<commit_message>
Missions: Content - Added mission type "kill_chain".
Former-commit-id: c61e4a58c9d0f3b8c27f8d9ab49033ce9b0cf369
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Missions.xlsx
+++ b/Docs/Content/HungryDragonContent_Missions.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10210"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hsemroud\Documents\Dragon\Docs\Content\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aortin/Documents/UBI/FD/Client/Docs/Content/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="10800"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="38300" windowHeight="19860"/>
   </bookViews>
   <sheets>
     <sheet name="missions" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="170">
   <si>
     <t>single_run</t>
   </si>
@@ -228,9 +228,6 @@
   </si>
   <si>
     <t>[tidDescSingleRun]</t>
-  </si>
-  <si>
-    <t>[canBeDuringOneRun]</t>
   </si>
   <si>
     <t>[weight]</t>
@@ -553,6 +550,15 @@
   </si>
   <si>
     <t>MISSIONS DEFINITIONS</t>
+  </si>
+  <si>
+    <t>[singleRunChance]</t>
+  </si>
+  <si>
+    <t>kill_chain</t>
+  </si>
+  <si>
+    <t>TID_MISSION_OBJECTIVE_KILL_CHAIN_DESC_SINGLE_RUN</t>
   </si>
 </sst>
 </file>
@@ -964,6 +970,16 @@
   </cellStyles>
   <dxfs count="67">
     <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -2022,16 +2038,6 @@
         </bottom>
       </border>
     </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -2046,94 +2052,94 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="missionDifficultyDefinitions" displayName="missionDifficultyDefinitions" ref="B47:K50" totalsRowShown="0" headerRowBorderDxfId="65" tableBorderDxfId="64">
-  <autoFilter ref="B47:K50"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="missionDifficultyDefinitions" displayName="missionDifficultyDefinitions" ref="B48:K51" totalsRowShown="0" headerRowBorderDxfId="66" tableBorderDxfId="65">
+  <autoFilter ref="B48:K51"/>
   <tableColumns count="10">
     <tableColumn id="1" name="{missionDifficultyDefinitions}"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="63"/>
-    <tableColumn id="7" name="[index]" dataDxfId="62"/>
-    <tableColumn id="3" name="[dragonsToUnlock]" dataDxfId="61"/>
-    <tableColumn id="4" name="[cooldownMinutes]" dataDxfId="60"/>
-    <tableColumn id="9" name="[maxRewardCoins]" dataDxfId="59"/>
-    <tableColumn id="5" name="[removeMissionPCCoefA]" dataDxfId="58"/>
-    <tableColumn id="6" name="[removeMissionPCCoefB]" dataDxfId="57"/>
-    <tableColumn id="8" name="[tidName]" dataDxfId="56"/>
-    <tableColumn id="10" name="[color]" dataDxfId="55"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="64"/>
+    <tableColumn id="7" name="[index]" dataDxfId="63"/>
+    <tableColumn id="3" name="[dragonsToUnlock]" dataDxfId="62"/>
+    <tableColumn id="4" name="[cooldownMinutes]" dataDxfId="61"/>
+    <tableColumn id="9" name="[maxRewardCoins]" dataDxfId="60"/>
+    <tableColumn id="5" name="[removeMissionPCCoefA]" dataDxfId="59"/>
+    <tableColumn id="6" name="[removeMissionPCCoefB]" dataDxfId="58"/>
+    <tableColumn id="8" name="[tidName]" dataDxfId="57"/>
+    <tableColumn id="10" name="[color]" dataDxfId="56"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table13303132" displayName="Table13303132" ref="B55:E65" totalsRowShown="0" headerRowDxfId="54" dataDxfId="52" headerRowBorderDxfId="53" tableBorderDxfId="51" totalsRowBorderDxfId="50">
-  <autoFilter ref="B55:E65"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table13303132" displayName="Table13303132" ref="B56:E66" totalsRowShown="0" headerRowDxfId="55" dataDxfId="53" headerRowBorderDxfId="54" tableBorderDxfId="52" totalsRowBorderDxfId="51">
+  <autoFilter ref="B56:E66"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="{missionDragonModifiersDefinitions}" dataDxfId="49"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="48"/>
-    <tableColumn id="7" name="[quantityModifier]" dataDxfId="47"/>
-    <tableColumn id="3" name="[missionSCRewardMultiplier]" dataDxfId="46"/>
+    <tableColumn id="1" name="{missionDragonModifiersDefinitions}" dataDxfId="50"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="49"/>
+    <tableColumn id="7" name="[quantityModifier]" dataDxfId="48"/>
+    <tableColumn id="3" name="[missionSCRewardMultiplier]" dataDxfId="47"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table1330313234" displayName="Table1330313234" ref="B69:D72" totalsRowShown="0" headerRowDxfId="45" dataDxfId="43" headerRowBorderDxfId="44" tableBorderDxfId="42" totalsRowBorderDxfId="41">
-  <autoFilter ref="B69:D72"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table1330313234" displayName="Table1330313234" ref="B70:D73" totalsRowShown="0" headerRowDxfId="46" dataDxfId="44" headerRowBorderDxfId="45" tableBorderDxfId="43" totalsRowBorderDxfId="42">
+  <autoFilter ref="B70:D73"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="{missionDifficultyModifiersDefinitions}" dataDxfId="40"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="39"/>
-    <tableColumn id="7" name="[quantityModifier]" dataDxfId="38"/>
+    <tableColumn id="1" name="{missionDifficultyModifiersDefinitions}" dataDxfId="41"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="40"/>
+    <tableColumn id="7" name="[quantityModifier]" dataDxfId="39"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table133031323435" displayName="Table133031323435" ref="B76:D77" totalsRowShown="0" headerRowDxfId="37" dataDxfId="35" headerRowBorderDxfId="36" tableBorderDxfId="34" totalsRowBorderDxfId="33">
-  <autoFilter ref="B76:D77"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table133031323435" displayName="Table133031323435" ref="B77:D78" totalsRowShown="0" headerRowDxfId="38" dataDxfId="36" headerRowBorderDxfId="37" tableBorderDxfId="35" totalsRowBorderDxfId="34">
+  <autoFilter ref="B77:D78"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="{missionOtherModifiersDefinitions}" dataDxfId="32"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="31"/>
-    <tableColumn id="7" name="[quantityModifier]" dataDxfId="30"/>
+    <tableColumn id="1" name="{missionOtherModifiersDefinitions}" dataDxfId="33"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="32"/>
+    <tableColumn id="7" name="[quantityModifier]" dataDxfId="31"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table13" displayName="Table13" ref="B35:I43" totalsRowShown="0" headerRowDxfId="29" dataDxfId="27" headerRowBorderDxfId="28" tableBorderDxfId="26" totalsRowBorderDxfId="25">
-  <autoFilter ref="B35:I43"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table13" displayName="Table13" ref="B35:I44" totalsRowShown="0" headerRowDxfId="30" dataDxfId="28" headerRowBorderDxfId="29" tableBorderDxfId="27" totalsRowBorderDxfId="26">
+  <autoFilter ref="B35:I44"/>
   <tableColumns count="8">
-    <tableColumn id="1" name="{missionTypeDefinitions}" dataDxfId="24"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="23"/>
-    <tableColumn id="3" name="[minTier]" dataDxfId="22"/>
-    <tableColumn id="6" name="[maxTier]" dataDxfId="21"/>
-    <tableColumn id="4" name="[weight]" dataDxfId="20"/>
-    <tableColumn id="5" name="[canBeDuringOneRun]" dataDxfId="19"/>
-    <tableColumn id="9" name="[tidDescSingleRun]" dataDxfId="18"/>
-    <tableColumn id="10" name="[tidDescMultiRun]" dataDxfId="17"/>
+    <tableColumn id="1" name="{missionTypeDefinitions}" dataDxfId="25"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="24"/>
+    <tableColumn id="3" name="[minTier]" dataDxfId="23"/>
+    <tableColumn id="6" name="[maxTier]" dataDxfId="22"/>
+    <tableColumn id="4" name="[weight]" dataDxfId="21"/>
+    <tableColumn id="5" name="[singleRunChance]" dataDxfId="20"/>
+    <tableColumn id="9" name="[tidDescSingleRun]" dataDxfId="19"/>
+    <tableColumn id="10" name="[tidDescMultiRun]" dataDxfId="18"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table1330" displayName="Table1330" ref="B4:M31" totalsRowShown="0" headerRowDxfId="16" dataDxfId="14" headerRowBorderDxfId="15" tableBorderDxfId="13" totalsRowBorderDxfId="12">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table1330" displayName="Table1330" ref="B4:M31" totalsRowShown="0" headerRowDxfId="17" dataDxfId="15" headerRowBorderDxfId="16" tableBorderDxfId="14" totalsRowBorderDxfId="13">
   <autoFilter ref="B4:M31"/>
   <tableColumns count="12">
-    <tableColumn id="1" name="{missionsDefinitions}" dataDxfId="11"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="10"/>
-    <tableColumn id="7" name="[type]" dataDxfId="9"/>
-    <tableColumn id="8" name="[weight]" dataDxfId="8"/>
-    <tableColumn id="11" name="[minTier]" dataDxfId="7"/>
-    <tableColumn id="12" name="[maxTier]" dataDxfId="6"/>
-    <tableColumn id="6" name="[params]" dataDxfId="5"/>
-    <tableColumn id="3" name="[objectiveBaseQuantityMin]" dataDxfId="4"/>
-    <tableColumn id="9" name="[objectiveBaseQuantityMax]" dataDxfId="3"/>
-    <tableColumn id="4" name="[icon]" dataDxfId="2"/>
-    <tableColumn id="5" name="[tidObjective]" dataDxfId="1"/>
-    <tableColumn id="10" name="[trackingSku]" dataDxfId="0"/>
+    <tableColumn id="1" name="{missionsDefinitions}" dataDxfId="12"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="11"/>
+    <tableColumn id="7" name="[type]" dataDxfId="10"/>
+    <tableColumn id="8" name="[weight]" dataDxfId="9"/>
+    <tableColumn id="11" name="[minTier]" dataDxfId="8"/>
+    <tableColumn id="12" name="[maxTier]" dataDxfId="7"/>
+    <tableColumn id="6" name="[params]" dataDxfId="6"/>
+    <tableColumn id="3" name="[objectiveBaseQuantityMin]" dataDxfId="5"/>
+    <tableColumn id="9" name="[objectiveBaseQuantityMax]" dataDxfId="4"/>
+    <tableColumn id="4" name="[icon]" dataDxfId="3"/>
+    <tableColumn id="5" name="[tidObjective]" dataDxfId="2"/>
+    <tableColumn id="10" name="[trackingSku]" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2405,34 +2411,34 @@
   <sheetPr>
     <tabColor theme="6"/>
   </sheetPr>
-  <dimension ref="B1:P77"/>
+  <dimension ref="B1:P78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="E42" sqref="E42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="3.7109375" customWidth="1"/>
-    <col min="2" max="2" width="59.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.6640625" customWidth="1"/>
+    <col min="2" max="2" width="59.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="36" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="42.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="58.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="42.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="58.6640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="60" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="49.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="49.5" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="52" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="28.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="28.83203125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="15" customWidth="1"/>
-    <col min="14" max="14" width="23.85546875" customWidth="1"/>
+    <col min="14" max="14" width="23.83203125" customWidth="1"/>
     <col min="15" max="16" width="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:16" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:16" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="2:16" ht="24" x14ac:dyDescent="0.3">
       <c r="B2" s="6" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C2" s="6"/>
       <c r="D2" s="6"/>
@@ -2445,19 +2451,19 @@
       <c r="K2" s="6"/>
       <c r="L2" s="6"/>
     </row>
-    <row r="3" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B3" s="20"/>
       <c r="C3" s="39"/>
       <c r="D3" s="39"/>
       <c r="E3" s="40" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="F3" s="40" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="G3" s="39"/>
       <c r="J3" s="41" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="K3" s="41"/>
       <c r="M3" s="41"/>
@@ -2465,50 +2471,50 @@
       <c r="O3" s="41"/>
       <c r="P3" s="41"/>
     </row>
-    <row r="4" spans="2:16" ht="107.25" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:16" ht="103" x14ac:dyDescent="0.2">
       <c r="B4" s="31" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C4" s="28" t="s">
         <v>3</v>
       </c>
       <c r="D4" s="38" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E4" s="38" t="s">
+        <v>68</v>
+      </c>
+      <c r="F4" s="38" t="s">
+        <v>70</v>
+      </c>
+      <c r="G4" s="38" t="s">
         <v>69</v>
       </c>
-      <c r="F4" s="38" t="s">
-        <v>71</v>
-      </c>
-      <c r="G4" s="38" t="s">
-        <v>70</v>
-      </c>
       <c r="H4" s="38" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="I4" s="38" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="J4" s="38" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="K4" s="37" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="L4" s="37" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="M4" s="36" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="5" spans="2:16" x14ac:dyDescent="0.25">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="5" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B5" s="27" t="s">
         <v>1</v>
       </c>
       <c r="C5" s="24" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D5" s="24" t="s">
         <v>65</v>
@@ -2523,7 +2529,7 @@
         <v>7</v>
       </c>
       <c r="H5" s="24" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="I5" s="24">
         <v>500</v>
@@ -2532,21 +2538,21 @@
         <v>600</v>
       </c>
       <c r="K5" s="34" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="L5" s="34" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="M5" s="32" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="6" spans="2:16" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="6" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B6" s="27" t="s">
         <v>1</v>
       </c>
       <c r="C6" s="24" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D6" s="23" t="s">
         <v>53</v>
@@ -2568,19 +2574,19 @@
         <v>600</v>
       </c>
       <c r="K6" s="34" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="L6" s="34"/>
       <c r="M6" s="32" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="7" spans="2:16" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="7" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B7" s="27" t="s">
         <v>1</v>
       </c>
       <c r="C7" s="24" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D7" s="24" t="s">
         <v>59</v>
@@ -2602,19 +2608,19 @@
         <v>10000</v>
       </c>
       <c r="K7" s="34" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="L7" s="34"/>
       <c r="M7" s="32" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="8" spans="2:16" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="8" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B8" s="27" t="s">
         <v>1</v>
       </c>
       <c r="C8" s="24" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D8" s="24" t="s">
         <v>65</v>
@@ -2629,7 +2635,7 @@
         <v>7</v>
       </c>
       <c r="H8" s="24" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="I8" s="24">
         <v>700</v>
@@ -2638,21 +2644,21 @@
         <v>750</v>
       </c>
       <c r="K8" s="34" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="L8" s="34" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="M8" s="32" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="9" spans="2:16" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="9" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B9" s="27" t="s">
         <v>1</v>
       </c>
       <c r="C9" s="24" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D9" s="24" t="s">
         <v>65</v>
@@ -2667,7 +2673,7 @@
         <v>7</v>
       </c>
       <c r="H9" s="24" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="I9" s="24">
         <v>25</v>
@@ -2676,21 +2682,21 @@
         <v>30</v>
       </c>
       <c r="K9" s="34" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="L9" s="34" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="M9" s="32" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="10" spans="2:16" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="10" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B10" s="27" t="s">
         <v>1</v>
       </c>
       <c r="C10" s="24" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D10" s="23" t="s">
         <v>56</v>
@@ -2705,7 +2711,7 @@
         <v>3</v>
       </c>
       <c r="H10" s="23" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="I10" s="24">
         <v>10</v>
@@ -2714,21 +2720,21 @@
         <v>12</v>
       </c>
       <c r="K10" s="34" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="L10" s="34" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="M10" s="32" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="11" spans="2:16" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="11" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B11" s="27" t="s">
         <v>1</v>
       </c>
       <c r="C11" s="24" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D11" s="23" t="s">
         <v>56</v>
@@ -2743,7 +2749,7 @@
         <v>7</v>
       </c>
       <c r="H11" s="23" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="I11" s="24">
         <v>8</v>
@@ -2752,21 +2758,21 @@
         <v>9</v>
       </c>
       <c r="K11" s="34" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="L11" s="34" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="M11" s="32" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="12" spans="2:16" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="12" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B12" s="27" t="s">
         <v>1</v>
       </c>
       <c r="C12" s="24" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D12" s="24" t="s">
         <v>50</v>
@@ -2781,7 +2787,7 @@
         <v>7</v>
       </c>
       <c r="H12" s="24" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="I12" s="24">
         <v>1000</v>
@@ -2790,21 +2796,21 @@
         <v>1200</v>
       </c>
       <c r="K12" s="34" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="L12" s="34" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="M12" s="32" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="13" spans="2:16" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="13" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B13" s="25" t="s">
         <v>1</v>
       </c>
       <c r="C13" s="23" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D13" s="24" t="s">
         <v>50</v>
@@ -2819,7 +2825,7 @@
         <v>1</v>
       </c>
       <c r="H13" s="23" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="I13" s="24">
         <v>1</v>
@@ -2828,21 +2834,21 @@
         <v>2</v>
       </c>
       <c r="K13" s="34" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="L13" s="34" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="M13" s="32" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="14" spans="2:16" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="14" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B14" s="25" t="s">
         <v>1</v>
       </c>
       <c r="C14" s="24" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D14" s="24" t="s">
         <v>65</v>
@@ -2857,7 +2863,7 @@
         <v>7</v>
       </c>
       <c r="H14" s="24" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="I14" s="24">
         <v>10</v>
@@ -2866,21 +2872,21 @@
         <v>11</v>
       </c>
       <c r="K14" s="34" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="L14" s="34" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="M14" s="32" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="15" spans="2:16" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="15" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B15" s="25" t="s">
         <v>1</v>
       </c>
       <c r="C15" s="24" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D15" s="24" t="s">
         <v>62</v>
@@ -2902,14 +2908,14 @@
         <v>6</v>
       </c>
       <c r="K15" s="34" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="L15" s="34"/>
       <c r="M15" s="32" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="16" spans="2:16" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="16" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B16" s="25" t="s">
         <v>1</v>
       </c>
@@ -2936,14 +2942,14 @@
         <v>800</v>
       </c>
       <c r="K16" s="34" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="L16" s="34"/>
       <c r="M16" s="32" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="17" spans="2:13" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="17" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B17" s="25" t="s">
         <v>1</v>
       </c>
@@ -2970,14 +2976,14 @@
         <v>400</v>
       </c>
       <c r="K17" s="34" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="L17" s="34"/>
       <c r="M17" s="32" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="18" spans="2:13" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="18" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B18" s="25" t="s">
         <v>1</v>
       </c>
@@ -3004,19 +3010,19 @@
         <v>500000</v>
       </c>
       <c r="K18" s="34" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="L18" s="34"/>
       <c r="M18" s="32" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="19" spans="2:13" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="19" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B19" s="25" t="s">
         <v>1</v>
       </c>
       <c r="C19" s="23" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D19" s="23" t="s">
         <v>65</v>
@@ -3031,7 +3037,7 @@
         <v>7</v>
       </c>
       <c r="H19" s="23" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="I19" s="24">
         <v>45</v>
@@ -3040,21 +3046,21 @@
         <v>55</v>
       </c>
       <c r="K19" s="35" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="L19" s="34" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="M19" s="32" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="20" spans="2:13" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="20" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B20" s="25" t="s">
         <v>1</v>
       </c>
       <c r="C20" s="23" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D20" s="23" t="s">
         <v>65</v>
@@ -3069,7 +3075,7 @@
         <v>7</v>
       </c>
       <c r="H20" s="23" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="I20" s="24">
         <v>40</v>
@@ -3078,21 +3084,21 @@
         <v>45</v>
       </c>
       <c r="K20" s="35" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="L20" s="34" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="M20" s="32" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="21" spans="2:13" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="21" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B21" s="25" t="s">
         <v>1</v>
       </c>
       <c r="C21" s="23" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D21" s="23" t="s">
         <v>65</v>
@@ -3107,7 +3113,7 @@
         <v>2</v>
       </c>
       <c r="H21" s="23" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="I21" s="23">
         <v>10</v>
@@ -3116,21 +3122,21 @@
         <v>12</v>
       </c>
       <c r="K21" s="35" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="L21" s="35" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="M21" s="32" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="22" spans="2:13" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="22" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B22" s="27" t="s">
         <v>1</v>
       </c>
       <c r="C22" s="24" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D22" s="23" t="s">
         <v>65</v>
@@ -3145,7 +3151,7 @@
         <v>1</v>
       </c>
       <c r="H22" s="23" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="I22" s="24">
         <v>5</v>
@@ -3154,21 +3160,21 @@
         <v>6</v>
       </c>
       <c r="K22" s="35" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="L22" s="35" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="M22" s="32" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="23" spans="2:13" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="23" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B23" s="27" t="s">
         <v>1</v>
       </c>
       <c r="C23" s="24" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D23" s="23" t="s">
         <v>65</v>
@@ -3183,7 +3189,7 @@
         <v>7</v>
       </c>
       <c r="H23" s="23" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="I23" s="24">
         <v>150</v>
@@ -3192,21 +3198,21 @@
         <v>200</v>
       </c>
       <c r="K23" s="35" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="L23" s="35" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="M23" s="32" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="24" spans="2:13" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="24" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B24" s="27" t="s">
         <v>1</v>
       </c>
       <c r="C24" s="24" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D24" s="23" t="s">
         <v>65</v>
@@ -3221,7 +3227,7 @@
         <v>7</v>
       </c>
       <c r="H24" s="23" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="I24" s="24">
         <v>5</v>
@@ -3230,21 +3236,21 @@
         <v>7</v>
       </c>
       <c r="K24" s="35" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="L24" s="35" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="M24" s="32" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="25" spans="2:13" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="25" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B25" s="27" t="s">
         <v>1</v>
       </c>
       <c r="C25" s="24" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D25" s="23" t="s">
         <v>65</v>
@@ -3259,7 +3265,7 @@
         <v>7</v>
       </c>
       <c r="H25" s="23" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="I25" s="24">
         <v>5</v>
@@ -3268,21 +3274,21 @@
         <v>7</v>
       </c>
       <c r="K25" s="35" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="L25" s="35" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="M25" s="32" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="26" spans="2:13" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="26" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B26" s="27" t="s">
         <v>1</v>
       </c>
       <c r="C26" s="24" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D26" s="23" t="s">
         <v>65</v>
@@ -3297,7 +3303,7 @@
         <v>7</v>
       </c>
       <c r="H26" s="23" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="I26" s="24">
         <v>3</v>
@@ -3306,21 +3312,21 @@
         <v>4</v>
       </c>
       <c r="K26" s="35" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="L26" s="35" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="M26" s="32" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="27" spans="2:13" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="27" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B27" s="27" t="s">
         <v>1</v>
       </c>
       <c r="C27" s="24" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D27" s="23" t="s">
         <v>65</v>
@@ -3335,7 +3341,7 @@
         <v>7</v>
       </c>
       <c r="H27" s="23" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="I27" s="24">
         <v>3</v>
@@ -3344,21 +3350,21 @@
         <v>3.5</v>
       </c>
       <c r="K27" s="35" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="L27" s="35" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="M27" s="32" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="28" spans="2:13" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="28" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B28" s="27" t="s">
         <v>1</v>
       </c>
       <c r="C28" s="24" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D28" s="23" t="s">
         <v>65</v>
@@ -3373,7 +3379,7 @@
         <v>7</v>
       </c>
       <c r="H28" s="23" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="I28" s="24">
         <v>8</v>
@@ -3382,21 +3388,21 @@
         <v>9</v>
       </c>
       <c r="K28" s="35" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="L28" s="35" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="M28" s="32" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="29" spans="2:13" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="29" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B29" s="27" t="s">
         <v>1</v>
       </c>
       <c r="C29" s="24" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D29" s="23" t="s">
         <v>65</v>
@@ -3411,7 +3417,7 @@
         <v>7</v>
       </c>
       <c r="H29" s="23" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="I29" s="24">
         <v>11</v>
@@ -3420,21 +3426,21 @@
         <v>12</v>
       </c>
       <c r="K29" s="35" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="L29" s="35" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="M29" s="32" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="30" spans="2:13" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="30" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B30" s="27" t="s">
         <v>1</v>
       </c>
       <c r="C30" s="24" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D30" s="23" t="s">
         <v>65</v>
@@ -3449,7 +3455,7 @@
         <v>7</v>
       </c>
       <c r="H30" s="23" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="I30" s="24">
         <v>3</v>
@@ -3458,16 +3464,16 @@
         <v>3.5</v>
       </c>
       <c r="K30" s="35" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="L30" s="35" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="M30" s="32" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="31" spans="2:13" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="31" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B31" s="27" t="s">
         <v>1</v>
       </c>
@@ -3494,14 +3500,14 @@
         <v>7000</v>
       </c>
       <c r="K31" s="34" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="L31" s="34"/>
       <c r="M31" s="32" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="32" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="32" spans="2:13" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B32" s="33"/>
       <c r="C32" s="33"/>
       <c r="D32" s="33"/>
@@ -3515,9 +3521,9 @@
       <c r="L32" s="33"/>
       <c r="M32" s="32"/>
     </row>
-    <row r="33" spans="2:13" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="33" spans="2:13" ht="24" x14ac:dyDescent="0.3">
       <c r="B33" s="6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C33" s="6"/>
       <c r="D33" s="6"/>
@@ -3530,7 +3536,7 @@
       <c r="K33" s="6"/>
       <c r="L33" s="6"/>
     </row>
-    <row r="34" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B34" s="20"/>
       <c r="C34" s="20"/>
       <c r="D34" s="20"/>
@@ -3541,24 +3547,24 @@
       <c r="I34" s="20"/>
       <c r="J34" s="20"/>
     </row>
-    <row r="35" spans="2:13" ht="96" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:13" ht="96" x14ac:dyDescent="0.2">
       <c r="B35" s="31" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C35" s="28" t="s">
         <v>3</v>
       </c>
       <c r="D35" s="30" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E35" s="30" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F35" s="30" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G35" s="29" t="s">
-        <v>68</v>
+        <v>167</v>
       </c>
       <c r="H35" s="28" t="s">
         <v>67</v>
@@ -3567,7 +3573,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="36" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B36" s="27" t="s">
         <v>1</v>
       </c>
@@ -3583,8 +3589,8 @@
       <c r="F36" s="24">
         <v>2</v>
       </c>
-      <c r="G36" s="26" t="b">
-        <v>1</v>
+      <c r="G36" s="26">
+        <v>0.3</v>
       </c>
       <c r="H36" s="26" t="s">
         <v>64</v>
@@ -3593,7 +3599,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="37" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B37" s="27" t="s">
         <v>1</v>
       </c>
@@ -3609,8 +3615,8 @@
       <c r="F37" s="24">
         <v>1</v>
       </c>
-      <c r="G37" s="26" t="b">
-        <v>1</v>
+      <c r="G37" s="26">
+        <v>0.3</v>
       </c>
       <c r="H37" s="26" t="s">
         <v>61</v>
@@ -3619,7 +3625,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="38" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B38" s="27" t="s">
         <v>1</v>
       </c>
@@ -3635,8 +3641,8 @@
       <c r="F38" s="24">
         <v>2</v>
       </c>
-      <c r="G38" s="26" t="b">
-        <v>1</v>
+      <c r="G38" s="26">
+        <v>0.3</v>
       </c>
       <c r="H38" s="26" t="s">
         <v>58</v>
@@ -3645,7 +3651,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="39" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B39" s="27" t="s">
         <v>1</v>
       </c>
@@ -3661,7 +3667,7 @@
       <c r="F39" s="24">
         <v>1</v>
       </c>
-      <c r="G39" s="26" t="b">
+      <c r="G39" s="26">
         <v>0</v>
       </c>
       <c r="H39" s="26" t="s">
@@ -3671,7 +3677,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="40" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B40" s="25" t="s">
         <v>1</v>
       </c>
@@ -3687,7 +3693,7 @@
       <c r="F40" s="23">
         <v>1</v>
       </c>
-      <c r="G40" s="26" t="b">
+      <c r="G40" s="26">
         <v>0</v>
       </c>
       <c r="H40" s="26" t="s">
@@ -3697,7 +3703,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="41" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B41" s="25" t="s">
         <v>1</v>
       </c>
@@ -3713,7 +3719,7 @@
       <c r="F41" s="24">
         <v>1</v>
       </c>
-      <c r="G41" s="26" t="b">
+      <c r="G41" s="26">
         <v>0</v>
       </c>
       <c r="H41" s="26" t="s">
@@ -3723,7 +3729,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="42" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B42" s="25" t="s">
         <v>1</v>
       </c>
@@ -3739,8 +3745,8 @@
       <c r="F42" s="24">
         <v>1</v>
       </c>
-      <c r="G42" s="26" t="b">
-        <v>1</v>
+      <c r="G42" s="26">
+        <v>0.3</v>
       </c>
       <c r="H42" s="26" t="s">
         <v>46</v>
@@ -3749,7 +3755,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="43" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B43" s="25" t="s">
         <v>1</v>
       </c>
@@ -3765,7 +3771,7 @@
       <c r="F43" s="23">
         <v>1</v>
       </c>
-      <c r="G43" s="22" t="b">
+      <c r="G43" s="22">
         <v>0</v>
       </c>
       <c r="H43" s="22" t="s">
@@ -3775,119 +3781,111 @@
         <v>42</v>
       </c>
     </row>
-    <row r="44" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="45" spans="2:13" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B45" s="6" t="s">
+    <row r="44" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B44" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="C44" s="23" t="s">
+        <v>168</v>
+      </c>
+      <c r="D44" s="23">
+        <v>0</v>
+      </c>
+      <c r="E44" s="24">
+        <v>7</v>
+      </c>
+      <c r="F44" s="23">
+        <v>1</v>
+      </c>
+      <c r="G44" s="22">
+        <v>1</v>
+      </c>
+      <c r="H44" s="26" t="s">
+        <v>169</v>
+      </c>
+      <c r="I44" s="26"/>
+    </row>
+    <row r="45" spans="2:13" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="46" spans="2:13" ht="24" x14ac:dyDescent="0.3">
+      <c r="B46" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="C45" s="6"/>
-      <c r="D45" s="6"/>
-      <c r="E45" s="6"/>
-      <c r="F45" s="6"/>
-      <c r="G45" s="6"/>
-      <c r="H45" s="6"/>
-      <c r="I45" s="6"/>
-      <c r="J45" s="6"/>
-      <c r="K45" s="6"/>
-      <c r="L45" s="6"/>
-      <c r="M45" s="6"/>
-    </row>
-    <row r="46" spans="2:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="B46" s="20"/>
-      <c r="C46" s="20"/>
-      <c r="D46" s="20"/>
-      <c r="E46" s="20"/>
-      <c r="F46" s="21" t="s">
+      <c r="C46" s="6"/>
+      <c r="D46" s="6"/>
+      <c r="E46" s="6"/>
+      <c r="F46" s="6"/>
+      <c r="G46" s="6"/>
+      <c r="H46" s="6"/>
+      <c r="I46" s="6"/>
+      <c r="J46" s="6"/>
+      <c r="K46" s="6"/>
+      <c r="L46" s="6"/>
+      <c r="M46" s="6"/>
+    </row>
+    <row r="47" spans="2:13" ht="30" x14ac:dyDescent="0.2">
+      <c r="B47" s="20"/>
+      <c r="C47" s="20"/>
+      <c r="D47" s="20"/>
+      <c r="E47" s="20"/>
+      <c r="F47" s="21" t="s">
         <v>40</v>
       </c>
-      <c r="G46" s="43" t="s">
+      <c r="G47" s="43" t="s">
         <v>39</v>
       </c>
-      <c r="H46" s="43"/>
-      <c r="I46" s="20"/>
-    </row>
-    <row r="47" spans="2:13" ht="142.5" x14ac:dyDescent="0.25">
-      <c r="B47" s="19" t="s">
+      <c r="H47" s="43"/>
+      <c r="I47" s="20"/>
+    </row>
+    <row r="48" spans="2:13" ht="137" x14ac:dyDescent="0.2">
+      <c r="B48" s="19" t="s">
         <v>38</v>
       </c>
-      <c r="C47" s="19" t="s">
+      <c r="C48" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="D47" s="18" t="s">
+      <c r="D48" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="E47" s="17" t="s">
+      <c r="E48" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="F47" s="17" t="s">
+      <c r="F48" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="G47" s="17" t="s">
+      <c r="G48" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="H47" s="16" t="s">
+      <c r="H48" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="I47" s="16" t="s">
+      <c r="I48" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="J47" s="15" t="s">
+      <c r="J48" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="K47" s="14" t="s">
+      <c r="K48" s="14" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="48" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B48" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="C48" s="11" t="s">
+    <row r="49" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B49" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="C49" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="D48" s="11">
+      <c r="D49" s="11">
         <v>0</v>
-      </c>
-      <c r="E48" s="10">
-        <v>0</v>
-      </c>
-      <c r="F48" s="10">
-        <v>15</v>
-      </c>
-      <c r="G48" s="10">
-        <v>200</v>
-      </c>
-      <c r="H48" s="9">
-        <v>0.5</v>
-      </c>
-      <c r="I48" s="9">
-        <v>1</v>
-      </c>
-      <c r="J48" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="K48" s="13" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="49" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B49" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="C49" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="D49" s="11">
-        <v>1</v>
       </c>
       <c r="E49" s="10">
         <v>0</v>
       </c>
       <c r="F49" s="10">
-        <v>60</v>
+        <v>15</v>
       </c>
       <c r="G49" s="10">
-        <v>300</v>
+        <v>200</v>
       </c>
       <c r="H49" s="9">
         <v>0.5</v>
@@ -3896,30 +3894,30 @@
         <v>1</v>
       </c>
       <c r="J49" s="8" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="K49" s="13" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="50" spans="2:11" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="50" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B50" s="12" t="s">
         <v>1</v>
       </c>
       <c r="C50" s="11" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D50" s="11">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E50" s="10">
         <v>0</v>
       </c>
       <c r="F50" s="10">
-        <v>240</v>
+        <v>60</v>
       </c>
       <c r="G50" s="10">
-        <v>600</v>
+        <v>300</v>
       </c>
       <c r="H50" s="9">
         <v>0.5</v>
@@ -3928,262 +3926,294 @@
         <v>1</v>
       </c>
       <c r="J50" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="K50" s="13" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="51" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B51" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="C51" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="D51" s="11">
+        <v>2</v>
+      </c>
+      <c r="E51" s="10">
+        <v>0</v>
+      </c>
+      <c r="F51" s="10">
+        <v>240</v>
+      </c>
+      <c r="G51" s="10">
+        <v>600</v>
+      </c>
+      <c r="H51" s="9">
+        <v>0.5</v>
+      </c>
+      <c r="I51" s="9">
+        <v>1</v>
+      </c>
+      <c r="J51" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="K50" s="7" t="s">
+      <c r="K51" s="7" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="52" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="53" spans="2:11" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B53" s="6" t="s">
+    <row r="53" spans="2:11" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="54" spans="2:11" ht="24" x14ac:dyDescent="0.3">
+      <c r="B54" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="C53" s="6"/>
-      <c r="D53" s="6"/>
-      <c r="E53" s="6"/>
-      <c r="F53" s="6"/>
-      <c r="G53" s="6"/>
-    </row>
-    <row r="55" spans="2:11" ht="135.75" x14ac:dyDescent="0.25">
-      <c r="B55" s="5" t="s">
+      <c r="C54" s="6"/>
+      <c r="D54" s="6"/>
+      <c r="E54" s="6"/>
+      <c r="F54" s="6"/>
+      <c r="G54" s="6"/>
+    </row>
+    <row r="56" spans="2:11" ht="135" x14ac:dyDescent="0.2">
+      <c r="B56" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="C55" s="4" t="s">
+      <c r="C56" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D55" s="3" t="s">
+      <c r="D56" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E55" s="3" t="s">
+      <c r="E56" s="3" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="56" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B56" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C56" s="1" t="s">
+    <row r="57" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B57" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C57" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D56" s="1">
+      <c r="D57" s="1">
         <v>0.1</v>
       </c>
-      <c r="E56" s="1">
+      <c r="E57" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="57" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B57" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C57" s="1" t="s">
+    <row r="58" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B58" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C58" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D57" s="1">
+      <c r="D58" s="1">
         <v>0.7</v>
       </c>
-      <c r="E57" s="1">
+      <c r="E58" s="1">
         <v>6</v>
       </c>
     </row>
-    <row r="58" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B58" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C58" s="1" t="s">
+    <row r="59" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B59" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C59" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D58" s="1">
-        <v>1</v>
-      </c>
-      <c r="E58" s="1">
+      <c r="D59" s="1">
+        <v>1</v>
+      </c>
+      <c r="E59" s="1">
         <v>12</v>
       </c>
     </row>
-    <row r="59" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B59" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C59" s="1" t="s">
+    <row r="60" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B60" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C60" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D59" s="1">
+      <c r="D60" s="1">
         <v>1.5</v>
       </c>
-      <c r="E59" s="1">
+      <c r="E60" s="1">
         <v>18</v>
       </c>
     </row>
-    <row r="60" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B60" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C60" s="1" t="s">
+    <row r="61" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B61" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C61" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D60" s="1">
+      <c r="D61" s="1">
         <v>2</v>
       </c>
-      <c r="E60" s="1">
+      <c r="E61" s="1">
         <v>26</v>
       </c>
     </row>
-    <row r="61" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B61" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C61" s="1" t="s">
+    <row r="62" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B62" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C62" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D61" s="1">
+      <c r="D62" s="1">
         <v>2.5</v>
       </c>
-      <c r="E61" s="1">
+      <c r="E62" s="1">
         <v>35</v>
       </c>
     </row>
-    <row r="62" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B62" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C62" s="1" t="s">
+    <row r="63" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B63" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C63" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D62" s="1">
+      <c r="D63" s="1">
         <v>3</v>
       </c>
-      <c r="E62" s="1">
+      <c r="E63" s="1">
         <v>45</v>
       </c>
     </row>
-    <row r="63" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B63" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C63" s="1" t="s">
+    <row r="64" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B64" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C64" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D63" s="1">
+      <c r="D64" s="1">
         <v>4</v>
       </c>
-      <c r="E63" s="1">
+      <c r="E64" s="1">
         <v>56</v>
       </c>
     </row>
-    <row r="64" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B64" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C64" s="1" t="s">
+    <row r="65" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B65" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C65" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D64" s="1">
+      <c r="D65" s="1">
         <v>5</v>
       </c>
-      <c r="E64" s="1">
+      <c r="E65" s="1">
         <v>67</v>
       </c>
     </row>
-    <row r="65" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B65" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C65" s="1" t="s">
+    <row r="66" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B66" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C66" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D65" s="1">
+      <c r="D66" s="1">
         <v>7</v>
       </c>
-      <c r="E65" s="1">
+      <c r="E66" s="1">
         <v>80</v>
       </c>
     </row>
-    <row r="66" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="67" spans="2:7" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B67" s="6" t="s">
+    <row r="67" spans="2:7" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="68" spans="2:7" ht="24" x14ac:dyDescent="0.3">
+      <c r="B68" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C67" s="6"/>
-      <c r="D67" s="6"/>
-      <c r="E67" s="6"/>
-      <c r="F67" s="6"/>
-      <c r="G67" s="6"/>
-    </row>
-    <row r="69" spans="2:7" ht="142.5" x14ac:dyDescent="0.25">
-      <c r="B69" s="5" t="s">
+      <c r="C68" s="6"/>
+      <c r="D68" s="6"/>
+      <c r="E68" s="6"/>
+      <c r="F68" s="6"/>
+      <c r="G68" s="6"/>
+    </row>
+    <row r="70" spans="2:7" ht="142" x14ac:dyDescent="0.2">
+      <c r="B70" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C69" s="4" t="s">
+      <c r="C70" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D69" s="3" t="s">
+      <c r="D70" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="70" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B70" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C70" s="1" t="s">
+    <row r="71" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B71" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C71" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D70" s="1">
+      <c r="D71" s="1">
         <v>0.05</v>
       </c>
     </row>
-    <row r="71" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B71" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C71" s="1" t="s">
+    <row r="72" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B72" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C72" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D71" s="1">
+      <c r="D72" s="1">
         <v>0.1</v>
       </c>
     </row>
-    <row r="72" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B72" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C72" s="1" t="s">
+    <row r="73" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B73" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C73" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D72" s="1">
+      <c r="D73" s="1">
         <v>0.2</v>
       </c>
     </row>
-    <row r="73" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="74" spans="2:7" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B74" s="6" t="s">
+    <row r="74" spans="2:7" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="75" spans="2:7" ht="24" x14ac:dyDescent="0.3">
+      <c r="B75" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C74" s="6"/>
-      <c r="D74" s="6"/>
-      <c r="E74" s="6"/>
-      <c r="F74" s="6"/>
-      <c r="G74" s="6"/>
-    </row>
-    <row r="76" spans="2:7" ht="132" x14ac:dyDescent="0.25">
-      <c r="B76" s="5" t="s">
+      <c r="C75" s="6"/>
+      <c r="D75" s="6"/>
+      <c r="E75" s="6"/>
+      <c r="F75" s="6"/>
+      <c r="G75" s="6"/>
+    </row>
+    <row r="77" spans="2:7" ht="131" x14ac:dyDescent="0.2">
+      <c r="B77" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C76" s="4" t="s">
+      <c r="C77" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D76" s="3" t="s">
+      <c r="D77" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="77" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B77" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C77" s="1" t="s">
+    <row r="78" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B78" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C78" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D77" s="1">
+      <c r="D78" s="1">
         <v>0.7</v>
       </c>
     </row>
@@ -4192,10 +4222,10 @@
     <mergeCell ref="J3:K3"/>
     <mergeCell ref="M3:P3"/>
     <mergeCell ref="F34:H34"/>
-    <mergeCell ref="G46:H46"/>
+    <mergeCell ref="G47:H47"/>
   </mergeCells>
-  <conditionalFormatting sqref="C48:D50">
-    <cfRule type="duplicateValues" dxfId="66" priority="1"/>
+  <conditionalFormatting sqref="C49:D51">
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Missions: Content - Added kill_chain_birds mission. Moved "singleRunChance" column from missionTypeDefinitions to missionDefinitions table.
Former-commit-id: cc6b651af50f7e535977e606decb75612791f2ab
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Missions.xlsx
+++ b/Docs/Content/HungryDragonContent_Missions.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="171">
   <si>
     <t>single_run</t>
   </si>
@@ -559,6 +559,9 @@
   </si>
   <si>
     <t>TID_MISSION_OBJECTIVE_KILL_CHAIN_DESC_SINGLE_RUN</t>
+  </si>
+  <si>
+    <t>kill_chain_birds</t>
   </si>
 </sst>
 </file>
@@ -705,7 +708,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -835,17 +838,6 @@
       <left style="thin">
         <color auto="1"/>
       </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
       <right style="thin">
         <color auto="1"/>
       </right>
@@ -857,7 +849,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1"/>
@@ -921,9 +913,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="45"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="45"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="45"/>
     </xf>
@@ -939,7 +928,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
@@ -981,6 +970,23 @@
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -1235,21 +1241,6 @@
         <bottom/>
         <vertical/>
         <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
       </border>
     </dxf>
     <dxf>
@@ -2052,8 +2043,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="missionDifficultyDefinitions" displayName="missionDifficultyDefinitions" ref="B48:K51" totalsRowShown="0" headerRowBorderDxfId="66" tableBorderDxfId="65">
-  <autoFilter ref="B48:K51"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="missionDifficultyDefinitions" displayName="missionDifficultyDefinitions" ref="B49:K52" totalsRowShown="0" headerRowBorderDxfId="66" tableBorderDxfId="65">
+  <autoFilter ref="B49:K52"/>
   <tableColumns count="10">
     <tableColumn id="1" name="{missionDifficultyDefinitions}"/>
     <tableColumn id="2" name="[sku]" dataDxfId="64"/>
@@ -2071,8 +2062,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table13303132" displayName="Table13303132" ref="B56:E66" totalsRowShown="0" headerRowDxfId="55" dataDxfId="53" headerRowBorderDxfId="54" tableBorderDxfId="52" totalsRowBorderDxfId="51">
-  <autoFilter ref="B56:E66"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table13303132" displayName="Table13303132" ref="B57:E67" totalsRowShown="0" headerRowDxfId="55" dataDxfId="53" headerRowBorderDxfId="54" tableBorderDxfId="52" totalsRowBorderDxfId="51">
+  <autoFilter ref="B57:E67"/>
   <tableColumns count="4">
     <tableColumn id="1" name="{missionDragonModifiersDefinitions}" dataDxfId="50"/>
     <tableColumn id="2" name="[sku]" dataDxfId="49"/>
@@ -2084,8 +2075,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table1330313234" displayName="Table1330313234" ref="B70:D73" totalsRowShown="0" headerRowDxfId="46" dataDxfId="44" headerRowBorderDxfId="45" tableBorderDxfId="43" totalsRowBorderDxfId="42">
-  <autoFilter ref="B70:D73"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table1330313234" displayName="Table1330313234" ref="B71:D74" totalsRowShown="0" headerRowDxfId="46" dataDxfId="44" headerRowBorderDxfId="45" tableBorderDxfId="43" totalsRowBorderDxfId="42">
+  <autoFilter ref="B71:D74"/>
   <tableColumns count="3">
     <tableColumn id="1" name="{missionDifficultyModifiersDefinitions}" dataDxfId="41"/>
     <tableColumn id="2" name="[sku]" dataDxfId="40"/>
@@ -2096,8 +2087,8 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table133031323435" displayName="Table133031323435" ref="B77:D78" totalsRowShown="0" headerRowDxfId="38" dataDxfId="36" headerRowBorderDxfId="37" tableBorderDxfId="35" totalsRowBorderDxfId="34">
-  <autoFilter ref="B77:D78"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table133031323435" displayName="Table133031323435" ref="B78:D79" totalsRowShown="0" headerRowDxfId="38" dataDxfId="36" headerRowBorderDxfId="37" tableBorderDxfId="35" totalsRowBorderDxfId="34">
+  <autoFilter ref="B78:D79"/>
   <tableColumns count="3">
     <tableColumn id="1" name="{missionOtherModifiersDefinitions}" dataDxfId="33"/>
     <tableColumn id="2" name="[sku]" dataDxfId="32"/>
@@ -2108,38 +2099,38 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table13" displayName="Table13" ref="B35:I44" totalsRowShown="0" headerRowDxfId="30" dataDxfId="28" headerRowBorderDxfId="29" tableBorderDxfId="27" totalsRowBorderDxfId="26">
-  <autoFilter ref="B35:I44"/>
-  <tableColumns count="8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table13" displayName="Table13" ref="B36:H45" totalsRowShown="0" headerRowDxfId="30" dataDxfId="28" headerRowBorderDxfId="29" tableBorderDxfId="27" totalsRowBorderDxfId="26">
+  <autoFilter ref="B36:H45"/>
+  <tableColumns count="7">
     <tableColumn id="1" name="{missionTypeDefinitions}" dataDxfId="25"/>
     <tableColumn id="2" name="[sku]" dataDxfId="24"/>
     <tableColumn id="3" name="[minTier]" dataDxfId="23"/>
     <tableColumn id="6" name="[maxTier]" dataDxfId="22"/>
     <tableColumn id="4" name="[weight]" dataDxfId="21"/>
-    <tableColumn id="5" name="[singleRunChance]" dataDxfId="20"/>
-    <tableColumn id="9" name="[tidDescSingleRun]" dataDxfId="19"/>
-    <tableColumn id="10" name="[tidDescMultiRun]" dataDxfId="18"/>
+    <tableColumn id="9" name="[tidDescSingleRun]" dataDxfId="20"/>
+    <tableColumn id="10" name="[tidDescMultiRun]" dataDxfId="19"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table1330" displayName="Table1330" ref="B4:M31" totalsRowShown="0" headerRowDxfId="17" dataDxfId="15" headerRowBorderDxfId="16" tableBorderDxfId="14" totalsRowBorderDxfId="13">
-  <autoFilter ref="B4:M31"/>
-  <tableColumns count="12">
-    <tableColumn id="1" name="{missionsDefinitions}" dataDxfId="12"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="11"/>
-    <tableColumn id="7" name="[type]" dataDxfId="10"/>
-    <tableColumn id="8" name="[weight]" dataDxfId="9"/>
-    <tableColumn id="11" name="[minTier]" dataDxfId="8"/>
-    <tableColumn id="12" name="[maxTier]" dataDxfId="7"/>
-    <tableColumn id="6" name="[params]" dataDxfId="6"/>
-    <tableColumn id="3" name="[objectiveBaseQuantityMin]" dataDxfId="5"/>
-    <tableColumn id="9" name="[objectiveBaseQuantityMax]" dataDxfId="4"/>
-    <tableColumn id="4" name="[icon]" dataDxfId="3"/>
-    <tableColumn id="5" name="[tidObjective]" dataDxfId="2"/>
-    <tableColumn id="10" name="[trackingSku]" dataDxfId="1"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table1330" displayName="Table1330" ref="B4:N32" totalsRowShown="0" headerRowDxfId="18" dataDxfId="16" headerRowBorderDxfId="17" tableBorderDxfId="15" totalsRowBorderDxfId="14">
+  <autoFilter ref="B4:N32"/>
+  <tableColumns count="13">
+    <tableColumn id="1" name="{missionsDefinitions}" dataDxfId="13"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="12"/>
+    <tableColumn id="7" name="[type]" dataDxfId="11"/>
+    <tableColumn id="8" name="[weight]" dataDxfId="10"/>
+    <tableColumn id="13" name="[singleRunChance]" dataDxfId="1"/>
+    <tableColumn id="11" name="[minTier]" dataDxfId="9"/>
+    <tableColumn id="12" name="[maxTier]" dataDxfId="8"/>
+    <tableColumn id="6" name="[params]" dataDxfId="7"/>
+    <tableColumn id="3" name="[objectiveBaseQuantityMin]" dataDxfId="6"/>
+    <tableColumn id="9" name="[objectiveBaseQuantityMax]" dataDxfId="5"/>
+    <tableColumn id="4" name="[icon]" dataDxfId="4"/>
+    <tableColumn id="5" name="[tidObjective]" dataDxfId="3"/>
+    <tableColumn id="10" name="[trackingSku]" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2411,26 +2402,26 @@
   <sheetPr>
     <tabColor theme="6"/>
   </sheetPr>
-  <dimension ref="B1:P78"/>
+  <dimension ref="B1:P79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="E42" sqref="E42"/>
+    <sheetView tabSelected="1" topLeftCell="A20" zoomScale="125" workbookViewId="0">
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="3.6640625" customWidth="1"/>
-    <col min="2" max="2" width="59.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17" customWidth="1"/>
     <col min="3" max="3" width="16.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="36" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="42.83203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="58.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="60" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.33203125" customWidth="1"/>
+    <col min="6" max="6" width="21" customWidth="1"/>
+    <col min="7" max="7" width="46.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="48" customWidth="1"/>
     <col min="9" max="9" width="49.5" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="52" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="28.83203125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="15" customWidth="1"/>
+    <col min="13" max="13" width="46.6640625" customWidth="1"/>
     <col min="14" max="14" width="23.83203125" customWidth="1"/>
     <col min="15" max="16" width="15" customWidth="1"/>
   </cols>
@@ -2453,59 +2444,62 @@
     </row>
     <row r="3" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B3" s="20"/>
-      <c r="C3" s="39"/>
-      <c r="D3" s="39"/>
-      <c r="E3" s="40" t="s">
+      <c r="C3" s="38"/>
+      <c r="D3" s="38"/>
+      <c r="E3" s="39" t="s">
         <v>165</v>
       </c>
-      <c r="F3" s="40" t="s">
+      <c r="F3" s="39" t="s">
         <v>164</v>
       </c>
-      <c r="G3" s="39"/>
-      <c r="J3" s="41" t="s">
+      <c r="G3" s="38"/>
+      <c r="J3" s="40" t="s">
         <v>163</v>
       </c>
-      <c r="K3" s="41"/>
-      <c r="M3" s="41"/>
-      <c r="N3" s="41"/>
-      <c r="O3" s="41"/>
-      <c r="P3" s="41"/>
-    </row>
-    <row r="4" spans="2:16" ht="103" x14ac:dyDescent="0.2">
-      <c r="B4" s="31" t="s">
+      <c r="K3" s="40"/>
+      <c r="M3" s="40"/>
+      <c r="N3" s="40"/>
+      <c r="O3" s="40"/>
+      <c r="P3" s="40"/>
+    </row>
+    <row r="4" spans="2:16" ht="108" x14ac:dyDescent="0.2">
+      <c r="B4" s="30" t="s">
         <v>162</v>
       </c>
       <c r="C4" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="38" t="s">
+      <c r="D4" s="37" t="s">
         <v>161</v>
       </c>
-      <c r="E4" s="38" t="s">
+      <c r="E4" s="37" t="s">
         <v>68</v>
       </c>
-      <c r="F4" s="38" t="s">
+      <c r="F4" s="37" t="s">
+        <v>167</v>
+      </c>
+      <c r="G4" s="37" t="s">
         <v>70</v>
       </c>
-      <c r="G4" s="38" t="s">
+      <c r="H4" s="37" t="s">
         <v>69</v>
       </c>
-      <c r="H4" s="38" t="s">
+      <c r="I4" s="37" t="s">
         <v>160</v>
       </c>
-      <c r="I4" s="38" t="s">
+      <c r="J4" s="37" t="s">
         <v>159</v>
       </c>
-      <c r="J4" s="38" t="s">
+      <c r="K4" s="37" t="s">
         <v>158</v>
       </c>
-      <c r="K4" s="37" t="s">
+      <c r="L4" s="36" t="s">
         <v>157</v>
       </c>
-      <c r="L4" s="37" t="s">
+      <c r="M4" s="36" t="s">
         <v>156</v>
       </c>
-      <c r="M4" s="36" t="s">
+      <c r="N4" s="35" t="s">
         <v>155</v>
       </c>
     </row>
@@ -2523,27 +2517,30 @@
         <v>0</v>
       </c>
       <c r="F5" s="24">
+        <v>0.3</v>
+      </c>
+      <c r="G5" s="24">
         <v>0</v>
       </c>
-      <c r="G5" s="24">
+      <c r="H5" s="24">
         <v>7</v>
       </c>
-      <c r="H5" s="24" t="s">
+      <c r="I5" s="24" t="s">
         <v>150</v>
       </c>
-      <c r="I5" s="24">
+      <c r="J5" s="24">
         <v>500</v>
       </c>
-      <c r="J5" s="34">
+      <c r="K5" s="33">
         <v>600</v>
       </c>
-      <c r="K5" s="34" t="s">
+      <c r="L5" s="33" t="s">
         <v>149</v>
       </c>
-      <c r="L5" s="34" t="s">
+      <c r="M5" s="33" t="s">
         <v>148</v>
       </c>
-      <c r="M5" s="32" t="s">
+      <c r="N5" s="31" t="s">
         <v>73</v>
       </c>
     </row>
@@ -2564,20 +2561,23 @@
         <v>0</v>
       </c>
       <c r="G6" s="24">
+        <v>0</v>
+      </c>
+      <c r="H6" s="24">
         <v>7</v>
       </c>
-      <c r="H6" s="24"/>
-      <c r="I6" s="24">
+      <c r="I6" s="24"/>
+      <c r="J6" s="24">
         <v>600</v>
       </c>
-      <c r="J6" s="34">
+      <c r="K6" s="33">
         <v>600</v>
       </c>
-      <c r="K6" s="34" t="s">
+      <c r="L6" s="33" t="s">
         <v>124</v>
       </c>
-      <c r="L6" s="34"/>
-      <c r="M6" s="32" t="s">
+      <c r="M6" s="33"/>
+      <c r="N6" s="31" t="s">
         <v>73</v>
       </c>
     </row>
@@ -2595,23 +2595,26 @@
         <v>0</v>
       </c>
       <c r="F7" s="24">
+        <v>0.3</v>
+      </c>
+      <c r="G7" s="24">
         <v>0</v>
       </c>
-      <c r="G7" s="24">
+      <c r="H7" s="24">
         <v>7</v>
       </c>
-      <c r="H7" s="24"/>
-      <c r="I7" s="24">
+      <c r="I7" s="24"/>
+      <c r="J7" s="24">
         <v>10000</v>
       </c>
-      <c r="J7" s="34">
+      <c r="K7" s="33">
         <v>10000</v>
       </c>
-      <c r="K7" s="34" t="s">
+      <c r="L7" s="33" t="s">
         <v>123</v>
       </c>
-      <c r="L7" s="34"/>
-      <c r="M7" s="32" t="s">
+      <c r="M7" s="33"/>
+      <c r="N7" s="31" t="s">
         <v>73</v>
       </c>
     </row>
@@ -2629,27 +2632,30 @@
         <v>1</v>
       </c>
       <c r="F8" s="24">
+        <v>0.3</v>
+      </c>
+      <c r="G8" s="24">
         <v>0</v>
       </c>
-      <c r="G8" s="24">
+      <c r="H8" s="24">
         <v>7</v>
       </c>
-      <c r="H8" s="24" t="s">
+      <c r="I8" s="24" t="s">
         <v>150</v>
       </c>
-      <c r="I8" s="24">
+      <c r="J8" s="24">
         <v>700</v>
       </c>
-      <c r="J8" s="34">
+      <c r="K8" s="33">
         <v>750</v>
       </c>
-      <c r="K8" s="34" t="s">
+      <c r="L8" s="33" t="s">
         <v>149</v>
       </c>
-      <c r="L8" s="34" t="s">
+      <c r="M8" s="33" t="s">
         <v>148</v>
       </c>
-      <c r="M8" s="32" t="s">
+      <c r="N8" s="31" t="s">
         <v>73</v>
       </c>
     </row>
@@ -2667,27 +2673,30 @@
         <v>1</v>
       </c>
       <c r="F9" s="24">
+        <v>0.3</v>
+      </c>
+      <c r="G9" s="24">
         <v>0</v>
       </c>
-      <c r="G9" s="24">
+      <c r="H9" s="24">
         <v>7</v>
       </c>
-      <c r="H9" s="24" t="s">
+      <c r="I9" s="24" t="s">
         <v>146</v>
       </c>
-      <c r="I9" s="24">
+      <c r="J9" s="24">
         <v>25</v>
       </c>
-      <c r="J9" s="34">
+      <c r="K9" s="33">
         <v>30</v>
       </c>
-      <c r="K9" s="34" t="s">
+      <c r="L9" s="33" t="s">
         <v>145</v>
       </c>
-      <c r="L9" s="34" t="s">
+      <c r="M9" s="33" t="s">
         <v>144</v>
       </c>
-      <c r="M9" s="32" t="s">
+      <c r="N9" s="31" t="s">
         <v>73</v>
       </c>
     </row>
@@ -2705,27 +2714,30 @@
         <v>1</v>
       </c>
       <c r="F10" s="24">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G10" s="24">
+        <v>1</v>
+      </c>
+      <c r="H10" s="24">
         <v>3</v>
       </c>
-      <c r="H10" s="23" t="s">
+      <c r="I10" s="23" t="s">
         <v>140</v>
       </c>
-      <c r="I10" s="24">
+      <c r="J10" s="24">
         <v>10</v>
       </c>
-      <c r="J10" s="34">
+      <c r="K10" s="33">
         <v>12</v>
       </c>
-      <c r="K10" s="34" t="s">
+      <c r="L10" s="33" t="s">
         <v>142</v>
       </c>
-      <c r="L10" s="34" t="s">
+      <c r="M10" s="33" t="s">
         <v>138</v>
       </c>
-      <c r="M10" s="32" t="s">
+      <c r="N10" s="31" t="s">
         <v>73</v>
       </c>
     </row>
@@ -2743,27 +2755,30 @@
         <v>0</v>
       </c>
       <c r="F11" s="24">
+        <v>0</v>
+      </c>
+      <c r="G11" s="24">
         <v>2</v>
       </c>
-      <c r="G11" s="24">
+      <c r="H11" s="24">
         <v>7</v>
       </c>
-      <c r="H11" s="23" t="s">
+      <c r="I11" s="23" t="s">
         <v>140</v>
       </c>
-      <c r="I11" s="24">
+      <c r="J11" s="24">
         <v>8</v>
       </c>
-      <c r="J11" s="23">
+      <c r="K11" s="23">
         <v>9</v>
       </c>
-      <c r="K11" s="34" t="s">
+      <c r="L11" s="33" t="s">
         <v>139</v>
       </c>
-      <c r="L11" s="34" t="s">
+      <c r="M11" s="33" t="s">
         <v>138</v>
       </c>
-      <c r="M11" s="32" t="s">
+      <c r="N11" s="31" t="s">
         <v>73</v>
       </c>
     </row>
@@ -2784,24 +2799,27 @@
         <v>0</v>
       </c>
       <c r="G12" s="24">
+        <v>0</v>
+      </c>
+      <c r="H12" s="24">
         <v>7</v>
       </c>
-      <c r="H12" s="24" t="s">
+      <c r="I12" s="24" t="s">
         <v>137</v>
       </c>
-      <c r="I12" s="24">
+      <c r="J12" s="24">
         <v>1000</v>
       </c>
-      <c r="J12" s="34">
+      <c r="K12" s="33">
         <v>1200</v>
       </c>
-      <c r="K12" s="34" t="s">
+      <c r="L12" s="33" t="s">
         <v>136</v>
       </c>
-      <c r="L12" s="34" t="s">
+      <c r="M12" s="33" t="s">
         <v>135</v>
       </c>
-      <c r="M12" s="32" t="s">
+      <c r="N12" s="31" t="s">
         <v>73</v>
       </c>
     </row>
@@ -2822,24 +2840,27 @@
         <v>0</v>
       </c>
       <c r="G13" s="24">
-        <v>1</v>
-      </c>
-      <c r="H13" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="H13" s="24">
+        <v>1</v>
+      </c>
+      <c r="I13" s="23" t="s">
         <v>134</v>
       </c>
-      <c r="I13" s="24">
-        <v>1</v>
-      </c>
-      <c r="J13" s="34">
+      <c r="J13" s="24">
+        <v>1</v>
+      </c>
+      <c r="K13" s="33">
         <v>2</v>
       </c>
-      <c r="K13" s="34" t="s">
+      <c r="L13" s="33" t="s">
         <v>133</v>
       </c>
-      <c r="L13" s="34" t="s">
+      <c r="M13" s="33" t="s">
         <v>132</v>
       </c>
-      <c r="M13" s="32" t="s">
+      <c r="N13" s="31" t="s">
         <v>73</v>
       </c>
     </row>
@@ -2857,27 +2878,30 @@
         <v>1</v>
       </c>
       <c r="F14" s="24">
-        <v>1</v>
+        <v>0.3</v>
       </c>
       <c r="G14" s="24">
+        <v>1</v>
+      </c>
+      <c r="H14" s="24">
         <v>7</v>
       </c>
-      <c r="H14" s="24" t="s">
+      <c r="I14" s="24" t="s">
         <v>130</v>
       </c>
-      <c r="I14" s="24">
+      <c r="J14" s="24">
         <v>10</v>
       </c>
-      <c r="J14" s="34">
+      <c r="K14" s="33">
         <v>11</v>
       </c>
-      <c r="K14" s="34" t="s">
+      <c r="L14" s="33" t="s">
         <v>129</v>
       </c>
-      <c r="L14" s="34" t="s">
+      <c r="M14" s="33" t="s">
         <v>128</v>
       </c>
-      <c r="M14" s="32" t="s">
+      <c r="N14" s="31" t="s">
         <v>73</v>
       </c>
     </row>
@@ -2895,23 +2919,26 @@
         <v>1</v>
       </c>
       <c r="F15" s="24">
+        <v>0.3</v>
+      </c>
+      <c r="G15" s="24">
         <v>0</v>
       </c>
-      <c r="G15" s="24">
+      <c r="H15" s="24">
         <v>7</v>
       </c>
-      <c r="H15" s="24"/>
-      <c r="I15" s="24">
+      <c r="I15" s="24"/>
+      <c r="J15" s="24">
         <v>5</v>
       </c>
-      <c r="J15" s="34">
+      <c r="K15" s="33">
         <v>6</v>
       </c>
-      <c r="K15" s="34" t="s">
+      <c r="L15" s="33" t="s">
         <v>126</v>
       </c>
-      <c r="L15" s="34"/>
-      <c r="M15" s="32" t="s">
+      <c r="M15" s="33"/>
+      <c r="N15" s="31" t="s">
         <v>73</v>
       </c>
     </row>
@@ -2932,24 +2959,27 @@
         <v>0</v>
       </c>
       <c r="G16" s="24">
+        <v>0</v>
+      </c>
+      <c r="H16" s="24">
         <v>7</v>
       </c>
-      <c r="H16" s="24"/>
-      <c r="I16" s="24">
+      <c r="I16" s="24"/>
+      <c r="J16" s="24">
         <v>700</v>
       </c>
-      <c r="J16" s="34">
+      <c r="K16" s="33">
         <v>800</v>
       </c>
-      <c r="K16" s="34" t="s">
+      <c r="L16" s="33" t="s">
         <v>125</v>
       </c>
-      <c r="L16" s="34"/>
-      <c r="M16" s="32" t="s">
+      <c r="M16" s="33"/>
+      <c r="N16" s="31" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="17" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B17" s="25" t="s">
         <v>1</v>
       </c>
@@ -2966,24 +2996,27 @@
         <v>0</v>
       </c>
       <c r="G17" s="24">
+        <v>0</v>
+      </c>
+      <c r="H17" s="24">
         <v>7</v>
       </c>
-      <c r="H17" s="24"/>
-      <c r="I17" s="24">
+      <c r="I17" s="24"/>
+      <c r="J17" s="24">
         <v>300</v>
       </c>
-      <c r="J17" s="34">
+      <c r="K17" s="33">
         <v>400</v>
       </c>
-      <c r="K17" s="34" t="s">
+      <c r="L17" s="33" t="s">
         <v>124</v>
       </c>
-      <c r="L17" s="34"/>
-      <c r="M17" s="32" t="s">
+      <c r="M17" s="33"/>
+      <c r="N17" s="31" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="18" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B18" s="25" t="s">
         <v>1</v>
       </c>
@@ -2997,27 +3030,30 @@
         <v>1</v>
       </c>
       <c r="F18" s="24">
+        <v>0.3</v>
+      </c>
+      <c r="G18" s="24">
         <v>0</v>
       </c>
-      <c r="G18" s="24">
+      <c r="H18" s="24">
         <v>7</v>
       </c>
-      <c r="H18" s="24"/>
-      <c r="I18" s="24">
+      <c r="I18" s="24"/>
+      <c r="J18" s="24">
         <v>400000</v>
       </c>
-      <c r="J18" s="34">
+      <c r="K18" s="33">
         <v>500000</v>
       </c>
-      <c r="K18" s="34" t="s">
+      <c r="L18" s="33" t="s">
         <v>123</v>
       </c>
-      <c r="L18" s="34"/>
-      <c r="M18" s="32" t="s">
+      <c r="M18" s="33"/>
+      <c r="N18" s="31" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="19" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B19" s="25" t="s">
         <v>1</v>
       </c>
@@ -3031,31 +3067,34 @@
         <v>1</v>
       </c>
       <c r="F19" s="24">
+        <v>0.3</v>
+      </c>
+      <c r="G19" s="24">
         <v>0</v>
       </c>
-      <c r="G19" s="24">
+      <c r="H19" s="24">
         <v>7</v>
       </c>
-      <c r="H19" s="23" t="s">
+      <c r="I19" s="23" t="s">
         <v>121</v>
       </c>
-      <c r="I19" s="24">
+      <c r="J19" s="24">
         <v>45</v>
       </c>
-      <c r="J19" s="34">
+      <c r="K19" s="33">
         <v>55</v>
       </c>
-      <c r="K19" s="35" t="s">
+      <c r="L19" s="34" t="s">
         <v>120</v>
       </c>
-      <c r="L19" s="34" t="s">
+      <c r="M19" s="33" t="s">
         <v>119</v>
       </c>
-      <c r="M19" s="32" t="s">
+      <c r="N19" s="31" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="20" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B20" s="25" t="s">
         <v>1</v>
       </c>
@@ -3069,31 +3108,34 @@
         <v>1</v>
       </c>
       <c r="F20" s="24">
+        <v>0.3</v>
+      </c>
+      <c r="G20" s="24">
         <v>0</v>
       </c>
-      <c r="G20" s="24">
+      <c r="H20" s="24">
         <v>7</v>
       </c>
-      <c r="H20" s="23" t="s">
+      <c r="I20" s="23" t="s">
         <v>117</v>
       </c>
-      <c r="I20" s="24">
+      <c r="J20" s="24">
         <v>40</v>
       </c>
-      <c r="J20" s="34">
+      <c r="K20" s="33">
         <v>45</v>
       </c>
-      <c r="K20" s="35" t="s">
+      <c r="L20" s="34" t="s">
         <v>116</v>
       </c>
-      <c r="L20" s="34" t="s">
+      <c r="M20" s="33" t="s">
         <v>115</v>
       </c>
-      <c r="M20" s="32" t="s">
+      <c r="N20" s="31" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="21" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B21" s="25" t="s">
         <v>1</v>
       </c>
@@ -3107,31 +3149,34 @@
         <v>1</v>
       </c>
       <c r="F21" s="24">
-        <v>1</v>
+        <v>0.3</v>
       </c>
       <c r="G21" s="24">
+        <v>1</v>
+      </c>
+      <c r="H21" s="24">
         <v>2</v>
       </c>
-      <c r="H21" s="23" t="s">
+      <c r="I21" s="23" t="s">
         <v>113</v>
       </c>
-      <c r="I21" s="23">
+      <c r="J21" s="23">
         <v>10</v>
       </c>
-      <c r="J21" s="35">
+      <c r="K21" s="34">
         <v>12</v>
       </c>
-      <c r="K21" s="35" t="s">
+      <c r="L21" s="34" t="s">
         <v>112</v>
       </c>
-      <c r="L21" s="35" t="s">
+      <c r="M21" s="34" t="s">
         <v>111</v>
       </c>
-      <c r="M21" s="32" t="s">
+      <c r="N21" s="31" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="22" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B22" s="27" t="s">
         <v>1</v>
       </c>
@@ -3145,31 +3190,34 @@
         <v>1</v>
       </c>
       <c r="F22" s="24">
+        <v>0.3</v>
+      </c>
+      <c r="G22" s="24">
         <v>0</v>
       </c>
-      <c r="G22" s="23">
-        <v>1</v>
-      </c>
-      <c r="H22" s="23" t="s">
+      <c r="H22" s="23">
+        <v>1</v>
+      </c>
+      <c r="I22" s="23" t="s">
         <v>109</v>
       </c>
-      <c r="I22" s="24">
+      <c r="J22" s="24">
         <v>5</v>
       </c>
-      <c r="J22" s="23">
+      <c r="K22" s="23">
         <v>6</v>
       </c>
-      <c r="K22" s="35" t="s">
+      <c r="L22" s="34" t="s">
         <v>108</v>
       </c>
-      <c r="L22" s="35" t="s">
+      <c r="M22" s="34" t="s">
         <v>107</v>
       </c>
-      <c r="M22" s="32" t="s">
+      <c r="N22" s="31" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="23" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B23" s="27" t="s">
         <v>1</v>
       </c>
@@ -3183,31 +3231,34 @@
         <v>1</v>
       </c>
       <c r="F23" s="24">
+        <v>0.3</v>
+      </c>
+      <c r="G23" s="24">
         <v>0</v>
       </c>
-      <c r="G23" s="35">
+      <c r="H23" s="34">
         <v>7</v>
       </c>
-      <c r="H23" s="23" t="s">
+      <c r="I23" s="23" t="s">
         <v>105</v>
       </c>
-      <c r="I23" s="24">
+      <c r="J23" s="24">
         <v>150</v>
       </c>
-      <c r="J23" s="23">
+      <c r="K23" s="23">
         <v>200</v>
       </c>
-      <c r="K23" s="35" t="s">
+      <c r="L23" s="34" t="s">
         <v>104</v>
       </c>
-      <c r="L23" s="35" t="s">
+      <c r="M23" s="34" t="s">
         <v>103</v>
       </c>
-      <c r="M23" s="32" t="s">
+      <c r="N23" s="31" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="24" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B24" s="27" t="s">
         <v>1</v>
       </c>
@@ -3221,31 +3272,34 @@
         <v>1</v>
       </c>
       <c r="F24" s="24">
+        <v>0.3</v>
+      </c>
+      <c r="G24" s="24">
         <v>2</v>
       </c>
-      <c r="G24" s="35">
+      <c r="H24" s="34">
         <v>7</v>
       </c>
-      <c r="H24" s="23" t="s">
+      <c r="I24" s="23" t="s">
         <v>101</v>
       </c>
-      <c r="I24" s="24">
+      <c r="J24" s="24">
         <v>5</v>
       </c>
-      <c r="J24" s="23">
+      <c r="K24" s="23">
         <v>7</v>
       </c>
-      <c r="K24" s="35" t="s">
+      <c r="L24" s="34" t="s">
         <v>100</v>
       </c>
-      <c r="L24" s="35" t="s">
+      <c r="M24" s="34" t="s">
         <v>99</v>
       </c>
-      <c r="M24" s="32" t="s">
+      <c r="N24" s="31" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="25" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B25" s="27" t="s">
         <v>1</v>
       </c>
@@ -3259,31 +3313,34 @@
         <v>1</v>
       </c>
       <c r="F25" s="24">
+        <v>0.3</v>
+      </c>
+      <c r="G25" s="24">
         <v>2</v>
       </c>
-      <c r="G25" s="35">
+      <c r="H25" s="34">
         <v>7</v>
       </c>
-      <c r="H25" s="23" t="s">
+      <c r="I25" s="23" t="s">
         <v>97</v>
       </c>
-      <c r="I25" s="24">
+      <c r="J25" s="24">
         <v>5</v>
       </c>
-      <c r="J25" s="23">
+      <c r="K25" s="23">
         <v>7</v>
       </c>
-      <c r="K25" s="35" t="s">
+      <c r="L25" s="34" t="s">
         <v>96</v>
       </c>
-      <c r="L25" s="35" t="s">
+      <c r="M25" s="34" t="s">
         <v>95</v>
       </c>
-      <c r="M25" s="32" t="s">
+      <c r="N25" s="31" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="26" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B26" s="27" t="s">
         <v>1</v>
       </c>
@@ -3297,31 +3354,34 @@
         <v>1</v>
       </c>
       <c r="F26" s="24">
+        <v>0.3</v>
+      </c>
+      <c r="G26" s="24">
         <v>2</v>
       </c>
-      <c r="G26" s="35">
+      <c r="H26" s="34">
         <v>7</v>
       </c>
-      <c r="H26" s="23" t="s">
+      <c r="I26" s="23" t="s">
         <v>93</v>
       </c>
-      <c r="I26" s="24">
+      <c r="J26" s="24">
         <v>3</v>
       </c>
-      <c r="J26" s="23">
+      <c r="K26" s="23">
         <v>4</v>
       </c>
-      <c r="K26" s="35" t="s">
+      <c r="L26" s="34" t="s">
         <v>92</v>
       </c>
-      <c r="L26" s="35" t="s">
+      <c r="M26" s="34" t="s">
         <v>91</v>
       </c>
-      <c r="M26" s="32" t="s">
+      <c r="N26" s="31" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="27" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B27" s="27" t="s">
         <v>1</v>
       </c>
@@ -3335,31 +3395,34 @@
         <v>1</v>
       </c>
       <c r="F27" s="24">
+        <v>0.3</v>
+      </c>
+      <c r="G27" s="24">
         <v>3</v>
       </c>
-      <c r="G27" s="35">
+      <c r="H27" s="34">
         <v>7</v>
       </c>
-      <c r="H27" s="23" t="s">
+      <c r="I27" s="23" t="s">
         <v>89</v>
       </c>
-      <c r="I27" s="24">
+      <c r="J27" s="24">
         <v>3</v>
       </c>
-      <c r="J27" s="23">
+      <c r="K27" s="23">
         <v>3.5</v>
       </c>
-      <c r="K27" s="35" t="s">
+      <c r="L27" s="34" t="s">
         <v>88</v>
       </c>
-      <c r="L27" s="35" t="s">
+      <c r="M27" s="34" t="s">
         <v>87</v>
       </c>
-      <c r="M27" s="32" t="s">
+      <c r="N27" s="31" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="28" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B28" s="27" t="s">
         <v>1</v>
       </c>
@@ -3373,31 +3436,34 @@
         <v>1</v>
       </c>
       <c r="F28" s="24">
-        <v>1</v>
-      </c>
-      <c r="G28" s="35">
+        <v>0.3</v>
+      </c>
+      <c r="G28" s="24">
+        <v>1</v>
+      </c>
+      <c r="H28" s="34">
         <v>7</v>
       </c>
-      <c r="H28" s="23" t="s">
+      <c r="I28" s="23" t="s">
         <v>85</v>
       </c>
-      <c r="I28" s="24">
+      <c r="J28" s="24">
         <v>8</v>
       </c>
-      <c r="J28" s="23">
+      <c r="K28" s="23">
         <v>9</v>
       </c>
-      <c r="K28" s="35" t="s">
+      <c r="L28" s="34" t="s">
         <v>84</v>
       </c>
-      <c r="L28" s="35" t="s">
+      <c r="M28" s="34" t="s">
         <v>83</v>
       </c>
-      <c r="M28" s="32" t="s">
+      <c r="N28" s="31" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="29" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B29" s="27" t="s">
         <v>1</v>
       </c>
@@ -3411,31 +3477,34 @@
         <v>1</v>
       </c>
       <c r="F29" s="24">
+        <v>0.3</v>
+      </c>
+      <c r="G29" s="24">
         <v>2</v>
       </c>
-      <c r="G29" s="35">
+      <c r="H29" s="34">
         <v>7</v>
       </c>
-      <c r="H29" s="23" t="s">
+      <c r="I29" s="23" t="s">
         <v>81</v>
       </c>
-      <c r="I29" s="24">
+      <c r="J29" s="24">
         <v>11</v>
       </c>
-      <c r="J29" s="23">
+      <c r="K29" s="23">
         <v>12</v>
       </c>
-      <c r="K29" s="35" t="s">
+      <c r="L29" s="34" t="s">
         <v>80</v>
       </c>
-      <c r="L29" s="35" t="s">
+      <c r="M29" s="34" t="s">
         <v>79</v>
       </c>
-      <c r="M29" s="32" t="s">
+      <c r="N29" s="31" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="30" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B30" s="27" t="s">
         <v>1</v>
       </c>
@@ -3449,31 +3518,34 @@
         <v>1</v>
       </c>
       <c r="F30" s="24">
+        <v>0.3</v>
+      </c>
+      <c r="G30" s="24">
         <v>3</v>
       </c>
-      <c r="G30" s="35">
+      <c r="H30" s="34">
         <v>7</v>
       </c>
-      <c r="H30" s="23" t="s">
+      <c r="I30" s="23" t="s">
         <v>77</v>
       </c>
-      <c r="I30" s="24">
+      <c r="J30" s="24">
         <v>3</v>
       </c>
-      <c r="J30" s="23">
+      <c r="K30" s="23">
         <v>3.5</v>
       </c>
-      <c r="K30" s="35" t="s">
+      <c r="L30" s="34" t="s">
         <v>76</v>
       </c>
-      <c r="L30" s="35" t="s">
+      <c r="M30" s="34" t="s">
         <v>75</v>
       </c>
-      <c r="M30" s="32" t="s">
+      <c r="N30" s="31" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="31" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B31" s="27" t="s">
         <v>1</v>
       </c>
@@ -3487,116 +3559,131 @@
         <v>1</v>
       </c>
       <c r="F31" s="24">
+        <v>0.3</v>
+      </c>
+      <c r="G31" s="24">
         <v>0</v>
       </c>
-      <c r="G31" s="35">
+      <c r="H31" s="34">
         <v>7</v>
       </c>
-      <c r="H31" s="23"/>
-      <c r="I31" s="24">
+      <c r="I31" s="23"/>
+      <c r="J31" s="24">
         <v>6000</v>
       </c>
-      <c r="J31" s="23">
+      <c r="K31" s="23">
         <v>7000</v>
       </c>
-      <c r="K31" s="34" t="s">
+      <c r="L31" s="33" t="s">
         <v>74</v>
       </c>
-      <c r="L31" s="34"/>
-      <c r="M31" s="32" t="s">
+      <c r="M31" s="33"/>
+      <c r="N31" s="31" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="32" spans="2:13" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="33"/>
-      <c r="C32" s="33"/>
-      <c r="D32" s="33"/>
-      <c r="E32" s="33"/>
-      <c r="F32" s="33"/>
-      <c r="G32" s="33"/>
-      <c r="H32" s="33"/>
-      <c r="I32" s="33"/>
-      <c r="J32" s="33"/>
-      <c r="K32" s="33"/>
-      <c r="L32" s="33"/>
-      <c r="M32" s="32"/>
-    </row>
-    <row r="33" spans="2:13" ht="24" x14ac:dyDescent="0.3">
-      <c r="B33" s="6" t="s">
+    <row r="32" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B32" s="27" t="s">
+        <v>1</v>
+      </c>
+      <c r="C32" s="24" t="s">
+        <v>170</v>
+      </c>
+      <c r="D32" s="23" t="s">
+        <v>168</v>
+      </c>
+      <c r="E32" s="23">
+        <v>1</v>
+      </c>
+      <c r="F32" s="23">
+        <v>1</v>
+      </c>
+      <c r="G32" s="24">
+        <v>0</v>
+      </c>
+      <c r="H32" s="23">
+        <v>7</v>
+      </c>
+      <c r="I32" s="23" t="s">
+        <v>150</v>
+      </c>
+      <c r="J32" s="24">
+        <v>999</v>
+      </c>
+      <c r="K32" s="23">
+        <v>999</v>
+      </c>
+      <c r="L32" s="33" t="s">
+        <v>149</v>
+      </c>
+      <c r="M32" s="33" t="s">
+        <v>148</v>
+      </c>
+      <c r="N32" s="31" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="33" spans="2:13" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B33" s="32"/>
+      <c r="C33" s="32"/>
+      <c r="D33" s="32"/>
+      <c r="E33" s="32"/>
+      <c r="F33" s="32"/>
+      <c r="G33" s="32"/>
+      <c r="H33" s="32"/>
+      <c r="I33" s="32"/>
+      <c r="J33" s="32"/>
+      <c r="K33" s="32"/>
+      <c r="L33" s="32"/>
+      <c r="M33" s="31"/>
+    </row>
+    <row r="34" spans="2:13" ht="24" x14ac:dyDescent="0.3">
+      <c r="B34" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="C33" s="6"/>
-      <c r="D33" s="6"/>
-      <c r="E33" s="6"/>
-      <c r="F33" s="6"/>
-      <c r="G33" s="6"/>
-      <c r="H33" s="6"/>
-      <c r="I33" s="6"/>
-      <c r="J33" s="6"/>
-      <c r="K33" s="6"/>
-      <c r="L33" s="6"/>
-    </row>
-    <row r="34" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B34" s="20"/>
-      <c r="C34" s="20"/>
-      <c r="D34" s="20"/>
-      <c r="E34" s="20"/>
-      <c r="F34" s="42"/>
-      <c r="G34" s="42"/>
-      <c r="H34" s="42"/>
-      <c r="I34" s="20"/>
-      <c r="J34" s="20"/>
-    </row>
-    <row r="35" spans="2:13" ht="96" x14ac:dyDescent="0.2">
-      <c r="B35" s="31" t="s">
+      <c r="C34" s="6"/>
+      <c r="D34" s="6"/>
+      <c r="E34" s="6"/>
+      <c r="F34" s="6"/>
+      <c r="G34" s="6"/>
+      <c r="H34" s="6"/>
+      <c r="I34" s="6"/>
+      <c r="J34" s="6"/>
+      <c r="K34" s="6"/>
+      <c r="L34" s="6"/>
+    </row>
+    <row r="35" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B35" s="20"/>
+      <c r="C35" s="20"/>
+      <c r="D35" s="20"/>
+      <c r="E35" s="20"/>
+      <c r="F35" s="41"/>
+      <c r="G35" s="41"/>
+      <c r="H35" s="41"/>
+      <c r="I35" s="20"/>
+      <c r="J35" s="20"/>
+    </row>
+    <row r="36" spans="2:13" ht="96" x14ac:dyDescent="0.2">
+      <c r="B36" s="30" t="s">
         <v>71</v>
       </c>
-      <c r="C35" s="28" t="s">
+      <c r="C36" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="D35" s="30" t="s">
+      <c r="D36" s="29" t="s">
         <v>70</v>
       </c>
-      <c r="E35" s="30" t="s">
+      <c r="E36" s="29" t="s">
         <v>69</v>
       </c>
-      <c r="F35" s="30" t="s">
+      <c r="F36" s="29" t="s">
         <v>68</v>
       </c>
-      <c r="G35" s="29" t="s">
-        <v>167</v>
-      </c>
-      <c r="H35" s="28" t="s">
+      <c r="G36" s="28" t="s">
         <v>67</v>
       </c>
-      <c r="I35" s="28" t="s">
+      <c r="H36" s="28" t="s">
         <v>66</v>
-      </c>
-    </row>
-    <row r="36" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B36" s="27" t="s">
-        <v>1</v>
-      </c>
-      <c r="C36" s="24" t="s">
-        <v>65</v>
-      </c>
-      <c r="D36" s="24">
-        <v>0</v>
-      </c>
-      <c r="E36" s="24">
-        <v>7</v>
-      </c>
-      <c r="F36" s="24">
-        <v>2</v>
-      </c>
-      <c r="G36" s="26">
-        <v>0.3</v>
-      </c>
-      <c r="H36" s="26" t="s">
-        <v>64</v>
-      </c>
-      <c r="I36" s="26" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="37" spans="2:13" x14ac:dyDescent="0.2">
@@ -3604,7 +3691,7 @@
         <v>1</v>
       </c>
       <c r="C37" s="24" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="D37" s="24">
         <v>0</v>
@@ -3613,16 +3700,13 @@
         <v>7</v>
       </c>
       <c r="F37" s="24">
-        <v>1</v>
-      </c>
-      <c r="G37" s="26">
-        <v>0.3</v>
+        <v>2</v>
+      </c>
+      <c r="G37" s="26" t="s">
+        <v>64</v>
       </c>
       <c r="H37" s="26" t="s">
-        <v>61</v>
-      </c>
-      <c r="I37" s="26" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
     </row>
     <row r="38" spans="2:13" x14ac:dyDescent="0.2">
@@ -3630,7 +3714,7 @@
         <v>1</v>
       </c>
       <c r="C38" s="24" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="D38" s="24">
         <v>0</v>
@@ -3639,16 +3723,13 @@
         <v>7</v>
       </c>
       <c r="F38" s="24">
-        <v>2</v>
-      </c>
-      <c r="G38" s="26">
-        <v>0.3</v>
+        <v>1</v>
+      </c>
+      <c r="G38" s="26" t="s">
+        <v>61</v>
       </c>
       <c r="H38" s="26" t="s">
-        <v>58</v>
-      </c>
-      <c r="I38" s="26" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
     </row>
     <row r="39" spans="2:13" x14ac:dyDescent="0.2">
@@ -3656,7 +3737,7 @@
         <v>1</v>
       </c>
       <c r="C39" s="24" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="D39" s="24">
         <v>0</v>
@@ -3665,68 +3746,59 @@
         <v>7</v>
       </c>
       <c r="F39" s="24">
-        <v>1</v>
-      </c>
-      <c r="G39" s="26">
-        <v>0</v>
+        <v>2</v>
+      </c>
+      <c r="G39" s="26" t="s">
+        <v>58</v>
       </c>
       <c r="H39" s="26" t="s">
-        <v>55</v>
-      </c>
-      <c r="I39" s="26" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
     </row>
     <row r="40" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B40" s="25" t="s">
-        <v>1</v>
-      </c>
-      <c r="C40" s="23" t="s">
-        <v>53</v>
-      </c>
-      <c r="D40" s="23">
+      <c r="B40" s="27" t="s">
+        <v>1</v>
+      </c>
+      <c r="C40" s="24" t="s">
+        <v>56</v>
+      </c>
+      <c r="D40" s="24">
         <v>0</v>
       </c>
       <c r="E40" s="24">
         <v>7</v>
       </c>
-      <c r="F40" s="23">
-        <v>1</v>
-      </c>
-      <c r="G40" s="26">
-        <v>0</v>
+      <c r="F40" s="24">
+        <v>1</v>
+      </c>
+      <c r="G40" s="26" t="s">
+        <v>55</v>
       </c>
       <c r="H40" s="26" t="s">
-        <v>52</v>
-      </c>
-      <c r="I40" s="26" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
     </row>
     <row r="41" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B41" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="C41" s="24" t="s">
-        <v>50</v>
-      </c>
-      <c r="D41" s="24">
+      <c r="C41" s="23" t="s">
+        <v>53</v>
+      </c>
+      <c r="D41" s="23">
         <v>0</v>
       </c>
       <c r="E41" s="24">
         <v>7</v>
       </c>
-      <c r="F41" s="24">
-        <v>1</v>
-      </c>
-      <c r="G41" s="26">
-        <v>0</v>
+      <c r="F41" s="23">
+        <v>1</v>
+      </c>
+      <c r="G41" s="26" t="s">
+        <v>52</v>
       </c>
       <c r="H41" s="26" t="s">
-        <v>49</v>
-      </c>
-      <c r="I41" s="26" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
     </row>
     <row r="42" spans="2:13" x14ac:dyDescent="0.2">
@@ -3734,7 +3806,7 @@
         <v>1</v>
       </c>
       <c r="C42" s="24" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="D42" s="24">
         <v>0</v>
@@ -3745,40 +3817,34 @@
       <c r="F42" s="24">
         <v>1</v>
       </c>
-      <c r="G42" s="26">
-        <v>0.3</v>
+      <c r="G42" s="26" t="s">
+        <v>49</v>
       </c>
       <c r="H42" s="26" t="s">
-        <v>46</v>
-      </c>
-      <c r="I42" s="26" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
     </row>
     <row r="43" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B43" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="C43" s="23" t="s">
-        <v>44</v>
-      </c>
-      <c r="D43" s="23">
+      <c r="C43" s="24" t="s">
+        <v>47</v>
+      </c>
+      <c r="D43" s="24">
         <v>0</v>
       </c>
       <c r="E43" s="24">
         <v>7</v>
       </c>
-      <c r="F43" s="23">
-        <v>1</v>
-      </c>
-      <c r="G43" s="22">
-        <v>0</v>
-      </c>
-      <c r="H43" s="22" t="s">
-        <v>43</v>
-      </c>
-      <c r="I43" s="22" t="s">
-        <v>42</v>
+      <c r="F43" s="24">
+        <v>1</v>
+      </c>
+      <c r="G43" s="26" t="s">
+        <v>46</v>
+      </c>
+      <c r="H43" s="26" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="44" spans="2:13" x14ac:dyDescent="0.2">
@@ -3786,7 +3852,7 @@
         <v>1</v>
       </c>
       <c r="C44" s="23" t="s">
-        <v>168</v>
+        <v>44</v>
       </c>
       <c r="D44" s="23">
         <v>0</v>
@@ -3797,107 +3863,95 @@
       <c r="F44" s="23">
         <v>1</v>
       </c>
-      <c r="G44" s="22">
-        <v>1</v>
-      </c>
-      <c r="H44" s="26" t="s">
+      <c r="G44" s="22" t="s">
+        <v>43</v>
+      </c>
+      <c r="H44" s="22" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="45" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B45" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="C45" s="23" t="s">
+        <v>168</v>
+      </c>
+      <c r="D45" s="23">
+        <v>0</v>
+      </c>
+      <c r="E45" s="24">
+        <v>7</v>
+      </c>
+      <c r="F45" s="23">
+        <v>1</v>
+      </c>
+      <c r="G45" s="26" t="s">
         <v>169</v>
       </c>
-      <c r="I44" s="26"/>
-    </row>
-    <row r="45" spans="2:13" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="46" spans="2:13" ht="24" x14ac:dyDescent="0.3">
-      <c r="B46" s="6" t="s">
+      <c r="H45" s="26"/>
+    </row>
+    <row r="46" spans="2:13" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="47" spans="2:13" ht="24" x14ac:dyDescent="0.3">
+      <c r="B47" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="C46" s="6"/>
-      <c r="D46" s="6"/>
-      <c r="E46" s="6"/>
-      <c r="F46" s="6"/>
-      <c r="G46" s="6"/>
-      <c r="H46" s="6"/>
-      <c r="I46" s="6"/>
-      <c r="J46" s="6"/>
-      <c r="K46" s="6"/>
-      <c r="L46" s="6"/>
-      <c r="M46" s="6"/>
-    </row>
-    <row r="47" spans="2:13" ht="30" x14ac:dyDescent="0.2">
-      <c r="B47" s="20"/>
-      <c r="C47" s="20"/>
-      <c r="D47" s="20"/>
-      <c r="E47" s="20"/>
-      <c r="F47" s="21" t="s">
+      <c r="C47" s="6"/>
+      <c r="D47" s="6"/>
+      <c r="E47" s="6"/>
+      <c r="F47" s="6"/>
+      <c r="G47" s="6"/>
+      <c r="H47" s="6"/>
+      <c r="I47" s="6"/>
+      <c r="J47" s="6"/>
+      <c r="K47" s="6"/>
+      <c r="L47" s="6"/>
+      <c r="M47" s="6"/>
+    </row>
+    <row r="48" spans="2:13" ht="45" x14ac:dyDescent="0.2">
+      <c r="B48" s="20"/>
+      <c r="C48" s="20"/>
+      <c r="D48" s="20"/>
+      <c r="E48" s="20"/>
+      <c r="F48" s="21" t="s">
         <v>40</v>
       </c>
-      <c r="G47" s="43" t="s">
+      <c r="G48" s="42" t="s">
         <v>39</v>
       </c>
-      <c r="H47" s="43"/>
-      <c r="I47" s="20"/>
-    </row>
-    <row r="48" spans="2:13" ht="137" x14ac:dyDescent="0.2">
-      <c r="B48" s="19" t="s">
+      <c r="H48" s="42"/>
+      <c r="I48" s="20"/>
+    </row>
+    <row r="49" spans="2:11" ht="137" x14ac:dyDescent="0.2">
+      <c r="B49" s="19" t="s">
         <v>38</v>
       </c>
-      <c r="C48" s="19" t="s">
+      <c r="C49" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="D48" s="18" t="s">
+      <c r="D49" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="E48" s="17" t="s">
+      <c r="E49" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="F48" s="17" t="s">
+      <c r="F49" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="G48" s="17" t="s">
+      <c r="G49" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="H48" s="16" t="s">
+      <c r="H49" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="I48" s="16" t="s">
+      <c r="I49" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="J48" s="15" t="s">
+      <c r="J49" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="K48" s="14" t="s">
+      <c r="K49" s="14" t="s">
         <v>30</v>
-      </c>
-    </row>
-    <row r="49" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B49" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="C49" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="D49" s="11">
-        <v>0</v>
-      </c>
-      <c r="E49" s="10">
-        <v>0</v>
-      </c>
-      <c r="F49" s="10">
-        <v>15</v>
-      </c>
-      <c r="G49" s="10">
-        <v>200</v>
-      </c>
-      <c r="H49" s="9">
-        <v>0.5</v>
-      </c>
-      <c r="I49" s="9">
-        <v>1</v>
-      </c>
-      <c r="J49" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="K49" s="13" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="50" spans="2:11" x14ac:dyDescent="0.2">
@@ -3905,19 +3959,19 @@
         <v>1</v>
       </c>
       <c r="C50" s="11" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D50" s="11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E50" s="10">
         <v>0</v>
       </c>
       <c r="F50" s="10">
-        <v>60</v>
+        <v>15</v>
       </c>
       <c r="G50" s="10">
-        <v>300</v>
+        <v>200</v>
       </c>
       <c r="H50" s="9">
         <v>0.5</v>
@@ -3926,10 +3980,10 @@
         <v>1</v>
       </c>
       <c r="J50" s="8" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="K50" s="13" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="51" spans="2:11" x14ac:dyDescent="0.2">
@@ -3937,19 +3991,19 @@
         <v>1</v>
       </c>
       <c r="C51" s="11" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D51" s="11">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E51" s="10">
         <v>0</v>
       </c>
       <c r="F51" s="10">
-        <v>240</v>
+        <v>60</v>
       </c>
       <c r="G51" s="10">
-        <v>600</v>
+        <v>300</v>
       </c>
       <c r="H51" s="9">
         <v>0.5</v>
@@ -3958,49 +4012,67 @@
         <v>1</v>
       </c>
       <c r="J51" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="K51" s="13" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="52" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B52" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="C52" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="D52" s="11">
+        <v>2</v>
+      </c>
+      <c r="E52" s="10">
+        <v>0</v>
+      </c>
+      <c r="F52" s="10">
+        <v>240</v>
+      </c>
+      <c r="G52" s="10">
+        <v>600</v>
+      </c>
+      <c r="H52" s="9">
+        <v>0.5</v>
+      </c>
+      <c r="I52" s="9">
+        <v>1</v>
+      </c>
+      <c r="J52" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="K51" s="7" t="s">
+      <c r="K52" s="7" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="53" spans="2:11" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="54" spans="2:11" ht="24" x14ac:dyDescent="0.3">
-      <c r="B54" s="6" t="s">
+    <row r="54" spans="2:11" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="55" spans="2:11" ht="24" x14ac:dyDescent="0.3">
+      <c r="B55" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="C54" s="6"/>
-      <c r="D54" s="6"/>
-      <c r="E54" s="6"/>
-      <c r="F54" s="6"/>
-      <c r="G54" s="6"/>
-    </row>
-    <row r="56" spans="2:11" ht="135" x14ac:dyDescent="0.2">
-      <c r="B56" s="5" t="s">
+      <c r="C55" s="6"/>
+      <c r="D55" s="6"/>
+      <c r="E55" s="6"/>
+      <c r="F55" s="6"/>
+      <c r="G55" s="6"/>
+    </row>
+    <row r="57" spans="2:11" ht="135" x14ac:dyDescent="0.2">
+      <c r="B57" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="C56" s="4" t="s">
+      <c r="C57" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D56" s="3" t="s">
+      <c r="D57" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E56" s="3" t="s">
+      <c r="E57" s="3" t="s">
         <v>21</v>
-      </c>
-    </row>
-    <row r="57" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B57" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C57" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D57" s="1">
-        <v>0.1</v>
-      </c>
-      <c r="E57" s="1">
-        <v>2</v>
       </c>
     </row>
     <row r="58" spans="2:11" x14ac:dyDescent="0.2">
@@ -4008,13 +4080,13 @@
         <v>1</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D58" s="1">
-        <v>0.7</v>
+        <v>0.1</v>
       </c>
       <c r="E58" s="1">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="59" spans="2:11" x14ac:dyDescent="0.2">
@@ -4022,13 +4094,13 @@
         <v>1</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D59" s="1">
-        <v>1</v>
+        <v>0.7</v>
       </c>
       <c r="E59" s="1">
-        <v>12</v>
+        <v>6</v>
       </c>
     </row>
     <row r="60" spans="2:11" x14ac:dyDescent="0.2">
@@ -4036,13 +4108,13 @@
         <v>1</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D60" s="1">
-        <v>1.5</v>
+        <v>1</v>
       </c>
       <c r="E60" s="1">
-        <v>18</v>
+        <v>12</v>
       </c>
     </row>
     <row r="61" spans="2:11" x14ac:dyDescent="0.2">
@@ -4050,13 +4122,13 @@
         <v>1</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D61" s="1">
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="E61" s="1">
-        <v>26</v>
+        <v>18</v>
       </c>
     </row>
     <row r="62" spans="2:11" x14ac:dyDescent="0.2">
@@ -4064,13 +4136,13 @@
         <v>1</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D62" s="1">
-        <v>2.5</v>
+        <v>2</v>
       </c>
       <c r="E62" s="1">
-        <v>35</v>
+        <v>26</v>
       </c>
     </row>
     <row r="63" spans="2:11" x14ac:dyDescent="0.2">
@@ -4078,13 +4150,13 @@
         <v>1</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D63" s="1">
-        <v>3</v>
+        <v>2.5</v>
       </c>
       <c r="E63" s="1">
-        <v>45</v>
+        <v>35</v>
       </c>
     </row>
     <row r="64" spans="2:11" x14ac:dyDescent="0.2">
@@ -4092,13 +4164,13 @@
         <v>1</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D64" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E64" s="1">
-        <v>56</v>
+        <v>45</v>
       </c>
     </row>
     <row r="65" spans="2:7" x14ac:dyDescent="0.2">
@@ -4106,13 +4178,13 @@
         <v>1</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D65" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E65" s="1">
-        <v>67</v>
+        <v>56</v>
       </c>
     </row>
     <row r="66" spans="2:7" x14ac:dyDescent="0.2">
@@ -4120,46 +4192,49 @@
         <v>1</v>
       </c>
       <c r="C66" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D66" s="1">
+        <v>5</v>
+      </c>
+      <c r="E66" s="1">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="67" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B67" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C67" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D66" s="1">
+      <c r="D67" s="1">
         <v>7</v>
       </c>
-      <c r="E66" s="1">
+      <c r="E67" s="1">
         <v>80</v>
       </c>
     </row>
-    <row r="67" spans="2:7" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="68" spans="2:7" ht="24" x14ac:dyDescent="0.3">
-      <c r="B68" s="6" t="s">
+    <row r="68" spans="2:7" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="69" spans="2:7" ht="24" x14ac:dyDescent="0.3">
+      <c r="B69" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C68" s="6"/>
-      <c r="D68" s="6"/>
-      <c r="E68" s="6"/>
-      <c r="F68" s="6"/>
-      <c r="G68" s="6"/>
-    </row>
-    <row r="70" spans="2:7" ht="142" x14ac:dyDescent="0.2">
-      <c r="B70" s="5" t="s">
+      <c r="C69" s="6"/>
+      <c r="D69" s="6"/>
+      <c r="E69" s="6"/>
+      <c r="F69" s="6"/>
+      <c r="G69" s="6"/>
+    </row>
+    <row r="71" spans="2:7" ht="142" x14ac:dyDescent="0.2">
+      <c r="B71" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C70" s="4" t="s">
+      <c r="C71" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D70" s="3" t="s">
+      <c r="D71" s="3" t="s">
         <v>2</v>
-      </c>
-    </row>
-    <row r="71" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B71" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C71" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D71" s="1">
-        <v>0.05</v>
       </c>
     </row>
     <row r="72" spans="2:7" x14ac:dyDescent="0.2">
@@ -4167,10 +4242,10 @@
         <v>1</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D72" s="1">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="73" spans="2:7" x14ac:dyDescent="0.2">
@@ -4178,42 +4253,53 @@
         <v>1</v>
       </c>
       <c r="C73" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D73" s="1">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="74" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B74" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C74" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D73" s="1">
+      <c r="D74" s="1">
         <v>0.2</v>
       </c>
     </row>
-    <row r="74" spans="2:7" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="75" spans="2:7" ht="24" x14ac:dyDescent="0.3">
-      <c r="B75" s="6" t="s">
+    <row r="75" spans="2:7" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="76" spans="2:7" ht="24" x14ac:dyDescent="0.3">
+      <c r="B76" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C75" s="6"/>
-      <c r="D75" s="6"/>
-      <c r="E75" s="6"/>
-      <c r="F75" s="6"/>
-      <c r="G75" s="6"/>
-    </row>
-    <row r="77" spans="2:7" ht="131" x14ac:dyDescent="0.2">
-      <c r="B77" s="5" t="s">
+      <c r="C76" s="6"/>
+      <c r="D76" s="6"/>
+      <c r="E76" s="6"/>
+      <c r="F76" s="6"/>
+      <c r="G76" s="6"/>
+    </row>
+    <row r="78" spans="2:7" ht="131" x14ac:dyDescent="0.2">
+      <c r="B78" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C77" s="4" t="s">
+      <c r="C78" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D77" s="3" t="s">
+      <c r="D78" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="78" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B78" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C78" s="1" t="s">
+    <row r="79" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B79" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C79" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D78" s="1">
+      <c r="D79" s="1">
         <v>0.7</v>
       </c>
     </row>
@@ -4221,10 +4307,10 @@
   <mergeCells count="4">
     <mergeCell ref="J3:K3"/>
     <mergeCell ref="M3:P3"/>
-    <mergeCell ref="F34:H34"/>
-    <mergeCell ref="G47:H47"/>
+    <mergeCell ref="F35:H35"/>
+    <mergeCell ref="G48:H48"/>
   </mergeCells>
-  <conditionalFormatting sqref="C49:D51">
+  <conditionalFormatting sqref="C50:D52">
     <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
[ CONTENT ] Added new missions using the new types of missons :)
Former-commit-id: 500e02b44661fa3a63789635f91b82277ba24e51
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Missions.xlsx
+++ b/Docs/Content/HungryDragonContent_Missions.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10210"/>
-  <workbookPr/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aortin/Documents/UBI/FD/Client/Docs/Content/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\dragon\client\Docs\Content\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="38300" windowHeight="19860"/>
+    <workbookView xWindow="0" yWindow="435" windowWidth="38295" windowHeight="19860"/>
   </bookViews>
   <sheets>
     <sheet name="missions" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="401" uniqueCount="213">
   <si>
     <t>single_run</t>
   </si>
@@ -251,9 +251,6 @@
     <t>icon_run</t>
   </si>
   <si>
-    <t>TID_MISSION_TROLL_DESC</t>
-  </si>
-  <si>
     <t>icon_troll</t>
   </si>
   <si>
@@ -263,9 +260,6 @@
     <t>troll</t>
   </si>
   <si>
-    <t>TID_MISSION_SOLDIERS_DESC</t>
-  </si>
-  <si>
     <t>icon_soldiers</t>
   </si>
   <si>
@@ -275,9 +269,6 @@
     <t>soldiers</t>
   </si>
   <si>
-    <t>TID_MISSION_ARCHER_DESC</t>
-  </si>
-  <si>
     <t>icon_archer</t>
   </si>
   <si>
@@ -287,9 +278,6 @@
     <t>archers</t>
   </si>
   <si>
-    <t>TID_MISSION_BOATMAN_DESC</t>
-  </si>
-  <si>
     <t>icon_fisherman</t>
   </si>
   <si>
@@ -299,9 +287,6 @@
     <t>boatFished</t>
   </si>
   <si>
-    <t>TID_MISSION_DRILLER_DESC</t>
-  </si>
-  <si>
     <t>icon_rocket</t>
   </si>
   <si>
@@ -311,9 +296,6 @@
     <t>guardian</t>
   </si>
   <si>
-    <t>TID_MISSION_LIONBIRD_DESC</t>
-  </si>
-  <si>
     <t>icon_lionbird</t>
   </si>
   <si>
@@ -323,9 +305,6 @@
     <t>lionbird</t>
   </si>
   <si>
-    <t>TID_MISSION_OWL_DESC</t>
-  </si>
-  <si>
     <t>icon_owl</t>
   </si>
   <si>
@@ -335,9 +314,6 @@
     <t>owls</t>
   </si>
   <si>
-    <t>TID_MISSION_BATS_DESC</t>
-  </si>
-  <si>
     <t>icon_bat_s</t>
   </si>
   <si>
@@ -347,9 +323,6 @@
     <t>bats</t>
   </si>
   <si>
-    <t>TID_MISSION_FLYINGPIG_DESC</t>
-  </si>
-  <si>
     <t>icon_flying_pig</t>
   </si>
   <si>
@@ -359,9 +332,6 @@
     <t>flyingPig</t>
   </si>
   <si>
-    <t>TID_MISSION_VULTURE_DESC</t>
-  </si>
-  <si>
     <t>icon_vulture</t>
   </si>
   <si>
@@ -371,9 +341,6 @@
     <t>vulture</t>
   </si>
   <si>
-    <t>TID_MISSION_GOBLINS_DESC</t>
-  </si>
-  <si>
     <t>icon_goblins</t>
   </si>
   <si>
@@ -383,9 +350,6 @@
     <t>goblins</t>
   </si>
   <si>
-    <t>TID_MISSION_SPIDERS_DESC</t>
-  </si>
-  <si>
     <t>icon_spiders</t>
   </si>
   <si>
@@ -410,9 +374,6 @@
     <t>fire_rushes</t>
   </si>
   <si>
-    <t>TID_MISSION_DRAGONS_DESC</t>
-  </si>
-  <si>
     <t>icon_dragon</t>
   </si>
   <si>
@@ -422,27 +383,18 @@
     <t>dragons</t>
   </si>
   <si>
-    <t>TID_MISSION_EGGS_DESC</t>
-  </si>
-  <si>
     <t>icon_egg</t>
   </si>
   <si>
     <t>eggs</t>
   </si>
   <si>
-    <t>TID_MISSION_COINS_DESC</t>
-  </si>
-  <si>
     <t>icon_money</t>
   </si>
   <si>
     <t>coins</t>
   </si>
   <si>
-    <t>TID_MISSION_HOUSES_DESC</t>
-  </si>
-  <si>
     <t>icon_cart</t>
   </si>
   <si>
@@ -458,19 +410,10 @@
     <t>houses</t>
   </si>
   <si>
-    <t>TID_MISSION_VILLAGERS_DESC</t>
-  </si>
-  <si>
     <t>icon_humans</t>
   </si>
   <si>
-    <t>Villager01;Villager02;BadFarmer;DrunkenMan;Merida;BoatFisher</t>
-  </si>
-  <si>
     <t>villagers</t>
-  </si>
-  <si>
-    <t>TID_MISSION_CANARIES_DESC</t>
   </si>
   <si>
     <t>icon_canary</t>
@@ -558,17 +501,200 @@
     <t>kill_chain</t>
   </si>
   <si>
-    <t>TID_MISSION_OBJECTIVE_KILL_CHAIN_DESC_SINGLE_RUN</t>
-  </si>
-  <si>
-    <t>kill_chain_birds</t>
+    <t>Sheep</t>
+  </si>
+  <si>
+    <t>SpiderSmall;SpiderRed</t>
+  </si>
+  <si>
+    <t>eat_gold</t>
+  </si>
+  <si>
+    <t>eat_suicidal</t>
+  </si>
+  <si>
+    <t>Worker</t>
+  </si>
+  <si>
+    <t>kill_chain_sheeps</t>
+  </si>
+  <si>
+    <t>eat_suicidal_goblins</t>
+  </si>
+  <si>
+    <t>eat_gold_generic</t>
+  </si>
+  <si>
+    <t>eat_gold_razorback</t>
+  </si>
+  <si>
+    <t>eat_gold_driller</t>
+  </si>
+  <si>
+    <t>eat_suicidal_cattle</t>
+  </si>
+  <si>
+    <t>Sheep; Cow; Horse</t>
+  </si>
+  <si>
+    <t>eat_suicidal_villagers</t>
+  </si>
+  <si>
+    <t>Villager01;Villager02</t>
+  </si>
+  <si>
+    <t>Hawk;OwlSmall;Vulture</t>
+  </si>
+  <si>
+    <t>eat_gold_fishes</t>
+  </si>
+  <si>
+    <t>Fish01_Generic;Fish02_Generic;Fish03_Generic</t>
+  </si>
+  <si>
+    <t>eat_gold_stingrayLarge</t>
+  </si>
+  <si>
+    <t>StingrayLarge</t>
+  </si>
+  <si>
+    <t>Razorback</t>
+  </si>
+  <si>
+    <t>eat_gold_piranha</t>
+  </si>
+  <si>
+    <t>Piranha</t>
+  </si>
+  <si>
+    <t>TID_EDIBLE_CANARY_PL</t>
+  </si>
+  <si>
+    <t>Villager01;Villager02;BadFarmer;DrunkenMan;BoatFisher</t>
+  </si>
+  <si>
+    <t>TID_MISSION_TARGET_VILLAGERS</t>
+  </si>
+  <si>
+    <t>TID_MISSION_TARGET_BUILDINGS</t>
+  </si>
+  <si>
+    <t>TID_EDIBLE_VULTURE_PL</t>
+  </si>
+  <si>
+    <t>TID_SC_NAME_PLURAL</t>
+  </si>
+  <si>
+    <t>TID_EGG_PLURAL</t>
+  </si>
+  <si>
+    <t>TID_EDIBLE_EVILDRAGON_PL</t>
+  </si>
+  <si>
+    <t>TID_EDIBLE_GOBLIN_PL</t>
+  </si>
+  <si>
+    <t>TID_EDIBLE_SPIDER_PL</t>
+  </si>
+  <si>
+    <t>TID_EDIBLE_FLYINGPIG_PL</t>
+  </si>
+  <si>
+    <t>TID_EDIBLE_BAT_PL</t>
+  </si>
+  <si>
+    <t>TID_EDIBLE_OWL_PL</t>
+  </si>
+  <si>
+    <t>TID_EDIBLE_LIONBIRD_PL</t>
+  </si>
+  <si>
+    <t>TID_EDIBLE_GOBLIN_DRILLER_PL</t>
+  </si>
+  <si>
+    <t>TID_EDIBLE_ARCHER_PL</t>
+  </si>
+  <si>
+    <t>TID_EDIBLE_SOLDIER_PL</t>
+  </si>
+  <si>
+    <t>TID_EDIBLE_TROLL_PL</t>
+  </si>
+  <si>
+    <t>TID_EDIBLE_SHEEP_PL</t>
+  </si>
+  <si>
+    <t>TID_EDIBLE_STINGRAY_PL</t>
+  </si>
+  <si>
+    <t>TID_EDIBLE_PIRANHA_PL</t>
+  </si>
+  <si>
+    <t>TID_EDIBLE_RAZORBACK_PL</t>
+  </si>
+  <si>
+    <t>TID_EDIBLE_FISH_PL</t>
+  </si>
+  <si>
+    <t>TID_MISSION_TARGET_BOATMAN</t>
+  </si>
+  <si>
+    <t>TID_MISSION_TARGET_BIRDSPREY</t>
+  </si>
+  <si>
+    <t>TID_MISSION_TARGET_CATTLE</t>
+  </si>
+  <si>
+    <t>TID_MISSION_OBJECTIVE_KILLCHAIN_DESC_SINGLE_RUN</t>
+  </si>
+  <si>
+    <t>TID_MISSION_OBJECTIVE_EATGOLD_DESC_SINGLE_RUN</t>
+  </si>
+  <si>
+    <t>TID_MISSION_OBJECTIVE_EATSUICIDAL_DESC_SINGLE_RUN</t>
+  </si>
+  <si>
+    <t>TID_MISSION_OBJECTIVE_EATHANG_DESC_SINGLE_RUN</t>
+  </si>
+  <si>
+    <t>TID_MISSION_OBJECTIVE_KILLCHAIN_DESC_MULTI_RUN</t>
+  </si>
+  <si>
+    <t>TID_MISSION_OBJECTIVE_EATHANG_DESC_MULTI_RUN</t>
+  </si>
+  <si>
+    <t>TID_MISSION_OBJECTIVE_EATGOLD_DESC_MULTI_RUN</t>
+  </si>
+  <si>
+    <t>TID_MISSION_OBJECTIVE_EATSUICIDAL_DESC_MULTI_RUN</t>
+  </si>
+  <si>
+    <t>eat_gold_birdsPrey</t>
+  </si>
+  <si>
+    <t>kill_chain_canary_01</t>
+  </si>
+  <si>
+    <t>Blue Canaries</t>
+  </si>
+  <si>
+    <t>TID_EDIBLE_CANARY_01_PL</t>
+  </si>
+  <si>
+    <t>eat_spec_anim_a</t>
+  </si>
+  <si>
+    <t>eat_chain</t>
+  </si>
+  <si>
+    <t>eat_spec_anim_a_spiders</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -611,6 +737,44 @@
       <i/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="4" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF0070C0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1" tint="4.9989318521683403E-2"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -708,7 +872,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -845,11 +1009,50 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color theme="8"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color theme="8"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color theme="8"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1"/>
@@ -946,6 +1149,67 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -959,14 +1223,88 @@
   </cellStyles>
   <dxfs count="67">
     <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom/>
+      </border>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -987,6 +1325,22 @@
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -997,110 +1351,10 @@
         <right style="thin">
           <color auto="1"/>
         </right>
-        <top/>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top/>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
         <top style="thin">
           <color auto="1"/>
         </top>
         <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
         <vertical/>
         <horizontal/>
       </border>
@@ -2029,6 +2283,16 @@
         </bottom>
       </border>
     </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -2043,94 +2307,94 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="missionDifficultyDefinitions" displayName="missionDifficultyDefinitions" ref="B49:K52" totalsRowShown="0" headerRowBorderDxfId="66" tableBorderDxfId="65">
-  <autoFilter ref="B49:K52"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="missionDifficultyDefinitions" displayName="missionDifficultyDefinitions" ref="B70:K73" totalsRowShown="0" headerRowBorderDxfId="65" tableBorderDxfId="64">
+  <autoFilter ref="B70:K73"/>
   <tableColumns count="10">
     <tableColumn id="1" name="{missionDifficultyDefinitions}"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="64"/>
-    <tableColumn id="7" name="[index]" dataDxfId="63"/>
-    <tableColumn id="3" name="[dragonsToUnlock]" dataDxfId="62"/>
-    <tableColumn id="4" name="[cooldownMinutes]" dataDxfId="61"/>
-    <tableColumn id="9" name="[maxRewardCoins]" dataDxfId="60"/>
-    <tableColumn id="5" name="[removeMissionPCCoefA]" dataDxfId="59"/>
-    <tableColumn id="6" name="[removeMissionPCCoefB]" dataDxfId="58"/>
-    <tableColumn id="8" name="[tidName]" dataDxfId="57"/>
-    <tableColumn id="10" name="[color]" dataDxfId="56"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="63"/>
+    <tableColumn id="7" name="[index]" dataDxfId="62"/>
+    <tableColumn id="3" name="[dragonsToUnlock]" dataDxfId="61"/>
+    <tableColumn id="4" name="[cooldownMinutes]" dataDxfId="60"/>
+    <tableColumn id="9" name="[maxRewardCoins]" dataDxfId="59"/>
+    <tableColumn id="5" name="[removeMissionPCCoefA]" dataDxfId="58"/>
+    <tableColumn id="6" name="[removeMissionPCCoefB]" dataDxfId="57"/>
+    <tableColumn id="8" name="[tidName]" dataDxfId="56"/>
+    <tableColumn id="10" name="[color]" dataDxfId="55"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table13303132" displayName="Table13303132" ref="B57:E67" totalsRowShown="0" headerRowDxfId="55" dataDxfId="53" headerRowBorderDxfId="54" tableBorderDxfId="52" totalsRowBorderDxfId="51">
-  <autoFilter ref="B57:E67"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table13303132" displayName="Table13303132" ref="B78:E88" totalsRowShown="0" headerRowDxfId="54" dataDxfId="52" headerRowBorderDxfId="53" tableBorderDxfId="51" totalsRowBorderDxfId="50">
+  <autoFilter ref="B78:E88"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="{missionDragonModifiersDefinitions}" dataDxfId="50"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="49"/>
-    <tableColumn id="7" name="[quantityModifier]" dataDxfId="48"/>
-    <tableColumn id="3" name="[missionSCRewardMultiplier]" dataDxfId="47"/>
+    <tableColumn id="1" name="{missionDragonModifiersDefinitions}" dataDxfId="49"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="48"/>
+    <tableColumn id="7" name="[quantityModifier]" dataDxfId="47"/>
+    <tableColumn id="3" name="[missionSCRewardMultiplier]" dataDxfId="46"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table1330313234" displayName="Table1330313234" ref="B71:D74" totalsRowShown="0" headerRowDxfId="46" dataDxfId="44" headerRowBorderDxfId="45" tableBorderDxfId="43" totalsRowBorderDxfId="42">
-  <autoFilter ref="B71:D74"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table1330313234" displayName="Table1330313234" ref="B92:D95" totalsRowShown="0" headerRowDxfId="45" dataDxfId="43" headerRowBorderDxfId="44" tableBorderDxfId="42" totalsRowBorderDxfId="41">
+  <autoFilter ref="B92:D95"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="{missionDifficultyModifiersDefinitions}" dataDxfId="41"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="40"/>
-    <tableColumn id="7" name="[quantityModifier]" dataDxfId="39"/>
+    <tableColumn id="1" name="{missionDifficultyModifiersDefinitions}" dataDxfId="40"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="39"/>
+    <tableColumn id="7" name="[quantityModifier]" dataDxfId="38"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table133031323435" displayName="Table133031323435" ref="B78:D79" totalsRowShown="0" headerRowDxfId="38" dataDxfId="36" headerRowBorderDxfId="37" tableBorderDxfId="35" totalsRowBorderDxfId="34">
-  <autoFilter ref="B78:D79"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table133031323435" displayName="Table133031323435" ref="B99:D100" totalsRowShown="0" headerRowDxfId="37" dataDxfId="35" headerRowBorderDxfId="36" tableBorderDxfId="34" totalsRowBorderDxfId="33">
+  <autoFilter ref="B99:D100"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="{missionOtherModifiersDefinitions}" dataDxfId="33"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="32"/>
-    <tableColumn id="7" name="[quantityModifier]" dataDxfId="31"/>
+    <tableColumn id="1" name="{missionOtherModifiersDefinitions}" dataDxfId="32"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="31"/>
+    <tableColumn id="7" name="[quantityModifier]" dataDxfId="30"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table13" displayName="Table13" ref="B36:H45" totalsRowShown="0" headerRowDxfId="30" dataDxfId="28" headerRowBorderDxfId="29" tableBorderDxfId="27" totalsRowBorderDxfId="26">
-  <autoFilter ref="B36:H45"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table13" displayName="Table13" ref="B53:H65" totalsRowShown="0" headerRowDxfId="29" dataDxfId="27" headerRowBorderDxfId="28" tableBorderDxfId="26" totalsRowBorderDxfId="25">
+  <autoFilter ref="B53:H65"/>
   <tableColumns count="7">
-    <tableColumn id="1" name="{missionTypeDefinitions}" dataDxfId="25"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="24"/>
-    <tableColumn id="3" name="[minTier]" dataDxfId="23"/>
-    <tableColumn id="6" name="[maxTier]" dataDxfId="22"/>
-    <tableColumn id="4" name="[weight]" dataDxfId="21"/>
-    <tableColumn id="9" name="[tidDescSingleRun]" dataDxfId="20"/>
-    <tableColumn id="10" name="[tidDescMultiRun]" dataDxfId="19"/>
+    <tableColumn id="1" name="{missionTypeDefinitions}" dataDxfId="24"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="23"/>
+    <tableColumn id="3" name="[minTier]" dataDxfId="22"/>
+    <tableColumn id="6" name="[maxTier]" dataDxfId="21"/>
+    <tableColumn id="4" name="[weight]" dataDxfId="20"/>
+    <tableColumn id="9" name="[tidDescSingleRun]" dataDxfId="19"/>
+    <tableColumn id="10" name="[tidDescMultiRun]" dataDxfId="18"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table1330" displayName="Table1330" ref="B4:N32" totalsRowShown="0" headerRowDxfId="18" dataDxfId="16" headerRowBorderDxfId="17" tableBorderDxfId="15" totalsRowBorderDxfId="14">
-  <autoFilter ref="B4:N32"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table1330" displayName="Table1330" ref="B4:N48" totalsRowShown="0" headerRowDxfId="17" dataDxfId="15" headerRowBorderDxfId="16" tableBorderDxfId="14" totalsRowBorderDxfId="13">
+  <autoFilter ref="B4:N48"/>
   <tableColumns count="13">
-    <tableColumn id="1" name="{missionsDefinitions}" dataDxfId="13"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="12"/>
-    <tableColumn id="7" name="[type]" dataDxfId="11"/>
-    <tableColumn id="8" name="[weight]" dataDxfId="10"/>
-    <tableColumn id="13" name="[singleRunChance]" dataDxfId="1"/>
-    <tableColumn id="11" name="[minTier]" dataDxfId="9"/>
-    <tableColumn id="12" name="[maxTier]" dataDxfId="8"/>
-    <tableColumn id="6" name="[params]" dataDxfId="7"/>
-    <tableColumn id="3" name="[objectiveBaseQuantityMin]" dataDxfId="6"/>
-    <tableColumn id="9" name="[objectiveBaseQuantityMax]" dataDxfId="5"/>
-    <tableColumn id="4" name="[icon]" dataDxfId="4"/>
-    <tableColumn id="5" name="[tidObjective]" dataDxfId="3"/>
-    <tableColumn id="10" name="[trackingSku]" dataDxfId="2"/>
+    <tableColumn id="1" name="{missionsDefinitions}" dataDxfId="12"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="11"/>
+    <tableColumn id="7" name="[type]" dataDxfId="10"/>
+    <tableColumn id="8" name="[weight]" dataDxfId="9"/>
+    <tableColumn id="13" name="[singleRunChance]" dataDxfId="8"/>
+    <tableColumn id="11" name="[minTier]" dataDxfId="7"/>
+    <tableColumn id="12" name="[maxTier]" dataDxfId="6"/>
+    <tableColumn id="6" name="[params]" dataDxfId="5"/>
+    <tableColumn id="3" name="[objectiveBaseQuantityMin]" dataDxfId="4"/>
+    <tableColumn id="9" name="[objectiveBaseQuantityMax]" dataDxfId="3"/>
+    <tableColumn id="4" name="[icon]" dataDxfId="2"/>
+    <tableColumn id="5" name="[tidObjective]" dataDxfId="1"/>
+    <tableColumn id="10" name="[trackingSku]" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2402,34 +2666,30 @@
   <sheetPr>
     <tabColor theme="6"/>
   </sheetPr>
-  <dimension ref="B1:P79"/>
+  <dimension ref="B1:P100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" zoomScale="125" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D40" sqref="D40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.6640625" customWidth="1"/>
-    <col min="2" max="2" width="17" customWidth="1"/>
-    <col min="3" max="3" width="16.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.33203125" customWidth="1"/>
-    <col min="6" max="6" width="21" customWidth="1"/>
-    <col min="7" max="7" width="46.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="48" customWidth="1"/>
-    <col min="9" max="9" width="49.5" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="52" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="28.83203125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="46.6640625" customWidth="1"/>
-    <col min="14" max="14" width="23.83203125" customWidth="1"/>
+    <col min="1" max="1" width="7" customWidth="1"/>
+    <col min="2" max="6" width="18.7109375" customWidth="1"/>
+    <col min="7" max="7" width="25.28515625" customWidth="1"/>
+    <col min="8" max="8" width="18.7109375" customWidth="1"/>
+    <col min="9" max="9" width="36" customWidth="1"/>
+    <col min="10" max="11" width="18.7109375" customWidth="1"/>
+    <col min="12" max="12" width="17.140625" customWidth="1"/>
+    <col min="13" max="13" width="26.140625" customWidth="1"/>
+    <col min="14" max="14" width="8.42578125" customWidth="1"/>
     <col min="15" max="16" width="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:16" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="2:16" ht="24" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:16" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B2" s="6" t="s">
-        <v>166</v>
+        <v>147</v>
       </c>
       <c r="C2" s="6"/>
       <c r="D2" s="6"/>
@@ -2442,41 +2702,41 @@
       <c r="K2" s="6"/>
       <c r="L2" s="6"/>
     </row>
-    <row r="3" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:16" ht="45" x14ac:dyDescent="0.25">
       <c r="B3" s="20"/>
       <c r="C3" s="38"/>
       <c r="D3" s="38"/>
       <c r="E3" s="39" t="s">
-        <v>165</v>
+        <v>146</v>
       </c>
       <c r="F3" s="39" t="s">
-        <v>164</v>
+        <v>145</v>
       </c>
       <c r="G3" s="38"/>
-      <c r="J3" s="40" t="s">
-        <v>163</v>
-      </c>
-      <c r="K3" s="40"/>
-      <c r="M3" s="40"/>
-      <c r="N3" s="40"/>
-      <c r="O3" s="40"/>
-      <c r="P3" s="40"/>
-    </row>
-    <row r="4" spans="2:16" ht="108" x14ac:dyDescent="0.2">
+      <c r="J3" s="61" t="s">
+        <v>144</v>
+      </c>
+      <c r="K3" s="61"/>
+      <c r="M3" s="61"/>
+      <c r="N3" s="61"/>
+      <c r="O3" s="61"/>
+      <c r="P3" s="61"/>
+    </row>
+    <row r="4" spans="2:16" ht="106.5" x14ac:dyDescent="0.25">
       <c r="B4" s="30" t="s">
-        <v>162</v>
+        <v>143</v>
       </c>
       <c r="C4" s="28" t="s">
         <v>3</v>
       </c>
       <c r="D4" s="37" t="s">
-        <v>161</v>
+        <v>142</v>
       </c>
       <c r="E4" s="37" t="s">
         <v>68</v>
       </c>
       <c r="F4" s="37" t="s">
-        <v>167</v>
+        <v>148</v>
       </c>
       <c r="G4" s="37" t="s">
         <v>70</v>
@@ -2485,30 +2745,30 @@
         <v>69</v>
       </c>
       <c r="I4" s="37" t="s">
-        <v>160</v>
+        <v>141</v>
       </c>
       <c r="J4" s="37" t="s">
-        <v>159</v>
+        <v>140</v>
       </c>
       <c r="K4" s="37" t="s">
-        <v>158</v>
+        <v>139</v>
       </c>
       <c r="L4" s="36" t="s">
-        <v>157</v>
+        <v>138</v>
       </c>
       <c r="M4" s="36" t="s">
-        <v>156</v>
+        <v>137</v>
       </c>
       <c r="N4" s="35" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="5" spans="2:16" x14ac:dyDescent="0.2">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="5" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B5" s="27" t="s">
         <v>1</v>
       </c>
       <c r="C5" s="24" t="s">
-        <v>154</v>
+        <v>135</v>
       </c>
       <c r="D5" s="24" t="s">
         <v>65</v>
@@ -2526,7 +2786,7 @@
         <v>7</v>
       </c>
       <c r="I5" s="24" t="s">
-        <v>150</v>
+        <v>131</v>
       </c>
       <c r="J5" s="24">
         <v>500</v>
@@ -2535,21 +2795,21 @@
         <v>600</v>
       </c>
       <c r="L5" s="33" t="s">
-        <v>149</v>
+        <v>130</v>
       </c>
       <c r="M5" s="33" t="s">
-        <v>148</v>
+        <v>172</v>
       </c>
       <c r="N5" s="31" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="6" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B6" s="27" t="s">
         <v>1</v>
       </c>
       <c r="C6" s="24" t="s">
-        <v>153</v>
+        <v>134</v>
       </c>
       <c r="D6" s="23" t="s">
         <v>53</v>
@@ -2574,19 +2834,19 @@
         <v>600</v>
       </c>
       <c r="L6" s="33" t="s">
-        <v>124</v>
+        <v>112</v>
       </c>
       <c r="M6" s="33"/>
       <c r="N6" s="31" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="7" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B7" s="27" t="s">
         <v>1</v>
       </c>
       <c r="C7" s="24" t="s">
-        <v>152</v>
+        <v>133</v>
       </c>
       <c r="D7" s="24" t="s">
         <v>59</v>
@@ -2611,19 +2871,19 @@
         <v>10000</v>
       </c>
       <c r="L7" s="33" t="s">
-        <v>123</v>
+        <v>111</v>
       </c>
       <c r="M7" s="33"/>
       <c r="N7" s="31" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="8" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B8" s="27" t="s">
         <v>1</v>
       </c>
       <c r="C8" s="24" t="s">
-        <v>151</v>
+        <v>132</v>
       </c>
       <c r="D8" s="24" t="s">
         <v>65</v>
@@ -2641,7 +2901,7 @@
         <v>7</v>
       </c>
       <c r="I8" s="24" t="s">
-        <v>150</v>
+        <v>131</v>
       </c>
       <c r="J8" s="24">
         <v>700</v>
@@ -2650,21 +2910,21 @@
         <v>750</v>
       </c>
       <c r="L8" s="33" t="s">
-        <v>149</v>
+        <v>130</v>
       </c>
       <c r="M8" s="33" t="s">
-        <v>148</v>
+        <v>172</v>
       </c>
       <c r="N8" s="31" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="9" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B9" s="27" t="s">
         <v>1</v>
       </c>
       <c r="C9" s="24" t="s">
-        <v>147</v>
+        <v>129</v>
       </c>
       <c r="D9" s="24" t="s">
         <v>65</v>
@@ -2682,7 +2942,7 @@
         <v>7</v>
       </c>
       <c r="I9" s="24" t="s">
-        <v>146</v>
+        <v>173</v>
       </c>
       <c r="J9" s="24">
         <v>25</v>
@@ -2691,21 +2951,21 @@
         <v>30</v>
       </c>
       <c r="L9" s="33" t="s">
-        <v>145</v>
-      </c>
-      <c r="M9" s="33" t="s">
-        <v>144</v>
+        <v>128</v>
+      </c>
+      <c r="M9" s="48" t="s">
+        <v>174</v>
       </c>
       <c r="N9" s="31" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="10" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B10" s="27" t="s">
         <v>1</v>
       </c>
       <c r="C10" s="24" t="s">
-        <v>143</v>
+        <v>127</v>
       </c>
       <c r="D10" s="23" t="s">
         <v>56</v>
@@ -2723,7 +2983,7 @@
         <v>3</v>
       </c>
       <c r="I10" s="23" t="s">
-        <v>140</v>
+        <v>124</v>
       </c>
       <c r="J10" s="24">
         <v>10</v>
@@ -2732,21 +2992,21 @@
         <v>12</v>
       </c>
       <c r="L10" s="33" t="s">
-        <v>142</v>
-      </c>
-      <c r="M10" s="33" t="s">
-        <v>138</v>
+        <v>126</v>
+      </c>
+      <c r="M10" s="48" t="s">
+        <v>175</v>
       </c>
       <c r="N10" s="31" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="11" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B11" s="27" t="s">
         <v>1</v>
       </c>
       <c r="C11" s="24" t="s">
-        <v>141</v>
+        <v>125</v>
       </c>
       <c r="D11" s="23" t="s">
         <v>56</v>
@@ -2764,7 +3024,7 @@
         <v>7</v>
       </c>
       <c r="I11" s="23" t="s">
-        <v>140</v>
+        <v>124</v>
       </c>
       <c r="J11" s="24">
         <v>8</v>
@@ -2773,21 +3033,21 @@
         <v>9</v>
       </c>
       <c r="L11" s="33" t="s">
-        <v>139</v>
-      </c>
-      <c r="M11" s="33" t="s">
-        <v>138</v>
+        <v>123</v>
+      </c>
+      <c r="M11" s="48" t="s">
+        <v>175</v>
       </c>
       <c r="N11" s="31" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="12" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B12" s="27" t="s">
         <v>1</v>
       </c>
       <c r="C12" s="24" t="s">
-        <v>137</v>
+        <v>122</v>
       </c>
       <c r="D12" s="24" t="s">
         <v>50</v>
@@ -2805,7 +3065,7 @@
         <v>7</v>
       </c>
       <c r="I12" s="24" t="s">
-        <v>137</v>
+        <v>122</v>
       </c>
       <c r="J12" s="24">
         <v>1000</v>
@@ -2814,21 +3074,21 @@
         <v>1200</v>
       </c>
       <c r="L12" s="33" t="s">
-        <v>136</v>
+        <v>121</v>
       </c>
       <c r="M12" s="33" t="s">
-        <v>135</v>
+        <v>177</v>
       </c>
       <c r="N12" s="31" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="13" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B13" s="25" t="s">
         <v>1</v>
       </c>
       <c r="C13" s="23" t="s">
-        <v>134</v>
+        <v>120</v>
       </c>
       <c r="D13" s="24" t="s">
         <v>50</v>
@@ -2846,7 +3106,7 @@
         <v>1</v>
       </c>
       <c r="I13" s="23" t="s">
-        <v>134</v>
+        <v>120</v>
       </c>
       <c r="J13" s="24">
         <v>1</v>
@@ -2855,21 +3115,21 @@
         <v>2</v>
       </c>
       <c r="L13" s="33" t="s">
-        <v>133</v>
+        <v>119</v>
       </c>
       <c r="M13" s="33" t="s">
-        <v>132</v>
+        <v>178</v>
       </c>
       <c r="N13" s="31" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="14" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B14" s="25" t="s">
         <v>1</v>
       </c>
       <c r="C14" s="24" t="s">
-        <v>131</v>
+        <v>118</v>
       </c>
       <c r="D14" s="24" t="s">
         <v>65</v>
@@ -2887,7 +3147,7 @@
         <v>7</v>
       </c>
       <c r="I14" s="24" t="s">
-        <v>130</v>
+        <v>117</v>
       </c>
       <c r="J14" s="24">
         <v>10</v>
@@ -2896,21 +3156,21 @@
         <v>11</v>
       </c>
       <c r="L14" s="33" t="s">
-        <v>129</v>
-      </c>
-      <c r="M14" s="33" t="s">
-        <v>128</v>
+        <v>116</v>
+      </c>
+      <c r="M14" s="48" t="s">
+        <v>179</v>
       </c>
       <c r="N14" s="31" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="15" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B15" s="25" t="s">
         <v>1</v>
       </c>
       <c r="C15" s="24" t="s">
-        <v>127</v>
+        <v>115</v>
       </c>
       <c r="D15" s="24" t="s">
         <v>62</v>
@@ -2935,14 +3195,14 @@
         <v>6</v>
       </c>
       <c r="L15" s="33" t="s">
-        <v>126</v>
+        <v>114</v>
       </c>
       <c r="M15" s="33"/>
       <c r="N15" s="31" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="16" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B16" s="25" t="s">
         <v>1</v>
       </c>
@@ -2972,14 +3232,14 @@
         <v>800</v>
       </c>
       <c r="L16" s="33" t="s">
-        <v>125</v>
+        <v>113</v>
       </c>
       <c r="M16" s="33"/>
       <c r="N16" s="31" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="17" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B17" s="25" t="s">
         <v>1</v>
       </c>
@@ -3009,14 +3269,14 @@
         <v>400</v>
       </c>
       <c r="L17" s="33" t="s">
-        <v>124</v>
+        <v>112</v>
       </c>
       <c r="M17" s="33"/>
       <c r="N17" s="31" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="18" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B18" s="25" t="s">
         <v>1</v>
       </c>
@@ -3046,19 +3306,19 @@
         <v>500000</v>
       </c>
       <c r="L18" s="33" t="s">
-        <v>123</v>
+        <v>111</v>
       </c>
       <c r="M18" s="33"/>
       <c r="N18" s="31" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="19" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B19" s="25" t="s">
         <v>1</v>
       </c>
       <c r="C19" s="23" t="s">
-        <v>122</v>
+        <v>110</v>
       </c>
       <c r="D19" s="23" t="s">
         <v>65</v>
@@ -3076,7 +3336,7 @@
         <v>7</v>
       </c>
       <c r="I19" s="23" t="s">
-        <v>121</v>
+        <v>109</v>
       </c>
       <c r="J19" s="24">
         <v>45</v>
@@ -3085,21 +3345,21 @@
         <v>55</v>
       </c>
       <c r="L19" s="34" t="s">
-        <v>120</v>
-      </c>
-      <c r="M19" s="33" t="s">
-        <v>119</v>
+        <v>108</v>
+      </c>
+      <c r="M19" s="48" t="s">
+        <v>181</v>
       </c>
       <c r="N19" s="31" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="20" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B20" s="25" t="s">
         <v>1</v>
       </c>
       <c r="C20" s="23" t="s">
-        <v>118</v>
+        <v>107</v>
       </c>
       <c r="D20" s="23" t="s">
         <v>65</v>
@@ -3117,7 +3377,7 @@
         <v>7</v>
       </c>
       <c r="I20" s="23" t="s">
-        <v>117</v>
+        <v>106</v>
       </c>
       <c r="J20" s="24">
         <v>40</v>
@@ -3126,21 +3386,21 @@
         <v>45</v>
       </c>
       <c r="L20" s="34" t="s">
-        <v>116</v>
+        <v>105</v>
       </c>
       <c r="M20" s="33" t="s">
-        <v>115</v>
+        <v>180</v>
       </c>
       <c r="N20" s="31" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="21" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B21" s="25" t="s">
         <v>1</v>
       </c>
       <c r="C21" s="23" t="s">
-        <v>114</v>
+        <v>104</v>
       </c>
       <c r="D21" s="23" t="s">
         <v>65</v>
@@ -3158,7 +3418,7 @@
         <v>2</v>
       </c>
       <c r="I21" s="23" t="s">
-        <v>113</v>
+        <v>103</v>
       </c>
       <c r="J21" s="23">
         <v>10</v>
@@ -3167,21 +3427,21 @@
         <v>12</v>
       </c>
       <c r="L21" s="34" t="s">
-        <v>112</v>
-      </c>
-      <c r="M21" s="34" t="s">
-        <v>111</v>
+        <v>102</v>
+      </c>
+      <c r="M21" s="51" t="s">
+        <v>176</v>
       </c>
       <c r="N21" s="31" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="22" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B22" s="27" t="s">
         <v>1</v>
       </c>
       <c r="C22" s="24" t="s">
-        <v>110</v>
+        <v>101</v>
       </c>
       <c r="D22" s="23" t="s">
         <v>65</v>
@@ -3199,7 +3459,7 @@
         <v>1</v>
       </c>
       <c r="I22" s="23" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="J22" s="24">
         <v>5</v>
@@ -3208,21 +3468,21 @@
         <v>6</v>
       </c>
       <c r="L22" s="34" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
       <c r="M22" s="34" t="s">
-        <v>107</v>
+        <v>182</v>
       </c>
       <c r="N22" s="31" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="23" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B23" s="27" t="s">
         <v>1</v>
       </c>
       <c r="C23" s="24" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="D23" s="23" t="s">
         <v>65</v>
@@ -3240,7 +3500,7 @@
         <v>7</v>
       </c>
       <c r="I23" s="23" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
       <c r="J23" s="24">
         <v>150</v>
@@ -3249,21 +3509,21 @@
         <v>200</v>
       </c>
       <c r="L23" s="34" t="s">
-        <v>104</v>
-      </c>
-      <c r="M23" s="34" t="s">
-        <v>103</v>
+        <v>96</v>
+      </c>
+      <c r="M23" s="51" t="s">
+        <v>183</v>
       </c>
       <c r="N23" s="31" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="24" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B24" s="27" t="s">
         <v>1</v>
       </c>
       <c r="C24" s="24" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="D24" s="23" t="s">
         <v>65</v>
@@ -3281,7 +3541,7 @@
         <v>7</v>
       </c>
       <c r="I24" s="23" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="J24" s="24">
         <v>5</v>
@@ -3290,21 +3550,21 @@
         <v>7</v>
       </c>
       <c r="L24" s="34" t="s">
-        <v>100</v>
-      </c>
-      <c r="M24" s="34" t="s">
-        <v>99</v>
+        <v>93</v>
+      </c>
+      <c r="M24" s="52" t="s">
+        <v>184</v>
       </c>
       <c r="N24" s="31" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="25" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B25" s="27" t="s">
         <v>1</v>
       </c>
       <c r="C25" s="24" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="D25" s="23" t="s">
         <v>65</v>
@@ -3322,7 +3582,7 @@
         <v>7</v>
       </c>
       <c r="I25" s="23" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="J25" s="24">
         <v>5</v>
@@ -3331,21 +3591,21 @@
         <v>7</v>
       </c>
       <c r="L25" s="34" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="M25" s="34" t="s">
-        <v>95</v>
+        <v>185</v>
       </c>
       <c r="N25" s="31" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="26" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B26" s="27" t="s">
         <v>1</v>
       </c>
       <c r="C26" s="24" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="D26" s="23" t="s">
         <v>65</v>
@@ -3363,7 +3623,7 @@
         <v>7</v>
       </c>
       <c r="I26" s="23" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="J26" s="24">
         <v>3</v>
@@ -3372,21 +3632,21 @@
         <v>4</v>
       </c>
       <c r="L26" s="34" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="M26" s="34" t="s">
-        <v>91</v>
+        <v>186</v>
       </c>
       <c r="N26" s="31" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="27" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B27" s="27" t="s">
         <v>1</v>
       </c>
       <c r="C27" s="24" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="D27" s="23" t="s">
         <v>65</v>
@@ -3404,7 +3664,7 @@
         <v>7</v>
       </c>
       <c r="I27" s="23" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="J27" s="24">
         <v>3</v>
@@ -3413,21 +3673,21 @@
         <v>3.5</v>
       </c>
       <c r="L27" s="34" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="M27" s="34" t="s">
-        <v>87</v>
+        <v>195</v>
       </c>
       <c r="N27" s="31" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="28" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B28" s="27" t="s">
         <v>1</v>
       </c>
       <c r="C28" s="24" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="D28" s="23" t="s">
         <v>65</v>
@@ -3445,7 +3705,7 @@
         <v>7</v>
       </c>
       <c r="I28" s="23" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="J28" s="24">
         <v>8</v>
@@ -3454,21 +3714,21 @@
         <v>9</v>
       </c>
       <c r="L28" s="34" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="M28" s="34" t="s">
-        <v>83</v>
+        <v>187</v>
       </c>
       <c r="N28" s="31" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="29" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B29" s="27" t="s">
         <v>1</v>
       </c>
       <c r="C29" s="24" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D29" s="23" t="s">
         <v>65</v>
@@ -3486,7 +3746,7 @@
         <v>7</v>
       </c>
       <c r="I29" s="23" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="J29" s="24">
         <v>11</v>
@@ -3495,21 +3755,21 @@
         <v>12</v>
       </c>
       <c r="L29" s="34" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="M29" s="34" t="s">
-        <v>79</v>
+        <v>188</v>
       </c>
       <c r="N29" s="31" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="30" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B30" s="27" t="s">
         <v>1</v>
       </c>
       <c r="C30" s="24" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D30" s="23" t="s">
         <v>65</v>
@@ -3527,7 +3787,7 @@
         <v>7</v>
       </c>
       <c r="I30" s="23" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="J30" s="24">
         <v>3</v>
@@ -3536,16 +3796,16 @@
         <v>3.5</v>
       </c>
       <c r="L30" s="34" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="M30" s="34" t="s">
-        <v>75</v>
+        <v>189</v>
       </c>
       <c r="N30" s="31" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="31" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B31" s="27" t="s">
         <v>1</v>
       </c>
@@ -3582,698 +3842,1117 @@
         <v>73</v>
       </c>
     </row>
-    <row r="32" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B32" s="27" t="s">
-        <v>1</v>
-      </c>
-      <c r="C32" s="24" t="s">
+    <row r="32" spans="2:14" s="44" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B32" s="53" t="s">
+        <v>1</v>
+      </c>
+      <c r="C32" s="54" t="s">
+        <v>155</v>
+      </c>
+      <c r="D32" s="55" t="s">
+        <v>149</v>
+      </c>
+      <c r="E32" s="55">
+        <v>1</v>
+      </c>
+      <c r="F32" s="55">
+        <v>0.3</v>
+      </c>
+      <c r="G32" s="54">
+        <v>0</v>
+      </c>
+      <c r="H32" s="55">
+        <v>7</v>
+      </c>
+      <c r="I32" s="55" t="s">
+        <v>150</v>
+      </c>
+      <c r="J32" s="54">
+        <v>99</v>
+      </c>
+      <c r="K32" s="55">
+        <v>99</v>
+      </c>
+      <c r="L32" s="49" t="s">
+        <v>130</v>
+      </c>
+      <c r="M32" s="49" t="s">
+        <v>190</v>
+      </c>
+      <c r="N32" s="56" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="33" spans="2:14" s="44" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B33" s="53" t="s">
+        <v>1</v>
+      </c>
+      <c r="C33" s="54" t="s">
+        <v>207</v>
+      </c>
+      <c r="D33" s="55" t="s">
+        <v>149</v>
+      </c>
+      <c r="E33" s="55">
+        <v>1</v>
+      </c>
+      <c r="F33" s="55">
+        <v>0.3</v>
+      </c>
+      <c r="G33" s="54">
+        <v>0</v>
+      </c>
+      <c r="H33" s="55">
+        <v>7</v>
+      </c>
+      <c r="I33" s="55" t="s">
+        <v>208</v>
+      </c>
+      <c r="J33" s="54">
+        <v>99</v>
+      </c>
+      <c r="K33" s="55">
+        <v>99</v>
+      </c>
+      <c r="L33" s="49" t="s">
+        <v>130</v>
+      </c>
+      <c r="M33" s="49" t="s">
+        <v>209</v>
+      </c>
+      <c r="N33" s="56" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="34" spans="2:14" s="44" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B34" s="53"/>
+      <c r="C34" s="54"/>
+      <c r="D34" s="55"/>
+      <c r="E34" s="55"/>
+      <c r="F34" s="55"/>
+      <c r="G34" s="54"/>
+      <c r="H34" s="55"/>
+      <c r="I34" s="55"/>
+      <c r="J34" s="54"/>
+      <c r="K34" s="55"/>
+      <c r="L34" s="49"/>
+      <c r="M34" s="58"/>
+      <c r="N34" s="56"/>
+    </row>
+    <row r="35" spans="2:14" s="44" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B35" s="53" t="s">
+        <v>1</v>
+      </c>
+      <c r="C35" s="54" t="s">
+        <v>212</v>
+      </c>
+      <c r="D35" s="55" t="s">
+        <v>210</v>
+      </c>
+      <c r="E35" s="55">
+        <v>1</v>
+      </c>
+      <c r="F35" s="55">
+        <v>0.3</v>
+      </c>
+      <c r="G35" s="54">
+        <v>0</v>
+      </c>
+      <c r="H35" s="55">
+        <v>7</v>
+      </c>
+      <c r="I35" s="55" t="s">
+        <v>151</v>
+      </c>
+      <c r="J35" s="54">
+        <v>99</v>
+      </c>
+      <c r="K35" s="55">
+        <v>99</v>
+      </c>
+      <c r="L35" s="49" t="s">
+        <v>130</v>
+      </c>
+      <c r="M35" s="49" t="s">
+        <v>181</v>
+      </c>
+      <c r="N35" s="56" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="36" spans="2:14" s="44" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B36" s="53"/>
+      <c r="C36" s="54"/>
+      <c r="D36" s="55"/>
+      <c r="E36" s="55"/>
+      <c r="F36" s="55"/>
+      <c r="G36" s="54"/>
+      <c r="H36" s="55"/>
+      <c r="I36" s="55"/>
+      <c r="J36" s="54"/>
+      <c r="K36" s="55"/>
+      <c r="L36" s="49"/>
+      <c r="M36" s="50"/>
+      <c r="N36" s="56"/>
+    </row>
+    <row r="37" spans="2:14" s="44" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B37" s="53" t="s">
+        <v>1</v>
+      </c>
+      <c r="C37" s="54" t="s">
+        <v>157</v>
+      </c>
+      <c r="D37" s="55" t="s">
+        <v>152</v>
+      </c>
+      <c r="E37" s="55">
+        <v>1</v>
+      </c>
+      <c r="F37" s="55">
+        <v>0.3</v>
+      </c>
+      <c r="G37" s="54">
+        <v>0</v>
+      </c>
+      <c r="H37" s="55">
+        <v>7</v>
+      </c>
+      <c r="I37" s="55"/>
+      <c r="J37" s="54">
+        <v>99</v>
+      </c>
+      <c r="K37" s="55">
+        <v>99</v>
+      </c>
+      <c r="L37" s="49" t="s">
+        <v>130</v>
+      </c>
+      <c r="M37" s="50"/>
+      <c r="N37" s="56" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="38" spans="2:14" s="44" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B38" s="53" t="s">
+        <v>1</v>
+      </c>
+      <c r="C38" s="54" t="s">
+        <v>167</v>
+      </c>
+      <c r="D38" s="55" t="s">
+        <v>152</v>
+      </c>
+      <c r="E38" s="55">
+        <v>1</v>
+      </c>
+      <c r="F38" s="55">
+        <v>0.3</v>
+      </c>
+      <c r="G38" s="54">
+        <v>3</v>
+      </c>
+      <c r="H38" s="55">
+        <v>7</v>
+      </c>
+      <c r="I38" s="55" t="s">
+        <v>168</v>
+      </c>
+      <c r="J38" s="54">
+        <v>99</v>
+      </c>
+      <c r="K38" s="55">
+        <v>99</v>
+      </c>
+      <c r="L38" s="49" t="s">
+        <v>130</v>
+      </c>
+      <c r="M38" s="55" t="s">
+        <v>191</v>
+      </c>
+      <c r="N38" s="56" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="39" spans="2:14" s="44" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B39" s="53"/>
+      <c r="C39" s="54" t="s">
         <v>170</v>
       </c>
-      <c r="D32" s="23" t="s">
-        <v>168</v>
-      </c>
-      <c r="E32" s="23">
-        <v>1</v>
-      </c>
-      <c r="F32" s="23">
-        <v>1</v>
-      </c>
-      <c r="G32" s="24">
+      <c r="D39" s="55" t="s">
+        <v>152</v>
+      </c>
+      <c r="E39" s="55">
+        <v>1</v>
+      </c>
+      <c r="F39" s="55">
+        <v>0.3</v>
+      </c>
+      <c r="G39" s="54">
+        <v>1</v>
+      </c>
+      <c r="H39" s="55">
+        <v>7</v>
+      </c>
+      <c r="I39" s="55" t="s">
+        <v>171</v>
+      </c>
+      <c r="J39" s="54">
+        <v>99</v>
+      </c>
+      <c r="K39" s="55">
+        <v>99</v>
+      </c>
+      <c r="L39" s="49" t="s">
+        <v>130</v>
+      </c>
+      <c r="M39" s="55" t="s">
+        <v>192</v>
+      </c>
+      <c r="N39" s="56" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="40" spans="2:14" s="44" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B40" s="53" t="s">
+        <v>1</v>
+      </c>
+      <c r="C40" s="54" t="s">
+        <v>158</v>
+      </c>
+      <c r="D40" s="55" t="s">
+        <v>152</v>
+      </c>
+      <c r="E40" s="55">
+        <v>1</v>
+      </c>
+      <c r="F40" s="55">
+        <v>0.3</v>
+      </c>
+      <c r="G40" s="54">
+        <v>2</v>
+      </c>
+      <c r="H40" s="55">
+        <v>7</v>
+      </c>
+      <c r="I40" s="55" t="s">
+        <v>169</v>
+      </c>
+      <c r="J40" s="54">
+        <v>99</v>
+      </c>
+      <c r="K40" s="55">
+        <v>99</v>
+      </c>
+      <c r="L40" s="49" t="s">
+        <v>130</v>
+      </c>
+      <c r="M40" s="55" t="s">
+        <v>193</v>
+      </c>
+      <c r="N40" s="56" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="41" spans="2:14" s="44" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B41" s="53"/>
+      <c r="C41" s="54" t="s">
+        <v>159</v>
+      </c>
+      <c r="D41" s="55" t="s">
+        <v>152</v>
+      </c>
+      <c r="E41" s="55">
+        <v>1</v>
+      </c>
+      <c r="F41" s="55">
+        <v>0.3</v>
+      </c>
+      <c r="G41" s="54">
+        <v>4</v>
+      </c>
+      <c r="H41" s="55">
+        <v>7</v>
+      </c>
+      <c r="I41" s="55" t="s">
+        <v>88</v>
+      </c>
+      <c r="J41" s="54">
+        <v>99</v>
+      </c>
+      <c r="K41" s="55">
+        <v>99</v>
+      </c>
+      <c r="L41" s="49" t="s">
+        <v>130</v>
+      </c>
+      <c r="M41" s="55" t="s">
+        <v>186</v>
+      </c>
+      <c r="N41" s="56" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="42" spans="2:14" s="44" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B42" s="53" t="s">
+        <v>1</v>
+      </c>
+      <c r="C42" s="54" t="s">
+        <v>165</v>
+      </c>
+      <c r="D42" s="55" t="s">
+        <v>152</v>
+      </c>
+      <c r="E42" s="55">
+        <v>1</v>
+      </c>
+      <c r="F42" s="55">
+        <v>0.3</v>
+      </c>
+      <c r="G42" s="54">
         <v>0</v>
       </c>
-      <c r="H32" s="23">
+      <c r="H42" s="55">
         <v>7</v>
       </c>
-      <c r="I32" s="23" t="s">
-        <v>150</v>
-      </c>
-      <c r="J32" s="24">
-        <v>999</v>
-      </c>
-      <c r="K32" s="23">
-        <v>999</v>
-      </c>
-      <c r="L32" s="33" t="s">
-        <v>149</v>
-      </c>
-      <c r="M32" s="33" t="s">
-        <v>148</v>
-      </c>
-      <c r="N32" s="31" t="s">
+      <c r="I42" s="55" t="s">
+        <v>166</v>
+      </c>
+      <c r="J42" s="54">
+        <v>99</v>
+      </c>
+      <c r="K42" s="55">
+        <v>99</v>
+      </c>
+      <c r="L42" s="49" t="s">
+        <v>130</v>
+      </c>
+      <c r="M42" s="50" t="s">
+        <v>194</v>
+      </c>
+      <c r="N42" s="56" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="33" spans="2:13" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B33" s="32"/>
-      <c r="C33" s="32"/>
-      <c r="D33" s="32"/>
-      <c r="E33" s="32"/>
-      <c r="F33" s="32"/>
-      <c r="G33" s="32"/>
-      <c r="H33" s="32"/>
-      <c r="I33" s="32"/>
-      <c r="J33" s="32"/>
-      <c r="K33" s="32"/>
-      <c r="L33" s="32"/>
-      <c r="M33" s="31"/>
-    </row>
-    <row r="34" spans="2:13" ht="24" x14ac:dyDescent="0.3">
-      <c r="B34" s="6" t="s">
+    <row r="43" spans="2:14" s="44" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B43" s="53" t="s">
+        <v>1</v>
+      </c>
+      <c r="C43" s="54" t="s">
+        <v>206</v>
+      </c>
+      <c r="D43" s="55" t="s">
+        <v>152</v>
+      </c>
+      <c r="E43" s="55">
+        <v>1</v>
+      </c>
+      <c r="F43" s="55">
+        <v>0.3</v>
+      </c>
+      <c r="G43" s="54">
+        <v>0</v>
+      </c>
+      <c r="H43" s="55">
+        <v>7</v>
+      </c>
+      <c r="I43" s="55" t="s">
+        <v>164</v>
+      </c>
+      <c r="J43" s="54">
+        <v>99</v>
+      </c>
+      <c r="K43" s="55">
+        <v>99</v>
+      </c>
+      <c r="L43" s="49" t="s">
+        <v>130</v>
+      </c>
+      <c r="M43" s="50" t="s">
+        <v>196</v>
+      </c>
+      <c r="N43" s="56" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="44" spans="2:14" s="44" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B44" s="53"/>
+      <c r="C44" s="54"/>
+      <c r="D44" s="55"/>
+      <c r="E44" s="55"/>
+      <c r="F44" s="55"/>
+      <c r="G44" s="54"/>
+      <c r="H44" s="55"/>
+      <c r="I44" s="55"/>
+      <c r="J44" s="54"/>
+      <c r="K44" s="55"/>
+      <c r="L44" s="49"/>
+      <c r="M44" s="50"/>
+      <c r="N44" s="56"/>
+    </row>
+    <row r="45" spans="2:14" s="44" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B45" s="53" t="s">
+        <v>1</v>
+      </c>
+      <c r="C45" s="54" t="s">
+        <v>156</v>
+      </c>
+      <c r="D45" s="55" t="s">
+        <v>153</v>
+      </c>
+      <c r="E45" s="55">
+        <v>1</v>
+      </c>
+      <c r="F45" s="55">
+        <v>0.3</v>
+      </c>
+      <c r="G45" s="54">
+        <v>0</v>
+      </c>
+      <c r="H45" s="55">
+        <v>7</v>
+      </c>
+      <c r="I45" s="55" t="s">
+        <v>154</v>
+      </c>
+      <c r="J45" s="54">
+        <v>99</v>
+      </c>
+      <c r="K45" s="55">
+        <v>99</v>
+      </c>
+      <c r="L45" s="49" t="s">
+        <v>130</v>
+      </c>
+      <c r="M45" s="50" t="s">
+        <v>180</v>
+      </c>
+      <c r="N45" s="56" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="46" spans="2:14" s="44" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B46" s="53" t="s">
+        <v>1</v>
+      </c>
+      <c r="C46" s="54" t="s">
+        <v>162</v>
+      </c>
+      <c r="D46" s="55" t="s">
+        <v>153</v>
+      </c>
+      <c r="E46" s="55">
+        <v>1</v>
+      </c>
+      <c r="F46" s="55">
+        <v>0.3</v>
+      </c>
+      <c r="G46" s="54">
+        <v>0</v>
+      </c>
+      <c r="H46" s="55">
+        <v>7</v>
+      </c>
+      <c r="I46" s="55" t="s">
+        <v>163</v>
+      </c>
+      <c r="J46" s="54">
+        <v>99</v>
+      </c>
+      <c r="K46" s="55">
+        <v>99</v>
+      </c>
+      <c r="L46" s="49" t="s">
+        <v>130</v>
+      </c>
+      <c r="M46" s="50" t="s">
+        <v>174</v>
+      </c>
+      <c r="N46" s="56" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="47" spans="2:14" s="44" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B47" s="53" t="s">
+        <v>1</v>
+      </c>
+      <c r="C47" s="54" t="s">
+        <v>160</v>
+      </c>
+      <c r="D47" s="55" t="s">
+        <v>153</v>
+      </c>
+      <c r="E47" s="55">
+        <v>1</v>
+      </c>
+      <c r="F47" s="55">
+        <v>0.3</v>
+      </c>
+      <c r="G47" s="54">
+        <v>0</v>
+      </c>
+      <c r="H47" s="55">
+        <v>7</v>
+      </c>
+      <c r="I47" s="55" t="s">
+        <v>161</v>
+      </c>
+      <c r="J47" s="54">
+        <v>99</v>
+      </c>
+      <c r="K47" s="55">
+        <v>99</v>
+      </c>
+      <c r="L47" s="49" t="s">
+        <v>130</v>
+      </c>
+      <c r="M47" s="50" t="s">
+        <v>197</v>
+      </c>
+      <c r="N47" s="56" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="48" spans="2:14" s="44" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B48" s="57"/>
+      <c r="C48" s="55"/>
+      <c r="D48" s="55"/>
+      <c r="E48" s="55"/>
+      <c r="F48" s="55"/>
+      <c r="G48" s="55"/>
+      <c r="H48" s="55"/>
+      <c r="I48" s="55"/>
+      <c r="J48" s="55"/>
+      <c r="K48" s="55"/>
+      <c r="L48" s="59"/>
+      <c r="M48" s="59"/>
+      <c r="N48" s="60"/>
+    </row>
+    <row r="49" spans="2:14" s="44" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B49" s="45"/>
+      <c r="C49" s="45"/>
+      <c r="D49" s="45"/>
+      <c r="E49" s="45"/>
+      <c r="F49" s="45"/>
+      <c r="G49" s="45"/>
+      <c r="H49" s="45"/>
+      <c r="I49" s="45"/>
+      <c r="J49" s="45"/>
+      <c r="K49" s="45"/>
+      <c r="L49" s="45"/>
+      <c r="M49" s="45"/>
+      <c r="N49" s="43"/>
+    </row>
+    <row r="50" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B50" s="32"/>
+      <c r="C50" s="32"/>
+      <c r="D50" s="32"/>
+      <c r="E50" s="32"/>
+      <c r="F50" s="32"/>
+      <c r="G50" s="32"/>
+      <c r="H50" s="32"/>
+      <c r="I50" s="32"/>
+      <c r="J50" s="32"/>
+      <c r="K50" s="32"/>
+      <c r="L50" s="32"/>
+      <c r="M50" s="31"/>
+    </row>
+    <row r="51" spans="2:14" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B51" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="C34" s="6"/>
-      <c r="D34" s="6"/>
-      <c r="E34" s="6"/>
-      <c r="F34" s="6"/>
-      <c r="G34" s="6"/>
-      <c r="H34" s="6"/>
-      <c r="I34" s="6"/>
-      <c r="J34" s="6"/>
-      <c r="K34" s="6"/>
-      <c r="L34" s="6"/>
-    </row>
-    <row r="35" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B35" s="20"/>
-      <c r="C35" s="20"/>
-      <c r="D35" s="20"/>
-      <c r="E35" s="20"/>
-      <c r="F35" s="41"/>
-      <c r="G35" s="41"/>
-      <c r="H35" s="41"/>
-      <c r="I35" s="20"/>
-      <c r="J35" s="20"/>
-    </row>
-    <row r="36" spans="2:13" ht="96" x14ac:dyDescent="0.2">
-      <c r="B36" s="30" t="s">
+      <c r="C51" s="6"/>
+      <c r="D51" s="6"/>
+      <c r="E51" s="6"/>
+      <c r="F51" s="6"/>
+      <c r="G51" s="6"/>
+      <c r="H51" s="6"/>
+      <c r="I51" s="6"/>
+      <c r="J51" s="6"/>
+      <c r="K51" s="6"/>
+      <c r="L51" s="6"/>
+    </row>
+    <row r="52" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B52" s="20"/>
+      <c r="C52" s="20"/>
+      <c r="D52" s="20"/>
+      <c r="E52" s="20"/>
+      <c r="F52" s="62"/>
+      <c r="G52" s="62"/>
+      <c r="H52" s="62"/>
+      <c r="I52" s="20"/>
+      <c r="J52" s="20"/>
+    </row>
+    <row r="53" spans="2:14" ht="96" x14ac:dyDescent="0.25">
+      <c r="B53" s="30" t="s">
         <v>71</v>
       </c>
-      <c r="C36" s="28" t="s">
+      <c r="C53" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="D36" s="29" t="s">
+      <c r="D53" s="29" t="s">
         <v>70</v>
       </c>
-      <c r="E36" s="29" t="s">
+      <c r="E53" s="29" t="s">
         <v>69</v>
       </c>
-      <c r="F36" s="29" t="s">
+      <c r="F53" s="29" t="s">
         <v>68</v>
       </c>
-      <c r="G36" s="28" t="s">
+      <c r="G53" s="28" t="s">
         <v>67</v>
       </c>
-      <c r="H36" s="28" t="s">
+      <c r="H53" s="28" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="37" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B37" s="27" t="s">
-        <v>1</v>
-      </c>
-      <c r="C37" s="24" t="s">
+    <row r="54" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B54" s="27" t="s">
+        <v>1</v>
+      </c>
+      <c r="C54" s="24" t="s">
         <v>65</v>
       </c>
-      <c r="D37" s="24">
+      <c r="D54" s="24">
         <v>0</v>
       </c>
-      <c r="E37" s="24">
+      <c r="E54" s="24">
         <v>7</v>
       </c>
-      <c r="F37" s="24">
+      <c r="F54" s="24">
         <v>2</v>
       </c>
-      <c r="G37" s="26" t="s">
+      <c r="G54" s="26" t="s">
         <v>64</v>
       </c>
-      <c r="H37" s="26" t="s">
+      <c r="H54" s="26" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="38" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B38" s="27" t="s">
-        <v>1</v>
-      </c>
-      <c r="C38" s="24" t="s">
+    <row r="55" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B55" s="27" t="s">
+        <v>1</v>
+      </c>
+      <c r="C55" s="24" t="s">
         <v>62</v>
       </c>
-      <c r="D38" s="24">
+      <c r="D55" s="24">
         <v>0</v>
       </c>
-      <c r="E38" s="24">
+      <c r="E55" s="24">
         <v>7</v>
       </c>
-      <c r="F38" s="24">
-        <v>1</v>
-      </c>
-      <c r="G38" s="26" t="s">
+      <c r="F55" s="24">
+        <v>1</v>
+      </c>
+      <c r="G55" s="26" t="s">
         <v>61</v>
       </c>
-      <c r="H38" s="26" t="s">
+      <c r="H55" s="26" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="39" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B39" s="27" t="s">
-        <v>1</v>
-      </c>
-      <c r="C39" s="24" t="s">
+    <row r="56" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B56" s="27" t="s">
+        <v>1</v>
+      </c>
+      <c r="C56" s="24" t="s">
         <v>59</v>
       </c>
-      <c r="D39" s="24">
+      <c r="D56" s="24">
         <v>0</v>
       </c>
-      <c r="E39" s="24">
+      <c r="E56" s="24">
         <v>7</v>
       </c>
-      <c r="F39" s="24">
+      <c r="F56" s="24">
         <v>2</v>
       </c>
-      <c r="G39" s="26" t="s">
+      <c r="G56" s="26" t="s">
         <v>58</v>
       </c>
-      <c r="H39" s="26" t="s">
+      <c r="H56" s="26" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="40" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B40" s="27" t="s">
-        <v>1</v>
-      </c>
-      <c r="C40" s="24" t="s">
+    <row r="57" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B57" s="27" t="s">
+        <v>1</v>
+      </c>
+      <c r="C57" s="24" t="s">
         <v>56</v>
       </c>
-      <c r="D40" s="24">
+      <c r="D57" s="24">
         <v>0</v>
       </c>
-      <c r="E40" s="24">
+      <c r="E57" s="24">
         <v>7</v>
       </c>
-      <c r="F40" s="24">
-        <v>1</v>
-      </c>
-      <c r="G40" s="26" t="s">
+      <c r="F57" s="24">
+        <v>1</v>
+      </c>
+      <c r="G57" s="26" t="s">
         <v>55</v>
       </c>
-      <c r="H40" s="26" t="s">
+      <c r="H57" s="26" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="41" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B41" s="25" t="s">
-        <v>1</v>
-      </c>
-      <c r="C41" s="23" t="s">
+    <row r="58" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B58" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="C58" s="23" t="s">
         <v>53</v>
       </c>
-      <c r="D41" s="23">
+      <c r="D58" s="23">
         <v>0</v>
       </c>
-      <c r="E41" s="24">
+      <c r="E58" s="24">
         <v>7</v>
       </c>
-      <c r="F41" s="23">
-        <v>1</v>
-      </c>
-      <c r="G41" s="26" t="s">
+      <c r="F58" s="23">
+        <v>1</v>
+      </c>
+      <c r="G58" s="26" t="s">
         <v>52</v>
       </c>
-      <c r="H41" s="26" t="s">
+      <c r="H58" s="26" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="42" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B42" s="25" t="s">
-        <v>1</v>
-      </c>
-      <c r="C42" s="24" t="s">
+    <row r="59" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B59" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="C59" s="24" t="s">
         <v>50</v>
       </c>
-      <c r="D42" s="24">
+      <c r="D59" s="24">
         <v>0</v>
       </c>
-      <c r="E42" s="24">
+      <c r="E59" s="24">
         <v>7</v>
       </c>
-      <c r="F42" s="24">
-        <v>1</v>
-      </c>
-      <c r="G42" s="26" t="s">
+      <c r="F59" s="24">
+        <v>1</v>
+      </c>
+      <c r="G59" s="26" t="s">
         <v>49</v>
       </c>
-      <c r="H42" s="26" t="s">
+      <c r="H59" s="26" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="43" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B43" s="25" t="s">
-        <v>1</v>
-      </c>
-      <c r="C43" s="24" t="s">
+    <row r="60" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B60" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="C60" s="24" t="s">
         <v>47</v>
       </c>
-      <c r="D43" s="24">
+      <c r="D60" s="24">
         <v>0</v>
       </c>
-      <c r="E43" s="24">
+      <c r="E60" s="24">
         <v>7</v>
       </c>
-      <c r="F43" s="24">
-        <v>1</v>
-      </c>
-      <c r="G43" s="26" t="s">
+      <c r="F60" s="24">
+        <v>1</v>
+      </c>
+      <c r="G60" s="26" t="s">
         <v>46</v>
       </c>
-      <c r="H43" s="26" t="s">
+      <c r="H60" s="26" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="44" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B44" s="25" t="s">
-        <v>1</v>
-      </c>
-      <c r="C44" s="23" t="s">
+    <row r="61" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B61" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="C61" s="23" t="s">
         <v>44</v>
       </c>
-      <c r="D44" s="23">
+      <c r="D61" s="23">
         <v>0</v>
       </c>
-      <c r="E44" s="24">
+      <c r="E61" s="24">
         <v>7</v>
       </c>
-      <c r="F44" s="23">
-        <v>1</v>
-      </c>
-      <c r="G44" s="22" t="s">
+      <c r="F61" s="23">
+        <v>1</v>
+      </c>
+      <c r="G61" s="22" t="s">
         <v>43</v>
       </c>
-      <c r="H44" s="22" t="s">
+      <c r="H61" s="22" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="45" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B45" s="25" t="s">
-        <v>1</v>
-      </c>
-      <c r="C45" s="23" t="s">
-        <v>168</v>
-      </c>
-      <c r="D45" s="23">
+    <row r="62" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B62" s="47" t="s">
+        <v>1</v>
+      </c>
+      <c r="C62" s="41" t="s">
+        <v>211</v>
+      </c>
+      <c r="D62" s="41">
         <v>0</v>
       </c>
-      <c r="E45" s="24">
+      <c r="E62" s="41">
         <v>7</v>
       </c>
-      <c r="F45" s="23">
-        <v>1</v>
-      </c>
-      <c r="G45" s="26" t="s">
-        <v>169</v>
-      </c>
-      <c r="H45" s="26"/>
-    </row>
-    <row r="46" spans="2:13" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="47" spans="2:13" ht="24" x14ac:dyDescent="0.3">
-      <c r="B47" s="6" t="s">
+      <c r="F62" s="41">
+        <v>1</v>
+      </c>
+      <c r="G62" s="42" t="s">
+        <v>198</v>
+      </c>
+      <c r="H62" s="42" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="63" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B63" s="47" t="s">
+        <v>1</v>
+      </c>
+      <c r="C63" s="41" t="s">
+        <v>210</v>
+      </c>
+      <c r="D63" s="41">
+        <v>0</v>
+      </c>
+      <c r="E63" s="41">
+        <v>7</v>
+      </c>
+      <c r="F63" s="41">
+        <v>2</v>
+      </c>
+      <c r="G63" s="46" t="s">
+        <v>201</v>
+      </c>
+      <c r="H63" s="46" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="64" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B64" s="47" t="s">
+        <v>1</v>
+      </c>
+      <c r="C64" s="41" t="s">
+        <v>152</v>
+      </c>
+      <c r="D64" s="41">
+        <v>0</v>
+      </c>
+      <c r="E64" s="41">
+        <v>7</v>
+      </c>
+      <c r="F64" s="41">
+        <v>2</v>
+      </c>
+      <c r="G64" s="46" t="s">
+        <v>199</v>
+      </c>
+      <c r="H64" s="46" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="65" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B65" s="47" t="s">
+        <v>1</v>
+      </c>
+      <c r="C65" s="41" t="s">
+        <v>153</v>
+      </c>
+      <c r="D65" s="41">
+        <v>0</v>
+      </c>
+      <c r="E65" s="41">
+        <v>7</v>
+      </c>
+      <c r="F65" s="41">
+        <v>2</v>
+      </c>
+      <c r="G65" s="46" t="s">
+        <v>200</v>
+      </c>
+      <c r="H65" s="46" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="66" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B66" s="40"/>
+      <c r="C66" s="40"/>
+      <c r="D66" s="40"/>
+      <c r="E66" s="40"/>
+      <c r="F66" s="40"/>
+      <c r="G66" s="40"/>
+      <c r="H66" s="40"/>
+    </row>
+    <row r="67" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="68" spans="2:13" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B68" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="C47" s="6"/>
-      <c r="D47" s="6"/>
-      <c r="E47" s="6"/>
-      <c r="F47" s="6"/>
-      <c r="G47" s="6"/>
-      <c r="H47" s="6"/>
-      <c r="I47" s="6"/>
-      <c r="J47" s="6"/>
-      <c r="K47" s="6"/>
-      <c r="L47" s="6"/>
-      <c r="M47" s="6"/>
-    </row>
-    <row r="48" spans="2:13" ht="45" x14ac:dyDescent="0.2">
-      <c r="B48" s="20"/>
-      <c r="C48" s="20"/>
-      <c r="D48" s="20"/>
-      <c r="E48" s="20"/>
-      <c r="F48" s="21" t="s">
+      <c r="C68" s="6"/>
+      <c r="D68" s="6"/>
+      <c r="E68" s="6"/>
+      <c r="F68" s="6"/>
+      <c r="G68" s="6"/>
+      <c r="H68" s="6"/>
+      <c r="I68" s="6"/>
+      <c r="J68" s="6"/>
+      <c r="K68" s="6"/>
+      <c r="L68" s="6"/>
+      <c r="M68" s="6"/>
+    </row>
+    <row r="69" spans="2:13" ht="60" x14ac:dyDescent="0.25">
+      <c r="B69" s="20"/>
+      <c r="C69" s="20"/>
+      <c r="D69" s="20"/>
+      <c r="E69" s="20"/>
+      <c r="F69" s="21" t="s">
         <v>40</v>
       </c>
-      <c r="G48" s="42" t="s">
+      <c r="G69" s="63" t="s">
         <v>39</v>
       </c>
-      <c r="H48" s="42"/>
-      <c r="I48" s="20"/>
-    </row>
-    <row r="49" spans="2:11" ht="137" x14ac:dyDescent="0.2">
-      <c r="B49" s="19" t="s">
+      <c r="H69" s="63"/>
+      <c r="I69" s="20"/>
+    </row>
+    <row r="70" spans="2:13" ht="142.5" x14ac:dyDescent="0.25">
+      <c r="B70" s="19" t="s">
         <v>38</v>
       </c>
-      <c r="C49" s="19" t="s">
+      <c r="C70" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="D49" s="18" t="s">
+      <c r="D70" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="E49" s="17" t="s">
+      <c r="E70" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="F49" s="17" t="s">
+      <c r="F70" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="G49" s="17" t="s">
+      <c r="G70" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="H49" s="16" t="s">
+      <c r="H70" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="I49" s="16" t="s">
+      <c r="I70" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="J49" s="15" t="s">
+      <c r="J70" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="K49" s="14" t="s">
+      <c r="K70" s="14" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="50" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B50" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="C50" s="11" t="s">
+    <row r="71" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B71" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="C71" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="D50" s="11">
+      <c r="D71" s="11">
         <v>0</v>
       </c>
-      <c r="E50" s="10">
+      <c r="E71" s="10">
         <v>0</v>
       </c>
-      <c r="F50" s="10">
+      <c r="F71" s="10">
         <v>15</v>
       </c>
-      <c r="G50" s="10">
+      <c r="G71" s="10">
         <v>200</v>
       </c>
-      <c r="H50" s="9">
+      <c r="H71" s="9">
         <v>0.5</v>
       </c>
-      <c r="I50" s="9">
-        <v>1</v>
-      </c>
-      <c r="J50" s="8" t="s">
+      <c r="I71" s="9">
+        <v>1</v>
+      </c>
+      <c r="J71" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="K50" s="13" t="s">
+      <c r="K71" s="13" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="51" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B51" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="C51" s="11" t="s">
+    <row r="72" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B72" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="C72" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="D51" s="11">
-        <v>1</v>
-      </c>
-      <c r="E51" s="10">
+      <c r="D72" s="11">
+        <v>1</v>
+      </c>
+      <c r="E72" s="10">
         <v>0</v>
       </c>
-      <c r="F51" s="10">
+      <c r="F72" s="10">
         <v>60</v>
       </c>
-      <c r="G51" s="10">
+      <c r="G72" s="10">
         <v>300</v>
       </c>
-      <c r="H51" s="9">
+      <c r="H72" s="9">
         <v>0.5</v>
       </c>
-      <c r="I51" s="9">
-        <v>1</v>
-      </c>
-      <c r="J51" s="8" t="s">
+      <c r="I72" s="9">
+        <v>1</v>
+      </c>
+      <c r="J72" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="K51" s="13" t="s">
+      <c r="K72" s="13" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="52" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B52" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="C52" s="11" t="s">
+    <row r="73" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B73" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="C73" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="D52" s="11">
+      <c r="D73" s="11">
         <v>2</v>
       </c>
-      <c r="E52" s="10">
+      <c r="E73" s="10">
         <v>0</v>
       </c>
-      <c r="F52" s="10">
+      <c r="F73" s="10">
         <v>240</v>
       </c>
-      <c r="G52" s="10">
+      <c r="G73" s="10">
         <v>600</v>
       </c>
-      <c r="H52" s="9">
+      <c r="H73" s="9">
         <v>0.5</v>
       </c>
-      <c r="I52" s="9">
-        <v>1</v>
-      </c>
-      <c r="J52" s="8" t="s">
+      <c r="I73" s="9">
+        <v>1</v>
+      </c>
+      <c r="J73" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="K52" s="7" t="s">
+      <c r="K73" s="7" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="54" spans="2:11" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="55" spans="2:11" ht="24" x14ac:dyDescent="0.3">
-      <c r="B55" s="6" t="s">
+    <row r="75" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="76" spans="2:13" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B76" s="6" t="s">
         <v>23</v>
-      </c>
-      <c r="C55" s="6"/>
-      <c r="D55" s="6"/>
-      <c r="E55" s="6"/>
-      <c r="F55" s="6"/>
-      <c r="G55" s="6"/>
-    </row>
-    <row r="57" spans="2:11" ht="135" x14ac:dyDescent="0.2">
-      <c r="B57" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="C57" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D57" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E57" s="3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="58" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B58" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C58" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D58" s="1">
-        <v>0.1</v>
-      </c>
-      <c r="E58" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="59" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B59" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C59" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D59" s="1">
-        <v>0.7</v>
-      </c>
-      <c r="E59" s="1">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="60" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B60" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C60" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D60" s="1">
-        <v>1</v>
-      </c>
-      <c r="E60" s="1">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="61" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B61" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C61" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D61" s="1">
-        <v>1.5</v>
-      </c>
-      <c r="E61" s="1">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="62" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B62" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C62" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D62" s="1">
-        <v>2</v>
-      </c>
-      <c r="E62" s="1">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="63" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B63" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C63" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D63" s="1">
-        <v>2.5</v>
-      </c>
-      <c r="E63" s="1">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="64" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B64" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C64" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D64" s="1">
-        <v>3</v>
-      </c>
-      <c r="E64" s="1">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="65" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B65" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C65" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D65" s="1">
-        <v>4</v>
-      </c>
-      <c r="E65" s="1">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="66" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B66" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C66" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D66" s="1">
-        <v>5</v>
-      </c>
-      <c r="E66" s="1">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="67" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B67" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C67" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D67" s="1">
-        <v>7</v>
-      </c>
-      <c r="E67" s="1">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="68" spans="2:7" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="69" spans="2:7" ht="24" x14ac:dyDescent="0.3">
-      <c r="B69" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C69" s="6"/>
-      <c r="D69" s="6"/>
-      <c r="E69" s="6"/>
-      <c r="F69" s="6"/>
-      <c r="G69" s="6"/>
-    </row>
-    <row r="71" spans="2:7" ht="142" x14ac:dyDescent="0.2">
-      <c r="B71" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C71" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D71" s="3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="72" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B72" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C72" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D72" s="1">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="73" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B73" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C73" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D73" s="1">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="74" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B74" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C74" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D74" s="1">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="75" spans="2:7" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="76" spans="2:7" ht="24" x14ac:dyDescent="0.3">
-      <c r="B76" s="6" t="s">
-        <v>5</v>
       </c>
       <c r="C76" s="6"/>
       <c r="D76" s="6"/>
@@ -4281,9 +4960,9 @@
       <c r="F76" s="6"/>
       <c r="G76" s="6"/>
     </row>
-    <row r="78" spans="2:7" ht="131" x14ac:dyDescent="0.2">
+    <row r="78" spans="2:13" ht="135.75" x14ac:dyDescent="0.25">
       <c r="B78" s="5" t="s">
-        <v>4</v>
+        <v>22</v>
       </c>
       <c r="C78" s="4" t="s">
         <v>3</v>
@@ -4291,15 +4970,235 @@
       <c r="D78" s="3" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="79" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="E78" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="79" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B79" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C79" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D79" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="E79" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="80" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B80" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C80" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D80" s="1">
+        <v>0.7</v>
+      </c>
+      <c r="E80" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="81" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B81" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C81" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D81" s="1">
+        <v>1</v>
+      </c>
+      <c r="E81" s="1">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="82" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B82" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C82" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D82" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="E82" s="1">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="83" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B83" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C83" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D83" s="1">
+        <v>2</v>
+      </c>
+      <c r="E83" s="1">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="84" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B84" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C84" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D84" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="E84" s="1">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="85" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B85" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C85" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D85" s="1">
+        <v>3</v>
+      </c>
+      <c r="E85" s="1">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="86" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B86" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C86" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D86" s="1">
+        <v>4</v>
+      </c>
+      <c r="E86" s="1">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="87" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B87" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C87" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D87" s="1">
+        <v>5</v>
+      </c>
+      <c r="E87" s="1">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="88" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B88" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C88" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D88" s="1">
+        <v>7</v>
+      </c>
+      <c r="E88" s="1">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="89" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="90" spans="2:7" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B90" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C90" s="6"/>
+      <c r="D90" s="6"/>
+      <c r="E90" s="6"/>
+      <c r="F90" s="6"/>
+      <c r="G90" s="6"/>
+    </row>
+    <row r="92" spans="2:7" ht="142.5" x14ac:dyDescent="0.25">
+      <c r="B92" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C92" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D92" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="93" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B93" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C93" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D93" s="1">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="94" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B94" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C94" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D94" s="1">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="95" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B95" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C95" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D95" s="1">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="96" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="97" spans="2:7" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B97" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C97" s="6"/>
+      <c r="D97" s="6"/>
+      <c r="E97" s="6"/>
+      <c r="F97" s="6"/>
+      <c r="G97" s="6"/>
+    </row>
+    <row r="99" spans="2:7" ht="132" x14ac:dyDescent="0.25">
+      <c r="B99" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C99" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D99" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="100" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B100" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C100" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D79" s="1">
+      <c r="D100" s="1">
         <v>0.7</v>
       </c>
     </row>
@@ -4307,11 +5206,11 @@
   <mergeCells count="4">
     <mergeCell ref="J3:K3"/>
     <mergeCell ref="M3:P3"/>
-    <mergeCell ref="F35:H35"/>
-    <mergeCell ref="G48:H48"/>
+    <mergeCell ref="F52:H52"/>
+    <mergeCell ref="G69:H69"/>
   </mergeCells>
-  <conditionalFormatting sqref="C50:D52">
-    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+  <conditionalFormatting sqref="C71:D73">
+    <cfRule type="duplicateValues" dxfId="66" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
[FIXED] [CONTENT] Renamed type of mission. In TrackerBase.cs it says kill_chain and in content it was named eat_chain.
Former-commit-id: 5d0772cc61f7b412d3379fa125235011217be2eb
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Missions.xlsx
+++ b/Docs/Content/HungryDragonContent_Missions.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="401" uniqueCount="213">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="407" uniqueCount="214">
   <si>
     <t>single_run</t>
   </si>
@@ -498,203 +498,206 @@
     <t>[singleRunChance]</t>
   </si>
   <si>
+    <t>Sheep</t>
+  </si>
+  <si>
+    <t>SpiderSmall;SpiderRed</t>
+  </si>
+  <si>
+    <t>eat_gold</t>
+  </si>
+  <si>
+    <t>eat_suicidal</t>
+  </si>
+  <si>
+    <t>Worker</t>
+  </si>
+  <si>
+    <t>eat_suicidal_goblins</t>
+  </si>
+  <si>
+    <t>eat_gold_generic</t>
+  </si>
+  <si>
+    <t>eat_gold_razorback</t>
+  </si>
+  <si>
+    <t>eat_gold_driller</t>
+  </si>
+  <si>
+    <t>eat_suicidal_cattle</t>
+  </si>
+  <si>
+    <t>Sheep; Cow; Horse</t>
+  </si>
+  <si>
+    <t>eat_suicidal_villagers</t>
+  </si>
+  <si>
+    <t>Villager01;Villager02</t>
+  </si>
+  <si>
+    <t>Hawk;OwlSmall;Vulture</t>
+  </si>
+  <si>
+    <t>eat_gold_fishes</t>
+  </si>
+  <si>
+    <t>Fish01_Generic;Fish02_Generic;Fish03_Generic</t>
+  </si>
+  <si>
+    <t>eat_gold_stingrayLarge</t>
+  </si>
+  <si>
+    <t>StingrayLarge</t>
+  </si>
+  <si>
+    <t>Razorback</t>
+  </si>
+  <si>
+    <t>eat_gold_piranha</t>
+  </si>
+  <si>
+    <t>Piranha</t>
+  </si>
+  <si>
+    <t>TID_EDIBLE_CANARY_PL</t>
+  </si>
+  <si>
+    <t>Villager01;Villager02;BadFarmer;DrunkenMan;BoatFisher</t>
+  </si>
+  <si>
+    <t>TID_MISSION_TARGET_VILLAGERS</t>
+  </si>
+  <si>
+    <t>TID_MISSION_TARGET_BUILDINGS</t>
+  </si>
+  <si>
+    <t>TID_EDIBLE_VULTURE_PL</t>
+  </si>
+  <si>
+    <t>TID_SC_NAME_PLURAL</t>
+  </si>
+  <si>
+    <t>TID_EGG_PLURAL</t>
+  </si>
+  <si>
+    <t>TID_EDIBLE_EVILDRAGON_PL</t>
+  </si>
+  <si>
+    <t>TID_EDIBLE_GOBLIN_PL</t>
+  </si>
+  <si>
+    <t>TID_EDIBLE_SPIDER_PL</t>
+  </si>
+  <si>
+    <t>TID_EDIBLE_FLYINGPIG_PL</t>
+  </si>
+  <si>
+    <t>TID_EDIBLE_BAT_PL</t>
+  </si>
+  <si>
+    <t>TID_EDIBLE_OWL_PL</t>
+  </si>
+  <si>
+    <t>TID_EDIBLE_LIONBIRD_PL</t>
+  </si>
+  <si>
+    <t>TID_EDIBLE_GOBLIN_DRILLER_PL</t>
+  </si>
+  <si>
+    <t>TID_EDIBLE_ARCHER_PL</t>
+  </si>
+  <si>
+    <t>TID_EDIBLE_SOLDIER_PL</t>
+  </si>
+  <si>
+    <t>TID_EDIBLE_TROLL_PL</t>
+  </si>
+  <si>
+    <t>TID_EDIBLE_SHEEP_PL</t>
+  </si>
+  <si>
+    <t>TID_EDIBLE_STINGRAY_PL</t>
+  </si>
+  <si>
+    <t>TID_EDIBLE_PIRANHA_PL</t>
+  </si>
+  <si>
+    <t>TID_EDIBLE_RAZORBACK_PL</t>
+  </si>
+  <si>
+    <t>TID_EDIBLE_FISH_PL</t>
+  </si>
+  <si>
+    <t>TID_MISSION_TARGET_BOATMAN</t>
+  </si>
+  <si>
+    <t>TID_MISSION_TARGET_BIRDSPREY</t>
+  </si>
+  <si>
+    <t>TID_MISSION_TARGET_CATTLE</t>
+  </si>
+  <si>
+    <t>TID_MISSION_OBJECTIVE_KILLCHAIN_DESC_SINGLE_RUN</t>
+  </si>
+  <si>
+    <t>TID_MISSION_OBJECTIVE_EATGOLD_DESC_SINGLE_RUN</t>
+  </si>
+  <si>
+    <t>TID_MISSION_OBJECTIVE_EATSUICIDAL_DESC_SINGLE_RUN</t>
+  </si>
+  <si>
+    <t>TID_MISSION_OBJECTIVE_EATHANG_DESC_SINGLE_RUN</t>
+  </si>
+  <si>
+    <t>TID_MISSION_OBJECTIVE_KILLCHAIN_DESC_MULTI_RUN</t>
+  </si>
+  <si>
+    <t>TID_MISSION_OBJECTIVE_EATHANG_DESC_MULTI_RUN</t>
+  </si>
+  <si>
+    <t>TID_MISSION_OBJECTIVE_EATGOLD_DESC_MULTI_RUN</t>
+  </si>
+  <si>
+    <t>TID_MISSION_OBJECTIVE_EATSUICIDAL_DESC_MULTI_RUN</t>
+  </si>
+  <si>
+    <t>eat_gold_birdsPrey</t>
+  </si>
+  <si>
+    <t>Blue Canaries</t>
+  </si>
+  <si>
+    <t>TID_EDIBLE_CANARY_01_PL</t>
+  </si>
+  <si>
+    <t>eat_spec_anim_a</t>
+  </si>
+  <si>
+    <t>eat_chain</t>
+  </si>
+  <si>
+    <t>eat_spec_anim_a_spiders</t>
+  </si>
+  <si>
+    <t>critical_time</t>
+  </si>
+  <si>
     <t>kill_chain</t>
   </si>
   <si>
-    <t>Sheep</t>
-  </si>
-  <si>
-    <t>SpiderSmall;SpiderRed</t>
-  </si>
-  <si>
-    <t>eat_gold</t>
-  </si>
-  <si>
-    <t>eat_suicidal</t>
-  </si>
-  <si>
-    <t>Worker</t>
-  </si>
-  <si>
     <t>kill_chain_sheeps</t>
   </si>
   <si>
-    <t>eat_suicidal_goblins</t>
-  </si>
-  <si>
-    <t>eat_gold_generic</t>
-  </si>
-  <si>
-    <t>eat_gold_razorback</t>
-  </si>
-  <si>
-    <t>eat_gold_driller</t>
-  </si>
-  <si>
-    <t>eat_suicidal_cattle</t>
-  </si>
-  <si>
-    <t>Sheep; Cow; Horse</t>
-  </si>
-  <si>
-    <t>eat_suicidal_villagers</t>
-  </si>
-  <si>
-    <t>Villager01;Villager02</t>
-  </si>
-  <si>
-    <t>Hawk;OwlSmall;Vulture</t>
-  </si>
-  <si>
-    <t>eat_gold_fishes</t>
-  </si>
-  <si>
-    <t>Fish01_Generic;Fish02_Generic;Fish03_Generic</t>
-  </si>
-  <si>
-    <t>eat_gold_stingrayLarge</t>
-  </si>
-  <si>
-    <t>StingrayLarge</t>
-  </si>
-  <si>
-    <t>Razorback</t>
-  </si>
-  <si>
-    <t>eat_gold_piranha</t>
-  </si>
-  <si>
-    <t>Piranha</t>
-  </si>
-  <si>
-    <t>TID_EDIBLE_CANARY_PL</t>
-  </si>
-  <si>
-    <t>Villager01;Villager02;BadFarmer;DrunkenMan;BoatFisher</t>
-  </si>
-  <si>
-    <t>TID_MISSION_TARGET_VILLAGERS</t>
-  </si>
-  <si>
-    <t>TID_MISSION_TARGET_BUILDINGS</t>
-  </si>
-  <si>
-    <t>TID_EDIBLE_VULTURE_PL</t>
-  </si>
-  <si>
-    <t>TID_SC_NAME_PLURAL</t>
-  </si>
-  <si>
-    <t>TID_EGG_PLURAL</t>
-  </si>
-  <si>
-    <t>TID_EDIBLE_EVILDRAGON_PL</t>
-  </si>
-  <si>
-    <t>TID_EDIBLE_GOBLIN_PL</t>
-  </si>
-  <si>
-    <t>TID_EDIBLE_SPIDER_PL</t>
-  </si>
-  <si>
-    <t>TID_EDIBLE_FLYINGPIG_PL</t>
-  </si>
-  <si>
-    <t>TID_EDIBLE_BAT_PL</t>
-  </si>
-  <si>
-    <t>TID_EDIBLE_OWL_PL</t>
-  </si>
-  <si>
-    <t>TID_EDIBLE_LIONBIRD_PL</t>
-  </si>
-  <si>
-    <t>TID_EDIBLE_GOBLIN_DRILLER_PL</t>
-  </si>
-  <si>
-    <t>TID_EDIBLE_ARCHER_PL</t>
-  </si>
-  <si>
-    <t>TID_EDIBLE_SOLDIER_PL</t>
-  </si>
-  <si>
-    <t>TID_EDIBLE_TROLL_PL</t>
-  </si>
-  <si>
-    <t>TID_EDIBLE_SHEEP_PL</t>
-  </si>
-  <si>
-    <t>TID_EDIBLE_STINGRAY_PL</t>
-  </si>
-  <si>
-    <t>TID_EDIBLE_PIRANHA_PL</t>
-  </si>
-  <si>
-    <t>TID_EDIBLE_RAZORBACK_PL</t>
-  </si>
-  <si>
-    <t>TID_EDIBLE_FISH_PL</t>
-  </si>
-  <si>
-    <t>TID_MISSION_TARGET_BOATMAN</t>
-  </si>
-  <si>
-    <t>TID_MISSION_TARGET_BIRDSPREY</t>
-  </si>
-  <si>
-    <t>TID_MISSION_TARGET_CATTLE</t>
-  </si>
-  <si>
-    <t>TID_MISSION_OBJECTIVE_KILLCHAIN_DESC_SINGLE_RUN</t>
-  </si>
-  <si>
-    <t>TID_MISSION_OBJECTIVE_EATGOLD_DESC_SINGLE_RUN</t>
-  </si>
-  <si>
-    <t>TID_MISSION_OBJECTIVE_EATSUICIDAL_DESC_SINGLE_RUN</t>
-  </si>
-  <si>
-    <t>TID_MISSION_OBJECTIVE_EATHANG_DESC_SINGLE_RUN</t>
-  </si>
-  <si>
-    <t>TID_MISSION_OBJECTIVE_KILLCHAIN_DESC_MULTI_RUN</t>
-  </si>
-  <si>
-    <t>TID_MISSION_OBJECTIVE_EATHANG_DESC_MULTI_RUN</t>
-  </si>
-  <si>
-    <t>TID_MISSION_OBJECTIVE_EATGOLD_DESC_MULTI_RUN</t>
-  </si>
-  <si>
-    <t>TID_MISSION_OBJECTIVE_EATSUICIDAL_DESC_MULTI_RUN</t>
-  </si>
-  <si>
-    <t>eat_gold_birdsPrey</t>
-  </si>
-  <si>
     <t>kill_chain_canary_01</t>
-  </si>
-  <si>
-    <t>Blue Canaries</t>
-  </si>
-  <si>
-    <t>TID_EDIBLE_CANARY_01_PL</t>
-  </si>
-  <si>
-    <t>eat_spec_anim_a</t>
-  </si>
-  <si>
-    <t>eat_chain</t>
-  </si>
-  <si>
-    <t>eat_spec_anim_a_spiders</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -768,13 +771,6 @@
     <font>
       <sz val="11"/>
       <color theme="1" tint="4.9989318521683403E-2"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -872,7 +868,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="15">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -1026,26 +1022,13 @@
     </border>
     <border>
       <left style="thin">
-        <color auto="1"/>
+        <color indexed="64"/>
       </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color theme="8"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
+      <right/>
+      <top/>
+      <bottom style="thin">
         <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color theme="8"/>
-      </top>
-      <bottom/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -1158,9 +1141,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1198,18 +1178,6 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1217,11 +1185,36 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="67">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -2283,16 +2276,6 @@
         </bottom>
       </border>
     </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -2307,94 +2290,94 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="missionDifficultyDefinitions" displayName="missionDifficultyDefinitions" ref="B70:K73" totalsRowShown="0" headerRowBorderDxfId="65" tableBorderDxfId="64">
-  <autoFilter ref="B70:K73"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="missionDifficultyDefinitions" displayName="missionDifficultyDefinitions" ref="B75:K78" totalsRowShown="0" headerRowBorderDxfId="66" tableBorderDxfId="65">
+  <autoFilter ref="B75:K78"/>
   <tableColumns count="10">
     <tableColumn id="1" name="{missionDifficultyDefinitions}"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="63"/>
-    <tableColumn id="7" name="[index]" dataDxfId="62"/>
-    <tableColumn id="3" name="[dragonsToUnlock]" dataDxfId="61"/>
-    <tableColumn id="4" name="[cooldownMinutes]" dataDxfId="60"/>
-    <tableColumn id="9" name="[maxRewardCoins]" dataDxfId="59"/>
-    <tableColumn id="5" name="[removeMissionPCCoefA]" dataDxfId="58"/>
-    <tableColumn id="6" name="[removeMissionPCCoefB]" dataDxfId="57"/>
-    <tableColumn id="8" name="[tidName]" dataDxfId="56"/>
-    <tableColumn id="10" name="[color]" dataDxfId="55"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="64"/>
+    <tableColumn id="7" name="[index]" dataDxfId="63"/>
+    <tableColumn id="3" name="[dragonsToUnlock]" dataDxfId="62"/>
+    <tableColumn id="4" name="[cooldownMinutes]" dataDxfId="61"/>
+    <tableColumn id="9" name="[maxRewardCoins]" dataDxfId="60"/>
+    <tableColumn id="5" name="[removeMissionPCCoefA]" dataDxfId="59"/>
+    <tableColumn id="6" name="[removeMissionPCCoefB]" dataDxfId="58"/>
+    <tableColumn id="8" name="[tidName]" dataDxfId="57"/>
+    <tableColumn id="10" name="[color]" dataDxfId="56"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table13303132" displayName="Table13303132" ref="B78:E88" totalsRowShown="0" headerRowDxfId="54" dataDxfId="52" headerRowBorderDxfId="53" tableBorderDxfId="51" totalsRowBorderDxfId="50">
-  <autoFilter ref="B78:E88"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table13303132" displayName="Table13303132" ref="B83:E93" totalsRowShown="0" headerRowDxfId="55" dataDxfId="53" headerRowBorderDxfId="54" tableBorderDxfId="52" totalsRowBorderDxfId="51">
+  <autoFilter ref="B83:E93"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="{missionDragonModifiersDefinitions}" dataDxfId="49"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="48"/>
-    <tableColumn id="7" name="[quantityModifier]" dataDxfId="47"/>
-    <tableColumn id="3" name="[missionSCRewardMultiplier]" dataDxfId="46"/>
+    <tableColumn id="1" name="{missionDragonModifiersDefinitions}" dataDxfId="50"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="49"/>
+    <tableColumn id="7" name="[quantityModifier]" dataDxfId="48"/>
+    <tableColumn id="3" name="[missionSCRewardMultiplier]" dataDxfId="47"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table1330313234" displayName="Table1330313234" ref="B92:D95" totalsRowShown="0" headerRowDxfId="45" dataDxfId="43" headerRowBorderDxfId="44" tableBorderDxfId="42" totalsRowBorderDxfId="41">
-  <autoFilter ref="B92:D95"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table1330313234" displayName="Table1330313234" ref="B97:D100" totalsRowShown="0" headerRowDxfId="46" dataDxfId="44" headerRowBorderDxfId="45" tableBorderDxfId="43" totalsRowBorderDxfId="42">
+  <autoFilter ref="B97:D100"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="{missionDifficultyModifiersDefinitions}" dataDxfId="40"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="39"/>
-    <tableColumn id="7" name="[quantityModifier]" dataDxfId="38"/>
+    <tableColumn id="1" name="{missionDifficultyModifiersDefinitions}" dataDxfId="41"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="40"/>
+    <tableColumn id="7" name="[quantityModifier]" dataDxfId="39"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table133031323435" displayName="Table133031323435" ref="B99:D100" totalsRowShown="0" headerRowDxfId="37" dataDxfId="35" headerRowBorderDxfId="36" tableBorderDxfId="34" totalsRowBorderDxfId="33">
-  <autoFilter ref="B99:D100"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table133031323435" displayName="Table133031323435" ref="B104:D105" totalsRowShown="0" headerRowDxfId="38" dataDxfId="36" headerRowBorderDxfId="37" tableBorderDxfId="35" totalsRowBorderDxfId="34">
+  <autoFilter ref="B104:D105"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="{missionOtherModifiersDefinitions}" dataDxfId="32"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="31"/>
-    <tableColumn id="7" name="[quantityModifier]" dataDxfId="30"/>
+    <tableColumn id="1" name="{missionOtherModifiersDefinitions}" dataDxfId="33"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="32"/>
+    <tableColumn id="7" name="[quantityModifier]" dataDxfId="31"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table13" displayName="Table13" ref="B53:H65" totalsRowShown="0" headerRowDxfId="29" dataDxfId="27" headerRowBorderDxfId="28" tableBorderDxfId="26" totalsRowBorderDxfId="25">
-  <autoFilter ref="B53:H65"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table13" displayName="Table13" ref="B54:H71" totalsRowShown="0" headerRowDxfId="30" dataDxfId="28" headerRowBorderDxfId="29" tableBorderDxfId="27" totalsRowBorderDxfId="26">
+  <autoFilter ref="B54:H71"/>
   <tableColumns count="7">
-    <tableColumn id="1" name="{missionTypeDefinitions}" dataDxfId="24"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="23"/>
-    <tableColumn id="3" name="[minTier]" dataDxfId="22"/>
-    <tableColumn id="6" name="[maxTier]" dataDxfId="21"/>
-    <tableColumn id="4" name="[weight]" dataDxfId="20"/>
-    <tableColumn id="9" name="[tidDescSingleRun]" dataDxfId="19"/>
-    <tableColumn id="10" name="[tidDescMultiRun]" dataDxfId="18"/>
+    <tableColumn id="1" name="{missionTypeDefinitions}" dataDxfId="25"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="24"/>
+    <tableColumn id="3" name="[minTier]" dataDxfId="23"/>
+    <tableColumn id="6" name="[maxTier]" dataDxfId="22"/>
+    <tableColumn id="4" name="[weight]" dataDxfId="21"/>
+    <tableColumn id="9" name="[tidDescSingleRun]" dataDxfId="20"/>
+    <tableColumn id="10" name="[tidDescMultiRun]" dataDxfId="19"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table1330" displayName="Table1330" ref="B4:N48" totalsRowShown="0" headerRowDxfId="17" dataDxfId="15" headerRowBorderDxfId="16" tableBorderDxfId="14" totalsRowBorderDxfId="13">
-  <autoFilter ref="B4:N48"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table1330" displayName="Table1330" ref="B4:N49" totalsRowShown="0" headerRowDxfId="18" dataDxfId="16" headerRowBorderDxfId="17" tableBorderDxfId="15" totalsRowBorderDxfId="14">
+  <autoFilter ref="B4:N49"/>
   <tableColumns count="13">
-    <tableColumn id="1" name="{missionsDefinitions}" dataDxfId="12"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="11"/>
-    <tableColumn id="7" name="[type]" dataDxfId="10"/>
-    <tableColumn id="8" name="[weight]" dataDxfId="9"/>
-    <tableColumn id="13" name="[singleRunChance]" dataDxfId="8"/>
-    <tableColumn id="11" name="[minTier]" dataDxfId="7"/>
-    <tableColumn id="12" name="[maxTier]" dataDxfId="6"/>
-    <tableColumn id="6" name="[params]" dataDxfId="5"/>
-    <tableColumn id="3" name="[objectiveBaseQuantityMin]" dataDxfId="4"/>
-    <tableColumn id="9" name="[objectiveBaseQuantityMax]" dataDxfId="3"/>
-    <tableColumn id="4" name="[icon]" dataDxfId="2"/>
-    <tableColumn id="5" name="[tidObjective]" dataDxfId="1"/>
-    <tableColumn id="10" name="[trackingSku]" dataDxfId="0"/>
+    <tableColumn id="1" name="{missionsDefinitions}" dataDxfId="13"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="12"/>
+    <tableColumn id="7" name="[type]" dataDxfId="11"/>
+    <tableColumn id="8" name="[weight]" dataDxfId="10"/>
+    <tableColumn id="13" name="[singleRunChance]" dataDxfId="9"/>
+    <tableColumn id="11" name="[minTier]" dataDxfId="8"/>
+    <tableColumn id="12" name="[maxTier]" dataDxfId="7"/>
+    <tableColumn id="6" name="[params]" dataDxfId="6"/>
+    <tableColumn id="3" name="[objectiveBaseQuantityMin]" dataDxfId="5"/>
+    <tableColumn id="9" name="[objectiveBaseQuantityMax]" dataDxfId="4"/>
+    <tableColumn id="4" name="[icon]" dataDxfId="3"/>
+    <tableColumn id="5" name="[tidObjective]" dataDxfId="2"/>
+    <tableColumn id="10" name="[trackingSku]" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2666,10 +2649,10 @@
   <sheetPr>
     <tabColor theme="6"/>
   </sheetPr>
-  <dimension ref="B1:P100"/>
+  <dimension ref="B1:P105"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D40" sqref="D40"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C44" sqref="C32:C44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2713,14 +2696,14 @@
         <v>145</v>
       </c>
       <c r="G3" s="38"/>
-      <c r="J3" s="61" t="s">
+      <c r="J3" s="56" t="s">
         <v>144</v>
       </c>
-      <c r="K3" s="61"/>
-      <c r="M3" s="61"/>
-      <c r="N3" s="61"/>
-      <c r="O3" s="61"/>
-      <c r="P3" s="61"/>
+      <c r="K3" s="56"/>
+      <c r="M3" s="56"/>
+      <c r="N3" s="56"/>
+      <c r="O3" s="56"/>
+      <c r="P3" s="56"/>
     </row>
     <row r="4" spans="2:16" ht="106.5" x14ac:dyDescent="0.25">
       <c r="B4" s="30" t="s">
@@ -2798,7 +2781,7 @@
         <v>130</v>
       </c>
       <c r="M5" s="33" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="N5" s="31" t="s">
         <v>73</v>
@@ -2913,7 +2896,7 @@
         <v>130</v>
       </c>
       <c r="M8" s="33" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="N8" s="31" t="s">
         <v>73</v>
@@ -2942,7 +2925,7 @@
         <v>7</v>
       </c>
       <c r="I9" s="24" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="J9" s="24">
         <v>25</v>
@@ -2953,8 +2936,8 @@
       <c r="L9" s="33" t="s">
         <v>128</v>
       </c>
-      <c r="M9" s="48" t="s">
-        <v>174</v>
+      <c r="M9" s="47" t="s">
+        <v>172</v>
       </c>
       <c r="N9" s="31" t="s">
         <v>73</v>
@@ -2994,8 +2977,8 @@
       <c r="L10" s="33" t="s">
         <v>126</v>
       </c>
-      <c r="M10" s="48" t="s">
-        <v>175</v>
+      <c r="M10" s="47" t="s">
+        <v>173</v>
       </c>
       <c r="N10" s="31" t="s">
         <v>73</v>
@@ -3035,8 +3018,8 @@
       <c r="L11" s="33" t="s">
         <v>123</v>
       </c>
-      <c r="M11" s="48" t="s">
-        <v>175</v>
+      <c r="M11" s="47" t="s">
+        <v>173</v>
       </c>
       <c r="N11" s="31" t="s">
         <v>73</v>
@@ -3077,7 +3060,7 @@
         <v>121</v>
       </c>
       <c r="M12" s="33" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="N12" s="31" t="s">
         <v>73</v>
@@ -3118,7 +3101,7 @@
         <v>119</v>
       </c>
       <c r="M13" s="33" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="N13" s="31" t="s">
         <v>73</v>
@@ -3158,8 +3141,8 @@
       <c r="L14" s="33" t="s">
         <v>116</v>
       </c>
-      <c r="M14" s="48" t="s">
-        <v>179</v>
+      <c r="M14" s="47" t="s">
+        <v>177</v>
       </c>
       <c r="N14" s="31" t="s">
         <v>73</v>
@@ -3347,8 +3330,8 @@
       <c r="L19" s="34" t="s">
         <v>108</v>
       </c>
-      <c r="M19" s="48" t="s">
-        <v>181</v>
+      <c r="M19" s="47" t="s">
+        <v>179</v>
       </c>
       <c r="N19" s="31" t="s">
         <v>73</v>
@@ -3389,7 +3372,7 @@
         <v>105</v>
       </c>
       <c r="M20" s="33" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="N20" s="31" t="s">
         <v>73</v>
@@ -3429,8 +3412,8 @@
       <c r="L21" s="34" t="s">
         <v>102</v>
       </c>
-      <c r="M21" s="51" t="s">
-        <v>176</v>
+      <c r="M21" s="50" t="s">
+        <v>174</v>
       </c>
       <c r="N21" s="31" t="s">
         <v>73</v>
@@ -3471,7 +3454,7 @@
         <v>99</v>
       </c>
       <c r="M22" s="34" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="N22" s="31" t="s">
         <v>73</v>
@@ -3511,8 +3494,8 @@
       <c r="L23" s="34" t="s">
         <v>96</v>
       </c>
-      <c r="M23" s="51" t="s">
-        <v>183</v>
+      <c r="M23" s="50" t="s">
+        <v>181</v>
       </c>
       <c r="N23" s="31" t="s">
         <v>73</v>
@@ -3552,8 +3535,8 @@
       <c r="L24" s="34" t="s">
         <v>93</v>
       </c>
-      <c r="M24" s="52" t="s">
-        <v>184</v>
+      <c r="M24" s="51" t="s">
+        <v>182</v>
       </c>
       <c r="N24" s="31" t="s">
         <v>73</v>
@@ -3594,7 +3577,7 @@
         <v>90</v>
       </c>
       <c r="M25" s="34" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="N25" s="31" t="s">
         <v>73</v>
@@ -3635,7 +3618,7 @@
         <v>87</v>
       </c>
       <c r="M26" s="34" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="N26" s="31" t="s">
         <v>73</v>
@@ -3676,7 +3659,7 @@
         <v>84</v>
       </c>
       <c r="M27" s="34" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="N27" s="31" t="s">
         <v>73</v>
@@ -3717,7 +3700,7 @@
         <v>81</v>
       </c>
       <c r="M28" s="34" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="N28" s="31" t="s">
         <v>73</v>
@@ -3758,7 +3741,7 @@
         <v>78</v>
       </c>
       <c r="M29" s="34" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="N29" s="31" t="s">
         <v>73</v>
@@ -3799,7 +3782,7 @@
         <v>75</v>
       </c>
       <c r="M30" s="34" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="N30" s="31" t="s">
         <v>73</v>
@@ -3842,690 +3825,704 @@
         <v>73</v>
       </c>
     </row>
-    <row r="32" spans="2:14" s="44" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="53" t="s">
-        <v>1</v>
-      </c>
-      <c r="C32" s="54" t="s">
+    <row r="32" spans="2:14" s="43" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B32" s="52" t="s">
+        <v>1</v>
+      </c>
+      <c r="C32" s="53" t="s">
+        <v>212</v>
+      </c>
+      <c r="D32" s="54" t="s">
+        <v>208</v>
+      </c>
+      <c r="E32" s="54">
+        <v>1</v>
+      </c>
+      <c r="F32" s="54">
+        <v>0.3</v>
+      </c>
+      <c r="G32" s="53">
+        <v>0</v>
+      </c>
+      <c r="H32" s="54">
+        <v>7</v>
+      </c>
+      <c r="I32" s="54" t="s">
+        <v>149</v>
+      </c>
+      <c r="J32" s="53">
+        <v>99</v>
+      </c>
+      <c r="K32" s="54">
+        <v>99</v>
+      </c>
+      <c r="L32" s="48" t="s">
+        <v>130</v>
+      </c>
+      <c r="M32" s="48" t="s">
+        <v>188</v>
+      </c>
+      <c r="N32" s="55" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="33" spans="2:14" s="43" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B33" s="52" t="s">
+        <v>1</v>
+      </c>
+      <c r="C33" s="53" t="s">
+        <v>213</v>
+      </c>
+      <c r="D33" s="54" t="s">
+        <v>208</v>
+      </c>
+      <c r="E33" s="54">
+        <v>1</v>
+      </c>
+      <c r="F33" s="54">
+        <v>0.3</v>
+      </c>
+      <c r="G33" s="53">
+        <v>0</v>
+      </c>
+      <c r="H33" s="54">
+        <v>7</v>
+      </c>
+      <c r="I33" s="54" t="s">
+        <v>205</v>
+      </c>
+      <c r="J33" s="53">
+        <v>99</v>
+      </c>
+      <c r="K33" s="54">
+        <v>99</v>
+      </c>
+      <c r="L33" s="48" t="s">
+        <v>130</v>
+      </c>
+      <c r="M33" s="48" t="s">
+        <v>206</v>
+      </c>
+      <c r="N33" s="55" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="34" spans="2:14" s="43" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B34" s="52" t="s">
+        <v>1</v>
+      </c>
+      <c r="C34" s="53" t="s">
+        <v>209</v>
+      </c>
+      <c r="D34" s="54" t="s">
+        <v>207</v>
+      </c>
+      <c r="E34" s="54">
+        <v>1</v>
+      </c>
+      <c r="F34" s="54">
+        <v>0.3</v>
+      </c>
+      <c r="G34" s="53">
+        <v>0</v>
+      </c>
+      <c r="H34" s="54">
+        <v>7</v>
+      </c>
+      <c r="I34" s="54" t="s">
+        <v>150</v>
+      </c>
+      <c r="J34" s="53">
+        <v>99</v>
+      </c>
+      <c r="K34" s="54">
+        <v>99</v>
+      </c>
+      <c r="L34" s="48" t="s">
+        <v>130</v>
+      </c>
+      <c r="M34" s="48" t="s">
+        <v>179</v>
+      </c>
+      <c r="N34" s="55" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="35" spans="2:14" s="43" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B35" s="52" t="s">
+        <v>1</v>
+      </c>
+      <c r="C35" s="53" t="s">
         <v>155</v>
       </c>
-      <c r="D32" s="55" t="s">
-        <v>149</v>
-      </c>
-      <c r="E32" s="55">
-        <v>1</v>
-      </c>
-      <c r="F32" s="55">
+      <c r="D35" s="54" t="s">
+        <v>151</v>
+      </c>
+      <c r="E35" s="54">
+        <v>1</v>
+      </c>
+      <c r="F35" s="54">
         <v>0.3</v>
       </c>
-      <c r="G32" s="54">
+      <c r="G35" s="53">
         <v>0</v>
       </c>
-      <c r="H32" s="55">
-        <v>7</v>
-      </c>
-      <c r="I32" s="55" t="s">
-        <v>150</v>
-      </c>
-      <c r="J32" s="54">
+      <c r="H35" s="54">
+        <v>7</v>
+      </c>
+      <c r="I35" s="54"/>
+      <c r="J35" s="53">
         <v>99</v>
       </c>
-      <c r="K32" s="55">
+      <c r="K35" s="54">
         <v>99</v>
       </c>
-      <c r="L32" s="49" t="s">
+      <c r="L35" s="48" t="s">
         <v>130</v>
       </c>
-      <c r="M32" s="49" t="s">
+      <c r="M35" s="49"/>
+      <c r="N35" s="55" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="36" spans="2:14" s="43" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B36" s="52" t="s">
+        <v>1</v>
+      </c>
+      <c r="C36" s="53" t="s">
+        <v>165</v>
+      </c>
+      <c r="D36" s="54" t="s">
+        <v>151</v>
+      </c>
+      <c r="E36" s="54">
+        <v>1</v>
+      </c>
+      <c r="F36" s="54">
+        <v>0.3</v>
+      </c>
+      <c r="G36" s="53">
+        <v>3</v>
+      </c>
+      <c r="H36" s="54">
+        <v>7</v>
+      </c>
+      <c r="I36" s="54" t="s">
+        <v>166</v>
+      </c>
+      <c r="J36" s="53">
+        <v>99</v>
+      </c>
+      <c r="K36" s="54">
+        <v>99</v>
+      </c>
+      <c r="L36" s="48" t="s">
+        <v>130</v>
+      </c>
+      <c r="M36" s="54" t="s">
+        <v>189</v>
+      </c>
+      <c r="N36" s="55" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="37" spans="2:14" s="43" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B37" s="52" t="s">
+        <v>1</v>
+      </c>
+      <c r="C37" s="53" t="s">
+        <v>168</v>
+      </c>
+      <c r="D37" s="54" t="s">
+        <v>151</v>
+      </c>
+      <c r="E37" s="54">
+        <v>1</v>
+      </c>
+      <c r="F37" s="54">
+        <v>0.3</v>
+      </c>
+      <c r="G37" s="53">
+        <v>1</v>
+      </c>
+      <c r="H37" s="54">
+        <v>7</v>
+      </c>
+      <c r="I37" s="54" t="s">
+        <v>169</v>
+      </c>
+      <c r="J37" s="53">
+        <v>99</v>
+      </c>
+      <c r="K37" s="54">
+        <v>99</v>
+      </c>
+      <c r="L37" s="48" t="s">
+        <v>130</v>
+      </c>
+      <c r="M37" s="54" t="s">
         <v>190</v>
       </c>
-      <c r="N32" s="56" t="s">
+      <c r="N37" s="55" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="33" spans="2:14" s="44" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B33" s="53" t="s">
-        <v>1</v>
-      </c>
-      <c r="C33" s="54" t="s">
-        <v>207</v>
-      </c>
-      <c r="D33" s="55" t="s">
-        <v>149</v>
-      </c>
-      <c r="E33" s="55">
-        <v>1</v>
-      </c>
-      <c r="F33" s="55">
+    <row r="38" spans="2:14" s="43" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B38" s="52" t="s">
+        <v>1</v>
+      </c>
+      <c r="C38" s="53" t="s">
+        <v>156</v>
+      </c>
+      <c r="D38" s="54" t="s">
+        <v>151</v>
+      </c>
+      <c r="E38" s="54">
+        <v>1</v>
+      </c>
+      <c r="F38" s="54">
         <v>0.3</v>
       </c>
-      <c r="G33" s="54">
+      <c r="G38" s="53">
+        <v>2</v>
+      </c>
+      <c r="H38" s="54">
+        <v>7</v>
+      </c>
+      <c r="I38" s="54" t="s">
+        <v>167</v>
+      </c>
+      <c r="J38" s="53">
+        <v>99</v>
+      </c>
+      <c r="K38" s="54">
+        <v>99</v>
+      </c>
+      <c r="L38" s="48" t="s">
+        <v>130</v>
+      </c>
+      <c r="M38" s="54" t="s">
+        <v>191</v>
+      </c>
+      <c r="N38" s="55" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="39" spans="2:14" s="43" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B39" s="52" t="s">
+        <v>1</v>
+      </c>
+      <c r="C39" s="53" t="s">
+        <v>157</v>
+      </c>
+      <c r="D39" s="54" t="s">
+        <v>151</v>
+      </c>
+      <c r="E39" s="54">
+        <v>1</v>
+      </c>
+      <c r="F39" s="54">
+        <v>0.3</v>
+      </c>
+      <c r="G39" s="53">
+        <v>4</v>
+      </c>
+      <c r="H39" s="54">
+        <v>7</v>
+      </c>
+      <c r="I39" s="54" t="s">
+        <v>88</v>
+      </c>
+      <c r="J39" s="53">
+        <v>99</v>
+      </c>
+      <c r="K39" s="54">
+        <v>99</v>
+      </c>
+      <c r="L39" s="48" t="s">
+        <v>130</v>
+      </c>
+      <c r="M39" s="54" t="s">
+        <v>184</v>
+      </c>
+      <c r="N39" s="55" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="40" spans="2:14" s="43" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B40" s="52" t="s">
+        <v>1</v>
+      </c>
+      <c r="C40" s="53" t="s">
+        <v>163</v>
+      </c>
+      <c r="D40" s="54" t="s">
+        <v>151</v>
+      </c>
+      <c r="E40" s="54">
+        <v>1</v>
+      </c>
+      <c r="F40" s="54">
+        <v>0.3</v>
+      </c>
+      <c r="G40" s="53">
         <v>0</v>
       </c>
-      <c r="H33" s="55">
-        <v>7</v>
-      </c>
-      <c r="I33" s="55" t="s">
-        <v>208</v>
-      </c>
-      <c r="J33" s="54">
+      <c r="H40" s="54">
+        <v>7</v>
+      </c>
+      <c r="I40" s="54" t="s">
+        <v>164</v>
+      </c>
+      <c r="J40" s="53">
         <v>99</v>
       </c>
-      <c r="K33" s="55">
+      <c r="K40" s="54">
         <v>99</v>
       </c>
-      <c r="L33" s="49" t="s">
+      <c r="L40" s="48" t="s">
         <v>130</v>
       </c>
-      <c r="M33" s="49" t="s">
-        <v>209</v>
-      </c>
-      <c r="N33" s="56" t="s">
+      <c r="M40" s="49" t="s">
+        <v>192</v>
+      </c>
+      <c r="N40" s="55" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="34" spans="2:14" s="44" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B34" s="53"/>
-      <c r="C34" s="54"/>
-      <c r="D34" s="55"/>
-      <c r="E34" s="55"/>
-      <c r="F34" s="55"/>
-      <c r="G34" s="54"/>
-      <c r="H34" s="55"/>
-      <c r="I34" s="55"/>
-      <c r="J34" s="54"/>
-      <c r="K34" s="55"/>
-      <c r="L34" s="49"/>
-      <c r="M34" s="58"/>
-      <c r="N34" s="56"/>
-    </row>
-    <row r="35" spans="2:14" s="44" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B35" s="53" t="s">
-        <v>1</v>
-      </c>
-      <c r="C35" s="54" t="s">
-        <v>212</v>
-      </c>
-      <c r="D35" s="55" t="s">
-        <v>210</v>
-      </c>
-      <c r="E35" s="55">
-        <v>1</v>
-      </c>
-      <c r="F35" s="55">
+    <row r="41" spans="2:14" s="43" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B41" s="52" t="s">
+        <v>1</v>
+      </c>
+      <c r="C41" s="53" t="s">
+        <v>204</v>
+      </c>
+      <c r="D41" s="54" t="s">
+        <v>151</v>
+      </c>
+      <c r="E41" s="54">
+        <v>1</v>
+      </c>
+      <c r="F41" s="54">
         <v>0.3</v>
       </c>
-      <c r="G35" s="54">
+      <c r="G41" s="53">
         <v>0</v>
       </c>
-      <c r="H35" s="55">
-        <v>7</v>
-      </c>
-      <c r="I35" s="55" t="s">
-        <v>151</v>
-      </c>
-      <c r="J35" s="54">
+      <c r="H41" s="54">
+        <v>7</v>
+      </c>
+      <c r="I41" s="54" t="s">
+        <v>162</v>
+      </c>
+      <c r="J41" s="53">
         <v>99</v>
       </c>
-      <c r="K35" s="55">
+      <c r="K41" s="54">
         <v>99</v>
       </c>
-      <c r="L35" s="49" t="s">
+      <c r="L41" s="48" t="s">
         <v>130</v>
       </c>
-      <c r="M35" s="49" t="s">
-        <v>181</v>
-      </c>
-      <c r="N35" s="56" t="s">
+      <c r="M41" s="49" t="s">
+        <v>194</v>
+      </c>
+      <c r="N41" s="55" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="36" spans="2:14" s="44" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B36" s="53"/>
-      <c r="C36" s="54"/>
-      <c r="D36" s="55"/>
-      <c r="E36" s="55"/>
-      <c r="F36" s="55"/>
-      <c r="G36" s="54"/>
-      <c r="H36" s="55"/>
-      <c r="I36" s="55"/>
-      <c r="J36" s="54"/>
-      <c r="K36" s="55"/>
-      <c r="L36" s="49"/>
-      <c r="M36" s="50"/>
-      <c r="N36" s="56"/>
-    </row>
-    <row r="37" spans="2:14" s="44" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B37" s="53" t="s">
-        <v>1</v>
-      </c>
-      <c r="C37" s="54" t="s">
-        <v>157</v>
-      </c>
-      <c r="D37" s="55" t="s">
+    <row r="42" spans="2:14" s="43" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B42" s="52" t="s">
+        <v>1</v>
+      </c>
+      <c r="C42" s="53" t="s">
+        <v>154</v>
+      </c>
+      <c r="D42" s="54" t="s">
         <v>152</v>
       </c>
-      <c r="E37" s="55">
-        <v>1</v>
-      </c>
-      <c r="F37" s="55">
+      <c r="E42" s="54">
+        <v>1</v>
+      </c>
+      <c r="F42" s="54">
         <v>0.3</v>
       </c>
-      <c r="G37" s="54">
+      <c r="G42" s="53">
+        <v>1</v>
+      </c>
+      <c r="H42" s="54">
+        <v>7</v>
+      </c>
+      <c r="I42" s="54" t="s">
+        <v>153</v>
+      </c>
+      <c r="J42" s="53">
+        <v>99</v>
+      </c>
+      <c r="K42" s="54">
+        <v>99</v>
+      </c>
+      <c r="L42" s="48" t="s">
+        <v>130</v>
+      </c>
+      <c r="M42" s="49" t="s">
+        <v>178</v>
+      </c>
+      <c r="N42" s="55" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="43" spans="2:14" s="43" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B43" s="52" t="s">
+        <v>1</v>
+      </c>
+      <c r="C43" s="53" t="s">
+        <v>160</v>
+      </c>
+      <c r="D43" s="54" t="s">
+        <v>152</v>
+      </c>
+      <c r="E43" s="54">
+        <v>1</v>
+      </c>
+      <c r="F43" s="54">
+        <v>0.3</v>
+      </c>
+      <c r="G43" s="53">
         <v>0</v>
       </c>
-      <c r="H37" s="55">
-        <v>7</v>
-      </c>
-      <c r="I37" s="55"/>
-      <c r="J37" s="54">
+      <c r="H43" s="54">
+        <v>7</v>
+      </c>
+      <c r="I43" s="54" t="s">
+        <v>161</v>
+      </c>
+      <c r="J43" s="53">
         <v>99</v>
       </c>
-      <c r="K37" s="55">
+      <c r="K43" s="54">
         <v>99</v>
       </c>
-      <c r="L37" s="49" t="s">
+      <c r="L43" s="48" t="s">
         <v>130</v>
       </c>
-      <c r="M37" s="50"/>
-      <c r="N37" s="56" t="s">
+      <c r="M43" s="49" t="s">
+        <v>172</v>
+      </c>
+      <c r="N43" s="55" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="38" spans="2:14" s="44" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B38" s="53" t="s">
-        <v>1</v>
-      </c>
-      <c r="C38" s="54" t="s">
-        <v>167</v>
-      </c>
-      <c r="D38" s="55" t="s">
+    <row r="44" spans="2:14" s="43" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B44" s="52" t="s">
+        <v>1</v>
+      </c>
+      <c r="C44" s="53" t="s">
+        <v>158</v>
+      </c>
+      <c r="D44" s="54" t="s">
         <v>152</v>
       </c>
-      <c r="E38" s="55">
-        <v>1</v>
-      </c>
-      <c r="F38" s="55">
+      <c r="E44" s="54">
+        <v>1</v>
+      </c>
+      <c r="F44" s="54">
         <v>0.3</v>
       </c>
-      <c r="G38" s="54">
+      <c r="G44" s="53">
+        <v>1</v>
+      </c>
+      <c r="H44" s="54">
+        <v>7</v>
+      </c>
+      <c r="I44" s="54" t="s">
+        <v>159</v>
+      </c>
+      <c r="J44" s="53">
+        <v>99</v>
+      </c>
+      <c r="K44" s="54">
+        <v>99</v>
+      </c>
+      <c r="L44" s="48" t="s">
+        <v>130</v>
+      </c>
+      <c r="M44" s="49" t="s">
+        <v>195</v>
+      </c>
+      <c r="N44" s="55" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="45" spans="2:14" s="43" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B45" s="52" t="s">
+        <v>1</v>
+      </c>
+      <c r="C45" s="53"/>
+      <c r="D45" s="54"/>
+      <c r="E45" s="54">
+        <v>1</v>
+      </c>
+      <c r="F45" s="54">
+        <v>0.3</v>
+      </c>
+      <c r="G45" s="53">
+        <v>1</v>
+      </c>
+      <c r="H45" s="54">
+        <v>7</v>
+      </c>
+      <c r="I45" s="54"/>
+      <c r="J45" s="53">
+        <v>99</v>
+      </c>
+      <c r="K45" s="54">
+        <v>99</v>
+      </c>
+      <c r="L45" s="48" t="s">
+        <v>130</v>
+      </c>
+      <c r="M45" s="49"/>
+      <c r="N45" s="55" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="46" spans="2:14" s="43" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B46" s="46"/>
+      <c r="C46" s="41"/>
+      <c r="D46" s="41"/>
+      <c r="E46" s="41"/>
+      <c r="F46" s="41"/>
+      <c r="G46" s="41"/>
+      <c r="H46" s="41"/>
+      <c r="I46" s="41"/>
+      <c r="J46" s="41"/>
+      <c r="K46" s="41"/>
+      <c r="L46" s="60"/>
+      <c r="M46" s="60"/>
+      <c r="N46" s="44"/>
+    </row>
+    <row r="47" spans="2:14" s="43" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B47" s="59"/>
+      <c r="C47" s="40"/>
+      <c r="D47" s="41"/>
+      <c r="E47" s="41"/>
+      <c r="F47" s="41"/>
+      <c r="G47" s="40"/>
+      <c r="H47" s="41"/>
+      <c r="I47" s="41"/>
+      <c r="J47" s="40"/>
+      <c r="K47" s="41"/>
+      <c r="L47" s="60"/>
+      <c r="M47" s="60"/>
+      <c r="N47" s="44"/>
+    </row>
+    <row r="48" spans="2:14" s="43" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B48" s="59"/>
+      <c r="C48" s="40"/>
+      <c r="D48" s="41"/>
+      <c r="E48" s="41"/>
+      <c r="F48" s="60"/>
+      <c r="G48" s="40"/>
+      <c r="H48" s="60"/>
+      <c r="I48" s="41"/>
+      <c r="J48" s="40"/>
+      <c r="K48" s="41"/>
+      <c r="L48" s="60"/>
+      <c r="M48" s="60"/>
+      <c r="N48" s="44"/>
+    </row>
+    <row r="49" spans="2:14" s="43" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B49" s="46"/>
+      <c r="C49" s="41"/>
+      <c r="D49" s="41"/>
+      <c r="E49" s="41"/>
+      <c r="F49" s="60"/>
+      <c r="G49" s="41"/>
+      <c r="H49" s="60"/>
+      <c r="I49" s="41"/>
+      <c r="J49" s="41"/>
+      <c r="K49" s="41"/>
+      <c r="L49" s="60"/>
+      <c r="M49" s="60"/>
+      <c r="N49" s="44"/>
+    </row>
+    <row r="50" spans="2:14" s="43" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B50" s="44"/>
+      <c r="C50" s="44"/>
+      <c r="D50" s="44"/>
+      <c r="E50" s="44"/>
+      <c r="F50" s="44"/>
+      <c r="G50" s="44"/>
+      <c r="H50" s="44"/>
+      <c r="I50" s="44"/>
+      <c r="J50" s="44"/>
+      <c r="K50" s="44"/>
+      <c r="L50" s="44"/>
+      <c r="M50" s="44"/>
+      <c r="N50" s="44"/>
+    </row>
+    <row r="51" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B51" s="32"/>
+      <c r="C51" s="32"/>
+      <c r="D51" s="32"/>
+      <c r="E51" s="32"/>
+      <c r="F51" s="32"/>
+      <c r="G51" s="32"/>
+      <c r="H51" s="32"/>
+      <c r="I51" s="32"/>
+      <c r="J51" s="32"/>
+      <c r="K51" s="32"/>
+      <c r="L51" s="32"/>
+      <c r="M51" s="31"/>
+    </row>
+    <row r="52" spans="2:14" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B52" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="C52" s="6"/>
+      <c r="D52" s="6"/>
+      <c r="E52" s="6"/>
+      <c r="F52" s="6"/>
+      <c r="G52" s="6"/>
+      <c r="H52" s="6"/>
+      <c r="I52" s="6"/>
+      <c r="J52" s="6"/>
+      <c r="K52" s="6"/>
+      <c r="L52" s="6"/>
+    </row>
+    <row r="53" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B53" s="20"/>
+      <c r="C53" s="20"/>
+      <c r="D53" s="20"/>
+      <c r="E53" s="20"/>
+      <c r="F53" s="57"/>
+      <c r="G53" s="57"/>
+      <c r="H53" s="57"/>
+      <c r="I53" s="20"/>
+      <c r="J53" s="20"/>
+    </row>
+    <row r="54" spans="2:14" ht="96" x14ac:dyDescent="0.25">
+      <c r="B54" s="30" t="s">
+        <v>71</v>
+      </c>
+      <c r="C54" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="H38" s="55">
-        <v>7</v>
-      </c>
-      <c r="I38" s="55" t="s">
-        <v>168</v>
-      </c>
-      <c r="J38" s="54">
-        <v>99</v>
-      </c>
-      <c r="K38" s="55">
-        <v>99</v>
-      </c>
-      <c r="L38" s="49" t="s">
-        <v>130</v>
-      </c>
-      <c r="M38" s="55" t="s">
-        <v>191</v>
-      </c>
-      <c r="N38" s="56" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="39" spans="2:14" s="44" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B39" s="53"/>
-      <c r="C39" s="54" t="s">
-        <v>170</v>
-      </c>
-      <c r="D39" s="55" t="s">
-        <v>152</v>
-      </c>
-      <c r="E39" s="55">
-        <v>1</v>
-      </c>
-      <c r="F39" s="55">
-        <v>0.3</v>
-      </c>
-      <c r="G39" s="54">
-        <v>1</v>
-      </c>
-      <c r="H39" s="55">
-        <v>7</v>
-      </c>
-      <c r="I39" s="55" t="s">
-        <v>171</v>
-      </c>
-      <c r="J39" s="54">
-        <v>99</v>
-      </c>
-      <c r="K39" s="55">
-        <v>99</v>
-      </c>
-      <c r="L39" s="49" t="s">
-        <v>130</v>
-      </c>
-      <c r="M39" s="55" t="s">
-        <v>192</v>
-      </c>
-      <c r="N39" s="56" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="40" spans="2:14" s="44" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B40" s="53" t="s">
-        <v>1</v>
-      </c>
-      <c r="C40" s="54" t="s">
-        <v>158</v>
-      </c>
-      <c r="D40" s="55" t="s">
-        <v>152</v>
-      </c>
-      <c r="E40" s="55">
-        <v>1</v>
-      </c>
-      <c r="F40" s="55">
-        <v>0.3</v>
-      </c>
-      <c r="G40" s="54">
-        <v>2</v>
-      </c>
-      <c r="H40" s="55">
-        <v>7</v>
-      </c>
-      <c r="I40" s="55" t="s">
-        <v>169</v>
-      </c>
-      <c r="J40" s="54">
-        <v>99</v>
-      </c>
-      <c r="K40" s="55">
-        <v>99</v>
-      </c>
-      <c r="L40" s="49" t="s">
-        <v>130</v>
-      </c>
-      <c r="M40" s="55" t="s">
-        <v>193</v>
-      </c>
-      <c r="N40" s="56" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="41" spans="2:14" s="44" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B41" s="53"/>
-      <c r="C41" s="54" t="s">
-        <v>159</v>
-      </c>
-      <c r="D41" s="55" t="s">
-        <v>152</v>
-      </c>
-      <c r="E41" s="55">
-        <v>1</v>
-      </c>
-      <c r="F41" s="55">
-        <v>0.3</v>
-      </c>
-      <c r="G41" s="54">
-        <v>4</v>
-      </c>
-      <c r="H41" s="55">
-        <v>7</v>
-      </c>
-      <c r="I41" s="55" t="s">
-        <v>88</v>
-      </c>
-      <c r="J41" s="54">
-        <v>99</v>
-      </c>
-      <c r="K41" s="55">
-        <v>99</v>
-      </c>
-      <c r="L41" s="49" t="s">
-        <v>130</v>
-      </c>
-      <c r="M41" s="55" t="s">
-        <v>186</v>
-      </c>
-      <c r="N41" s="56" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="42" spans="2:14" s="44" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B42" s="53" t="s">
-        <v>1</v>
-      </c>
-      <c r="C42" s="54" t="s">
-        <v>165</v>
-      </c>
-      <c r="D42" s="55" t="s">
-        <v>152</v>
-      </c>
-      <c r="E42" s="55">
-        <v>1</v>
-      </c>
-      <c r="F42" s="55">
-        <v>0.3</v>
-      </c>
-      <c r="G42" s="54">
-        <v>0</v>
-      </c>
-      <c r="H42" s="55">
-        <v>7</v>
-      </c>
-      <c r="I42" s="55" t="s">
-        <v>166</v>
-      </c>
-      <c r="J42" s="54">
-        <v>99</v>
-      </c>
-      <c r="K42" s="55">
-        <v>99</v>
-      </c>
-      <c r="L42" s="49" t="s">
-        <v>130</v>
-      </c>
-      <c r="M42" s="50" t="s">
-        <v>194</v>
-      </c>
-      <c r="N42" s="56" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="43" spans="2:14" s="44" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B43" s="53" t="s">
-        <v>1</v>
-      </c>
-      <c r="C43" s="54" t="s">
-        <v>206</v>
-      </c>
-      <c r="D43" s="55" t="s">
-        <v>152</v>
-      </c>
-      <c r="E43" s="55">
-        <v>1</v>
-      </c>
-      <c r="F43" s="55">
-        <v>0.3</v>
-      </c>
-      <c r="G43" s="54">
-        <v>0</v>
-      </c>
-      <c r="H43" s="55">
-        <v>7</v>
-      </c>
-      <c r="I43" s="55" t="s">
-        <v>164</v>
-      </c>
-      <c r="J43" s="54">
-        <v>99</v>
-      </c>
-      <c r="K43" s="55">
-        <v>99</v>
-      </c>
-      <c r="L43" s="49" t="s">
-        <v>130</v>
-      </c>
-      <c r="M43" s="50" t="s">
-        <v>196</v>
-      </c>
-      <c r="N43" s="56" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="44" spans="2:14" s="44" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B44" s="53"/>
-      <c r="C44" s="54"/>
-      <c r="D44" s="55"/>
-      <c r="E44" s="55"/>
-      <c r="F44" s="55"/>
-      <c r="G44" s="54"/>
-      <c r="H44" s="55"/>
-      <c r="I44" s="55"/>
-      <c r="J44" s="54"/>
-      <c r="K44" s="55"/>
-      <c r="L44" s="49"/>
-      <c r="M44" s="50"/>
-      <c r="N44" s="56"/>
-    </row>
-    <row r="45" spans="2:14" s="44" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B45" s="53" t="s">
-        <v>1</v>
-      </c>
-      <c r="C45" s="54" t="s">
-        <v>156</v>
-      </c>
-      <c r="D45" s="55" t="s">
-        <v>153</v>
-      </c>
-      <c r="E45" s="55">
-        <v>1</v>
-      </c>
-      <c r="F45" s="55">
-        <v>0.3</v>
-      </c>
-      <c r="G45" s="54">
-        <v>0</v>
-      </c>
-      <c r="H45" s="55">
-        <v>7</v>
-      </c>
-      <c r="I45" s="55" t="s">
-        <v>154</v>
-      </c>
-      <c r="J45" s="54">
-        <v>99</v>
-      </c>
-      <c r="K45" s="55">
-        <v>99</v>
-      </c>
-      <c r="L45" s="49" t="s">
-        <v>130</v>
-      </c>
-      <c r="M45" s="50" t="s">
-        <v>180</v>
-      </c>
-      <c r="N45" s="56" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="46" spans="2:14" s="44" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B46" s="53" t="s">
-        <v>1</v>
-      </c>
-      <c r="C46" s="54" t="s">
-        <v>162</v>
-      </c>
-      <c r="D46" s="55" t="s">
-        <v>153</v>
-      </c>
-      <c r="E46" s="55">
-        <v>1</v>
-      </c>
-      <c r="F46" s="55">
-        <v>0.3</v>
-      </c>
-      <c r="G46" s="54">
-        <v>0</v>
-      </c>
-      <c r="H46" s="55">
-        <v>7</v>
-      </c>
-      <c r="I46" s="55" t="s">
-        <v>163</v>
-      </c>
-      <c r="J46" s="54">
-        <v>99</v>
-      </c>
-      <c r="K46" s="55">
-        <v>99</v>
-      </c>
-      <c r="L46" s="49" t="s">
-        <v>130</v>
-      </c>
-      <c r="M46" s="50" t="s">
-        <v>174</v>
-      </c>
-      <c r="N46" s="56" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="47" spans="2:14" s="44" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B47" s="53" t="s">
-        <v>1</v>
-      </c>
-      <c r="C47" s="54" t="s">
-        <v>160</v>
-      </c>
-      <c r="D47" s="55" t="s">
-        <v>153</v>
-      </c>
-      <c r="E47" s="55">
-        <v>1</v>
-      </c>
-      <c r="F47" s="55">
-        <v>0.3</v>
-      </c>
-      <c r="G47" s="54">
-        <v>0</v>
-      </c>
-      <c r="H47" s="55">
-        <v>7</v>
-      </c>
-      <c r="I47" s="55" t="s">
-        <v>161</v>
-      </c>
-      <c r="J47" s="54">
-        <v>99</v>
-      </c>
-      <c r="K47" s="55">
-        <v>99</v>
-      </c>
-      <c r="L47" s="49" t="s">
-        <v>130</v>
-      </c>
-      <c r="M47" s="50" t="s">
-        <v>197</v>
-      </c>
-      <c r="N47" s="56" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="48" spans="2:14" s="44" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B48" s="57"/>
-      <c r="C48" s="55"/>
-      <c r="D48" s="55"/>
-      <c r="E48" s="55"/>
-      <c r="F48" s="55"/>
-      <c r="G48" s="55"/>
-      <c r="H48" s="55"/>
-      <c r="I48" s="55"/>
-      <c r="J48" s="55"/>
-      <c r="K48" s="55"/>
-      <c r="L48" s="59"/>
-      <c r="M48" s="59"/>
-      <c r="N48" s="60"/>
-    </row>
-    <row r="49" spans="2:14" s="44" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B49" s="45"/>
-      <c r="C49" s="45"/>
-      <c r="D49" s="45"/>
-      <c r="E49" s="45"/>
-      <c r="F49" s="45"/>
-      <c r="G49" s="45"/>
-      <c r="H49" s="45"/>
-      <c r="I49" s="45"/>
-      <c r="J49" s="45"/>
-      <c r="K49" s="45"/>
-      <c r="L49" s="45"/>
-      <c r="M49" s="45"/>
-      <c r="N49" s="43"/>
-    </row>
-    <row r="50" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B50" s="32"/>
-      <c r="C50" s="32"/>
-      <c r="D50" s="32"/>
-      <c r="E50" s="32"/>
-      <c r="F50" s="32"/>
-      <c r="G50" s="32"/>
-      <c r="H50" s="32"/>
-      <c r="I50" s="32"/>
-      <c r="J50" s="32"/>
-      <c r="K50" s="32"/>
-      <c r="L50" s="32"/>
-      <c r="M50" s="31"/>
-    </row>
-    <row r="51" spans="2:14" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B51" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="C51" s="6"/>
-      <c r="D51" s="6"/>
-      <c r="E51" s="6"/>
-      <c r="F51" s="6"/>
-      <c r="G51" s="6"/>
-      <c r="H51" s="6"/>
-      <c r="I51" s="6"/>
-      <c r="J51" s="6"/>
-      <c r="K51" s="6"/>
-      <c r="L51" s="6"/>
-    </row>
-    <row r="52" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B52" s="20"/>
-      <c r="C52" s="20"/>
-      <c r="D52" s="20"/>
-      <c r="E52" s="20"/>
-      <c r="F52" s="62"/>
-      <c r="G52" s="62"/>
-      <c r="H52" s="62"/>
-      <c r="I52" s="20"/>
-      <c r="J52" s="20"/>
-    </row>
-    <row r="53" spans="2:14" ht="96" x14ac:dyDescent="0.25">
-      <c r="B53" s="30" t="s">
-        <v>71</v>
-      </c>
-      <c r="C53" s="28" t="s">
-        <v>3</v>
-      </c>
-      <c r="D53" s="29" t="s">
+      <c r="D54" s="29" t="s">
         <v>70</v>
       </c>
-      <c r="E53" s="29" t="s">
+      <c r="E54" s="29" t="s">
         <v>69</v>
       </c>
-      <c r="F53" s="29" t="s">
+      <c r="F54" s="29" t="s">
         <v>68</v>
       </c>
-      <c r="G53" s="28" t="s">
+      <c r="G54" s="28" t="s">
         <v>67</v>
       </c>
-      <c r="H53" s="28" t="s">
+      <c r="H54" s="28" t="s">
         <v>66</v>
-      </c>
-    </row>
-    <row r="54" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B54" s="27" t="s">
-        <v>1</v>
-      </c>
-      <c r="C54" s="24" t="s">
-        <v>65</v>
-      </c>
-      <c r="D54" s="24">
-        <v>0</v>
-      </c>
-      <c r="E54" s="24">
-        <v>7</v>
-      </c>
-      <c r="F54" s="24">
-        <v>2</v>
-      </c>
-      <c r="G54" s="26" t="s">
-        <v>64</v>
-      </c>
-      <c r="H54" s="26" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="55" spans="2:14" x14ac:dyDescent="0.25">
@@ -4533,7 +4530,7 @@
         <v>1</v>
       </c>
       <c r="C55" s="24" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="D55" s="24">
         <v>0</v>
@@ -4542,13 +4539,13 @@
         <v>7</v>
       </c>
       <c r="F55" s="24">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G55" s="26" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="H55" s="26" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
     </row>
     <row r="56" spans="2:14" x14ac:dyDescent="0.25">
@@ -4556,7 +4553,7 @@
         <v>1</v>
       </c>
       <c r="C56" s="24" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="D56" s="24">
         <v>0</v>
@@ -4565,13 +4562,13 @@
         <v>7</v>
       </c>
       <c r="F56" s="24">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G56" s="26" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="H56" s="26" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
     </row>
     <row r="57" spans="2:14" x14ac:dyDescent="0.25">
@@ -4579,7 +4576,7 @@
         <v>1</v>
       </c>
       <c r="C57" s="24" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="D57" s="24">
         <v>0</v>
@@ -4588,59 +4585,59 @@
         <v>7</v>
       </c>
       <c r="F57" s="24">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G57" s="26" t="s">
+        <v>58</v>
+      </c>
+      <c r="H57" s="26" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="58" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B58" s="27" t="s">
+        <v>1</v>
+      </c>
+      <c r="C58" s="24" t="s">
+        <v>56</v>
+      </c>
+      <c r="D58" s="24">
+        <v>0</v>
+      </c>
+      <c r="E58" s="24">
+        <v>7</v>
+      </c>
+      <c r="F58" s="24">
+        <v>1</v>
+      </c>
+      <c r="G58" s="26" t="s">
         <v>55</v>
       </c>
-      <c r="H57" s="26" t="s">
+      <c r="H58" s="26" t="s">
         <v>54</v>
-      </c>
-    </row>
-    <row r="58" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B58" s="25" t="s">
-        <v>1</v>
-      </c>
-      <c r="C58" s="23" t="s">
-        <v>53</v>
-      </c>
-      <c r="D58" s="23">
-        <v>0</v>
-      </c>
-      <c r="E58" s="24">
-        <v>7</v>
-      </c>
-      <c r="F58" s="23">
-        <v>1</v>
-      </c>
-      <c r="G58" s="26" t="s">
-        <v>52</v>
-      </c>
-      <c r="H58" s="26" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="59" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B59" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="C59" s="24" t="s">
-        <v>50</v>
-      </c>
-      <c r="D59" s="24">
+      <c r="C59" s="23" t="s">
+        <v>53</v>
+      </c>
+      <c r="D59" s="23">
         <v>0</v>
       </c>
       <c r="E59" s="24">
         <v>7</v>
       </c>
-      <c r="F59" s="24">
+      <c r="F59" s="23">
         <v>1</v>
       </c>
       <c r="G59" s="26" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="H59" s="26" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
     </row>
     <row r="60" spans="2:14" x14ac:dyDescent="0.25">
@@ -4648,7 +4645,7 @@
         <v>1</v>
       </c>
       <c r="C60" s="24" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="D60" s="24">
         <v>0</v>
@@ -4660,64 +4657,64 @@
         <v>1</v>
       </c>
       <c r="G60" s="26" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="H60" s="26" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
     </row>
     <row r="61" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B61" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="C61" s="23" t="s">
+      <c r="C61" s="24" t="s">
+        <v>47</v>
+      </c>
+      <c r="D61" s="24">
+        <v>0</v>
+      </c>
+      <c r="E61" s="24">
+        <v>7</v>
+      </c>
+      <c r="F61" s="24">
+        <v>1</v>
+      </c>
+      <c r="G61" s="26" t="s">
+        <v>46</v>
+      </c>
+      <c r="H61" s="26" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="62" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B62" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="C62" s="23" t="s">
         <v>44</v>
       </c>
-      <c r="D61" s="23">
+      <c r="D62" s="23">
         <v>0</v>
       </c>
-      <c r="E61" s="24">
-        <v>7</v>
-      </c>
-      <c r="F61" s="23">
-        <v>1</v>
-      </c>
-      <c r="G61" s="22" t="s">
+      <c r="E62" s="24">
+        <v>7</v>
+      </c>
+      <c r="F62" s="23">
+        <v>1</v>
+      </c>
+      <c r="G62" s="22" t="s">
         <v>43</v>
       </c>
-      <c r="H61" s="22" t="s">
+      <c r="H62" s="22" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="62" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B62" s="47" t="s">
-        <v>1</v>
-      </c>
-      <c r="C62" s="41" t="s">
+    <row r="63" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B63" s="46" t="s">
+        <v>1</v>
+      </c>
+      <c r="C63" s="41" t="s">
         <v>211</v>
-      </c>
-      <c r="D62" s="41">
-        <v>0</v>
-      </c>
-      <c r="E62" s="41">
-        <v>7</v>
-      </c>
-      <c r="F62" s="41">
-        <v>1</v>
-      </c>
-      <c r="G62" s="42" t="s">
-        <v>198</v>
-      </c>
-      <c r="H62" s="42" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="63" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B63" s="47" t="s">
-        <v>1</v>
-      </c>
-      <c r="C63" s="41" t="s">
-        <v>210</v>
       </c>
       <c r="D63" s="41">
         <v>0</v>
@@ -4726,21 +4723,21 @@
         <v>7</v>
       </c>
       <c r="F63" s="41">
-        <v>2</v>
-      </c>
-      <c r="G63" s="46" t="s">
-        <v>201</v>
-      </c>
-      <c r="H63" s="46" t="s">
-        <v>203</v>
+        <v>1</v>
+      </c>
+      <c r="G63" s="42" t="s">
+        <v>196</v>
+      </c>
+      <c r="H63" s="42" t="s">
+        <v>200</v>
       </c>
     </row>
     <row r="64" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B64" s="47" t="s">
+      <c r="B64" s="46" t="s">
         <v>1</v>
       </c>
       <c r="C64" s="41" t="s">
-        <v>152</v>
+        <v>207</v>
       </c>
       <c r="D64" s="41">
         <v>0</v>
@@ -4751,19 +4748,19 @@
       <c r="F64" s="41">
         <v>2</v>
       </c>
-      <c r="G64" s="46" t="s">
+      <c r="G64" s="45" t="s">
         <v>199</v>
       </c>
-      <c r="H64" s="46" t="s">
-        <v>204</v>
+      <c r="H64" s="45" t="s">
+        <v>201</v>
       </c>
     </row>
     <row r="65" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B65" s="47" t="s">
+      <c r="B65" s="46" t="s">
         <v>1</v>
       </c>
       <c r="C65" s="41" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="D65" s="41">
         <v>0</v>
@@ -4774,274 +4771,265 @@
       <c r="F65" s="41">
         <v>2</v>
       </c>
-      <c r="G65" s="46" t="s">
+      <c r="G65" s="45" t="s">
+        <v>197</v>
+      </c>
+      <c r="H65" s="45" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="66" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B66" s="46" t="s">
+        <v>1</v>
+      </c>
+      <c r="C66" s="41" t="s">
+        <v>152</v>
+      </c>
+      <c r="D66" s="41">
+        <v>0</v>
+      </c>
+      <c r="E66" s="41">
+        <v>7</v>
+      </c>
+      <c r="F66" s="41">
+        <v>2</v>
+      </c>
+      <c r="G66" s="45" t="s">
+        <v>198</v>
+      </c>
+      <c r="H66" s="45" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="67" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B67" s="59"/>
+      <c r="C67" s="40" t="s">
+        <v>210</v>
+      </c>
+      <c r="D67" s="40"/>
+      <c r="E67" s="40"/>
+      <c r="F67" s="40"/>
+      <c r="G67" s="61"/>
+      <c r="H67" s="61"/>
+    </row>
+    <row r="68" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B68" s="59"/>
+      <c r="C68" s="40"/>
+      <c r="D68" s="40"/>
+      <c r="E68" s="40"/>
+      <c r="F68" s="40"/>
+      <c r="G68" s="62"/>
+      <c r="H68" s="62"/>
+    </row>
+    <row r="69" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B69" s="59"/>
+      <c r="C69" s="40"/>
+      <c r="D69" s="40"/>
+      <c r="E69" s="40"/>
+      <c r="F69" s="40"/>
+      <c r="G69" s="62"/>
+      <c r="H69" s="62"/>
+    </row>
+    <row r="70" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B70" s="59"/>
+      <c r="C70" s="40"/>
+      <c r="D70" s="40"/>
+      <c r="E70" s="40"/>
+      <c r="F70" s="40"/>
+      <c r="G70" s="62"/>
+      <c r="H70" s="62"/>
+    </row>
+    <row r="71" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B71" s="46"/>
+      <c r="C71" s="41"/>
+      <c r="D71" s="41"/>
+      <c r="E71" s="41"/>
+      <c r="F71" s="41"/>
+      <c r="G71" s="63"/>
+      <c r="H71" s="63"/>
+    </row>
+    <row r="72" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="73" spans="2:13" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B73" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="C73" s="6"/>
+      <c r="D73" s="6"/>
+      <c r="E73" s="6"/>
+      <c r="F73" s="6"/>
+      <c r="G73" s="6"/>
+      <c r="H73" s="6"/>
+      <c r="I73" s="6"/>
+      <c r="J73" s="6"/>
+      <c r="K73" s="6"/>
+      <c r="L73" s="6"/>
+      <c r="M73" s="6"/>
+    </row>
+    <row r="74" spans="2:13" ht="60" x14ac:dyDescent="0.25">
+      <c r="B74" s="20"/>
+      <c r="C74" s="20"/>
+      <c r="D74" s="20"/>
+      <c r="E74" s="20"/>
+      <c r="F74" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="G74" s="58" t="s">
+        <v>39</v>
+      </c>
+      <c r="H74" s="58"/>
+      <c r="I74" s="20"/>
+    </row>
+    <row r="75" spans="2:13" ht="142.5" x14ac:dyDescent="0.25">
+      <c r="B75" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="C75" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="D75" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="E75" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="F75" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="G75" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="H75" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="I75" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="J75" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="K75" s="14" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="76" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B76" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="C76" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="D76" s="11">
+        <v>0</v>
+      </c>
+      <c r="E76" s="10">
+        <v>0</v>
+      </c>
+      <c r="F76" s="10">
+        <v>15</v>
+      </c>
+      <c r="G76" s="10">
         <v>200</v>
       </c>
-      <c r="H65" s="46" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="66" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B66" s="40"/>
-      <c r="C66" s="40"/>
-      <c r="D66" s="40"/>
-      <c r="E66" s="40"/>
-      <c r="F66" s="40"/>
-      <c r="G66" s="40"/>
-      <c r="H66" s="40"/>
-    </row>
-    <row r="67" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="68" spans="2:13" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B68" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="C68" s="6"/>
-      <c r="D68" s="6"/>
-      <c r="E68" s="6"/>
-      <c r="F68" s="6"/>
-      <c r="G68" s="6"/>
-      <c r="H68" s="6"/>
-      <c r="I68" s="6"/>
-      <c r="J68" s="6"/>
-      <c r="K68" s="6"/>
-      <c r="L68" s="6"/>
-      <c r="M68" s="6"/>
-    </row>
-    <row r="69" spans="2:13" ht="60" x14ac:dyDescent="0.25">
-      <c r="B69" s="20"/>
-      <c r="C69" s="20"/>
-      <c r="D69" s="20"/>
-      <c r="E69" s="20"/>
-      <c r="F69" s="21" t="s">
-        <v>40</v>
-      </c>
-      <c r="G69" s="63" t="s">
-        <v>39</v>
-      </c>
-      <c r="H69" s="63"/>
-      <c r="I69" s="20"/>
-    </row>
-    <row r="70" spans="2:13" ht="142.5" x14ac:dyDescent="0.25">
-      <c r="B70" s="19" t="s">
-        <v>38</v>
-      </c>
-      <c r="C70" s="19" t="s">
+      <c r="H76" s="9">
+        <v>0.5</v>
+      </c>
+      <c r="I76" s="9">
+        <v>1</v>
+      </c>
+      <c r="J76" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="K76" s="13" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="77" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B77" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="C77" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D77" s="11">
+        <v>1</v>
+      </c>
+      <c r="E77" s="10">
+        <v>0</v>
+      </c>
+      <c r="F77" s="10">
+        <v>60</v>
+      </c>
+      <c r="G77" s="10">
+        <v>300</v>
+      </c>
+      <c r="H77" s="9">
+        <v>0.5</v>
+      </c>
+      <c r="I77" s="9">
+        <v>1</v>
+      </c>
+      <c r="J77" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="K77" s="13" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="78" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B78" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="C78" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="D78" s="11">
+        <v>2</v>
+      </c>
+      <c r="E78" s="10">
+        <v>0</v>
+      </c>
+      <c r="F78" s="10">
+        <v>240</v>
+      </c>
+      <c r="G78" s="10">
+        <v>600</v>
+      </c>
+      <c r="H78" s="9">
+        <v>0.5</v>
+      </c>
+      <c r="I78" s="9">
+        <v>1</v>
+      </c>
+      <c r="J78" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="K78" s="7" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="80" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="81" spans="2:7" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B81" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C81" s="6"/>
+      <c r="D81" s="6"/>
+      <c r="E81" s="6"/>
+      <c r="F81" s="6"/>
+      <c r="G81" s="6"/>
+    </row>
+    <row r="83" spans="2:7" ht="135.75" x14ac:dyDescent="0.25">
+      <c r="B83" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C83" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D70" s="18" t="s">
-        <v>37</v>
-      </c>
-      <c r="E70" s="17" t="s">
-        <v>36</v>
-      </c>
-      <c r="F70" s="17" t="s">
-        <v>35</v>
-      </c>
-      <c r="G70" s="17" t="s">
-        <v>34</v>
-      </c>
-      <c r="H70" s="16" t="s">
-        <v>33</v>
-      </c>
-      <c r="I70" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="J70" s="15" t="s">
-        <v>31</v>
-      </c>
-      <c r="K70" s="14" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="71" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B71" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="C71" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="D71" s="11">
-        <v>0</v>
-      </c>
-      <c r="E71" s="10">
-        <v>0</v>
-      </c>
-      <c r="F71" s="10">
-        <v>15</v>
-      </c>
-      <c r="G71" s="10">
-        <v>200</v>
-      </c>
-      <c r="H71" s="9">
-        <v>0.5</v>
-      </c>
-      <c r="I71" s="9">
-        <v>1</v>
-      </c>
-      <c r="J71" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="K71" s="13" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="72" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B72" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="C72" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="D72" s="11">
-        <v>1</v>
-      </c>
-      <c r="E72" s="10">
-        <v>0</v>
-      </c>
-      <c r="F72" s="10">
-        <v>60</v>
-      </c>
-      <c r="G72" s="10">
-        <v>300</v>
-      </c>
-      <c r="H72" s="9">
-        <v>0.5</v>
-      </c>
-      <c r="I72" s="9">
-        <v>1</v>
-      </c>
-      <c r="J72" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="K72" s="13" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="73" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B73" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="C73" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="D73" s="11">
+      <c r="D83" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E73" s="10">
-        <v>0</v>
-      </c>
-      <c r="F73" s="10">
-        <v>240</v>
-      </c>
-      <c r="G73" s="10">
-        <v>600</v>
-      </c>
-      <c r="H73" s="9">
-        <v>0.5</v>
-      </c>
-      <c r="I73" s="9">
-        <v>1</v>
-      </c>
-      <c r="J73" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="K73" s="7" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="75" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="76" spans="2:13" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B76" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="C76" s="6"/>
-      <c r="D76" s="6"/>
-      <c r="E76" s="6"/>
-      <c r="F76" s="6"/>
-      <c r="G76" s="6"/>
-    </row>
-    <row r="78" spans="2:13" ht="135.75" x14ac:dyDescent="0.25">
-      <c r="B78" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="C78" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D78" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E78" s="3" t="s">
+      <c r="E83" s="3" t="s">
         <v>21</v>
-      </c>
-    </row>
-    <row r="79" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B79" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C79" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D79" s="1">
-        <v>0.1</v>
-      </c>
-      <c r="E79" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="80" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B80" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C80" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D80" s="1">
-        <v>0.7</v>
-      </c>
-      <c r="E80" s="1">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="81" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B81" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C81" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D81" s="1">
-        <v>1</v>
-      </c>
-      <c r="E81" s="1">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="82" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B82" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C82" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D82" s="1">
-        <v>1.5</v>
-      </c>
-      <c r="E82" s="1">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="83" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B83" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C83" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D83" s="1">
-        <v>2</v>
-      </c>
-      <c r="E83" s="1">
-        <v>26</v>
       </c>
     </row>
     <row r="84" spans="2:7" x14ac:dyDescent="0.25">
@@ -5049,13 +5037,13 @@
         <v>1</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="D84" s="1">
-        <v>2.5</v>
+        <v>0.1</v>
       </c>
       <c r="E84" s="1">
-        <v>35</v>
+        <v>2</v>
       </c>
     </row>
     <row r="85" spans="2:7" x14ac:dyDescent="0.25">
@@ -5063,13 +5051,13 @@
         <v>1</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="D85" s="1">
-        <v>3</v>
+        <v>0.7</v>
       </c>
       <c r="E85" s="1">
-        <v>45</v>
+        <v>6</v>
       </c>
     </row>
     <row r="86" spans="2:7" x14ac:dyDescent="0.25">
@@ -5077,13 +5065,13 @@
         <v>1</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="D86" s="1">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E86" s="1">
-        <v>56</v>
+        <v>12</v>
       </c>
     </row>
     <row r="87" spans="2:7" x14ac:dyDescent="0.25">
@@ -5091,13 +5079,13 @@
         <v>1</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="D87" s="1">
-        <v>5</v>
+        <v>1.5</v>
       </c>
       <c r="E87" s="1">
-        <v>67</v>
+        <v>18</v>
       </c>
     </row>
     <row r="88" spans="2:7" x14ac:dyDescent="0.25">
@@ -5105,35 +5093,69 @@
         <v>1</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="D88" s="1">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="E88" s="1">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="89" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="90" spans="2:7" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B90" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C90" s="6"/>
-      <c r="D90" s="6"/>
-      <c r="E90" s="6"/>
-      <c r="F90" s="6"/>
-      <c r="G90" s="6"/>
-    </row>
-    <row r="92" spans="2:7" ht="142.5" x14ac:dyDescent="0.25">
-      <c r="B92" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C92" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="89" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B89" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C89" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D89" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="E89" s="1">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="90" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B90" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C90" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D90" s="1">
         <v>3</v>
       </c>
-      <c r="D92" s="3" t="s">
-        <v>2</v>
+      <c r="E90" s="1">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="91" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B91" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C91" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D91" s="1">
+        <v>4</v>
+      </c>
+      <c r="E91" s="1">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="92" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B92" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C92" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D92" s="1">
+        <v>5</v>
+      </c>
+      <c r="E92" s="1">
+        <v>67</v>
       </c>
     </row>
     <row r="93" spans="2:7" x14ac:dyDescent="0.25">
@@ -5141,54 +5163,57 @@
         <v>1</v>
       </c>
       <c r="C93" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D93" s="1">
+        <v>7</v>
+      </c>
+      <c r="E93" s="1">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="94" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="95" spans="2:7" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B95" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C95" s="6"/>
+      <c r="D95" s="6"/>
+      <c r="E95" s="6"/>
+      <c r="F95" s="6"/>
+      <c r="G95" s="6"/>
+    </row>
+    <row r="97" spans="2:7" ht="142.5" x14ac:dyDescent="0.25">
+      <c r="B97" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C97" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D97" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="98" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B98" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C98" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D93" s="1">
+      <c r="D98" s="1">
         <v>0.05</v>
       </c>
     </row>
-    <row r="94" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B94" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C94" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D94" s="1">
+    <row r="99" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B99" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C99" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D99" s="1">
         <v>0.1</v>
-      </c>
-    </row>
-    <row r="95" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B95" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C95" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D95" s="1">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="96" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="97" spans="2:7" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B97" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C97" s="6"/>
-      <c r="D97" s="6"/>
-      <c r="E97" s="6"/>
-      <c r="F97" s="6"/>
-      <c r="G97" s="6"/>
-    </row>
-    <row r="99" spans="2:7" ht="132" x14ac:dyDescent="0.25">
-      <c r="B99" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C99" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D99" s="3" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="100" spans="2:7" x14ac:dyDescent="0.25">
@@ -5196,9 +5221,42 @@
         <v>1</v>
       </c>
       <c r="C100" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D100" s="1">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="101" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="102" spans="2:7" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B102" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C102" s="6"/>
+      <c r="D102" s="6"/>
+      <c r="E102" s="6"/>
+      <c r="F102" s="6"/>
+      <c r="G102" s="6"/>
+    </row>
+    <row r="104" spans="2:7" ht="132" x14ac:dyDescent="0.25">
+      <c r="B104" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C104" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D104" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="105" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B105" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C105" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D100" s="1">
+      <c r="D105" s="1">
         <v>0.7</v>
       </c>
     </row>
@@ -5206,11 +5264,11 @@
   <mergeCells count="4">
     <mergeCell ref="J3:K3"/>
     <mergeCell ref="M3:P3"/>
-    <mergeCell ref="F52:H52"/>
-    <mergeCell ref="G69:H69"/>
+    <mergeCell ref="F53:H53"/>
+    <mergeCell ref="G74:H74"/>
   </mergeCells>
-  <conditionalFormatting sqref="C71:D73">
-    <cfRule type="duplicateValues" dxfId="66" priority="1"/>
+  <conditionalFormatting sqref="C76:D78">
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
[FIX] [CONTENT] changedname appearing in [type] (in previous commits I changed only the [sku] )
Former-commit-id: 4c36eb8915210e6ea7b7fe50719dd9ce7205d6c5
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Missions.xlsx
+++ b/Docs/Content/HungryDragonContent_Missions.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="407" uniqueCount="214">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="407" uniqueCount="213">
   <si>
     <t>single_run</t>
   </si>
@@ -673,9 +673,6 @@
   </si>
   <si>
     <t>eat_spec_anim_a</t>
-  </si>
-  <si>
-    <t>eat_chain</t>
   </si>
   <si>
     <t>eat_spec_anim_a_spiders</t>
@@ -1178,13 +1175,6 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1200,21 +1190,18 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="67">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -2276,6 +2263,16 @@
         </bottom>
       </border>
     </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -2290,94 +2287,94 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="missionDifficultyDefinitions" displayName="missionDifficultyDefinitions" ref="B75:K78" totalsRowShown="0" headerRowBorderDxfId="66" tableBorderDxfId="65">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="missionDifficultyDefinitions" displayName="missionDifficultyDefinitions" ref="B75:K78" totalsRowShown="0" headerRowBorderDxfId="65" tableBorderDxfId="64">
   <autoFilter ref="B75:K78"/>
   <tableColumns count="10">
     <tableColumn id="1" name="{missionDifficultyDefinitions}"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="64"/>
-    <tableColumn id="7" name="[index]" dataDxfId="63"/>
-    <tableColumn id="3" name="[dragonsToUnlock]" dataDxfId="62"/>
-    <tableColumn id="4" name="[cooldownMinutes]" dataDxfId="61"/>
-    <tableColumn id="9" name="[maxRewardCoins]" dataDxfId="60"/>
-    <tableColumn id="5" name="[removeMissionPCCoefA]" dataDxfId="59"/>
-    <tableColumn id="6" name="[removeMissionPCCoefB]" dataDxfId="58"/>
-    <tableColumn id="8" name="[tidName]" dataDxfId="57"/>
-    <tableColumn id="10" name="[color]" dataDxfId="56"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="63"/>
+    <tableColumn id="7" name="[index]" dataDxfId="62"/>
+    <tableColumn id="3" name="[dragonsToUnlock]" dataDxfId="61"/>
+    <tableColumn id="4" name="[cooldownMinutes]" dataDxfId="60"/>
+    <tableColumn id="9" name="[maxRewardCoins]" dataDxfId="59"/>
+    <tableColumn id="5" name="[removeMissionPCCoefA]" dataDxfId="58"/>
+    <tableColumn id="6" name="[removeMissionPCCoefB]" dataDxfId="57"/>
+    <tableColumn id="8" name="[tidName]" dataDxfId="56"/>
+    <tableColumn id="10" name="[color]" dataDxfId="55"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table13303132" displayName="Table13303132" ref="B83:E93" totalsRowShown="0" headerRowDxfId="55" dataDxfId="53" headerRowBorderDxfId="54" tableBorderDxfId="52" totalsRowBorderDxfId="51">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table13303132" displayName="Table13303132" ref="B83:E93" totalsRowShown="0" headerRowDxfId="54" dataDxfId="52" headerRowBorderDxfId="53" tableBorderDxfId="51" totalsRowBorderDxfId="50">
   <autoFilter ref="B83:E93"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="{missionDragonModifiersDefinitions}" dataDxfId="50"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="49"/>
-    <tableColumn id="7" name="[quantityModifier]" dataDxfId="48"/>
-    <tableColumn id="3" name="[missionSCRewardMultiplier]" dataDxfId="47"/>
+    <tableColumn id="1" name="{missionDragonModifiersDefinitions}" dataDxfId="49"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="48"/>
+    <tableColumn id="7" name="[quantityModifier]" dataDxfId="47"/>
+    <tableColumn id="3" name="[missionSCRewardMultiplier]" dataDxfId="46"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table1330313234" displayName="Table1330313234" ref="B97:D100" totalsRowShown="0" headerRowDxfId="46" dataDxfId="44" headerRowBorderDxfId="45" tableBorderDxfId="43" totalsRowBorderDxfId="42">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table1330313234" displayName="Table1330313234" ref="B97:D100" totalsRowShown="0" headerRowDxfId="45" dataDxfId="43" headerRowBorderDxfId="44" tableBorderDxfId="42" totalsRowBorderDxfId="41">
   <autoFilter ref="B97:D100"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="{missionDifficultyModifiersDefinitions}" dataDxfId="41"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="40"/>
-    <tableColumn id="7" name="[quantityModifier]" dataDxfId="39"/>
+    <tableColumn id="1" name="{missionDifficultyModifiersDefinitions}" dataDxfId="40"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="39"/>
+    <tableColumn id="7" name="[quantityModifier]" dataDxfId="38"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table133031323435" displayName="Table133031323435" ref="B104:D105" totalsRowShown="0" headerRowDxfId="38" dataDxfId="36" headerRowBorderDxfId="37" tableBorderDxfId="35" totalsRowBorderDxfId="34">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table133031323435" displayName="Table133031323435" ref="B104:D105" totalsRowShown="0" headerRowDxfId="37" dataDxfId="35" headerRowBorderDxfId="36" tableBorderDxfId="34" totalsRowBorderDxfId="33">
   <autoFilter ref="B104:D105"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="{missionOtherModifiersDefinitions}" dataDxfId="33"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="32"/>
-    <tableColumn id="7" name="[quantityModifier]" dataDxfId="31"/>
+    <tableColumn id="1" name="{missionOtherModifiersDefinitions}" dataDxfId="32"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="31"/>
+    <tableColumn id="7" name="[quantityModifier]" dataDxfId="30"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table13" displayName="Table13" ref="B54:H71" totalsRowShown="0" headerRowDxfId="30" dataDxfId="28" headerRowBorderDxfId="29" tableBorderDxfId="27" totalsRowBorderDxfId="26">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table13" displayName="Table13" ref="B54:H71" totalsRowShown="0" headerRowDxfId="29" dataDxfId="27" headerRowBorderDxfId="28" tableBorderDxfId="26" totalsRowBorderDxfId="25">
   <autoFilter ref="B54:H71"/>
   <tableColumns count="7">
-    <tableColumn id="1" name="{missionTypeDefinitions}" dataDxfId="25"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="24"/>
-    <tableColumn id="3" name="[minTier]" dataDxfId="23"/>
-    <tableColumn id="6" name="[maxTier]" dataDxfId="22"/>
-    <tableColumn id="4" name="[weight]" dataDxfId="21"/>
-    <tableColumn id="9" name="[tidDescSingleRun]" dataDxfId="20"/>
-    <tableColumn id="10" name="[tidDescMultiRun]" dataDxfId="19"/>
+    <tableColumn id="1" name="{missionTypeDefinitions}" dataDxfId="24"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="23"/>
+    <tableColumn id="3" name="[minTier]" dataDxfId="22"/>
+    <tableColumn id="6" name="[maxTier]" dataDxfId="21"/>
+    <tableColumn id="4" name="[weight]" dataDxfId="20"/>
+    <tableColumn id="9" name="[tidDescSingleRun]" dataDxfId="19"/>
+    <tableColumn id="10" name="[tidDescMultiRun]" dataDxfId="18"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table1330" displayName="Table1330" ref="B4:N49" totalsRowShown="0" headerRowDxfId="18" dataDxfId="16" headerRowBorderDxfId="17" tableBorderDxfId="15" totalsRowBorderDxfId="14">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table1330" displayName="Table1330" ref="B4:N49" totalsRowShown="0" headerRowDxfId="17" dataDxfId="15" headerRowBorderDxfId="16" tableBorderDxfId="14" totalsRowBorderDxfId="13">
   <autoFilter ref="B4:N49"/>
   <tableColumns count="13">
-    <tableColumn id="1" name="{missionsDefinitions}" dataDxfId="13"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="12"/>
-    <tableColumn id="7" name="[type]" dataDxfId="11"/>
-    <tableColumn id="8" name="[weight]" dataDxfId="10"/>
-    <tableColumn id="13" name="[singleRunChance]" dataDxfId="9"/>
-    <tableColumn id="11" name="[minTier]" dataDxfId="8"/>
-    <tableColumn id="12" name="[maxTier]" dataDxfId="7"/>
-    <tableColumn id="6" name="[params]" dataDxfId="6"/>
-    <tableColumn id="3" name="[objectiveBaseQuantityMin]" dataDxfId="5"/>
-    <tableColumn id="9" name="[objectiveBaseQuantityMax]" dataDxfId="4"/>
-    <tableColumn id="4" name="[icon]" dataDxfId="3"/>
-    <tableColumn id="5" name="[tidObjective]" dataDxfId="2"/>
-    <tableColumn id="10" name="[trackingSku]" dataDxfId="1"/>
+    <tableColumn id="1" name="{missionsDefinitions}" dataDxfId="12"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="11"/>
+    <tableColumn id="7" name="[type]" dataDxfId="10"/>
+    <tableColumn id="8" name="[weight]" dataDxfId="9"/>
+    <tableColumn id="13" name="[singleRunChance]" dataDxfId="8"/>
+    <tableColumn id="11" name="[minTier]" dataDxfId="7"/>
+    <tableColumn id="12" name="[maxTier]" dataDxfId="6"/>
+    <tableColumn id="6" name="[params]" dataDxfId="5"/>
+    <tableColumn id="3" name="[objectiveBaseQuantityMin]" dataDxfId="4"/>
+    <tableColumn id="9" name="[objectiveBaseQuantityMax]" dataDxfId="3"/>
+    <tableColumn id="4" name="[icon]" dataDxfId="2"/>
+    <tableColumn id="5" name="[tidObjective]" dataDxfId="1"/>
+    <tableColumn id="10" name="[trackingSku]" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2652,13 +2649,15 @@
   <dimension ref="B1:P105"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C44" sqref="C32:C44"/>
+      <selection activeCell="D40" sqref="D40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="7" customWidth="1"/>
-    <col min="2" max="6" width="18.7109375" customWidth="1"/>
+    <col min="2" max="2" width="18.7109375" customWidth="1"/>
+    <col min="3" max="3" width="21" customWidth="1"/>
+    <col min="4" max="6" width="18.7109375" customWidth="1"/>
     <col min="7" max="7" width="25.28515625" customWidth="1"/>
     <col min="8" max="8" width="18.7109375" customWidth="1"/>
     <col min="9" max="9" width="36" customWidth="1"/>
@@ -2696,14 +2695,14 @@
         <v>145</v>
       </c>
       <c r="G3" s="38"/>
-      <c r="J3" s="56" t="s">
+      <c r="J3" s="61" t="s">
         <v>144</v>
       </c>
-      <c r="K3" s="56"/>
-      <c r="M3" s="56"/>
-      <c r="N3" s="56"/>
-      <c r="O3" s="56"/>
-      <c r="P3" s="56"/>
+      <c r="K3" s="61"/>
+      <c r="M3" s="61"/>
+      <c r="N3" s="61"/>
+      <c r="O3" s="61"/>
+      <c r="P3" s="61"/>
     </row>
     <row r="4" spans="2:16" ht="106.5" x14ac:dyDescent="0.25">
       <c r="B4" s="30" t="s">
@@ -3830,10 +3829,10 @@
         <v>1</v>
       </c>
       <c r="C32" s="53" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D32" s="54" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="E32" s="54">
         <v>1</v>
@@ -3871,10 +3870,10 @@
         <v>1</v>
       </c>
       <c r="C33" s="53" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D33" s="54" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="E33" s="54">
         <v>1</v>
@@ -3912,7 +3911,7 @@
         <v>1</v>
       </c>
       <c r="C34" s="53" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="D34" s="54" t="s">
         <v>207</v>
@@ -4398,12 +4397,12 @@
       <c r="I46" s="41"/>
       <c r="J46" s="41"/>
       <c r="K46" s="41"/>
-      <c r="L46" s="60"/>
-      <c r="M46" s="60"/>
+      <c r="L46" s="57"/>
+      <c r="M46" s="57"/>
       <c r="N46" s="44"/>
     </row>
     <row r="47" spans="2:14" s="43" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B47" s="59"/>
+      <c r="B47" s="56"/>
       <c r="C47" s="40"/>
       <c r="D47" s="41"/>
       <c r="E47" s="41"/>
@@ -4413,23 +4412,23 @@
       <c r="I47" s="41"/>
       <c r="J47" s="40"/>
       <c r="K47" s="41"/>
-      <c r="L47" s="60"/>
-      <c r="M47" s="60"/>
+      <c r="L47" s="57"/>
+      <c r="M47" s="57"/>
       <c r="N47" s="44"/>
     </row>
     <row r="48" spans="2:14" s="43" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B48" s="59"/>
+      <c r="B48" s="56"/>
       <c r="C48" s="40"/>
       <c r="D48" s="41"/>
       <c r="E48" s="41"/>
-      <c r="F48" s="60"/>
+      <c r="F48" s="57"/>
       <c r="G48" s="40"/>
-      <c r="H48" s="60"/>
+      <c r="H48" s="57"/>
       <c r="I48" s="41"/>
       <c r="J48" s="40"/>
       <c r="K48" s="41"/>
-      <c r="L48" s="60"/>
-      <c r="M48" s="60"/>
+      <c r="L48" s="57"/>
+      <c r="M48" s="57"/>
       <c r="N48" s="44"/>
     </row>
     <row r="49" spans="2:14" s="43" customFormat="1" x14ac:dyDescent="0.25">
@@ -4437,14 +4436,14 @@
       <c r="C49" s="41"/>
       <c r="D49" s="41"/>
       <c r="E49" s="41"/>
-      <c r="F49" s="60"/>
+      <c r="F49" s="57"/>
       <c r="G49" s="41"/>
-      <c r="H49" s="60"/>
+      <c r="H49" s="57"/>
       <c r="I49" s="41"/>
       <c r="J49" s="41"/>
       <c r="K49" s="41"/>
-      <c r="L49" s="60"/>
-      <c r="M49" s="60"/>
+      <c r="L49" s="57"/>
+      <c r="M49" s="57"/>
       <c r="N49" s="44"/>
     </row>
     <row r="50" spans="2:14" s="43" customFormat="1" x14ac:dyDescent="0.25">
@@ -4496,9 +4495,9 @@
       <c r="C53" s="20"/>
       <c r="D53" s="20"/>
       <c r="E53" s="20"/>
-      <c r="F53" s="57"/>
-      <c r="G53" s="57"/>
-      <c r="H53" s="57"/>
+      <c r="F53" s="62"/>
+      <c r="G53" s="62"/>
+      <c r="H53" s="62"/>
       <c r="I53" s="20"/>
       <c r="J53" s="20"/>
     </row>
@@ -4714,7 +4713,7 @@
         <v>1</v>
       </c>
       <c r="C63" s="41" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D63" s="41">
         <v>0</v>
@@ -4802,42 +4801,42 @@
       </c>
     </row>
     <row r="67" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B67" s="59"/>
+      <c r="B67" s="56"/>
       <c r="C67" s="40" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D67" s="40"/>
       <c r="E67" s="40"/>
       <c r="F67" s="40"/>
-      <c r="G67" s="61"/>
-      <c r="H67" s="61"/>
+      <c r="G67" s="58"/>
+      <c r="H67" s="58"/>
     </row>
     <row r="68" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B68" s="59"/>
+      <c r="B68" s="56"/>
       <c r="C68" s="40"/>
       <c r="D68" s="40"/>
       <c r="E68" s="40"/>
       <c r="F68" s="40"/>
-      <c r="G68" s="62"/>
-      <c r="H68" s="62"/>
+      <c r="G68" s="59"/>
+      <c r="H68" s="59"/>
     </row>
     <row r="69" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B69" s="59"/>
+      <c r="B69" s="56"/>
       <c r="C69" s="40"/>
       <c r="D69" s="40"/>
       <c r="E69" s="40"/>
       <c r="F69" s="40"/>
-      <c r="G69" s="62"/>
-      <c r="H69" s="62"/>
+      <c r="G69" s="59"/>
+      <c r="H69" s="59"/>
     </row>
     <row r="70" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B70" s="59"/>
+      <c r="B70" s="56"/>
       <c r="C70" s="40"/>
       <c r="D70" s="40"/>
       <c r="E70" s="40"/>
       <c r="F70" s="40"/>
-      <c r="G70" s="62"/>
-      <c r="H70" s="62"/>
+      <c r="G70" s="59"/>
+      <c r="H70" s="59"/>
     </row>
     <row r="71" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B71" s="46"/>
@@ -4845,8 +4844,8 @@
       <c r="D71" s="41"/>
       <c r="E71" s="41"/>
       <c r="F71" s="41"/>
-      <c r="G71" s="63"/>
-      <c r="H71" s="63"/>
+      <c r="G71" s="60"/>
+      <c r="H71" s="60"/>
     </row>
     <row r="72" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="73" spans="2:13" ht="23.25" x14ac:dyDescent="0.35">
@@ -4873,10 +4872,10 @@
       <c r="F74" s="21" t="s">
         <v>40</v>
       </c>
-      <c r="G74" s="58" t="s">
+      <c r="G74" s="63" t="s">
         <v>39</v>
       </c>
-      <c r="H74" s="58"/>
+      <c r="H74" s="63"/>
       <c r="I74" s="20"/>
     </row>
     <row r="75" spans="2:13" ht="142.5" x14ac:dyDescent="0.25">
@@ -5268,7 +5267,7 @@
     <mergeCell ref="G74:H74"/>
   </mergeCells>
   <conditionalFormatting sqref="C76:D78">
-    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="66" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
[CONTENT] Added last new missions (critical_time, destroy and eat_dizzy)
Former-commit-id: 98ce852f56c5dd5323842881efc51c5911e9b38e
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Missions.xlsx
+++ b/Docs/Content/HungryDragonContent_Missions.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="407" uniqueCount="213">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="430" uniqueCount="221">
   <si>
     <t>single_run</t>
   </si>
@@ -516,9 +516,6 @@
     <t>eat_suicidal_goblins</t>
   </si>
   <si>
-    <t>eat_gold_generic</t>
-  </si>
-  <si>
     <t>eat_gold_razorback</t>
   </si>
   <si>
@@ -688,6 +685,33 @@
   </si>
   <si>
     <t>kill_chain_canary_01</t>
+  </si>
+  <si>
+    <t>eat_dizzy</t>
+  </si>
+  <si>
+    <t>destroy</t>
+  </si>
+  <si>
+    <t>destroy_mineSmall</t>
+  </si>
+  <si>
+    <t>eat_dizzy_gen</t>
+  </si>
+  <si>
+    <t>eat_gold_gen</t>
+  </si>
+  <si>
+    <t>TID_MISSION_OBJECTIVE_CRITICALTIME_DESC_SINGLE_RUN</t>
+  </si>
+  <si>
+    <t>TID_MISSION_OBJECTIVE_EATDIZZY_DESC_SINGLE_RUN</t>
+  </si>
+  <si>
+    <t>TID_MISSION_OBJECTIVE_CRITICALTIME_DESC_MULTI_RUN</t>
+  </si>
+  <si>
+    <t>TID_MISSION_OBJECTIVE_EATDIZZY_DESC_MULTI_RUN</t>
   </si>
 </sst>
 </file>
@@ -1032,7 +1056,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="64">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1"/>
@@ -1178,12 +1202,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2287,8 +2305,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="missionDifficultyDefinitions" displayName="missionDifficultyDefinitions" ref="B75:K78" totalsRowShown="0" headerRowBorderDxfId="65" tableBorderDxfId="64">
-  <autoFilter ref="B75:K78"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="missionDifficultyDefinitions" displayName="missionDifficultyDefinitions" ref="B74:K77" totalsRowShown="0" headerRowBorderDxfId="65" tableBorderDxfId="64">
+  <autoFilter ref="B74:K77"/>
   <tableColumns count="10">
     <tableColumn id="1" name="{missionDifficultyDefinitions}"/>
     <tableColumn id="2" name="[sku]" dataDxfId="63"/>
@@ -2306,8 +2324,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table13303132" displayName="Table13303132" ref="B83:E93" totalsRowShown="0" headerRowDxfId="54" dataDxfId="52" headerRowBorderDxfId="53" tableBorderDxfId="51" totalsRowBorderDxfId="50">
-  <autoFilter ref="B83:E93"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table13303132" displayName="Table13303132" ref="B82:E92" totalsRowShown="0" headerRowDxfId="54" dataDxfId="52" headerRowBorderDxfId="53" tableBorderDxfId="51" totalsRowBorderDxfId="50">
+  <autoFilter ref="B82:E92"/>
   <tableColumns count="4">
     <tableColumn id="1" name="{missionDragonModifiersDefinitions}" dataDxfId="49"/>
     <tableColumn id="2" name="[sku]" dataDxfId="48"/>
@@ -2319,8 +2337,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table1330313234" displayName="Table1330313234" ref="B97:D100" totalsRowShown="0" headerRowDxfId="45" dataDxfId="43" headerRowBorderDxfId="44" tableBorderDxfId="42" totalsRowBorderDxfId="41">
-  <autoFilter ref="B97:D100"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table1330313234" displayName="Table1330313234" ref="B96:D99" totalsRowShown="0" headerRowDxfId="45" dataDxfId="43" headerRowBorderDxfId="44" tableBorderDxfId="42" totalsRowBorderDxfId="41">
+  <autoFilter ref="B96:D99"/>
   <tableColumns count="3">
     <tableColumn id="1" name="{missionDifficultyModifiersDefinitions}" dataDxfId="40"/>
     <tableColumn id="2" name="[sku]" dataDxfId="39"/>
@@ -2331,8 +2349,8 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table133031323435" displayName="Table133031323435" ref="B104:D105" totalsRowShown="0" headerRowDxfId="37" dataDxfId="35" headerRowBorderDxfId="36" tableBorderDxfId="34" totalsRowBorderDxfId="33">
-  <autoFilter ref="B104:D105"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table133031323435" displayName="Table133031323435" ref="B103:D104" totalsRowShown="0" headerRowDxfId="37" dataDxfId="35" headerRowBorderDxfId="36" tableBorderDxfId="34" totalsRowBorderDxfId="33">
+  <autoFilter ref="B103:D104"/>
   <tableColumns count="3">
     <tableColumn id="1" name="{missionOtherModifiersDefinitions}" dataDxfId="32"/>
     <tableColumn id="2" name="[sku]" dataDxfId="31"/>
@@ -2343,8 +2361,8 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table13" displayName="Table13" ref="B54:H71" totalsRowShown="0" headerRowDxfId="29" dataDxfId="27" headerRowBorderDxfId="28" tableBorderDxfId="26" totalsRowBorderDxfId="25">
-  <autoFilter ref="B54:H71"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table13" displayName="Table13" ref="B53:H70" totalsRowShown="0" headerRowDxfId="29" dataDxfId="27" headerRowBorderDxfId="28" tableBorderDxfId="26" totalsRowBorderDxfId="25">
+  <autoFilter ref="B53:H70"/>
   <tableColumns count="7">
     <tableColumn id="1" name="{missionTypeDefinitions}" dataDxfId="24"/>
     <tableColumn id="2" name="[sku]" dataDxfId="23"/>
@@ -2359,8 +2377,8 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table1330" displayName="Table1330" ref="B4:N49" totalsRowShown="0" headerRowDxfId="17" dataDxfId="15" headerRowBorderDxfId="16" tableBorderDxfId="14" totalsRowBorderDxfId="13">
-  <autoFilter ref="B4:N49"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table1330" displayName="Table1330" ref="B4:N48" totalsRowShown="0" headerRowDxfId="17" dataDxfId="15" headerRowBorderDxfId="16" tableBorderDxfId="14" totalsRowBorderDxfId="13">
+  <autoFilter ref="B4:N48"/>
   <tableColumns count="13">
     <tableColumn id="1" name="{missionsDefinitions}" dataDxfId="12"/>
     <tableColumn id="2" name="[sku]" dataDxfId="11"/>
@@ -2646,10 +2664,10 @@
   <sheetPr>
     <tabColor theme="6"/>
   </sheetPr>
-  <dimension ref="B1:P105"/>
+  <dimension ref="B1:P104"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D40" sqref="D40"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H66" sqref="H66:H68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2658,8 +2676,8 @@
     <col min="2" max="2" width="18.7109375" customWidth="1"/>
     <col min="3" max="3" width="21" customWidth="1"/>
     <col min="4" max="6" width="18.7109375" customWidth="1"/>
-    <col min="7" max="7" width="25.28515625" customWidth="1"/>
-    <col min="8" max="8" width="18.7109375" customWidth="1"/>
+    <col min="7" max="7" width="42" customWidth="1"/>
+    <col min="8" max="8" width="35.5703125" customWidth="1"/>
     <col min="9" max="9" width="36" customWidth="1"/>
     <col min="10" max="11" width="18.7109375" customWidth="1"/>
     <col min="12" max="12" width="17.140625" customWidth="1"/>
@@ -2695,14 +2713,14 @@
         <v>145</v>
       </c>
       <c r="G3" s="38"/>
-      <c r="J3" s="61" t="s">
+      <c r="J3" s="59" t="s">
         <v>144</v>
       </c>
-      <c r="K3" s="61"/>
-      <c r="M3" s="61"/>
-      <c r="N3" s="61"/>
-      <c r="O3" s="61"/>
-      <c r="P3" s="61"/>
+      <c r="K3" s="59"/>
+      <c r="M3" s="59"/>
+      <c r="N3" s="59"/>
+      <c r="O3" s="59"/>
+      <c r="P3" s="59"/>
     </row>
     <row r="4" spans="2:16" ht="106.5" x14ac:dyDescent="0.25">
       <c r="B4" s="30" t="s">
@@ -2780,7 +2798,7 @@
         <v>130</v>
       </c>
       <c r="M5" s="33" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="N5" s="31" t="s">
         <v>73</v>
@@ -2895,7 +2913,7 @@
         <v>130</v>
       </c>
       <c r="M8" s="33" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="N8" s="31" t="s">
         <v>73</v>
@@ -2924,7 +2942,7 @@
         <v>7</v>
       </c>
       <c r="I9" s="24" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="J9" s="24">
         <v>25</v>
@@ -2936,7 +2954,7 @@
         <v>128</v>
       </c>
       <c r="M9" s="47" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="N9" s="31" t="s">
         <v>73</v>
@@ -2977,7 +2995,7 @@
         <v>126</v>
       </c>
       <c r="M10" s="47" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="N10" s="31" t="s">
         <v>73</v>
@@ -3018,7 +3036,7 @@
         <v>123</v>
       </c>
       <c r="M11" s="47" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="N11" s="31" t="s">
         <v>73</v>
@@ -3059,7 +3077,7 @@
         <v>121</v>
       </c>
       <c r="M12" s="33" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="N12" s="31" t="s">
         <v>73</v>
@@ -3100,7 +3118,7 @@
         <v>119</v>
       </c>
       <c r="M13" s="33" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="N13" s="31" t="s">
         <v>73</v>
@@ -3141,7 +3159,7 @@
         <v>116</v>
       </c>
       <c r="M14" s="47" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="N14" s="31" t="s">
         <v>73</v>
@@ -3330,7 +3348,7 @@
         <v>108</v>
       </c>
       <c r="M19" s="47" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="N19" s="31" t="s">
         <v>73</v>
@@ -3371,7 +3389,7 @@
         <v>105</v>
       </c>
       <c r="M20" s="33" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="N20" s="31" t="s">
         <v>73</v>
@@ -3412,7 +3430,7 @@
         <v>102</v>
       </c>
       <c r="M21" s="50" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="N21" s="31" t="s">
         <v>73</v>
@@ -3453,7 +3471,7 @@
         <v>99</v>
       </c>
       <c r="M22" s="34" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="N22" s="31" t="s">
         <v>73</v>
@@ -3494,7 +3512,7 @@
         <v>96</v>
       </c>
       <c r="M23" s="50" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="N23" s="31" t="s">
         <v>73</v>
@@ -3535,7 +3553,7 @@
         <v>93</v>
       </c>
       <c r="M24" s="51" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="N24" s="31" t="s">
         <v>73</v>
@@ -3576,7 +3594,7 @@
         <v>90</v>
       </c>
       <c r="M25" s="34" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="N25" s="31" t="s">
         <v>73</v>
@@ -3617,7 +3635,7 @@
         <v>87</v>
       </c>
       <c r="M26" s="34" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="N26" s="31" t="s">
         <v>73</v>
@@ -3658,7 +3676,7 @@
         <v>84</v>
       </c>
       <c r="M27" s="34" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="N27" s="31" t="s">
         <v>73</v>
@@ -3699,7 +3717,7 @@
         <v>81</v>
       </c>
       <c r="M28" s="34" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="N28" s="31" t="s">
         <v>73</v>
@@ -3740,7 +3758,7 @@
         <v>78</v>
       </c>
       <c r="M29" s="34" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="N29" s="31" t="s">
         <v>73</v>
@@ -3781,7 +3799,7 @@
         <v>75</v>
       </c>
       <c r="M30" s="34" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="N30" s="31" t="s">
         <v>73</v>
@@ -3829,10 +3847,10 @@
         <v>1</v>
       </c>
       <c r="C32" s="53" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D32" s="54" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="E32" s="54">
         <v>1</v>
@@ -3859,7 +3877,7 @@
         <v>130</v>
       </c>
       <c r="M32" s="48" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="N32" s="55" t="s">
         <v>73</v>
@@ -3870,10 +3888,10 @@
         <v>1</v>
       </c>
       <c r="C33" s="53" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D33" s="54" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="E33" s="54">
         <v>1</v>
@@ -3888,7 +3906,7 @@
         <v>7</v>
       </c>
       <c r="I33" s="54" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="J33" s="53">
         <v>99</v>
@@ -3900,7 +3918,7 @@
         <v>130</v>
       </c>
       <c r="M33" s="48" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="N33" s="55" t="s">
         <v>73</v>
@@ -3911,10 +3929,10 @@
         <v>1</v>
       </c>
       <c r="C34" s="53" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D34" s="54" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="E34" s="54">
         <v>1</v>
@@ -3941,7 +3959,7 @@
         <v>130</v>
       </c>
       <c r="M34" s="48" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="N34" s="55" t="s">
         <v>73</v>
@@ -3952,7 +3970,7 @@
         <v>1</v>
       </c>
       <c r="C35" s="53" t="s">
-        <v>155</v>
+        <v>216</v>
       </c>
       <c r="D35" s="54" t="s">
         <v>151</v>
@@ -3989,7 +4007,7 @@
         <v>1</v>
       </c>
       <c r="C36" s="53" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D36" s="54" t="s">
         <v>151</v>
@@ -4007,7 +4025,7 @@
         <v>7</v>
       </c>
       <c r="I36" s="54" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="J36" s="53">
         <v>99</v>
@@ -4019,7 +4037,7 @@
         <v>130</v>
       </c>
       <c r="M36" s="54" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="N36" s="55" t="s">
         <v>73</v>
@@ -4030,7 +4048,7 @@
         <v>1</v>
       </c>
       <c r="C37" s="53" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D37" s="54" t="s">
         <v>151</v>
@@ -4048,7 +4066,7 @@
         <v>7</v>
       </c>
       <c r="I37" s="54" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="J37" s="53">
         <v>99</v>
@@ -4060,7 +4078,7 @@
         <v>130</v>
       </c>
       <c r="M37" s="54" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="N37" s="55" t="s">
         <v>73</v>
@@ -4071,7 +4089,7 @@
         <v>1</v>
       </c>
       <c r="C38" s="53" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D38" s="54" t="s">
         <v>151</v>
@@ -4089,7 +4107,7 @@
         <v>7</v>
       </c>
       <c r="I38" s="54" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="J38" s="53">
         <v>99</v>
@@ -4101,7 +4119,7 @@
         <v>130</v>
       </c>
       <c r="M38" s="54" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="N38" s="55" t="s">
         <v>73</v>
@@ -4112,7 +4130,7 @@
         <v>1</v>
       </c>
       <c r="C39" s="53" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D39" s="54" t="s">
         <v>151</v>
@@ -4142,7 +4160,7 @@
         <v>130</v>
       </c>
       <c r="M39" s="54" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="N39" s="55" t="s">
         <v>73</v>
@@ -4153,7 +4171,7 @@
         <v>1</v>
       </c>
       <c r="C40" s="53" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D40" s="54" t="s">
         <v>151</v>
@@ -4171,7 +4189,7 @@
         <v>7</v>
       </c>
       <c r="I40" s="54" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="J40" s="53">
         <v>99</v>
@@ -4183,7 +4201,7 @@
         <v>130</v>
       </c>
       <c r="M40" s="49" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="N40" s="55" t="s">
         <v>73</v>
@@ -4194,7 +4212,7 @@
         <v>1</v>
       </c>
       <c r="C41" s="53" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D41" s="54" t="s">
         <v>151</v>
@@ -4212,7 +4230,7 @@
         <v>7</v>
       </c>
       <c r="I41" s="54" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="J41" s="53">
         <v>99</v>
@@ -4224,7 +4242,7 @@
         <v>130</v>
       </c>
       <c r="M41" s="49" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="N41" s="55" t="s">
         <v>73</v>
@@ -4265,7 +4283,7 @@
         <v>130</v>
       </c>
       <c r="M42" s="49" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="N42" s="55" t="s">
         <v>73</v>
@@ -4276,7 +4294,7 @@
         <v>1</v>
       </c>
       <c r="C43" s="53" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D43" s="54" t="s">
         <v>152</v>
@@ -4294,7 +4312,7 @@
         <v>7</v>
       </c>
       <c r="I43" s="54" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="J43" s="53">
         <v>99</v>
@@ -4306,7 +4324,7 @@
         <v>130</v>
       </c>
       <c r="M43" s="49" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="N43" s="55" t="s">
         <v>73</v>
@@ -4317,7 +4335,7 @@
         <v>1</v>
       </c>
       <c r="C44" s="53" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D44" s="54" t="s">
         <v>152</v>
@@ -4335,7 +4353,7 @@
         <v>7</v>
       </c>
       <c r="I44" s="54" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="J44" s="53">
         <v>99</v>
@@ -4347,7 +4365,7 @@
         <v>130</v>
       </c>
       <c r="M44" s="49" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="N44" s="55" t="s">
         <v>73</v>
@@ -4357,16 +4375,20 @@
       <c r="B45" s="52" t="s">
         <v>1</v>
       </c>
-      <c r="C45" s="53"/>
-      <c r="D45" s="54"/>
+      <c r="C45" s="40" t="s">
+        <v>208</v>
+      </c>
+      <c r="D45" s="40" t="s">
+        <v>208</v>
+      </c>
       <c r="E45" s="54">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F45" s="54">
-        <v>0.3</v>
+        <v>0</v>
       </c>
       <c r="G45" s="53">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H45" s="54">
         <v>7</v>
@@ -4387,141 +4409,193 @@
       </c>
     </row>
     <row r="46" spans="2:14" s="43" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B46" s="46"/>
-      <c r="C46" s="41"/>
-      <c r="D46" s="41"/>
-      <c r="E46" s="41"/>
-      <c r="F46" s="41"/>
-      <c r="G46" s="41"/>
-      <c r="H46" s="41"/>
+      <c r="B46" s="52" t="s">
+        <v>1</v>
+      </c>
+      <c r="C46" s="40" t="s">
+        <v>215</v>
+      </c>
+      <c r="D46" s="40" t="s">
+        <v>212</v>
+      </c>
+      <c r="E46" s="54">
+        <v>1</v>
+      </c>
+      <c r="F46" s="54">
+        <v>0.3</v>
+      </c>
+      <c r="G46" s="53">
+        <v>0</v>
+      </c>
+      <c r="H46" s="54">
+        <v>7</v>
+      </c>
       <c r="I46" s="41"/>
-      <c r="J46" s="41"/>
-      <c r="K46" s="41"/>
-      <c r="L46" s="57"/>
-      <c r="M46" s="57"/>
-      <c r="N46" s="44"/>
+      <c r="J46" s="53">
+        <v>99</v>
+      </c>
+      <c r="K46" s="54">
+        <v>99</v>
+      </c>
+      <c r="L46" s="48" t="s">
+        <v>130</v>
+      </c>
+      <c r="M46" s="41"/>
+      <c r="N46" s="55" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="47" spans="2:14" s="43" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B47" s="56"/>
-      <c r="C47" s="40"/>
-      <c r="D47" s="41"/>
-      <c r="E47" s="41"/>
-      <c r="F47" s="41"/>
-      <c r="G47" s="40"/>
-      <c r="H47" s="41"/>
+      <c r="B47" s="52" t="s">
+        <v>1</v>
+      </c>
+      <c r="C47" s="40" t="s">
+        <v>214</v>
+      </c>
+      <c r="D47" s="40" t="s">
+        <v>213</v>
+      </c>
+      <c r="E47" s="54">
+        <v>1</v>
+      </c>
+      <c r="F47" s="54">
+        <v>0.3</v>
+      </c>
+      <c r="G47" s="53">
+        <v>0</v>
+      </c>
+      <c r="H47" s="54">
+        <v>7</v>
+      </c>
       <c r="I47" s="41"/>
-      <c r="J47" s="40"/>
-      <c r="K47" s="41"/>
-      <c r="L47" s="57"/>
-      <c r="M47" s="57"/>
-      <c r="N47" s="44"/>
+      <c r="J47" s="53">
+        <v>99</v>
+      </c>
+      <c r="K47" s="54">
+        <v>99</v>
+      </c>
+      <c r="L47" s="48" t="s">
+        <v>130</v>
+      </c>
+      <c r="M47" s="41"/>
+      <c r="N47" s="55" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="48" spans="2:14" s="43" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B48" s="56"/>
+      <c r="B48" s="52"/>
       <c r="C48" s="40"/>
-      <c r="D48" s="41"/>
-      <c r="E48" s="41"/>
-      <c r="F48" s="57"/>
-      <c r="G48" s="40"/>
-      <c r="H48" s="57"/>
+      <c r="D48" s="40"/>
+      <c r="E48" s="54"/>
+      <c r="F48" s="54"/>
+      <c r="G48" s="53"/>
+      <c r="H48" s="54"/>
       <c r="I48" s="41"/>
-      <c r="J48" s="40"/>
-      <c r="K48" s="41"/>
-      <c r="L48" s="57"/>
-      <c r="M48" s="57"/>
-      <c r="N48" s="44"/>
+      <c r="J48" s="53"/>
+      <c r="K48" s="54"/>
+      <c r="L48" s="48"/>
+      <c r="M48" s="41"/>
+      <c r="N48" s="55"/>
     </row>
     <row r="49" spans="2:14" s="43" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B49" s="46"/>
-      <c r="C49" s="41"/>
-      <c r="D49" s="41"/>
-      <c r="E49" s="41"/>
-      <c r="F49" s="57"/>
-      <c r="G49" s="41"/>
-      <c r="H49" s="57"/>
-      <c r="I49" s="41"/>
-      <c r="J49" s="41"/>
-      <c r="K49" s="41"/>
-      <c r="L49" s="57"/>
-      <c r="M49" s="57"/>
+      <c r="B49" s="44"/>
+      <c r="C49" s="44"/>
+      <c r="D49" s="44"/>
+      <c r="E49" s="44"/>
+      <c r="F49" s="44"/>
+      <c r="G49" s="44"/>
+      <c r="H49" s="44"/>
+      <c r="I49" s="44"/>
+      <c r="J49" s="44"/>
+      <c r="K49" s="44"/>
+      <c r="L49" s="44"/>
+      <c r="M49" s="44"/>
       <c r="N49" s="44"/>
     </row>
-    <row r="50" spans="2:14" s="43" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B50" s="44"/>
-      <c r="C50" s="44"/>
-      <c r="D50" s="44"/>
-      <c r="E50" s="44"/>
-      <c r="F50" s="44"/>
-      <c r="G50" s="44"/>
-      <c r="H50" s="44"/>
-      <c r="I50" s="44"/>
-      <c r="J50" s="44"/>
-      <c r="K50" s="44"/>
-      <c r="L50" s="44"/>
-      <c r="M50" s="44"/>
-      <c r="N50" s="44"/>
-    </row>
-    <row r="51" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B51" s="32"/>
-      <c r="C51" s="32"/>
-      <c r="D51" s="32"/>
-      <c r="E51" s="32"/>
-      <c r="F51" s="32"/>
-      <c r="G51" s="32"/>
-      <c r="H51" s="32"/>
-      <c r="I51" s="32"/>
-      <c r="J51" s="32"/>
-      <c r="K51" s="32"/>
-      <c r="L51" s="32"/>
-      <c r="M51" s="31"/>
-    </row>
-    <row r="52" spans="2:14" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B52" s="6" t="s">
+    <row r="50" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B50" s="32"/>
+      <c r="C50" s="32"/>
+      <c r="D50" s="32"/>
+      <c r="E50" s="32"/>
+      <c r="F50" s="32"/>
+      <c r="G50" s="32"/>
+      <c r="H50" s="32"/>
+      <c r="I50" s="32"/>
+      <c r="J50" s="32"/>
+      <c r="K50" s="32"/>
+      <c r="L50" s="32"/>
+      <c r="M50" s="31"/>
+    </row>
+    <row r="51" spans="2:14" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B51" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="C52" s="6"/>
-      <c r="D52" s="6"/>
-      <c r="E52" s="6"/>
-      <c r="F52" s="6"/>
-      <c r="G52" s="6"/>
-      <c r="H52" s="6"/>
-      <c r="I52" s="6"/>
-      <c r="J52" s="6"/>
-      <c r="K52" s="6"/>
-      <c r="L52" s="6"/>
-    </row>
-    <row r="53" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B53" s="20"/>
-      <c r="C53" s="20"/>
-      <c r="D53" s="20"/>
-      <c r="E53" s="20"/>
-      <c r="F53" s="62"/>
-      <c r="G53" s="62"/>
-      <c r="H53" s="62"/>
-      <c r="I53" s="20"/>
-      <c r="J53" s="20"/>
-    </row>
-    <row r="54" spans="2:14" ht="96" x14ac:dyDescent="0.25">
-      <c r="B54" s="30" t="s">
+      <c r="C51" s="6"/>
+      <c r="D51" s="6"/>
+      <c r="E51" s="6"/>
+      <c r="F51" s="6"/>
+      <c r="G51" s="6"/>
+      <c r="H51" s="6"/>
+      <c r="I51" s="6"/>
+      <c r="J51" s="6"/>
+      <c r="K51" s="6"/>
+      <c r="L51" s="6"/>
+    </row>
+    <row r="52" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B52" s="20"/>
+      <c r="C52" s="20"/>
+      <c r="D52" s="20"/>
+      <c r="E52" s="20"/>
+      <c r="F52" s="60"/>
+      <c r="G52" s="60"/>
+      <c r="H52" s="60"/>
+      <c r="I52" s="20"/>
+      <c r="J52" s="20"/>
+    </row>
+    <row r="53" spans="2:14" ht="96" x14ac:dyDescent="0.25">
+      <c r="B53" s="30" t="s">
         <v>71</v>
       </c>
-      <c r="C54" s="28" t="s">
+      <c r="C53" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="D54" s="29" t="s">
+      <c r="D53" s="29" t="s">
         <v>70</v>
       </c>
-      <c r="E54" s="29" t="s">
+      <c r="E53" s="29" t="s">
         <v>69</v>
       </c>
-      <c r="F54" s="29" t="s">
+      <c r="F53" s="29" t="s">
         <v>68</v>
       </c>
-      <c r="G54" s="28" t="s">
+      <c r="G53" s="28" t="s">
         <v>67</v>
       </c>
-      <c r="H54" s="28" t="s">
+      <c r="H53" s="28" t="s">
         <v>66</v>
+      </c>
+    </row>
+    <row r="54" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B54" s="27" t="s">
+        <v>1</v>
+      </c>
+      <c r="C54" s="24" t="s">
+        <v>65</v>
+      </c>
+      <c r="D54" s="24">
+        <v>0</v>
+      </c>
+      <c r="E54" s="24">
+        <v>7</v>
+      </c>
+      <c r="F54" s="24">
+        <v>2</v>
+      </c>
+      <c r="G54" s="26" t="s">
+        <v>64</v>
+      </c>
+      <c r="H54" s="26" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="55" spans="2:14" x14ac:dyDescent="0.25">
@@ -4529,7 +4603,7 @@
         <v>1</v>
       </c>
       <c r="C55" s="24" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="D55" s="24">
         <v>0</v>
@@ -4538,13 +4612,13 @@
         <v>7</v>
       </c>
       <c r="F55" s="24">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G55" s="26" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="H55" s="26" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
     <row r="56" spans="2:14" x14ac:dyDescent="0.25">
@@ -4552,7 +4626,7 @@
         <v>1</v>
       </c>
       <c r="C56" s="24" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D56" s="24">
         <v>0</v>
@@ -4561,13 +4635,13 @@
         <v>7</v>
       </c>
       <c r="F56" s="24">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G56" s="26" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="H56" s="26" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="57" spans="2:14" x14ac:dyDescent="0.25">
@@ -4575,7 +4649,7 @@
         <v>1</v>
       </c>
       <c r="C57" s="24" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D57" s="24">
         <v>0</v>
@@ -4584,59 +4658,59 @@
         <v>7</v>
       </c>
       <c r="F57" s="24">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G57" s="26" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="H57" s="26" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="58" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B58" s="27" t="s">
-        <v>1</v>
-      </c>
-      <c r="C58" s="24" t="s">
-        <v>56</v>
-      </c>
-      <c r="D58" s="24">
+      <c r="B58" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="C58" s="23" t="s">
+        <v>53</v>
+      </c>
+      <c r="D58" s="23">
         <v>0</v>
       </c>
       <c r="E58" s="24">
         <v>7</v>
       </c>
-      <c r="F58" s="24">
+      <c r="F58" s="23">
         <v>1</v>
       </c>
       <c r="G58" s="26" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="H58" s="26" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="59" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B59" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="C59" s="23" t="s">
-        <v>53</v>
-      </c>
-      <c r="D59" s="23">
+      <c r="C59" s="24" t="s">
+        <v>50</v>
+      </c>
+      <c r="D59" s="24">
         <v>0</v>
       </c>
       <c r="E59" s="24">
         <v>7</v>
       </c>
-      <c r="F59" s="23">
+      <c r="F59" s="24">
         <v>1</v>
       </c>
       <c r="G59" s="26" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="H59" s="26" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="60" spans="2:14" x14ac:dyDescent="0.25">
@@ -4644,7 +4718,7 @@
         <v>1</v>
       </c>
       <c r="C60" s="24" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D60" s="24">
         <v>0</v>
@@ -4656,56 +4730,56 @@
         <v>1</v>
       </c>
       <c r="G60" s="26" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="H60" s="26" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="61" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B61" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="C61" s="24" t="s">
-        <v>47</v>
-      </c>
-      <c r="D61" s="24">
+      <c r="C61" s="23" t="s">
+        <v>44</v>
+      </c>
+      <c r="D61" s="23">
         <v>0</v>
       </c>
       <c r="E61" s="24">
         <v>7</v>
       </c>
-      <c r="F61" s="24">
-        <v>1</v>
-      </c>
-      <c r="G61" s="26" t="s">
-        <v>46</v>
-      </c>
-      <c r="H61" s="26" t="s">
-        <v>45</v>
+      <c r="F61" s="23">
+        <v>1</v>
+      </c>
+      <c r="G61" s="22" t="s">
+        <v>43</v>
+      </c>
+      <c r="H61" s="22" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="62" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B62" s="25" t="s">
-        <v>1</v>
-      </c>
-      <c r="C62" s="23" t="s">
-        <v>44</v>
-      </c>
-      <c r="D62" s="23">
-        <v>0</v>
-      </c>
-      <c r="E62" s="24">
-        <v>7</v>
-      </c>
-      <c r="F62" s="23">
-        <v>1</v>
-      </c>
-      <c r="G62" s="22" t="s">
-        <v>43</v>
-      </c>
-      <c r="H62" s="22" t="s">
-        <v>42</v>
+      <c r="B62" s="46" t="s">
+        <v>1</v>
+      </c>
+      <c r="C62" s="41" t="s">
+        <v>209</v>
+      </c>
+      <c r="D62" s="41">
+        <v>0</v>
+      </c>
+      <c r="E62" s="41">
+        <v>7</v>
+      </c>
+      <c r="F62" s="41">
+        <v>1</v>
+      </c>
+      <c r="G62" s="42" t="s">
+        <v>195</v>
+      </c>
+      <c r="H62" s="42" t="s">
+        <v>199</v>
       </c>
     </row>
     <row r="63" spans="2:14" x14ac:dyDescent="0.25">
@@ -4713,7 +4787,7 @@
         <v>1</v>
       </c>
       <c r="C63" s="41" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="D63" s="41">
         <v>0</v>
@@ -4722,12 +4796,12 @@
         <v>7</v>
       </c>
       <c r="F63" s="41">
-        <v>1</v>
-      </c>
-      <c r="G63" s="42" t="s">
-        <v>196</v>
-      </c>
-      <c r="H63" s="42" t="s">
+        <v>2</v>
+      </c>
+      <c r="G63" s="45" t="s">
+        <v>198</v>
+      </c>
+      <c r="H63" s="45" t="s">
         <v>200</v>
       </c>
     </row>
@@ -4736,7 +4810,7 @@
         <v>1</v>
       </c>
       <c r="C64" s="41" t="s">
-        <v>207</v>
+        <v>151</v>
       </c>
       <c r="D64" s="41">
         <v>0</v>
@@ -4748,7 +4822,7 @@
         <v>2</v>
       </c>
       <c r="G64" s="45" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="H64" s="45" t="s">
         <v>201</v>
@@ -4759,7 +4833,7 @@
         <v>1</v>
       </c>
       <c r="C65" s="41" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="D65" s="41">
         <v>0</v>
@@ -4781,8 +4855,8 @@
       <c r="B66" s="46" t="s">
         <v>1</v>
       </c>
-      <c r="C66" s="41" t="s">
-        <v>152</v>
+      <c r="C66" s="40" t="s">
+        <v>208</v>
       </c>
       <c r="D66" s="41">
         <v>0</v>
@@ -4791,34 +4865,60 @@
         <v>7</v>
       </c>
       <c r="F66" s="41">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G66" s="45" t="s">
-        <v>198</v>
+        <v>217</v>
       </c>
       <c r="H66" s="45" t="s">
-        <v>203</v>
+        <v>219</v>
       </c>
     </row>
     <row r="67" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B67" s="56"/>
+      <c r="B67" s="46" t="s">
+        <v>1</v>
+      </c>
       <c r="C67" s="40" t="s">
-        <v>209</v>
-      </c>
-      <c r="D67" s="40"/>
-      <c r="E67" s="40"/>
-      <c r="F67" s="40"/>
-      <c r="G67" s="58"/>
-      <c r="H67" s="58"/>
+        <v>212</v>
+      </c>
+      <c r="D67" s="41">
+        <v>0</v>
+      </c>
+      <c r="E67" s="41">
+        <v>7</v>
+      </c>
+      <c r="F67" s="41">
+        <v>1</v>
+      </c>
+      <c r="G67" s="45" t="s">
+        <v>218</v>
+      </c>
+      <c r="H67" s="45" t="s">
+        <v>220</v>
+      </c>
     </row>
     <row r="68" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B68" s="56"/>
-      <c r="C68" s="40"/>
-      <c r="D68" s="40"/>
-      <c r="E68" s="40"/>
-      <c r="F68" s="40"/>
-      <c r="G68" s="59"/>
-      <c r="H68" s="59"/>
+      <c r="B68" s="46" t="s">
+        <v>1</v>
+      </c>
+      <c r="C68" s="40" t="s">
+        <v>213</v>
+      </c>
+      <c r="D68" s="41">
+        <v>0</v>
+      </c>
+      <c r="E68" s="41">
+        <v>7</v>
+      </c>
+      <c r="F68" s="41">
+        <v>1</v>
+      </c>
+      <c r="G68" s="45" t="s">
+        <v>55</v>
+      </c>
+      <c r="H68" s="45" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="69" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B69" s="56"/>
@@ -4826,88 +4926,111 @@
       <c r="D69" s="40"/>
       <c r="E69" s="40"/>
       <c r="F69" s="40"/>
-      <c r="G69" s="59"/>
-      <c r="H69" s="59"/>
+      <c r="G69" s="57"/>
+      <c r="H69" s="57"/>
     </row>
     <row r="70" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B70" s="56"/>
-      <c r="C70" s="40"/>
-      <c r="D70" s="40"/>
-      <c r="E70" s="40"/>
-      <c r="F70" s="40"/>
-      <c r="G70" s="59"/>
-      <c r="H70" s="59"/>
-    </row>
-    <row r="71" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B71" s="46"/>
-      <c r="C71" s="41"/>
-      <c r="D71" s="41"/>
-      <c r="E71" s="41"/>
-      <c r="F71" s="41"/>
-      <c r="G71" s="60"/>
-      <c r="H71" s="60"/>
-    </row>
-    <row r="72" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="73" spans="2:13" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B73" s="6" t="s">
+      <c r="B70" s="46"/>
+      <c r="C70" s="41"/>
+      <c r="D70" s="41"/>
+      <c r="E70" s="41"/>
+      <c r="F70" s="41"/>
+      <c r="G70" s="58"/>
+      <c r="H70" s="58"/>
+    </row>
+    <row r="71" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="72" spans="2:13" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B72" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="C73" s="6"/>
-      <c r="D73" s="6"/>
-      <c r="E73" s="6"/>
-      <c r="F73" s="6"/>
-      <c r="G73" s="6"/>
-      <c r="H73" s="6"/>
-      <c r="I73" s="6"/>
-      <c r="J73" s="6"/>
-      <c r="K73" s="6"/>
-      <c r="L73" s="6"/>
-      <c r="M73" s="6"/>
-    </row>
-    <row r="74" spans="2:13" ht="60" x14ac:dyDescent="0.25">
-      <c r="B74" s="20"/>
-      <c r="C74" s="20"/>
-      <c r="D74" s="20"/>
-      <c r="E74" s="20"/>
-      <c r="F74" s="21" t="s">
+      <c r="C72" s="6"/>
+      <c r="D72" s="6"/>
+      <c r="E72" s="6"/>
+      <c r="F72" s="6"/>
+      <c r="G72" s="6"/>
+      <c r="H72" s="6"/>
+      <c r="I72" s="6"/>
+      <c r="J72" s="6"/>
+      <c r="K72" s="6"/>
+      <c r="L72" s="6"/>
+      <c r="M72" s="6"/>
+    </row>
+    <row r="73" spans="2:13" ht="60" x14ac:dyDescent="0.25">
+      <c r="B73" s="20"/>
+      <c r="C73" s="20"/>
+      <c r="D73" s="20"/>
+      <c r="E73" s="20"/>
+      <c r="F73" s="21" t="s">
         <v>40</v>
       </c>
-      <c r="G74" s="63" t="s">
+      <c r="G73" s="61" t="s">
         <v>39</v>
       </c>
-      <c r="H74" s="63"/>
-      <c r="I74" s="20"/>
-    </row>
-    <row r="75" spans="2:13" ht="142.5" x14ac:dyDescent="0.25">
-      <c r="B75" s="19" t="s">
+      <c r="H73" s="61"/>
+      <c r="I73" s="20"/>
+    </row>
+    <row r="74" spans="2:13" ht="142.5" x14ac:dyDescent="0.25">
+      <c r="B74" s="19" t="s">
         <v>38</v>
       </c>
-      <c r="C75" s="19" t="s">
+      <c r="C74" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="D75" s="18" t="s">
+      <c r="D74" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="E75" s="17" t="s">
+      <c r="E74" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="F75" s="17" t="s">
+      <c r="F74" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="G75" s="17" t="s">
+      <c r="G74" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="H75" s="16" t="s">
+      <c r="H74" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="I75" s="16" t="s">
+      <c r="I74" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="J75" s="15" t="s">
+      <c r="J74" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="K75" s="14" t="s">
+      <c r="K74" s="14" t="s">
         <v>30</v>
+      </c>
+    </row>
+    <row r="75" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B75" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="C75" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="D75" s="11">
+        <v>0</v>
+      </c>
+      <c r="E75" s="10">
+        <v>0</v>
+      </c>
+      <c r="F75" s="10">
+        <v>15</v>
+      </c>
+      <c r="G75" s="10">
+        <v>200</v>
+      </c>
+      <c r="H75" s="9">
+        <v>0.5</v>
+      </c>
+      <c r="I75" s="9">
+        <v>1</v>
+      </c>
+      <c r="J75" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="K75" s="13" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="76" spans="2:13" x14ac:dyDescent="0.25">
@@ -4915,19 +5038,19 @@
         <v>1</v>
       </c>
       <c r="C76" s="11" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D76" s="11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E76" s="10">
         <v>0</v>
       </c>
       <c r="F76" s="10">
-        <v>15</v>
+        <v>60</v>
       </c>
       <c r="G76" s="10">
-        <v>200</v>
+        <v>300</v>
       </c>
       <c r="H76" s="9">
         <v>0.5</v>
@@ -4936,10 +5059,10 @@
         <v>1</v>
       </c>
       <c r="J76" s="8" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="K76" s="13" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="77" spans="2:13" x14ac:dyDescent="0.25">
@@ -4947,19 +5070,19 @@
         <v>1</v>
       </c>
       <c r="C77" s="11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D77" s="11">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E77" s="10">
         <v>0</v>
       </c>
       <c r="F77" s="10">
-        <v>60</v>
+        <v>240</v>
       </c>
       <c r="G77" s="10">
-        <v>300</v>
+        <v>600</v>
       </c>
       <c r="H77" s="9">
         <v>0.5</v>
@@ -4968,67 +5091,49 @@
         <v>1</v>
       </c>
       <c r="J77" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="K77" s="13" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="78" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B78" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="C78" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="D78" s="11">
+        <v>25</v>
+      </c>
+      <c r="K77" s="7" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="79" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="80" spans="2:13" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B80" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C80" s="6"/>
+      <c r="D80" s="6"/>
+      <c r="E80" s="6"/>
+      <c r="F80" s="6"/>
+      <c r="G80" s="6"/>
+    </row>
+    <row r="82" spans="2:7" ht="135.75" x14ac:dyDescent="0.25">
+      <c r="B82" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C82" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D82" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E78" s="10">
-        <v>0</v>
-      </c>
-      <c r="F78" s="10">
-        <v>240</v>
-      </c>
-      <c r="G78" s="10">
-        <v>600</v>
-      </c>
-      <c r="H78" s="9">
-        <v>0.5</v>
-      </c>
-      <c r="I78" s="9">
-        <v>1</v>
-      </c>
-      <c r="J78" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="K78" s="7" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="80" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="81" spans="2:7" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B81" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="C81" s="6"/>
-      <c r="D81" s="6"/>
-      <c r="E81" s="6"/>
-      <c r="F81" s="6"/>
-      <c r="G81" s="6"/>
-    </row>
-    <row r="83" spans="2:7" ht="135.75" x14ac:dyDescent="0.25">
-      <c r="B83" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="C83" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D83" s="3" t="s">
+      <c r="E82" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="83" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B83" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C83" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D83" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="E83" s="1">
         <v>2</v>
-      </c>
-      <c r="E83" s="3" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="84" spans="2:7" x14ac:dyDescent="0.25">
@@ -5036,13 +5141,13 @@
         <v>1</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D84" s="1">
-        <v>0.1</v>
+        <v>0.7</v>
       </c>
       <c r="E84" s="1">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="85" spans="2:7" x14ac:dyDescent="0.25">
@@ -5050,13 +5155,13 @@
         <v>1</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D85" s="1">
-        <v>0.7</v>
+        <v>1</v>
       </c>
       <c r="E85" s="1">
-        <v>6</v>
+        <v>12</v>
       </c>
     </row>
     <row r="86" spans="2:7" x14ac:dyDescent="0.25">
@@ -5064,13 +5169,13 @@
         <v>1</v>
       </c>
       <c r="C86" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D86" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="E86" s="1">
         <v>18</v>
-      </c>
-      <c r="D86" s="1">
-        <v>1</v>
-      </c>
-      <c r="E86" s="1">
-        <v>12</v>
       </c>
     </row>
     <row r="87" spans="2:7" x14ac:dyDescent="0.25">
@@ -5078,13 +5183,13 @@
         <v>1</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D87" s="1">
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="E87" s="1">
-        <v>18</v>
+        <v>26</v>
       </c>
     </row>
     <row r="88" spans="2:7" x14ac:dyDescent="0.25">
@@ -5092,13 +5197,13 @@
         <v>1</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D88" s="1">
-        <v>2</v>
+        <v>2.5</v>
       </c>
       <c r="E88" s="1">
-        <v>26</v>
+        <v>35</v>
       </c>
     </row>
     <row r="89" spans="2:7" x14ac:dyDescent="0.25">
@@ -5106,13 +5211,13 @@
         <v>1</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D89" s="1">
-        <v>2.5</v>
+        <v>3</v>
       </c>
       <c r="E89" s="1">
-        <v>35</v>
+        <v>45</v>
       </c>
     </row>
     <row r="90" spans="2:7" x14ac:dyDescent="0.25">
@@ -5120,13 +5225,13 @@
         <v>1</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D90" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E90" s="1">
-        <v>45</v>
+        <v>56</v>
       </c>
     </row>
     <row r="91" spans="2:7" x14ac:dyDescent="0.25">
@@ -5134,13 +5239,13 @@
         <v>1</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D91" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E91" s="1">
-        <v>56</v>
+        <v>67</v>
       </c>
     </row>
     <row r="92" spans="2:7" x14ac:dyDescent="0.25">
@@ -5148,49 +5253,46 @@
         <v>1</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D92" s="1">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="E92" s="1">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="93" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B93" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C93" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D93" s="1">
-        <v>7</v>
-      </c>
-      <c r="E93" s="1">
         <v>80</v>
       </c>
     </row>
-    <row r="94" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="95" spans="2:7" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B95" s="6" t="s">
+    <row r="93" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="94" spans="2:7" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B94" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C95" s="6"/>
-      <c r="D95" s="6"/>
-      <c r="E95" s="6"/>
-      <c r="F95" s="6"/>
-      <c r="G95" s="6"/>
-    </row>
-    <row r="97" spans="2:7" ht="142.5" x14ac:dyDescent="0.25">
-      <c r="B97" s="5" t="s">
+      <c r="C94" s="6"/>
+      <c r="D94" s="6"/>
+      <c r="E94" s="6"/>
+      <c r="F94" s="6"/>
+      <c r="G94" s="6"/>
+    </row>
+    <row r="96" spans="2:7" ht="142.5" x14ac:dyDescent="0.25">
+      <c r="B96" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C97" s="4" t="s">
+      <c r="C96" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D97" s="3" t="s">
+      <c r="D96" s="3" t="s">
         <v>2</v>
+      </c>
+    </row>
+    <row r="97" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B97" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C97" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D97" s="1">
+        <v>0.05</v>
       </c>
     </row>
     <row r="98" spans="2:7" x14ac:dyDescent="0.25">
@@ -5198,10 +5300,10 @@
         <v>1</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D98" s="1">
-        <v>0.05</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="99" spans="2:7" x14ac:dyDescent="0.25">
@@ -5209,53 +5311,42 @@
         <v>1</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D99" s="1">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="100" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B100" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C100" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D100" s="1">
         <v>0.2</v>
       </c>
     </row>
-    <row r="101" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="102" spans="2:7" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B102" s="6" t="s">
+    <row r="100" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="101" spans="2:7" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B101" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C102" s="6"/>
-      <c r="D102" s="6"/>
-      <c r="E102" s="6"/>
-      <c r="F102" s="6"/>
-      <c r="G102" s="6"/>
-    </row>
-    <row r="104" spans="2:7" ht="132" x14ac:dyDescent="0.25">
-      <c r="B104" s="5" t="s">
+      <c r="C101" s="6"/>
+      <c r="D101" s="6"/>
+      <c r="E101" s="6"/>
+      <c r="F101" s="6"/>
+      <c r="G101" s="6"/>
+    </row>
+    <row r="103" spans="2:7" ht="132" x14ac:dyDescent="0.25">
+      <c r="B103" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C104" s="4" t="s">
+      <c r="C103" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D104" s="3" t="s">
+      <c r="D103" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="105" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B105" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C105" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D105" s="1">
+    <row r="104" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B104" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C104" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D104" s="1">
         <v>0.7</v>
       </c>
     </row>
@@ -5263,10 +5354,10 @@
   <mergeCells count="4">
     <mergeCell ref="J3:K3"/>
     <mergeCell ref="M3:P3"/>
-    <mergeCell ref="F53:H53"/>
-    <mergeCell ref="G74:H74"/>
+    <mergeCell ref="F52:H52"/>
+    <mergeCell ref="G73:H73"/>
   </mergeCells>
-  <conditionalFormatting sqref="C76:D78">
+  <conditionalFormatting sqref="C75:D77">
     <cfRule type="duplicateValues" dxfId="66" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
[FIX] [CONTENT] Removed useless tid multi run for mission critical_time
Former-commit-id: c808265986705b675b2d20b60aad601f5dd3a166
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Missions.xlsx
+++ b/Docs/Content/HungryDragonContent_Missions.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="430" uniqueCount="221">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="429" uniqueCount="220">
   <si>
     <t>single_run</t>
   </si>
@@ -706,9 +706,6 @@
   </si>
   <si>
     <t>TID_MISSION_OBJECTIVE_EATDIZZY_DESC_SINGLE_RUN</t>
-  </si>
-  <si>
-    <t>TID_MISSION_OBJECTIVE_CRITICALTIME_DESC_MULTI_RUN</t>
   </si>
   <si>
     <t>TID_MISSION_OBJECTIVE_EATDIZZY_DESC_MULTI_RUN</t>
@@ -2666,8 +2663,8 @@
   </sheetPr>
   <dimension ref="B1:P104"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H66" sqref="H66:H68"/>
+    <sheetView tabSelected="1" topLeftCell="D46" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I66" sqref="I66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4870,9 +4867,7 @@
       <c r="G66" s="45" t="s">
         <v>217</v>
       </c>
-      <c r="H66" s="45" t="s">
-        <v>219</v>
-      </c>
+      <c r="H66" s="45"/>
     </row>
     <row r="67" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B67" s="46" t="s">
@@ -4894,7 +4889,7 @@
         <v>218</v>
       </c>
       <c r="H67" s="45" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="68" spans="2:13" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
[CONTENT] Added new missions for eat_gold type
Former-commit-id: 52be9f25585e3262757b5837c3d9963b1a9efaf5
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Missions.xlsx
+++ b/Docs/Content/HungryDragonContent_Missions.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="429" uniqueCount="220">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="441" uniqueCount="223">
   <si>
     <t>single_run</t>
   </si>
@@ -660,12 +660,6 @@
     <t>TID_MISSION_OBJECTIVE_EATSUICIDAL_DESC_MULTI_RUN</t>
   </si>
   <si>
-    <t>eat_gold_birdsPrey</t>
-  </si>
-  <si>
-    <t>Blue Canaries</t>
-  </si>
-  <si>
     <t>TID_EDIBLE_CANARY_01_PL</t>
   </si>
   <si>
@@ -709,6 +703,21 @@
   </si>
   <si>
     <t>TID_MISSION_OBJECTIVE_EATDIZZY_DESC_MULTI_RUN</t>
+  </si>
+  <si>
+    <t>eat_gold_birds</t>
+  </si>
+  <si>
+    <t>eat_gold_goblins</t>
+  </si>
+  <si>
+    <t>eat_gold_cattle</t>
+  </si>
+  <si>
+    <t>eat_gold_birdsOfPrey</t>
+  </si>
+  <si>
+    <t>Canary01_Flock</t>
   </si>
 </sst>
 </file>
@@ -886,7 +895,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="14">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -1038,22 +1047,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="62">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1"/>
@@ -1196,12 +1194,6 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1217,6 +1209,16 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="67">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -2278,16 +2280,6 @@
         </bottom>
       </border>
     </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -2302,94 +2294,94 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="missionDifficultyDefinitions" displayName="missionDifficultyDefinitions" ref="B74:K77" totalsRowShown="0" headerRowBorderDxfId="65" tableBorderDxfId="64">
-  <autoFilter ref="B74:K77"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="missionDifficultyDefinitions" displayName="missionDifficultyDefinitions" ref="B76:K79" totalsRowShown="0" headerRowBorderDxfId="66" tableBorderDxfId="65">
+  <autoFilter ref="B76:K79"/>
   <tableColumns count="10">
     <tableColumn id="1" name="{missionDifficultyDefinitions}"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="63"/>
-    <tableColumn id="7" name="[index]" dataDxfId="62"/>
-    <tableColumn id="3" name="[dragonsToUnlock]" dataDxfId="61"/>
-    <tableColumn id="4" name="[cooldownMinutes]" dataDxfId="60"/>
-    <tableColumn id="9" name="[maxRewardCoins]" dataDxfId="59"/>
-    <tableColumn id="5" name="[removeMissionPCCoefA]" dataDxfId="58"/>
-    <tableColumn id="6" name="[removeMissionPCCoefB]" dataDxfId="57"/>
-    <tableColumn id="8" name="[tidName]" dataDxfId="56"/>
-    <tableColumn id="10" name="[color]" dataDxfId="55"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="64"/>
+    <tableColumn id="7" name="[index]" dataDxfId="63"/>
+    <tableColumn id="3" name="[dragonsToUnlock]" dataDxfId="62"/>
+    <tableColumn id="4" name="[cooldownMinutes]" dataDxfId="61"/>
+    <tableColumn id="9" name="[maxRewardCoins]" dataDxfId="60"/>
+    <tableColumn id="5" name="[removeMissionPCCoefA]" dataDxfId="59"/>
+    <tableColumn id="6" name="[removeMissionPCCoefB]" dataDxfId="58"/>
+    <tableColumn id="8" name="[tidName]" dataDxfId="57"/>
+    <tableColumn id="10" name="[color]" dataDxfId="56"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table13303132" displayName="Table13303132" ref="B82:E92" totalsRowShown="0" headerRowDxfId="54" dataDxfId="52" headerRowBorderDxfId="53" tableBorderDxfId="51" totalsRowBorderDxfId="50">
-  <autoFilter ref="B82:E92"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table13303132" displayName="Table13303132" ref="B84:E94" totalsRowShown="0" headerRowDxfId="55" dataDxfId="53" headerRowBorderDxfId="54" tableBorderDxfId="52" totalsRowBorderDxfId="51">
+  <autoFilter ref="B84:E94"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="{missionDragonModifiersDefinitions}" dataDxfId="49"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="48"/>
-    <tableColumn id="7" name="[quantityModifier]" dataDxfId="47"/>
-    <tableColumn id="3" name="[missionSCRewardMultiplier]" dataDxfId="46"/>
+    <tableColumn id="1" name="{missionDragonModifiersDefinitions}" dataDxfId="50"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="49"/>
+    <tableColumn id="7" name="[quantityModifier]" dataDxfId="48"/>
+    <tableColumn id="3" name="[missionSCRewardMultiplier]" dataDxfId="47"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table1330313234" displayName="Table1330313234" ref="B96:D99" totalsRowShown="0" headerRowDxfId="45" dataDxfId="43" headerRowBorderDxfId="44" tableBorderDxfId="42" totalsRowBorderDxfId="41">
-  <autoFilter ref="B96:D99"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table1330313234" displayName="Table1330313234" ref="B98:D101" totalsRowShown="0" headerRowDxfId="46" dataDxfId="44" headerRowBorderDxfId="45" tableBorderDxfId="43" totalsRowBorderDxfId="42">
+  <autoFilter ref="B98:D101"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="{missionDifficultyModifiersDefinitions}" dataDxfId="40"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="39"/>
-    <tableColumn id="7" name="[quantityModifier]" dataDxfId="38"/>
+    <tableColumn id="1" name="{missionDifficultyModifiersDefinitions}" dataDxfId="41"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="40"/>
+    <tableColumn id="7" name="[quantityModifier]" dataDxfId="39"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table133031323435" displayName="Table133031323435" ref="B103:D104" totalsRowShown="0" headerRowDxfId="37" dataDxfId="35" headerRowBorderDxfId="36" tableBorderDxfId="34" totalsRowBorderDxfId="33">
-  <autoFilter ref="B103:D104"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table133031323435" displayName="Table133031323435" ref="B105:D106" totalsRowShown="0" headerRowDxfId="38" dataDxfId="36" headerRowBorderDxfId="37" tableBorderDxfId="35" totalsRowBorderDxfId="34">
+  <autoFilter ref="B105:D106"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="{missionOtherModifiersDefinitions}" dataDxfId="32"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="31"/>
-    <tableColumn id="7" name="[quantityModifier]" dataDxfId="30"/>
+    <tableColumn id="1" name="{missionOtherModifiersDefinitions}" dataDxfId="33"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="32"/>
+    <tableColumn id="7" name="[quantityModifier]" dataDxfId="31"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table13" displayName="Table13" ref="B53:H70" totalsRowShown="0" headerRowDxfId="29" dataDxfId="27" headerRowBorderDxfId="28" tableBorderDxfId="26" totalsRowBorderDxfId="25">
-  <autoFilter ref="B53:H70"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table13" displayName="Table13" ref="B56:H72" totalsRowShown="0" headerRowDxfId="30" dataDxfId="28" headerRowBorderDxfId="29" tableBorderDxfId="27" totalsRowBorderDxfId="26">
+  <autoFilter ref="B56:H72"/>
   <tableColumns count="7">
-    <tableColumn id="1" name="{missionTypeDefinitions}" dataDxfId="24"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="23"/>
-    <tableColumn id="3" name="[minTier]" dataDxfId="22"/>
-    <tableColumn id="6" name="[maxTier]" dataDxfId="21"/>
-    <tableColumn id="4" name="[weight]" dataDxfId="20"/>
-    <tableColumn id="9" name="[tidDescSingleRun]" dataDxfId="19"/>
-    <tableColumn id="10" name="[tidDescMultiRun]" dataDxfId="18"/>
+    <tableColumn id="1" name="{missionTypeDefinitions}" dataDxfId="25"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="24"/>
+    <tableColumn id="3" name="[minTier]" dataDxfId="23"/>
+    <tableColumn id="6" name="[maxTier]" dataDxfId="22"/>
+    <tableColumn id="4" name="[weight]" dataDxfId="21"/>
+    <tableColumn id="9" name="[tidDescSingleRun]" dataDxfId="20"/>
+    <tableColumn id="10" name="[tidDescMultiRun]" dataDxfId="19"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table1330" displayName="Table1330" ref="B4:N48" totalsRowShown="0" headerRowDxfId="17" dataDxfId="15" headerRowBorderDxfId="16" tableBorderDxfId="14" totalsRowBorderDxfId="13">
-  <autoFilter ref="B4:N48"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table1330" displayName="Table1330" ref="B4:N51" totalsRowShown="0" headerRowDxfId="18" dataDxfId="16" headerRowBorderDxfId="17" tableBorderDxfId="15" totalsRowBorderDxfId="14">
+  <autoFilter ref="B4:N51"/>
   <tableColumns count="13">
-    <tableColumn id="1" name="{missionsDefinitions}" dataDxfId="12"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="11"/>
-    <tableColumn id="7" name="[type]" dataDxfId="10"/>
-    <tableColumn id="8" name="[weight]" dataDxfId="9"/>
-    <tableColumn id="13" name="[singleRunChance]" dataDxfId="8"/>
-    <tableColumn id="11" name="[minTier]" dataDxfId="7"/>
-    <tableColumn id="12" name="[maxTier]" dataDxfId="6"/>
-    <tableColumn id="6" name="[params]" dataDxfId="5"/>
-    <tableColumn id="3" name="[objectiveBaseQuantityMin]" dataDxfId="4"/>
-    <tableColumn id="9" name="[objectiveBaseQuantityMax]" dataDxfId="3"/>
-    <tableColumn id="4" name="[icon]" dataDxfId="2"/>
-    <tableColumn id="5" name="[tidObjective]" dataDxfId="1"/>
-    <tableColumn id="10" name="[trackingSku]" dataDxfId="0"/>
+    <tableColumn id="1" name="{missionsDefinitions}" dataDxfId="13"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="12"/>
+    <tableColumn id="7" name="[type]" dataDxfId="11"/>
+    <tableColumn id="8" name="[weight]" dataDxfId="10"/>
+    <tableColumn id="13" name="[singleRunChance]" dataDxfId="9"/>
+    <tableColumn id="11" name="[minTier]" dataDxfId="8"/>
+    <tableColumn id="12" name="[maxTier]" dataDxfId="7"/>
+    <tableColumn id="6" name="[params]" dataDxfId="6"/>
+    <tableColumn id="3" name="[objectiveBaseQuantityMin]" dataDxfId="5"/>
+    <tableColumn id="9" name="[objectiveBaseQuantityMax]" dataDxfId="4"/>
+    <tableColumn id="4" name="[icon]" dataDxfId="3"/>
+    <tableColumn id="5" name="[tidObjective]" dataDxfId="2"/>
+    <tableColumn id="10" name="[trackingSku]" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2661,10 +2653,10 @@
   <sheetPr>
     <tabColor theme="6"/>
   </sheetPr>
-  <dimension ref="B1:P104"/>
+  <dimension ref="B1:P106"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D46" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I66" sqref="I66"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E69" sqref="E69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2710,14 +2702,14 @@
         <v>145</v>
       </c>
       <c r="G3" s="38"/>
-      <c r="J3" s="59" t="s">
+      <c r="J3" s="57" t="s">
         <v>144</v>
       </c>
-      <c r="K3" s="59"/>
-      <c r="M3" s="59"/>
-      <c r="N3" s="59"/>
-      <c r="O3" s="59"/>
-      <c r="P3" s="59"/>
+      <c r="K3" s="57"/>
+      <c r="M3" s="57"/>
+      <c r="N3" s="57"/>
+      <c r="O3" s="57"/>
+      <c r="P3" s="57"/>
     </row>
     <row r="4" spans="2:16" ht="106.5" x14ac:dyDescent="0.25">
       <c r="B4" s="30" t="s">
@@ -3844,10 +3836,10 @@
         <v>1</v>
       </c>
       <c r="C32" s="53" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="D32" s="54" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="E32" s="54">
         <v>1</v>
@@ -3885,10 +3877,10 @@
         <v>1</v>
       </c>
       <c r="C33" s="53" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="D33" s="54" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="E33" s="54">
         <v>1</v>
@@ -3903,7 +3895,7 @@
         <v>7</v>
       </c>
       <c r="I33" s="54" t="s">
-        <v>204</v>
+        <v>222</v>
       </c>
       <c r="J33" s="53">
         <v>99</v>
@@ -3915,7 +3907,7 @@
         <v>130</v>
       </c>
       <c r="M33" s="48" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="N33" s="55" t="s">
         <v>73</v>
@@ -3926,10 +3918,10 @@
         <v>1</v>
       </c>
       <c r="C34" s="53" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="D34" s="54" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="E34" s="54">
         <v>1</v>
@@ -3967,7 +3959,7 @@
         <v>1</v>
       </c>
       <c r="C35" s="53" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="D35" s="54" t="s">
         <v>151</v>
@@ -4209,7 +4201,7 @@
         <v>1</v>
       </c>
       <c r="C41" s="53" t="s">
-        <v>203</v>
+        <v>221</v>
       </c>
       <c r="D41" s="54" t="s">
         <v>151</v>
@@ -4250,10 +4242,10 @@
         <v>1</v>
       </c>
       <c r="C42" s="53" t="s">
-        <v>154</v>
+        <v>218</v>
       </c>
       <c r="D42" s="54" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="E42" s="54">
         <v>1</v>
@@ -4262,39 +4254,29 @@
         <v>0.3</v>
       </c>
       <c r="G42" s="53">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H42" s="54">
         <v>7</v>
       </c>
       <c r="I42" s="54" t="s">
-        <v>153</v>
-      </c>
-      <c r="J42" s="53">
-        <v>99</v>
-      </c>
-      <c r="K42" s="54">
-        <v>99</v>
-      </c>
-      <c r="L42" s="48" t="s">
-        <v>130</v>
-      </c>
-      <c r="M42" s="49" t="s">
-        <v>177</v>
-      </c>
-      <c r="N42" s="55" t="s">
-        <v>73</v>
-      </c>
+        <v>131</v>
+      </c>
+      <c r="J42" s="53"/>
+      <c r="K42" s="54"/>
+      <c r="L42" s="48"/>
+      <c r="M42" s="48"/>
+      <c r="N42" s="55"/>
     </row>
     <row r="43" spans="2:14" s="43" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B43" s="52" t="s">
         <v>1</v>
       </c>
       <c r="C43" s="53" t="s">
-        <v>159</v>
+        <v>220</v>
       </c>
       <c r="D43" s="54" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="E43" s="54">
         <v>1</v>
@@ -4309,33 +4291,23 @@
         <v>7</v>
       </c>
       <c r="I43" s="54" t="s">
-        <v>160</v>
-      </c>
-      <c r="J43" s="53">
-        <v>99</v>
-      </c>
-      <c r="K43" s="54">
-        <v>99</v>
-      </c>
-      <c r="L43" s="48" t="s">
-        <v>130</v>
-      </c>
-      <c r="M43" s="49" t="s">
-        <v>171</v>
-      </c>
-      <c r="N43" s="55" t="s">
-        <v>73</v>
-      </c>
+        <v>158</v>
+      </c>
+      <c r="J43" s="53"/>
+      <c r="K43" s="54"/>
+      <c r="L43" s="48"/>
+      <c r="M43" s="48"/>
+      <c r="N43" s="55"/>
     </row>
     <row r="44" spans="2:14" s="43" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B44" s="52" t="s">
         <v>1</v>
       </c>
       <c r="C44" s="53" t="s">
-        <v>157</v>
+        <v>219</v>
       </c>
       <c r="D44" s="54" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="E44" s="54">
         <v>1</v>
@@ -4344,53 +4316,45 @@
         <v>0.3</v>
       </c>
       <c r="G44" s="53">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H44" s="54">
         <v>7</v>
       </c>
       <c r="I44" s="54" t="s">
-        <v>158</v>
-      </c>
-      <c r="J44" s="53">
-        <v>99</v>
-      </c>
-      <c r="K44" s="54">
-        <v>99</v>
-      </c>
-      <c r="L44" s="48" t="s">
-        <v>130</v>
-      </c>
-      <c r="M44" s="49" t="s">
-        <v>194</v>
-      </c>
-      <c r="N44" s="55" t="s">
-        <v>73</v>
-      </c>
+        <v>106</v>
+      </c>
+      <c r="J44" s="53"/>
+      <c r="K44" s="54"/>
+      <c r="L44" s="48"/>
+      <c r="M44" s="48"/>
+      <c r="N44" s="55"/>
     </row>
     <row r="45" spans="2:14" s="43" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B45" s="52" t="s">
         <v>1</v>
       </c>
-      <c r="C45" s="40" t="s">
-        <v>208</v>
-      </c>
-      <c r="D45" s="40" t="s">
-        <v>208</v>
+      <c r="C45" s="53" t="s">
+        <v>154</v>
+      </c>
+      <c r="D45" s="54" t="s">
+        <v>152</v>
       </c>
       <c r="E45" s="54">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F45" s="54">
-        <v>0</v>
+        <v>0.3</v>
       </c>
       <c r="G45" s="53">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H45" s="54">
         <v>7</v>
       </c>
-      <c r="I45" s="54"/>
+      <c r="I45" s="54" t="s">
+        <v>153</v>
+      </c>
       <c r="J45" s="53">
         <v>99</v>
       </c>
@@ -4400,7 +4364,9 @@
       <c r="L45" s="48" t="s">
         <v>130</v>
       </c>
-      <c r="M45" s="49"/>
+      <c r="M45" s="49" t="s">
+        <v>177</v>
+      </c>
       <c r="N45" s="55" t="s">
         <v>73</v>
       </c>
@@ -4409,11 +4375,11 @@
       <c r="B46" s="52" t="s">
         <v>1</v>
       </c>
-      <c r="C46" s="40" t="s">
-        <v>215</v>
-      </c>
-      <c r="D46" s="40" t="s">
-        <v>212</v>
+      <c r="C46" s="53" t="s">
+        <v>159</v>
+      </c>
+      <c r="D46" s="54" t="s">
+        <v>152</v>
       </c>
       <c r="E46" s="54">
         <v>1</v>
@@ -4427,7 +4393,9 @@
       <c r="H46" s="54">
         <v>7</v>
       </c>
-      <c r="I46" s="41"/>
+      <c r="I46" s="54" t="s">
+        <v>160</v>
+      </c>
       <c r="J46" s="53">
         <v>99</v>
       </c>
@@ -4437,7 +4405,9 @@
       <c r="L46" s="48" t="s">
         <v>130</v>
       </c>
-      <c r="M46" s="41"/>
+      <c r="M46" s="49" t="s">
+        <v>171</v>
+      </c>
       <c r="N46" s="55" t="s">
         <v>73</v>
       </c>
@@ -4446,11 +4416,11 @@
       <c r="B47" s="52" t="s">
         <v>1</v>
       </c>
-      <c r="C47" s="40" t="s">
-        <v>214</v>
-      </c>
-      <c r="D47" s="40" t="s">
-        <v>213</v>
+      <c r="C47" s="53" t="s">
+        <v>157</v>
+      </c>
+      <c r="D47" s="54" t="s">
+        <v>152</v>
       </c>
       <c r="E47" s="54">
         <v>1</v>
@@ -4459,12 +4429,14 @@
         <v>0.3</v>
       </c>
       <c r="G47" s="53">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H47" s="54">
         <v>7</v>
       </c>
-      <c r="I47" s="41"/>
+      <c r="I47" s="54" t="s">
+        <v>158</v>
+      </c>
       <c r="J47" s="53">
         <v>99</v>
       </c>
@@ -4474,171 +4446,215 @@
       <c r="L47" s="48" t="s">
         <v>130</v>
       </c>
-      <c r="M47" s="41"/>
+      <c r="M47" s="49" t="s">
+        <v>194</v>
+      </c>
       <c r="N47" s="55" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="48" spans="2:14" s="43" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B48" s="52"/>
-      <c r="C48" s="40"/>
-      <c r="D48" s="40"/>
-      <c r="E48" s="54"/>
-      <c r="F48" s="54"/>
-      <c r="G48" s="53"/>
-      <c r="H48" s="54"/>
-      <c r="I48" s="41"/>
-      <c r="J48" s="53"/>
-      <c r="K48" s="54"/>
-      <c r="L48" s="48"/>
-      <c r="M48" s="41"/>
-      <c r="N48" s="55"/>
+      <c r="B48" s="52" t="s">
+        <v>1</v>
+      </c>
+      <c r="C48" s="40" t="s">
+        <v>206</v>
+      </c>
+      <c r="D48" s="40" t="s">
+        <v>206</v>
+      </c>
+      <c r="E48" s="54">
+        <v>0</v>
+      </c>
+      <c r="F48" s="54">
+        <v>0</v>
+      </c>
+      <c r="G48" s="53">
+        <v>0</v>
+      </c>
+      <c r="H48" s="54">
+        <v>7</v>
+      </c>
+      <c r="I48" s="54"/>
+      <c r="J48" s="53">
+        <v>99</v>
+      </c>
+      <c r="K48" s="54">
+        <v>99</v>
+      </c>
+      <c r="L48" s="48" t="s">
+        <v>130</v>
+      </c>
+      <c r="M48" s="49"/>
+      <c r="N48" s="55" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="49" spans="2:14" s="43" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B49" s="44"/>
-      <c r="C49" s="44"/>
-      <c r="D49" s="44"/>
-      <c r="E49" s="44"/>
-      <c r="F49" s="44"/>
-      <c r="G49" s="44"/>
-      <c r="H49" s="44"/>
-      <c r="I49" s="44"/>
-      <c r="J49" s="44"/>
-      <c r="K49" s="44"/>
-      <c r="L49" s="44"/>
-      <c r="M49" s="44"/>
-      <c r="N49" s="44"/>
-    </row>
-    <row r="50" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B50" s="32"/>
-      <c r="C50" s="32"/>
-      <c r="D50" s="32"/>
-      <c r="E50" s="32"/>
-      <c r="F50" s="32"/>
-      <c r="G50" s="32"/>
-      <c r="H50" s="32"/>
-      <c r="I50" s="32"/>
-      <c r="J50" s="32"/>
-      <c r="K50" s="32"/>
-      <c r="L50" s="32"/>
-      <c r="M50" s="31"/>
-    </row>
-    <row r="51" spans="2:14" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B51" s="6" t="s">
+      <c r="B49" s="52" t="s">
+        <v>1</v>
+      </c>
+      <c r="C49" s="40" t="s">
+        <v>213</v>
+      </c>
+      <c r="D49" s="40" t="s">
+        <v>210</v>
+      </c>
+      <c r="E49" s="54">
+        <v>1</v>
+      </c>
+      <c r="F49" s="54">
+        <v>0.3</v>
+      </c>
+      <c r="G49" s="53">
+        <v>0</v>
+      </c>
+      <c r="H49" s="54">
+        <v>7</v>
+      </c>
+      <c r="I49" s="41"/>
+      <c r="J49" s="53">
+        <v>99</v>
+      </c>
+      <c r="K49" s="54">
+        <v>99</v>
+      </c>
+      <c r="L49" s="48" t="s">
+        <v>130</v>
+      </c>
+      <c r="M49" s="41"/>
+      <c r="N49" s="55" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="50" spans="2:14" s="43" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B50" s="52" t="s">
+        <v>1</v>
+      </c>
+      <c r="C50" s="40" t="s">
+        <v>212</v>
+      </c>
+      <c r="D50" s="40" t="s">
+        <v>211</v>
+      </c>
+      <c r="E50" s="54">
+        <v>1</v>
+      </c>
+      <c r="F50" s="54">
+        <v>0.3</v>
+      </c>
+      <c r="G50" s="53">
+        <v>0</v>
+      </c>
+      <c r="H50" s="54">
+        <v>7</v>
+      </c>
+      <c r="I50" s="41"/>
+      <c r="J50" s="53">
+        <v>99</v>
+      </c>
+      <c r="K50" s="54">
+        <v>99</v>
+      </c>
+      <c r="L50" s="48" t="s">
+        <v>130</v>
+      </c>
+      <c r="M50" s="41"/>
+      <c r="N50" s="55" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="51" spans="2:14" s="43" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B51" s="52"/>
+      <c r="C51" s="40"/>
+      <c r="D51" s="40"/>
+      <c r="E51" s="54"/>
+      <c r="F51" s="54"/>
+      <c r="G51" s="53"/>
+      <c r="H51" s="54"/>
+      <c r="I51" s="41"/>
+      <c r="J51" s="53"/>
+      <c r="K51" s="54"/>
+      <c r="L51" s="48"/>
+      <c r="M51" s="41"/>
+      <c r="N51" s="55"/>
+    </row>
+    <row r="52" spans="2:14" s="43" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B52" s="44"/>
+      <c r="C52" s="44"/>
+      <c r="D52" s="44"/>
+      <c r="E52" s="44"/>
+      <c r="F52" s="44"/>
+      <c r="G52" s="44"/>
+      <c r="H52" s="44"/>
+      <c r="I52" s="44"/>
+      <c r="J52" s="44"/>
+      <c r="K52" s="44"/>
+      <c r="L52" s="44"/>
+      <c r="M52" s="44"/>
+      <c r="N52" s="44"/>
+    </row>
+    <row r="53" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B53" s="32"/>
+      <c r="C53" s="32"/>
+      <c r="D53" s="32"/>
+      <c r="E53" s="32"/>
+      <c r="F53" s="32"/>
+      <c r="G53" s="32"/>
+      <c r="H53" s="32"/>
+      <c r="I53" s="32"/>
+      <c r="J53" s="32"/>
+      <c r="K53" s="32"/>
+      <c r="L53" s="32"/>
+      <c r="M53" s="31"/>
+    </row>
+    <row r="54" spans="2:14" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B54" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="C51" s="6"/>
-      <c r="D51" s="6"/>
-      <c r="E51" s="6"/>
-      <c r="F51" s="6"/>
-      <c r="G51" s="6"/>
-      <c r="H51" s="6"/>
-      <c r="I51" s="6"/>
-      <c r="J51" s="6"/>
-      <c r="K51" s="6"/>
-      <c r="L51" s="6"/>
-    </row>
-    <row r="52" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B52" s="20"/>
-      <c r="C52" s="20"/>
-      <c r="D52" s="20"/>
-      <c r="E52" s="20"/>
-      <c r="F52" s="60"/>
-      <c r="G52" s="60"/>
-      <c r="H52" s="60"/>
-      <c r="I52" s="20"/>
-      <c r="J52" s="20"/>
-    </row>
-    <row r="53" spans="2:14" ht="96" x14ac:dyDescent="0.25">
-      <c r="B53" s="30" t="s">
+      <c r="C54" s="6"/>
+      <c r="D54" s="6"/>
+      <c r="E54" s="6"/>
+      <c r="F54" s="6"/>
+      <c r="G54" s="6"/>
+      <c r="H54" s="6"/>
+      <c r="I54" s="6"/>
+      <c r="J54" s="6"/>
+      <c r="K54" s="6"/>
+      <c r="L54" s="6"/>
+    </row>
+    <row r="55" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B55" s="20"/>
+      <c r="C55" s="20"/>
+      <c r="D55" s="20"/>
+      <c r="E55" s="20"/>
+      <c r="F55" s="58"/>
+      <c r="G55" s="58"/>
+      <c r="H55" s="58"/>
+      <c r="I55" s="20"/>
+      <c r="J55" s="20"/>
+    </row>
+    <row r="56" spans="2:14" ht="96" x14ac:dyDescent="0.25">
+      <c r="B56" s="30" t="s">
         <v>71</v>
       </c>
-      <c r="C53" s="28" t="s">
+      <c r="C56" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="D53" s="29" t="s">
+      <c r="D56" s="29" t="s">
         <v>70</v>
       </c>
-      <c r="E53" s="29" t="s">
+      <c r="E56" s="29" t="s">
         <v>69</v>
       </c>
-      <c r="F53" s="29" t="s">
+      <c r="F56" s="29" t="s">
         <v>68</v>
       </c>
-      <c r="G53" s="28" t="s">
+      <c r="G56" s="28" t="s">
         <v>67</v>
       </c>
-      <c r="H53" s="28" t="s">
+      <c r="H56" s="28" t="s">
         <v>66</v>
-      </c>
-    </row>
-    <row r="54" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B54" s="27" t="s">
-        <v>1</v>
-      </c>
-      <c r="C54" s="24" t="s">
-        <v>65</v>
-      </c>
-      <c r="D54" s="24">
-        <v>0</v>
-      </c>
-      <c r="E54" s="24">
-        <v>7</v>
-      </c>
-      <c r="F54" s="24">
-        <v>2</v>
-      </c>
-      <c r="G54" s="26" t="s">
-        <v>64</v>
-      </c>
-      <c r="H54" s="26" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="55" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B55" s="27" t="s">
-        <v>1</v>
-      </c>
-      <c r="C55" s="24" t="s">
-        <v>62</v>
-      </c>
-      <c r="D55" s="24">
-        <v>0</v>
-      </c>
-      <c r="E55" s="24">
-        <v>7</v>
-      </c>
-      <c r="F55" s="24">
-        <v>1</v>
-      </c>
-      <c r="G55" s="26" t="s">
-        <v>61</v>
-      </c>
-      <c r="H55" s="26" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="56" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B56" s="27" t="s">
-        <v>1</v>
-      </c>
-      <c r="C56" s="24" t="s">
-        <v>59</v>
-      </c>
-      <c r="D56" s="24">
-        <v>0</v>
-      </c>
-      <c r="E56" s="24">
-        <v>7</v>
-      </c>
-      <c r="F56" s="24">
-        <v>2</v>
-      </c>
-      <c r="G56" s="26" t="s">
-        <v>58</v>
-      </c>
-      <c r="H56" s="26" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="57" spans="2:14" x14ac:dyDescent="0.25">
@@ -4646,91 +4662,91 @@
         <v>1</v>
       </c>
       <c r="C57" s="24" t="s">
+        <v>65</v>
+      </c>
+      <c r="D57" s="24">
+        <v>0</v>
+      </c>
+      <c r="E57" s="24">
+        <v>7</v>
+      </c>
+      <c r="F57" s="24">
+        <v>2</v>
+      </c>
+      <c r="G57" s="26" t="s">
+        <v>64</v>
+      </c>
+      <c r="H57" s="26" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="58" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B58" s="27" t="s">
+        <v>1</v>
+      </c>
+      <c r="C58" s="24" t="s">
+        <v>62</v>
+      </c>
+      <c r="D58" s="24">
+        <v>0</v>
+      </c>
+      <c r="E58" s="24">
+        <v>7</v>
+      </c>
+      <c r="F58" s="24">
+        <v>1</v>
+      </c>
+      <c r="G58" s="26" t="s">
+        <v>61</v>
+      </c>
+      <c r="H58" s="26" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="59" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B59" s="27" t="s">
+        <v>1</v>
+      </c>
+      <c r="C59" s="24" t="s">
+        <v>59</v>
+      </c>
+      <c r="D59" s="24">
+        <v>0</v>
+      </c>
+      <c r="E59" s="24">
+        <v>7</v>
+      </c>
+      <c r="F59" s="24">
+        <v>2</v>
+      </c>
+      <c r="G59" s="26" t="s">
+        <v>58</v>
+      </c>
+      <c r="H59" s="26" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="60" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B60" s="27" t="s">
+        <v>1</v>
+      </c>
+      <c r="C60" s="24" t="s">
         <v>56</v>
       </c>
-      <c r="D57" s="24">
-        <v>0</v>
-      </c>
-      <c r="E57" s="24">
-        <v>7</v>
-      </c>
-      <c r="F57" s="24">
-        <v>1</v>
-      </c>
-      <c r="G57" s="26" t="s">
+      <c r="D60" s="24">
+        <v>0</v>
+      </c>
+      <c r="E60" s="24">
+        <v>7</v>
+      </c>
+      <c r="F60" s="24">
+        <v>1</v>
+      </c>
+      <c r="G60" s="26" t="s">
         <v>55</v>
       </c>
-      <c r="H57" s="26" t="s">
+      <c r="H60" s="26" t="s">
         <v>54</v>
-      </c>
-    </row>
-    <row r="58" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B58" s="25" t="s">
-        <v>1</v>
-      </c>
-      <c r="C58" s="23" t="s">
-        <v>53</v>
-      </c>
-      <c r="D58" s="23">
-        <v>0</v>
-      </c>
-      <c r="E58" s="24">
-        <v>7</v>
-      </c>
-      <c r="F58" s="23">
-        <v>1</v>
-      </c>
-      <c r="G58" s="26" t="s">
-        <v>52</v>
-      </c>
-      <c r="H58" s="26" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="59" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B59" s="25" t="s">
-        <v>1</v>
-      </c>
-      <c r="C59" s="24" t="s">
-        <v>50</v>
-      </c>
-      <c r="D59" s="24">
-        <v>0</v>
-      </c>
-      <c r="E59" s="24">
-        <v>7</v>
-      </c>
-      <c r="F59" s="24">
-        <v>1</v>
-      </c>
-      <c r="G59" s="26" t="s">
-        <v>49</v>
-      </c>
-      <c r="H59" s="26" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="60" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B60" s="25" t="s">
-        <v>1</v>
-      </c>
-      <c r="C60" s="24" t="s">
-        <v>47</v>
-      </c>
-      <c r="D60" s="24">
-        <v>0</v>
-      </c>
-      <c r="E60" s="24">
-        <v>7</v>
-      </c>
-      <c r="F60" s="24">
-        <v>1</v>
-      </c>
-      <c r="G60" s="26" t="s">
-        <v>46</v>
-      </c>
-      <c r="H60" s="26" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="61" spans="2:14" x14ac:dyDescent="0.25">
@@ -4738,91 +4754,91 @@
         <v>1</v>
       </c>
       <c r="C61" s="23" t="s">
+        <v>53</v>
+      </c>
+      <c r="D61" s="23">
+        <v>0</v>
+      </c>
+      <c r="E61" s="24">
+        <v>7</v>
+      </c>
+      <c r="F61" s="23">
+        <v>1</v>
+      </c>
+      <c r="G61" s="26" t="s">
+        <v>52</v>
+      </c>
+      <c r="H61" s="26" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="62" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B62" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="C62" s="24" t="s">
+        <v>50</v>
+      </c>
+      <c r="D62" s="24">
+        <v>0</v>
+      </c>
+      <c r="E62" s="24">
+        <v>7</v>
+      </c>
+      <c r="F62" s="24">
+        <v>1</v>
+      </c>
+      <c r="G62" s="26" t="s">
+        <v>49</v>
+      </c>
+      <c r="H62" s="26" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="63" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B63" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="C63" s="24" t="s">
+        <v>47</v>
+      </c>
+      <c r="D63" s="24">
+        <v>0</v>
+      </c>
+      <c r="E63" s="24">
+        <v>7</v>
+      </c>
+      <c r="F63" s="24">
+        <v>1</v>
+      </c>
+      <c r="G63" s="26" t="s">
+        <v>46</v>
+      </c>
+      <c r="H63" s="26" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="64" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B64" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="C64" s="23" t="s">
         <v>44</v>
       </c>
-      <c r="D61" s="23">
-        <v>0</v>
-      </c>
-      <c r="E61" s="24">
-        <v>7</v>
-      </c>
-      <c r="F61" s="23">
-        <v>1</v>
-      </c>
-      <c r="G61" s="22" t="s">
+      <c r="D64" s="23">
+        <v>0</v>
+      </c>
+      <c r="E64" s="24">
+        <v>7</v>
+      </c>
+      <c r="F64" s="23">
+        <v>1</v>
+      </c>
+      <c r="G64" s="22" t="s">
         <v>43</v>
       </c>
-      <c r="H61" s="22" t="s">
+      <c r="H64" s="22" t="s">
         <v>42</v>
-      </c>
-    </row>
-    <row r="62" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B62" s="46" t="s">
-        <v>1</v>
-      </c>
-      <c r="C62" s="41" t="s">
-        <v>209</v>
-      </c>
-      <c r="D62" s="41">
-        <v>0</v>
-      </c>
-      <c r="E62" s="41">
-        <v>7</v>
-      </c>
-      <c r="F62" s="41">
-        <v>1</v>
-      </c>
-      <c r="G62" s="42" t="s">
-        <v>195</v>
-      </c>
-      <c r="H62" s="42" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="63" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B63" s="46" t="s">
-        <v>1</v>
-      </c>
-      <c r="C63" s="41" t="s">
-        <v>206</v>
-      </c>
-      <c r="D63" s="41">
-        <v>0</v>
-      </c>
-      <c r="E63" s="41">
-        <v>7</v>
-      </c>
-      <c r="F63" s="41">
-        <v>2</v>
-      </c>
-      <c r="G63" s="45" t="s">
-        <v>198</v>
-      </c>
-      <c r="H63" s="45" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="64" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B64" s="46" t="s">
-        <v>1</v>
-      </c>
-      <c r="C64" s="41" t="s">
-        <v>151</v>
-      </c>
-      <c r="D64" s="41">
-        <v>0</v>
-      </c>
-      <c r="E64" s="41">
-        <v>7</v>
-      </c>
-      <c r="F64" s="41">
-        <v>2</v>
-      </c>
-      <c r="G64" s="45" t="s">
-        <v>196</v>
-      </c>
-      <c r="H64" s="45" t="s">
-        <v>201</v>
       </c>
     </row>
     <row r="65" spans="2:13" x14ac:dyDescent="0.25">
@@ -4830,7 +4846,7 @@
         <v>1</v>
       </c>
       <c r="C65" s="41" t="s">
-        <v>152</v>
+        <v>207</v>
       </c>
       <c r="D65" s="41">
         <v>0</v>
@@ -4839,21 +4855,21 @@
         <v>7</v>
       </c>
       <c r="F65" s="41">
-        <v>2</v>
-      </c>
-      <c r="G65" s="45" t="s">
-        <v>197</v>
-      </c>
-      <c r="H65" s="45" t="s">
-        <v>202</v>
+        <v>1</v>
+      </c>
+      <c r="G65" s="42" t="s">
+        <v>195</v>
+      </c>
+      <c r="H65" s="42" t="s">
+        <v>199</v>
       </c>
     </row>
     <row r="66" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B66" s="46" t="s">
         <v>1</v>
       </c>
-      <c r="C66" s="40" t="s">
-        <v>208</v>
+      <c r="C66" s="41" t="s">
+        <v>204</v>
       </c>
       <c r="D66" s="41">
         <v>0</v>
@@ -4862,19 +4878,21 @@
         <v>7</v>
       </c>
       <c r="F66" s="41">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G66" s="45" t="s">
-        <v>217</v>
-      </c>
-      <c r="H66" s="45"/>
+        <v>198</v>
+      </c>
+      <c r="H66" s="45" t="s">
+        <v>200</v>
+      </c>
     </row>
     <row r="67" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B67" s="46" t="s">
         <v>1</v>
       </c>
-      <c r="C67" s="40" t="s">
-        <v>212</v>
+      <c r="C67" s="41" t="s">
+        <v>151</v>
       </c>
       <c r="D67" s="41">
         <v>0</v>
@@ -4883,21 +4901,21 @@
         <v>7</v>
       </c>
       <c r="F67" s="41">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G67" s="45" t="s">
-        <v>218</v>
+        <v>196</v>
       </c>
       <c r="H67" s="45" t="s">
-        <v>219</v>
+        <v>201</v>
       </c>
     </row>
     <row r="68" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B68" s="46" t="s">
         <v>1</v>
       </c>
-      <c r="C68" s="40" t="s">
-        <v>213</v>
+      <c r="C68" s="41" t="s">
+        <v>152</v>
       </c>
       <c r="D68" s="41">
         <v>0</v>
@@ -4906,158 +4924,152 @@
         <v>7</v>
       </c>
       <c r="F68" s="41">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G68" s="45" t="s">
+        <v>197</v>
+      </c>
+      <c r="H68" s="45" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="69" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B69" s="46" t="s">
+        <v>1</v>
+      </c>
+      <c r="C69" s="40" t="s">
+        <v>206</v>
+      </c>
+      <c r="D69" s="41">
+        <v>0</v>
+      </c>
+      <c r="E69" s="41">
+        <v>7</v>
+      </c>
+      <c r="F69" s="41">
+        <v>1</v>
+      </c>
+      <c r="G69" s="45" t="s">
+        <v>215</v>
+      </c>
+      <c r="H69" s="45"/>
+    </row>
+    <row r="70" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B70" s="46" t="s">
+        <v>1</v>
+      </c>
+      <c r="C70" s="40" t="s">
+        <v>210</v>
+      </c>
+      <c r="D70" s="41">
+        <v>0</v>
+      </c>
+      <c r="E70" s="41">
+        <v>7</v>
+      </c>
+      <c r="F70" s="41">
+        <v>1</v>
+      </c>
+      <c r="G70" s="45" t="s">
+        <v>216</v>
+      </c>
+      <c r="H70" s="45" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="71" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B71" s="46" t="s">
+        <v>1</v>
+      </c>
+      <c r="C71" s="40" t="s">
+        <v>211</v>
+      </c>
+      <c r="D71" s="41">
+        <v>0</v>
+      </c>
+      <c r="E71" s="41">
+        <v>7</v>
+      </c>
+      <c r="F71" s="41">
+        <v>1</v>
+      </c>
+      <c r="G71" s="45" t="s">
         <v>55</v>
       </c>
-      <c r="H68" s="45" t="s">
+      <c r="H71" s="45" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="69" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B69" s="56"/>
-      <c r="C69" s="40"/>
-      <c r="D69" s="40"/>
-      <c r="E69" s="40"/>
-      <c r="F69" s="40"/>
-      <c r="G69" s="57"/>
-      <c r="H69" s="57"/>
-    </row>
-    <row r="70" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B70" s="46"/>
-      <c r="C70" s="41"/>
-      <c r="D70" s="41"/>
-      <c r="E70" s="41"/>
-      <c r="F70" s="41"/>
-      <c r="G70" s="58"/>
-      <c r="H70" s="58"/>
-    </row>
-    <row r="71" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="72" spans="2:13" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B72" s="6" t="s">
+    <row r="72" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B72" s="46"/>
+      <c r="C72" s="41"/>
+      <c r="D72" s="41"/>
+      <c r="E72" s="41"/>
+      <c r="F72" s="41"/>
+      <c r="G72" s="56"/>
+      <c r="H72" s="56"/>
+    </row>
+    <row r="73" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="74" spans="2:13" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B74" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="C72" s="6"/>
-      <c r="D72" s="6"/>
-      <c r="E72" s="6"/>
-      <c r="F72" s="6"/>
-      <c r="G72" s="6"/>
-      <c r="H72" s="6"/>
-      <c r="I72" s="6"/>
-      <c r="J72" s="6"/>
-      <c r="K72" s="6"/>
-      <c r="L72" s="6"/>
-      <c r="M72" s="6"/>
-    </row>
-    <row r="73" spans="2:13" ht="60" x14ac:dyDescent="0.25">
-      <c r="B73" s="20"/>
-      <c r="C73" s="20"/>
-      <c r="D73" s="20"/>
-      <c r="E73" s="20"/>
-      <c r="F73" s="21" t="s">
+      <c r="C74" s="6"/>
+      <c r="D74" s="6"/>
+      <c r="E74" s="6"/>
+      <c r="F74" s="6"/>
+      <c r="G74" s="6"/>
+      <c r="H74" s="6"/>
+      <c r="I74" s="6"/>
+      <c r="J74" s="6"/>
+      <c r="K74" s="6"/>
+      <c r="L74" s="6"/>
+      <c r="M74" s="6"/>
+    </row>
+    <row r="75" spans="2:13" ht="60" x14ac:dyDescent="0.25">
+      <c r="B75" s="20"/>
+      <c r="C75" s="20"/>
+      <c r="D75" s="20"/>
+      <c r="E75" s="20"/>
+      <c r="F75" s="21" t="s">
         <v>40</v>
       </c>
-      <c r="G73" s="61" t="s">
+      <c r="G75" s="59" t="s">
         <v>39</v>
       </c>
-      <c r="H73" s="61"/>
-      <c r="I73" s="20"/>
-    </row>
-    <row r="74" spans="2:13" ht="142.5" x14ac:dyDescent="0.25">
-      <c r="B74" s="19" t="s">
+      <c r="H75" s="59"/>
+      <c r="I75" s="20"/>
+    </row>
+    <row r="76" spans="2:13" ht="142.5" x14ac:dyDescent="0.25">
+      <c r="B76" s="19" t="s">
         <v>38</v>
       </c>
-      <c r="C74" s="19" t="s">
+      <c r="C76" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="D74" s="18" t="s">
+      <c r="D76" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="E74" s="17" t="s">
+      <c r="E76" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="F74" s="17" t="s">
+      <c r="F76" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="G74" s="17" t="s">
+      <c r="G76" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="H74" s="16" t="s">
+      <c r="H76" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="I74" s="16" t="s">
+      <c r="I76" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="J74" s="15" t="s">
+      <c r="J76" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="K74" s="14" t="s">
+      <c r="K76" s="14" t="s">
         <v>30</v>
-      </c>
-    </row>
-    <row r="75" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B75" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="C75" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="D75" s="11">
-        <v>0</v>
-      </c>
-      <c r="E75" s="10">
-        <v>0</v>
-      </c>
-      <c r="F75" s="10">
-        <v>15</v>
-      </c>
-      <c r="G75" s="10">
-        <v>200</v>
-      </c>
-      <c r="H75" s="9">
-        <v>0.5</v>
-      </c>
-      <c r="I75" s="9">
-        <v>1</v>
-      </c>
-      <c r="J75" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="K75" s="13" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="76" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B76" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="C76" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="D76" s="11">
-        <v>1</v>
-      </c>
-      <c r="E76" s="10">
-        <v>0</v>
-      </c>
-      <c r="F76" s="10">
-        <v>60</v>
-      </c>
-      <c r="G76" s="10">
-        <v>300</v>
-      </c>
-      <c r="H76" s="9">
-        <v>0.5</v>
-      </c>
-      <c r="I76" s="9">
-        <v>1</v>
-      </c>
-      <c r="J76" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="K76" s="13" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="77" spans="2:13" x14ac:dyDescent="0.25">
@@ -5065,19 +5077,19 @@
         <v>1</v>
       </c>
       <c r="C77" s="11" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D77" s="11">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E77" s="10">
         <v>0</v>
       </c>
       <c r="F77" s="10">
-        <v>240</v>
+        <v>15</v>
       </c>
       <c r="G77" s="10">
-        <v>600</v>
+        <v>200</v>
       </c>
       <c r="H77" s="9">
         <v>0.5</v>
@@ -5086,63 +5098,99 @@
         <v>1</v>
       </c>
       <c r="J77" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="K77" s="13" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="78" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B78" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="C78" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D78" s="11">
+        <v>1</v>
+      </c>
+      <c r="E78" s="10">
+        <v>0</v>
+      </c>
+      <c r="F78" s="10">
+        <v>60</v>
+      </c>
+      <c r="G78" s="10">
+        <v>300</v>
+      </c>
+      <c r="H78" s="9">
+        <v>0.5</v>
+      </c>
+      <c r="I78" s="9">
+        <v>1</v>
+      </c>
+      <c r="J78" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="K78" s="13" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="79" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B79" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="C79" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="D79" s="11">
+        <v>2</v>
+      </c>
+      <c r="E79" s="10">
+        <v>0</v>
+      </c>
+      <c r="F79" s="10">
+        <v>240</v>
+      </c>
+      <c r="G79" s="10">
+        <v>600</v>
+      </c>
+      <c r="H79" s="9">
+        <v>0.5</v>
+      </c>
+      <c r="I79" s="9">
+        <v>1</v>
+      </c>
+      <c r="J79" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="K77" s="7" t="s">
+      <c r="K79" s="7" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="79" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="80" spans="2:13" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B80" s="6" t="s">
+    <row r="81" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="82" spans="2:7" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B82" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="C80" s="6"/>
-      <c r="D80" s="6"/>
-      <c r="E80" s="6"/>
-      <c r="F80" s="6"/>
-      <c r="G80" s="6"/>
-    </row>
-    <row r="82" spans="2:7" ht="135.75" x14ac:dyDescent="0.25">
-      <c r="B82" s="5" t="s">
+      <c r="C82" s="6"/>
+      <c r="D82" s="6"/>
+      <c r="E82" s="6"/>
+      <c r="F82" s="6"/>
+      <c r="G82" s="6"/>
+    </row>
+    <row r="84" spans="2:7" ht="135.75" x14ac:dyDescent="0.25">
+      <c r="B84" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="C82" s="4" t="s">
+      <c r="C84" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D82" s="3" t="s">
+      <c r="D84" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E82" s="3" t="s">
+      <c r="E84" s="3" t="s">
         <v>21</v>
-      </c>
-    </row>
-    <row r="83" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B83" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C83" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D83" s="1">
-        <v>0.1</v>
-      </c>
-      <c r="E83" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="84" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B84" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C84" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D84" s="1">
-        <v>0.7</v>
-      </c>
-      <c r="E84" s="1">
-        <v>6</v>
       </c>
     </row>
     <row r="85" spans="2:7" x14ac:dyDescent="0.25">
@@ -5150,13 +5198,13 @@
         <v>1</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D85" s="1">
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="E85" s="1">
-        <v>12</v>
+        <v>2</v>
       </c>
     </row>
     <row r="86" spans="2:7" x14ac:dyDescent="0.25">
@@ -5164,13 +5212,13 @@
         <v>1</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D86" s="1">
-        <v>1.5</v>
+        <v>0.7</v>
       </c>
       <c r="E86" s="1">
-        <v>18</v>
+        <v>6</v>
       </c>
     </row>
     <row r="87" spans="2:7" x14ac:dyDescent="0.25">
@@ -5178,13 +5226,13 @@
         <v>1</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D87" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E87" s="1">
-        <v>26</v>
+        <v>12</v>
       </c>
     </row>
     <row r="88" spans="2:7" x14ac:dyDescent="0.25">
@@ -5192,13 +5240,13 @@
         <v>1</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D88" s="1">
-        <v>2.5</v>
+        <v>1.5</v>
       </c>
       <c r="E88" s="1">
-        <v>35</v>
+        <v>18</v>
       </c>
     </row>
     <row r="89" spans="2:7" x14ac:dyDescent="0.25">
@@ -5206,13 +5254,13 @@
         <v>1</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D89" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E89" s="1">
-        <v>45</v>
+        <v>26</v>
       </c>
     </row>
     <row r="90" spans="2:7" x14ac:dyDescent="0.25">
@@ -5220,13 +5268,13 @@
         <v>1</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D90" s="1">
-        <v>4</v>
+        <v>2.5</v>
       </c>
       <c r="E90" s="1">
-        <v>56</v>
+        <v>35</v>
       </c>
     </row>
     <row r="91" spans="2:7" x14ac:dyDescent="0.25">
@@ -5234,13 +5282,13 @@
         <v>1</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D91" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E91" s="1">
-        <v>67</v>
+        <v>45</v>
       </c>
     </row>
     <row r="92" spans="2:7" x14ac:dyDescent="0.25">
@@ -5248,57 +5296,63 @@
         <v>1</v>
       </c>
       <c r="C92" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D92" s="1">
+        <v>4</v>
+      </c>
+      <c r="E92" s="1">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="93" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B93" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C93" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D93" s="1">
+        <v>5</v>
+      </c>
+      <c r="E93" s="1">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="94" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B94" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C94" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D92" s="1">
-        <v>7</v>
-      </c>
-      <c r="E92" s="1">
+      <c r="D94" s="1">
+        <v>7</v>
+      </c>
+      <c r="E94" s="1">
         <v>80</v>
       </c>
     </row>
-    <row r="93" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="94" spans="2:7" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B94" s="6" t="s">
+    <row r="95" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="96" spans="2:7" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B96" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C94" s="6"/>
-      <c r="D94" s="6"/>
-      <c r="E94" s="6"/>
-      <c r="F94" s="6"/>
-      <c r="G94" s="6"/>
-    </row>
-    <row r="96" spans="2:7" ht="142.5" x14ac:dyDescent="0.25">
-      <c r="B96" s="5" t="s">
+      <c r="C96" s="6"/>
+      <c r="D96" s="6"/>
+      <c r="E96" s="6"/>
+      <c r="F96" s="6"/>
+      <c r="G96" s="6"/>
+    </row>
+    <row r="98" spans="2:7" ht="142.5" x14ac:dyDescent="0.25">
+      <c r="B98" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C96" s="4" t="s">
+      <c r="C98" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D96" s="3" t="s">
+      <c r="D98" s="3" t="s">
         <v>2</v>
-      </c>
-    </row>
-    <row r="97" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B97" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C97" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D97" s="1">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="98" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B98" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C98" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D98" s="1">
-        <v>0.1</v>
       </c>
     </row>
     <row r="99" spans="2:7" x14ac:dyDescent="0.25">
@@ -5306,42 +5360,64 @@
         <v>1</v>
       </c>
       <c r="C99" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D99" s="1">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="100" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B100" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C100" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D100" s="1">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="101" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B101" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C101" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D99" s="1">
+      <c r="D101" s="1">
         <v>0.2</v>
       </c>
     </row>
-    <row r="100" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="101" spans="2:7" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B101" s="6" t="s">
+    <row r="102" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="103" spans="2:7" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B103" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C101" s="6"/>
-      <c r="D101" s="6"/>
-      <c r="E101" s="6"/>
-      <c r="F101" s="6"/>
-      <c r="G101" s="6"/>
-    </row>
-    <row r="103" spans="2:7" ht="132" x14ac:dyDescent="0.25">
-      <c r="B103" s="5" t="s">
+      <c r="C103" s="6"/>
+      <c r="D103" s="6"/>
+      <c r="E103" s="6"/>
+      <c r="F103" s="6"/>
+      <c r="G103" s="6"/>
+    </row>
+    <row r="105" spans="2:7" ht="132" x14ac:dyDescent="0.25">
+      <c r="B105" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C103" s="4" t="s">
+      <c r="C105" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D103" s="3" t="s">
+      <c r="D105" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="104" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B104" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C104" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D104" s="1">
+    <row r="106" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B106" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C106" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D106" s="1">
         <v>0.7</v>
       </c>
     </row>
@@ -5349,11 +5425,11 @@
   <mergeCells count="4">
     <mergeCell ref="J3:K3"/>
     <mergeCell ref="M3:P3"/>
-    <mergeCell ref="F52:H52"/>
-    <mergeCell ref="G73:H73"/>
+    <mergeCell ref="F55:H55"/>
+    <mergeCell ref="G75:H75"/>
   </mergeCells>
-  <conditionalFormatting sqref="C75:D77">
-    <cfRule type="duplicateValues" dxfId="66" priority="1"/>
+  <conditionalFormatting sqref="C77:D79">
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Content - First balancing for the new missions
Former-commit-id: aa9420feaa93797ae9233aa2179a44db7b475360
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Missions.xlsx
+++ b/Docs/Content/HungryDragonContent_Missions.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\dragon\client\Docs\Content\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hsemroud\Documents\Dragon\Docs\Content\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="missions" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913" calcMode="manual"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="441" uniqueCount="223">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="422" uniqueCount="214">
   <si>
     <t>single_run</t>
   </si>
@@ -291,9 +291,6 @@
   </si>
   <si>
     <t>Driller</t>
-  </si>
-  <si>
-    <t>guardian</t>
   </si>
   <si>
     <t>icon_lionbird</t>
@@ -516,15 +513,6 @@
     <t>eat_suicidal_goblins</t>
   </si>
   <si>
-    <t>eat_gold_razorback</t>
-  </si>
-  <si>
-    <t>eat_gold_driller</t>
-  </si>
-  <si>
-    <t>eat_suicidal_cattle</t>
-  </si>
-  <si>
     <t>Sheep; Cow; Horse</t>
   </si>
   <si>
@@ -534,30 +522,6 @@
     <t>Villager01;Villager02</t>
   </si>
   <si>
-    <t>Hawk;OwlSmall;Vulture</t>
-  </si>
-  <si>
-    <t>eat_gold_fishes</t>
-  </si>
-  <si>
-    <t>Fish01_Generic;Fish02_Generic;Fish03_Generic</t>
-  </si>
-  <si>
-    <t>eat_gold_stingrayLarge</t>
-  </si>
-  <si>
-    <t>StingrayLarge</t>
-  </si>
-  <si>
-    <t>Razorback</t>
-  </si>
-  <si>
-    <t>eat_gold_piranha</t>
-  </si>
-  <si>
-    <t>Piranha</t>
-  </si>
-  <si>
     <t>TID_EDIBLE_CANARY_PL</t>
   </si>
   <si>
@@ -618,24 +582,15 @@
     <t>TID_EDIBLE_STINGRAY_PL</t>
   </si>
   <si>
-    <t>TID_EDIBLE_PIRANHA_PL</t>
-  </si>
-  <si>
     <t>TID_EDIBLE_RAZORBACK_PL</t>
   </si>
   <si>
-    <t>TID_EDIBLE_FISH_PL</t>
-  </si>
-  <si>
     <t>TID_MISSION_TARGET_BOATMAN</t>
   </si>
   <si>
     <t>TID_MISSION_TARGET_BIRDSPREY</t>
   </si>
   <si>
-    <t>TID_MISSION_TARGET_CATTLE</t>
-  </si>
-  <si>
     <t>TID_MISSION_OBJECTIVE_KILLCHAIN_DESC_SINGLE_RUN</t>
   </si>
   <si>
@@ -678,9 +633,6 @@
     <t>kill_chain_sheeps</t>
   </si>
   <si>
-    <t>kill_chain_canary_01</t>
-  </si>
-  <si>
     <t>eat_dizzy</t>
   </si>
   <si>
@@ -690,9 +642,6 @@
     <t>destroy_mineSmall</t>
   </si>
   <si>
-    <t>eat_dizzy_gen</t>
-  </si>
-  <si>
     <t>eat_gold_gen</t>
   </si>
   <si>
@@ -717,7 +666,31 @@
     <t>eat_gold_birdsOfPrey</t>
   </si>
   <si>
-    <t>Canary01_Flock</t>
+    <t>eat_gold_stingrays</t>
+  </si>
+  <si>
+    <t>StingraySmall;StingrayLarge</t>
+  </si>
+  <si>
+    <t>kill_chain_humans</t>
+  </si>
+  <si>
+    <t>kill_chain_canaries</t>
+  </si>
+  <si>
+    <t>driller</t>
+  </si>
+  <si>
+    <t>eat_gold_witch</t>
+  </si>
+  <si>
+    <t>Hawk;OwlSmall;OwlBig;Vulture</t>
+  </si>
+  <si>
+    <t>witches</t>
+  </si>
+  <si>
+    <t>GoodWitch;GoodWitch2;BadWitch;Witch</t>
   </si>
 </sst>
 </file>
@@ -1051,7 +1024,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1"/>
@@ -1194,9 +1167,6 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1209,16 +1179,6 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="67">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -2280,6 +2240,16 @@
         </bottom>
       </border>
     </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -2294,94 +2264,94 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="missionDifficultyDefinitions" displayName="missionDifficultyDefinitions" ref="B76:K79" totalsRowShown="0" headerRowBorderDxfId="66" tableBorderDxfId="65">
-  <autoFilter ref="B76:K79"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="missionDifficultyDefinitions" displayName="missionDifficultyDefinitions" ref="B71:K74" totalsRowShown="0" headerRowBorderDxfId="65" tableBorderDxfId="64">
+  <autoFilter ref="B71:K74"/>
   <tableColumns count="10">
     <tableColumn id="1" name="{missionDifficultyDefinitions}"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="64"/>
-    <tableColumn id="7" name="[index]" dataDxfId="63"/>
-    <tableColumn id="3" name="[dragonsToUnlock]" dataDxfId="62"/>
-    <tableColumn id="4" name="[cooldownMinutes]" dataDxfId="61"/>
-    <tableColumn id="9" name="[maxRewardCoins]" dataDxfId="60"/>
-    <tableColumn id="5" name="[removeMissionPCCoefA]" dataDxfId="59"/>
-    <tableColumn id="6" name="[removeMissionPCCoefB]" dataDxfId="58"/>
-    <tableColumn id="8" name="[tidName]" dataDxfId="57"/>
-    <tableColumn id="10" name="[color]" dataDxfId="56"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="63"/>
+    <tableColumn id="7" name="[index]" dataDxfId="62"/>
+    <tableColumn id="3" name="[dragonsToUnlock]" dataDxfId="61"/>
+    <tableColumn id="4" name="[cooldownMinutes]" dataDxfId="60"/>
+    <tableColumn id="9" name="[maxRewardCoins]" dataDxfId="59"/>
+    <tableColumn id="5" name="[removeMissionPCCoefA]" dataDxfId="58"/>
+    <tableColumn id="6" name="[removeMissionPCCoefB]" dataDxfId="57"/>
+    <tableColumn id="8" name="[tidName]" dataDxfId="56"/>
+    <tableColumn id="10" name="[color]" dataDxfId="55"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table13303132" displayName="Table13303132" ref="B84:E94" totalsRowShown="0" headerRowDxfId="55" dataDxfId="53" headerRowBorderDxfId="54" tableBorderDxfId="52" totalsRowBorderDxfId="51">
-  <autoFilter ref="B84:E94"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table13303132" displayName="Table13303132" ref="B79:E89" totalsRowShown="0" headerRowDxfId="54" dataDxfId="52" headerRowBorderDxfId="53" tableBorderDxfId="51" totalsRowBorderDxfId="50">
+  <autoFilter ref="B79:E89"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="{missionDragonModifiersDefinitions}" dataDxfId="50"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="49"/>
-    <tableColumn id="7" name="[quantityModifier]" dataDxfId="48"/>
-    <tableColumn id="3" name="[missionSCRewardMultiplier]" dataDxfId="47"/>
+    <tableColumn id="1" name="{missionDragonModifiersDefinitions}" dataDxfId="49"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="48"/>
+    <tableColumn id="7" name="[quantityModifier]" dataDxfId="47"/>
+    <tableColumn id="3" name="[missionSCRewardMultiplier]" dataDxfId="46"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table1330313234" displayName="Table1330313234" ref="B98:D101" totalsRowShown="0" headerRowDxfId="46" dataDxfId="44" headerRowBorderDxfId="45" tableBorderDxfId="43" totalsRowBorderDxfId="42">
-  <autoFilter ref="B98:D101"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table1330313234" displayName="Table1330313234" ref="B93:D96" totalsRowShown="0" headerRowDxfId="45" dataDxfId="43" headerRowBorderDxfId="44" tableBorderDxfId="42" totalsRowBorderDxfId="41">
+  <autoFilter ref="B93:D96"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="{missionDifficultyModifiersDefinitions}" dataDxfId="41"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="40"/>
-    <tableColumn id="7" name="[quantityModifier]" dataDxfId="39"/>
+    <tableColumn id="1" name="{missionDifficultyModifiersDefinitions}" dataDxfId="40"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="39"/>
+    <tableColumn id="7" name="[quantityModifier]" dataDxfId="38"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table133031323435" displayName="Table133031323435" ref="B105:D106" totalsRowShown="0" headerRowDxfId="38" dataDxfId="36" headerRowBorderDxfId="37" tableBorderDxfId="35" totalsRowBorderDxfId="34">
-  <autoFilter ref="B105:D106"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table133031323435" displayName="Table133031323435" ref="B100:D101" totalsRowShown="0" headerRowDxfId="37" dataDxfId="35" headerRowBorderDxfId="36" tableBorderDxfId="34" totalsRowBorderDxfId="33">
+  <autoFilter ref="B100:D101"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="{missionOtherModifiersDefinitions}" dataDxfId="33"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="32"/>
-    <tableColumn id="7" name="[quantityModifier]" dataDxfId="31"/>
+    <tableColumn id="1" name="{missionOtherModifiersDefinitions}" dataDxfId="32"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="31"/>
+    <tableColumn id="7" name="[quantityModifier]" dataDxfId="30"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table13" displayName="Table13" ref="B56:H72" totalsRowShown="0" headerRowDxfId="30" dataDxfId="28" headerRowBorderDxfId="29" tableBorderDxfId="27" totalsRowBorderDxfId="26">
-  <autoFilter ref="B56:H72"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table13" displayName="Table13" ref="B52:H67" totalsRowShown="0" headerRowDxfId="29" dataDxfId="27" headerRowBorderDxfId="28" tableBorderDxfId="26" totalsRowBorderDxfId="25">
+  <autoFilter ref="B52:H67"/>
   <tableColumns count="7">
-    <tableColumn id="1" name="{missionTypeDefinitions}" dataDxfId="25"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="24"/>
-    <tableColumn id="3" name="[minTier]" dataDxfId="23"/>
-    <tableColumn id="6" name="[maxTier]" dataDxfId="22"/>
-    <tableColumn id="4" name="[weight]" dataDxfId="21"/>
-    <tableColumn id="9" name="[tidDescSingleRun]" dataDxfId="20"/>
-    <tableColumn id="10" name="[tidDescMultiRun]" dataDxfId="19"/>
+    <tableColumn id="1" name="{missionTypeDefinitions}" dataDxfId="24"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="23"/>
+    <tableColumn id="3" name="[minTier]" dataDxfId="22"/>
+    <tableColumn id="6" name="[maxTier]" dataDxfId="21"/>
+    <tableColumn id="4" name="[weight]" dataDxfId="20"/>
+    <tableColumn id="9" name="[tidDescSingleRun]" dataDxfId="19"/>
+    <tableColumn id="10" name="[tidDescMultiRun]" dataDxfId="18"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table1330" displayName="Table1330" ref="B4:N51" totalsRowShown="0" headerRowDxfId="18" dataDxfId="16" headerRowBorderDxfId="17" tableBorderDxfId="15" totalsRowBorderDxfId="14">
-  <autoFilter ref="B4:N51"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table1330" displayName="Table1330" ref="B4:N47" totalsRowShown="0" headerRowDxfId="17" dataDxfId="15" headerRowBorderDxfId="16" tableBorderDxfId="14" totalsRowBorderDxfId="13">
+  <autoFilter ref="B4:N47"/>
   <tableColumns count="13">
-    <tableColumn id="1" name="{missionsDefinitions}" dataDxfId="13"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="12"/>
-    <tableColumn id="7" name="[type]" dataDxfId="11"/>
-    <tableColumn id="8" name="[weight]" dataDxfId="10"/>
-    <tableColumn id="13" name="[singleRunChance]" dataDxfId="9"/>
-    <tableColumn id="11" name="[minTier]" dataDxfId="8"/>
-    <tableColumn id="12" name="[maxTier]" dataDxfId="7"/>
-    <tableColumn id="6" name="[params]" dataDxfId="6"/>
-    <tableColumn id="3" name="[objectiveBaseQuantityMin]" dataDxfId="5"/>
-    <tableColumn id="9" name="[objectiveBaseQuantityMax]" dataDxfId="4"/>
-    <tableColumn id="4" name="[icon]" dataDxfId="3"/>
-    <tableColumn id="5" name="[tidObjective]" dataDxfId="2"/>
-    <tableColumn id="10" name="[trackingSku]" dataDxfId="1"/>
+    <tableColumn id="1" name="{missionsDefinitions}" dataDxfId="12"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="11"/>
+    <tableColumn id="7" name="[type]" dataDxfId="10"/>
+    <tableColumn id="8" name="[weight]" dataDxfId="9"/>
+    <tableColumn id="13" name="[singleRunChance]" dataDxfId="8"/>
+    <tableColumn id="11" name="[minTier]" dataDxfId="7"/>
+    <tableColumn id="12" name="[maxTier]" dataDxfId="6"/>
+    <tableColumn id="6" name="[params]" dataDxfId="5"/>
+    <tableColumn id="3" name="[objectiveBaseQuantityMin]" dataDxfId="4"/>
+    <tableColumn id="9" name="[objectiveBaseQuantityMax]" dataDxfId="3"/>
+    <tableColumn id="4" name="[icon]" dataDxfId="2"/>
+    <tableColumn id="5" name="[tidObjective]" dataDxfId="1"/>
+    <tableColumn id="10" name="[trackingSku]" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2653,21 +2623,21 @@
   <sheetPr>
     <tabColor theme="6"/>
   </sheetPr>
-  <dimension ref="B1:P106"/>
+  <dimension ref="B1:P101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E69" sqref="E69"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G39" sqref="G39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="7" customWidth="1"/>
     <col min="2" max="2" width="18.7109375" customWidth="1"/>
-    <col min="3" max="3" width="21" customWidth="1"/>
+    <col min="3" max="3" width="24.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="6" width="18.7109375" customWidth="1"/>
     <col min="7" max="7" width="42" customWidth="1"/>
     <col min="8" max="8" width="35.5703125" customWidth="1"/>
-    <col min="9" max="9" width="36" customWidth="1"/>
+    <col min="9" max="9" width="59.85546875" bestFit="1" customWidth="1"/>
     <col min="10" max="11" width="18.7109375" customWidth="1"/>
     <col min="12" max="12" width="17.140625" customWidth="1"/>
     <col min="13" max="13" width="26.140625" customWidth="1"/>
@@ -2678,7 +2648,7 @@
     <row r="1" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:16" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B2" s="6" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C2" s="6"/>
       <c r="D2" s="6"/>
@@ -2696,36 +2666,36 @@
       <c r="C3" s="38"/>
       <c r="D3" s="38"/>
       <c r="E3" s="39" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="F3" s="39" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G3" s="38"/>
-      <c r="J3" s="57" t="s">
-        <v>144</v>
-      </c>
-      <c r="K3" s="57"/>
-      <c r="M3" s="57"/>
-      <c r="N3" s="57"/>
-      <c r="O3" s="57"/>
-      <c r="P3" s="57"/>
+      <c r="J3" s="56" t="s">
+        <v>143</v>
+      </c>
+      <c r="K3" s="56"/>
+      <c r="M3" s="56"/>
+      <c r="N3" s="56"/>
+      <c r="O3" s="56"/>
+      <c r="P3" s="56"/>
     </row>
     <row r="4" spans="2:16" ht="106.5" x14ac:dyDescent="0.25">
       <c r="B4" s="30" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C4" s="28" t="s">
         <v>3</v>
       </c>
       <c r="D4" s="37" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E4" s="37" t="s">
         <v>68</v>
       </c>
       <c r="F4" s="37" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="G4" s="37" t="s">
         <v>70</v>
@@ -2734,22 +2704,22 @@
         <v>69</v>
       </c>
       <c r="I4" s="37" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="J4" s="37" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="K4" s="37" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="L4" s="36" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="M4" s="36" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="N4" s="35" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="5" spans="2:16" x14ac:dyDescent="0.25">
@@ -2757,7 +2727,7 @@
         <v>1</v>
       </c>
       <c r="C5" s="24" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D5" s="24" t="s">
         <v>65</v>
@@ -2775,7 +2745,7 @@
         <v>7</v>
       </c>
       <c r="I5" s="24" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="J5" s="24">
         <v>500</v>
@@ -2784,10 +2754,10 @@
         <v>600</v>
       </c>
       <c r="L5" s="33" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="M5" s="33" t="s">
-        <v>169</v>
+        <v>157</v>
       </c>
       <c r="N5" s="31" t="s">
         <v>73</v>
@@ -2798,7 +2768,7 @@
         <v>1</v>
       </c>
       <c r="C6" s="24" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D6" s="23" t="s">
         <v>53</v>
@@ -2823,7 +2793,7 @@
         <v>600</v>
       </c>
       <c r="L6" s="33" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="M6" s="33"/>
       <c r="N6" s="31" t="s">
@@ -2835,7 +2805,7 @@
         <v>1</v>
       </c>
       <c r="C7" s="24" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D7" s="24" t="s">
         <v>59</v>
@@ -2860,7 +2830,7 @@
         <v>10000</v>
       </c>
       <c r="L7" s="33" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="M7" s="33"/>
       <c r="N7" s="31" t="s">
@@ -2872,7 +2842,7 @@
         <v>1</v>
       </c>
       <c r="C8" s="24" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D8" s="24" t="s">
         <v>65</v>
@@ -2890,7 +2860,7 @@
         <v>7</v>
       </c>
       <c r="I8" s="24" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="J8" s="24">
         <v>700</v>
@@ -2899,10 +2869,10 @@
         <v>750</v>
       </c>
       <c r="L8" s="33" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="M8" s="33" t="s">
-        <v>169</v>
+        <v>157</v>
       </c>
       <c r="N8" s="31" t="s">
         <v>73</v>
@@ -2913,7 +2883,7 @@
         <v>1</v>
       </c>
       <c r="C9" s="24" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D9" s="24" t="s">
         <v>65</v>
@@ -2931,7 +2901,7 @@
         <v>7</v>
       </c>
       <c r="I9" s="24" t="s">
-        <v>170</v>
+        <v>158</v>
       </c>
       <c r="J9" s="24">
         <v>25</v>
@@ -2940,10 +2910,10 @@
         <v>30</v>
       </c>
       <c r="L9" s="33" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="M9" s="47" t="s">
-        <v>171</v>
+        <v>159</v>
       </c>
       <c r="N9" s="31" t="s">
         <v>73</v>
@@ -2954,7 +2924,7 @@
         <v>1</v>
       </c>
       <c r="C10" s="24" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D10" s="23" t="s">
         <v>56</v>
@@ -2972,7 +2942,7 @@
         <v>3</v>
       </c>
       <c r="I10" s="23" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="J10" s="24">
         <v>10</v>
@@ -2981,10 +2951,10 @@
         <v>12</v>
       </c>
       <c r="L10" s="33" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="M10" s="47" t="s">
-        <v>172</v>
+        <v>160</v>
       </c>
       <c r="N10" s="31" t="s">
         <v>73</v>
@@ -2995,7 +2965,7 @@
         <v>1</v>
       </c>
       <c r="C11" s="24" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D11" s="23" t="s">
         <v>56</v>
@@ -3013,7 +2983,7 @@
         <v>7</v>
       </c>
       <c r="I11" s="23" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="J11" s="24">
         <v>8</v>
@@ -3022,10 +2992,10 @@
         <v>9</v>
       </c>
       <c r="L11" s="33" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="M11" s="47" t="s">
-        <v>172</v>
+        <v>160</v>
       </c>
       <c r="N11" s="31" t="s">
         <v>73</v>
@@ -3036,7 +3006,7 @@
         <v>1</v>
       </c>
       <c r="C12" s="24" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D12" s="24" t="s">
         <v>50</v>
@@ -3054,7 +3024,7 @@
         <v>7</v>
       </c>
       <c r="I12" s="24" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="J12" s="24">
         <v>1000</v>
@@ -3063,10 +3033,10 @@
         <v>1200</v>
       </c>
       <c r="L12" s="33" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="M12" s="33" t="s">
-        <v>174</v>
+        <v>162</v>
       </c>
       <c r="N12" s="31" t="s">
         <v>73</v>
@@ -3077,7 +3047,7 @@
         <v>1</v>
       </c>
       <c r="C13" s="23" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D13" s="24" t="s">
         <v>50</v>
@@ -3095,7 +3065,7 @@
         <v>1</v>
       </c>
       <c r="I13" s="23" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="J13" s="24">
         <v>1</v>
@@ -3104,10 +3074,10 @@
         <v>2</v>
       </c>
       <c r="L13" s="33" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="M13" s="33" t="s">
-        <v>175</v>
+        <v>163</v>
       </c>
       <c r="N13" s="31" t="s">
         <v>73</v>
@@ -3118,7 +3088,7 @@
         <v>1</v>
       </c>
       <c r="C14" s="24" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D14" s="24" t="s">
         <v>65</v>
@@ -3136,7 +3106,7 @@
         <v>7</v>
       </c>
       <c r="I14" s="24" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="J14" s="24">
         <v>10</v>
@@ -3145,10 +3115,10 @@
         <v>11</v>
       </c>
       <c r="L14" s="33" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="M14" s="47" t="s">
-        <v>176</v>
+        <v>164</v>
       </c>
       <c r="N14" s="31" t="s">
         <v>73</v>
@@ -3159,7 +3129,7 @@
         <v>1</v>
       </c>
       <c r="C15" s="24" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D15" s="24" t="s">
         <v>62</v>
@@ -3184,7 +3154,7 @@
         <v>6</v>
       </c>
       <c r="L15" s="33" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="M15" s="33"/>
       <c r="N15" s="31" t="s">
@@ -3208,7 +3178,7 @@
         <v>0</v>
       </c>
       <c r="G16" s="24">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H16" s="24">
         <v>7</v>
@@ -3221,7 +3191,7 @@
         <v>800</v>
       </c>
       <c r="L16" s="33" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="M16" s="33"/>
       <c r="N16" s="31" t="s">
@@ -3258,7 +3228,7 @@
         <v>400</v>
       </c>
       <c r="L17" s="33" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="M17" s="33"/>
       <c r="N17" s="31" t="s">
@@ -3295,7 +3265,7 @@
         <v>500000</v>
       </c>
       <c r="L18" s="33" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="M18" s="33"/>
       <c r="N18" s="31" t="s">
@@ -3307,7 +3277,7 @@
         <v>1</v>
       </c>
       <c r="C19" s="23" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D19" s="23" t="s">
         <v>65</v>
@@ -3325,7 +3295,7 @@
         <v>7</v>
       </c>
       <c r="I19" s="23" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="J19" s="24">
         <v>45</v>
@@ -3334,10 +3304,10 @@
         <v>55</v>
       </c>
       <c r="L19" s="34" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="M19" s="47" t="s">
-        <v>178</v>
+        <v>166</v>
       </c>
       <c r="N19" s="31" t="s">
         <v>73</v>
@@ -3348,7 +3318,7 @@
         <v>1</v>
       </c>
       <c r="C20" s="23" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D20" s="23" t="s">
         <v>65</v>
@@ -3366,7 +3336,7 @@
         <v>7</v>
       </c>
       <c r="I20" s="23" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="J20" s="24">
         <v>40</v>
@@ -3375,10 +3345,10 @@
         <v>45</v>
       </c>
       <c r="L20" s="34" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="M20" s="33" t="s">
-        <v>177</v>
+        <v>165</v>
       </c>
       <c r="N20" s="31" t="s">
         <v>73</v>
@@ -3389,7 +3359,7 @@
         <v>1</v>
       </c>
       <c r="C21" s="23" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D21" s="23" t="s">
         <v>65</v>
@@ -3407,7 +3377,7 @@
         <v>2</v>
       </c>
       <c r="I21" s="23" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="J21" s="23">
         <v>10</v>
@@ -3416,10 +3386,10 @@
         <v>12</v>
       </c>
       <c r="L21" s="34" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="M21" s="50" t="s">
-        <v>173</v>
+        <v>161</v>
       </c>
       <c r="N21" s="31" t="s">
         <v>73</v>
@@ -3430,7 +3400,7 @@
         <v>1</v>
       </c>
       <c r="C22" s="24" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D22" s="23" t="s">
         <v>65</v>
@@ -3448,7 +3418,7 @@
         <v>1</v>
       </c>
       <c r="I22" s="23" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="J22" s="24">
         <v>5</v>
@@ -3457,10 +3427,10 @@
         <v>6</v>
       </c>
       <c r="L22" s="34" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="M22" s="34" t="s">
-        <v>179</v>
+        <v>167</v>
       </c>
       <c r="N22" s="31" t="s">
         <v>73</v>
@@ -3471,7 +3441,7 @@
         <v>1</v>
       </c>
       <c r="C23" s="24" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D23" s="23" t="s">
         <v>65</v>
@@ -3489,7 +3459,7 @@
         <v>7</v>
       </c>
       <c r="I23" s="23" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="J23" s="24">
         <v>150</v>
@@ -3498,10 +3468,10 @@
         <v>200</v>
       </c>
       <c r="L23" s="34" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="M23" s="50" t="s">
-        <v>180</v>
+        <v>168</v>
       </c>
       <c r="N23" s="31" t="s">
         <v>73</v>
@@ -3512,7 +3482,7 @@
         <v>1</v>
       </c>
       <c r="C24" s="24" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D24" s="23" t="s">
         <v>65</v>
@@ -3530,7 +3500,7 @@
         <v>7</v>
       </c>
       <c r="I24" s="23" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="J24" s="24">
         <v>5</v>
@@ -3539,10 +3509,10 @@
         <v>7</v>
       </c>
       <c r="L24" s="34" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="M24" s="51" t="s">
-        <v>181</v>
+        <v>169</v>
       </c>
       <c r="N24" s="31" t="s">
         <v>73</v>
@@ -3553,7 +3523,7 @@
         <v>1</v>
       </c>
       <c r="C25" s="24" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D25" s="23" t="s">
         <v>65</v>
@@ -3571,7 +3541,7 @@
         <v>7</v>
       </c>
       <c r="I25" s="23" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="J25" s="24">
         <v>5</v>
@@ -3580,10 +3550,10 @@
         <v>7</v>
       </c>
       <c r="L25" s="34" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="M25" s="34" t="s">
-        <v>182</v>
+        <v>170</v>
       </c>
       <c r="N25" s="31" t="s">
         <v>73</v>
@@ -3594,7 +3564,7 @@
         <v>1</v>
       </c>
       <c r="C26" s="24" t="s">
-        <v>89</v>
+        <v>209</v>
       </c>
       <c r="D26" s="23" t="s">
         <v>65</v>
@@ -3624,7 +3594,7 @@
         <v>87</v>
       </c>
       <c r="M26" s="34" t="s">
-        <v>183</v>
+        <v>171</v>
       </c>
       <c r="N26" s="31" t="s">
         <v>73</v>
@@ -3665,7 +3635,7 @@
         <v>84</v>
       </c>
       <c r="M27" s="34" t="s">
-        <v>192</v>
+        <v>178</v>
       </c>
       <c r="N27" s="31" t="s">
         <v>73</v>
@@ -3706,7 +3676,7 @@
         <v>81</v>
       </c>
       <c r="M28" s="34" t="s">
-        <v>184</v>
+        <v>172</v>
       </c>
       <c r="N28" s="31" t="s">
         <v>73</v>
@@ -3747,7 +3717,7 @@
         <v>78</v>
       </c>
       <c r="M29" s="34" t="s">
-        <v>185</v>
+        <v>173</v>
       </c>
       <c r="N29" s="31" t="s">
         <v>73</v>
@@ -3788,7 +3758,7 @@
         <v>75</v>
       </c>
       <c r="M30" s="34" t="s">
-        <v>186</v>
+        <v>174</v>
       </c>
       <c r="N30" s="31" t="s">
         <v>73</v>
@@ -3831,44 +3801,44 @@
         <v>73</v>
       </c>
     </row>
-    <row r="32" spans="2:14" s="43" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="52" t="s">
-        <v>1</v>
-      </c>
-      <c r="C32" s="53" t="s">
-        <v>208</v>
-      </c>
-      <c r="D32" s="54" t="s">
-        <v>207</v>
-      </c>
-      <c r="E32" s="54">
-        <v>1</v>
-      </c>
-      <c r="F32" s="54">
+    <row r="32" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B32" s="27" t="s">
+        <v>1</v>
+      </c>
+      <c r="C32" s="24" t="s">
+        <v>212</v>
+      </c>
+      <c r="D32" s="23" t="s">
+        <v>65</v>
+      </c>
+      <c r="E32" s="23">
+        <v>1</v>
+      </c>
+      <c r="F32" s="24">
         <v>0.3</v>
       </c>
-      <c r="G32" s="53">
-        <v>0</v>
-      </c>
-      <c r="H32" s="54">
-        <v>7</v>
-      </c>
-      <c r="I32" s="54" t="s">
-        <v>149</v>
-      </c>
-      <c r="J32" s="53">
-        <v>99</v>
-      </c>
-      <c r="K32" s="54">
-        <v>99</v>
-      </c>
-      <c r="L32" s="48" t="s">
-        <v>130</v>
-      </c>
-      <c r="M32" s="48" t="s">
-        <v>187</v>
-      </c>
-      <c r="N32" s="55" t="s">
+      <c r="G32" s="24">
+        <v>1</v>
+      </c>
+      <c r="H32" s="34">
+        <v>7</v>
+      </c>
+      <c r="I32" s="23" t="s">
+        <v>213</v>
+      </c>
+      <c r="J32" s="24">
+        <v>10</v>
+      </c>
+      <c r="K32" s="23">
+        <v>12</v>
+      </c>
+      <c r="L32" s="33" t="s">
+        <v>81</v>
+      </c>
+      <c r="M32" s="33" t="s">
+        <v>172</v>
+      </c>
+      <c r="N32" s="31" t="s">
         <v>73</v>
       </c>
     </row>
@@ -3877,37 +3847,37 @@
         <v>1</v>
       </c>
       <c r="C33" s="53" t="s">
-        <v>209</v>
+        <v>193</v>
       </c>
       <c r="D33" s="54" t="s">
-        <v>207</v>
+        <v>192</v>
       </c>
       <c r="E33" s="54">
         <v>1</v>
       </c>
       <c r="F33" s="54">
-        <v>0.3</v>
+        <v>1</v>
       </c>
       <c r="G33" s="53">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H33" s="54">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="I33" s="54" t="s">
-        <v>222</v>
+        <v>148</v>
       </c>
       <c r="J33" s="53">
-        <v>99</v>
+        <v>10</v>
       </c>
       <c r="K33" s="54">
-        <v>99</v>
+        <v>11</v>
       </c>
       <c r="L33" s="48" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="M33" s="48" t="s">
-        <v>203</v>
+        <v>175</v>
       </c>
       <c r="N33" s="55" t="s">
         <v>73</v>
@@ -3918,37 +3888,37 @@
         <v>1</v>
       </c>
       <c r="C34" s="53" t="s">
-        <v>205</v>
+        <v>208</v>
       </c>
       <c r="D34" s="54" t="s">
-        <v>204</v>
+        <v>192</v>
       </c>
       <c r="E34" s="54">
         <v>1</v>
       </c>
       <c r="F34" s="54">
-        <v>0.3</v>
+        <v>1</v>
       </c>
       <c r="G34" s="53">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H34" s="54">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="I34" s="54" t="s">
+        <v>130</v>
+      </c>
+      <c r="J34" s="53">
         <v>150</v>
       </c>
-      <c r="J34" s="53">
-        <v>99</v>
-      </c>
       <c r="K34" s="54">
-        <v>99</v>
+        <v>160</v>
       </c>
       <c r="L34" s="48" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="M34" s="48" t="s">
-        <v>178</v>
+        <v>188</v>
       </c>
       <c r="N34" s="55" t="s">
         <v>73</v>
@@ -3959,34 +3929,38 @@
         <v>1</v>
       </c>
       <c r="C35" s="53" t="s">
-        <v>214</v>
+        <v>207</v>
       </c>
       <c r="D35" s="54" t="s">
-        <v>151</v>
+        <v>192</v>
       </c>
       <c r="E35" s="54">
         <v>1</v>
       </c>
       <c r="F35" s="54">
-        <v>0.3</v>
+        <v>1</v>
       </c>
       <c r="G35" s="53">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H35" s="54">
-        <v>7</v>
-      </c>
-      <c r="I35" s="54"/>
+        <v>2</v>
+      </c>
+      <c r="I35" s="54" t="s">
+        <v>158</v>
+      </c>
       <c r="J35" s="53">
-        <v>99</v>
+        <v>15</v>
       </c>
       <c r="K35" s="54">
-        <v>99</v>
+        <v>16</v>
       </c>
       <c r="L35" s="48" t="s">
-        <v>130</v>
-      </c>
-      <c r="M35" s="49"/>
+        <v>129</v>
+      </c>
+      <c r="M35" s="48" t="s">
+        <v>188</v>
+      </c>
       <c r="N35" s="55" t="s">
         <v>73</v>
       </c>
@@ -3996,10 +3970,10 @@
         <v>1</v>
       </c>
       <c r="C36" s="53" t="s">
-        <v>164</v>
+        <v>190</v>
       </c>
       <c r="D36" s="54" t="s">
-        <v>151</v>
+        <v>189</v>
       </c>
       <c r="E36" s="54">
         <v>1</v>
@@ -4008,25 +3982,25 @@
         <v>0.3</v>
       </c>
       <c r="G36" s="53">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="H36" s="54">
         <v>7</v>
       </c>
       <c r="I36" s="54" t="s">
-        <v>165</v>
+        <v>149</v>
       </c>
       <c r="J36" s="53">
-        <v>99</v>
+        <v>8</v>
       </c>
       <c r="K36" s="54">
-        <v>99</v>
+        <v>9</v>
       </c>
       <c r="L36" s="48" t="s">
-        <v>130</v>
-      </c>
-      <c r="M36" s="54" t="s">
-        <v>188</v>
+        <v>129</v>
+      </c>
+      <c r="M36" s="48" t="s">
+        <v>166</v>
       </c>
       <c r="N36" s="55" t="s">
         <v>73</v>
@@ -4037,10 +4011,10 @@
         <v>1</v>
       </c>
       <c r="C37" s="53" t="s">
-        <v>167</v>
+        <v>197</v>
       </c>
       <c r="D37" s="54" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E37" s="54">
         <v>1</v>
@@ -4049,26 +4023,22 @@
         <v>0.3</v>
       </c>
       <c r="G37" s="53">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H37" s="54">
         <v>7</v>
       </c>
-      <c r="I37" s="54" t="s">
-        <v>168</v>
-      </c>
+      <c r="I37" s="54"/>
       <c r="J37" s="53">
-        <v>99</v>
+        <v>80</v>
       </c>
       <c r="K37" s="54">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="L37" s="48" t="s">
-        <v>130</v>
-      </c>
-      <c r="M37" s="54" t="s">
-        <v>189</v>
-      </c>
+        <v>129</v>
+      </c>
+      <c r="M37" s="49"/>
       <c r="N37" s="55" t="s">
         <v>73</v>
       </c>
@@ -4078,10 +4048,10 @@
         <v>1</v>
       </c>
       <c r="C38" s="53" t="s">
-        <v>155</v>
+        <v>205</v>
       </c>
       <c r="D38" s="54" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E38" s="54">
         <v>1</v>
@@ -4090,25 +4060,25 @@
         <v>0.3</v>
       </c>
       <c r="G38" s="53">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H38" s="54">
         <v>7</v>
       </c>
       <c r="I38" s="54" t="s">
-        <v>166</v>
+        <v>206</v>
       </c>
       <c r="J38" s="53">
-        <v>99</v>
+        <v>5</v>
       </c>
       <c r="K38" s="54">
-        <v>99</v>
+        <v>7</v>
       </c>
       <c r="L38" s="48" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="M38" s="54" t="s">
-        <v>190</v>
+        <v>176</v>
       </c>
       <c r="N38" s="55" t="s">
         <v>73</v>
@@ -4119,10 +4089,10 @@
         <v>1</v>
       </c>
       <c r="C39" s="53" t="s">
-        <v>156</v>
+        <v>210</v>
       </c>
       <c r="D39" s="54" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E39" s="54">
         <v>1</v>
@@ -4131,25 +4101,25 @@
         <v>0.3</v>
       </c>
       <c r="G39" s="53">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H39" s="54">
         <v>7</v>
       </c>
       <c r="I39" s="54" t="s">
-        <v>88</v>
+        <v>213</v>
       </c>
       <c r="J39" s="53">
-        <v>99</v>
+        <v>5</v>
       </c>
       <c r="K39" s="54">
-        <v>99</v>
+        <v>7</v>
       </c>
       <c r="L39" s="48" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="M39" s="54" t="s">
-        <v>183</v>
+        <v>177</v>
       </c>
       <c r="N39" s="55" t="s">
         <v>73</v>
@@ -4160,10 +4130,10 @@
         <v>1</v>
       </c>
       <c r="C40" s="53" t="s">
-        <v>162</v>
+        <v>204</v>
       </c>
       <c r="D40" s="54" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E40" s="54">
         <v>1</v>
@@ -4172,25 +4142,25 @@
         <v>0.3</v>
       </c>
       <c r="G40" s="53">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H40" s="54">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="I40" s="54" t="s">
-        <v>163</v>
+        <v>211</v>
       </c>
       <c r="J40" s="53">
-        <v>99</v>
+        <v>30</v>
       </c>
       <c r="K40" s="54">
-        <v>99</v>
+        <v>35</v>
       </c>
       <c r="L40" s="48" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="M40" s="49" t="s">
-        <v>191</v>
+        <v>179</v>
       </c>
       <c r="N40" s="55" t="s">
         <v>73</v>
@@ -4201,10 +4171,10 @@
         <v>1</v>
       </c>
       <c r="C41" s="53" t="s">
-        <v>221</v>
+        <v>201</v>
       </c>
       <c r="D41" s="54" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E41" s="54">
         <v>1</v>
@@ -4213,39 +4183,33 @@
         <v>0.3</v>
       </c>
       <c r="G41" s="53">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H41" s="54">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="I41" s="54" t="s">
-        <v>161</v>
+        <v>130</v>
       </c>
       <c r="J41" s="53">
-        <v>99</v>
+        <v>30</v>
       </c>
       <c r="K41" s="54">
-        <v>99</v>
-      </c>
-      <c r="L41" s="48" t="s">
-        <v>130</v>
-      </c>
-      <c r="M41" s="49" t="s">
-        <v>193</v>
-      </c>
-      <c r="N41" s="55" t="s">
-        <v>73</v>
-      </c>
+        <v>35</v>
+      </c>
+      <c r="L41" s="48"/>
+      <c r="M41" s="48"/>
+      <c r="N41" s="55"/>
     </row>
     <row r="42" spans="2:14" s="43" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B42" s="52" t="s">
         <v>1</v>
       </c>
       <c r="C42" s="53" t="s">
-        <v>218</v>
+        <v>203</v>
       </c>
       <c r="D42" s="54" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E42" s="54">
         <v>1</v>
@@ -4254,16 +4218,20 @@
         <v>0.3</v>
       </c>
       <c r="G42" s="53">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H42" s="54">
         <v>7</v>
       </c>
       <c r="I42" s="54" t="s">
-        <v>131</v>
-      </c>
-      <c r="J42" s="53"/>
-      <c r="K42" s="54"/>
+        <v>154</v>
+      </c>
+      <c r="J42" s="53">
+        <v>10</v>
+      </c>
+      <c r="K42" s="54">
+        <v>12</v>
+      </c>
       <c r="L42" s="48"/>
       <c r="M42" s="48"/>
       <c r="N42" s="55"/>
@@ -4273,10 +4241,10 @@
         <v>1</v>
       </c>
       <c r="C43" s="53" t="s">
-        <v>220</v>
+        <v>202</v>
       </c>
       <c r="D43" s="54" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E43" s="54">
         <v>1</v>
@@ -4291,10 +4259,14 @@
         <v>7</v>
       </c>
       <c r="I43" s="54" t="s">
-        <v>158</v>
-      </c>
-      <c r="J43" s="53"/>
-      <c r="K43" s="54"/>
+        <v>105</v>
+      </c>
+      <c r="J43" s="53">
+        <v>10</v>
+      </c>
+      <c r="K43" s="54">
+        <v>12</v>
+      </c>
       <c r="L43" s="48"/>
       <c r="M43" s="48"/>
       <c r="N43" s="55"/>
@@ -4304,7 +4276,7 @@
         <v>1</v>
       </c>
       <c r="C44" s="53" t="s">
-        <v>219</v>
+        <v>153</v>
       </c>
       <c r="D44" s="54" t="s">
         <v>151</v>
@@ -4316,29 +4288,39 @@
         <v>0.3</v>
       </c>
       <c r="G44" s="53">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H44" s="54">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="I44" s="54" t="s">
-        <v>106</v>
-      </c>
-      <c r="J44" s="53"/>
-      <c r="K44" s="54"/>
-      <c r="L44" s="48"/>
-      <c r="M44" s="48"/>
-      <c r="N44" s="55"/>
+        <v>152</v>
+      </c>
+      <c r="J44" s="53">
+        <v>5</v>
+      </c>
+      <c r="K44" s="54">
+        <v>6</v>
+      </c>
+      <c r="L44" s="48" t="s">
+        <v>129</v>
+      </c>
+      <c r="M44" s="49" t="s">
+        <v>165</v>
+      </c>
+      <c r="N44" s="55" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="45" spans="2:14" s="43" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B45" s="52" t="s">
         <v>1</v>
       </c>
       <c r="C45" s="53" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="D45" s="54" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="E45" s="54">
         <v>1</v>
@@ -4350,22 +4332,22 @@
         <v>1</v>
       </c>
       <c r="H45" s="54">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="I45" s="54" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="J45" s="53">
-        <v>99</v>
+        <v>5</v>
       </c>
       <c r="K45" s="54">
-        <v>99</v>
+        <v>6</v>
       </c>
       <c r="L45" s="48" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="M45" s="49" t="s">
-        <v>177</v>
+        <v>159</v>
       </c>
       <c r="N45" s="55" t="s">
         <v>73</v>
@@ -4375,39 +4357,35 @@
       <c r="B46" s="52" t="s">
         <v>1</v>
       </c>
-      <c r="C46" s="53" t="s">
-        <v>159</v>
-      </c>
-      <c r="D46" s="54" t="s">
-        <v>152</v>
+      <c r="C46" s="40" t="s">
+        <v>191</v>
+      </c>
+      <c r="D46" s="40" t="s">
+        <v>191</v>
       </c>
       <c r="E46" s="54">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F46" s="54">
-        <v>0.3</v>
+        <v>1</v>
       </c>
       <c r="G46" s="53">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H46" s="54">
         <v>7</v>
       </c>
-      <c r="I46" s="54" t="s">
-        <v>160</v>
-      </c>
+      <c r="I46" s="54"/>
       <c r="J46" s="53">
-        <v>99</v>
+        <v>25</v>
       </c>
       <c r="K46" s="54">
-        <v>99</v>
+        <v>27</v>
       </c>
       <c r="L46" s="48" t="s">
-        <v>130</v>
-      </c>
-      <c r="M46" s="49" t="s">
-        <v>171</v>
-      </c>
+        <v>129</v>
+      </c>
+      <c r="M46" s="49"/>
       <c r="N46" s="55" t="s">
         <v>73</v>
       </c>
@@ -4416,276 +4394,238 @@
       <c r="B47" s="52" t="s">
         <v>1</v>
       </c>
-      <c r="C47" s="53" t="s">
-        <v>157</v>
-      </c>
-      <c r="D47" s="54" t="s">
-        <v>152</v>
+      <c r="C47" s="40" t="s">
+        <v>196</v>
+      </c>
+      <c r="D47" s="40" t="s">
+        <v>195</v>
       </c>
       <c r="E47" s="54">
         <v>1</v>
       </c>
       <c r="F47" s="54">
-        <v>0.3</v>
+        <v>1</v>
       </c>
       <c r="G47" s="53">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H47" s="54">
         <v>7</v>
       </c>
-      <c r="I47" s="54" t="s">
-        <v>158</v>
-      </c>
+      <c r="I47" s="41"/>
       <c r="J47" s="53">
-        <v>99</v>
+        <v>20</v>
       </c>
       <c r="K47" s="54">
-        <v>99</v>
+        <v>22</v>
       </c>
       <c r="L47" s="48" t="s">
-        <v>130</v>
-      </c>
-      <c r="M47" s="49" t="s">
-        <v>194</v>
-      </c>
+        <v>129</v>
+      </c>
+      <c r="M47" s="41"/>
       <c r="N47" s="55" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="48" spans="2:14" s="43" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B48" s="52" t="s">
-        <v>1</v>
-      </c>
-      <c r="C48" s="40" t="s">
-        <v>206</v>
-      </c>
-      <c r="D48" s="40" t="s">
-        <v>206</v>
-      </c>
-      <c r="E48" s="54">
+      <c r="B48" s="44"/>
+      <c r="C48" s="44"/>
+      <c r="D48" s="44"/>
+      <c r="E48" s="44"/>
+      <c r="F48" s="44"/>
+      <c r="G48" s="44"/>
+      <c r="H48" s="44"/>
+      <c r="I48" s="44"/>
+      <c r="J48" s="44"/>
+      <c r="K48" s="44"/>
+      <c r="L48" s="44"/>
+      <c r="M48" s="44"/>
+      <c r="N48" s="44"/>
+    </row>
+    <row r="49" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B49" s="32"/>
+      <c r="C49" s="32"/>
+      <c r="D49" s="32"/>
+      <c r="E49" s="32"/>
+      <c r="F49" s="32"/>
+      <c r="G49" s="32"/>
+      <c r="H49" s="32"/>
+      <c r="I49" s="32"/>
+      <c r="J49" s="32"/>
+      <c r="K49" s="32"/>
+      <c r="L49" s="32"/>
+      <c r="M49" s="31"/>
+    </row>
+    <row r="50" spans="2:13" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B50" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="C50" s="6"/>
+      <c r="D50" s="6"/>
+      <c r="E50" s="6"/>
+      <c r="F50" s="6"/>
+      <c r="G50" s="6"/>
+      <c r="H50" s="6"/>
+      <c r="I50" s="6"/>
+      <c r="J50" s="6"/>
+      <c r="K50" s="6"/>
+      <c r="L50" s="6"/>
+    </row>
+    <row r="51" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B51" s="20"/>
+      <c r="C51" s="20"/>
+      <c r="D51" s="20"/>
+      <c r="E51" s="20"/>
+      <c r="F51" s="57"/>
+      <c r="G51" s="57"/>
+      <c r="H51" s="57"/>
+      <c r="I51" s="20"/>
+      <c r="J51" s="20"/>
+    </row>
+    <row r="52" spans="2:13" ht="96" x14ac:dyDescent="0.25">
+      <c r="B52" s="30" t="s">
+        <v>71</v>
+      </c>
+      <c r="C52" s="28" t="s">
+        <v>3</v>
+      </c>
+      <c r="D52" s="29" t="s">
+        <v>70</v>
+      </c>
+      <c r="E52" s="29" t="s">
+        <v>69</v>
+      </c>
+      <c r="F52" s="29" t="s">
+        <v>68</v>
+      </c>
+      <c r="G52" s="28" t="s">
+        <v>67</v>
+      </c>
+      <c r="H52" s="28" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="53" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B53" s="27" t="s">
+        <v>1</v>
+      </c>
+      <c r="C53" s="24" t="s">
+        <v>65</v>
+      </c>
+      <c r="D53" s="24">
         <v>0</v>
       </c>
-      <c r="F48" s="54">
+      <c r="E53" s="24">
+        <v>7</v>
+      </c>
+      <c r="F53" s="24">
+        <v>2</v>
+      </c>
+      <c r="G53" s="26" t="s">
+        <v>64</v>
+      </c>
+      <c r="H53" s="26" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="54" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B54" s="27" t="s">
+        <v>1</v>
+      </c>
+      <c r="C54" s="24" t="s">
+        <v>62</v>
+      </c>
+      <c r="D54" s="24">
         <v>0</v>
       </c>
-      <c r="G48" s="53">
+      <c r="E54" s="24">
+        <v>7</v>
+      </c>
+      <c r="F54" s="24">
+        <v>1</v>
+      </c>
+      <c r="G54" s="26" t="s">
+        <v>61</v>
+      </c>
+      <c r="H54" s="26" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="55" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B55" s="27" t="s">
+        <v>1</v>
+      </c>
+      <c r="C55" s="24" t="s">
+        <v>59</v>
+      </c>
+      <c r="D55" s="24">
         <v>0</v>
       </c>
-      <c r="H48" s="54">
-        <v>7</v>
-      </c>
-      <c r="I48" s="54"/>
-      <c r="J48" s="53">
-        <v>99</v>
-      </c>
-      <c r="K48" s="54">
-        <v>99</v>
-      </c>
-      <c r="L48" s="48" t="s">
-        <v>130</v>
-      </c>
-      <c r="M48" s="49"/>
-      <c r="N48" s="55" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="49" spans="2:14" s="43" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B49" s="52" t="s">
-        <v>1</v>
-      </c>
-      <c r="C49" s="40" t="s">
-        <v>213</v>
-      </c>
-      <c r="D49" s="40" t="s">
-        <v>210</v>
-      </c>
-      <c r="E49" s="54">
-        <v>1</v>
-      </c>
-      <c r="F49" s="54">
-        <v>0.3</v>
-      </c>
-      <c r="G49" s="53">
+      <c r="E55" s="24">
+        <v>7</v>
+      </c>
+      <c r="F55" s="24">
+        <v>2</v>
+      </c>
+      <c r="G55" s="26" t="s">
+        <v>58</v>
+      </c>
+      <c r="H55" s="26" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="56" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B56" s="27" t="s">
+        <v>1</v>
+      </c>
+      <c r="C56" s="24" t="s">
+        <v>56</v>
+      </c>
+      <c r="D56" s="24">
         <v>0</v>
       </c>
-      <c r="H49" s="54">
-        <v>7</v>
-      </c>
-      <c r="I49" s="41"/>
-      <c r="J49" s="53">
-        <v>99</v>
-      </c>
-      <c r="K49" s="54">
-        <v>99</v>
-      </c>
-      <c r="L49" s="48" t="s">
-        <v>130</v>
-      </c>
-      <c r="M49" s="41"/>
-      <c r="N49" s="55" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="50" spans="2:14" s="43" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B50" s="52" t="s">
-        <v>1</v>
-      </c>
-      <c r="C50" s="40" t="s">
-        <v>212</v>
-      </c>
-      <c r="D50" s="40" t="s">
-        <v>211</v>
-      </c>
-      <c r="E50" s="54">
-        <v>1</v>
-      </c>
-      <c r="F50" s="54">
-        <v>0.3</v>
-      </c>
-      <c r="G50" s="53">
+      <c r="E56" s="24">
+        <v>7</v>
+      </c>
+      <c r="F56" s="24">
+        <v>1</v>
+      </c>
+      <c r="G56" s="26" t="s">
+        <v>55</v>
+      </c>
+      <c r="H56" s="26" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="57" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B57" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="C57" s="23" t="s">
+        <v>53</v>
+      </c>
+      <c r="D57" s="23">
         <v>0</v>
       </c>
-      <c r="H50" s="54">
-        <v>7</v>
-      </c>
-      <c r="I50" s="41"/>
-      <c r="J50" s="53">
-        <v>99</v>
-      </c>
-      <c r="K50" s="54">
-        <v>99</v>
-      </c>
-      <c r="L50" s="48" t="s">
-        <v>130</v>
-      </c>
-      <c r="M50" s="41"/>
-      <c r="N50" s="55" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="51" spans="2:14" s="43" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B51" s="52"/>
-      <c r="C51" s="40"/>
-      <c r="D51" s="40"/>
-      <c r="E51" s="54"/>
-      <c r="F51" s="54"/>
-      <c r="G51" s="53"/>
-      <c r="H51" s="54"/>
-      <c r="I51" s="41"/>
-      <c r="J51" s="53"/>
-      <c r="K51" s="54"/>
-      <c r="L51" s="48"/>
-      <c r="M51" s="41"/>
-      <c r="N51" s="55"/>
-    </row>
-    <row r="52" spans="2:14" s="43" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B52" s="44"/>
-      <c r="C52" s="44"/>
-      <c r="D52" s="44"/>
-      <c r="E52" s="44"/>
-      <c r="F52" s="44"/>
-      <c r="G52" s="44"/>
-      <c r="H52" s="44"/>
-      <c r="I52" s="44"/>
-      <c r="J52" s="44"/>
-      <c r="K52" s="44"/>
-      <c r="L52" s="44"/>
-      <c r="M52" s="44"/>
-      <c r="N52" s="44"/>
-    </row>
-    <row r="53" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B53" s="32"/>
-      <c r="C53" s="32"/>
-      <c r="D53" s="32"/>
-      <c r="E53" s="32"/>
-      <c r="F53" s="32"/>
-      <c r="G53" s="32"/>
-      <c r="H53" s="32"/>
-      <c r="I53" s="32"/>
-      <c r="J53" s="32"/>
-      <c r="K53" s="32"/>
-      <c r="L53" s="32"/>
-      <c r="M53" s="31"/>
-    </row>
-    <row r="54" spans="2:14" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B54" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="C54" s="6"/>
-      <c r="D54" s="6"/>
-      <c r="E54" s="6"/>
-      <c r="F54" s="6"/>
-      <c r="G54" s="6"/>
-      <c r="H54" s="6"/>
-      <c r="I54" s="6"/>
-      <c r="J54" s="6"/>
-      <c r="K54" s="6"/>
-      <c r="L54" s="6"/>
-    </row>
-    <row r="55" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B55" s="20"/>
-      <c r="C55" s="20"/>
-      <c r="D55" s="20"/>
-      <c r="E55" s="20"/>
-      <c r="F55" s="58"/>
-      <c r="G55" s="58"/>
-      <c r="H55" s="58"/>
-      <c r="I55" s="20"/>
-      <c r="J55" s="20"/>
-    </row>
-    <row r="56" spans="2:14" ht="96" x14ac:dyDescent="0.25">
-      <c r="B56" s="30" t="s">
-        <v>71</v>
-      </c>
-      <c r="C56" s="28" t="s">
-        <v>3</v>
-      </c>
-      <c r="D56" s="29" t="s">
-        <v>70</v>
-      </c>
-      <c r="E56" s="29" t="s">
-        <v>69</v>
-      </c>
-      <c r="F56" s="29" t="s">
-        <v>68</v>
-      </c>
-      <c r="G56" s="28" t="s">
-        <v>67</v>
-      </c>
-      <c r="H56" s="28" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="57" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B57" s="27" t="s">
-        <v>1</v>
-      </c>
-      <c r="C57" s="24" t="s">
-        <v>65</v>
-      </c>
-      <c r="D57" s="24">
-        <v>0</v>
-      </c>
       <c r="E57" s="24">
         <v>7</v>
       </c>
-      <c r="F57" s="24">
-        <v>2</v>
+      <c r="F57" s="23">
+        <v>1</v>
       </c>
       <c r="G57" s="26" t="s">
-        <v>64</v>
+        <v>52</v>
       </c>
       <c r="H57" s="26" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="58" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B58" s="27" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="58" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B58" s="25" t="s">
         <v>1</v>
       </c>
       <c r="C58" s="24" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="D58" s="24">
         <v>0</v>
@@ -4697,18 +4637,18 @@
         <v>1</v>
       </c>
       <c r="G58" s="26" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="H58" s="26" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="59" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B59" s="27" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="59" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B59" s="25" t="s">
         <v>1</v>
       </c>
       <c r="C59" s="24" t="s">
-        <v>59</v>
+        <v>47</v>
       </c>
       <c r="D59" s="24">
         <v>0</v>
@@ -4717,136 +4657,136 @@
         <v>7</v>
       </c>
       <c r="F59" s="24">
+        <v>1</v>
+      </c>
+      <c r="G59" s="26" t="s">
+        <v>46</v>
+      </c>
+      <c r="H59" s="26" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="60" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B60" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="C60" s="23" t="s">
+        <v>44</v>
+      </c>
+      <c r="D60" s="23">
+        <v>0</v>
+      </c>
+      <c r="E60" s="24">
+        <v>7</v>
+      </c>
+      <c r="F60" s="23">
+        <v>1</v>
+      </c>
+      <c r="G60" s="22" t="s">
+        <v>43</v>
+      </c>
+      <c r="H60" s="22" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="61" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B61" s="46" t="s">
+        <v>1</v>
+      </c>
+      <c r="C61" s="41" t="s">
+        <v>192</v>
+      </c>
+      <c r="D61" s="41">
+        <v>0</v>
+      </c>
+      <c r="E61" s="41">
+        <v>7</v>
+      </c>
+      <c r="F61" s="41">
+        <v>1</v>
+      </c>
+      <c r="G61" s="42" t="s">
+        <v>180</v>
+      </c>
+      <c r="H61" s="42" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="62" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B62" s="46" t="s">
+        <v>1</v>
+      </c>
+      <c r="C62" s="41" t="s">
+        <v>189</v>
+      </c>
+      <c r="D62" s="41">
+        <v>0</v>
+      </c>
+      <c r="E62" s="41">
+        <v>7</v>
+      </c>
+      <c r="F62" s="41">
         <v>2</v>
       </c>
-      <c r="G59" s="26" t="s">
-        <v>58</v>
-      </c>
-      <c r="H59" s="26" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="60" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B60" s="27" t="s">
-        <v>1</v>
-      </c>
-      <c r="C60" s="24" t="s">
-        <v>56</v>
-      </c>
-      <c r="D60" s="24">
+      <c r="G62" s="45" t="s">
+        <v>183</v>
+      </c>
+      <c r="H62" s="45" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="63" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B63" s="46" t="s">
+        <v>1</v>
+      </c>
+      <c r="C63" s="41" t="s">
+        <v>150</v>
+      </c>
+      <c r="D63" s="41">
         <v>0</v>
       </c>
-      <c r="E60" s="24">
-        <v>7</v>
-      </c>
-      <c r="F60" s="24">
-        <v>1</v>
-      </c>
-      <c r="G60" s="26" t="s">
-        <v>55</v>
-      </c>
-      <c r="H60" s="26" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="61" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B61" s="25" t="s">
-        <v>1</v>
-      </c>
-      <c r="C61" s="23" t="s">
-        <v>53</v>
-      </c>
-      <c r="D61" s="23">
+      <c r="E63" s="41">
+        <v>7</v>
+      </c>
+      <c r="F63" s="41">
+        <v>2</v>
+      </c>
+      <c r="G63" s="45" t="s">
+        <v>181</v>
+      </c>
+      <c r="H63" s="45" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="64" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B64" s="46" t="s">
+        <v>1</v>
+      </c>
+      <c r="C64" s="41" t="s">
+        <v>151</v>
+      </c>
+      <c r="D64" s="41">
         <v>0</v>
       </c>
-      <c r="E61" s="24">
-        <v>7</v>
-      </c>
-      <c r="F61" s="23">
-        <v>1</v>
-      </c>
-      <c r="G61" s="26" t="s">
-        <v>52</v>
-      </c>
-      <c r="H61" s="26" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="62" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B62" s="25" t="s">
-        <v>1</v>
-      </c>
-      <c r="C62" s="24" t="s">
-        <v>50</v>
-      </c>
-      <c r="D62" s="24">
-        <v>0</v>
-      </c>
-      <c r="E62" s="24">
-        <v>7</v>
-      </c>
-      <c r="F62" s="24">
-        <v>1</v>
-      </c>
-      <c r="G62" s="26" t="s">
-        <v>49</v>
-      </c>
-      <c r="H62" s="26" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="63" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B63" s="25" t="s">
-        <v>1</v>
-      </c>
-      <c r="C63" s="24" t="s">
-        <v>47</v>
-      </c>
-      <c r="D63" s="24">
-        <v>0</v>
-      </c>
-      <c r="E63" s="24">
-        <v>7</v>
-      </c>
-      <c r="F63" s="24">
-        <v>1</v>
-      </c>
-      <c r="G63" s="26" t="s">
-        <v>46</v>
-      </c>
-      <c r="H63" s="26" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="64" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B64" s="25" t="s">
-        <v>1</v>
-      </c>
-      <c r="C64" s="23" t="s">
-        <v>44</v>
-      </c>
-      <c r="D64" s="23">
-        <v>0</v>
-      </c>
-      <c r="E64" s="24">
-        <v>7</v>
-      </c>
-      <c r="F64" s="23">
-        <v>1</v>
-      </c>
-      <c r="G64" s="22" t="s">
-        <v>43</v>
-      </c>
-      <c r="H64" s="22" t="s">
-        <v>42</v>
+      <c r="E64" s="41">
+        <v>7</v>
+      </c>
+      <c r="F64" s="41">
+        <v>2</v>
+      </c>
+      <c r="G64" s="45" t="s">
+        <v>182</v>
+      </c>
+      <c r="H64" s="45" t="s">
+        <v>187</v>
       </c>
     </row>
     <row r="65" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B65" s="46" t="s">
         <v>1</v>
       </c>
-      <c r="C65" s="41" t="s">
-        <v>207</v>
+      <c r="C65" s="40" t="s">
+        <v>191</v>
       </c>
       <c r="D65" s="41">
         <v>0</v>
@@ -4857,19 +4797,17 @@
       <c r="F65" s="41">
         <v>1</v>
       </c>
-      <c r="G65" s="42" t="s">
-        <v>195</v>
-      </c>
-      <c r="H65" s="42" t="s">
-        <v>199</v>
-      </c>
+      <c r="G65" s="45" t="s">
+        <v>198</v>
+      </c>
+      <c r="H65" s="45"/>
     </row>
     <row r="66" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B66" s="46" t="s">
         <v>1</v>
       </c>
-      <c r="C66" s="41" t="s">
-        <v>204</v>
+      <c r="C66" s="40" t="s">
+        <v>194</v>
       </c>
       <c r="D66" s="41">
         <v>0</v>
@@ -4878,10 +4816,10 @@
         <v>7</v>
       </c>
       <c r="F66" s="41">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G66" s="45" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="H66" s="45" t="s">
         <v>200</v>
@@ -4891,8 +4829,8 @@
       <c r="B67" s="46" t="s">
         <v>1</v>
       </c>
-      <c r="C67" s="41" t="s">
-        <v>151</v>
+      <c r="C67" s="40" t="s">
+        <v>195</v>
       </c>
       <c r="D67" s="41">
         <v>0</v>
@@ -4901,296 +4839,267 @@
         <v>7</v>
       </c>
       <c r="F67" s="41">
+        <v>1</v>
+      </c>
+      <c r="G67" s="45" t="s">
+        <v>55</v>
+      </c>
+      <c r="H67" s="45" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="68" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="69" spans="2:13" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B69" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="C69" s="6"/>
+      <c r="D69" s="6"/>
+      <c r="E69" s="6"/>
+      <c r="F69" s="6"/>
+      <c r="G69" s="6"/>
+      <c r="H69" s="6"/>
+      <c r="I69" s="6"/>
+      <c r="J69" s="6"/>
+      <c r="K69" s="6"/>
+      <c r="L69" s="6"/>
+      <c r="M69" s="6"/>
+    </row>
+    <row r="70" spans="2:13" ht="60" x14ac:dyDescent="0.25">
+      <c r="B70" s="20"/>
+      <c r="C70" s="20"/>
+      <c r="D70" s="20"/>
+      <c r="E70" s="20"/>
+      <c r="F70" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="G70" s="58" t="s">
+        <v>39</v>
+      </c>
+      <c r="H70" s="58"/>
+      <c r="I70" s="20"/>
+    </row>
+    <row r="71" spans="2:13" ht="142.5" x14ac:dyDescent="0.25">
+      <c r="B71" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="C71" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="D71" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="E71" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="F71" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="G71" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="H71" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="I71" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="J71" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="K71" s="14" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="72" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B72" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="C72" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="D72" s="11">
+        <v>0</v>
+      </c>
+      <c r="E72" s="10">
+        <v>0</v>
+      </c>
+      <c r="F72" s="10">
+        <v>15</v>
+      </c>
+      <c r="G72" s="10">
+        <v>200</v>
+      </c>
+      <c r="H72" s="9">
+        <v>0.5</v>
+      </c>
+      <c r="I72" s="9">
+        <v>1</v>
+      </c>
+      <c r="J72" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="K72" s="13" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="73" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B73" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="C73" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D73" s="11">
+        <v>1</v>
+      </c>
+      <c r="E73" s="10">
+        <v>0</v>
+      </c>
+      <c r="F73" s="10">
+        <v>60</v>
+      </c>
+      <c r="G73" s="10">
+        <v>300</v>
+      </c>
+      <c r="H73" s="9">
+        <v>0.5</v>
+      </c>
+      <c r="I73" s="9">
+        <v>1</v>
+      </c>
+      <c r="J73" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="K73" s="13" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="74" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B74" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="C74" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="D74" s="11">
         <v>2</v>
       </c>
-      <c r="G67" s="45" t="s">
-        <v>196</v>
-      </c>
-      <c r="H67" s="45" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="68" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B68" s="46" t="s">
-        <v>1</v>
-      </c>
-      <c r="C68" s="41" t="s">
-        <v>152</v>
-      </c>
-      <c r="D68" s="41">
+      <c r="E74" s="10">
         <v>0</v>
       </c>
-      <c r="E68" s="41">
-        <v>7</v>
-      </c>
-      <c r="F68" s="41">
+      <c r="F74" s="10">
+        <v>240</v>
+      </c>
+      <c r="G74" s="10">
+        <v>600</v>
+      </c>
+      <c r="H74" s="9">
+        <v>0.5</v>
+      </c>
+      <c r="I74" s="9">
+        <v>1</v>
+      </c>
+      <c r="J74" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="K74" s="7" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="76" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="77" spans="2:13" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B77" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C77" s="6"/>
+      <c r="D77" s="6"/>
+      <c r="E77" s="6"/>
+      <c r="F77" s="6"/>
+      <c r="G77" s="6"/>
+    </row>
+    <row r="79" spans="2:13" ht="135.75" x14ac:dyDescent="0.25">
+      <c r="B79" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C79" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D79" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="G68" s="45" t="s">
-        <v>197</v>
-      </c>
-      <c r="H68" s="45" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="69" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B69" s="46" t="s">
-        <v>1</v>
-      </c>
-      <c r="C69" s="40" t="s">
-        <v>206</v>
-      </c>
-      <c r="D69" s="41">
-        <v>0</v>
-      </c>
-      <c r="E69" s="41">
-        <v>7</v>
-      </c>
-      <c r="F69" s="41">
-        <v>1</v>
-      </c>
-      <c r="G69" s="45" t="s">
-        <v>215</v>
-      </c>
-      <c r="H69" s="45"/>
-    </row>
-    <row r="70" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B70" s="46" t="s">
-        <v>1</v>
-      </c>
-      <c r="C70" s="40" t="s">
-        <v>210</v>
-      </c>
-      <c r="D70" s="41">
-        <v>0</v>
-      </c>
-      <c r="E70" s="41">
-        <v>7</v>
-      </c>
-      <c r="F70" s="41">
-        <v>1</v>
-      </c>
-      <c r="G70" s="45" t="s">
-        <v>216</v>
-      </c>
-      <c r="H70" s="45" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="71" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B71" s="46" t="s">
-        <v>1</v>
-      </c>
-      <c r="C71" s="40" t="s">
-        <v>211</v>
-      </c>
-      <c r="D71" s="41">
-        <v>0</v>
-      </c>
-      <c r="E71" s="41">
-        <v>7</v>
-      </c>
-      <c r="F71" s="41">
-        <v>1</v>
-      </c>
-      <c r="G71" s="45" t="s">
-        <v>55</v>
-      </c>
-      <c r="H71" s="45" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="72" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B72" s="46"/>
-      <c r="C72" s="41"/>
-      <c r="D72" s="41"/>
-      <c r="E72" s="41"/>
-      <c r="F72" s="41"/>
-      <c r="G72" s="56"/>
-      <c r="H72" s="56"/>
-    </row>
-    <row r="73" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="74" spans="2:13" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B74" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="C74" s="6"/>
-      <c r="D74" s="6"/>
-      <c r="E74" s="6"/>
-      <c r="F74" s="6"/>
-      <c r="G74" s="6"/>
-      <c r="H74" s="6"/>
-      <c r="I74" s="6"/>
-      <c r="J74" s="6"/>
-      <c r="K74" s="6"/>
-      <c r="L74" s="6"/>
-      <c r="M74" s="6"/>
-    </row>
-    <row r="75" spans="2:13" ht="60" x14ac:dyDescent="0.25">
-      <c r="B75" s="20"/>
-      <c r="C75" s="20"/>
-      <c r="D75" s="20"/>
-      <c r="E75" s="20"/>
-      <c r="F75" s="21" t="s">
-        <v>40</v>
-      </c>
-      <c r="G75" s="59" t="s">
-        <v>39</v>
-      </c>
-      <c r="H75" s="59"/>
-      <c r="I75" s="20"/>
-    </row>
-    <row r="76" spans="2:13" ht="142.5" x14ac:dyDescent="0.25">
-      <c r="B76" s="19" t="s">
-        <v>38</v>
-      </c>
-      <c r="C76" s="19" t="s">
-        <v>3</v>
-      </c>
-      <c r="D76" s="18" t="s">
-        <v>37</v>
-      </c>
-      <c r="E76" s="17" t="s">
-        <v>36</v>
-      </c>
-      <c r="F76" s="17" t="s">
-        <v>35</v>
-      </c>
-      <c r="G76" s="17" t="s">
-        <v>34</v>
-      </c>
-      <c r="H76" s="16" t="s">
-        <v>33</v>
-      </c>
-      <c r="I76" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="J76" s="15" t="s">
-        <v>31</v>
-      </c>
-      <c r="K76" s="14" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="77" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B77" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="C77" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="D77" s="11">
-        <v>0</v>
-      </c>
-      <c r="E77" s="10">
-        <v>0</v>
-      </c>
-      <c r="F77" s="10">
-        <v>15</v>
-      </c>
-      <c r="G77" s="10">
-        <v>200</v>
-      </c>
-      <c r="H77" s="9">
-        <v>0.5</v>
-      </c>
-      <c r="I77" s="9">
-        <v>1</v>
-      </c>
-      <c r="J77" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="K77" s="13" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="78" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B78" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="C78" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="D78" s="11">
-        <v>1</v>
-      </c>
-      <c r="E78" s="10">
-        <v>0</v>
-      </c>
-      <c r="F78" s="10">
-        <v>60</v>
-      </c>
-      <c r="G78" s="10">
-        <v>300</v>
-      </c>
-      <c r="H78" s="9">
-        <v>0.5</v>
-      </c>
-      <c r="I78" s="9">
-        <v>1</v>
-      </c>
-      <c r="J78" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="K78" s="13" t="s">
+      <c r="E79" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="80" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B80" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C80" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D80" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="E80" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="81" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B81" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C81" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D81" s="1">
+        <v>0.7</v>
+      </c>
+      <c r="E81" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="82" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B82" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C82" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D82" s="1">
+        <v>1</v>
+      </c>
+      <c r="E82" s="1">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="83" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B83" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C83" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D83" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="E83" s="1">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="84" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B84" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C84" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D84" s="1">
+        <v>2</v>
+      </c>
+      <c r="E84" s="1">
         <v>26</v>
-      </c>
-    </row>
-    <row r="79" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B79" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="C79" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="D79" s="11">
-        <v>2</v>
-      </c>
-      <c r="E79" s="10">
-        <v>0</v>
-      </c>
-      <c r="F79" s="10">
-        <v>240</v>
-      </c>
-      <c r="G79" s="10">
-        <v>600</v>
-      </c>
-      <c r="H79" s="9">
-        <v>0.5</v>
-      </c>
-      <c r="I79" s="9">
-        <v>1</v>
-      </c>
-      <c r="J79" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="K79" s="7" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="81" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="82" spans="2:7" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B82" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="C82" s="6"/>
-      <c r="D82" s="6"/>
-      <c r="E82" s="6"/>
-      <c r="F82" s="6"/>
-      <c r="G82" s="6"/>
-    </row>
-    <row r="84" spans="2:7" ht="135.75" x14ac:dyDescent="0.25">
-      <c r="B84" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="C84" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D84" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E84" s="3" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="85" spans="2:7" x14ac:dyDescent="0.25">
@@ -5198,13 +5107,13 @@
         <v>1</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="D85" s="1">
-        <v>0.1</v>
+        <v>2.5</v>
       </c>
       <c r="E85" s="1">
-        <v>2</v>
+        <v>35</v>
       </c>
     </row>
     <row r="86" spans="2:7" x14ac:dyDescent="0.25">
@@ -5212,13 +5121,13 @@
         <v>1</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="D86" s="1">
-        <v>0.7</v>
+        <v>3</v>
       </c>
       <c r="E86" s="1">
-        <v>6</v>
+        <v>45</v>
       </c>
     </row>
     <row r="87" spans="2:7" x14ac:dyDescent="0.25">
@@ -5226,13 +5135,13 @@
         <v>1</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="D87" s="1">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E87" s="1">
-        <v>12</v>
+        <v>56</v>
       </c>
     </row>
     <row r="88" spans="2:7" x14ac:dyDescent="0.25">
@@ -5240,13 +5149,13 @@
         <v>1</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="D88" s="1">
-        <v>1.5</v>
+        <v>5</v>
       </c>
       <c r="E88" s="1">
-        <v>18</v>
+        <v>67</v>
       </c>
     </row>
     <row r="89" spans="2:7" x14ac:dyDescent="0.25">
@@ -5254,69 +5163,35 @@
         <v>1</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="D89" s="1">
+        <v>7</v>
+      </c>
+      <c r="E89" s="1">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="90" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="91" spans="2:7" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B91" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C91" s="6"/>
+      <c r="D91" s="6"/>
+      <c r="E91" s="6"/>
+      <c r="F91" s="6"/>
+      <c r="G91" s="6"/>
+    </row>
+    <row r="93" spans="2:7" ht="142.5" x14ac:dyDescent="0.25">
+      <c r="B93" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C93" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D93" s="3" t="s">
         <v>2</v>
-      </c>
-      <c r="E89" s="1">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="90" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B90" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C90" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D90" s="1">
-        <v>2.5</v>
-      </c>
-      <c r="E90" s="1">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="91" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B91" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C91" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D91" s="1">
-        <v>3</v>
-      </c>
-      <c r="E91" s="1">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="92" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B92" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C92" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D92" s="1">
-        <v>4</v>
-      </c>
-      <c r="E92" s="1">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="93" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B93" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C93" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D93" s="1">
-        <v>5</v>
-      </c>
-      <c r="E93" s="1">
-        <v>67</v>
       </c>
     </row>
     <row r="94" spans="2:7" x14ac:dyDescent="0.25">
@@ -5324,57 +5199,54 @@
         <v>1</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="D94" s="1">
-        <v>7</v>
-      </c>
-      <c r="E94" s="1">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="95" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="96" spans="2:7" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B96" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C96" s="6"/>
-      <c r="D96" s="6"/>
-      <c r="E96" s="6"/>
-      <c r="F96" s="6"/>
-      <c r="G96" s="6"/>
-    </row>
-    <row r="98" spans="2:7" ht="142.5" x14ac:dyDescent="0.25">
-      <c r="B98" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C98" s="4" t="s">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="95" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B95" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C95" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D95" s="1">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="96" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B96" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C96" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D96" s="1">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="97" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="98" spans="2:7" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B98" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C98" s="6"/>
+      <c r="D98" s="6"/>
+      <c r="E98" s="6"/>
+      <c r="F98" s="6"/>
+      <c r="G98" s="6"/>
+    </row>
+    <row r="100" spans="2:7" ht="132" x14ac:dyDescent="0.25">
+      <c r="B100" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C100" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D98" s="3" t="s">
+      <c r="D100" s="3" t="s">
         <v>2</v>
-      </c>
-    </row>
-    <row r="99" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B99" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C99" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D99" s="1">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="100" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B100" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C100" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D100" s="1">
-        <v>0.1</v>
       </c>
     </row>
     <row r="101" spans="2:7" x14ac:dyDescent="0.25">
@@ -5382,42 +5254,9 @@
         <v>1</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="D101" s="1">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="102" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="103" spans="2:7" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B103" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C103" s="6"/>
-      <c r="D103" s="6"/>
-      <c r="E103" s="6"/>
-      <c r="F103" s="6"/>
-      <c r="G103" s="6"/>
-    </row>
-    <row r="105" spans="2:7" ht="132" x14ac:dyDescent="0.25">
-      <c r="B105" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C105" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D105" s="3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="106" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B106" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C106" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D106" s="1">
         <v>0.7</v>
       </c>
     </row>
@@ -5425,11 +5264,11 @@
   <mergeCells count="4">
     <mergeCell ref="J3:K3"/>
     <mergeCell ref="M3:P3"/>
-    <mergeCell ref="F55:H55"/>
-    <mergeCell ref="G75:H75"/>
+    <mergeCell ref="F51:H51"/>
+    <mergeCell ref="G70:H70"/>
   </mergeCells>
-  <conditionalFormatting sqref="C77:D79">
-    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+  <conditionalFormatting sqref="C72:D74">
+    <cfRule type="duplicateValues" dxfId="66" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Content - Balancing for new missions (until gold_witch)
Former-commit-id: bcc3f43de0178ffda389120376ba36a87cf94b7e
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Missions.xlsx
+++ b/Docs/Content/HungryDragonContent_Missions.xlsx
@@ -2625,8 +2625,8 @@
   </sheetPr>
   <dimension ref="B1:P101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G39" sqref="G39"/>
+    <sheetView tabSelected="1" topLeftCell="B13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3868,10 +3868,10 @@
         <v>148</v>
       </c>
       <c r="J33" s="53">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="K33" s="54">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="L33" s="48" t="s">
         <v>129</v>
@@ -4030,10 +4030,10 @@
       </c>
       <c r="I37" s="54"/>
       <c r="J37" s="53">
-        <v>80</v>
+        <v>50</v>
       </c>
       <c r="K37" s="54">
-        <v>100</v>
+        <v>55</v>
       </c>
       <c r="L37" s="48" t="s">
         <v>129</v>
@@ -4069,10 +4069,10 @@
         <v>206</v>
       </c>
       <c r="J38" s="53">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="K38" s="54">
-        <v>7</v>
+        <v>4.5</v>
       </c>
       <c r="L38" s="48" t="s">
         <v>129</v>
@@ -4104,16 +4104,16 @@
         <v>2</v>
       </c>
       <c r="H39" s="54">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="I39" s="54" t="s">
         <v>213</v>
       </c>
       <c r="J39" s="53">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="K39" s="54">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="L39" s="48" t="s">
         <v>129</v>

</xml_diff>

<commit_message>
Content - Balancing next step Gold preys until birds
Former-commit-id: c57ea1e748d7a8467d8abc54b045330bcd33b5d5
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Missions.xlsx
+++ b/Docs/Content/HungryDragonContent_Missions.xlsx
@@ -2626,7 +2626,7 @@
   <dimension ref="B1:P101"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H28" sqref="H28"/>
+      <selection activeCell="C41" sqref="C41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4142,7 +4142,7 @@
         <v>0.3</v>
       </c>
       <c r="G40" s="53">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H40" s="54">
         <v>2</v>
@@ -4151,10 +4151,10 @@
         <v>211</v>
       </c>
       <c r="J40" s="53">
-        <v>30</v>
+        <v>3</v>
       </c>
       <c r="K40" s="54">
-        <v>35</v>
+        <v>3</v>
       </c>
       <c r="L40" s="48" t="s">
         <v>129</v>
@@ -4192,10 +4192,10 @@
         <v>130</v>
       </c>
       <c r="J41" s="53">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="K41" s="54">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="L41" s="48"/>
       <c r="M41" s="48"/>

</xml_diff>

<commit_message>
Final balancing for the new missions
Former-commit-id: 336c2acf2b31ca2fc1e44673f9e4e9959d57bfcc
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Missions.xlsx
+++ b/Docs/Content/HungryDragonContent_Missions.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="422" uniqueCount="214">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="415" uniqueCount="212">
   <si>
     <t>single_run</t>
   </si>
@@ -513,15 +513,6 @@
     <t>eat_suicidal_goblins</t>
   </si>
   <si>
-    <t>Sheep; Cow; Horse</t>
-  </si>
-  <si>
-    <t>eat_suicidal_villagers</t>
-  </si>
-  <si>
-    <t>Villager01;Villager02</t>
-  </si>
-  <si>
     <t>TID_EDIBLE_CANARY_PL</t>
   </si>
   <si>
@@ -691,6 +682,9 @@
   </si>
   <si>
     <t>GoodWitch;GoodWitch2;BadWitch;Witch</t>
+  </si>
+  <si>
+    <t>Sheep;Cow;Horse</t>
   </si>
 </sst>
 </file>
@@ -1180,6 +1174,16 @@
   </cellStyles>
   <dxfs count="67">
     <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -2240,16 +2244,6 @@
         </bottom>
       </border>
     </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -2264,94 +2258,94 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="missionDifficultyDefinitions" displayName="missionDifficultyDefinitions" ref="B71:K74" totalsRowShown="0" headerRowBorderDxfId="65" tableBorderDxfId="64">
-  <autoFilter ref="B71:K74"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="missionDifficultyDefinitions" displayName="missionDifficultyDefinitions" ref="B70:K73" totalsRowShown="0" headerRowBorderDxfId="66" tableBorderDxfId="65">
+  <autoFilter ref="B70:K73"/>
   <tableColumns count="10">
     <tableColumn id="1" name="{missionDifficultyDefinitions}"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="63"/>
-    <tableColumn id="7" name="[index]" dataDxfId="62"/>
-    <tableColumn id="3" name="[dragonsToUnlock]" dataDxfId="61"/>
-    <tableColumn id="4" name="[cooldownMinutes]" dataDxfId="60"/>
-    <tableColumn id="9" name="[maxRewardCoins]" dataDxfId="59"/>
-    <tableColumn id="5" name="[removeMissionPCCoefA]" dataDxfId="58"/>
-    <tableColumn id="6" name="[removeMissionPCCoefB]" dataDxfId="57"/>
-    <tableColumn id="8" name="[tidName]" dataDxfId="56"/>
-    <tableColumn id="10" name="[color]" dataDxfId="55"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="64"/>
+    <tableColumn id="7" name="[index]" dataDxfId="63"/>
+    <tableColumn id="3" name="[dragonsToUnlock]" dataDxfId="62"/>
+    <tableColumn id="4" name="[cooldownMinutes]" dataDxfId="61"/>
+    <tableColumn id="9" name="[maxRewardCoins]" dataDxfId="60"/>
+    <tableColumn id="5" name="[removeMissionPCCoefA]" dataDxfId="59"/>
+    <tableColumn id="6" name="[removeMissionPCCoefB]" dataDxfId="58"/>
+    <tableColumn id="8" name="[tidName]" dataDxfId="57"/>
+    <tableColumn id="10" name="[color]" dataDxfId="56"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table13303132" displayName="Table13303132" ref="B79:E89" totalsRowShown="0" headerRowDxfId="54" dataDxfId="52" headerRowBorderDxfId="53" tableBorderDxfId="51" totalsRowBorderDxfId="50">
-  <autoFilter ref="B79:E89"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table13303132" displayName="Table13303132" ref="B78:E88" totalsRowShown="0" headerRowDxfId="55" dataDxfId="53" headerRowBorderDxfId="54" tableBorderDxfId="52" totalsRowBorderDxfId="51">
+  <autoFilter ref="B78:E88"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="{missionDragonModifiersDefinitions}" dataDxfId="49"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="48"/>
-    <tableColumn id="7" name="[quantityModifier]" dataDxfId="47"/>
-    <tableColumn id="3" name="[missionSCRewardMultiplier]" dataDxfId="46"/>
+    <tableColumn id="1" name="{missionDragonModifiersDefinitions}" dataDxfId="50"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="49"/>
+    <tableColumn id="7" name="[quantityModifier]" dataDxfId="48"/>
+    <tableColumn id="3" name="[missionSCRewardMultiplier]" dataDxfId="47"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table1330313234" displayName="Table1330313234" ref="B93:D96" totalsRowShown="0" headerRowDxfId="45" dataDxfId="43" headerRowBorderDxfId="44" tableBorderDxfId="42" totalsRowBorderDxfId="41">
-  <autoFilter ref="B93:D96"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table1330313234" displayName="Table1330313234" ref="B92:D95" totalsRowShown="0" headerRowDxfId="46" dataDxfId="44" headerRowBorderDxfId="45" tableBorderDxfId="43" totalsRowBorderDxfId="42">
+  <autoFilter ref="B92:D95"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="{missionDifficultyModifiersDefinitions}" dataDxfId="40"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="39"/>
-    <tableColumn id="7" name="[quantityModifier]" dataDxfId="38"/>
+    <tableColumn id="1" name="{missionDifficultyModifiersDefinitions}" dataDxfId="41"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="40"/>
+    <tableColumn id="7" name="[quantityModifier]" dataDxfId="39"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table133031323435" displayName="Table133031323435" ref="B100:D101" totalsRowShown="0" headerRowDxfId="37" dataDxfId="35" headerRowBorderDxfId="36" tableBorderDxfId="34" totalsRowBorderDxfId="33">
-  <autoFilter ref="B100:D101"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table133031323435" displayName="Table133031323435" ref="B99:D100" totalsRowShown="0" headerRowDxfId="38" dataDxfId="36" headerRowBorderDxfId="37" tableBorderDxfId="35" totalsRowBorderDxfId="34">
+  <autoFilter ref="B99:D100"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="{missionOtherModifiersDefinitions}" dataDxfId="32"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="31"/>
-    <tableColumn id="7" name="[quantityModifier]" dataDxfId="30"/>
+    <tableColumn id="1" name="{missionOtherModifiersDefinitions}" dataDxfId="33"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="32"/>
+    <tableColumn id="7" name="[quantityModifier]" dataDxfId="31"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table13" displayName="Table13" ref="B52:H67" totalsRowShown="0" headerRowDxfId="29" dataDxfId="27" headerRowBorderDxfId="28" tableBorderDxfId="26" totalsRowBorderDxfId="25">
-  <autoFilter ref="B52:H67"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table13" displayName="Table13" ref="B51:H66" totalsRowShown="0" headerRowDxfId="30" dataDxfId="28" headerRowBorderDxfId="29" tableBorderDxfId="27" totalsRowBorderDxfId="26">
+  <autoFilter ref="B51:H66"/>
   <tableColumns count="7">
-    <tableColumn id="1" name="{missionTypeDefinitions}" dataDxfId="24"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="23"/>
-    <tableColumn id="3" name="[minTier]" dataDxfId="22"/>
-    <tableColumn id="6" name="[maxTier]" dataDxfId="21"/>
-    <tableColumn id="4" name="[weight]" dataDxfId="20"/>
-    <tableColumn id="9" name="[tidDescSingleRun]" dataDxfId="19"/>
-    <tableColumn id="10" name="[tidDescMultiRun]" dataDxfId="18"/>
+    <tableColumn id="1" name="{missionTypeDefinitions}" dataDxfId="25"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="24"/>
+    <tableColumn id="3" name="[minTier]" dataDxfId="23"/>
+    <tableColumn id="6" name="[maxTier]" dataDxfId="22"/>
+    <tableColumn id="4" name="[weight]" dataDxfId="21"/>
+    <tableColumn id="9" name="[tidDescSingleRun]" dataDxfId="20"/>
+    <tableColumn id="10" name="[tidDescMultiRun]" dataDxfId="19"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table1330" displayName="Table1330" ref="B4:N47" totalsRowShown="0" headerRowDxfId="17" dataDxfId="15" headerRowBorderDxfId="16" tableBorderDxfId="14" totalsRowBorderDxfId="13">
-  <autoFilter ref="B4:N47"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table1330" displayName="Table1330" ref="B4:N46" totalsRowShown="0" headerRowDxfId="18" dataDxfId="16" headerRowBorderDxfId="17" tableBorderDxfId="15" totalsRowBorderDxfId="14">
+  <autoFilter ref="B4:N46"/>
   <tableColumns count="13">
-    <tableColumn id="1" name="{missionsDefinitions}" dataDxfId="12"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="11"/>
-    <tableColumn id="7" name="[type]" dataDxfId="10"/>
-    <tableColumn id="8" name="[weight]" dataDxfId="9"/>
-    <tableColumn id="13" name="[singleRunChance]" dataDxfId="8"/>
-    <tableColumn id="11" name="[minTier]" dataDxfId="7"/>
-    <tableColumn id="12" name="[maxTier]" dataDxfId="6"/>
-    <tableColumn id="6" name="[params]" dataDxfId="5"/>
-    <tableColumn id="3" name="[objectiveBaseQuantityMin]" dataDxfId="4"/>
-    <tableColumn id="9" name="[objectiveBaseQuantityMax]" dataDxfId="3"/>
-    <tableColumn id="4" name="[icon]" dataDxfId="2"/>
-    <tableColumn id="5" name="[tidObjective]" dataDxfId="1"/>
-    <tableColumn id="10" name="[trackingSku]" dataDxfId="0"/>
+    <tableColumn id="1" name="{missionsDefinitions}" dataDxfId="13"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="12"/>
+    <tableColumn id="7" name="[type]" dataDxfId="11"/>
+    <tableColumn id="8" name="[weight]" dataDxfId="10"/>
+    <tableColumn id="13" name="[singleRunChance]" dataDxfId="9"/>
+    <tableColumn id="11" name="[minTier]" dataDxfId="8"/>
+    <tableColumn id="12" name="[maxTier]" dataDxfId="7"/>
+    <tableColumn id="6" name="[params]" dataDxfId="6"/>
+    <tableColumn id="3" name="[objectiveBaseQuantityMin]" dataDxfId="5"/>
+    <tableColumn id="9" name="[objectiveBaseQuantityMax]" dataDxfId="4"/>
+    <tableColumn id="4" name="[icon]" dataDxfId="3"/>
+    <tableColumn id="5" name="[tidObjective]" dataDxfId="2"/>
+    <tableColumn id="10" name="[trackingSku]" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2623,10 +2617,10 @@
   <sheetPr>
     <tabColor theme="6"/>
   </sheetPr>
-  <dimension ref="B1:P101"/>
+  <dimension ref="B1:P100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C41" sqref="C41"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E41" sqref="E41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2635,8 +2629,8 @@
     <col min="2" max="2" width="18.7109375" customWidth="1"/>
     <col min="3" max="3" width="24.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="6" width="18.7109375" customWidth="1"/>
-    <col min="7" max="7" width="42" customWidth="1"/>
-    <col min="8" max="8" width="35.5703125" customWidth="1"/>
+    <col min="7" max="7" width="55.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="54.5703125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="59.85546875" bestFit="1" customWidth="1"/>
     <col min="10" max="11" width="18.7109375" customWidth="1"/>
     <col min="12" max="12" width="17.140625" customWidth="1"/>
@@ -2757,7 +2751,7 @@
         <v>129</v>
       </c>
       <c r="M5" s="33" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="N5" s="31" t="s">
         <v>73</v>
@@ -2872,7 +2866,7 @@
         <v>129</v>
       </c>
       <c r="M8" s="33" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="N8" s="31" t="s">
         <v>73</v>
@@ -2901,7 +2895,7 @@
         <v>7</v>
       </c>
       <c r="I9" s="24" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="J9" s="24">
         <v>25</v>
@@ -2913,7 +2907,7 @@
         <v>127</v>
       </c>
       <c r="M9" s="47" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="N9" s="31" t="s">
         <v>73</v>
@@ -2954,7 +2948,7 @@
         <v>125</v>
       </c>
       <c r="M10" s="47" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="N10" s="31" t="s">
         <v>73</v>
@@ -2995,7 +2989,7 @@
         <v>122</v>
       </c>
       <c r="M11" s="47" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="N11" s="31" t="s">
         <v>73</v>
@@ -3036,7 +3030,7 @@
         <v>120</v>
       </c>
       <c r="M12" s="33" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="N12" s="31" t="s">
         <v>73</v>
@@ -3077,7 +3071,7 @@
         <v>118</v>
       </c>
       <c r="M13" s="33" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="N13" s="31" t="s">
         <v>73</v>
@@ -3118,7 +3112,7 @@
         <v>115</v>
       </c>
       <c r="M14" s="47" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="N14" s="31" t="s">
         <v>73</v>
@@ -3307,7 +3301,7 @@
         <v>107</v>
       </c>
       <c r="M19" s="47" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="N19" s="31" t="s">
         <v>73</v>
@@ -3348,7 +3342,7 @@
         <v>104</v>
       </c>
       <c r="M20" s="33" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="N20" s="31" t="s">
         <v>73</v>
@@ -3389,7 +3383,7 @@
         <v>101</v>
       </c>
       <c r="M21" s="50" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="N21" s="31" t="s">
         <v>73</v>
@@ -3430,7 +3424,7 @@
         <v>98</v>
       </c>
       <c r="M22" s="34" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="N22" s="31" t="s">
         <v>73</v>
@@ -3471,7 +3465,7 @@
         <v>95</v>
       </c>
       <c r="M23" s="50" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="N23" s="31" t="s">
         <v>73</v>
@@ -3512,7 +3506,7 @@
         <v>92</v>
       </c>
       <c r="M24" s="51" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="N24" s="31" t="s">
         <v>73</v>
@@ -3553,7 +3547,7 @@
         <v>89</v>
       </c>
       <c r="M25" s="34" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="N25" s="31" t="s">
         <v>73</v>
@@ -3564,7 +3558,7 @@
         <v>1</v>
       </c>
       <c r="C26" s="24" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="D26" s="23" t="s">
         <v>65</v>
@@ -3594,7 +3588,7 @@
         <v>87</v>
       </c>
       <c r="M26" s="34" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="N26" s="31" t="s">
         <v>73</v>
@@ -3635,7 +3629,7 @@
         <v>84</v>
       </c>
       <c r="M27" s="34" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="N27" s="31" t="s">
         <v>73</v>
@@ -3676,7 +3670,7 @@
         <v>81</v>
       </c>
       <c r="M28" s="34" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="N28" s="31" t="s">
         <v>73</v>
@@ -3717,7 +3711,7 @@
         <v>78</v>
       </c>
       <c r="M29" s="34" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="N29" s="31" t="s">
         <v>73</v>
@@ -3758,7 +3752,7 @@
         <v>75</v>
       </c>
       <c r="M30" s="34" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="N30" s="31" t="s">
         <v>73</v>
@@ -3806,7 +3800,7 @@
         <v>1</v>
       </c>
       <c r="C32" s="24" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="D32" s="23" t="s">
         <v>65</v>
@@ -3824,7 +3818,7 @@
         <v>7</v>
       </c>
       <c r="I32" s="23" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="J32" s="24">
         <v>10</v>
@@ -3836,7 +3830,7 @@
         <v>81</v>
       </c>
       <c r="M32" s="33" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="N32" s="31" t="s">
         <v>73</v>
@@ -3847,10 +3841,10 @@
         <v>1</v>
       </c>
       <c r="C33" s="53" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="D33" s="54" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="E33" s="54">
         <v>1</v>
@@ -3877,7 +3871,7 @@
         <v>129</v>
       </c>
       <c r="M33" s="48" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="N33" s="55" t="s">
         <v>73</v>
@@ -3888,10 +3882,10 @@
         <v>1</v>
       </c>
       <c r="C34" s="53" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="D34" s="54" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="E34" s="54">
         <v>1</v>
@@ -3918,7 +3912,7 @@
         <v>129</v>
       </c>
       <c r="M34" s="48" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="N34" s="55" t="s">
         <v>73</v>
@@ -3929,10 +3923,10 @@
         <v>1</v>
       </c>
       <c r="C35" s="53" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="D35" s="54" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="E35" s="54">
         <v>1</v>
@@ -3947,7 +3941,7 @@
         <v>2</v>
       </c>
       <c r="I35" s="54" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="J35" s="53">
         <v>15</v>
@@ -3959,7 +3953,7 @@
         <v>129</v>
       </c>
       <c r="M35" s="48" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="N35" s="55" t="s">
         <v>73</v>
@@ -3970,10 +3964,10 @@
         <v>1</v>
       </c>
       <c r="C36" s="53" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="D36" s="54" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="E36" s="54">
         <v>1</v>
@@ -4000,7 +3994,7 @@
         <v>129</v>
       </c>
       <c r="M36" s="48" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="N36" s="55" t="s">
         <v>73</v>
@@ -4011,7 +4005,7 @@
         <v>1</v>
       </c>
       <c r="C37" s="53" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="D37" s="54" t="s">
         <v>150</v>
@@ -4048,7 +4042,7 @@
         <v>1</v>
       </c>
       <c r="C38" s="53" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="D38" s="54" t="s">
         <v>150</v>
@@ -4066,7 +4060,7 @@
         <v>7</v>
       </c>
       <c r="I38" s="54" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="J38" s="53">
         <v>4</v>
@@ -4078,7 +4072,7 @@
         <v>129</v>
       </c>
       <c r="M38" s="54" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="N38" s="55" t="s">
         <v>73</v>
@@ -4089,7 +4083,7 @@
         <v>1</v>
       </c>
       <c r="C39" s="53" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="D39" s="54" t="s">
         <v>150</v>
@@ -4107,7 +4101,7 @@
         <v>3</v>
       </c>
       <c r="I39" s="54" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="J39" s="53">
         <v>3</v>
@@ -4119,7 +4113,7 @@
         <v>129</v>
       </c>
       <c r="M39" s="54" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="N39" s="55" t="s">
         <v>73</v>
@@ -4130,7 +4124,7 @@
         <v>1</v>
       </c>
       <c r="C40" s="53" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="D40" s="54" t="s">
         <v>150</v>
@@ -4148,7 +4142,7 @@
         <v>2</v>
       </c>
       <c r="I40" s="54" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="J40" s="53">
         <v>3</v>
@@ -4160,7 +4154,7 @@
         <v>129</v>
       </c>
       <c r="M40" s="49" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="N40" s="55" t="s">
         <v>73</v>
@@ -4171,7 +4165,7 @@
         <v>1</v>
       </c>
       <c r="C41" s="53" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="D41" s="54" t="s">
         <v>150</v>
@@ -4206,7 +4200,7 @@
         <v>1</v>
       </c>
       <c r="C42" s="53" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="D42" s="54" t="s">
         <v>150</v>
@@ -4224,13 +4218,13 @@
         <v>7</v>
       </c>
       <c r="I42" s="54" t="s">
-        <v>154</v>
+        <v>211</v>
       </c>
       <c r="J42" s="53">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="K42" s="54">
-        <v>12</v>
+        <v>5.5</v>
       </c>
       <c r="L42" s="48"/>
       <c r="M42" s="48"/>
@@ -4241,7 +4235,7 @@
         <v>1</v>
       </c>
       <c r="C43" s="53" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="D43" s="54" t="s">
         <v>150</v>
@@ -4262,10 +4256,10 @@
         <v>105</v>
       </c>
       <c r="J43" s="53">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="K43" s="54">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="L43" s="48"/>
       <c r="M43" s="48"/>
@@ -4306,7 +4300,7 @@
         <v>129</v>
       </c>
       <c r="M44" s="49" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="N44" s="55" t="s">
         <v>73</v>
@@ -4316,39 +4310,35 @@
       <c r="B45" s="52" t="s">
         <v>1</v>
       </c>
-      <c r="C45" s="53" t="s">
-        <v>155</v>
-      </c>
-      <c r="D45" s="54" t="s">
-        <v>151</v>
+      <c r="C45" s="40" t="s">
+        <v>188</v>
+      </c>
+      <c r="D45" s="40" t="s">
+        <v>188</v>
       </c>
       <c r="E45" s="54">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F45" s="54">
-        <v>0.3</v>
+        <v>1</v>
       </c>
       <c r="G45" s="53">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H45" s="54">
-        <v>3</v>
-      </c>
-      <c r="I45" s="54" t="s">
-        <v>156</v>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="I45" s="54"/>
       <c r="J45" s="53">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="K45" s="54">
-        <v>6</v>
+        <v>27</v>
       </c>
       <c r="L45" s="48" t="s">
         <v>129</v>
       </c>
-      <c r="M45" s="49" t="s">
-        <v>159</v>
-      </c>
+      <c r="M45" s="49"/>
       <c r="N45" s="55" t="s">
         <v>73</v>
       </c>
@@ -4358,159 +4348,145 @@
         <v>1</v>
       </c>
       <c r="C46" s="40" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="D46" s="40" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="E46" s="54">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F46" s="54">
         <v>1</v>
       </c>
       <c r="G46" s="53">
+        <v>1</v>
+      </c>
+      <c r="H46" s="54">
         <v>2</v>
       </c>
-      <c r="H46" s="54">
-        <v>7</v>
-      </c>
-      <c r="I46" s="54"/>
+      <c r="I46" s="41"/>
       <c r="J46" s="53">
-        <v>25</v>
+        <v>50</v>
       </c>
       <c r="K46" s="54">
-        <v>27</v>
+        <v>52</v>
       </c>
       <c r="L46" s="48" t="s">
         <v>129</v>
       </c>
-      <c r="M46" s="49"/>
+      <c r="M46" s="41"/>
       <c r="N46" s="55" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="47" spans="2:14" s="43" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B47" s="52" t="s">
-        <v>1</v>
-      </c>
-      <c r="C47" s="40" t="s">
-        <v>196</v>
-      </c>
-      <c r="D47" s="40" t="s">
-        <v>195</v>
-      </c>
-      <c r="E47" s="54">
-        <v>1</v>
-      </c>
-      <c r="F47" s="54">
-        <v>1</v>
-      </c>
-      <c r="G47" s="53">
+      <c r="B47" s="44"/>
+      <c r="C47" s="44"/>
+      <c r="D47" s="44"/>
+      <c r="E47" s="44"/>
+      <c r="F47" s="44"/>
+      <c r="G47" s="44"/>
+      <c r="H47" s="44"/>
+      <c r="I47" s="44"/>
+      <c r="J47" s="44"/>
+      <c r="K47" s="44"/>
+      <c r="L47" s="44"/>
+      <c r="M47" s="44"/>
+      <c r="N47" s="44"/>
+    </row>
+    <row r="48" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B48" s="32"/>
+      <c r="C48" s="32"/>
+      <c r="D48" s="32"/>
+      <c r="E48" s="32"/>
+      <c r="F48" s="32"/>
+      <c r="G48" s="32"/>
+      <c r="H48" s="32"/>
+      <c r="I48" s="32"/>
+      <c r="J48" s="32"/>
+      <c r="K48" s="32"/>
+      <c r="L48" s="32"/>
+      <c r="M48" s="31"/>
+    </row>
+    <row r="49" spans="2:12" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B49" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="C49" s="6"/>
+      <c r="D49" s="6"/>
+      <c r="E49" s="6"/>
+      <c r="F49" s="6"/>
+      <c r="G49" s="6"/>
+      <c r="H49" s="6"/>
+      <c r="I49" s="6"/>
+      <c r="J49" s="6"/>
+      <c r="K49" s="6"/>
+      <c r="L49" s="6"/>
+    </row>
+    <row r="50" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B50" s="20"/>
+      <c r="C50" s="20"/>
+      <c r="D50" s="20"/>
+      <c r="E50" s="20"/>
+      <c r="F50" s="57"/>
+      <c r="G50" s="57"/>
+      <c r="H50" s="57"/>
+      <c r="I50" s="20"/>
+      <c r="J50" s="20"/>
+    </row>
+    <row r="51" spans="2:12" ht="96" x14ac:dyDescent="0.25">
+      <c r="B51" s="30" t="s">
+        <v>71</v>
+      </c>
+      <c r="C51" s="28" t="s">
+        <v>3</v>
+      </c>
+      <c r="D51" s="29" t="s">
+        <v>70</v>
+      </c>
+      <c r="E51" s="29" t="s">
+        <v>69</v>
+      </c>
+      <c r="F51" s="29" t="s">
+        <v>68</v>
+      </c>
+      <c r="G51" s="28" t="s">
+        <v>67</v>
+      </c>
+      <c r="H51" s="28" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="52" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B52" s="27" t="s">
+        <v>1</v>
+      </c>
+      <c r="C52" s="24" t="s">
+        <v>65</v>
+      </c>
+      <c r="D52" s="24">
         <v>0</v>
       </c>
-      <c r="H47" s="54">
+      <c r="E52" s="24">
         <v>7</v>
       </c>
-      <c r="I47" s="41"/>
-      <c r="J47" s="53">
-        <v>20</v>
-      </c>
-      <c r="K47" s="54">
-        <v>22</v>
-      </c>
-      <c r="L47" s="48" t="s">
-        <v>129</v>
-      </c>
-      <c r="M47" s="41"/>
-      <c r="N47" s="55" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="48" spans="2:14" s="43" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B48" s="44"/>
-      <c r="C48" s="44"/>
-      <c r="D48" s="44"/>
-      <c r="E48" s="44"/>
-      <c r="F48" s="44"/>
-      <c r="G48" s="44"/>
-      <c r="H48" s="44"/>
-      <c r="I48" s="44"/>
-      <c r="J48" s="44"/>
-      <c r="K48" s="44"/>
-      <c r="L48" s="44"/>
-      <c r="M48" s="44"/>
-      <c r="N48" s="44"/>
-    </row>
-    <row r="49" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B49" s="32"/>
-      <c r="C49" s="32"/>
-      <c r="D49" s="32"/>
-      <c r="E49" s="32"/>
-      <c r="F49" s="32"/>
-      <c r="G49" s="32"/>
-      <c r="H49" s="32"/>
-      <c r="I49" s="32"/>
-      <c r="J49" s="32"/>
-      <c r="K49" s="32"/>
-      <c r="L49" s="32"/>
-      <c r="M49" s="31"/>
-    </row>
-    <row r="50" spans="2:13" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B50" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="C50" s="6"/>
-      <c r="D50" s="6"/>
-      <c r="E50" s="6"/>
-      <c r="F50" s="6"/>
-      <c r="G50" s="6"/>
-      <c r="H50" s="6"/>
-      <c r="I50" s="6"/>
-      <c r="J50" s="6"/>
-      <c r="K50" s="6"/>
-      <c r="L50" s="6"/>
-    </row>
-    <row r="51" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B51" s="20"/>
-      <c r="C51" s="20"/>
-      <c r="D51" s="20"/>
-      <c r="E51" s="20"/>
-      <c r="F51" s="57"/>
-      <c r="G51" s="57"/>
-      <c r="H51" s="57"/>
-      <c r="I51" s="20"/>
-      <c r="J51" s="20"/>
-    </row>
-    <row r="52" spans="2:13" ht="96" x14ac:dyDescent="0.25">
-      <c r="B52" s="30" t="s">
-        <v>71</v>
-      </c>
-      <c r="C52" s="28" t="s">
-        <v>3</v>
-      </c>
-      <c r="D52" s="29" t="s">
-        <v>70</v>
-      </c>
-      <c r="E52" s="29" t="s">
-        <v>69</v>
-      </c>
-      <c r="F52" s="29" t="s">
-        <v>68</v>
-      </c>
-      <c r="G52" s="28" t="s">
-        <v>67</v>
-      </c>
-      <c r="H52" s="28" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="53" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="F52" s="24">
+        <v>2</v>
+      </c>
+      <c r="G52" s="26" t="s">
+        <v>64</v>
+      </c>
+      <c r="H52" s="26" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="53" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B53" s="27" t="s">
         <v>1</v>
       </c>
       <c r="C53" s="24" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="D53" s="24">
         <v>0</v>
@@ -4519,21 +4495,21 @@
         <v>7</v>
       </c>
       <c r="F53" s="24">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G53" s="26" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="H53" s="26" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="54" spans="2:13" x14ac:dyDescent="0.25">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="54" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B54" s="27" t="s">
         <v>1</v>
       </c>
       <c r="C54" s="24" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D54" s="24">
         <v>0</v>
@@ -4542,21 +4518,21 @@
         <v>7</v>
       </c>
       <c r="F54" s="24">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G54" s="26" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="H54" s="26" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="55" spans="2:13" x14ac:dyDescent="0.25">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="55" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B55" s="27" t="s">
         <v>1</v>
       </c>
       <c r="C55" s="24" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D55" s="24">
         <v>0</v>
@@ -4565,67 +4541,67 @@
         <v>7</v>
       </c>
       <c r="F55" s="24">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G55" s="26" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="H55" s="26" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="56" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B56" s="27" t="s">
-        <v>1</v>
-      </c>
-      <c r="C56" s="24" t="s">
-        <v>56</v>
-      </c>
-      <c r="D56" s="24">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="56" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B56" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="C56" s="23" t="s">
+        <v>53</v>
+      </c>
+      <c r="D56" s="23">
         <v>0</v>
       </c>
       <c r="E56" s="24">
         <v>7</v>
       </c>
-      <c r="F56" s="24">
+      <c r="F56" s="23">
         <v>1</v>
       </c>
       <c r="G56" s="26" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="H56" s="26" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="57" spans="2:13" x14ac:dyDescent="0.25">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="57" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B57" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="C57" s="23" t="s">
-        <v>53</v>
-      </c>
-      <c r="D57" s="23">
+      <c r="C57" s="24" t="s">
+        <v>50</v>
+      </c>
+      <c r="D57" s="24">
         <v>0</v>
       </c>
       <c r="E57" s="24">
         <v>7</v>
       </c>
-      <c r="F57" s="23">
+      <c r="F57" s="24">
         <v>1</v>
       </c>
       <c r="G57" s="26" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="H57" s="26" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="58" spans="2:13" x14ac:dyDescent="0.25">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="58" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B58" s="25" t="s">
         <v>1</v>
       </c>
       <c r="C58" s="24" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D58" s="24">
         <v>0</v>
@@ -4637,64 +4613,64 @@
         <v>1</v>
       </c>
       <c r="G58" s="26" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="H58" s="26" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="59" spans="2:13" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="59" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B59" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="C59" s="24" t="s">
-        <v>47</v>
-      </c>
-      <c r="D59" s="24">
+      <c r="C59" s="23" t="s">
+        <v>44</v>
+      </c>
+      <c r="D59" s="23">
         <v>0</v>
       </c>
       <c r="E59" s="24">
         <v>7</v>
       </c>
-      <c r="F59" s="24">
-        <v>1</v>
-      </c>
-      <c r="G59" s="26" t="s">
-        <v>46</v>
-      </c>
-      <c r="H59" s="26" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="60" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B60" s="25" t="s">
-        <v>1</v>
-      </c>
-      <c r="C60" s="23" t="s">
-        <v>44</v>
-      </c>
-      <c r="D60" s="23">
+      <c r="F59" s="23">
+        <v>1</v>
+      </c>
+      <c r="G59" s="22" t="s">
+        <v>43</v>
+      </c>
+      <c r="H59" s="22" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="60" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B60" s="46" t="s">
+        <v>1</v>
+      </c>
+      <c r="C60" s="41" t="s">
+        <v>189</v>
+      </c>
+      <c r="D60" s="41">
         <v>0</v>
       </c>
-      <c r="E60" s="24">
+      <c r="E60" s="41">
         <v>7</v>
       </c>
-      <c r="F60" s="23">
-        <v>1</v>
-      </c>
-      <c r="G60" s="22" t="s">
-        <v>43</v>
-      </c>
-      <c r="H60" s="22" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="61" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="F60" s="41">
+        <v>1</v>
+      </c>
+      <c r="G60" s="42" t="s">
+        <v>177</v>
+      </c>
+      <c r="H60" s="42" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="61" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B61" s="46" t="s">
         <v>1</v>
       </c>
       <c r="C61" s="41" t="s">
-        <v>192</v>
+        <v>186</v>
       </c>
       <c r="D61" s="41">
         <v>0</v>
@@ -4703,21 +4679,21 @@
         <v>7</v>
       </c>
       <c r="F61" s="41">
-        <v>1</v>
-      </c>
-      <c r="G61" s="42" t="s">
+        <v>2</v>
+      </c>
+      <c r="G61" s="45" t="s">
         <v>180</v>
       </c>
-      <c r="H61" s="42" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="62" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="H61" s="45" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="62" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B62" s="46" t="s">
         <v>1</v>
       </c>
       <c r="C62" s="41" t="s">
-        <v>189</v>
+        <v>150</v>
       </c>
       <c r="D62" s="41">
         <v>0</v>
@@ -4729,18 +4705,18 @@
         <v>2</v>
       </c>
       <c r="G62" s="45" t="s">
+        <v>178</v>
+      </c>
+      <c r="H62" s="45" t="s">
         <v>183</v>
       </c>
-      <c r="H62" s="45" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="63" spans="2:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="63" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B63" s="46" t="s">
         <v>1</v>
       </c>
       <c r="C63" s="41" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="D63" s="41">
         <v>0</v>
@@ -4752,18 +4728,18 @@
         <v>2</v>
       </c>
       <c r="G63" s="45" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="H63" s="45" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="64" spans="2:13" x14ac:dyDescent="0.25">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="64" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B64" s="46" t="s">
         <v>1</v>
       </c>
-      <c r="C64" s="41" t="s">
-        <v>151</v>
+      <c r="C64" s="40" t="s">
+        <v>188</v>
       </c>
       <c r="D64" s="41">
         <v>0</v>
@@ -4772,14 +4748,12 @@
         <v>7</v>
       </c>
       <c r="F64" s="41">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G64" s="45" t="s">
-        <v>182</v>
-      </c>
-      <c r="H64" s="45" t="s">
-        <v>187</v>
-      </c>
+        <v>195</v>
+      </c>
+      <c r="H64" s="45"/>
     </row>
     <row r="65" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B65" s="46" t="s">
@@ -4798,16 +4772,18 @@
         <v>1</v>
       </c>
       <c r="G65" s="45" t="s">
-        <v>198</v>
-      </c>
-      <c r="H65" s="45"/>
+        <v>196</v>
+      </c>
+      <c r="H65" s="45" t="s">
+        <v>197</v>
+      </c>
     </row>
     <row r="66" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B66" s="46" t="s">
         <v>1</v>
       </c>
       <c r="C66" s="40" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="D66" s="41">
         <v>0</v>
@@ -4819,96 +4795,105 @@
         <v>1</v>
       </c>
       <c r="G66" s="45" t="s">
-        <v>199</v>
+        <v>55</v>
       </c>
       <c r="H66" s="45" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="67" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="68" spans="2:13" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B68" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="C68" s="6"/>
+      <c r="D68" s="6"/>
+      <c r="E68" s="6"/>
+      <c r="F68" s="6"/>
+      <c r="G68" s="6"/>
+      <c r="H68" s="6"/>
+      <c r="I68" s="6"/>
+      <c r="J68" s="6"/>
+      <c r="K68" s="6"/>
+      <c r="L68" s="6"/>
+      <c r="M68" s="6"/>
+    </row>
+    <row r="69" spans="2:13" ht="60" x14ac:dyDescent="0.25">
+      <c r="B69" s="20"/>
+      <c r="C69" s="20"/>
+      <c r="D69" s="20"/>
+      <c r="E69" s="20"/>
+      <c r="F69" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="G69" s="58" t="s">
+        <v>39</v>
+      </c>
+      <c r="H69" s="58"/>
+      <c r="I69" s="20"/>
+    </row>
+    <row r="70" spans="2:13" ht="142.5" x14ac:dyDescent="0.25">
+      <c r="B70" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="C70" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="D70" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="E70" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="F70" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="G70" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="H70" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="I70" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="J70" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="K70" s="14" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="71" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B71" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="C71" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="D71" s="11">
+        <v>0</v>
+      </c>
+      <c r="E71" s="10">
+        <v>0</v>
+      </c>
+      <c r="F71" s="10">
+        <v>15</v>
+      </c>
+      <c r="G71" s="10">
         <v>200</v>
       </c>
-    </row>
-    <row r="67" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B67" s="46" t="s">
-        <v>1</v>
-      </c>
-      <c r="C67" s="40" t="s">
-        <v>195</v>
-      </c>
-      <c r="D67" s="41">
-        <v>0</v>
-      </c>
-      <c r="E67" s="41">
-        <v>7</v>
-      </c>
-      <c r="F67" s="41">
-        <v>1</v>
-      </c>
-      <c r="G67" s="45" t="s">
-        <v>55</v>
-      </c>
-      <c r="H67" s="45" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="68" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="69" spans="2:13" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B69" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="C69" s="6"/>
-      <c r="D69" s="6"/>
-      <c r="E69" s="6"/>
-      <c r="F69" s="6"/>
-      <c r="G69" s="6"/>
-      <c r="H69" s="6"/>
-      <c r="I69" s="6"/>
-      <c r="J69" s="6"/>
-      <c r="K69" s="6"/>
-      <c r="L69" s="6"/>
-      <c r="M69" s="6"/>
-    </row>
-    <row r="70" spans="2:13" ht="60" x14ac:dyDescent="0.25">
-      <c r="B70" s="20"/>
-      <c r="C70" s="20"/>
-      <c r="D70" s="20"/>
-      <c r="E70" s="20"/>
-      <c r="F70" s="21" t="s">
-        <v>40</v>
-      </c>
-      <c r="G70" s="58" t="s">
-        <v>39</v>
-      </c>
-      <c r="H70" s="58"/>
-      <c r="I70" s="20"/>
-    </row>
-    <row r="71" spans="2:13" ht="142.5" x14ac:dyDescent="0.25">
-      <c r="B71" s="19" t="s">
-        <v>38</v>
-      </c>
-      <c r="C71" s="19" t="s">
-        <v>3</v>
-      </c>
-      <c r="D71" s="18" t="s">
-        <v>37</v>
-      </c>
-      <c r="E71" s="17" t="s">
-        <v>36</v>
-      </c>
-      <c r="F71" s="17" t="s">
-        <v>35</v>
-      </c>
-      <c r="G71" s="17" t="s">
-        <v>34</v>
-      </c>
-      <c r="H71" s="16" t="s">
-        <v>33</v>
-      </c>
-      <c r="I71" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="J71" s="15" t="s">
-        <v>31</v>
-      </c>
-      <c r="K71" s="14" t="s">
-        <v>30</v>
+      <c r="H71" s="9">
+        <v>0.5</v>
+      </c>
+      <c r="I71" s="9">
+        <v>1</v>
+      </c>
+      <c r="J71" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="K71" s="13" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="72" spans="2:13" x14ac:dyDescent="0.25">
@@ -4916,19 +4901,19 @@
         <v>1</v>
       </c>
       <c r="C72" s="11" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D72" s="11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E72" s="10">
         <v>0</v>
       </c>
       <c r="F72" s="10">
-        <v>15</v>
+        <v>60</v>
       </c>
       <c r="G72" s="10">
-        <v>200</v>
+        <v>300</v>
       </c>
       <c r="H72" s="9">
         <v>0.5</v>
@@ -4937,10 +4922,10 @@
         <v>1</v>
       </c>
       <c r="J72" s="8" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="K72" s="13" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="73" spans="2:13" x14ac:dyDescent="0.25">
@@ -4948,19 +4933,19 @@
         <v>1</v>
       </c>
       <c r="C73" s="11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D73" s="11">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E73" s="10">
         <v>0</v>
       </c>
       <c r="F73" s="10">
-        <v>60</v>
+        <v>240</v>
       </c>
       <c r="G73" s="10">
-        <v>300</v>
+        <v>600</v>
       </c>
       <c r="H73" s="9">
         <v>0.5</v>
@@ -4969,67 +4954,49 @@
         <v>1</v>
       </c>
       <c r="J73" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="K73" s="13" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="74" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B74" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="C74" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="D74" s="11">
+        <v>25</v>
+      </c>
+      <c r="K73" s="7" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="75" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="76" spans="2:13" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B76" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C76" s="6"/>
+      <c r="D76" s="6"/>
+      <c r="E76" s="6"/>
+      <c r="F76" s="6"/>
+      <c r="G76" s="6"/>
+    </row>
+    <row r="78" spans="2:13" ht="135.75" x14ac:dyDescent="0.25">
+      <c r="B78" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C78" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D78" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E74" s="10">
-        <v>0</v>
-      </c>
-      <c r="F74" s="10">
-        <v>240</v>
-      </c>
-      <c r="G74" s="10">
-        <v>600</v>
-      </c>
-      <c r="H74" s="9">
-        <v>0.5</v>
-      </c>
-      <c r="I74" s="9">
-        <v>1</v>
-      </c>
-      <c r="J74" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="K74" s="7" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="76" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="77" spans="2:13" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B77" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="C77" s="6"/>
-      <c r="D77" s="6"/>
-      <c r="E77" s="6"/>
-      <c r="F77" s="6"/>
-      <c r="G77" s="6"/>
-    </row>
-    <row r="79" spans="2:13" ht="135.75" x14ac:dyDescent="0.25">
-      <c r="B79" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="C79" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D79" s="3" t="s">
+      <c r="E78" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="79" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B79" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C79" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D79" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="E79" s="1">
         <v>2</v>
-      </c>
-      <c r="E79" s="3" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="80" spans="2:13" x14ac:dyDescent="0.25">
@@ -5037,13 +5004,13 @@
         <v>1</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D80" s="1">
-        <v>0.1</v>
+        <v>0.7</v>
       </c>
       <c r="E80" s="1">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="81" spans="2:7" x14ac:dyDescent="0.25">
@@ -5051,13 +5018,13 @@
         <v>1</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D81" s="1">
-        <v>0.7</v>
+        <v>1</v>
       </c>
       <c r="E81" s="1">
-        <v>6</v>
+        <v>12</v>
       </c>
     </row>
     <row r="82" spans="2:7" x14ac:dyDescent="0.25">
@@ -5065,13 +5032,13 @@
         <v>1</v>
       </c>
       <c r="C82" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D82" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="E82" s="1">
         <v>18</v>
-      </c>
-      <c r="D82" s="1">
-        <v>1</v>
-      </c>
-      <c r="E82" s="1">
-        <v>12</v>
       </c>
     </row>
     <row r="83" spans="2:7" x14ac:dyDescent="0.25">
@@ -5079,13 +5046,13 @@
         <v>1</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D83" s="1">
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="E83" s="1">
-        <v>18</v>
+        <v>26</v>
       </c>
     </row>
     <row r="84" spans="2:7" x14ac:dyDescent="0.25">
@@ -5093,13 +5060,13 @@
         <v>1</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D84" s="1">
-        <v>2</v>
+        <v>2.5</v>
       </c>
       <c r="E84" s="1">
-        <v>26</v>
+        <v>35</v>
       </c>
     </row>
     <row r="85" spans="2:7" x14ac:dyDescent="0.25">
@@ -5107,13 +5074,13 @@
         <v>1</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D85" s="1">
-        <v>2.5</v>
+        <v>3</v>
       </c>
       <c r="E85" s="1">
-        <v>35</v>
+        <v>45</v>
       </c>
     </row>
     <row r="86" spans="2:7" x14ac:dyDescent="0.25">
@@ -5121,13 +5088,13 @@
         <v>1</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D86" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E86" s="1">
-        <v>45</v>
+        <v>56</v>
       </c>
     </row>
     <row r="87" spans="2:7" x14ac:dyDescent="0.25">
@@ -5135,13 +5102,13 @@
         <v>1</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D87" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E87" s="1">
-        <v>56</v>
+        <v>67</v>
       </c>
     </row>
     <row r="88" spans="2:7" x14ac:dyDescent="0.25">
@@ -5149,49 +5116,46 @@
         <v>1</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D88" s="1">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="E88" s="1">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="89" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B89" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C89" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D89" s="1">
-        <v>7</v>
-      </c>
-      <c r="E89" s="1">
         <v>80</v>
       </c>
     </row>
-    <row r="90" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="91" spans="2:7" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B91" s="6" t="s">
+    <row r="89" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="90" spans="2:7" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B90" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C91" s="6"/>
-      <c r="D91" s="6"/>
-      <c r="E91" s="6"/>
-      <c r="F91" s="6"/>
-      <c r="G91" s="6"/>
-    </row>
-    <row r="93" spans="2:7" ht="142.5" x14ac:dyDescent="0.25">
-      <c r="B93" s="5" t="s">
+      <c r="C90" s="6"/>
+      <c r="D90" s="6"/>
+      <c r="E90" s="6"/>
+      <c r="F90" s="6"/>
+      <c r="G90" s="6"/>
+    </row>
+    <row r="92" spans="2:7" ht="142.5" x14ac:dyDescent="0.25">
+      <c r="B92" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C93" s="4" t="s">
+      <c r="C92" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D93" s="3" t="s">
+      <c r="D92" s="3" t="s">
         <v>2</v>
+      </c>
+    </row>
+    <row r="93" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B93" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C93" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D93" s="1">
+        <v>0.05</v>
       </c>
     </row>
     <row r="94" spans="2:7" x14ac:dyDescent="0.25">
@@ -5199,10 +5163,10 @@
         <v>1</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D94" s="1">
-        <v>0.05</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="95" spans="2:7" x14ac:dyDescent="0.25">
@@ -5210,53 +5174,42 @@
         <v>1</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D95" s="1">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="96" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B96" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C96" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D96" s="1">
         <v>0.2</v>
       </c>
     </row>
-    <row r="97" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="98" spans="2:7" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B98" s="6" t="s">
+    <row r="96" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="97" spans="2:7" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B97" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C98" s="6"/>
-      <c r="D98" s="6"/>
-      <c r="E98" s="6"/>
-      <c r="F98" s="6"/>
-      <c r="G98" s="6"/>
-    </row>
-    <row r="100" spans="2:7" ht="132" x14ac:dyDescent="0.25">
-      <c r="B100" s="5" t="s">
+      <c r="C97" s="6"/>
+      <c r="D97" s="6"/>
+      <c r="E97" s="6"/>
+      <c r="F97" s="6"/>
+      <c r="G97" s="6"/>
+    </row>
+    <row r="99" spans="2:7" ht="132" x14ac:dyDescent="0.25">
+      <c r="B99" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C100" s="4" t="s">
+      <c r="C99" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D100" s="3" t="s">
+      <c r="D99" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="101" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B101" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C101" s="1" t="s">
+    <row r="100" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B100" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C100" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D101" s="1">
+      <c r="D100" s="1">
         <v>0.7</v>
       </c>
     </row>
@@ -5264,11 +5217,11 @@
   <mergeCells count="4">
     <mergeCell ref="J3:K3"/>
     <mergeCell ref="M3:P3"/>
-    <mergeCell ref="F51:H51"/>
-    <mergeCell ref="G70:H70"/>
+    <mergeCell ref="F50:H50"/>
+    <mergeCell ref="G69:H69"/>
   </mergeCells>
-  <conditionalFormatting sqref="C72:D74">
-    <cfRule type="duplicateValues" dxfId="66" priority="1"/>
+  <conditionalFormatting sqref="C71:D73">
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Content - Add missing tids and missing icons - Final balance
Former-commit-id: a94258b1023bd9dc40ee81f770cdd95a9fc85379
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Missions.xlsx
+++ b/Docs/Content/HungryDragonContent_Missions.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="415" uniqueCount="212">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="404" uniqueCount="221">
   <si>
     <t>single_run</t>
   </si>
@@ -495,9 +495,6 @@
     <t>[singleRunChance]</t>
   </si>
   <si>
-    <t>Sheep</t>
-  </si>
-  <si>
     <t>SpiderSmall;SpiderRed</t>
   </si>
   <si>
@@ -507,12 +504,6 @@
     <t>eat_suicidal</t>
   </si>
   <si>
-    <t>Worker</t>
-  </si>
-  <si>
-    <t>eat_suicidal_goblins</t>
-  </si>
-  <si>
     <t>TID_EDIBLE_CANARY_PL</t>
   </si>
   <si>
@@ -567,15 +558,9 @@
     <t>TID_EDIBLE_TROLL_PL</t>
   </si>
   <si>
-    <t>TID_EDIBLE_SHEEP_PL</t>
-  </si>
-  <si>
     <t>TID_EDIBLE_STINGRAY_PL</t>
   </si>
   <si>
-    <t>TID_EDIBLE_RAZORBACK_PL</t>
-  </si>
-  <si>
     <t>TID_MISSION_TARGET_BOATMAN</t>
   </si>
   <si>
@@ -606,9 +591,6 @@
     <t>TID_MISSION_OBJECTIVE_EATSUICIDAL_DESC_MULTI_RUN</t>
   </si>
   <si>
-    <t>TID_EDIBLE_CANARY_01_PL</t>
-  </si>
-  <si>
     <t>eat_spec_anim_a</t>
   </si>
   <si>
@@ -621,9 +603,6 @@
     <t>kill_chain</t>
   </si>
   <si>
-    <t>kill_chain_sheeps</t>
-  </si>
-  <si>
     <t>eat_dizzy</t>
   </si>
   <si>
@@ -678,13 +657,61 @@
     <t>Hawk;OwlSmall;OwlBig;Vulture</t>
   </si>
   <si>
-    <t>witches</t>
-  </si>
-  <si>
     <t>GoodWitch;GoodWitch2;BadWitch;Witch</t>
   </si>
   <si>
     <t>Sheep;Cow;Horse</t>
+  </si>
+  <si>
+    <t>icon_hanging_spiders</t>
+  </si>
+  <si>
+    <t>icon_eat_gold_gen</t>
+  </si>
+  <si>
+    <t>icon_eat_gold_stingrays</t>
+  </si>
+  <si>
+    <t>icon_eat_gold_witch</t>
+  </si>
+  <si>
+    <t>icon_eat_gold_preybirds</t>
+  </si>
+  <si>
+    <t>icon_eat_gold_goblins</t>
+  </si>
+  <si>
+    <t>icon_eat_gold_cattle</t>
+  </si>
+  <si>
+    <t>icon_eat_gold_birds</t>
+  </si>
+  <si>
+    <t>icon_kill_chain_canaries</t>
+  </si>
+  <si>
+    <t>icon_kill_chain_humans</t>
+  </si>
+  <si>
+    <t>icon_destroy_mines</t>
+  </si>
+  <si>
+    <t>icon_critical_time</t>
+  </si>
+  <si>
+    <t>TID_MISSION_OBJECTIVE_DESTROYNODIE_DESC_SINGLE_RUN</t>
+  </si>
+  <si>
+    <t>TID_MISSION_OBJECTIVE_DESTROYNODIE_DESC_MULTI_RUN</t>
+  </si>
+  <si>
+    <t>TID_EDIBLE_CATTLE</t>
+  </si>
+  <si>
+    <t>TID_EDIBLE_GEN</t>
+  </si>
+  <si>
+    <t>TID_EDIBLE_WITCH_PL</t>
   </si>
 </sst>
 </file>
@@ -2258,8 +2285,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="missionDifficultyDefinitions" displayName="missionDifficultyDefinitions" ref="B70:K73" totalsRowShown="0" headerRowBorderDxfId="66" tableBorderDxfId="65">
-  <autoFilter ref="B70:K73"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="missionDifficultyDefinitions" displayName="missionDifficultyDefinitions" ref="B67:K70" totalsRowShown="0" headerRowBorderDxfId="66" tableBorderDxfId="65">
+  <autoFilter ref="B67:K70"/>
   <tableColumns count="10">
     <tableColumn id="1" name="{missionDifficultyDefinitions}"/>
     <tableColumn id="2" name="[sku]" dataDxfId="64"/>
@@ -2277,8 +2304,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table13303132" displayName="Table13303132" ref="B78:E88" totalsRowShown="0" headerRowDxfId="55" dataDxfId="53" headerRowBorderDxfId="54" tableBorderDxfId="52" totalsRowBorderDxfId="51">
-  <autoFilter ref="B78:E88"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table13303132" displayName="Table13303132" ref="B75:E85" totalsRowShown="0" headerRowDxfId="55" dataDxfId="53" headerRowBorderDxfId="54" tableBorderDxfId="52" totalsRowBorderDxfId="51">
+  <autoFilter ref="B75:E85"/>
   <tableColumns count="4">
     <tableColumn id="1" name="{missionDragonModifiersDefinitions}" dataDxfId="50"/>
     <tableColumn id="2" name="[sku]" dataDxfId="49"/>
@@ -2290,8 +2317,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table1330313234" displayName="Table1330313234" ref="B92:D95" totalsRowShown="0" headerRowDxfId="46" dataDxfId="44" headerRowBorderDxfId="45" tableBorderDxfId="43" totalsRowBorderDxfId="42">
-  <autoFilter ref="B92:D95"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table1330313234" displayName="Table1330313234" ref="B89:D92" totalsRowShown="0" headerRowDxfId="46" dataDxfId="44" headerRowBorderDxfId="45" tableBorderDxfId="43" totalsRowBorderDxfId="42">
+  <autoFilter ref="B89:D92"/>
   <tableColumns count="3">
     <tableColumn id="1" name="{missionDifficultyModifiersDefinitions}" dataDxfId="41"/>
     <tableColumn id="2" name="[sku]" dataDxfId="40"/>
@@ -2302,8 +2329,8 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table133031323435" displayName="Table133031323435" ref="B99:D100" totalsRowShown="0" headerRowDxfId="38" dataDxfId="36" headerRowBorderDxfId="37" tableBorderDxfId="35" totalsRowBorderDxfId="34">
-  <autoFilter ref="B99:D100"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table133031323435" displayName="Table133031323435" ref="B96:D97" totalsRowShown="0" headerRowDxfId="38" dataDxfId="36" headerRowBorderDxfId="37" tableBorderDxfId="35" totalsRowBorderDxfId="34">
+  <autoFilter ref="B96:D97"/>
   <tableColumns count="3">
     <tableColumn id="1" name="{missionOtherModifiersDefinitions}" dataDxfId="33"/>
     <tableColumn id="2" name="[sku]" dataDxfId="32"/>
@@ -2314,8 +2341,8 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table13" displayName="Table13" ref="B51:H66" totalsRowShown="0" headerRowDxfId="30" dataDxfId="28" headerRowBorderDxfId="29" tableBorderDxfId="27" totalsRowBorderDxfId="26">
-  <autoFilter ref="B51:H66"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table13" displayName="Table13" ref="B48:H63" totalsRowShown="0" headerRowDxfId="30" dataDxfId="28" headerRowBorderDxfId="29" tableBorderDxfId="27" totalsRowBorderDxfId="26">
+  <autoFilter ref="B48:H63"/>
   <tableColumns count="7">
     <tableColumn id="1" name="{missionTypeDefinitions}" dataDxfId="25"/>
     <tableColumn id="2" name="[sku]" dataDxfId="24"/>
@@ -2330,8 +2357,8 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table1330" displayName="Table1330" ref="B4:N46" totalsRowShown="0" headerRowDxfId="18" dataDxfId="16" headerRowBorderDxfId="17" tableBorderDxfId="15" totalsRowBorderDxfId="14">
-  <autoFilter ref="B4:N46"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table1330" displayName="Table1330" ref="B4:N43" totalsRowShown="0" headerRowDxfId="18" dataDxfId="16" headerRowBorderDxfId="17" tableBorderDxfId="15" totalsRowBorderDxfId="14">
+  <autoFilter ref="B4:N43"/>
   <tableColumns count="13">
     <tableColumn id="1" name="{missionsDefinitions}" dataDxfId="13"/>
     <tableColumn id="2" name="[sku]" dataDxfId="12"/>
@@ -2617,10 +2644,10 @@
   <sheetPr>
     <tabColor theme="6"/>
   </sheetPr>
-  <dimension ref="B1:P100"/>
+  <dimension ref="B1:P97"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E41" sqref="E41"/>
+    <sheetView tabSelected="1" topLeftCell="A46" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E57" sqref="E57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2633,8 +2660,8 @@
     <col min="8" max="8" width="54.5703125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="59.85546875" bestFit="1" customWidth="1"/>
     <col min="10" max="11" width="18.7109375" customWidth="1"/>
-    <col min="12" max="12" width="17.140625" customWidth="1"/>
-    <col min="13" max="13" width="26.140625" customWidth="1"/>
+    <col min="12" max="12" width="23.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="32.28515625" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="8.42578125" customWidth="1"/>
     <col min="15" max="16" width="15" customWidth="1"/>
   </cols>
@@ -2751,7 +2778,7 @@
         <v>129</v>
       </c>
       <c r="M5" s="33" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="N5" s="31" t="s">
         <v>73</v>
@@ -2866,7 +2893,7 @@
         <v>129</v>
       </c>
       <c r="M8" s="33" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="N8" s="31" t="s">
         <v>73</v>
@@ -2895,7 +2922,7 @@
         <v>7</v>
       </c>
       <c r="I9" s="24" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="J9" s="24">
         <v>25</v>
@@ -2907,7 +2934,7 @@
         <v>127</v>
       </c>
       <c r="M9" s="47" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="N9" s="31" t="s">
         <v>73</v>
@@ -2948,7 +2975,7 @@
         <v>125</v>
       </c>
       <c r="M10" s="47" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="N10" s="31" t="s">
         <v>73</v>
@@ -2989,7 +3016,7 @@
         <v>122</v>
       </c>
       <c r="M11" s="47" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="N11" s="31" t="s">
         <v>73</v>
@@ -3030,7 +3057,7 @@
         <v>120</v>
       </c>
       <c r="M12" s="33" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="N12" s="31" t="s">
         <v>73</v>
@@ -3071,7 +3098,7 @@
         <v>118</v>
       </c>
       <c r="M13" s="33" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="N13" s="31" t="s">
         <v>73</v>
@@ -3112,7 +3139,7 @@
         <v>115</v>
       </c>
       <c r="M14" s="47" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="N14" s="31" t="s">
         <v>73</v>
@@ -3301,7 +3328,7 @@
         <v>107</v>
       </c>
       <c r="M19" s="47" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="N19" s="31" t="s">
         <v>73</v>
@@ -3342,7 +3369,7 @@
         <v>104</v>
       </c>
       <c r="M20" s="33" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="N20" s="31" t="s">
         <v>73</v>
@@ -3383,7 +3410,7 @@
         <v>101</v>
       </c>
       <c r="M21" s="50" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="N21" s="31" t="s">
         <v>73</v>
@@ -3424,7 +3451,7 @@
         <v>98</v>
       </c>
       <c r="M22" s="34" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="N22" s="31" t="s">
         <v>73</v>
@@ -3465,7 +3492,7 @@
         <v>95</v>
       </c>
       <c r="M23" s="50" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="N23" s="31" t="s">
         <v>73</v>
@@ -3506,7 +3533,7 @@
         <v>92</v>
       </c>
       <c r="M24" s="51" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="N24" s="31" t="s">
         <v>73</v>
@@ -3547,7 +3574,7 @@
         <v>89</v>
       </c>
       <c r="M25" s="34" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="N25" s="31" t="s">
         <v>73</v>
@@ -3558,7 +3585,7 @@
         <v>1</v>
       </c>
       <c r="C26" s="24" t="s">
-        <v>206</v>
+        <v>199</v>
       </c>
       <c r="D26" s="23" t="s">
         <v>65</v>
@@ -3588,7 +3615,7 @@
         <v>87</v>
       </c>
       <c r="M26" s="34" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="N26" s="31" t="s">
         <v>73</v>
@@ -3629,7 +3656,7 @@
         <v>84</v>
       </c>
       <c r="M27" s="34" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="N27" s="31" t="s">
         <v>73</v>
@@ -3670,7 +3697,7 @@
         <v>81</v>
       </c>
       <c r="M28" s="34" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="N28" s="31" t="s">
         <v>73</v>
@@ -3711,7 +3738,7 @@
         <v>78</v>
       </c>
       <c r="M29" s="34" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="N29" s="31" t="s">
         <v>73</v>
@@ -3752,7 +3779,7 @@
         <v>75</v>
       </c>
       <c r="M30" s="34" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="N30" s="31" t="s">
         <v>73</v>
@@ -3795,44 +3822,44 @@
         <v>73</v>
       </c>
     </row>
-    <row r="32" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B32" s="27" t="s">
-        <v>1</v>
-      </c>
-      <c r="C32" s="24" t="s">
-        <v>209</v>
-      </c>
-      <c r="D32" s="23" t="s">
-        <v>65</v>
-      </c>
-      <c r="E32" s="23">
-        <v>1</v>
-      </c>
-      <c r="F32" s="24">
-        <v>0.3</v>
-      </c>
-      <c r="G32" s="24">
-        <v>1</v>
-      </c>
-      <c r="H32" s="34">
-        <v>7</v>
-      </c>
-      <c r="I32" s="23" t="s">
-        <v>210</v>
-      </c>
-      <c r="J32" s="24">
-        <v>10</v>
-      </c>
-      <c r="K32" s="23">
-        <v>12</v>
-      </c>
-      <c r="L32" s="33" t="s">
-        <v>81</v>
-      </c>
-      <c r="M32" s="33" t="s">
-        <v>169</v>
-      </c>
-      <c r="N32" s="31" t="s">
+    <row r="32" spans="2:14" s="43" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B32" s="52" t="s">
+        <v>1</v>
+      </c>
+      <c r="C32" s="53" t="s">
+        <v>198</v>
+      </c>
+      <c r="D32" s="54" t="s">
+        <v>183</v>
+      </c>
+      <c r="E32" s="54">
+        <v>0</v>
+      </c>
+      <c r="F32" s="54">
+        <v>1</v>
+      </c>
+      <c r="G32" s="53">
+        <v>1</v>
+      </c>
+      <c r="H32" s="54">
+        <v>2</v>
+      </c>
+      <c r="I32" s="54" t="s">
+        <v>130</v>
+      </c>
+      <c r="J32" s="53">
+        <v>150</v>
+      </c>
+      <c r="K32" s="54">
+        <v>160</v>
+      </c>
+      <c r="L32" s="48" t="s">
+        <v>212</v>
+      </c>
+      <c r="M32" s="48" t="s">
+        <v>151</v>
+      </c>
+      <c r="N32" s="55" t="s">
         <v>73</v>
       </c>
     </row>
@@ -3841,13 +3868,13 @@
         <v>1</v>
       </c>
       <c r="C33" s="53" t="s">
-        <v>190</v>
+        <v>197</v>
       </c>
       <c r="D33" s="54" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
       <c r="E33" s="54">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F33" s="54">
         <v>1</v>
@@ -3859,19 +3886,19 @@
         <v>2</v>
       </c>
       <c r="I33" s="54" t="s">
-        <v>148</v>
+        <v>152</v>
       </c>
       <c r="J33" s="53">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="K33" s="54">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="L33" s="48" t="s">
-        <v>129</v>
+        <v>213</v>
       </c>
       <c r="M33" s="48" t="s">
-        <v>172</v>
+        <v>153</v>
       </c>
       <c r="N33" s="55" t="s">
         <v>73</v>
@@ -3882,37 +3909,37 @@
         <v>1</v>
       </c>
       <c r="C34" s="53" t="s">
-        <v>205</v>
+        <v>181</v>
       </c>
       <c r="D34" s="54" t="s">
-        <v>189</v>
+        <v>180</v>
       </c>
       <c r="E34" s="54">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F34" s="54">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G34" s="53">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H34" s="54">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="I34" s="54" t="s">
-        <v>130</v>
+        <v>148</v>
       </c>
       <c r="J34" s="53">
-        <v>150</v>
+        <v>8</v>
       </c>
       <c r="K34" s="54">
+        <v>9</v>
+      </c>
+      <c r="L34" s="48" t="s">
+        <v>204</v>
+      </c>
+      <c r="M34" s="48" t="s">
         <v>160</v>
-      </c>
-      <c r="L34" s="48" t="s">
-        <v>129</v>
-      </c>
-      <c r="M34" s="48" t="s">
-        <v>185</v>
       </c>
       <c r="N34" s="55" t="s">
         <v>73</v>
@@ -3923,37 +3950,35 @@
         <v>1</v>
       </c>
       <c r="C35" s="53" t="s">
-        <v>204</v>
+        <v>187</v>
       </c>
       <c r="D35" s="54" t="s">
-        <v>189</v>
+        <v>149</v>
       </c>
       <c r="E35" s="54">
         <v>1</v>
       </c>
       <c r="F35" s="54">
-        <v>1</v>
+        <v>0.3</v>
       </c>
       <c r="G35" s="53">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H35" s="54">
-        <v>2</v>
-      </c>
-      <c r="I35" s="54" t="s">
-        <v>155</v>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="I35" s="54"/>
       <c r="J35" s="53">
-        <v>15</v>
+        <v>50</v>
       </c>
       <c r="K35" s="54">
-        <v>16</v>
+        <v>55</v>
       </c>
       <c r="L35" s="48" t="s">
-        <v>129</v>
-      </c>
-      <c r="M35" s="48" t="s">
-        <v>185</v>
+        <v>205</v>
+      </c>
+      <c r="M35" s="49" t="s">
+        <v>219</v>
       </c>
       <c r="N35" s="55" t="s">
         <v>73</v>
@@ -3964,10 +3989,10 @@
         <v>1</v>
       </c>
       <c r="C36" s="53" t="s">
-        <v>187</v>
+        <v>195</v>
       </c>
       <c r="D36" s="54" t="s">
-        <v>186</v>
+        <v>149</v>
       </c>
       <c r="E36" s="54">
         <v>1</v>
@@ -3976,25 +4001,25 @@
         <v>0.3</v>
       </c>
       <c r="G36" s="53">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H36" s="54">
         <v>7</v>
       </c>
       <c r="I36" s="54" t="s">
-        <v>149</v>
+        <v>196</v>
       </c>
       <c r="J36" s="53">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="K36" s="54">
-        <v>9</v>
+        <v>4.5</v>
       </c>
       <c r="L36" s="48" t="s">
-        <v>129</v>
-      </c>
-      <c r="M36" s="48" t="s">
-        <v>163</v>
+        <v>206</v>
+      </c>
+      <c r="M36" s="54" t="s">
+        <v>169</v>
       </c>
       <c r="N36" s="55" t="s">
         <v>73</v>
@@ -4005,10 +4030,10 @@
         <v>1</v>
       </c>
       <c r="C37" s="53" t="s">
-        <v>194</v>
+        <v>200</v>
       </c>
       <c r="D37" s="54" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E37" s="54">
         <v>1</v>
@@ -4017,22 +4042,26 @@
         <v>0.3</v>
       </c>
       <c r="G37" s="53">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H37" s="54">
-        <v>7</v>
-      </c>
-      <c r="I37" s="54"/>
+        <v>3</v>
+      </c>
+      <c r="I37" s="54" t="s">
+        <v>202</v>
+      </c>
       <c r="J37" s="53">
-        <v>50</v>
+        <v>3</v>
       </c>
       <c r="K37" s="54">
-        <v>55</v>
+        <v>4</v>
       </c>
       <c r="L37" s="48" t="s">
-        <v>129</v>
-      </c>
-      <c r="M37" s="49"/>
+        <v>207</v>
+      </c>
+      <c r="M37" s="54" t="s">
+        <v>220</v>
+      </c>
       <c r="N37" s="55" t="s">
         <v>73</v>
       </c>
@@ -4042,10 +4071,10 @@
         <v>1</v>
       </c>
       <c r="C38" s="53" t="s">
-        <v>202</v>
+        <v>194</v>
       </c>
       <c r="D38" s="54" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E38" s="54">
         <v>1</v>
@@ -4054,25 +4083,25 @@
         <v>0.3</v>
       </c>
       <c r="G38" s="53">
+        <v>2</v>
+      </c>
+      <c r="H38" s="54">
+        <v>2</v>
+      </c>
+      <c r="I38" s="54" t="s">
+        <v>201</v>
+      </c>
+      <c r="J38" s="53">
         <v>3</v>
       </c>
-      <c r="H38" s="54">
-        <v>7</v>
-      </c>
-      <c r="I38" s="54" t="s">
-        <v>203</v>
-      </c>
-      <c r="J38" s="53">
-        <v>4</v>
-      </c>
       <c r="K38" s="54">
-        <v>4.5</v>
+        <v>3</v>
       </c>
       <c r="L38" s="48" t="s">
-        <v>129</v>
-      </c>
-      <c r="M38" s="54" t="s">
-        <v>173</v>
+        <v>208</v>
+      </c>
+      <c r="M38" s="49" t="s">
+        <v>171</v>
       </c>
       <c r="N38" s="55" t="s">
         <v>73</v>
@@ -4083,10 +4112,10 @@
         <v>1</v>
       </c>
       <c r="C39" s="53" t="s">
-        <v>207</v>
+        <v>191</v>
       </c>
       <c r="D39" s="54" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E39" s="54">
         <v>1</v>
@@ -4095,25 +4124,25 @@
         <v>0.3</v>
       </c>
       <c r="G39" s="53">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H39" s="54">
         <v>3</v>
       </c>
       <c r="I39" s="54" t="s">
-        <v>210</v>
+        <v>130</v>
       </c>
       <c r="J39" s="53">
-        <v>3</v>
+        <v>25</v>
       </c>
       <c r="K39" s="54">
-        <v>4</v>
+        <v>27</v>
       </c>
       <c r="L39" s="48" t="s">
-        <v>129</v>
-      </c>
-      <c r="M39" s="54" t="s">
-        <v>174</v>
+        <v>211</v>
+      </c>
+      <c r="M39" s="48" t="s">
+        <v>151</v>
       </c>
       <c r="N39" s="55" t="s">
         <v>73</v>
@@ -4124,10 +4153,10 @@
         <v>1</v>
       </c>
       <c r="C40" s="53" t="s">
-        <v>201</v>
+        <v>193</v>
       </c>
       <c r="D40" s="54" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E40" s="54">
         <v>1</v>
@@ -4136,25 +4165,25 @@
         <v>0.3</v>
       </c>
       <c r="G40" s="53">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H40" s="54">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="I40" s="54" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="J40" s="53">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="K40" s="54">
-        <v>3</v>
+        <v>5.5</v>
       </c>
       <c r="L40" s="48" t="s">
-        <v>129</v>
-      </c>
-      <c r="M40" s="49" t="s">
-        <v>176</v>
+        <v>210</v>
+      </c>
+      <c r="M40" s="48" t="s">
+        <v>218</v>
       </c>
       <c r="N40" s="55" t="s">
         <v>73</v>
@@ -4165,10 +4194,10 @@
         <v>1</v>
       </c>
       <c r="C41" s="53" t="s">
-        <v>198</v>
+        <v>192</v>
       </c>
       <c r="D41" s="54" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E41" s="54">
         <v>1</v>
@@ -4177,293 +4206,257 @@
         <v>0.3</v>
       </c>
       <c r="G41" s="53">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H41" s="54">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="I41" s="54" t="s">
-        <v>130</v>
+        <v>105</v>
       </c>
       <c r="J41" s="53">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="K41" s="54">
-        <v>27</v>
-      </c>
-      <c r="L41" s="48"/>
-      <c r="M41" s="48"/>
-      <c r="N41" s="55"/>
+        <v>18</v>
+      </c>
+      <c r="L41" s="48" t="s">
+        <v>209</v>
+      </c>
+      <c r="M41" s="48" t="s">
+        <v>159</v>
+      </c>
+      <c r="N41" s="55" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="42" spans="2:14" s="43" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B42" s="52" t="s">
         <v>1</v>
       </c>
-      <c r="C42" s="53" t="s">
-        <v>200</v>
-      </c>
-      <c r="D42" s="54" t="s">
-        <v>150</v>
+      <c r="C42" s="40" t="s">
+        <v>182</v>
+      </c>
+      <c r="D42" s="40" t="s">
+        <v>182</v>
       </c>
       <c r="E42" s="54">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F42" s="54">
-        <v>0.3</v>
+        <v>1</v>
       </c>
       <c r="G42" s="53">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H42" s="54">
         <v>7</v>
       </c>
-      <c r="I42" s="54" t="s">
-        <v>211</v>
-      </c>
+      <c r="I42" s="54"/>
       <c r="J42" s="53">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="K42" s="54">
-        <v>5.5</v>
-      </c>
-      <c r="L42" s="48"/>
-      <c r="M42" s="48"/>
-      <c r="N42" s="55"/>
+        <v>27</v>
+      </c>
+      <c r="L42" s="48" t="s">
+        <v>215</v>
+      </c>
+      <c r="M42" s="49"/>
+      <c r="N42" s="55" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="43" spans="2:14" s="43" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B43" s="52" t="s">
         <v>1</v>
       </c>
-      <c r="C43" s="53" t="s">
-        <v>199</v>
-      </c>
-      <c r="D43" s="54" t="s">
-        <v>150</v>
+      <c r="C43" s="40" t="s">
+        <v>186</v>
+      </c>
+      <c r="D43" s="40" t="s">
+        <v>185</v>
       </c>
       <c r="E43" s="54">
         <v>1</v>
       </c>
       <c r="F43" s="54">
-        <v>0.3</v>
+        <v>1</v>
       </c>
       <c r="G43" s="53">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H43" s="54">
+        <v>2</v>
+      </c>
+      <c r="I43" s="41"/>
+      <c r="J43" s="53">
+        <v>50</v>
+      </c>
+      <c r="K43" s="54">
+        <v>52</v>
+      </c>
+      <c r="L43" s="48" t="s">
+        <v>214</v>
+      </c>
+      <c r="M43" s="41"/>
+      <c r="N43" s="55" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="44" spans="2:14" s="43" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B44" s="44"/>
+      <c r="C44" s="44"/>
+      <c r="D44" s="44"/>
+      <c r="E44" s="44"/>
+      <c r="F44" s="44"/>
+      <c r="G44" s="44"/>
+      <c r="H44" s="44"/>
+      <c r="I44" s="44"/>
+      <c r="J44" s="44"/>
+      <c r="K44" s="44"/>
+      <c r="L44" s="44"/>
+      <c r="M44" s="44"/>
+      <c r="N44" s="44"/>
+    </row>
+    <row r="45" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B45" s="32"/>
+      <c r="C45" s="32"/>
+      <c r="D45" s="32"/>
+      <c r="E45" s="32"/>
+      <c r="F45" s="32"/>
+      <c r="G45" s="32"/>
+      <c r="H45" s="32"/>
+      <c r="I45" s="32"/>
+      <c r="J45" s="32"/>
+      <c r="K45" s="32"/>
+      <c r="L45" s="32"/>
+      <c r="M45" s="31"/>
+    </row>
+    <row r="46" spans="2:14" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B46" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="C46" s="6"/>
+      <c r="D46" s="6"/>
+      <c r="E46" s="6"/>
+      <c r="F46" s="6"/>
+      <c r="G46" s="6"/>
+      <c r="H46" s="6"/>
+      <c r="I46" s="6"/>
+      <c r="J46" s="6"/>
+      <c r="K46" s="6"/>
+      <c r="L46" s="6"/>
+    </row>
+    <row r="47" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B47" s="20"/>
+      <c r="C47" s="20"/>
+      <c r="D47" s="20"/>
+      <c r="E47" s="20"/>
+      <c r="F47" s="57"/>
+      <c r="G47" s="57"/>
+      <c r="H47" s="57"/>
+      <c r="I47" s="20"/>
+      <c r="J47" s="20"/>
+    </row>
+    <row r="48" spans="2:14" ht="96" x14ac:dyDescent="0.25">
+      <c r="B48" s="30" t="s">
+        <v>71</v>
+      </c>
+      <c r="C48" s="28" t="s">
+        <v>3</v>
+      </c>
+      <c r="D48" s="29" t="s">
+        <v>70</v>
+      </c>
+      <c r="E48" s="29" t="s">
+        <v>69</v>
+      </c>
+      <c r="F48" s="29" t="s">
+        <v>68</v>
+      </c>
+      <c r="G48" s="28" t="s">
+        <v>67</v>
+      </c>
+      <c r="H48" s="28" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="49" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B49" s="27" t="s">
+        <v>1</v>
+      </c>
+      <c r="C49" s="24" t="s">
+        <v>65</v>
+      </c>
+      <c r="D49" s="24">
+        <v>0</v>
+      </c>
+      <c r="E49" s="24">
         <v>7</v>
       </c>
-      <c r="I43" s="54" t="s">
-        <v>105</v>
-      </c>
-      <c r="J43" s="53">
-        <v>17</v>
-      </c>
-      <c r="K43" s="54">
-        <v>18</v>
-      </c>
-      <c r="L43" s="48"/>
-      <c r="M43" s="48"/>
-      <c r="N43" s="55"/>
-    </row>
-    <row r="44" spans="2:14" s="43" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B44" s="52" t="s">
-        <v>1</v>
-      </c>
-      <c r="C44" s="53" t="s">
-        <v>153</v>
-      </c>
-      <c r="D44" s="54" t="s">
-        <v>151</v>
-      </c>
-      <c r="E44" s="54">
-        <v>1</v>
-      </c>
-      <c r="F44" s="54">
-        <v>0.3</v>
-      </c>
-      <c r="G44" s="53">
-        <v>1</v>
-      </c>
-      <c r="H44" s="54">
-        <v>3</v>
-      </c>
-      <c r="I44" s="54" t="s">
-        <v>152</v>
-      </c>
-      <c r="J44" s="53">
-        <v>5</v>
-      </c>
-      <c r="K44" s="54">
-        <v>6</v>
-      </c>
-      <c r="L44" s="48" t="s">
-        <v>129</v>
-      </c>
-      <c r="M44" s="49" t="s">
-        <v>162</v>
-      </c>
-      <c r="N44" s="55" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="45" spans="2:14" s="43" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B45" s="52" t="s">
-        <v>1</v>
-      </c>
-      <c r="C45" s="40" t="s">
-        <v>188</v>
-      </c>
-      <c r="D45" s="40" t="s">
-        <v>188</v>
-      </c>
-      <c r="E45" s="54">
-        <v>0</v>
-      </c>
-      <c r="F45" s="54">
-        <v>1</v>
-      </c>
-      <c r="G45" s="53">
+      <c r="F49" s="24">
         <v>2</v>
       </c>
-      <c r="H45" s="54">
+      <c r="G49" s="26" t="s">
+        <v>64</v>
+      </c>
+      <c r="H49" s="26" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="50" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B50" s="27" t="s">
+        <v>1</v>
+      </c>
+      <c r="C50" s="24" t="s">
+        <v>62</v>
+      </c>
+      <c r="D50" s="24">
+        <v>0</v>
+      </c>
+      <c r="E50" s="24">
         <v>7</v>
       </c>
-      <c r="I45" s="54"/>
-      <c r="J45" s="53">
-        <v>25</v>
-      </c>
-      <c r="K45" s="54">
-        <v>27</v>
-      </c>
-      <c r="L45" s="48" t="s">
-        <v>129</v>
-      </c>
-      <c r="M45" s="49"/>
-      <c r="N45" s="55" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="46" spans="2:14" s="43" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B46" s="52" t="s">
-        <v>1</v>
-      </c>
-      <c r="C46" s="40" t="s">
-        <v>193</v>
-      </c>
-      <c r="D46" s="40" t="s">
-        <v>192</v>
-      </c>
-      <c r="E46" s="54">
-        <v>1</v>
-      </c>
-      <c r="F46" s="54">
-        <v>1</v>
-      </c>
-      <c r="G46" s="53">
-        <v>1</v>
-      </c>
-      <c r="H46" s="54">
+      <c r="F50" s="24">
+        <v>1</v>
+      </c>
+      <c r="G50" s="26" t="s">
+        <v>61</v>
+      </c>
+      <c r="H50" s="26" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="51" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B51" s="27" t="s">
+        <v>1</v>
+      </c>
+      <c r="C51" s="24" t="s">
+        <v>59</v>
+      </c>
+      <c r="D51" s="24">
+        <v>0</v>
+      </c>
+      <c r="E51" s="24">
+        <v>7</v>
+      </c>
+      <c r="F51" s="24">
         <v>2</v>
       </c>
-      <c r="I46" s="41"/>
-      <c r="J46" s="53">
-        <v>50</v>
-      </c>
-      <c r="K46" s="54">
-        <v>52</v>
-      </c>
-      <c r="L46" s="48" t="s">
-        <v>129</v>
-      </c>
-      <c r="M46" s="41"/>
-      <c r="N46" s="55" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="47" spans="2:14" s="43" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B47" s="44"/>
-      <c r="C47" s="44"/>
-      <c r="D47" s="44"/>
-      <c r="E47" s="44"/>
-      <c r="F47" s="44"/>
-      <c r="G47" s="44"/>
-      <c r="H47" s="44"/>
-      <c r="I47" s="44"/>
-      <c r="J47" s="44"/>
-      <c r="K47" s="44"/>
-      <c r="L47" s="44"/>
-      <c r="M47" s="44"/>
-      <c r="N47" s="44"/>
-    </row>
-    <row r="48" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B48" s="32"/>
-      <c r="C48" s="32"/>
-      <c r="D48" s="32"/>
-      <c r="E48" s="32"/>
-      <c r="F48" s="32"/>
-      <c r="G48" s="32"/>
-      <c r="H48" s="32"/>
-      <c r="I48" s="32"/>
-      <c r="J48" s="32"/>
-      <c r="K48" s="32"/>
-      <c r="L48" s="32"/>
-      <c r="M48" s="31"/>
-    </row>
-    <row r="49" spans="2:12" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B49" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="C49" s="6"/>
-      <c r="D49" s="6"/>
-      <c r="E49" s="6"/>
-      <c r="F49" s="6"/>
-      <c r="G49" s="6"/>
-      <c r="H49" s="6"/>
-      <c r="I49" s="6"/>
-      <c r="J49" s="6"/>
-      <c r="K49" s="6"/>
-      <c r="L49" s="6"/>
-    </row>
-    <row r="50" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B50" s="20"/>
-      <c r="C50" s="20"/>
-      <c r="D50" s="20"/>
-      <c r="E50" s="20"/>
-      <c r="F50" s="57"/>
-      <c r="G50" s="57"/>
-      <c r="H50" s="57"/>
-      <c r="I50" s="20"/>
-      <c r="J50" s="20"/>
-    </row>
-    <row r="51" spans="2:12" ht="96" x14ac:dyDescent="0.25">
-      <c r="B51" s="30" t="s">
-        <v>71</v>
-      </c>
-      <c r="C51" s="28" t="s">
-        <v>3</v>
-      </c>
-      <c r="D51" s="29" t="s">
-        <v>70</v>
-      </c>
-      <c r="E51" s="29" t="s">
-        <v>69</v>
-      </c>
-      <c r="F51" s="29" t="s">
-        <v>68</v>
-      </c>
-      <c r="G51" s="28" t="s">
-        <v>67</v>
-      </c>
-      <c r="H51" s="28" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="52" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="G51" s="26" t="s">
+        <v>58</v>
+      </c>
+      <c r="H51" s="26" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="52" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B52" s="27" t="s">
         <v>1</v>
       </c>
       <c r="C52" s="24" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="D52" s="24">
         <v>0</v>
@@ -4472,44 +4465,44 @@
         <v>7</v>
       </c>
       <c r="F52" s="24">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G52" s="26" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="H52" s="26" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="53" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B53" s="27" t="s">
-        <v>1</v>
-      </c>
-      <c r="C53" s="24" t="s">
-        <v>62</v>
-      </c>
-      <c r="D53" s="24">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="53" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B53" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="C53" s="23" t="s">
+        <v>53</v>
+      </c>
+      <c r="D53" s="23">
         <v>0</v>
       </c>
       <c r="E53" s="24">
         <v>7</v>
       </c>
-      <c r="F53" s="24">
+      <c r="F53" s="23">
         <v>1</v>
       </c>
       <c r="G53" s="26" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="H53" s="26" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="54" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B54" s="27" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="54" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B54" s="25" t="s">
         <v>1</v>
       </c>
       <c r="C54" s="24" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="D54" s="24">
         <v>0</v>
@@ -4518,21 +4511,21 @@
         <v>7</v>
       </c>
       <c r="F54" s="24">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G54" s="26" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="H54" s="26" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="55" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B55" s="27" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="55" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B55" s="25" t="s">
         <v>1</v>
       </c>
       <c r="C55" s="24" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="D55" s="24">
         <v>0</v>
@@ -4544,18 +4537,18 @@
         <v>1</v>
       </c>
       <c r="G55" s="26" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="H55" s="26" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="56" spans="2:12" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="56" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B56" s="25" t="s">
         <v>1</v>
       </c>
       <c r="C56" s="23" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="D56" s="23">
         <v>0</v>
@@ -4566,88 +4559,88 @@
       <c r="F56" s="23">
         <v>1</v>
       </c>
-      <c r="G56" s="26" t="s">
-        <v>52</v>
-      </c>
-      <c r="H56" s="26" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="57" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B57" s="25" t="s">
-        <v>1</v>
-      </c>
-      <c r="C57" s="24" t="s">
-        <v>50</v>
-      </c>
-      <c r="D57" s="24">
-        <v>0</v>
-      </c>
-      <c r="E57" s="24">
+      <c r="G56" s="22" t="s">
+        <v>43</v>
+      </c>
+      <c r="H56" s="22" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="57" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B57" s="46" t="s">
+        <v>1</v>
+      </c>
+      <c r="C57" s="41" t="s">
+        <v>183</v>
+      </c>
+      <c r="D57" s="41">
+        <v>0</v>
+      </c>
+      <c r="E57" s="41">
         <v>7</v>
       </c>
-      <c r="F57" s="24">
-        <v>1</v>
-      </c>
-      <c r="G57" s="26" t="s">
-        <v>49</v>
-      </c>
-      <c r="H57" s="26" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="58" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B58" s="25" t="s">
-        <v>1</v>
-      </c>
-      <c r="C58" s="24" t="s">
-        <v>47</v>
-      </c>
-      <c r="D58" s="24">
-        <v>0</v>
-      </c>
-      <c r="E58" s="24">
+      <c r="F57" s="41">
+        <v>0</v>
+      </c>
+      <c r="G57" s="42" t="s">
+        <v>172</v>
+      </c>
+      <c r="H57" s="42" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="58" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B58" s="46" t="s">
+        <v>1</v>
+      </c>
+      <c r="C58" s="41" t="s">
+        <v>180</v>
+      </c>
+      <c r="D58" s="41">
+        <v>0</v>
+      </c>
+      <c r="E58" s="41">
         <v>7</v>
       </c>
-      <c r="F58" s="24">
-        <v>1</v>
-      </c>
-      <c r="G58" s="26" t="s">
-        <v>46</v>
-      </c>
-      <c r="H58" s="26" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="59" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B59" s="25" t="s">
-        <v>1</v>
-      </c>
-      <c r="C59" s="23" t="s">
-        <v>44</v>
-      </c>
-      <c r="D59" s="23">
-        <v>0</v>
-      </c>
-      <c r="E59" s="24">
+      <c r="F58" s="41">
+        <v>0</v>
+      </c>
+      <c r="G58" s="45" t="s">
+        <v>175</v>
+      </c>
+      <c r="H58" s="45" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="59" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B59" s="46" t="s">
+        <v>1</v>
+      </c>
+      <c r="C59" s="41" t="s">
+        <v>149</v>
+      </c>
+      <c r="D59" s="41">
+        <v>0</v>
+      </c>
+      <c r="E59" s="41">
         <v>7</v>
       </c>
-      <c r="F59" s="23">
-        <v>1</v>
-      </c>
-      <c r="G59" s="22" t="s">
-        <v>43</v>
-      </c>
-      <c r="H59" s="22" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="60" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="F59" s="41">
+        <v>2</v>
+      </c>
+      <c r="G59" s="45" t="s">
+        <v>173</v>
+      </c>
+      <c r="H59" s="45" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="60" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B60" s="46" t="s">
         <v>1</v>
       </c>
       <c r="C60" s="41" t="s">
-        <v>189</v>
+        <v>150</v>
       </c>
       <c r="D60" s="41">
         <v>0</v>
@@ -4656,21 +4649,21 @@
         <v>7</v>
       </c>
       <c r="F60" s="41">
-        <v>1</v>
-      </c>
-      <c r="G60" s="42" t="s">
-        <v>177</v>
-      </c>
-      <c r="H60" s="42" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="61" spans="2:12" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="G60" s="45" t="s">
+        <v>174</v>
+      </c>
+      <c r="H60" s="45" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="61" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B61" s="46" t="s">
         <v>1</v>
       </c>
-      <c r="C61" s="41" t="s">
-        <v>186</v>
+      <c r="C61" s="40" t="s">
+        <v>182</v>
       </c>
       <c r="D61" s="41">
         <v>0</v>
@@ -4679,21 +4672,19 @@
         <v>7</v>
       </c>
       <c r="F61" s="41">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G61" s="45" t="s">
-        <v>180</v>
-      </c>
-      <c r="H61" s="45" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="62" spans="2:12" x14ac:dyDescent="0.25">
+        <v>188</v>
+      </c>
+      <c r="H61" s="45"/>
+    </row>
+    <row r="62" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B62" s="46" t="s">
         <v>1</v>
       </c>
-      <c r="C62" s="41" t="s">
-        <v>150</v>
+      <c r="C62" s="40" t="s">
+        <v>184</v>
       </c>
       <c r="D62" s="41">
         <v>0</v>
@@ -4702,21 +4693,21 @@
         <v>7</v>
       </c>
       <c r="F62" s="41">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G62" s="45" t="s">
-        <v>178</v>
+        <v>189</v>
       </c>
       <c r="H62" s="45" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="63" spans="2:12" x14ac:dyDescent="0.25">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="63" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B63" s="46" t="s">
         <v>1</v>
       </c>
-      <c r="C63" s="41" t="s">
-        <v>151</v>
+      <c r="C63" s="40" t="s">
+        <v>185</v>
       </c>
       <c r="D63" s="41">
         <v>0</v>
@@ -4725,264 +4716,239 @@
         <v>7</v>
       </c>
       <c r="F63" s="41">
+        <v>1</v>
+      </c>
+      <c r="G63" s="45" t="s">
+        <v>216</v>
+      </c>
+      <c r="H63" s="45" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="64" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="65" spans="2:13" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B65" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="C65" s="6"/>
+      <c r="D65" s="6"/>
+      <c r="E65" s="6"/>
+      <c r="F65" s="6"/>
+      <c r="G65" s="6"/>
+      <c r="H65" s="6"/>
+      <c r="I65" s="6"/>
+      <c r="J65" s="6"/>
+      <c r="K65" s="6"/>
+      <c r="L65" s="6"/>
+      <c r="M65" s="6"/>
+    </row>
+    <row r="66" spans="2:13" ht="60" x14ac:dyDescent="0.25">
+      <c r="B66" s="20"/>
+      <c r="C66" s="20"/>
+      <c r="D66" s="20"/>
+      <c r="E66" s="20"/>
+      <c r="F66" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="G66" s="58" t="s">
+        <v>39</v>
+      </c>
+      <c r="H66" s="58"/>
+      <c r="I66" s="20"/>
+    </row>
+    <row r="67" spans="2:13" ht="142.5" x14ac:dyDescent="0.25">
+      <c r="B67" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="C67" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="D67" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="E67" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="F67" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="G67" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="H67" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="I67" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="J67" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="K67" s="14" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="68" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B68" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="C68" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="D68" s="11">
+        <v>0</v>
+      </c>
+      <c r="E68" s="10">
+        <v>0</v>
+      </c>
+      <c r="F68" s="10">
+        <v>15</v>
+      </c>
+      <c r="G68" s="10">
+        <v>200</v>
+      </c>
+      <c r="H68" s="9">
+        <v>0.5</v>
+      </c>
+      <c r="I68" s="9">
+        <v>1</v>
+      </c>
+      <c r="J68" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="K68" s="13" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="69" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B69" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="C69" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D69" s="11">
+        <v>1</v>
+      </c>
+      <c r="E69" s="10">
+        <v>0</v>
+      </c>
+      <c r="F69" s="10">
+        <v>60</v>
+      </c>
+      <c r="G69" s="10">
+        <v>300</v>
+      </c>
+      <c r="H69" s="9">
+        <v>0.5</v>
+      </c>
+      <c r="I69" s="9">
+        <v>1</v>
+      </c>
+      <c r="J69" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="K69" s="13" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="70" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B70" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="C70" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="D70" s="11">
         <v>2</v>
       </c>
-      <c r="G63" s="45" t="s">
-        <v>179</v>
-      </c>
-      <c r="H63" s="45" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="64" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B64" s="46" t="s">
-        <v>1</v>
-      </c>
-      <c r="C64" s="40" t="s">
-        <v>188</v>
-      </c>
-      <c r="D64" s="41">
-        <v>0</v>
-      </c>
-      <c r="E64" s="41">
-        <v>7</v>
-      </c>
-      <c r="F64" s="41">
-        <v>1</v>
-      </c>
-      <c r="G64" s="45" t="s">
-        <v>195</v>
-      </c>
-      <c r="H64" s="45"/>
-    </row>
-    <row r="65" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B65" s="46" t="s">
-        <v>1</v>
-      </c>
-      <c r="C65" s="40" t="s">
-        <v>191</v>
-      </c>
-      <c r="D65" s="41">
-        <v>0</v>
-      </c>
-      <c r="E65" s="41">
-        <v>7</v>
-      </c>
-      <c r="F65" s="41">
-        <v>1</v>
-      </c>
-      <c r="G65" s="45" t="s">
-        <v>196</v>
-      </c>
-      <c r="H65" s="45" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="66" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B66" s="46" t="s">
-        <v>1</v>
-      </c>
-      <c r="C66" s="40" t="s">
-        <v>192</v>
-      </c>
-      <c r="D66" s="41">
-        <v>0</v>
-      </c>
-      <c r="E66" s="41">
-        <v>7</v>
-      </c>
-      <c r="F66" s="41">
-        <v>1</v>
-      </c>
-      <c r="G66" s="45" t="s">
-        <v>55</v>
-      </c>
-      <c r="H66" s="45" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="67" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="68" spans="2:13" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B68" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="C68" s="6"/>
-      <c r="D68" s="6"/>
-      <c r="E68" s="6"/>
-      <c r="F68" s="6"/>
-      <c r="G68" s="6"/>
-      <c r="H68" s="6"/>
-      <c r="I68" s="6"/>
-      <c r="J68" s="6"/>
-      <c r="K68" s="6"/>
-      <c r="L68" s="6"/>
-      <c r="M68" s="6"/>
-    </row>
-    <row r="69" spans="2:13" ht="60" x14ac:dyDescent="0.25">
-      <c r="B69" s="20"/>
-      <c r="C69" s="20"/>
-      <c r="D69" s="20"/>
-      <c r="E69" s="20"/>
-      <c r="F69" s="21" t="s">
-        <v>40</v>
-      </c>
-      <c r="G69" s="58" t="s">
-        <v>39</v>
-      </c>
-      <c r="H69" s="58"/>
-      <c r="I69" s="20"/>
-    </row>
-    <row r="70" spans="2:13" ht="142.5" x14ac:dyDescent="0.25">
-      <c r="B70" s="19" t="s">
-        <v>38</v>
-      </c>
-      <c r="C70" s="19" t="s">
+      <c r="E70" s="10">
+        <v>0</v>
+      </c>
+      <c r="F70" s="10">
+        <v>240</v>
+      </c>
+      <c r="G70" s="10">
+        <v>600</v>
+      </c>
+      <c r="H70" s="9">
+        <v>0.5</v>
+      </c>
+      <c r="I70" s="9">
+        <v>1</v>
+      </c>
+      <c r="J70" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="K70" s="7" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="72" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="73" spans="2:13" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B73" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C73" s="6"/>
+      <c r="D73" s="6"/>
+      <c r="E73" s="6"/>
+      <c r="F73" s="6"/>
+      <c r="G73" s="6"/>
+    </row>
+    <row r="75" spans="2:13" ht="135.75" x14ac:dyDescent="0.25">
+      <c r="B75" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C75" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D70" s="18" t="s">
-        <v>37</v>
-      </c>
-      <c r="E70" s="17" t="s">
-        <v>36</v>
-      </c>
-      <c r="F70" s="17" t="s">
-        <v>35</v>
-      </c>
-      <c r="G70" s="17" t="s">
-        <v>34</v>
-      </c>
-      <c r="H70" s="16" t="s">
-        <v>33</v>
-      </c>
-      <c r="I70" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="J70" s="15" t="s">
-        <v>31</v>
-      </c>
-      <c r="K70" s="14" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="71" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B71" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="C71" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="D71" s="11">
-        <v>0</v>
-      </c>
-      <c r="E71" s="10">
-        <v>0</v>
-      </c>
-      <c r="F71" s="10">
-        <v>15</v>
-      </c>
-      <c r="G71" s="10">
-        <v>200</v>
-      </c>
-      <c r="H71" s="9">
-        <v>0.5</v>
-      </c>
-      <c r="I71" s="9">
-        <v>1</v>
-      </c>
-      <c r="J71" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="K71" s="13" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="72" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B72" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="C72" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="D72" s="11">
-        <v>1</v>
-      </c>
-      <c r="E72" s="10">
-        <v>0</v>
-      </c>
-      <c r="F72" s="10">
-        <v>60</v>
-      </c>
-      <c r="G72" s="10">
-        <v>300</v>
-      </c>
-      <c r="H72" s="9">
-        <v>0.5</v>
-      </c>
-      <c r="I72" s="9">
-        <v>1</v>
-      </c>
-      <c r="J72" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="K72" s="13" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="73" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B73" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="C73" s="11" t="s">
+      <c r="D75" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E75" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="76" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B76" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C76" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D76" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="E76" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="77" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B77" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C77" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D77" s="1">
+        <v>0.7</v>
+      </c>
+      <c r="E77" s="1">
         <v>6</v>
       </c>
-      <c r="D73" s="11">
-        <v>2</v>
-      </c>
-      <c r="E73" s="10">
-        <v>0</v>
-      </c>
-      <c r="F73" s="10">
-        <v>240</v>
-      </c>
-      <c r="G73" s="10">
-        <v>600</v>
-      </c>
-      <c r="H73" s="9">
-        <v>0.5</v>
-      </c>
-      <c r="I73" s="9">
-        <v>1</v>
-      </c>
-      <c r="J73" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="K73" s="7" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="75" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="76" spans="2:13" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B76" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="C76" s="6"/>
-      <c r="D76" s="6"/>
-      <c r="E76" s="6"/>
-      <c r="F76" s="6"/>
-      <c r="G76" s="6"/>
-    </row>
-    <row r="78" spans="2:13" ht="135.75" x14ac:dyDescent="0.25">
-      <c r="B78" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="C78" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D78" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E78" s="3" t="s">
-        <v>21</v>
+    </row>
+    <row r="78" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B78" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C78" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D78" s="1">
+        <v>1</v>
+      </c>
+      <c r="E78" s="1">
+        <v>12</v>
       </c>
     </row>
     <row r="79" spans="2:13" x14ac:dyDescent="0.25">
@@ -4990,13 +4956,13 @@
         <v>1</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="D79" s="1">
-        <v>0.1</v>
+        <v>1.5</v>
       </c>
       <c r="E79" s="1">
-        <v>2</v>
+        <v>18</v>
       </c>
     </row>
     <row r="80" spans="2:13" x14ac:dyDescent="0.25">
@@ -5004,13 +4970,13 @@
         <v>1</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D80" s="1">
-        <v>0.7</v>
+        <v>2</v>
       </c>
       <c r="E80" s="1">
-        <v>6</v>
+        <v>26</v>
       </c>
     </row>
     <row r="81" spans="2:7" x14ac:dyDescent="0.25">
@@ -5018,13 +4984,13 @@
         <v>1</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D81" s="1">
-        <v>1</v>
+        <v>2.5</v>
       </c>
       <c r="E81" s="1">
-        <v>12</v>
+        <v>35</v>
       </c>
     </row>
     <row r="82" spans="2:7" x14ac:dyDescent="0.25">
@@ -5032,13 +4998,13 @@
         <v>1</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="D82" s="1">
-        <v>1.5</v>
+        <v>3</v>
       </c>
       <c r="E82" s="1">
-        <v>18</v>
+        <v>45</v>
       </c>
     </row>
     <row r="83" spans="2:7" x14ac:dyDescent="0.25">
@@ -5046,13 +5012,13 @@
         <v>1</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D83" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E83" s="1">
-        <v>26</v>
+        <v>56</v>
       </c>
     </row>
     <row r="84" spans="2:7" x14ac:dyDescent="0.25">
@@ -5060,13 +5026,13 @@
         <v>1</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="D84" s="1">
-        <v>2.5</v>
+        <v>5</v>
       </c>
       <c r="E84" s="1">
-        <v>35</v>
+        <v>67</v>
       </c>
     </row>
     <row r="85" spans="2:7" x14ac:dyDescent="0.25">
@@ -5074,142 +5040,100 @@
         <v>1</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D85" s="1">
+        <v>7</v>
+      </c>
+      <c r="E85" s="1">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="86" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="87" spans="2:7" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B87" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C87" s="6"/>
+      <c r="D87" s="6"/>
+      <c r="E87" s="6"/>
+      <c r="F87" s="6"/>
+      <c r="G87" s="6"/>
+    </row>
+    <row r="89" spans="2:7" ht="142.5" x14ac:dyDescent="0.25">
+      <c r="B89" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C89" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E85" s="1">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="86" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B86" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C86" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D86" s="1">
+      <c r="D89" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="90" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B90" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C90" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D90" s="1">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="91" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B91" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C91" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D91" s="1">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="92" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B92" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C92" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D92" s="1">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="93" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="94" spans="2:7" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B94" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C94" s="6"/>
+      <c r="D94" s="6"/>
+      <c r="E94" s="6"/>
+      <c r="F94" s="6"/>
+      <c r="G94" s="6"/>
+    </row>
+    <row r="96" spans="2:7" ht="132" x14ac:dyDescent="0.25">
+      <c r="B96" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="E86" s="1">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="87" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B87" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C87" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D87" s="1">
-        <v>5</v>
-      </c>
-      <c r="E87" s="1">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="88" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B88" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C88" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D88" s="1">
-        <v>7</v>
-      </c>
-      <c r="E88" s="1">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="89" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="90" spans="2:7" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B90" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C90" s="6"/>
-      <c r="D90" s="6"/>
-      <c r="E90" s="6"/>
-      <c r="F90" s="6"/>
-      <c r="G90" s="6"/>
-    </row>
-    <row r="92" spans="2:7" ht="142.5" x14ac:dyDescent="0.25">
-      <c r="B92" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C92" s="4" t="s">
+      <c r="C96" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D92" s="3" t="s">
+      <c r="D96" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="93" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B93" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C93" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D93" s="1">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="94" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B94" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C94" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D94" s="1">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="95" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B95" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C95" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D95" s="1">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="96" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="97" spans="2:7" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B97" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C97" s="6"/>
-      <c r="D97" s="6"/>
-      <c r="E97" s="6"/>
-      <c r="F97" s="6"/>
-      <c r="G97" s="6"/>
-    </row>
-    <row r="99" spans="2:7" ht="132" x14ac:dyDescent="0.25">
-      <c r="B99" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C99" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D99" s="3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="100" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B100" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C100" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D100" s="1">
+    <row r="97" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B97" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C97" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D97" s="1">
         <v>0.7</v>
       </c>
     </row>
@@ -5217,10 +5141,10 @@
   <mergeCells count="4">
     <mergeCell ref="J3:K3"/>
     <mergeCell ref="M3:P3"/>
-    <mergeCell ref="F50:H50"/>
-    <mergeCell ref="G69:H69"/>
+    <mergeCell ref="F47:H47"/>
+    <mergeCell ref="G66:H66"/>
   </mergeCells>
-  <conditionalFormatting sqref="C71:D73">
+  <conditionalFormatting sqref="C68:D70">
     <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Content - Adjust Dive missions
Former-commit-id: 6338a078178ef4a3591ed3a055968c85701f6212
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Missions.xlsx
+++ b/Docs/Content/HungryDragonContent_Missions.xlsx
@@ -1182,13 +1182,6 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1201,21 +1194,18 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="67">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -2277,6 +2267,16 @@
         </bottom>
       </border>
     </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -2291,97 +2291,97 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="missionDifficultyDefinitions" displayName="missionDifficultyDefinitions" ref="B67:K70" totalsRowShown="0" headerRowBorderDxfId="66" tableBorderDxfId="65">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="missionDifficultyDefinitions" displayName="missionDifficultyDefinitions" ref="B67:K70" totalsRowShown="0" headerRowBorderDxfId="65" tableBorderDxfId="64">
   <autoFilter ref="B67:K70"/>
   <tableColumns count="10">
     <tableColumn id="1" name="{missionDifficultyDefinitions}"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="64"/>
-    <tableColumn id="7" name="[index]" dataDxfId="63"/>
-    <tableColumn id="3" name="[dragonsToUnlock]" dataDxfId="62"/>
-    <tableColumn id="4" name="[cooldownMinutes]" dataDxfId="61"/>
-    <tableColumn id="9" name="[maxRewardCoins]" dataDxfId="60"/>
-    <tableColumn id="5" name="[removeMissionPCCoefA]" dataDxfId="59"/>
-    <tableColumn id="6" name="[removeMissionPCCoefB]" dataDxfId="58"/>
-    <tableColumn id="8" name="[tidName]" dataDxfId="57"/>
-    <tableColumn id="10" name="[color]" dataDxfId="56"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="63"/>
+    <tableColumn id="7" name="[index]" dataDxfId="62"/>
+    <tableColumn id="3" name="[dragonsToUnlock]" dataDxfId="61"/>
+    <tableColumn id="4" name="[cooldownMinutes]" dataDxfId="60"/>
+    <tableColumn id="9" name="[maxRewardCoins]" dataDxfId="59"/>
+    <tableColumn id="5" name="[removeMissionPCCoefA]" dataDxfId="58"/>
+    <tableColumn id="6" name="[removeMissionPCCoefB]" dataDxfId="57"/>
+    <tableColumn id="8" name="[tidName]" dataDxfId="56"/>
+    <tableColumn id="10" name="[color]" dataDxfId="55"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table13303132" displayName="Table13303132" ref="B75:E85" totalsRowShown="0" headerRowDxfId="55" dataDxfId="53" headerRowBorderDxfId="54" tableBorderDxfId="52" totalsRowBorderDxfId="51">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table13303132" displayName="Table13303132" ref="B75:E85" totalsRowShown="0" headerRowDxfId="54" dataDxfId="52" headerRowBorderDxfId="53" tableBorderDxfId="51" totalsRowBorderDxfId="50">
   <autoFilter ref="B75:E85"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="{missionDragonModifiersDefinitions}" dataDxfId="50"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="49"/>
-    <tableColumn id="7" name="[quantityModifier]" dataDxfId="48"/>
-    <tableColumn id="3" name="[missionSCRewardMultiplier]" dataDxfId="47"/>
+    <tableColumn id="1" name="{missionDragonModifiersDefinitions}" dataDxfId="49"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="48"/>
+    <tableColumn id="7" name="[quantityModifier]" dataDxfId="47"/>
+    <tableColumn id="3" name="[missionSCRewardMultiplier]" dataDxfId="46"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table1330313234" displayName="Table1330313234" ref="B89:D92" totalsRowShown="0" headerRowDxfId="46" dataDxfId="44" headerRowBorderDxfId="45" tableBorderDxfId="43" totalsRowBorderDxfId="42">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table1330313234" displayName="Table1330313234" ref="B89:D92" totalsRowShown="0" headerRowDxfId="45" dataDxfId="43" headerRowBorderDxfId="44" tableBorderDxfId="42" totalsRowBorderDxfId="41">
   <autoFilter ref="B89:D92"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="{missionDifficultyModifiersDefinitions}" dataDxfId="41"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="40"/>
-    <tableColumn id="7" name="[quantityModifier]" dataDxfId="39"/>
+    <tableColumn id="1" name="{missionDifficultyModifiersDefinitions}" dataDxfId="40"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="39"/>
+    <tableColumn id="7" name="[quantityModifier]" dataDxfId="38"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table133031323435" displayName="Table133031323435" ref="B96:D97" totalsRowShown="0" headerRowDxfId="38" dataDxfId="36" headerRowBorderDxfId="37" tableBorderDxfId="35" totalsRowBorderDxfId="34">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table133031323435" displayName="Table133031323435" ref="B96:D97" totalsRowShown="0" headerRowDxfId="37" dataDxfId="35" headerRowBorderDxfId="36" tableBorderDxfId="34" totalsRowBorderDxfId="33">
   <autoFilter ref="B96:D97"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="{missionOtherModifiersDefinitions}" dataDxfId="33"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="32"/>
-    <tableColumn id="7" name="[quantityModifier]" dataDxfId="31"/>
+    <tableColumn id="1" name="{missionOtherModifiersDefinitions}" dataDxfId="32"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="31"/>
+    <tableColumn id="7" name="[quantityModifier]" dataDxfId="30"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table13" displayName="Table13" ref="B48:H63" totalsRowShown="0" headerRowDxfId="30" dataDxfId="28" headerRowBorderDxfId="29" tableBorderDxfId="27" totalsRowBorderDxfId="26">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table13" displayName="Table13" ref="B48:H63" totalsRowShown="0" headerRowDxfId="29" dataDxfId="27" headerRowBorderDxfId="28" tableBorderDxfId="26" totalsRowBorderDxfId="25">
   <autoFilter ref="B48:H63"/>
   <tableColumns count="7">
-    <tableColumn id="1" name="{missionTypeDefinitions}" dataDxfId="25"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="24"/>
-    <tableColumn id="3" name="[minTier]" dataDxfId="23"/>
-    <tableColumn id="6" name="[maxTier]" dataDxfId="22"/>
-    <tableColumn id="4" name="[weight]" dataDxfId="21"/>
-    <tableColumn id="9" name="[tidDescSingleRun]" dataDxfId="20"/>
-    <tableColumn id="10" name="[tidDescMultiRun]" dataDxfId="19"/>
+    <tableColumn id="1" name="{missionTypeDefinitions}" dataDxfId="24"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="23"/>
+    <tableColumn id="3" name="[minTier]" dataDxfId="22"/>
+    <tableColumn id="6" name="[maxTier]" dataDxfId="21"/>
+    <tableColumn id="4" name="[weight]" dataDxfId="20"/>
+    <tableColumn id="9" name="[tidDescSingleRun]" dataDxfId="19"/>
+    <tableColumn id="10" name="[tidDescMultiRun]" dataDxfId="18"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table1330" displayName="Table1330" ref="B4:N43" totalsRowShown="0" headerRowDxfId="18" dataDxfId="16" headerRowBorderDxfId="17" tableBorderDxfId="15" totalsRowBorderDxfId="14">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table1330" displayName="Table1330" ref="B4:N43" totalsRowShown="0" headerRowDxfId="17" dataDxfId="15" headerRowBorderDxfId="16" tableBorderDxfId="14" totalsRowBorderDxfId="13">
   <autoFilter ref="B4:N43"/>
   <sortState ref="B5:N43">
     <sortCondition descending="1" ref="H4:H43"/>
   </sortState>
   <tableColumns count="13">
-    <tableColumn id="1" name="{missionsDefinitions}" dataDxfId="13"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="12"/>
-    <tableColumn id="7" name="[type]" dataDxfId="11"/>
-    <tableColumn id="8" name="[weight]" dataDxfId="10"/>
-    <tableColumn id="13" name="[singleRunChance]" dataDxfId="9"/>
-    <tableColumn id="11" name="[minTier]" dataDxfId="8"/>
-    <tableColumn id="12" name="[maxTier]" dataDxfId="7"/>
-    <tableColumn id="6" name="[params]" dataDxfId="6"/>
-    <tableColumn id="3" name="[objectiveBaseQuantityMin]" dataDxfId="5"/>
-    <tableColumn id="9" name="[objectiveBaseQuantityMax]" dataDxfId="4"/>
-    <tableColumn id="4" name="[icon]" dataDxfId="3"/>
-    <tableColumn id="5" name="[tidObjective]" dataDxfId="2"/>
-    <tableColumn id="10" name="[trackingSku]" dataDxfId="1"/>
+    <tableColumn id="1" name="{missionsDefinitions}" dataDxfId="12"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="11"/>
+    <tableColumn id="7" name="[type]" dataDxfId="10"/>
+    <tableColumn id="8" name="[weight]" dataDxfId="9"/>
+    <tableColumn id="13" name="[singleRunChance]" dataDxfId="8"/>
+    <tableColumn id="11" name="[minTier]" dataDxfId="7"/>
+    <tableColumn id="12" name="[maxTier]" dataDxfId="6"/>
+    <tableColumn id="6" name="[params]" dataDxfId="5"/>
+    <tableColumn id="3" name="[objectiveBaseQuantityMin]" dataDxfId="4"/>
+    <tableColumn id="9" name="[objectiveBaseQuantityMax]" dataDxfId="3"/>
+    <tableColumn id="4" name="[icon]" dataDxfId="2"/>
+    <tableColumn id="5" name="[tidObjective]" dataDxfId="1"/>
+    <tableColumn id="10" name="[trackingSku]" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2655,8 +2655,8 @@
   </sheetPr>
   <dimension ref="B1:P97"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="H33" sqref="B9:H33"/>
+    <sheetView tabSelected="1" topLeftCell="H7" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2702,14 +2702,14 @@
         <v>144</v>
       </c>
       <c r="G3" s="38"/>
-      <c r="J3" s="54" t="s">
+      <c r="J3" s="58" t="s">
         <v>143</v>
       </c>
-      <c r="K3" s="54"/>
-      <c r="M3" s="54"/>
-      <c r="N3" s="54"/>
-      <c r="O3" s="54"/>
-      <c r="P3" s="54"/>
+      <c r="K3" s="58"/>
+      <c r="M3" s="58"/>
+      <c r="N3" s="58"/>
+      <c r="O3" s="58"/>
+      <c r="P3" s="58"/>
     </row>
     <row r="4" spans="2:16" ht="106.5" x14ac:dyDescent="0.25">
       <c r="B4" s="30" t="s">
@@ -3133,10 +3133,10 @@
       </c>
       <c r="I14" s="24"/>
       <c r="J14" s="24">
-        <v>700</v>
+        <v>350</v>
       </c>
       <c r="K14" s="33">
-        <v>800</v>
+        <v>400</v>
       </c>
       <c r="L14" s="33" t="s">
         <v>112</v>
@@ -3377,7 +3377,7 @@
       <c r="L20" s="34" t="s">
         <v>92</v>
       </c>
-      <c r="M20" s="58" t="s">
+      <c r="M20" s="55" t="s">
         <v>163</v>
       </c>
       <c r="N20" s="31" t="s">
@@ -3686,7 +3686,7 @@
       <c r="G28" s="51">
         <v>0</v>
       </c>
-      <c r="H28" s="57">
+      <c r="H28" s="54">
         <v>7</v>
       </c>
       <c r="I28" s="52" t="s">
@@ -3698,10 +3698,10 @@
       <c r="K28" s="52">
         <v>9</v>
       </c>
-      <c r="L28" s="57" t="s">
+      <c r="L28" s="54" t="s">
         <v>204</v>
       </c>
-      <c r="M28" s="57" t="s">
+      <c r="M28" s="54" t="s">
         <v>160</v>
       </c>
       <c r="N28" s="53" t="s">
@@ -3727,7 +3727,7 @@
       <c r="G29" s="51">
         <v>0</v>
       </c>
-      <c r="H29" s="57">
+      <c r="H29" s="54">
         <v>7</v>
       </c>
       <c r="I29" s="52"/>
@@ -3737,10 +3737,10 @@
       <c r="K29" s="52">
         <v>55</v>
       </c>
-      <c r="L29" s="57" t="s">
+      <c r="L29" s="54" t="s">
         <v>205</v>
       </c>
-      <c r="M29" s="57" t="s">
+      <c r="M29" s="54" t="s">
         <v>219</v>
       </c>
       <c r="N29" s="53" t="s">
@@ -3766,7 +3766,7 @@
       <c r="G30" s="51">
         <v>3</v>
       </c>
-      <c r="H30" s="57">
+      <c r="H30" s="54">
         <v>7</v>
       </c>
       <c r="I30" s="52" t="s">
@@ -3778,10 +3778,10 @@
       <c r="K30" s="52">
         <v>4.5</v>
       </c>
-      <c r="L30" s="57" t="s">
+      <c r="L30" s="54" t="s">
         <v>206</v>
       </c>
-      <c r="M30" s="57" t="s">
+      <c r="M30" s="54" t="s">
         <v>169</v>
       </c>
       <c r="N30" s="53" t="s">
@@ -3807,7 +3807,7 @@
       <c r="G31" s="51">
         <v>3</v>
       </c>
-      <c r="H31" s="57">
+      <c r="H31" s="54">
         <v>7</v>
       </c>
       <c r="I31" s="52" t="s">
@@ -4064,7 +4064,7 @@
       <c r="L37" s="33" t="s">
         <v>101</v>
       </c>
-      <c r="M37" s="60" t="s">
+      <c r="M37" s="57" t="s">
         <v>155</v>
       </c>
       <c r="N37" s="31" t="s">
@@ -4265,7 +4265,7 @@
       <c r="L42" s="33" t="s">
         <v>118</v>
       </c>
-      <c r="M42" s="59" t="s">
+      <c r="M42" s="56" t="s">
         <v>157</v>
       </c>
       <c r="N42" s="31" t="s">
@@ -4362,9 +4362,9 @@
       <c r="C47" s="20"/>
       <c r="D47" s="20"/>
       <c r="E47" s="20"/>
-      <c r="F47" s="55"/>
-      <c r="G47" s="55"/>
-      <c r="H47" s="55"/>
+      <c r="F47" s="59"/>
+      <c r="G47" s="59"/>
+      <c r="H47" s="59"/>
       <c r="I47" s="20"/>
       <c r="J47" s="20"/>
     </row>
@@ -4759,10 +4759,10 @@
       <c r="F66" s="21" t="s">
         <v>40</v>
       </c>
-      <c r="G66" s="56" t="s">
+      <c r="G66" s="60" t="s">
         <v>39</v>
       </c>
-      <c r="H66" s="56"/>
+      <c r="H66" s="60"/>
       <c r="I66" s="20"/>
     </row>
     <row r="67" spans="2:13" ht="142.5" x14ac:dyDescent="0.25">
@@ -5154,7 +5154,7 @@
     <mergeCell ref="G66:H66"/>
   </mergeCells>
   <conditionalFormatting sqref="C68:D70">
-    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="66" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Content - Add jawfrey coefficient for generating missions
Former-commit-id: 609dcb2fb7217e8c3c6bcb9054258059c723fb71
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Missions.xlsx
+++ b/Docs/Content/HungryDragonContent_Missions.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="404" uniqueCount="221">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="406" uniqueCount="222">
   <si>
     <t>single_run</t>
   </si>
@@ -712,6 +712,9 @@
   </si>
   <si>
     <t>TID_EDIBLE_WITCH_PL</t>
+  </si>
+  <si>
+    <t>dragon_jawfrey</t>
   </si>
 </sst>
 </file>
@@ -1207,6 +1210,16 @@
   </cellStyles>
   <dxfs count="67">
     <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -2267,16 +2280,6 @@
         </bottom>
       </border>
     </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -2291,97 +2294,97 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="missionDifficultyDefinitions" displayName="missionDifficultyDefinitions" ref="B67:K70" totalsRowShown="0" headerRowBorderDxfId="65" tableBorderDxfId="64">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="missionDifficultyDefinitions" displayName="missionDifficultyDefinitions" ref="B67:K70" totalsRowShown="0" headerRowBorderDxfId="66" tableBorderDxfId="65">
   <autoFilter ref="B67:K70"/>
   <tableColumns count="10">
     <tableColumn id="1" name="{missionDifficultyDefinitions}"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="63"/>
-    <tableColumn id="7" name="[index]" dataDxfId="62"/>
-    <tableColumn id="3" name="[dragonsToUnlock]" dataDxfId="61"/>
-    <tableColumn id="4" name="[cooldownMinutes]" dataDxfId="60"/>
-    <tableColumn id="9" name="[maxRewardCoins]" dataDxfId="59"/>
-    <tableColumn id="5" name="[removeMissionPCCoefA]" dataDxfId="58"/>
-    <tableColumn id="6" name="[removeMissionPCCoefB]" dataDxfId="57"/>
-    <tableColumn id="8" name="[tidName]" dataDxfId="56"/>
-    <tableColumn id="10" name="[color]" dataDxfId="55"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="64"/>
+    <tableColumn id="7" name="[index]" dataDxfId="63"/>
+    <tableColumn id="3" name="[dragonsToUnlock]" dataDxfId="62"/>
+    <tableColumn id="4" name="[cooldownMinutes]" dataDxfId="61"/>
+    <tableColumn id="9" name="[maxRewardCoins]" dataDxfId="60"/>
+    <tableColumn id="5" name="[removeMissionPCCoefA]" dataDxfId="59"/>
+    <tableColumn id="6" name="[removeMissionPCCoefB]" dataDxfId="58"/>
+    <tableColumn id="8" name="[tidName]" dataDxfId="57"/>
+    <tableColumn id="10" name="[color]" dataDxfId="56"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table13303132" displayName="Table13303132" ref="B75:E85" totalsRowShown="0" headerRowDxfId="54" dataDxfId="52" headerRowBorderDxfId="53" tableBorderDxfId="51" totalsRowBorderDxfId="50">
-  <autoFilter ref="B75:E85"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table13303132" displayName="Table13303132" ref="B75:E86" totalsRowShown="0" headerRowDxfId="55" dataDxfId="53" headerRowBorderDxfId="54" tableBorderDxfId="52" totalsRowBorderDxfId="51">
+  <autoFilter ref="B75:E86"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="{missionDragonModifiersDefinitions}" dataDxfId="49"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="48"/>
-    <tableColumn id="7" name="[quantityModifier]" dataDxfId="47"/>
-    <tableColumn id="3" name="[missionSCRewardMultiplier]" dataDxfId="46"/>
+    <tableColumn id="1" name="{missionDragonModifiersDefinitions}" dataDxfId="50"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="49"/>
+    <tableColumn id="7" name="[quantityModifier]" dataDxfId="48"/>
+    <tableColumn id="3" name="[missionSCRewardMultiplier]" dataDxfId="47"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table1330313234" displayName="Table1330313234" ref="B89:D92" totalsRowShown="0" headerRowDxfId="45" dataDxfId="43" headerRowBorderDxfId="44" tableBorderDxfId="42" totalsRowBorderDxfId="41">
-  <autoFilter ref="B89:D92"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table1330313234" displayName="Table1330313234" ref="B90:D93" totalsRowShown="0" headerRowDxfId="46" dataDxfId="44" headerRowBorderDxfId="45" tableBorderDxfId="43" totalsRowBorderDxfId="42">
+  <autoFilter ref="B90:D93"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="{missionDifficultyModifiersDefinitions}" dataDxfId="40"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="39"/>
-    <tableColumn id="7" name="[quantityModifier]" dataDxfId="38"/>
+    <tableColumn id="1" name="{missionDifficultyModifiersDefinitions}" dataDxfId="41"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="40"/>
+    <tableColumn id="7" name="[quantityModifier]" dataDxfId="39"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table133031323435" displayName="Table133031323435" ref="B96:D97" totalsRowShown="0" headerRowDxfId="37" dataDxfId="35" headerRowBorderDxfId="36" tableBorderDxfId="34" totalsRowBorderDxfId="33">
-  <autoFilter ref="B96:D97"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table133031323435" displayName="Table133031323435" ref="B97:D98" totalsRowShown="0" headerRowDxfId="38" dataDxfId="36" headerRowBorderDxfId="37" tableBorderDxfId="35" totalsRowBorderDxfId="34">
+  <autoFilter ref="B97:D98"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="{missionOtherModifiersDefinitions}" dataDxfId="32"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="31"/>
-    <tableColumn id="7" name="[quantityModifier]" dataDxfId="30"/>
+    <tableColumn id="1" name="{missionOtherModifiersDefinitions}" dataDxfId="33"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="32"/>
+    <tableColumn id="7" name="[quantityModifier]" dataDxfId="31"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table13" displayName="Table13" ref="B48:H63" totalsRowShown="0" headerRowDxfId="29" dataDxfId="27" headerRowBorderDxfId="28" tableBorderDxfId="26" totalsRowBorderDxfId="25">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table13" displayName="Table13" ref="B48:H63" totalsRowShown="0" headerRowDxfId="30" dataDxfId="28" headerRowBorderDxfId="29" tableBorderDxfId="27" totalsRowBorderDxfId="26">
   <autoFilter ref="B48:H63"/>
   <tableColumns count="7">
-    <tableColumn id="1" name="{missionTypeDefinitions}" dataDxfId="24"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="23"/>
-    <tableColumn id="3" name="[minTier]" dataDxfId="22"/>
-    <tableColumn id="6" name="[maxTier]" dataDxfId="21"/>
-    <tableColumn id="4" name="[weight]" dataDxfId="20"/>
-    <tableColumn id="9" name="[tidDescSingleRun]" dataDxfId="19"/>
-    <tableColumn id="10" name="[tidDescMultiRun]" dataDxfId="18"/>
+    <tableColumn id="1" name="{missionTypeDefinitions}" dataDxfId="25"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="24"/>
+    <tableColumn id="3" name="[minTier]" dataDxfId="23"/>
+    <tableColumn id="6" name="[maxTier]" dataDxfId="22"/>
+    <tableColumn id="4" name="[weight]" dataDxfId="21"/>
+    <tableColumn id="9" name="[tidDescSingleRun]" dataDxfId="20"/>
+    <tableColumn id="10" name="[tidDescMultiRun]" dataDxfId="19"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table1330" displayName="Table1330" ref="B4:N43" totalsRowShown="0" headerRowDxfId="17" dataDxfId="15" headerRowBorderDxfId="16" tableBorderDxfId="14" totalsRowBorderDxfId="13">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table1330" displayName="Table1330" ref="B4:N43" totalsRowShown="0" headerRowDxfId="18" dataDxfId="16" headerRowBorderDxfId="17" tableBorderDxfId="15" totalsRowBorderDxfId="14">
   <autoFilter ref="B4:N43"/>
   <sortState ref="B5:N43">
     <sortCondition descending="1" ref="H4:H43"/>
   </sortState>
   <tableColumns count="13">
-    <tableColumn id="1" name="{missionsDefinitions}" dataDxfId="12"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="11"/>
-    <tableColumn id="7" name="[type]" dataDxfId="10"/>
-    <tableColumn id="8" name="[weight]" dataDxfId="9"/>
-    <tableColumn id="13" name="[singleRunChance]" dataDxfId="8"/>
-    <tableColumn id="11" name="[minTier]" dataDxfId="7"/>
-    <tableColumn id="12" name="[maxTier]" dataDxfId="6"/>
-    <tableColumn id="6" name="[params]" dataDxfId="5"/>
-    <tableColumn id="3" name="[objectiveBaseQuantityMin]" dataDxfId="4"/>
-    <tableColumn id="9" name="[objectiveBaseQuantityMax]" dataDxfId="3"/>
-    <tableColumn id="4" name="[icon]" dataDxfId="2"/>
-    <tableColumn id="5" name="[tidObjective]" dataDxfId="1"/>
-    <tableColumn id="10" name="[trackingSku]" dataDxfId="0"/>
+    <tableColumn id="1" name="{missionsDefinitions}" dataDxfId="13"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="12"/>
+    <tableColumn id="7" name="[type]" dataDxfId="11"/>
+    <tableColumn id="8" name="[weight]" dataDxfId="10"/>
+    <tableColumn id="13" name="[singleRunChance]" dataDxfId="9"/>
+    <tableColumn id="11" name="[minTier]" dataDxfId="8"/>
+    <tableColumn id="12" name="[maxTier]" dataDxfId="7"/>
+    <tableColumn id="6" name="[params]" dataDxfId="6"/>
+    <tableColumn id="3" name="[objectiveBaseQuantityMin]" dataDxfId="5"/>
+    <tableColumn id="9" name="[objectiveBaseQuantityMax]" dataDxfId="4"/>
+    <tableColumn id="4" name="[icon]" dataDxfId="3"/>
+    <tableColumn id="5" name="[tidObjective]" dataDxfId="2"/>
+    <tableColumn id="10" name="[trackingSku]" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2653,10 +2656,10 @@
   <sheetPr>
     <tabColor theme="6"/>
   </sheetPr>
-  <dimension ref="B1:P97"/>
+  <dimension ref="B1:P98"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H7" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
+    <sheetView tabSelected="1" topLeftCell="A73" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F79" sqref="F79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5035,13 +5038,13 @@
         <v>1</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>12</v>
+        <v>221</v>
       </c>
       <c r="D84" s="1">
-        <v>5</v>
+        <v>4.5</v>
       </c>
       <c r="E84" s="1">
-        <v>67</v>
+        <v>62</v>
       </c>
     </row>
     <row r="85" spans="2:7" x14ac:dyDescent="0.25">
@@ -5049,46 +5052,49 @@
         <v>1</v>
       </c>
       <c r="C85" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D85" s="1">
+        <v>5</v>
+      </c>
+      <c r="E85" s="1">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="86" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B86" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C86" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D85" s="1">
+      <c r="D86" s="1">
         <v>7</v>
       </c>
-      <c r="E85" s="1">
+      <c r="E86" s="1">
         <v>80</v>
       </c>
     </row>
-    <row r="86" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="87" spans="2:7" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B87" s="6" t="s">
+    <row r="87" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="88" spans="2:7" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B88" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C87" s="6"/>
-      <c r="D87" s="6"/>
-      <c r="E87" s="6"/>
-      <c r="F87" s="6"/>
-      <c r="G87" s="6"/>
-    </row>
-    <row r="89" spans="2:7" ht="142.5" x14ac:dyDescent="0.25">
-      <c r="B89" s="5" t="s">
+      <c r="C88" s="6"/>
+      <c r="D88" s="6"/>
+      <c r="E88" s="6"/>
+      <c r="F88" s="6"/>
+      <c r="G88" s="6"/>
+    </row>
+    <row r="90" spans="2:7" ht="142.5" x14ac:dyDescent="0.25">
+      <c r="B90" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C89" s="4" t="s">
+      <c r="C90" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D89" s="3" t="s">
+      <c r="D90" s="3" t="s">
         <v>2</v>
-      </c>
-    </row>
-    <row r="90" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B90" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C90" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D90" s="1">
-        <v>0.05</v>
       </c>
     </row>
     <row r="91" spans="2:7" x14ac:dyDescent="0.25">
@@ -5096,10 +5102,10 @@
         <v>1</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D91" s="1">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="92" spans="2:7" x14ac:dyDescent="0.25">
@@ -5107,42 +5113,53 @@
         <v>1</v>
       </c>
       <c r="C92" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D92" s="1">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="93" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B93" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C93" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D92" s="1">
+      <c r="D93" s="1">
         <v>0.2</v>
       </c>
     </row>
-    <row r="93" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="94" spans="2:7" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B94" s="6" t="s">
+    <row r="94" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="95" spans="2:7" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B95" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C94" s="6"/>
-      <c r="D94" s="6"/>
-      <c r="E94" s="6"/>
-      <c r="F94" s="6"/>
-      <c r="G94" s="6"/>
-    </row>
-    <row r="96" spans="2:7" ht="132" x14ac:dyDescent="0.25">
-      <c r="B96" s="5" t="s">
+      <c r="C95" s="6"/>
+      <c r="D95" s="6"/>
+      <c r="E95" s="6"/>
+      <c r="F95" s="6"/>
+      <c r="G95" s="6"/>
+    </row>
+    <row r="97" spans="2:4" ht="132" x14ac:dyDescent="0.25">
+      <c r="B97" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C96" s="4" t="s">
+      <c r="C97" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D96" s="3" t="s">
+      <c r="D97" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="97" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B97" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C97" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D97" s="1">
+    <row r="98" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B98" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C98" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D98" s="1">
         <v>0.7</v>
       </c>
     </row>
@@ -5154,7 +5171,7 @@
     <mergeCell ref="G66:H66"/>
   </mergeCells>
   <conditionalFormatting sqref="C68:D70">
-    <cfRule type="duplicateValues" dxfId="66" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Content - Missing tids and Jawfrey balance
Former-commit-id: 8a10214904585f2b5c1fd7ed4ab0124bcd871217
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Missions.xlsx
+++ b/Docs/Content/HungryDragonContent_Missions.xlsx
@@ -561,9 +561,6 @@
     <t>TID_EDIBLE_STINGRAY_PL</t>
   </si>
   <si>
-    <t>TID_MISSION_TARGET_BOATMAN</t>
-  </si>
-  <si>
     <t>TID_MISSION_TARGET_BIRDSPREY</t>
   </si>
   <si>
@@ -715,6 +712,9 @@
   </si>
   <si>
     <t>dragon_jawfrey</t>
+  </si>
+  <si>
+    <t>TID_MISSION_TARGET_BOATMAN_PL</t>
   </si>
 </sst>
 </file>
@@ -1210,16 +1210,6 @@
   </cellStyles>
   <dxfs count="67">
     <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -2280,6 +2270,16 @@
         </bottom>
       </border>
     </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -2294,97 +2294,97 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="missionDifficultyDefinitions" displayName="missionDifficultyDefinitions" ref="B67:K70" totalsRowShown="0" headerRowBorderDxfId="66" tableBorderDxfId="65">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="missionDifficultyDefinitions" displayName="missionDifficultyDefinitions" ref="B67:K70" totalsRowShown="0" headerRowBorderDxfId="65" tableBorderDxfId="64">
   <autoFilter ref="B67:K70"/>
   <tableColumns count="10">
     <tableColumn id="1" name="{missionDifficultyDefinitions}"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="64"/>
-    <tableColumn id="7" name="[index]" dataDxfId="63"/>
-    <tableColumn id="3" name="[dragonsToUnlock]" dataDxfId="62"/>
-    <tableColumn id="4" name="[cooldownMinutes]" dataDxfId="61"/>
-    <tableColumn id="9" name="[maxRewardCoins]" dataDxfId="60"/>
-    <tableColumn id="5" name="[removeMissionPCCoefA]" dataDxfId="59"/>
-    <tableColumn id="6" name="[removeMissionPCCoefB]" dataDxfId="58"/>
-    <tableColumn id="8" name="[tidName]" dataDxfId="57"/>
-    <tableColumn id="10" name="[color]" dataDxfId="56"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="63"/>
+    <tableColumn id="7" name="[index]" dataDxfId="62"/>
+    <tableColumn id="3" name="[dragonsToUnlock]" dataDxfId="61"/>
+    <tableColumn id="4" name="[cooldownMinutes]" dataDxfId="60"/>
+    <tableColumn id="9" name="[maxRewardCoins]" dataDxfId="59"/>
+    <tableColumn id="5" name="[removeMissionPCCoefA]" dataDxfId="58"/>
+    <tableColumn id="6" name="[removeMissionPCCoefB]" dataDxfId="57"/>
+    <tableColumn id="8" name="[tidName]" dataDxfId="56"/>
+    <tableColumn id="10" name="[color]" dataDxfId="55"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table13303132" displayName="Table13303132" ref="B75:E86" totalsRowShown="0" headerRowDxfId="55" dataDxfId="53" headerRowBorderDxfId="54" tableBorderDxfId="52" totalsRowBorderDxfId="51">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table13303132" displayName="Table13303132" ref="B75:E86" totalsRowShown="0" headerRowDxfId="54" dataDxfId="52" headerRowBorderDxfId="53" tableBorderDxfId="51" totalsRowBorderDxfId="50">
   <autoFilter ref="B75:E86"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="{missionDragonModifiersDefinitions}" dataDxfId="50"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="49"/>
-    <tableColumn id="7" name="[quantityModifier]" dataDxfId="48"/>
-    <tableColumn id="3" name="[missionSCRewardMultiplier]" dataDxfId="47"/>
+    <tableColumn id="1" name="{missionDragonModifiersDefinitions}" dataDxfId="49"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="48"/>
+    <tableColumn id="7" name="[quantityModifier]" dataDxfId="47"/>
+    <tableColumn id="3" name="[missionSCRewardMultiplier]" dataDxfId="46"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table1330313234" displayName="Table1330313234" ref="B90:D93" totalsRowShown="0" headerRowDxfId="46" dataDxfId="44" headerRowBorderDxfId="45" tableBorderDxfId="43" totalsRowBorderDxfId="42">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table1330313234" displayName="Table1330313234" ref="B90:D93" totalsRowShown="0" headerRowDxfId="45" dataDxfId="43" headerRowBorderDxfId="44" tableBorderDxfId="42" totalsRowBorderDxfId="41">
   <autoFilter ref="B90:D93"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="{missionDifficultyModifiersDefinitions}" dataDxfId="41"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="40"/>
-    <tableColumn id="7" name="[quantityModifier]" dataDxfId="39"/>
+    <tableColumn id="1" name="{missionDifficultyModifiersDefinitions}" dataDxfId="40"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="39"/>
+    <tableColumn id="7" name="[quantityModifier]" dataDxfId="38"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table133031323435" displayName="Table133031323435" ref="B97:D98" totalsRowShown="0" headerRowDxfId="38" dataDxfId="36" headerRowBorderDxfId="37" tableBorderDxfId="35" totalsRowBorderDxfId="34">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table133031323435" displayName="Table133031323435" ref="B97:D98" totalsRowShown="0" headerRowDxfId="37" dataDxfId="35" headerRowBorderDxfId="36" tableBorderDxfId="34" totalsRowBorderDxfId="33">
   <autoFilter ref="B97:D98"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="{missionOtherModifiersDefinitions}" dataDxfId="33"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="32"/>
-    <tableColumn id="7" name="[quantityModifier]" dataDxfId="31"/>
+    <tableColumn id="1" name="{missionOtherModifiersDefinitions}" dataDxfId="32"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="31"/>
+    <tableColumn id="7" name="[quantityModifier]" dataDxfId="30"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table13" displayName="Table13" ref="B48:H63" totalsRowShown="0" headerRowDxfId="30" dataDxfId="28" headerRowBorderDxfId="29" tableBorderDxfId="27" totalsRowBorderDxfId="26">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table13" displayName="Table13" ref="B48:H63" totalsRowShown="0" headerRowDxfId="29" dataDxfId="27" headerRowBorderDxfId="28" tableBorderDxfId="26" totalsRowBorderDxfId="25">
   <autoFilter ref="B48:H63"/>
   <tableColumns count="7">
-    <tableColumn id="1" name="{missionTypeDefinitions}" dataDxfId="25"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="24"/>
-    <tableColumn id="3" name="[minTier]" dataDxfId="23"/>
-    <tableColumn id="6" name="[maxTier]" dataDxfId="22"/>
-    <tableColumn id="4" name="[weight]" dataDxfId="21"/>
-    <tableColumn id="9" name="[tidDescSingleRun]" dataDxfId="20"/>
-    <tableColumn id="10" name="[tidDescMultiRun]" dataDxfId="19"/>
+    <tableColumn id="1" name="{missionTypeDefinitions}" dataDxfId="24"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="23"/>
+    <tableColumn id="3" name="[minTier]" dataDxfId="22"/>
+    <tableColumn id="6" name="[maxTier]" dataDxfId="21"/>
+    <tableColumn id="4" name="[weight]" dataDxfId="20"/>
+    <tableColumn id="9" name="[tidDescSingleRun]" dataDxfId="19"/>
+    <tableColumn id="10" name="[tidDescMultiRun]" dataDxfId="18"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table1330" displayName="Table1330" ref="B4:N43" totalsRowShown="0" headerRowDxfId="18" dataDxfId="16" headerRowBorderDxfId="17" tableBorderDxfId="15" totalsRowBorderDxfId="14">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table1330" displayName="Table1330" ref="B4:N43" totalsRowShown="0" headerRowDxfId="17" dataDxfId="15" headerRowBorderDxfId="16" tableBorderDxfId="14" totalsRowBorderDxfId="13">
   <autoFilter ref="B4:N43"/>
   <sortState ref="B5:N43">
     <sortCondition descending="1" ref="H4:H43"/>
   </sortState>
   <tableColumns count="13">
-    <tableColumn id="1" name="{missionsDefinitions}" dataDxfId="13"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="12"/>
-    <tableColumn id="7" name="[type]" dataDxfId="11"/>
-    <tableColumn id="8" name="[weight]" dataDxfId="10"/>
-    <tableColumn id="13" name="[singleRunChance]" dataDxfId="9"/>
-    <tableColumn id="11" name="[minTier]" dataDxfId="8"/>
-    <tableColumn id="12" name="[maxTier]" dataDxfId="7"/>
-    <tableColumn id="6" name="[params]" dataDxfId="6"/>
-    <tableColumn id="3" name="[objectiveBaseQuantityMin]" dataDxfId="5"/>
-    <tableColumn id="9" name="[objectiveBaseQuantityMax]" dataDxfId="4"/>
-    <tableColumn id="4" name="[icon]" dataDxfId="3"/>
-    <tableColumn id="5" name="[tidObjective]" dataDxfId="2"/>
-    <tableColumn id="10" name="[trackingSku]" dataDxfId="1"/>
+    <tableColumn id="1" name="{missionsDefinitions}" dataDxfId="12"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="11"/>
+    <tableColumn id="7" name="[type]" dataDxfId="10"/>
+    <tableColumn id="8" name="[weight]" dataDxfId="9"/>
+    <tableColumn id="13" name="[singleRunChance]" dataDxfId="8"/>
+    <tableColumn id="11" name="[minTier]" dataDxfId="7"/>
+    <tableColumn id="12" name="[maxTier]" dataDxfId="6"/>
+    <tableColumn id="6" name="[params]" dataDxfId="5"/>
+    <tableColumn id="3" name="[objectiveBaseQuantityMin]" dataDxfId="4"/>
+    <tableColumn id="9" name="[objectiveBaseQuantityMax]" dataDxfId="3"/>
+    <tableColumn id="4" name="[icon]" dataDxfId="2"/>
+    <tableColumn id="5" name="[tidObjective]" dataDxfId="1"/>
+    <tableColumn id="10" name="[trackingSku]" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2658,8 +2658,8 @@
   </sheetPr>
   <dimension ref="B1:P98"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A73" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F79" sqref="F79"/>
+    <sheetView tabSelected="1" topLeftCell="J7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M22" sqref="M22:M23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2673,7 +2673,7 @@
     <col min="9" max="9" width="59.85546875" bestFit="1" customWidth="1"/>
     <col min="10" max="11" width="18.7109375" customWidth="1"/>
     <col min="12" max="12" width="23.5703125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="32.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="34.42578125" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="8.42578125" customWidth="1"/>
     <col min="15" max="16" width="15" customWidth="1"/>
   </cols>
@@ -3433,7 +3433,7 @@
         <v>1</v>
       </c>
       <c r="C22" s="24" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D22" s="23" t="s">
         <v>65</v>
@@ -3504,7 +3504,7 @@
         <v>84</v>
       </c>
       <c r="M23" s="34" t="s">
-        <v>170</v>
+        <v>221</v>
       </c>
       <c r="N23" s="31" t="s">
         <v>73</v>
@@ -3675,10 +3675,10 @@
         <v>1</v>
       </c>
       <c r="C28" s="51" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D28" s="52" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E28" s="52">
         <v>0</v>
@@ -3702,7 +3702,7 @@
         <v>9</v>
       </c>
       <c r="L28" s="54" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="M28" s="54" t="s">
         <v>160</v>
@@ -3716,7 +3716,7 @@
         <v>1</v>
       </c>
       <c r="C29" s="51" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D29" s="52" t="s">
         <v>149</v>
@@ -3741,10 +3741,10 @@
         <v>55</v>
       </c>
       <c r="L29" s="54" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="M29" s="54" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="N29" s="53" t="s">
         <v>73</v>
@@ -3755,7 +3755,7 @@
         <v>1</v>
       </c>
       <c r="C30" s="51" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D30" s="52" t="s">
         <v>149</v>
@@ -3773,7 +3773,7 @@
         <v>7</v>
       </c>
       <c r="I30" s="52" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="J30" s="51">
         <v>4</v>
@@ -3782,7 +3782,7 @@
         <v>4.5</v>
       </c>
       <c r="L30" s="54" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="M30" s="54" t="s">
         <v>169</v>
@@ -3796,7 +3796,7 @@
         <v>1</v>
       </c>
       <c r="C31" s="51" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D31" s="52" t="s">
         <v>149</v>
@@ -3814,7 +3814,7 @@
         <v>7</v>
       </c>
       <c r="I31" s="52" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="J31" s="51">
         <v>5</v>
@@ -3823,10 +3823,10 @@
         <v>5.5</v>
       </c>
       <c r="L31" s="48" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="M31" s="48" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="N31" s="53" t="s">
         <v>73</v>
@@ -3837,7 +3837,7 @@
         <v>1</v>
       </c>
       <c r="C32" s="51" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D32" s="52" t="s">
         <v>149</v>
@@ -3864,7 +3864,7 @@
         <v>18</v>
       </c>
       <c r="L32" s="48" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="M32" s="48" t="s">
         <v>159</v>
@@ -3878,10 +3878,10 @@
         <v>1</v>
       </c>
       <c r="C33" s="40" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D33" s="41" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="E33" s="52">
         <v>0</v>
@@ -3903,7 +3903,7 @@
         <v>27</v>
       </c>
       <c r="L33" s="48" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="M33" s="48"/>
       <c r="N33" s="53" t="s">
@@ -3956,7 +3956,7 @@
         <v>1</v>
       </c>
       <c r="C35" s="51" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D35" s="52" t="s">
         <v>149</v>
@@ -3974,7 +3974,7 @@
         <v>3</v>
       </c>
       <c r="I35" s="52" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="J35" s="51">
         <v>3</v>
@@ -3983,10 +3983,10 @@
         <v>4</v>
       </c>
       <c r="L35" s="48" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="M35" s="49" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="N35" s="53" t="s">
         <v>73</v>
@@ -3997,7 +3997,7 @@
         <v>1</v>
       </c>
       <c r="C36" s="51" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D36" s="52" t="s">
         <v>149</v>
@@ -4024,7 +4024,7 @@
         <v>27</v>
       </c>
       <c r="L36" s="48" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="M36" s="52" t="s">
         <v>151</v>
@@ -4079,10 +4079,10 @@
         <v>1</v>
       </c>
       <c r="C38" s="51" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D38" s="52" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="E38" s="52">
         <v>0</v>
@@ -4106,7 +4106,7 @@
         <v>160</v>
       </c>
       <c r="L38" s="48" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="M38" s="49" t="s">
         <v>151</v>
@@ -4120,10 +4120,10 @@
         <v>1</v>
       </c>
       <c r="C39" s="51" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D39" s="52" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="E39" s="52">
         <v>0</v>
@@ -4147,7 +4147,7 @@
         <v>16</v>
       </c>
       <c r="L39" s="48" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="M39" s="48" t="s">
         <v>153</v>
@@ -4161,7 +4161,7 @@
         <v>1</v>
       </c>
       <c r="C40" s="51" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D40" s="52" t="s">
         <v>149</v>
@@ -4179,7 +4179,7 @@
         <v>2</v>
       </c>
       <c r="I40" s="52" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="J40" s="51">
         <v>3</v>
@@ -4188,10 +4188,10 @@
         <v>3</v>
       </c>
       <c r="L40" s="48" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="M40" s="48" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="N40" s="53" t="s">
         <v>73</v>
@@ -4202,10 +4202,10 @@
         <v>1</v>
       </c>
       <c r="C41" s="40" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D41" s="41" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="E41" s="52">
         <v>1</v>
@@ -4227,7 +4227,7 @@
         <v>52</v>
       </c>
       <c r="L41" s="48" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="M41" s="42"/>
       <c r="N41" s="53" t="s">
@@ -4583,7 +4583,7 @@
         <v>1</v>
       </c>
       <c r="C57" s="41" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D57" s="41">
         <v>0</v>
@@ -4595,10 +4595,10 @@
         <v>0</v>
       </c>
       <c r="G57" s="42" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="H57" s="42" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="58" spans="2:8" x14ac:dyDescent="0.25">
@@ -4606,7 +4606,7 @@
         <v>1</v>
       </c>
       <c r="C58" s="41" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D58" s="41">
         <v>0</v>
@@ -4618,10 +4618,10 @@
         <v>0</v>
       </c>
       <c r="G58" s="45" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="H58" s="45" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="59" spans="2:8" x14ac:dyDescent="0.25">
@@ -4641,10 +4641,10 @@
         <v>2</v>
       </c>
       <c r="G59" s="45" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="H59" s="45" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="60" spans="2:8" x14ac:dyDescent="0.25">
@@ -4664,10 +4664,10 @@
         <v>0</v>
       </c>
       <c r="G60" s="45" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H60" s="45" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="61" spans="2:8" x14ac:dyDescent="0.25">
@@ -4675,7 +4675,7 @@
         <v>1</v>
       </c>
       <c r="C61" s="40" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D61" s="41">
         <v>0</v>
@@ -4687,7 +4687,7 @@
         <v>1</v>
       </c>
       <c r="G61" s="45" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="H61" s="45"/>
     </row>
@@ -4696,7 +4696,7 @@
         <v>1</v>
       </c>
       <c r="C62" s="40" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D62" s="41">
         <v>0</v>
@@ -4708,10 +4708,10 @@
         <v>0</v>
       </c>
       <c r="G62" s="45" t="s">
+        <v>188</v>
+      </c>
+      <c r="H62" s="45" t="s">
         <v>189</v>
-      </c>
-      <c r="H62" s="45" t="s">
-        <v>190</v>
       </c>
     </row>
     <row r="63" spans="2:8" x14ac:dyDescent="0.25">
@@ -4719,7 +4719,7 @@
         <v>1</v>
       </c>
       <c r="C63" s="40" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D63" s="41">
         <v>0</v>
@@ -4731,10 +4731,10 @@
         <v>1</v>
       </c>
       <c r="G63" s="45" t="s">
+        <v>215</v>
+      </c>
+      <c r="H63" s="45" t="s">
         <v>216</v>
-      </c>
-      <c r="H63" s="45" t="s">
-        <v>217</v>
       </c>
     </row>
     <row r="64" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -5038,7 +5038,7 @@
         <v>1</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="D84" s="1">
         <v>4.5</v>
@@ -5171,7 +5171,7 @@
     <mergeCell ref="G66:H66"/>
   </mergeCells>
   <conditionalFormatting sqref="C68:D70">
-    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="66" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Adding sku "MineSmall" to mission related to destroy small mines
Former-commit-id: 2700eec2bf2a3e8a48ee16599d8f0d817cd27388
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Missions.xlsx
+++ b/Docs/Content/HungryDragonContent_Missions.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hsemroud\Documents\Dragon\Docs\Content\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\dragon\client\Docs\Content\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="406" uniqueCount="222">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="407" uniqueCount="223">
   <si>
     <t>single_run</t>
   </si>
@@ -715,6 +715,9 @@
   </si>
   <si>
     <t>TID_MISSION_TARGET_BOATMAN_PL</t>
+  </si>
+  <si>
+    <t>MineSmall</t>
   </si>
 </sst>
 </file>
@@ -2658,8 +2661,8 @@
   </sheetPr>
   <dimension ref="B1:P98"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M22" sqref="M22:M23"/>
+    <sheetView tabSelected="1" topLeftCell="C7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I41" sqref="I41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4219,7 +4222,9 @@
       <c r="H41" s="52">
         <v>2</v>
       </c>
-      <c r="I41" s="41"/>
+      <c r="I41" s="41" t="s">
+        <v>222</v>
+      </c>
       <c r="J41" s="51">
         <v>50</v>
       </c>

</xml_diff>

<commit_message>
Reviewing some missions... I noticed that we had 2 owls time ago: Big and Small, now we have: Big and White, so modified those params in 2 missions related to owls
Former-commit-id: e059d23db7c575cc58697a058290d122ec3b658e
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Missions.xlsx
+++ b/Docs/Content/HungryDragonContent_Missions.xlsx
@@ -305,9 +305,6 @@
     <t>icon_owl</t>
   </si>
   <si>
-    <t>OwlBig;OwlSmall</t>
-  </si>
-  <si>
     <t>owls</t>
   </si>
   <si>
@@ -651,9 +648,6 @@
     <t>eat_gold_witch</t>
   </si>
   <si>
-    <t>Hawk;OwlSmall;OwlBig;Vulture</t>
-  </si>
-  <si>
     <t>GoodWitch;GoodWitch2;BadWitch;Witch</t>
   </si>
   <si>
@@ -718,6 +712,12 @@
   </si>
   <si>
     <t>MineSmall</t>
+  </si>
+  <si>
+    <t>OwlBig;OwlWhite</t>
+  </si>
+  <si>
+    <t>Hawk;OwlWhite;OwlBig;Vulture</t>
   </si>
 </sst>
 </file>
@@ -2661,8 +2661,8 @@
   </sheetPr>
   <dimension ref="B1:P98"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I41" sqref="I41"/>
+    <sheetView tabSelected="1" topLeftCell="F4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2684,7 +2684,7 @@
     <row r="1" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:16" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B2" s="6" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C2" s="6"/>
       <c r="D2" s="6"/>
@@ -2702,14 +2702,14 @@
       <c r="C3" s="38"/>
       <c r="D3" s="38"/>
       <c r="E3" s="39" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="F3" s="39" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="G3" s="38"/>
       <c r="J3" s="58" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="K3" s="58"/>
       <c r="M3" s="58"/>
@@ -2719,19 +2719,19 @@
     </row>
     <row r="4" spans="2:16" ht="106.5" x14ac:dyDescent="0.25">
       <c r="B4" s="30" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C4" s="28" t="s">
         <v>3</v>
       </c>
       <c r="D4" s="37" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E4" s="37" t="s">
         <v>68</v>
       </c>
       <c r="F4" s="37" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="G4" s="37" t="s">
         <v>70</v>
@@ -2740,22 +2740,22 @@
         <v>69</v>
       </c>
       <c r="I4" s="37" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="J4" s="37" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="K4" s="37" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="L4" s="36" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="M4" s="36" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="N4" s="35" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="5" spans="2:16" x14ac:dyDescent="0.25">
@@ -2763,7 +2763,7 @@
         <v>1</v>
       </c>
       <c r="C5" s="24" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D5" s="24" t="s">
         <v>65</v>
@@ -2781,7 +2781,7 @@
         <v>7</v>
       </c>
       <c r="I5" s="24" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="J5" s="24">
         <v>500</v>
@@ -2790,10 +2790,10 @@
         <v>600</v>
       </c>
       <c r="L5" s="33" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="M5" s="33" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="N5" s="31" t="s">
         <v>73</v>
@@ -2804,7 +2804,7 @@
         <v>1</v>
       </c>
       <c r="C6" s="24" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D6" s="23" t="s">
         <v>53</v>
@@ -2829,7 +2829,7 @@
         <v>600</v>
       </c>
       <c r="L6" s="33" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="M6" s="33"/>
       <c r="N6" s="31" t="s">
@@ -2841,7 +2841,7 @@
         <v>1</v>
       </c>
       <c r="C7" s="24" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D7" s="24" t="s">
         <v>59</v>
@@ -2866,7 +2866,7 @@
         <v>10000</v>
       </c>
       <c r="L7" s="33" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="M7" s="33"/>
       <c r="N7" s="31" t="s">
@@ -2878,7 +2878,7 @@
         <v>1</v>
       </c>
       <c r="C8" s="24" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D8" s="24" t="s">
         <v>65</v>
@@ -2896,7 +2896,7 @@
         <v>7</v>
       </c>
       <c r="I8" s="24" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="J8" s="24">
         <v>700</v>
@@ -2905,10 +2905,10 @@
         <v>750</v>
       </c>
       <c r="L8" s="33" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="M8" s="33" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="N8" s="31" t="s">
         <v>73</v>
@@ -2919,7 +2919,7 @@
         <v>1</v>
       </c>
       <c r="C9" s="24" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D9" s="24" t="s">
         <v>65</v>
@@ -2937,7 +2937,7 @@
         <v>7</v>
       </c>
       <c r="I9" s="24" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="J9" s="24">
         <v>25</v>
@@ -2946,10 +2946,10 @@
         <v>30</v>
       </c>
       <c r="L9" s="33" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="M9" s="47" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="N9" s="31" t="s">
         <v>73</v>
@@ -2960,7 +2960,7 @@
         <v>1</v>
       </c>
       <c r="C10" s="24" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D10" s="23" t="s">
         <v>56</v>
@@ -2978,7 +2978,7 @@
         <v>7</v>
       </c>
       <c r="I10" s="23" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="J10" s="24">
         <v>8</v>
@@ -2987,10 +2987,10 @@
         <v>9</v>
       </c>
       <c r="L10" s="33" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="M10" s="47" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="N10" s="31" t="s">
         <v>73</v>
@@ -3001,7 +3001,7 @@
         <v>1</v>
       </c>
       <c r="C11" s="24" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D11" s="23" t="s">
         <v>50</v>
@@ -3019,7 +3019,7 @@
         <v>7</v>
       </c>
       <c r="I11" s="23" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="J11" s="24">
         <v>1000</v>
@@ -3028,10 +3028,10 @@
         <v>1200</v>
       </c>
       <c r="L11" s="33" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="M11" s="33" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="N11" s="31" t="s">
         <v>73</v>
@@ -3042,7 +3042,7 @@
         <v>1</v>
       </c>
       <c r="C12" s="24" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D12" s="24" t="s">
         <v>65</v>
@@ -3060,7 +3060,7 @@
         <v>7</v>
       </c>
       <c r="I12" s="24" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="J12" s="24">
         <v>10</v>
@@ -3069,10 +3069,10 @@
         <v>11</v>
       </c>
       <c r="L12" s="33" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="M12" s="47" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="N12" s="31" t="s">
         <v>73</v>
@@ -3083,7 +3083,7 @@
         <v>1</v>
       </c>
       <c r="C13" s="23" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D13" s="24" t="s">
         <v>62</v>
@@ -3108,7 +3108,7 @@
         <v>6</v>
       </c>
       <c r="L13" s="33" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="M13" s="33"/>
       <c r="N13" s="31" t="s">
@@ -3145,7 +3145,7 @@
         <v>400</v>
       </c>
       <c r="L14" s="33" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="M14" s="33"/>
       <c r="N14" s="31" t="s">
@@ -3182,7 +3182,7 @@
         <v>400</v>
       </c>
       <c r="L15" s="33" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="M15" s="33"/>
       <c r="N15" s="31" t="s">
@@ -3219,7 +3219,7 @@
         <v>500000</v>
       </c>
       <c r="L16" s="33" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="M16" s="33"/>
       <c r="N16" s="31" t="s">
@@ -3231,7 +3231,7 @@
         <v>1</v>
       </c>
       <c r="C17" s="23" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D17" s="23" t="s">
         <v>65</v>
@@ -3249,7 +3249,7 @@
         <v>7</v>
       </c>
       <c r="I17" s="24" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="J17" s="24">
         <v>45</v>
@@ -3258,10 +3258,10 @@
         <v>55</v>
       </c>
       <c r="L17" s="33" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="M17" s="47" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="N17" s="31" t="s">
         <v>73</v>
@@ -3272,7 +3272,7 @@
         <v>1</v>
       </c>
       <c r="C18" s="24" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D18" s="24" t="s">
         <v>65</v>
@@ -3290,7 +3290,7 @@
         <v>7</v>
       </c>
       <c r="I18" s="24" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="J18" s="24">
         <v>40</v>
@@ -3299,10 +3299,10 @@
         <v>45</v>
       </c>
       <c r="L18" s="33" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="M18" s="33" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="N18" s="31" t="s">
         <v>73</v>
@@ -3313,7 +3313,7 @@
         <v>1</v>
       </c>
       <c r="C19" s="23" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D19" s="23" t="s">
         <v>65</v>
@@ -3331,7 +3331,7 @@
         <v>7</v>
       </c>
       <c r="I19" s="23" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="J19" s="24">
         <v>150</v>
@@ -3340,10 +3340,10 @@
         <v>200</v>
       </c>
       <c r="L19" s="34" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="M19" s="47" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="N19" s="31" t="s">
         <v>73</v>
@@ -3354,7 +3354,7 @@
         <v>1</v>
       </c>
       <c r="C20" s="23" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D20" s="23" t="s">
         <v>65</v>
@@ -3372,7 +3372,7 @@
         <v>7</v>
       </c>
       <c r="I20" s="23" t="s">
-        <v>93</v>
+        <v>221</v>
       </c>
       <c r="J20" s="24">
         <v>5</v>
@@ -3384,7 +3384,7 @@
         <v>92</v>
       </c>
       <c r="M20" s="55" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="N20" s="31" t="s">
         <v>73</v>
@@ -3425,7 +3425,7 @@
         <v>89</v>
       </c>
       <c r="M21" s="34" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="N21" s="31" t="s">
         <v>73</v>
@@ -3436,7 +3436,7 @@
         <v>1</v>
       </c>
       <c r="C22" s="24" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D22" s="23" t="s">
         <v>65</v>
@@ -3466,7 +3466,7 @@
         <v>87</v>
       </c>
       <c r="M22" s="34" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="N22" s="31" t="s">
         <v>73</v>
@@ -3507,7 +3507,7 @@
         <v>84</v>
       </c>
       <c r="M23" s="34" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="N23" s="31" t="s">
         <v>73</v>
@@ -3548,7 +3548,7 @@
         <v>81</v>
       </c>
       <c r="M24" s="34" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="N24" s="31" t="s">
         <v>73</v>
@@ -3589,7 +3589,7 @@
         <v>78</v>
       </c>
       <c r="M25" s="34" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="N25" s="31" t="s">
         <v>73</v>
@@ -3630,7 +3630,7 @@
         <v>75</v>
       </c>
       <c r="M26" s="34" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="N26" s="31" t="s">
         <v>73</v>
@@ -3678,10 +3678,10 @@
         <v>1</v>
       </c>
       <c r="C28" s="51" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D28" s="52" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E28" s="52">
         <v>0</v>
@@ -3696,7 +3696,7 @@
         <v>7</v>
       </c>
       <c r="I28" s="52" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="J28" s="51">
         <v>8</v>
@@ -3705,10 +3705,10 @@
         <v>9</v>
       </c>
       <c r="L28" s="54" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="M28" s="54" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="N28" s="53" t="s">
         <v>73</v>
@@ -3719,10 +3719,10 @@
         <v>1</v>
       </c>
       <c r="C29" s="51" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D29" s="52" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E29" s="52">
         <v>1</v>
@@ -3744,10 +3744,10 @@
         <v>55</v>
       </c>
       <c r="L29" s="54" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="M29" s="54" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="N29" s="53" t="s">
         <v>73</v>
@@ -3758,10 +3758,10 @@
         <v>1</v>
       </c>
       <c r="C30" s="51" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D30" s="52" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E30" s="52">
         <v>1</v>
@@ -3776,7 +3776,7 @@
         <v>7</v>
       </c>
       <c r="I30" s="52" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="J30" s="51">
         <v>4</v>
@@ -3785,10 +3785,10 @@
         <v>4.5</v>
       </c>
       <c r="L30" s="54" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="M30" s="54" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="N30" s="53" t="s">
         <v>73</v>
@@ -3799,10 +3799,10 @@
         <v>1</v>
       </c>
       <c r="C31" s="51" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D31" s="52" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E31" s="52">
         <v>1</v>
@@ -3817,7 +3817,7 @@
         <v>7</v>
       </c>
       <c r="I31" s="52" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="J31" s="51">
         <v>5</v>
@@ -3826,10 +3826,10 @@
         <v>5.5</v>
       </c>
       <c r="L31" s="48" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="M31" s="48" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="N31" s="53" t="s">
         <v>73</v>
@@ -3840,10 +3840,10 @@
         <v>1</v>
       </c>
       <c r="C32" s="51" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D32" s="52" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E32" s="52">
         <v>1</v>
@@ -3858,7 +3858,7 @@
         <v>7</v>
       </c>
       <c r="I32" s="52" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="J32" s="51">
         <v>17</v>
@@ -3867,10 +3867,10 @@
         <v>18</v>
       </c>
       <c r="L32" s="48" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="M32" s="48" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="N32" s="53" t="s">
         <v>73</v>
@@ -3881,10 +3881,10 @@
         <v>1</v>
       </c>
       <c r="C33" s="40" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D33" s="41" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="E33" s="52">
         <v>0</v>
@@ -3906,7 +3906,7 @@
         <v>27</v>
       </c>
       <c r="L33" s="48" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="M33" s="48"/>
       <c r="N33" s="53" t="s">
@@ -3918,7 +3918,7 @@
         <v>1</v>
       </c>
       <c r="C34" s="24" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D34" s="23" t="s">
         <v>56</v>
@@ -3936,7 +3936,7 @@
         <v>3</v>
       </c>
       <c r="I34" s="23" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="J34" s="24">
         <v>10</v>
@@ -3945,10 +3945,10 @@
         <v>12</v>
       </c>
       <c r="L34" s="33" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="M34" s="47" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="N34" s="31" t="s">
         <v>73</v>
@@ -3959,10 +3959,10 @@
         <v>1</v>
       </c>
       <c r="C35" s="51" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D35" s="52" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E35" s="52">
         <v>1</v>
@@ -3977,7 +3977,7 @@
         <v>3</v>
       </c>
       <c r="I35" s="52" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="J35" s="51">
         <v>3</v>
@@ -3986,10 +3986,10 @@
         <v>4</v>
       </c>
       <c r="L35" s="48" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="M35" s="49" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="N35" s="53" t="s">
         <v>73</v>
@@ -4000,10 +4000,10 @@
         <v>1</v>
       </c>
       <c r="C36" s="51" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D36" s="52" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E36" s="52">
         <v>1</v>
@@ -4018,7 +4018,7 @@
         <v>3</v>
       </c>
       <c r="I36" s="52" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="J36" s="51">
         <v>25</v>
@@ -4027,10 +4027,10 @@
         <v>27</v>
       </c>
       <c r="L36" s="48" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="M36" s="52" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="N36" s="53" t="s">
         <v>73</v>
@@ -4041,7 +4041,7 @@
         <v>1</v>
       </c>
       <c r="C37" s="24" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D37" s="23" t="s">
         <v>65</v>
@@ -4059,7 +4059,7 @@
         <v>2</v>
       </c>
       <c r="I37" s="23" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="J37" s="24">
         <v>10</v>
@@ -4068,10 +4068,10 @@
         <v>12</v>
       </c>
       <c r="L37" s="33" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="M37" s="57" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="N37" s="31" t="s">
         <v>73</v>
@@ -4082,10 +4082,10 @@
         <v>1</v>
       </c>
       <c r="C38" s="51" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D38" s="52" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="E38" s="52">
         <v>0</v>
@@ -4100,7 +4100,7 @@
         <v>2</v>
       </c>
       <c r="I38" s="52" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="J38" s="51">
         <v>150</v>
@@ -4109,10 +4109,10 @@
         <v>160</v>
       </c>
       <c r="L38" s="48" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="M38" s="49" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="N38" s="53" t="s">
         <v>73</v>
@@ -4123,10 +4123,10 @@
         <v>1</v>
       </c>
       <c r="C39" s="51" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D39" s="52" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="E39" s="52">
         <v>0</v>
@@ -4141,7 +4141,7 @@
         <v>2</v>
       </c>
       <c r="I39" s="52" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="J39" s="51">
         <v>15</v>
@@ -4150,10 +4150,10 @@
         <v>16</v>
       </c>
       <c r="L39" s="48" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="M39" s="48" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="N39" s="53" t="s">
         <v>73</v>
@@ -4164,10 +4164,10 @@
         <v>1</v>
       </c>
       <c r="C40" s="51" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D40" s="52" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E40" s="52">
         <v>1</v>
@@ -4182,7 +4182,7 @@
         <v>2</v>
       </c>
       <c r="I40" s="52" t="s">
-        <v>200</v>
+        <v>222</v>
       </c>
       <c r="J40" s="51">
         <v>3</v>
@@ -4191,10 +4191,10 @@
         <v>3</v>
       </c>
       <c r="L40" s="48" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="M40" s="48" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="N40" s="53" t="s">
         <v>73</v>
@@ -4205,10 +4205,10 @@
         <v>1</v>
       </c>
       <c r="C41" s="40" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D41" s="41" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="E41" s="52">
         <v>1</v>
@@ -4223,7 +4223,7 @@
         <v>2</v>
       </c>
       <c r="I41" s="41" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="J41" s="51">
         <v>50</v>
@@ -4232,7 +4232,7 @@
         <v>52</v>
       </c>
       <c r="L41" s="48" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="M41" s="42"/>
       <c r="N41" s="53" t="s">
@@ -4244,7 +4244,7 @@
         <v>1</v>
       </c>
       <c r="C42" s="24" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D42" s="24" t="s">
         <v>50</v>
@@ -4262,7 +4262,7 @@
         <v>1</v>
       </c>
       <c r="I42" s="23" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="J42" s="24">
         <v>1</v>
@@ -4271,10 +4271,10 @@
         <v>2</v>
       </c>
       <c r="L42" s="33" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="M42" s="56" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="N42" s="31" t="s">
         <v>73</v>
@@ -4285,7 +4285,7 @@
         <v>1</v>
       </c>
       <c r="C43" s="24" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D43" s="24" t="s">
         <v>65</v>
@@ -4303,7 +4303,7 @@
         <v>1</v>
       </c>
       <c r="I43" s="23" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="J43" s="24">
         <v>5</v>
@@ -4312,10 +4312,10 @@
         <v>6</v>
       </c>
       <c r="L43" s="33" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="M43" s="23" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="N43" s="31" t="s">
         <v>73</v>
@@ -4588,7 +4588,7 @@
         <v>1</v>
       </c>
       <c r="C57" s="41" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D57" s="41">
         <v>0</v>
@@ -4600,10 +4600,10 @@
         <v>0</v>
       </c>
       <c r="G57" s="42" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="H57" s="42" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="58" spans="2:8" x14ac:dyDescent="0.25">
@@ -4611,7 +4611,7 @@
         <v>1</v>
       </c>
       <c r="C58" s="41" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D58" s="41">
         <v>0</v>
@@ -4623,10 +4623,10 @@
         <v>0</v>
       </c>
       <c r="G58" s="45" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H58" s="45" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="59" spans="2:8" x14ac:dyDescent="0.25">
@@ -4634,7 +4634,7 @@
         <v>1</v>
       </c>
       <c r="C59" s="41" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D59" s="41">
         <v>0</v>
@@ -4646,10 +4646,10 @@
         <v>2</v>
       </c>
       <c r="G59" s="45" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="H59" s="45" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="60" spans="2:8" x14ac:dyDescent="0.25">
@@ -4657,7 +4657,7 @@
         <v>1</v>
       </c>
       <c r="C60" s="41" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D60" s="41">
         <v>0</v>
@@ -4669,10 +4669,10 @@
         <v>0</v>
       </c>
       <c r="G60" s="45" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="H60" s="45" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="61" spans="2:8" x14ac:dyDescent="0.25">
@@ -4680,7 +4680,7 @@
         <v>1</v>
       </c>
       <c r="C61" s="40" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D61" s="41">
         <v>0</v>
@@ -4692,7 +4692,7 @@
         <v>1</v>
       </c>
       <c r="G61" s="45" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="H61" s="45"/>
     </row>
@@ -4701,7 +4701,7 @@
         <v>1</v>
       </c>
       <c r="C62" s="40" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D62" s="41">
         <v>0</v>
@@ -4713,10 +4713,10 @@
         <v>0</v>
       </c>
       <c r="G62" s="45" t="s">
+        <v>187</v>
+      </c>
+      <c r="H62" s="45" t="s">
         <v>188</v>
-      </c>
-      <c r="H62" s="45" t="s">
-        <v>189</v>
       </c>
     </row>
     <row r="63" spans="2:8" x14ac:dyDescent="0.25">
@@ -4724,7 +4724,7 @@
         <v>1</v>
       </c>
       <c r="C63" s="40" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D63" s="41">
         <v>0</v>
@@ -4736,10 +4736,10 @@
         <v>1</v>
       </c>
       <c r="G63" s="45" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="H63" s="45" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="64" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -5043,7 +5043,7 @@
         <v>1</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="D84" s="1">
         <v>4.5</v>

</xml_diff>

<commit_message>
Content - Remove all float from mission engine (min and max coef)
Former-commit-id: 0a1bae0f54a5d766e8fb9acc95c89d0429e444e3
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Missions.xlsx
+++ b/Docs/Content/HungryDragonContent_Missions.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\dragon\client\Docs\Content\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hsemroud\Documents\Dragon\Docs\Content\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="missions" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="162913" calcMode="manual" calcCompleted="0" calcOnSave="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -2661,8 +2661,8 @@
   </sheetPr>
   <dimension ref="B1:P98"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+    <sheetView tabSelected="1" topLeftCell="F16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K40" sqref="K40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3501,7 +3501,7 @@
         <v>3</v>
       </c>
       <c r="K23" s="23">
-        <v>3.5</v>
+        <v>3</v>
       </c>
       <c r="L23" s="34" t="s">
         <v>84</v>
@@ -3624,7 +3624,7 @@
         <v>3</v>
       </c>
       <c r="K26" s="23">
-        <v>3.5</v>
+        <v>3</v>
       </c>
       <c r="L26" s="34" t="s">
         <v>75</v>
@@ -3782,7 +3782,7 @@
         <v>4</v>
       </c>
       <c r="K30" s="52">
-        <v>4.5</v>
+        <v>4</v>
       </c>
       <c r="L30" s="54" t="s">
         <v>203</v>
@@ -3823,7 +3823,7 @@
         <v>5</v>
       </c>
       <c r="K31" s="52">
-        <v>5.5</v>
+        <v>5</v>
       </c>
       <c r="L31" s="48" t="s">
         <v>207</v>

</xml_diff>

<commit_message>
Content - Disable troll mission
Former-commit-id: 479128eb9ae5f79bc1ab8a04f9196d29a58108c8
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Missions.xlsx
+++ b/Docs/Content/HungryDragonContent_Missions.xlsx
@@ -2661,8 +2661,8 @@
   </sheetPr>
   <dimension ref="B1:P98"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F16" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K40" sqref="K40"/>
+    <sheetView tabSelected="1" topLeftCell="D10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3606,7 +3606,7 @@
         <v>65</v>
       </c>
       <c r="E26" s="23">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F26" s="24">
         <v>0.3</v>

</xml_diff>

<commit_message>
Content - Fix mission for Goldheist
Former-commit-id: 06a52cc8a00d6c1833693603ace37c18ea1d8838
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Missions.xlsx
+++ b/Docs/Content/HungryDragonContent_Missions.xlsx
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="missions" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913" calcOnSave="0"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="409" uniqueCount="223">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="409" uniqueCount="224">
   <si>
     <t>single_run</t>
   </si>
@@ -718,6 +718,9 @@
   </si>
   <si>
     <t>Hawk;OwlWhite;OwlBig;Vulture</t>
+  </si>
+  <si>
+    <t>dragon_goldheist</t>
   </si>
 </sst>
 </file>
@@ -1200,6 +1203,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1207,22 +1211,11 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="67">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -2284,6 +2277,16 @@
         </bottom>
       </border>
     </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -2298,97 +2301,97 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="missionDifficultyDefinitions" displayName="missionDifficultyDefinitions" ref="B67:K70" totalsRowShown="0" headerRowBorderDxfId="66" tableBorderDxfId="65">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="missionDifficultyDefinitions" displayName="missionDifficultyDefinitions" ref="B67:K70" totalsRowShown="0" headerRowBorderDxfId="65" tableBorderDxfId="64">
   <autoFilter ref="B67:K70"/>
   <tableColumns count="10">
     <tableColumn id="1" name="{missionDifficultyDefinitions}"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="64"/>
-    <tableColumn id="7" name="[index]" dataDxfId="63"/>
-    <tableColumn id="3" name="[dragonsToUnlock]" dataDxfId="62"/>
-    <tableColumn id="4" name="[cooldownMinutes]" dataDxfId="61"/>
-    <tableColumn id="9" name="[maxRewardCoins]" dataDxfId="60"/>
-    <tableColumn id="5" name="[removeMissionPCCoefA]" dataDxfId="59"/>
-    <tableColumn id="6" name="[removeMissionPCCoefB]" dataDxfId="58"/>
-    <tableColumn id="8" name="[tidName]" dataDxfId="57"/>
-    <tableColumn id="10" name="[color]" dataDxfId="56"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="63"/>
+    <tableColumn id="7" name="[index]" dataDxfId="62"/>
+    <tableColumn id="3" name="[dragonsToUnlock]" dataDxfId="61"/>
+    <tableColumn id="4" name="[cooldownMinutes]" dataDxfId="60"/>
+    <tableColumn id="9" name="[maxRewardCoins]" dataDxfId="59"/>
+    <tableColumn id="5" name="[removeMissionPCCoefA]" dataDxfId="58"/>
+    <tableColumn id="6" name="[removeMissionPCCoefB]" dataDxfId="57"/>
+    <tableColumn id="8" name="[tidName]" dataDxfId="56"/>
+    <tableColumn id="10" name="[color]" dataDxfId="55"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table13303132" displayName="Table13303132" ref="B75:E87" totalsRowShown="0" headerRowDxfId="55" dataDxfId="53" headerRowBorderDxfId="54" tableBorderDxfId="52" totalsRowBorderDxfId="51">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table13303132" displayName="Table13303132" ref="B75:E87" totalsRowShown="0" headerRowDxfId="54" dataDxfId="52" headerRowBorderDxfId="53" tableBorderDxfId="51" totalsRowBorderDxfId="50">
   <autoFilter ref="B75:E87"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="{missionDragonModifiersDefinitions}" dataDxfId="50"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="49"/>
-    <tableColumn id="7" name="[quantityModifier]" dataDxfId="48"/>
-    <tableColumn id="3" name="[missionSCRewardMultiplier]" dataDxfId="47"/>
+    <tableColumn id="1" name="{missionDragonModifiersDefinitions}" dataDxfId="49"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="48"/>
+    <tableColumn id="7" name="[quantityModifier]" dataDxfId="47"/>
+    <tableColumn id="3" name="[missionSCRewardMultiplier]" dataDxfId="46"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table1330313234" displayName="Table1330313234" ref="B91:D94" totalsRowShown="0" headerRowDxfId="46" dataDxfId="44" headerRowBorderDxfId="45" tableBorderDxfId="43" totalsRowBorderDxfId="42">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table1330313234" displayName="Table1330313234" ref="B91:D94" totalsRowShown="0" headerRowDxfId="45" dataDxfId="43" headerRowBorderDxfId="44" tableBorderDxfId="42" totalsRowBorderDxfId="41">
   <autoFilter ref="B91:D94"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="{missionDifficultyModifiersDefinitions}" dataDxfId="41"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="40"/>
-    <tableColumn id="7" name="[quantityModifier]" dataDxfId="39"/>
+    <tableColumn id="1" name="{missionDifficultyModifiersDefinitions}" dataDxfId="40"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="39"/>
+    <tableColumn id="7" name="[quantityModifier]" dataDxfId="38"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table133031323435" displayName="Table133031323435" ref="B98:D99" totalsRowShown="0" headerRowDxfId="38" dataDxfId="36" headerRowBorderDxfId="37" tableBorderDxfId="35" totalsRowBorderDxfId="34">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table133031323435" displayName="Table133031323435" ref="B98:D99" totalsRowShown="0" headerRowDxfId="37" dataDxfId="35" headerRowBorderDxfId="36" tableBorderDxfId="34" totalsRowBorderDxfId="33">
   <autoFilter ref="B98:D99"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="{missionOtherModifiersDefinitions}" dataDxfId="33"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="32"/>
-    <tableColumn id="7" name="[quantityModifier]" dataDxfId="31"/>
+    <tableColumn id="1" name="{missionOtherModifiersDefinitions}" dataDxfId="32"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="31"/>
+    <tableColumn id="7" name="[quantityModifier]" dataDxfId="30"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table13" displayName="Table13" ref="B48:H63" totalsRowShown="0" headerRowDxfId="30" dataDxfId="28" headerRowBorderDxfId="29" tableBorderDxfId="27" totalsRowBorderDxfId="26">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table13" displayName="Table13" ref="B48:H63" totalsRowShown="0" headerRowDxfId="29" dataDxfId="27" headerRowBorderDxfId="28" tableBorderDxfId="26" totalsRowBorderDxfId="25">
   <autoFilter ref="B48:H63"/>
   <tableColumns count="7">
-    <tableColumn id="1" name="{missionTypeDefinitions}" dataDxfId="25"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="24"/>
-    <tableColumn id="3" name="[minTier]" dataDxfId="23"/>
-    <tableColumn id="6" name="[maxTier]" dataDxfId="22"/>
-    <tableColumn id="4" name="[weight]" dataDxfId="21"/>
-    <tableColumn id="9" name="[tidDescSingleRun]" dataDxfId="20"/>
-    <tableColumn id="10" name="[tidDescMultiRun]" dataDxfId="19"/>
+    <tableColumn id="1" name="{missionTypeDefinitions}" dataDxfId="24"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="23"/>
+    <tableColumn id="3" name="[minTier]" dataDxfId="22"/>
+    <tableColumn id="6" name="[maxTier]" dataDxfId="21"/>
+    <tableColumn id="4" name="[weight]" dataDxfId="20"/>
+    <tableColumn id="9" name="[tidDescSingleRun]" dataDxfId="19"/>
+    <tableColumn id="10" name="[tidDescMultiRun]" dataDxfId="18"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table1330" displayName="Table1330" ref="B4:N43" totalsRowShown="0" headerRowDxfId="18" dataDxfId="16" headerRowBorderDxfId="17" tableBorderDxfId="15" totalsRowBorderDxfId="14">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table1330" displayName="Table1330" ref="B4:N43" totalsRowShown="0" headerRowDxfId="17" dataDxfId="15" headerRowBorderDxfId="16" tableBorderDxfId="14" totalsRowBorderDxfId="13">
   <autoFilter ref="B4:N43"/>
   <sortState ref="B5:N43">
     <sortCondition descending="1" ref="H4:H43"/>
   </sortState>
   <tableColumns count="13">
-    <tableColumn id="1" name="{missionsDefinitions}" dataDxfId="13"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="12"/>
-    <tableColumn id="7" name="[type]" dataDxfId="11"/>
-    <tableColumn id="8" name="[weight]" dataDxfId="10"/>
-    <tableColumn id="13" name="[singleRunChance]" dataDxfId="9"/>
-    <tableColumn id="11" name="[minTier]" dataDxfId="8"/>
-    <tableColumn id="12" name="[maxTier]" dataDxfId="7"/>
-    <tableColumn id="6" name="[params]" dataDxfId="6"/>
-    <tableColumn id="3" name="[objectiveBaseQuantityMin]" dataDxfId="5"/>
-    <tableColumn id="9" name="[objectiveBaseQuantityMax]" dataDxfId="4"/>
-    <tableColumn id="4" name="[icon]" dataDxfId="3"/>
-    <tableColumn id="5" name="[tidObjective]" dataDxfId="2"/>
-    <tableColumn id="10" name="[trackingSku]" dataDxfId="1"/>
+    <tableColumn id="1" name="{missionsDefinitions}" dataDxfId="12"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="11"/>
+    <tableColumn id="7" name="[type]" dataDxfId="10"/>
+    <tableColumn id="8" name="[weight]" dataDxfId="9"/>
+    <tableColumn id="13" name="[singleRunChance]" dataDxfId="8"/>
+    <tableColumn id="11" name="[minTier]" dataDxfId="7"/>
+    <tableColumn id="12" name="[maxTier]" dataDxfId="6"/>
+    <tableColumn id="6" name="[params]" dataDxfId="5"/>
+    <tableColumn id="3" name="[objectiveBaseQuantityMin]" dataDxfId="4"/>
+    <tableColumn id="9" name="[objectiveBaseQuantityMax]" dataDxfId="3"/>
+    <tableColumn id="4" name="[icon]" dataDxfId="2"/>
+    <tableColumn id="5" name="[tidObjective]" dataDxfId="1"/>
+    <tableColumn id="10" name="[trackingSku]" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2663,7 +2666,7 @@
   <dimension ref="B1:P99"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A73" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H86" sqref="H86"/>
+      <selection activeCell="G84" sqref="G84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2709,14 +2712,14 @@
         <v>143</v>
       </c>
       <c r="G3" s="38"/>
-      <c r="J3" s="58" t="s">
+      <c r="J3" s="59" t="s">
         <v>142</v>
       </c>
-      <c r="K3" s="58"/>
-      <c r="M3" s="58"/>
-      <c r="N3" s="58"/>
-      <c r="O3" s="58"/>
-      <c r="P3" s="58"/>
+      <c r="K3" s="59"/>
+      <c r="M3" s="59"/>
+      <c r="N3" s="59"/>
+      <c r="O3" s="59"/>
+      <c r="P3" s="59"/>
     </row>
     <row r="4" spans="2:16" ht="106.5" x14ac:dyDescent="0.25">
       <c r="B4" s="30" t="s">
@@ -4371,9 +4374,9 @@
       <c r="C47" s="20"/>
       <c r="D47" s="20"/>
       <c r="E47" s="20"/>
-      <c r="F47" s="59"/>
-      <c r="G47" s="59"/>
-      <c r="H47" s="59"/>
+      <c r="F47" s="60"/>
+      <c r="G47" s="60"/>
+      <c r="H47" s="60"/>
       <c r="I47" s="20"/>
       <c r="J47" s="20"/>
     </row>
@@ -4768,10 +4771,10 @@
       <c r="F66" s="21" t="s">
         <v>40</v>
       </c>
-      <c r="G66" s="60" t="s">
+      <c r="G66" s="61" t="s">
         <v>39</v>
       </c>
-      <c r="H66" s="60"/>
+      <c r="H66" s="61"/>
       <c r="I66" s="20"/>
     </row>
     <row r="67" spans="2:13" ht="142.5" x14ac:dyDescent="0.25">
@@ -5086,13 +5089,13 @@
         <v>1</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D87" s="61">
+        <v>223</v>
+      </c>
+      <c r="D87" s="58">
         <v>7.5</v>
       </c>
       <c r="E87" s="1">
-        <v>80</v>
+        <v>85</v>
       </c>
     </row>
     <row r="88" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -5191,7 +5194,7 @@
     <mergeCell ref="G66:H66"/>
   </mergeCells>
   <conditionalFormatting sqref="C68:D70">
-    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="66" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Content - Fix  special mission content
Former-commit-id: 49d6363d28a59f3225af3b9701413d614d213fc5
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Missions.xlsx
+++ b/Docs/Content/HungryDragonContent_Missions.xlsx
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="missions" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="162913" calcMode="manual"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="409" uniqueCount="224">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="413" uniqueCount="228">
   <si>
     <t>single_run</t>
   </si>
@@ -721,6 +721,18 @@
   </si>
   <si>
     <t>dragon_goldheist</t>
+  </si>
+  <si>
+    <t>missionEasy</t>
+  </si>
+  <si>
+    <t>missionMedium</t>
+  </si>
+  <si>
+    <t>missionHard</t>
+  </si>
+  <si>
+    <t>[difficulty]</t>
   </si>
 </sst>
 </file>
@@ -1215,7 +1227,56 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="67">
+  <dxfs count="68">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -2277,16 +2338,6 @@
         </bottom>
       </border>
     </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -2301,97 +2352,98 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="missionDifficultyDefinitions" displayName="missionDifficultyDefinitions" ref="B67:K70" totalsRowShown="0" headerRowBorderDxfId="65" tableBorderDxfId="64">
-  <autoFilter ref="B67:K70"/>
-  <tableColumns count="10">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="missionDifficultyDefinitions" displayName="missionDifficultyDefinitions" ref="B67:L70" totalsRowShown="0" headerRowBorderDxfId="67" tableBorderDxfId="66">
+  <autoFilter ref="B67:L70"/>
+  <tableColumns count="11">
     <tableColumn id="1" name="{missionDifficultyDefinitions}"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="63"/>
-    <tableColumn id="7" name="[index]" dataDxfId="62"/>
-    <tableColumn id="3" name="[dragonsToUnlock]" dataDxfId="61"/>
-    <tableColumn id="4" name="[cooldownMinutes]" dataDxfId="60"/>
-    <tableColumn id="9" name="[maxRewardCoins]" dataDxfId="59"/>
-    <tableColumn id="5" name="[removeMissionPCCoefA]" dataDxfId="58"/>
-    <tableColumn id="6" name="[removeMissionPCCoefB]" dataDxfId="57"/>
-    <tableColumn id="8" name="[tidName]" dataDxfId="56"/>
-    <tableColumn id="10" name="[color]" dataDxfId="55"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="65"/>
+    <tableColumn id="11" name="[difficulty]" dataDxfId="0"/>
+    <tableColumn id="7" name="[index]" dataDxfId="64"/>
+    <tableColumn id="3" name="[dragonsToUnlock]" dataDxfId="63"/>
+    <tableColumn id="4" name="[cooldownMinutes]" dataDxfId="62"/>
+    <tableColumn id="9" name="[maxRewardCoins]" dataDxfId="61"/>
+    <tableColumn id="5" name="[removeMissionPCCoefA]" dataDxfId="60"/>
+    <tableColumn id="6" name="[removeMissionPCCoefB]" dataDxfId="59"/>
+    <tableColumn id="8" name="[tidName]" dataDxfId="58"/>
+    <tableColumn id="10" name="[color]" dataDxfId="57"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table13303132" displayName="Table13303132" ref="B75:E87" totalsRowShown="0" headerRowDxfId="54" dataDxfId="52" headerRowBorderDxfId="53" tableBorderDxfId="51" totalsRowBorderDxfId="50">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table13303132" displayName="Table13303132" ref="B75:E87" totalsRowShown="0" headerRowDxfId="56" dataDxfId="54" headerRowBorderDxfId="55" tableBorderDxfId="53" totalsRowBorderDxfId="52">
   <autoFilter ref="B75:E87"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="{missionDragonModifiersDefinitions}" dataDxfId="49"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="48"/>
-    <tableColumn id="7" name="[quantityModifier]" dataDxfId="47"/>
-    <tableColumn id="3" name="[missionSCRewardMultiplier]" dataDxfId="46"/>
+    <tableColumn id="1" name="{missionDragonModifiersDefinitions}" dataDxfId="51"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="50"/>
+    <tableColumn id="7" name="[quantityModifier]" dataDxfId="49"/>
+    <tableColumn id="3" name="[missionSCRewardMultiplier]" dataDxfId="48"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table1330313234" displayName="Table1330313234" ref="B91:D94" totalsRowShown="0" headerRowDxfId="45" dataDxfId="43" headerRowBorderDxfId="44" tableBorderDxfId="42" totalsRowBorderDxfId="41">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table1330313234" displayName="Table1330313234" ref="B91:D94" totalsRowShown="0" headerRowDxfId="47" dataDxfId="45" headerRowBorderDxfId="46" tableBorderDxfId="44" totalsRowBorderDxfId="43">
   <autoFilter ref="B91:D94"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="{missionDifficultyModifiersDefinitions}" dataDxfId="40"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="39"/>
-    <tableColumn id="7" name="[quantityModifier]" dataDxfId="38"/>
+    <tableColumn id="1" name="{missionDifficultyModifiersDefinitions}" dataDxfId="42"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="41"/>
+    <tableColumn id="7" name="[quantityModifier]" dataDxfId="40"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table133031323435" displayName="Table133031323435" ref="B98:D99" totalsRowShown="0" headerRowDxfId="37" dataDxfId="35" headerRowBorderDxfId="36" tableBorderDxfId="34" totalsRowBorderDxfId="33">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table133031323435" displayName="Table133031323435" ref="B98:D99" totalsRowShown="0" headerRowDxfId="39" dataDxfId="37" headerRowBorderDxfId="38" tableBorderDxfId="36" totalsRowBorderDxfId="35">
   <autoFilter ref="B98:D99"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="{missionOtherModifiersDefinitions}" dataDxfId="32"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="31"/>
-    <tableColumn id="7" name="[quantityModifier]" dataDxfId="30"/>
+    <tableColumn id="1" name="{missionOtherModifiersDefinitions}" dataDxfId="34"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="33"/>
+    <tableColumn id="7" name="[quantityModifier]" dataDxfId="32"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table13" displayName="Table13" ref="B48:H63" totalsRowShown="0" headerRowDxfId="29" dataDxfId="27" headerRowBorderDxfId="28" tableBorderDxfId="26" totalsRowBorderDxfId="25">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table13" displayName="Table13" ref="B48:H63" totalsRowShown="0" headerRowDxfId="31" dataDxfId="29" headerRowBorderDxfId="30" tableBorderDxfId="28" totalsRowBorderDxfId="27">
   <autoFilter ref="B48:H63"/>
   <tableColumns count="7">
-    <tableColumn id="1" name="{missionTypeDefinitions}" dataDxfId="24"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="23"/>
-    <tableColumn id="3" name="[minTier]" dataDxfId="22"/>
-    <tableColumn id="6" name="[maxTier]" dataDxfId="21"/>
-    <tableColumn id="4" name="[weight]" dataDxfId="20"/>
-    <tableColumn id="9" name="[tidDescSingleRun]" dataDxfId="19"/>
-    <tableColumn id="10" name="[tidDescMultiRun]" dataDxfId="18"/>
+    <tableColumn id="1" name="{missionTypeDefinitions}" dataDxfId="26"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="25"/>
+    <tableColumn id="3" name="[minTier]" dataDxfId="24"/>
+    <tableColumn id="6" name="[maxTier]" dataDxfId="23"/>
+    <tableColumn id="4" name="[weight]" dataDxfId="22"/>
+    <tableColumn id="9" name="[tidDescSingleRun]" dataDxfId="21"/>
+    <tableColumn id="10" name="[tidDescMultiRun]" dataDxfId="20"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table1330" displayName="Table1330" ref="B4:N43" totalsRowShown="0" headerRowDxfId="17" dataDxfId="15" headerRowBorderDxfId="16" tableBorderDxfId="14" totalsRowBorderDxfId="13">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table1330" displayName="Table1330" ref="B4:N43" totalsRowShown="0" headerRowDxfId="19" dataDxfId="17" headerRowBorderDxfId="18" tableBorderDxfId="16" totalsRowBorderDxfId="15">
   <autoFilter ref="B4:N43"/>
-  <sortState ref="B5:N43">
-    <sortCondition descending="1" ref="H4:H43"/>
+  <sortState ref="B5:O43">
+    <sortCondition descending="1" ref="I4:I43"/>
   </sortState>
   <tableColumns count="13">
-    <tableColumn id="1" name="{missionsDefinitions}" dataDxfId="12"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="11"/>
-    <tableColumn id="7" name="[type]" dataDxfId="10"/>
-    <tableColumn id="8" name="[weight]" dataDxfId="9"/>
-    <tableColumn id="13" name="[singleRunChance]" dataDxfId="8"/>
-    <tableColumn id="11" name="[minTier]" dataDxfId="7"/>
-    <tableColumn id="12" name="[maxTier]" dataDxfId="6"/>
-    <tableColumn id="6" name="[params]" dataDxfId="5"/>
-    <tableColumn id="3" name="[objectiveBaseQuantityMin]" dataDxfId="4"/>
-    <tableColumn id="9" name="[objectiveBaseQuantityMax]" dataDxfId="3"/>
-    <tableColumn id="4" name="[icon]" dataDxfId="2"/>
-    <tableColumn id="5" name="[tidObjective]" dataDxfId="1"/>
-    <tableColumn id="10" name="[trackingSku]" dataDxfId="0"/>
+    <tableColumn id="1" name="{missionsDefinitions}" dataDxfId="14"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="13"/>
+    <tableColumn id="7" name="[type]" dataDxfId="12"/>
+    <tableColumn id="8" name="[weight]" dataDxfId="11"/>
+    <tableColumn id="13" name="[singleRunChance]" dataDxfId="10"/>
+    <tableColumn id="11" name="[minTier]" dataDxfId="9"/>
+    <tableColumn id="12" name="[maxTier]" dataDxfId="8"/>
+    <tableColumn id="6" name="[params]" dataDxfId="7"/>
+    <tableColumn id="3" name="[objectiveBaseQuantityMin]" dataDxfId="6"/>
+    <tableColumn id="9" name="[objectiveBaseQuantityMax]" dataDxfId="5"/>
+    <tableColumn id="4" name="[icon]" dataDxfId="4"/>
+    <tableColumn id="5" name="[tidObjective]" dataDxfId="3"/>
+    <tableColumn id="10" name="[trackingSku]" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2665,8 +2717,8 @@
   </sheetPr>
   <dimension ref="B1:P99"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A73" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G84" sqref="G84"/>
+    <sheetView tabSelected="1" topLeftCell="A67" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D69" sqref="D69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4785,27 +4837,30 @@
         <v>3</v>
       </c>
       <c r="D67" s="18" t="s">
+        <v>227</v>
+      </c>
+      <c r="E67" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="E67" s="17" t="s">
+      <c r="F67" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="F67" s="17" t="s">
+      <c r="G67" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="G67" s="17" t="s">
+      <c r="H67" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="H67" s="16" t="s">
+      <c r="I67" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="I67" s="16" t="s">
+      <c r="J67" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="J67" s="15" t="s">
+      <c r="K67" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="K67" s="14" t="s">
+      <c r="L67" s="14" t="s">
         <v>30</v>
       </c>
     </row>
@@ -4814,30 +4869,33 @@
         <v>1</v>
       </c>
       <c r="C68" s="11" t="s">
+        <v>224</v>
+      </c>
+      <c r="D68" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="D68" s="11">
-        <v>0</v>
-      </c>
-      <c r="E68" s="10">
+      <c r="E68" s="11">
         <v>0</v>
       </c>
       <c r="F68" s="10">
+        <v>0</v>
+      </c>
+      <c r="G68" s="10">
         <v>15</v>
       </c>
-      <c r="G68" s="10">
+      <c r="H68" s="10">
         <v>200</v>
       </c>
-      <c r="H68" s="9">
+      <c r="I68" s="9">
         <v>0.5</v>
       </c>
-      <c r="I68" s="9">
-        <v>1</v>
-      </c>
-      <c r="J68" s="8" t="s">
+      <c r="J68" s="9">
+        <v>1</v>
+      </c>
+      <c r="K68" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="K68" s="13" t="s">
+      <c r="L68" s="13" t="s">
         <v>28</v>
       </c>
     </row>
@@ -4846,30 +4904,33 @@
         <v>1</v>
       </c>
       <c r="C69" s="11" t="s">
+        <v>225</v>
+      </c>
+      <c r="D69" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="D69" s="11">
-        <v>1</v>
-      </c>
-      <c r="E69" s="10">
-        <v>0</v>
+      <c r="E69" s="11">
+        <v>1</v>
       </c>
       <c r="F69" s="10">
+        <v>0</v>
+      </c>
+      <c r="G69" s="10">
         <v>60</v>
       </c>
-      <c r="G69" s="10">
+      <c r="H69" s="10">
         <v>300</v>
       </c>
-      <c r="H69" s="9">
+      <c r="I69" s="9">
         <v>0.5</v>
       </c>
-      <c r="I69" s="9">
-        <v>1</v>
-      </c>
-      <c r="J69" s="8" t="s">
+      <c r="J69" s="9">
+        <v>1</v>
+      </c>
+      <c r="K69" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="K69" s="13" t="s">
+      <c r="L69" s="13" t="s">
         <v>26</v>
       </c>
     </row>
@@ -4878,30 +4939,33 @@
         <v>1</v>
       </c>
       <c r="C70" s="11" t="s">
+        <v>226</v>
+      </c>
+      <c r="D70" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="D70" s="11">
+      <c r="E70" s="11">
         <v>2</v>
       </c>
-      <c r="E70" s="10">
-        <v>0</v>
-      </c>
       <c r="F70" s="10">
+        <v>0</v>
+      </c>
+      <c r="G70" s="10">
         <v>240</v>
       </c>
-      <c r="G70" s="10">
+      <c r="H70" s="10">
         <v>600</v>
       </c>
-      <c r="H70" s="9">
+      <c r="I70" s="9">
         <v>0.5</v>
       </c>
-      <c r="I70" s="9">
-        <v>1</v>
-      </c>
-      <c r="J70" s="8" t="s">
+      <c r="J70" s="9">
+        <v>1</v>
+      </c>
+      <c r="K70" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="K70" s="7" t="s">
+      <c r="L70" s="7" t="s">
         <v>24</v>
       </c>
     </row>
@@ -5193,8 +5257,8 @@
     <mergeCell ref="F47:H47"/>
     <mergeCell ref="G66:H66"/>
   </mergeCells>
-  <conditionalFormatting sqref="C68:D70">
-    <cfRule type="duplicateValues" dxfId="66" priority="1"/>
+  <conditionalFormatting sqref="C68:E70">
+    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Content - Fix collumns names
Former-commit-id: ae82991b0b38d5ea674964eb4b04ac92a1eb0dc8
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Missions.xlsx
+++ b/Docs/Content/HungryDragonContent_Missions.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="413" uniqueCount="228">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="417" uniqueCount="231">
   <si>
     <t>single_run</t>
   </si>
@@ -733,6 +733,15 @@
   </si>
   <si>
     <t>[difficulty]</t>
+  </si>
+  <si>
+    <t>modifierEasy</t>
+  </si>
+  <si>
+    <t>modifierMedium</t>
+  </si>
+  <si>
+    <t>modifierHard</t>
   </si>
 </sst>
 </file>
@@ -1227,7 +1236,1002 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="68">
+  <dxfs count="69">
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="45" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="45" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="45" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="45" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="45" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -1269,982 +2273,6 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top/>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top/>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <border>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="45" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <border>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="45" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <border>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="45" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <border>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="45" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <border>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="45" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
         <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
@@ -2352,12 +2380,12 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="missionDifficultyDefinitions" displayName="missionDifficultyDefinitions" ref="B67:L70" totalsRowShown="0" headerRowBorderDxfId="67" tableBorderDxfId="66">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="missionDifficultyDefinitions" displayName="missionDifficultyDefinitions" ref="B67:L70" totalsRowShown="0" headerRowBorderDxfId="68" tableBorderDxfId="67">
   <autoFilter ref="B67:L70"/>
   <tableColumns count="11">
     <tableColumn id="1" name="{missionDifficultyDefinitions}"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="65"/>
-    <tableColumn id="11" name="[difficulty]" dataDxfId="0"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="66"/>
+    <tableColumn id="11" name="[difficulty]" dataDxfId="65"/>
     <tableColumn id="7" name="[index]" dataDxfId="64"/>
     <tableColumn id="3" name="[dragonsToUnlock]" dataDxfId="63"/>
     <tableColumn id="4" name="[cooldownMinutes]" dataDxfId="62"/>
@@ -2385,11 +2413,12 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table1330313234" displayName="Table1330313234" ref="B91:D94" totalsRowShown="0" headerRowDxfId="47" dataDxfId="45" headerRowBorderDxfId="46" tableBorderDxfId="44" totalsRowBorderDxfId="43">
-  <autoFilter ref="B91:D94"/>
-  <tableColumns count="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table1330313234" displayName="Table1330313234" ref="B91:E94" totalsRowShown="0" headerRowDxfId="47" dataDxfId="45" headerRowBorderDxfId="46" tableBorderDxfId="44" totalsRowBorderDxfId="43">
+  <autoFilter ref="B91:E94"/>
+  <tableColumns count="4">
     <tableColumn id="1" name="{missionDifficultyModifiersDefinitions}" dataDxfId="42"/>
     <tableColumn id="2" name="[sku]" dataDxfId="41"/>
+    <tableColumn id="3" name="[difficulty]" dataDxfId="0"/>
     <tableColumn id="7" name="[quantityModifier]" dataDxfId="40"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -2427,8 +2456,8 @@
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table1330" displayName="Table1330" ref="B4:N43" totalsRowShown="0" headerRowDxfId="19" dataDxfId="17" headerRowBorderDxfId="18" tableBorderDxfId="16" totalsRowBorderDxfId="15">
   <autoFilter ref="B4:N43"/>
-  <sortState ref="B5:O43">
-    <sortCondition descending="1" ref="I4:I43"/>
+  <sortState ref="B5:P43">
+    <sortCondition descending="1" ref="J4:J43"/>
   </sortState>
   <tableColumns count="13">
     <tableColumn id="1" name="{missionsDefinitions}" dataDxfId="14"/>
@@ -2717,8 +2746,8 @@
   </sheetPr>
   <dimension ref="B1:P99"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A67" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D69" sqref="D69"/>
+    <sheetView tabSelected="1" topLeftCell="A82" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D92" sqref="D92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5180,7 +5209,10 @@
       <c r="C91" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D91" s="3" t="s">
+      <c r="D91" s="4" t="s">
+        <v>227</v>
+      </c>
+      <c r="E91" s="3" t="s">
         <v>2</v>
       </c>
     </row>
@@ -5189,9 +5221,12 @@
         <v>1</v>
       </c>
       <c r="C92" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="D92" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D92" s="1">
+      <c r="E92" s="1">
         <v>0.05</v>
       </c>
     </row>
@@ -5200,9 +5235,12 @@
         <v>1</v>
       </c>
       <c r="C93" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="D93" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D93" s="1">
+      <c r="E93" s="1">
         <v>0.1</v>
       </c>
     </row>
@@ -5211,9 +5249,12 @@
         <v>1</v>
       </c>
       <c r="C94" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="D94" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D94" s="1">
+      <c r="E94" s="1">
         <v>0.2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Allows to show 3d models instead of images in the mission icon in the missions/ lab missions screen.
Former-commit-id: b54e93270ec9ee0a207e42657c12a7d860637487
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Missions.xlsx
+++ b/Docs/Content/HungryDragonContent_Missions.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10114"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/msana/Workspace/Dragon/client_ios/Docs/Content/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\dragon\client\Docs\Content\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B78AC90E-5775-FA4D-9E20-722D5638D363}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="38300" windowHeight="19860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="38295" windowHeight="19860"/>
   </bookViews>
   <sheets>
     <sheet name="missions" sheetId="1" r:id="rId1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="433" uniqueCount="243">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="434" uniqueCount="244">
   <si>
     <t>single_run</t>
   </si>
@@ -780,11 +779,14 @@
   <si>
     <t>TID_MISSION_OBJECTIVE_KILL_EQUIPABLE_DESC_MULTI_RUN</t>
   </si>
+  <si>
+    <t>[is3dIcon]</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1112,7 +1114,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="66">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1"/>
@@ -1262,6 +1264,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1269,14 +1274,48 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment textRotation="45"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="69">
+  <dxfs count="70">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="8"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -2420,99 +2459,100 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="missionDifficultyDefinitions" displayName="missionDifficultyDefinitions" ref="B71:L74" totalsRowShown="0" headerRowBorderDxfId="68" tableBorderDxfId="67">
-  <autoFilter ref="B71:L74" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="missionDifficultyDefinitions" displayName="missionDifficultyDefinitions" ref="B71:L74" totalsRowShown="0" headerRowBorderDxfId="69" tableBorderDxfId="68">
+  <autoFilter ref="B71:L74"/>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="{missionDifficultyDefinitions}"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="[sku]" dataDxfId="66"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="[difficulty]" dataDxfId="65"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="[index]" dataDxfId="64"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="[dragonsToUnlock]" dataDxfId="63"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="[cooldownMinutes]" dataDxfId="62"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="[maxRewardCoins]" dataDxfId="61"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="[removeMissionPCCoefA]" dataDxfId="60"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="[removeMissionPCCoefB]" dataDxfId="59"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="[tidName]" dataDxfId="58"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="[color]" dataDxfId="57"/>
+    <tableColumn id="1" name="{missionDifficultyDefinitions}"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="67"/>
+    <tableColumn id="11" name="[difficulty]" dataDxfId="66"/>
+    <tableColumn id="7" name="[index]" dataDxfId="65"/>
+    <tableColumn id="3" name="[dragonsToUnlock]" dataDxfId="64"/>
+    <tableColumn id="4" name="[cooldownMinutes]" dataDxfId="63"/>
+    <tableColumn id="9" name="[maxRewardCoins]" dataDxfId="62"/>
+    <tableColumn id="5" name="[removeMissionPCCoefA]" dataDxfId="61"/>
+    <tableColumn id="6" name="[removeMissionPCCoefB]" dataDxfId="60"/>
+    <tableColumn id="8" name="[tidName]" dataDxfId="59"/>
+    <tableColumn id="10" name="[color]" dataDxfId="58"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table13303132" displayName="Table13303132" ref="B79:E91" totalsRowShown="0" headerRowDxfId="56" dataDxfId="54" headerRowBorderDxfId="55" tableBorderDxfId="53" totalsRowBorderDxfId="52">
-  <autoFilter ref="B79:E91" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table13303132" displayName="Table13303132" ref="B79:E91" totalsRowShown="0" headerRowDxfId="57" dataDxfId="55" headerRowBorderDxfId="56" tableBorderDxfId="54" totalsRowBorderDxfId="53">
+  <autoFilter ref="B79:E91"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="{missionDragonModifiersDefinitions}" dataDxfId="51"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="[sku]" dataDxfId="50"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="[quantityModifier]" dataDxfId="49"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="[missionSCRewardMultiplier]" dataDxfId="48"/>
+    <tableColumn id="1" name="{missionDragonModifiersDefinitions}" dataDxfId="52"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="51"/>
+    <tableColumn id="7" name="[quantityModifier]" dataDxfId="50"/>
+    <tableColumn id="3" name="[missionSCRewardMultiplier]" dataDxfId="49"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table1330313234" displayName="Table1330313234" ref="B95:E98" totalsRowShown="0" headerRowDxfId="47" dataDxfId="45" headerRowBorderDxfId="46" tableBorderDxfId="44" totalsRowBorderDxfId="43">
-  <autoFilter ref="B95:E98" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table1330313234" displayName="Table1330313234" ref="B95:E98" totalsRowShown="0" headerRowDxfId="48" dataDxfId="46" headerRowBorderDxfId="47" tableBorderDxfId="45" totalsRowBorderDxfId="44">
+  <autoFilter ref="B95:E98"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="{missionDifficultyModifiersDefinitions}" dataDxfId="42"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="[sku]" dataDxfId="41"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="[difficulty]" dataDxfId="40"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0200-000007000000}" name="[quantityModifier]" dataDxfId="39"/>
+    <tableColumn id="1" name="{missionDifficultyModifiersDefinitions}" dataDxfId="43"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="42"/>
+    <tableColumn id="3" name="[difficulty]" dataDxfId="41"/>
+    <tableColumn id="7" name="[quantityModifier]" dataDxfId="40"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="Table133031323435" displayName="Table133031323435" ref="B102:D103" totalsRowShown="0" headerRowDxfId="38" dataDxfId="36" headerRowBorderDxfId="37" tableBorderDxfId="35" totalsRowBorderDxfId="34">
-  <autoFilter ref="B102:D103" xr:uid="{00000000-0009-0000-0100-000004000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table133031323435" displayName="Table133031323435" ref="B102:D103" totalsRowShown="0" headerRowDxfId="39" dataDxfId="37" headerRowBorderDxfId="38" tableBorderDxfId="36" totalsRowBorderDxfId="35">
+  <autoFilter ref="B102:D103"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="{missionOtherModifiersDefinitions}" dataDxfId="33"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0300-000002000000}" name="[sku]" dataDxfId="32"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0300-000007000000}" name="[quantityModifier]" dataDxfId="31"/>
+    <tableColumn id="1" name="{missionOtherModifiersDefinitions}" dataDxfId="34"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="33"/>
+    <tableColumn id="7" name="[quantityModifier]" dataDxfId="32"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{00000000-000C-0000-FFFF-FFFF04000000}" name="Table13" displayName="Table13" ref="B48:H67" totalsRowShown="0" headerRowDxfId="30" dataDxfId="28" headerRowBorderDxfId="29" tableBorderDxfId="27" totalsRowBorderDxfId="26">
-  <autoFilter ref="B48:H67" xr:uid="{00000000-0009-0000-0100-000005000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table13" displayName="Table13" ref="B48:H67" totalsRowShown="0" headerRowDxfId="31" dataDxfId="29" headerRowBorderDxfId="30" tableBorderDxfId="28" totalsRowBorderDxfId="27">
+  <autoFilter ref="B48:H67"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0400-000001000000}" name="{missionTypeDefinitions}" dataDxfId="25"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0400-000002000000}" name="[sku]" dataDxfId="24"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0400-000003000000}" name="[minTier]" dataDxfId="23"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0400-000006000000}" name="[maxTier]" dataDxfId="22"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0400-000004000000}" name="[weight]" dataDxfId="21"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0400-000009000000}" name="[tidDescSingleRun]" dataDxfId="20"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0400-00000A000000}" name="[tidDescMultiRun]" dataDxfId="19"/>
+    <tableColumn id="1" name="{missionTypeDefinitions}" dataDxfId="26"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="25"/>
+    <tableColumn id="3" name="[minTier]" dataDxfId="24"/>
+    <tableColumn id="6" name="[maxTier]" dataDxfId="23"/>
+    <tableColumn id="4" name="[weight]" dataDxfId="22"/>
+    <tableColumn id="9" name="[tidDescSingleRun]" dataDxfId="21"/>
+    <tableColumn id="10" name="[tidDescMultiRun]" dataDxfId="20"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{00000000-000C-0000-FFFF-FFFF05000000}" name="Table1330" displayName="Table1330" ref="B4:N43" totalsRowShown="0" headerRowDxfId="18" dataDxfId="16" headerRowBorderDxfId="17" tableBorderDxfId="15" totalsRowBorderDxfId="14">
-  <autoFilter ref="B4:N43" xr:uid="{00000000-0009-0000-0100-000006000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table1330" displayName="Table1330" ref="B4:O43" totalsRowShown="0" headerRowDxfId="19" dataDxfId="17" headerRowBorderDxfId="18" tableBorderDxfId="16" totalsRowBorderDxfId="15">
+  <autoFilter ref="B4:O43"/>
   <sortState ref="B5:P43">
     <sortCondition descending="1" ref="J4:J43"/>
   </sortState>
-  <tableColumns count="13">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0500-000001000000}" name="{missionsDefinitions}" dataDxfId="13"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0500-000002000000}" name="[sku]" dataDxfId="12"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0500-000007000000}" name="[type]" dataDxfId="11"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0500-000008000000}" name="[weight]" dataDxfId="10"/>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0500-00000D000000}" name="[singleRunChance]" dataDxfId="9"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0500-00000B000000}" name="[minTier]" dataDxfId="8"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0500-00000C000000}" name="[maxTier]" dataDxfId="7"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0500-000006000000}" name="[params]" dataDxfId="6"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0500-000003000000}" name="[objectiveBaseQuantityMin]" dataDxfId="5"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0500-000009000000}" name="[objectiveBaseQuantityMax]" dataDxfId="4"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0500-000004000000}" name="[icon]" dataDxfId="3"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0500-000005000000}" name="[tidObjective]" dataDxfId="2"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0500-00000A000000}" name="[trackingSku]" dataDxfId="1"/>
+  <tableColumns count="14">
+    <tableColumn id="1" name="{missionsDefinitions}" dataDxfId="14"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="13"/>
+    <tableColumn id="7" name="[type]" dataDxfId="12"/>
+    <tableColumn id="8" name="[weight]" dataDxfId="11"/>
+    <tableColumn id="13" name="[singleRunChance]" dataDxfId="10"/>
+    <tableColumn id="11" name="[minTier]" dataDxfId="9"/>
+    <tableColumn id="12" name="[maxTier]" dataDxfId="8"/>
+    <tableColumn id="6" name="[params]" dataDxfId="7"/>
+    <tableColumn id="3" name="[objectiveBaseQuantityMin]" dataDxfId="6"/>
+    <tableColumn id="9" name="[objectiveBaseQuantityMax]" dataDxfId="5"/>
+    <tableColumn id="4" name="[icon]" dataDxfId="4"/>
+    <tableColumn id="14" name="[is3dIcon]" dataDxfId="0"/>
+    <tableColumn id="5" name="[tidObjective]" dataDxfId="3"/>
+    <tableColumn id="10" name="[trackingSku]" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2780,34 +2820,35 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="6"/>
   </sheetPr>
-  <dimension ref="B1:P103"/>
+  <dimension ref="B1:Q103"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H64" sqref="H64"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M34" sqref="M34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="7" customWidth="1"/>
-    <col min="2" max="2" width="18.6640625" customWidth="1"/>
-    <col min="3" max="3" width="24.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="6" width="18.6640625" customWidth="1"/>
-    <col min="7" max="7" width="55.83203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="54.5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="59.83203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="18.6640625" customWidth="1"/>
-    <col min="12" max="12" width="23.5" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="34.5" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="8.5" customWidth="1"/>
-    <col min="15" max="16" width="15" customWidth="1"/>
+    <col min="2" max="2" width="18.7109375" customWidth="1"/>
+    <col min="3" max="3" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="18.7109375" customWidth="1"/>
+    <col min="7" max="7" width="55.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="54.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="59.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="18.7109375" customWidth="1"/>
+    <col min="12" max="12" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="23.42578125" customWidth="1"/>
+    <col min="14" max="14" width="34.42578125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="8.42578125" customWidth="1"/>
+    <col min="16" max="17" width="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:16" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="2:16" ht="24" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:17" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B2" s="6" t="s">
         <v>145</v>
       </c>
@@ -2821,8 +2862,9 @@
       <c r="J2" s="6"/>
       <c r="K2" s="6"/>
       <c r="L2" s="6"/>
-    </row>
-    <row r="3" spans="2:16" ht="32" x14ac:dyDescent="0.2">
+      <c r="M2" s="63"/>
+    </row>
+    <row r="3" spans="2:17" ht="45" x14ac:dyDescent="0.25">
       <c r="B3" s="20"/>
       <c r="C3" s="38"/>
       <c r="D3" s="38"/>
@@ -2833,16 +2875,16 @@
         <v>143</v>
       </c>
       <c r="G3" s="38"/>
-      <c r="J3" s="59" t="s">
+      <c r="J3" s="60" t="s">
         <v>142</v>
       </c>
-      <c r="K3" s="59"/>
-      <c r="M3" s="59"/>
-      <c r="N3" s="59"/>
-      <c r="O3" s="59"/>
-      <c r="P3" s="59"/>
-    </row>
-    <row r="4" spans="2:16" ht="103" x14ac:dyDescent="0.2">
+      <c r="K3" s="60"/>
+      <c r="N3" s="60"/>
+      <c r="O3" s="60"/>
+      <c r="P3" s="60"/>
+      <c r="Q3" s="60"/>
+    </row>
+    <row r="4" spans="2:17" ht="107.25" x14ac:dyDescent="0.25">
       <c r="B4" s="30" t="s">
         <v>141</v>
       </c>
@@ -2877,13 +2919,16 @@
         <v>136</v>
       </c>
       <c r="M4" s="36" t="s">
+        <v>243</v>
+      </c>
+      <c r="N4" s="36" t="s">
         <v>135</v>
       </c>
-      <c r="N4" s="35" t="s">
+      <c r="O4" s="35" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="5" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B5" s="27" t="s">
         <v>1</v>
       </c>
@@ -2917,14 +2962,17 @@
       <c r="L5" s="33" t="s">
         <v>128</v>
       </c>
-      <c r="M5" s="33" t="s">
+      <c r="M5" s="33" t="b">
+        <v>0</v>
+      </c>
+      <c r="N5" s="33" t="s">
         <v>150</v>
       </c>
-      <c r="N5" s="31" t="s">
+      <c r="O5" s="31" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="6" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B6" s="27" t="s">
         <v>1</v>
       </c>
@@ -2956,12 +3004,15 @@
       <c r="L6" s="33" t="s">
         <v>110</v>
       </c>
-      <c r="M6" s="33"/>
-      <c r="N6" s="31" t="s">
+      <c r="M6" s="33" t="b">
+        <v>0</v>
+      </c>
+      <c r="N6" s="33"/>
+      <c r="O6" s="31" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="7" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B7" s="27" t="s">
         <v>1</v>
       </c>
@@ -2993,12 +3044,15 @@
       <c r="L7" s="33" t="s">
         <v>109</v>
       </c>
-      <c r="M7" s="33"/>
-      <c r="N7" s="31" t="s">
+      <c r="M7" s="33" t="b">
+        <v>0</v>
+      </c>
+      <c r="N7" s="33"/>
+      <c r="O7" s="31" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="8" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B8" s="27" t="s">
         <v>1</v>
       </c>
@@ -3032,14 +3086,17 @@
       <c r="L8" s="33" t="s">
         <v>128</v>
       </c>
-      <c r="M8" s="33" t="s">
+      <c r="M8" s="33" t="b">
+        <v>0</v>
+      </c>
+      <c r="N8" s="33" t="s">
         <v>150</v>
       </c>
-      <c r="N8" s="31" t="s">
+      <c r="O8" s="31" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="9" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B9" s="27" t="s">
         <v>1</v>
       </c>
@@ -3073,14 +3130,17 @@
       <c r="L9" s="33" t="s">
         <v>126</v>
       </c>
-      <c r="M9" s="47" t="s">
+      <c r="M9" s="33" t="b">
+        <v>0</v>
+      </c>
+      <c r="N9" s="47" t="s">
         <v>152</v>
       </c>
-      <c r="N9" s="31" t="s">
+      <c r="O9" s="31" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="10" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B10" s="27" t="s">
         <v>1</v>
       </c>
@@ -3114,14 +3174,17 @@
       <c r="L10" s="33" t="s">
         <v>121</v>
       </c>
-      <c r="M10" s="47" t="s">
+      <c r="M10" s="33" t="b">
+        <v>0</v>
+      </c>
+      <c r="N10" s="47" t="s">
         <v>153</v>
       </c>
-      <c r="N10" s="31" t="s">
+      <c r="O10" s="31" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="11" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B11" s="27" t="s">
         <v>1</v>
       </c>
@@ -3155,14 +3218,17 @@
       <c r="L11" s="33" t="s">
         <v>119</v>
       </c>
-      <c r="M11" s="33" t="s">
+      <c r="M11" s="33" t="b">
+        <v>0</v>
+      </c>
+      <c r="N11" s="33" t="s">
         <v>155</v>
       </c>
-      <c r="N11" s="31" t="s">
+      <c r="O11" s="31" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="12" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B12" s="27" t="s">
         <v>1</v>
       </c>
@@ -3196,14 +3262,17 @@
       <c r="L12" s="33" t="s">
         <v>114</v>
       </c>
-      <c r="M12" s="47" t="s">
+      <c r="M12" s="33" t="b">
+        <v>0</v>
+      </c>
+      <c r="N12" s="47" t="s">
         <v>157</v>
       </c>
-      <c r="N12" s="31" t="s">
+      <c r="O12" s="31" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="13" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B13" s="25" t="s">
         <v>1</v>
       </c>
@@ -3235,12 +3304,15 @@
       <c r="L13" s="33" t="s">
         <v>112</v>
       </c>
-      <c r="M13" s="33"/>
-      <c r="N13" s="31" t="s">
+      <c r="M13" s="33" t="b">
+        <v>0</v>
+      </c>
+      <c r="N13" s="33"/>
+      <c r="O13" s="31" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="14" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B14" s="25" t="s">
         <v>1</v>
       </c>
@@ -3272,12 +3344,15 @@
       <c r="L14" s="33" t="s">
         <v>111</v>
       </c>
-      <c r="M14" s="33"/>
-      <c r="N14" s="31" t="s">
+      <c r="M14" s="33" t="b">
+        <v>0</v>
+      </c>
+      <c r="N14" s="33"/>
+      <c r="O14" s="31" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="15" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B15" s="25" t="s">
         <v>1</v>
       </c>
@@ -3309,12 +3384,15 @@
       <c r="L15" s="33" t="s">
         <v>110</v>
       </c>
-      <c r="M15" s="33"/>
-      <c r="N15" s="31" t="s">
+      <c r="M15" s="33" t="b">
+        <v>0</v>
+      </c>
+      <c r="N15" s="33"/>
+      <c r="O15" s="31" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="16" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B16" s="25" t="s">
         <v>1</v>
       </c>
@@ -3346,12 +3424,15 @@
       <c r="L16" s="33" t="s">
         <v>109</v>
       </c>
-      <c r="M16" s="33"/>
-      <c r="N16" s="31" t="s">
+      <c r="M16" s="33" t="b">
+        <v>0</v>
+      </c>
+      <c r="N16" s="33"/>
+      <c r="O16" s="31" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="17" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B17" s="25" t="s">
         <v>1</v>
       </c>
@@ -3385,14 +3466,17 @@
       <c r="L17" s="33" t="s">
         <v>106</v>
       </c>
-      <c r="M17" s="47" t="s">
+      <c r="M17" s="33" t="b">
+        <v>0</v>
+      </c>
+      <c r="N17" s="47" t="s">
         <v>159</v>
       </c>
-      <c r="N17" s="31" t="s">
+      <c r="O17" s="31" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="18" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B18" s="25" t="s">
         <v>1</v>
       </c>
@@ -3426,14 +3510,17 @@
       <c r="L18" s="33" t="s">
         <v>103</v>
       </c>
-      <c r="M18" s="33" t="s">
+      <c r="M18" s="33" t="b">
+        <v>0</v>
+      </c>
+      <c r="N18" s="33" t="s">
         <v>158</v>
       </c>
-      <c r="N18" s="31" t="s">
+      <c r="O18" s="31" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="19" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B19" s="25" t="s">
         <v>1</v>
       </c>
@@ -3467,14 +3554,17 @@
       <c r="L19" s="34" t="s">
         <v>94</v>
       </c>
-      <c r="M19" s="47" t="s">
+      <c r="M19" s="33" t="b">
+        <v>0</v>
+      </c>
+      <c r="N19" s="47" t="s">
         <v>161</v>
       </c>
-      <c r="N19" s="31" t="s">
+      <c r="O19" s="31" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="20" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B20" s="25" t="s">
         <v>1</v>
       </c>
@@ -3508,14 +3598,17 @@
       <c r="L20" s="34" t="s">
         <v>92</v>
       </c>
-      <c r="M20" s="55" t="s">
+      <c r="M20" s="33" t="b">
+        <v>0</v>
+      </c>
+      <c r="N20" s="55" t="s">
         <v>162</v>
       </c>
-      <c r="N20" s="31" t="s">
+      <c r="O20" s="31" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="21" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B21" s="25" t="s">
         <v>1</v>
       </c>
@@ -3549,14 +3642,17 @@
       <c r="L21" s="34" t="s">
         <v>89</v>
       </c>
-      <c r="M21" s="34" t="s">
+      <c r="M21" s="33" t="b">
+        <v>0</v>
+      </c>
+      <c r="N21" s="34" t="s">
         <v>163</v>
       </c>
-      <c r="N21" s="31" t="s">
+      <c r="O21" s="31" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="22" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B22" s="27" t="s">
         <v>1</v>
       </c>
@@ -3590,14 +3686,17 @@
       <c r="L22" s="34" t="s">
         <v>87</v>
       </c>
-      <c r="M22" s="34" t="s">
+      <c r="M22" s="33" t="b">
+        <v>0</v>
+      </c>
+      <c r="N22" s="34" t="s">
         <v>164</v>
       </c>
-      <c r="N22" s="31" t="s">
+      <c r="O22" s="31" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="23" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B23" s="27" t="s">
         <v>1</v>
       </c>
@@ -3631,14 +3730,17 @@
       <c r="L23" s="34" t="s">
         <v>84</v>
       </c>
-      <c r="M23" s="34" t="s">
+      <c r="M23" s="33" t="b">
+        <v>0</v>
+      </c>
+      <c r="N23" s="34" t="s">
         <v>219</v>
       </c>
-      <c r="N23" s="31" t="s">
+      <c r="O23" s="31" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="24" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B24" s="27" t="s">
         <v>1</v>
       </c>
@@ -3672,14 +3774,17 @@
       <c r="L24" s="34" t="s">
         <v>81</v>
       </c>
-      <c r="M24" s="34" t="s">
+      <c r="M24" s="33" t="b">
+        <v>0</v>
+      </c>
+      <c r="N24" s="34" t="s">
         <v>165</v>
       </c>
-      <c r="N24" s="31" t="s">
+      <c r="O24" s="31" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="25" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B25" s="27" t="s">
         <v>1</v>
       </c>
@@ -3713,14 +3818,17 @@
       <c r="L25" s="34" t="s">
         <v>78</v>
       </c>
-      <c r="M25" s="34" t="s">
+      <c r="M25" s="33" t="b">
+        <v>0</v>
+      </c>
+      <c r="N25" s="34" t="s">
         <v>166</v>
       </c>
-      <c r="N25" s="31" t="s">
+      <c r="O25" s="31" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="26" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B26" s="27" t="s">
         <v>1</v>
       </c>
@@ -3754,14 +3862,17 @@
       <c r="L26" s="34" t="s">
         <v>75</v>
       </c>
-      <c r="M26" s="34" t="s">
+      <c r="M26" s="33" t="b">
+        <v>0</v>
+      </c>
+      <c r="N26" s="34" t="s">
         <v>167</v>
       </c>
-      <c r="N26" s="31" t="s">
+      <c r="O26" s="31" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="27" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B27" s="27" t="s">
         <v>1</v>
       </c>
@@ -3793,12 +3904,15 @@
       <c r="L27" s="34" t="s">
         <v>74</v>
       </c>
-      <c r="M27" s="34"/>
-      <c r="N27" s="31" t="s">
+      <c r="M27" s="33" t="b">
+        <v>0</v>
+      </c>
+      <c r="N27" s="34"/>
+      <c r="O27" s="31" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="28" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B28" s="50" t="s">
         <v>1</v>
       </c>
@@ -3832,14 +3946,17 @@
       <c r="L28" s="54" t="s">
         <v>201</v>
       </c>
-      <c r="M28" s="54" t="s">
+      <c r="M28" s="33" t="b">
+        <v>0</v>
+      </c>
+      <c r="N28" s="54" t="s">
         <v>159</v>
       </c>
-      <c r="N28" s="53" t="s">
+      <c r="O28" s="53" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="29" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B29" s="50" t="s">
         <v>1</v>
       </c>
@@ -3871,14 +3988,17 @@
       <c r="L29" s="54" t="s">
         <v>202</v>
       </c>
-      <c r="M29" s="54" t="s">
+      <c r="M29" s="33" t="b">
+        <v>0</v>
+      </c>
+      <c r="N29" s="54" t="s">
         <v>216</v>
       </c>
-      <c r="N29" s="53" t="s">
+      <c r="O29" s="53" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="30" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B30" s="50" t="s">
         <v>1</v>
       </c>
@@ -3912,14 +4032,17 @@
       <c r="L30" s="54" t="s">
         <v>203</v>
       </c>
-      <c r="M30" s="54" t="s">
+      <c r="M30" s="33" t="b">
+        <v>0</v>
+      </c>
+      <c r="N30" s="54" t="s">
         <v>168</v>
       </c>
-      <c r="N30" s="53" t="s">
+      <c r="O30" s="53" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="31" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B31" s="50" t="s">
         <v>1</v>
       </c>
@@ -3953,14 +4076,17 @@
       <c r="L31" s="48" t="s">
         <v>207</v>
       </c>
-      <c r="M31" s="48" t="s">
+      <c r="M31" s="33" t="b">
+        <v>0</v>
+      </c>
+      <c r="N31" s="48" t="s">
         <v>215</v>
       </c>
-      <c r="N31" s="53" t="s">
+      <c r="O31" s="53" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="32" spans="2:14" s="43" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:15" s="43" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B32" s="50" t="s">
         <v>1</v>
       </c>
@@ -3994,14 +4120,17 @@
       <c r="L32" s="48" t="s">
         <v>206</v>
       </c>
-      <c r="M32" s="48" t="s">
+      <c r="M32" s="33" t="b">
+        <v>0</v>
+      </c>
+      <c r="N32" s="48" t="s">
         <v>158</v>
       </c>
-      <c r="N32" s="53" t="s">
+      <c r="O32" s="53" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="33" spans="2:14" s="43" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:15" s="43" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B33" s="50" t="s">
         <v>1</v>
       </c>
@@ -4033,12 +4162,15 @@
       <c r="L33" s="48" t="s">
         <v>212</v>
       </c>
-      <c r="M33" s="48"/>
-      <c r="N33" s="53" t="s">
+      <c r="M33" s="33" t="b">
+        <v>0</v>
+      </c>
+      <c r="N33" s="48"/>
+      <c r="O33" s="53" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="34" spans="2:14" s="43" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:15" s="43" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B34" s="27" t="s">
         <v>1</v>
       </c>
@@ -4072,14 +4204,17 @@
       <c r="L34" s="33" t="s">
         <v>124</v>
       </c>
-      <c r="M34" s="47" t="s">
+      <c r="M34" s="33" t="b">
+        <v>0</v>
+      </c>
+      <c r="N34" s="47" t="s">
         <v>153</v>
       </c>
-      <c r="N34" s="31" t="s">
+      <c r="O34" s="31" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="35" spans="2:14" s="43" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:15" s="43" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B35" s="50" t="s">
         <v>1</v>
       </c>
@@ -4113,14 +4248,17 @@
       <c r="L35" s="48" t="s">
         <v>204</v>
       </c>
-      <c r="M35" s="49" t="s">
+      <c r="M35" s="33" t="b">
+        <v>0</v>
+      </c>
+      <c r="N35" s="49" t="s">
         <v>217</v>
       </c>
-      <c r="N35" s="53" t="s">
+      <c r="O35" s="53" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="36" spans="2:14" s="43" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:15" s="43" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B36" s="50" t="s">
         <v>1</v>
       </c>
@@ -4154,14 +4292,17 @@
       <c r="L36" s="48" t="s">
         <v>208</v>
       </c>
-      <c r="M36" s="52" t="s">
+      <c r="M36" s="33" t="b">
+        <v>0</v>
+      </c>
+      <c r="N36" s="52" t="s">
         <v>150</v>
       </c>
-      <c r="N36" s="53" t="s">
+      <c r="O36" s="53" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="37" spans="2:14" s="43" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="2:15" s="43" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B37" s="27" t="s">
         <v>1</v>
       </c>
@@ -4195,14 +4336,17 @@
       <c r="L37" s="33" t="s">
         <v>100</v>
       </c>
-      <c r="M37" s="57" t="s">
+      <c r="M37" s="33" t="b">
+        <v>0</v>
+      </c>
+      <c r="N37" s="57" t="s">
         <v>154</v>
       </c>
-      <c r="N37" s="31" t="s">
+      <c r="O37" s="31" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="38" spans="2:14" s="43" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="2:15" s="43" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B38" s="50" t="s">
         <v>1</v>
       </c>
@@ -4236,14 +4380,17 @@
       <c r="L38" s="48" t="s">
         <v>209</v>
       </c>
-      <c r="M38" s="49" t="s">
+      <c r="M38" s="33" t="b">
+        <v>0</v>
+      </c>
+      <c r="N38" s="49" t="s">
         <v>150</v>
       </c>
-      <c r="N38" s="53" t="s">
+      <c r="O38" s="53" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="39" spans="2:14" s="43" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="2:15" s="43" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B39" s="50" t="s">
         <v>1</v>
       </c>
@@ -4277,14 +4424,17 @@
       <c r="L39" s="48" t="s">
         <v>210</v>
       </c>
-      <c r="M39" s="48" t="s">
+      <c r="M39" s="33" t="b">
+        <v>0</v>
+      </c>
+      <c r="N39" s="48" t="s">
         <v>152</v>
       </c>
-      <c r="N39" s="53" t="s">
+      <c r="O39" s="53" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="40" spans="2:14" s="43" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="2:15" s="43" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B40" s="50" t="s">
         <v>1</v>
       </c>
@@ -4318,14 +4468,17 @@
       <c r="L40" s="48" t="s">
         <v>205</v>
       </c>
-      <c r="M40" s="48" t="s">
+      <c r="M40" s="33" t="b">
+        <v>0</v>
+      </c>
+      <c r="N40" s="48" t="s">
         <v>169</v>
       </c>
-      <c r="N40" s="53" t="s">
+      <c r="O40" s="53" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="41" spans="2:14" s="43" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="2:15" s="43" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B41" s="50" t="s">
         <v>1</v>
       </c>
@@ -4359,12 +4512,15 @@
       <c r="L41" s="48" t="s">
         <v>211</v>
       </c>
-      <c r="M41" s="42"/>
-      <c r="N41" s="53" t="s">
+      <c r="M41" s="33" t="b">
+        <v>0</v>
+      </c>
+      <c r="N41" s="42"/>
+      <c r="O41" s="53" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="42" spans="2:14" s="43" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="2:15" s="43" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B42" s="27" t="s">
         <v>1</v>
       </c>
@@ -4398,14 +4554,17 @@
       <c r="L42" s="33" t="s">
         <v>117</v>
       </c>
-      <c r="M42" s="56" t="s">
+      <c r="M42" s="33" t="b">
+        <v>0</v>
+      </c>
+      <c r="N42" s="56" t="s">
         <v>156</v>
       </c>
-      <c r="N42" s="31" t="s">
+      <c r="O42" s="31" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="43" spans="2:14" s="43" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="2:15" s="43" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B43" s="27" t="s">
         <v>1</v>
       </c>
@@ -4439,14 +4598,17 @@
       <c r="L43" s="33" t="s">
         <v>97</v>
       </c>
-      <c r="M43" s="23" t="s">
+      <c r="M43" s="33" t="b">
+        <v>0</v>
+      </c>
+      <c r="N43" s="23" t="s">
         <v>160</v>
       </c>
-      <c r="N43" s="31" t="s">
+      <c r="O43" s="31" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="44" spans="2:14" s="43" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="2:15" s="43" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B44" s="44"/>
       <c r="C44" s="44"/>
       <c r="D44" s="44"/>
@@ -4460,8 +4622,9 @@
       <c r="L44" s="44"/>
       <c r="M44" s="44"/>
       <c r="N44" s="44"/>
-    </row>
-    <row r="45" spans="2:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="O44" s="44"/>
+    </row>
+    <row r="45" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B45" s="32"/>
       <c r="C45" s="32"/>
       <c r="D45" s="32"/>
@@ -4473,9 +4636,10 @@
       <c r="J45" s="32"/>
       <c r="K45" s="32"/>
       <c r="L45" s="32"/>
-      <c r="M45" s="31"/>
-    </row>
-    <row r="46" spans="2:14" ht="24" x14ac:dyDescent="0.3">
+      <c r="M45" s="32"/>
+      <c r="N45" s="31"/>
+    </row>
+    <row r="46" spans="2:15" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B46" s="6" t="s">
         <v>72</v>
       </c>
@@ -4489,19 +4653,20 @@
       <c r="J46" s="6"/>
       <c r="K46" s="6"/>
       <c r="L46" s="6"/>
-    </row>
-    <row r="47" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="M46" s="63"/>
+    </row>
+    <row r="47" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B47" s="20"/>
       <c r="C47" s="20"/>
       <c r="D47" s="20"/>
       <c r="E47" s="20"/>
-      <c r="F47" s="60"/>
-      <c r="G47" s="60"/>
-      <c r="H47" s="60"/>
+      <c r="F47" s="61"/>
+      <c r="G47" s="61"/>
+      <c r="H47" s="61"/>
       <c r="I47" s="20"/>
       <c r="J47" s="20"/>
     </row>
-    <row r="48" spans="2:14" ht="93" x14ac:dyDescent="0.2">
+    <row r="48" spans="2:15" ht="96" x14ac:dyDescent="0.25">
       <c r="B48" s="30" t="s">
         <v>71</v>
       </c>
@@ -4524,7 +4689,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="49" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="49" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B49" s="27" t="s">
         <v>1</v>
       </c>
@@ -4547,7 +4712,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="50" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="50" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B50" s="27" t="s">
         <v>1</v>
       </c>
@@ -4570,7 +4735,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="51" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="51" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B51" s="27" t="s">
         <v>1</v>
       </c>
@@ -4593,7 +4758,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="52" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="52" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B52" s="27" t="s">
         <v>1</v>
       </c>
@@ -4616,7 +4781,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="53" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="53" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B53" s="25" t="s">
         <v>1</v>
       </c>
@@ -4639,7 +4804,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="54" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="54" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B54" s="25" t="s">
         <v>1</v>
       </c>
@@ -4662,7 +4827,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="55" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="55" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B55" s="25" t="s">
         <v>1</v>
       </c>
@@ -4685,7 +4850,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="56" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="56" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B56" s="25" t="s">
         <v>1</v>
       </c>
@@ -4708,7 +4873,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="57" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="57" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B57" s="46" t="s">
         <v>1</v>
       </c>
@@ -4731,7 +4896,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="58" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="58" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B58" s="46" t="s">
         <v>1</v>
       </c>
@@ -4754,7 +4919,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="59" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="59" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B59" s="46" t="s">
         <v>1</v>
       </c>
@@ -4777,7 +4942,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="60" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="60" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B60" s="46" t="s">
         <v>1</v>
       </c>
@@ -4800,7 +4965,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="61" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="61" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B61" s="46" t="s">
         <v>1</v>
       </c>
@@ -4823,7 +4988,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="62" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="62" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B62" s="46" t="s">
         <v>1</v>
       </c>
@@ -4846,8 +5011,8 @@
         <v>239</v>
       </c>
     </row>
-    <row r="63" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B63" s="62" t="s">
+    <row r="63" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B63" s="59" t="s">
         <v>1</v>
       </c>
       <c r="C63" s="40" t="s">
@@ -4869,7 +5034,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="64" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="64" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B64" s="46" t="s">
         <v>1</v>
       </c>
@@ -4892,7 +5057,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="65" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="65" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B65" s="46" t="s">
         <v>1</v>
       </c>
@@ -4913,7 +5078,7 @@
       </c>
       <c r="H65" s="45"/>
     </row>
-    <row r="66" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="66" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B66" s="46" t="s">
         <v>1</v>
       </c>
@@ -4936,7 +5101,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="67" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="67" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B67" s="46" t="s">
         <v>1</v>
       </c>
@@ -4959,8 +5124,8 @@
         <v>214</v>
       </c>
     </row>
-    <row r="68" spans="2:13" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="69" spans="2:13" ht="24" x14ac:dyDescent="0.3">
+    <row r="68" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="69" spans="2:14" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B69" s="6" t="s">
         <v>41</v>
       </c>
@@ -4975,8 +5140,9 @@
       <c r="K69" s="6"/>
       <c r="L69" s="6"/>
       <c r="M69" s="6"/>
-    </row>
-    <row r="70" spans="2:13" ht="64" x14ac:dyDescent="0.2">
+      <c r="N69" s="6"/>
+    </row>
+    <row r="70" spans="2:14" ht="60" x14ac:dyDescent="0.25">
       <c r="B70" s="20"/>
       <c r="C70" s="20"/>
       <c r="D70" s="20"/>
@@ -4984,13 +5150,13 @@
       <c r="F70" s="21" t="s">
         <v>40</v>
       </c>
-      <c r="G70" s="61" t="s">
+      <c r="G70" s="62" t="s">
         <v>39</v>
       </c>
-      <c r="H70" s="61"/>
+      <c r="H70" s="62"/>
       <c r="I70" s="20"/>
     </row>
-    <row r="71" spans="2:13" ht="137" x14ac:dyDescent="0.2">
+    <row r="71" spans="2:14" ht="142.5" x14ac:dyDescent="0.25">
       <c r="B71" s="19" t="s">
         <v>38</v>
       </c>
@@ -5024,8 +5190,9 @@
       <c r="L71" s="14" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="72" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="M71" s="64"/>
+    </row>
+    <row r="72" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B72" s="12" t="s">
         <v>1</v>
       </c>
@@ -5059,8 +5226,9 @@
       <c r="L72" s="13" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="73" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="M72" s="65"/>
+    </row>
+    <row r="73" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B73" s="12" t="s">
         <v>1</v>
       </c>
@@ -5094,8 +5262,9 @@
       <c r="L73" s="13" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="74" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="M73" s="65"/>
+    </row>
+    <row r="74" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B74" s="12" t="s">
         <v>1</v>
       </c>
@@ -5129,9 +5298,10 @@
       <c r="L74" s="7" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="76" spans="2:13" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="77" spans="2:13" ht="24" x14ac:dyDescent="0.3">
+      <c r="M74" s="65"/>
+    </row>
+    <row r="76" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="77" spans="2:14" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B77" s="6" t="s">
         <v>23</v>
       </c>
@@ -5141,7 +5311,7 @@
       <c r="F77" s="6"/>
       <c r="G77" s="6"/>
     </row>
-    <row r="79" spans="2:13" ht="132" x14ac:dyDescent="0.2">
+    <row r="79" spans="2:14" ht="135.75" x14ac:dyDescent="0.25">
       <c r="B79" s="5" t="s">
         <v>22</v>
       </c>
@@ -5155,7 +5325,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="80" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="80" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B80" s="2" t="s">
         <v>1</v>
       </c>
@@ -5169,7 +5339,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="81" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="81" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B81" s="2" t="s">
         <v>1</v>
       </c>
@@ -5183,7 +5353,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="82" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="82" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B82" s="2" t="s">
         <v>1</v>
       </c>
@@ -5197,7 +5367,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="83" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="83" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B83" s="2" t="s">
         <v>1</v>
       </c>
@@ -5211,7 +5381,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="84" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="84" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B84" s="2" t="s">
         <v>1</v>
       </c>
@@ -5225,7 +5395,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="85" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="85" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B85" s="2" t="s">
         <v>1</v>
       </c>
@@ -5239,7 +5409,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="86" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="86" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B86" s="2" t="s">
         <v>1</v>
       </c>
@@ -5253,7 +5423,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="87" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="87" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B87" s="2" t="s">
         <v>1</v>
       </c>
@@ -5267,7 +5437,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="88" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="88" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B88" s="2" t="s">
         <v>1</v>
       </c>
@@ -5281,7 +5451,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="89" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="89" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B89" s="2" t="s">
         <v>1</v>
       </c>
@@ -5295,7 +5465,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="90" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="90" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B90" s="2" t="s">
         <v>1</v>
       </c>
@@ -5309,7 +5479,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="91" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="91" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B91" s="2" t="s">
         <v>1</v>
       </c>
@@ -5323,8 +5493,8 @@
         <v>85</v>
       </c>
     </row>
-    <row r="92" spans="2:7" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="93" spans="2:7" ht="24" x14ac:dyDescent="0.3">
+    <row r="92" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="93" spans="2:7" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B93" s="6" t="s">
         <v>10</v>
       </c>
@@ -5334,7 +5504,7 @@
       <c r="F93" s="6"/>
       <c r="G93" s="6"/>
     </row>
-    <row r="95" spans="2:7" ht="142" x14ac:dyDescent="0.2">
+    <row r="95" spans="2:7" ht="142.5" x14ac:dyDescent="0.25">
       <c r="B95" s="5" t="s">
         <v>9</v>
       </c>
@@ -5348,7 +5518,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="96" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="96" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B96" s="2" t="s">
         <v>1</v>
       </c>
@@ -5362,7 +5532,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="97" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="97" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B97" s="2" t="s">
         <v>1</v>
       </c>
@@ -5376,7 +5546,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="98" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="98" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B98" s="2" t="s">
         <v>1</v>
       </c>
@@ -5390,8 +5560,8 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="99" spans="2:7" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="100" spans="2:7" ht="24" x14ac:dyDescent="0.3">
+    <row r="99" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="100" spans="2:7" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B100" s="6" t="s">
         <v>5</v>
       </c>
@@ -5401,7 +5571,7 @@
       <c r="F100" s="6"/>
       <c r="G100" s="6"/>
     </row>
-    <row r="102" spans="2:7" ht="131" x14ac:dyDescent="0.2">
+    <row r="102" spans="2:7" ht="132" x14ac:dyDescent="0.25">
       <c r="B102" s="5" t="s">
         <v>4</v>
       </c>
@@ -5412,7 +5582,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="103" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="103" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B103" s="2" t="s">
         <v>1</v>
       </c>
@@ -5426,12 +5596,12 @@
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="J3:K3"/>
-    <mergeCell ref="M3:P3"/>
+    <mergeCell ref="N3:Q3"/>
     <mergeCell ref="F47:H47"/>
     <mergeCell ref="G70:H70"/>
   </mergeCells>
   <conditionalFormatting sqref="C72:E74">
-    <cfRule type="duplicateValues" dxfId="0" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Fixed missions tracking bug
Former-commit-id: 1e732f4e2dccfcf2d4ba0db4519be0ecdb3d6219
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Missions.xlsx
+++ b/Docs/Content/HungryDragonContent_Missions.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10114"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/msana/Workspace/Dragon/client_ios/Docs/Content/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\dragon\client\Docs\Content\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B78AC90E-5775-FA4D-9E20-722D5638D363}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="38300" windowHeight="19860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="38295" windowHeight="19860"/>
   </bookViews>
   <sheets>
     <sheet name="missions" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913" calcMode="manual"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="433" uniqueCount="243">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="394" uniqueCount="242">
   <si>
     <t>single_run</t>
   </si>
@@ -244,9 +243,6 @@
   </si>
   <si>
     <t>MISSION TYPE DEFINITIONS</t>
-  </si>
-  <si>
-    <t>id</t>
   </si>
   <si>
     <t>icon_run</t>
@@ -784,7 +780,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1112,7 +1108,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1"/>
@@ -1246,9 +1242,6 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1262,6 +1255,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1269,24 +1265,11 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="69">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -2406,6 +2389,16 @@
         </bottom>
       </border>
     </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -2420,99 +2413,101 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="missionDifficultyDefinitions" displayName="missionDifficultyDefinitions" ref="B71:L74" totalsRowShown="0" headerRowBorderDxfId="68" tableBorderDxfId="67">
-  <autoFilter ref="B71:L74" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="missionDifficultyDefinitions" displayName="missionDifficultyDefinitions" ref="B71:L74" totalsRowShown="0" headerRowBorderDxfId="67" tableBorderDxfId="66">
+  <autoFilter ref="B71:L74"/>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="{missionDifficultyDefinitions}"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="[sku]" dataDxfId="66"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="[difficulty]" dataDxfId="65"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="[index]" dataDxfId="64"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="[dragonsToUnlock]" dataDxfId="63"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="[cooldownMinutes]" dataDxfId="62"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="[maxRewardCoins]" dataDxfId="61"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="[removeMissionPCCoefA]" dataDxfId="60"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="[removeMissionPCCoefB]" dataDxfId="59"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="[tidName]" dataDxfId="58"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="[color]" dataDxfId="57"/>
+    <tableColumn id="1" name="{missionDifficultyDefinitions}"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="65"/>
+    <tableColumn id="11" name="[difficulty]" dataDxfId="64"/>
+    <tableColumn id="7" name="[index]" dataDxfId="63"/>
+    <tableColumn id="3" name="[dragonsToUnlock]" dataDxfId="62"/>
+    <tableColumn id="4" name="[cooldownMinutes]" dataDxfId="61"/>
+    <tableColumn id="9" name="[maxRewardCoins]" dataDxfId="60"/>
+    <tableColumn id="5" name="[removeMissionPCCoefA]" dataDxfId="59"/>
+    <tableColumn id="6" name="[removeMissionPCCoefB]" dataDxfId="58"/>
+    <tableColumn id="8" name="[tidName]" dataDxfId="57"/>
+    <tableColumn id="10" name="[color]" dataDxfId="56"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table13303132" displayName="Table13303132" ref="B79:E91" totalsRowShown="0" headerRowDxfId="56" dataDxfId="54" headerRowBorderDxfId="55" tableBorderDxfId="53" totalsRowBorderDxfId="52">
-  <autoFilter ref="B79:E91" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table13303132" displayName="Table13303132" ref="B79:E91" totalsRowShown="0" headerRowDxfId="55" dataDxfId="53" headerRowBorderDxfId="54" tableBorderDxfId="52" totalsRowBorderDxfId="51">
+  <autoFilter ref="B79:E91"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="{missionDragonModifiersDefinitions}" dataDxfId="51"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="[sku]" dataDxfId="50"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="[quantityModifier]" dataDxfId="49"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="[missionSCRewardMultiplier]" dataDxfId="48"/>
+    <tableColumn id="1" name="{missionDragonModifiersDefinitions}" dataDxfId="50"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="49"/>
+    <tableColumn id="7" name="[quantityModifier]" dataDxfId="48"/>
+    <tableColumn id="3" name="[missionSCRewardMultiplier]" dataDxfId="47"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table1330313234" displayName="Table1330313234" ref="B95:E98" totalsRowShown="0" headerRowDxfId="47" dataDxfId="45" headerRowBorderDxfId="46" tableBorderDxfId="44" totalsRowBorderDxfId="43">
-  <autoFilter ref="B95:E98" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table1330313234" displayName="Table1330313234" ref="B95:E98" totalsRowShown="0" headerRowDxfId="46" dataDxfId="44" headerRowBorderDxfId="45" tableBorderDxfId="43" totalsRowBorderDxfId="42">
+  <autoFilter ref="B95:E98"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="{missionDifficultyModifiersDefinitions}" dataDxfId="42"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="[sku]" dataDxfId="41"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="[difficulty]" dataDxfId="40"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0200-000007000000}" name="[quantityModifier]" dataDxfId="39"/>
+    <tableColumn id="1" name="{missionDifficultyModifiersDefinitions}" dataDxfId="41"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="40"/>
+    <tableColumn id="3" name="[difficulty]" dataDxfId="39"/>
+    <tableColumn id="7" name="[quantityModifier]" dataDxfId="38"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="Table133031323435" displayName="Table133031323435" ref="B102:D103" totalsRowShown="0" headerRowDxfId="38" dataDxfId="36" headerRowBorderDxfId="37" tableBorderDxfId="35" totalsRowBorderDxfId="34">
-  <autoFilter ref="B102:D103" xr:uid="{00000000-0009-0000-0100-000004000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table133031323435" displayName="Table133031323435" ref="B102:D103" totalsRowShown="0" headerRowDxfId="37" dataDxfId="35" headerRowBorderDxfId="36" tableBorderDxfId="34" totalsRowBorderDxfId="33">
+  <autoFilter ref="B102:D103"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="{missionOtherModifiersDefinitions}" dataDxfId="33"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0300-000002000000}" name="[sku]" dataDxfId="32"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0300-000007000000}" name="[quantityModifier]" dataDxfId="31"/>
+    <tableColumn id="1" name="{missionOtherModifiersDefinitions}" dataDxfId="32"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="31"/>
+    <tableColumn id="7" name="[quantityModifier]" dataDxfId="30"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{00000000-000C-0000-FFFF-FFFF04000000}" name="Table13" displayName="Table13" ref="B48:H67" totalsRowShown="0" headerRowDxfId="30" dataDxfId="28" headerRowBorderDxfId="29" tableBorderDxfId="27" totalsRowBorderDxfId="26">
-  <autoFilter ref="B48:H67" xr:uid="{00000000-0009-0000-0100-000005000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table13" displayName="Table13" ref="B48:H67" totalsRowShown="0" headerRowDxfId="29" dataDxfId="27" headerRowBorderDxfId="28" tableBorderDxfId="26" totalsRowBorderDxfId="25">
+  <autoFilter ref="B48:H67"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0400-000001000000}" name="{missionTypeDefinitions}" dataDxfId="25"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0400-000002000000}" name="[sku]" dataDxfId="24"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0400-000003000000}" name="[minTier]" dataDxfId="23"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0400-000006000000}" name="[maxTier]" dataDxfId="22"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0400-000004000000}" name="[weight]" dataDxfId="21"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0400-000009000000}" name="[tidDescSingleRun]" dataDxfId="20"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0400-00000A000000}" name="[tidDescMultiRun]" dataDxfId="19"/>
+    <tableColumn id="1" name="{missionTypeDefinitions}" dataDxfId="24"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="23"/>
+    <tableColumn id="3" name="[minTier]" dataDxfId="22"/>
+    <tableColumn id="6" name="[maxTier]" dataDxfId="21"/>
+    <tableColumn id="4" name="[weight]" dataDxfId="20"/>
+    <tableColumn id="9" name="[tidDescSingleRun]" dataDxfId="19"/>
+    <tableColumn id="10" name="[tidDescMultiRun]" dataDxfId="18"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{00000000-000C-0000-FFFF-FFFF05000000}" name="Table1330" displayName="Table1330" ref="B4:N43" totalsRowShown="0" headerRowDxfId="18" dataDxfId="16" headerRowBorderDxfId="17" tableBorderDxfId="15" totalsRowBorderDxfId="14">
-  <autoFilter ref="B4:N43" xr:uid="{00000000-0009-0000-0100-000006000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table1330" displayName="Table1330" ref="B4:N43" totalsRowShown="0" headerRowDxfId="17" dataDxfId="15" headerRowBorderDxfId="16" tableBorderDxfId="14" totalsRowBorderDxfId="13">
+  <autoFilter ref="B4:N43"/>
   <sortState ref="B5:P43">
     <sortCondition descending="1" ref="J4:J43"/>
   </sortState>
   <tableColumns count="13">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0500-000001000000}" name="{missionsDefinitions}" dataDxfId="13"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0500-000002000000}" name="[sku]" dataDxfId="12"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0500-000007000000}" name="[type]" dataDxfId="11"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0500-000008000000}" name="[weight]" dataDxfId="10"/>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0500-00000D000000}" name="[singleRunChance]" dataDxfId="9"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0500-00000B000000}" name="[minTier]" dataDxfId="8"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0500-00000C000000}" name="[maxTier]" dataDxfId="7"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0500-000006000000}" name="[params]" dataDxfId="6"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0500-000003000000}" name="[objectiveBaseQuantityMin]" dataDxfId="5"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0500-000009000000}" name="[objectiveBaseQuantityMax]" dataDxfId="4"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0500-000004000000}" name="[icon]" dataDxfId="3"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0500-000005000000}" name="[tidObjective]" dataDxfId="2"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0500-00000A000000}" name="[trackingSku]" dataDxfId="1"/>
+    <tableColumn id="1" name="{missionsDefinitions}" dataDxfId="12"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="11"/>
+    <tableColumn id="7" name="[type]" dataDxfId="10"/>
+    <tableColumn id="8" name="[weight]" dataDxfId="9"/>
+    <tableColumn id="13" name="[singleRunChance]" dataDxfId="8"/>
+    <tableColumn id="11" name="[minTier]" dataDxfId="7"/>
+    <tableColumn id="12" name="[maxTier]" dataDxfId="6"/>
+    <tableColumn id="6" name="[params]" dataDxfId="5"/>
+    <tableColumn id="3" name="[objectiveBaseQuantityMin]" dataDxfId="4"/>
+    <tableColumn id="9" name="[objectiveBaseQuantityMax]" dataDxfId="3"/>
+    <tableColumn id="4" name="[icon]" dataDxfId="2"/>
+    <tableColumn id="5" name="[tidObjective]" dataDxfId="1"/>
+    <tableColumn id="10" name="[trackingSku]" dataDxfId="0">
+      <calculatedColumnFormula>Table1330[[#This Row],['[sku']]]</calculatedColumnFormula>
+    </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2780,36 +2775,36 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="6"/>
   </sheetPr>
   <dimension ref="B1:P103"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H64" sqref="H64"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="O9" sqref="O9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="7" customWidth="1"/>
-    <col min="2" max="2" width="18.6640625" customWidth="1"/>
-    <col min="3" max="3" width="24.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="6" width="18.6640625" customWidth="1"/>
-    <col min="7" max="7" width="55.83203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="54.5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="59.83203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="18.6640625" customWidth="1"/>
-    <col min="12" max="12" width="23.5" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="34.5" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="8.5" customWidth="1"/>
+    <col min="2" max="2" width="18.7109375" customWidth="1"/>
+    <col min="3" max="3" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="18.7109375" customWidth="1"/>
+    <col min="7" max="7" width="55.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="54.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="59.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="18.7109375" customWidth="1"/>
+    <col min="12" max="12" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="34.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="28" customWidth="1"/>
     <col min="15" max="16" width="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:16" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="2:16" ht="24" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:16" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B2" s="6" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C2" s="6"/>
       <c r="D2" s="6"/>
@@ -2822,19 +2817,19 @@
       <c r="K2" s="6"/>
       <c r="L2" s="6"/>
     </row>
-    <row r="3" spans="2:16" ht="32" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:16" ht="45" x14ac:dyDescent="0.25">
       <c r="B3" s="20"/>
       <c r="C3" s="38"/>
       <c r="D3" s="38"/>
       <c r="E3" s="39" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="F3" s="39" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G3" s="38"/>
       <c r="J3" s="59" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="K3" s="59"/>
       <c r="M3" s="59"/>
@@ -2842,21 +2837,21 @@
       <c r="O3" s="59"/>
       <c r="P3" s="59"/>
     </row>
-    <row r="4" spans="2:16" ht="103" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:16" ht="106.5" x14ac:dyDescent="0.25">
       <c r="B4" s="30" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C4" s="28" t="s">
         <v>3</v>
       </c>
       <c r="D4" s="37" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E4" s="37" t="s">
         <v>68</v>
       </c>
       <c r="F4" s="37" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="G4" s="37" t="s">
         <v>70</v>
@@ -2865,30 +2860,30 @@
         <v>69</v>
       </c>
       <c r="I4" s="37" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="J4" s="37" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="K4" s="37" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="L4" s="36" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="M4" s="36" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="N4" s="35" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="5" spans="2:16" x14ac:dyDescent="0.2">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="5" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B5" s="27" t="s">
         <v>1</v>
       </c>
       <c r="C5" s="24" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D5" s="24" t="s">
         <v>65</v>
@@ -2906,7 +2901,7 @@
         <v>7</v>
       </c>
       <c r="I5" s="24" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="J5" s="24">
         <v>500</v>
@@ -2915,21 +2910,22 @@
         <v>600</v>
       </c>
       <c r="L5" s="33" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="M5" s="33" t="s">
-        <v>150</v>
-      </c>
-      <c r="N5" s="31" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="6" spans="2:16" x14ac:dyDescent="0.2">
+        <v>149</v>
+      </c>
+      <c r="N5" s="31" t="str">
+        <f>Table1330[[#This Row],['[sku']]]</f>
+        <v>ftux1</v>
+      </c>
+    </row>
+    <row r="6" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B6" s="27" t="s">
         <v>1</v>
       </c>
       <c r="C6" s="24" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D6" s="23" t="s">
         <v>53</v>
@@ -2954,19 +2950,20 @@
         <v>600</v>
       </c>
       <c r="L6" s="33" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="M6" s="33"/>
-      <c r="N6" s="31" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="7" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="N6" s="31" t="str">
+        <f>Table1330[[#This Row],['[sku']]]</f>
+        <v>ftux2</v>
+      </c>
+    </row>
+    <row r="7" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B7" s="27" t="s">
         <v>1</v>
       </c>
       <c r="C7" s="24" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D7" s="24" t="s">
         <v>59</v>
@@ -2991,19 +2988,20 @@
         <v>10000</v>
       </c>
       <c r="L7" s="33" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="M7" s="33"/>
-      <c r="N7" s="31" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="8" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="N7" s="31" t="str">
+        <f>Table1330[[#This Row],['[sku']]]</f>
+        <v>ftux3</v>
+      </c>
+    </row>
+    <row r="8" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B8" s="27" t="s">
         <v>1</v>
       </c>
       <c r="C8" s="24" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D8" s="24" t="s">
         <v>65</v>
@@ -3021,7 +3019,7 @@
         <v>7</v>
       </c>
       <c r="I8" s="24" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="J8" s="24">
         <v>700</v>
@@ -3030,21 +3028,22 @@
         <v>750</v>
       </c>
       <c r="L8" s="33" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="M8" s="33" t="s">
-        <v>150</v>
-      </c>
-      <c r="N8" s="31" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="9" spans="2:16" x14ac:dyDescent="0.2">
+        <v>149</v>
+      </c>
+      <c r="N8" s="31" t="str">
+        <f>Table1330[[#This Row],['[sku']]]</f>
+        <v>birds</v>
+      </c>
+    </row>
+    <row r="9" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B9" s="27" t="s">
         <v>1</v>
       </c>
       <c r="C9" s="24" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D9" s="24" t="s">
         <v>65</v>
@@ -3062,7 +3061,7 @@
         <v>7</v>
       </c>
       <c r="I9" s="24" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="J9" s="24">
         <v>25</v>
@@ -3071,21 +3070,22 @@
         <v>30</v>
       </c>
       <c r="L9" s="33" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="M9" s="47" t="s">
-        <v>152</v>
-      </c>
-      <c r="N9" s="31" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="10" spans="2:16" x14ac:dyDescent="0.2">
+        <v>151</v>
+      </c>
+      <c r="N9" s="31" t="str">
+        <f>Table1330[[#This Row],['[sku']]]</f>
+        <v>villagers</v>
+      </c>
+    </row>
+    <row r="10" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B10" s="27" t="s">
         <v>1</v>
       </c>
       <c r="C10" s="24" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D10" s="23" t="s">
         <v>56</v>
@@ -3103,7 +3103,7 @@
         <v>7</v>
       </c>
       <c r="I10" s="23" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="J10" s="24">
         <v>8</v>
@@ -3112,21 +3112,22 @@
         <v>9</v>
       </c>
       <c r="L10" s="33" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="M10" s="47" t="s">
-        <v>153</v>
-      </c>
-      <c r="N10" s="31" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="11" spans="2:16" x14ac:dyDescent="0.2">
+        <v>152</v>
+      </c>
+      <c r="N10" s="31" t="str">
+        <f>Table1330[[#This Row],['[sku']]]</f>
+        <v>small_decos</v>
+      </c>
+    </row>
+    <row r="11" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B11" s="27" t="s">
         <v>1</v>
       </c>
       <c r="C11" s="24" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D11" s="23" t="s">
         <v>50</v>
@@ -3144,7 +3145,7 @@
         <v>7</v>
       </c>
       <c r="I11" s="23" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="J11" s="24">
         <v>1000</v>
@@ -3153,21 +3154,22 @@
         <v>1200</v>
       </c>
       <c r="L11" s="33" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="M11" s="33" t="s">
-        <v>155</v>
-      </c>
-      <c r="N11" s="31" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="12" spans="2:16" x14ac:dyDescent="0.2">
+        <v>154</v>
+      </c>
+      <c r="N11" s="31" t="str">
+        <f>Table1330[[#This Row],['[sku']]]</f>
+        <v>coins</v>
+      </c>
+    </row>
+    <row r="12" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B12" s="27" t="s">
         <v>1</v>
       </c>
       <c r="C12" s="24" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D12" s="24" t="s">
         <v>65</v>
@@ -3185,7 +3187,7 @@
         <v>7</v>
       </c>
       <c r="I12" s="24" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="J12" s="24">
         <v>10</v>
@@ -3194,21 +3196,22 @@
         <v>11</v>
       </c>
       <c r="L12" s="33" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="M12" s="47" t="s">
-        <v>157</v>
-      </c>
-      <c r="N12" s="31" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="13" spans="2:16" x14ac:dyDescent="0.2">
+        <v>156</v>
+      </c>
+      <c r="N12" s="31" t="str">
+        <f>Table1330[[#This Row],['[sku']]]</f>
+        <v>dragons</v>
+      </c>
+    </row>
+    <row r="13" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B13" s="25" t="s">
         <v>1</v>
       </c>
       <c r="C13" s="23" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D13" s="24" t="s">
         <v>62</v>
@@ -3233,14 +3236,15 @@
         <v>6</v>
       </c>
       <c r="L13" s="33" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="M13" s="33"/>
-      <c r="N13" s="31" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="14" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="N13" s="31" t="str">
+        <f>Table1330[[#This Row],['[sku']]]</f>
+        <v>fire_rushes</v>
+      </c>
+    </row>
+    <row r="14" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B14" s="25" t="s">
         <v>1</v>
       </c>
@@ -3270,14 +3274,15 @@
         <v>400</v>
       </c>
       <c r="L14" s="33" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="M14" s="33"/>
-      <c r="N14" s="31" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="15" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="N14" s="31" t="str">
+        <f>Table1330[[#This Row],['[sku']]]</f>
+        <v>dive</v>
+      </c>
+    </row>
+    <row r="15" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B15" s="25" t="s">
         <v>1</v>
       </c>
@@ -3307,14 +3312,15 @@
         <v>400</v>
       </c>
       <c r="L15" s="33" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="M15" s="33"/>
-      <c r="N15" s="31" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="16" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="N15" s="31" t="str">
+        <f>Table1330[[#This Row],['[sku']]]</f>
+        <v>survive_time</v>
+      </c>
+    </row>
+    <row r="16" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B16" s="25" t="s">
         <v>1</v>
       </c>
@@ -3344,19 +3350,20 @@
         <v>500000</v>
       </c>
       <c r="L16" s="33" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="M16" s="33"/>
-      <c r="N16" s="31" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="17" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="N16" s="31" t="str">
+        <f>Table1330[[#This Row],['[sku']]]</f>
+        <v>score</v>
+      </c>
+    </row>
+    <row r="17" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B17" s="25" t="s">
         <v>1</v>
       </c>
       <c r="C17" s="23" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D17" s="23" t="s">
         <v>65</v>
@@ -3374,7 +3381,7 @@
         <v>7</v>
       </c>
       <c r="I17" s="24" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="J17" s="24">
         <v>45</v>
@@ -3383,21 +3390,22 @@
         <v>55</v>
       </c>
       <c r="L17" s="33" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="M17" s="47" t="s">
-        <v>159</v>
-      </c>
-      <c r="N17" s="31" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="18" spans="2:14" x14ac:dyDescent="0.2">
+        <v>158</v>
+      </c>
+      <c r="N17" s="31" t="str">
+        <f>Table1330[[#This Row],['[sku']]]</f>
+        <v>spiders</v>
+      </c>
+    </row>
+    <row r="18" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B18" s="25" t="s">
         <v>1</v>
       </c>
       <c r="C18" s="24" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D18" s="24" t="s">
         <v>65</v>
@@ -3415,7 +3423,7 @@
         <v>7</v>
       </c>
       <c r="I18" s="24" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="J18" s="24">
         <v>40</v>
@@ -3424,21 +3432,22 @@
         <v>45</v>
       </c>
       <c r="L18" s="33" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="M18" s="33" t="s">
-        <v>158</v>
-      </c>
-      <c r="N18" s="31" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="19" spans="2:14" x14ac:dyDescent="0.2">
+        <v>157</v>
+      </c>
+      <c r="N18" s="31" t="str">
+        <f>Table1330[[#This Row],['[sku']]]</f>
+        <v>goblins</v>
+      </c>
+    </row>
+    <row r="19" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B19" s="25" t="s">
         <v>1</v>
       </c>
       <c r="C19" s="23" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D19" s="23" t="s">
         <v>65</v>
@@ -3456,7 +3465,7 @@
         <v>7</v>
       </c>
       <c r="I19" s="23" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="J19" s="24">
         <v>150</v>
@@ -3465,21 +3474,22 @@
         <v>200</v>
       </c>
       <c r="L19" s="34" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="M19" s="47" t="s">
-        <v>161</v>
-      </c>
-      <c r="N19" s="31" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="20" spans="2:14" x14ac:dyDescent="0.2">
+        <v>160</v>
+      </c>
+      <c r="N19" s="31" t="str">
+        <f>Table1330[[#This Row],['[sku']]]</f>
+        <v>bats</v>
+      </c>
+    </row>
+    <row r="20" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B20" s="25" t="s">
         <v>1</v>
       </c>
       <c r="C20" s="23" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D20" s="23" t="s">
         <v>65</v>
@@ -3497,7 +3507,7 @@
         <v>7</v>
       </c>
       <c r="I20" s="23" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="J20" s="24">
         <v>5</v>
@@ -3506,21 +3516,22 @@
         <v>7</v>
       </c>
       <c r="L20" s="34" t="s">
-        <v>92</v>
-      </c>
-      <c r="M20" s="55" t="s">
-        <v>162</v>
-      </c>
-      <c r="N20" s="31" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="21" spans="2:14" x14ac:dyDescent="0.2">
+        <v>91</v>
+      </c>
+      <c r="M20" s="54" t="s">
+        <v>161</v>
+      </c>
+      <c r="N20" s="31" t="str">
+        <f>Table1330[[#This Row],['[sku']]]</f>
+        <v>owls</v>
+      </c>
+    </row>
+    <row r="21" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B21" s="25" t="s">
         <v>1</v>
       </c>
       <c r="C21" s="23" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D21" s="23" t="s">
         <v>65</v>
@@ -3538,7 +3549,7 @@
         <v>7</v>
       </c>
       <c r="I21" s="23" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="J21" s="23">
         <v>5</v>
@@ -3547,21 +3558,22 @@
         <v>7</v>
       </c>
       <c r="L21" s="34" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="M21" s="34" t="s">
-        <v>163</v>
-      </c>
-      <c r="N21" s="31" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="22" spans="2:14" x14ac:dyDescent="0.2">
+        <v>162</v>
+      </c>
+      <c r="N21" s="31" t="str">
+        <f>Table1330[[#This Row],['[sku']]]</f>
+        <v>lionbird</v>
+      </c>
+    </row>
+    <row r="22" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B22" s="27" t="s">
         <v>1</v>
       </c>
       <c r="C22" s="24" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D22" s="23" t="s">
         <v>65</v>
@@ -3579,7 +3591,7 @@
         <v>7</v>
       </c>
       <c r="I22" s="23" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="J22" s="24">
         <v>3</v>
@@ -3588,21 +3600,22 @@
         <v>4</v>
       </c>
       <c r="L22" s="34" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="M22" s="34" t="s">
-        <v>164</v>
-      </c>
-      <c r="N22" s="31" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="23" spans="2:14" x14ac:dyDescent="0.2">
+        <v>163</v>
+      </c>
+      <c r="N22" s="31" t="str">
+        <f>Table1330[[#This Row],['[sku']]]</f>
+        <v>driller</v>
+      </c>
+    </row>
+    <row r="23" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B23" s="27" t="s">
         <v>1</v>
       </c>
       <c r="C23" s="24" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D23" s="23" t="s">
         <v>65</v>
@@ -3620,7 +3633,7 @@
         <v>7</v>
       </c>
       <c r="I23" s="23" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="J23" s="24">
         <v>3</v>
@@ -3629,21 +3642,22 @@
         <v>3</v>
       </c>
       <c r="L23" s="34" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="M23" s="34" t="s">
-        <v>219</v>
-      </c>
-      <c r="N23" s="31" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="24" spans="2:14" x14ac:dyDescent="0.2">
+        <v>218</v>
+      </c>
+      <c r="N23" s="31" t="str">
+        <f>Table1330[[#This Row],['[sku']]]</f>
+        <v>boatFished</v>
+      </c>
+    </row>
+    <row r="24" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B24" s="27" t="s">
         <v>1</v>
       </c>
       <c r="C24" s="24" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D24" s="23" t="s">
         <v>65</v>
@@ -3661,7 +3675,7 @@
         <v>7</v>
       </c>
       <c r="I24" s="23" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J24" s="24">
         <v>8</v>
@@ -3670,21 +3684,22 @@
         <v>9</v>
       </c>
       <c r="L24" s="34" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="M24" s="34" t="s">
-        <v>165</v>
-      </c>
-      <c r="N24" s="31" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="25" spans="2:14" x14ac:dyDescent="0.2">
+        <v>164</v>
+      </c>
+      <c r="N24" s="31" t="str">
+        <f>Table1330[[#This Row],['[sku']]]</f>
+        <v>archers</v>
+      </c>
+    </row>
+    <row r="25" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B25" s="27" t="s">
         <v>1</v>
       </c>
       <c r="C25" s="24" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D25" s="23" t="s">
         <v>65</v>
@@ -3702,7 +3717,7 @@
         <v>7</v>
       </c>
       <c r="I25" s="23" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="J25" s="24">
         <v>11</v>
@@ -3711,21 +3726,22 @@
         <v>12</v>
       </c>
       <c r="L25" s="34" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="M25" s="34" t="s">
-        <v>166</v>
-      </c>
-      <c r="N25" s="31" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="26" spans="2:14" x14ac:dyDescent="0.2">
+        <v>165</v>
+      </c>
+      <c r="N25" s="31" t="str">
+        <f>Table1330[[#This Row],['[sku']]]</f>
+        <v>soldiers</v>
+      </c>
+    </row>
+    <row r="26" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B26" s="27" t="s">
         <v>1</v>
       </c>
       <c r="C26" s="24" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D26" s="23" t="s">
         <v>65</v>
@@ -3743,7 +3759,7 @@
         <v>7</v>
       </c>
       <c r="I26" s="23" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="J26" s="24">
         <v>3</v>
@@ -3752,16 +3768,17 @@
         <v>3</v>
       </c>
       <c r="L26" s="34" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="M26" s="34" t="s">
-        <v>167</v>
-      </c>
-      <c r="N26" s="31" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="27" spans="2:14" x14ac:dyDescent="0.2">
+        <v>166</v>
+      </c>
+      <c r="N26" s="31" t="str">
+        <f>Table1330[[#This Row],['[sku']]]</f>
+        <v>troll</v>
+      </c>
+    </row>
+    <row r="27" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B27" s="27" t="s">
         <v>1</v>
       </c>
@@ -3791,22 +3808,23 @@
         <v>7000</v>
       </c>
       <c r="L27" s="34" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="M27" s="34"/>
-      <c r="N27" s="31" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="28" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="N27" s="31" t="str">
+        <f>Table1330[[#This Row],['[sku']]]</f>
+        <v>distance</v>
+      </c>
+    </row>
+    <row r="28" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B28" s="50" t="s">
         <v>1</v>
       </c>
       <c r="C28" s="51" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D28" s="52" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E28" s="52">
         <v>0</v>
@@ -3817,11 +3835,11 @@
       <c r="G28" s="51">
         <v>0</v>
       </c>
-      <c r="H28" s="54">
+      <c r="H28" s="53">
         <v>7</v>
       </c>
       <c r="I28" s="52" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="J28" s="51">
         <v>8</v>
@@ -3829,25 +3847,26 @@
       <c r="K28" s="52">
         <v>9</v>
       </c>
-      <c r="L28" s="54" t="s">
-        <v>201</v>
-      </c>
-      <c r="M28" s="54" t="s">
-        <v>159</v>
-      </c>
-      <c r="N28" s="53" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="29" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="L28" s="53" t="s">
+        <v>200</v>
+      </c>
+      <c r="M28" s="53" t="s">
+        <v>158</v>
+      </c>
+      <c r="N28" s="31" t="str">
+        <f>Table1330[[#This Row],['[sku']]]</f>
+        <v>eat_spec_anim_a_spiders</v>
+      </c>
+    </row>
+    <row r="29" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B29" s="50" t="s">
         <v>1</v>
       </c>
       <c r="C29" s="51" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D29" s="52" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E29" s="52">
         <v>1</v>
@@ -3858,7 +3877,7 @@
       <c r="G29" s="51">
         <v>0</v>
       </c>
-      <c r="H29" s="54">
+      <c r="H29" s="53">
         <v>7</v>
       </c>
       <c r="I29" s="52"/>
@@ -3868,25 +3887,26 @@
       <c r="K29" s="52">
         <v>55</v>
       </c>
-      <c r="L29" s="54" t="s">
-        <v>202</v>
-      </c>
-      <c r="M29" s="54" t="s">
-        <v>216</v>
-      </c>
-      <c r="N29" s="53" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="30" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="L29" s="53" t="s">
+        <v>201</v>
+      </c>
+      <c r="M29" s="53" t="s">
+        <v>215</v>
+      </c>
+      <c r="N29" s="31" t="str">
+        <f>Table1330[[#This Row],['[sku']]]</f>
+        <v>eat_gold_gen</v>
+      </c>
+    </row>
+    <row r="30" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B30" s="50" t="s">
         <v>1</v>
       </c>
       <c r="C30" s="51" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D30" s="52" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E30" s="52">
         <v>1</v>
@@ -3897,11 +3917,11 @@
       <c r="G30" s="51">
         <v>3</v>
       </c>
-      <c r="H30" s="54">
+      <c r="H30" s="53">
         <v>7</v>
       </c>
       <c r="I30" s="52" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="J30" s="51">
         <v>4</v>
@@ -3909,25 +3929,26 @@
       <c r="K30" s="52">
         <v>4</v>
       </c>
-      <c r="L30" s="54" t="s">
-        <v>203</v>
-      </c>
-      <c r="M30" s="54" t="s">
-        <v>168</v>
-      </c>
-      <c r="N30" s="53" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="31" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="L30" s="53" t="s">
+        <v>202</v>
+      </c>
+      <c r="M30" s="53" t="s">
+        <v>167</v>
+      </c>
+      <c r="N30" s="31" t="str">
+        <f>Table1330[[#This Row],['[sku']]]</f>
+        <v>eat_gold_stingrays</v>
+      </c>
+    </row>
+    <row r="31" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B31" s="50" t="s">
         <v>1</v>
       </c>
       <c r="C31" s="51" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D31" s="52" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E31" s="52">
         <v>1</v>
@@ -3938,11 +3959,11 @@
       <c r="G31" s="51">
         <v>3</v>
       </c>
-      <c r="H31" s="54">
+      <c r="H31" s="53">
         <v>7</v>
       </c>
       <c r="I31" s="52" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="J31" s="51">
         <v>5</v>
@@ -3951,24 +3972,25 @@
         <v>5</v>
       </c>
       <c r="L31" s="48" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="M31" s="48" t="s">
-        <v>215</v>
-      </c>
-      <c r="N31" s="53" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="32" spans="2:14" s="43" customFormat="1" x14ac:dyDescent="0.2">
+        <v>214</v>
+      </c>
+      <c r="N31" s="31" t="str">
+        <f>Table1330[[#This Row],['[sku']]]</f>
+        <v>eat_gold_cattle</v>
+      </c>
+    </row>
+    <row r="32" spans="2:14" s="43" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B32" s="50" t="s">
         <v>1</v>
       </c>
       <c r="C32" s="51" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D32" s="52" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E32" s="52">
         <v>1</v>
@@ -3983,7 +4005,7 @@
         <v>7</v>
       </c>
       <c r="I32" s="52" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="J32" s="51">
         <v>17</v>
@@ -3992,24 +4014,25 @@
         <v>18</v>
       </c>
       <c r="L32" s="48" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="M32" s="48" t="s">
-        <v>158</v>
-      </c>
-      <c r="N32" s="53" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="33" spans="2:14" s="43" customFormat="1" x14ac:dyDescent="0.2">
+        <v>157</v>
+      </c>
+      <c r="N32" s="31" t="str">
+        <f>Table1330[[#This Row],['[sku']]]</f>
+        <v>eat_gold_goblins</v>
+      </c>
+    </row>
+    <row r="33" spans="2:14" s="43" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B33" s="50" t="s">
         <v>1</v>
       </c>
       <c r="C33" s="40" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D33" s="41" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E33" s="52">
         <v>0</v>
@@ -4031,19 +4054,20 @@
         <v>27</v>
       </c>
       <c r="L33" s="48" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="M33" s="48"/>
-      <c r="N33" s="53" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="34" spans="2:14" s="43" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="N33" s="31" t="str">
+        <f>Table1330[[#This Row],['[sku']]]</f>
+        <v>critical_time</v>
+      </c>
+    </row>
+    <row r="34" spans="2:14" s="43" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B34" s="27" t="s">
         <v>1</v>
       </c>
       <c r="C34" s="24" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D34" s="23" t="s">
         <v>56</v>
@@ -4061,7 +4085,7 @@
         <v>3</v>
       </c>
       <c r="I34" s="23" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="J34" s="24">
         <v>10</v>
@@ -4070,24 +4094,25 @@
         <v>12</v>
       </c>
       <c r="L34" s="33" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="M34" s="47" t="s">
-        <v>153</v>
-      </c>
-      <c r="N34" s="31" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="35" spans="2:14" s="43" customFormat="1" x14ac:dyDescent="0.2">
+        <v>152</v>
+      </c>
+      <c r="N34" s="31" t="str">
+        <f>Table1330[[#This Row],['[sku']]]</f>
+        <v>houses</v>
+      </c>
+    </row>
+    <row r="35" spans="2:14" s="43" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B35" s="50" t="s">
         <v>1</v>
       </c>
       <c r="C35" s="51" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D35" s="52" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E35" s="52">
         <v>1</v>
@@ -4102,7 +4127,7 @@
         <v>3</v>
       </c>
       <c r="I35" s="52" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="J35" s="51">
         <v>3</v>
@@ -4111,24 +4136,25 @@
         <v>4</v>
       </c>
       <c r="L35" s="48" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="M35" s="49" t="s">
-        <v>217</v>
-      </c>
-      <c r="N35" s="53" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="36" spans="2:14" s="43" customFormat="1" x14ac:dyDescent="0.2">
+        <v>216</v>
+      </c>
+      <c r="N35" s="31" t="str">
+        <f>Table1330[[#This Row],['[sku']]]</f>
+        <v>eat_gold_witch</v>
+      </c>
+    </row>
+    <row r="36" spans="2:14" s="43" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B36" s="50" t="s">
         <v>1</v>
       </c>
       <c r="C36" s="51" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D36" s="52" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E36" s="52">
         <v>1</v>
@@ -4143,7 +4169,7 @@
         <v>3</v>
       </c>
       <c r="I36" s="52" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="J36" s="51">
         <v>25</v>
@@ -4152,21 +4178,22 @@
         <v>27</v>
       </c>
       <c r="L36" s="48" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="M36" s="52" t="s">
-        <v>150</v>
-      </c>
-      <c r="N36" s="53" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="37" spans="2:14" s="43" customFormat="1" x14ac:dyDescent="0.2">
+        <v>149</v>
+      </c>
+      <c r="N36" s="31" t="str">
+        <f>Table1330[[#This Row],['[sku']]]</f>
+        <v>eat_gold_birds</v>
+      </c>
+    </row>
+    <row r="37" spans="2:14" s="43" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B37" s="27" t="s">
         <v>1</v>
       </c>
       <c r="C37" s="24" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D37" s="23" t="s">
         <v>65</v>
@@ -4184,7 +4211,7 @@
         <v>2</v>
       </c>
       <c r="I37" s="23" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="J37" s="24">
         <v>10</v>
@@ -4193,24 +4220,25 @@
         <v>12</v>
       </c>
       <c r="L37" s="33" t="s">
-        <v>100</v>
-      </c>
-      <c r="M37" s="57" t="s">
-        <v>154</v>
-      </c>
-      <c r="N37" s="31" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="38" spans="2:14" s="43" customFormat="1" x14ac:dyDescent="0.2">
+        <v>99</v>
+      </c>
+      <c r="M37" s="56" t="s">
+        <v>153</v>
+      </c>
+      <c r="N37" s="31" t="str">
+        <f>Table1330[[#This Row],['[sku']]]</f>
+        <v>vulture</v>
+      </c>
+    </row>
+    <row r="38" spans="2:14" s="43" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B38" s="50" t="s">
         <v>1</v>
       </c>
       <c r="C38" s="51" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D38" s="52" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="E38" s="52">
         <v>0</v>
@@ -4225,7 +4253,7 @@
         <v>2</v>
       </c>
       <c r="I38" s="52" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="J38" s="51">
         <v>150</v>
@@ -4234,24 +4262,25 @@
         <v>160</v>
       </c>
       <c r="L38" s="48" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="M38" s="49" t="s">
-        <v>150</v>
-      </c>
-      <c r="N38" s="53" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="39" spans="2:14" s="43" customFormat="1" x14ac:dyDescent="0.2">
+        <v>149</v>
+      </c>
+      <c r="N38" s="31" t="str">
+        <f>Table1330[[#This Row],['[sku']]]</f>
+        <v>kill_chain_canaries</v>
+      </c>
+    </row>
+    <row r="39" spans="2:14" s="43" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B39" s="50" t="s">
         <v>1</v>
       </c>
       <c r="C39" s="51" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D39" s="52" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="E39" s="52">
         <v>0</v>
@@ -4266,7 +4295,7 @@
         <v>2</v>
       </c>
       <c r="I39" s="52" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="J39" s="51">
         <v>15</v>
@@ -4275,24 +4304,25 @@
         <v>16</v>
       </c>
       <c r="L39" s="48" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="M39" s="48" t="s">
-        <v>152</v>
-      </c>
-      <c r="N39" s="53" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="40" spans="2:14" s="43" customFormat="1" x14ac:dyDescent="0.2">
+        <v>151</v>
+      </c>
+      <c r="N39" s="31" t="str">
+        <f>Table1330[[#This Row],['[sku']]]</f>
+        <v>kill_chain_humans</v>
+      </c>
+    </row>
+    <row r="40" spans="2:14" s="43" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B40" s="50" t="s">
         <v>1</v>
       </c>
       <c r="C40" s="51" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D40" s="52" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E40" s="52">
         <v>1</v>
@@ -4307,7 +4337,7 @@
         <v>2</v>
       </c>
       <c r="I40" s="52" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="J40" s="51">
         <v>3</v>
@@ -4316,24 +4346,25 @@
         <v>3</v>
       </c>
       <c r="L40" s="48" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="M40" s="48" t="s">
-        <v>169</v>
-      </c>
-      <c r="N40" s="53" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="41" spans="2:14" s="43" customFormat="1" x14ac:dyDescent="0.2">
+        <v>168</v>
+      </c>
+      <c r="N40" s="31" t="str">
+        <f>Table1330[[#This Row],['[sku']]]</f>
+        <v>eat_gold_birdsOfPrey</v>
+      </c>
+    </row>
+    <row r="41" spans="2:14" s="43" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B41" s="50" t="s">
         <v>1</v>
       </c>
       <c r="C41" s="40" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D41" s="41" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="E41" s="52">
         <v>1</v>
@@ -4348,7 +4379,7 @@
         <v>2</v>
       </c>
       <c r="I41" s="41" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="J41" s="51">
         <v>50</v>
@@ -4357,19 +4388,20 @@
         <v>52</v>
       </c>
       <c r="L41" s="48" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="M41" s="42"/>
-      <c r="N41" s="53" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="42" spans="2:14" s="43" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="N41" s="31" t="str">
+        <f>Table1330[[#This Row],['[sku']]]</f>
+        <v>destroy_mineSmall</v>
+      </c>
+    </row>
+    <row r="42" spans="2:14" s="43" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B42" s="27" t="s">
         <v>1</v>
       </c>
       <c r="C42" s="24" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D42" s="24" t="s">
         <v>50</v>
@@ -4387,7 +4419,7 @@
         <v>1</v>
       </c>
       <c r="I42" s="23" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="J42" s="24">
         <v>1</v>
@@ -4396,21 +4428,22 @@
         <v>2</v>
       </c>
       <c r="L42" s="33" t="s">
-        <v>117</v>
-      </c>
-      <c r="M42" s="56" t="s">
-        <v>156</v>
-      </c>
-      <c r="N42" s="31" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="43" spans="2:14" s="43" customFormat="1" x14ac:dyDescent="0.2">
+        <v>116</v>
+      </c>
+      <c r="M42" s="55" t="s">
+        <v>155</v>
+      </c>
+      <c r="N42" s="31" t="str">
+        <f>Table1330[[#This Row],['[sku']]]</f>
+        <v>eggs</v>
+      </c>
+    </row>
+    <row r="43" spans="2:14" s="43" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B43" s="27" t="s">
         <v>1</v>
       </c>
       <c r="C43" s="24" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D43" s="24" t="s">
         <v>65</v>
@@ -4428,7 +4461,7 @@
         <v>1</v>
       </c>
       <c r="I43" s="23" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="J43" s="24">
         <v>5</v>
@@ -4437,16 +4470,17 @@
         <v>6</v>
       </c>
       <c r="L43" s="33" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="M43" s="23" t="s">
-        <v>160</v>
-      </c>
-      <c r="N43" s="31" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="44" spans="2:14" s="43" customFormat="1" x14ac:dyDescent="0.2">
+        <v>159</v>
+      </c>
+      <c r="N43" s="31" t="str">
+        <f>Table1330[[#This Row],['[sku']]]</f>
+        <v>flyingPig</v>
+      </c>
+    </row>
+    <row r="44" spans="2:14" s="43" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B44" s="44"/>
       <c r="C44" s="44"/>
       <c r="D44" s="44"/>
@@ -4461,7 +4495,7 @@
       <c r="M44" s="44"/>
       <c r="N44" s="44"/>
     </row>
-    <row r="45" spans="2:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B45" s="32"/>
       <c r="C45" s="32"/>
       <c r="D45" s="32"/>
@@ -4475,7 +4509,7 @@
       <c r="L45" s="32"/>
       <c r="M45" s="31"/>
     </row>
-    <row r="46" spans="2:14" ht="24" x14ac:dyDescent="0.3">
+    <row r="46" spans="2:14" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B46" s="6" t="s">
         <v>72</v>
       </c>
@@ -4490,7 +4524,7 @@
       <c r="K46" s="6"/>
       <c r="L46" s="6"/>
     </row>
-    <row r="47" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="47" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B47" s="20"/>
       <c r="C47" s="20"/>
       <c r="D47" s="20"/>
@@ -4501,7 +4535,7 @@
       <c r="I47" s="20"/>
       <c r="J47" s="20"/>
     </row>
-    <row r="48" spans="2:14" ht="93" x14ac:dyDescent="0.2">
+    <row r="48" spans="2:14" ht="96" x14ac:dyDescent="0.25">
       <c r="B48" s="30" t="s">
         <v>71</v>
       </c>
@@ -4524,7 +4558,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="49" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="49" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B49" s="27" t="s">
         <v>1</v>
       </c>
@@ -4547,7 +4581,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="50" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="50" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B50" s="27" t="s">
         <v>1</v>
       </c>
@@ -4570,7 +4604,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="51" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="51" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B51" s="27" t="s">
         <v>1</v>
       </c>
@@ -4593,7 +4627,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="52" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="52" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B52" s="27" t="s">
         <v>1</v>
       </c>
@@ -4616,7 +4650,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="53" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="53" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B53" s="25" t="s">
         <v>1</v>
       </c>
@@ -4639,7 +4673,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="54" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="54" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B54" s="25" t="s">
         <v>1</v>
       </c>
@@ -4662,7 +4696,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="55" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="55" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B55" s="25" t="s">
         <v>1</v>
       </c>
@@ -4685,7 +4719,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="56" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="56" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B56" s="25" t="s">
         <v>1</v>
       </c>
@@ -4708,12 +4742,12 @@
         <v>42</v>
       </c>
     </row>
-    <row r="57" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="57" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B57" s="46" t="s">
         <v>1</v>
       </c>
       <c r="C57" s="41" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D57" s="41">
         <v>0</v>
@@ -4725,18 +4759,18 @@
         <v>0</v>
       </c>
       <c r="G57" s="42" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="H57" s="42" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="58" spans="2:8" x14ac:dyDescent="0.2">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="58" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B58" s="46" t="s">
         <v>1</v>
       </c>
       <c r="C58" s="41" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D58" s="41">
         <v>0</v>
@@ -4748,18 +4782,18 @@
         <v>0</v>
       </c>
       <c r="G58" s="45" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="H58" s="45" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="59" spans="2:8" x14ac:dyDescent="0.2">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="59" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B59" s="46" t="s">
         <v>1</v>
       </c>
       <c r="C59" s="41" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D59" s="41">
         <v>0</v>
@@ -4771,18 +4805,18 @@
         <v>2</v>
       </c>
       <c r="G59" s="45" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="H59" s="45" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="60" spans="2:8" x14ac:dyDescent="0.2">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="60" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B60" s="46" t="s">
         <v>1</v>
       </c>
       <c r="C60" s="40" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="D60" s="41">
         <v>0</v>
@@ -4794,18 +4828,18 @@
         <v>1</v>
       </c>
       <c r="G60" s="45" t="s">
+        <v>231</v>
+      </c>
+      <c r="H60" s="45" t="s">
         <v>232</v>
       </c>
-      <c r="H60" s="45" t="s">
+    </row>
+    <row r="61" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B61" s="46" t="s">
+        <v>1</v>
+      </c>
+      <c r="C61" s="40" t="s">
         <v>233</v>
-      </c>
-    </row>
-    <row r="61" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B61" s="46" t="s">
-        <v>1</v>
-      </c>
-      <c r="C61" s="40" t="s">
-        <v>234</v>
       </c>
       <c r="D61" s="41">
         <v>0</v>
@@ -4817,18 +4851,18 @@
         <v>1</v>
       </c>
       <c r="G61" s="45" t="s">
+        <v>234</v>
+      </c>
+      <c r="H61" s="45" t="s">
         <v>235</v>
       </c>
-      <c r="H61" s="45" t="s">
+    </row>
+    <row r="62" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B62" s="46" t="s">
+        <v>1</v>
+      </c>
+      <c r="C62" s="40" t="s">
         <v>236</v>
-      </c>
-    </row>
-    <row r="62" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B62" s="46" t="s">
-        <v>1</v>
-      </c>
-      <c r="C62" s="40" t="s">
-        <v>237</v>
       </c>
       <c r="D62" s="41">
         <v>0</v>
@@ -4840,18 +4874,18 @@
         <v>1</v>
       </c>
       <c r="G62" s="45" t="s">
+        <v>237</v>
+      </c>
+      <c r="H62" s="45" t="s">
         <v>238</v>
       </c>
-      <c r="H62" s="45" t="s">
+    </row>
+    <row r="63" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B63" s="58" t="s">
+        <v>1</v>
+      </c>
+      <c r="C63" s="40" t="s">
         <v>239</v>
-      </c>
-    </row>
-    <row r="63" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B63" s="62" t="s">
-        <v>1</v>
-      </c>
-      <c r="C63" s="40" t="s">
-        <v>240</v>
       </c>
       <c r="D63" s="40">
         <v>0</v>
@@ -4863,18 +4897,18 @@
         <v>1</v>
       </c>
       <c r="G63" s="45" t="s">
+        <v>240</v>
+      </c>
+      <c r="H63" s="45" t="s">
         <v>241</v>
       </c>
-      <c r="H63" s="45" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="64" spans="2:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="64" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B64" s="46" t="s">
         <v>1</v>
       </c>
       <c r="C64" s="41" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D64" s="41">
         <v>0</v>
@@ -4886,18 +4920,18 @@
         <v>0</v>
       </c>
       <c r="G64" s="45" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="H64" s="45" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="65" spans="2:13" x14ac:dyDescent="0.2">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="65" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B65" s="46" t="s">
         <v>1</v>
       </c>
       <c r="C65" s="40" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D65" s="41">
         <v>0</v>
@@ -4909,16 +4943,16 @@
         <v>1</v>
       </c>
       <c r="G65" s="45" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="H65" s="45"/>
     </row>
-    <row r="66" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="66" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B66" s="46" t="s">
         <v>1</v>
       </c>
       <c r="C66" s="40" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D66" s="41">
         <v>0</v>
@@ -4930,18 +4964,18 @@
         <v>0</v>
       </c>
       <c r="G66" s="45" t="s">
+        <v>186</v>
+      </c>
+      <c r="H66" s="45" t="s">
         <v>187</v>
       </c>
-      <c r="H66" s="45" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="67" spans="2:13" x14ac:dyDescent="0.2">
+    </row>
+    <row r="67" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B67" s="46" t="s">
         <v>1</v>
       </c>
       <c r="C67" s="40" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D67" s="41">
         <v>0</v>
@@ -4953,14 +4987,14 @@
         <v>1</v>
       </c>
       <c r="G67" s="45" t="s">
+        <v>212</v>
+      </c>
+      <c r="H67" s="45" t="s">
         <v>213</v>
       </c>
-      <c r="H67" s="45" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="68" spans="2:13" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="69" spans="2:13" ht="24" x14ac:dyDescent="0.3">
+    </row>
+    <row r="68" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="69" spans="2:13" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B69" s="6" t="s">
         <v>41</v>
       </c>
@@ -4976,7 +5010,7 @@
       <c r="L69" s="6"/>
       <c r="M69" s="6"/>
     </row>
-    <row r="70" spans="2:13" ht="64" x14ac:dyDescent="0.2">
+    <row r="70" spans="2:13" ht="60" x14ac:dyDescent="0.25">
       <c r="B70" s="20"/>
       <c r="C70" s="20"/>
       <c r="D70" s="20"/>
@@ -4990,7 +5024,7 @@
       <c r="H70" s="61"/>
       <c r="I70" s="20"/>
     </row>
-    <row r="71" spans="2:13" ht="137" x14ac:dyDescent="0.2">
+    <row r="71" spans="2:13" ht="142.5" x14ac:dyDescent="0.25">
       <c r="B71" s="19" t="s">
         <v>38</v>
       </c>
@@ -4998,7 +5032,7 @@
         <v>3</v>
       </c>
       <c r="D71" s="18" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="E71" s="18" t="s">
         <v>37</v>
@@ -5025,12 +5059,12 @@
         <v>30</v>
       </c>
     </row>
-    <row r="72" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="72" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B72" s="12" t="s">
         <v>1</v>
       </c>
       <c r="C72" s="11" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="D72" s="11" t="s">
         <v>8</v>
@@ -5060,12 +5094,12 @@
         <v>28</v>
       </c>
     </row>
-    <row r="73" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="73" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B73" s="12" t="s">
         <v>1</v>
       </c>
       <c r="C73" s="11" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D73" s="11" t="s">
         <v>7</v>
@@ -5095,12 +5129,12 @@
         <v>26</v>
       </c>
     </row>
-    <row r="74" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="74" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B74" s="12" t="s">
         <v>1</v>
       </c>
       <c r="C74" s="11" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="D74" s="11" t="s">
         <v>6</v>
@@ -5130,8 +5164,8 @@
         <v>24</v>
       </c>
     </row>
-    <row r="76" spans="2:13" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="77" spans="2:13" ht="24" x14ac:dyDescent="0.3">
+    <row r="76" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="77" spans="2:13" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B77" s="6" t="s">
         <v>23</v>
       </c>
@@ -5141,7 +5175,7 @@
       <c r="F77" s="6"/>
       <c r="G77" s="6"/>
     </row>
-    <row r="79" spans="2:13" ht="132" x14ac:dyDescent="0.2">
+    <row r="79" spans="2:13" ht="135.75" x14ac:dyDescent="0.25">
       <c r="B79" s="5" t="s">
         <v>22</v>
       </c>
@@ -5155,7 +5189,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="80" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="80" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B80" s="2" t="s">
         <v>1</v>
       </c>
@@ -5169,7 +5203,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="81" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="81" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B81" s="2" t="s">
         <v>1</v>
       </c>
@@ -5183,7 +5217,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="82" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="82" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B82" s="2" t="s">
         <v>1</v>
       </c>
@@ -5197,7 +5231,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="83" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="83" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B83" s="2" t="s">
         <v>1</v>
       </c>
@@ -5211,7 +5245,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="84" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="84" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B84" s="2" t="s">
         <v>1</v>
       </c>
@@ -5225,7 +5259,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="85" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="85" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B85" s="2" t="s">
         <v>1</v>
       </c>
@@ -5239,7 +5273,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="86" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="86" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B86" s="2" t="s">
         <v>1</v>
       </c>
@@ -5253,7 +5287,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="87" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="87" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B87" s="2" t="s">
         <v>1</v>
       </c>
@@ -5267,12 +5301,12 @@
         <v>56</v>
       </c>
     </row>
-    <row r="88" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="88" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B88" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D88" s="1">
         <v>4.5</v>
@@ -5281,7 +5315,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="89" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="89" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B89" s="2" t="s">
         <v>1</v>
       </c>
@@ -5295,7 +5329,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="90" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="90" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B90" s="2" t="s">
         <v>1</v>
       </c>
@@ -5309,22 +5343,22 @@
         <v>80</v>
       </c>
     </row>
-    <row r="91" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="91" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B91" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>223</v>
-      </c>
-      <c r="D91" s="58">
+        <v>222</v>
+      </c>
+      <c r="D91" s="57">
         <v>7.5</v>
       </c>
       <c r="E91" s="1">
         <v>85</v>
       </c>
     </row>
-    <row r="92" spans="2:7" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="93" spans="2:7" ht="24" x14ac:dyDescent="0.3">
+    <row r="92" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="93" spans="2:7" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B93" s="6" t="s">
         <v>10</v>
       </c>
@@ -5334,7 +5368,7 @@
       <c r="F93" s="6"/>
       <c r="G93" s="6"/>
     </row>
-    <row r="95" spans="2:7" ht="142" x14ac:dyDescent="0.2">
+    <row r="95" spans="2:7" ht="142.5" x14ac:dyDescent="0.25">
       <c r="B95" s="5" t="s">
         <v>9</v>
       </c>
@@ -5342,18 +5376,18 @@
         <v>3</v>
       </c>
       <c r="D95" s="4" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="E95" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="96" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="96" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B96" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="D96" s="1" t="s">
         <v>8</v>
@@ -5362,12 +5396,12 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="97" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="97" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B97" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="D97" s="1" t="s">
         <v>7</v>
@@ -5376,12 +5410,12 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="98" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="98" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B98" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D98" s="1" t="s">
         <v>6</v>
@@ -5390,8 +5424,8 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="99" spans="2:7" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="100" spans="2:7" ht="24" x14ac:dyDescent="0.3">
+    <row r="99" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="100" spans="2:7" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B100" s="6" t="s">
         <v>5</v>
       </c>
@@ -5401,7 +5435,7 @@
       <c r="F100" s="6"/>
       <c r="G100" s="6"/>
     </row>
-    <row r="102" spans="2:7" ht="131" x14ac:dyDescent="0.2">
+    <row r="102" spans="2:7" ht="132" x14ac:dyDescent="0.25">
       <c r="B102" s="5" t="s">
         <v>4</v>
       </c>
@@ -5412,7 +5446,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="103" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="103" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B103" s="2" t="s">
         <v>1</v>
       </c>
@@ -5431,7 +5465,7 @@
     <mergeCell ref="G70:H70"/>
   </mergeCells>
   <conditionalFormatting sqref="C72:E74">
-    <cfRule type="duplicateValues" dxfId="0" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="68" priority="2"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Created a new table for the 3d Icons
Former-commit-id: f39e9ebc736c54906974c229a92e8e05624a7f16
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Missions.xlsx
+++ b/Docs/Content/HungryDragonContent_Missions.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="394" uniqueCount="242">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="546" uniqueCount="306">
   <si>
     <t>single_run</t>
   </si>
@@ -776,12 +776,204 @@
   <si>
     <t>TID_MISSION_OBJECTIVE_KILL_EQUIPABLE_DESC_MULTI_RUN</t>
   </si>
+  <si>
+    <t>Icon Definitions</t>
+  </si>
+  <si>
+    <t>{iconDefinitions}</t>
+  </si>
+  <si>
+    <t>[asset]</t>
+  </si>
+  <si>
+    <t>[icon3d]</t>
+  </si>
+  <si>
+    <t>icon_easter_bunny</t>
+  </si>
+  <si>
+    <t>icon_easter_egg</t>
+  </si>
+  <si>
+    <t>icon_firerush</t>
+  </si>
+  <si>
+    <t>icon_football</t>
+  </si>
+  <si>
+    <t>icon_goblin_castle</t>
+  </si>
+  <si>
+    <t>icon_heart</t>
+  </si>
+  <si>
+    <t>icon_mexican_pepper</t>
+  </si>
+  <si>
+    <t>icon_mission_destory_gift</t>
+  </si>
+  <si>
+    <t>icon_mission_kill_in_love_all</t>
+  </si>
+  <si>
+    <t>icon_mooncake</t>
+  </si>
+  <si>
+    <t>icon_pumpkin</t>
+  </si>
+  <si>
+    <t>icon_rabbit</t>
+  </si>
+  <si>
+    <t>icon_red_envelope</t>
+  </si>
+  <si>
+    <t>icon_sheep</t>
+  </si>
+  <si>
+    <t>icon_snorkel_cocktail</t>
+  </si>
+  <si>
+    <t>icon_stpatrick_balloon</t>
+  </si>
+  <si>
+    <t>icon_stpatrick_kill</t>
+  </si>
+  <si>
+    <t>icon_ufo_disguise_humanoids</t>
+  </si>
+  <si>
+    <t>icon_unknown</t>
+  </si>
+  <si>
+    <t>icon_watermelon</t>
+  </si>
+  <si>
+    <t>icon_witch</t>
+  </si>
+  <si>
+    <t>PF_icon_archer</t>
+  </si>
+  <si>
+    <t>PF_icon_bat_s</t>
+  </si>
+  <si>
+    <t>PF_icon_canary</t>
+  </si>
+  <si>
+    <t>PF_icon_dragon</t>
+  </si>
+  <si>
+    <t>PF_icon_easter_bunny</t>
+  </si>
+  <si>
+    <t>PF_icon_easter_egg</t>
+  </si>
+  <si>
+    <t>PF_icon_eat_gold_birds</t>
+  </si>
+  <si>
+    <t>PF_icon_eat_gold_cattle</t>
+  </si>
+  <si>
+    <t>PF_icon_eat_gold_gen</t>
+  </si>
+  <si>
+    <t>PF_icon_eat_gold_goblins</t>
+  </si>
+  <si>
+    <t>PF_icon_eat_gold_preybirds</t>
+  </si>
+  <si>
+    <t>PF_icon_eat_gold_stingrays</t>
+  </si>
+  <si>
+    <t>PF_icon_eat_gold_witch</t>
+  </si>
+  <si>
+    <t>PF_icon_egg</t>
+  </si>
+  <si>
+    <t>PF_icon_fisherman</t>
+  </si>
+  <si>
+    <t>PF_icon_flying_pig</t>
+  </si>
+  <si>
+    <t>PF_icon_football</t>
+  </si>
+  <si>
+    <t>PF_icon_goblin_castle</t>
+  </si>
+  <si>
+    <t>PF_icon_goblins</t>
+  </si>
+  <si>
+    <t>PF_icon_humans</t>
+  </si>
+  <si>
+    <t>PF_icon_lionbird</t>
+  </si>
+  <si>
+    <t>PF_icon_mexican_pepper</t>
+  </si>
+  <si>
+    <t>PF_icon_mission_destory_gift</t>
+  </si>
+  <si>
+    <t>PF_icon_mooncake</t>
+  </si>
+  <si>
+    <t>PF_icon_owl</t>
+  </si>
+  <si>
+    <t>PF_icon_pumpkin</t>
+  </si>
+  <si>
+    <t>PF_icon_rabbit</t>
+  </si>
+  <si>
+    <t>PF_icon_red_envelope</t>
+  </si>
+  <si>
+    <t>PF_icon_rocket</t>
+  </si>
+  <si>
+    <t>PF_icon_sheep</t>
+  </si>
+  <si>
+    <t>PF_icon_snorkel_cocktail</t>
+  </si>
+  <si>
+    <t>PF_icon_soldiers</t>
+  </si>
+  <si>
+    <t>PF_icon_spiders</t>
+  </si>
+  <si>
+    <t>PF_icon_stpatrick_balloon</t>
+  </si>
+  <si>
+    <t>PF_icon_stpatrick_kill</t>
+  </si>
+  <si>
+    <t>PF_icon_ufo_disguise_humanoids</t>
+  </si>
+  <si>
+    <t>PF_icon_vulture</t>
+  </si>
+  <si>
+    <t>PF_icon_watermelon</t>
+  </si>
+  <si>
+    <t>PF_icon_witch</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -855,6 +1047,21 @@
     <font>
       <sz val="11"/>
       <color theme="1" tint="4.9989318521683403E-2"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF172B4D"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1108,7 +1315,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="62">
+  <cellXfs count="66">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1"/>
@@ -1265,11 +1472,29 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment textRotation="45"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment textRotation="45"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="69">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -2389,16 +2614,6 @@
         </bottom>
       </border>
     </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -2413,99 +2628,99 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="missionDifficultyDefinitions" displayName="missionDifficultyDefinitions" ref="B71:L74" totalsRowShown="0" headerRowBorderDxfId="67" tableBorderDxfId="66">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="missionDifficultyDefinitions" displayName="missionDifficultyDefinitions" ref="B71:L74" totalsRowShown="0" headerRowBorderDxfId="68" tableBorderDxfId="67">
   <autoFilter ref="B71:L74"/>
   <tableColumns count="11">
     <tableColumn id="1" name="{missionDifficultyDefinitions}"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="65"/>
-    <tableColumn id="11" name="[difficulty]" dataDxfId="64"/>
-    <tableColumn id="7" name="[index]" dataDxfId="63"/>
-    <tableColumn id="3" name="[dragonsToUnlock]" dataDxfId="62"/>
-    <tableColumn id="4" name="[cooldownMinutes]" dataDxfId="61"/>
-    <tableColumn id="9" name="[maxRewardCoins]" dataDxfId="60"/>
-    <tableColumn id="5" name="[removeMissionPCCoefA]" dataDxfId="59"/>
-    <tableColumn id="6" name="[removeMissionPCCoefB]" dataDxfId="58"/>
-    <tableColumn id="8" name="[tidName]" dataDxfId="57"/>
-    <tableColumn id="10" name="[color]" dataDxfId="56"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="66"/>
+    <tableColumn id="11" name="[difficulty]" dataDxfId="65"/>
+    <tableColumn id="7" name="[index]" dataDxfId="64"/>
+    <tableColumn id="3" name="[dragonsToUnlock]" dataDxfId="63"/>
+    <tableColumn id="4" name="[cooldownMinutes]" dataDxfId="62"/>
+    <tableColumn id="9" name="[maxRewardCoins]" dataDxfId="61"/>
+    <tableColumn id="5" name="[removeMissionPCCoefA]" dataDxfId="60"/>
+    <tableColumn id="6" name="[removeMissionPCCoefB]" dataDxfId="59"/>
+    <tableColumn id="8" name="[tidName]" dataDxfId="58"/>
+    <tableColumn id="10" name="[color]" dataDxfId="57"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table13303132" displayName="Table13303132" ref="B79:E91" totalsRowShown="0" headerRowDxfId="55" dataDxfId="53" headerRowBorderDxfId="54" tableBorderDxfId="52" totalsRowBorderDxfId="51">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table13303132" displayName="Table13303132" ref="B79:E91" totalsRowShown="0" headerRowDxfId="56" dataDxfId="54" headerRowBorderDxfId="55" tableBorderDxfId="53" totalsRowBorderDxfId="52">
   <autoFilter ref="B79:E91"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="{missionDragonModifiersDefinitions}" dataDxfId="50"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="49"/>
-    <tableColumn id="7" name="[quantityModifier]" dataDxfId="48"/>
-    <tableColumn id="3" name="[missionSCRewardMultiplier]" dataDxfId="47"/>
+    <tableColumn id="1" name="{missionDragonModifiersDefinitions}" dataDxfId="51"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="50"/>
+    <tableColumn id="7" name="[quantityModifier]" dataDxfId="49"/>
+    <tableColumn id="3" name="[missionSCRewardMultiplier]" dataDxfId="48"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table1330313234" displayName="Table1330313234" ref="B95:E98" totalsRowShown="0" headerRowDxfId="46" dataDxfId="44" headerRowBorderDxfId="45" tableBorderDxfId="43" totalsRowBorderDxfId="42">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table1330313234" displayName="Table1330313234" ref="B95:E98" totalsRowShown="0" headerRowDxfId="47" dataDxfId="45" headerRowBorderDxfId="46" tableBorderDxfId="44" totalsRowBorderDxfId="43">
   <autoFilter ref="B95:E98"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="{missionDifficultyModifiersDefinitions}" dataDxfId="41"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="40"/>
-    <tableColumn id="3" name="[difficulty]" dataDxfId="39"/>
-    <tableColumn id="7" name="[quantityModifier]" dataDxfId="38"/>
+    <tableColumn id="1" name="{missionDifficultyModifiersDefinitions}" dataDxfId="42"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="41"/>
+    <tableColumn id="3" name="[difficulty]" dataDxfId="40"/>
+    <tableColumn id="7" name="[quantityModifier]" dataDxfId="39"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table133031323435" displayName="Table133031323435" ref="B102:D103" totalsRowShown="0" headerRowDxfId="37" dataDxfId="35" headerRowBorderDxfId="36" tableBorderDxfId="34" totalsRowBorderDxfId="33">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table133031323435" displayName="Table133031323435" ref="B102:D103" totalsRowShown="0" headerRowDxfId="38" dataDxfId="36" headerRowBorderDxfId="37" tableBorderDxfId="35" totalsRowBorderDxfId="34">
   <autoFilter ref="B102:D103"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="{missionOtherModifiersDefinitions}" dataDxfId="32"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="31"/>
-    <tableColumn id="7" name="[quantityModifier]" dataDxfId="30"/>
+    <tableColumn id="1" name="{missionOtherModifiersDefinitions}" dataDxfId="33"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="32"/>
+    <tableColumn id="7" name="[quantityModifier]" dataDxfId="31"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table13" displayName="Table13" ref="B48:H67" totalsRowShown="0" headerRowDxfId="29" dataDxfId="27" headerRowBorderDxfId="28" tableBorderDxfId="26" totalsRowBorderDxfId="25">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table13" displayName="Table13" ref="B48:H67" totalsRowShown="0" headerRowDxfId="30" dataDxfId="28" headerRowBorderDxfId="29" tableBorderDxfId="27" totalsRowBorderDxfId="26">
   <autoFilter ref="B48:H67"/>
   <tableColumns count="7">
-    <tableColumn id="1" name="{missionTypeDefinitions}" dataDxfId="24"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="23"/>
-    <tableColumn id="3" name="[minTier]" dataDxfId="22"/>
-    <tableColumn id="6" name="[maxTier]" dataDxfId="21"/>
-    <tableColumn id="4" name="[weight]" dataDxfId="20"/>
-    <tableColumn id="9" name="[tidDescSingleRun]" dataDxfId="19"/>
-    <tableColumn id="10" name="[tidDescMultiRun]" dataDxfId="18"/>
+    <tableColumn id="1" name="{missionTypeDefinitions}" dataDxfId="25"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="24"/>
+    <tableColumn id="3" name="[minTier]" dataDxfId="23"/>
+    <tableColumn id="6" name="[maxTier]" dataDxfId="22"/>
+    <tableColumn id="4" name="[weight]" dataDxfId="21"/>
+    <tableColumn id="9" name="[tidDescSingleRun]" dataDxfId="20"/>
+    <tableColumn id="10" name="[tidDescMultiRun]" dataDxfId="19"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table1330" displayName="Table1330" ref="B4:N43" totalsRowShown="0" headerRowDxfId="17" dataDxfId="15" headerRowBorderDxfId="16" tableBorderDxfId="14" totalsRowBorderDxfId="13">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table1330" displayName="Table1330" ref="B4:N43" totalsRowShown="0" headerRowDxfId="18" dataDxfId="16" headerRowBorderDxfId="17" tableBorderDxfId="15" totalsRowBorderDxfId="14">
   <autoFilter ref="B4:N43"/>
   <sortState ref="B5:P43">
     <sortCondition descending="1" ref="J4:J43"/>
   </sortState>
   <tableColumns count="13">
-    <tableColumn id="1" name="{missionsDefinitions}" dataDxfId="12"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="11"/>
-    <tableColumn id="7" name="[type]" dataDxfId="10"/>
-    <tableColumn id="8" name="[weight]" dataDxfId="9"/>
-    <tableColumn id="13" name="[singleRunChance]" dataDxfId="8"/>
-    <tableColumn id="11" name="[minTier]" dataDxfId="7"/>
-    <tableColumn id="12" name="[maxTier]" dataDxfId="6"/>
-    <tableColumn id="6" name="[params]" dataDxfId="5"/>
-    <tableColumn id="3" name="[objectiveBaseQuantityMin]" dataDxfId="4"/>
-    <tableColumn id="9" name="[objectiveBaseQuantityMax]" dataDxfId="3"/>
-    <tableColumn id="4" name="[icon]" dataDxfId="2"/>
-    <tableColumn id="5" name="[tidObjective]" dataDxfId="1"/>
-    <tableColumn id="10" name="[trackingSku]" dataDxfId="0">
+    <tableColumn id="1" name="{missionsDefinitions}" dataDxfId="13"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="12"/>
+    <tableColumn id="7" name="[type]" dataDxfId="11"/>
+    <tableColumn id="8" name="[weight]" dataDxfId="10"/>
+    <tableColumn id="13" name="[singleRunChance]" dataDxfId="9"/>
+    <tableColumn id="11" name="[minTier]" dataDxfId="8"/>
+    <tableColumn id="12" name="[maxTier]" dataDxfId="7"/>
+    <tableColumn id="6" name="[params]" dataDxfId="6"/>
+    <tableColumn id="3" name="[objectiveBaseQuantityMin]" dataDxfId="5"/>
+    <tableColumn id="9" name="[objectiveBaseQuantityMax]" dataDxfId="4"/>
+    <tableColumn id="4" name="[icon]" dataDxfId="3"/>
+    <tableColumn id="5" name="[tidObjective]" dataDxfId="2"/>
+    <tableColumn id="10" name="[trackingSku]" dataDxfId="1">
       <calculatedColumnFormula>Table1330[[#This Row],['[sku']]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2779,18 +2994,19 @@
   <sheetPr>
     <tabColor theme="6"/>
   </sheetPr>
-  <dimension ref="B1:P103"/>
+  <dimension ref="B1:P156"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O9" sqref="O9"/>
+    <sheetView tabSelected="1" topLeftCell="A121" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G109" sqref="G109"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="7" customWidth="1"/>
     <col min="2" max="2" width="18.7109375" customWidth="1"/>
-    <col min="3" max="3" width="24.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="6" width="18.7109375" customWidth="1"/>
+    <col min="3" max="3" width="30.140625" customWidth="1"/>
+    <col min="4" max="4" width="34.140625" customWidth="1"/>
+    <col min="5" max="6" width="18.7109375" customWidth="1"/>
     <col min="7" max="7" width="55.85546875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="54.42578125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="59.85546875" bestFit="1" customWidth="1"/>
@@ -4367,7 +4583,7 @@
         <v>182</v>
       </c>
       <c r="E41" s="52">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F41" s="52">
         <v>1</v>
@@ -5457,6 +5673,717 @@
         <v>0.7</v>
       </c>
     </row>
+    <row r="104" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="105" spans="2:7" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B105" s="6" t="s">
+        <v>242</v>
+      </c>
+      <c r="C105" s="6"/>
+      <c r="D105" s="6"/>
+      <c r="E105" s="6"/>
+      <c r="F105" s="6"/>
+      <c r="G105" s="6"/>
+    </row>
+    <row r="107" spans="2:7" ht="68.25" x14ac:dyDescent="0.25">
+      <c r="B107" s="63" t="s">
+        <v>243</v>
+      </c>
+      <c r="C107" s="63" t="s">
+        <v>3</v>
+      </c>
+      <c r="D107" s="64" t="s">
+        <v>244</v>
+      </c>
+      <c r="E107" s="64" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="108" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B108" s="62" t="s">
+        <v>1</v>
+      </c>
+      <c r="C108" s="65" t="s">
+        <v>80</v>
+      </c>
+      <c r="D108" s="65" t="s">
+        <v>267</v>
+      </c>
+      <c r="E108" s="62" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="109" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B109" s="62" t="s">
+        <v>1</v>
+      </c>
+      <c r="C109" s="65" t="s">
+        <v>93</v>
+      </c>
+      <c r="D109" s="65" t="s">
+        <v>268</v>
+      </c>
+      <c r="E109" s="62" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="110" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B110" s="62" t="s">
+        <v>1</v>
+      </c>
+      <c r="C110" s="65" t="s">
+        <v>127</v>
+      </c>
+      <c r="D110" s="65" t="s">
+        <v>269</v>
+      </c>
+      <c r="E110" s="62" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="111" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B111" s="62" t="s">
+        <v>1</v>
+      </c>
+      <c r="C111" s="65" t="s">
+        <v>109</v>
+      </c>
+      <c r="D111" s="65" t="s">
+        <v>109</v>
+      </c>
+      <c r="E111" s="62" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="112" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B112" s="62" t="s">
+        <v>1</v>
+      </c>
+      <c r="C112" s="65" t="s">
+        <v>123</v>
+      </c>
+      <c r="D112" s="65" t="s">
+        <v>123</v>
+      </c>
+      <c r="E112" s="62" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="113" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B113" s="62" t="s">
+        <v>1</v>
+      </c>
+      <c r="C113" s="65" t="s">
+        <v>110</v>
+      </c>
+      <c r="D113" s="65" t="s">
+        <v>110</v>
+      </c>
+      <c r="E113" s="62" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="114" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B114" s="62" t="s">
+        <v>1</v>
+      </c>
+      <c r="C114" s="65" t="s">
+        <v>113</v>
+      </c>
+      <c r="D114" s="65" t="s">
+        <v>270</v>
+      </c>
+      <c r="E114" s="62" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="115" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B115" s="62" t="s">
+        <v>1</v>
+      </c>
+      <c r="C115" s="65" t="s">
+        <v>246</v>
+      </c>
+      <c r="D115" s="65" t="s">
+        <v>271</v>
+      </c>
+      <c r="E115" s="62" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="116" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B116" s="62" t="s">
+        <v>1</v>
+      </c>
+      <c r="C116" s="65" t="s">
+        <v>247</v>
+      </c>
+      <c r="D116" s="65" t="s">
+        <v>272</v>
+      </c>
+      <c r="E116" s="62" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="117" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B117" s="62" t="s">
+        <v>1</v>
+      </c>
+      <c r="C117" s="65" t="s">
+        <v>207</v>
+      </c>
+      <c r="D117" s="65" t="s">
+        <v>273</v>
+      </c>
+      <c r="E117" s="62" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="118" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B118" s="62" t="s">
+        <v>1</v>
+      </c>
+      <c r="C118" s="65" t="s">
+        <v>206</v>
+      </c>
+      <c r="D118" s="65" t="s">
+        <v>274</v>
+      </c>
+      <c r="E118" s="62" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="119" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B119" s="62" t="s">
+        <v>1</v>
+      </c>
+      <c r="C119" s="65" t="s">
+        <v>201</v>
+      </c>
+      <c r="D119" s="65" t="s">
+        <v>275</v>
+      </c>
+      <c r="E119" s="62" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="120" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B120" s="62" t="s">
+        <v>1</v>
+      </c>
+      <c r="C120" s="65" t="s">
+        <v>205</v>
+      </c>
+      <c r="D120" s="65" t="s">
+        <v>276</v>
+      </c>
+      <c r="E120" s="62" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="121" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B121" s="62" t="s">
+        <v>1</v>
+      </c>
+      <c r="C121" s="65" t="s">
+        <v>204</v>
+      </c>
+      <c r="D121" s="65" t="s">
+        <v>277</v>
+      </c>
+      <c r="E121" s="62" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="122" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B122" s="62" t="s">
+        <v>1</v>
+      </c>
+      <c r="C122" s="65" t="s">
+        <v>202</v>
+      </c>
+      <c r="D122" s="65" t="s">
+        <v>278</v>
+      </c>
+      <c r="E122" s="62" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="123" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B123" s="62" t="s">
+        <v>1</v>
+      </c>
+      <c r="C123" s="65" t="s">
+        <v>203</v>
+      </c>
+      <c r="D123" s="65" t="s">
+        <v>279</v>
+      </c>
+      <c r="E123" s="62" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="124" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B124" s="62" t="s">
+        <v>1</v>
+      </c>
+      <c r="C124" s="65" t="s">
+        <v>116</v>
+      </c>
+      <c r="D124" s="65" t="s">
+        <v>280</v>
+      </c>
+      <c r="E124" s="62" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="125" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B125" s="62" t="s">
+        <v>1</v>
+      </c>
+      <c r="C125" s="65" t="s">
+        <v>248</v>
+      </c>
+      <c r="D125" s="65" t="s">
+        <v>248</v>
+      </c>
+      <c r="E125" s="62" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="126" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B126" s="62" t="s">
+        <v>1</v>
+      </c>
+      <c r="C126" s="65" t="s">
+        <v>83</v>
+      </c>
+      <c r="D126" s="65" t="s">
+        <v>281</v>
+      </c>
+      <c r="E126" s="62" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="127" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B127" s="62" t="s">
+        <v>1</v>
+      </c>
+      <c r="C127" s="65" t="s">
+        <v>96</v>
+      </c>
+      <c r="D127" s="65" t="s">
+        <v>282</v>
+      </c>
+      <c r="E127" s="62" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="128" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B128" s="62" t="s">
+        <v>1</v>
+      </c>
+      <c r="C128" s="65" t="s">
+        <v>249</v>
+      </c>
+      <c r="D128" s="65" t="s">
+        <v>283</v>
+      </c>
+      <c r="E128" s="62" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="129" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B129" s="62" t="s">
+        <v>1</v>
+      </c>
+      <c r="C129" s="65" t="s">
+        <v>250</v>
+      </c>
+      <c r="D129" s="65" t="s">
+        <v>284</v>
+      </c>
+      <c r="E129" s="62" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="130" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B130" s="62" t="s">
+        <v>1</v>
+      </c>
+      <c r="C130" s="65" t="s">
+        <v>102</v>
+      </c>
+      <c r="D130" s="65" t="s">
+        <v>285</v>
+      </c>
+      <c r="E130" s="62" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="131" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B131" s="62" t="s">
+        <v>1</v>
+      </c>
+      <c r="C131" s="65" t="s">
+        <v>251</v>
+      </c>
+      <c r="D131" s="65" t="s">
+        <v>251</v>
+      </c>
+      <c r="E131" s="62" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="132" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B132" s="62" t="s">
+        <v>1</v>
+      </c>
+      <c r="C132" s="65" t="s">
+        <v>125</v>
+      </c>
+      <c r="D132" s="65" t="s">
+        <v>286</v>
+      </c>
+      <c r="E132" s="62" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="133" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B133" s="62" t="s">
+        <v>1</v>
+      </c>
+      <c r="C133" s="65" t="s">
+        <v>88</v>
+      </c>
+      <c r="D133" s="65" t="s">
+        <v>287</v>
+      </c>
+      <c r="E133" s="62" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="134" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B134" s="62" t="s">
+        <v>1</v>
+      </c>
+      <c r="C134" s="65" t="s">
+        <v>252</v>
+      </c>
+      <c r="D134" s="65" t="s">
+        <v>288</v>
+      </c>
+      <c r="E134" s="62" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="135" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B135" s="62" t="s">
+        <v>1</v>
+      </c>
+      <c r="C135" s="65" t="s">
+        <v>253</v>
+      </c>
+      <c r="D135" s="65" t="s">
+        <v>289</v>
+      </c>
+      <c r="E135" s="62" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="136" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B136" s="62" t="s">
+        <v>1</v>
+      </c>
+      <c r="C136" s="65" t="s">
+        <v>254</v>
+      </c>
+      <c r="D136" s="65" t="s">
+        <v>254</v>
+      </c>
+      <c r="E136" s="62" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="137" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B137" s="62" t="s">
+        <v>1</v>
+      </c>
+      <c r="C137" s="65" t="s">
+        <v>118</v>
+      </c>
+      <c r="D137" s="65" t="s">
+        <v>118</v>
+      </c>
+      <c r="E137" s="62" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="138" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B138" s="62" t="s">
+        <v>1</v>
+      </c>
+      <c r="C138" s="65" t="s">
+        <v>255</v>
+      </c>
+      <c r="D138" s="65" t="s">
+        <v>290</v>
+      </c>
+      <c r="E138" s="62" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="139" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B139" s="62" t="s">
+        <v>1</v>
+      </c>
+      <c r="C139" s="65" t="s">
+        <v>91</v>
+      </c>
+      <c r="D139" s="65" t="s">
+        <v>291</v>
+      </c>
+      <c r="E139" s="62" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="140" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B140" s="62" t="s">
+        <v>1</v>
+      </c>
+      <c r="C140" s="65" t="s">
+        <v>256</v>
+      </c>
+      <c r="D140" s="65" t="s">
+        <v>292</v>
+      </c>
+      <c r="E140" s="62" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="141" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B141" s="62" t="s">
+        <v>1</v>
+      </c>
+      <c r="C141" s="65" t="s">
+        <v>257</v>
+      </c>
+      <c r="D141" s="65" t="s">
+        <v>293</v>
+      </c>
+      <c r="E141" s="62" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="142" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B142" s="62" t="s">
+        <v>1</v>
+      </c>
+      <c r="C142" s="65" t="s">
+        <v>258</v>
+      </c>
+      <c r="D142" s="65" t="s">
+        <v>294</v>
+      </c>
+      <c r="E142" s="62" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="143" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B143" s="62" t="s">
+        <v>1</v>
+      </c>
+      <c r="C143" s="65" t="s">
+        <v>86</v>
+      </c>
+      <c r="D143" s="65" t="s">
+        <v>295</v>
+      </c>
+      <c r="E143" s="62" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="144" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B144" s="62" t="s">
+        <v>1</v>
+      </c>
+      <c r="C144" s="65" t="s">
+        <v>73</v>
+      </c>
+      <c r="D144" s="65" t="s">
+        <v>73</v>
+      </c>
+      <c r="E144" s="62" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="145" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B145" s="62" t="s">
+        <v>1</v>
+      </c>
+      <c r="C145" s="65" t="s">
+        <v>108</v>
+      </c>
+      <c r="D145" s="65" t="s">
+        <v>108</v>
+      </c>
+      <c r="E145" s="62" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="146" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B146" s="62" t="s">
+        <v>1</v>
+      </c>
+      <c r="C146" s="65" t="s">
+        <v>259</v>
+      </c>
+      <c r="D146" s="65" t="s">
+        <v>296</v>
+      </c>
+      <c r="E146" s="62" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="147" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B147" s="62" t="s">
+        <v>1</v>
+      </c>
+      <c r="C147" s="65" t="s">
+        <v>260</v>
+      </c>
+      <c r="D147" s="65" t="s">
+        <v>297</v>
+      </c>
+      <c r="E147" s="62" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="148" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B148" s="62" t="s">
+        <v>1</v>
+      </c>
+      <c r="C148" s="65" t="s">
+        <v>77</v>
+      </c>
+      <c r="D148" s="65" t="s">
+        <v>298</v>
+      </c>
+      <c r="E148" s="62" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="149" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B149" s="62" t="s">
+        <v>1</v>
+      </c>
+      <c r="C149" s="65" t="s">
+        <v>105</v>
+      </c>
+      <c r="D149" s="65" t="s">
+        <v>299</v>
+      </c>
+      <c r="E149" s="62" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="150" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B150" s="62" t="s">
+        <v>1</v>
+      </c>
+      <c r="C150" s="65" t="s">
+        <v>261</v>
+      </c>
+      <c r="D150" s="65" t="s">
+        <v>300</v>
+      </c>
+      <c r="E150" s="62" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="151" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B151" s="62" t="s">
+        <v>1</v>
+      </c>
+      <c r="C151" s="65" t="s">
+        <v>262</v>
+      </c>
+      <c r="D151" s="65" t="s">
+        <v>301</v>
+      </c>
+      <c r="E151" s="62" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="152" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B152" s="62" t="s">
+        <v>1</v>
+      </c>
+      <c r="C152" s="65" t="s">
+        <v>263</v>
+      </c>
+      <c r="D152" s="65" t="s">
+        <v>302</v>
+      </c>
+      <c r="E152" s="62" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="153" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B153" s="62" t="s">
+        <v>1</v>
+      </c>
+      <c r="C153" s="65" t="s">
+        <v>264</v>
+      </c>
+      <c r="D153" s="65" t="s">
+        <v>264</v>
+      </c>
+      <c r="E153" s="62" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="154" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B154" s="62" t="s">
+        <v>1</v>
+      </c>
+      <c r="C154" s="65" t="s">
+        <v>99</v>
+      </c>
+      <c r="D154" s="65" t="s">
+        <v>303</v>
+      </c>
+      <c r="E154" s="62" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="155" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B155" s="62" t="s">
+        <v>1</v>
+      </c>
+      <c r="C155" s="65" t="s">
+        <v>265</v>
+      </c>
+      <c r="D155" s="65" t="s">
+        <v>304</v>
+      </c>
+      <c r="E155" s="62" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="156" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B156" s="62" t="s">
+        <v>1</v>
+      </c>
+      <c r="C156" s="65" t="s">
+        <v>266</v>
+      </c>
+      <c r="D156" s="65" t="s">
+        <v>305</v>
+      </c>
+      <c r="E156" s="62" t="b">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="J3:K3"/>
@@ -5465,7 +6392,7 @@
     <mergeCell ref="G70:H70"/>
   </mergeCells>
   <conditionalFormatting sqref="C72:E74">
-    <cfRule type="duplicateValues" dxfId="68" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="2"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Introduce BaseIcon component to deal with 2d/3d icons Fix bug in catalog generated json.
Former-commit-id: 180300653dea2ab60b8d291fed1eab2d035a744c
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Missions.xlsx
+++ b/Docs/Content/HungryDragonContent_Missions.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="434" uniqueCount="244">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="433" uniqueCount="244">
   <si>
     <t>single_run</t>
   </si>
@@ -780,7 +780,7 @@
     <t>TID_MISSION_OBJECTIVE_KILL_EQUIPABLE_DESC_MULTI_RUN</t>
   </si>
   <si>
-    <t>[is3dIcon]</t>
+    <t>icon_pet_bruce</t>
   </si>
 </sst>
 </file>
@@ -1267,6 +1267,11 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment textRotation="45"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1274,48 +1279,11 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment textRotation="45"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="70">
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="8"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top/>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
+  <dxfs count="69">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -2459,100 +2427,99 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="missionDifficultyDefinitions" displayName="missionDifficultyDefinitions" ref="B71:L74" totalsRowShown="0" headerRowBorderDxfId="69" tableBorderDxfId="68">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="missionDifficultyDefinitions" displayName="missionDifficultyDefinitions" ref="B71:L74" totalsRowShown="0" headerRowBorderDxfId="68" tableBorderDxfId="67">
   <autoFilter ref="B71:L74"/>
   <tableColumns count="11">
     <tableColumn id="1" name="{missionDifficultyDefinitions}"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="67"/>
-    <tableColumn id="11" name="[difficulty]" dataDxfId="66"/>
-    <tableColumn id="7" name="[index]" dataDxfId="65"/>
-    <tableColumn id="3" name="[dragonsToUnlock]" dataDxfId="64"/>
-    <tableColumn id="4" name="[cooldownMinutes]" dataDxfId="63"/>
-    <tableColumn id="9" name="[maxRewardCoins]" dataDxfId="62"/>
-    <tableColumn id="5" name="[removeMissionPCCoefA]" dataDxfId="61"/>
-    <tableColumn id="6" name="[removeMissionPCCoefB]" dataDxfId="60"/>
-    <tableColumn id="8" name="[tidName]" dataDxfId="59"/>
-    <tableColumn id="10" name="[color]" dataDxfId="58"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="66"/>
+    <tableColumn id="11" name="[difficulty]" dataDxfId="65"/>
+    <tableColumn id="7" name="[index]" dataDxfId="64"/>
+    <tableColumn id="3" name="[dragonsToUnlock]" dataDxfId="63"/>
+    <tableColumn id="4" name="[cooldownMinutes]" dataDxfId="62"/>
+    <tableColumn id="9" name="[maxRewardCoins]" dataDxfId="61"/>
+    <tableColumn id="5" name="[removeMissionPCCoefA]" dataDxfId="60"/>
+    <tableColumn id="6" name="[removeMissionPCCoefB]" dataDxfId="59"/>
+    <tableColumn id="8" name="[tidName]" dataDxfId="58"/>
+    <tableColumn id="10" name="[color]" dataDxfId="57"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table13303132" displayName="Table13303132" ref="B79:E91" totalsRowShown="0" headerRowDxfId="57" dataDxfId="55" headerRowBorderDxfId="56" tableBorderDxfId="54" totalsRowBorderDxfId="53">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table13303132" displayName="Table13303132" ref="B79:E91" totalsRowShown="0" headerRowDxfId="56" dataDxfId="54" headerRowBorderDxfId="55" tableBorderDxfId="53" totalsRowBorderDxfId="52">
   <autoFilter ref="B79:E91"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="{missionDragonModifiersDefinitions}" dataDxfId="52"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="51"/>
-    <tableColumn id="7" name="[quantityModifier]" dataDxfId="50"/>
-    <tableColumn id="3" name="[missionSCRewardMultiplier]" dataDxfId="49"/>
+    <tableColumn id="1" name="{missionDragonModifiersDefinitions}" dataDxfId="51"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="50"/>
+    <tableColumn id="7" name="[quantityModifier]" dataDxfId="49"/>
+    <tableColumn id="3" name="[missionSCRewardMultiplier]" dataDxfId="48"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table1330313234" displayName="Table1330313234" ref="B95:E98" totalsRowShown="0" headerRowDxfId="48" dataDxfId="46" headerRowBorderDxfId="47" tableBorderDxfId="45" totalsRowBorderDxfId="44">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table1330313234" displayName="Table1330313234" ref="B95:E98" totalsRowShown="0" headerRowDxfId="47" dataDxfId="45" headerRowBorderDxfId="46" tableBorderDxfId="44" totalsRowBorderDxfId="43">
   <autoFilter ref="B95:E98"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="{missionDifficultyModifiersDefinitions}" dataDxfId="43"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="42"/>
-    <tableColumn id="3" name="[difficulty]" dataDxfId="41"/>
-    <tableColumn id="7" name="[quantityModifier]" dataDxfId="40"/>
+    <tableColumn id="1" name="{missionDifficultyModifiersDefinitions}" dataDxfId="42"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="41"/>
+    <tableColumn id="3" name="[difficulty]" dataDxfId="40"/>
+    <tableColumn id="7" name="[quantityModifier]" dataDxfId="39"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table133031323435" displayName="Table133031323435" ref="B102:D103" totalsRowShown="0" headerRowDxfId="39" dataDxfId="37" headerRowBorderDxfId="38" tableBorderDxfId="36" totalsRowBorderDxfId="35">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table133031323435" displayName="Table133031323435" ref="B102:D103" totalsRowShown="0" headerRowDxfId="38" dataDxfId="36" headerRowBorderDxfId="37" tableBorderDxfId="35" totalsRowBorderDxfId="34">
   <autoFilter ref="B102:D103"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="{missionOtherModifiersDefinitions}" dataDxfId="34"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="33"/>
-    <tableColumn id="7" name="[quantityModifier]" dataDxfId="32"/>
+    <tableColumn id="1" name="{missionOtherModifiersDefinitions}" dataDxfId="33"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="32"/>
+    <tableColumn id="7" name="[quantityModifier]" dataDxfId="31"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table13" displayName="Table13" ref="B48:H67" totalsRowShown="0" headerRowDxfId="31" dataDxfId="29" headerRowBorderDxfId="30" tableBorderDxfId="28" totalsRowBorderDxfId="27">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table13" displayName="Table13" ref="B48:H67" totalsRowShown="0" headerRowDxfId="30" dataDxfId="28" headerRowBorderDxfId="29" tableBorderDxfId="27" totalsRowBorderDxfId="26">
   <autoFilter ref="B48:H67"/>
   <tableColumns count="7">
-    <tableColumn id="1" name="{missionTypeDefinitions}" dataDxfId="26"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="25"/>
-    <tableColumn id="3" name="[minTier]" dataDxfId="24"/>
-    <tableColumn id="6" name="[maxTier]" dataDxfId="23"/>
-    <tableColumn id="4" name="[weight]" dataDxfId="22"/>
-    <tableColumn id="9" name="[tidDescSingleRun]" dataDxfId="21"/>
-    <tableColumn id="10" name="[tidDescMultiRun]" dataDxfId="20"/>
+    <tableColumn id="1" name="{missionTypeDefinitions}" dataDxfId="25"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="24"/>
+    <tableColumn id="3" name="[minTier]" dataDxfId="23"/>
+    <tableColumn id="6" name="[maxTier]" dataDxfId="22"/>
+    <tableColumn id="4" name="[weight]" dataDxfId="21"/>
+    <tableColumn id="9" name="[tidDescSingleRun]" dataDxfId="20"/>
+    <tableColumn id="10" name="[tidDescMultiRun]" dataDxfId="19"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table1330" displayName="Table1330" ref="B4:O43" totalsRowShown="0" headerRowDxfId="19" dataDxfId="17" headerRowBorderDxfId="18" tableBorderDxfId="16" totalsRowBorderDxfId="15">
-  <autoFilter ref="B4:O43"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table1330" displayName="Table1330" ref="B4:N43" totalsRowShown="0" headerRowDxfId="18" dataDxfId="16" headerRowBorderDxfId="17" tableBorderDxfId="15" totalsRowBorderDxfId="14">
+  <autoFilter ref="B4:N43"/>
   <sortState ref="B5:P43">
     <sortCondition descending="1" ref="J4:J43"/>
   </sortState>
-  <tableColumns count="14">
-    <tableColumn id="1" name="{missionsDefinitions}" dataDxfId="14"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="13"/>
-    <tableColumn id="7" name="[type]" dataDxfId="12"/>
-    <tableColumn id="8" name="[weight]" dataDxfId="11"/>
-    <tableColumn id="13" name="[singleRunChance]" dataDxfId="10"/>
-    <tableColumn id="11" name="[minTier]" dataDxfId="9"/>
-    <tableColumn id="12" name="[maxTier]" dataDxfId="8"/>
-    <tableColumn id="6" name="[params]" dataDxfId="7"/>
-    <tableColumn id="3" name="[objectiveBaseQuantityMin]" dataDxfId="6"/>
-    <tableColumn id="9" name="[objectiveBaseQuantityMax]" dataDxfId="5"/>
-    <tableColumn id="4" name="[icon]" dataDxfId="4"/>
-    <tableColumn id="14" name="[is3dIcon]" dataDxfId="0"/>
-    <tableColumn id="5" name="[tidObjective]" dataDxfId="3"/>
-    <tableColumn id="10" name="[trackingSku]" dataDxfId="2"/>
+  <tableColumns count="13">
+    <tableColumn id="1" name="{missionsDefinitions}" dataDxfId="13"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="12"/>
+    <tableColumn id="7" name="[type]" dataDxfId="11"/>
+    <tableColumn id="8" name="[weight]" dataDxfId="10"/>
+    <tableColumn id="13" name="[singleRunChance]" dataDxfId="9"/>
+    <tableColumn id="11" name="[minTier]" dataDxfId="8"/>
+    <tableColumn id="12" name="[maxTier]" dataDxfId="7"/>
+    <tableColumn id="6" name="[params]" dataDxfId="6"/>
+    <tableColumn id="3" name="[objectiveBaseQuantityMin]" dataDxfId="5"/>
+    <tableColumn id="9" name="[objectiveBaseQuantityMax]" dataDxfId="4"/>
+    <tableColumn id="4" name="[icon]" dataDxfId="3"/>
+    <tableColumn id="5" name="[tidObjective]" dataDxfId="2"/>
+    <tableColumn id="10" name="[trackingSku]" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2827,7 +2794,7 @@
   <dimension ref="B1:Q103"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="G1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M34" sqref="M34"/>
+      <selection activeCell="L5" sqref="L5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2862,7 +2829,7 @@
       <c r="J2" s="6"/>
       <c r="K2" s="6"/>
       <c r="L2" s="6"/>
-      <c r="M2" s="63"/>
+      <c r="M2" s="60"/>
     </row>
     <row r="3" spans="2:17" ht="45" x14ac:dyDescent="0.25">
       <c r="B3" s="20"/>
@@ -2875,14 +2842,14 @@
         <v>143</v>
       </c>
       <c r="G3" s="38"/>
-      <c r="J3" s="60" t="s">
+      <c r="J3" s="63" t="s">
         <v>142</v>
       </c>
-      <c r="K3" s="60"/>
-      <c r="N3" s="60"/>
-      <c r="O3" s="60"/>
-      <c r="P3" s="60"/>
-      <c r="Q3" s="60"/>
+      <c r="K3" s="63"/>
+      <c r="N3" s="63"/>
+      <c r="O3" s="63"/>
+      <c r="P3" s="63"/>
+      <c r="Q3" s="63"/>
     </row>
     <row r="4" spans="2:17" ht="107.25" x14ac:dyDescent="0.25">
       <c r="B4" s="30" t="s">
@@ -2919,12 +2886,9 @@
         <v>136</v>
       </c>
       <c r="M4" s="36" t="s">
-        <v>243</v>
-      </c>
-      <c r="N4" s="36" t="s">
         <v>135</v>
       </c>
-      <c r="O4" s="35" t="s">
+      <c r="N4" s="35" t="s">
         <v>134</v>
       </c>
     </row>
@@ -2960,15 +2924,12 @@
         <v>600</v>
       </c>
       <c r="L5" s="33" t="s">
-        <v>128</v>
-      </c>
-      <c r="M5" s="33" t="b">
-        <v>0</v>
-      </c>
-      <c r="N5" s="33" t="s">
+        <v>243</v>
+      </c>
+      <c r="M5" s="33" t="s">
         <v>150</v>
       </c>
-      <c r="O5" s="31" t="s">
+      <c r="N5" s="31" t="s">
         <v>73</v>
       </c>
     </row>
@@ -3004,11 +2965,8 @@
       <c r="L6" s="33" t="s">
         <v>110</v>
       </c>
-      <c r="M6" s="33" t="b">
-        <v>0</v>
-      </c>
-      <c r="N6" s="33"/>
-      <c r="O6" s="31" t="s">
+      <c r="M6" s="33"/>
+      <c r="N6" s="31" t="s">
         <v>73</v>
       </c>
     </row>
@@ -3044,11 +3002,8 @@
       <c r="L7" s="33" t="s">
         <v>109</v>
       </c>
-      <c r="M7" s="33" t="b">
-        <v>0</v>
-      </c>
-      <c r="N7" s="33"/>
-      <c r="O7" s="31" t="s">
+      <c r="M7" s="33"/>
+      <c r="N7" s="31" t="s">
         <v>73</v>
       </c>
     </row>
@@ -3086,13 +3041,10 @@
       <c r="L8" s="33" t="s">
         <v>128</v>
       </c>
-      <c r="M8" s="33" t="b">
-        <v>0</v>
-      </c>
-      <c r="N8" s="33" t="s">
+      <c r="M8" s="33" t="s">
         <v>150</v>
       </c>
-      <c r="O8" s="31" t="s">
+      <c r="N8" s="31" t="s">
         <v>73</v>
       </c>
     </row>
@@ -3130,13 +3082,10 @@
       <c r="L9" s="33" t="s">
         <v>126</v>
       </c>
-      <c r="M9" s="33" t="b">
-        <v>0</v>
-      </c>
-      <c r="N9" s="47" t="s">
+      <c r="M9" s="47" t="s">
         <v>152</v>
       </c>
-      <c r="O9" s="31" t="s">
+      <c r="N9" s="31" t="s">
         <v>73</v>
       </c>
     </row>
@@ -3174,13 +3123,10 @@
       <c r="L10" s="33" t="s">
         <v>121</v>
       </c>
-      <c r="M10" s="33" t="b">
-        <v>0</v>
-      </c>
-      <c r="N10" s="47" t="s">
+      <c r="M10" s="47" t="s">
         <v>153</v>
       </c>
-      <c r="O10" s="31" t="s">
+      <c r="N10" s="31" t="s">
         <v>73</v>
       </c>
     </row>
@@ -3218,13 +3164,10 @@
       <c r="L11" s="33" t="s">
         <v>119</v>
       </c>
-      <c r="M11" s="33" t="b">
-        <v>0</v>
-      </c>
-      <c r="N11" s="33" t="s">
+      <c r="M11" s="33" t="s">
         <v>155</v>
       </c>
-      <c r="O11" s="31" t="s">
+      <c r="N11" s="31" t="s">
         <v>73</v>
       </c>
     </row>
@@ -3262,13 +3205,10 @@
       <c r="L12" s="33" t="s">
         <v>114</v>
       </c>
-      <c r="M12" s="33" t="b">
-        <v>0</v>
-      </c>
-      <c r="N12" s="47" t="s">
+      <c r="M12" s="47" t="s">
         <v>157</v>
       </c>
-      <c r="O12" s="31" t="s">
+      <c r="N12" s="31" t="s">
         <v>73</v>
       </c>
     </row>
@@ -3304,11 +3244,8 @@
       <c r="L13" s="33" t="s">
         <v>112</v>
       </c>
-      <c r="M13" s="33" t="b">
-        <v>0</v>
-      </c>
-      <c r="N13" s="33"/>
-      <c r="O13" s="31" t="s">
+      <c r="M13" s="33"/>
+      <c r="N13" s="31" t="s">
         <v>73</v>
       </c>
     </row>
@@ -3344,11 +3281,8 @@
       <c r="L14" s="33" t="s">
         <v>111</v>
       </c>
-      <c r="M14" s="33" t="b">
-        <v>0</v>
-      </c>
-      <c r="N14" s="33"/>
-      <c r="O14" s="31" t="s">
+      <c r="M14" s="33"/>
+      <c r="N14" s="31" t="s">
         <v>73</v>
       </c>
     </row>
@@ -3384,11 +3318,8 @@
       <c r="L15" s="33" t="s">
         <v>110</v>
       </c>
-      <c r="M15" s="33" t="b">
-        <v>0</v>
-      </c>
-      <c r="N15" s="33"/>
-      <c r="O15" s="31" t="s">
+      <c r="M15" s="33"/>
+      <c r="N15" s="31" t="s">
         <v>73</v>
       </c>
     </row>
@@ -3424,15 +3355,12 @@
       <c r="L16" s="33" t="s">
         <v>109</v>
       </c>
-      <c r="M16" s="33" t="b">
-        <v>0</v>
-      </c>
-      <c r="N16" s="33"/>
-      <c r="O16" s="31" t="s">
+      <c r="M16" s="33"/>
+      <c r="N16" s="31" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="17" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B17" s="25" t="s">
         <v>1</v>
       </c>
@@ -3466,17 +3394,14 @@
       <c r="L17" s="33" t="s">
         <v>106</v>
       </c>
-      <c r="M17" s="33" t="b">
-        <v>0</v>
-      </c>
-      <c r="N17" s="47" t="s">
+      <c r="M17" s="47" t="s">
         <v>159</v>
       </c>
-      <c r="O17" s="31" t="s">
+      <c r="N17" s="31" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="18" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B18" s="25" t="s">
         <v>1</v>
       </c>
@@ -3510,17 +3435,14 @@
       <c r="L18" s="33" t="s">
         <v>103</v>
       </c>
-      <c r="M18" s="33" t="b">
-        <v>0</v>
-      </c>
-      <c r="N18" s="33" t="s">
+      <c r="M18" s="33" t="s">
         <v>158</v>
       </c>
-      <c r="O18" s="31" t="s">
+      <c r="N18" s="31" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="19" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B19" s="25" t="s">
         <v>1</v>
       </c>
@@ -3554,17 +3476,14 @@
       <c r="L19" s="34" t="s">
         <v>94</v>
       </c>
-      <c r="M19" s="33" t="b">
-        <v>0</v>
-      </c>
-      <c r="N19" s="47" t="s">
+      <c r="M19" s="47" t="s">
         <v>161</v>
       </c>
-      <c r="O19" s="31" t="s">
+      <c r="N19" s="31" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="20" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B20" s="25" t="s">
         <v>1</v>
       </c>
@@ -3598,17 +3517,14 @@
       <c r="L20" s="34" t="s">
         <v>92</v>
       </c>
-      <c r="M20" s="33" t="b">
-        <v>0</v>
-      </c>
-      <c r="N20" s="55" t="s">
+      <c r="M20" s="55" t="s">
         <v>162</v>
       </c>
-      <c r="O20" s="31" t="s">
+      <c r="N20" s="31" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="21" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B21" s="25" t="s">
         <v>1</v>
       </c>
@@ -3642,17 +3558,14 @@
       <c r="L21" s="34" t="s">
         <v>89</v>
       </c>
-      <c r="M21" s="33" t="b">
-        <v>0</v>
-      </c>
-      <c r="N21" s="34" t="s">
+      <c r="M21" s="34" t="s">
         <v>163</v>
       </c>
-      <c r="O21" s="31" t="s">
+      <c r="N21" s="31" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="22" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B22" s="27" t="s">
         <v>1</v>
       </c>
@@ -3686,17 +3599,14 @@
       <c r="L22" s="34" t="s">
         <v>87</v>
       </c>
-      <c r="M22" s="33" t="b">
-        <v>0</v>
-      </c>
-      <c r="N22" s="34" t="s">
+      <c r="M22" s="34" t="s">
         <v>164</v>
       </c>
-      <c r="O22" s="31" t="s">
+      <c r="N22" s="31" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="23" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B23" s="27" t="s">
         <v>1</v>
       </c>
@@ -3730,17 +3640,14 @@
       <c r="L23" s="34" t="s">
         <v>84</v>
       </c>
-      <c r="M23" s="33" t="b">
-        <v>0</v>
-      </c>
-      <c r="N23" s="34" t="s">
+      <c r="M23" s="34" t="s">
         <v>219</v>
       </c>
-      <c r="O23" s="31" t="s">
+      <c r="N23" s="31" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="24" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B24" s="27" t="s">
         <v>1</v>
       </c>
@@ -3774,17 +3681,14 @@
       <c r="L24" s="34" t="s">
         <v>81</v>
       </c>
-      <c r="M24" s="33" t="b">
-        <v>0</v>
-      </c>
-      <c r="N24" s="34" t="s">
+      <c r="M24" s="34" t="s">
         <v>165</v>
       </c>
-      <c r="O24" s="31" t="s">
+      <c r="N24" s="31" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="25" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B25" s="27" t="s">
         <v>1</v>
       </c>
@@ -3818,17 +3722,14 @@
       <c r="L25" s="34" t="s">
         <v>78</v>
       </c>
-      <c r="M25" s="33" t="b">
-        <v>0</v>
-      </c>
-      <c r="N25" s="34" t="s">
+      <c r="M25" s="34" t="s">
         <v>166</v>
       </c>
-      <c r="O25" s="31" t="s">
+      <c r="N25" s="31" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="26" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B26" s="27" t="s">
         <v>1</v>
       </c>
@@ -3862,17 +3763,14 @@
       <c r="L26" s="34" t="s">
         <v>75</v>
       </c>
-      <c r="M26" s="33" t="b">
-        <v>0</v>
-      </c>
-      <c r="N26" s="34" t="s">
+      <c r="M26" s="34" t="s">
         <v>167</v>
       </c>
-      <c r="O26" s="31" t="s">
+      <c r="N26" s="31" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="27" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B27" s="27" t="s">
         <v>1</v>
       </c>
@@ -3904,15 +3802,12 @@
       <c r="L27" s="34" t="s">
         <v>74</v>
       </c>
-      <c r="M27" s="33" t="b">
-        <v>0</v>
-      </c>
-      <c r="N27" s="34"/>
-      <c r="O27" s="31" t="s">
+      <c r="M27" s="34"/>
+      <c r="N27" s="31" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="28" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B28" s="50" t="s">
         <v>1</v>
       </c>
@@ -3946,17 +3841,14 @@
       <c r="L28" s="54" t="s">
         <v>201</v>
       </c>
-      <c r="M28" s="33" t="b">
-        <v>0</v>
-      </c>
-      <c r="N28" s="54" t="s">
+      <c r="M28" s="54" t="s">
         <v>159</v>
       </c>
-      <c r="O28" s="53" t="s">
+      <c r="N28" s="53" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="29" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B29" s="50" t="s">
         <v>1</v>
       </c>
@@ -3988,17 +3880,14 @@
       <c r="L29" s="54" t="s">
         <v>202</v>
       </c>
-      <c r="M29" s="33" t="b">
-        <v>0</v>
-      </c>
-      <c r="N29" s="54" t="s">
+      <c r="M29" s="54" t="s">
         <v>216</v>
       </c>
-      <c r="O29" s="53" t="s">
+      <c r="N29" s="53" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="30" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B30" s="50" t="s">
         <v>1</v>
       </c>
@@ -4032,17 +3921,14 @@
       <c r="L30" s="54" t="s">
         <v>203</v>
       </c>
-      <c r="M30" s="33" t="b">
-        <v>0</v>
-      </c>
-      <c r="N30" s="54" t="s">
+      <c r="M30" s="54" t="s">
         <v>168</v>
       </c>
-      <c r="O30" s="53" t="s">
+      <c r="N30" s="53" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="31" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B31" s="50" t="s">
         <v>1</v>
       </c>
@@ -4076,17 +3962,14 @@
       <c r="L31" s="48" t="s">
         <v>207</v>
       </c>
-      <c r="M31" s="33" t="b">
-        <v>0</v>
-      </c>
-      <c r="N31" s="48" t="s">
+      <c r="M31" s="48" t="s">
         <v>215</v>
       </c>
-      <c r="O31" s="53" t="s">
+      <c r="N31" s="53" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="32" spans="2:15" s="43" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:14" s="43" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B32" s="50" t="s">
         <v>1</v>
       </c>
@@ -4120,13 +4003,10 @@
       <c r="L32" s="48" t="s">
         <v>206</v>
       </c>
-      <c r="M32" s="33" t="b">
-        <v>0</v>
-      </c>
-      <c r="N32" s="48" t="s">
+      <c r="M32" s="48" t="s">
         <v>158</v>
       </c>
-      <c r="O32" s="53" t="s">
+      <c r="N32" s="53" t="s">
         <v>73</v>
       </c>
     </row>
@@ -4162,11 +4042,8 @@
       <c r="L33" s="48" t="s">
         <v>212</v>
       </c>
-      <c r="M33" s="33" t="b">
-        <v>0</v>
-      </c>
-      <c r="N33" s="48"/>
-      <c r="O33" s="53" t="s">
+      <c r="M33" s="48"/>
+      <c r="N33" s="53" t="s">
         <v>73</v>
       </c>
     </row>
@@ -4204,13 +4081,10 @@
       <c r="L34" s="33" t="s">
         <v>124</v>
       </c>
-      <c r="M34" s="33" t="b">
-        <v>0</v>
-      </c>
-      <c r="N34" s="47" t="s">
+      <c r="M34" s="47" t="s">
         <v>153</v>
       </c>
-      <c r="O34" s="31" t="s">
+      <c r="N34" s="31" t="s">
         <v>73</v>
       </c>
     </row>
@@ -4248,13 +4122,10 @@
       <c r="L35" s="48" t="s">
         <v>204</v>
       </c>
-      <c r="M35" s="33" t="b">
-        <v>0</v>
-      </c>
-      <c r="N35" s="49" t="s">
+      <c r="M35" s="49" t="s">
         <v>217</v>
       </c>
-      <c r="O35" s="53" t="s">
+      <c r="N35" s="53" t="s">
         <v>73</v>
       </c>
     </row>
@@ -4292,13 +4163,10 @@
       <c r="L36" s="48" t="s">
         <v>208</v>
       </c>
-      <c r="M36" s="33" t="b">
-        <v>0</v>
-      </c>
-      <c r="N36" s="52" t="s">
+      <c r="M36" s="52" t="s">
         <v>150</v>
       </c>
-      <c r="O36" s="53" t="s">
+      <c r="N36" s="53" t="s">
         <v>73</v>
       </c>
     </row>
@@ -4336,13 +4204,10 @@
       <c r="L37" s="33" t="s">
         <v>100</v>
       </c>
-      <c r="M37" s="33" t="b">
-        <v>0</v>
-      </c>
-      <c r="N37" s="57" t="s">
+      <c r="M37" s="57" t="s">
         <v>154</v>
       </c>
-      <c r="O37" s="31" t="s">
+      <c r="N37" s="31" t="s">
         <v>73</v>
       </c>
     </row>
@@ -4380,13 +4245,10 @@
       <c r="L38" s="48" t="s">
         <v>209</v>
       </c>
-      <c r="M38" s="33" t="b">
-        <v>0</v>
-      </c>
-      <c r="N38" s="49" t="s">
+      <c r="M38" s="49" t="s">
         <v>150</v>
       </c>
-      <c r="O38" s="53" t="s">
+      <c r="N38" s="53" t="s">
         <v>73</v>
       </c>
     </row>
@@ -4424,13 +4286,10 @@
       <c r="L39" s="48" t="s">
         <v>210</v>
       </c>
-      <c r="M39" s="33" t="b">
-        <v>0</v>
-      </c>
-      <c r="N39" s="48" t="s">
+      <c r="M39" s="48" t="s">
         <v>152</v>
       </c>
-      <c r="O39" s="53" t="s">
+      <c r="N39" s="53" t="s">
         <v>73</v>
       </c>
     </row>
@@ -4468,13 +4327,10 @@
       <c r="L40" s="48" t="s">
         <v>205</v>
       </c>
-      <c r="M40" s="33" t="b">
-        <v>0</v>
-      </c>
-      <c r="N40" s="48" t="s">
+      <c r="M40" s="48" t="s">
         <v>169</v>
       </c>
-      <c r="O40" s="53" t="s">
+      <c r="N40" s="53" t="s">
         <v>73</v>
       </c>
     </row>
@@ -4512,11 +4368,8 @@
       <c r="L41" s="48" t="s">
         <v>211</v>
       </c>
-      <c r="M41" s="33" t="b">
-        <v>0</v>
-      </c>
-      <c r="N41" s="42"/>
-      <c r="O41" s="53" t="s">
+      <c r="M41" s="42"/>
+      <c r="N41" s="53" t="s">
         <v>73</v>
       </c>
     </row>
@@ -4554,13 +4407,10 @@
       <c r="L42" s="33" t="s">
         <v>117</v>
       </c>
-      <c r="M42" s="33" t="b">
-        <v>0</v>
-      </c>
-      <c r="N42" s="56" t="s">
+      <c r="M42" s="56" t="s">
         <v>156</v>
       </c>
-      <c r="O42" s="31" t="s">
+      <c r="N42" s="31" t="s">
         <v>73</v>
       </c>
     </row>
@@ -4598,13 +4448,10 @@
       <c r="L43" s="33" t="s">
         <v>97</v>
       </c>
-      <c r="M43" s="33" t="b">
-        <v>0</v>
-      </c>
-      <c r="N43" s="23" t="s">
+      <c r="M43" s="23" t="s">
         <v>160</v>
       </c>
-      <c r="O43" s="31" t="s">
+      <c r="N43" s="31" t="s">
         <v>73</v>
       </c>
     </row>
@@ -4653,16 +4500,16 @@
       <c r="J46" s="6"/>
       <c r="K46" s="6"/>
       <c r="L46" s="6"/>
-      <c r="M46" s="63"/>
+      <c r="M46" s="60"/>
     </row>
     <row r="47" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B47" s="20"/>
       <c r="C47" s="20"/>
       <c r="D47" s="20"/>
       <c r="E47" s="20"/>
-      <c r="F47" s="61"/>
-      <c r="G47" s="61"/>
-      <c r="H47" s="61"/>
+      <c r="F47" s="64"/>
+      <c r="G47" s="64"/>
+      <c r="H47" s="64"/>
       <c r="I47" s="20"/>
       <c r="J47" s="20"/>
     </row>
@@ -5150,10 +4997,10 @@
       <c r="F70" s="21" t="s">
         <v>40</v>
       </c>
-      <c r="G70" s="62" t="s">
+      <c r="G70" s="65" t="s">
         <v>39</v>
       </c>
-      <c r="H70" s="62"/>
+      <c r="H70" s="65"/>
       <c r="I70" s="20"/>
     </row>
     <row r="71" spans="2:14" ht="142.5" x14ac:dyDescent="0.25">
@@ -5190,7 +5037,7 @@
       <c r="L71" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="M71" s="64"/>
+      <c r="M71" s="61"/>
     </row>
     <row r="72" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B72" s="12" t="s">
@@ -5226,7 +5073,7 @@
       <c r="L72" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="M72" s="65"/>
+      <c r="M72" s="62"/>
     </row>
     <row r="73" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B73" s="12" t="s">
@@ -5262,7 +5109,7 @@
       <c r="L73" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="M73" s="65"/>
+      <c r="M73" s="62"/>
     </row>
     <row r="74" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B74" s="12" t="s">
@@ -5298,7 +5145,7 @@
       <c r="L74" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="M74" s="65"/>
+      <c r="M74" s="62"/>
     </row>
     <row r="76" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="77" spans="2:14" ht="23.25" x14ac:dyDescent="0.35">
@@ -5601,7 +5448,7 @@
     <mergeCell ref="G70:H70"/>
   </mergeCells>
   <conditionalFormatting sqref="C72:E74">
-    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="2"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Missions deactivated + nomenclature changed
Former-commit-id: 8e7ce21978adf8c1b21867e3289c06564c731e6a
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Missions.xlsx
+++ b/Docs/Content/HungryDragonContent_Missions.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="536" uniqueCount="305">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="539" uniqueCount="305">
   <si>
     <t>single_run</t>
   </si>
@@ -1312,7 +1312,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="66">
+  <cellXfs count="65">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1"/>
@@ -1435,9 +1435,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2993,8 +2990,8 @@
   </sheetPr>
   <dimension ref="B1:P156"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A92" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F102" sqref="F102"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3041,14 +3038,14 @@
         <v>141</v>
       </c>
       <c r="G3" s="38"/>
-      <c r="J3" s="63" t="s">
+      <c r="J3" s="62" t="s">
         <v>140</v>
       </c>
-      <c r="K3" s="63"/>
-      <c r="M3" s="63"/>
-      <c r="N3" s="63"/>
-      <c r="O3" s="63"/>
-      <c r="P3" s="63"/>
+      <c r="K3" s="62"/>
+      <c r="M3" s="62"/>
+      <c r="N3" s="62"/>
+      <c r="O3" s="62"/>
+      <c r="P3" s="62"/>
     </row>
     <row r="4" spans="2:16" ht="106.5" x14ac:dyDescent="0.25">
       <c r="B4" s="30" t="s">
@@ -3092,7 +3089,9 @@
       </c>
     </row>
     <row r="5" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B5" s="27"/>
+      <c r="B5" s="27" t="s">
+        <v>1</v>
+      </c>
       <c r="C5" s="24" t="s">
         <v>131</v>
       </c>
@@ -3132,7 +3131,9 @@
       </c>
     </row>
     <row r="6" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B6" s="27"/>
+      <c r="B6" s="27" t="s">
+        <v>1</v>
+      </c>
       <c r="C6" s="24" t="s">
         <v>130</v>
       </c>
@@ -3168,7 +3169,9 @@
       </c>
     </row>
     <row r="7" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B7" s="27"/>
+      <c r="B7" s="27" t="s">
+        <v>1</v>
+      </c>
       <c r="C7" s="24" t="s">
         <v>129</v>
       </c>
@@ -3723,7 +3726,7 @@
       <c r="L20" s="34" t="s">
         <v>91</v>
       </c>
-      <c r="M20" s="54" t="s">
+      <c r="M20" s="53" t="s">
         <v>160</v>
       </c>
       <c r="N20" s="31" t="str">
@@ -4020,38 +4023,38 @@
       </c>
     </row>
     <row r="28" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B28" s="50"/>
-      <c r="C28" s="51" t="s">
+      <c r="B28" s="27"/>
+      <c r="C28" s="50" t="s">
         <v>177</v>
       </c>
-      <c r="D28" s="52" t="s">
+      <c r="D28" s="51" t="s">
         <v>176</v>
       </c>
-      <c r="E28" s="52">
-        <v>0</v>
-      </c>
-      <c r="F28" s="51">
-        <v>0</v>
-      </c>
-      <c r="G28" s="51">
-        <v>0</v>
-      </c>
-      <c r="H28" s="53">
+      <c r="E28" s="51">
+        <v>0</v>
+      </c>
+      <c r="F28" s="50">
+        <v>0</v>
+      </c>
+      <c r="G28" s="50">
+        <v>0</v>
+      </c>
+      <c r="H28" s="52">
         <v>7</v>
       </c>
-      <c r="I28" s="52" t="s">
+      <c r="I28" s="51" t="s">
         <v>145</v>
       </c>
-      <c r="J28" s="51">
+      <c r="J28" s="50">
         <v>8</v>
       </c>
-      <c r="K28" s="52">
+      <c r="K28" s="51">
         <v>9</v>
       </c>
-      <c r="L28" s="53" t="s">
+      <c r="L28" s="52" t="s">
         <v>199</v>
       </c>
-      <c r="M28" s="53" t="s">
+      <c r="M28" s="52" t="s">
         <v>157</v>
       </c>
       <c r="N28" s="31" t="str">
@@ -4060,38 +4063,38 @@
       </c>
     </row>
     <row r="29" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B29" s="50" t="s">
-        <v>1</v>
-      </c>
-      <c r="C29" s="51" t="s">
+      <c r="B29" s="27" t="s">
+        <v>1</v>
+      </c>
+      <c r="C29" s="50" t="s">
         <v>183</v>
       </c>
-      <c r="D29" s="52" t="s">
+      <c r="D29" s="51" t="s">
         <v>146</v>
       </c>
-      <c r="E29" s="52">
-        <v>1</v>
-      </c>
-      <c r="F29" s="51">
+      <c r="E29" s="51">
+        <v>1</v>
+      </c>
+      <c r="F29" s="50">
         <v>0.3</v>
       </c>
-      <c r="G29" s="51">
-        <v>0</v>
-      </c>
-      <c r="H29" s="53">
+      <c r="G29" s="50">
+        <v>0</v>
+      </c>
+      <c r="H29" s="52">
         <v>7</v>
       </c>
-      <c r="I29" s="52"/>
-      <c r="J29" s="51">
+      <c r="I29" s="51"/>
+      <c r="J29" s="50">
         <v>50</v>
       </c>
-      <c r="K29" s="52">
+      <c r="K29" s="51">
         <v>55</v>
       </c>
-      <c r="L29" s="53" t="s">
+      <c r="L29" s="52" t="s">
         <v>200</v>
       </c>
-      <c r="M29" s="53" t="s">
+      <c r="M29" s="52" t="s">
         <v>214</v>
       </c>
       <c r="N29" s="31" t="str">
@@ -4100,40 +4103,40 @@
       </c>
     </row>
     <row r="30" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B30" s="50" t="s">
-        <v>1</v>
-      </c>
-      <c r="C30" s="51" t="s">
+      <c r="B30" s="27" t="s">
+        <v>1</v>
+      </c>
+      <c r="C30" s="50" t="s">
         <v>191</v>
       </c>
-      <c r="D30" s="52" t="s">
+      <c r="D30" s="51" t="s">
         <v>146</v>
       </c>
-      <c r="E30" s="52">
-        <v>1</v>
-      </c>
-      <c r="F30" s="51">
+      <c r="E30" s="51">
+        <v>1</v>
+      </c>
+      <c r="F30" s="50">
         <v>0.3</v>
       </c>
-      <c r="G30" s="51">
+      <c r="G30" s="50">
         <v>3</v>
       </c>
-      <c r="H30" s="53">
+      <c r="H30" s="52">
         <v>7</v>
       </c>
-      <c r="I30" s="52" t="s">
+      <c r="I30" s="51" t="s">
         <v>192</v>
       </c>
-      <c r="J30" s="51">
+      <c r="J30" s="50">
         <v>4</v>
       </c>
-      <c r="K30" s="52">
+      <c r="K30" s="51">
         <v>4</v>
       </c>
-      <c r="L30" s="53" t="s">
+      <c r="L30" s="52" t="s">
         <v>201</v>
       </c>
-      <c r="M30" s="53" t="s">
+      <c r="M30" s="52" t="s">
         <v>166</v>
       </c>
       <c r="N30" s="31" t="str">
@@ -4142,34 +4145,34 @@
       </c>
     </row>
     <row r="31" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B31" s="50" t="s">
-        <v>1</v>
-      </c>
-      <c r="C31" s="51" t="s">
+      <c r="B31" s="27" t="s">
+        <v>1</v>
+      </c>
+      <c r="C31" s="50" t="s">
         <v>189</v>
       </c>
-      <c r="D31" s="52" t="s">
+      <c r="D31" s="51" t="s">
         <v>146</v>
       </c>
-      <c r="E31" s="52">
-        <v>1</v>
-      </c>
-      <c r="F31" s="51">
+      <c r="E31" s="51">
+        <v>1</v>
+      </c>
+      <c r="F31" s="50">
         <v>0.3</v>
       </c>
-      <c r="G31" s="51">
+      <c r="G31" s="50">
         <v>3</v>
       </c>
-      <c r="H31" s="53">
+      <c r="H31" s="52">
         <v>7</v>
       </c>
-      <c r="I31" s="52" t="s">
+      <c r="I31" s="51" t="s">
         <v>198</v>
       </c>
-      <c r="J31" s="51">
+      <c r="J31" s="50">
         <v>5</v>
       </c>
-      <c r="K31" s="52">
+      <c r="K31" s="51">
         <v>5</v>
       </c>
       <c r="L31" s="48" t="s">
@@ -4184,34 +4187,34 @@
       </c>
     </row>
     <row r="32" spans="2:14" s="43" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="50" t="s">
-        <v>1</v>
-      </c>
-      <c r="C32" s="51" t="s">
+      <c r="B32" s="27" t="s">
+        <v>1</v>
+      </c>
+      <c r="C32" s="50" t="s">
         <v>188</v>
       </c>
-      <c r="D32" s="52" t="s">
+      <c r="D32" s="51" t="s">
         <v>146</v>
       </c>
-      <c r="E32" s="52">
-        <v>1</v>
-      </c>
-      <c r="F32" s="52">
+      <c r="E32" s="51">
+        <v>1</v>
+      </c>
+      <c r="F32" s="51">
         <v>0.3</v>
       </c>
-      <c r="G32" s="51">
-        <v>0</v>
-      </c>
-      <c r="H32" s="52">
+      <c r="G32" s="50">
+        <v>0</v>
+      </c>
+      <c r="H32" s="51">
         <v>7</v>
       </c>
-      <c r="I32" s="52" t="s">
+      <c r="I32" s="51" t="s">
         <v>103</v>
       </c>
-      <c r="J32" s="51">
+      <c r="J32" s="50">
         <v>17</v>
       </c>
-      <c r="K32" s="52">
+      <c r="K32" s="51">
         <v>18</v>
       </c>
       <c r="L32" s="48" t="s">
@@ -4226,30 +4229,30 @@
       </c>
     </row>
     <row r="33" spans="2:14" s="43" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B33" s="50"/>
+      <c r="B33" s="27"/>
       <c r="C33" s="40" t="s">
         <v>178</v>
       </c>
       <c r="D33" s="41" t="s">
         <v>178</v>
       </c>
-      <c r="E33" s="52">
-        <v>0</v>
-      </c>
-      <c r="F33" s="52">
-        <v>1</v>
-      </c>
-      <c r="G33" s="51">
+      <c r="E33" s="51">
+        <v>0</v>
+      </c>
+      <c r="F33" s="51">
+        <v>1</v>
+      </c>
+      <c r="G33" s="50">
         <v>2</v>
       </c>
-      <c r="H33" s="52">
+      <c r="H33" s="51">
         <v>7</v>
       </c>
-      <c r="I33" s="52"/>
-      <c r="J33" s="51">
+      <c r="I33" s="51"/>
+      <c r="J33" s="50">
         <v>25</v>
       </c>
-      <c r="K33" s="52">
+      <c r="K33" s="51">
         <v>27</v>
       </c>
       <c r="L33" s="48" t="s">
@@ -4304,34 +4307,34 @@
       </c>
     </row>
     <row r="35" spans="2:14" s="43" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B35" s="50" t="s">
-        <v>1</v>
-      </c>
-      <c r="C35" s="51" t="s">
+      <c r="B35" s="27" t="s">
+        <v>1</v>
+      </c>
+      <c r="C35" s="50" t="s">
         <v>196</v>
       </c>
-      <c r="D35" s="52" t="s">
+      <c r="D35" s="51" t="s">
         <v>146</v>
       </c>
-      <c r="E35" s="52">
-        <v>1</v>
-      </c>
-      <c r="F35" s="52">
+      <c r="E35" s="51">
+        <v>1</v>
+      </c>
+      <c r="F35" s="51">
         <v>0.3</v>
       </c>
-      <c r="G35" s="51">
+      <c r="G35" s="50">
         <v>2</v>
       </c>
-      <c r="H35" s="52">
+      <c r="H35" s="51">
         <v>3</v>
       </c>
-      <c r="I35" s="52" t="s">
+      <c r="I35" s="51" t="s">
         <v>197</v>
       </c>
-      <c r="J35" s="51">
+      <c r="J35" s="50">
         <v>3</v>
       </c>
-      <c r="K35" s="52">
+      <c r="K35" s="51">
         <v>4</v>
       </c>
       <c r="L35" s="48" t="s">
@@ -4346,40 +4349,40 @@
       </c>
     </row>
     <row r="36" spans="2:14" s="43" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B36" s="50" t="s">
-        <v>1</v>
-      </c>
-      <c r="C36" s="51" t="s">
+      <c r="B36" s="27" t="s">
+        <v>1</v>
+      </c>
+      <c r="C36" s="50" t="s">
         <v>187</v>
       </c>
-      <c r="D36" s="52" t="s">
+      <c r="D36" s="51" t="s">
         <v>146</v>
       </c>
-      <c r="E36" s="52">
-        <v>1</v>
-      </c>
-      <c r="F36" s="52">
+      <c r="E36" s="51">
+        <v>1</v>
+      </c>
+      <c r="F36" s="51">
         <v>0.3</v>
       </c>
-      <c r="G36" s="51">
-        <v>1</v>
-      </c>
-      <c r="H36" s="52">
+      <c r="G36" s="50">
+        <v>1</v>
+      </c>
+      <c r="H36" s="51">
         <v>3</v>
       </c>
-      <c r="I36" s="52" t="s">
+      <c r="I36" s="51" t="s">
         <v>127</v>
       </c>
-      <c r="J36" s="51">
+      <c r="J36" s="50">
         <v>25</v>
       </c>
-      <c r="K36" s="52">
+      <c r="K36" s="51">
         <v>27</v>
       </c>
       <c r="L36" s="48" t="s">
         <v>206</v>
       </c>
-      <c r="M36" s="52" t="s">
+      <c r="M36" s="51" t="s">
         <v>148</v>
       </c>
       <c r="N36" s="31" t="str">
@@ -4421,7 +4424,7 @@
       <c r="L37" s="33" t="s">
         <v>99</v>
       </c>
-      <c r="M37" s="56" t="s">
+      <c r="M37" s="55" t="s">
         <v>152</v>
       </c>
       <c r="N37" s="31" t="str">
@@ -4430,32 +4433,32 @@
       </c>
     </row>
     <row r="38" spans="2:14" s="43" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B38" s="50"/>
-      <c r="C38" s="51" t="s">
+      <c r="B38" s="27"/>
+      <c r="C38" s="50" t="s">
         <v>194</v>
       </c>
-      <c r="D38" s="52" t="s">
+      <c r="D38" s="51" t="s">
         <v>179</v>
       </c>
-      <c r="E38" s="52">
-        <v>0</v>
-      </c>
-      <c r="F38" s="52">
-        <v>1</v>
-      </c>
-      <c r="G38" s="51">
-        <v>1</v>
-      </c>
-      <c r="H38" s="52">
+      <c r="E38" s="51">
+        <v>0</v>
+      </c>
+      <c r="F38" s="51">
+        <v>1</v>
+      </c>
+      <c r="G38" s="50">
+        <v>1</v>
+      </c>
+      <c r="H38" s="51">
         <v>2</v>
       </c>
-      <c r="I38" s="52" t="s">
+      <c r="I38" s="51" t="s">
         <v>127</v>
       </c>
-      <c r="J38" s="51">
+      <c r="J38" s="50">
         <v>150</v>
       </c>
-      <c r="K38" s="52">
+      <c r="K38" s="51">
         <v>160</v>
       </c>
       <c r="L38" s="48" t="s">
@@ -4470,32 +4473,32 @@
       </c>
     </row>
     <row r="39" spans="2:14" s="43" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B39" s="50"/>
-      <c r="C39" s="51" t="s">
+      <c r="B39" s="27"/>
+      <c r="C39" s="50" t="s">
         <v>193</v>
       </c>
-      <c r="D39" s="52" t="s">
+      <c r="D39" s="51" t="s">
         <v>179</v>
       </c>
-      <c r="E39" s="52">
-        <v>0</v>
-      </c>
-      <c r="F39" s="52">
-        <v>1</v>
-      </c>
-      <c r="G39" s="51">
-        <v>1</v>
-      </c>
-      <c r="H39" s="52">
+      <c r="E39" s="51">
+        <v>0</v>
+      </c>
+      <c r="F39" s="51">
+        <v>1</v>
+      </c>
+      <c r="G39" s="50">
+        <v>1</v>
+      </c>
+      <c r="H39" s="51">
         <v>2</v>
       </c>
-      <c r="I39" s="52" t="s">
+      <c r="I39" s="51" t="s">
         <v>149</v>
       </c>
-      <c r="J39" s="51">
+      <c r="J39" s="50">
         <v>15</v>
       </c>
-      <c r="K39" s="52">
+      <c r="K39" s="51">
         <v>16</v>
       </c>
       <c r="L39" s="48" t="s">
@@ -4510,34 +4513,34 @@
       </c>
     </row>
     <row r="40" spans="2:14" s="43" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B40" s="50" t="s">
-        <v>1</v>
-      </c>
-      <c r="C40" s="51" t="s">
+      <c r="B40" s="27" t="s">
+        <v>1</v>
+      </c>
+      <c r="C40" s="50" t="s">
         <v>190</v>
       </c>
-      <c r="D40" s="52" t="s">
+      <c r="D40" s="51" t="s">
         <v>146</v>
       </c>
-      <c r="E40" s="52">
-        <v>1</v>
-      </c>
-      <c r="F40" s="52">
+      <c r="E40" s="51">
+        <v>1</v>
+      </c>
+      <c r="F40" s="51">
         <v>0.3</v>
       </c>
-      <c r="G40" s="51">
+      <c r="G40" s="50">
         <v>2</v>
       </c>
-      <c r="H40" s="52">
+      <c r="H40" s="51">
         <v>2</v>
       </c>
-      <c r="I40" s="52" t="s">
+      <c r="I40" s="51" t="s">
         <v>220</v>
       </c>
-      <c r="J40" s="51">
+      <c r="J40" s="50">
         <v>3</v>
       </c>
-      <c r="K40" s="52">
+      <c r="K40" s="51">
         <v>3</v>
       </c>
       <c r="L40" s="48" t="s">
@@ -4552,32 +4555,32 @@
       </c>
     </row>
     <row r="41" spans="2:14" s="43" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B41" s="50"/>
+      <c r="B41" s="27"/>
       <c r="C41" s="40" t="s">
         <v>182</v>
       </c>
       <c r="D41" s="41" t="s">
         <v>181</v>
       </c>
-      <c r="E41" s="52">
-        <v>0</v>
-      </c>
-      <c r="F41" s="52">
-        <v>1</v>
-      </c>
-      <c r="G41" s="51">
-        <v>1</v>
-      </c>
-      <c r="H41" s="52">
+      <c r="E41" s="51">
+        <v>0</v>
+      </c>
+      <c r="F41" s="51">
+        <v>1</v>
+      </c>
+      <c r="G41" s="50">
+        <v>1</v>
+      </c>
+      <c r="H41" s="51">
         <v>2</v>
       </c>
       <c r="I41" s="41" t="s">
         <v>218</v>
       </c>
-      <c r="J41" s="51">
+      <c r="J41" s="50">
         <v>50</v>
       </c>
-      <c r="K41" s="52">
+      <c r="K41" s="51">
         <v>52</v>
       </c>
       <c r="L41" s="48" t="s">
@@ -4623,7 +4626,7 @@
       <c r="L42" s="33" t="s">
         <v>115</v>
       </c>
-      <c r="M42" s="55" t="s">
+      <c r="M42" s="54" t="s">
         <v>154</v>
       </c>
       <c r="N42" s="31" t="str">
@@ -4722,9 +4725,9 @@
       <c r="C47" s="20"/>
       <c r="D47" s="20"/>
       <c r="E47" s="20"/>
-      <c r="F47" s="64"/>
-      <c r="G47" s="64"/>
-      <c r="H47" s="64"/>
+      <c r="F47" s="63"/>
+      <c r="G47" s="63"/>
+      <c r="H47" s="63"/>
       <c r="I47" s="20"/>
       <c r="J47" s="20"/>
     </row>
@@ -5074,7 +5077,7 @@
       </c>
     </row>
     <row r="63" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B63" s="58" t="s">
+      <c r="B63" s="57" t="s">
         <v>1</v>
       </c>
       <c r="C63" s="40" t="s">
@@ -5211,10 +5214,10 @@
       <c r="F70" s="21" t="s">
         <v>40</v>
       </c>
-      <c r="G70" s="65" t="s">
+      <c r="G70" s="64" t="s">
         <v>39</v>
       </c>
-      <c r="H70" s="65"/>
+      <c r="H70" s="64"/>
       <c r="I70" s="20"/>
     </row>
     <row r="71" spans="2:13" ht="142.5" x14ac:dyDescent="0.25">
@@ -5543,7 +5546,7 @@
       <c r="C91" s="1" t="s">
         <v>221</v>
       </c>
-      <c r="D91" s="57">
+      <c r="D91" s="56">
         <v>7.5</v>
       </c>
       <c r="E91" s="1">
@@ -5662,702 +5665,702 @@
       <c r="G105" s="6"/>
     </row>
     <row r="107" spans="2:7" ht="68.25" x14ac:dyDescent="0.25">
-      <c r="B107" s="60" t="s">
+      <c r="B107" s="59" t="s">
         <v>242</v>
       </c>
-      <c r="C107" s="60" t="s">
+      <c r="C107" s="59" t="s">
         <v>3</v>
       </c>
-      <c r="D107" s="61" t="s">
+      <c r="D107" s="60" t="s">
         <v>243</v>
       </c>
-      <c r="E107" s="61" t="s">
+      <c r="E107" s="60" t="s">
         <v>244</v>
       </c>
     </row>
     <row r="108" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B108" s="59" t="s">
-        <v>1</v>
-      </c>
-      <c r="C108" s="62" t="s">
+      <c r="B108" s="58" t="s">
+        <v>1</v>
+      </c>
+      <c r="C108" s="61" t="s">
         <v>80</v>
       </c>
-      <c r="D108" s="62" t="s">
+      <c r="D108" s="61" t="s">
         <v>265</v>
       </c>
-      <c r="E108" s="59" t="b">
+      <c r="E108" s="58" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="109" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B109" s="59" t="s">
-        <v>1</v>
-      </c>
-      <c r="C109" s="62" t="s">
+      <c r="B109" s="58" t="s">
+        <v>1</v>
+      </c>
+      <c r="C109" s="61" t="s">
         <v>93</v>
       </c>
-      <c r="D109" s="62" t="s">
+      <c r="D109" s="61" t="s">
         <v>266</v>
       </c>
-      <c r="E109" s="59" t="b">
+      <c r="E109" s="58" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="110" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B110" s="59" t="s">
-        <v>1</v>
-      </c>
-      <c r="C110" s="62" t="s">
+      <c r="B110" s="58" t="s">
+        <v>1</v>
+      </c>
+      <c r="C110" s="61" t="s">
         <v>126</v>
       </c>
-      <c r="D110" s="62" t="s">
+      <c r="D110" s="61" t="s">
         <v>267</v>
       </c>
-      <c r="E110" s="59" t="b">
+      <c r="E110" s="58" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="111" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B111" s="59" t="s">
-        <v>1</v>
-      </c>
-      <c r="C111" s="62" t="s">
+      <c r="B111" s="58" t="s">
+        <v>1</v>
+      </c>
+      <c r="C111" s="61" t="s">
         <v>109</v>
       </c>
-      <c r="D111" s="62" t="s">
+      <c r="D111" s="61" t="s">
         <v>109</v>
       </c>
-      <c r="E111" s="59" t="b">
+      <c r="E111" s="58" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="112" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B112" s="59" t="s">
-        <v>1</v>
-      </c>
-      <c r="C112" s="62" t="s">
+      <c r="B112" s="58" t="s">
+        <v>1</v>
+      </c>
+      <c r="C112" s="61" t="s">
         <v>122</v>
       </c>
-      <c r="D112" s="62" t="s">
+      <c r="D112" s="61" t="s">
         <v>122</v>
       </c>
-      <c r="E112" s="59" t="b">
+      <c r="E112" s="58" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="113" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B113" s="59" t="s">
-        <v>1</v>
-      </c>
-      <c r="C113" s="62" t="s">
+      <c r="B113" s="58" t="s">
+        <v>1</v>
+      </c>
+      <c r="C113" s="61" t="s">
         <v>110</v>
       </c>
-      <c r="D113" s="62" t="s">
+      <c r="D113" s="61" t="s">
         <v>110</v>
       </c>
-      <c r="E113" s="59" t="b">
+      <c r="E113" s="58" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="114" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B114" s="59" t="s">
-        <v>1</v>
-      </c>
-      <c r="C114" s="62" t="s">
+      <c r="B114" s="58" t="s">
+        <v>1</v>
+      </c>
+      <c r="C114" s="61" t="s">
         <v>112</v>
       </c>
-      <c r="D114" s="62" t="s">
+      <c r="D114" s="61" t="s">
         <v>268</v>
       </c>
-      <c r="E114" s="59" t="b">
+      <c r="E114" s="58" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="115" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B115" s="59" t="s">
-        <v>1</v>
-      </c>
-      <c r="C115" s="62" t="s">
+      <c r="B115" s="58" t="s">
+        <v>1</v>
+      </c>
+      <c r="C115" s="61" t="s">
         <v>245</v>
       </c>
-      <c r="D115" s="62" t="s">
+      <c r="D115" s="61" t="s">
         <v>269</v>
       </c>
-      <c r="E115" s="59" t="b">
+      <c r="E115" s="58" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="116" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B116" s="59" t="s">
-        <v>1</v>
-      </c>
-      <c r="C116" s="62" t="s">
+      <c r="B116" s="58" t="s">
+        <v>1</v>
+      </c>
+      <c r="C116" s="61" t="s">
         <v>246</v>
       </c>
-      <c r="D116" s="62" t="s">
+      <c r="D116" s="61" t="s">
         <v>270</v>
       </c>
-      <c r="E116" s="59" t="b">
+      <c r="E116" s="58" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="117" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B117" s="59" t="s">
-        <v>1</v>
-      </c>
-      <c r="C117" s="62" t="s">
+      <c r="B117" s="58" t="s">
+        <v>1</v>
+      </c>
+      <c r="C117" s="61" t="s">
         <v>206</v>
       </c>
-      <c r="D117" s="62" t="s">
+      <c r="D117" s="61" t="s">
         <v>271</v>
       </c>
-      <c r="E117" s="59" t="b">
+      <c r="E117" s="58" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="118" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B118" s="59" t="s">
-        <v>1</v>
-      </c>
-      <c r="C118" s="62" t="s">
+      <c r="B118" s="58" t="s">
+        <v>1</v>
+      </c>
+      <c r="C118" s="61" t="s">
         <v>205</v>
       </c>
-      <c r="D118" s="62" t="s">
+      <c r="D118" s="61" t="s">
         <v>272</v>
       </c>
-      <c r="E118" s="59" t="b">
+      <c r="E118" s="58" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="119" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B119" s="59" t="s">
-        <v>1</v>
-      </c>
-      <c r="C119" s="62" t="s">
+      <c r="B119" s="58" t="s">
+        <v>1</v>
+      </c>
+      <c r="C119" s="61" t="s">
         <v>200</v>
       </c>
-      <c r="D119" s="62" t="s">
+      <c r="D119" s="61" t="s">
         <v>273</v>
       </c>
-      <c r="E119" s="59" t="b">
+      <c r="E119" s="58" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="120" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B120" s="59" t="s">
-        <v>1</v>
-      </c>
-      <c r="C120" s="62" t="s">
+      <c r="B120" s="58" t="s">
+        <v>1</v>
+      </c>
+      <c r="C120" s="61" t="s">
         <v>204</v>
       </c>
-      <c r="D120" s="62" t="s">
+      <c r="D120" s="61" t="s">
         <v>274</v>
       </c>
-      <c r="E120" s="59" t="b">
+      <c r="E120" s="58" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="121" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B121" s="59" t="s">
-        <v>1</v>
-      </c>
-      <c r="C121" s="62" t="s">
+      <c r="B121" s="58" t="s">
+        <v>1</v>
+      </c>
+      <c r="C121" s="61" t="s">
         <v>203</v>
       </c>
-      <c r="D121" s="62" t="s">
+      <c r="D121" s="61" t="s">
         <v>275</v>
       </c>
-      <c r="E121" s="59" t="b">
+      <c r="E121" s="58" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="122" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B122" s="59" t="s">
-        <v>1</v>
-      </c>
-      <c r="C122" s="62" t="s">
+      <c r="B122" s="58" t="s">
+        <v>1</v>
+      </c>
+      <c r="C122" s="61" t="s">
         <v>201</v>
       </c>
-      <c r="D122" s="62" t="s">
+      <c r="D122" s="61" t="s">
         <v>276</v>
       </c>
-      <c r="E122" s="59" t="b">
+      <c r="E122" s="58" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="123" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B123" s="59" t="s">
-        <v>1</v>
-      </c>
-      <c r="C123" s="62" t="s">
+      <c r="B123" s="58" t="s">
+        <v>1</v>
+      </c>
+      <c r="C123" s="61" t="s">
         <v>202</v>
       </c>
-      <c r="D123" s="62" t="s">
+      <c r="D123" s="61" t="s">
         <v>277</v>
       </c>
-      <c r="E123" s="59" t="b">
+      <c r="E123" s="58" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="124" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B124" s="59" t="s">
-        <v>1</v>
-      </c>
-      <c r="C124" s="62" t="s">
+      <c r="B124" s="58" t="s">
+        <v>1</v>
+      </c>
+      <c r="C124" s="61" t="s">
         <v>115</v>
       </c>
-      <c r="D124" s="62" t="s">
+      <c r="D124" s="61" t="s">
         <v>278</v>
       </c>
-      <c r="E124" s="59" t="b">
+      <c r="E124" s="58" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="125" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B125" s="59" t="s">
-        <v>1</v>
-      </c>
-      <c r="C125" s="62" t="s">
+      <c r="B125" s="58" t="s">
+        <v>1</v>
+      </c>
+      <c r="C125" s="61" t="s">
         <v>247</v>
       </c>
-      <c r="D125" s="62" t="s">
+      <c r="D125" s="61" t="s">
         <v>247</v>
       </c>
-      <c r="E125" s="59" t="b">
+      <c r="E125" s="58" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="126" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B126" s="59" t="s">
-        <v>1</v>
-      </c>
-      <c r="C126" s="62" t="s">
+      <c r="B126" s="58" t="s">
+        <v>1</v>
+      </c>
+      <c r="C126" s="61" t="s">
         <v>83</v>
       </c>
-      <c r="D126" s="62" t="s">
+      <c r="D126" s="61" t="s">
         <v>279</v>
       </c>
-      <c r="E126" s="59" t="b">
+      <c r="E126" s="58" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="127" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B127" s="59" t="s">
-        <v>1</v>
-      </c>
-      <c r="C127" s="62" t="s">
+      <c r="B127" s="58" t="s">
+        <v>1</v>
+      </c>
+      <c r="C127" s="61" t="s">
         <v>96</v>
       </c>
-      <c r="D127" s="62" t="s">
+      <c r="D127" s="61" t="s">
         <v>280</v>
       </c>
-      <c r="E127" s="59" t="b">
+      <c r="E127" s="58" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="128" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B128" s="59" t="s">
-        <v>1</v>
-      </c>
-      <c r="C128" s="62" t="s">
+      <c r="B128" s="58" t="s">
+        <v>1</v>
+      </c>
+      <c r="C128" s="61" t="s">
         <v>248</v>
       </c>
-      <c r="D128" s="62" t="s">
+      <c r="D128" s="61" t="s">
         <v>281</v>
       </c>
-      <c r="E128" s="59" t="b">
+      <c r="E128" s="58" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="129" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B129" s="59" t="s">
-        <v>1</v>
-      </c>
-      <c r="C129" s="62" t="s">
+      <c r="B129" s="58" t="s">
+        <v>1</v>
+      </c>
+      <c r="C129" s="61" t="s">
         <v>249</v>
       </c>
-      <c r="D129" s="62" t="s">
+      <c r="D129" s="61" t="s">
         <v>282</v>
       </c>
-      <c r="E129" s="59" t="b">
+      <c r="E129" s="58" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="130" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B130" s="59" t="s">
-        <v>1</v>
-      </c>
-      <c r="C130" s="62" t="s">
+      <c r="B130" s="58" t="s">
+        <v>1</v>
+      </c>
+      <c r="C130" s="61" t="s">
         <v>102</v>
       </c>
-      <c r="D130" s="62" t="s">
+      <c r="D130" s="61" t="s">
         <v>283</v>
       </c>
-      <c r="E130" s="59" t="b">
+      <c r="E130" s="58" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="131" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B131" s="59" t="s">
-        <v>1</v>
-      </c>
-      <c r="C131" s="62" t="s">
+      <c r="B131" s="58" t="s">
+        <v>1</v>
+      </c>
+      <c r="C131" s="61" t="s">
         <v>250</v>
       </c>
-      <c r="D131" s="62" t="s">
+      <c r="D131" s="61" t="s">
         <v>250</v>
       </c>
-      <c r="E131" s="59" t="b">
+      <c r="E131" s="58" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="132" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B132" s="59" t="s">
-        <v>1</v>
-      </c>
-      <c r="C132" s="62" t="s">
+      <c r="B132" s="58" t="s">
+        <v>1</v>
+      </c>
+      <c r="C132" s="61" t="s">
         <v>124</v>
       </c>
-      <c r="D132" s="62" t="s">
+      <c r="D132" s="61" t="s">
         <v>284</v>
       </c>
-      <c r="E132" s="59" t="b">
+      <c r="E132" s="58" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="133" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B133" s="59" t="s">
-        <v>1</v>
-      </c>
-      <c r="C133" s="62" t="s">
+      <c r="B133" s="58" t="s">
+        <v>1</v>
+      </c>
+      <c r="C133" s="61" t="s">
         <v>88</v>
       </c>
-      <c r="D133" s="62" t="s">
+      <c r="D133" s="61" t="s">
         <v>285</v>
       </c>
-      <c r="E133" s="59" t="b">
+      <c r="E133" s="58" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="134" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B134" s="59" t="s">
-        <v>1</v>
-      </c>
-      <c r="C134" s="62" t="s">
+      <c r="B134" s="58" t="s">
+        <v>1</v>
+      </c>
+      <c r="C134" s="61" t="s">
         <v>251</v>
       </c>
-      <c r="D134" s="62" t="s">
+      <c r="D134" s="61" t="s">
         <v>286</v>
       </c>
-      <c r="E134" s="59" t="b">
+      <c r="E134" s="58" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="135" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B135" s="59" t="s">
-        <v>1</v>
-      </c>
-      <c r="C135" s="62" t="s">
+      <c r="B135" s="58" t="s">
+        <v>1</v>
+      </c>
+      <c r="C135" s="61" t="s">
         <v>303</v>
       </c>
-      <c r="D135" s="62" t="s">
+      <c r="D135" s="61" t="s">
         <v>304</v>
       </c>
-      <c r="E135" s="59" t="b">
+      <c r="E135" s="58" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="136" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B136" s="59" t="s">
-        <v>1</v>
-      </c>
-      <c r="C136" s="62" t="s">
+      <c r="B136" s="58" t="s">
+        <v>1</v>
+      </c>
+      <c r="C136" s="61" t="s">
         <v>252</v>
       </c>
-      <c r="D136" s="62" t="s">
+      <c r="D136" s="61" t="s">
         <v>252</v>
       </c>
-      <c r="E136" s="59" t="b">
+      <c r="E136" s="58" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="137" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B137" s="59" t="s">
-        <v>1</v>
-      </c>
-      <c r="C137" s="62" t="s">
+      <c r="B137" s="58" t="s">
+        <v>1</v>
+      </c>
+      <c r="C137" s="61" t="s">
         <v>117</v>
       </c>
-      <c r="D137" s="62" t="s">
+      <c r="D137" s="61" t="s">
         <v>117</v>
       </c>
-      <c r="E137" s="59" t="b">
+      <c r="E137" s="58" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="138" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B138" s="59" t="s">
-        <v>1</v>
-      </c>
-      <c r="C138" s="62" t="s">
+      <c r="B138" s="58" t="s">
+        <v>1</v>
+      </c>
+      <c r="C138" s="61" t="s">
         <v>253</v>
       </c>
-      <c r="D138" s="62" t="s">
+      <c r="D138" s="61" t="s">
         <v>287</v>
       </c>
-      <c r="E138" s="59" t="b">
+      <c r="E138" s="58" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="139" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B139" s="59" t="s">
-        <v>1</v>
-      </c>
-      <c r="C139" s="62" t="s">
+      <c r="B139" s="58" t="s">
+        <v>1</v>
+      </c>
+      <c r="C139" s="61" t="s">
         <v>91</v>
       </c>
-      <c r="D139" s="62" t="s">
+      <c r="D139" s="61" t="s">
         <v>288</v>
       </c>
-      <c r="E139" s="59" t="b">
+      <c r="E139" s="58" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="140" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B140" s="59" t="s">
-        <v>1</v>
-      </c>
-      <c r="C140" s="62" t="s">
+      <c r="B140" s="58" t="s">
+        <v>1</v>
+      </c>
+      <c r="C140" s="61" t="s">
         <v>254</v>
       </c>
-      <c r="D140" s="62" t="s">
+      <c r="D140" s="61" t="s">
         <v>289</v>
       </c>
-      <c r="E140" s="59" t="b">
+      <c r="E140" s="58" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="141" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B141" s="59" t="s">
-        <v>1</v>
-      </c>
-      <c r="C141" s="62" t="s">
+      <c r="B141" s="58" t="s">
+        <v>1</v>
+      </c>
+      <c r="C141" s="61" t="s">
         <v>255</v>
       </c>
-      <c r="D141" s="62" t="s">
+      <c r="D141" s="61" t="s">
         <v>290</v>
       </c>
-      <c r="E141" s="59" t="b">
+      <c r="E141" s="58" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="142" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B142" s="59" t="s">
-        <v>1</v>
-      </c>
-      <c r="C142" s="62" t="s">
+      <c r="B142" s="58" t="s">
+        <v>1</v>
+      </c>
+      <c r="C142" s="61" t="s">
         <v>256</v>
       </c>
-      <c r="D142" s="62" t="s">
+      <c r="D142" s="61" t="s">
         <v>291</v>
       </c>
-      <c r="E142" s="59" t="b">
+      <c r="E142" s="58" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="143" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B143" s="59" t="s">
-        <v>1</v>
-      </c>
-      <c r="C143" s="62" t="s">
+      <c r="B143" s="58" t="s">
+        <v>1</v>
+      </c>
+      <c r="C143" s="61" t="s">
         <v>86</v>
       </c>
-      <c r="D143" s="62" t="s">
+      <c r="D143" s="61" t="s">
         <v>292</v>
       </c>
-      <c r="E143" s="59" t="b">
+      <c r="E143" s="58" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="144" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B144" s="59" t="s">
-        <v>1</v>
-      </c>
-      <c r="C144" s="62" t="s">
+      <c r="B144" s="58" t="s">
+        <v>1</v>
+      </c>
+      <c r="C144" s="61" t="s">
         <v>73</v>
       </c>
-      <c r="D144" s="62" t="s">
+      <c r="D144" s="61" t="s">
         <v>73</v>
       </c>
-      <c r="E144" s="59" t="b">
+      <c r="E144" s="58" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="145" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B145" s="59" t="s">
-        <v>1</v>
-      </c>
-      <c r="C145" s="62" t="s">
+      <c r="B145" s="58" t="s">
+        <v>1</v>
+      </c>
+      <c r="C145" s="61" t="s">
         <v>108</v>
       </c>
-      <c r="D145" s="62" t="s">
+      <c r="D145" s="61" t="s">
         <v>108</v>
       </c>
-      <c r="E145" s="59" t="b">
+      <c r="E145" s="58" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="146" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B146" s="59" t="s">
-        <v>1</v>
-      </c>
-      <c r="C146" s="62" t="s">
+      <c r="B146" s="58" t="s">
+        <v>1</v>
+      </c>
+      <c r="C146" s="61" t="s">
         <v>257</v>
       </c>
-      <c r="D146" s="62" t="s">
+      <c r="D146" s="61" t="s">
         <v>293</v>
       </c>
-      <c r="E146" s="59" t="b">
+      <c r="E146" s="58" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="147" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B147" s="59" t="s">
-        <v>1</v>
-      </c>
-      <c r="C147" s="62" t="s">
+      <c r="B147" s="58" t="s">
+        <v>1</v>
+      </c>
+      <c r="C147" s="61" t="s">
         <v>258</v>
       </c>
-      <c r="D147" s="62" t="s">
+      <c r="D147" s="61" t="s">
         <v>294</v>
       </c>
-      <c r="E147" s="59" t="b">
+      <c r="E147" s="58" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="148" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B148" s="59" t="s">
-        <v>1</v>
-      </c>
-      <c r="C148" s="62" t="s">
+      <c r="B148" s="58" t="s">
+        <v>1</v>
+      </c>
+      <c r="C148" s="61" t="s">
         <v>77</v>
       </c>
-      <c r="D148" s="62" t="s">
+      <c r="D148" s="61" t="s">
         <v>295</v>
       </c>
-      <c r="E148" s="59" t="b">
+      <c r="E148" s="58" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="149" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B149" s="59" t="s">
-        <v>1</v>
-      </c>
-      <c r="C149" s="62" t="s">
+      <c r="B149" s="58" t="s">
+        <v>1</v>
+      </c>
+      <c r="C149" s="61" t="s">
         <v>105</v>
       </c>
-      <c r="D149" s="62" t="s">
+      <c r="D149" s="61" t="s">
         <v>296</v>
       </c>
-      <c r="E149" s="59" t="b">
+      <c r="E149" s="58" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="150" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B150" s="59" t="s">
-        <v>1</v>
-      </c>
-      <c r="C150" s="62" t="s">
+      <c r="B150" s="58" t="s">
+        <v>1</v>
+      </c>
+      <c r="C150" s="61" t="s">
         <v>259</v>
       </c>
-      <c r="D150" s="62" t="s">
+      <c r="D150" s="61" t="s">
         <v>297</v>
       </c>
-      <c r="E150" s="59" t="b">
+      <c r="E150" s="58" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="151" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B151" s="59" t="s">
-        <v>1</v>
-      </c>
-      <c r="C151" s="62" t="s">
+      <c r="B151" s="58" t="s">
+        <v>1</v>
+      </c>
+      <c r="C151" s="61" t="s">
         <v>260</v>
       </c>
-      <c r="D151" s="62" t="s">
+      <c r="D151" s="61" t="s">
         <v>298</v>
       </c>
-      <c r="E151" s="59" t="b">
+      <c r="E151" s="58" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="152" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B152" s="59" t="s">
-        <v>1</v>
-      </c>
-      <c r="C152" s="62" t="s">
+      <c r="B152" s="58" t="s">
+        <v>1</v>
+      </c>
+      <c r="C152" s="61" t="s">
         <v>261</v>
       </c>
-      <c r="D152" s="62" t="s">
+      <c r="D152" s="61" t="s">
         <v>299</v>
       </c>
-      <c r="E152" s="59" t="b">
+      <c r="E152" s="58" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="153" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B153" s="59" t="s">
-        <v>1</v>
-      </c>
-      <c r="C153" s="62" t="s">
+      <c r="B153" s="58" t="s">
+        <v>1</v>
+      </c>
+      <c r="C153" s="61" t="s">
         <v>262</v>
       </c>
-      <c r="D153" s="62" t="s">
+      <c r="D153" s="61" t="s">
         <v>262</v>
       </c>
-      <c r="E153" s="59" t="b">
+      <c r="E153" s="58" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="154" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B154" s="59" t="s">
-        <v>1</v>
-      </c>
-      <c r="C154" s="62" t="s">
+      <c r="B154" s="58" t="s">
+        <v>1</v>
+      </c>
+      <c r="C154" s="61" t="s">
         <v>99</v>
       </c>
-      <c r="D154" s="62" t="s">
+      <c r="D154" s="61" t="s">
         <v>300</v>
       </c>
-      <c r="E154" s="59" t="b">
+      <c r="E154" s="58" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="155" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B155" s="59" t="s">
-        <v>1</v>
-      </c>
-      <c r="C155" s="62" t="s">
+      <c r="B155" s="58" t="s">
+        <v>1</v>
+      </c>
+      <c r="C155" s="61" t="s">
         <v>263</v>
       </c>
-      <c r="D155" s="62" t="s">
+      <c r="D155" s="61" t="s">
         <v>301</v>
       </c>
-      <c r="E155" s="59" t="b">
+      <c r="E155" s="58" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="156" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B156" s="59" t="s">
-        <v>1</v>
-      </c>
-      <c r="C156" s="62" t="s">
+      <c r="B156" s="58" t="s">
+        <v>1</v>
+      </c>
+      <c r="C156" s="61" t="s">
         <v>264</v>
       </c>
-      <c r="D156" s="62" t="s">
+      <c r="D156" s="61" t="s">
         <v>302</v>
       </c>
-      <c r="E156" s="59" t="b">
+      <c r="E156" s="58" t="b">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Adding new enemy dragon to the mission related to kill enemy dragons. Also adding Dark Dragon mission multipliers
Former-commit-id: de686de3dbb70637fd555f0a0c248627442abf28
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Missions.xlsx
+++ b/Docs/Content/HungryDragonContent_Missions.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="539" uniqueCount="306">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="541" uniqueCount="307">
   <si>
     <t>single_run</t>
   </si>
@@ -363,9 +363,6 @@
   </si>
   <si>
     <t>icon_dragon</t>
-  </si>
-  <si>
-    <t>EnemyTier0;EnemyTier1;EnemyTier2;EnemyTier3;EnemyTier4</t>
   </si>
   <si>
     <t>dragons</t>
@@ -967,6 +964,12 @@
   </si>
   <si>
     <t>PF_icon_heart</t>
+  </si>
+  <si>
+    <t>EnemyTier0;EnemyTier1;EnemyTier2;EnemyTier3;EnemyTier4;EnemyTier5</t>
+  </si>
+  <si>
+    <t>dragon_dark</t>
   </si>
 </sst>
 </file>
@@ -1284,7 +1287,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1"/>
@@ -1394,13 +1397,6 @@
       <alignment textRotation="45"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1413,11 +1409,29 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="69">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
@@ -2569,16 +2583,6 @@
         </bottom>
       </border>
     </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -2593,99 +2597,99 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="missionDifficultyDefinitions" displayName="missionDifficultyDefinitions" ref="B71:L74" totalsRowShown="0" headerRowBorderDxfId="67" tableBorderDxfId="66">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="missionDifficultyDefinitions" displayName="missionDifficultyDefinitions" ref="B71:L74" totalsRowShown="0" headerRowBorderDxfId="68" tableBorderDxfId="67">
   <autoFilter ref="B71:L74"/>
   <tableColumns count="11">
     <tableColumn id="1" name="{missionDifficultyDefinitions}"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="65"/>
-    <tableColumn id="11" name="[difficulty]" dataDxfId="64"/>
-    <tableColumn id="7" name="[index]" dataDxfId="63"/>
-    <tableColumn id="3" name="[dragonsToUnlock]" dataDxfId="62"/>
-    <tableColumn id="4" name="[cooldownMinutes]" dataDxfId="61"/>
-    <tableColumn id="9" name="[maxRewardCoins]" dataDxfId="60"/>
-    <tableColumn id="5" name="[removeMissionPCCoefA]" dataDxfId="59"/>
-    <tableColumn id="6" name="[removeMissionPCCoefB]" dataDxfId="58"/>
-    <tableColumn id="8" name="[tidName]" dataDxfId="57"/>
-    <tableColumn id="10" name="[color]" dataDxfId="56"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="66"/>
+    <tableColumn id="11" name="[difficulty]" dataDxfId="65"/>
+    <tableColumn id="7" name="[index]" dataDxfId="64"/>
+    <tableColumn id="3" name="[dragonsToUnlock]" dataDxfId="63"/>
+    <tableColumn id="4" name="[cooldownMinutes]" dataDxfId="62"/>
+    <tableColumn id="9" name="[maxRewardCoins]" dataDxfId="61"/>
+    <tableColumn id="5" name="[removeMissionPCCoefA]" dataDxfId="60"/>
+    <tableColumn id="6" name="[removeMissionPCCoefB]" dataDxfId="59"/>
+    <tableColumn id="8" name="[tidName]" dataDxfId="58"/>
+    <tableColumn id="10" name="[color]" dataDxfId="57"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table13303132" displayName="Table13303132" ref="B79:E91" totalsRowShown="0" headerRowDxfId="55" dataDxfId="53" headerRowBorderDxfId="54" tableBorderDxfId="52" totalsRowBorderDxfId="51">
-  <autoFilter ref="B79:E91"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table13303132" displayName="Table13303132" ref="B79:E92" totalsRowShown="0" headerRowDxfId="56" dataDxfId="54" headerRowBorderDxfId="55" tableBorderDxfId="53" totalsRowBorderDxfId="52">
+  <autoFilter ref="B79:E92"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="{missionDragonModifiersDefinitions}" dataDxfId="50"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="49"/>
-    <tableColumn id="7" name="[quantityModifier]" dataDxfId="48"/>
-    <tableColumn id="3" name="[missionSCRewardMultiplier]" dataDxfId="47"/>
+    <tableColumn id="1" name="{missionDragonModifiersDefinitions}" dataDxfId="51"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="50"/>
+    <tableColumn id="7" name="[quantityModifier]" dataDxfId="49"/>
+    <tableColumn id="3" name="[missionSCRewardMultiplier]" dataDxfId="48"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table1330313234" displayName="Table1330313234" ref="B95:E98" totalsRowShown="0" headerRowDxfId="46" dataDxfId="44" headerRowBorderDxfId="45" tableBorderDxfId="43" totalsRowBorderDxfId="42">
-  <autoFilter ref="B95:E98"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table1330313234" displayName="Table1330313234" ref="B96:E99" totalsRowShown="0" headerRowDxfId="47" dataDxfId="45" headerRowBorderDxfId="46" tableBorderDxfId="44" totalsRowBorderDxfId="43">
+  <autoFilter ref="B96:E99"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="{missionDifficultyModifiersDefinitions}" dataDxfId="41"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="40"/>
-    <tableColumn id="3" name="[difficulty]" dataDxfId="39"/>
-    <tableColumn id="7" name="[quantityModifier]" dataDxfId="38"/>
+    <tableColumn id="1" name="{missionDifficultyModifiersDefinitions}" dataDxfId="42"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="41"/>
+    <tableColumn id="3" name="[difficulty]" dataDxfId="40"/>
+    <tableColumn id="7" name="[quantityModifier]" dataDxfId="39"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table133031323435" displayName="Table133031323435" ref="B102:D103" totalsRowShown="0" headerRowDxfId="37" dataDxfId="35" headerRowBorderDxfId="36" tableBorderDxfId="34" totalsRowBorderDxfId="33">
-  <autoFilter ref="B102:D103"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table133031323435" displayName="Table133031323435" ref="B103:D104" totalsRowShown="0" headerRowDxfId="38" dataDxfId="36" headerRowBorderDxfId="37" tableBorderDxfId="35" totalsRowBorderDxfId="34">
+  <autoFilter ref="B103:D104"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="{missionOtherModifiersDefinitions}" dataDxfId="32"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="31"/>
-    <tableColumn id="7" name="[quantityModifier]" dataDxfId="30"/>
+    <tableColumn id="1" name="{missionOtherModifiersDefinitions}" dataDxfId="33"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="32"/>
+    <tableColumn id="7" name="[quantityModifier]" dataDxfId="31"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table13" displayName="Table13" ref="B48:H67" totalsRowShown="0" headerRowDxfId="29" dataDxfId="27" headerRowBorderDxfId="28" tableBorderDxfId="26" totalsRowBorderDxfId="25">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table13" displayName="Table13" ref="B48:H67" totalsRowShown="0" headerRowDxfId="30" dataDxfId="28" headerRowBorderDxfId="29" tableBorderDxfId="27" totalsRowBorderDxfId="26">
   <autoFilter ref="B48:H67"/>
   <tableColumns count="7">
-    <tableColumn id="1" name="{missionTypeDefinitions}" dataDxfId="24"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="23"/>
-    <tableColumn id="3" name="[minTier]" dataDxfId="22"/>
-    <tableColumn id="6" name="[maxTier]" dataDxfId="21"/>
-    <tableColumn id="4" name="[weight]" dataDxfId="20"/>
-    <tableColumn id="9" name="[tidDescSingleRun]" dataDxfId="19"/>
-    <tableColumn id="10" name="[tidDescMultiRun]" dataDxfId="18"/>
+    <tableColumn id="1" name="{missionTypeDefinitions}" dataDxfId="25"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="24"/>
+    <tableColumn id="3" name="[minTier]" dataDxfId="23"/>
+    <tableColumn id="6" name="[maxTier]" dataDxfId="22"/>
+    <tableColumn id="4" name="[weight]" dataDxfId="21"/>
+    <tableColumn id="9" name="[tidDescSingleRun]" dataDxfId="20"/>
+    <tableColumn id="10" name="[tidDescMultiRun]" dataDxfId="19"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table1330" displayName="Table1330" ref="B4:N43" totalsRowShown="0" headerRowDxfId="17" dataDxfId="15" headerRowBorderDxfId="16" tableBorderDxfId="14" totalsRowBorderDxfId="13">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table1330" displayName="Table1330" ref="B4:N43" totalsRowShown="0" headerRowDxfId="18" dataDxfId="16" headerRowBorderDxfId="17" tableBorderDxfId="15" totalsRowBorderDxfId="14">
   <autoFilter ref="B4:N43"/>
   <sortState ref="B5:P43">
     <sortCondition descending="1" ref="J4:J43"/>
   </sortState>
   <tableColumns count="13">
-    <tableColumn id="1" name="{missionsDefinitions}" dataDxfId="12"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="11"/>
-    <tableColumn id="7" name="[type]" dataDxfId="10"/>
-    <tableColumn id="8" name="[weight]" dataDxfId="9"/>
-    <tableColumn id="13" name="[singleRunChance]" dataDxfId="8"/>
-    <tableColumn id="11" name="[minTier]" dataDxfId="7"/>
-    <tableColumn id="12" name="[maxTier]" dataDxfId="6"/>
-    <tableColumn id="6" name="[params]" dataDxfId="5"/>
-    <tableColumn id="3" name="[objectiveBaseQuantityMin]" dataDxfId="4"/>
-    <tableColumn id="9" name="[objectiveBaseQuantityMax]" dataDxfId="3"/>
-    <tableColumn id="4" name="[icon]" dataDxfId="2"/>
-    <tableColumn id="5" name="[tidObjective]" dataDxfId="1"/>
-    <tableColumn id="10" name="[trackingSku]" dataDxfId="0">
+    <tableColumn id="1" name="{missionsDefinitions}" dataDxfId="13"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="12"/>
+    <tableColumn id="7" name="[type]" dataDxfId="11"/>
+    <tableColumn id="8" name="[weight]" dataDxfId="10"/>
+    <tableColumn id="13" name="[singleRunChance]" dataDxfId="9"/>
+    <tableColumn id="11" name="[minTier]" dataDxfId="8"/>
+    <tableColumn id="12" name="[maxTier]" dataDxfId="7"/>
+    <tableColumn id="6" name="[params]" dataDxfId="6"/>
+    <tableColumn id="3" name="[objectiveBaseQuantityMin]" dataDxfId="5"/>
+    <tableColumn id="9" name="[objectiveBaseQuantityMax]" dataDxfId="4"/>
+    <tableColumn id="4" name="[icon]" dataDxfId="3"/>
+    <tableColumn id="5" name="[tidObjective]" dataDxfId="2"/>
+    <tableColumn id="10" name="[trackingSku]" dataDxfId="1">
       <calculatedColumnFormula>Table1330[[#This Row],['[sku']]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2959,10 +2963,10 @@
   <sheetPr>
     <tabColor theme="6"/>
   </sheetPr>
-  <dimension ref="B1:P156"/>
+  <dimension ref="B1:P157"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B34" sqref="B34"/>
+    <sheetView tabSelected="1" topLeftCell="A73" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F91" sqref="F91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2985,7 +2989,7 @@
     <row r="1" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:16" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B2" s="6" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C2" s="6"/>
       <c r="D2" s="6"/>
@@ -3003,36 +3007,36 @@
       <c r="C3" s="38"/>
       <c r="D3" s="38"/>
       <c r="E3" s="39" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F3" s="39" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="G3" s="38"/>
-      <c r="J3" s="47" t="s">
-        <v>140</v>
-      </c>
-      <c r="K3" s="47"/>
-      <c r="M3" s="47"/>
-      <c r="N3" s="47"/>
-      <c r="O3" s="47"/>
-      <c r="P3" s="47"/>
+      <c r="J3" s="51" t="s">
+        <v>139</v>
+      </c>
+      <c r="K3" s="51"/>
+      <c r="M3" s="51"/>
+      <c r="N3" s="51"/>
+      <c r="O3" s="51"/>
+      <c r="P3" s="51"/>
     </row>
     <row r="4" spans="2:16" ht="106.5" x14ac:dyDescent="0.25">
       <c r="B4" s="30" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C4" s="28" t="s">
         <v>3</v>
       </c>
       <c r="D4" s="37" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E4" s="37" t="s">
         <v>68</v>
       </c>
       <c r="F4" s="37" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="G4" s="37" t="s">
         <v>70</v>
@@ -3041,22 +3045,22 @@
         <v>69</v>
       </c>
       <c r="I4" s="37" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="J4" s="37" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="K4" s="37" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="L4" s="36" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="M4" s="36" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="N4" s="35" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="5" spans="2:16" x14ac:dyDescent="0.25">
@@ -3064,7 +3068,7 @@
         <v>1</v>
       </c>
       <c r="C5" s="24" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D5" s="24" t="s">
         <v>65</v>
@@ -3082,7 +3086,7 @@
         <v>7</v>
       </c>
       <c r="I5" s="24" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="J5" s="24">
         <v>500</v>
@@ -3091,10 +3095,10 @@
         <v>600</v>
       </c>
       <c r="L5" s="24" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="M5" s="24" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="N5" s="24" t="str">
         <f>Table1330[[#This Row],['[sku']]]</f>
@@ -3106,7 +3110,7 @@
         <v>1</v>
       </c>
       <c r="C6" s="24" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D6" s="23" t="s">
         <v>53</v>
@@ -3144,7 +3148,7 @@
         <v>1</v>
       </c>
       <c r="C7" s="24" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D7" s="24" t="s">
         <v>59</v>
@@ -3182,7 +3186,7 @@
         <v>1</v>
       </c>
       <c r="C8" s="24" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D8" s="24" t="s">
         <v>65</v>
@@ -3200,7 +3204,7 @@
         <v>7</v>
       </c>
       <c r="I8" s="24" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="J8" s="24">
         <v>700</v>
@@ -3209,10 +3213,10 @@
         <v>750</v>
       </c>
       <c r="L8" s="24" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="M8" s="24" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="N8" s="24" t="str">
         <f>Table1330[[#This Row],['[sku']]]</f>
@@ -3224,7 +3228,7 @@
         <v>1</v>
       </c>
       <c r="C9" s="24" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D9" s="24" t="s">
         <v>65</v>
@@ -3242,7 +3246,7 @@
         <v>7</v>
       </c>
       <c r="I9" s="24" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="J9" s="24">
         <v>25</v>
@@ -3251,10 +3255,10 @@
         <v>30</v>
       </c>
       <c r="L9" s="24" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="M9" s="24" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="N9" s="24" t="str">
         <f>Table1330[[#This Row],['[sku']]]</f>
@@ -3262,41 +3266,41 @@
       </c>
     </row>
     <row r="10" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B10" s="50"/>
-      <c r="C10" s="51" t="s">
-        <v>121</v>
-      </c>
-      <c r="D10" s="52" t="s">
+      <c r="B10" s="47"/>
+      <c r="C10" s="48" t="s">
+        <v>120</v>
+      </c>
+      <c r="D10" s="49" t="s">
         <v>56</v>
       </c>
-      <c r="E10" s="51">
-        <v>0</v>
-      </c>
-      <c r="F10" s="51">
-        <v>0</v>
-      </c>
-      <c r="G10" s="51">
+      <c r="E10" s="48">
+        <v>0</v>
+      </c>
+      <c r="F10" s="48">
+        <v>0</v>
+      </c>
+      <c r="G10" s="48">
         <v>2</v>
       </c>
-      <c r="H10" s="51">
+      <c r="H10" s="48">
         <v>7</v>
       </c>
-      <c r="I10" s="52" t="s">
-        <v>120</v>
-      </c>
-      <c r="J10" s="51">
+      <c r="I10" s="49" t="s">
+        <v>119</v>
+      </c>
+      <c r="J10" s="48">
         <v>8</v>
       </c>
-      <c r="K10" s="53">
+      <c r="K10" s="50">
         <v>9</v>
       </c>
-      <c r="L10" s="51" t="s">
-        <v>119</v>
-      </c>
-      <c r="M10" s="51" t="s">
-        <v>151</v>
-      </c>
-      <c r="N10" s="51" t="str">
+      <c r="L10" s="48" t="s">
+        <v>118</v>
+      </c>
+      <c r="M10" s="48" t="s">
+        <v>150</v>
+      </c>
+      <c r="N10" s="48" t="str">
         <f>Table1330[[#This Row],['[sku']]]</f>
         <v>small_decos</v>
       </c>
@@ -3306,7 +3310,7 @@
         <v>1</v>
       </c>
       <c r="C11" s="24" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D11" s="23" t="s">
         <v>50</v>
@@ -3324,7 +3328,7 @@
         <v>7</v>
       </c>
       <c r="I11" s="23" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="J11" s="24">
         <v>1000</v>
@@ -3333,10 +3337,10 @@
         <v>1200</v>
       </c>
       <c r="L11" s="24" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="M11" s="24" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="N11" s="24" t="str">
         <f>Table1330[[#This Row],['[sku']]]</f>
@@ -3348,7 +3352,7 @@
         <v>1</v>
       </c>
       <c r="C12" s="24" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D12" s="24" t="s">
         <v>65</v>
@@ -3366,7 +3370,7 @@
         <v>7</v>
       </c>
       <c r="I12" s="24" t="s">
-        <v>113</v>
+        <v>305</v>
       </c>
       <c r="J12" s="24">
         <v>10</v>
@@ -3378,7 +3382,7 @@
         <v>112</v>
       </c>
       <c r="M12" s="24" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="N12" s="24" t="str">
         <f>Table1330[[#This Row],['[sku']]]</f>
@@ -3415,7 +3419,7 @@
         <v>6</v>
       </c>
       <c r="L13" s="24" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="M13" s="24"/>
       <c r="N13" s="24" t="str">
@@ -3572,7 +3576,7 @@
         <v>105</v>
       </c>
       <c r="M17" s="24" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="N17" s="24" t="str">
         <f>Table1330[[#This Row],['[sku']]]</f>
@@ -3614,7 +3618,7 @@
         <v>102</v>
       </c>
       <c r="M18" s="24" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="N18" s="24" t="str">
         <f>Table1330[[#This Row],['[sku']]]</f>
@@ -3656,7 +3660,7 @@
         <v>93</v>
       </c>
       <c r="M19" s="24" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="N19" s="24" t="str">
         <f>Table1330[[#This Row],['[sku']]]</f>
@@ -3686,7 +3690,7 @@
         <v>7</v>
       </c>
       <c r="I20" s="23" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="J20" s="24">
         <v>5</v>
@@ -3698,7 +3702,7 @@
         <v>91</v>
       </c>
       <c r="M20" s="24" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="N20" s="24" t="str">
         <f>Table1330[[#This Row],['[sku']]]</f>
@@ -3740,7 +3744,7 @@
         <v>88</v>
       </c>
       <c r="M21" s="24" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="N21" s="24" t="str">
         <f>Table1330[[#This Row],['[sku']]]</f>
@@ -3752,7 +3756,7 @@
         <v>1</v>
       </c>
       <c r="C22" s="24" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D22" s="23" t="s">
         <v>65</v>
@@ -3782,7 +3786,7 @@
         <v>86</v>
       </c>
       <c r="M22" s="24" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="N22" s="24" t="str">
         <f>Table1330[[#This Row],['[sku']]]</f>
@@ -3824,7 +3828,7 @@
         <v>83</v>
       </c>
       <c r="M23" s="24" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="N23" s="24" t="str">
         <f>Table1330[[#This Row],['[sku']]]</f>
@@ -3866,7 +3870,7 @@
         <v>80</v>
       </c>
       <c r="M24" s="24" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="N24" s="24" t="str">
         <f>Table1330[[#This Row],['[sku']]]</f>
@@ -3908,7 +3912,7 @@
         <v>77</v>
       </c>
       <c r="M25" s="24" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="N25" s="24" t="str">
         <f>Table1330[[#This Row],['[sku']]]</f>
@@ -3916,41 +3920,41 @@
       </c>
     </row>
     <row r="26" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B26" s="50"/>
-      <c r="C26" s="51" t="s">
+      <c r="B26" s="47"/>
+      <c r="C26" s="48" t="s">
         <v>76</v>
       </c>
-      <c r="D26" s="52" t="s">
+      <c r="D26" s="49" t="s">
         <v>65</v>
       </c>
-      <c r="E26" s="51">
-        <v>0</v>
-      </c>
-      <c r="F26" s="51">
+      <c r="E26" s="48">
+        <v>0</v>
+      </c>
+      <c r="F26" s="48">
         <v>0.3</v>
       </c>
-      <c r="G26" s="51">
+      <c r="G26" s="48">
         <v>3</v>
       </c>
-      <c r="H26" s="51">
+      <c r="H26" s="48">
         <v>7</v>
       </c>
-      <c r="I26" s="52" t="s">
+      <c r="I26" s="49" t="s">
         <v>75</v>
       </c>
-      <c r="J26" s="51">
+      <c r="J26" s="48">
         <v>3</v>
       </c>
-      <c r="K26" s="53">
+      <c r="K26" s="50">
         <v>3</v>
       </c>
-      <c r="L26" s="51" t="s">
+      <c r="L26" s="48" t="s">
         <v>74</v>
       </c>
-      <c r="M26" s="51" t="s">
-        <v>165</v>
-      </c>
-      <c r="N26" s="51" t="str">
+      <c r="M26" s="48" t="s">
+        <v>164</v>
+      </c>
+      <c r="N26" s="48" t="str">
         <f>Table1330[[#This Row],['[sku']]]</f>
         <v>troll</v>
       </c>
@@ -3996,10 +4000,10 @@
     <row r="28" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B28" s="27"/>
       <c r="C28" s="23" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D28" s="24" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E28" s="24">
         <v>0</v>
@@ -4014,7 +4018,7 @@
         <v>7</v>
       </c>
       <c r="I28" s="24" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="J28" s="24">
         <v>8</v>
@@ -4023,10 +4027,10 @@
         <v>9</v>
       </c>
       <c r="L28" s="24" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="M28" s="24" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="N28" s="24" t="str">
         <f>Table1330[[#This Row],['[sku']]]</f>
@@ -4038,10 +4042,10 @@
         <v>1</v>
       </c>
       <c r="C29" s="23" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D29" s="24" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E29" s="24">
         <v>1</v>
@@ -4063,10 +4067,10 @@
         <v>55</v>
       </c>
       <c r="L29" s="24" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="M29" s="24" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="N29" s="24" t="str">
         <f>Table1330[[#This Row],['[sku']]]</f>
@@ -4078,10 +4082,10 @@
         <v>1</v>
       </c>
       <c r="C30" s="23" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D30" s="23" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E30" s="24">
         <v>1</v>
@@ -4096,7 +4100,7 @@
         <v>7</v>
       </c>
       <c r="I30" s="24" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="J30" s="24">
         <v>4</v>
@@ -4105,10 +4109,10 @@
         <v>4</v>
       </c>
       <c r="L30" s="24" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="M30" s="24" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="N30" s="24" t="str">
         <f>Table1330[[#This Row],['[sku']]]</f>
@@ -4120,10 +4124,10 @@
         <v>1</v>
       </c>
       <c r="C31" s="23" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D31" s="23" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E31" s="24">
         <v>1</v>
@@ -4138,7 +4142,7 @@
         <v>7</v>
       </c>
       <c r="I31" s="23" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="J31" s="24">
         <v>5</v>
@@ -4147,10 +4151,10 @@
         <v>5</v>
       </c>
       <c r="L31" s="24" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="M31" s="24" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="N31" s="24" t="str">
         <f>Table1330[[#This Row],['[sku']]]</f>
@@ -4162,10 +4166,10 @@
         <v>1</v>
       </c>
       <c r="C32" s="23" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D32" s="24" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E32" s="24">
         <v>1</v>
@@ -4189,10 +4193,10 @@
         <v>18</v>
       </c>
       <c r="L32" s="24" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="M32" s="24" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="N32" s="24" t="str">
         <f>Table1330[[#This Row],['[sku']]]</f>
@@ -4200,37 +4204,37 @@
       </c>
     </row>
     <row r="33" spans="2:14" s="40" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B33" s="50"/>
-      <c r="C33" s="51" t="s">
-        <v>178</v>
-      </c>
-      <c r="D33" s="52" t="s">
-        <v>178</v>
-      </c>
-      <c r="E33" s="51">
-        <v>0</v>
-      </c>
-      <c r="F33" s="51">
-        <v>1</v>
-      </c>
-      <c r="G33" s="51">
+      <c r="B33" s="47"/>
+      <c r="C33" s="48" t="s">
+        <v>177</v>
+      </c>
+      <c r="D33" s="49" t="s">
+        <v>177</v>
+      </c>
+      <c r="E33" s="48">
+        <v>0</v>
+      </c>
+      <c r="F33" s="48">
+        <v>1</v>
+      </c>
+      <c r="G33" s="48">
         <v>2</v>
       </c>
-      <c r="H33" s="51">
+      <c r="H33" s="48">
         <v>7</v>
       </c>
-      <c r="I33" s="52"/>
-      <c r="J33" s="51">
+      <c r="I33" s="49"/>
+      <c r="J33" s="48">
         <v>25</v>
       </c>
-      <c r="K33" s="53">
+      <c r="K33" s="50">
         <v>27</v>
       </c>
-      <c r="L33" s="51" t="s">
-        <v>210</v>
-      </c>
-      <c r="M33" s="51"/>
-      <c r="N33" s="51" t="str">
+      <c r="L33" s="48" t="s">
+        <v>209</v>
+      </c>
+      <c r="M33" s="48"/>
+      <c r="N33" s="48" t="str">
         <f>Table1330[[#This Row],['[sku']]]</f>
         <v>critical_time</v>
       </c>
@@ -4240,7 +4244,7 @@
         <v>1</v>
       </c>
       <c r="C34" s="23" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D34" s="23" t="s">
         <v>56</v>
@@ -4258,7 +4262,7 @@
         <v>3</v>
       </c>
       <c r="I34" s="23" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="J34" s="24">
         <v>10</v>
@@ -4267,10 +4271,10 @@
         <v>12</v>
       </c>
       <c r="L34" s="24" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="M34" s="24" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="N34" s="24" t="str">
         <f>Table1330[[#This Row],['[sku']]]</f>
@@ -4282,10 +4286,10 @@
         <v>1</v>
       </c>
       <c r="C35" s="23" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D35" s="23" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E35" s="23">
         <v>1</v>
@@ -4300,7 +4304,7 @@
         <v>3</v>
       </c>
       <c r="I35" s="24" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="J35" s="24">
         <v>3</v>
@@ -4309,10 +4313,10 @@
         <v>4</v>
       </c>
       <c r="L35" s="24" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="M35" s="24" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="N35" s="24" t="str">
         <f>Table1330[[#This Row],['[sku']]]</f>
@@ -4324,10 +4328,10 @@
         <v>1</v>
       </c>
       <c r="C36" s="24" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D36" s="23" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E36" s="23">
         <v>1</v>
@@ -4342,7 +4346,7 @@
         <v>3</v>
       </c>
       <c r="I36" s="24" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="J36" s="24">
         <v>25</v>
@@ -4351,10 +4355,10 @@
         <v>27</v>
       </c>
       <c r="L36" s="24" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="M36" s="24" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="N36" s="24" t="str">
         <f>Table1330[[#This Row],['[sku']]]</f>
@@ -4396,7 +4400,7 @@
         <v>99</v>
       </c>
       <c r="M37" s="24" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="N37" s="24" t="str">
         <f>Table1330[[#This Row],['[sku']]]</f>
@@ -4404,81 +4408,81 @@
       </c>
     </row>
     <row r="38" spans="2:14" s="40" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B38" s="50"/>
-      <c r="C38" s="51" t="s">
-        <v>194</v>
-      </c>
-      <c r="D38" s="52" t="s">
-        <v>179</v>
-      </c>
-      <c r="E38" s="51">
-        <v>0</v>
-      </c>
-      <c r="F38" s="51">
-        <v>1</v>
-      </c>
-      <c r="G38" s="51">
-        <v>1</v>
-      </c>
-      <c r="H38" s="51">
+      <c r="B38" s="47"/>
+      <c r="C38" s="48" t="s">
+        <v>193</v>
+      </c>
+      <c r="D38" s="49" t="s">
+        <v>178</v>
+      </c>
+      <c r="E38" s="48">
+        <v>0</v>
+      </c>
+      <c r="F38" s="48">
+        <v>1</v>
+      </c>
+      <c r="G38" s="48">
+        <v>1</v>
+      </c>
+      <c r="H38" s="48">
         <v>2</v>
       </c>
-      <c r="I38" s="52" t="s">
-        <v>127</v>
-      </c>
-      <c r="J38" s="51">
+      <c r="I38" s="49" t="s">
+        <v>126</v>
+      </c>
+      <c r="J38" s="48">
         <v>150</v>
       </c>
-      <c r="K38" s="53">
+      <c r="K38" s="50">
         <v>160</v>
       </c>
-      <c r="L38" s="51" t="s">
-        <v>207</v>
-      </c>
-      <c r="M38" s="51" t="s">
-        <v>148</v>
-      </c>
-      <c r="N38" s="51" t="str">
+      <c r="L38" s="48" t="s">
+        <v>206</v>
+      </c>
+      <c r="M38" s="48" t="s">
+        <v>147</v>
+      </c>
+      <c r="N38" s="48" t="str">
         <f>Table1330[[#This Row],['[sku']]]</f>
         <v>kill_chain_canaries</v>
       </c>
     </row>
     <row r="39" spans="2:14" s="40" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B39" s="50"/>
-      <c r="C39" s="51" t="s">
-        <v>193</v>
-      </c>
-      <c r="D39" s="52" t="s">
-        <v>179</v>
-      </c>
-      <c r="E39" s="51">
-        <v>0</v>
-      </c>
-      <c r="F39" s="51">
-        <v>1</v>
-      </c>
-      <c r="G39" s="51">
-        <v>1</v>
-      </c>
-      <c r="H39" s="51">
+      <c r="B39" s="47"/>
+      <c r="C39" s="48" t="s">
+        <v>192</v>
+      </c>
+      <c r="D39" s="49" t="s">
+        <v>178</v>
+      </c>
+      <c r="E39" s="48">
+        <v>0</v>
+      </c>
+      <c r="F39" s="48">
+        <v>1</v>
+      </c>
+      <c r="G39" s="48">
+        <v>1</v>
+      </c>
+      <c r="H39" s="48">
         <v>2</v>
       </c>
-      <c r="I39" s="52" t="s">
+      <c r="I39" s="49" t="s">
+        <v>148</v>
+      </c>
+      <c r="J39" s="48">
+        <v>15</v>
+      </c>
+      <c r="K39" s="50">
+        <v>16</v>
+      </c>
+      <c r="L39" s="48" t="s">
+        <v>207</v>
+      </c>
+      <c r="M39" s="48" t="s">
         <v>149</v>
       </c>
-      <c r="J39" s="51">
-        <v>15</v>
-      </c>
-      <c r="K39" s="53">
-        <v>16</v>
-      </c>
-      <c r="L39" s="51" t="s">
-        <v>208</v>
-      </c>
-      <c r="M39" s="51" t="s">
-        <v>150</v>
-      </c>
-      <c r="N39" s="51" t="str">
+      <c r="N39" s="48" t="str">
         <f>Table1330[[#This Row],['[sku']]]</f>
         <v>kill_chain_humans</v>
       </c>
@@ -4488,10 +4492,10 @@
         <v>1</v>
       </c>
       <c r="C40" s="24" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D40" s="23" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E40" s="23">
         <v>1</v>
@@ -4506,7 +4510,7 @@
         <v>2</v>
       </c>
       <c r="I40" s="23" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="J40" s="24">
         <v>3</v>
@@ -4515,10 +4519,10 @@
         <v>3</v>
       </c>
       <c r="L40" s="24" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="M40" s="24" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="N40" s="24" t="str">
         <f>Table1330[[#This Row],['[sku']]]</f>
@@ -4526,39 +4530,39 @@
       </c>
     </row>
     <row r="41" spans="2:14" s="40" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B41" s="50"/>
-      <c r="C41" s="51" t="s">
-        <v>182</v>
-      </c>
-      <c r="D41" s="52" t="s">
+      <c r="B41" s="47"/>
+      <c r="C41" s="48" t="s">
         <v>181</v>
       </c>
-      <c r="E41" s="51">
-        <v>0</v>
-      </c>
-      <c r="F41" s="51">
-        <v>1</v>
-      </c>
-      <c r="G41" s="51">
-        <v>1</v>
-      </c>
-      <c r="H41" s="51">
+      <c r="D41" s="49" t="s">
+        <v>180</v>
+      </c>
+      <c r="E41" s="48">
+        <v>0</v>
+      </c>
+      <c r="F41" s="48">
+        <v>1</v>
+      </c>
+      <c r="G41" s="48">
+        <v>1</v>
+      </c>
+      <c r="H41" s="48">
         <v>2</v>
       </c>
-      <c r="I41" s="52" t="s">
-        <v>218</v>
-      </c>
-      <c r="J41" s="51">
+      <c r="I41" s="49" t="s">
+        <v>217</v>
+      </c>
+      <c r="J41" s="48">
         <v>50</v>
       </c>
-      <c r="K41" s="53">
+      <c r="K41" s="50">
         <v>52</v>
       </c>
-      <c r="L41" s="51" t="s">
-        <v>209</v>
-      </c>
-      <c r="M41" s="51"/>
-      <c r="N41" s="51" t="str">
+      <c r="L41" s="48" t="s">
+        <v>208</v>
+      </c>
+      <c r="M41" s="48"/>
+      <c r="N41" s="48" t="str">
         <f>Table1330[[#This Row],['[sku']]]</f>
         <v>destroy_mineSmall</v>
       </c>
@@ -4568,7 +4572,7 @@
         <v>1</v>
       </c>
       <c r="C42" s="24" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D42" s="24" t="s">
         <v>50</v>
@@ -4586,7 +4590,7 @@
         <v>1</v>
       </c>
       <c r="I42" s="23" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="J42" s="24">
         <v>1</v>
@@ -4595,10 +4599,10 @@
         <v>2</v>
       </c>
       <c r="L42" s="24" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="M42" s="24" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="N42" s="24" t="str">
         <f>Table1330[[#This Row],['[sku']]]</f>
@@ -4640,7 +4644,7 @@
         <v>96</v>
       </c>
       <c r="M43" s="24" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="N43" s="24" t="str">
         <f>Table1330[[#This Row],['[sku']]]</f>
@@ -4696,9 +4700,9 @@
       <c r="C47" s="20"/>
       <c r="D47" s="20"/>
       <c r="E47" s="20"/>
-      <c r="F47" s="48"/>
-      <c r="G47" s="48"/>
-      <c r="H47" s="48"/>
+      <c r="F47" s="52"/>
+      <c r="G47" s="52"/>
+      <c r="H47" s="52"/>
       <c r="I47" s="20"/>
       <c r="J47" s="20"/>
     </row>
@@ -4914,7 +4918,7 @@
         <v>1</v>
       </c>
       <c r="C57" s="24" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D57" s="24">
         <v>0</v>
@@ -4926,10 +4930,10 @@
         <v>0</v>
       </c>
       <c r="G57" s="26" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="H57" s="26" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="58" spans="2:8" x14ac:dyDescent="0.25">
@@ -4937,7 +4941,7 @@
         <v>1</v>
       </c>
       <c r="C58" s="24" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D58" s="24">
         <v>0</v>
@@ -4949,10 +4953,10 @@
         <v>0</v>
       </c>
       <c r="G58" s="26" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="H58" s="26" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="59" spans="2:8" x14ac:dyDescent="0.25">
@@ -4960,7 +4964,7 @@
         <v>1</v>
       </c>
       <c r="C59" s="24" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D59" s="24">
         <v>0</v>
@@ -4972,10 +4976,10 @@
         <v>2</v>
       </c>
       <c r="G59" s="26" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="H59" s="26" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="60" spans="2:8" x14ac:dyDescent="0.25">
@@ -4983,7 +4987,7 @@
         <v>1</v>
       </c>
       <c r="C60" s="24" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="D60" s="24">
         <v>0</v>
@@ -4995,10 +4999,10 @@
         <v>1</v>
       </c>
       <c r="G60" s="26" t="s">
+        <v>229</v>
+      </c>
+      <c r="H60" s="26" t="s">
         <v>230</v>
-      </c>
-      <c r="H60" s="26" t="s">
-        <v>231</v>
       </c>
     </row>
     <row r="61" spans="2:8" x14ac:dyDescent="0.25">
@@ -5006,7 +5010,7 @@
         <v>1</v>
       </c>
       <c r="C61" s="23" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="D61" s="23">
         <v>0</v>
@@ -5018,10 +5022,10 @@
         <v>1</v>
       </c>
       <c r="G61" s="26" t="s">
+        <v>232</v>
+      </c>
+      <c r="H61" s="26" t="s">
         <v>233</v>
-      </c>
-      <c r="H61" s="26" t="s">
-        <v>234</v>
       </c>
     </row>
     <row r="62" spans="2:8" x14ac:dyDescent="0.25">
@@ -5029,7 +5033,7 @@
         <v>1</v>
       </c>
       <c r="C62" s="24" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D62" s="24">
         <v>0</v>
@@ -5041,10 +5045,10 @@
         <v>1</v>
       </c>
       <c r="G62" s="26" t="s">
+        <v>235</v>
+      </c>
+      <c r="H62" s="26" t="s">
         <v>236</v>
-      </c>
-      <c r="H62" s="26" t="s">
-        <v>237</v>
       </c>
     </row>
     <row r="63" spans="2:8" x14ac:dyDescent="0.25">
@@ -5052,7 +5056,7 @@
         <v>1</v>
       </c>
       <c r="C63" s="24" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="D63" s="24">
         <v>0</v>
@@ -5064,10 +5068,10 @@
         <v>1</v>
       </c>
       <c r="G63" s="26" t="s">
+        <v>238</v>
+      </c>
+      <c r="H63" s="26" t="s">
         <v>239</v>
-      </c>
-      <c r="H63" s="26" t="s">
-        <v>240</v>
       </c>
     </row>
     <row r="64" spans="2:8" x14ac:dyDescent="0.25">
@@ -5075,7 +5079,7 @@
         <v>1</v>
       </c>
       <c r="C64" s="23" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D64" s="23">
         <v>0</v>
@@ -5087,10 +5091,10 @@
         <v>0</v>
       </c>
       <c r="G64" s="22" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="H64" s="22" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="65" spans="2:13" x14ac:dyDescent="0.25">
@@ -5098,7 +5102,7 @@
         <v>1</v>
       </c>
       <c r="C65" s="24" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D65" s="24">
         <v>0</v>
@@ -5110,7 +5114,7 @@
         <v>1</v>
       </c>
       <c r="G65" s="26" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="H65" s="26"/>
     </row>
@@ -5119,7 +5123,7 @@
         <v>1</v>
       </c>
       <c r="C66" s="24" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D66" s="24">
         <v>0</v>
@@ -5131,10 +5135,10 @@
         <v>0</v>
       </c>
       <c r="G66" s="26" t="s">
+        <v>184</v>
+      </c>
+      <c r="H66" s="26" t="s">
         <v>185</v>
-      </c>
-      <c r="H66" s="26" t="s">
-        <v>186</v>
       </c>
     </row>
     <row r="67" spans="2:13" x14ac:dyDescent="0.25">
@@ -5142,7 +5146,7 @@
         <v>1</v>
       </c>
       <c r="C67" s="24" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D67" s="24">
         <v>0</v>
@@ -5154,10 +5158,10 @@
         <v>1</v>
       </c>
       <c r="G67" s="26" t="s">
+        <v>210</v>
+      </c>
+      <c r="H67" s="26" t="s">
         <v>211</v>
-      </c>
-      <c r="H67" s="26" t="s">
-        <v>212</v>
       </c>
     </row>
     <row r="68" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -5185,10 +5189,10 @@
       <c r="F70" s="21" t="s">
         <v>40</v>
       </c>
-      <c r="G70" s="49" t="s">
+      <c r="G70" s="53" t="s">
         <v>39</v>
       </c>
-      <c r="H70" s="49"/>
+      <c r="H70" s="53"/>
       <c r="I70" s="20"/>
     </row>
     <row r="71" spans="2:13" ht="142.5" x14ac:dyDescent="0.25">
@@ -5199,7 +5203,7 @@
         <v>3</v>
       </c>
       <c r="D71" s="18" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="E71" s="18" t="s">
         <v>37</v>
@@ -5231,7 +5235,7 @@
         <v>1</v>
       </c>
       <c r="C72" s="11" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="D72" s="11" t="s">
         <v>8</v>
@@ -5266,7 +5270,7 @@
         <v>1</v>
       </c>
       <c r="C73" s="11" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D73" s="11" t="s">
         <v>7</v>
@@ -5301,7 +5305,7 @@
         <v>1</v>
       </c>
       <c r="C74" s="11" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="D74" s="11" t="s">
         <v>6</v>
@@ -5473,7 +5477,7 @@
         <v>1</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D88" s="1">
         <v>4.5</v>
@@ -5515,7 +5519,7 @@
         <v>1</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="D91" s="42">
         <v>7.5</v>
@@ -5524,43 +5528,43 @@
         <v>85</v>
       </c>
     </row>
-    <row r="92" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="93" spans="2:7" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B93" s="6" t="s">
+    <row r="92" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B92" s="54" t="s">
+        <v>1</v>
+      </c>
+      <c r="C92" s="42" t="s">
+        <v>306</v>
+      </c>
+      <c r="D92" s="42">
+        <v>8</v>
+      </c>
+      <c r="E92" s="42">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="93" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="94" spans="2:7" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B94" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C93" s="6"/>
-      <c r="D93" s="6"/>
-      <c r="E93" s="6"/>
-      <c r="F93" s="6"/>
-      <c r="G93" s="6"/>
-    </row>
-    <row r="95" spans="2:7" ht="142.5" x14ac:dyDescent="0.25">
-      <c r="B95" s="5" t="s">
+      <c r="C94" s="6"/>
+      <c r="D94" s="6"/>
+      <c r="E94" s="6"/>
+      <c r="F94" s="6"/>
+      <c r="G94" s="6"/>
+    </row>
+    <row r="96" spans="2:7" ht="142.5" x14ac:dyDescent="0.25">
+      <c r="B96" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C95" s="4" t="s">
+      <c r="C96" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D95" s="4" t="s">
-        <v>225</v>
-      </c>
-      <c r="E95" s="3" t="s">
+      <c r="D96" s="4" t="s">
+        <v>224</v>
+      </c>
+      <c r="E96" s="3" t="s">
         <v>2</v>
-      </c>
-    </row>
-    <row r="96" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B96" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C96" s="1" t="s">
-        <v>226</v>
-      </c>
-      <c r="D96" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E96" s="1">
-        <v>0.05</v>
       </c>
     </row>
     <row r="97" spans="2:7" x14ac:dyDescent="0.25">
@@ -5568,13 +5572,13 @@
         <v>1</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="D97" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E97" s="1">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="98" spans="2:7" x14ac:dyDescent="0.25">
@@ -5582,85 +5586,85 @@
         <v>1</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="D98" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E98" s="1">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="99" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B99" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C99" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="D99" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E98" s="1">
+      <c r="E99" s="1">
         <v>0.2</v>
       </c>
     </row>
-    <row r="99" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="100" spans="2:7" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B100" s="6" t="s">
+    <row r="100" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="101" spans="2:7" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B101" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C100" s="6"/>
-      <c r="D100" s="6"/>
-      <c r="E100" s="6"/>
-      <c r="F100" s="6"/>
-      <c r="G100" s="6"/>
-    </row>
-    <row r="102" spans="2:7" ht="132" x14ac:dyDescent="0.25">
-      <c r="B102" s="5" t="s">
+      <c r="C101" s="6"/>
+      <c r="D101" s="6"/>
+      <c r="E101" s="6"/>
+      <c r="F101" s="6"/>
+      <c r="G101" s="6"/>
+    </row>
+    <row r="103" spans="2:7" ht="132" x14ac:dyDescent="0.25">
+      <c r="B103" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C102" s="4" t="s">
+      <c r="C103" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D102" s="3" t="s">
+      <c r="D103" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="103" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B103" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C103" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D103" s="1">
+    <row r="104" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B104" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C104" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D104" s="1">
         <v>0.7</v>
       </c>
     </row>
-    <row r="104" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="105" spans="2:7" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B105" s="6" t="s">
+    <row r="105" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="106" spans="2:7" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B106" s="6" t="s">
+        <v>240</v>
+      </c>
+      <c r="C106" s="6"/>
+      <c r="D106" s="6"/>
+      <c r="E106" s="6"/>
+      <c r="F106" s="6"/>
+      <c r="G106" s="6"/>
+    </row>
+    <row r="108" spans="2:7" ht="68.25" x14ac:dyDescent="0.25">
+      <c r="B108" s="44" t="s">
         <v>241</v>
       </c>
-      <c r="C105" s="6"/>
-      <c r="D105" s="6"/>
-      <c r="E105" s="6"/>
-      <c r="F105" s="6"/>
-      <c r="G105" s="6"/>
-    </row>
-    <row r="107" spans="2:7" ht="68.25" x14ac:dyDescent="0.25">
-      <c r="B107" s="44" t="s">
+      <c r="C108" s="44" t="s">
+        <v>3</v>
+      </c>
+      <c r="D108" s="45" t="s">
         <v>242</v>
       </c>
-      <c r="C107" s="44" t="s">
-        <v>3</v>
-      </c>
-      <c r="D107" s="45" t="s">
+      <c r="E108" s="45" t="s">
         <v>243</v>
-      </c>
-      <c r="E107" s="45" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="108" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B108" s="43" t="s">
-        <v>1</v>
-      </c>
-      <c r="C108" s="46" t="s">
-        <v>80</v>
-      </c>
-      <c r="D108" s="46" t="s">
-        <v>265</v>
-      </c>
-      <c r="E108" s="43" t="b">
-        <v>1</v>
       </c>
     </row>
     <row r="109" spans="2:7" x14ac:dyDescent="0.25">
@@ -5668,10 +5672,10 @@
         <v>1</v>
       </c>
       <c r="C109" s="46" t="s">
-        <v>93</v>
+        <v>80</v>
       </c>
       <c r="D109" s="46" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="E109" s="43" t="b">
         <v>1</v>
@@ -5682,10 +5686,10 @@
         <v>1</v>
       </c>
       <c r="C110" s="46" t="s">
-        <v>126</v>
+        <v>93</v>
       </c>
       <c r="D110" s="46" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="E110" s="43" t="b">
         <v>1</v>
@@ -5696,13 +5700,13 @@
         <v>1</v>
       </c>
       <c r="C111" s="46" t="s">
-        <v>109</v>
+        <v>125</v>
       </c>
       <c r="D111" s="46" t="s">
-        <v>109</v>
+        <v>266</v>
       </c>
       <c r="E111" s="43" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="112" spans="2:7" x14ac:dyDescent="0.25">
@@ -5710,10 +5714,10 @@
         <v>1</v>
       </c>
       <c r="C112" s="46" t="s">
-        <v>122</v>
+        <v>109</v>
       </c>
       <c r="D112" s="46" t="s">
-        <v>122</v>
+        <v>109</v>
       </c>
       <c r="E112" s="43" t="b">
         <v>0</v>
@@ -5724,10 +5728,10 @@
         <v>1</v>
       </c>
       <c r="C113" s="46" t="s">
-        <v>110</v>
+        <v>121</v>
       </c>
       <c r="D113" s="46" t="s">
-        <v>110</v>
+        <v>121</v>
       </c>
       <c r="E113" s="43" t="b">
         <v>0</v>
@@ -5738,13 +5742,13 @@
         <v>1</v>
       </c>
       <c r="C114" s="46" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D114" s="46" t="s">
-        <v>268</v>
+        <v>110</v>
       </c>
       <c r="E114" s="43" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="115" spans="2:5" x14ac:dyDescent="0.25">
@@ -5752,10 +5756,10 @@
         <v>1</v>
       </c>
       <c r="C115" s="46" t="s">
-        <v>245</v>
+        <v>112</v>
       </c>
       <c r="D115" s="46" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="E115" s="43" t="b">
         <v>1</v>
@@ -5766,10 +5770,10 @@
         <v>1</v>
       </c>
       <c r="C116" s="46" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="D116" s="46" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="E116" s="43" t="b">
         <v>1</v>
@@ -5780,10 +5784,10 @@
         <v>1</v>
       </c>
       <c r="C117" s="46" t="s">
-        <v>206</v>
+        <v>245</v>
       </c>
       <c r="D117" s="46" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="E117" s="43" t="b">
         <v>1</v>
@@ -5797,7 +5801,7 @@
         <v>205</v>
       </c>
       <c r="D118" s="46" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="E118" s="43" t="b">
         <v>1</v>
@@ -5808,10 +5812,10 @@
         <v>1</v>
       </c>
       <c r="C119" s="46" t="s">
-        <v>200</v>
+        <v>204</v>
       </c>
       <c r="D119" s="46" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="E119" s="43" t="b">
         <v>1</v>
@@ -5822,10 +5826,10 @@
         <v>1</v>
       </c>
       <c r="C120" s="46" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="D120" s="46" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="E120" s="43" t="b">
         <v>1</v>
@@ -5839,7 +5843,7 @@
         <v>203</v>
       </c>
       <c r="D121" s="46" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="E121" s="43" t="b">
         <v>1</v>
@@ -5850,10 +5854,10 @@
         <v>1</v>
       </c>
       <c r="C122" s="46" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="D122" s="46" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="E122" s="43" t="b">
         <v>1</v>
@@ -5864,10 +5868,10 @@
         <v>1</v>
       </c>
       <c r="C123" s="46" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="D123" s="46" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="E123" s="43" t="b">
         <v>1</v>
@@ -5878,10 +5882,10 @@
         <v>1</v>
       </c>
       <c r="C124" s="46" t="s">
-        <v>115</v>
+        <v>201</v>
       </c>
       <c r="D124" s="46" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="E124" s="43" t="b">
         <v>1</v>
@@ -5892,13 +5896,13 @@
         <v>1</v>
       </c>
       <c r="C125" s="46" t="s">
-        <v>247</v>
+        <v>114</v>
       </c>
       <c r="D125" s="46" t="s">
-        <v>247</v>
+        <v>277</v>
       </c>
       <c r="E125" s="43" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="126" spans="2:5" x14ac:dyDescent="0.25">
@@ -5906,13 +5910,13 @@
         <v>1</v>
       </c>
       <c r="C126" s="46" t="s">
-        <v>83</v>
+        <v>246</v>
       </c>
       <c r="D126" s="46" t="s">
-        <v>279</v>
+        <v>246</v>
       </c>
       <c r="E126" s="43" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="127" spans="2:5" x14ac:dyDescent="0.25">
@@ -5920,10 +5924,10 @@
         <v>1</v>
       </c>
       <c r="C127" s="46" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="D127" s="46" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="E127" s="43" t="b">
         <v>1</v>
@@ -5934,10 +5938,10 @@
         <v>1</v>
       </c>
       <c r="C128" s="46" t="s">
-        <v>248</v>
+        <v>96</v>
       </c>
       <c r="D128" s="46" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="E128" s="43" t="b">
         <v>1</v>
@@ -5948,10 +5952,10 @@
         <v>1</v>
       </c>
       <c r="C129" s="46" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="D129" s="46" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="E129" s="43" t="b">
         <v>1</v>
@@ -5962,10 +5966,10 @@
         <v>1</v>
       </c>
       <c r="C130" s="46" t="s">
-        <v>102</v>
+        <v>248</v>
       </c>
       <c r="D130" s="46" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="E130" s="43" t="b">
         <v>1</v>
@@ -5976,10 +5980,10 @@
         <v>1</v>
       </c>
       <c r="C131" s="46" t="s">
-        <v>250</v>
+        <v>102</v>
       </c>
       <c r="D131" s="46" t="s">
-        <v>305</v>
+        <v>282</v>
       </c>
       <c r="E131" s="43" t="b">
         <v>1</v>
@@ -5990,10 +5994,10 @@
         <v>1</v>
       </c>
       <c r="C132" s="46" t="s">
-        <v>124</v>
+        <v>249</v>
       </c>
       <c r="D132" s="46" t="s">
-        <v>284</v>
+        <v>304</v>
       </c>
       <c r="E132" s="43" t="b">
         <v>1</v>
@@ -6004,10 +6008,10 @@
         <v>1</v>
       </c>
       <c r="C133" s="46" t="s">
-        <v>88</v>
+        <v>123</v>
       </c>
       <c r="D133" s="46" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="E133" s="43" t="b">
         <v>1</v>
@@ -6018,10 +6022,10 @@
         <v>1</v>
       </c>
       <c r="C134" s="46" t="s">
-        <v>251</v>
+        <v>88</v>
       </c>
       <c r="D134" s="46" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="E134" s="43" t="b">
         <v>1</v>
@@ -6032,10 +6036,10 @@
         <v>1</v>
       </c>
       <c r="C135" s="46" t="s">
-        <v>303</v>
+        <v>250</v>
       </c>
       <c r="D135" s="46" t="s">
-        <v>304</v>
+        <v>285</v>
       </c>
       <c r="E135" s="43" t="b">
         <v>1</v>
@@ -6046,13 +6050,13 @@
         <v>1</v>
       </c>
       <c r="C136" s="46" t="s">
-        <v>252</v>
+        <v>302</v>
       </c>
       <c r="D136" s="46" t="s">
-        <v>252</v>
+        <v>303</v>
       </c>
       <c r="E136" s="43" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="137" spans="2:5" x14ac:dyDescent="0.25">
@@ -6060,10 +6064,10 @@
         <v>1</v>
       </c>
       <c r="C137" s="46" t="s">
-        <v>117</v>
+        <v>251</v>
       </c>
       <c r="D137" s="46" t="s">
-        <v>117</v>
+        <v>251</v>
       </c>
       <c r="E137" s="43" t="b">
         <v>0</v>
@@ -6074,13 +6078,13 @@
         <v>1</v>
       </c>
       <c r="C138" s="46" t="s">
-        <v>253</v>
+        <v>116</v>
       </c>
       <c r="D138" s="46" t="s">
-        <v>287</v>
+        <v>116</v>
       </c>
       <c r="E138" s="43" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="139" spans="2:5" x14ac:dyDescent="0.25">
@@ -6088,10 +6092,10 @@
         <v>1</v>
       </c>
       <c r="C139" s="46" t="s">
-        <v>91</v>
+        <v>252</v>
       </c>
       <c r="D139" s="46" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="E139" s="43" t="b">
         <v>1</v>
@@ -6102,10 +6106,10 @@
         <v>1</v>
       </c>
       <c r="C140" s="46" t="s">
-        <v>254</v>
+        <v>91</v>
       </c>
       <c r="D140" s="46" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="E140" s="43" t="b">
         <v>1</v>
@@ -6116,10 +6120,10 @@
         <v>1</v>
       </c>
       <c r="C141" s="46" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="D141" s="46" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="E141" s="43" t="b">
         <v>1</v>
@@ -6130,10 +6134,10 @@
         <v>1</v>
       </c>
       <c r="C142" s="46" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="D142" s="46" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="E142" s="43" t="b">
         <v>1</v>
@@ -6144,10 +6148,10 @@
         <v>1</v>
       </c>
       <c r="C143" s="46" t="s">
-        <v>86</v>
+        <v>255</v>
       </c>
       <c r="D143" s="46" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="E143" s="43" t="b">
         <v>1</v>
@@ -6158,13 +6162,13 @@
         <v>1</v>
       </c>
       <c r="C144" s="46" t="s">
-        <v>73</v>
+        <v>86</v>
       </c>
       <c r="D144" s="46" t="s">
-        <v>73</v>
+        <v>291</v>
       </c>
       <c r="E144" s="43" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="145" spans="2:5" x14ac:dyDescent="0.25">
@@ -6172,10 +6176,10 @@
         <v>1</v>
       </c>
       <c r="C145" s="46" t="s">
-        <v>108</v>
+        <v>73</v>
       </c>
       <c r="D145" s="46" t="s">
-        <v>108</v>
+        <v>73</v>
       </c>
       <c r="E145" s="43" t="b">
         <v>0</v>
@@ -6186,13 +6190,13 @@
         <v>1</v>
       </c>
       <c r="C146" s="46" t="s">
-        <v>257</v>
+        <v>108</v>
       </c>
       <c r="D146" s="46" t="s">
-        <v>293</v>
+        <v>108</v>
       </c>
       <c r="E146" s="43" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="147" spans="2:5" x14ac:dyDescent="0.25">
@@ -6200,10 +6204,10 @@
         <v>1</v>
       </c>
       <c r="C147" s="46" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="D147" s="46" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="E147" s="43" t="b">
         <v>1</v>
@@ -6214,10 +6218,10 @@
         <v>1</v>
       </c>
       <c r="C148" s="46" t="s">
-        <v>77</v>
+        <v>257</v>
       </c>
       <c r="D148" s="46" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="E148" s="43" t="b">
         <v>1</v>
@@ -6228,10 +6232,10 @@
         <v>1</v>
       </c>
       <c r="C149" s="46" t="s">
-        <v>105</v>
+        <v>77</v>
       </c>
       <c r="D149" s="46" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="E149" s="43" t="b">
         <v>1</v>
@@ -6242,10 +6246,10 @@
         <v>1</v>
       </c>
       <c r="C150" s="46" t="s">
-        <v>259</v>
+        <v>105</v>
       </c>
       <c r="D150" s="46" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="E150" s="43" t="b">
         <v>1</v>
@@ -6256,10 +6260,10 @@
         <v>1</v>
       </c>
       <c r="C151" s="46" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="D151" s="46" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="E151" s="43" t="b">
         <v>1</v>
@@ -6270,10 +6274,10 @@
         <v>1</v>
       </c>
       <c r="C152" s="46" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="D152" s="46" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="E152" s="43" t="b">
         <v>1</v>
@@ -6284,13 +6288,13 @@
         <v>1</v>
       </c>
       <c r="C153" s="46" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="D153" s="46" t="s">
-        <v>262</v>
+        <v>298</v>
       </c>
       <c r="E153" s="43" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="154" spans="2:5" x14ac:dyDescent="0.25">
@@ -6298,13 +6302,13 @@
         <v>1</v>
       </c>
       <c r="C154" s="46" t="s">
-        <v>99</v>
+        <v>261</v>
       </c>
       <c r="D154" s="46" t="s">
-        <v>300</v>
+        <v>261</v>
       </c>
       <c r="E154" s="43" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="155" spans="2:5" x14ac:dyDescent="0.25">
@@ -6312,10 +6316,10 @@
         <v>1</v>
       </c>
       <c r="C155" s="46" t="s">
-        <v>263</v>
+        <v>99</v>
       </c>
       <c r="D155" s="46" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="E155" s="43" t="b">
         <v>1</v>
@@ -6326,12 +6330,26 @@
         <v>1</v>
       </c>
       <c r="C156" s="46" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="D156" s="46" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="E156" s="43" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="157" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B157" s="43" t="s">
+        <v>1</v>
+      </c>
+      <c r="C157" s="46" t="s">
+        <v>263</v>
+      </c>
+      <c r="D157" s="46" t="s">
+        <v>301</v>
+      </c>
+      <c r="E157" s="43" t="b">
         <v>1</v>
       </c>
     </row>
@@ -6343,7 +6361,7 @@
     <mergeCell ref="G70:H70"/>
   </mergeCells>
   <conditionalFormatting sqref="C72:E74">
-    <cfRule type="duplicateValues" dxfId="68" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="2"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
added icons anniversary to content
Former-commit-id: c400007eb676f8e11b14169dc2538112b3d08bb9
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Missions.xlsx
+++ b/Docs/Content/HungryDragonContent_Missions.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\dragon\Docs\Content\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\dragon\client\Docs\Content\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="missions" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="162913" calcOnSave="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="541" uniqueCount="307">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="550" uniqueCount="313">
   <si>
     <t>single_run</t>
   </si>
@@ -970,6 +970,24 @@
   </si>
   <si>
     <t>dragon_dark</t>
+  </si>
+  <si>
+    <t>PF_icon_1stAnniversaryCake</t>
+  </si>
+  <si>
+    <t>PF_icon_AnniversaryCandle</t>
+  </si>
+  <si>
+    <t>PF_icon_Party_Hat</t>
+  </si>
+  <si>
+    <t>icon_1stAnniversaryCake</t>
+  </si>
+  <si>
+    <t>icon_AnniversaryCandle</t>
+  </si>
+  <si>
+    <t>icon_Party_Hat</t>
   </si>
 </sst>
 </file>
@@ -1409,6 +1427,7 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1416,22 +1435,11 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="69">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
@@ -2583,6 +2591,16 @@
         </bottom>
       </border>
     </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -2597,99 +2615,99 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="missionDifficultyDefinitions" displayName="missionDifficultyDefinitions" ref="B71:L74" totalsRowShown="0" headerRowBorderDxfId="68" tableBorderDxfId="67">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="missionDifficultyDefinitions" displayName="missionDifficultyDefinitions" ref="B71:L74" totalsRowShown="0" headerRowBorderDxfId="67" tableBorderDxfId="66">
   <autoFilter ref="B71:L74"/>
   <tableColumns count="11">
     <tableColumn id="1" name="{missionDifficultyDefinitions}"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="66"/>
-    <tableColumn id="11" name="[difficulty]" dataDxfId="65"/>
-    <tableColumn id="7" name="[index]" dataDxfId="64"/>
-    <tableColumn id="3" name="[dragonsToUnlock]" dataDxfId="63"/>
-    <tableColumn id="4" name="[cooldownMinutes]" dataDxfId="62"/>
-    <tableColumn id="9" name="[maxRewardCoins]" dataDxfId="61"/>
-    <tableColumn id="5" name="[removeMissionPCCoefA]" dataDxfId="60"/>
-    <tableColumn id="6" name="[removeMissionPCCoefB]" dataDxfId="59"/>
-    <tableColumn id="8" name="[tidName]" dataDxfId="58"/>
-    <tableColumn id="10" name="[color]" dataDxfId="57"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="65"/>
+    <tableColumn id="11" name="[difficulty]" dataDxfId="64"/>
+    <tableColumn id="7" name="[index]" dataDxfId="63"/>
+    <tableColumn id="3" name="[dragonsToUnlock]" dataDxfId="62"/>
+    <tableColumn id="4" name="[cooldownMinutes]" dataDxfId="61"/>
+    <tableColumn id="9" name="[maxRewardCoins]" dataDxfId="60"/>
+    <tableColumn id="5" name="[removeMissionPCCoefA]" dataDxfId="59"/>
+    <tableColumn id="6" name="[removeMissionPCCoefB]" dataDxfId="58"/>
+    <tableColumn id="8" name="[tidName]" dataDxfId="57"/>
+    <tableColumn id="10" name="[color]" dataDxfId="56"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table13303132" displayName="Table13303132" ref="B79:E92" totalsRowShown="0" headerRowDxfId="56" dataDxfId="54" headerRowBorderDxfId="55" tableBorderDxfId="53" totalsRowBorderDxfId="52">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table13303132" displayName="Table13303132" ref="B79:E92" totalsRowShown="0" headerRowDxfId="55" dataDxfId="53" headerRowBorderDxfId="54" tableBorderDxfId="52" totalsRowBorderDxfId="51">
   <autoFilter ref="B79:E92"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="{missionDragonModifiersDefinitions}" dataDxfId="51"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="50"/>
-    <tableColumn id="7" name="[quantityModifier]" dataDxfId="49"/>
-    <tableColumn id="3" name="[missionSCRewardMultiplier]" dataDxfId="48"/>
+    <tableColumn id="1" name="{missionDragonModifiersDefinitions}" dataDxfId="50"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="49"/>
+    <tableColumn id="7" name="[quantityModifier]" dataDxfId="48"/>
+    <tableColumn id="3" name="[missionSCRewardMultiplier]" dataDxfId="47"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table1330313234" displayName="Table1330313234" ref="B96:E99" totalsRowShown="0" headerRowDxfId="47" dataDxfId="45" headerRowBorderDxfId="46" tableBorderDxfId="44" totalsRowBorderDxfId="43">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table1330313234" displayName="Table1330313234" ref="B96:E99" totalsRowShown="0" headerRowDxfId="46" dataDxfId="44" headerRowBorderDxfId="45" tableBorderDxfId="43" totalsRowBorderDxfId="42">
   <autoFilter ref="B96:E99"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="{missionDifficultyModifiersDefinitions}" dataDxfId="42"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="41"/>
-    <tableColumn id="3" name="[difficulty]" dataDxfId="40"/>
-    <tableColumn id="7" name="[quantityModifier]" dataDxfId="39"/>
+    <tableColumn id="1" name="{missionDifficultyModifiersDefinitions}" dataDxfId="41"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="40"/>
+    <tableColumn id="3" name="[difficulty]" dataDxfId="39"/>
+    <tableColumn id="7" name="[quantityModifier]" dataDxfId="38"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table133031323435" displayName="Table133031323435" ref="B103:D104" totalsRowShown="0" headerRowDxfId="38" dataDxfId="36" headerRowBorderDxfId="37" tableBorderDxfId="35" totalsRowBorderDxfId="34">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table133031323435" displayName="Table133031323435" ref="B103:D104" totalsRowShown="0" headerRowDxfId="37" dataDxfId="35" headerRowBorderDxfId="36" tableBorderDxfId="34" totalsRowBorderDxfId="33">
   <autoFilter ref="B103:D104"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="{missionOtherModifiersDefinitions}" dataDxfId="33"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="32"/>
-    <tableColumn id="7" name="[quantityModifier]" dataDxfId="31"/>
+    <tableColumn id="1" name="{missionOtherModifiersDefinitions}" dataDxfId="32"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="31"/>
+    <tableColumn id="7" name="[quantityModifier]" dataDxfId="30"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table13" displayName="Table13" ref="B48:H67" totalsRowShown="0" headerRowDxfId="30" dataDxfId="28" headerRowBorderDxfId="29" tableBorderDxfId="27" totalsRowBorderDxfId="26">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table13" displayName="Table13" ref="B48:H67" totalsRowShown="0" headerRowDxfId="29" dataDxfId="27" headerRowBorderDxfId="28" tableBorderDxfId="26" totalsRowBorderDxfId="25">
   <autoFilter ref="B48:H67"/>
   <tableColumns count="7">
-    <tableColumn id="1" name="{missionTypeDefinitions}" dataDxfId="25"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="24"/>
-    <tableColumn id="3" name="[minTier]" dataDxfId="23"/>
-    <tableColumn id="6" name="[maxTier]" dataDxfId="22"/>
-    <tableColumn id="4" name="[weight]" dataDxfId="21"/>
-    <tableColumn id="9" name="[tidDescSingleRun]" dataDxfId="20"/>
-    <tableColumn id="10" name="[tidDescMultiRun]" dataDxfId="19"/>
+    <tableColumn id="1" name="{missionTypeDefinitions}" dataDxfId="24"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="23"/>
+    <tableColumn id="3" name="[minTier]" dataDxfId="22"/>
+    <tableColumn id="6" name="[maxTier]" dataDxfId="21"/>
+    <tableColumn id="4" name="[weight]" dataDxfId="20"/>
+    <tableColumn id="9" name="[tidDescSingleRun]" dataDxfId="19"/>
+    <tableColumn id="10" name="[tidDescMultiRun]" dataDxfId="18"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table1330" displayName="Table1330" ref="B4:N43" totalsRowShown="0" headerRowDxfId="18" dataDxfId="16" headerRowBorderDxfId="17" tableBorderDxfId="15" totalsRowBorderDxfId="14">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table1330" displayName="Table1330" ref="B4:N43" totalsRowShown="0" headerRowDxfId="17" dataDxfId="15" headerRowBorderDxfId="16" tableBorderDxfId="14" totalsRowBorderDxfId="13">
   <autoFilter ref="B4:N43"/>
   <sortState ref="B5:P43">
     <sortCondition descending="1" ref="J4:J43"/>
   </sortState>
   <tableColumns count="13">
-    <tableColumn id="1" name="{missionsDefinitions}" dataDxfId="13"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="12"/>
-    <tableColumn id="7" name="[type]" dataDxfId="11"/>
-    <tableColumn id="8" name="[weight]" dataDxfId="10"/>
-    <tableColumn id="13" name="[singleRunChance]" dataDxfId="9"/>
-    <tableColumn id="11" name="[minTier]" dataDxfId="8"/>
-    <tableColumn id="12" name="[maxTier]" dataDxfId="7"/>
-    <tableColumn id="6" name="[params]" dataDxfId="6"/>
-    <tableColumn id="3" name="[objectiveBaseQuantityMin]" dataDxfId="5"/>
-    <tableColumn id="9" name="[objectiveBaseQuantityMax]" dataDxfId="4"/>
-    <tableColumn id="4" name="[icon]" dataDxfId="3"/>
-    <tableColumn id="5" name="[tidObjective]" dataDxfId="2"/>
-    <tableColumn id="10" name="[trackingSku]" dataDxfId="1">
+    <tableColumn id="1" name="{missionsDefinitions}" dataDxfId="12"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="11"/>
+    <tableColumn id="7" name="[type]" dataDxfId="10"/>
+    <tableColumn id="8" name="[weight]" dataDxfId="9"/>
+    <tableColumn id="13" name="[singleRunChance]" dataDxfId="8"/>
+    <tableColumn id="11" name="[minTier]" dataDxfId="7"/>
+    <tableColumn id="12" name="[maxTier]" dataDxfId="6"/>
+    <tableColumn id="6" name="[params]" dataDxfId="5"/>
+    <tableColumn id="3" name="[objectiveBaseQuantityMin]" dataDxfId="4"/>
+    <tableColumn id="9" name="[objectiveBaseQuantityMax]" dataDxfId="3"/>
+    <tableColumn id="4" name="[icon]" dataDxfId="2"/>
+    <tableColumn id="5" name="[tidObjective]" dataDxfId="1"/>
+    <tableColumn id="10" name="[trackingSku]" dataDxfId="0">
       <calculatedColumnFormula>Table1330[[#This Row],['[sku']]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2963,10 +2981,10 @@
   <sheetPr>
     <tabColor theme="6"/>
   </sheetPr>
-  <dimension ref="B1:P157"/>
+  <dimension ref="B1:P160"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A73" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F91" sqref="F91"/>
+    <sheetView tabSelected="1" topLeftCell="A130" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C161" sqref="C161"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3013,14 +3031,14 @@
         <v>140</v>
       </c>
       <c r="G3" s="38"/>
-      <c r="J3" s="51" t="s">
+      <c r="J3" s="52" t="s">
         <v>139</v>
       </c>
-      <c r="K3" s="51"/>
-      <c r="M3" s="51"/>
-      <c r="N3" s="51"/>
-      <c r="O3" s="51"/>
-      <c r="P3" s="51"/>
+      <c r="K3" s="52"/>
+      <c r="M3" s="52"/>
+      <c r="N3" s="52"/>
+      <c r="O3" s="52"/>
+      <c r="P3" s="52"/>
     </row>
     <row r="4" spans="2:16" ht="106.5" x14ac:dyDescent="0.25">
       <c r="B4" s="30" t="s">
@@ -4700,9 +4718,9 @@
       <c r="C47" s="20"/>
       <c r="D47" s="20"/>
       <c r="E47" s="20"/>
-      <c r="F47" s="52"/>
-      <c r="G47" s="52"/>
-      <c r="H47" s="52"/>
+      <c r="F47" s="53"/>
+      <c r="G47" s="53"/>
+      <c r="H47" s="53"/>
       <c r="I47" s="20"/>
       <c r="J47" s="20"/>
     </row>
@@ -5189,10 +5207,10 @@
       <c r="F70" s="21" t="s">
         <v>40</v>
       </c>
-      <c r="G70" s="53" t="s">
+      <c r="G70" s="54" t="s">
         <v>39</v>
       </c>
-      <c r="H70" s="53"/>
+      <c r="H70" s="54"/>
       <c r="I70" s="20"/>
     </row>
     <row r="71" spans="2:13" ht="142.5" x14ac:dyDescent="0.25">
@@ -5529,7 +5547,7 @@
       </c>
     </row>
     <row r="92" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B92" s="54" t="s">
+      <c r="B92" s="51" t="s">
         <v>1</v>
       </c>
       <c r="C92" s="42" t="s">
@@ -6350,6 +6368,48 @@
         <v>301</v>
       </c>
       <c r="E157" s="43" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="158" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B158" s="43" t="s">
+        <v>1</v>
+      </c>
+      <c r="C158" s="46" t="s">
+        <v>310</v>
+      </c>
+      <c r="D158" s="46" t="s">
+        <v>307</v>
+      </c>
+      <c r="E158" s="43" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="159" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B159" s="43" t="s">
+        <v>1</v>
+      </c>
+      <c r="C159" s="46" t="s">
+        <v>311</v>
+      </c>
+      <c r="D159" s="46" t="s">
+        <v>308</v>
+      </c>
+      <c r="E159" s="43" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="160" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B160" s="43" t="s">
+        <v>1</v>
+      </c>
+      <c r="C160" s="46" t="s">
+        <v>312</v>
+      </c>
+      <c r="D160" s="46" t="s">
+        <v>309</v>
+      </c>
+      <c r="E160" s="43" t="b">
         <v>1</v>
       </c>
     </row>
@@ -6361,7 +6421,7 @@
     <mergeCell ref="G70:H70"/>
   </mergeCells>
   <conditionalFormatting sqref="C72:E74">
-    <cfRule type="duplicateValues" dxfId="0" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="68" priority="2"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
added two new mission types related to Hungry birthday mode Tournaments
Former-commit-id: 89a58486c281672142f4a74620bace12da61c34f
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Missions.xlsx
+++ b/Docs/Content/HungryDragonContent_Missions.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="550" uniqueCount="313">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="556" uniqueCount="317">
   <si>
     <t>single_run</t>
   </si>
@@ -988,6 +988,18 @@
   </si>
   <si>
     <t>icon_Party_Hat</t>
+  </si>
+  <si>
+    <t>birthday_mode_count</t>
+  </si>
+  <si>
+    <t>TID_EVENT_TOURNAMENT_TIME_LIMIT_HUNGRY_BIRTHDAY_MODE</t>
+  </si>
+  <si>
+    <t>birthday_stay_mode_time</t>
+  </si>
+  <si>
+    <t>TID_EVENT_TOURNAMENT_TIME_LIMIT_STAY_HUNGRY_BIRTHDAY_MODE</t>
   </si>
 </sst>
 </file>
@@ -1441,6 +1453,16 @@
   </cellStyles>
   <dxfs count="69">
     <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
@@ -2591,16 +2613,6 @@
         </bottom>
       </border>
     </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -2615,99 +2627,99 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="missionDifficultyDefinitions" displayName="missionDifficultyDefinitions" ref="B71:L74" totalsRowShown="0" headerRowBorderDxfId="67" tableBorderDxfId="66">
-  <autoFilter ref="B71:L74"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="missionDifficultyDefinitions" displayName="missionDifficultyDefinitions" ref="B73:L76" totalsRowShown="0" headerRowBorderDxfId="68" tableBorderDxfId="67">
+  <autoFilter ref="B73:L76"/>
   <tableColumns count="11">
     <tableColumn id="1" name="{missionDifficultyDefinitions}"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="65"/>
-    <tableColumn id="11" name="[difficulty]" dataDxfId="64"/>
-    <tableColumn id="7" name="[index]" dataDxfId="63"/>
-    <tableColumn id="3" name="[dragonsToUnlock]" dataDxfId="62"/>
-    <tableColumn id="4" name="[cooldownMinutes]" dataDxfId="61"/>
-    <tableColumn id="9" name="[maxRewardCoins]" dataDxfId="60"/>
-    <tableColumn id="5" name="[removeMissionPCCoefA]" dataDxfId="59"/>
-    <tableColumn id="6" name="[removeMissionPCCoefB]" dataDxfId="58"/>
-    <tableColumn id="8" name="[tidName]" dataDxfId="57"/>
-    <tableColumn id="10" name="[color]" dataDxfId="56"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="66"/>
+    <tableColumn id="11" name="[difficulty]" dataDxfId="65"/>
+    <tableColumn id="7" name="[index]" dataDxfId="64"/>
+    <tableColumn id="3" name="[dragonsToUnlock]" dataDxfId="63"/>
+    <tableColumn id="4" name="[cooldownMinutes]" dataDxfId="62"/>
+    <tableColumn id="9" name="[maxRewardCoins]" dataDxfId="61"/>
+    <tableColumn id="5" name="[removeMissionPCCoefA]" dataDxfId="60"/>
+    <tableColumn id="6" name="[removeMissionPCCoefB]" dataDxfId="59"/>
+    <tableColumn id="8" name="[tidName]" dataDxfId="58"/>
+    <tableColumn id="10" name="[color]" dataDxfId="57"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table13303132" displayName="Table13303132" ref="B79:E92" totalsRowShown="0" headerRowDxfId="55" dataDxfId="53" headerRowBorderDxfId="54" tableBorderDxfId="52" totalsRowBorderDxfId="51">
-  <autoFilter ref="B79:E92"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table13303132" displayName="Table13303132" ref="B81:E94" totalsRowShown="0" headerRowDxfId="56" dataDxfId="54" headerRowBorderDxfId="55" tableBorderDxfId="53" totalsRowBorderDxfId="52">
+  <autoFilter ref="B81:E94"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="{missionDragonModifiersDefinitions}" dataDxfId="50"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="49"/>
-    <tableColumn id="7" name="[quantityModifier]" dataDxfId="48"/>
-    <tableColumn id="3" name="[missionSCRewardMultiplier]" dataDxfId="47"/>
+    <tableColumn id="1" name="{missionDragonModifiersDefinitions}" dataDxfId="51"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="50"/>
+    <tableColumn id="7" name="[quantityModifier]" dataDxfId="49"/>
+    <tableColumn id="3" name="[missionSCRewardMultiplier]" dataDxfId="48"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table1330313234" displayName="Table1330313234" ref="B96:E99" totalsRowShown="0" headerRowDxfId="46" dataDxfId="44" headerRowBorderDxfId="45" tableBorderDxfId="43" totalsRowBorderDxfId="42">
-  <autoFilter ref="B96:E99"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table1330313234" displayName="Table1330313234" ref="B98:E101" totalsRowShown="0" headerRowDxfId="47" dataDxfId="45" headerRowBorderDxfId="46" tableBorderDxfId="44" totalsRowBorderDxfId="43">
+  <autoFilter ref="B98:E101"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="{missionDifficultyModifiersDefinitions}" dataDxfId="41"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="40"/>
-    <tableColumn id="3" name="[difficulty]" dataDxfId="39"/>
-    <tableColumn id="7" name="[quantityModifier]" dataDxfId="38"/>
+    <tableColumn id="1" name="{missionDifficultyModifiersDefinitions}" dataDxfId="42"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="41"/>
+    <tableColumn id="3" name="[difficulty]" dataDxfId="40"/>
+    <tableColumn id="7" name="[quantityModifier]" dataDxfId="39"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table133031323435" displayName="Table133031323435" ref="B103:D104" totalsRowShown="0" headerRowDxfId="37" dataDxfId="35" headerRowBorderDxfId="36" tableBorderDxfId="34" totalsRowBorderDxfId="33">
-  <autoFilter ref="B103:D104"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table133031323435" displayName="Table133031323435" ref="B105:D106" totalsRowShown="0" headerRowDxfId="38" dataDxfId="36" headerRowBorderDxfId="37" tableBorderDxfId="35" totalsRowBorderDxfId="34">
+  <autoFilter ref="B105:D106"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="{missionOtherModifiersDefinitions}" dataDxfId="32"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="31"/>
-    <tableColumn id="7" name="[quantityModifier]" dataDxfId="30"/>
+    <tableColumn id="1" name="{missionOtherModifiersDefinitions}" dataDxfId="33"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="32"/>
+    <tableColumn id="7" name="[quantityModifier]" dataDxfId="31"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table13" displayName="Table13" ref="B48:H67" totalsRowShown="0" headerRowDxfId="29" dataDxfId="27" headerRowBorderDxfId="28" tableBorderDxfId="26" totalsRowBorderDxfId="25">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table13" displayName="Table13" ref="B48:H67" totalsRowShown="0" headerRowDxfId="30" dataDxfId="28" headerRowBorderDxfId="29" tableBorderDxfId="27" totalsRowBorderDxfId="26">
   <autoFilter ref="B48:H67"/>
   <tableColumns count="7">
-    <tableColumn id="1" name="{missionTypeDefinitions}" dataDxfId="24"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="23"/>
-    <tableColumn id="3" name="[minTier]" dataDxfId="22"/>
-    <tableColumn id="6" name="[maxTier]" dataDxfId="21"/>
-    <tableColumn id="4" name="[weight]" dataDxfId="20"/>
-    <tableColumn id="9" name="[tidDescSingleRun]" dataDxfId="19"/>
-    <tableColumn id="10" name="[tidDescMultiRun]" dataDxfId="18"/>
+    <tableColumn id="1" name="{missionTypeDefinitions}" dataDxfId="25"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="24"/>
+    <tableColumn id="3" name="[minTier]" dataDxfId="23"/>
+    <tableColumn id="6" name="[maxTier]" dataDxfId="22"/>
+    <tableColumn id="4" name="[weight]" dataDxfId="21"/>
+    <tableColumn id="9" name="[tidDescSingleRun]" dataDxfId="20"/>
+    <tableColumn id="10" name="[tidDescMultiRun]" dataDxfId="19"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table1330" displayName="Table1330" ref="B4:N43" totalsRowShown="0" headerRowDxfId="17" dataDxfId="15" headerRowBorderDxfId="16" tableBorderDxfId="14" totalsRowBorderDxfId="13">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table1330" displayName="Table1330" ref="B4:N43" totalsRowShown="0" headerRowDxfId="18" dataDxfId="16" headerRowBorderDxfId="17" tableBorderDxfId="15" totalsRowBorderDxfId="14">
   <autoFilter ref="B4:N43"/>
   <sortState ref="B5:P43">
     <sortCondition descending="1" ref="J4:J43"/>
   </sortState>
   <tableColumns count="13">
-    <tableColumn id="1" name="{missionsDefinitions}" dataDxfId="12"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="11"/>
-    <tableColumn id="7" name="[type]" dataDxfId="10"/>
-    <tableColumn id="8" name="[weight]" dataDxfId="9"/>
-    <tableColumn id="13" name="[singleRunChance]" dataDxfId="8"/>
-    <tableColumn id="11" name="[minTier]" dataDxfId="7"/>
-    <tableColumn id="12" name="[maxTier]" dataDxfId="6"/>
-    <tableColumn id="6" name="[params]" dataDxfId="5"/>
-    <tableColumn id="3" name="[objectiveBaseQuantityMin]" dataDxfId="4"/>
-    <tableColumn id="9" name="[objectiveBaseQuantityMax]" dataDxfId="3"/>
-    <tableColumn id="4" name="[icon]" dataDxfId="2"/>
-    <tableColumn id="5" name="[tidObjective]" dataDxfId="1"/>
-    <tableColumn id="10" name="[trackingSku]" dataDxfId="0">
+    <tableColumn id="1" name="{missionsDefinitions}" dataDxfId="13"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="12"/>
+    <tableColumn id="7" name="[type]" dataDxfId="11"/>
+    <tableColumn id="8" name="[weight]" dataDxfId="10"/>
+    <tableColumn id="13" name="[singleRunChance]" dataDxfId="9"/>
+    <tableColumn id="11" name="[minTier]" dataDxfId="8"/>
+    <tableColumn id="12" name="[maxTier]" dataDxfId="7"/>
+    <tableColumn id="6" name="[params]" dataDxfId="6"/>
+    <tableColumn id="3" name="[objectiveBaseQuantityMin]" dataDxfId="5"/>
+    <tableColumn id="9" name="[objectiveBaseQuantityMax]" dataDxfId="4"/>
+    <tableColumn id="4" name="[icon]" dataDxfId="3"/>
+    <tableColumn id="5" name="[tidObjective]" dataDxfId="2"/>
+    <tableColumn id="10" name="[trackingSku]" dataDxfId="1">
       <calculatedColumnFormula>Table1330[[#This Row],['[sku']]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2981,10 +2993,10 @@
   <sheetPr>
     <tabColor theme="6"/>
   </sheetPr>
-  <dimension ref="B1:P160"/>
+  <dimension ref="B1:P162"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A130" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C161" sqref="C161"/>
+    <sheetView tabSelected="1" topLeftCell="B49" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C69" sqref="C69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5182,140 +5194,112 @@
         <v>211</v>
       </c>
     </row>
-    <row r="68" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="69" spans="2:13" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B69" s="6" t="s">
+    <row r="68" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B68" s="27" t="s">
+        <v>1</v>
+      </c>
+      <c r="C68" s="24" t="s">
+        <v>313</v>
+      </c>
+      <c r="D68" s="24">
+        <v>0</v>
+      </c>
+      <c r="E68" s="24">
+        <v>7</v>
+      </c>
+      <c r="F68" s="24">
+        <v>1</v>
+      </c>
+      <c r="G68" s="26" t="s">
+        <v>314</v>
+      </c>
+      <c r="H68" s="26"/>
+    </row>
+    <row r="69" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B69" s="27" t="s">
+        <v>1</v>
+      </c>
+      <c r="C69" s="24" t="s">
+        <v>315</v>
+      </c>
+      <c r="D69" s="24">
+        <v>0</v>
+      </c>
+      <c r="E69" s="24">
+        <v>7</v>
+      </c>
+      <c r="F69" s="24">
+        <v>1</v>
+      </c>
+      <c r="G69" s="26" t="s">
+        <v>316</v>
+      </c>
+      <c r="H69" s="26"/>
+    </row>
+    <row r="70" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="71" spans="2:13" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B71" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="C69" s="6"/>
-      <c r="D69" s="6"/>
-      <c r="E69" s="6"/>
-      <c r="F69" s="6"/>
-      <c r="G69" s="6"/>
-      <c r="H69" s="6"/>
-      <c r="I69" s="6"/>
-      <c r="J69" s="6"/>
-      <c r="K69" s="6"/>
-      <c r="L69" s="6"/>
-      <c r="M69" s="6"/>
-    </row>
-    <row r="70" spans="2:13" ht="60" x14ac:dyDescent="0.25">
-      <c r="B70" s="20"/>
-      <c r="C70" s="20"/>
-      <c r="D70" s="20"/>
-      <c r="E70" s="20"/>
-      <c r="F70" s="21" t="s">
+      <c r="C71" s="6"/>
+      <c r="D71" s="6"/>
+      <c r="E71" s="6"/>
+      <c r="F71" s="6"/>
+      <c r="G71" s="6"/>
+      <c r="H71" s="6"/>
+      <c r="I71" s="6"/>
+      <c r="J71" s="6"/>
+      <c r="K71" s="6"/>
+      <c r="L71" s="6"/>
+      <c r="M71" s="6"/>
+    </row>
+    <row r="72" spans="2:13" ht="60" x14ac:dyDescent="0.25">
+      <c r="B72" s="20"/>
+      <c r="C72" s="20"/>
+      <c r="D72" s="20"/>
+      <c r="E72" s="20"/>
+      <c r="F72" s="21" t="s">
         <v>40</v>
       </c>
-      <c r="G70" s="54" t="s">
+      <c r="G72" s="54" t="s">
         <v>39</v>
       </c>
-      <c r="H70" s="54"/>
-      <c r="I70" s="20"/>
-    </row>
-    <row r="71" spans="2:13" ht="142.5" x14ac:dyDescent="0.25">
-      <c r="B71" s="19" t="s">
+      <c r="H72" s="54"/>
+      <c r="I72" s="20"/>
+    </row>
+    <row r="73" spans="2:13" ht="142.5" x14ac:dyDescent="0.25">
+      <c r="B73" s="19" t="s">
         <v>38</v>
       </c>
-      <c r="C71" s="19" t="s">
+      <c r="C73" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="D71" s="18" t="s">
+      <c r="D73" s="18" t="s">
         <v>224</v>
       </c>
-      <c r="E71" s="18" t="s">
+      <c r="E73" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="F71" s="17" t="s">
+      <c r="F73" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="G71" s="17" t="s">
+      <c r="G73" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="H71" s="17" t="s">
+      <c r="H73" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="I71" s="16" t="s">
+      <c r="I73" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="J71" s="16" t="s">
+      <c r="J73" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="K71" s="15" t="s">
+      <c r="K73" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="L71" s="14" t="s">
+      <c r="L73" s="14" t="s">
         <v>30</v>
-      </c>
-    </row>
-    <row r="72" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B72" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="C72" s="11" t="s">
-        <v>221</v>
-      </c>
-      <c r="D72" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="E72" s="11">
-        <v>0</v>
-      </c>
-      <c r="F72" s="10">
-        <v>0</v>
-      </c>
-      <c r="G72" s="10">
-        <v>15</v>
-      </c>
-      <c r="H72" s="10">
-        <v>200</v>
-      </c>
-      <c r="I72" s="9">
-        <v>0.5</v>
-      </c>
-      <c r="J72" s="9">
-        <v>1</v>
-      </c>
-      <c r="K72" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="L72" s="13" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="73" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B73" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="C73" s="11" t="s">
-        <v>222</v>
-      </c>
-      <c r="D73" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="E73" s="11">
-        <v>1</v>
-      </c>
-      <c r="F73" s="10">
-        <v>0</v>
-      </c>
-      <c r="G73" s="10">
-        <v>60</v>
-      </c>
-      <c r="H73" s="10">
-        <v>300</v>
-      </c>
-      <c r="I73" s="9">
-        <v>0.5</v>
-      </c>
-      <c r="J73" s="9">
-        <v>1</v>
-      </c>
-      <c r="K73" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="L73" s="13" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="74" spans="2:13" x14ac:dyDescent="0.25">
@@ -5323,22 +5307,22 @@
         <v>1</v>
       </c>
       <c r="C74" s="11" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="D74" s="11" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="E74" s="11">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F74" s="10">
         <v>0</v>
       </c>
       <c r="G74" s="10">
-        <v>240</v>
+        <v>15</v>
       </c>
       <c r="H74" s="10">
-        <v>600</v>
+        <v>200</v>
       </c>
       <c r="I74" s="9">
         <v>0.5</v>
@@ -5347,63 +5331,105 @@
         <v>1</v>
       </c>
       <c r="K74" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="L74" s="13" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="75" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B75" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="C75" s="11" t="s">
+        <v>222</v>
+      </c>
+      <c r="D75" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="E75" s="11">
+        <v>1</v>
+      </c>
+      <c r="F75" s="10">
+        <v>0</v>
+      </c>
+      <c r="G75" s="10">
+        <v>60</v>
+      </c>
+      <c r="H75" s="10">
+        <v>300</v>
+      </c>
+      <c r="I75" s="9">
+        <v>0.5</v>
+      </c>
+      <c r="J75" s="9">
+        <v>1</v>
+      </c>
+      <c r="K75" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="L75" s="13" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="76" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B76" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="C76" s="11" t="s">
+        <v>223</v>
+      </c>
+      <c r="D76" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="E76" s="11">
+        <v>2</v>
+      </c>
+      <c r="F76" s="10">
+        <v>0</v>
+      </c>
+      <c r="G76" s="10">
+        <v>240</v>
+      </c>
+      <c r="H76" s="10">
+        <v>600</v>
+      </c>
+      <c r="I76" s="9">
+        <v>0.5</v>
+      </c>
+      <c r="J76" s="9">
+        <v>1</v>
+      </c>
+      <c r="K76" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="L74" s="7" t="s">
+      <c r="L76" s="7" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="76" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="77" spans="2:13" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B77" s="6" t="s">
+    <row r="78" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="79" spans="2:13" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B79" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="C77" s="6"/>
-      <c r="D77" s="6"/>
-      <c r="E77" s="6"/>
-      <c r="F77" s="6"/>
-      <c r="G77" s="6"/>
-    </row>
-    <row r="79" spans="2:13" ht="135.75" x14ac:dyDescent="0.25">
-      <c r="B79" s="5" t="s">
+      <c r="C79" s="6"/>
+      <c r="D79" s="6"/>
+      <c r="E79" s="6"/>
+      <c r="F79" s="6"/>
+      <c r="G79" s="6"/>
+    </row>
+    <row r="81" spans="2:7" ht="135.75" x14ac:dyDescent="0.25">
+      <c r="B81" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="C79" s="4" t="s">
+      <c r="C81" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D79" s="3" t="s">
+      <c r="D81" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E79" s="3" t="s">
+      <c r="E81" s="3" t="s">
         <v>21</v>
-      </c>
-    </row>
-    <row r="80" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B80" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C80" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D80" s="1">
-        <v>0.1</v>
-      </c>
-      <c r="E80" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="81" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B81" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C81" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D81" s="1">
-        <v>0.7</v>
-      </c>
-      <c r="E81" s="1">
-        <v>6</v>
       </c>
     </row>
     <row r="82" spans="2:7" x14ac:dyDescent="0.25">
@@ -5411,13 +5437,13 @@
         <v>1</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D82" s="1">
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="E82" s="1">
-        <v>12</v>
+        <v>2</v>
       </c>
     </row>
     <row r="83" spans="2:7" x14ac:dyDescent="0.25">
@@ -5425,13 +5451,13 @@
         <v>1</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D83" s="1">
-        <v>1.5</v>
+        <v>0.7</v>
       </c>
       <c r="E83" s="1">
-        <v>18</v>
+        <v>6</v>
       </c>
     </row>
     <row r="84" spans="2:7" x14ac:dyDescent="0.25">
@@ -5439,13 +5465,13 @@
         <v>1</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D84" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E84" s="1">
-        <v>26</v>
+        <v>12</v>
       </c>
     </row>
     <row r="85" spans="2:7" x14ac:dyDescent="0.25">
@@ -5453,13 +5479,13 @@
         <v>1</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D85" s="1">
-        <v>2.5</v>
+        <v>1.5</v>
       </c>
       <c r="E85" s="1">
-        <v>35</v>
+        <v>18</v>
       </c>
     </row>
     <row r="86" spans="2:7" x14ac:dyDescent="0.25">
@@ -5467,13 +5493,13 @@
         <v>1</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D86" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E86" s="1">
-        <v>45</v>
+        <v>26</v>
       </c>
     </row>
     <row r="87" spans="2:7" x14ac:dyDescent="0.25">
@@ -5481,13 +5507,13 @@
         <v>1</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D87" s="1">
-        <v>4</v>
+        <v>2.5</v>
       </c>
       <c r="E87" s="1">
-        <v>56</v>
+        <v>35</v>
       </c>
     </row>
     <row r="88" spans="2:7" x14ac:dyDescent="0.25">
@@ -5495,13 +5521,13 @@
         <v>1</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>215</v>
+        <v>14</v>
       </c>
       <c r="D88" s="1">
-        <v>4.5</v>
+        <v>3</v>
       </c>
       <c r="E88" s="1">
-        <v>62</v>
+        <v>45</v>
       </c>
     </row>
     <row r="89" spans="2:7" x14ac:dyDescent="0.25">
@@ -5509,13 +5535,13 @@
         <v>1</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D89" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E89" s="1">
-        <v>67</v>
+        <v>56</v>
       </c>
     </row>
     <row r="90" spans="2:7" x14ac:dyDescent="0.25">
@@ -5523,13 +5549,13 @@
         <v>1</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>11</v>
+        <v>215</v>
       </c>
       <c r="D90" s="1">
-        <v>7</v>
+        <v>4.5</v>
       </c>
       <c r="E90" s="1">
-        <v>80</v>
+        <v>62</v>
       </c>
     </row>
     <row r="91" spans="2:7" x14ac:dyDescent="0.25">
@@ -5537,80 +5563,80 @@
         <v>1</v>
       </c>
       <c r="C91" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D91" s="1">
+        <v>5</v>
+      </c>
+      <c r="E91" s="1">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="92" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B92" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C92" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D92" s="1">
+        <v>7</v>
+      </c>
+      <c r="E92" s="1">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="93" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B93" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C93" s="1" t="s">
         <v>220</v>
       </c>
-      <c r="D91" s="42">
+      <c r="D93" s="42">
         <v>7.5</v>
       </c>
-      <c r="E91" s="1">
+      <c r="E93" s="1">
         <v>85</v>
       </c>
     </row>
-    <row r="92" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B92" s="51" t="s">
-        <v>1</v>
-      </c>
-      <c r="C92" s="42" t="s">
+    <row r="94" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B94" s="51" t="s">
+        <v>1</v>
+      </c>
+      <c r="C94" s="42" t="s">
         <v>306</v>
       </c>
-      <c r="D92" s="42">
+      <c r="D94" s="42">
         <v>8</v>
       </c>
-      <c r="E92" s="42">
+      <c r="E94" s="42">
         <v>90</v>
       </c>
     </row>
-    <row r="93" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="94" spans="2:7" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B94" s="6" t="s">
+    <row r="95" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="96" spans="2:7" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B96" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C94" s="6"/>
-      <c r="D94" s="6"/>
-      <c r="E94" s="6"/>
-      <c r="F94" s="6"/>
-      <c r="G94" s="6"/>
-    </row>
-    <row r="96" spans="2:7" ht="142.5" x14ac:dyDescent="0.25">
-      <c r="B96" s="5" t="s">
+      <c r="C96" s="6"/>
+      <c r="D96" s="6"/>
+      <c r="E96" s="6"/>
+      <c r="F96" s="6"/>
+      <c r="G96" s="6"/>
+    </row>
+    <row r="98" spans="2:7" ht="142.5" x14ac:dyDescent="0.25">
+      <c r="B98" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C96" s="4" t="s">
+      <c r="C98" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D96" s="4" t="s">
+      <c r="D98" s="4" t="s">
         <v>224</v>
       </c>
-      <c r="E96" s="3" t="s">
+      <c r="E98" s="3" t="s">
         <v>2</v>
-      </c>
-    </row>
-    <row r="97" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B97" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C97" s="1" t="s">
-        <v>225</v>
-      </c>
-      <c r="D97" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E97" s="1">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="98" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B98" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C98" s="1" t="s">
-        <v>226</v>
-      </c>
-      <c r="D98" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E98" s="1">
-        <v>0.1</v>
       </c>
     </row>
     <row r="99" spans="2:7" x14ac:dyDescent="0.25">
@@ -5618,99 +5644,99 @@
         <v>1</v>
       </c>
       <c r="C99" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="D99" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E99" s="1">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="100" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B100" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C100" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="D100" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E100" s="1">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="101" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B101" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C101" s="1" t="s">
         <v>227</v>
       </c>
-      <c r="D99" s="1" t="s">
+      <c r="D101" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E99" s="1">
+      <c r="E101" s="1">
         <v>0.2</v>
       </c>
     </row>
-    <row r="100" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="101" spans="2:7" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B101" s="6" t="s">
+    <row r="102" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="103" spans="2:7" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B103" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C101" s="6"/>
-      <c r="D101" s="6"/>
-      <c r="E101" s="6"/>
-      <c r="F101" s="6"/>
-      <c r="G101" s="6"/>
-    </row>
-    <row r="103" spans="2:7" ht="132" x14ac:dyDescent="0.25">
-      <c r="B103" s="5" t="s">
+      <c r="C103" s="6"/>
+      <c r="D103" s="6"/>
+      <c r="E103" s="6"/>
+      <c r="F103" s="6"/>
+      <c r="G103" s="6"/>
+    </row>
+    <row r="105" spans="2:7" ht="132" x14ac:dyDescent="0.25">
+      <c r="B105" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C103" s="4" t="s">
+      <c r="C105" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D103" s="3" t="s">
+      <c r="D105" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="104" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B104" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C104" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D104" s="1">
+    <row r="106" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B106" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C106" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D106" s="1">
         <v>0.7</v>
       </c>
     </row>
-    <row r="105" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="106" spans="2:7" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B106" s="6" t="s">
+    <row r="107" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="108" spans="2:7" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B108" s="6" t="s">
         <v>240</v>
       </c>
-      <c r="C106" s="6"/>
-      <c r="D106" s="6"/>
-      <c r="E106" s="6"/>
-      <c r="F106" s="6"/>
-      <c r="G106" s="6"/>
-    </row>
-    <row r="108" spans="2:7" ht="68.25" x14ac:dyDescent="0.25">
-      <c r="B108" s="44" t="s">
+      <c r="C108" s="6"/>
+      <c r="D108" s="6"/>
+      <c r="E108" s="6"/>
+      <c r="F108" s="6"/>
+      <c r="G108" s="6"/>
+    </row>
+    <row r="110" spans="2:7" ht="68.25" x14ac:dyDescent="0.25">
+      <c r="B110" s="44" t="s">
         <v>241</v>
       </c>
-      <c r="C108" s="44" t="s">
+      <c r="C110" s="44" t="s">
         <v>3</v>
       </c>
-      <c r="D108" s="45" t="s">
+      <c r="D110" s="45" t="s">
         <v>242</v>
       </c>
-      <c r="E108" s="45" t="s">
+      <c r="E110" s="45" t="s">
         <v>243</v>
-      </c>
-    </row>
-    <row r="109" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B109" s="43" t="s">
-        <v>1</v>
-      </c>
-      <c r="C109" s="46" t="s">
-        <v>80</v>
-      </c>
-      <c r="D109" s="46" t="s">
-        <v>264</v>
-      </c>
-      <c r="E109" s="43" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="110" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B110" s="43" t="s">
-        <v>1</v>
-      </c>
-      <c r="C110" s="46" t="s">
-        <v>93</v>
-      </c>
-      <c r="D110" s="46" t="s">
-        <v>265</v>
-      </c>
-      <c r="E110" s="43" t="b">
-        <v>1</v>
       </c>
     </row>
     <row r="111" spans="2:7" x14ac:dyDescent="0.25">
@@ -5718,10 +5744,10 @@
         <v>1</v>
       </c>
       <c r="C111" s="46" t="s">
-        <v>125</v>
+        <v>80</v>
       </c>
       <c r="D111" s="46" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="E111" s="43" t="b">
         <v>1</v>
@@ -5732,13 +5758,13 @@
         <v>1</v>
       </c>
       <c r="C112" s="46" t="s">
-        <v>109</v>
+        <v>93</v>
       </c>
       <c r="D112" s="46" t="s">
-        <v>109</v>
+        <v>265</v>
       </c>
       <c r="E112" s="43" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="113" spans="2:5" x14ac:dyDescent="0.25">
@@ -5746,13 +5772,13 @@
         <v>1</v>
       </c>
       <c r="C113" s="46" t="s">
-        <v>121</v>
+        <v>125</v>
       </c>
       <c r="D113" s="46" t="s">
-        <v>121</v>
+        <v>266</v>
       </c>
       <c r="E113" s="43" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="114" spans="2:5" x14ac:dyDescent="0.25">
@@ -5760,10 +5786,10 @@
         <v>1</v>
       </c>
       <c r="C114" s="46" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D114" s="46" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E114" s="43" t="b">
         <v>0</v>
@@ -5774,13 +5800,13 @@
         <v>1</v>
       </c>
       <c r="C115" s="46" t="s">
-        <v>112</v>
+        <v>121</v>
       </c>
       <c r="D115" s="46" t="s">
-        <v>267</v>
+        <v>121</v>
       </c>
       <c r="E115" s="43" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="116" spans="2:5" x14ac:dyDescent="0.25">
@@ -5788,13 +5814,13 @@
         <v>1</v>
       </c>
       <c r="C116" s="46" t="s">
-        <v>244</v>
+        <v>110</v>
       </c>
       <c r="D116" s="46" t="s">
-        <v>268</v>
+        <v>110</v>
       </c>
       <c r="E116" s="43" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="117" spans="2:5" x14ac:dyDescent="0.25">
@@ -5802,10 +5828,10 @@
         <v>1</v>
       </c>
       <c r="C117" s="46" t="s">
-        <v>245</v>
+        <v>112</v>
       </c>
       <c r="D117" s="46" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="E117" s="43" t="b">
         <v>1</v>
@@ -5816,10 +5842,10 @@
         <v>1</v>
       </c>
       <c r="C118" s="46" t="s">
-        <v>205</v>
+        <v>244</v>
       </c>
       <c r="D118" s="46" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="E118" s="43" t="b">
         <v>1</v>
@@ -5830,10 +5856,10 @@
         <v>1</v>
       </c>
       <c r="C119" s="46" t="s">
-        <v>204</v>
+        <v>245</v>
       </c>
       <c r="D119" s="46" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="E119" s="43" t="b">
         <v>1</v>
@@ -5844,10 +5870,10 @@
         <v>1</v>
       </c>
       <c r="C120" s="46" t="s">
-        <v>199</v>
+        <v>205</v>
       </c>
       <c r="D120" s="46" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="E120" s="43" t="b">
         <v>1</v>
@@ -5858,10 +5884,10 @@
         <v>1</v>
       </c>
       <c r="C121" s="46" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="D121" s="46" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="E121" s="43" t="b">
         <v>1</v>
@@ -5872,10 +5898,10 @@
         <v>1</v>
       </c>
       <c r="C122" s="46" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="D122" s="46" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="E122" s="43" t="b">
         <v>1</v>
@@ -5886,10 +5912,10 @@
         <v>1</v>
       </c>
       <c r="C123" s="46" t="s">
-        <v>200</v>
+        <v>203</v>
       </c>
       <c r="D123" s="46" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="E123" s="43" t="b">
         <v>1</v>
@@ -5900,10 +5926,10 @@
         <v>1</v>
       </c>
       <c r="C124" s="46" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="D124" s="46" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="E124" s="43" t="b">
         <v>1</v>
@@ -5914,10 +5940,10 @@
         <v>1</v>
       </c>
       <c r="C125" s="46" t="s">
-        <v>114</v>
+        <v>200</v>
       </c>
       <c r="D125" s="46" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="E125" s="43" t="b">
         <v>1</v>
@@ -5928,13 +5954,13 @@
         <v>1</v>
       </c>
       <c r="C126" s="46" t="s">
-        <v>246</v>
+        <v>201</v>
       </c>
       <c r="D126" s="46" t="s">
-        <v>246</v>
+        <v>276</v>
       </c>
       <c r="E126" s="43" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="127" spans="2:5" x14ac:dyDescent="0.25">
@@ -5942,10 +5968,10 @@
         <v>1</v>
       </c>
       <c r="C127" s="46" t="s">
-        <v>83</v>
+        <v>114</v>
       </c>
       <c r="D127" s="46" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="E127" s="43" t="b">
         <v>1</v>
@@ -5956,13 +5982,13 @@
         <v>1</v>
       </c>
       <c r="C128" s="46" t="s">
-        <v>96</v>
+        <v>246</v>
       </c>
       <c r="D128" s="46" t="s">
-        <v>279</v>
+        <v>246</v>
       </c>
       <c r="E128" s="43" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="129" spans="2:5" x14ac:dyDescent="0.25">
@@ -5970,10 +5996,10 @@
         <v>1</v>
       </c>
       <c r="C129" s="46" t="s">
-        <v>247</v>
+        <v>83</v>
       </c>
       <c r="D129" s="46" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="E129" s="43" t="b">
         <v>1</v>
@@ -5984,10 +6010,10 @@
         <v>1</v>
       </c>
       <c r="C130" s="46" t="s">
-        <v>248</v>
+        <v>96</v>
       </c>
       <c r="D130" s="46" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="E130" s="43" t="b">
         <v>1</v>
@@ -5998,10 +6024,10 @@
         <v>1</v>
       </c>
       <c r="C131" s="46" t="s">
-        <v>102</v>
+        <v>247</v>
       </c>
       <c r="D131" s="46" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="E131" s="43" t="b">
         <v>1</v>
@@ -6012,10 +6038,10 @@
         <v>1</v>
       </c>
       <c r="C132" s="46" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D132" s="46" t="s">
-        <v>304</v>
+        <v>281</v>
       </c>
       <c r="E132" s="43" t="b">
         <v>1</v>
@@ -6026,10 +6052,10 @@
         <v>1</v>
       </c>
       <c r="C133" s="46" t="s">
-        <v>123</v>
+        <v>102</v>
       </c>
       <c r="D133" s="46" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="E133" s="43" t="b">
         <v>1</v>
@@ -6040,10 +6066,10 @@
         <v>1</v>
       </c>
       <c r="C134" s="46" t="s">
-        <v>88</v>
+        <v>249</v>
       </c>
       <c r="D134" s="46" t="s">
-        <v>284</v>
+        <v>304</v>
       </c>
       <c r="E134" s="43" t="b">
         <v>1</v>
@@ -6054,10 +6080,10 @@
         <v>1</v>
       </c>
       <c r="C135" s="46" t="s">
-        <v>250</v>
+        <v>123</v>
       </c>
       <c r="D135" s="46" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="E135" s="43" t="b">
         <v>1</v>
@@ -6068,10 +6094,10 @@
         <v>1</v>
       </c>
       <c r="C136" s="46" t="s">
-        <v>302</v>
+        <v>88</v>
       </c>
       <c r="D136" s="46" t="s">
-        <v>303</v>
+        <v>284</v>
       </c>
       <c r="E136" s="43" t="b">
         <v>1</v>
@@ -6082,13 +6108,13 @@
         <v>1</v>
       </c>
       <c r="C137" s="46" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="D137" s="46" t="s">
-        <v>251</v>
+        <v>285</v>
       </c>
       <c r="E137" s="43" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="138" spans="2:5" x14ac:dyDescent="0.25">
@@ -6096,13 +6122,13 @@
         <v>1</v>
       </c>
       <c r="C138" s="46" t="s">
-        <v>116</v>
+        <v>302</v>
       </c>
       <c r="D138" s="46" t="s">
-        <v>116</v>
+        <v>303</v>
       </c>
       <c r="E138" s="43" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="139" spans="2:5" x14ac:dyDescent="0.25">
@@ -6110,13 +6136,13 @@
         <v>1</v>
       </c>
       <c r="C139" s="46" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="D139" s="46" t="s">
-        <v>286</v>
+        <v>251</v>
       </c>
       <c r="E139" s="43" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="140" spans="2:5" x14ac:dyDescent="0.25">
@@ -6124,13 +6150,13 @@
         <v>1</v>
       </c>
       <c r="C140" s="46" t="s">
-        <v>91</v>
+        <v>116</v>
       </c>
       <c r="D140" s="46" t="s">
-        <v>287</v>
+        <v>116</v>
       </c>
       <c r="E140" s="43" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="141" spans="2:5" x14ac:dyDescent="0.25">
@@ -6138,10 +6164,10 @@
         <v>1</v>
       </c>
       <c r="C141" s="46" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="D141" s="46" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="E141" s="43" t="b">
         <v>1</v>
@@ -6152,10 +6178,10 @@
         <v>1</v>
       </c>
       <c r="C142" s="46" t="s">
-        <v>254</v>
+        <v>91</v>
       </c>
       <c r="D142" s="46" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="E142" s="43" t="b">
         <v>1</v>
@@ -6166,10 +6192,10 @@
         <v>1</v>
       </c>
       <c r="C143" s="46" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="D143" s="46" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="E143" s="43" t="b">
         <v>1</v>
@@ -6180,10 +6206,10 @@
         <v>1</v>
       </c>
       <c r="C144" s="46" t="s">
-        <v>86</v>
+        <v>254</v>
       </c>
       <c r="D144" s="46" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="E144" s="43" t="b">
         <v>1</v>
@@ -6194,13 +6220,13 @@
         <v>1</v>
       </c>
       <c r="C145" s="46" t="s">
-        <v>73</v>
+        <v>255</v>
       </c>
       <c r="D145" s="46" t="s">
-        <v>73</v>
+        <v>290</v>
       </c>
       <c r="E145" s="43" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="146" spans="2:5" x14ac:dyDescent="0.25">
@@ -6208,13 +6234,13 @@
         <v>1</v>
       </c>
       <c r="C146" s="46" t="s">
-        <v>108</v>
+        <v>86</v>
       </c>
       <c r="D146" s="46" t="s">
-        <v>108</v>
+        <v>291</v>
       </c>
       <c r="E146" s="43" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="147" spans="2:5" x14ac:dyDescent="0.25">
@@ -6222,13 +6248,13 @@
         <v>1</v>
       </c>
       <c r="C147" s="46" t="s">
-        <v>256</v>
+        <v>73</v>
       </c>
       <c r="D147" s="46" t="s">
-        <v>292</v>
+        <v>73</v>
       </c>
       <c r="E147" s="43" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="148" spans="2:5" x14ac:dyDescent="0.25">
@@ -6236,13 +6262,13 @@
         <v>1</v>
       </c>
       <c r="C148" s="46" t="s">
-        <v>257</v>
+        <v>108</v>
       </c>
       <c r="D148" s="46" t="s">
-        <v>293</v>
+        <v>108</v>
       </c>
       <c r="E148" s="43" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="149" spans="2:5" x14ac:dyDescent="0.25">
@@ -6250,10 +6276,10 @@
         <v>1</v>
       </c>
       <c r="C149" s="46" t="s">
-        <v>77</v>
+        <v>256</v>
       </c>
       <c r="D149" s="46" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="E149" s="43" t="b">
         <v>1</v>
@@ -6264,10 +6290,10 @@
         <v>1</v>
       </c>
       <c r="C150" s="46" t="s">
-        <v>105</v>
+        <v>257</v>
       </c>
       <c r="D150" s="46" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="E150" s="43" t="b">
         <v>1</v>
@@ -6278,10 +6304,10 @@
         <v>1</v>
       </c>
       <c r="C151" s="46" t="s">
-        <v>258</v>
+        <v>77</v>
       </c>
       <c r="D151" s="46" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="E151" s="43" t="b">
         <v>1</v>
@@ -6292,10 +6318,10 @@
         <v>1</v>
       </c>
       <c r="C152" s="46" t="s">
-        <v>259</v>
+        <v>105</v>
       </c>
       <c r="D152" s="46" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="E152" s="43" t="b">
         <v>1</v>
@@ -6306,10 +6332,10 @@
         <v>1</v>
       </c>
       <c r="C153" s="46" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="D153" s="46" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="E153" s="43" t="b">
         <v>1</v>
@@ -6320,13 +6346,13 @@
         <v>1</v>
       </c>
       <c r="C154" s="46" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="D154" s="46" t="s">
-        <v>261</v>
+        <v>297</v>
       </c>
       <c r="E154" s="43" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="155" spans="2:5" x14ac:dyDescent="0.25">
@@ -6334,10 +6360,10 @@
         <v>1</v>
       </c>
       <c r="C155" s="46" t="s">
-        <v>99</v>
+        <v>260</v>
       </c>
       <c r="D155" s="46" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="E155" s="43" t="b">
         <v>1</v>
@@ -6348,13 +6374,13 @@
         <v>1</v>
       </c>
       <c r="C156" s="46" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="D156" s="46" t="s">
-        <v>300</v>
+        <v>261</v>
       </c>
       <c r="E156" s="43" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="157" spans="2:5" x14ac:dyDescent="0.25">
@@ -6362,10 +6388,10 @@
         <v>1</v>
       </c>
       <c r="C157" s="46" t="s">
-        <v>263</v>
+        <v>99</v>
       </c>
       <c r="D157" s="46" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="E157" s="43" t="b">
         <v>1</v>
@@ -6376,10 +6402,10 @@
         <v>1</v>
       </c>
       <c r="C158" s="46" t="s">
-        <v>310</v>
+        <v>262</v>
       </c>
       <c r="D158" s="46" t="s">
-        <v>307</v>
+        <v>300</v>
       </c>
       <c r="E158" s="43" t="b">
         <v>1</v>
@@ -6390,10 +6416,10 @@
         <v>1</v>
       </c>
       <c r="C159" s="46" t="s">
-        <v>311</v>
+        <v>263</v>
       </c>
       <c r="D159" s="46" t="s">
-        <v>308</v>
+        <v>301</v>
       </c>
       <c r="E159" s="43" t="b">
         <v>1</v>
@@ -6404,12 +6430,40 @@
         <v>1</v>
       </c>
       <c r="C160" s="46" t="s">
+        <v>310</v>
+      </c>
+      <c r="D160" s="46" t="s">
+        <v>307</v>
+      </c>
+      <c r="E160" s="43" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="161" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B161" s="43" t="s">
+        <v>1</v>
+      </c>
+      <c r="C161" s="46" t="s">
+        <v>311</v>
+      </c>
+      <c r="D161" s="46" t="s">
+        <v>308</v>
+      </c>
+      <c r="E161" s="43" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="162" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B162" s="43" t="s">
+        <v>1</v>
+      </c>
+      <c r="C162" s="46" t="s">
         <v>312</v>
       </c>
-      <c r="D160" s="46" t="s">
+      <c r="D162" s="46" t="s">
         <v>309</v>
       </c>
-      <c r="E160" s="43" t="b">
+      <c r="E162" s="43" t="b">
         <v>1</v>
       </c>
     </row>
@@ -6418,10 +6472,10 @@
     <mergeCell ref="J3:K3"/>
     <mergeCell ref="M3:P3"/>
     <mergeCell ref="F47:H47"/>
-    <mergeCell ref="G70:H70"/>
+    <mergeCell ref="G72:H72"/>
   </mergeCells>
-  <conditionalFormatting sqref="C72:E74">
-    <cfRule type="duplicateValues" dxfId="68" priority="2"/>
+  <conditionalFormatting sqref="C74:E76">
+    <cfRule type="duplicateValues" dxfId="0" priority="2"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
New Tournaments Definitionss added
Former-commit-id: bcb0ffef0f3ea2c1840925a448d783bae9d16244
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Missions.xlsx
+++ b/Docs/Content/HungryDragonContent_Missions.xlsx
@@ -5,14 +5,15 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\dragon\client\Docs\Content\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\dragon\client\Docs\Content\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="38295" windowHeight="19860"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="38295" windowHeight="19860" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="missions" sheetId="1" r:id="rId1"/>
+    <sheet name="tournaments" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913" calcOnSave="0"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="556" uniqueCount="317">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1061" uniqueCount="454">
   <si>
     <t>single_run</t>
   </si>
@@ -1000,6 +1001,419 @@
   </si>
   <si>
     <t>TID_EVENT_TOURNAMENT_TIME_LIMIT_STAY_HUNGRY_BIRTHDAY_MODE</t>
+  </si>
+  <si>
+    <t>TOURNAMENTS DEFINITIONS</t>
+  </si>
+  <si>
+    <t>{tournamentsDefinitions}</t>
+  </si>
+  <si>
+    <t>[gameMode]</t>
+  </si>
+  <si>
+    <t>[target]</t>
+  </si>
+  <si>
+    <t>[category]</t>
+  </si>
+  <si>
+    <t>TID_EVENT_TOURNAMENT_KILL_NORMAL_ARCHERS</t>
+  </si>
+  <si>
+    <t>0 --&gt; Normal Mode
+1 --&gt; Time Attack Mode
+2 --&gt; Time Limit Mode</t>
+  </si>
+  <si>
+    <t>Archers</t>
+  </si>
+  <si>
+    <t>TID_EVENT_TOURNAMENT_KILL_TIME_LIMIT_ARCHERS</t>
+  </si>
+  <si>
+    <t>TID_EVENT_TOURNAMENT_KILL_TIME_ATTACK_ARCHERS</t>
+  </si>
+  <si>
+    <t>TID_EVENT_TOURNAMENT_KILL_NORMAL_GOBLINS</t>
+  </si>
+  <si>
+    <t>Bomber;WorkerWagon;Spartakus;Guardian;Miner;Worker;Driller;Kamikaze;Unka;GoblinWarMachine</t>
+  </si>
+  <si>
+    <t>Goblins</t>
+  </si>
+  <si>
+    <t>TID_EVENT_TOURNAMENT_KILL_TIME_LIMIT_GOBLINS</t>
+  </si>
+  <si>
+    <t>TID_EVENT_TOURNAMENT_KILL_TIME_ATTACK_GOBLINS</t>
+  </si>
+  <si>
+    <t>TID_EVENT_TOURNAMENT_KILL_NORMAL_BIRDS</t>
+  </si>
+  <si>
+    <t>Canary01_Flock;Canary02_Flock;Canary03_Flock;Canary04_Flock;Hawk;OwlWhite;OwlBig;Vulture;Starling_Flock;CrowFlock</t>
+  </si>
+  <si>
+    <t>Birds</t>
+  </si>
+  <si>
+    <t>TID_EVENT_TOURNAMENT_KILL_TIME_LIMIT_BIRDS</t>
+  </si>
+  <si>
+    <t>TID_EVENT_TOURNAMENT_KILL_TIME_ATTACK_BIRDS</t>
+  </si>
+  <si>
+    <t>TID_EVENT_TOURNAMENT_NORMAL_SURVIVE_TIME</t>
+  </si>
+  <si>
+    <t>TID_EVENT_TOURNAMENT_DESTROY_NORMAL_HOUSES</t>
+  </si>
+  <si>
+    <t>Buildings</t>
+  </si>
+  <si>
+    <t>TID_EVENT_TOURNAMENT_DESTROY_TIME_LIMIT_HOUSES</t>
+  </si>
+  <si>
+    <t>TID_EVENT_TOURNAMENT_DESTROY_TIME_ATTACK_HOUSES</t>
+  </si>
+  <si>
+    <t>TID_EVENT_TOURNAMENT_KILL_NORMAL_DRAGONS</t>
+  </si>
+  <si>
+    <t>TID_EVENT_TOURNAMENT_KILL_TIME_LIMIT_DRAGONS</t>
+  </si>
+  <si>
+    <t>TID_EVENT_TOURNAMENT_KILL_TIME_ATTACK_DRAGONS</t>
+  </si>
+  <si>
+    <t>EnemyTier0;EnemyTier1;EnemyTier2;EnemyTier3;EnemyTier5</t>
+  </si>
+  <si>
+    <t>Dragons</t>
+  </si>
+  <si>
+    <t>TID_EVENT_TOURNAMENT_KILL_NORMAL_FLYINGBUNNIES</t>
+  </si>
+  <si>
+    <t>TID_EVENT_TOURNAMENT_KILL_TIME_LIMIT_FLYINGBUNNIES</t>
+  </si>
+  <si>
+    <t>TID_EVENT_TOURNAMENT_KILL_TIME_ATTACK_FLYINGBUNNIES</t>
+  </si>
+  <si>
+    <t>TID_EVENT_TOURNAMENT_KILL_NORMAL_EASTER_EGGS</t>
+  </si>
+  <si>
+    <t>TID_EVENT_TOURNAMENT_KILL_TIME_LIMIT_EASTER_EGGS</t>
+  </si>
+  <si>
+    <t>easter_egg</t>
+  </si>
+  <si>
+    <t>TID_EVENT_TOURNAMENT_NORMAL_FIRERUSH</t>
+  </si>
+  <si>
+    <t>TID_EVENT_TOURNAMENT_TIME_LIMIT_FIRERUSH</t>
+  </si>
+  <si>
+    <t>TID_EVENT_TOURNAMENT_TIME_ATTACK_FIRERUSH</t>
+  </si>
+  <si>
+    <t>TID_EVENT_TOURNAMENT_KILL_NORMAL_FISH</t>
+  </si>
+  <si>
+    <t>TID_EVENT_TOURNAMENT_KILL_TIME_LIMIT_FISH</t>
+  </si>
+  <si>
+    <t>TID_EVENT_TOURNAMENT_KILL_TIME_ATTACK_FISH</t>
+  </si>
+  <si>
+    <t>Fish01_Generic;FishDark;StingraySmall;Piranha;Fish03_Generic;PiranhaDark;StingrayLarge;Fish02_Generic;Shark;JellyfishBlue;JellyfishRed</t>
+  </si>
+  <si>
+    <t>Fish</t>
+  </si>
+  <si>
+    <t>icon_fish</t>
+  </si>
+  <si>
+    <t>TID_EVENT_TOURNAMENT_KILL_NORMAL_GHOST</t>
+  </si>
+  <si>
+    <t>TID_EVENT_TOURNAMENT_KILL_TIME_LIMIT_GHOST</t>
+  </si>
+  <si>
+    <t>TID_EVENT_TOURNAMENT_KILL_TIME_ATTACK_GHOST</t>
+  </si>
+  <si>
+    <t>Ghost01;Ghost02;Ghost03</t>
+  </si>
+  <si>
+    <t>Ghosts</t>
+  </si>
+  <si>
+    <t>icon_ghost</t>
+  </si>
+  <si>
+    <t>TID_EVENT_TOURNAMENT_KILL_NORMAL_FLYINGPIGS</t>
+  </si>
+  <si>
+    <t>TID_EVENT_TOURNAMENT_KILL_TIME_LIMIT_FLYINGPIGS</t>
+  </si>
+  <si>
+    <t>TID_EVENT_TOURNAMENT_KILL_TIME_ATTACK_FLYINGPIGS</t>
+  </si>
+  <si>
+    <t>TID_EVENT_TOURNAMENT_DESTROY_NORMAL_SPIDERS</t>
+  </si>
+  <si>
+    <t>TID_EVENT_TOURNAMENT_DESTROY_TIME_LIMIT_SPIDERS</t>
+  </si>
+  <si>
+    <t>TID_EVENT_TOURNAMENT_DESTROY_TIME_ATTACK_SPIDER</t>
+  </si>
+  <si>
+    <t>SpiderSmall;SpiderGreenTurret;SpiderRed</t>
+  </si>
+  <si>
+    <t>Spiders</t>
+  </si>
+  <si>
+    <t>icon_spider</t>
+  </si>
+  <si>
+    <t>TID_EVENT_TOURNAMENT_KILL_IN_LOVE_NORMAL_ALL</t>
+  </si>
+  <si>
+    <t>TID_EVENT_TOURNAMENT_KILL_IN_LOVE_TIME_LIMIT_ALL</t>
+  </si>
+  <si>
+    <t>TID_EVENT_TOURNAMENT_KILL_IN_LOVE_TIME_ATTACK_ALL</t>
+  </si>
+  <si>
+    <t>NPCs</t>
+  </si>
+  <si>
+    <t>TID_EVENT_TOURNAMENT_KILL_NORMAL_HUMANS</t>
+  </si>
+  <si>
+    <t>TID_EVENT_TOURNAMENT_KILL_TIME_LIMIT_HUMANS</t>
+  </si>
+  <si>
+    <t>TID_EVENT_TOURNAMENT_KILL_TIME_ATTACK_HUMANS</t>
+  </si>
+  <si>
+    <t>RichMan;BoatFisher;BakerWoman;BadFarmer;Soldier;Archer01;Archer02;ShieldMan;DrunkenMan;Catapulter;Villager01;Villager02</t>
+  </si>
+  <si>
+    <t>Humans</t>
+  </si>
+  <si>
+    <t>TID_EVENT_TOURNAMENT_NORMAL_COLLECT_COINS</t>
+  </si>
+  <si>
+    <t>TID_EVENT_TOURNAMENT_TIME_LIMIT_COLLECT_COINS</t>
+  </si>
+  <si>
+    <t>TID_EVENT_TOURNAMENT_TIME_ATTACK_COLLECT_COINS</t>
+  </si>
+  <si>
+    <t>TID_EVENT_TOURNAMENT_KILL_NORMAL_MOONCAKES</t>
+  </si>
+  <si>
+    <t>TID_EVENT_TOURNAMENT_KILL_TIME_LIMIT_MOONCAKES</t>
+  </si>
+  <si>
+    <t>TID_EVENT_TOURNAMENT_KILL_TIME_ATTACK_MOONCAKES</t>
+  </si>
+  <si>
+    <t>moonCake</t>
+  </si>
+  <si>
+    <t>TID_EVENT_TOURNAMENT_NORMAL_DISTANCE</t>
+  </si>
+  <si>
+    <t>TID_EVENT_TOURNAMENT_TIME_LIMIT_DISTANCE</t>
+  </si>
+  <si>
+    <t>TID_EVENT_TOURNAMENT_TIME_ATTACK_DISTANCE</t>
+  </si>
+  <si>
+    <t>TID_EVENT_TOURNAMENT_NORMAL_SCORE</t>
+  </si>
+  <si>
+    <t>TID_EVENT_TOURNAMENT_TIME_LIMIT_SCORE</t>
+  </si>
+  <si>
+    <t>TID_EVENT_TOURNAMENT_TIME_ATTACK_SCORE</t>
+  </si>
+  <si>
+    <t>TID_EVENT_TOURNAMENT_KILL_WEARING_NORMAL_STPATRICK</t>
+  </si>
+  <si>
+    <t>TID_EVENT_TOURNAMENT_KILL_TIME_LIMIT_STPATRICK</t>
+  </si>
+  <si>
+    <t>TID_EVENT_TOURNAMENT_KILL_TIME_ATTACK_STPATRICK</t>
+  </si>
+  <si>
+    <t>*TID_LEPRECHAUN_HAT</t>
+  </si>
+  <si>
+    <t>TID_EVENT_TOURNAMENT_KILL_NORMAL_TROLLS</t>
+  </si>
+  <si>
+    <t>TID_EVENT_TOURNAMENT_KILL_TIME_LIMIT_TROLLS</t>
+  </si>
+  <si>
+    <t>TID_EVENT_TOURNAMENT_KILL_TIME_ATTACK_TROLLS</t>
+  </si>
+  <si>
+    <t>TID_EVENT_TOURNAMENT_KILL_WEARING_NORMAL_UFO_DAY_DISGUISE</t>
+  </si>
+  <si>
+    <t>TID_EVENT_TOURNAMENT_WEARING_KILL_TIME_LIMIT_UFO_DAY_DISGUISE</t>
+  </si>
+  <si>
+    <t>TID_EVENT_TOURNAMENT_WEARING_KILL_TIME_ATTACK_UFO_DAY_DISGUISE</t>
+  </si>
+  <si>
+    <t>*TID_ALIEN_MASK ; TID_FOIL_PAPER_HAT</t>
+  </si>
+  <si>
+    <t>TID_EVENT_TOURNAMENT_KILL_NORMAL_WITCHES</t>
+  </si>
+  <si>
+    <t>TID_EVENT_TOURNAMENT_KILL_TIME_LIMIT_WITCHES</t>
+  </si>
+  <si>
+    <t>TID_EVENT_TOURNAMENT_KILL_TIME_ATTACK_WITCHES</t>
+  </si>
+  <si>
+    <t>Witch;BadWitch;GoodWitch;GoodWitch02</t>
+  </si>
+  <si>
+    <t>Witch</t>
+  </si>
+  <si>
+    <t>TID_EVENT_TOURNAMENT_KILL_STUNNED_NORMAL_ALL</t>
+  </si>
+  <si>
+    <t>TID_EVENT_TOURNAMENT_KILL_STUNNED_TIME_LIMIT_ALL</t>
+  </si>
+  <si>
+    <t>TID_EVENT_TOURNAMENT_KILL_STUNNED_TIME_ATTACK_ALL</t>
+  </si>
+  <si>
+    <t>icon_stunned</t>
+  </si>
+  <si>
+    <t>TID_EVENT_TOURNAMENT_KILL_FROZEN_NORMAL_ALL</t>
+  </si>
+  <si>
+    <t>TID_EVENT_TOURNAMENT_KILL_FROZEN_TIME_LIMIT_ALL</t>
+  </si>
+  <si>
+    <t>TID_EVENT_TOURNAMENT_KILL_FROZEN_TIME_ATTACK_ALL</t>
+  </si>
+  <si>
+    <t>icon_frozen</t>
+  </si>
+  <si>
+    <t>TID_EVENT_TOURNAMENT_NORMAL_HUNGRY_BIRTHDAY_MODE</t>
+  </si>
+  <si>
+    <t>TID_EVENT_TOURNAMENT_TIME_ATTACK_HUNGRY_BIRTHDAY_MODE</t>
+  </si>
+  <si>
+    <t>TID_EVENT_TOURNAMENT_NORMAL_STAY_HUNGRY_BIRTHDAY_MODE</t>
+  </si>
+  <si>
+    <t>FlyingBunny</t>
+  </si>
+  <si>
+    <t>TID_EVENT_TOURNAMENT_KILL_NORMAL_FAIRIES</t>
+  </si>
+  <si>
+    <t>TID_EVENT_TOURNAMENT_KILL_TIME_LIMIT_FAIRIES</t>
+  </si>
+  <si>
+    <t>TID_EVENT_TOURNAMENT_KILL_TIME_ATTACK_FAIRIES</t>
+  </si>
+  <si>
+    <t>FairySmall;FairyBig</t>
+  </si>
+  <si>
+    <t>icon_fairy</t>
+  </si>
+  <si>
+    <t>Fairies</t>
+  </si>
+  <si>
+    <t>TID_EVENT_TOURNAMENT_KILL_NORMAL_ROCKETGOBLINS</t>
+  </si>
+  <si>
+    <t>TID_EVENT_TOURNAMENT_KILL_TIME_LIMIT_ROCKETGOBLINS</t>
+  </si>
+  <si>
+    <t>TID_EVENT_TOURNAMENT_KILL_TIME_ATTACK_ROCKETGOBLINS</t>
+  </si>
+  <si>
+    <t>TID_EVENT_TOURNAMENT_KILL_NORMAL_SUMMER_ITEMS</t>
+  </si>
+  <si>
+    <t>TID_EVENT_TOURNAMENT_KILL_TIME_LIMIT_SUMMER_ITEMS</t>
+  </si>
+  <si>
+    <t>TID_EVENT_TOURNAMENT_KILL_TIME_ATTACK_SUMMER_ITEMS</t>
+  </si>
+  <si>
+    <t>PreSummer_01_cocktail;PreSummer_03_snorkel</t>
+  </si>
+  <si>
+    <t>Summer Items</t>
+  </si>
+  <si>
+    <t>TID_EVENT_TOURNAMENT_NORMAL_BIRTHDAY_CANDLE</t>
+  </si>
+  <si>
+    <t>TID_EVENT_TOURNAMENT_TIME_LIMIT_BIRTHDAY_CANDLE</t>
+  </si>
+  <si>
+    <t>TID_EVENT_TOURNAMENT_TIME_ATTACK_BIRTHDAY_CANDLE</t>
+  </si>
+  <si>
+    <t>AnniversaryCandle</t>
+  </si>
+  <si>
+    <t>TID_EVENT_TOURNAMENT_WEARING_NORMAL_BIRTHDAY</t>
+  </si>
+  <si>
+    <t>TID_EVENT_TOURNAMENT_WEARING_TIME_LIMIT_BIRTHDAY</t>
+  </si>
+  <si>
+    <t>TID_EVENT_TOURNAMENT_WEARING_TIME_ATTACK_BIRTHDAY</t>
+  </si>
+  <si>
+    <t>*TID_ANNIVERSARY_HAT</t>
+  </si>
+  <si>
+    <t>TID_EVENT_TOURNAMENT_KILL_GOLDEN_NORMAL_ALL</t>
+  </si>
+  <si>
+    <t>TID_EVENT_TOURNAMENT_KILL_GOLDEN_TIME_LIMIT_ALL</t>
+  </si>
+  <si>
+    <t>TID_EVENT_TOURNAMENT_KILL_GOLDEN_TIME_ATTACK_ALL</t>
+  </si>
+  <si>
+    <t>kill_golden</t>
+  </si>
+  <si>
+    <t>icon_golden</t>
   </si>
 </sst>
 </file>
@@ -1317,7 +1731,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1"/>
@@ -1443,9 +1857,22 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2995,8 +3422,8 @@
   </sheetPr>
   <dimension ref="B1:P162"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B49" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C69" sqref="C69"/>
+    <sheetView topLeftCell="A124" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C162" sqref="C162"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3043,14 +3470,14 @@
         <v>140</v>
       </c>
       <c r="G3" s="38"/>
-      <c r="J3" s="52" t="s">
+      <c r="J3" s="53" t="s">
         <v>139</v>
       </c>
-      <c r="K3" s="52"/>
-      <c r="M3" s="52"/>
-      <c r="N3" s="52"/>
-      <c r="O3" s="52"/>
-      <c r="P3" s="52"/>
+      <c r="K3" s="53"/>
+      <c r="M3" s="53"/>
+      <c r="N3" s="53"/>
+      <c r="O3" s="53"/>
+      <c r="P3" s="53"/>
     </row>
     <row r="4" spans="2:16" ht="106.5" x14ac:dyDescent="0.25">
       <c r="B4" s="30" t="s">
@@ -4730,9 +5157,9 @@
       <c r="C47" s="20"/>
       <c r="D47" s="20"/>
       <c r="E47" s="20"/>
-      <c r="F47" s="53"/>
-      <c r="G47" s="53"/>
-      <c r="H47" s="53"/>
+      <c r="F47" s="54"/>
+      <c r="G47" s="54"/>
+      <c r="H47" s="54"/>
       <c r="I47" s="20"/>
       <c r="J47" s="20"/>
     </row>
@@ -5261,10 +5688,10 @@
       <c r="F72" s="21" t="s">
         <v>40</v>
       </c>
-      <c r="G72" s="54" t="s">
+      <c r="G72" s="55" t="s">
         <v>39</v>
       </c>
-      <c r="H72" s="54"/>
+      <c r="H72" s="55"/>
       <c r="I72" s="20"/>
     </row>
     <row r="73" spans="2:13" ht="142.5" x14ac:dyDescent="0.25">
@@ -6488,4 +6915,2110 @@
     <tablePart r:id="rId7"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G99"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="28.42578125" customWidth="1"/>
+    <col min="2" max="2" width="73.85546875" customWidth="1"/>
+    <col min="3" max="3" width="34" customWidth="1"/>
+    <col min="4" max="4" width="26.28515625" customWidth="1"/>
+    <col min="5" max="5" width="128.85546875" customWidth="1"/>
+    <col min="6" max="6" width="27.140625" customWidth="1"/>
+    <col min="7" max="7" width="32.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="1:7" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A2" s="6" t="s">
+        <v>317</v>
+      </c>
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+    </row>
+    <row r="3" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A3" s="20"/>
+      <c r="B3" s="52"/>
+      <c r="D3" s="52" t="s">
+        <v>323</v>
+      </c>
+      <c r="E3" s="39"/>
+      <c r="F3" s="52"/>
+    </row>
+    <row r="4" spans="1:7" ht="97.5" x14ac:dyDescent="0.25">
+      <c r="A4" s="30" t="s">
+        <v>318</v>
+      </c>
+      <c r="B4" s="28" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="37" t="s">
+        <v>137</v>
+      </c>
+      <c r="D4" s="37" t="s">
+        <v>319</v>
+      </c>
+      <c r="E4" s="37" t="s">
+        <v>320</v>
+      </c>
+      <c r="F4" s="37" t="s">
+        <v>321</v>
+      </c>
+      <c r="G4" s="37" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="56" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" s="46" t="s">
+        <v>322</v>
+      </c>
+      <c r="C5" s="56" t="s">
+        <v>65</v>
+      </c>
+      <c r="D5" s="56">
+        <v>0</v>
+      </c>
+      <c r="E5" s="46" t="s">
+        <v>81</v>
+      </c>
+      <c r="F5" s="56" t="s">
+        <v>324</v>
+      </c>
+      <c r="G5" s="59" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="56" t="s">
+        <v>1</v>
+      </c>
+      <c r="B6" s="46" t="s">
+        <v>325</v>
+      </c>
+      <c r="C6" s="56" t="s">
+        <v>65</v>
+      </c>
+      <c r="D6" s="56">
+        <v>2</v>
+      </c>
+      <c r="E6" s="46" t="s">
+        <v>81</v>
+      </c>
+      <c r="F6" s="56" t="s">
+        <v>324</v>
+      </c>
+      <c r="G6" s="59" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="56" t="s">
+        <v>1</v>
+      </c>
+      <c r="B7" s="46" t="s">
+        <v>326</v>
+      </c>
+      <c r="C7" s="56" t="s">
+        <v>65</v>
+      </c>
+      <c r="D7" s="56">
+        <v>1</v>
+      </c>
+      <c r="E7" s="46" t="s">
+        <v>81</v>
+      </c>
+      <c r="F7" s="56" t="s">
+        <v>324</v>
+      </c>
+      <c r="G7" s="59" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="56" t="s">
+        <v>1</v>
+      </c>
+      <c r="B8" s="46" t="s">
+        <v>327</v>
+      </c>
+      <c r="C8" s="56" t="s">
+        <v>65</v>
+      </c>
+      <c r="D8" s="56">
+        <v>0</v>
+      </c>
+      <c r="E8" s="46" t="s">
+        <v>328</v>
+      </c>
+      <c r="F8" s="56" t="s">
+        <v>329</v>
+      </c>
+      <c r="G8" s="59" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="56" t="s">
+        <v>1</v>
+      </c>
+      <c r="B9" s="46" t="s">
+        <v>330</v>
+      </c>
+      <c r="C9" s="56" t="s">
+        <v>65</v>
+      </c>
+      <c r="D9" s="56">
+        <v>2</v>
+      </c>
+      <c r="E9" s="46" t="s">
+        <v>328</v>
+      </c>
+      <c r="F9" s="56" t="s">
+        <v>329</v>
+      </c>
+      <c r="G9" s="59" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="56" t="s">
+        <v>1</v>
+      </c>
+      <c r="B10" s="46" t="s">
+        <v>331</v>
+      </c>
+      <c r="C10" s="56" t="s">
+        <v>65</v>
+      </c>
+      <c r="D10" s="56">
+        <v>1</v>
+      </c>
+      <c r="E10" s="46" t="s">
+        <v>328</v>
+      </c>
+      <c r="F10" s="56" t="s">
+        <v>329</v>
+      </c>
+      <c r="G10" s="59" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="56" t="s">
+        <v>1</v>
+      </c>
+      <c r="B11" s="46" t="s">
+        <v>332</v>
+      </c>
+      <c r="C11" s="56" t="s">
+        <v>65</v>
+      </c>
+      <c r="D11" s="56">
+        <v>0</v>
+      </c>
+      <c r="E11" s="46" t="s">
+        <v>333</v>
+      </c>
+      <c r="F11" s="56" t="s">
+        <v>334</v>
+      </c>
+      <c r="G11" s="59" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="56" t="s">
+        <v>1</v>
+      </c>
+      <c r="B12" s="46" t="s">
+        <v>335</v>
+      </c>
+      <c r="C12" s="56" t="s">
+        <v>65</v>
+      </c>
+      <c r="D12" s="56">
+        <v>2</v>
+      </c>
+      <c r="E12" s="46" t="s">
+        <v>333</v>
+      </c>
+      <c r="F12" s="56" t="s">
+        <v>334</v>
+      </c>
+      <c r="G12" s="59" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="56" t="s">
+        <v>1</v>
+      </c>
+      <c r="B13" s="46" t="s">
+        <v>336</v>
+      </c>
+      <c r="C13" s="56" t="s">
+        <v>65</v>
+      </c>
+      <c r="D13" s="56">
+        <v>1</v>
+      </c>
+      <c r="E13" s="46" t="s">
+        <v>333</v>
+      </c>
+      <c r="F13" s="56" t="s">
+        <v>334</v>
+      </c>
+      <c r="G13" s="59" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="56" t="s">
+        <v>1</v>
+      </c>
+      <c r="B14" s="46" t="s">
+        <v>337</v>
+      </c>
+      <c r="C14" s="56" t="s">
+        <v>53</v>
+      </c>
+      <c r="D14" s="56">
+        <v>0</v>
+      </c>
+      <c r="E14" s="56"/>
+      <c r="F14" s="56"/>
+      <c r="G14" s="59" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="56" t="s">
+        <v>1</v>
+      </c>
+      <c r="B15" s="46" t="s">
+        <v>338</v>
+      </c>
+      <c r="C15" s="56" t="s">
+        <v>180</v>
+      </c>
+      <c r="D15" s="56">
+        <v>0</v>
+      </c>
+      <c r="E15" s="46" t="s">
+        <v>119</v>
+      </c>
+      <c r="F15" s="56" t="s">
+        <v>339</v>
+      </c>
+      <c r="G15" s="59" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="56" t="s">
+        <v>1</v>
+      </c>
+      <c r="B16" s="46" t="s">
+        <v>340</v>
+      </c>
+      <c r="C16" s="56" t="s">
+        <v>180</v>
+      </c>
+      <c r="D16" s="56">
+        <v>2</v>
+      </c>
+      <c r="E16" s="46" t="s">
+        <v>119</v>
+      </c>
+      <c r="F16" s="56" t="s">
+        <v>339</v>
+      </c>
+      <c r="G16" s="59" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="56" t="s">
+        <v>1</v>
+      </c>
+      <c r="B17" s="46" t="s">
+        <v>341</v>
+      </c>
+      <c r="C17" s="56" t="s">
+        <v>180</v>
+      </c>
+      <c r="D17" s="56">
+        <v>1</v>
+      </c>
+      <c r="E17" s="46" t="s">
+        <v>119</v>
+      </c>
+      <c r="F17" s="56" t="s">
+        <v>339</v>
+      </c>
+      <c r="G17" s="59" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="56" t="s">
+        <v>1</v>
+      </c>
+      <c r="B18" s="46" t="s">
+        <v>342</v>
+      </c>
+      <c r="C18" s="56" t="s">
+        <v>65</v>
+      </c>
+      <c r="D18" s="56">
+        <v>0</v>
+      </c>
+      <c r="E18" s="46" t="s">
+        <v>345</v>
+      </c>
+      <c r="F18" s="56" t="s">
+        <v>346</v>
+      </c>
+      <c r="G18" s="59" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="56" t="s">
+        <v>1</v>
+      </c>
+      <c r="B19" s="46" t="s">
+        <v>343</v>
+      </c>
+      <c r="C19" s="56" t="s">
+        <v>65</v>
+      </c>
+      <c r="D19" s="56">
+        <v>2</v>
+      </c>
+      <c r="E19" s="46" t="s">
+        <v>345</v>
+      </c>
+      <c r="F19" s="56" t="s">
+        <v>346</v>
+      </c>
+      <c r="G19" s="59" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="56" t="s">
+        <v>1</v>
+      </c>
+      <c r="B20" s="46" t="s">
+        <v>344</v>
+      </c>
+      <c r="C20" s="56" t="s">
+        <v>65</v>
+      </c>
+      <c r="D20" s="56">
+        <v>1</v>
+      </c>
+      <c r="E20" s="46" t="s">
+        <v>345</v>
+      </c>
+      <c r="F20" s="56" t="s">
+        <v>346</v>
+      </c>
+      <c r="G20" s="59" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="56" t="s">
+        <v>1</v>
+      </c>
+      <c r="B21" s="46" t="s">
+        <v>347</v>
+      </c>
+      <c r="C21" s="56" t="s">
+        <v>65</v>
+      </c>
+      <c r="D21" s="56">
+        <v>0</v>
+      </c>
+      <c r="E21" s="46" t="s">
+        <v>426</v>
+      </c>
+      <c r="F21" s="56"/>
+      <c r="G21" s="58" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="56" t="s">
+        <v>1</v>
+      </c>
+      <c r="B22" s="46" t="s">
+        <v>348</v>
+      </c>
+      <c r="C22" s="56" t="s">
+        <v>65</v>
+      </c>
+      <c r="D22" s="56">
+        <v>2</v>
+      </c>
+      <c r="E22" s="46" t="s">
+        <v>426</v>
+      </c>
+      <c r="F22" s="56"/>
+      <c r="G22" s="58" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" s="56" t="s">
+        <v>1</v>
+      </c>
+      <c r="B23" s="46" t="s">
+        <v>349</v>
+      </c>
+      <c r="C23" s="56" t="s">
+        <v>65</v>
+      </c>
+      <c r="D23" s="56">
+        <v>1</v>
+      </c>
+      <c r="E23" s="46" t="s">
+        <v>426</v>
+      </c>
+      <c r="F23" s="56"/>
+      <c r="G23" s="58" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="56" t="s">
+        <v>1</v>
+      </c>
+      <c r="B24" s="46" t="s">
+        <v>350</v>
+      </c>
+      <c r="C24" s="56" t="s">
+        <v>50</v>
+      </c>
+      <c r="D24" s="56">
+        <v>0</v>
+      </c>
+      <c r="E24" s="46" t="s">
+        <v>352</v>
+      </c>
+      <c r="F24" s="56"/>
+      <c r="G24" s="59" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" s="56" t="s">
+        <v>1</v>
+      </c>
+      <c r="B25" s="46" t="s">
+        <v>351</v>
+      </c>
+      <c r="C25" s="56" t="s">
+        <v>50</v>
+      </c>
+      <c r="D25" s="56">
+        <v>2</v>
+      </c>
+      <c r="E25" s="46" t="s">
+        <v>352</v>
+      </c>
+      <c r="F25" s="56"/>
+      <c r="G25" s="59" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" s="56" t="s">
+        <v>1</v>
+      </c>
+      <c r="B26" s="46" t="s">
+        <v>353</v>
+      </c>
+      <c r="C26" s="56" t="s">
+        <v>62</v>
+      </c>
+      <c r="D26" s="56">
+        <v>2</v>
+      </c>
+      <c r="E26" s="56"/>
+      <c r="F26" s="56"/>
+      <c r="G26" s="59" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" s="56" t="s">
+        <v>1</v>
+      </c>
+      <c r="B27" s="46" t="s">
+        <v>354</v>
+      </c>
+      <c r="C27" s="56" t="s">
+        <v>62</v>
+      </c>
+      <c r="D27" s="56">
+        <v>1</v>
+      </c>
+      <c r="E27" s="56"/>
+      <c r="F27" s="56"/>
+      <c r="G27" s="59" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" s="56" t="s">
+        <v>1</v>
+      </c>
+      <c r="B28" s="46" t="s">
+        <v>355</v>
+      </c>
+      <c r="C28" s="56" t="s">
+        <v>62</v>
+      </c>
+      <c r="D28" s="56">
+        <v>2</v>
+      </c>
+      <c r="E28" s="56"/>
+      <c r="F28" s="56"/>
+      <c r="G28" s="59" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" s="56" t="s">
+        <v>1</v>
+      </c>
+      <c r="B29" s="46" t="s">
+        <v>356</v>
+      </c>
+      <c r="C29" s="56" t="s">
+        <v>65</v>
+      </c>
+      <c r="D29" s="56">
+        <v>0</v>
+      </c>
+      <c r="E29" s="46" t="s">
+        <v>359</v>
+      </c>
+      <c r="F29" s="56" t="s">
+        <v>360</v>
+      </c>
+      <c r="G29" s="56" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" s="56" t="s">
+        <v>1</v>
+      </c>
+      <c r="B30" s="46" t="s">
+        <v>357</v>
+      </c>
+      <c r="C30" s="56" t="s">
+        <v>65</v>
+      </c>
+      <c r="D30" s="56">
+        <v>1</v>
+      </c>
+      <c r="E30" s="46" t="s">
+        <v>359</v>
+      </c>
+      <c r="F30" s="56" t="s">
+        <v>360</v>
+      </c>
+      <c r="G30" s="56" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" s="56" t="s">
+        <v>1</v>
+      </c>
+      <c r="B31" s="46" t="s">
+        <v>358</v>
+      </c>
+      <c r="C31" s="56" t="s">
+        <v>65</v>
+      </c>
+      <c r="D31" s="56">
+        <v>2</v>
+      </c>
+      <c r="E31" s="46" t="s">
+        <v>359</v>
+      </c>
+      <c r="F31" s="56" t="s">
+        <v>360</v>
+      </c>
+      <c r="G31" s="56" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" s="56" t="s">
+        <v>1</v>
+      </c>
+      <c r="B32" s="46" t="s">
+        <v>362</v>
+      </c>
+      <c r="C32" s="56" t="s">
+        <v>65</v>
+      </c>
+      <c r="D32" s="56">
+        <v>0</v>
+      </c>
+      <c r="E32" s="46" t="s">
+        <v>365</v>
+      </c>
+      <c r="F32" s="56" t="s">
+        <v>366</v>
+      </c>
+      <c r="G32" s="56" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33" s="56" t="s">
+        <v>1</v>
+      </c>
+      <c r="B33" s="46" t="s">
+        <v>363</v>
+      </c>
+      <c r="C33" s="56" t="s">
+        <v>65</v>
+      </c>
+      <c r="D33" s="56">
+        <v>2</v>
+      </c>
+      <c r="E33" s="46" t="s">
+        <v>365</v>
+      </c>
+      <c r="F33" s="56" t="s">
+        <v>366</v>
+      </c>
+      <c r="G33" s="56" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A34" s="56" t="s">
+        <v>1</v>
+      </c>
+      <c r="B34" s="46" t="s">
+        <v>364</v>
+      </c>
+      <c r="C34" s="56" t="s">
+        <v>65</v>
+      </c>
+      <c r="D34" s="56">
+        <v>1</v>
+      </c>
+      <c r="E34" s="46" t="s">
+        <v>365</v>
+      </c>
+      <c r="F34" s="56" t="s">
+        <v>366</v>
+      </c>
+      <c r="G34" s="56" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A35" s="56" t="s">
+        <v>1</v>
+      </c>
+      <c r="B35" s="46" t="s">
+        <v>368</v>
+      </c>
+      <c r="C35" s="56" t="s">
+        <v>65</v>
+      </c>
+      <c r="D35" s="56">
+        <v>0</v>
+      </c>
+      <c r="E35" s="46" t="s">
+        <v>97</v>
+      </c>
+      <c r="F35" s="56"/>
+      <c r="G35" s="58" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A36" s="56" t="s">
+        <v>1</v>
+      </c>
+      <c r="B36" s="46" t="s">
+        <v>369</v>
+      </c>
+      <c r="C36" s="56" t="s">
+        <v>65</v>
+      </c>
+      <c r="D36" s="56">
+        <v>2</v>
+      </c>
+      <c r="E36" s="46" t="s">
+        <v>97</v>
+      </c>
+      <c r="F36" s="56"/>
+      <c r="G36" s="58" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A37" s="56" t="s">
+        <v>1</v>
+      </c>
+      <c r="B37" s="46" t="s">
+        <v>370</v>
+      </c>
+      <c r="C37" s="56" t="s">
+        <v>65</v>
+      </c>
+      <c r="D37" s="56">
+        <v>1</v>
+      </c>
+      <c r="E37" s="46" t="s">
+        <v>97</v>
+      </c>
+      <c r="F37" s="56"/>
+      <c r="G37" s="58" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A38" s="56" t="s">
+        <v>1</v>
+      </c>
+      <c r="B38" s="46" t="s">
+        <v>371</v>
+      </c>
+      <c r="C38" s="56" t="s">
+        <v>65</v>
+      </c>
+      <c r="D38" s="56">
+        <v>0</v>
+      </c>
+      <c r="E38" s="57" t="s">
+        <v>374</v>
+      </c>
+      <c r="F38" s="56" t="s">
+        <v>375</v>
+      </c>
+      <c r="G38" s="56" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A39" s="56" t="s">
+        <v>1</v>
+      </c>
+      <c r="B39" s="46" t="s">
+        <v>372</v>
+      </c>
+      <c r="C39" s="56" t="s">
+        <v>65</v>
+      </c>
+      <c r="D39" s="56">
+        <v>2</v>
+      </c>
+      <c r="E39" s="57" t="s">
+        <v>374</v>
+      </c>
+      <c r="F39" s="56" t="s">
+        <v>375</v>
+      </c>
+      <c r="G39" s="56" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A40" s="56" t="s">
+        <v>1</v>
+      </c>
+      <c r="B40" s="46" t="s">
+        <v>373</v>
+      </c>
+      <c r="C40" s="56" t="s">
+        <v>65</v>
+      </c>
+      <c r="D40" s="56">
+        <v>1</v>
+      </c>
+      <c r="E40" s="57" t="s">
+        <v>374</v>
+      </c>
+      <c r="F40" s="56" t="s">
+        <v>375</v>
+      </c>
+      <c r="G40" s="56" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A41" s="56" t="s">
+        <v>1</v>
+      </c>
+      <c r="B41" s="46" t="s">
+        <v>377</v>
+      </c>
+      <c r="C41" s="56" t="s">
+        <v>231</v>
+      </c>
+      <c r="D41" s="56">
+        <v>0</v>
+      </c>
+      <c r="E41" s="56"/>
+      <c r="F41" s="56" t="s">
+        <v>380</v>
+      </c>
+      <c r="G41" s="58" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A42" s="56" t="s">
+        <v>1</v>
+      </c>
+      <c r="B42" s="46" t="s">
+        <v>378</v>
+      </c>
+      <c r="C42" s="56" t="s">
+        <v>231</v>
+      </c>
+      <c r="D42" s="56">
+        <v>2</v>
+      </c>
+      <c r="E42" s="56"/>
+      <c r="F42" s="56" t="s">
+        <v>380</v>
+      </c>
+      <c r="G42" s="58" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A43" s="56" t="s">
+        <v>1</v>
+      </c>
+      <c r="B43" s="46" t="s">
+        <v>379</v>
+      </c>
+      <c r="C43" s="56" t="s">
+        <v>231</v>
+      </c>
+      <c r="D43" s="56">
+        <v>1</v>
+      </c>
+      <c r="E43" s="56"/>
+      <c r="F43" s="56" t="s">
+        <v>380</v>
+      </c>
+      <c r="G43" s="58" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A44" s="56" t="s">
+        <v>1</v>
+      </c>
+      <c r="B44" s="46" t="s">
+        <v>381</v>
+      </c>
+      <c r="C44" s="56" t="s">
+        <v>65</v>
+      </c>
+      <c r="D44" s="56">
+        <v>0</v>
+      </c>
+      <c r="E44" s="46" t="s">
+        <v>384</v>
+      </c>
+      <c r="F44" s="56" t="s">
+        <v>385</v>
+      </c>
+      <c r="G44" s="58" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A45" s="56" t="s">
+        <v>1</v>
+      </c>
+      <c r="B45" s="46" t="s">
+        <v>382</v>
+      </c>
+      <c r="C45" s="56" t="s">
+        <v>65</v>
+      </c>
+      <c r="D45" s="56">
+        <v>2</v>
+      </c>
+      <c r="E45" s="46" t="s">
+        <v>384</v>
+      </c>
+      <c r="F45" s="56" t="s">
+        <v>385</v>
+      </c>
+      <c r="G45" s="58" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A46" s="56" t="s">
+        <v>1</v>
+      </c>
+      <c r="B46" s="46" t="s">
+        <v>383</v>
+      </c>
+      <c r="C46" s="56" t="s">
+        <v>65</v>
+      </c>
+      <c r="D46" s="56">
+        <v>1</v>
+      </c>
+      <c r="E46" s="46" t="s">
+        <v>384</v>
+      </c>
+      <c r="F46" s="56" t="s">
+        <v>385</v>
+      </c>
+      <c r="G46" s="58" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A47" s="56" t="s">
+        <v>1</v>
+      </c>
+      <c r="B47" s="46" t="s">
+        <v>386</v>
+      </c>
+      <c r="C47" s="56" t="s">
+        <v>50</v>
+      </c>
+      <c r="D47" s="56">
+        <v>0</v>
+      </c>
+      <c r="E47" s="46" t="s">
+        <v>117</v>
+      </c>
+      <c r="F47" s="56"/>
+      <c r="G47" s="58" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A48" s="56" t="s">
+        <v>1</v>
+      </c>
+      <c r="B48" s="46" t="s">
+        <v>387</v>
+      </c>
+      <c r="C48" s="56" t="s">
+        <v>50</v>
+      </c>
+      <c r="D48" s="56">
+        <v>2</v>
+      </c>
+      <c r="E48" s="46" t="s">
+        <v>117</v>
+      </c>
+      <c r="F48" s="56"/>
+      <c r="G48" s="58" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A49" s="56" t="s">
+        <v>1</v>
+      </c>
+      <c r="B49" s="46" t="s">
+        <v>388</v>
+      </c>
+      <c r="C49" s="56" t="s">
+        <v>50</v>
+      </c>
+      <c r="D49" s="56">
+        <v>1</v>
+      </c>
+      <c r="E49" s="46" t="s">
+        <v>117</v>
+      </c>
+      <c r="F49" s="56"/>
+      <c r="G49" s="58" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A50" s="56" t="s">
+        <v>1</v>
+      </c>
+      <c r="B50" s="46" t="s">
+        <v>389</v>
+      </c>
+      <c r="C50" s="56" t="s">
+        <v>50</v>
+      </c>
+      <c r="D50" s="56">
+        <v>0</v>
+      </c>
+      <c r="E50" s="46" t="s">
+        <v>392</v>
+      </c>
+      <c r="F50" s="56"/>
+      <c r="G50" s="58" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A51" s="56" t="s">
+        <v>1</v>
+      </c>
+      <c r="B51" s="46" t="s">
+        <v>390</v>
+      </c>
+      <c r="C51" s="56" t="s">
+        <v>50</v>
+      </c>
+      <c r="D51" s="56">
+        <v>2</v>
+      </c>
+      <c r="E51" s="46" t="s">
+        <v>392</v>
+      </c>
+      <c r="F51" s="56"/>
+      <c r="G51" s="58" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A52" s="56" t="s">
+        <v>1</v>
+      </c>
+      <c r="B52" s="46" t="s">
+        <v>391</v>
+      </c>
+      <c r="C52" s="56" t="s">
+        <v>50</v>
+      </c>
+      <c r="D52" s="56">
+        <v>1</v>
+      </c>
+      <c r="E52" s="46" t="s">
+        <v>392</v>
+      </c>
+      <c r="F52" s="56"/>
+      <c r="G52" s="58" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A53" s="56" t="s">
+        <v>1</v>
+      </c>
+      <c r="B53" s="46" t="s">
+        <v>393</v>
+      </c>
+      <c r="C53" s="56" t="s">
+        <v>47</v>
+      </c>
+      <c r="D53" s="56">
+        <v>0</v>
+      </c>
+      <c r="E53" s="56"/>
+      <c r="F53" s="56"/>
+      <c r="G53" s="58" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A54" s="56" t="s">
+        <v>1</v>
+      </c>
+      <c r="B54" s="46" t="s">
+        <v>394</v>
+      </c>
+      <c r="C54" s="56" t="s">
+        <v>47</v>
+      </c>
+      <c r="D54" s="56">
+        <v>2</v>
+      </c>
+      <c r="E54" s="56"/>
+      <c r="F54" s="56"/>
+      <c r="G54" s="58" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A55" s="56" t="s">
+        <v>1</v>
+      </c>
+      <c r="B55" s="46" t="s">
+        <v>395</v>
+      </c>
+      <c r="C55" s="56" t="s">
+        <v>47</v>
+      </c>
+      <c r="D55" s="56">
+        <v>1</v>
+      </c>
+      <c r="E55" s="56"/>
+      <c r="F55" s="56"/>
+      <c r="G55" s="58" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A56" s="56" t="s">
+        <v>1</v>
+      </c>
+      <c r="B56" s="46" t="s">
+        <v>396</v>
+      </c>
+      <c r="C56" s="56" t="s">
+        <v>59</v>
+      </c>
+      <c r="D56" s="56">
+        <v>0</v>
+      </c>
+      <c r="E56" s="56"/>
+      <c r="F56" s="56"/>
+      <c r="G56" s="58" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A57" s="56" t="s">
+        <v>1</v>
+      </c>
+      <c r="B57" s="46" t="s">
+        <v>397</v>
+      </c>
+      <c r="C57" s="56" t="s">
+        <v>59</v>
+      </c>
+      <c r="D57" s="56">
+        <v>2</v>
+      </c>
+      <c r="E57" s="56"/>
+      <c r="F57" s="56"/>
+      <c r="G57" s="58" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A58" s="56" t="s">
+        <v>1</v>
+      </c>
+      <c r="B58" s="46" t="s">
+        <v>398</v>
+      </c>
+      <c r="C58" s="56" t="s">
+        <v>59</v>
+      </c>
+      <c r="D58" s="56">
+        <v>1</v>
+      </c>
+      <c r="E58" s="57"/>
+      <c r="F58" s="56"/>
+      <c r="G58" s="58" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A59" s="56" t="s">
+        <v>1</v>
+      </c>
+      <c r="B59" s="46" t="s">
+        <v>399</v>
+      </c>
+      <c r="C59" s="56" t="s">
+        <v>237</v>
+      </c>
+      <c r="D59" s="56">
+        <v>0</v>
+      </c>
+      <c r="E59" s="46" t="s">
+        <v>402</v>
+      </c>
+      <c r="F59" s="56"/>
+      <c r="G59" s="58" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A60" s="56" t="s">
+        <v>1</v>
+      </c>
+      <c r="B60" s="46" t="s">
+        <v>400</v>
+      </c>
+      <c r="C60" s="56" t="s">
+        <v>237</v>
+      </c>
+      <c r="D60" s="56">
+        <v>2</v>
+      </c>
+      <c r="E60" s="46" t="s">
+        <v>402</v>
+      </c>
+      <c r="F60" s="56"/>
+      <c r="G60" s="58" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A61" s="56" t="s">
+        <v>1</v>
+      </c>
+      <c r="B61" s="46" t="s">
+        <v>401</v>
+      </c>
+      <c r="C61" s="56" t="s">
+        <v>237</v>
+      </c>
+      <c r="D61" s="56">
+        <v>1</v>
+      </c>
+      <c r="E61" s="46" t="s">
+        <v>402</v>
+      </c>
+      <c r="F61" s="56"/>
+      <c r="G61" s="58" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A62" s="56" t="s">
+        <v>1</v>
+      </c>
+      <c r="B62" s="46" t="s">
+        <v>403</v>
+      </c>
+      <c r="C62" s="56" t="s">
+        <v>65</v>
+      </c>
+      <c r="D62" s="56">
+        <v>0</v>
+      </c>
+      <c r="E62" s="46" t="s">
+        <v>75</v>
+      </c>
+      <c r="F62" s="56"/>
+      <c r="G62" s="56" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A63" s="56" t="s">
+        <v>1</v>
+      </c>
+      <c r="B63" s="46" t="s">
+        <v>404</v>
+      </c>
+      <c r="C63" s="56" t="s">
+        <v>65</v>
+      </c>
+      <c r="D63" s="56">
+        <v>2</v>
+      </c>
+      <c r="E63" s="46" t="s">
+        <v>75</v>
+      </c>
+      <c r="F63" s="56"/>
+      <c r="G63" s="56" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A64" s="56" t="s">
+        <v>1</v>
+      </c>
+      <c r="B64" s="46" t="s">
+        <v>405</v>
+      </c>
+      <c r="C64" s="56" t="s">
+        <v>65</v>
+      </c>
+      <c r="D64" s="56">
+        <v>1</v>
+      </c>
+      <c r="E64" s="46" t="s">
+        <v>75</v>
+      </c>
+      <c r="F64" s="56"/>
+      <c r="G64" s="56" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A65" s="56" t="s">
+        <v>1</v>
+      </c>
+      <c r="B65" s="46" t="s">
+        <v>406</v>
+      </c>
+      <c r="C65" s="56" t="s">
+        <v>237</v>
+      </c>
+      <c r="D65" s="56">
+        <v>0</v>
+      </c>
+      <c r="E65" s="46" t="s">
+        <v>409</v>
+      </c>
+      <c r="F65" s="56"/>
+      <c r="G65" s="58" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A66" s="56" t="s">
+        <v>1</v>
+      </c>
+      <c r="B66" s="46" t="s">
+        <v>407</v>
+      </c>
+      <c r="C66" s="56" t="s">
+        <v>237</v>
+      </c>
+      <c r="D66" s="56">
+        <v>2</v>
+      </c>
+      <c r="E66" s="46" t="s">
+        <v>409</v>
+      </c>
+      <c r="F66" s="56"/>
+      <c r="G66" s="58" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A67" s="56" t="s">
+        <v>1</v>
+      </c>
+      <c r="B67" s="46" t="s">
+        <v>408</v>
+      </c>
+      <c r="C67" s="56" t="s">
+        <v>237</v>
+      </c>
+      <c r="D67" s="56">
+        <v>1</v>
+      </c>
+      <c r="E67" s="46" t="s">
+        <v>409</v>
+      </c>
+      <c r="F67" s="56"/>
+      <c r="G67" s="58" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A68" s="56" t="s">
+        <v>1</v>
+      </c>
+      <c r="B68" s="46" t="s">
+        <v>410</v>
+      </c>
+      <c r="C68" s="56" t="s">
+        <v>65</v>
+      </c>
+      <c r="D68" s="56">
+        <v>0</v>
+      </c>
+      <c r="E68" s="46" t="s">
+        <v>413</v>
+      </c>
+      <c r="F68" s="56" t="s">
+        <v>414</v>
+      </c>
+      <c r="G68" s="58" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A69" s="56" t="s">
+        <v>1</v>
+      </c>
+      <c r="B69" s="46" t="s">
+        <v>411</v>
+      </c>
+      <c r="C69" s="56" t="s">
+        <v>65</v>
+      </c>
+      <c r="D69" s="56">
+        <v>2</v>
+      </c>
+      <c r="E69" s="46" t="s">
+        <v>413</v>
+      </c>
+      <c r="F69" s="56" t="s">
+        <v>414</v>
+      </c>
+      <c r="G69" s="58" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A70" s="56" t="s">
+        <v>1</v>
+      </c>
+      <c r="B70" s="46" t="s">
+        <v>412</v>
+      </c>
+      <c r="C70" s="56" t="s">
+        <v>65</v>
+      </c>
+      <c r="D70" s="56">
+        <v>1</v>
+      </c>
+      <c r="E70" s="46" t="s">
+        <v>413</v>
+      </c>
+      <c r="F70" s="56" t="s">
+        <v>414</v>
+      </c>
+      <c r="G70" s="58" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A71" s="56" t="s">
+        <v>1</v>
+      </c>
+      <c r="B71" s="46" t="s">
+        <v>415</v>
+      </c>
+      <c r="C71" s="56" t="s">
+        <v>228</v>
+      </c>
+      <c r="D71" s="56">
+        <v>0</v>
+      </c>
+      <c r="E71" s="56"/>
+      <c r="F71" s="56" t="s">
+        <v>380</v>
+      </c>
+      <c r="G71" s="56" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A72" s="56" t="s">
+        <v>1</v>
+      </c>
+      <c r="B72" s="46" t="s">
+        <v>416</v>
+      </c>
+      <c r="C72" s="56" t="s">
+        <v>228</v>
+      </c>
+      <c r="D72" s="56">
+        <v>2</v>
+      </c>
+      <c r="E72" s="56"/>
+      <c r="F72" s="56" t="s">
+        <v>380</v>
+      </c>
+      <c r="G72" s="56" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A73" s="56" t="s">
+        <v>1</v>
+      </c>
+      <c r="B73" s="46" t="s">
+        <v>417</v>
+      </c>
+      <c r="C73" s="56" t="s">
+        <v>228</v>
+      </c>
+      <c r="D73" s="56">
+        <v>1</v>
+      </c>
+      <c r="E73" s="56"/>
+      <c r="F73" s="56" t="s">
+        <v>380</v>
+      </c>
+      <c r="G73" s="56" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A74" s="56" t="s">
+        <v>1</v>
+      </c>
+      <c r="B74" s="46" t="s">
+        <v>419</v>
+      </c>
+      <c r="C74" s="56" t="s">
+        <v>234</v>
+      </c>
+      <c r="D74" s="56">
+        <v>0</v>
+      </c>
+      <c r="E74" s="56"/>
+      <c r="F74" s="56" t="s">
+        <v>380</v>
+      </c>
+      <c r="G74" s="56" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A75" s="56" t="s">
+        <v>1</v>
+      </c>
+      <c r="B75" s="46" t="s">
+        <v>420</v>
+      </c>
+      <c r="C75" s="56" t="s">
+        <v>234</v>
+      </c>
+      <c r="D75" s="56">
+        <v>2</v>
+      </c>
+      <c r="E75" s="56"/>
+      <c r="F75" s="56" t="s">
+        <v>380</v>
+      </c>
+      <c r="G75" s="56" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A76" s="56" t="s">
+        <v>1</v>
+      </c>
+      <c r="B76" s="46" t="s">
+        <v>421</v>
+      </c>
+      <c r="C76" s="56" t="s">
+        <v>234</v>
+      </c>
+      <c r="D76" s="56">
+        <v>1</v>
+      </c>
+      <c r="E76" s="56"/>
+      <c r="F76" s="56" t="s">
+        <v>380</v>
+      </c>
+      <c r="G76" s="56" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A77" s="56" t="s">
+        <v>1</v>
+      </c>
+      <c r="B77" s="46" t="s">
+        <v>423</v>
+      </c>
+      <c r="C77" s="59" t="s">
+        <v>313</v>
+      </c>
+      <c r="D77" s="56">
+        <v>0</v>
+      </c>
+      <c r="E77" s="56"/>
+      <c r="F77" s="56"/>
+      <c r="G77" s="58" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A78" s="56" t="s">
+        <v>1</v>
+      </c>
+      <c r="B78" s="46" t="s">
+        <v>314</v>
+      </c>
+      <c r="C78" s="59" t="s">
+        <v>313</v>
+      </c>
+      <c r="D78" s="56">
+        <v>2</v>
+      </c>
+      <c r="E78" s="56"/>
+      <c r="F78" s="56"/>
+      <c r="G78" s="58" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A79" s="56" t="s">
+        <v>1</v>
+      </c>
+      <c r="B79" s="46" t="s">
+        <v>424</v>
+      </c>
+      <c r="C79" s="59" t="s">
+        <v>313</v>
+      </c>
+      <c r="D79" s="56">
+        <v>1</v>
+      </c>
+      <c r="E79" s="56"/>
+      <c r="F79" s="56"/>
+      <c r="G79" s="58" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A80" s="56" t="s">
+        <v>1</v>
+      </c>
+      <c r="B80" s="46" t="s">
+        <v>425</v>
+      </c>
+      <c r="C80" s="59" t="s">
+        <v>315</v>
+      </c>
+      <c r="D80" s="56">
+        <v>0</v>
+      </c>
+      <c r="E80" s="57"/>
+      <c r="F80" s="56"/>
+      <c r="G80" s="58" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A81" s="56" t="s">
+        <v>1</v>
+      </c>
+      <c r="B81" s="46" t="s">
+        <v>316</v>
+      </c>
+      <c r="C81" s="59" t="s">
+        <v>315</v>
+      </c>
+      <c r="D81" s="56">
+        <v>2</v>
+      </c>
+      <c r="E81" s="56"/>
+      <c r="F81" s="56"/>
+      <c r="G81" s="58" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A82" s="56" t="s">
+        <v>1</v>
+      </c>
+      <c r="B82" s="46" t="s">
+        <v>427</v>
+      </c>
+      <c r="C82" s="56" t="s">
+        <v>65</v>
+      </c>
+      <c r="D82" s="56">
+        <v>0</v>
+      </c>
+      <c r="E82" s="57" t="s">
+        <v>430</v>
+      </c>
+      <c r="F82" s="56" t="s">
+        <v>432</v>
+      </c>
+      <c r="G82" s="56" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A83" s="56" t="s">
+        <v>1</v>
+      </c>
+      <c r="B83" s="46" t="s">
+        <v>428</v>
+      </c>
+      <c r="C83" s="56" t="s">
+        <v>65</v>
+      </c>
+      <c r="D83" s="56">
+        <v>2</v>
+      </c>
+      <c r="E83" s="57" t="s">
+        <v>430</v>
+      </c>
+      <c r="F83" s="56" t="s">
+        <v>432</v>
+      </c>
+      <c r="G83" s="56" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A84" s="56" t="s">
+        <v>1</v>
+      </c>
+      <c r="B84" s="46" t="s">
+        <v>429</v>
+      </c>
+      <c r="C84" s="56" t="s">
+        <v>65</v>
+      </c>
+      <c r="D84" s="56">
+        <v>1</v>
+      </c>
+      <c r="E84" s="57" t="s">
+        <v>430</v>
+      </c>
+      <c r="F84" s="56" t="s">
+        <v>432</v>
+      </c>
+      <c r="G84" s="56" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A85" s="56" t="s">
+        <v>1</v>
+      </c>
+      <c r="B85" s="46" t="s">
+        <v>433</v>
+      </c>
+      <c r="C85" s="56" t="s">
+        <v>65</v>
+      </c>
+      <c r="D85" s="56">
+        <v>0</v>
+      </c>
+      <c r="E85" s="46" t="s">
+        <v>87</v>
+      </c>
+      <c r="F85" s="56"/>
+      <c r="G85" s="58" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A86" s="56" t="s">
+        <v>1</v>
+      </c>
+      <c r="B86" s="46" t="s">
+        <v>434</v>
+      </c>
+      <c r="C86" s="56" t="s">
+        <v>65</v>
+      </c>
+      <c r="D86" s="56">
+        <v>2</v>
+      </c>
+      <c r="E86" s="46" t="s">
+        <v>87</v>
+      </c>
+      <c r="F86" s="56"/>
+      <c r="G86" s="58" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A87" s="56" t="s">
+        <v>1</v>
+      </c>
+      <c r="B87" s="46" t="s">
+        <v>435</v>
+      </c>
+      <c r="C87" s="56" t="s">
+        <v>65</v>
+      </c>
+      <c r="D87" s="56">
+        <v>1</v>
+      </c>
+      <c r="E87" s="46" t="s">
+        <v>87</v>
+      </c>
+      <c r="F87" s="56"/>
+      <c r="G87" s="58" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A88" s="56" t="s">
+        <v>1</v>
+      </c>
+      <c r="B88" s="46" t="s">
+        <v>436</v>
+      </c>
+      <c r="C88" s="56" t="s">
+        <v>50</v>
+      </c>
+      <c r="D88" s="56">
+        <v>0</v>
+      </c>
+      <c r="E88" s="46" t="s">
+        <v>439</v>
+      </c>
+      <c r="F88" s="56" t="s">
+        <v>440</v>
+      </c>
+      <c r="G88" s="58" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A89" s="56" t="s">
+        <v>1</v>
+      </c>
+      <c r="B89" s="46" t="s">
+        <v>437</v>
+      </c>
+      <c r="C89" s="56" t="s">
+        <v>50</v>
+      </c>
+      <c r="D89" s="56">
+        <v>2</v>
+      </c>
+      <c r="E89" s="46" t="s">
+        <v>439</v>
+      </c>
+      <c r="F89" s="56" t="s">
+        <v>440</v>
+      </c>
+      <c r="G89" s="58" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A90" s="56" t="s">
+        <v>1</v>
+      </c>
+      <c r="B90" s="46" t="s">
+        <v>438</v>
+      </c>
+      <c r="C90" s="56" t="s">
+        <v>50</v>
+      </c>
+      <c r="D90" s="56">
+        <v>1</v>
+      </c>
+      <c r="E90" s="46" t="s">
+        <v>439</v>
+      </c>
+      <c r="F90" s="56" t="s">
+        <v>440</v>
+      </c>
+      <c r="G90" s="58" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A91" s="56" t="s">
+        <v>1</v>
+      </c>
+      <c r="B91" s="46" t="s">
+        <v>441</v>
+      </c>
+      <c r="C91" s="56" t="s">
+        <v>50</v>
+      </c>
+      <c r="D91" s="56">
+        <v>0</v>
+      </c>
+      <c r="E91" s="46" t="s">
+        <v>444</v>
+      </c>
+      <c r="F91" s="56"/>
+      <c r="G91" s="58" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A92" s="56" t="s">
+        <v>1</v>
+      </c>
+      <c r="B92" s="46" t="s">
+        <v>442</v>
+      </c>
+      <c r="C92" s="56" t="s">
+        <v>50</v>
+      </c>
+      <c r="D92" s="56">
+        <v>2</v>
+      </c>
+      <c r="E92" s="46" t="s">
+        <v>444</v>
+      </c>
+      <c r="F92" s="56"/>
+      <c r="G92" s="58" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A93" s="56" t="s">
+        <v>1</v>
+      </c>
+      <c r="B93" s="46" t="s">
+        <v>443</v>
+      </c>
+      <c r="C93" s="56" t="s">
+        <v>50</v>
+      </c>
+      <c r="D93" s="56">
+        <v>1</v>
+      </c>
+      <c r="E93" s="46" t="s">
+        <v>444</v>
+      </c>
+      <c r="F93" s="56"/>
+      <c r="G93" s="58" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A94" s="56" t="s">
+        <v>1</v>
+      </c>
+      <c r="B94" s="46" t="s">
+        <v>445</v>
+      </c>
+      <c r="C94" s="56" t="s">
+        <v>237</v>
+      </c>
+      <c r="D94" s="56">
+        <v>0</v>
+      </c>
+      <c r="E94" s="46" t="s">
+        <v>448</v>
+      </c>
+      <c r="F94" s="56"/>
+      <c r="G94" s="58" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A95" s="56" t="s">
+        <v>1</v>
+      </c>
+      <c r="B95" s="46" t="s">
+        <v>446</v>
+      </c>
+      <c r="C95" s="56" t="s">
+        <v>237</v>
+      </c>
+      <c r="D95" s="56">
+        <v>2</v>
+      </c>
+      <c r="E95" s="46" t="s">
+        <v>448</v>
+      </c>
+      <c r="F95" s="56"/>
+      <c r="G95" s="58" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A96" s="56" t="s">
+        <v>1</v>
+      </c>
+      <c r="B96" s="46" t="s">
+        <v>447</v>
+      </c>
+      <c r="C96" s="56" t="s">
+        <v>237</v>
+      </c>
+      <c r="D96" s="56">
+        <v>1</v>
+      </c>
+      <c r="E96" s="46" t="s">
+        <v>448</v>
+      </c>
+      <c r="F96" s="56"/>
+      <c r="G96" s="58" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A97" s="56" t="s">
+        <v>1</v>
+      </c>
+      <c r="B97" s="46" t="s">
+        <v>449</v>
+      </c>
+      <c r="C97" s="56" t="s">
+        <v>452</v>
+      </c>
+      <c r="D97" s="56">
+        <v>0</v>
+      </c>
+      <c r="E97" s="56"/>
+      <c r="F97" s="56" t="s">
+        <v>380</v>
+      </c>
+      <c r="G97" s="56" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A98" s="56" t="s">
+        <v>1</v>
+      </c>
+      <c r="B98" s="46" t="s">
+        <v>450</v>
+      </c>
+      <c r="C98" s="56" t="s">
+        <v>452</v>
+      </c>
+      <c r="D98" s="56">
+        <v>2</v>
+      </c>
+      <c r="E98" s="56"/>
+      <c r="F98" s="56" t="s">
+        <v>380</v>
+      </c>
+      <c r="G98" s="56" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A99" s="56" t="s">
+        <v>1</v>
+      </c>
+      <c r="B99" s="46" t="s">
+        <v>451</v>
+      </c>
+      <c r="C99" s="56" t="s">
+        <v>452</v>
+      </c>
+      <c r="D99" s="56">
+        <v>1</v>
+      </c>
+      <c r="E99" s="56"/>
+      <c r="F99" s="56" t="s">
+        <v>380</v>
+      </c>
+      <c r="G99" s="56" t="s">
+        <v>453</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added new categories for tournament filters!
Former-commit-id: 6d4bbe68c2ad907eb43a85b8951cc5149cc816be
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Missions.xlsx
+++ b/Docs/Content/HungryDragonContent_Missions.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1061" uniqueCount="454">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1049" uniqueCount="453">
   <si>
     <t>single_run</t>
   </si>
@@ -1192,9 +1192,6 @@
   </si>
   <si>
     <t>TID_EVENT_TOURNAMENT_KILL_IN_LOVE_TIME_ATTACK_ALL</t>
-  </si>
-  <si>
-    <t>NPCs</t>
   </si>
   <si>
     <t>TID_EVENT_TOURNAMENT_KILL_NORMAL_HUMANS</t>
@@ -1857,13 +1854,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1874,21 +1864,18 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="69">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
@@ -3040,6 +3027,16 @@
         </bottom>
       </border>
     </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -3054,99 +3051,99 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="missionDifficultyDefinitions" displayName="missionDifficultyDefinitions" ref="B73:L76" totalsRowShown="0" headerRowBorderDxfId="68" tableBorderDxfId="67">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="missionDifficultyDefinitions" displayName="missionDifficultyDefinitions" ref="B73:L76" totalsRowShown="0" headerRowBorderDxfId="67" tableBorderDxfId="66">
   <autoFilter ref="B73:L76"/>
   <tableColumns count="11">
     <tableColumn id="1" name="{missionDifficultyDefinitions}"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="66"/>
-    <tableColumn id="11" name="[difficulty]" dataDxfId="65"/>
-    <tableColumn id="7" name="[index]" dataDxfId="64"/>
-    <tableColumn id="3" name="[dragonsToUnlock]" dataDxfId="63"/>
-    <tableColumn id="4" name="[cooldownMinutes]" dataDxfId="62"/>
-    <tableColumn id="9" name="[maxRewardCoins]" dataDxfId="61"/>
-    <tableColumn id="5" name="[removeMissionPCCoefA]" dataDxfId="60"/>
-    <tableColumn id="6" name="[removeMissionPCCoefB]" dataDxfId="59"/>
-    <tableColumn id="8" name="[tidName]" dataDxfId="58"/>
-    <tableColumn id="10" name="[color]" dataDxfId="57"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="65"/>
+    <tableColumn id="11" name="[difficulty]" dataDxfId="64"/>
+    <tableColumn id="7" name="[index]" dataDxfId="63"/>
+    <tableColumn id="3" name="[dragonsToUnlock]" dataDxfId="62"/>
+    <tableColumn id="4" name="[cooldownMinutes]" dataDxfId="61"/>
+    <tableColumn id="9" name="[maxRewardCoins]" dataDxfId="60"/>
+    <tableColumn id="5" name="[removeMissionPCCoefA]" dataDxfId="59"/>
+    <tableColumn id="6" name="[removeMissionPCCoefB]" dataDxfId="58"/>
+    <tableColumn id="8" name="[tidName]" dataDxfId="57"/>
+    <tableColumn id="10" name="[color]" dataDxfId="56"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table13303132" displayName="Table13303132" ref="B81:E94" totalsRowShown="0" headerRowDxfId="56" dataDxfId="54" headerRowBorderDxfId="55" tableBorderDxfId="53" totalsRowBorderDxfId="52">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table13303132" displayName="Table13303132" ref="B81:E94" totalsRowShown="0" headerRowDxfId="55" dataDxfId="53" headerRowBorderDxfId="54" tableBorderDxfId="52" totalsRowBorderDxfId="51">
   <autoFilter ref="B81:E94"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="{missionDragonModifiersDefinitions}" dataDxfId="51"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="50"/>
-    <tableColumn id="7" name="[quantityModifier]" dataDxfId="49"/>
-    <tableColumn id="3" name="[missionSCRewardMultiplier]" dataDxfId="48"/>
+    <tableColumn id="1" name="{missionDragonModifiersDefinitions}" dataDxfId="50"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="49"/>
+    <tableColumn id="7" name="[quantityModifier]" dataDxfId="48"/>
+    <tableColumn id="3" name="[missionSCRewardMultiplier]" dataDxfId="47"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table1330313234" displayName="Table1330313234" ref="B98:E101" totalsRowShown="0" headerRowDxfId="47" dataDxfId="45" headerRowBorderDxfId="46" tableBorderDxfId="44" totalsRowBorderDxfId="43">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table1330313234" displayName="Table1330313234" ref="B98:E101" totalsRowShown="0" headerRowDxfId="46" dataDxfId="44" headerRowBorderDxfId="45" tableBorderDxfId="43" totalsRowBorderDxfId="42">
   <autoFilter ref="B98:E101"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="{missionDifficultyModifiersDefinitions}" dataDxfId="42"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="41"/>
-    <tableColumn id="3" name="[difficulty]" dataDxfId="40"/>
-    <tableColumn id="7" name="[quantityModifier]" dataDxfId="39"/>
+    <tableColumn id="1" name="{missionDifficultyModifiersDefinitions}" dataDxfId="41"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="40"/>
+    <tableColumn id="3" name="[difficulty]" dataDxfId="39"/>
+    <tableColumn id="7" name="[quantityModifier]" dataDxfId="38"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table133031323435" displayName="Table133031323435" ref="B105:D106" totalsRowShown="0" headerRowDxfId="38" dataDxfId="36" headerRowBorderDxfId="37" tableBorderDxfId="35" totalsRowBorderDxfId="34">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table133031323435" displayName="Table133031323435" ref="B105:D106" totalsRowShown="0" headerRowDxfId="37" dataDxfId="35" headerRowBorderDxfId="36" tableBorderDxfId="34" totalsRowBorderDxfId="33">
   <autoFilter ref="B105:D106"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="{missionOtherModifiersDefinitions}" dataDxfId="33"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="32"/>
-    <tableColumn id="7" name="[quantityModifier]" dataDxfId="31"/>
+    <tableColumn id="1" name="{missionOtherModifiersDefinitions}" dataDxfId="32"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="31"/>
+    <tableColumn id="7" name="[quantityModifier]" dataDxfId="30"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table13" displayName="Table13" ref="B48:H67" totalsRowShown="0" headerRowDxfId="30" dataDxfId="28" headerRowBorderDxfId="29" tableBorderDxfId="27" totalsRowBorderDxfId="26">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table13" displayName="Table13" ref="B48:H67" totalsRowShown="0" headerRowDxfId="29" dataDxfId="27" headerRowBorderDxfId="28" tableBorderDxfId="26" totalsRowBorderDxfId="25">
   <autoFilter ref="B48:H67"/>
   <tableColumns count="7">
-    <tableColumn id="1" name="{missionTypeDefinitions}" dataDxfId="25"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="24"/>
-    <tableColumn id="3" name="[minTier]" dataDxfId="23"/>
-    <tableColumn id="6" name="[maxTier]" dataDxfId="22"/>
-    <tableColumn id="4" name="[weight]" dataDxfId="21"/>
-    <tableColumn id="9" name="[tidDescSingleRun]" dataDxfId="20"/>
-    <tableColumn id="10" name="[tidDescMultiRun]" dataDxfId="19"/>
+    <tableColumn id="1" name="{missionTypeDefinitions}" dataDxfId="24"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="23"/>
+    <tableColumn id="3" name="[minTier]" dataDxfId="22"/>
+    <tableColumn id="6" name="[maxTier]" dataDxfId="21"/>
+    <tableColumn id="4" name="[weight]" dataDxfId="20"/>
+    <tableColumn id="9" name="[tidDescSingleRun]" dataDxfId="19"/>
+    <tableColumn id="10" name="[tidDescMultiRun]" dataDxfId="18"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table1330" displayName="Table1330" ref="B4:N43" totalsRowShown="0" headerRowDxfId="18" dataDxfId="16" headerRowBorderDxfId="17" tableBorderDxfId="15" totalsRowBorderDxfId="14">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table1330" displayName="Table1330" ref="B4:N43" totalsRowShown="0" headerRowDxfId="17" dataDxfId="15" headerRowBorderDxfId="16" tableBorderDxfId="14" totalsRowBorderDxfId="13">
   <autoFilter ref="B4:N43"/>
   <sortState ref="B5:P43">
     <sortCondition descending="1" ref="J4:J43"/>
   </sortState>
   <tableColumns count="13">
-    <tableColumn id="1" name="{missionsDefinitions}" dataDxfId="13"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="12"/>
-    <tableColumn id="7" name="[type]" dataDxfId="11"/>
-    <tableColumn id="8" name="[weight]" dataDxfId="10"/>
-    <tableColumn id="13" name="[singleRunChance]" dataDxfId="9"/>
-    <tableColumn id="11" name="[minTier]" dataDxfId="8"/>
-    <tableColumn id="12" name="[maxTier]" dataDxfId="7"/>
-    <tableColumn id="6" name="[params]" dataDxfId="6"/>
-    <tableColumn id="3" name="[objectiveBaseQuantityMin]" dataDxfId="5"/>
-    <tableColumn id="9" name="[objectiveBaseQuantityMax]" dataDxfId="4"/>
-    <tableColumn id="4" name="[icon]" dataDxfId="3"/>
-    <tableColumn id="5" name="[tidObjective]" dataDxfId="2"/>
-    <tableColumn id="10" name="[trackingSku]" dataDxfId="1">
+    <tableColumn id="1" name="{missionsDefinitions}" dataDxfId="12"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="11"/>
+    <tableColumn id="7" name="[type]" dataDxfId="10"/>
+    <tableColumn id="8" name="[weight]" dataDxfId="9"/>
+    <tableColumn id="13" name="[singleRunChance]" dataDxfId="8"/>
+    <tableColumn id="11" name="[minTier]" dataDxfId="7"/>
+    <tableColumn id="12" name="[maxTier]" dataDxfId="6"/>
+    <tableColumn id="6" name="[params]" dataDxfId="5"/>
+    <tableColumn id="3" name="[objectiveBaseQuantityMin]" dataDxfId="4"/>
+    <tableColumn id="9" name="[objectiveBaseQuantityMax]" dataDxfId="3"/>
+    <tableColumn id="4" name="[icon]" dataDxfId="2"/>
+    <tableColumn id="5" name="[tidObjective]" dataDxfId="1"/>
+    <tableColumn id="10" name="[trackingSku]" dataDxfId="0">
       <calculatedColumnFormula>Table1330[[#This Row],['[sku']]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -3470,14 +3467,14 @@
         <v>140</v>
       </c>
       <c r="G3" s="38"/>
-      <c r="J3" s="53" t="s">
+      <c r="J3" s="57" t="s">
         <v>139</v>
       </c>
-      <c r="K3" s="53"/>
-      <c r="M3" s="53"/>
-      <c r="N3" s="53"/>
-      <c r="O3" s="53"/>
-      <c r="P3" s="53"/>
+      <c r="K3" s="57"/>
+      <c r="M3" s="57"/>
+      <c r="N3" s="57"/>
+      <c r="O3" s="57"/>
+      <c r="P3" s="57"/>
     </row>
     <row r="4" spans="2:16" ht="106.5" x14ac:dyDescent="0.25">
       <c r="B4" s="30" t="s">
@@ -5157,9 +5154,9 @@
       <c r="C47" s="20"/>
       <c r="D47" s="20"/>
       <c r="E47" s="20"/>
-      <c r="F47" s="54"/>
-      <c r="G47" s="54"/>
-      <c r="H47" s="54"/>
+      <c r="F47" s="58"/>
+      <c r="G47" s="58"/>
+      <c r="H47" s="58"/>
       <c r="I47" s="20"/>
       <c r="J47" s="20"/>
     </row>
@@ -5688,10 +5685,10 @@
       <c r="F72" s="21" t="s">
         <v>40</v>
       </c>
-      <c r="G72" s="55" t="s">
+      <c r="G72" s="59" t="s">
         <v>39</v>
       </c>
-      <c r="H72" s="55"/>
+      <c r="H72" s="59"/>
       <c r="I72" s="20"/>
     </row>
     <row r="73" spans="2:13" ht="142.5" x14ac:dyDescent="0.25">
@@ -6902,7 +6899,7 @@
     <mergeCell ref="G72:H72"/>
   </mergeCells>
   <conditionalFormatting sqref="C74:E76">
-    <cfRule type="duplicateValues" dxfId="0" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="68" priority="2"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -6921,8 +6918,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G99"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6981,2040 +6978,2016 @@
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="56" t="s">
+      <c r="A5" s="53" t="s">
         <v>1</v>
       </c>
       <c r="B5" s="46" t="s">
         <v>322</v>
       </c>
-      <c r="C5" s="56" t="s">
+      <c r="C5" s="53" t="s">
         <v>65</v>
       </c>
-      <c r="D5" s="56">
+      <c r="D5" s="53">
         <v>0</v>
       </c>
       <c r="E5" s="46" t="s">
         <v>81</v>
       </c>
-      <c r="F5" s="56" t="s">
+      <c r="F5" s="53" t="s">
         <v>324</v>
       </c>
-      <c r="G5" s="59" t="s">
+      <c r="G5" s="56" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="56" t="s">
+      <c r="A6" s="53" t="s">
         <v>1</v>
       </c>
       <c r="B6" s="46" t="s">
         <v>325</v>
       </c>
-      <c r="C6" s="56" t="s">
+      <c r="C6" s="53" t="s">
         <v>65</v>
       </c>
-      <c r="D6" s="56">
+      <c r="D6" s="53">
         <v>2</v>
       </c>
       <c r="E6" s="46" t="s">
         <v>81</v>
       </c>
-      <c r="F6" s="56" t="s">
+      <c r="F6" s="53" t="s">
         <v>324</v>
       </c>
-      <c r="G6" s="59" t="s">
+      <c r="G6" s="56" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="56" t="s">
+      <c r="A7" s="53" t="s">
         <v>1</v>
       </c>
       <c r="B7" s="46" t="s">
         <v>326</v>
       </c>
-      <c r="C7" s="56" t="s">
+      <c r="C7" s="53" t="s">
         <v>65</v>
       </c>
-      <c r="D7" s="56">
+      <c r="D7" s="53">
         <v>1</v>
       </c>
       <c r="E7" s="46" t="s">
         <v>81</v>
       </c>
-      <c r="F7" s="56" t="s">
+      <c r="F7" s="53" t="s">
         <v>324</v>
       </c>
-      <c r="G7" s="59" t="s">
+      <c r="G7" s="56" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="56" t="s">
+      <c r="A8" s="53" t="s">
         <v>1</v>
       </c>
       <c r="B8" s="46" t="s">
         <v>327</v>
       </c>
-      <c r="C8" s="56" t="s">
+      <c r="C8" s="53" t="s">
         <v>65</v>
       </c>
-      <c r="D8" s="56">
+      <c r="D8" s="53">
         <v>0</v>
       </c>
       <c r="E8" s="46" t="s">
         <v>328</v>
       </c>
-      <c r="F8" s="56" t="s">
+      <c r="F8" s="53" t="s">
         <v>329</v>
       </c>
-      <c r="G8" s="59" t="s">
+      <c r="G8" s="56" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="56" t="s">
+      <c r="A9" s="53" t="s">
         <v>1</v>
       </c>
       <c r="B9" s="46" t="s">
         <v>330</v>
       </c>
-      <c r="C9" s="56" t="s">
+      <c r="C9" s="53" t="s">
         <v>65</v>
       </c>
-      <c r="D9" s="56">
+      <c r="D9" s="53">
         <v>2</v>
       </c>
       <c r="E9" s="46" t="s">
         <v>328</v>
       </c>
-      <c r="F9" s="56" t="s">
+      <c r="F9" s="53" t="s">
         <v>329</v>
       </c>
-      <c r="G9" s="59" t="s">
+      <c r="G9" s="56" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="56" t="s">
+      <c r="A10" s="53" t="s">
         <v>1</v>
       </c>
       <c r="B10" s="46" t="s">
         <v>331</v>
       </c>
-      <c r="C10" s="56" t="s">
+      <c r="C10" s="53" t="s">
         <v>65</v>
       </c>
-      <c r="D10" s="56">
+      <c r="D10" s="53">
         <v>1</v>
       </c>
       <c r="E10" s="46" t="s">
         <v>328</v>
       </c>
-      <c r="F10" s="56" t="s">
+      <c r="F10" s="53" t="s">
         <v>329</v>
       </c>
-      <c r="G10" s="59" t="s">
+      <c r="G10" s="56" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="56" t="s">
+      <c r="A11" s="53" t="s">
         <v>1</v>
       </c>
       <c r="B11" s="46" t="s">
         <v>332</v>
       </c>
-      <c r="C11" s="56" t="s">
+      <c r="C11" s="53" t="s">
         <v>65</v>
       </c>
-      <c r="D11" s="56">
+      <c r="D11" s="53">
         <v>0</v>
       </c>
       <c r="E11" s="46" t="s">
         <v>333</v>
       </c>
-      <c r="F11" s="56" t="s">
+      <c r="F11" s="53" t="s">
         <v>334</v>
       </c>
-      <c r="G11" s="59" t="s">
+      <c r="G11" s="56" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="56" t="s">
+      <c r="A12" s="53" t="s">
         <v>1</v>
       </c>
       <c r="B12" s="46" t="s">
         <v>335</v>
       </c>
-      <c r="C12" s="56" t="s">
+      <c r="C12" s="53" t="s">
         <v>65</v>
       </c>
-      <c r="D12" s="56">
+      <c r="D12" s="53">
         <v>2</v>
       </c>
       <c r="E12" s="46" t="s">
         <v>333</v>
       </c>
-      <c r="F12" s="56" t="s">
+      <c r="F12" s="53" t="s">
         <v>334</v>
       </c>
-      <c r="G12" s="59" t="s">
+      <c r="G12" s="56" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="56" t="s">
+      <c r="A13" s="53" t="s">
         <v>1</v>
       </c>
       <c r="B13" s="46" t="s">
         <v>336</v>
       </c>
-      <c r="C13" s="56" t="s">
+      <c r="C13" s="53" t="s">
         <v>65</v>
       </c>
-      <c r="D13" s="56">
+      <c r="D13" s="53">
         <v>1</v>
       </c>
       <c r="E13" s="46" t="s">
         <v>333</v>
       </c>
-      <c r="F13" s="56" t="s">
+      <c r="F13" s="53" t="s">
         <v>334</v>
       </c>
-      <c r="G13" s="59" t="s">
+      <c r="G13" s="56" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="56" t="s">
+      <c r="A14" s="53" t="s">
         <v>1</v>
       </c>
       <c r="B14" s="46" t="s">
         <v>337</v>
       </c>
-      <c r="C14" s="56" t="s">
+      <c r="C14" s="53" t="s">
         <v>53</v>
       </c>
-      <c r="D14" s="56">
-        <v>0</v>
-      </c>
-      <c r="E14" s="56"/>
-      <c r="F14" s="56"/>
-      <c r="G14" s="59" t="s">
+      <c r="D14" s="53">
+        <v>0</v>
+      </c>
+      <c r="E14" s="53"/>
+      <c r="F14" s="53"/>
+      <c r="G14" s="56" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="56" t="s">
+      <c r="A15" s="53" t="s">
         <v>1</v>
       </c>
       <c r="B15" s="46" t="s">
         <v>338</v>
       </c>
-      <c r="C15" s="56" t="s">
+      <c r="C15" s="53" t="s">
         <v>180</v>
       </c>
-      <c r="D15" s="56">
+      <c r="D15" s="53">
         <v>0</v>
       </c>
       <c r="E15" s="46" t="s">
         <v>119</v>
       </c>
-      <c r="F15" s="56" t="s">
+      <c r="F15" s="53" t="s">
         <v>339</v>
       </c>
-      <c r="G15" s="59" t="s">
+      <c r="G15" s="56" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="56" t="s">
+      <c r="A16" s="53" t="s">
         <v>1</v>
       </c>
       <c r="B16" s="46" t="s">
         <v>340</v>
       </c>
-      <c r="C16" s="56" t="s">
+      <c r="C16" s="53" t="s">
         <v>180</v>
       </c>
-      <c r="D16" s="56">
+      <c r="D16" s="53">
         <v>2</v>
       </c>
       <c r="E16" s="46" t="s">
         <v>119</v>
       </c>
-      <c r="F16" s="56" t="s">
+      <c r="F16" s="53" t="s">
         <v>339</v>
       </c>
-      <c r="G16" s="59" t="s">
+      <c r="G16" s="56" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="56" t="s">
+      <c r="A17" s="53" t="s">
         <v>1</v>
       </c>
       <c r="B17" s="46" t="s">
         <v>341</v>
       </c>
-      <c r="C17" s="56" t="s">
+      <c r="C17" s="53" t="s">
         <v>180</v>
       </c>
-      <c r="D17" s="56">
+      <c r="D17" s="53">
         <v>1</v>
       </c>
       <c r="E17" s="46" t="s">
         <v>119</v>
       </c>
-      <c r="F17" s="56" t="s">
+      <c r="F17" s="53" t="s">
         <v>339</v>
       </c>
-      <c r="G17" s="59" t="s">
+      <c r="G17" s="56" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="56" t="s">
+      <c r="A18" s="53" t="s">
         <v>1</v>
       </c>
       <c r="B18" s="46" t="s">
         <v>342</v>
       </c>
-      <c r="C18" s="56" t="s">
+      <c r="C18" s="53" t="s">
         <v>65</v>
       </c>
-      <c r="D18" s="56">
+      <c r="D18" s="53">
         <v>0</v>
       </c>
       <c r="E18" s="46" t="s">
         <v>345</v>
       </c>
-      <c r="F18" s="56" t="s">
+      <c r="F18" s="53" t="s">
         <v>346</v>
       </c>
-      <c r="G18" s="59" t="s">
+      <c r="G18" s="56" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="56" t="s">
+      <c r="A19" s="53" t="s">
         <v>1</v>
       </c>
       <c r="B19" s="46" t="s">
         <v>343</v>
       </c>
-      <c r="C19" s="56" t="s">
+      <c r="C19" s="53" t="s">
         <v>65</v>
       </c>
-      <c r="D19" s="56">
+      <c r="D19" s="53">
         <v>2</v>
       </c>
       <c r="E19" s="46" t="s">
         <v>345</v>
       </c>
-      <c r="F19" s="56" t="s">
+      <c r="F19" s="53" t="s">
         <v>346</v>
       </c>
-      <c r="G19" s="59" t="s">
+      <c r="G19" s="56" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="56" t="s">
+      <c r="A20" s="53" t="s">
         <v>1</v>
       </c>
       <c r="B20" s="46" t="s">
         <v>344</v>
       </c>
-      <c r="C20" s="56" t="s">
+      <c r="C20" s="53" t="s">
         <v>65</v>
       </c>
-      <c r="D20" s="56">
+      <c r="D20" s="53">
         <v>1</v>
       </c>
       <c r="E20" s="46" t="s">
         <v>345</v>
       </c>
-      <c r="F20" s="56" t="s">
+      <c r="F20" s="53" t="s">
         <v>346</v>
       </c>
-      <c r="G20" s="59" t="s">
+      <c r="G20" s="56" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="56" t="s">
+      <c r="A21" s="53" t="s">
         <v>1</v>
       </c>
       <c r="B21" s="46" t="s">
         <v>347</v>
       </c>
-      <c r="C21" s="56" t="s">
+      <c r="C21" s="53" t="s">
         <v>65</v>
       </c>
-      <c r="D21" s="56">
+      <c r="D21" s="53">
         <v>0</v>
       </c>
       <c r="E21" s="46" t="s">
-        <v>426</v>
-      </c>
-      <c r="F21" s="56"/>
-      <c r="G21" s="58" t="s">
+        <v>425</v>
+      </c>
+      <c r="F21" s="53"/>
+      <c r="G21" s="55" t="s">
         <v>254</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="56" t="s">
+      <c r="A22" s="53" t="s">
         <v>1</v>
       </c>
       <c r="B22" s="46" t="s">
         <v>348</v>
       </c>
-      <c r="C22" s="56" t="s">
+      <c r="C22" s="53" t="s">
         <v>65</v>
       </c>
-      <c r="D22" s="56">
+      <c r="D22" s="53">
         <v>2</v>
       </c>
       <c r="E22" s="46" t="s">
-        <v>426</v>
-      </c>
-      <c r="F22" s="56"/>
-      <c r="G22" s="58" t="s">
+        <v>425</v>
+      </c>
+      <c r="F22" s="53"/>
+      <c r="G22" s="55" t="s">
         <v>254</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="56" t="s">
+      <c r="A23" s="53" t="s">
         <v>1</v>
       </c>
       <c r="B23" s="46" t="s">
         <v>349</v>
       </c>
-      <c r="C23" s="56" t="s">
+      <c r="C23" s="53" t="s">
         <v>65</v>
       </c>
-      <c r="D23" s="56">
+      <c r="D23" s="53">
         <v>1</v>
       </c>
       <c r="E23" s="46" t="s">
-        <v>426</v>
-      </c>
-      <c r="F23" s="56"/>
-      <c r="G23" s="58" t="s">
+        <v>425</v>
+      </c>
+      <c r="F23" s="53"/>
+      <c r="G23" s="55" t="s">
         <v>254</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="56" t="s">
+      <c r="A24" s="53" t="s">
         <v>1</v>
       </c>
       <c r="B24" s="46" t="s">
         <v>350</v>
       </c>
-      <c r="C24" s="56" t="s">
+      <c r="C24" s="53" t="s">
         <v>50</v>
       </c>
-      <c r="D24" s="56">
+      <c r="D24" s="53">
         <v>0</v>
       </c>
       <c r="E24" s="46" t="s">
         <v>352</v>
       </c>
-      <c r="F24" s="56"/>
-      <c r="G24" s="59" t="s">
+      <c r="F24" s="53"/>
+      <c r="G24" s="56" t="s">
         <v>245</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="56" t="s">
+      <c r="A25" s="53" t="s">
         <v>1</v>
       </c>
       <c r="B25" s="46" t="s">
         <v>351</v>
       </c>
-      <c r="C25" s="56" t="s">
+      <c r="C25" s="53" t="s">
         <v>50</v>
       </c>
-      <c r="D25" s="56">
+      <c r="D25" s="53">
         <v>2</v>
       </c>
       <c r="E25" s="46" t="s">
         <v>352</v>
       </c>
-      <c r="F25" s="56"/>
-      <c r="G25" s="59" t="s">
+      <c r="F25" s="53"/>
+      <c r="G25" s="56" t="s">
         <v>245</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="56" t="s">
+      <c r="A26" s="53" t="s">
         <v>1</v>
       </c>
       <c r="B26" s="46" t="s">
         <v>353</v>
       </c>
-      <c r="C26" s="56" t="s">
+      <c r="C26" s="53" t="s">
         <v>62</v>
       </c>
-      <c r="D26" s="56">
+      <c r="D26" s="53">
         <v>2</v>
       </c>
-      <c r="E26" s="56"/>
-      <c r="F26" s="56"/>
-      <c r="G26" s="59" t="s">
+      <c r="E26" s="53"/>
+      <c r="F26" s="53"/>
+      <c r="G26" s="56" t="s">
         <v>246</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="56" t="s">
+      <c r="A27" s="53" t="s">
         <v>1</v>
       </c>
       <c r="B27" s="46" t="s">
         <v>354</v>
       </c>
-      <c r="C27" s="56" t="s">
+      <c r="C27" s="53" t="s">
         <v>62</v>
       </c>
-      <c r="D27" s="56">
-        <v>1</v>
-      </c>
-      <c r="E27" s="56"/>
-      <c r="F27" s="56"/>
-      <c r="G27" s="59" t="s">
+      <c r="D27" s="53">
+        <v>1</v>
+      </c>
+      <c r="E27" s="53"/>
+      <c r="F27" s="53"/>
+      <c r="G27" s="56" t="s">
         <v>246</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="56" t="s">
+      <c r="A28" s="53" t="s">
         <v>1</v>
       </c>
       <c r="B28" s="46" t="s">
         <v>355</v>
       </c>
-      <c r="C28" s="56" t="s">
+      <c r="C28" s="53" t="s">
         <v>62</v>
       </c>
-      <c r="D28" s="56">
+      <c r="D28" s="53">
         <v>2</v>
       </c>
-      <c r="E28" s="56"/>
-      <c r="F28" s="56"/>
-      <c r="G28" s="59" t="s">
+      <c r="E28" s="53"/>
+      <c r="F28" s="53"/>
+      <c r="G28" s="56" t="s">
         <v>246</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" s="56" t="s">
+      <c r="A29" s="53" t="s">
         <v>1</v>
       </c>
       <c r="B29" s="46" t="s">
         <v>356</v>
       </c>
-      <c r="C29" s="56" t="s">
+      <c r="C29" s="53" t="s">
         <v>65</v>
       </c>
-      <c r="D29" s="56">
+      <c r="D29" s="53">
         <v>0</v>
       </c>
       <c r="E29" s="46" t="s">
         <v>359</v>
       </c>
-      <c r="F29" s="56" t="s">
+      <c r="F29" s="53" t="s">
         <v>360</v>
       </c>
-      <c r="G29" s="56" t="s">
+      <c r="G29" s="53" t="s">
         <v>361</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" s="56" t="s">
+      <c r="A30" s="53" t="s">
         <v>1</v>
       </c>
       <c r="B30" s="46" t="s">
         <v>357</v>
       </c>
-      <c r="C30" s="56" t="s">
+      <c r="C30" s="53" t="s">
         <v>65</v>
       </c>
-      <c r="D30" s="56">
+      <c r="D30" s="53">
         <v>1</v>
       </c>
       <c r="E30" s="46" t="s">
         <v>359</v>
       </c>
-      <c r="F30" s="56" t="s">
+      <c r="F30" s="53" t="s">
         <v>360</v>
       </c>
-      <c r="G30" s="56" t="s">
+      <c r="G30" s="53" t="s">
         <v>361</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A31" s="56" t="s">
+      <c r="A31" s="53" t="s">
         <v>1</v>
       </c>
       <c r="B31" s="46" t="s">
         <v>358</v>
       </c>
-      <c r="C31" s="56" t="s">
+      <c r="C31" s="53" t="s">
         <v>65</v>
       </c>
-      <c r="D31" s="56">
+      <c r="D31" s="53">
         <v>2</v>
       </c>
       <c r="E31" s="46" t="s">
         <v>359</v>
       </c>
-      <c r="F31" s="56" t="s">
+      <c r="F31" s="53" t="s">
         <v>360</v>
       </c>
-      <c r="G31" s="56" t="s">
+      <c r="G31" s="53" t="s">
         <v>361</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32" s="56" t="s">
+      <c r="A32" s="53" t="s">
         <v>1</v>
       </c>
       <c r="B32" s="46" t="s">
         <v>362</v>
       </c>
-      <c r="C32" s="56" t="s">
+      <c r="C32" s="53" t="s">
         <v>65</v>
       </c>
-      <c r="D32" s="56">
+      <c r="D32" s="53">
         <v>0</v>
       </c>
       <c r="E32" s="46" t="s">
         <v>365</v>
       </c>
-      <c r="F32" s="56" t="s">
+      <c r="F32" s="53" t="s">
         <v>366</v>
       </c>
-      <c r="G32" s="56" t="s">
+      <c r="G32" s="53" t="s">
         <v>367</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A33" s="56" t="s">
+      <c r="A33" s="53" t="s">
         <v>1</v>
       </c>
       <c r="B33" s="46" t="s">
         <v>363</v>
       </c>
-      <c r="C33" s="56" t="s">
+      <c r="C33" s="53" t="s">
         <v>65</v>
       </c>
-      <c r="D33" s="56">
+      <c r="D33" s="53">
         <v>2</v>
       </c>
       <c r="E33" s="46" t="s">
         <v>365</v>
       </c>
-      <c r="F33" s="56" t="s">
+      <c r="F33" s="53" t="s">
         <v>366</v>
       </c>
-      <c r="G33" s="56" t="s">
+      <c r="G33" s="53" t="s">
         <v>367</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A34" s="56" t="s">
+      <c r="A34" s="53" t="s">
         <v>1</v>
       </c>
       <c r="B34" s="46" t="s">
         <v>364</v>
       </c>
-      <c r="C34" s="56" t="s">
+      <c r="C34" s="53" t="s">
         <v>65</v>
       </c>
-      <c r="D34" s="56">
+      <c r="D34" s="53">
         <v>1</v>
       </c>
       <c r="E34" s="46" t="s">
         <v>365</v>
       </c>
-      <c r="F34" s="56" t="s">
+      <c r="F34" s="53" t="s">
         <v>366</v>
       </c>
-      <c r="G34" s="56" t="s">
+      <c r="G34" s="53" t="s">
         <v>367</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A35" s="56" t="s">
+      <c r="A35" s="53" t="s">
         <v>1</v>
       </c>
       <c r="B35" s="46" t="s">
         <v>368</v>
       </c>
-      <c r="C35" s="56" t="s">
+      <c r="C35" s="53" t="s">
         <v>65</v>
       </c>
-      <c r="D35" s="56">
+      <c r="D35" s="53">
         <v>0</v>
       </c>
       <c r="E35" s="46" t="s">
         <v>97</v>
       </c>
-      <c r="F35" s="56"/>
-      <c r="G35" s="58" t="s">
+      <c r="F35" s="53"/>
+      <c r="G35" s="55" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A36" s="56" t="s">
+      <c r="A36" s="53" t="s">
         <v>1</v>
       </c>
       <c r="B36" s="46" t="s">
         <v>369</v>
       </c>
-      <c r="C36" s="56" t="s">
+      <c r="C36" s="53" t="s">
         <v>65</v>
       </c>
-      <c r="D36" s="56">
+      <c r="D36" s="53">
         <v>2</v>
       </c>
       <c r="E36" s="46" t="s">
         <v>97</v>
       </c>
-      <c r="F36" s="56"/>
-      <c r="G36" s="58" t="s">
+      <c r="F36" s="53"/>
+      <c r="G36" s="55" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A37" s="56" t="s">
+      <c r="A37" s="53" t="s">
         <v>1</v>
       </c>
       <c r="B37" s="46" t="s">
         <v>370</v>
       </c>
-      <c r="C37" s="56" t="s">
+      <c r="C37" s="53" t="s">
         <v>65</v>
       </c>
-      <c r="D37" s="56">
+      <c r="D37" s="53">
         <v>1</v>
       </c>
       <c r="E37" s="46" t="s">
         <v>97</v>
       </c>
-      <c r="F37" s="56"/>
-      <c r="G37" s="58" t="s">
+      <c r="F37" s="53"/>
+      <c r="G37" s="55" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A38" s="56" t="s">
+      <c r="A38" s="53" t="s">
         <v>1</v>
       </c>
       <c r="B38" s="46" t="s">
         <v>371</v>
       </c>
-      <c r="C38" s="56" t="s">
+      <c r="C38" s="53" t="s">
         <v>65</v>
       </c>
-      <c r="D38" s="56">
-        <v>0</v>
-      </c>
-      <c r="E38" s="57" t="s">
+      <c r="D38" s="53">
+        <v>0</v>
+      </c>
+      <c r="E38" s="54" t="s">
         <v>374</v>
       </c>
-      <c r="F38" s="56" t="s">
+      <c r="F38" s="53" t="s">
         <v>375</v>
       </c>
-      <c r="G38" s="56" t="s">
+      <c r="G38" s="53" t="s">
         <v>376</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A39" s="56" t="s">
+      <c r="A39" s="53" t="s">
         <v>1</v>
       </c>
       <c r="B39" s="46" t="s">
         <v>372</v>
       </c>
-      <c r="C39" s="56" t="s">
+      <c r="C39" s="53" t="s">
         <v>65</v>
       </c>
-      <c r="D39" s="56">
+      <c r="D39" s="53">
         <v>2</v>
       </c>
-      <c r="E39" s="57" t="s">
+      <c r="E39" s="54" t="s">
         <v>374</v>
       </c>
-      <c r="F39" s="56" t="s">
+      <c r="F39" s="53" t="s">
         <v>375</v>
       </c>
-      <c r="G39" s="56" t="s">
+      <c r="G39" s="53" t="s">
         <v>376</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A40" s="56" t="s">
+      <c r="A40" s="53" t="s">
         <v>1</v>
       </c>
       <c r="B40" s="46" t="s">
         <v>373</v>
       </c>
-      <c r="C40" s="56" t="s">
+      <c r="C40" s="53" t="s">
         <v>65</v>
       </c>
-      <c r="D40" s="56">
-        <v>1</v>
-      </c>
-      <c r="E40" s="57" t="s">
+      <c r="D40" s="53">
+        <v>1</v>
+      </c>
+      <c r="E40" s="54" t="s">
         <v>374</v>
       </c>
-      <c r="F40" s="56" t="s">
+      <c r="F40" s="53" t="s">
         <v>375</v>
       </c>
-      <c r="G40" s="56" t="s">
+      <c r="G40" s="53" t="s">
         <v>376</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A41" s="56" t="s">
+      <c r="A41" s="53" t="s">
         <v>1</v>
       </c>
       <c r="B41" s="46" t="s">
         <v>377</v>
       </c>
-      <c r="C41" s="56" t="s">
+      <c r="C41" s="53" t="s">
         <v>231</v>
       </c>
-      <c r="D41" s="56">
-        <v>0</v>
-      </c>
-      <c r="E41" s="56"/>
-      <c r="F41" s="56" t="s">
-        <v>380</v>
-      </c>
-      <c r="G41" s="58" t="s">
+      <c r="D41" s="53">
+        <v>0</v>
+      </c>
+      <c r="E41" s="53"/>
+      <c r="F41" s="53"/>
+      <c r="G41" s="55" t="s">
         <v>251</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A42" s="56" t="s">
+      <c r="A42" s="53" t="s">
         <v>1</v>
       </c>
       <c r="B42" s="46" t="s">
         <v>378</v>
       </c>
-      <c r="C42" s="56" t="s">
+      <c r="C42" s="53" t="s">
         <v>231</v>
       </c>
-      <c r="D42" s="56">
+      <c r="D42" s="53">
         <v>2</v>
       </c>
-      <c r="E42" s="56"/>
-      <c r="F42" s="56" t="s">
-        <v>380</v>
-      </c>
-      <c r="G42" s="58" t="s">
+      <c r="E42" s="53"/>
+      <c r="F42" s="53"/>
+      <c r="G42" s="55" t="s">
         <v>251</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A43" s="56" t="s">
+      <c r="A43" s="53" t="s">
         <v>1</v>
       </c>
       <c r="B43" s="46" t="s">
         <v>379</v>
       </c>
-      <c r="C43" s="56" t="s">
+      <c r="C43" s="53" t="s">
         <v>231</v>
       </c>
-      <c r="D43" s="56">
-        <v>1</v>
-      </c>
-      <c r="E43" s="56"/>
-      <c r="F43" s="56" t="s">
+      <c r="D43" s="53">
+        <v>1</v>
+      </c>
+      <c r="E43" s="53"/>
+      <c r="F43" s="53"/>
+      <c r="G43" s="55" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A44" s="53" t="s">
+        <v>1</v>
+      </c>
+      <c r="B44" s="46" t="s">
         <v>380</v>
       </c>
-      <c r="G43" s="58" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A44" s="56" t="s">
-        <v>1</v>
-      </c>
-      <c r="B44" s="46" t="s">
+      <c r="C44" s="53" t="s">
+        <v>65</v>
+      </c>
+      <c r="D44" s="53">
+        <v>0</v>
+      </c>
+      <c r="E44" s="46" t="s">
+        <v>383</v>
+      </c>
+      <c r="F44" s="53" t="s">
+        <v>384</v>
+      </c>
+      <c r="G44" s="55" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A45" s="53" t="s">
+        <v>1</v>
+      </c>
+      <c r="B45" s="46" t="s">
         <v>381</v>
       </c>
-      <c r="C44" s="56" t="s">
+      <c r="C45" s="53" t="s">
         <v>65</v>
       </c>
-      <c r="D44" s="56">
-        <v>0</v>
-      </c>
-      <c r="E44" s="46" t="s">
+      <c r="D45" s="53">
+        <v>2</v>
+      </c>
+      <c r="E45" s="46" t="s">
+        <v>383</v>
+      </c>
+      <c r="F45" s="53" t="s">
         <v>384</v>
       </c>
-      <c r="F44" s="56" t="s">
+      <c r="G45" s="55" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A46" s="53" t="s">
+        <v>1</v>
+      </c>
+      <c r="B46" s="46" t="s">
+        <v>382</v>
+      </c>
+      <c r="C46" s="53" t="s">
+        <v>65</v>
+      </c>
+      <c r="D46" s="53">
+        <v>1</v>
+      </c>
+      <c r="E46" s="46" t="s">
+        <v>383</v>
+      </c>
+      <c r="F46" s="53" t="s">
+        <v>384</v>
+      </c>
+      <c r="G46" s="55" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A47" s="53" t="s">
+        <v>1</v>
+      </c>
+      <c r="B47" s="46" t="s">
         <v>385</v>
       </c>
-      <c r="G44" s="58" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A45" s="56" t="s">
-        <v>1</v>
-      </c>
-      <c r="B45" s="46" t="s">
-        <v>382</v>
-      </c>
-      <c r="C45" s="56" t="s">
-        <v>65</v>
-      </c>
-      <c r="D45" s="56">
-        <v>2</v>
-      </c>
-      <c r="E45" s="46" t="s">
-        <v>384</v>
-      </c>
-      <c r="F45" s="56" t="s">
-        <v>385</v>
-      </c>
-      <c r="G45" s="58" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A46" s="56" t="s">
-        <v>1</v>
-      </c>
-      <c r="B46" s="46" t="s">
-        <v>383</v>
-      </c>
-      <c r="C46" s="56" t="s">
-        <v>65</v>
-      </c>
-      <c r="D46" s="56">
-        <v>1</v>
-      </c>
-      <c r="E46" s="46" t="s">
-        <v>384</v>
-      </c>
-      <c r="F46" s="56" t="s">
-        <v>385</v>
-      </c>
-      <c r="G46" s="58" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A47" s="56" t="s">
-        <v>1</v>
-      </c>
-      <c r="B47" s="46" t="s">
-        <v>386</v>
-      </c>
-      <c r="C47" s="56" t="s">
+      <c r="C47" s="53" t="s">
         <v>50</v>
       </c>
-      <c r="D47" s="56">
+      <c r="D47" s="53">
         <v>0</v>
       </c>
       <c r="E47" s="46" t="s">
         <v>117</v>
       </c>
-      <c r="F47" s="56"/>
-      <c r="G47" s="58" t="s">
+      <c r="F47" s="53"/>
+      <c r="G47" s="55" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A48" s="56" t="s">
+      <c r="A48" s="53" t="s">
         <v>1</v>
       </c>
       <c r="B48" s="46" t="s">
-        <v>387</v>
-      </c>
-      <c r="C48" s="56" t="s">
+        <v>386</v>
+      </c>
+      <c r="C48" s="53" t="s">
         <v>50</v>
       </c>
-      <c r="D48" s="56">
+      <c r="D48" s="53">
         <v>2</v>
       </c>
       <c r="E48" s="46" t="s">
         <v>117</v>
       </c>
-      <c r="F48" s="56"/>
-      <c r="G48" s="58" t="s">
+      <c r="F48" s="53"/>
+      <c r="G48" s="55" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A49" s="56" t="s">
+      <c r="A49" s="53" t="s">
         <v>1</v>
       </c>
       <c r="B49" s="46" t="s">
-        <v>388</v>
-      </c>
-      <c r="C49" s="56" t="s">
+        <v>387</v>
+      </c>
+      <c r="C49" s="53" t="s">
         <v>50</v>
       </c>
-      <c r="D49" s="56">
+      <c r="D49" s="53">
         <v>1</v>
       </c>
       <c r="E49" s="46" t="s">
         <v>117</v>
       </c>
-      <c r="F49" s="56"/>
-      <c r="G49" s="58" t="s">
+      <c r="F49" s="53"/>
+      <c r="G49" s="55" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A50" s="56" t="s">
+      <c r="A50" s="53" t="s">
         <v>1</v>
       </c>
       <c r="B50" s="46" t="s">
+        <v>388</v>
+      </c>
+      <c r="C50" s="53" t="s">
+        <v>50</v>
+      </c>
+      <c r="D50" s="53">
+        <v>0</v>
+      </c>
+      <c r="E50" s="46" t="s">
+        <v>391</v>
+      </c>
+      <c r="F50" s="53"/>
+      <c r="G50" s="55" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A51" s="53" t="s">
+        <v>1</v>
+      </c>
+      <c r="B51" s="46" t="s">
         <v>389</v>
       </c>
-      <c r="C50" s="56" t="s">
+      <c r="C51" s="53" t="s">
         <v>50</v>
       </c>
-      <c r="D50" s="56">
-        <v>0</v>
-      </c>
-      <c r="E50" s="46" t="s">
+      <c r="D51" s="53">
+        <v>2</v>
+      </c>
+      <c r="E51" s="46" t="s">
+        <v>391</v>
+      </c>
+      <c r="F51" s="53"/>
+      <c r="G51" s="55" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A52" s="53" t="s">
+        <v>1</v>
+      </c>
+      <c r="B52" s="46" t="s">
+        <v>390</v>
+      </c>
+      <c r="C52" s="53" t="s">
+        <v>50</v>
+      </c>
+      <c r="D52" s="53">
+        <v>1</v>
+      </c>
+      <c r="E52" s="46" t="s">
+        <v>391</v>
+      </c>
+      <c r="F52" s="53"/>
+      <c r="G52" s="55" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A53" s="53" t="s">
+        <v>1</v>
+      </c>
+      <c r="B53" s="46" t="s">
         <v>392</v>
       </c>
-      <c r="F50" s="56"/>
-      <c r="G50" s="58" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A51" s="56" t="s">
-        <v>1</v>
-      </c>
-      <c r="B51" s="46" t="s">
-        <v>390</v>
-      </c>
-      <c r="C51" s="56" t="s">
-        <v>50</v>
-      </c>
-      <c r="D51" s="56">
+      <c r="C53" s="53" t="s">
+        <v>47</v>
+      </c>
+      <c r="D53" s="53">
+        <v>0</v>
+      </c>
+      <c r="E53" s="53"/>
+      <c r="F53" s="53"/>
+      <c r="G53" s="55" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A54" s="53" t="s">
+        <v>1</v>
+      </c>
+      <c r="B54" s="46" t="s">
+        <v>393</v>
+      </c>
+      <c r="C54" s="53" t="s">
+        <v>47</v>
+      </c>
+      <c r="D54" s="53">
         <v>2</v>
       </c>
-      <c r="E51" s="46" t="s">
-        <v>392</v>
-      </c>
-      <c r="F51" s="56"/>
-      <c r="G51" s="58" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A52" s="56" t="s">
-        <v>1</v>
-      </c>
-      <c r="B52" s="46" t="s">
-        <v>391</v>
-      </c>
-      <c r="C52" s="56" t="s">
-        <v>50</v>
-      </c>
-      <c r="D52" s="56">
-        <v>1</v>
-      </c>
-      <c r="E52" s="46" t="s">
-        <v>392</v>
-      </c>
-      <c r="F52" s="56"/>
-      <c r="G52" s="58" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A53" s="56" t="s">
-        <v>1</v>
-      </c>
-      <c r="B53" s="46" t="s">
-        <v>393</v>
-      </c>
-      <c r="C53" s="56" t="s">
+      <c r="E54" s="53"/>
+      <c r="F54" s="53"/>
+      <c r="G54" s="55" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A55" s="53" t="s">
+        <v>1</v>
+      </c>
+      <c r="B55" s="46" t="s">
+        <v>394</v>
+      </c>
+      <c r="C55" s="53" t="s">
         <v>47</v>
       </c>
-      <c r="D53" s="56">
-        <v>0</v>
-      </c>
-      <c r="E53" s="56"/>
-      <c r="F53" s="56"/>
-      <c r="G53" s="58" t="s">
+      <c r="D55" s="53">
+        <v>1</v>
+      </c>
+      <c r="E55" s="53"/>
+      <c r="F55" s="53"/>
+      <c r="G55" s="55" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A54" s="56" t="s">
-        <v>1</v>
-      </c>
-      <c r="B54" s="46" t="s">
-        <v>394</v>
-      </c>
-      <c r="C54" s="56" t="s">
-        <v>47</v>
-      </c>
-      <c r="D54" s="56">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A56" s="53" t="s">
+        <v>1</v>
+      </c>
+      <c r="B56" s="46" t="s">
+        <v>395</v>
+      </c>
+      <c r="C56" s="53" t="s">
+        <v>59</v>
+      </c>
+      <c r="D56" s="53">
+        <v>0</v>
+      </c>
+      <c r="E56" s="53"/>
+      <c r="F56" s="53"/>
+      <c r="G56" s="55" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A57" s="53" t="s">
+        <v>1</v>
+      </c>
+      <c r="B57" s="46" t="s">
+        <v>396</v>
+      </c>
+      <c r="C57" s="53" t="s">
+        <v>59</v>
+      </c>
+      <c r="D57" s="53">
         <v>2</v>
       </c>
-      <c r="E54" s="56"/>
-      <c r="F54" s="56"/>
-      <c r="G54" s="58" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A55" s="56" t="s">
-        <v>1</v>
-      </c>
-      <c r="B55" s="46" t="s">
-        <v>395</v>
-      </c>
-      <c r="C55" s="56" t="s">
-        <v>47</v>
-      </c>
-      <c r="D55" s="56">
-        <v>1</v>
-      </c>
-      <c r="E55" s="56"/>
-      <c r="F55" s="56"/>
-      <c r="G55" s="58" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A56" s="56" t="s">
-        <v>1</v>
-      </c>
-      <c r="B56" s="46" t="s">
-        <v>396</v>
-      </c>
-      <c r="C56" s="56" t="s">
+      <c r="E57" s="53"/>
+      <c r="F57" s="53"/>
+      <c r="G57" s="55" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A58" s="53" t="s">
+        <v>1</v>
+      </c>
+      <c r="B58" s="46" t="s">
+        <v>397</v>
+      </c>
+      <c r="C58" s="53" t="s">
         <v>59</v>
       </c>
-      <c r="D56" s="56">
-        <v>0</v>
-      </c>
-      <c r="E56" s="56"/>
-      <c r="F56" s="56"/>
-      <c r="G56" s="58" t="s">
+      <c r="D58" s="53">
+        <v>1</v>
+      </c>
+      <c r="E58" s="54"/>
+      <c r="F58" s="53"/>
+      <c r="G58" s="55" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A57" s="56" t="s">
-        <v>1</v>
-      </c>
-      <c r="B57" s="46" t="s">
-        <v>397</v>
-      </c>
-      <c r="C57" s="56" t="s">
-        <v>59</v>
-      </c>
-      <c r="D57" s="56">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A59" s="53" t="s">
+        <v>1</v>
+      </c>
+      <c r="B59" s="46" t="s">
+        <v>398</v>
+      </c>
+      <c r="C59" s="53" t="s">
+        <v>237</v>
+      </c>
+      <c r="D59" s="53">
+        <v>0</v>
+      </c>
+      <c r="E59" s="46" t="s">
+        <v>401</v>
+      </c>
+      <c r="F59" s="53"/>
+      <c r="G59" s="55" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A60" s="53" t="s">
+        <v>1</v>
+      </c>
+      <c r="B60" s="46" t="s">
+        <v>399</v>
+      </c>
+      <c r="C60" s="53" t="s">
+        <v>237</v>
+      </c>
+      <c r="D60" s="53">
         <v>2</v>
       </c>
-      <c r="E57" s="56"/>
-      <c r="F57" s="56"/>
-      <c r="G57" s="58" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A58" s="56" t="s">
-        <v>1</v>
-      </c>
-      <c r="B58" s="46" t="s">
-        <v>398</v>
-      </c>
-      <c r="C58" s="56" t="s">
-        <v>59</v>
-      </c>
-      <c r="D58" s="56">
-        <v>1</v>
-      </c>
-      <c r="E58" s="57"/>
-      <c r="F58" s="56"/>
-      <c r="G58" s="58" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A59" s="56" t="s">
-        <v>1</v>
-      </c>
-      <c r="B59" s="46" t="s">
-        <v>399</v>
-      </c>
-      <c r="C59" s="56" t="s">
+      <c r="E60" s="46" t="s">
+        <v>401</v>
+      </c>
+      <c r="F60" s="53"/>
+      <c r="G60" s="55" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A61" s="53" t="s">
+        <v>1</v>
+      </c>
+      <c r="B61" s="46" t="s">
+        <v>400</v>
+      </c>
+      <c r="C61" s="53" t="s">
         <v>237</v>
       </c>
-      <c r="D59" s="56">
-        <v>0</v>
-      </c>
-      <c r="E59" s="46" t="s">
+      <c r="D61" s="53">
+        <v>1</v>
+      </c>
+      <c r="E61" s="46" t="s">
+        <v>401</v>
+      </c>
+      <c r="F61" s="53"/>
+      <c r="G61" s="55" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A62" s="53" t="s">
+        <v>1</v>
+      </c>
+      <c r="B62" s="46" t="s">
         <v>402</v>
       </c>
-      <c r="F59" s="56"/>
-      <c r="G59" s="58" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A60" s="56" t="s">
-        <v>1</v>
-      </c>
-      <c r="B60" s="46" t="s">
-        <v>400</v>
-      </c>
-      <c r="C60" s="56" t="s">
-        <v>237</v>
-      </c>
-      <c r="D60" s="56">
-        <v>2</v>
-      </c>
-      <c r="E60" s="46" t="s">
-        <v>402</v>
-      </c>
-      <c r="F60" s="56"/>
-      <c r="G60" s="58" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A61" s="56" t="s">
-        <v>1</v>
-      </c>
-      <c r="B61" s="46" t="s">
-        <v>401</v>
-      </c>
-      <c r="C61" s="56" t="s">
-        <v>237</v>
-      </c>
-      <c r="D61" s="56">
-        <v>1</v>
-      </c>
-      <c r="E61" s="46" t="s">
-        <v>402</v>
-      </c>
-      <c r="F61" s="56"/>
-      <c r="G61" s="58" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A62" s="56" t="s">
-        <v>1</v>
-      </c>
-      <c r="B62" s="46" t="s">
-        <v>403</v>
-      </c>
-      <c r="C62" s="56" t="s">
+      <c r="C62" s="53" t="s">
         <v>65</v>
       </c>
-      <c r="D62" s="56">
+      <c r="D62" s="53">
         <v>0</v>
       </c>
       <c r="E62" s="46" t="s">
         <v>75</v>
       </c>
-      <c r="F62" s="56"/>
-      <c r="G62" s="56" t="s">
+      <c r="F62" s="53"/>
+      <c r="G62" s="53" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A63" s="56" t="s">
+      <c r="A63" s="53" t="s">
         <v>1</v>
       </c>
       <c r="B63" s="46" t="s">
-        <v>404</v>
-      </c>
-      <c r="C63" s="56" t="s">
+        <v>403</v>
+      </c>
+      <c r="C63" s="53" t="s">
         <v>65</v>
       </c>
-      <c r="D63" s="56">
+      <c r="D63" s="53">
         <v>2</v>
       </c>
       <c r="E63" s="46" t="s">
         <v>75</v>
       </c>
-      <c r="F63" s="56"/>
-      <c r="G63" s="56" t="s">
+      <c r="F63" s="53"/>
+      <c r="G63" s="53" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A64" s="56" t="s">
+      <c r="A64" s="53" t="s">
         <v>1</v>
       </c>
       <c r="B64" s="46" t="s">
-        <v>405</v>
-      </c>
-      <c r="C64" s="56" t="s">
+        <v>404</v>
+      </c>
+      <c r="C64" s="53" t="s">
         <v>65</v>
       </c>
-      <c r="D64" s="56">
+      <c r="D64" s="53">
         <v>1</v>
       </c>
       <c r="E64" s="46" t="s">
         <v>75</v>
       </c>
-      <c r="F64" s="56"/>
-      <c r="G64" s="56" t="s">
+      <c r="F64" s="53"/>
+      <c r="G64" s="53" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A65" s="56" t="s">
+      <c r="A65" s="53" t="s">
         <v>1</v>
       </c>
       <c r="B65" s="46" t="s">
+        <v>405</v>
+      </c>
+      <c r="C65" s="53" t="s">
+        <v>237</v>
+      </c>
+      <c r="D65" s="53">
+        <v>0</v>
+      </c>
+      <c r="E65" s="46" t="s">
+        <v>408</v>
+      </c>
+      <c r="F65" s="53"/>
+      <c r="G65" s="55" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A66" s="53" t="s">
+        <v>1</v>
+      </c>
+      <c r="B66" s="46" t="s">
         <v>406</v>
       </c>
-      <c r="C65" s="56" t="s">
+      <c r="C66" s="53" t="s">
         <v>237</v>
       </c>
-      <c r="D65" s="56">
-        <v>0</v>
-      </c>
-      <c r="E65" s="46" t="s">
+      <c r="D66" s="53">
+        <v>2</v>
+      </c>
+      <c r="E66" s="46" t="s">
+        <v>408</v>
+      </c>
+      <c r="F66" s="53"/>
+      <c r="G66" s="55" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A67" s="53" t="s">
+        <v>1</v>
+      </c>
+      <c r="B67" s="46" t="s">
+        <v>407</v>
+      </c>
+      <c r="C67" s="53" t="s">
+        <v>237</v>
+      </c>
+      <c r="D67" s="53">
+        <v>1</v>
+      </c>
+      <c r="E67" s="46" t="s">
+        <v>408</v>
+      </c>
+      <c r="F67" s="53"/>
+      <c r="G67" s="55" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A68" s="53" t="s">
+        <v>1</v>
+      </c>
+      <c r="B68" s="46" t="s">
         <v>409</v>
       </c>
-      <c r="F65" s="56"/>
-      <c r="G65" s="58" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A66" s="56" t="s">
-        <v>1</v>
-      </c>
-      <c r="B66" s="46" t="s">
-        <v>407</v>
-      </c>
-      <c r="C66" s="56" t="s">
-        <v>237</v>
-      </c>
-      <c r="D66" s="56">
+      <c r="C68" s="53" t="s">
+        <v>65</v>
+      </c>
+      <c r="D68" s="53">
+        <v>0</v>
+      </c>
+      <c r="E68" s="46" t="s">
+        <v>412</v>
+      </c>
+      <c r="F68" s="53" t="s">
+        <v>413</v>
+      </c>
+      <c r="G68" s="55" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A69" s="53" t="s">
+        <v>1</v>
+      </c>
+      <c r="B69" s="46" t="s">
+        <v>410</v>
+      </c>
+      <c r="C69" s="53" t="s">
+        <v>65</v>
+      </c>
+      <c r="D69" s="53">
         <v>2</v>
       </c>
-      <c r="E66" s="46" t="s">
-        <v>409</v>
-      </c>
-      <c r="F66" s="56"/>
-      <c r="G66" s="58" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A67" s="56" t="s">
-        <v>1</v>
-      </c>
-      <c r="B67" s="46" t="s">
-        <v>408</v>
-      </c>
-      <c r="C67" s="56" t="s">
-        <v>237</v>
-      </c>
-      <c r="D67" s="56">
-        <v>1</v>
-      </c>
-      <c r="E67" s="46" t="s">
-        <v>409</v>
-      </c>
-      <c r="F67" s="56"/>
-      <c r="G67" s="58" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A68" s="56" t="s">
-        <v>1</v>
-      </c>
-      <c r="B68" s="46" t="s">
-        <v>410</v>
-      </c>
-      <c r="C68" s="56" t="s">
+      <c r="E69" s="46" t="s">
+        <v>412</v>
+      </c>
+      <c r="F69" s="53" t="s">
+        <v>413</v>
+      </c>
+      <c r="G69" s="55" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A70" s="53" t="s">
+        <v>1</v>
+      </c>
+      <c r="B70" s="46" t="s">
+        <v>411</v>
+      </c>
+      <c r="C70" s="53" t="s">
         <v>65</v>
       </c>
-      <c r="D68" s="56">
-        <v>0</v>
-      </c>
-      <c r="E68" s="46" t="s">
+      <c r="D70" s="53">
+        <v>1</v>
+      </c>
+      <c r="E70" s="46" t="s">
+        <v>412</v>
+      </c>
+      <c r="F70" s="53" t="s">
         <v>413</v>
       </c>
-      <c r="F68" s="56" t="s">
+      <c r="G70" s="55" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A71" s="53" t="s">
+        <v>1</v>
+      </c>
+      <c r="B71" s="46" t="s">
         <v>414</v>
       </c>
-      <c r="G68" s="58" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A69" s="56" t="s">
-        <v>1</v>
-      </c>
-      <c r="B69" s="46" t="s">
-        <v>411</v>
-      </c>
-      <c r="C69" s="56" t="s">
-        <v>65</v>
-      </c>
-      <c r="D69" s="56">
+      <c r="C71" s="53" t="s">
+        <v>228</v>
+      </c>
+      <c r="D71" s="53">
+        <v>0</v>
+      </c>
+      <c r="E71" s="53"/>
+      <c r="F71" s="53"/>
+      <c r="G71" s="53" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A72" s="53" t="s">
+        <v>1</v>
+      </c>
+      <c r="B72" s="46" t="s">
+        <v>415</v>
+      </c>
+      <c r="C72" s="53" t="s">
+        <v>228</v>
+      </c>
+      <c r="D72" s="53">
         <v>2</v>
       </c>
-      <c r="E69" s="46" t="s">
-        <v>413</v>
-      </c>
-      <c r="F69" s="56" t="s">
-        <v>414</v>
-      </c>
-      <c r="G69" s="58" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A70" s="56" t="s">
-        <v>1</v>
-      </c>
-      <c r="B70" s="46" t="s">
-        <v>412</v>
-      </c>
-      <c r="C70" s="56" t="s">
-        <v>65</v>
-      </c>
-      <c r="D70" s="56">
-        <v>1</v>
-      </c>
-      <c r="E70" s="46" t="s">
-        <v>413</v>
-      </c>
-      <c r="F70" s="56" t="s">
-        <v>414</v>
-      </c>
-      <c r="G70" s="58" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A71" s="56" t="s">
-        <v>1</v>
-      </c>
-      <c r="B71" s="46" t="s">
-        <v>415</v>
-      </c>
-      <c r="C71" s="56" t="s">
+      <c r="E72" s="53"/>
+      <c r="F72" s="53"/>
+      <c r="G72" s="53" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A73" s="53" t="s">
+        <v>1</v>
+      </c>
+      <c r="B73" s="46" t="s">
+        <v>416</v>
+      </c>
+      <c r="C73" s="53" t="s">
         <v>228</v>
       </c>
-      <c r="D71" s="56">
-        <v>0</v>
-      </c>
-      <c r="E71" s="56"/>
-      <c r="F71" s="56" t="s">
-        <v>380</v>
-      </c>
-      <c r="G71" s="56" t="s">
+      <c r="D73" s="53">
+        <v>1</v>
+      </c>
+      <c r="E73" s="53"/>
+      <c r="F73" s="53"/>
+      <c r="G73" s="53" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A74" s="53" t="s">
+        <v>1</v>
+      </c>
+      <c r="B74" s="46" t="s">
         <v>418</v>
       </c>
-    </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A72" s="56" t="s">
-        <v>1</v>
-      </c>
-      <c r="B72" s="46" t="s">
-        <v>416</v>
-      </c>
-      <c r="C72" s="56" t="s">
-        <v>228</v>
-      </c>
-      <c r="D72" s="56">
+      <c r="C74" s="53" t="s">
+        <v>234</v>
+      </c>
+      <c r="D74" s="53">
+        <v>0</v>
+      </c>
+      <c r="E74" s="53"/>
+      <c r="F74" s="53"/>
+      <c r="G74" s="53" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A75" s="53" t="s">
+        <v>1</v>
+      </c>
+      <c r="B75" s="46" t="s">
+        <v>419</v>
+      </c>
+      <c r="C75" s="53" t="s">
+        <v>234</v>
+      </c>
+      <c r="D75" s="53">
         <v>2</v>
       </c>
-      <c r="E72" s="56"/>
-      <c r="F72" s="56" t="s">
-        <v>380</v>
-      </c>
-      <c r="G72" s="56" t="s">
-        <v>418</v>
-      </c>
-    </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A73" s="56" t="s">
-        <v>1</v>
-      </c>
-      <c r="B73" s="46" t="s">
-        <v>417</v>
-      </c>
-      <c r="C73" s="56" t="s">
-        <v>228</v>
-      </c>
-      <c r="D73" s="56">
-        <v>1</v>
-      </c>
-      <c r="E73" s="56"/>
-      <c r="F73" s="56" t="s">
-        <v>380</v>
-      </c>
-      <c r="G73" s="56" t="s">
-        <v>418</v>
-      </c>
-    </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A74" s="56" t="s">
-        <v>1</v>
-      </c>
-      <c r="B74" s="46" t="s">
-        <v>419</v>
-      </c>
-      <c r="C74" s="56" t="s">
+      <c r="E75" s="53"/>
+      <c r="F75" s="53"/>
+      <c r="G75" s="53" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A76" s="53" t="s">
+        <v>1</v>
+      </c>
+      <c r="B76" s="46" t="s">
+        <v>420</v>
+      </c>
+      <c r="C76" s="53" t="s">
         <v>234</v>
       </c>
-      <c r="D74" s="56">
-        <v>0</v>
-      </c>
-      <c r="E74" s="56"/>
-      <c r="F74" s="56" t="s">
-        <v>380</v>
-      </c>
-      <c r="G74" s="56" t="s">
+      <c r="D76" s="53">
+        <v>1</v>
+      </c>
+      <c r="E76" s="53"/>
+      <c r="F76" s="53"/>
+      <c r="G76" s="53" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A77" s="53" t="s">
+        <v>1</v>
+      </c>
+      <c r="B77" s="46" t="s">
         <v>422</v>
       </c>
-    </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A75" s="56" t="s">
-        <v>1</v>
-      </c>
-      <c r="B75" s="46" t="s">
-        <v>420</v>
-      </c>
-      <c r="C75" s="56" t="s">
-        <v>234</v>
-      </c>
-      <c r="D75" s="56">
-        <v>2</v>
-      </c>
-      <c r="E75" s="56"/>
-      <c r="F75" s="56" t="s">
-        <v>380</v>
-      </c>
-      <c r="G75" s="56" t="s">
-        <v>422</v>
-      </c>
-    </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A76" s="56" t="s">
-        <v>1</v>
-      </c>
-      <c r="B76" s="46" t="s">
-        <v>421</v>
-      </c>
-      <c r="C76" s="56" t="s">
-        <v>234</v>
-      </c>
-      <c r="D76" s="56">
-        <v>1</v>
-      </c>
-      <c r="E76" s="56"/>
-      <c r="F76" s="56" t="s">
-        <v>380</v>
-      </c>
-      <c r="G76" s="56" t="s">
-        <v>422</v>
-      </c>
-    </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A77" s="56" t="s">
-        <v>1</v>
-      </c>
-      <c r="B77" s="46" t="s">
-        <v>423</v>
-      </c>
-      <c r="C77" s="59" t="s">
+      <c r="C77" s="56" t="s">
         <v>313</v>
       </c>
-      <c r="D77" s="56">
-        <v>0</v>
-      </c>
-      <c r="E77" s="56"/>
-      <c r="F77" s="56"/>
-      <c r="G77" s="58" t="s">
+      <c r="D77" s="53">
+        <v>0</v>
+      </c>
+      <c r="E77" s="53"/>
+      <c r="F77" s="53"/>
+      <c r="G77" s="55" t="s">
         <v>310</v>
       </c>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A78" s="56" t="s">
+      <c r="A78" s="53" t="s">
         <v>1</v>
       </c>
       <c r="B78" s="46" t="s">
         <v>314</v>
       </c>
-      <c r="C78" s="59" t="s">
+      <c r="C78" s="56" t="s">
         <v>313</v>
       </c>
-      <c r="D78" s="56">
+      <c r="D78" s="53">
         <v>2</v>
       </c>
-      <c r="E78" s="56"/>
-      <c r="F78" s="56"/>
-      <c r="G78" s="58" t="s">
+      <c r="E78" s="53"/>
+      <c r="F78" s="53"/>
+      <c r="G78" s="55" t="s">
         <v>310</v>
       </c>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A79" s="56" t="s">
+      <c r="A79" s="53" t="s">
         <v>1</v>
       </c>
       <c r="B79" s="46" t="s">
+        <v>423</v>
+      </c>
+      <c r="C79" s="56" t="s">
+        <v>313</v>
+      </c>
+      <c r="D79" s="53">
+        <v>1</v>
+      </c>
+      <c r="E79" s="53"/>
+      <c r="F79" s="53"/>
+      <c r="G79" s="55" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A80" s="53" t="s">
+        <v>1</v>
+      </c>
+      <c r="B80" s="46" t="s">
         <v>424</v>
       </c>
-      <c r="C79" s="59" t="s">
-        <v>313</v>
-      </c>
-      <c r="D79" s="56">
-        <v>1</v>
-      </c>
-      <c r="E79" s="56"/>
-      <c r="F79" s="56"/>
-      <c r="G79" s="58" t="s">
+      <c r="C80" s="56" t="s">
+        <v>315</v>
+      </c>
+      <c r="D80" s="53">
+        <v>0</v>
+      </c>
+      <c r="E80" s="54"/>
+      <c r="F80" s="53"/>
+      <c r="G80" s="55" t="s">
         <v>310</v>
       </c>
     </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A80" s="56" t="s">
-        <v>1</v>
-      </c>
-      <c r="B80" s="46" t="s">
-        <v>425</v>
-      </c>
-      <c r="C80" s="59" t="s">
-        <v>315</v>
-      </c>
-      <c r="D80" s="56">
-        <v>0</v>
-      </c>
-      <c r="E80" s="57"/>
-      <c r="F80" s="56"/>
-      <c r="G80" s="58" t="s">
-        <v>310</v>
-      </c>
-    </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A81" s="56" t="s">
+      <c r="A81" s="53" t="s">
         <v>1</v>
       </c>
       <c r="B81" s="46" t="s">
         <v>316</v>
       </c>
-      <c r="C81" s="59" t="s">
+      <c r="C81" s="56" t="s">
         <v>315</v>
       </c>
-      <c r="D81" s="56">
+      <c r="D81" s="53">
         <v>2</v>
       </c>
-      <c r="E81" s="56"/>
-      <c r="F81" s="56"/>
-      <c r="G81" s="58" t="s">
+      <c r="E81" s="53"/>
+      <c r="F81" s="53"/>
+      <c r="G81" s="55" t="s">
         <v>310</v>
       </c>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A82" s="56" t="s">
+      <c r="A82" s="53" t="s">
         <v>1</v>
       </c>
       <c r="B82" s="46" t="s">
+        <v>426</v>
+      </c>
+      <c r="C82" s="53" t="s">
+        <v>65</v>
+      </c>
+      <c r="D82" s="53">
+        <v>0</v>
+      </c>
+      <c r="E82" s="54" t="s">
+        <v>429</v>
+      </c>
+      <c r="F82" s="53" t="s">
+        <v>431</v>
+      </c>
+      <c r="G82" s="53" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A83" s="53" t="s">
+        <v>1</v>
+      </c>
+      <c r="B83" s="46" t="s">
         <v>427</v>
       </c>
-      <c r="C82" s="56" t="s">
+      <c r="C83" s="53" t="s">
         <v>65</v>
       </c>
-      <c r="D82" s="56">
-        <v>0</v>
-      </c>
-      <c r="E82" s="57" t="s">
+      <c r="D83" s="53">
+        <v>2</v>
+      </c>
+      <c r="E83" s="54" t="s">
+        <v>429</v>
+      </c>
+      <c r="F83" s="53" t="s">
+        <v>431</v>
+      </c>
+      <c r="G83" s="53" t="s">
         <v>430</v>
       </c>
-      <c r="F82" s="56" t="s">
+    </row>
+    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A84" s="53" t="s">
+        <v>1</v>
+      </c>
+      <c r="B84" s="46" t="s">
+        <v>428</v>
+      </c>
+      <c r="C84" s="53" t="s">
+        <v>65</v>
+      </c>
+      <c r="D84" s="53">
+        <v>1</v>
+      </c>
+      <c r="E84" s="54" t="s">
+        <v>429</v>
+      </c>
+      <c r="F84" s="53" t="s">
+        <v>431</v>
+      </c>
+      <c r="G84" s="53" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A85" s="53" t="s">
+        <v>1</v>
+      </c>
+      <c r="B85" s="46" t="s">
         <v>432</v>
       </c>
-      <c r="G82" s="56" t="s">
-        <v>431</v>
-      </c>
-    </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A83" s="56" t="s">
-        <v>1</v>
-      </c>
-      <c r="B83" s="46" t="s">
-        <v>428</v>
-      </c>
-      <c r="C83" s="56" t="s">
+      <c r="C85" s="53" t="s">
         <v>65</v>
       </c>
-      <c r="D83" s="56">
-        <v>2</v>
-      </c>
-      <c r="E83" s="57" t="s">
-        <v>430</v>
-      </c>
-      <c r="F83" s="56" t="s">
-        <v>432</v>
-      </c>
-      <c r="G83" s="56" t="s">
-        <v>431</v>
-      </c>
-    </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A84" s="56" t="s">
-        <v>1</v>
-      </c>
-      <c r="B84" s="46" t="s">
-        <v>429</v>
-      </c>
-      <c r="C84" s="56" t="s">
-        <v>65</v>
-      </c>
-      <c r="D84" s="56">
-        <v>1</v>
-      </c>
-      <c r="E84" s="57" t="s">
-        <v>430</v>
-      </c>
-      <c r="F84" s="56" t="s">
-        <v>432</v>
-      </c>
-      <c r="G84" s="56" t="s">
-        <v>431</v>
-      </c>
-    </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A85" s="56" t="s">
-        <v>1</v>
-      </c>
-      <c r="B85" s="46" t="s">
-        <v>433</v>
-      </c>
-      <c r="C85" s="56" t="s">
-        <v>65</v>
-      </c>
-      <c r="D85" s="56">
+      <c r="D85" s="53">
         <v>0</v>
       </c>
       <c r="E85" s="46" t="s">
         <v>87</v>
       </c>
-      <c r="F85" s="56"/>
-      <c r="G85" s="58" t="s">
+      <c r="F85" s="53"/>
+      <c r="G85" s="55" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A86" s="56" t="s">
+      <c r="A86" s="53" t="s">
         <v>1</v>
       </c>
       <c r="B86" s="46" t="s">
-        <v>434</v>
-      </c>
-      <c r="C86" s="56" t="s">
+        <v>433</v>
+      </c>
+      <c r="C86" s="53" t="s">
         <v>65</v>
       </c>
-      <c r="D86" s="56">
+      <c r="D86" s="53">
         <v>2</v>
       </c>
       <c r="E86" s="46" t="s">
         <v>87</v>
       </c>
-      <c r="F86" s="56"/>
-      <c r="G86" s="58" t="s">
+      <c r="F86" s="53"/>
+      <c r="G86" s="55" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A87" s="56" t="s">
+      <c r="A87" s="53" t="s">
         <v>1</v>
       </c>
       <c r="B87" s="46" t="s">
-        <v>435</v>
-      </c>
-      <c r="C87" s="56" t="s">
+        <v>434</v>
+      </c>
+      <c r="C87" s="53" t="s">
         <v>65</v>
       </c>
-      <c r="D87" s="56">
+      <c r="D87" s="53">
         <v>1</v>
       </c>
       <c r="E87" s="46" t="s">
         <v>87</v>
       </c>
-      <c r="F87" s="56"/>
-      <c r="G87" s="58" t="s">
+      <c r="F87" s="53"/>
+      <c r="G87" s="55" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A88" s="56" t="s">
+      <c r="A88" s="53" t="s">
         <v>1</v>
       </c>
       <c r="B88" s="46" t="s">
+        <v>435</v>
+      </c>
+      <c r="C88" s="53" t="s">
+        <v>50</v>
+      </c>
+      <c r="D88" s="53">
+        <v>0</v>
+      </c>
+      <c r="E88" s="46" t="s">
+        <v>438</v>
+      </c>
+      <c r="F88" s="53" t="s">
+        <v>439</v>
+      </c>
+      <c r="G88" s="55" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A89" s="53" t="s">
+        <v>1</v>
+      </c>
+      <c r="B89" s="46" t="s">
         <v>436</v>
       </c>
-      <c r="C88" s="56" t="s">
+      <c r="C89" s="53" t="s">
         <v>50</v>
       </c>
-      <c r="D88" s="56">
-        <v>0</v>
-      </c>
-      <c r="E88" s="46" t="s">
+      <c r="D89" s="53">
+        <v>2</v>
+      </c>
+      <c r="E89" s="46" t="s">
+        <v>438</v>
+      </c>
+      <c r="F89" s="53" t="s">
         <v>439</v>
       </c>
-      <c r="F88" s="56" t="s">
+      <c r="G89" s="55" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A90" s="53" t="s">
+        <v>1</v>
+      </c>
+      <c r="B90" s="46" t="s">
+        <v>437</v>
+      </c>
+      <c r="C90" s="53" t="s">
+        <v>50</v>
+      </c>
+      <c r="D90" s="53">
+        <v>1</v>
+      </c>
+      <c r="E90" s="46" t="s">
+        <v>438</v>
+      </c>
+      <c r="F90" s="53" t="s">
+        <v>439</v>
+      </c>
+      <c r="G90" s="55" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A91" s="53" t="s">
+        <v>1</v>
+      </c>
+      <c r="B91" s="46" t="s">
         <v>440</v>
       </c>
-      <c r="G88" s="58" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A89" s="56" t="s">
-        <v>1</v>
-      </c>
-      <c r="B89" s="46" t="s">
-        <v>437</v>
-      </c>
-      <c r="C89" s="56" t="s">
+      <c r="C91" s="53" t="s">
         <v>50</v>
       </c>
-      <c r="D89" s="56">
+      <c r="D91" s="53">
+        <v>0</v>
+      </c>
+      <c r="E91" s="46" t="s">
+        <v>443</v>
+      </c>
+      <c r="F91" s="53"/>
+      <c r="G91" s="55" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A92" s="53" t="s">
+        <v>1</v>
+      </c>
+      <c r="B92" s="46" t="s">
+        <v>441</v>
+      </c>
+      <c r="C92" s="53" t="s">
+        <v>50</v>
+      </c>
+      <c r="D92" s="53">
         <v>2</v>
       </c>
-      <c r="E89" s="46" t="s">
-        <v>439</v>
-      </c>
-      <c r="F89" s="56" t="s">
-        <v>440</v>
-      </c>
-      <c r="G89" s="58" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A90" s="56" t="s">
-        <v>1</v>
-      </c>
-      <c r="B90" s="46" t="s">
-        <v>438</v>
-      </c>
-      <c r="C90" s="56" t="s">
+      <c r="E92" s="46" t="s">
+        <v>443</v>
+      </c>
+      <c r="F92" s="53"/>
+      <c r="G92" s="55" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A93" s="53" t="s">
+        <v>1</v>
+      </c>
+      <c r="B93" s="46" t="s">
+        <v>442</v>
+      </c>
+      <c r="C93" s="53" t="s">
         <v>50</v>
       </c>
-      <c r="D90" s="56">
-        <v>1</v>
-      </c>
-      <c r="E90" s="46" t="s">
-        <v>439</v>
-      </c>
-      <c r="F90" s="56" t="s">
-        <v>440</v>
-      </c>
-      <c r="G90" s="58" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A91" s="56" t="s">
-        <v>1</v>
-      </c>
-      <c r="B91" s="46" t="s">
-        <v>441</v>
-      </c>
-      <c r="C91" s="56" t="s">
-        <v>50</v>
-      </c>
-      <c r="D91" s="56">
-        <v>0</v>
-      </c>
-      <c r="E91" s="46" t="s">
+      <c r="D93" s="53">
+        <v>1</v>
+      </c>
+      <c r="E93" s="46" t="s">
+        <v>443</v>
+      </c>
+      <c r="F93" s="53"/>
+      <c r="G93" s="55" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A94" s="53" t="s">
+        <v>1</v>
+      </c>
+      <c r="B94" s="46" t="s">
         <v>444</v>
       </c>
-      <c r="F91" s="56"/>
-      <c r="G91" s="58" t="s">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A92" s="56" t="s">
-        <v>1</v>
-      </c>
-      <c r="B92" s="46" t="s">
-        <v>442</v>
-      </c>
-      <c r="C92" s="56" t="s">
-        <v>50</v>
-      </c>
-      <c r="D92" s="56">
+      <c r="C94" s="53" t="s">
+        <v>237</v>
+      </c>
+      <c r="D94" s="53">
+        <v>0</v>
+      </c>
+      <c r="E94" s="46" t="s">
+        <v>447</v>
+      </c>
+      <c r="F94" s="53"/>
+      <c r="G94" s="55" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A95" s="53" t="s">
+        <v>1</v>
+      </c>
+      <c r="B95" s="46" t="s">
+        <v>445</v>
+      </c>
+      <c r="C95" s="53" t="s">
+        <v>237</v>
+      </c>
+      <c r="D95" s="53">
         <v>2</v>
       </c>
-      <c r="E92" s="46" t="s">
-        <v>444</v>
-      </c>
-      <c r="F92" s="56"/>
-      <c r="G92" s="58" t="s">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A93" s="56" t="s">
-        <v>1</v>
-      </c>
-      <c r="B93" s="46" t="s">
-        <v>443</v>
-      </c>
-      <c r="C93" s="56" t="s">
-        <v>50</v>
-      </c>
-      <c r="D93" s="56">
-        <v>1</v>
-      </c>
-      <c r="E93" s="46" t="s">
-        <v>444</v>
-      </c>
-      <c r="F93" s="56"/>
-      <c r="G93" s="58" t="s">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A94" s="56" t="s">
-        <v>1</v>
-      </c>
-      <c r="B94" s="46" t="s">
-        <v>445</v>
-      </c>
-      <c r="C94" s="56" t="s">
+      <c r="E95" s="46" t="s">
+        <v>447</v>
+      </c>
+      <c r="F95" s="53"/>
+      <c r="G95" s="55" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A96" s="53" t="s">
+        <v>1</v>
+      </c>
+      <c r="B96" s="46" t="s">
+        <v>446</v>
+      </c>
+      <c r="C96" s="53" t="s">
         <v>237</v>
       </c>
-      <c r="D94" s="56">
-        <v>0</v>
-      </c>
-      <c r="E94" s="46" t="s">
+      <c r="D96" s="53">
+        <v>1</v>
+      </c>
+      <c r="E96" s="46" t="s">
+        <v>447</v>
+      </c>
+      <c r="F96" s="53"/>
+      <c r="G96" s="55" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A97" s="53" t="s">
+        <v>1</v>
+      </c>
+      <c r="B97" s="46" t="s">
         <v>448</v>
       </c>
-      <c r="F94" s="56"/>
-      <c r="G94" s="58" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A95" s="56" t="s">
-        <v>1</v>
-      </c>
-      <c r="B95" s="46" t="s">
-        <v>446</v>
-      </c>
-      <c r="C95" s="56" t="s">
-        <v>237</v>
-      </c>
-      <c r="D95" s="56">
+      <c r="C97" s="53" t="s">
+        <v>451</v>
+      </c>
+      <c r="D97" s="53">
+        <v>0</v>
+      </c>
+      <c r="E97" s="53"/>
+      <c r="F97" s="53"/>
+      <c r="G97" s="53" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A98" s="53" t="s">
+        <v>1</v>
+      </c>
+      <c r="B98" s="46" t="s">
+        <v>449</v>
+      </c>
+      <c r="C98" s="53" t="s">
+        <v>451</v>
+      </c>
+      <c r="D98" s="53">
         <v>2</v>
       </c>
-      <c r="E95" s="46" t="s">
-        <v>448</v>
-      </c>
-      <c r="F95" s="56"/>
-      <c r="G95" s="58" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A96" s="56" t="s">
-        <v>1</v>
-      </c>
-      <c r="B96" s="46" t="s">
-        <v>447</v>
-      </c>
-      <c r="C96" s="56" t="s">
-        <v>237</v>
-      </c>
-      <c r="D96" s="56">
-        <v>1</v>
-      </c>
-      <c r="E96" s="46" t="s">
-        <v>448</v>
-      </c>
-      <c r="F96" s="56"/>
-      <c r="G96" s="58" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A97" s="56" t="s">
-        <v>1</v>
-      </c>
-      <c r="B97" s="46" t="s">
-        <v>449</v>
-      </c>
-      <c r="C97" s="56" t="s">
+      <c r="E98" s="53"/>
+      <c r="F98" s="53"/>
+      <c r="G98" s="53" t="s">
         <v>452</v>
       </c>
-      <c r="D97" s="56">
-        <v>0</v>
-      </c>
-      <c r="E97" s="56"/>
-      <c r="F97" s="56" t="s">
-        <v>380</v>
-      </c>
-      <c r="G97" s="56" t="s">
-        <v>453</v>
-      </c>
-    </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A98" s="56" t="s">
-        <v>1</v>
-      </c>
-      <c r="B98" s="46" t="s">
+    </row>
+    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A99" s="53" t="s">
+        <v>1</v>
+      </c>
+      <c r="B99" s="46" t="s">
         <v>450</v>
       </c>
-      <c r="C98" s="56" t="s">
+      <c r="C99" s="53" t="s">
+        <v>451</v>
+      </c>
+      <c r="D99" s="53">
+        <v>1</v>
+      </c>
+      <c r="E99" s="53"/>
+      <c r="F99" s="53"/>
+      <c r="G99" s="53" t="s">
         <v>452</v>
-      </c>
-      <c r="D98" s="56">
-        <v>2</v>
-      </c>
-      <c r="E98" s="56"/>
-      <c r="F98" s="56" t="s">
-        <v>380</v>
-      </c>
-      <c r="G98" s="56" t="s">
-        <v>453</v>
-      </c>
-    </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A99" s="56" t="s">
-        <v>1</v>
-      </c>
-      <c r="B99" s="46" t="s">
-        <v>451</v>
-      </c>
-      <c r="C99" s="56" t="s">
-        <v>452</v>
-      </c>
-      <c r="D99" s="56">
-        <v>1</v>
-      </c>
-      <c r="E99" s="56"/>
-      <c r="F99" s="56" t="s">
-        <v>380</v>
-      </c>
-      <c r="G99" s="56" t="s">
-        <v>453</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
adjustments forest event, added icon name to missions content
Former-commit-id: 5b438b7ca09bc022c75d2f5dae7e87f71cd617fe
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Missions.xlsx
+++ b/Docs/Content/HungryDragonContent_Missions.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\dragon\client\Docs\Content\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\dragon\client\Docs\Content\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="38295" windowHeight="19860" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="38295" windowHeight="19860"/>
   </bookViews>
   <sheets>
     <sheet name="missions" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1061" uniqueCount="454">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1070" uniqueCount="460">
   <si>
     <t>single_run</t>
   </si>
@@ -1414,6 +1414,24 @@
   </si>
   <si>
     <t>icon_golden</t>
+  </si>
+  <si>
+    <t>PF_icon_humans_halloween</t>
+  </si>
+  <si>
+    <t>PF_icon_grave_zombie</t>
+  </si>
+  <si>
+    <t>PF_icon_masks_halloween</t>
+  </si>
+  <si>
+    <t>icon_humans_halloween</t>
+  </si>
+  <si>
+    <t>icon_grave_zombie</t>
+  </si>
+  <si>
+    <t>icon_masks_halloween</t>
   </si>
 </sst>
 </file>
@@ -1857,13 +1875,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1874,21 +1885,18 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="69">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
@@ -3040,6 +3048,16 @@
         </bottom>
       </border>
     </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -3054,99 +3072,99 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="missionDifficultyDefinitions" displayName="missionDifficultyDefinitions" ref="B73:L76" totalsRowShown="0" headerRowBorderDxfId="68" tableBorderDxfId="67">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="missionDifficultyDefinitions" displayName="missionDifficultyDefinitions" ref="B73:L76" totalsRowShown="0" headerRowBorderDxfId="67" tableBorderDxfId="66">
   <autoFilter ref="B73:L76"/>
   <tableColumns count="11">
     <tableColumn id="1" name="{missionDifficultyDefinitions}"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="66"/>
-    <tableColumn id="11" name="[difficulty]" dataDxfId="65"/>
-    <tableColumn id="7" name="[index]" dataDxfId="64"/>
-    <tableColumn id="3" name="[dragonsToUnlock]" dataDxfId="63"/>
-    <tableColumn id="4" name="[cooldownMinutes]" dataDxfId="62"/>
-    <tableColumn id="9" name="[maxRewardCoins]" dataDxfId="61"/>
-    <tableColumn id="5" name="[removeMissionPCCoefA]" dataDxfId="60"/>
-    <tableColumn id="6" name="[removeMissionPCCoefB]" dataDxfId="59"/>
-    <tableColumn id="8" name="[tidName]" dataDxfId="58"/>
-    <tableColumn id="10" name="[color]" dataDxfId="57"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="65"/>
+    <tableColumn id="11" name="[difficulty]" dataDxfId="64"/>
+    <tableColumn id="7" name="[index]" dataDxfId="63"/>
+    <tableColumn id="3" name="[dragonsToUnlock]" dataDxfId="62"/>
+    <tableColumn id="4" name="[cooldownMinutes]" dataDxfId="61"/>
+    <tableColumn id="9" name="[maxRewardCoins]" dataDxfId="60"/>
+    <tableColumn id="5" name="[removeMissionPCCoefA]" dataDxfId="59"/>
+    <tableColumn id="6" name="[removeMissionPCCoefB]" dataDxfId="58"/>
+    <tableColumn id="8" name="[tidName]" dataDxfId="57"/>
+    <tableColumn id="10" name="[color]" dataDxfId="56"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table13303132" displayName="Table13303132" ref="B81:E94" totalsRowShown="0" headerRowDxfId="56" dataDxfId="54" headerRowBorderDxfId="55" tableBorderDxfId="53" totalsRowBorderDxfId="52">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table13303132" displayName="Table13303132" ref="B81:E94" totalsRowShown="0" headerRowDxfId="55" dataDxfId="53" headerRowBorderDxfId="54" tableBorderDxfId="52" totalsRowBorderDxfId="51">
   <autoFilter ref="B81:E94"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="{missionDragonModifiersDefinitions}" dataDxfId="51"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="50"/>
-    <tableColumn id="7" name="[quantityModifier]" dataDxfId="49"/>
-    <tableColumn id="3" name="[missionSCRewardMultiplier]" dataDxfId="48"/>
+    <tableColumn id="1" name="{missionDragonModifiersDefinitions}" dataDxfId="50"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="49"/>
+    <tableColumn id="7" name="[quantityModifier]" dataDxfId="48"/>
+    <tableColumn id="3" name="[missionSCRewardMultiplier]" dataDxfId="47"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table1330313234" displayName="Table1330313234" ref="B98:E101" totalsRowShown="0" headerRowDxfId="47" dataDxfId="45" headerRowBorderDxfId="46" tableBorderDxfId="44" totalsRowBorderDxfId="43">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table1330313234" displayName="Table1330313234" ref="B98:E101" totalsRowShown="0" headerRowDxfId="46" dataDxfId="44" headerRowBorderDxfId="45" tableBorderDxfId="43" totalsRowBorderDxfId="42">
   <autoFilter ref="B98:E101"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="{missionDifficultyModifiersDefinitions}" dataDxfId="42"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="41"/>
-    <tableColumn id="3" name="[difficulty]" dataDxfId="40"/>
-    <tableColumn id="7" name="[quantityModifier]" dataDxfId="39"/>
+    <tableColumn id="1" name="{missionDifficultyModifiersDefinitions}" dataDxfId="41"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="40"/>
+    <tableColumn id="3" name="[difficulty]" dataDxfId="39"/>
+    <tableColumn id="7" name="[quantityModifier]" dataDxfId="38"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table133031323435" displayName="Table133031323435" ref="B105:D106" totalsRowShown="0" headerRowDxfId="38" dataDxfId="36" headerRowBorderDxfId="37" tableBorderDxfId="35" totalsRowBorderDxfId="34">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table133031323435" displayName="Table133031323435" ref="B105:D106" totalsRowShown="0" headerRowDxfId="37" dataDxfId="35" headerRowBorderDxfId="36" tableBorderDxfId="34" totalsRowBorderDxfId="33">
   <autoFilter ref="B105:D106"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="{missionOtherModifiersDefinitions}" dataDxfId="33"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="32"/>
-    <tableColumn id="7" name="[quantityModifier]" dataDxfId="31"/>
+    <tableColumn id="1" name="{missionOtherModifiersDefinitions}" dataDxfId="32"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="31"/>
+    <tableColumn id="7" name="[quantityModifier]" dataDxfId="30"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table13" displayName="Table13" ref="B48:H67" totalsRowShown="0" headerRowDxfId="30" dataDxfId="28" headerRowBorderDxfId="29" tableBorderDxfId="27" totalsRowBorderDxfId="26">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table13" displayName="Table13" ref="B48:H67" totalsRowShown="0" headerRowDxfId="29" dataDxfId="27" headerRowBorderDxfId="28" tableBorderDxfId="26" totalsRowBorderDxfId="25">
   <autoFilter ref="B48:H67"/>
   <tableColumns count="7">
-    <tableColumn id="1" name="{missionTypeDefinitions}" dataDxfId="25"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="24"/>
-    <tableColumn id="3" name="[minTier]" dataDxfId="23"/>
-    <tableColumn id="6" name="[maxTier]" dataDxfId="22"/>
-    <tableColumn id="4" name="[weight]" dataDxfId="21"/>
-    <tableColumn id="9" name="[tidDescSingleRun]" dataDxfId="20"/>
-    <tableColumn id="10" name="[tidDescMultiRun]" dataDxfId="19"/>
+    <tableColumn id="1" name="{missionTypeDefinitions}" dataDxfId="24"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="23"/>
+    <tableColumn id="3" name="[minTier]" dataDxfId="22"/>
+    <tableColumn id="6" name="[maxTier]" dataDxfId="21"/>
+    <tableColumn id="4" name="[weight]" dataDxfId="20"/>
+    <tableColumn id="9" name="[tidDescSingleRun]" dataDxfId="19"/>
+    <tableColumn id="10" name="[tidDescMultiRun]" dataDxfId="18"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table1330" displayName="Table1330" ref="B4:N43" totalsRowShown="0" headerRowDxfId="18" dataDxfId="16" headerRowBorderDxfId="17" tableBorderDxfId="15" totalsRowBorderDxfId="14">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table1330" displayName="Table1330" ref="B4:N43" totalsRowShown="0" headerRowDxfId="17" dataDxfId="15" headerRowBorderDxfId="16" tableBorderDxfId="14" totalsRowBorderDxfId="13">
   <autoFilter ref="B4:N43"/>
   <sortState ref="B5:P43">
     <sortCondition descending="1" ref="J4:J43"/>
   </sortState>
   <tableColumns count="13">
-    <tableColumn id="1" name="{missionsDefinitions}" dataDxfId="13"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="12"/>
-    <tableColumn id="7" name="[type]" dataDxfId="11"/>
-    <tableColumn id="8" name="[weight]" dataDxfId="10"/>
-    <tableColumn id="13" name="[singleRunChance]" dataDxfId="9"/>
-    <tableColumn id="11" name="[minTier]" dataDxfId="8"/>
-    <tableColumn id="12" name="[maxTier]" dataDxfId="7"/>
-    <tableColumn id="6" name="[params]" dataDxfId="6"/>
-    <tableColumn id="3" name="[objectiveBaseQuantityMin]" dataDxfId="5"/>
-    <tableColumn id="9" name="[objectiveBaseQuantityMax]" dataDxfId="4"/>
-    <tableColumn id="4" name="[icon]" dataDxfId="3"/>
-    <tableColumn id="5" name="[tidObjective]" dataDxfId="2"/>
-    <tableColumn id="10" name="[trackingSku]" dataDxfId="1">
+    <tableColumn id="1" name="{missionsDefinitions}" dataDxfId="12"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="11"/>
+    <tableColumn id="7" name="[type]" dataDxfId="10"/>
+    <tableColumn id="8" name="[weight]" dataDxfId="9"/>
+    <tableColumn id="13" name="[singleRunChance]" dataDxfId="8"/>
+    <tableColumn id="11" name="[minTier]" dataDxfId="7"/>
+    <tableColumn id="12" name="[maxTier]" dataDxfId="6"/>
+    <tableColumn id="6" name="[params]" dataDxfId="5"/>
+    <tableColumn id="3" name="[objectiveBaseQuantityMin]" dataDxfId="4"/>
+    <tableColumn id="9" name="[objectiveBaseQuantityMax]" dataDxfId="3"/>
+    <tableColumn id="4" name="[icon]" dataDxfId="2"/>
+    <tableColumn id="5" name="[tidObjective]" dataDxfId="1"/>
+    <tableColumn id="10" name="[trackingSku]" dataDxfId="0">
       <calculatedColumnFormula>Table1330[[#This Row],['[sku']]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -3420,10 +3438,10 @@
   <sheetPr>
     <tabColor theme="6"/>
   </sheetPr>
-  <dimension ref="B1:P162"/>
+  <dimension ref="B1:P165"/>
   <sheetViews>
-    <sheetView topLeftCell="A124" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C162" sqref="C162"/>
+    <sheetView tabSelected="1" topLeftCell="A133" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C168" sqref="C168"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3470,14 +3488,14 @@
         <v>140</v>
       </c>
       <c r="G3" s="38"/>
-      <c r="J3" s="53" t="s">
+      <c r="J3" s="57" t="s">
         <v>139</v>
       </c>
-      <c r="K3" s="53"/>
-      <c r="M3" s="53"/>
-      <c r="N3" s="53"/>
-      <c r="O3" s="53"/>
-      <c r="P3" s="53"/>
+      <c r="K3" s="57"/>
+      <c r="M3" s="57"/>
+      <c r="N3" s="57"/>
+      <c r="O3" s="57"/>
+      <c r="P3" s="57"/>
     </row>
     <row r="4" spans="2:16" ht="106.5" x14ac:dyDescent="0.25">
       <c r="B4" s="30" t="s">
@@ -5157,9 +5175,9 @@
       <c r="C47" s="20"/>
       <c r="D47" s="20"/>
       <c r="E47" s="20"/>
-      <c r="F47" s="54"/>
-      <c r="G47" s="54"/>
-      <c r="H47" s="54"/>
+      <c r="F47" s="58"/>
+      <c r="G47" s="58"/>
+      <c r="H47" s="58"/>
       <c r="I47" s="20"/>
       <c r="J47" s="20"/>
     </row>
@@ -5688,10 +5706,10 @@
       <c r="F72" s="21" t="s">
         <v>40</v>
       </c>
-      <c r="G72" s="55" t="s">
+      <c r="G72" s="59" t="s">
         <v>39</v>
       </c>
-      <c r="H72" s="55"/>
+      <c r="H72" s="59"/>
       <c r="I72" s="20"/>
     </row>
     <row r="73" spans="2:13" ht="142.5" x14ac:dyDescent="0.25">
@@ -6891,6 +6909,48 @@
         <v>309</v>
       </c>
       <c r="E162" s="43" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="163" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B163" s="43" t="s">
+        <v>1</v>
+      </c>
+      <c r="C163" s="46" t="s">
+        <v>457</v>
+      </c>
+      <c r="D163" s="46" t="s">
+        <v>454</v>
+      </c>
+      <c r="E163" s="43" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="164" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B164" s="43" t="s">
+        <v>1</v>
+      </c>
+      <c r="C164" s="46" t="s">
+        <v>458</v>
+      </c>
+      <c r="D164" s="46" t="s">
+        <v>455</v>
+      </c>
+      <c r="E164" s="43" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="165" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B165" s="43" t="s">
+        <v>1</v>
+      </c>
+      <c r="C165" s="46" t="s">
+        <v>459</v>
+      </c>
+      <c r="D165" s="46" t="s">
+        <v>456</v>
+      </c>
+      <c r="E165" s="43" t="b">
         <v>1</v>
       </c>
     </row>
@@ -6902,7 +6962,7 @@
     <mergeCell ref="G72:H72"/>
   </mergeCells>
   <conditionalFormatting sqref="C74:E76">
-    <cfRule type="duplicateValues" dxfId="0" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="68" priority="2"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -6921,7 +6981,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G99"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A82" workbookViewId="0">
       <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
@@ -6981,2039 +7041,2039 @@
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="56" t="s">
+      <c r="A5" s="53" t="s">
         <v>1</v>
       </c>
       <c r="B5" s="46" t="s">
         <v>322</v>
       </c>
-      <c r="C5" s="56" t="s">
+      <c r="C5" s="53" t="s">
         <v>65</v>
       </c>
-      <c r="D5" s="56">
+      <c r="D5" s="53">
         <v>0</v>
       </c>
       <c r="E5" s="46" t="s">
         <v>81</v>
       </c>
-      <c r="F5" s="56" t="s">
+      <c r="F5" s="53" t="s">
         <v>324</v>
       </c>
-      <c r="G5" s="59" t="s">
+      <c r="G5" s="56" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="56" t="s">
+      <c r="A6" s="53" t="s">
         <v>1</v>
       </c>
       <c r="B6" s="46" t="s">
         <v>325</v>
       </c>
-      <c r="C6" s="56" t="s">
+      <c r="C6" s="53" t="s">
         <v>65</v>
       </c>
-      <c r="D6" s="56">
+      <c r="D6" s="53">
         <v>2</v>
       </c>
       <c r="E6" s="46" t="s">
         <v>81</v>
       </c>
-      <c r="F6" s="56" t="s">
+      <c r="F6" s="53" t="s">
         <v>324</v>
       </c>
-      <c r="G6" s="59" t="s">
+      <c r="G6" s="56" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="56" t="s">
+      <c r="A7" s="53" t="s">
         <v>1</v>
       </c>
       <c r="B7" s="46" t="s">
         <v>326</v>
       </c>
-      <c r="C7" s="56" t="s">
+      <c r="C7" s="53" t="s">
         <v>65</v>
       </c>
-      <c r="D7" s="56">
+      <c r="D7" s="53">
         <v>1</v>
       </c>
       <c r="E7" s="46" t="s">
         <v>81</v>
       </c>
-      <c r="F7" s="56" t="s">
+      <c r="F7" s="53" t="s">
         <v>324</v>
       </c>
-      <c r="G7" s="59" t="s">
+      <c r="G7" s="56" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="56" t="s">
+      <c r="A8" s="53" t="s">
         <v>1</v>
       </c>
       <c r="B8" s="46" t="s">
         <v>327</v>
       </c>
-      <c r="C8" s="56" t="s">
+      <c r="C8" s="53" t="s">
         <v>65</v>
       </c>
-      <c r="D8" s="56">
+      <c r="D8" s="53">
         <v>0</v>
       </c>
       <c r="E8" s="46" t="s">
         <v>328</v>
       </c>
-      <c r="F8" s="56" t="s">
+      <c r="F8" s="53" t="s">
         <v>329</v>
       </c>
-      <c r="G8" s="59" t="s">
+      <c r="G8" s="56" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="56" t="s">
+      <c r="A9" s="53" t="s">
         <v>1</v>
       </c>
       <c r="B9" s="46" t="s">
         <v>330</v>
       </c>
-      <c r="C9" s="56" t="s">
+      <c r="C9" s="53" t="s">
         <v>65</v>
       </c>
-      <c r="D9" s="56">
+      <c r="D9" s="53">
         <v>2</v>
       </c>
       <c r="E9" s="46" t="s">
         <v>328</v>
       </c>
-      <c r="F9" s="56" t="s">
+      <c r="F9" s="53" t="s">
         <v>329</v>
       </c>
-      <c r="G9" s="59" t="s">
+      <c r="G9" s="56" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="56" t="s">
+      <c r="A10" s="53" t="s">
         <v>1</v>
       </c>
       <c r="B10" s="46" t="s">
         <v>331</v>
       </c>
-      <c r="C10" s="56" t="s">
+      <c r="C10" s="53" t="s">
         <v>65</v>
       </c>
-      <c r="D10" s="56">
+      <c r="D10" s="53">
         <v>1</v>
       </c>
       <c r="E10" s="46" t="s">
         <v>328</v>
       </c>
-      <c r="F10" s="56" t="s">
+      <c r="F10" s="53" t="s">
         <v>329</v>
       </c>
-      <c r="G10" s="59" t="s">
+      <c r="G10" s="56" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="56" t="s">
+      <c r="A11" s="53" t="s">
         <v>1</v>
       </c>
       <c r="B11" s="46" t="s">
         <v>332</v>
       </c>
-      <c r="C11" s="56" t="s">
+      <c r="C11" s="53" t="s">
         <v>65</v>
       </c>
-      <c r="D11" s="56">
+      <c r="D11" s="53">
         <v>0</v>
       </c>
       <c r="E11" s="46" t="s">
         <v>333</v>
       </c>
-      <c r="F11" s="56" t="s">
+      <c r="F11" s="53" t="s">
         <v>334</v>
       </c>
-      <c r="G11" s="59" t="s">
+      <c r="G11" s="56" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="56" t="s">
+      <c r="A12" s="53" t="s">
         <v>1</v>
       </c>
       <c r="B12" s="46" t="s">
         <v>335</v>
       </c>
-      <c r="C12" s="56" t="s">
+      <c r="C12" s="53" t="s">
         <v>65</v>
       </c>
-      <c r="D12" s="56">
+      <c r="D12" s="53">
         <v>2</v>
       </c>
       <c r="E12" s="46" t="s">
         <v>333</v>
       </c>
-      <c r="F12" s="56" t="s">
+      <c r="F12" s="53" t="s">
         <v>334</v>
       </c>
-      <c r="G12" s="59" t="s">
+      <c r="G12" s="56" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="56" t="s">
+      <c r="A13" s="53" t="s">
         <v>1</v>
       </c>
       <c r="B13" s="46" t="s">
         <v>336</v>
       </c>
-      <c r="C13" s="56" t="s">
+      <c r="C13" s="53" t="s">
         <v>65</v>
       </c>
-      <c r="D13" s="56">
+      <c r="D13" s="53">
         <v>1</v>
       </c>
       <c r="E13" s="46" t="s">
         <v>333</v>
       </c>
-      <c r="F13" s="56" t="s">
+      <c r="F13" s="53" t="s">
         <v>334</v>
       </c>
-      <c r="G13" s="59" t="s">
+      <c r="G13" s="56" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="56" t="s">
+      <c r="A14" s="53" t="s">
         <v>1</v>
       </c>
       <c r="B14" s="46" t="s">
         <v>337</v>
       </c>
-      <c r="C14" s="56" t="s">
+      <c r="C14" s="53" t="s">
         <v>53</v>
       </c>
-      <c r="D14" s="56">
-        <v>0</v>
-      </c>
-      <c r="E14" s="56"/>
-      <c r="F14" s="56"/>
-      <c r="G14" s="59" t="s">
+      <c r="D14" s="53">
+        <v>0</v>
+      </c>
+      <c r="E14" s="53"/>
+      <c r="F14" s="53"/>
+      <c r="G14" s="56" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="56" t="s">
+      <c r="A15" s="53" t="s">
         <v>1</v>
       </c>
       <c r="B15" s="46" t="s">
         <v>338</v>
       </c>
-      <c r="C15" s="56" t="s">
+      <c r="C15" s="53" t="s">
         <v>180</v>
       </c>
-      <c r="D15" s="56">
+      <c r="D15" s="53">
         <v>0</v>
       </c>
       <c r="E15" s="46" t="s">
         <v>119</v>
       </c>
-      <c r="F15" s="56" t="s">
+      <c r="F15" s="53" t="s">
         <v>339</v>
       </c>
-      <c r="G15" s="59" t="s">
+      <c r="G15" s="56" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="56" t="s">
+      <c r="A16" s="53" t="s">
         <v>1</v>
       </c>
       <c r="B16" s="46" t="s">
         <v>340</v>
       </c>
-      <c r="C16" s="56" t="s">
+      <c r="C16" s="53" t="s">
         <v>180</v>
       </c>
-      <c r="D16" s="56">
+      <c r="D16" s="53">
         <v>2</v>
       </c>
       <c r="E16" s="46" t="s">
         <v>119</v>
       </c>
-      <c r="F16" s="56" t="s">
+      <c r="F16" s="53" t="s">
         <v>339</v>
       </c>
-      <c r="G16" s="59" t="s">
+      <c r="G16" s="56" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="56" t="s">
+      <c r="A17" s="53" t="s">
         <v>1</v>
       </c>
       <c r="B17" s="46" t="s">
         <v>341</v>
       </c>
-      <c r="C17" s="56" t="s">
+      <c r="C17" s="53" t="s">
         <v>180</v>
       </c>
-      <c r="D17" s="56">
+      <c r="D17" s="53">
         <v>1</v>
       </c>
       <c r="E17" s="46" t="s">
         <v>119</v>
       </c>
-      <c r="F17" s="56" t="s">
+      <c r="F17" s="53" t="s">
         <v>339</v>
       </c>
-      <c r="G17" s="59" t="s">
+      <c r="G17" s="56" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="56" t="s">
+      <c r="A18" s="53" t="s">
         <v>1</v>
       </c>
       <c r="B18" s="46" t="s">
         <v>342</v>
       </c>
-      <c r="C18" s="56" t="s">
+      <c r="C18" s="53" t="s">
         <v>65</v>
       </c>
-      <c r="D18" s="56">
+      <c r="D18" s="53">
         <v>0</v>
       </c>
       <c r="E18" s="46" t="s">
         <v>345</v>
       </c>
-      <c r="F18" s="56" t="s">
+      <c r="F18" s="53" t="s">
         <v>346</v>
       </c>
-      <c r="G18" s="59" t="s">
+      <c r="G18" s="56" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="56" t="s">
+      <c r="A19" s="53" t="s">
         <v>1</v>
       </c>
       <c r="B19" s="46" t="s">
         <v>343</v>
       </c>
-      <c r="C19" s="56" t="s">
+      <c r="C19" s="53" t="s">
         <v>65</v>
       </c>
-      <c r="D19" s="56">
+      <c r="D19" s="53">
         <v>2</v>
       </c>
       <c r="E19" s="46" t="s">
         <v>345</v>
       </c>
-      <c r="F19" s="56" t="s">
+      <c r="F19" s="53" t="s">
         <v>346</v>
       </c>
-      <c r="G19" s="59" t="s">
+      <c r="G19" s="56" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="56" t="s">
+      <c r="A20" s="53" t="s">
         <v>1</v>
       </c>
       <c r="B20" s="46" t="s">
         <v>344</v>
       </c>
-      <c r="C20" s="56" t="s">
+      <c r="C20" s="53" t="s">
         <v>65</v>
       </c>
-      <c r="D20" s="56">
+      <c r="D20" s="53">
         <v>1</v>
       </c>
       <c r="E20" s="46" t="s">
         <v>345</v>
       </c>
-      <c r="F20" s="56" t="s">
+      <c r="F20" s="53" t="s">
         <v>346</v>
       </c>
-      <c r="G20" s="59" t="s">
+      <c r="G20" s="56" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="56" t="s">
+      <c r="A21" s="53" t="s">
         <v>1</v>
       </c>
       <c r="B21" s="46" t="s">
         <v>347</v>
       </c>
-      <c r="C21" s="56" t="s">
+      <c r="C21" s="53" t="s">
         <v>65</v>
       </c>
-      <c r="D21" s="56">
+      <c r="D21" s="53">
         <v>0</v>
       </c>
       <c r="E21" s="46" t="s">
         <v>426</v>
       </c>
-      <c r="F21" s="56"/>
-      <c r="G21" s="58" t="s">
+      <c r="F21" s="53"/>
+      <c r="G21" s="55" t="s">
         <v>254</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="56" t="s">
+      <c r="A22" s="53" t="s">
         <v>1</v>
       </c>
       <c r="B22" s="46" t="s">
         <v>348</v>
       </c>
-      <c r="C22" s="56" t="s">
+      <c r="C22" s="53" t="s">
         <v>65</v>
       </c>
-      <c r="D22" s="56">
+      <c r="D22" s="53">
         <v>2</v>
       </c>
       <c r="E22" s="46" t="s">
         <v>426</v>
       </c>
-      <c r="F22" s="56"/>
-      <c r="G22" s="58" t="s">
+      <c r="F22" s="53"/>
+      <c r="G22" s="55" t="s">
         <v>254</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="56" t="s">
+      <c r="A23" s="53" t="s">
         <v>1</v>
       </c>
       <c r="B23" s="46" t="s">
         <v>349</v>
       </c>
-      <c r="C23" s="56" t="s">
+      <c r="C23" s="53" t="s">
         <v>65</v>
       </c>
-      <c r="D23" s="56">
+      <c r="D23" s="53">
         <v>1</v>
       </c>
       <c r="E23" s="46" t="s">
         <v>426</v>
       </c>
-      <c r="F23" s="56"/>
-      <c r="G23" s="58" t="s">
+      <c r="F23" s="53"/>
+      <c r="G23" s="55" t="s">
         <v>254</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="56" t="s">
+      <c r="A24" s="53" t="s">
         <v>1</v>
       </c>
       <c r="B24" s="46" t="s">
         <v>350</v>
       </c>
-      <c r="C24" s="56" t="s">
+      <c r="C24" s="53" t="s">
         <v>50</v>
       </c>
-      <c r="D24" s="56">
+      <c r="D24" s="53">
         <v>0</v>
       </c>
       <c r="E24" s="46" t="s">
         <v>352</v>
       </c>
-      <c r="F24" s="56"/>
-      <c r="G24" s="59" t="s">
+      <c r="F24" s="53"/>
+      <c r="G24" s="56" t="s">
         <v>245</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="56" t="s">
+      <c r="A25" s="53" t="s">
         <v>1</v>
       </c>
       <c r="B25" s="46" t="s">
         <v>351</v>
       </c>
-      <c r="C25" s="56" t="s">
+      <c r="C25" s="53" t="s">
         <v>50</v>
       </c>
-      <c r="D25" s="56">
+      <c r="D25" s="53">
         <v>2</v>
       </c>
       <c r="E25" s="46" t="s">
         <v>352</v>
       </c>
-      <c r="F25" s="56"/>
-      <c r="G25" s="59" t="s">
+      <c r="F25" s="53"/>
+      <c r="G25" s="56" t="s">
         <v>245</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="56" t="s">
+      <c r="A26" s="53" t="s">
         <v>1</v>
       </c>
       <c r="B26" s="46" t="s">
         <v>353</v>
       </c>
-      <c r="C26" s="56" t="s">
+      <c r="C26" s="53" t="s">
         <v>62</v>
       </c>
-      <c r="D26" s="56">
+      <c r="D26" s="53">
         <v>2</v>
       </c>
-      <c r="E26" s="56"/>
-      <c r="F26" s="56"/>
-      <c r="G26" s="59" t="s">
+      <c r="E26" s="53"/>
+      <c r="F26" s="53"/>
+      <c r="G26" s="56" t="s">
         <v>246</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="56" t="s">
+      <c r="A27" s="53" t="s">
         <v>1</v>
       </c>
       <c r="B27" s="46" t="s">
         <v>354</v>
       </c>
-      <c r="C27" s="56" t="s">
+      <c r="C27" s="53" t="s">
         <v>62</v>
       </c>
-      <c r="D27" s="56">
-        <v>1</v>
-      </c>
-      <c r="E27" s="56"/>
-      <c r="F27" s="56"/>
-      <c r="G27" s="59" t="s">
+      <c r="D27" s="53">
+        <v>1</v>
+      </c>
+      <c r="E27" s="53"/>
+      <c r="F27" s="53"/>
+      <c r="G27" s="56" t="s">
         <v>246</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="56" t="s">
+      <c r="A28" s="53" t="s">
         <v>1</v>
       </c>
       <c r="B28" s="46" t="s">
         <v>355</v>
       </c>
-      <c r="C28" s="56" t="s">
+      <c r="C28" s="53" t="s">
         <v>62</v>
       </c>
-      <c r="D28" s="56">
+      <c r="D28" s="53">
         <v>2</v>
       </c>
-      <c r="E28" s="56"/>
-      <c r="F28" s="56"/>
-      <c r="G28" s="59" t="s">
+      <c r="E28" s="53"/>
+      <c r="F28" s="53"/>
+      <c r="G28" s="56" t="s">
         <v>246</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" s="56" t="s">
+      <c r="A29" s="53" t="s">
         <v>1</v>
       </c>
       <c r="B29" s="46" t="s">
         <v>356</v>
       </c>
-      <c r="C29" s="56" t="s">
+      <c r="C29" s="53" t="s">
         <v>65</v>
       </c>
-      <c r="D29" s="56">
+      <c r="D29" s="53">
         <v>0</v>
       </c>
       <c r="E29" s="46" t="s">
         <v>359</v>
       </c>
-      <c r="F29" s="56" t="s">
+      <c r="F29" s="53" t="s">
         <v>360</v>
       </c>
-      <c r="G29" s="56" t="s">
+      <c r="G29" s="53" t="s">
         <v>361</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" s="56" t="s">
+      <c r="A30" s="53" t="s">
         <v>1</v>
       </c>
       <c r="B30" s="46" t="s">
         <v>357</v>
       </c>
-      <c r="C30" s="56" t="s">
+      <c r="C30" s="53" t="s">
         <v>65</v>
       </c>
-      <c r="D30" s="56">
+      <c r="D30" s="53">
         <v>1</v>
       </c>
       <c r="E30" s="46" t="s">
         <v>359</v>
       </c>
-      <c r="F30" s="56" t="s">
+      <c r="F30" s="53" t="s">
         <v>360</v>
       </c>
-      <c r="G30" s="56" t="s">
+      <c r="G30" s="53" t="s">
         <v>361</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A31" s="56" t="s">
+      <c r="A31" s="53" t="s">
         <v>1</v>
       </c>
       <c r="B31" s="46" t="s">
         <v>358</v>
       </c>
-      <c r="C31" s="56" t="s">
+      <c r="C31" s="53" t="s">
         <v>65</v>
       </c>
-      <c r="D31" s="56">
+      <c r="D31" s="53">
         <v>2</v>
       </c>
       <c r="E31" s="46" t="s">
         <v>359</v>
       </c>
-      <c r="F31" s="56" t="s">
+      <c r="F31" s="53" t="s">
         <v>360</v>
       </c>
-      <c r="G31" s="56" t="s">
+      <c r="G31" s="53" t="s">
         <v>361</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32" s="56" t="s">
+      <c r="A32" s="53" t="s">
         <v>1</v>
       </c>
       <c r="B32" s="46" t="s">
         <v>362</v>
       </c>
-      <c r="C32" s="56" t="s">
+      <c r="C32" s="53" t="s">
         <v>65</v>
       </c>
-      <c r="D32" s="56">
+      <c r="D32" s="53">
         <v>0</v>
       </c>
       <c r="E32" s="46" t="s">
         <v>365</v>
       </c>
-      <c r="F32" s="56" t="s">
+      <c r="F32" s="53" t="s">
         <v>366</v>
       </c>
-      <c r="G32" s="56" t="s">
+      <c r="G32" s="53" t="s">
         <v>367</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A33" s="56" t="s">
+      <c r="A33" s="53" t="s">
         <v>1</v>
       </c>
       <c r="B33" s="46" t="s">
         <v>363</v>
       </c>
-      <c r="C33" s="56" t="s">
+      <c r="C33" s="53" t="s">
         <v>65</v>
       </c>
-      <c r="D33" s="56">
+      <c r="D33" s="53">
         <v>2</v>
       </c>
       <c r="E33" s="46" t="s">
         <v>365</v>
       </c>
-      <c r="F33" s="56" t="s">
+      <c r="F33" s="53" t="s">
         <v>366</v>
       </c>
-      <c r="G33" s="56" t="s">
+      <c r="G33" s="53" t="s">
         <v>367</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A34" s="56" t="s">
+      <c r="A34" s="53" t="s">
         <v>1</v>
       </c>
       <c r="B34" s="46" t="s">
         <v>364</v>
       </c>
-      <c r="C34" s="56" t="s">
+      <c r="C34" s="53" t="s">
         <v>65</v>
       </c>
-      <c r="D34" s="56">
+      <c r="D34" s="53">
         <v>1</v>
       </c>
       <c r="E34" s="46" t="s">
         <v>365</v>
       </c>
-      <c r="F34" s="56" t="s">
+      <c r="F34" s="53" t="s">
         <v>366</v>
       </c>
-      <c r="G34" s="56" t="s">
+      <c r="G34" s="53" t="s">
         <v>367</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A35" s="56" t="s">
+      <c r="A35" s="53" t="s">
         <v>1</v>
       </c>
       <c r="B35" s="46" t="s">
         <v>368</v>
       </c>
-      <c r="C35" s="56" t="s">
+      <c r="C35" s="53" t="s">
         <v>65</v>
       </c>
-      <c r="D35" s="56">
+      <c r="D35" s="53">
         <v>0</v>
       </c>
       <c r="E35" s="46" t="s">
         <v>97</v>
       </c>
-      <c r="F35" s="56"/>
-      <c r="G35" s="58" t="s">
+      <c r="F35" s="53"/>
+      <c r="G35" s="55" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A36" s="56" t="s">
+      <c r="A36" s="53" t="s">
         <v>1</v>
       </c>
       <c r="B36" s="46" t="s">
         <v>369</v>
       </c>
-      <c r="C36" s="56" t="s">
+      <c r="C36" s="53" t="s">
         <v>65</v>
       </c>
-      <c r="D36" s="56">
+      <c r="D36" s="53">
         <v>2</v>
       </c>
       <c r="E36" s="46" t="s">
         <v>97</v>
       </c>
-      <c r="F36" s="56"/>
-      <c r="G36" s="58" t="s">
+      <c r="F36" s="53"/>
+      <c r="G36" s="55" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A37" s="56" t="s">
+      <c r="A37" s="53" t="s">
         <v>1</v>
       </c>
       <c r="B37" s="46" t="s">
         <v>370</v>
       </c>
-      <c r="C37" s="56" t="s">
+      <c r="C37" s="53" t="s">
         <v>65</v>
       </c>
-      <c r="D37" s="56">
+      <c r="D37" s="53">
         <v>1</v>
       </c>
       <c r="E37" s="46" t="s">
         <v>97</v>
       </c>
-      <c r="F37" s="56"/>
-      <c r="G37" s="58" t="s">
+      <c r="F37" s="53"/>
+      <c r="G37" s="55" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A38" s="56" t="s">
+      <c r="A38" s="53" t="s">
         <v>1</v>
       </c>
       <c r="B38" s="46" t="s">
         <v>371</v>
       </c>
-      <c r="C38" s="56" t="s">
+      <c r="C38" s="53" t="s">
         <v>65</v>
       </c>
-      <c r="D38" s="56">
-        <v>0</v>
-      </c>
-      <c r="E38" s="57" t="s">
+      <c r="D38" s="53">
+        <v>0</v>
+      </c>
+      <c r="E38" s="54" t="s">
         <v>374</v>
       </c>
-      <c r="F38" s="56" t="s">
+      <c r="F38" s="53" t="s">
         <v>375</v>
       </c>
-      <c r="G38" s="56" t="s">
+      <c r="G38" s="53" t="s">
         <v>376</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A39" s="56" t="s">
+      <c r="A39" s="53" t="s">
         <v>1</v>
       </c>
       <c r="B39" s="46" t="s">
         <v>372</v>
       </c>
-      <c r="C39" s="56" t="s">
+      <c r="C39" s="53" t="s">
         <v>65</v>
       </c>
-      <c r="D39" s="56">
+      <c r="D39" s="53">
         <v>2</v>
       </c>
-      <c r="E39" s="57" t="s">
+      <c r="E39" s="54" t="s">
         <v>374</v>
       </c>
-      <c r="F39" s="56" t="s">
+      <c r="F39" s="53" t="s">
         <v>375</v>
       </c>
-      <c r="G39" s="56" t="s">
+      <c r="G39" s="53" t="s">
         <v>376</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A40" s="56" t="s">
+      <c r="A40" s="53" t="s">
         <v>1</v>
       </c>
       <c r="B40" s="46" t="s">
         <v>373</v>
       </c>
-      <c r="C40" s="56" t="s">
+      <c r="C40" s="53" t="s">
         <v>65</v>
       </c>
-      <c r="D40" s="56">
-        <v>1</v>
-      </c>
-      <c r="E40" s="57" t="s">
+      <c r="D40" s="53">
+        <v>1</v>
+      </c>
+      <c r="E40" s="54" t="s">
         <v>374</v>
       </c>
-      <c r="F40" s="56" t="s">
+      <c r="F40" s="53" t="s">
         <v>375</v>
       </c>
-      <c r="G40" s="56" t="s">
+      <c r="G40" s="53" t="s">
         <v>376</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A41" s="56" t="s">
+      <c r="A41" s="53" t="s">
         <v>1</v>
       </c>
       <c r="B41" s="46" t="s">
         <v>377</v>
       </c>
-      <c r="C41" s="56" t="s">
+      <c r="C41" s="53" t="s">
         <v>231</v>
       </c>
-      <c r="D41" s="56">
-        <v>0</v>
-      </c>
-      <c r="E41" s="56"/>
-      <c r="F41" s="56" t="s">
+      <c r="D41" s="53">
+        <v>0</v>
+      </c>
+      <c r="E41" s="53"/>
+      <c r="F41" s="53" t="s">
         <v>380</v>
       </c>
-      <c r="G41" s="58" t="s">
+      <c r="G41" s="55" t="s">
         <v>251</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A42" s="56" t="s">
+      <c r="A42" s="53" t="s">
         <v>1</v>
       </c>
       <c r="B42" s="46" t="s">
         <v>378</v>
       </c>
-      <c r="C42" s="56" t="s">
+      <c r="C42" s="53" t="s">
         <v>231</v>
       </c>
-      <c r="D42" s="56">
+      <c r="D42" s="53">
         <v>2</v>
       </c>
-      <c r="E42" s="56"/>
-      <c r="F42" s="56" t="s">
+      <c r="E42" s="53"/>
+      <c r="F42" s="53" t="s">
         <v>380</v>
       </c>
-      <c r="G42" s="58" t="s">
+      <c r="G42" s="55" t="s">
         <v>251</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A43" s="56" t="s">
+      <c r="A43" s="53" t="s">
         <v>1</v>
       </c>
       <c r="B43" s="46" t="s">
         <v>379</v>
       </c>
-      <c r="C43" s="56" t="s">
+      <c r="C43" s="53" t="s">
         <v>231</v>
       </c>
-      <c r="D43" s="56">
-        <v>1</v>
-      </c>
-      <c r="E43" s="56"/>
-      <c r="F43" s="56" t="s">
+      <c r="D43" s="53">
+        <v>1</v>
+      </c>
+      <c r="E43" s="53"/>
+      <c r="F43" s="53" t="s">
         <v>380</v>
       </c>
-      <c r="G43" s="58" t="s">
+      <c r="G43" s="55" t="s">
         <v>251</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A44" s="56" t="s">
+      <c r="A44" s="53" t="s">
         <v>1</v>
       </c>
       <c r="B44" s="46" t="s">
         <v>381</v>
       </c>
-      <c r="C44" s="56" t="s">
+      <c r="C44" s="53" t="s">
         <v>65</v>
       </c>
-      <c r="D44" s="56">
+      <c r="D44" s="53">
         <v>0</v>
       </c>
       <c r="E44" s="46" t="s">
         <v>384</v>
       </c>
-      <c r="F44" s="56" t="s">
+      <c r="F44" s="53" t="s">
         <v>385</v>
       </c>
-      <c r="G44" s="58" t="s">
+      <c r="G44" s="55" t="s">
         <v>123</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A45" s="56" t="s">
+      <c r="A45" s="53" t="s">
         <v>1</v>
       </c>
       <c r="B45" s="46" t="s">
         <v>382</v>
       </c>
-      <c r="C45" s="56" t="s">
+      <c r="C45" s="53" t="s">
         <v>65</v>
       </c>
-      <c r="D45" s="56">
+      <c r="D45" s="53">
         <v>2</v>
       </c>
       <c r="E45" s="46" t="s">
         <v>384</v>
       </c>
-      <c r="F45" s="56" t="s">
+      <c r="F45" s="53" t="s">
         <v>385</v>
       </c>
-      <c r="G45" s="58" t="s">
+      <c r="G45" s="55" t="s">
         <v>123</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A46" s="56" t="s">
+      <c r="A46" s="53" t="s">
         <v>1</v>
       </c>
       <c r="B46" s="46" t="s">
         <v>383</v>
       </c>
-      <c r="C46" s="56" t="s">
+      <c r="C46" s="53" t="s">
         <v>65</v>
       </c>
-      <c r="D46" s="56">
+      <c r="D46" s="53">
         <v>1</v>
       </c>
       <c r="E46" s="46" t="s">
         <v>384</v>
       </c>
-      <c r="F46" s="56" t="s">
+      <c r="F46" s="53" t="s">
         <v>385</v>
       </c>
-      <c r="G46" s="58" t="s">
+      <c r="G46" s="55" t="s">
         <v>123</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A47" s="56" t="s">
+      <c r="A47" s="53" t="s">
         <v>1</v>
       </c>
       <c r="B47" s="46" t="s">
         <v>386</v>
       </c>
-      <c r="C47" s="56" t="s">
+      <c r="C47" s="53" t="s">
         <v>50</v>
       </c>
-      <c r="D47" s="56">
+      <c r="D47" s="53">
         <v>0</v>
       </c>
       <c r="E47" s="46" t="s">
         <v>117</v>
       </c>
-      <c r="F47" s="56"/>
-      <c r="G47" s="58" t="s">
+      <c r="F47" s="53"/>
+      <c r="G47" s="55" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A48" s="56" t="s">
+      <c r="A48" s="53" t="s">
         <v>1</v>
       </c>
       <c r="B48" s="46" t="s">
         <v>387</v>
       </c>
-      <c r="C48" s="56" t="s">
+      <c r="C48" s="53" t="s">
         <v>50</v>
       </c>
-      <c r="D48" s="56">
+      <c r="D48" s="53">
         <v>2</v>
       </c>
       <c r="E48" s="46" t="s">
         <v>117</v>
       </c>
-      <c r="F48" s="56"/>
-      <c r="G48" s="58" t="s">
+      <c r="F48" s="53"/>
+      <c r="G48" s="55" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A49" s="56" t="s">
+      <c r="A49" s="53" t="s">
         <v>1</v>
       </c>
       <c r="B49" s="46" t="s">
         <v>388</v>
       </c>
-      <c r="C49" s="56" t="s">
+      <c r="C49" s="53" t="s">
         <v>50</v>
       </c>
-      <c r="D49" s="56">
+      <c r="D49" s="53">
         <v>1</v>
       </c>
       <c r="E49" s="46" t="s">
         <v>117</v>
       </c>
-      <c r="F49" s="56"/>
-      <c r="G49" s="58" t="s">
+      <c r="F49" s="53"/>
+      <c r="G49" s="55" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A50" s="56" t="s">
+      <c r="A50" s="53" t="s">
         <v>1</v>
       </c>
       <c r="B50" s="46" t="s">
         <v>389</v>
       </c>
-      <c r="C50" s="56" t="s">
+      <c r="C50" s="53" t="s">
         <v>50</v>
       </c>
-      <c r="D50" s="56">
+      <c r="D50" s="53">
         <v>0</v>
       </c>
       <c r="E50" s="46" t="s">
         <v>392</v>
       </c>
-      <c r="F50" s="56"/>
-      <c r="G50" s="58" t="s">
+      <c r="F50" s="53"/>
+      <c r="G50" s="55" t="s">
         <v>252</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A51" s="56" t="s">
+      <c r="A51" s="53" t="s">
         <v>1</v>
       </c>
       <c r="B51" s="46" t="s">
         <v>390</v>
       </c>
-      <c r="C51" s="56" t="s">
+      <c r="C51" s="53" t="s">
         <v>50</v>
       </c>
-      <c r="D51" s="56">
+      <c r="D51" s="53">
         <v>2</v>
       </c>
       <c r="E51" s="46" t="s">
         <v>392</v>
       </c>
-      <c r="F51" s="56"/>
-      <c r="G51" s="58" t="s">
+      <c r="F51" s="53"/>
+      <c r="G51" s="55" t="s">
         <v>252</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A52" s="56" t="s">
+      <c r="A52" s="53" t="s">
         <v>1</v>
       </c>
       <c r="B52" s="46" t="s">
         <v>391</v>
       </c>
-      <c r="C52" s="56" t="s">
+      <c r="C52" s="53" t="s">
         <v>50</v>
       </c>
-      <c r="D52" s="56">
+      <c r="D52" s="53">
         <v>1</v>
       </c>
       <c r="E52" s="46" t="s">
         <v>392</v>
       </c>
-      <c r="F52" s="56"/>
-      <c r="G52" s="58" t="s">
+      <c r="F52" s="53"/>
+      <c r="G52" s="55" t="s">
         <v>252</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A53" s="56" t="s">
+      <c r="A53" s="53" t="s">
         <v>1</v>
       </c>
       <c r="B53" s="46" t="s">
         <v>393</v>
       </c>
-      <c r="C53" s="56" t="s">
+      <c r="C53" s="53" t="s">
         <v>47</v>
       </c>
-      <c r="D53" s="56">
-        <v>0</v>
-      </c>
-      <c r="E53" s="56"/>
-      <c r="F53" s="56"/>
-      <c r="G53" s="58" t="s">
+      <c r="D53" s="53">
+        <v>0</v>
+      </c>
+      <c r="E53" s="53"/>
+      <c r="F53" s="53"/>
+      <c r="G53" s="55" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A54" s="56" t="s">
+      <c r="A54" s="53" t="s">
         <v>1</v>
       </c>
       <c r="B54" s="46" t="s">
         <v>394</v>
       </c>
-      <c r="C54" s="56" t="s">
+      <c r="C54" s="53" t="s">
         <v>47</v>
       </c>
-      <c r="D54" s="56">
+      <c r="D54" s="53">
         <v>2</v>
       </c>
-      <c r="E54" s="56"/>
-      <c r="F54" s="56"/>
-      <c r="G54" s="58" t="s">
+      <c r="E54" s="53"/>
+      <c r="F54" s="53"/>
+      <c r="G54" s="55" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A55" s="56" t="s">
+      <c r="A55" s="53" t="s">
         <v>1</v>
       </c>
       <c r="B55" s="46" t="s">
         <v>395</v>
       </c>
-      <c r="C55" s="56" t="s">
+      <c r="C55" s="53" t="s">
         <v>47</v>
       </c>
-      <c r="D55" s="56">
-        <v>1</v>
-      </c>
-      <c r="E55" s="56"/>
-      <c r="F55" s="56"/>
-      <c r="G55" s="58" t="s">
+      <c r="D55" s="53">
+        <v>1</v>
+      </c>
+      <c r="E55" s="53"/>
+      <c r="F55" s="53"/>
+      <c r="G55" s="55" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A56" s="56" t="s">
+      <c r="A56" s="53" t="s">
         <v>1</v>
       </c>
       <c r="B56" s="46" t="s">
         <v>396</v>
       </c>
-      <c r="C56" s="56" t="s">
+      <c r="C56" s="53" t="s">
         <v>59</v>
       </c>
-      <c r="D56" s="56">
-        <v>0</v>
-      </c>
-      <c r="E56" s="56"/>
-      <c r="F56" s="56"/>
-      <c r="G56" s="58" t="s">
+      <c r="D56" s="53">
+        <v>0</v>
+      </c>
+      <c r="E56" s="53"/>
+      <c r="F56" s="53"/>
+      <c r="G56" s="55" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A57" s="56" t="s">
+      <c r="A57" s="53" t="s">
         <v>1</v>
       </c>
       <c r="B57" s="46" t="s">
         <v>397</v>
       </c>
-      <c r="C57" s="56" t="s">
+      <c r="C57" s="53" t="s">
         <v>59</v>
       </c>
-      <c r="D57" s="56">
+      <c r="D57" s="53">
         <v>2</v>
       </c>
-      <c r="E57" s="56"/>
-      <c r="F57" s="56"/>
-      <c r="G57" s="58" t="s">
+      <c r="E57" s="53"/>
+      <c r="F57" s="53"/>
+      <c r="G57" s="55" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A58" s="56" t="s">
+      <c r="A58" s="53" t="s">
         <v>1</v>
       </c>
       <c r="B58" s="46" t="s">
         <v>398</v>
       </c>
-      <c r="C58" s="56" t="s">
+      <c r="C58" s="53" t="s">
         <v>59</v>
       </c>
-      <c r="D58" s="56">
-        <v>1</v>
-      </c>
-      <c r="E58" s="57"/>
-      <c r="F58" s="56"/>
-      <c r="G58" s="58" t="s">
+      <c r="D58" s="53">
+        <v>1</v>
+      </c>
+      <c r="E58" s="54"/>
+      <c r="F58" s="53"/>
+      <c r="G58" s="55" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A59" s="56" t="s">
+      <c r="A59" s="53" t="s">
         <v>1</v>
       </c>
       <c r="B59" s="46" t="s">
         <v>399</v>
       </c>
-      <c r="C59" s="56" t="s">
+      <c r="C59" s="53" t="s">
         <v>237</v>
       </c>
-      <c r="D59" s="56">
+      <c r="D59" s="53">
         <v>0</v>
       </c>
       <c r="E59" s="46" t="s">
         <v>402</v>
       </c>
-      <c r="F59" s="56"/>
-      <c r="G59" s="58" t="s">
+      <c r="F59" s="53"/>
+      <c r="G59" s="55" t="s">
         <v>259</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A60" s="56" t="s">
+      <c r="A60" s="53" t="s">
         <v>1</v>
       </c>
       <c r="B60" s="46" t="s">
         <v>400</v>
       </c>
-      <c r="C60" s="56" t="s">
+      <c r="C60" s="53" t="s">
         <v>237</v>
       </c>
-      <c r="D60" s="56">
+      <c r="D60" s="53">
         <v>2</v>
       </c>
       <c r="E60" s="46" t="s">
         <v>402</v>
       </c>
-      <c r="F60" s="56"/>
-      <c r="G60" s="58" t="s">
+      <c r="F60" s="53"/>
+      <c r="G60" s="55" t="s">
         <v>259</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A61" s="56" t="s">
+      <c r="A61" s="53" t="s">
         <v>1</v>
       </c>
       <c r="B61" s="46" t="s">
         <v>401</v>
       </c>
-      <c r="C61" s="56" t="s">
+      <c r="C61" s="53" t="s">
         <v>237</v>
       </c>
-      <c r="D61" s="56">
+      <c r="D61" s="53">
         <v>1</v>
       </c>
       <c r="E61" s="46" t="s">
         <v>402</v>
       </c>
-      <c r="F61" s="56"/>
-      <c r="G61" s="58" t="s">
+      <c r="F61" s="53"/>
+      <c r="G61" s="55" t="s">
         <v>259</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A62" s="56" t="s">
+      <c r="A62" s="53" t="s">
         <v>1</v>
       </c>
       <c r="B62" s="46" t="s">
         <v>403</v>
       </c>
-      <c r="C62" s="56" t="s">
+      <c r="C62" s="53" t="s">
         <v>65</v>
       </c>
-      <c r="D62" s="56">
+      <c r="D62" s="53">
         <v>0</v>
       </c>
       <c r="E62" s="46" t="s">
         <v>75</v>
       </c>
-      <c r="F62" s="56"/>
-      <c r="G62" s="56" t="s">
+      <c r="F62" s="53"/>
+      <c r="G62" s="53" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A63" s="56" t="s">
+      <c r="A63" s="53" t="s">
         <v>1</v>
       </c>
       <c r="B63" s="46" t="s">
         <v>404</v>
       </c>
-      <c r="C63" s="56" t="s">
+      <c r="C63" s="53" t="s">
         <v>65</v>
       </c>
-      <c r="D63" s="56">
+      <c r="D63" s="53">
         <v>2</v>
       </c>
       <c r="E63" s="46" t="s">
         <v>75</v>
       </c>
-      <c r="F63" s="56"/>
-      <c r="G63" s="56" t="s">
+      <c r="F63" s="53"/>
+      <c r="G63" s="53" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A64" s="56" t="s">
+      <c r="A64" s="53" t="s">
         <v>1</v>
       </c>
       <c r="B64" s="46" t="s">
         <v>405</v>
       </c>
-      <c r="C64" s="56" t="s">
+      <c r="C64" s="53" t="s">
         <v>65</v>
       </c>
-      <c r="D64" s="56">
+      <c r="D64" s="53">
         <v>1</v>
       </c>
       <c r="E64" s="46" t="s">
         <v>75</v>
       </c>
-      <c r="F64" s="56"/>
-      <c r="G64" s="56" t="s">
+      <c r="F64" s="53"/>
+      <c r="G64" s="53" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A65" s="56" t="s">
+      <c r="A65" s="53" t="s">
         <v>1</v>
       </c>
       <c r="B65" s="46" t="s">
         <v>406</v>
       </c>
-      <c r="C65" s="56" t="s">
+      <c r="C65" s="53" t="s">
         <v>237</v>
       </c>
-      <c r="D65" s="56">
+      <c r="D65" s="53">
         <v>0</v>
       </c>
       <c r="E65" s="46" t="s">
         <v>409</v>
       </c>
-      <c r="F65" s="56"/>
-      <c r="G65" s="58" t="s">
+      <c r="F65" s="53"/>
+      <c r="G65" s="55" t="s">
         <v>260</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A66" s="56" t="s">
+      <c r="A66" s="53" t="s">
         <v>1</v>
       </c>
       <c r="B66" s="46" t="s">
         <v>407</v>
       </c>
-      <c r="C66" s="56" t="s">
+      <c r="C66" s="53" t="s">
         <v>237</v>
       </c>
-      <c r="D66" s="56">
+      <c r="D66" s="53">
         <v>2</v>
       </c>
       <c r="E66" s="46" t="s">
         <v>409</v>
       </c>
-      <c r="F66" s="56"/>
-      <c r="G66" s="58" t="s">
+      <c r="F66" s="53"/>
+      <c r="G66" s="55" t="s">
         <v>260</v>
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A67" s="56" t="s">
+      <c r="A67" s="53" t="s">
         <v>1</v>
       </c>
       <c r="B67" s="46" t="s">
         <v>408</v>
       </c>
-      <c r="C67" s="56" t="s">
+      <c r="C67" s="53" t="s">
         <v>237</v>
       </c>
-      <c r="D67" s="56">
+      <c r="D67" s="53">
         <v>1</v>
       </c>
       <c r="E67" s="46" t="s">
         <v>409</v>
       </c>
-      <c r="F67" s="56"/>
-      <c r="G67" s="58" t="s">
+      <c r="F67" s="53"/>
+      <c r="G67" s="55" t="s">
         <v>260</v>
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A68" s="56" t="s">
+      <c r="A68" s="53" t="s">
         <v>1</v>
       </c>
       <c r="B68" s="46" t="s">
         <v>410</v>
       </c>
-      <c r="C68" s="56" t="s">
+      <c r="C68" s="53" t="s">
         <v>65</v>
       </c>
-      <c r="D68" s="56">
+      <c r="D68" s="53">
         <v>0</v>
       </c>
       <c r="E68" s="46" t="s">
         <v>413</v>
       </c>
-      <c r="F68" s="56" t="s">
+      <c r="F68" s="53" t="s">
         <v>414</v>
       </c>
-      <c r="G68" s="58" t="s">
+      <c r="G68" s="55" t="s">
         <v>263</v>
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A69" s="56" t="s">
+      <c r="A69" s="53" t="s">
         <v>1</v>
       </c>
       <c r="B69" s="46" t="s">
         <v>411</v>
       </c>
-      <c r="C69" s="56" t="s">
+      <c r="C69" s="53" t="s">
         <v>65</v>
       </c>
-      <c r="D69" s="56">
+      <c r="D69" s="53">
         <v>2</v>
       </c>
       <c r="E69" s="46" t="s">
         <v>413</v>
       </c>
-      <c r="F69" s="56" t="s">
+      <c r="F69" s="53" t="s">
         <v>414</v>
       </c>
-      <c r="G69" s="58" t="s">
+      <c r="G69" s="55" t="s">
         <v>263</v>
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A70" s="56" t="s">
+      <c r="A70" s="53" t="s">
         <v>1</v>
       </c>
       <c r="B70" s="46" t="s">
         <v>412</v>
       </c>
-      <c r="C70" s="56" t="s">
+      <c r="C70" s="53" t="s">
         <v>65</v>
       </c>
-      <c r="D70" s="56">
+      <c r="D70" s="53">
         <v>1</v>
       </c>
       <c r="E70" s="46" t="s">
         <v>413</v>
       </c>
-      <c r="F70" s="56" t="s">
+      <c r="F70" s="53" t="s">
         <v>414</v>
       </c>
-      <c r="G70" s="58" t="s">
+      <c r="G70" s="55" t="s">
         <v>263</v>
       </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A71" s="56" t="s">
+      <c r="A71" s="53" t="s">
         <v>1</v>
       </c>
       <c r="B71" s="46" t="s">
         <v>415</v>
       </c>
-      <c r="C71" s="56" t="s">
+      <c r="C71" s="53" t="s">
         <v>228</v>
       </c>
-      <c r="D71" s="56">
-        <v>0</v>
-      </c>
-      <c r="E71" s="56"/>
-      <c r="F71" s="56" t="s">
+      <c r="D71" s="53">
+        <v>0</v>
+      </c>
+      <c r="E71" s="53"/>
+      <c r="F71" s="53" t="s">
         <v>380</v>
       </c>
-      <c r="G71" s="56" t="s">
+      <c r="G71" s="53" t="s">
         <v>418</v>
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A72" s="56" t="s">
+      <c r="A72" s="53" t="s">
         <v>1</v>
       </c>
       <c r="B72" s="46" t="s">
         <v>416</v>
       </c>
-      <c r="C72" s="56" t="s">
+      <c r="C72" s="53" t="s">
         <v>228</v>
       </c>
-      <c r="D72" s="56">
+      <c r="D72" s="53">
         <v>2</v>
       </c>
-      <c r="E72" s="56"/>
-      <c r="F72" s="56" t="s">
+      <c r="E72" s="53"/>
+      <c r="F72" s="53" t="s">
         <v>380</v>
       </c>
-      <c r="G72" s="56" t="s">
+      <c r="G72" s="53" t="s">
         <v>418</v>
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A73" s="56" t="s">
+      <c r="A73" s="53" t="s">
         <v>1</v>
       </c>
       <c r="B73" s="46" t="s">
         <v>417</v>
       </c>
-      <c r="C73" s="56" t="s">
+      <c r="C73" s="53" t="s">
         <v>228</v>
       </c>
-      <c r="D73" s="56">
-        <v>1</v>
-      </c>
-      <c r="E73" s="56"/>
-      <c r="F73" s="56" t="s">
+      <c r="D73" s="53">
+        <v>1</v>
+      </c>
+      <c r="E73" s="53"/>
+      <c r="F73" s="53" t="s">
         <v>380</v>
       </c>
-      <c r="G73" s="56" t="s">
+      <c r="G73" s="53" t="s">
         <v>418</v>
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A74" s="56" t="s">
+      <c r="A74" s="53" t="s">
         <v>1</v>
       </c>
       <c r="B74" s="46" t="s">
         <v>419</v>
       </c>
-      <c r="C74" s="56" t="s">
+      <c r="C74" s="53" t="s">
         <v>234</v>
       </c>
-      <c r="D74" s="56">
-        <v>0</v>
-      </c>
-      <c r="E74" s="56"/>
-      <c r="F74" s="56" t="s">
+      <c r="D74" s="53">
+        <v>0</v>
+      </c>
+      <c r="E74" s="53"/>
+      <c r="F74" s="53" t="s">
         <v>380</v>
       </c>
-      <c r="G74" s="56" t="s">
+      <c r="G74" s="53" t="s">
         <v>422</v>
       </c>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A75" s="56" t="s">
+      <c r="A75" s="53" t="s">
         <v>1</v>
       </c>
       <c r="B75" s="46" t="s">
         <v>420</v>
       </c>
-      <c r="C75" s="56" t="s">
+      <c r="C75" s="53" t="s">
         <v>234</v>
       </c>
-      <c r="D75" s="56">
+      <c r="D75" s="53">
         <v>2</v>
       </c>
-      <c r="E75" s="56"/>
-      <c r="F75" s="56" t="s">
+      <c r="E75" s="53"/>
+      <c r="F75" s="53" t="s">
         <v>380</v>
       </c>
-      <c r="G75" s="56" t="s">
+      <c r="G75" s="53" t="s">
         <v>422</v>
       </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A76" s="56" t="s">
+      <c r="A76" s="53" t="s">
         <v>1</v>
       </c>
       <c r="B76" s="46" t="s">
         <v>421</v>
       </c>
-      <c r="C76" s="56" t="s">
+      <c r="C76" s="53" t="s">
         <v>234</v>
       </c>
-      <c r="D76" s="56">
-        <v>1</v>
-      </c>
-      <c r="E76" s="56"/>
-      <c r="F76" s="56" t="s">
+      <c r="D76" s="53">
+        <v>1</v>
+      </c>
+      <c r="E76" s="53"/>
+      <c r="F76" s="53" t="s">
         <v>380</v>
       </c>
-      <c r="G76" s="56" t="s">
+      <c r="G76" s="53" t="s">
         <v>422</v>
       </c>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A77" s="56" t="s">
+      <c r="A77" s="53" t="s">
         <v>1</v>
       </c>
       <c r="B77" s="46" t="s">
         <v>423</v>
       </c>
-      <c r="C77" s="59" t="s">
+      <c r="C77" s="56" t="s">
         <v>313</v>
       </c>
-      <c r="D77" s="56">
-        <v>0</v>
-      </c>
-      <c r="E77" s="56"/>
-      <c r="F77" s="56"/>
-      <c r="G77" s="58" t="s">
+      <c r="D77" s="53">
+        <v>0</v>
+      </c>
+      <c r="E77" s="53"/>
+      <c r="F77" s="53"/>
+      <c r="G77" s="55" t="s">
         <v>310</v>
       </c>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A78" s="56" t="s">
+      <c r="A78" s="53" t="s">
         <v>1</v>
       </c>
       <c r="B78" s="46" t="s">
         <v>314</v>
       </c>
-      <c r="C78" s="59" t="s">
+      <c r="C78" s="56" t="s">
         <v>313</v>
       </c>
-      <c r="D78" s="56">
+      <c r="D78" s="53">
         <v>2</v>
       </c>
-      <c r="E78" s="56"/>
-      <c r="F78" s="56"/>
-      <c r="G78" s="58" t="s">
+      <c r="E78" s="53"/>
+      <c r="F78" s="53"/>
+      <c r="G78" s="55" t="s">
         <v>310</v>
       </c>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A79" s="56" t="s">
+      <c r="A79" s="53" t="s">
         <v>1</v>
       </c>
       <c r="B79" s="46" t="s">
         <v>424</v>
       </c>
-      <c r="C79" s="59" t="s">
+      <c r="C79" s="56" t="s">
         <v>313</v>
       </c>
-      <c r="D79" s="56">
-        <v>1</v>
-      </c>
-      <c r="E79" s="56"/>
-      <c r="F79" s="56"/>
-      <c r="G79" s="58" t="s">
+      <c r="D79" s="53">
+        <v>1</v>
+      </c>
+      <c r="E79" s="53"/>
+      <c r="F79" s="53"/>
+      <c r="G79" s="55" t="s">
         <v>310</v>
       </c>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A80" s="56" t="s">
+      <c r="A80" s="53" t="s">
         <v>1</v>
       </c>
       <c r="B80" s="46" t="s">
         <v>425</v>
       </c>
-      <c r="C80" s="59" t="s">
+      <c r="C80" s="56" t="s">
         <v>315</v>
       </c>
-      <c r="D80" s="56">
-        <v>0</v>
-      </c>
-      <c r="E80" s="57"/>
-      <c r="F80" s="56"/>
-      <c r="G80" s="58" t="s">
+      <c r="D80" s="53">
+        <v>0</v>
+      </c>
+      <c r="E80" s="54"/>
+      <c r="F80" s="53"/>
+      <c r="G80" s="55" t="s">
         <v>310</v>
       </c>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A81" s="56" t="s">
+      <c r="A81" s="53" t="s">
         <v>1</v>
       </c>
       <c r="B81" s="46" t="s">
         <v>316</v>
       </c>
-      <c r="C81" s="59" t="s">
+      <c r="C81" s="56" t="s">
         <v>315</v>
       </c>
-      <c r="D81" s="56">
+      <c r="D81" s="53">
         <v>2</v>
       </c>
-      <c r="E81" s="56"/>
-      <c r="F81" s="56"/>
-      <c r="G81" s="58" t="s">
+      <c r="E81" s="53"/>
+      <c r="F81" s="53"/>
+      <c r="G81" s="55" t="s">
         <v>310</v>
       </c>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A82" s="56" t="s">
+      <c r="A82" s="53" t="s">
         <v>1</v>
       </c>
       <c r="B82" s="46" t="s">
         <v>427</v>
       </c>
-      <c r="C82" s="56" t="s">
+      <c r="C82" s="53" t="s">
         <v>65</v>
       </c>
-      <c r="D82" s="56">
-        <v>0</v>
-      </c>
-      <c r="E82" s="57" t="s">
+      <c r="D82" s="53">
+        <v>0</v>
+      </c>
+      <c r="E82" s="54" t="s">
         <v>430</v>
       </c>
-      <c r="F82" s="56" t="s">
+      <c r="F82" s="53" t="s">
         <v>432</v>
       </c>
-      <c r="G82" s="56" t="s">
+      <c r="G82" s="53" t="s">
         <v>431</v>
       </c>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A83" s="56" t="s">
+      <c r="A83" s="53" t="s">
         <v>1</v>
       </c>
       <c r="B83" s="46" t="s">
         <v>428</v>
       </c>
-      <c r="C83" s="56" t="s">
+      <c r="C83" s="53" t="s">
         <v>65</v>
       </c>
-      <c r="D83" s="56">
+      <c r="D83" s="53">
         <v>2</v>
       </c>
-      <c r="E83" s="57" t="s">
+      <c r="E83" s="54" t="s">
         <v>430</v>
       </c>
-      <c r="F83" s="56" t="s">
+      <c r="F83" s="53" t="s">
         <v>432</v>
       </c>
-      <c r="G83" s="56" t="s">
+      <c r="G83" s="53" t="s">
         <v>431</v>
       </c>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A84" s="56" t="s">
+      <c r="A84" s="53" t="s">
         <v>1</v>
       </c>
       <c r="B84" s="46" t="s">
         <v>429</v>
       </c>
-      <c r="C84" s="56" t="s">
+      <c r="C84" s="53" t="s">
         <v>65</v>
       </c>
-      <c r="D84" s="56">
-        <v>1</v>
-      </c>
-      <c r="E84" s="57" t="s">
+      <c r="D84" s="53">
+        <v>1</v>
+      </c>
+      <c r="E84" s="54" t="s">
         <v>430</v>
       </c>
-      <c r="F84" s="56" t="s">
+      <c r="F84" s="53" t="s">
         <v>432</v>
       </c>
-      <c r="G84" s="56" t="s">
+      <c r="G84" s="53" t="s">
         <v>431</v>
       </c>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A85" s="56" t="s">
+      <c r="A85" s="53" t="s">
         <v>1</v>
       </c>
       <c r="B85" s="46" t="s">
         <v>433</v>
       </c>
-      <c r="C85" s="56" t="s">
+      <c r="C85" s="53" t="s">
         <v>65</v>
       </c>
-      <c r="D85" s="56">
+      <c r="D85" s="53">
         <v>0</v>
       </c>
       <c r="E85" s="46" t="s">
         <v>87</v>
       </c>
-      <c r="F85" s="56"/>
-      <c r="G85" s="58" t="s">
+      <c r="F85" s="53"/>
+      <c r="G85" s="55" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A86" s="56" t="s">
+      <c r="A86" s="53" t="s">
         <v>1</v>
       </c>
       <c r="B86" s="46" t="s">
         <v>434</v>
       </c>
-      <c r="C86" s="56" t="s">
+      <c r="C86" s="53" t="s">
         <v>65</v>
       </c>
-      <c r="D86" s="56">
+      <c r="D86" s="53">
         <v>2</v>
       </c>
       <c r="E86" s="46" t="s">
         <v>87</v>
       </c>
-      <c r="F86" s="56"/>
-      <c r="G86" s="58" t="s">
+      <c r="F86" s="53"/>
+      <c r="G86" s="55" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A87" s="56" t="s">
+      <c r="A87" s="53" t="s">
         <v>1</v>
       </c>
       <c r="B87" s="46" t="s">
         <v>435</v>
       </c>
-      <c r="C87" s="56" t="s">
+      <c r="C87" s="53" t="s">
         <v>65</v>
       </c>
-      <c r="D87" s="56">
+      <c r="D87" s="53">
         <v>1</v>
       </c>
       <c r="E87" s="46" t="s">
         <v>87</v>
       </c>
-      <c r="F87" s="56"/>
-      <c r="G87" s="58" t="s">
+      <c r="F87" s="53"/>
+      <c r="G87" s="55" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A88" s="56" t="s">
+      <c r="A88" s="53" t="s">
         <v>1</v>
       </c>
       <c r="B88" s="46" t="s">
         <v>436</v>
       </c>
-      <c r="C88" s="56" t="s">
+      <c r="C88" s="53" t="s">
         <v>50</v>
       </c>
-      <c r="D88" s="56">
+      <c r="D88" s="53">
         <v>0</v>
       </c>
       <c r="E88" s="46" t="s">
         <v>439</v>
       </c>
-      <c r="F88" s="56" t="s">
+      <c r="F88" s="53" t="s">
         <v>440</v>
       </c>
-      <c r="G88" s="58" t="s">
+      <c r="G88" s="55" t="s">
         <v>257</v>
       </c>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A89" s="56" t="s">
+      <c r="A89" s="53" t="s">
         <v>1</v>
       </c>
       <c r="B89" s="46" t="s">
         <v>437</v>
       </c>
-      <c r="C89" s="56" t="s">
+      <c r="C89" s="53" t="s">
         <v>50</v>
       </c>
-      <c r="D89" s="56">
+      <c r="D89" s="53">
         <v>2</v>
       </c>
       <c r="E89" s="46" t="s">
         <v>439</v>
       </c>
-      <c r="F89" s="56" t="s">
+      <c r="F89" s="53" t="s">
         <v>440</v>
       </c>
-      <c r="G89" s="58" t="s">
+      <c r="G89" s="55" t="s">
         <v>257</v>
       </c>
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A90" s="56" t="s">
+      <c r="A90" s="53" t="s">
         <v>1</v>
       </c>
       <c r="B90" s="46" t="s">
         <v>438</v>
       </c>
-      <c r="C90" s="56" t="s">
+      <c r="C90" s="53" t="s">
         <v>50</v>
       </c>
-      <c r="D90" s="56">
+      <c r="D90" s="53">
         <v>1</v>
       </c>
       <c r="E90" s="46" t="s">
         <v>439</v>
       </c>
-      <c r="F90" s="56" t="s">
+      <c r="F90" s="53" t="s">
         <v>440</v>
       </c>
-      <c r="G90" s="58" t="s">
+      <c r="G90" s="55" t="s">
         <v>257</v>
       </c>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A91" s="56" t="s">
+      <c r="A91" s="53" t="s">
         <v>1</v>
       </c>
       <c r="B91" s="46" t="s">
         <v>441</v>
       </c>
-      <c r="C91" s="56" t="s">
+      <c r="C91" s="53" t="s">
         <v>50</v>
       </c>
-      <c r="D91" s="56">
+      <c r="D91" s="53">
         <v>0</v>
       </c>
       <c r="E91" s="46" t="s">
         <v>444</v>
       </c>
-      <c r="F91" s="56"/>
-      <c r="G91" s="58" t="s">
+      <c r="F91" s="53"/>
+      <c r="G91" s="55" t="s">
         <v>311</v>
       </c>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A92" s="56" t="s">
+      <c r="A92" s="53" t="s">
         <v>1</v>
       </c>
       <c r="B92" s="46" t="s">
         <v>442</v>
       </c>
-      <c r="C92" s="56" t="s">
+      <c r="C92" s="53" t="s">
         <v>50</v>
       </c>
-      <c r="D92" s="56">
+      <c r="D92" s="53">
         <v>2</v>
       </c>
       <c r="E92" s="46" t="s">
         <v>444</v>
       </c>
-      <c r="F92" s="56"/>
-      <c r="G92" s="58" t="s">
+      <c r="F92" s="53"/>
+      <c r="G92" s="55" t="s">
         <v>311</v>
       </c>
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A93" s="56" t="s">
+      <c r="A93" s="53" t="s">
         <v>1</v>
       </c>
       <c r="B93" s="46" t="s">
         <v>443</v>
       </c>
-      <c r="C93" s="56" t="s">
+      <c r="C93" s="53" t="s">
         <v>50</v>
       </c>
-      <c r="D93" s="56">
+      <c r="D93" s="53">
         <v>1</v>
       </c>
       <c r="E93" s="46" t="s">
         <v>444</v>
       </c>
-      <c r="F93" s="56"/>
-      <c r="G93" s="58" t="s">
+      <c r="F93" s="53"/>
+      <c r="G93" s="55" t="s">
         <v>311</v>
       </c>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A94" s="56" t="s">
+      <c r="A94" s="53" t="s">
         <v>1</v>
       </c>
       <c r="B94" s="46" t="s">
         <v>445</v>
       </c>
-      <c r="C94" s="56" t="s">
+      <c r="C94" s="53" t="s">
         <v>237</v>
       </c>
-      <c r="D94" s="56">
+      <c r="D94" s="53">
         <v>0</v>
       </c>
       <c r="E94" s="46" t="s">
         <v>448</v>
       </c>
-      <c r="F94" s="56"/>
-      <c r="G94" s="58" t="s">
+      <c r="F94" s="53"/>
+      <c r="G94" s="55" t="s">
         <v>312</v>
       </c>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A95" s="56" t="s">
+      <c r="A95" s="53" t="s">
         <v>1</v>
       </c>
       <c r="B95" s="46" t="s">
         <v>446</v>
       </c>
-      <c r="C95" s="56" t="s">
+      <c r="C95" s="53" t="s">
         <v>237</v>
       </c>
-      <c r="D95" s="56">
+      <c r="D95" s="53">
         <v>2</v>
       </c>
       <c r="E95" s="46" t="s">
         <v>448</v>
       </c>
-      <c r="F95" s="56"/>
-      <c r="G95" s="58" t="s">
+      <c r="F95" s="53"/>
+      <c r="G95" s="55" t="s">
         <v>312</v>
       </c>
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A96" s="56" t="s">
+      <c r="A96" s="53" t="s">
         <v>1</v>
       </c>
       <c r="B96" s="46" t="s">
         <v>447</v>
       </c>
-      <c r="C96" s="56" t="s">
+      <c r="C96" s="53" t="s">
         <v>237</v>
       </c>
-      <c r="D96" s="56">
+      <c r="D96" s="53">
         <v>1</v>
       </c>
       <c r="E96" s="46" t="s">
         <v>448</v>
       </c>
-      <c r="F96" s="56"/>
-      <c r="G96" s="58" t="s">
+      <c r="F96" s="53"/>
+      <c r="G96" s="55" t="s">
         <v>312</v>
       </c>
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A97" s="56" t="s">
+      <c r="A97" s="53" t="s">
         <v>1</v>
       </c>
       <c r="B97" s="46" t="s">
         <v>449</v>
       </c>
-      <c r="C97" s="56" t="s">
+      <c r="C97" s="53" t="s">
         <v>452</v>
       </c>
-      <c r="D97" s="56">
-        <v>0</v>
-      </c>
-      <c r="E97" s="56"/>
-      <c r="F97" s="56" t="s">
+      <c r="D97" s="53">
+        <v>0</v>
+      </c>
+      <c r="E97" s="53"/>
+      <c r="F97" s="53" t="s">
         <v>380</v>
       </c>
-      <c r="G97" s="56" t="s">
+      <c r="G97" s="53" t="s">
         <v>453</v>
       </c>
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A98" s="56" t="s">
+      <c r="A98" s="53" t="s">
         <v>1</v>
       </c>
       <c r="B98" s="46" t="s">
         <v>450</v>
       </c>
-      <c r="C98" s="56" t="s">
+      <c r="C98" s="53" t="s">
         <v>452</v>
       </c>
-      <c r="D98" s="56">
+      <c r="D98" s="53">
         <v>2</v>
       </c>
-      <c r="E98" s="56"/>
-      <c r="F98" s="56" t="s">
+      <c r="E98" s="53"/>
+      <c r="F98" s="53" t="s">
         <v>380</v>
       </c>
-      <c r="G98" s="56" t="s">
+      <c r="G98" s="53" t="s">
         <v>453</v>
       </c>
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A99" s="56" t="s">
+      <c r="A99" s="53" t="s">
         <v>1</v>
       </c>
       <c r="B99" s="46" t="s">
         <v>451</v>
       </c>
-      <c r="C99" s="56" t="s">
+      <c r="C99" s="53" t="s">
         <v>452</v>
       </c>
-      <c r="D99" s="56">
-        <v>1</v>
-      </c>
-      <c r="E99" s="56"/>
-      <c r="F99" s="56" t="s">
+      <c r="D99" s="53">
+        <v>1</v>
+      </c>
+      <c r="E99" s="53"/>
+      <c r="F99" s="53" t="s">
         <v>380</v>
       </c>
-      <c r="G99" s="56" t="s">
+      <c r="G99" s="53" t="s">
         <v>453</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Adding mission modifiers for Legendary dragons
Former-commit-id: bd7be1a90a7624e0f4d7bc3271d9e337d3dbc3be
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Missions.xlsx
+++ b/Docs/Content/HungryDragonContent_Missions.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\dragon\client\Docs\Content\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\dragon\Docs\Content\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="38295" windowHeight="19860" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="38295" windowHeight="19860"/>
   </bookViews>
   <sheets>
     <sheet name="missions" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1049" uniqueCount="453">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1059" uniqueCount="458">
   <si>
     <t>single_run</t>
   </si>
@@ -1411,6 +1411,21 @@
   </si>
   <si>
     <t>icon_golden</t>
+  </si>
+  <si>
+    <t>dragon_electric</t>
+  </si>
+  <si>
+    <t>dragon_helicopter</t>
+  </si>
+  <si>
+    <t>dragon_hedgehog</t>
+  </si>
+  <si>
+    <t>dragon_ice</t>
+  </si>
+  <si>
+    <t>dragon_dino</t>
   </si>
 </sst>
 </file>
@@ -1877,6 +1892,16 @@
   </cellStyles>
   <dxfs count="69">
     <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
@@ -3027,16 +3052,6 @@
         </bottom>
       </border>
     </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -3051,99 +3066,99 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="missionDifficultyDefinitions" displayName="missionDifficultyDefinitions" ref="B73:L76" totalsRowShown="0" headerRowBorderDxfId="67" tableBorderDxfId="66">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="missionDifficultyDefinitions" displayName="missionDifficultyDefinitions" ref="B73:L76" totalsRowShown="0" headerRowBorderDxfId="68" tableBorderDxfId="67">
   <autoFilter ref="B73:L76"/>
   <tableColumns count="11">
     <tableColumn id="1" name="{missionDifficultyDefinitions}"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="65"/>
-    <tableColumn id="11" name="[difficulty]" dataDxfId="64"/>
-    <tableColumn id="7" name="[index]" dataDxfId="63"/>
-    <tableColumn id="3" name="[dragonsToUnlock]" dataDxfId="62"/>
-    <tableColumn id="4" name="[cooldownMinutes]" dataDxfId="61"/>
-    <tableColumn id="9" name="[maxRewardCoins]" dataDxfId="60"/>
-    <tableColumn id="5" name="[removeMissionPCCoefA]" dataDxfId="59"/>
-    <tableColumn id="6" name="[removeMissionPCCoefB]" dataDxfId="58"/>
-    <tableColumn id="8" name="[tidName]" dataDxfId="57"/>
-    <tableColumn id="10" name="[color]" dataDxfId="56"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="66"/>
+    <tableColumn id="11" name="[difficulty]" dataDxfId="65"/>
+    <tableColumn id="7" name="[index]" dataDxfId="64"/>
+    <tableColumn id="3" name="[dragonsToUnlock]" dataDxfId="63"/>
+    <tableColumn id="4" name="[cooldownMinutes]" dataDxfId="62"/>
+    <tableColumn id="9" name="[maxRewardCoins]" dataDxfId="61"/>
+    <tableColumn id="5" name="[removeMissionPCCoefA]" dataDxfId="60"/>
+    <tableColumn id="6" name="[removeMissionPCCoefB]" dataDxfId="59"/>
+    <tableColumn id="8" name="[tidName]" dataDxfId="58"/>
+    <tableColumn id="10" name="[color]" dataDxfId="57"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table13303132" displayName="Table13303132" ref="B81:E94" totalsRowShown="0" headerRowDxfId="55" dataDxfId="53" headerRowBorderDxfId="54" tableBorderDxfId="52" totalsRowBorderDxfId="51">
-  <autoFilter ref="B81:E94"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table13303132" displayName="Table13303132" ref="B81:E99" totalsRowShown="0" headerRowDxfId="56" dataDxfId="54" headerRowBorderDxfId="55" tableBorderDxfId="53" totalsRowBorderDxfId="52">
+  <autoFilter ref="B81:E99"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="{missionDragonModifiersDefinitions}" dataDxfId="50"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="49"/>
-    <tableColumn id="7" name="[quantityModifier]" dataDxfId="48"/>
-    <tableColumn id="3" name="[missionSCRewardMultiplier]" dataDxfId="47"/>
+    <tableColumn id="1" name="{missionDragonModifiersDefinitions}" dataDxfId="51"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="50"/>
+    <tableColumn id="7" name="[quantityModifier]" dataDxfId="49"/>
+    <tableColumn id="3" name="[missionSCRewardMultiplier]" dataDxfId="48"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table1330313234" displayName="Table1330313234" ref="B98:E101" totalsRowShown="0" headerRowDxfId="46" dataDxfId="44" headerRowBorderDxfId="45" tableBorderDxfId="43" totalsRowBorderDxfId="42">
-  <autoFilter ref="B98:E101"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table1330313234" displayName="Table1330313234" ref="B103:E106" totalsRowShown="0" headerRowDxfId="47" dataDxfId="45" headerRowBorderDxfId="46" tableBorderDxfId="44" totalsRowBorderDxfId="43">
+  <autoFilter ref="B103:E106"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="{missionDifficultyModifiersDefinitions}" dataDxfId="41"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="40"/>
-    <tableColumn id="3" name="[difficulty]" dataDxfId="39"/>
-    <tableColumn id="7" name="[quantityModifier]" dataDxfId="38"/>
+    <tableColumn id="1" name="{missionDifficultyModifiersDefinitions}" dataDxfId="42"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="41"/>
+    <tableColumn id="3" name="[difficulty]" dataDxfId="40"/>
+    <tableColumn id="7" name="[quantityModifier]" dataDxfId="39"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table133031323435" displayName="Table133031323435" ref="B105:D106" totalsRowShown="0" headerRowDxfId="37" dataDxfId="35" headerRowBorderDxfId="36" tableBorderDxfId="34" totalsRowBorderDxfId="33">
-  <autoFilter ref="B105:D106"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table133031323435" displayName="Table133031323435" ref="B110:D111" totalsRowShown="0" headerRowDxfId="38" dataDxfId="36" headerRowBorderDxfId="37" tableBorderDxfId="35" totalsRowBorderDxfId="34">
+  <autoFilter ref="B110:D111"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="{missionOtherModifiersDefinitions}" dataDxfId="32"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="31"/>
-    <tableColumn id="7" name="[quantityModifier]" dataDxfId="30"/>
+    <tableColumn id="1" name="{missionOtherModifiersDefinitions}" dataDxfId="33"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="32"/>
+    <tableColumn id="7" name="[quantityModifier]" dataDxfId="31"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table13" displayName="Table13" ref="B48:H67" totalsRowShown="0" headerRowDxfId="29" dataDxfId="27" headerRowBorderDxfId="28" tableBorderDxfId="26" totalsRowBorderDxfId="25">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table13" displayName="Table13" ref="B48:H67" totalsRowShown="0" headerRowDxfId="30" dataDxfId="28" headerRowBorderDxfId="29" tableBorderDxfId="27" totalsRowBorderDxfId="26">
   <autoFilter ref="B48:H67"/>
   <tableColumns count="7">
-    <tableColumn id="1" name="{missionTypeDefinitions}" dataDxfId="24"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="23"/>
-    <tableColumn id="3" name="[minTier]" dataDxfId="22"/>
-    <tableColumn id="6" name="[maxTier]" dataDxfId="21"/>
-    <tableColumn id="4" name="[weight]" dataDxfId="20"/>
-    <tableColumn id="9" name="[tidDescSingleRun]" dataDxfId="19"/>
-    <tableColumn id="10" name="[tidDescMultiRun]" dataDxfId="18"/>
+    <tableColumn id="1" name="{missionTypeDefinitions}" dataDxfId="25"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="24"/>
+    <tableColumn id="3" name="[minTier]" dataDxfId="23"/>
+    <tableColumn id="6" name="[maxTier]" dataDxfId="22"/>
+    <tableColumn id="4" name="[weight]" dataDxfId="21"/>
+    <tableColumn id="9" name="[tidDescSingleRun]" dataDxfId="20"/>
+    <tableColumn id="10" name="[tidDescMultiRun]" dataDxfId="19"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table1330" displayName="Table1330" ref="B4:N43" totalsRowShown="0" headerRowDxfId="17" dataDxfId="15" headerRowBorderDxfId="16" tableBorderDxfId="14" totalsRowBorderDxfId="13">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table1330" displayName="Table1330" ref="B4:N43" totalsRowShown="0" headerRowDxfId="18" dataDxfId="16" headerRowBorderDxfId="17" tableBorderDxfId="15" totalsRowBorderDxfId="14">
   <autoFilter ref="B4:N43"/>
   <sortState ref="B5:P43">
     <sortCondition descending="1" ref="J4:J43"/>
   </sortState>
   <tableColumns count="13">
-    <tableColumn id="1" name="{missionsDefinitions}" dataDxfId="12"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="11"/>
-    <tableColumn id="7" name="[type]" dataDxfId="10"/>
-    <tableColumn id="8" name="[weight]" dataDxfId="9"/>
-    <tableColumn id="13" name="[singleRunChance]" dataDxfId="8"/>
-    <tableColumn id="11" name="[minTier]" dataDxfId="7"/>
-    <tableColumn id="12" name="[maxTier]" dataDxfId="6"/>
-    <tableColumn id="6" name="[params]" dataDxfId="5"/>
-    <tableColumn id="3" name="[objectiveBaseQuantityMin]" dataDxfId="4"/>
-    <tableColumn id="9" name="[objectiveBaseQuantityMax]" dataDxfId="3"/>
-    <tableColumn id="4" name="[icon]" dataDxfId="2"/>
-    <tableColumn id="5" name="[tidObjective]" dataDxfId="1"/>
-    <tableColumn id="10" name="[trackingSku]" dataDxfId="0">
+    <tableColumn id="1" name="{missionsDefinitions}" dataDxfId="13"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="12"/>
+    <tableColumn id="7" name="[type]" dataDxfId="11"/>
+    <tableColumn id="8" name="[weight]" dataDxfId="10"/>
+    <tableColumn id="13" name="[singleRunChance]" dataDxfId="9"/>
+    <tableColumn id="11" name="[minTier]" dataDxfId="8"/>
+    <tableColumn id="12" name="[maxTier]" dataDxfId="7"/>
+    <tableColumn id="6" name="[params]" dataDxfId="6"/>
+    <tableColumn id="3" name="[objectiveBaseQuantityMin]" dataDxfId="5"/>
+    <tableColumn id="9" name="[objectiveBaseQuantityMax]" dataDxfId="4"/>
+    <tableColumn id="4" name="[icon]" dataDxfId="3"/>
+    <tableColumn id="5" name="[tidObjective]" dataDxfId="2"/>
+    <tableColumn id="10" name="[trackingSku]" dataDxfId="1">
       <calculatedColumnFormula>Table1330[[#This Row],['[sku']]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -3417,10 +3432,10 @@
   <sheetPr>
     <tabColor theme="6"/>
   </sheetPr>
-  <dimension ref="B1:P162"/>
+  <dimension ref="B1:P167"/>
   <sheetViews>
-    <sheetView topLeftCell="A124" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C162" sqref="C162"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G95" sqref="G95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5842,7 +5857,7 @@
       <c r="F79" s="6"/>
       <c r="G79" s="6"/>
     </row>
-    <row r="81" spans="2:7" ht="135.75" x14ac:dyDescent="0.25">
+    <row r="81" spans="2:5" ht="135.75" x14ac:dyDescent="0.25">
       <c r="B81" s="5" t="s">
         <v>22</v>
       </c>
@@ -5856,7 +5871,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="82" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="82" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B82" s="2" t="s">
         <v>1</v>
       </c>
@@ -5870,7 +5885,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="83" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="83" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B83" s="2" t="s">
         <v>1</v>
       </c>
@@ -5884,7 +5899,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="84" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="84" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B84" s="2" t="s">
         <v>1</v>
       </c>
@@ -5898,7 +5913,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="85" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="85" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B85" s="2" t="s">
         <v>1</v>
       </c>
@@ -5912,7 +5927,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="86" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="86" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B86" s="2" t="s">
         <v>1</v>
       </c>
@@ -5926,7 +5941,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="87" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="87" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B87" s="2" t="s">
         <v>1</v>
       </c>
@@ -5940,7 +5955,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="88" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="88" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B88" s="2" t="s">
         <v>1</v>
       </c>
@@ -5954,7 +5969,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="89" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="89" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B89" s="2" t="s">
         <v>1</v>
       </c>
@@ -5968,7 +5983,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="90" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="90" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B90" s="2" t="s">
         <v>1</v>
       </c>
@@ -5982,7 +5997,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="91" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="91" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B91" s="2" t="s">
         <v>1</v>
       </c>
@@ -5996,7 +6011,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="92" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="92" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B92" s="2" t="s">
         <v>1</v>
       </c>
@@ -6010,7 +6025,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="93" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="93" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B93" s="2" t="s">
         <v>1</v>
       </c>
@@ -6024,7 +6039,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="94" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="94" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B94" s="51" t="s">
         <v>1</v>
       </c>
@@ -6038,93 +6053,127 @@
         <v>90</v>
       </c>
     </row>
-    <row r="95" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="96" spans="2:7" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B96" s="6" t="s">
+    <row r="95" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B95" s="51" t="s">
+        <v>1</v>
+      </c>
+      <c r="C95" s="42" t="s">
+        <v>453</v>
+      </c>
+      <c r="D95" s="42">
+        <v>8</v>
+      </c>
+      <c r="E95" s="42">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="96" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B96" s="51" t="s">
+        <v>1</v>
+      </c>
+      <c r="C96" s="42" t="s">
+        <v>454</v>
+      </c>
+      <c r="D96" s="42">
+        <v>8</v>
+      </c>
+      <c r="E96" s="42">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="97" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B97" s="51" t="s">
+        <v>1</v>
+      </c>
+      <c r="C97" s="42" t="s">
+        <v>455</v>
+      </c>
+      <c r="D97" s="42">
+        <v>8</v>
+      </c>
+      <c r="E97" s="42">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="98" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B98" s="51" t="s">
+        <v>1</v>
+      </c>
+      <c r="C98" s="42" t="s">
+        <v>456</v>
+      </c>
+      <c r="D98" s="42">
+        <v>8</v>
+      </c>
+      <c r="E98" s="42">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="99" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B99" s="51" t="s">
+        <v>1</v>
+      </c>
+      <c r="C99" s="42" t="s">
+        <v>457</v>
+      </c>
+      <c r="D99" s="42">
+        <v>8</v>
+      </c>
+      <c r="E99" s="42">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="100" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="101" spans="2:7" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B101" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C96" s="6"/>
-      <c r="D96" s="6"/>
-      <c r="E96" s="6"/>
-      <c r="F96" s="6"/>
-      <c r="G96" s="6"/>
-    </row>
-    <row r="98" spans="2:7" ht="142.5" x14ac:dyDescent="0.25">
-      <c r="B98" s="5" t="s">
+      <c r="C101" s="6"/>
+      <c r="D101" s="6"/>
+      <c r="E101" s="6"/>
+      <c r="F101" s="6"/>
+      <c r="G101" s="6"/>
+    </row>
+    <row r="103" spans="2:7" ht="142.5" x14ac:dyDescent="0.25">
+      <c r="B103" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C98" s="4" t="s">
+      <c r="C103" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D98" s="4" t="s">
+      <c r="D103" s="4" t="s">
         <v>224</v>
       </c>
-      <c r="E98" s="3" t="s">
+      <c r="E103" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="99" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B99" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C99" s="1" t="s">
+    <row r="104" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B104" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C104" s="1" t="s">
         <v>225</v>
       </c>
-      <c r="D99" s="1" t="s">
+      <c r="D104" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E99" s="1">
+      <c r="E104" s="1">
         <v>0.05</v>
       </c>
     </row>
-    <row r="100" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B100" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C100" s="1" t="s">
+    <row r="105" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B105" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C105" s="1" t="s">
         <v>226</v>
       </c>
-      <c r="D100" s="1" t="s">
+      <c r="D105" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E100" s="1">
+      <c r="E105" s="1">
         <v>0.1</v>
-      </c>
-    </row>
-    <row r="101" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B101" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C101" s="1" t="s">
-        <v>227</v>
-      </c>
-      <c r="D101" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E101" s="1">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="102" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="103" spans="2:7" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B103" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C103" s="6"/>
-      <c r="D103" s="6"/>
-      <c r="E103" s="6"/>
-      <c r="F103" s="6"/>
-      <c r="G103" s="6"/>
-    </row>
-    <row r="105" spans="2:7" ht="132" x14ac:dyDescent="0.25">
-      <c r="B105" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C105" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D105" s="3" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="106" spans="2:7" x14ac:dyDescent="0.25">
@@ -6132,16 +6181,19 @@
         <v>1</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D106" s="1">
-        <v>0.7</v>
+        <v>227</v>
+      </c>
+      <c r="D106" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E106" s="1">
+        <v>0.2</v>
       </c>
     </row>
     <row r="107" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="108" spans="2:7" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B108" s="6" t="s">
-        <v>240</v>
+        <v>5</v>
       </c>
       <c r="C108" s="6"/>
       <c r="D108" s="6"/>
@@ -6149,270 +6201,233 @@
       <c r="F108" s="6"/>
       <c r="G108" s="6"/>
     </row>
-    <row r="110" spans="2:7" ht="68.25" x14ac:dyDescent="0.25">
-      <c r="B110" s="44" t="s">
+    <row r="110" spans="2:7" ht="132" x14ac:dyDescent="0.25">
+      <c r="B110" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C110" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D110" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="111" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B111" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C111" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D111" s="1">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="112" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="113" spans="2:7" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B113" s="6" t="s">
+        <v>240</v>
+      </c>
+      <c r="C113" s="6"/>
+      <c r="D113" s="6"/>
+      <c r="E113" s="6"/>
+      <c r="F113" s="6"/>
+      <c r="G113" s="6"/>
+    </row>
+    <row r="115" spans="2:7" ht="68.25" x14ac:dyDescent="0.25">
+      <c r="B115" s="44" t="s">
         <v>241</v>
       </c>
-      <c r="C110" s="44" t="s">
+      <c r="C115" s="44" t="s">
         <v>3</v>
       </c>
-      <c r="D110" s="45" t="s">
+      <c r="D115" s="45" t="s">
         <v>242</v>
       </c>
-      <c r="E110" s="45" t="s">
+      <c r="E115" s="45" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="111" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B111" s="43" t="s">
-        <v>1</v>
-      </c>
-      <c r="C111" s="46" t="s">
+    <row r="116" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B116" s="43" t="s">
+        <v>1</v>
+      </c>
+      <c r="C116" s="46" t="s">
         <v>80</v>
       </c>
-      <c r="D111" s="46" t="s">
+      <c r="D116" s="46" t="s">
         <v>264</v>
       </c>
-      <c r="E111" s="43" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="112" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B112" s="43" t="s">
-        <v>1</v>
-      </c>
-      <c r="C112" s="46" t="s">
+      <c r="E116" s="43" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="117" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B117" s="43" t="s">
+        <v>1</v>
+      </c>
+      <c r="C117" s="46" t="s">
         <v>93</v>
       </c>
-      <c r="D112" s="46" t="s">
+      <c r="D117" s="46" t="s">
         <v>265</v>
       </c>
-      <c r="E112" s="43" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="113" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B113" s="43" t="s">
-        <v>1</v>
-      </c>
-      <c r="C113" s="46" t="s">
+      <c r="E117" s="43" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="118" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B118" s="43" t="s">
+        <v>1</v>
+      </c>
+      <c r="C118" s="46" t="s">
         <v>125</v>
       </c>
-      <c r="D113" s="46" t="s">
+      <c r="D118" s="46" t="s">
         <v>266</v>
       </c>
-      <c r="E113" s="43" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="114" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B114" s="43" t="s">
-        <v>1</v>
-      </c>
-      <c r="C114" s="46" t="s">
+      <c r="E118" s="43" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="119" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B119" s="43" t="s">
+        <v>1</v>
+      </c>
+      <c r="C119" s="46" t="s">
         <v>109</v>
       </c>
-      <c r="D114" s="46" t="s">
+      <c r="D119" s="46" t="s">
         <v>109</v>
       </c>
-      <c r="E114" s="43" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="115" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B115" s="43" t="s">
-        <v>1</v>
-      </c>
-      <c r="C115" s="46" t="s">
+      <c r="E119" s="43" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="120" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B120" s="43" t="s">
+        <v>1</v>
+      </c>
+      <c r="C120" s="46" t="s">
         <v>121</v>
       </c>
-      <c r="D115" s="46" t="s">
+      <c r="D120" s="46" t="s">
         <v>121</v>
       </c>
-      <c r="E115" s="43" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="116" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B116" s="43" t="s">
-        <v>1</v>
-      </c>
-      <c r="C116" s="46" t="s">
+      <c r="E120" s="43" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="121" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B121" s="43" t="s">
+        <v>1</v>
+      </c>
+      <c r="C121" s="46" t="s">
         <v>110</v>
       </c>
-      <c r="D116" s="46" t="s">
+      <c r="D121" s="46" t="s">
         <v>110</v>
       </c>
-      <c r="E116" s="43" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="117" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B117" s="43" t="s">
-        <v>1</v>
-      </c>
-      <c r="C117" s="46" t="s">
+      <c r="E121" s="43" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="122" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B122" s="43" t="s">
+        <v>1</v>
+      </c>
+      <c r="C122" s="46" t="s">
         <v>112</v>
       </c>
-      <c r="D117" s="46" t="s">
+      <c r="D122" s="46" t="s">
         <v>267</v>
       </c>
-      <c r="E117" s="43" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="118" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B118" s="43" t="s">
-        <v>1</v>
-      </c>
-      <c r="C118" s="46" t="s">
+      <c r="E122" s="43" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="123" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B123" s="43" t="s">
+        <v>1</v>
+      </c>
+      <c r="C123" s="46" t="s">
         <v>244</v>
       </c>
-      <c r="D118" s="46" t="s">
+      <c r="D123" s="46" t="s">
         <v>268</v>
       </c>
-      <c r="E118" s="43" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="119" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B119" s="43" t="s">
-        <v>1</v>
-      </c>
-      <c r="C119" s="46" t="s">
+      <c r="E123" s="43" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="124" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B124" s="43" t="s">
+        <v>1</v>
+      </c>
+      <c r="C124" s="46" t="s">
         <v>245</v>
       </c>
-      <c r="D119" s="46" t="s">
+      <c r="D124" s="46" t="s">
         <v>269</v>
       </c>
-      <c r="E119" s="43" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="120" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B120" s="43" t="s">
-        <v>1</v>
-      </c>
-      <c r="C120" s="46" t="s">
+      <c r="E124" s="43" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="125" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B125" s="43" t="s">
+        <v>1</v>
+      </c>
+      <c r="C125" s="46" t="s">
         <v>205</v>
       </c>
-      <c r="D120" s="46" t="s">
+      <c r="D125" s="46" t="s">
         <v>270</v>
       </c>
-      <c r="E120" s="43" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="121" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B121" s="43" t="s">
-        <v>1</v>
-      </c>
-      <c r="C121" s="46" t="s">
+      <c r="E125" s="43" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="126" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B126" s="43" t="s">
+        <v>1</v>
+      </c>
+      <c r="C126" s="46" t="s">
         <v>204</v>
       </c>
-      <c r="D121" s="46" t="s">
+      <c r="D126" s="46" t="s">
         <v>271</v>
       </c>
-      <c r="E121" s="43" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="122" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B122" s="43" t="s">
-        <v>1</v>
-      </c>
-      <c r="C122" s="46" t="s">
+      <c r="E126" s="43" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="127" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B127" s="43" t="s">
+        <v>1</v>
+      </c>
+      <c r="C127" s="46" t="s">
         <v>199</v>
       </c>
-      <c r="D122" s="46" t="s">
+      <c r="D127" s="46" t="s">
         <v>272</v>
       </c>
-      <c r="E122" s="43" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="123" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B123" s="43" t="s">
-        <v>1</v>
-      </c>
-      <c r="C123" s="46" t="s">
+      <c r="E127" s="43" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="128" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B128" s="43" t="s">
+        <v>1</v>
+      </c>
+      <c r="C128" s="46" t="s">
         <v>203</v>
       </c>
-      <c r="D123" s="46" t="s">
+      <c r="D128" s="46" t="s">
         <v>273</v>
       </c>
-      <c r="E123" s="43" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="124" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B124" s="43" t="s">
-        <v>1</v>
-      </c>
-      <c r="C124" s="46" t="s">
-        <v>202</v>
-      </c>
-      <c r="D124" s="46" t="s">
-        <v>274</v>
-      </c>
-      <c r="E124" s="43" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="125" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B125" s="43" t="s">
-        <v>1</v>
-      </c>
-      <c r="C125" s="46" t="s">
-        <v>200</v>
-      </c>
-      <c r="D125" s="46" t="s">
-        <v>275</v>
-      </c>
-      <c r="E125" s="43" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="126" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B126" s="43" t="s">
-        <v>1</v>
-      </c>
-      <c r="C126" s="46" t="s">
-        <v>201</v>
-      </c>
-      <c r="D126" s="46" t="s">
-        <v>276</v>
-      </c>
-      <c r="E126" s="43" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="127" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B127" s="43" t="s">
-        <v>1</v>
-      </c>
-      <c r="C127" s="46" t="s">
-        <v>114</v>
-      </c>
-      <c r="D127" s="46" t="s">
-        <v>277</v>
-      </c>
-      <c r="E127" s="43" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="128" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B128" s="43" t="s">
-        <v>1</v>
-      </c>
-      <c r="C128" s="46" t="s">
-        <v>246</v>
-      </c>
-      <c r="D128" s="46" t="s">
-        <v>246</v>
-      </c>
       <c r="E128" s="43" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="129" spans="2:5" x14ac:dyDescent="0.25">
@@ -6420,10 +6435,10 @@
         <v>1</v>
       </c>
       <c r="C129" s="46" t="s">
-        <v>83</v>
+        <v>202</v>
       </c>
       <c r="D129" s="46" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="E129" s="43" t="b">
         <v>1</v>
@@ -6434,10 +6449,10 @@
         <v>1</v>
       </c>
       <c r="C130" s="46" t="s">
-        <v>96</v>
+        <v>200</v>
       </c>
       <c r="D130" s="46" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="E130" s="43" t="b">
         <v>1</v>
@@ -6448,10 +6463,10 @@
         <v>1</v>
       </c>
       <c r="C131" s="46" t="s">
-        <v>247</v>
+        <v>201</v>
       </c>
       <c r="D131" s="46" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
       <c r="E131" s="43" t="b">
         <v>1</v>
@@ -6462,10 +6477,10 @@
         <v>1</v>
       </c>
       <c r="C132" s="46" t="s">
-        <v>248</v>
+        <v>114</v>
       </c>
       <c r="D132" s="46" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
       <c r="E132" s="43" t="b">
         <v>1</v>
@@ -6476,13 +6491,13 @@
         <v>1</v>
       </c>
       <c r="C133" s="46" t="s">
-        <v>102</v>
+        <v>246</v>
       </c>
       <c r="D133" s="46" t="s">
-        <v>282</v>
+        <v>246</v>
       </c>
       <c r="E133" s="43" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="134" spans="2:5" x14ac:dyDescent="0.25">
@@ -6490,10 +6505,10 @@
         <v>1</v>
       </c>
       <c r="C134" s="46" t="s">
-        <v>249</v>
+        <v>83</v>
       </c>
       <c r="D134" s="46" t="s">
-        <v>304</v>
+        <v>278</v>
       </c>
       <c r="E134" s="43" t="b">
         <v>1</v>
@@ -6504,10 +6519,10 @@
         <v>1</v>
       </c>
       <c r="C135" s="46" t="s">
-        <v>123</v>
+        <v>96</v>
       </c>
       <c r="D135" s="46" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
       <c r="E135" s="43" t="b">
         <v>1</v>
@@ -6518,10 +6533,10 @@
         <v>1</v>
       </c>
       <c r="C136" s="46" t="s">
-        <v>88</v>
+        <v>247</v>
       </c>
       <c r="D136" s="46" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="E136" s="43" t="b">
         <v>1</v>
@@ -6532,10 +6547,10 @@
         <v>1</v>
       </c>
       <c r="C137" s="46" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="D137" s="46" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
       <c r="E137" s="43" t="b">
         <v>1</v>
@@ -6546,10 +6561,10 @@
         <v>1</v>
       </c>
       <c r="C138" s="46" t="s">
-        <v>302</v>
+        <v>102</v>
       </c>
       <c r="D138" s="46" t="s">
-        <v>303</v>
+        <v>282</v>
       </c>
       <c r="E138" s="43" t="b">
         <v>1</v>
@@ -6560,13 +6575,13 @@
         <v>1</v>
       </c>
       <c r="C139" s="46" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="D139" s="46" t="s">
-        <v>251</v>
+        <v>304</v>
       </c>
       <c r="E139" s="43" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="140" spans="2:5" x14ac:dyDescent="0.25">
@@ -6574,13 +6589,13 @@
         <v>1</v>
       </c>
       <c r="C140" s="46" t="s">
-        <v>116</v>
+        <v>123</v>
       </c>
       <c r="D140" s="46" t="s">
-        <v>116</v>
+        <v>283</v>
       </c>
       <c r="E140" s="43" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="141" spans="2:5" x14ac:dyDescent="0.25">
@@ -6588,10 +6603,10 @@
         <v>1</v>
       </c>
       <c r="C141" s="46" t="s">
-        <v>252</v>
+        <v>88</v>
       </c>
       <c r="D141" s="46" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="E141" s="43" t="b">
         <v>1</v>
@@ -6602,10 +6617,10 @@
         <v>1</v>
       </c>
       <c r="C142" s="46" t="s">
-        <v>91</v>
+        <v>250</v>
       </c>
       <c r="D142" s="46" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="E142" s="43" t="b">
         <v>1</v>
@@ -6616,10 +6631,10 @@
         <v>1</v>
       </c>
       <c r="C143" s="46" t="s">
-        <v>253</v>
+        <v>302</v>
       </c>
       <c r="D143" s="46" t="s">
-        <v>288</v>
+        <v>303</v>
       </c>
       <c r="E143" s="43" t="b">
         <v>1</v>
@@ -6630,13 +6645,13 @@
         <v>1</v>
       </c>
       <c r="C144" s="46" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="D144" s="46" t="s">
-        <v>289</v>
+        <v>251</v>
       </c>
       <c r="E144" s="43" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="145" spans="2:5" x14ac:dyDescent="0.25">
@@ -6644,13 +6659,13 @@
         <v>1</v>
       </c>
       <c r="C145" s="46" t="s">
-        <v>255</v>
+        <v>116</v>
       </c>
       <c r="D145" s="46" t="s">
-        <v>290</v>
+        <v>116</v>
       </c>
       <c r="E145" s="43" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="146" spans="2:5" x14ac:dyDescent="0.25">
@@ -6658,10 +6673,10 @@
         <v>1</v>
       </c>
       <c r="C146" s="46" t="s">
-        <v>86</v>
+        <v>252</v>
       </c>
       <c r="D146" s="46" t="s">
-        <v>291</v>
+        <v>286</v>
       </c>
       <c r="E146" s="43" t="b">
         <v>1</v>
@@ -6672,13 +6687,13 @@
         <v>1</v>
       </c>
       <c r="C147" s="46" t="s">
-        <v>73</v>
+        <v>91</v>
       </c>
       <c r="D147" s="46" t="s">
-        <v>73</v>
+        <v>287</v>
       </c>
       <c r="E147" s="43" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="148" spans="2:5" x14ac:dyDescent="0.25">
@@ -6686,13 +6701,13 @@
         <v>1</v>
       </c>
       <c r="C148" s="46" t="s">
-        <v>108</v>
+        <v>253</v>
       </c>
       <c r="D148" s="46" t="s">
-        <v>108</v>
+        <v>288</v>
       </c>
       <c r="E148" s="43" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="149" spans="2:5" x14ac:dyDescent="0.25">
@@ -6700,10 +6715,10 @@
         <v>1</v>
       </c>
       <c r="C149" s="46" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="D149" s="46" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="E149" s="43" t="b">
         <v>1</v>
@@ -6714,10 +6729,10 @@
         <v>1</v>
       </c>
       <c r="C150" s="46" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="D150" s="46" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="E150" s="43" t="b">
         <v>1</v>
@@ -6728,10 +6743,10 @@
         <v>1</v>
       </c>
       <c r="C151" s="46" t="s">
-        <v>77</v>
+        <v>86</v>
       </c>
       <c r="D151" s="46" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="E151" s="43" t="b">
         <v>1</v>
@@ -6742,13 +6757,13 @@
         <v>1</v>
       </c>
       <c r="C152" s="46" t="s">
-        <v>105</v>
+        <v>73</v>
       </c>
       <c r="D152" s="46" t="s">
-        <v>295</v>
+        <v>73</v>
       </c>
       <c r="E152" s="43" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="153" spans="2:5" x14ac:dyDescent="0.25">
@@ -6756,13 +6771,13 @@
         <v>1</v>
       </c>
       <c r="C153" s="46" t="s">
-        <v>258</v>
+        <v>108</v>
       </c>
       <c r="D153" s="46" t="s">
-        <v>296</v>
+        <v>108</v>
       </c>
       <c r="E153" s="43" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="154" spans="2:5" x14ac:dyDescent="0.25">
@@ -6770,10 +6785,10 @@
         <v>1</v>
       </c>
       <c r="C154" s="46" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="D154" s="46" t="s">
-        <v>297</v>
+        <v>292</v>
       </c>
       <c r="E154" s="43" t="b">
         <v>1</v>
@@ -6784,10 +6799,10 @@
         <v>1</v>
       </c>
       <c r="C155" s="46" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="D155" s="46" t="s">
-        <v>298</v>
+        <v>293</v>
       </c>
       <c r="E155" s="43" t="b">
         <v>1</v>
@@ -6798,13 +6813,13 @@
         <v>1</v>
       </c>
       <c r="C156" s="46" t="s">
-        <v>261</v>
+        <v>77</v>
       </c>
       <c r="D156" s="46" t="s">
-        <v>261</v>
+        <v>294</v>
       </c>
       <c r="E156" s="43" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="157" spans="2:5" x14ac:dyDescent="0.25">
@@ -6812,10 +6827,10 @@
         <v>1</v>
       </c>
       <c r="C157" s="46" t="s">
-        <v>99</v>
+        <v>105</v>
       </c>
       <c r="D157" s="46" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="E157" s="43" t="b">
         <v>1</v>
@@ -6826,10 +6841,10 @@
         <v>1</v>
       </c>
       <c r="C158" s="46" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="D158" s="46" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="E158" s="43" t="b">
         <v>1</v>
@@ -6840,10 +6855,10 @@
         <v>1</v>
       </c>
       <c r="C159" s="46" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="D159" s="46" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
       <c r="E159" s="43" t="b">
         <v>1</v>
@@ -6854,10 +6869,10 @@
         <v>1</v>
       </c>
       <c r="C160" s="46" t="s">
-        <v>310</v>
+        <v>260</v>
       </c>
       <c r="D160" s="46" t="s">
-        <v>307</v>
+        <v>298</v>
       </c>
       <c r="E160" s="43" t="b">
         <v>1</v>
@@ -6868,13 +6883,13 @@
         <v>1</v>
       </c>
       <c r="C161" s="46" t="s">
-        <v>311</v>
+        <v>261</v>
       </c>
       <c r="D161" s="46" t="s">
-        <v>308</v>
+        <v>261</v>
       </c>
       <c r="E161" s="43" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="162" spans="2:5" x14ac:dyDescent="0.25">
@@ -6882,12 +6897,82 @@
         <v>1</v>
       </c>
       <c r="C162" s="46" t="s">
+        <v>99</v>
+      </c>
+      <c r="D162" s="46" t="s">
+        <v>299</v>
+      </c>
+      <c r="E162" s="43" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="163" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B163" s="43" t="s">
+        <v>1</v>
+      </c>
+      <c r="C163" s="46" t="s">
+        <v>262</v>
+      </c>
+      <c r="D163" s="46" t="s">
+        <v>300</v>
+      </c>
+      <c r="E163" s="43" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="164" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B164" s="43" t="s">
+        <v>1</v>
+      </c>
+      <c r="C164" s="46" t="s">
+        <v>263</v>
+      </c>
+      <c r="D164" s="46" t="s">
+        <v>301</v>
+      </c>
+      <c r="E164" s="43" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="165" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B165" s="43" t="s">
+        <v>1</v>
+      </c>
+      <c r="C165" s="46" t="s">
+        <v>310</v>
+      </c>
+      <c r="D165" s="46" t="s">
+        <v>307</v>
+      </c>
+      <c r="E165" s="43" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="166" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B166" s="43" t="s">
+        <v>1</v>
+      </c>
+      <c r="C166" s="46" t="s">
+        <v>311</v>
+      </c>
+      <c r="D166" s="46" t="s">
+        <v>308</v>
+      </c>
+      <c r="E166" s="43" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="167" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B167" s="43" t="s">
+        <v>1</v>
+      </c>
+      <c r="C167" s="46" t="s">
         <v>312</v>
       </c>
-      <c r="D162" s="46" t="s">
+      <c r="D167" s="46" t="s">
         <v>309</v>
       </c>
-      <c r="E162" s="43" t="b">
+      <c r="E167" s="43" t="b">
         <v>1</v>
       </c>
     </row>
@@ -6899,7 +6984,7 @@
     <mergeCell ref="G72:H72"/>
   </mergeCells>
   <conditionalFormatting sqref="C74:E76">
-    <cfRule type="duplicateValues" dxfId="68" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="2"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -6918,7 +7003,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G99"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Setting missions a bit more difficult for Legendary dragons
Former-commit-id: 9788ce7aeb6f57b141e802f0b412604d6e6e536d
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Missions.xlsx
+++ b/Docs/Content/HungryDragonContent_Missions.xlsx
@@ -1892,16 +1892,6 @@
   </cellStyles>
   <dxfs count="69">
     <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
@@ -3052,6 +3042,16 @@
         </bottom>
       </border>
     </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -3066,99 +3066,99 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="missionDifficultyDefinitions" displayName="missionDifficultyDefinitions" ref="B73:L76" totalsRowShown="0" headerRowBorderDxfId="68" tableBorderDxfId="67">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="missionDifficultyDefinitions" displayName="missionDifficultyDefinitions" ref="B73:L76" totalsRowShown="0" headerRowBorderDxfId="67" tableBorderDxfId="66">
   <autoFilter ref="B73:L76"/>
   <tableColumns count="11">
     <tableColumn id="1" name="{missionDifficultyDefinitions}"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="66"/>
-    <tableColumn id="11" name="[difficulty]" dataDxfId="65"/>
-    <tableColumn id="7" name="[index]" dataDxfId="64"/>
-    <tableColumn id="3" name="[dragonsToUnlock]" dataDxfId="63"/>
-    <tableColumn id="4" name="[cooldownMinutes]" dataDxfId="62"/>
-    <tableColumn id="9" name="[maxRewardCoins]" dataDxfId="61"/>
-    <tableColumn id="5" name="[removeMissionPCCoefA]" dataDxfId="60"/>
-    <tableColumn id="6" name="[removeMissionPCCoefB]" dataDxfId="59"/>
-    <tableColumn id="8" name="[tidName]" dataDxfId="58"/>
-    <tableColumn id="10" name="[color]" dataDxfId="57"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="65"/>
+    <tableColumn id="11" name="[difficulty]" dataDxfId="64"/>
+    <tableColumn id="7" name="[index]" dataDxfId="63"/>
+    <tableColumn id="3" name="[dragonsToUnlock]" dataDxfId="62"/>
+    <tableColumn id="4" name="[cooldownMinutes]" dataDxfId="61"/>
+    <tableColumn id="9" name="[maxRewardCoins]" dataDxfId="60"/>
+    <tableColumn id="5" name="[removeMissionPCCoefA]" dataDxfId="59"/>
+    <tableColumn id="6" name="[removeMissionPCCoefB]" dataDxfId="58"/>
+    <tableColumn id="8" name="[tidName]" dataDxfId="57"/>
+    <tableColumn id="10" name="[color]" dataDxfId="56"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table13303132" displayName="Table13303132" ref="B81:E99" totalsRowShown="0" headerRowDxfId="56" dataDxfId="54" headerRowBorderDxfId="55" tableBorderDxfId="53" totalsRowBorderDxfId="52">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table13303132" displayName="Table13303132" ref="B81:E99" totalsRowShown="0" headerRowDxfId="55" dataDxfId="53" headerRowBorderDxfId="54" tableBorderDxfId="52" totalsRowBorderDxfId="51">
   <autoFilter ref="B81:E99"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="{missionDragonModifiersDefinitions}" dataDxfId="51"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="50"/>
-    <tableColumn id="7" name="[quantityModifier]" dataDxfId="49"/>
-    <tableColumn id="3" name="[missionSCRewardMultiplier]" dataDxfId="48"/>
+    <tableColumn id="1" name="{missionDragonModifiersDefinitions}" dataDxfId="50"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="49"/>
+    <tableColumn id="7" name="[quantityModifier]" dataDxfId="48"/>
+    <tableColumn id="3" name="[missionSCRewardMultiplier]" dataDxfId="47"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table1330313234" displayName="Table1330313234" ref="B103:E106" totalsRowShown="0" headerRowDxfId="47" dataDxfId="45" headerRowBorderDxfId="46" tableBorderDxfId="44" totalsRowBorderDxfId="43">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table1330313234" displayName="Table1330313234" ref="B103:E106" totalsRowShown="0" headerRowDxfId="46" dataDxfId="44" headerRowBorderDxfId="45" tableBorderDxfId="43" totalsRowBorderDxfId="42">
   <autoFilter ref="B103:E106"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="{missionDifficultyModifiersDefinitions}" dataDxfId="42"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="41"/>
-    <tableColumn id="3" name="[difficulty]" dataDxfId="40"/>
-    <tableColumn id="7" name="[quantityModifier]" dataDxfId="39"/>
+    <tableColumn id="1" name="{missionDifficultyModifiersDefinitions}" dataDxfId="41"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="40"/>
+    <tableColumn id="3" name="[difficulty]" dataDxfId="39"/>
+    <tableColumn id="7" name="[quantityModifier]" dataDxfId="38"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table133031323435" displayName="Table133031323435" ref="B110:D111" totalsRowShown="0" headerRowDxfId="38" dataDxfId="36" headerRowBorderDxfId="37" tableBorderDxfId="35" totalsRowBorderDxfId="34">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table133031323435" displayName="Table133031323435" ref="B110:D111" totalsRowShown="0" headerRowDxfId="37" dataDxfId="35" headerRowBorderDxfId="36" tableBorderDxfId="34" totalsRowBorderDxfId="33">
   <autoFilter ref="B110:D111"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="{missionOtherModifiersDefinitions}" dataDxfId="33"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="32"/>
-    <tableColumn id="7" name="[quantityModifier]" dataDxfId="31"/>
+    <tableColumn id="1" name="{missionOtherModifiersDefinitions}" dataDxfId="32"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="31"/>
+    <tableColumn id="7" name="[quantityModifier]" dataDxfId="30"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table13" displayName="Table13" ref="B48:H67" totalsRowShown="0" headerRowDxfId="30" dataDxfId="28" headerRowBorderDxfId="29" tableBorderDxfId="27" totalsRowBorderDxfId="26">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table13" displayName="Table13" ref="B48:H67" totalsRowShown="0" headerRowDxfId="29" dataDxfId="27" headerRowBorderDxfId="28" tableBorderDxfId="26" totalsRowBorderDxfId="25">
   <autoFilter ref="B48:H67"/>
   <tableColumns count="7">
-    <tableColumn id="1" name="{missionTypeDefinitions}" dataDxfId="25"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="24"/>
-    <tableColumn id="3" name="[minTier]" dataDxfId="23"/>
-    <tableColumn id="6" name="[maxTier]" dataDxfId="22"/>
-    <tableColumn id="4" name="[weight]" dataDxfId="21"/>
-    <tableColumn id="9" name="[tidDescSingleRun]" dataDxfId="20"/>
-    <tableColumn id="10" name="[tidDescMultiRun]" dataDxfId="19"/>
+    <tableColumn id="1" name="{missionTypeDefinitions}" dataDxfId="24"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="23"/>
+    <tableColumn id="3" name="[minTier]" dataDxfId="22"/>
+    <tableColumn id="6" name="[maxTier]" dataDxfId="21"/>
+    <tableColumn id="4" name="[weight]" dataDxfId="20"/>
+    <tableColumn id="9" name="[tidDescSingleRun]" dataDxfId="19"/>
+    <tableColumn id="10" name="[tidDescMultiRun]" dataDxfId="18"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table1330" displayName="Table1330" ref="B4:N43" totalsRowShown="0" headerRowDxfId="18" dataDxfId="16" headerRowBorderDxfId="17" tableBorderDxfId="15" totalsRowBorderDxfId="14">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table1330" displayName="Table1330" ref="B4:N43" totalsRowShown="0" headerRowDxfId="17" dataDxfId="15" headerRowBorderDxfId="16" tableBorderDxfId="14" totalsRowBorderDxfId="13">
   <autoFilter ref="B4:N43"/>
   <sortState ref="B5:P43">
     <sortCondition descending="1" ref="J4:J43"/>
   </sortState>
   <tableColumns count="13">
-    <tableColumn id="1" name="{missionsDefinitions}" dataDxfId="13"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="12"/>
-    <tableColumn id="7" name="[type]" dataDxfId="11"/>
-    <tableColumn id="8" name="[weight]" dataDxfId="10"/>
-    <tableColumn id="13" name="[singleRunChance]" dataDxfId="9"/>
-    <tableColumn id="11" name="[minTier]" dataDxfId="8"/>
-    <tableColumn id="12" name="[maxTier]" dataDxfId="7"/>
-    <tableColumn id="6" name="[params]" dataDxfId="6"/>
-    <tableColumn id="3" name="[objectiveBaseQuantityMin]" dataDxfId="5"/>
-    <tableColumn id="9" name="[objectiveBaseQuantityMax]" dataDxfId="4"/>
-    <tableColumn id="4" name="[icon]" dataDxfId="3"/>
-    <tableColumn id="5" name="[tidObjective]" dataDxfId="2"/>
-    <tableColumn id="10" name="[trackingSku]" dataDxfId="1">
+    <tableColumn id="1" name="{missionsDefinitions}" dataDxfId="12"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="11"/>
+    <tableColumn id="7" name="[type]" dataDxfId="10"/>
+    <tableColumn id="8" name="[weight]" dataDxfId="9"/>
+    <tableColumn id="13" name="[singleRunChance]" dataDxfId="8"/>
+    <tableColumn id="11" name="[minTier]" dataDxfId="7"/>
+    <tableColumn id="12" name="[maxTier]" dataDxfId="6"/>
+    <tableColumn id="6" name="[params]" dataDxfId="5"/>
+    <tableColumn id="3" name="[objectiveBaseQuantityMin]" dataDxfId="4"/>
+    <tableColumn id="9" name="[objectiveBaseQuantityMax]" dataDxfId="3"/>
+    <tableColumn id="4" name="[icon]" dataDxfId="2"/>
+    <tableColumn id="5" name="[tidObjective]" dataDxfId="1"/>
+    <tableColumn id="10" name="[trackingSku]" dataDxfId="0">
       <calculatedColumnFormula>Table1330[[#This Row],['[sku']]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -3434,8 +3434,8 @@
   </sheetPr>
   <dimension ref="B1:P167"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G95" sqref="G95"/>
+    <sheetView tabSelected="1" topLeftCell="A82" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G92" sqref="G92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6061,7 +6061,7 @@
         <v>453</v>
       </c>
       <c r="D95" s="42">
-        <v>8</v>
+        <v>8.5</v>
       </c>
       <c r="E95" s="42">
         <v>90</v>
@@ -6075,7 +6075,7 @@
         <v>454</v>
       </c>
       <c r="D96" s="42">
-        <v>8</v>
+        <v>8.5</v>
       </c>
       <c r="E96" s="42">
         <v>90</v>
@@ -6089,7 +6089,7 @@
         <v>455</v>
       </c>
       <c r="D97" s="42">
-        <v>8</v>
+        <v>8.5</v>
       </c>
       <c r="E97" s="42">
         <v>90</v>
@@ -6103,7 +6103,7 @@
         <v>456</v>
       </c>
       <c r="D98" s="42">
-        <v>8</v>
+        <v>8.5</v>
       </c>
       <c r="E98" s="42">
         <v>90</v>
@@ -6117,7 +6117,7 @@
         <v>457</v>
       </c>
       <c r="D99" s="42">
-        <v>8</v>
+        <v>8.5</v>
       </c>
       <c r="E99" s="42">
         <v>90</v>
@@ -6984,7 +6984,7 @@
     <mergeCell ref="G72:H72"/>
   </mergeCells>
   <conditionalFormatting sqref="C74:E76">
-    <cfRule type="duplicateValues" dxfId="0" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="68" priority="2"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
New missions for Halloween
Former-commit-id: 95eb27e6946455f5ff61722290368523e7810c84
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Missions.xlsx
+++ b/Docs/Content/HungryDragonContent_Missions.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1059" uniqueCount="458">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1074" uniqueCount="467">
   <si>
     <t>single_run</t>
   </si>
@@ -1427,12 +1427,39 @@
   <si>
     <t>dragon_dino</t>
   </si>
+  <si>
+    <t>halloween_zombie</t>
+  </si>
+  <si>
+    <t>halloween_creatures</t>
+  </si>
+  <si>
+    <t>kill_disguise</t>
+  </si>
+  <si>
+    <t>Villager02;Villager03;Villager04;Worker01;Worker02;WorkerWife;Troll;Cow;Horse;Sheep;EnemyTier0;EnemyTier1;EnemyTier2;EnemyTier3;EnemyTier4;EnemyTier5</t>
+  </si>
+  <si>
+    <t>TID_ENTITY_DISGUISE_HALLOWEEN</t>
+  </si>
+  <si>
+    <t>TID_EDIBLE_ZOMBIE_PL</t>
+  </si>
+  <si>
+    <t>TID_MISSION_OBJECTIVE_KILL_DISGUISE_DESC_SINGLE_RUN</t>
+  </si>
+  <si>
+    <t>TID_MISSION_OBJECTIVE_KILL_DISGUISE_DESC_MULTI_RUN</t>
+  </si>
+  <si>
+    <t>Villager01;BakerWoman;BoatFisher;Ground_Zombie</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1505,6 +1532,13 @@
     <font>
       <sz val="11"/>
       <color theme="0" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1602,7 +1636,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -1739,11 +1773,20 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1"/>
@@ -1879,6 +1922,15 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1891,29 +1943,6 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="69">
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
@@ -2601,6 +2630,29 @@
         <horizontal style="thin">
           <color indexed="64"/>
         </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
       </border>
     </dxf>
     <dxf>
@@ -3070,8 +3122,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="missionDifficultyDefinitions" displayName="missionDifficultyDefinitions" ref="B73:L76" totalsRowShown="0" headerRowBorderDxfId="67" tableBorderDxfId="66">
-  <autoFilter ref="B73:L76"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="missionDifficultyDefinitions" displayName="missionDifficultyDefinitions" ref="B76:L79" totalsRowShown="0" headerRowBorderDxfId="67" tableBorderDxfId="66">
+  <autoFilter ref="B76:L79"/>
   <tableColumns count="11">
     <tableColumn id="1" name="{missionDifficultyDefinitions}"/>
     <tableColumn id="2" name="[sku]" dataDxfId="65"/>
@@ -3090,79 +3142,79 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table13303132" displayName="Table13303132" ref="B81:E99" totalsRowShown="0" headerRowDxfId="55" dataDxfId="53" headerRowBorderDxfId="54" tableBorderDxfId="52" totalsRowBorderDxfId="51">
-  <autoFilter ref="B81:E99"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table13303132" displayName="Table13303132" ref="B84:E102" totalsRowShown="0" headerRowDxfId="55" dataDxfId="53" headerRowBorderDxfId="54" tableBorderDxfId="52" totalsRowBorderDxfId="51">
+  <autoFilter ref="B84:E102"/>
   <tableColumns count="4">
     <tableColumn id="1" name="{missionDragonModifiersDefinitions}" dataDxfId="50"/>
     <tableColumn id="2" name="[sku]" dataDxfId="49"/>
     <tableColumn id="7" name="[quantityModifier]" dataDxfId="48"/>
-    <tableColumn id="3" name="[missionSCRewardMultiplier]" dataDxfId="0"/>
+    <tableColumn id="3" name="[missionSCRewardMultiplier]" dataDxfId="47"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table1330313234" displayName="Table1330313234" ref="B103:E106" totalsRowShown="0" headerRowDxfId="47" dataDxfId="45" headerRowBorderDxfId="46" tableBorderDxfId="44" totalsRowBorderDxfId="43">
-  <autoFilter ref="B103:E106"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table1330313234" displayName="Table1330313234" ref="B106:E109" totalsRowShown="0" headerRowDxfId="46" dataDxfId="44" headerRowBorderDxfId="45" tableBorderDxfId="43" totalsRowBorderDxfId="42">
+  <autoFilter ref="B106:E109"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="{missionDifficultyModifiersDefinitions}" dataDxfId="42"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="41"/>
-    <tableColumn id="3" name="[difficulty]" dataDxfId="40"/>
-    <tableColumn id="7" name="[quantityModifier]" dataDxfId="39"/>
+    <tableColumn id="1" name="{missionDifficultyModifiersDefinitions}" dataDxfId="41"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="40"/>
+    <tableColumn id="3" name="[difficulty]" dataDxfId="39"/>
+    <tableColumn id="7" name="[quantityModifier]" dataDxfId="38"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table133031323435" displayName="Table133031323435" ref="B110:D111" totalsRowShown="0" headerRowDxfId="38" dataDxfId="36" headerRowBorderDxfId="37" tableBorderDxfId="35" totalsRowBorderDxfId="34">
-  <autoFilter ref="B110:D111"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table133031323435" displayName="Table133031323435" ref="B113:D114" totalsRowShown="0" headerRowDxfId="37" dataDxfId="35" headerRowBorderDxfId="36" tableBorderDxfId="34" totalsRowBorderDxfId="33">
+  <autoFilter ref="B113:D114"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="{missionOtherModifiersDefinitions}" dataDxfId="33"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="32"/>
-    <tableColumn id="7" name="[quantityModifier]" dataDxfId="31"/>
+    <tableColumn id="1" name="{missionOtherModifiersDefinitions}" dataDxfId="32"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="31"/>
+    <tableColumn id="7" name="[quantityModifier]" dataDxfId="30"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table13" displayName="Table13" ref="B48:H67" totalsRowShown="0" headerRowDxfId="30" dataDxfId="28" headerRowBorderDxfId="29" tableBorderDxfId="27" totalsRowBorderDxfId="26">
-  <autoFilter ref="B48:H67"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table13" displayName="Table13" ref="B50:H69" totalsRowShown="0" headerRowDxfId="29" dataDxfId="27" headerRowBorderDxfId="28" tableBorderDxfId="26" totalsRowBorderDxfId="25">
+  <autoFilter ref="B50:H69"/>
   <tableColumns count="7">
-    <tableColumn id="1" name="{missionTypeDefinitions}" dataDxfId="25"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="24"/>
-    <tableColumn id="3" name="[minTier]" dataDxfId="23"/>
-    <tableColumn id="6" name="[maxTier]" dataDxfId="22"/>
-    <tableColumn id="4" name="[weight]" dataDxfId="21"/>
-    <tableColumn id="9" name="[tidDescSingleRun]" dataDxfId="20"/>
-    <tableColumn id="10" name="[tidDescMultiRun]" dataDxfId="19"/>
+    <tableColumn id="1" name="{missionTypeDefinitions}" dataDxfId="24"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="23"/>
+    <tableColumn id="3" name="[minTier]" dataDxfId="22"/>
+    <tableColumn id="6" name="[maxTier]" dataDxfId="21"/>
+    <tableColumn id="4" name="[weight]" dataDxfId="20"/>
+    <tableColumn id="9" name="[tidDescSingleRun]" dataDxfId="19"/>
+    <tableColumn id="10" name="[tidDescMultiRun]" dataDxfId="18"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table1330" displayName="Table1330" ref="B4:N43" totalsRowShown="0" headerRowDxfId="18" dataDxfId="16" headerRowBorderDxfId="17" tableBorderDxfId="15" totalsRowBorderDxfId="14">
-  <autoFilter ref="B4:N43"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table1330" displayName="Table1330" ref="B4:N45" totalsRowShown="0" headerRowDxfId="17" dataDxfId="15" headerRowBorderDxfId="16" tableBorderDxfId="14" totalsRowBorderDxfId="13">
+  <autoFilter ref="B4:N45"/>
   <sortState ref="B5:P43">
     <sortCondition descending="1" ref="J4:J43"/>
   </sortState>
   <tableColumns count="13">
-    <tableColumn id="1" name="{missionsDefinitions}" dataDxfId="13"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="12"/>
-    <tableColumn id="7" name="[type]" dataDxfId="11"/>
-    <tableColumn id="8" name="[weight]" dataDxfId="10"/>
-    <tableColumn id="13" name="[singleRunChance]" dataDxfId="9"/>
-    <tableColumn id="11" name="[minTier]" dataDxfId="8"/>
-    <tableColumn id="12" name="[maxTier]" dataDxfId="7"/>
-    <tableColumn id="6" name="[params]" dataDxfId="6"/>
-    <tableColumn id="3" name="[objectiveBaseQuantityMin]" dataDxfId="5"/>
-    <tableColumn id="9" name="[objectiveBaseQuantityMax]" dataDxfId="4"/>
-    <tableColumn id="4" name="[icon]" dataDxfId="3"/>
-    <tableColumn id="5" name="[tidObjective]" dataDxfId="2"/>
-    <tableColumn id="10" name="[trackingSku]" dataDxfId="1">
+    <tableColumn id="1" name="{missionsDefinitions}" dataDxfId="12"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="11"/>
+    <tableColumn id="7" name="[type]" dataDxfId="10"/>
+    <tableColumn id="8" name="[weight]" dataDxfId="9"/>
+    <tableColumn id="13" name="[singleRunChance]" dataDxfId="8"/>
+    <tableColumn id="11" name="[minTier]" dataDxfId="7"/>
+    <tableColumn id="12" name="[maxTier]" dataDxfId="6"/>
+    <tableColumn id="6" name="[params]" dataDxfId="5"/>
+    <tableColumn id="3" name="[objectiveBaseQuantityMin]" dataDxfId="4"/>
+    <tableColumn id="9" name="[objectiveBaseQuantityMax]" dataDxfId="3"/>
+    <tableColumn id="4" name="[icon]" dataDxfId="2"/>
+    <tableColumn id="5" name="[tidObjective]" dataDxfId="1"/>
+    <tableColumn id="10" name="[trackingSku]" dataDxfId="0">
       <calculatedColumnFormula>Table1330[[#This Row],['[sku']]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -3436,10 +3488,10 @@
   <sheetPr>
     <tabColor theme="6"/>
   </sheetPr>
-  <dimension ref="B1:P167"/>
+  <dimension ref="B1:P170"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A76" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G86" sqref="G86"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I44" sqref="I44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3486,14 +3538,14 @@
         <v>140</v>
       </c>
       <c r="G3" s="38"/>
-      <c r="J3" s="57" t="s">
+      <c r="J3" s="60" t="s">
         <v>139</v>
       </c>
-      <c r="K3" s="57"/>
-      <c r="M3" s="57"/>
-      <c r="N3" s="57"/>
-      <c r="O3" s="57"/>
-      <c r="P3" s="57"/>
+      <c r="K3" s="60"/>
+      <c r="M3" s="60"/>
+      <c r="N3" s="60"/>
+      <c r="O3" s="60"/>
+      <c r="P3" s="60"/>
     </row>
     <row r="4" spans="2:16" ht="106.5" x14ac:dyDescent="0.25">
       <c r="B4" s="30" t="s">
@@ -3697,9 +3749,7 @@
       </c>
     </row>
     <row r="9" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B9" s="27" t="s">
-        <v>1</v>
-      </c>
+      <c r="B9" s="27"/>
       <c r="C9" s="24" t="s">
         <v>124</v>
       </c>
@@ -5125,135 +5175,173 @@
       </c>
     </row>
     <row r="44" spans="2:14" s="40" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B44" s="41"/>
-      <c r="C44" s="41"/>
-      <c r="D44" s="41"/>
-      <c r="E44" s="41"/>
-      <c r="F44" s="41"/>
-      <c r="G44" s="41"/>
-      <c r="H44" s="41"/>
-      <c r="I44" s="41"/>
-      <c r="J44" s="41"/>
-      <c r="K44" s="41"/>
-      <c r="L44" s="41"/>
-      <c r="M44" s="41"/>
-      <c r="N44" s="41"/>
-    </row>
-    <row r="45" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B45" s="32"/>
-      <c r="C45" s="32"/>
-      <c r="D45" s="32"/>
-      <c r="E45" s="32"/>
-      <c r="F45" s="32"/>
-      <c r="G45" s="32"/>
-      <c r="H45" s="32"/>
-      <c r="I45" s="32"/>
-      <c r="J45" s="32"/>
-      <c r="K45" s="32"/>
-      <c r="L45" s="32"/>
-      <c r="M45" s="31"/>
-    </row>
-    <row r="46" spans="2:14" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B46" s="6" t="s">
+      <c r="B44" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="C44" s="23" t="s">
+        <v>458</v>
+      </c>
+      <c r="D44" s="23" t="s">
+        <v>65</v>
+      </c>
+      <c r="E44" s="23">
+        <v>1</v>
+      </c>
+      <c r="F44" s="23">
+        <v>0.3</v>
+      </c>
+      <c r="G44" s="23">
+        <v>0</v>
+      </c>
+      <c r="H44" s="23">
+        <v>7</v>
+      </c>
+      <c r="I44" s="23" t="s">
+        <v>466</v>
+      </c>
+      <c r="J44" s="23">
+        <v>25</v>
+      </c>
+      <c r="K44" s="23">
+        <v>30</v>
+      </c>
+      <c r="L44" s="58" t="s">
+        <v>123</v>
+      </c>
+      <c r="M44" s="23" t="s">
+        <v>463</v>
+      </c>
+      <c r="N44" s="23" t="str">
+        <f>Table1330[[#This Row],['[sku']]]</f>
+        <v>halloween_zombie</v>
+      </c>
+    </row>
+    <row r="45" spans="2:14" s="40" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B45" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="C45" s="23" t="s">
+        <v>459</v>
+      </c>
+      <c r="D45" s="23" t="s">
+        <v>460</v>
+      </c>
+      <c r="E45" s="23">
+        <v>1</v>
+      </c>
+      <c r="F45" s="23">
+        <v>0.3</v>
+      </c>
+      <c r="G45" s="23">
+        <v>0</v>
+      </c>
+      <c r="H45" s="23">
+        <v>7</v>
+      </c>
+      <c r="I45" s="23" t="s">
+        <v>461</v>
+      </c>
+      <c r="J45" s="23">
+        <v>25</v>
+      </c>
+      <c r="K45" s="23">
+        <v>30</v>
+      </c>
+      <c r="L45" s="58" t="s">
+        <v>123</v>
+      </c>
+      <c r="M45" s="23" t="s">
+        <v>462</v>
+      </c>
+      <c r="N45" s="23" t="str">
+        <f>Table1330[[#This Row],['[sku']]]</f>
+        <v>halloween_creatures</v>
+      </c>
+    </row>
+    <row r="46" spans="2:14" s="40" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B46" s="41"/>
+      <c r="C46" s="41"/>
+      <c r="D46" s="59"/>
+      <c r="E46" s="41"/>
+      <c r="F46" s="41"/>
+      <c r="G46" s="41"/>
+      <c r="H46" s="41"/>
+      <c r="I46" s="41"/>
+      <c r="J46" s="41"/>
+      <c r="K46" s="41"/>
+      <c r="L46" s="41"/>
+      <c r="M46" s="41"/>
+      <c r="N46" s="41"/>
+    </row>
+    <row r="47" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B47" s="32"/>
+      <c r="C47" s="32"/>
+      <c r="D47" s="32"/>
+      <c r="E47" s="32"/>
+      <c r="F47" s="32"/>
+      <c r="G47" s="32"/>
+      <c r="H47" s="32"/>
+      <c r="I47" s="32"/>
+      <c r="J47" s="32"/>
+      <c r="K47" s="32"/>
+      <c r="L47" s="32"/>
+      <c r="M47" s="31"/>
+    </row>
+    <row r="48" spans="2:14" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B48" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="C46" s="6"/>
-      <c r="D46" s="6"/>
-      <c r="E46" s="6"/>
-      <c r="F46" s="6"/>
-      <c r="G46" s="6"/>
-      <c r="H46" s="6"/>
-      <c r="I46" s="6"/>
-      <c r="J46" s="6"/>
-      <c r="K46" s="6"/>
-      <c r="L46" s="6"/>
-    </row>
-    <row r="47" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B47" s="20"/>
-      <c r="C47" s="20"/>
-      <c r="D47" s="20"/>
-      <c r="E47" s="20"/>
-      <c r="F47" s="58"/>
-      <c r="G47" s="58"/>
-      <c r="H47" s="58"/>
-      <c r="I47" s="20"/>
-      <c r="J47" s="20"/>
-    </row>
-    <row r="48" spans="2:14" ht="96" x14ac:dyDescent="0.25">
-      <c r="B48" s="30" t="s">
+      <c r="C48" s="6"/>
+      <c r="D48" s="6"/>
+      <c r="E48" s="6"/>
+      <c r="F48" s="6"/>
+      <c r="G48" s="6"/>
+      <c r="H48" s="6"/>
+      <c r="I48" s="6"/>
+      <c r="J48" s="6"/>
+      <c r="K48" s="6"/>
+      <c r="L48" s="6"/>
+    </row>
+    <row r="49" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B49" s="20"/>
+      <c r="C49" s="20"/>
+      <c r="D49" s="20"/>
+      <c r="E49" s="20"/>
+      <c r="F49" s="61"/>
+      <c r="G49" s="61"/>
+      <c r="H49" s="61"/>
+      <c r="I49" s="20"/>
+      <c r="J49" s="20"/>
+    </row>
+    <row r="50" spans="2:10" ht="96" x14ac:dyDescent="0.25">
+      <c r="B50" s="30" t="s">
         <v>71</v>
       </c>
-      <c r="C48" s="28" t="s">
+      <c r="C50" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="D48" s="29" t="s">
+      <c r="D50" s="29" t="s">
         <v>70</v>
       </c>
-      <c r="E48" s="29" t="s">
+      <c r="E50" s="29" t="s">
         <v>69</v>
       </c>
-      <c r="F48" s="29" t="s">
+      <c r="F50" s="29" t="s">
         <v>68</v>
       </c>
-      <c r="G48" s="28" t="s">
+      <c r="G50" s="28" t="s">
         <v>67</v>
       </c>
-      <c r="H48" s="28" t="s">
+      <c r="H50" s="28" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="49" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B49" s="27" t="s">
-        <v>1</v>
-      </c>
-      <c r="C49" s="24" t="s">
+    <row r="51" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B51" s="27" t="s">
+        <v>1</v>
+      </c>
+      <c r="C51" s="24" t="s">
         <v>65</v>
-      </c>
-      <c r="D49" s="24">
-        <v>0</v>
-      </c>
-      <c r="E49" s="24">
-        <v>7</v>
-      </c>
-      <c r="F49" s="24">
-        <v>2</v>
-      </c>
-      <c r="G49" s="26" t="s">
-        <v>64</v>
-      </c>
-      <c r="H49" s="26" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="50" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B50" s="27" t="s">
-        <v>1</v>
-      </c>
-      <c r="C50" s="24" t="s">
-        <v>62</v>
-      </c>
-      <c r="D50" s="24">
-        <v>0</v>
-      </c>
-      <c r="E50" s="24">
-        <v>7</v>
-      </c>
-      <c r="F50" s="24">
-        <v>1</v>
-      </c>
-      <c r="G50" s="26" t="s">
-        <v>61</v>
-      </c>
-      <c r="H50" s="26" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="51" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B51" s="27" t="s">
-        <v>1</v>
-      </c>
-      <c r="C51" s="24" t="s">
-        <v>59</v>
       </c>
       <c r="D51" s="24">
         <v>0</v>
@@ -5265,18 +5353,18 @@
         <v>2</v>
       </c>
       <c r="G51" s="26" t="s">
-        <v>58</v>
+        <v>64</v>
       </c>
       <c r="H51" s="26" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="52" spans="2:8" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="52" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B52" s="27" t="s">
         <v>1</v>
       </c>
       <c r="C52" s="24" t="s">
-        <v>56</v>
+        <v>62</v>
       </c>
       <c r="D52" s="24">
         <v>0</v>
@@ -5288,41 +5376,41 @@
         <v>1</v>
       </c>
       <c r="G52" s="26" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="H52" s="26" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="53" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B53" s="25" t="s">
-        <v>1</v>
-      </c>
-      <c r="C53" s="23" t="s">
-        <v>53</v>
-      </c>
-      <c r="D53" s="23">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="53" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B53" s="27" t="s">
+        <v>1</v>
+      </c>
+      <c r="C53" s="24" t="s">
+        <v>59</v>
+      </c>
+      <c r="D53" s="24">
         <v>0</v>
       </c>
       <c r="E53" s="24">
         <v>7</v>
       </c>
-      <c r="F53" s="23">
-        <v>1</v>
+      <c r="F53" s="24">
+        <v>2</v>
       </c>
       <c r="G53" s="26" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="H53" s="26" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="54" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B54" s="25" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="54" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B54" s="27" t="s">
         <v>1</v>
       </c>
       <c r="C54" s="24" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="D54" s="24">
         <v>0</v>
@@ -5334,64 +5422,64 @@
         <v>1</v>
       </c>
       <c r="G54" s="26" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="H54" s="26" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="55" spans="2:8" x14ac:dyDescent="0.25">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="55" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B55" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="C55" s="24" t="s">
-        <v>47</v>
-      </c>
-      <c r="D55" s="24">
+      <c r="C55" s="23" t="s">
+        <v>53</v>
+      </c>
+      <c r="D55" s="23">
         <v>0</v>
       </c>
       <c r="E55" s="24">
         <v>7</v>
       </c>
-      <c r="F55" s="24">
+      <c r="F55" s="23">
         <v>1</v>
       </c>
       <c r="G55" s="26" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="H55" s="26" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="56" spans="2:8" x14ac:dyDescent="0.25">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="56" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B56" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="C56" s="23" t="s">
-        <v>44</v>
-      </c>
-      <c r="D56" s="23">
+      <c r="C56" s="24" t="s">
+        <v>50</v>
+      </c>
+      <c r="D56" s="24">
         <v>0</v>
       </c>
       <c r="E56" s="24">
         <v>7</v>
       </c>
-      <c r="F56" s="23">
-        <v>1</v>
-      </c>
-      <c r="G56" s="22" t="s">
-        <v>43</v>
-      </c>
-      <c r="H56" s="22" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="57" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B57" s="27" t="s">
+      <c r="F56" s="24">
+        <v>1</v>
+      </c>
+      <c r="G56" s="26" t="s">
+        <v>49</v>
+      </c>
+      <c r="H56" s="26" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="57" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B57" s="25" t="s">
         <v>1</v>
       </c>
       <c r="C57" s="24" t="s">
-        <v>178</v>
+        <v>47</v>
       </c>
       <c r="D57" s="24">
         <v>0</v>
@@ -5400,44 +5488,44 @@
         <v>7</v>
       </c>
       <c r="F57" s="24">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G57" s="26" t="s">
-        <v>167</v>
+        <v>46</v>
       </c>
       <c r="H57" s="26" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="58" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B58" s="27" t="s">
-        <v>1</v>
-      </c>
-      <c r="C58" s="24" t="s">
-        <v>175</v>
-      </c>
-      <c r="D58" s="24">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="58" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B58" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="C58" s="23" t="s">
+        <v>44</v>
+      </c>
+      <c r="D58" s="23">
         <v>0</v>
       </c>
       <c r="E58" s="24">
         <v>7</v>
       </c>
-      <c r="F58" s="24">
-        <v>0</v>
-      </c>
-      <c r="G58" s="26" t="s">
-        <v>170</v>
-      </c>
-      <c r="H58" s="26" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="59" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="F58" s="23">
+        <v>1</v>
+      </c>
+      <c r="G58" s="22" t="s">
+        <v>43</v>
+      </c>
+      <c r="H58" s="22" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="59" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B59" s="27" t="s">
         <v>1</v>
       </c>
       <c r="C59" s="24" t="s">
-        <v>145</v>
+        <v>178</v>
       </c>
       <c r="D59" s="24">
         <v>0</v>
@@ -5446,21 +5534,21 @@
         <v>7</v>
       </c>
       <c r="F59" s="24">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G59" s="26" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="H59" s="26" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="60" spans="2:8" x14ac:dyDescent="0.25">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="60" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B60" s="27" t="s">
         <v>1</v>
       </c>
       <c r="C60" s="24" t="s">
-        <v>228</v>
+        <v>175</v>
       </c>
       <c r="D60" s="24">
         <v>0</v>
@@ -5469,44 +5557,44 @@
         <v>7</v>
       </c>
       <c r="F60" s="24">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G60" s="26" t="s">
-        <v>229</v>
+        <v>170</v>
       </c>
       <c r="H60" s="26" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="61" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B61" s="25" t="s">
-        <v>1</v>
-      </c>
-      <c r="C61" s="23" t="s">
-        <v>231</v>
-      </c>
-      <c r="D61" s="23">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="61" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B61" s="27" t="s">
+        <v>1</v>
+      </c>
+      <c r="C61" s="24" t="s">
+        <v>145</v>
+      </c>
+      <c r="D61" s="24">
         <v>0</v>
       </c>
       <c r="E61" s="24">
         <v>7</v>
       </c>
-      <c r="F61" s="23">
-        <v>1</v>
+      <c r="F61" s="24">
+        <v>2</v>
       </c>
       <c r="G61" s="26" t="s">
-        <v>232</v>
+        <v>168</v>
       </c>
       <c r="H61" s="26" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="62" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B62" s="25" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="62" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B62" s="27" t="s">
         <v>1</v>
       </c>
       <c r="C62" s="24" t="s">
-        <v>234</v>
+        <v>228</v>
       </c>
       <c r="D62" s="24">
         <v>0</v>
@@ -5518,64 +5606,64 @@
         <v>1</v>
       </c>
       <c r="G62" s="26" t="s">
-        <v>235</v>
+        <v>229</v>
       </c>
       <c r="H62" s="26" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="63" spans="2:8" x14ac:dyDescent="0.25">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="63" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B63" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="C63" s="24" t="s">
-        <v>237</v>
-      </c>
-      <c r="D63" s="24">
+      <c r="C63" s="23" t="s">
+        <v>231</v>
+      </c>
+      <c r="D63" s="23">
         <v>0</v>
       </c>
       <c r="E63" s="24">
         <v>7</v>
       </c>
-      <c r="F63" s="24">
+      <c r="F63" s="23">
         <v>1</v>
       </c>
       <c r="G63" s="26" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
       <c r="H63" s="26" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="64" spans="2:8" x14ac:dyDescent="0.25">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="64" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B64" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="C64" s="23" t="s">
-        <v>146</v>
-      </c>
-      <c r="D64" s="23">
+      <c r="C64" s="24" t="s">
+        <v>234</v>
+      </c>
+      <c r="D64" s="24">
         <v>0</v>
       </c>
       <c r="E64" s="24">
         <v>7</v>
       </c>
-      <c r="F64" s="23">
-        <v>0</v>
-      </c>
-      <c r="G64" s="22" t="s">
-        <v>169</v>
-      </c>
-      <c r="H64" s="22" t="s">
-        <v>174</v>
+      <c r="F64" s="24">
+        <v>1</v>
+      </c>
+      <c r="G64" s="26" t="s">
+        <v>235</v>
+      </c>
+      <c r="H64" s="26" t="s">
+        <v>236</v>
       </c>
     </row>
     <row r="65" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B65" s="27" t="s">
+      <c r="B65" s="25" t="s">
         <v>1</v>
       </c>
       <c r="C65" s="24" t="s">
-        <v>177</v>
+        <v>237</v>
       </c>
       <c r="D65" s="24">
         <v>0</v>
@@ -5587,31 +5675,33 @@
         <v>1</v>
       </c>
       <c r="G65" s="26" t="s">
-        <v>183</v>
-      </c>
-      <c r="H65" s="26"/>
+        <v>238</v>
+      </c>
+      <c r="H65" s="26" t="s">
+        <v>239</v>
+      </c>
     </row>
     <row r="66" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B66" s="27" t="s">
-        <v>1</v>
-      </c>
-      <c r="C66" s="24" t="s">
-        <v>179</v>
-      </c>
-      <c r="D66" s="24">
+      <c r="B66" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="C66" s="23" t="s">
+        <v>146</v>
+      </c>
+      <c r="D66" s="23">
         <v>0</v>
       </c>
       <c r="E66" s="24">
         <v>7</v>
       </c>
-      <c r="F66" s="24">
-        <v>0</v>
-      </c>
-      <c r="G66" s="26" t="s">
-        <v>184</v>
-      </c>
-      <c r="H66" s="26" t="s">
-        <v>185</v>
+      <c r="F66" s="23">
+        <v>0</v>
+      </c>
+      <c r="G66" s="22" t="s">
+        <v>169</v>
+      </c>
+      <c r="H66" s="22" t="s">
+        <v>174</v>
       </c>
     </row>
     <row r="67" spans="2:13" x14ac:dyDescent="0.25">
@@ -5619,7 +5709,7 @@
         <v>1</v>
       </c>
       <c r="C67" s="24" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="D67" s="24">
         <v>0</v>
@@ -5631,18 +5721,16 @@
         <v>1</v>
       </c>
       <c r="G67" s="26" t="s">
-        <v>210</v>
-      </c>
-      <c r="H67" s="26" t="s">
-        <v>211</v>
-      </c>
+        <v>183</v>
+      </c>
+      <c r="H67" s="26"/>
     </row>
     <row r="68" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B68" s="27" t="s">
         <v>1</v>
       </c>
       <c r="C68" s="24" t="s">
-        <v>313</v>
+        <v>179</v>
       </c>
       <c r="D68" s="24">
         <v>0</v>
@@ -5651,19 +5739,21 @@
         <v>7</v>
       </c>
       <c r="F68" s="24">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G68" s="26" t="s">
-        <v>314</v>
-      </c>
-      <c r="H68" s="26"/>
+        <v>184</v>
+      </c>
+      <c r="H68" s="26" t="s">
+        <v>185</v>
+      </c>
     </row>
     <row r="69" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B69" s="27" t="s">
         <v>1</v>
       </c>
       <c r="C69" s="24" t="s">
-        <v>315</v>
+        <v>180</v>
       </c>
       <c r="D69" s="24">
         <v>0</v>
@@ -5675,414 +5765,439 @@
         <v>1</v>
       </c>
       <c r="G69" s="26" t="s">
+        <v>210</v>
+      </c>
+      <c r="H69" s="26" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="70" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B70" s="27" t="s">
+        <v>1</v>
+      </c>
+      <c r="C70" s="24" t="s">
+        <v>313</v>
+      </c>
+      <c r="D70" s="24">
+        <v>0</v>
+      </c>
+      <c r="E70" s="24">
+        <v>7</v>
+      </c>
+      <c r="F70" s="24">
+        <v>1</v>
+      </c>
+      <c r="G70" s="26" t="s">
+        <v>314</v>
+      </c>
+      <c r="H70" s="26"/>
+    </row>
+    <row r="71" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B71" s="27" t="s">
+        <v>1</v>
+      </c>
+      <c r="C71" s="24" t="s">
+        <v>315</v>
+      </c>
+      <c r="D71" s="24">
+        <v>0</v>
+      </c>
+      <c r="E71" s="24">
+        <v>7</v>
+      </c>
+      <c r="F71" s="24">
+        <v>1</v>
+      </c>
+      <c r="G71" s="26" t="s">
         <v>316</v>
       </c>
-      <c r="H69" s="26"/>
-    </row>
-    <row r="70" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="71" spans="2:13" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B71" s="6" t="s">
+      <c r="H71" s="26"/>
+    </row>
+    <row r="72" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B72" s="53" t="s">
+        <v>1</v>
+      </c>
+      <c r="C72" s="53" t="s">
+        <v>460</v>
+      </c>
+      <c r="D72" s="53">
+        <v>0</v>
+      </c>
+      <c r="E72" s="53">
+        <v>7</v>
+      </c>
+      <c r="F72" s="53">
+        <v>2</v>
+      </c>
+      <c r="G72" s="57" t="s">
+        <v>464</v>
+      </c>
+      <c r="H72" s="53" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="73" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="74" spans="2:13" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B74" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="C71" s="6"/>
-      <c r="D71" s="6"/>
-      <c r="E71" s="6"/>
-      <c r="F71" s="6"/>
-      <c r="G71" s="6"/>
-      <c r="H71" s="6"/>
-      <c r="I71" s="6"/>
-      <c r="J71" s="6"/>
-      <c r="K71" s="6"/>
-      <c r="L71" s="6"/>
-      <c r="M71" s="6"/>
-    </row>
-    <row r="72" spans="2:13" ht="60" x14ac:dyDescent="0.25">
-      <c r="B72" s="20"/>
-      <c r="C72" s="20"/>
-      <c r="D72" s="20"/>
-      <c r="E72" s="20"/>
-      <c r="F72" s="21" t="s">
+      <c r="C74" s="6"/>
+      <c r="D74" s="6"/>
+      <c r="E74" s="6"/>
+      <c r="F74" s="6"/>
+      <c r="G74" s="6"/>
+      <c r="H74" s="6"/>
+      <c r="I74" s="6"/>
+      <c r="J74" s="6"/>
+      <c r="K74" s="6"/>
+      <c r="L74" s="6"/>
+      <c r="M74" s="6"/>
+    </row>
+    <row r="75" spans="2:13" ht="60" x14ac:dyDescent="0.25">
+      <c r="B75" s="20"/>
+      <c r="C75" s="20"/>
+      <c r="D75" s="20"/>
+      <c r="E75" s="20"/>
+      <c r="F75" s="21" t="s">
         <v>40</v>
       </c>
-      <c r="G72" s="59" t="s">
+      <c r="G75" s="62" t="s">
         <v>39</v>
       </c>
-      <c r="H72" s="59"/>
-      <c r="I72" s="20"/>
-    </row>
-    <row r="73" spans="2:13" ht="142.5" x14ac:dyDescent="0.25">
-      <c r="B73" s="19" t="s">
+      <c r="H75" s="62"/>
+      <c r="I75" s="20"/>
+    </row>
+    <row r="76" spans="2:13" ht="142.5" x14ac:dyDescent="0.25">
+      <c r="B76" s="19" t="s">
         <v>38</v>
       </c>
-      <c r="C73" s="19" t="s">
+      <c r="C76" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="D73" s="18" t="s">
+      <c r="D76" s="18" t="s">
         <v>224</v>
       </c>
-      <c r="E73" s="18" t="s">
+      <c r="E76" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="F73" s="17" t="s">
+      <c r="F76" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="G73" s="17" t="s">
+      <c r="G76" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="H73" s="17" t="s">
+      <c r="H76" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="I73" s="16" t="s">
+      <c r="I76" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="J73" s="16" t="s">
+      <c r="J76" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="K73" s="15" t="s">
+      <c r="K76" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="L73" s="14" t="s">
+      <c r="L76" s="14" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="74" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B74" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="C74" s="11" t="s">
+    <row r="77" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B77" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="C77" s="11" t="s">
         <v>221</v>
       </c>
-      <c r="D74" s="11" t="s">
+      <c r="D77" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="E74" s="11">
-        <v>0</v>
-      </c>
-      <c r="F74" s="10">
-        <v>0</v>
-      </c>
-      <c r="G74" s="10">
+      <c r="E77" s="11">
+        <v>0</v>
+      </c>
+      <c r="F77" s="10">
+        <v>0</v>
+      </c>
+      <c r="G77" s="10">
         <v>15</v>
       </c>
-      <c r="H74" s="10">
+      <c r="H77" s="10">
         <v>200</v>
       </c>
-      <c r="I74" s="9">
+      <c r="I77" s="9">
         <v>0.5</v>
       </c>
-      <c r="J74" s="9">
-        <v>1</v>
-      </c>
-      <c r="K74" s="8" t="s">
+      <c r="J77" s="9">
+        <v>1</v>
+      </c>
+      <c r="K77" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="L74" s="13" t="s">
+      <c r="L77" s="13" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="75" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B75" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="C75" s="11" t="s">
+    <row r="78" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B78" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="C78" s="11" t="s">
         <v>222</v>
       </c>
-      <c r="D75" s="11" t="s">
+      <c r="D78" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="E75" s="11">
-        <v>1</v>
-      </c>
-      <c r="F75" s="10">
-        <v>0</v>
-      </c>
-      <c r="G75" s="10">
+      <c r="E78" s="11">
+        <v>1</v>
+      </c>
+      <c r="F78" s="10">
+        <v>0</v>
+      </c>
+      <c r="G78" s="10">
         <v>60</v>
       </c>
-      <c r="H75" s="10">
+      <c r="H78" s="10">
         <v>300</v>
       </c>
-      <c r="I75" s="9">
+      <c r="I78" s="9">
         <v>0.5</v>
       </c>
-      <c r="J75" s="9">
-        <v>1</v>
-      </c>
-      <c r="K75" s="8" t="s">
+      <c r="J78" s="9">
+        <v>1</v>
+      </c>
+      <c r="K78" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="L75" s="13" t="s">
+      <c r="L78" s="13" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="76" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B76" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="C76" s="11" t="s">
+    <row r="79" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B79" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="C79" s="11" t="s">
         <v>223</v>
       </c>
-      <c r="D76" s="11" t="s">
+      <c r="D79" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="E76" s="11">
+      <c r="E79" s="11">
         <v>2</v>
       </c>
-      <c r="F76" s="10">
-        <v>0</v>
-      </c>
-      <c r="G76" s="10">
+      <c r="F79" s="10">
+        <v>0</v>
+      </c>
+      <c r="G79" s="10">
         <v>240</v>
       </c>
-      <c r="H76" s="10">
+      <c r="H79" s="10">
         <v>600</v>
       </c>
-      <c r="I76" s="9">
+      <c r="I79" s="9">
         <v>0.5</v>
       </c>
-      <c r="J76" s="9">
-        <v>1</v>
-      </c>
-      <c r="K76" s="8" t="s">
+      <c r="J79" s="9">
+        <v>1</v>
+      </c>
+      <c r="K79" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="L76" s="7" t="s">
+      <c r="L79" s="7" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="78" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="79" spans="2:13" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B79" s="6" t="s">
+    <row r="81" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="82" spans="2:7" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B82" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="C79" s="6"/>
-      <c r="D79" s="6"/>
-      <c r="E79" s="6"/>
-      <c r="F79" s="6"/>
-      <c r="G79" s="6"/>
-    </row>
-    <row r="81" spans="2:5" ht="135.75" x14ac:dyDescent="0.25">
-      <c r="B81" s="5" t="s">
+      <c r="C82" s="6"/>
+      <c r="D82" s="6"/>
+      <c r="E82" s="6"/>
+      <c r="F82" s="6"/>
+      <c r="G82" s="6"/>
+    </row>
+    <row r="84" spans="2:7" ht="135.75" x14ac:dyDescent="0.25">
+      <c r="B84" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="C81" s="4" t="s">
+      <c r="C84" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D81" s="3" t="s">
+      <c r="D84" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E81" s="3" t="s">
+      <c r="E84" s="3" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="82" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B82" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C82" s="1" t="s">
+    <row r="85" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B85" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C85" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D82" s="1">
+      <c r="D85" s="1">
         <v>0.1</v>
       </c>
-      <c r="E82" s="1">
+      <c r="E85" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="83" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B83" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C83" s="1" t="s">
+    <row r="86" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B86" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C86" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D83" s="1">
+      <c r="D86" s="1">
         <v>0.7</v>
       </c>
-      <c r="E83" s="1">
+      <c r="E86" s="1">
         <v>6</v>
       </c>
     </row>
-    <row r="84" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B84" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C84" s="1" t="s">
+    <row r="87" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B87" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C87" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D84" s="1">
-        <v>1</v>
-      </c>
-      <c r="E84" s="1">
+      <c r="D87" s="1">
+        <v>1</v>
+      </c>
+      <c r="E87" s="1">
         <v>12</v>
       </c>
     </row>
-    <row r="85" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B85" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C85" s="1" t="s">
+    <row r="88" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B88" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C88" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D85" s="1">
+      <c r="D88" s="1">
         <v>1.5</v>
       </c>
-      <c r="E85" s="1">
+      <c r="E88" s="1">
         <v>18</v>
       </c>
     </row>
-    <row r="86" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B86" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C86" s="1" t="s">
+    <row r="89" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B89" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C89" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D86" s="1">
+      <c r="D89" s="1">
         <v>2</v>
       </c>
-      <c r="E86" s="1">
+      <c r="E89" s="1">
         <v>26</v>
       </c>
     </row>
-    <row r="87" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B87" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C87" s="1" t="s">
+    <row r="90" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B90" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C90" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D87" s="1">
+      <c r="D90" s="1">
         <v>2.5</v>
       </c>
-      <c r="E87" s="1">
+      <c r="E90" s="1">
         <v>35</v>
       </c>
     </row>
-    <row r="88" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B88" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C88" s="1" t="s">
+    <row r="91" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B91" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C91" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D88" s="1">
+      <c r="D91" s="1">
         <v>3</v>
       </c>
-      <c r="E88" s="1">
+      <c r="E91" s="1">
         <v>45</v>
       </c>
     </row>
-    <row r="89" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B89" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C89" s="1" t="s">
+    <row r="92" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B92" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C92" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D89" s="1">
+      <c r="D92" s="1">
         <v>4</v>
       </c>
-      <c r="E89" s="1">
+      <c r="E92" s="1">
         <v>56</v>
       </c>
     </row>
-    <row r="90" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B90" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C90" s="1" t="s">
+    <row r="93" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B93" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C93" s="1" t="s">
         <v>215</v>
       </c>
-      <c r="D90" s="1">
+      <c r="D93" s="1">
         <v>4.5</v>
       </c>
-      <c r="E90" s="1">
+      <c r="E93" s="1">
         <v>62</v>
       </c>
     </row>
-    <row r="91" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B91" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C91" s="1" t="s">
+    <row r="94" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B94" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C94" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D91" s="1">
+      <c r="D94" s="1">
         <v>5</v>
       </c>
-      <c r="E91" s="1">
+      <c r="E94" s="1">
         <v>65</v>
       </c>
     </row>
-    <row r="92" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B92" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C92" s="1" t="s">
+    <row r="95" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B95" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C95" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D92" s="1">
+      <c r="D95" s="1">
         <v>7</v>
       </c>
-      <c r="E92" s="1">
+      <c r="E95" s="1">
         <v>70</v>
       </c>
     </row>
-    <row r="93" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B93" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C93" s="1" t="s">
+    <row r="96" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B96" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C96" s="1" t="s">
         <v>220</v>
       </c>
-      <c r="D93" s="42">
+      <c r="D96" s="42">
         <v>7.5</v>
       </c>
-      <c r="E93" s="42">
+      <c r="E96" s="42">
         <v>70</v>
-      </c>
-    </row>
-    <row r="94" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B94" s="51" t="s">
-        <v>1</v>
-      </c>
-      <c r="C94" s="42" t="s">
-        <v>306</v>
-      </c>
-      <c r="D94" s="42">
-        <v>8</v>
-      </c>
-      <c r="E94" s="42">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="95" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B95" s="51" t="s">
-        <v>1</v>
-      </c>
-      <c r="C95" s="42" t="s">
-        <v>453</v>
-      </c>
-      <c r="D95" s="42">
-        <v>8.5</v>
-      </c>
-      <c r="E95" s="42">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="96" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B96" s="51" t="s">
-        <v>1</v>
-      </c>
-      <c r="C96" s="42" t="s">
-        <v>454</v>
-      </c>
-      <c r="D96" s="42">
-        <v>8.5</v>
-      </c>
-      <c r="E96" s="42">
-        <v>75</v>
       </c>
     </row>
     <row r="97" spans="2:7" x14ac:dyDescent="0.25">
@@ -6090,13 +6205,13 @@
         <v>1</v>
       </c>
       <c r="C97" s="42" t="s">
-        <v>455</v>
+        <v>306</v>
       </c>
       <c r="D97" s="42">
-        <v>8.5</v>
+        <v>8</v>
       </c>
       <c r="E97" s="42">
-        <v>75</v>
+        <v>70</v>
       </c>
     </row>
     <row r="98" spans="2:7" x14ac:dyDescent="0.25">
@@ -6104,7 +6219,7 @@
         <v>1</v>
       </c>
       <c r="C98" s="42" t="s">
-        <v>456</v>
+        <v>453</v>
       </c>
       <c r="D98" s="42">
         <v>8.5</v>
@@ -6118,7 +6233,7 @@
         <v>1</v>
       </c>
       <c r="C99" s="42" t="s">
-        <v>457</v>
+        <v>454</v>
       </c>
       <c r="D99" s="42">
         <v>8.5</v>
@@ -6127,171 +6242,171 @@
         <v>75</v>
       </c>
     </row>
-    <row r="100" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="101" spans="2:7" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B101" s="6" t="s">
+    <row r="100" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B100" s="51" t="s">
+        <v>1</v>
+      </c>
+      <c r="C100" s="42" t="s">
+        <v>455</v>
+      </c>
+      <c r="D100" s="42">
+        <v>8.5</v>
+      </c>
+      <c r="E100" s="42">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="101" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B101" s="51" t="s">
+        <v>1</v>
+      </c>
+      <c r="C101" s="42" t="s">
+        <v>456</v>
+      </c>
+      <c r="D101" s="42">
+        <v>8.5</v>
+      </c>
+      <c r="E101" s="42">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="102" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B102" s="51" t="s">
+        <v>1</v>
+      </c>
+      <c r="C102" s="42" t="s">
+        <v>457</v>
+      </c>
+      <c r="D102" s="42">
+        <v>8.5</v>
+      </c>
+      <c r="E102" s="42">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="103" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="104" spans="2:7" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B104" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C101" s="6"/>
-      <c r="D101" s="6"/>
-      <c r="E101" s="6"/>
-      <c r="F101" s="6"/>
-      <c r="G101" s="6"/>
-    </row>
-    <row r="103" spans="2:7" ht="142.5" x14ac:dyDescent="0.25">
-      <c r="B103" s="5" t="s">
+      <c r="C104" s="6"/>
+      <c r="D104" s="6"/>
+      <c r="E104" s="6"/>
+      <c r="F104" s="6"/>
+      <c r="G104" s="6"/>
+    </row>
+    <row r="106" spans="2:7" ht="142.5" x14ac:dyDescent="0.25">
+      <c r="B106" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C103" s="4" t="s">
+      <c r="C106" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D103" s="4" t="s">
+      <c r="D106" s="4" t="s">
         <v>224</v>
       </c>
-      <c r="E103" s="3" t="s">
+      <c r="E106" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="104" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B104" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C104" s="1" t="s">
+    <row r="107" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B107" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C107" s="1" t="s">
         <v>225</v>
       </c>
-      <c r="D104" s="1" t="s">
+      <c r="D107" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E104" s="1">
+      <c r="E107" s="1">
         <v>0.05</v>
       </c>
     </row>
-    <row r="105" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B105" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C105" s="1" t="s">
+    <row r="108" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B108" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C108" s="1" t="s">
         <v>226</v>
       </c>
-      <c r="D105" s="1" t="s">
+      <c r="D108" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E105" s="1">
+      <c r="E108" s="1">
         <v>0.1</v>
       </c>
     </row>
-    <row r="106" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B106" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C106" s="1" t="s">
+    <row r="109" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B109" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C109" s="1" t="s">
         <v>227</v>
       </c>
-      <c r="D106" s="1" t="s">
+      <c r="D109" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E106" s="1">
+      <c r="E109" s="1">
         <v>0.2</v>
       </c>
     </row>
-    <row r="107" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="108" spans="2:7" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B108" s="6" t="s">
+    <row r="110" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="111" spans="2:7" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B111" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C108" s="6"/>
-      <c r="D108" s="6"/>
-      <c r="E108" s="6"/>
-      <c r="F108" s="6"/>
-      <c r="G108" s="6"/>
-    </row>
-    <row r="110" spans="2:7" ht="132" x14ac:dyDescent="0.25">
-      <c r="B110" s="5" t="s">
+      <c r="C111" s="6"/>
+      <c r="D111" s="6"/>
+      <c r="E111" s="6"/>
+      <c r="F111" s="6"/>
+      <c r="G111" s="6"/>
+    </row>
+    <row r="113" spans="2:7" ht="132" x14ac:dyDescent="0.25">
+      <c r="B113" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C110" s="4" t="s">
+      <c r="C113" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D110" s="3" t="s">
+      <c r="D113" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="111" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B111" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C111" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D111" s="1">
+    <row r="114" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B114" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C114" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D114" s="1">
         <v>0.7</v>
       </c>
     </row>
-    <row r="112" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="113" spans="2:7" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B113" s="6" t="s">
+    <row r="115" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="116" spans="2:7" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B116" s="6" t="s">
         <v>240</v>
       </c>
-      <c r="C113" s="6"/>
-      <c r="D113" s="6"/>
-      <c r="E113" s="6"/>
-      <c r="F113" s="6"/>
-      <c r="G113" s="6"/>
-    </row>
-    <row r="115" spans="2:7" ht="68.25" x14ac:dyDescent="0.25">
-      <c r="B115" s="44" t="s">
+      <c r="C116" s="6"/>
+      <c r="D116" s="6"/>
+      <c r="E116" s="6"/>
+      <c r="F116" s="6"/>
+      <c r="G116" s="6"/>
+    </row>
+    <row r="118" spans="2:7" ht="68.25" x14ac:dyDescent="0.25">
+      <c r="B118" s="44" t="s">
         <v>241</v>
       </c>
-      <c r="C115" s="44" t="s">
+      <c r="C118" s="44" t="s">
         <v>3</v>
       </c>
-      <c r="D115" s="45" t="s">
+      <c r="D118" s="45" t="s">
         <v>242</v>
       </c>
-      <c r="E115" s="45" t="s">
+      <c r="E118" s="45" t="s">
         <v>243</v>
-      </c>
-    </row>
-    <row r="116" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B116" s="43" t="s">
-        <v>1</v>
-      </c>
-      <c r="C116" s="46" t="s">
-        <v>80</v>
-      </c>
-      <c r="D116" s="46" t="s">
-        <v>264</v>
-      </c>
-      <c r="E116" s="43" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="117" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B117" s="43" t="s">
-        <v>1</v>
-      </c>
-      <c r="C117" s="46" t="s">
-        <v>93</v>
-      </c>
-      <c r="D117" s="46" t="s">
-        <v>265</v>
-      </c>
-      <c r="E117" s="43" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="118" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B118" s="43" t="s">
-        <v>1</v>
-      </c>
-      <c r="C118" s="46" t="s">
-        <v>125</v>
-      </c>
-      <c r="D118" s="46" t="s">
-        <v>266</v>
-      </c>
-      <c r="E118" s="43" t="b">
-        <v>1</v>
       </c>
     </row>
     <row r="119" spans="2:7" x14ac:dyDescent="0.25">
@@ -6299,13 +6414,13 @@
         <v>1</v>
       </c>
       <c r="C119" s="46" t="s">
-        <v>109</v>
+        <v>80</v>
       </c>
       <c r="D119" s="46" t="s">
-        <v>109</v>
+        <v>264</v>
       </c>
       <c r="E119" s="43" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="120" spans="2:7" x14ac:dyDescent="0.25">
@@ -6313,13 +6428,13 @@
         <v>1</v>
       </c>
       <c r="C120" s="46" t="s">
-        <v>121</v>
+        <v>93</v>
       </c>
       <c r="D120" s="46" t="s">
-        <v>121</v>
+        <v>265</v>
       </c>
       <c r="E120" s="43" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="121" spans="2:7" x14ac:dyDescent="0.25">
@@ -6327,13 +6442,13 @@
         <v>1</v>
       </c>
       <c r="C121" s="46" t="s">
-        <v>110</v>
+        <v>125</v>
       </c>
       <c r="D121" s="46" t="s">
-        <v>110</v>
+        <v>266</v>
       </c>
       <c r="E121" s="43" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="122" spans="2:7" x14ac:dyDescent="0.25">
@@ -6341,13 +6456,13 @@
         <v>1</v>
       </c>
       <c r="C122" s="46" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="D122" s="46" t="s">
-        <v>267</v>
+        <v>109</v>
       </c>
       <c r="E122" s="43" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="123" spans="2:7" x14ac:dyDescent="0.25">
@@ -6355,13 +6470,13 @@
         <v>1</v>
       </c>
       <c r="C123" s="46" t="s">
-        <v>244</v>
+        <v>121</v>
       </c>
       <c r="D123" s="46" t="s">
-        <v>268</v>
+        <v>121</v>
       </c>
       <c r="E123" s="43" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="124" spans="2:7" x14ac:dyDescent="0.25">
@@ -6369,13 +6484,13 @@
         <v>1</v>
       </c>
       <c r="C124" s="46" t="s">
-        <v>245</v>
+        <v>110</v>
       </c>
       <c r="D124" s="46" t="s">
-        <v>269</v>
+        <v>110</v>
       </c>
       <c r="E124" s="43" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="125" spans="2:7" x14ac:dyDescent="0.25">
@@ -6383,10 +6498,10 @@
         <v>1</v>
       </c>
       <c r="C125" s="46" t="s">
-        <v>205</v>
+        <v>112</v>
       </c>
       <c r="D125" s="46" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="E125" s="43" t="b">
         <v>1</v>
@@ -6397,10 +6512,10 @@
         <v>1</v>
       </c>
       <c r="C126" s="46" t="s">
-        <v>204</v>
+        <v>244</v>
       </c>
       <c r="D126" s="46" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="E126" s="43" t="b">
         <v>1</v>
@@ -6411,10 +6526,10 @@
         <v>1</v>
       </c>
       <c r="C127" s="46" t="s">
-        <v>199</v>
+        <v>245</v>
       </c>
       <c r="D127" s="46" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="E127" s="43" t="b">
         <v>1</v>
@@ -6425,10 +6540,10 @@
         <v>1</v>
       </c>
       <c r="C128" s="46" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="D128" s="46" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="E128" s="43" t="b">
         <v>1</v>
@@ -6439,10 +6554,10 @@
         <v>1</v>
       </c>
       <c r="C129" s="46" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="D129" s="46" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="E129" s="43" t="b">
         <v>1</v>
@@ -6453,10 +6568,10 @@
         <v>1</v>
       </c>
       <c r="C130" s="46" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D130" s="46" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="E130" s="43" t="b">
         <v>1</v>
@@ -6467,10 +6582,10 @@
         <v>1</v>
       </c>
       <c r="C131" s="46" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="D131" s="46" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="E131" s="43" t="b">
         <v>1</v>
@@ -6481,10 +6596,10 @@
         <v>1</v>
       </c>
       <c r="C132" s="46" t="s">
-        <v>114</v>
+        <v>202</v>
       </c>
       <c r="D132" s="46" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="E132" s="43" t="b">
         <v>1</v>
@@ -6495,13 +6610,13 @@
         <v>1</v>
       </c>
       <c r="C133" s="46" t="s">
-        <v>246</v>
+        <v>200</v>
       </c>
       <c r="D133" s="46" t="s">
-        <v>246</v>
+        <v>275</v>
       </c>
       <c r="E133" s="43" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="134" spans="2:5" x14ac:dyDescent="0.25">
@@ -6509,10 +6624,10 @@
         <v>1</v>
       </c>
       <c r="C134" s="46" t="s">
-        <v>83</v>
+        <v>201</v>
       </c>
       <c r="D134" s="46" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="E134" s="43" t="b">
         <v>1</v>
@@ -6523,10 +6638,10 @@
         <v>1</v>
       </c>
       <c r="C135" s="46" t="s">
-        <v>96</v>
+        <v>114</v>
       </c>
       <c r="D135" s="46" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="E135" s="43" t="b">
         <v>1</v>
@@ -6537,13 +6652,13 @@
         <v>1</v>
       </c>
       <c r="C136" s="46" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="D136" s="46" t="s">
-        <v>280</v>
+        <v>246</v>
       </c>
       <c r="E136" s="43" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="137" spans="2:5" x14ac:dyDescent="0.25">
@@ -6551,10 +6666,10 @@
         <v>1</v>
       </c>
       <c r="C137" s="46" t="s">
-        <v>248</v>
+        <v>83</v>
       </c>
       <c r="D137" s="46" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="E137" s="43" t="b">
         <v>1</v>
@@ -6565,10 +6680,10 @@
         <v>1</v>
       </c>
       <c r="C138" s="46" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="D138" s="46" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="E138" s="43" t="b">
         <v>1</v>
@@ -6579,10 +6694,10 @@
         <v>1</v>
       </c>
       <c r="C139" s="46" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="D139" s="46" t="s">
-        <v>304</v>
+        <v>280</v>
       </c>
       <c r="E139" s="43" t="b">
         <v>1</v>
@@ -6593,10 +6708,10 @@
         <v>1</v>
       </c>
       <c r="C140" s="46" t="s">
-        <v>123</v>
+        <v>248</v>
       </c>
       <c r="D140" s="46" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="E140" s="43" t="b">
         <v>1</v>
@@ -6607,10 +6722,10 @@
         <v>1</v>
       </c>
       <c r="C141" s="46" t="s">
-        <v>88</v>
+        <v>102</v>
       </c>
       <c r="D141" s="46" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="E141" s="43" t="b">
         <v>1</v>
@@ -6621,10 +6736,10 @@
         <v>1</v>
       </c>
       <c r="C142" s="46" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="D142" s="46" t="s">
-        <v>285</v>
+        <v>304</v>
       </c>
       <c r="E142" s="43" t="b">
         <v>1</v>
@@ -6635,10 +6750,10 @@
         <v>1</v>
       </c>
       <c r="C143" s="46" t="s">
-        <v>302</v>
+        <v>123</v>
       </c>
       <c r="D143" s="46" t="s">
-        <v>303</v>
+        <v>283</v>
       </c>
       <c r="E143" s="43" t="b">
         <v>1</v>
@@ -6649,13 +6764,13 @@
         <v>1</v>
       </c>
       <c r="C144" s="46" t="s">
-        <v>251</v>
+        <v>88</v>
       </c>
       <c r="D144" s="46" t="s">
-        <v>251</v>
+        <v>284</v>
       </c>
       <c r="E144" s="43" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="145" spans="2:5" x14ac:dyDescent="0.25">
@@ -6663,13 +6778,13 @@
         <v>1</v>
       </c>
       <c r="C145" s="46" t="s">
-        <v>116</v>
+        <v>250</v>
       </c>
       <c r="D145" s="46" t="s">
-        <v>116</v>
+        <v>285</v>
       </c>
       <c r="E145" s="43" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="146" spans="2:5" x14ac:dyDescent="0.25">
@@ -6677,10 +6792,10 @@
         <v>1</v>
       </c>
       <c r="C146" s="46" t="s">
-        <v>252</v>
+        <v>302</v>
       </c>
       <c r="D146" s="46" t="s">
-        <v>286</v>
+        <v>303</v>
       </c>
       <c r="E146" s="43" t="b">
         <v>1</v>
@@ -6691,13 +6806,13 @@
         <v>1</v>
       </c>
       <c r="C147" s="46" t="s">
-        <v>91</v>
+        <v>251</v>
       </c>
       <c r="D147" s="46" t="s">
-        <v>287</v>
+        <v>251</v>
       </c>
       <c r="E147" s="43" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="148" spans="2:5" x14ac:dyDescent="0.25">
@@ -6705,13 +6820,13 @@
         <v>1</v>
       </c>
       <c r="C148" s="46" t="s">
-        <v>253</v>
+        <v>116</v>
       </c>
       <c r="D148" s="46" t="s">
-        <v>288</v>
+        <v>116</v>
       </c>
       <c r="E148" s="43" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="149" spans="2:5" x14ac:dyDescent="0.25">
@@ -6719,10 +6834,10 @@
         <v>1</v>
       </c>
       <c r="C149" s="46" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="D149" s="46" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="E149" s="43" t="b">
         <v>1</v>
@@ -6733,10 +6848,10 @@
         <v>1</v>
       </c>
       <c r="C150" s="46" t="s">
-        <v>255</v>
+        <v>91</v>
       </c>
       <c r="D150" s="46" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="E150" s="43" t="b">
         <v>1</v>
@@ -6747,10 +6862,10 @@
         <v>1</v>
       </c>
       <c r="C151" s="46" t="s">
-        <v>86</v>
+        <v>253</v>
       </c>
       <c r="D151" s="46" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="E151" s="43" t="b">
         <v>1</v>
@@ -6761,13 +6876,13 @@
         <v>1</v>
       </c>
       <c r="C152" s="46" t="s">
-        <v>73</v>
+        <v>254</v>
       </c>
       <c r="D152" s="46" t="s">
-        <v>73</v>
+        <v>289</v>
       </c>
       <c r="E152" s="43" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="153" spans="2:5" x14ac:dyDescent="0.25">
@@ -6775,13 +6890,13 @@
         <v>1</v>
       </c>
       <c r="C153" s="46" t="s">
-        <v>108</v>
+        <v>255</v>
       </c>
       <c r="D153" s="46" t="s">
-        <v>108</v>
+        <v>290</v>
       </c>
       <c r="E153" s="43" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="154" spans="2:5" x14ac:dyDescent="0.25">
@@ -6789,10 +6904,10 @@
         <v>1</v>
       </c>
       <c r="C154" s="46" t="s">
-        <v>256</v>
+        <v>86</v>
       </c>
       <c r="D154" s="46" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="E154" s="43" t="b">
         <v>1</v>
@@ -6803,13 +6918,13 @@
         <v>1</v>
       </c>
       <c r="C155" s="46" t="s">
-        <v>257</v>
+        <v>73</v>
       </c>
       <c r="D155" s="46" t="s">
-        <v>293</v>
+        <v>73</v>
       </c>
       <c r="E155" s="43" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="156" spans="2:5" x14ac:dyDescent="0.25">
@@ -6817,13 +6932,13 @@
         <v>1</v>
       </c>
       <c r="C156" s="46" t="s">
-        <v>77</v>
+        <v>108</v>
       </c>
       <c r="D156" s="46" t="s">
-        <v>294</v>
+        <v>108</v>
       </c>
       <c r="E156" s="43" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="157" spans="2:5" x14ac:dyDescent="0.25">
@@ -6831,10 +6946,10 @@
         <v>1</v>
       </c>
       <c r="C157" s="46" t="s">
-        <v>105</v>
+        <v>256</v>
       </c>
       <c r="D157" s="46" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="E157" s="43" t="b">
         <v>1</v>
@@ -6845,10 +6960,10 @@
         <v>1</v>
       </c>
       <c r="C158" s="46" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="D158" s="46" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="E158" s="43" t="b">
         <v>1</v>
@@ -6859,10 +6974,10 @@
         <v>1</v>
       </c>
       <c r="C159" s="46" t="s">
-        <v>259</v>
+        <v>77</v>
       </c>
       <c r="D159" s="46" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="E159" s="43" t="b">
         <v>1</v>
@@ -6873,10 +6988,10 @@
         <v>1</v>
       </c>
       <c r="C160" s="46" t="s">
-        <v>260</v>
+        <v>105</v>
       </c>
       <c r="D160" s="46" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="E160" s="43" t="b">
         <v>1</v>
@@ -6887,13 +7002,13 @@
         <v>1</v>
       </c>
       <c r="C161" s="46" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="D161" s="46" t="s">
-        <v>261</v>
+        <v>296</v>
       </c>
       <c r="E161" s="43" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="162" spans="2:5" x14ac:dyDescent="0.25">
@@ -6901,10 +7016,10 @@
         <v>1</v>
       </c>
       <c r="C162" s="46" t="s">
-        <v>99</v>
+        <v>259</v>
       </c>
       <c r="D162" s="46" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="E162" s="43" t="b">
         <v>1</v>
@@ -6915,10 +7030,10 @@
         <v>1</v>
       </c>
       <c r="C163" s="46" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="D163" s="46" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="E163" s="43" t="b">
         <v>1</v>
@@ -6929,13 +7044,13 @@
         <v>1</v>
       </c>
       <c r="C164" s="46" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="D164" s="46" t="s">
-        <v>301</v>
+        <v>261</v>
       </c>
       <c r="E164" s="43" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="165" spans="2:5" x14ac:dyDescent="0.25">
@@ -6943,10 +7058,10 @@
         <v>1</v>
       </c>
       <c r="C165" s="46" t="s">
-        <v>310</v>
+        <v>99</v>
       </c>
       <c r="D165" s="46" t="s">
-        <v>307</v>
+        <v>299</v>
       </c>
       <c r="E165" s="43" t="b">
         <v>1</v>
@@ -6957,10 +7072,10 @@
         <v>1</v>
       </c>
       <c r="C166" s="46" t="s">
-        <v>311</v>
+        <v>262</v>
       </c>
       <c r="D166" s="46" t="s">
-        <v>308</v>
+        <v>300</v>
       </c>
       <c r="E166" s="43" t="b">
         <v>1</v>
@@ -6971,12 +7086,54 @@
         <v>1</v>
       </c>
       <c r="C167" s="46" t="s">
+        <v>263</v>
+      </c>
+      <c r="D167" s="46" t="s">
+        <v>301</v>
+      </c>
+      <c r="E167" s="43" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="168" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B168" s="43" t="s">
+        <v>1</v>
+      </c>
+      <c r="C168" s="46" t="s">
+        <v>310</v>
+      </c>
+      <c r="D168" s="46" t="s">
+        <v>307</v>
+      </c>
+      <c r="E168" s="43" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="169" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B169" s="43" t="s">
+        <v>1</v>
+      </c>
+      <c r="C169" s="46" t="s">
+        <v>311</v>
+      </c>
+      <c r="D169" s="46" t="s">
+        <v>308</v>
+      </c>
+      <c r="E169" s="43" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="170" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B170" s="43" t="s">
+        <v>1</v>
+      </c>
+      <c r="C170" s="46" t="s">
         <v>312</v>
       </c>
-      <c r="D167" s="46" t="s">
+      <c r="D170" s="46" t="s">
         <v>309</v>
       </c>
-      <c r="E167" s="43" t="b">
+      <c r="E170" s="43" t="b">
         <v>1</v>
       </c>
     </row>
@@ -6984,10 +7141,10 @@
   <mergeCells count="4">
     <mergeCell ref="J3:K3"/>
     <mergeCell ref="M3:P3"/>
-    <mergeCell ref="F47:H47"/>
-    <mergeCell ref="G72:H72"/>
+    <mergeCell ref="F49:H49"/>
+    <mergeCell ref="G75:H75"/>
   </mergeCells>
-  <conditionalFormatting sqref="C74:E76">
+  <conditionalFormatting sqref="C77:E79">
     <cfRule type="duplicateValues" dxfId="68" priority="2"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Fix a mission type (that as now it is not exported, there is no xml to commit)
Former-commit-id: 564ffa455ae81e1f6a83b93bb78549dbcafe4908
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Missions.xlsx
+++ b/Docs/Content/HungryDragonContent_Missions.xlsx
@@ -24,8 +24,32 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Jose Camacho</author>
+  </authors>
+  <commentList>
+    <comment ref="B9" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>*Add this mission once Halloween is over</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1074" uniqueCount="467">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1074" uniqueCount="468">
   <si>
     <t>single_run</t>
   </si>
@@ -1454,12 +1478,15 @@
   <si>
     <t>Villager01;BakerWoman;BoatFisher;Ground_Zombie</t>
   </si>
+  <si>
+    <t>Villager01;Villager02;Villager03;Villager04;VillagerGirl;BakerWoman;BadFarmer;BoatFisher</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1542,6 +1569,13 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="8"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="16">
@@ -3484,14 +3518,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="6"/>
   </sheetPr>
   <dimension ref="B1:P170"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I44" sqref="I44"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3769,7 +3803,7 @@
         <v>7</v>
       </c>
       <c r="I9" s="24" t="s">
-        <v>148</v>
+        <v>467</v>
       </c>
       <c r="J9" s="24">
         <v>25</v>
@@ -7149,13 +7183,14 @@
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
   <tableParts count="6">
-    <tablePart r:id="rId2"/>
     <tablePart r:id="rId3"/>
     <tablePart r:id="rId4"/>
     <tablePart r:id="rId5"/>
     <tablePart r:id="rId6"/>
     <tablePart r:id="rId7"/>
+    <tablePart r:id="rId8"/>
   </tableParts>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Adding new icons for tournaments in content
Former-commit-id: e78433e49ff38db608e797ed2e0806f43b46b0f2
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Missions.xlsx
+++ b/Docs/Content/HungryDragonContent_Missions.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\dragon\Docs\Content\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\dragon\client\Docs\Content\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="38295" windowHeight="19860" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="38295" windowHeight="19860"/>
   </bookViews>
   <sheets>
     <sheet name="missions" sheetId="1" r:id="rId1"/>
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1083" uniqueCount="474">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1107" uniqueCount="484">
   <si>
     <t>single_run</t>
   </si>
@@ -1501,6 +1501,36 @@
   </si>
   <si>
     <t>dragon_dino</t>
+  </si>
+  <si>
+    <t>PF_icon_fish</t>
+  </si>
+  <si>
+    <t>PF_icon_ghost</t>
+  </si>
+  <si>
+    <t>PF_icon_troll</t>
+  </si>
+  <si>
+    <t>PF_icon_stun</t>
+  </si>
+  <si>
+    <t>PF_icon_freeze</t>
+  </si>
+  <si>
+    <t>PF_icon_fairy</t>
+  </si>
+  <si>
+    <t>PF_icon_eat_gold</t>
+  </si>
+  <si>
+    <t>icon_stun</t>
+  </si>
+  <si>
+    <t>icon_freeze</t>
+  </si>
+  <si>
+    <t>icon_eat_gold</t>
   </si>
 </sst>
 </file>
@@ -1968,13 +1998,6 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1990,55 +2013,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="69">
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -2727,6 +2713,40 @@
         <horizontal style="thin">
           <color indexed="64"/>
         </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
       </border>
     </dxf>
     <dxf>
@@ -3155,6 +3175,16 @@
         </bottom>
       </border>
     </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -3174,109 +3204,111 @@
     <sheetNames>
       <sheetName val="missions"/>
       <sheetName val="tournaments"/>
+      <sheetName val="HungryDragonContent_MissionsLD"/>
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0"/>
       <sheetData sheetId="1" refreshError="1"/>
+      <sheetData sheetId="2" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="missionDifficultyDefinitions" displayName="missionDifficultyDefinitions" ref="B76:L79" totalsRowShown="0" headerRowBorderDxfId="68" tableBorderDxfId="67">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="missionDifficultyDefinitions" displayName="missionDifficultyDefinitions" ref="B76:L79" totalsRowShown="0" headerRowBorderDxfId="67" tableBorderDxfId="66">
   <autoFilter ref="B76:L79"/>
   <tableColumns count="11">
     <tableColumn id="1" name="{missionDifficultyDefinitions}"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="66"/>
-    <tableColumn id="11" name="[difficulty]" dataDxfId="65"/>
-    <tableColumn id="7" name="[index]" dataDxfId="64"/>
-    <tableColumn id="3" name="[dragonsToUnlock]" dataDxfId="63"/>
-    <tableColumn id="4" name="[cooldownMinutes]" dataDxfId="62"/>
-    <tableColumn id="9" name="[maxRewardCoins]" dataDxfId="61"/>
-    <tableColumn id="5" name="[removeMissionPCCoefA]" dataDxfId="60"/>
-    <tableColumn id="6" name="[removeMissionPCCoefB]" dataDxfId="59"/>
-    <tableColumn id="8" name="[tidName]" dataDxfId="58"/>
-    <tableColumn id="10" name="[color]" dataDxfId="57"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="65"/>
+    <tableColumn id="11" name="[difficulty]" dataDxfId="64"/>
+    <tableColumn id="7" name="[index]" dataDxfId="63"/>
+    <tableColumn id="3" name="[dragonsToUnlock]" dataDxfId="62"/>
+    <tableColumn id="4" name="[cooldownMinutes]" dataDxfId="61"/>
+    <tableColumn id="9" name="[maxRewardCoins]" dataDxfId="60"/>
+    <tableColumn id="5" name="[removeMissionPCCoefA]" dataDxfId="59"/>
+    <tableColumn id="6" name="[removeMissionPCCoefB]" dataDxfId="58"/>
+    <tableColumn id="8" name="[tidName]" dataDxfId="57"/>
+    <tableColumn id="10" name="[color]" dataDxfId="56"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table13303132" displayName="Table13303132" ref="B84:E102" totalsRowShown="0" headerRowDxfId="56" dataDxfId="54" headerRowBorderDxfId="55" tableBorderDxfId="53" totalsRowBorderDxfId="52">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table13303132" displayName="Table13303132" ref="B84:E102" totalsRowShown="0" headerRowDxfId="55" dataDxfId="53" headerRowBorderDxfId="54" tableBorderDxfId="52" totalsRowBorderDxfId="51">
   <autoFilter ref="B84:E102"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="{missionDragonModifiersDefinitions}" dataDxfId="51"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="50"/>
-    <tableColumn id="7" name="[quantityModifier]" dataDxfId="1"/>
-    <tableColumn id="3" name="[missionSCRewardMultiplier]" dataDxfId="0"/>
+    <tableColumn id="1" name="{missionDragonModifiersDefinitions}" dataDxfId="50"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="49"/>
+    <tableColumn id="7" name="[quantityModifier]" dataDxfId="48"/>
+    <tableColumn id="3" name="[missionSCRewardMultiplier]" dataDxfId="47"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table1330313234" displayName="Table1330313234" ref="B106:E109" totalsRowShown="0" headerRowDxfId="49" dataDxfId="47" headerRowBorderDxfId="48" tableBorderDxfId="46" totalsRowBorderDxfId="45">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table1330313234" displayName="Table1330313234" ref="B106:E109" totalsRowShown="0" headerRowDxfId="46" dataDxfId="44" headerRowBorderDxfId="45" tableBorderDxfId="43" totalsRowBorderDxfId="42">
   <autoFilter ref="B106:E109"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="{missionDifficultyModifiersDefinitions}" dataDxfId="44"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="43"/>
-    <tableColumn id="3" name="[difficulty]" dataDxfId="42"/>
-    <tableColumn id="7" name="[quantityModifier]" dataDxfId="41"/>
+    <tableColumn id="1" name="{missionDifficultyModifiersDefinitions}" dataDxfId="41"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="40"/>
+    <tableColumn id="3" name="[difficulty]" dataDxfId="39"/>
+    <tableColumn id="7" name="[quantityModifier]" dataDxfId="38"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table133031323435" displayName="Table133031323435" ref="B113:D114" totalsRowShown="0" headerRowDxfId="40" dataDxfId="38" headerRowBorderDxfId="39" tableBorderDxfId="37" totalsRowBorderDxfId="36">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table133031323435" displayName="Table133031323435" ref="B113:D114" totalsRowShown="0" headerRowDxfId="37" dataDxfId="35" headerRowBorderDxfId="36" tableBorderDxfId="34" totalsRowBorderDxfId="33">
   <autoFilter ref="B113:D114"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="{missionOtherModifiersDefinitions}" dataDxfId="35"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="34"/>
-    <tableColumn id="7" name="[quantityModifier]" dataDxfId="33"/>
+    <tableColumn id="1" name="{missionOtherModifiersDefinitions}" dataDxfId="32"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="31"/>
+    <tableColumn id="7" name="[quantityModifier]" dataDxfId="30"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table13" displayName="Table13" ref="B50:H69" totalsRowShown="0" headerRowDxfId="32" dataDxfId="30" headerRowBorderDxfId="31" tableBorderDxfId="29" totalsRowBorderDxfId="28">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table13" displayName="Table13" ref="B50:H69" totalsRowShown="0" headerRowDxfId="29" dataDxfId="27" headerRowBorderDxfId="28" tableBorderDxfId="26" totalsRowBorderDxfId="25">
   <autoFilter ref="B50:H69"/>
   <tableColumns count="7">
-    <tableColumn id="1" name="{missionTypeDefinitions}" dataDxfId="27"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="26"/>
-    <tableColumn id="3" name="[minTier]" dataDxfId="25"/>
-    <tableColumn id="6" name="[maxTier]" dataDxfId="24"/>
-    <tableColumn id="4" name="[weight]" dataDxfId="23"/>
-    <tableColumn id="9" name="[tidDescSingleRun]" dataDxfId="22"/>
-    <tableColumn id="10" name="[tidDescMultiRun]" dataDxfId="21"/>
+    <tableColumn id="1" name="{missionTypeDefinitions}" dataDxfId="24"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="23"/>
+    <tableColumn id="3" name="[minTier]" dataDxfId="22"/>
+    <tableColumn id="6" name="[maxTier]" dataDxfId="21"/>
+    <tableColumn id="4" name="[weight]" dataDxfId="20"/>
+    <tableColumn id="9" name="[tidDescSingleRun]" dataDxfId="19"/>
+    <tableColumn id="10" name="[tidDescMultiRun]" dataDxfId="18"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table1330" displayName="Table1330" ref="B4:N45" totalsRowShown="0" headerRowDxfId="20" dataDxfId="18" headerRowBorderDxfId="19" tableBorderDxfId="17" totalsRowBorderDxfId="16">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table1330" displayName="Table1330" ref="B4:N45" totalsRowShown="0" headerRowDxfId="17" dataDxfId="15" headerRowBorderDxfId="16" tableBorderDxfId="14" totalsRowBorderDxfId="13">
   <autoFilter ref="B4:N45"/>
   <sortState ref="B5:P43">
     <sortCondition descending="1" ref="J4:J43"/>
   </sortState>
   <tableColumns count="13">
-    <tableColumn id="1" name="{missionsDefinitions}" dataDxfId="15"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="14"/>
-    <tableColumn id="7" name="[type]" dataDxfId="13"/>
-    <tableColumn id="8" name="[weight]" dataDxfId="12"/>
-    <tableColumn id="13" name="[singleRunChance]" dataDxfId="11"/>
-    <tableColumn id="11" name="[minTier]" dataDxfId="10"/>
-    <tableColumn id="12" name="[maxTier]" dataDxfId="9"/>
-    <tableColumn id="6" name="[params]" dataDxfId="8"/>
-    <tableColumn id="3" name="[objectiveBaseQuantityMin]" dataDxfId="7"/>
-    <tableColumn id="9" name="[objectiveBaseQuantityMax]" dataDxfId="6"/>
-    <tableColumn id="4" name="[icon]" dataDxfId="5"/>
-    <tableColumn id="5" name="[tidObjective]" dataDxfId="4"/>
-    <tableColumn id="10" name="[trackingSku]" dataDxfId="3">
+    <tableColumn id="1" name="{missionsDefinitions}" dataDxfId="12"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="11"/>
+    <tableColumn id="7" name="[type]" dataDxfId="10"/>
+    <tableColumn id="8" name="[weight]" dataDxfId="9"/>
+    <tableColumn id="13" name="[singleRunChance]" dataDxfId="8"/>
+    <tableColumn id="11" name="[minTier]" dataDxfId="7"/>
+    <tableColumn id="12" name="[maxTier]" dataDxfId="6"/>
+    <tableColumn id="6" name="[params]" dataDxfId="5"/>
+    <tableColumn id="3" name="[objectiveBaseQuantityMin]" dataDxfId="4"/>
+    <tableColumn id="9" name="[objectiveBaseQuantityMax]" dataDxfId="3"/>
+    <tableColumn id="4" name="[icon]" dataDxfId="2"/>
+    <tableColumn id="5" name="[tidObjective]" dataDxfId="1"/>
+    <tableColumn id="10" name="[trackingSku]" dataDxfId="0">
       <calculatedColumnFormula>[1]!Table1330[[#This Row],['[sku']]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -3550,10 +3582,10 @@
   <sheetPr>
     <tabColor theme="6"/>
   </sheetPr>
-  <dimension ref="B1:P173"/>
+  <dimension ref="B1:P181"/>
   <sheetViews>
-    <sheetView topLeftCell="A133" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G86" sqref="G86"/>
+    <sheetView tabSelected="1" topLeftCell="A151" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D185" sqref="D185"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3600,14 +3632,14 @@
         <v>140</v>
       </c>
       <c r="G3" s="38"/>
-      <c r="J3" s="57" t="s">
+      <c r="J3" s="62" t="s">
         <v>139</v>
       </c>
-      <c r="K3" s="57"/>
-      <c r="M3" s="57"/>
-      <c r="N3" s="57"/>
-      <c r="O3" s="57"/>
-      <c r="P3" s="57"/>
+      <c r="K3" s="62"/>
+      <c r="M3" s="62"/>
+      <c r="N3" s="62"/>
+      <c r="O3" s="62"/>
+      <c r="P3" s="62"/>
     </row>
     <row r="4" spans="2:16" ht="106.5" x14ac:dyDescent="0.25">
       <c r="B4" s="30" t="s">
@@ -5267,13 +5299,13 @@
       <c r="K44" s="23">
         <v>30</v>
       </c>
-      <c r="L44" s="62" t="s">
+      <c r="L44" s="59" t="s">
         <v>123</v>
       </c>
       <c r="M44" s="24" t="s">
         <v>462</v>
       </c>
-      <c r="N44" s="63" t="str">
+      <c r="N44" s="60" t="str">
         <f>[1]!Table1330[[#This Row],['[sku']]]</f>
         <v>halloween_zombie</v>
       </c>
@@ -5309,13 +5341,13 @@
       <c r="K45" s="23">
         <v>30</v>
       </c>
-      <c r="L45" s="61" t="s">
+      <c r="L45" s="58" t="s">
         <v>123</v>
       </c>
       <c r="M45" s="23" t="s">
         <v>466</v>
       </c>
-      <c r="N45" s="64" t="str">
+      <c r="N45" s="61" t="str">
         <f>[1]!Table1330[[#This Row],['[sku']]]</f>
         <v>halloween_creatures</v>
       </c>
@@ -5369,9 +5401,9 @@
       <c r="C49" s="20"/>
       <c r="D49" s="20"/>
       <c r="E49" s="20"/>
-      <c r="F49" s="58"/>
-      <c r="G49" s="58"/>
-      <c r="H49" s="58"/>
+      <c r="F49" s="63"/>
+      <c r="G49" s="63"/>
+      <c r="H49" s="63"/>
       <c r="I49" s="20"/>
       <c r="J49" s="20"/>
     </row>
@@ -5891,7 +5923,7 @@
       <c r="F72" s="53">
         <v>2</v>
       </c>
-      <c r="G72" s="60" t="s">
+      <c r="G72" s="57" t="s">
         <v>467</v>
       </c>
       <c r="H72" s="53" t="s">
@@ -5923,10 +5955,10 @@
       <c r="F75" s="21" t="s">
         <v>40</v>
       </c>
-      <c r="G75" s="59" t="s">
+      <c r="G75" s="64" t="s">
         <v>39</v>
       </c>
-      <c r="H75" s="59"/>
+      <c r="H75" s="64"/>
       <c r="I75" s="20"/>
     </row>
     <row r="76" spans="2:13" ht="142.5" x14ac:dyDescent="0.25">
@@ -7238,6 +7270,118 @@
         <v>458</v>
       </c>
       <c r="E173" s="43" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="174" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B174" s="43" t="s">
+        <v>1</v>
+      </c>
+      <c r="C174" s="46" t="s">
+        <v>361</v>
+      </c>
+      <c r="D174" s="46" t="s">
+        <v>474</v>
+      </c>
+      <c r="E174" s="43" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="175" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B175" s="43" t="s">
+        <v>1</v>
+      </c>
+      <c r="C175" s="46" t="s">
+        <v>367</v>
+      </c>
+      <c r="D175" s="46" t="s">
+        <v>475</v>
+      </c>
+      <c r="E175" s="43" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="176" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B176" s="43" t="s">
+        <v>1</v>
+      </c>
+      <c r="C176" s="46" t="s">
+        <v>105</v>
+      </c>
+      <c r="D176" s="46" t="s">
+        <v>295</v>
+      </c>
+      <c r="E176" s="43" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="177" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B177" s="43" t="s">
+        <v>1</v>
+      </c>
+      <c r="C177" s="46" t="s">
+        <v>74</v>
+      </c>
+      <c r="D177" s="46" t="s">
+        <v>476</v>
+      </c>
+      <c r="E177" s="43" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="178" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B178" s="43" t="s">
+        <v>1</v>
+      </c>
+      <c r="C178" s="46" t="s">
+        <v>481</v>
+      </c>
+      <c r="D178" s="46" t="s">
+        <v>477</v>
+      </c>
+      <c r="E178" s="43" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="179" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B179" s="43" t="s">
+        <v>1</v>
+      </c>
+      <c r="C179" s="46" t="s">
+        <v>482</v>
+      </c>
+      <c r="D179" s="46" t="s">
+        <v>478</v>
+      </c>
+      <c r="E179" s="43" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="180" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B180" s="43" t="s">
+        <v>1</v>
+      </c>
+      <c r="C180" s="46" t="s">
+        <v>430</v>
+      </c>
+      <c r="D180" s="46" t="s">
+        <v>479</v>
+      </c>
+      <c r="E180" s="43" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="181" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B181" s="43" t="s">
+        <v>1</v>
+      </c>
+      <c r="C181" s="46" t="s">
+        <v>483</v>
+      </c>
+      <c r="D181" s="46" t="s">
+        <v>480</v>
+      </c>
+      <c r="E181" s="43" t="b">
         <v>1</v>
       </c>
     </row>
@@ -7249,7 +7393,7 @@
     <mergeCell ref="G75:H75"/>
   </mergeCells>
   <conditionalFormatting sqref="C77:E79">
-    <cfRule type="duplicateValues" dxfId="2" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="68" priority="2"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -7269,7 +7413,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G99"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
+    <sheetView topLeftCell="A61" workbookViewId="0">
       <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Fixing a bug. Duplicated sku and another fix related to using folder references in the excel
Former-commit-id: 1be03cf2416c616962b9fc6f59df1bbd8b1423f6
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Missions.xlsx
+++ b/Docs/Content/HungryDragonContent_Missions.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\dragon\client\Docs\Content\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\dragon\Docs\Content\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -15,9 +15,6 @@
     <sheet name="missions" sheetId="1" r:id="rId1"/>
     <sheet name="tournaments" sheetId="2" r:id="rId2"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId3"/>
-  </externalReferences>
   <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -52,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1107" uniqueCount="484">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1138" uniqueCount="486">
   <si>
     <t>single_run</t>
   </si>
@@ -1531,6 +1528,12 @@
   </si>
   <si>
     <t>icon_eat_gold</t>
+  </si>
+  <si>
+    <t>zombies</t>
+  </si>
+  <si>
+    <t>halloween</t>
   </si>
 </sst>
 </file>
@@ -1862,7 +1865,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="65">
+  <cellXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1"/>
@@ -1998,9 +2001,6 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2020,6 +2020,15 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2048,6 +2057,16 @@
           <color indexed="64"/>
         </horizontal>
       </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -3175,16 +3194,6 @@
         </bottom>
       </border>
     </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -3198,119 +3207,100 @@
 </styleSheet>
 </file>
 
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="missions"/>
-      <sheetName val="tournaments"/>
-      <sheetName val="HungryDragonContent_MissionsLD"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1" refreshError="1"/>
-      <sheetData sheetId="2" refreshError="1"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="missionDifficultyDefinitions" displayName="missionDifficultyDefinitions" ref="B76:L79" totalsRowShown="0" headerRowBorderDxfId="67" tableBorderDxfId="66">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="missionDifficultyDefinitions" displayName="missionDifficultyDefinitions" ref="B76:L79" totalsRowShown="0" headerRowBorderDxfId="68" tableBorderDxfId="67">
   <autoFilter ref="B76:L79"/>
   <tableColumns count="11">
     <tableColumn id="1" name="{missionDifficultyDefinitions}"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="65"/>
-    <tableColumn id="11" name="[difficulty]" dataDxfId="64"/>
-    <tableColumn id="7" name="[index]" dataDxfId="63"/>
-    <tableColumn id="3" name="[dragonsToUnlock]" dataDxfId="62"/>
-    <tableColumn id="4" name="[cooldownMinutes]" dataDxfId="61"/>
-    <tableColumn id="9" name="[maxRewardCoins]" dataDxfId="60"/>
-    <tableColumn id="5" name="[removeMissionPCCoefA]" dataDxfId="59"/>
-    <tableColumn id="6" name="[removeMissionPCCoefB]" dataDxfId="58"/>
-    <tableColumn id="8" name="[tidName]" dataDxfId="57"/>
-    <tableColumn id="10" name="[color]" dataDxfId="56"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="66"/>
+    <tableColumn id="11" name="[difficulty]" dataDxfId="65"/>
+    <tableColumn id="7" name="[index]" dataDxfId="64"/>
+    <tableColumn id="3" name="[dragonsToUnlock]" dataDxfId="63"/>
+    <tableColumn id="4" name="[cooldownMinutes]" dataDxfId="62"/>
+    <tableColumn id="9" name="[maxRewardCoins]" dataDxfId="61"/>
+    <tableColumn id="5" name="[removeMissionPCCoefA]" dataDxfId="60"/>
+    <tableColumn id="6" name="[removeMissionPCCoefB]" dataDxfId="59"/>
+    <tableColumn id="8" name="[tidName]" dataDxfId="58"/>
+    <tableColumn id="10" name="[color]" dataDxfId="57"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table13303132" displayName="Table13303132" ref="B84:E102" totalsRowShown="0" headerRowDxfId="55" dataDxfId="53" headerRowBorderDxfId="54" tableBorderDxfId="52" totalsRowBorderDxfId="51">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table13303132" displayName="Table13303132" ref="B84:E102" totalsRowShown="0" headerRowDxfId="56" dataDxfId="54" headerRowBorderDxfId="55" tableBorderDxfId="53" totalsRowBorderDxfId="52">
   <autoFilter ref="B84:E102"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="{missionDragonModifiersDefinitions}" dataDxfId="50"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="49"/>
-    <tableColumn id="7" name="[quantityModifier]" dataDxfId="48"/>
-    <tableColumn id="3" name="[missionSCRewardMultiplier]" dataDxfId="47"/>
+    <tableColumn id="1" name="{missionDragonModifiersDefinitions}" dataDxfId="51"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="50"/>
+    <tableColumn id="7" name="[quantityModifier]" dataDxfId="49"/>
+    <tableColumn id="3" name="[missionSCRewardMultiplier]" dataDxfId="48"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table1330313234" displayName="Table1330313234" ref="B106:E109" totalsRowShown="0" headerRowDxfId="46" dataDxfId="44" headerRowBorderDxfId="45" tableBorderDxfId="43" totalsRowBorderDxfId="42">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table1330313234" displayName="Table1330313234" ref="B106:E109" totalsRowShown="0" headerRowDxfId="47" dataDxfId="45" headerRowBorderDxfId="46" tableBorderDxfId="44" totalsRowBorderDxfId="43">
   <autoFilter ref="B106:E109"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="{missionDifficultyModifiersDefinitions}" dataDxfId="41"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="40"/>
-    <tableColumn id="3" name="[difficulty]" dataDxfId="39"/>
-    <tableColumn id="7" name="[quantityModifier]" dataDxfId="38"/>
+    <tableColumn id="1" name="{missionDifficultyModifiersDefinitions}" dataDxfId="42"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="41"/>
+    <tableColumn id="3" name="[difficulty]" dataDxfId="40"/>
+    <tableColumn id="7" name="[quantityModifier]" dataDxfId="39"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table133031323435" displayName="Table133031323435" ref="B113:D114" totalsRowShown="0" headerRowDxfId="37" dataDxfId="35" headerRowBorderDxfId="36" tableBorderDxfId="34" totalsRowBorderDxfId="33">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table133031323435" displayName="Table133031323435" ref="B113:D114" totalsRowShown="0" headerRowDxfId="38" dataDxfId="36" headerRowBorderDxfId="37" tableBorderDxfId="35" totalsRowBorderDxfId="34">
   <autoFilter ref="B113:D114"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="{missionOtherModifiersDefinitions}" dataDxfId="32"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="31"/>
-    <tableColumn id="7" name="[quantityModifier]" dataDxfId="30"/>
+    <tableColumn id="1" name="{missionOtherModifiersDefinitions}" dataDxfId="33"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="32"/>
+    <tableColumn id="7" name="[quantityModifier]" dataDxfId="31"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table13" displayName="Table13" ref="B50:H69" totalsRowShown="0" headerRowDxfId="29" dataDxfId="27" headerRowBorderDxfId="28" tableBorderDxfId="26" totalsRowBorderDxfId="25">
-  <autoFilter ref="B50:H69"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table13" displayName="Table13" ref="B50:H72" totalsRowShown="0" headerRowDxfId="30" dataDxfId="28" headerRowBorderDxfId="29" tableBorderDxfId="27" totalsRowBorderDxfId="26">
+  <autoFilter ref="B50:H72"/>
   <tableColumns count="7">
-    <tableColumn id="1" name="{missionTypeDefinitions}" dataDxfId="24"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="23"/>
-    <tableColumn id="3" name="[minTier]" dataDxfId="22"/>
-    <tableColumn id="6" name="[maxTier]" dataDxfId="21"/>
-    <tableColumn id="4" name="[weight]" dataDxfId="20"/>
-    <tableColumn id="9" name="[tidDescSingleRun]" dataDxfId="19"/>
-    <tableColumn id="10" name="[tidDescMultiRun]" dataDxfId="18"/>
+    <tableColumn id="1" name="{missionTypeDefinitions}" dataDxfId="25"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="24"/>
+    <tableColumn id="3" name="[minTier]" dataDxfId="23"/>
+    <tableColumn id="6" name="[maxTier]" dataDxfId="22"/>
+    <tableColumn id="4" name="[weight]" dataDxfId="21"/>
+    <tableColumn id="9" name="[tidDescSingleRun]" dataDxfId="20"/>
+    <tableColumn id="10" name="[tidDescMultiRun]" dataDxfId="19"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table1330" displayName="Table1330" ref="B4:N45" totalsRowShown="0" headerRowDxfId="17" dataDxfId="15" headerRowBorderDxfId="16" tableBorderDxfId="14" totalsRowBorderDxfId="13">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table1330" displayName="Table1330" ref="B4:N45" totalsRowShown="0" headerRowDxfId="18" dataDxfId="16" headerRowBorderDxfId="17" tableBorderDxfId="15" totalsRowBorderDxfId="14">
   <autoFilter ref="B4:N45"/>
   <sortState ref="B5:P43">
     <sortCondition descending="1" ref="J4:J43"/>
   </sortState>
   <tableColumns count="13">
-    <tableColumn id="1" name="{missionsDefinitions}" dataDxfId="12"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="11"/>
-    <tableColumn id="7" name="[type]" dataDxfId="10"/>
-    <tableColumn id="8" name="[weight]" dataDxfId="9"/>
-    <tableColumn id="13" name="[singleRunChance]" dataDxfId="8"/>
-    <tableColumn id="11" name="[minTier]" dataDxfId="7"/>
-    <tableColumn id="12" name="[maxTier]" dataDxfId="6"/>
-    <tableColumn id="6" name="[params]" dataDxfId="5"/>
-    <tableColumn id="3" name="[objectiveBaseQuantityMin]" dataDxfId="4"/>
-    <tableColumn id="9" name="[objectiveBaseQuantityMax]" dataDxfId="3"/>
-    <tableColumn id="4" name="[icon]" dataDxfId="2"/>
-    <tableColumn id="5" name="[tidObjective]" dataDxfId="1"/>
-    <tableColumn id="10" name="[trackingSku]" dataDxfId="0">
-      <calculatedColumnFormula>[1]!Table1330[[#This Row],['[sku']]]</calculatedColumnFormula>
-    </tableColumn>
+    <tableColumn id="1" name="{missionsDefinitions}" dataDxfId="13"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="12"/>
+    <tableColumn id="7" name="[type]" dataDxfId="11"/>
+    <tableColumn id="8" name="[weight]" dataDxfId="10"/>
+    <tableColumn id="13" name="[singleRunChance]" dataDxfId="9"/>
+    <tableColumn id="11" name="[minTier]" dataDxfId="8"/>
+    <tableColumn id="12" name="[maxTier]" dataDxfId="7"/>
+    <tableColumn id="6" name="[params]" dataDxfId="6"/>
+    <tableColumn id="3" name="[objectiveBaseQuantityMin]" dataDxfId="5"/>
+    <tableColumn id="9" name="[objectiveBaseQuantityMax]" dataDxfId="4"/>
+    <tableColumn id="4" name="[icon]" dataDxfId="3"/>
+    <tableColumn id="5" name="[tidObjective]" dataDxfId="2"/>
+    <tableColumn id="10" name="[trackingSku]" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3582,10 +3572,10 @@
   <sheetPr>
     <tabColor theme="6"/>
   </sheetPr>
-  <dimension ref="B1:P181"/>
+  <dimension ref="B1:P180"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A151" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D185" sqref="D185"/>
+    <sheetView tabSelected="1" topLeftCell="A139" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N5" sqref="N5:N17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3632,16 +3622,16 @@
         <v>140</v>
       </c>
       <c r="G3" s="38"/>
-      <c r="J3" s="62" t="s">
+      <c r="J3" s="61" t="s">
         <v>139</v>
       </c>
-      <c r="K3" s="62"/>
-      <c r="M3" s="62"/>
-      <c r="N3" s="62"/>
-      <c r="O3" s="62"/>
-      <c r="P3" s="62"/>
-    </row>
-    <row r="4" spans="2:16" ht="106.5" x14ac:dyDescent="0.25">
+      <c r="K3" s="61"/>
+      <c r="M3" s="61"/>
+      <c r="N3" s="61"/>
+      <c r="O3" s="61"/>
+      <c r="P3" s="61"/>
+    </row>
+    <row r="4" spans="2:16" ht="107.25" x14ac:dyDescent="0.25">
       <c r="B4" s="30" t="s">
         <v>138</v>
       </c>
@@ -3719,9 +3709,8 @@
       <c r="M5" s="24" t="s">
         <v>147</v>
       </c>
-      <c r="N5" s="24" t="str">
-        <f>[1]!Table1330[[#This Row],['[sku']]]</f>
-        <v>ftux1</v>
+      <c r="N5" s="59" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="6" spans="2:16" x14ac:dyDescent="0.25">
@@ -3757,9 +3746,8 @@
         <v>109</v>
       </c>
       <c r="M6" s="24"/>
-      <c r="N6" s="24" t="str">
-        <f>[1]!Table1330[[#This Row],['[sku']]]</f>
-        <v>ftux2</v>
+      <c r="N6" s="60" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="7" spans="2:16" x14ac:dyDescent="0.25">
@@ -3795,9 +3783,8 @@
         <v>108</v>
       </c>
       <c r="M7" s="24"/>
-      <c r="N7" s="24" t="str">
-        <f>[1]!Table1330[[#This Row],['[sku']]]</f>
-        <v>ftux3</v>
+      <c r="N7" s="59" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="8" spans="2:16" x14ac:dyDescent="0.25">
@@ -3837,9 +3824,8 @@
       <c r="M8" s="24" t="s">
         <v>147</v>
       </c>
-      <c r="N8" s="24" t="str">
-        <f>[1]!Table1330[[#This Row],['[sku']]]</f>
-        <v>birds</v>
+      <c r="N8" s="60" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="9" spans="2:16" x14ac:dyDescent="0.25">
@@ -3877,9 +3863,8 @@
       <c r="M9" s="24" t="s">
         <v>149</v>
       </c>
-      <c r="N9" s="24" t="str">
-        <f>[1]!Table1330[[#This Row],['[sku']]]</f>
-        <v>villagers</v>
+      <c r="N9" s="59" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="10" spans="2:16" x14ac:dyDescent="0.25">
@@ -3917,10 +3902,7 @@
       <c r="M10" s="48" t="s">
         <v>150</v>
       </c>
-      <c r="N10" s="48" t="str">
-        <f>[1]!Table1330[[#This Row],['[sku']]]</f>
-        <v>small_decos</v>
-      </c>
+      <c r="N10" s="60"/>
     </row>
     <row r="11" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B11" s="27" t="s">
@@ -3959,9 +3941,8 @@
       <c r="M11" s="24" t="s">
         <v>152</v>
       </c>
-      <c r="N11" s="24" t="str">
-        <f>[1]!Table1330[[#This Row],['[sku']]]</f>
-        <v>coins</v>
+      <c r="N11" s="59" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="12" spans="2:16" x14ac:dyDescent="0.25">
@@ -4001,9 +3982,8 @@
       <c r="M12" s="24" t="s">
         <v>154</v>
       </c>
-      <c r="N12" s="24" t="str">
-        <f>[1]!Table1330[[#This Row],['[sku']]]</f>
-        <v>dragons</v>
+      <c r="N12" s="60" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="13" spans="2:16" x14ac:dyDescent="0.25">
@@ -4039,9 +4019,8 @@
         <v>246</v>
       </c>
       <c r="M13" s="24"/>
-      <c r="N13" s="24" t="str">
-        <f>[1]!Table1330[[#This Row],['[sku']]]</f>
-        <v>fire_rushes</v>
+      <c r="N13" s="60" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="14" spans="2:16" x14ac:dyDescent="0.25">
@@ -4077,9 +4056,8 @@
         <v>110</v>
       </c>
       <c r="M14" s="24"/>
-      <c r="N14" s="24" t="str">
-        <f>[1]!Table1330[[#This Row],['[sku']]]</f>
-        <v>dive</v>
+      <c r="N14" s="59" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="15" spans="2:16" x14ac:dyDescent="0.25">
@@ -4115,9 +4093,8 @@
         <v>109</v>
       </c>
       <c r="M15" s="24"/>
-      <c r="N15" s="24" t="str">
-        <f>[1]!Table1330[[#This Row],['[sku']]]</f>
-        <v>survive_time</v>
+      <c r="N15" s="60" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="16" spans="2:16" x14ac:dyDescent="0.25">
@@ -4153,9 +4130,8 @@
         <v>108</v>
       </c>
       <c r="M16" s="24"/>
-      <c r="N16" s="24" t="str">
-        <f>[1]!Table1330[[#This Row],['[sku']]]</f>
-        <v>score</v>
+      <c r="N16" s="59" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="17" spans="2:14" x14ac:dyDescent="0.25">
@@ -4195,9 +4171,8 @@
       <c r="M17" s="24" t="s">
         <v>156</v>
       </c>
-      <c r="N17" s="24" t="str">
-        <f>[1]!Table1330[[#This Row],['[sku']]]</f>
-        <v>spiders</v>
+      <c r="N17" s="60" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="18" spans="2:14" x14ac:dyDescent="0.25">
@@ -4237,9 +4212,8 @@
       <c r="M18" s="24" t="s">
         <v>155</v>
       </c>
-      <c r="N18" s="24" t="str">
-        <f>[1]!Table1330[[#This Row],['[sku']]]</f>
-        <v>goblins</v>
+      <c r="N18" s="60" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="19" spans="2:14" x14ac:dyDescent="0.25">
@@ -4279,9 +4253,8 @@
       <c r="M19" s="24" t="s">
         <v>158</v>
       </c>
-      <c r="N19" s="24" t="str">
-        <f>[1]!Table1330[[#This Row],['[sku']]]</f>
-        <v>bats</v>
+      <c r="N19" s="59" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="20" spans="2:14" x14ac:dyDescent="0.25">
@@ -4321,9 +4294,8 @@
       <c r="M20" s="24" t="s">
         <v>159</v>
       </c>
-      <c r="N20" s="24" t="str">
-        <f>[1]!Table1330[[#This Row],['[sku']]]</f>
-        <v>owls</v>
+      <c r="N20" s="60" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="21" spans="2:14" x14ac:dyDescent="0.25">
@@ -4363,9 +4335,8 @@
       <c r="M21" s="24" t="s">
         <v>160</v>
       </c>
-      <c r="N21" s="24" t="str">
-        <f>[1]!Table1330[[#This Row],['[sku']]]</f>
-        <v>lionbird</v>
+      <c r="N21" s="60" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="22" spans="2:14" x14ac:dyDescent="0.25">
@@ -4405,9 +4376,8 @@
       <c r="M22" s="24" t="s">
         <v>161</v>
       </c>
-      <c r="N22" s="24" t="str">
-        <f>[1]!Table1330[[#This Row],['[sku']]]</f>
-        <v>driller</v>
+      <c r="N22" s="59" t="s">
+        <v>194</v>
       </c>
     </row>
     <row r="23" spans="2:14" x14ac:dyDescent="0.25">
@@ -4447,9 +4417,8 @@
       <c r="M23" s="24" t="s">
         <v>216</v>
       </c>
-      <c r="N23" s="24" t="str">
-        <f>[1]!Table1330[[#This Row],['[sku']]]</f>
-        <v>boatFished</v>
+      <c r="N23" s="60" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="24" spans="2:14" x14ac:dyDescent="0.25">
@@ -4489,9 +4458,8 @@
       <c r="M24" s="24" t="s">
         <v>162</v>
       </c>
-      <c r="N24" s="24" t="str">
-        <f>[1]!Table1330[[#This Row],['[sku']]]</f>
-        <v>archers</v>
+      <c r="N24" s="59" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="25" spans="2:14" x14ac:dyDescent="0.25">
@@ -4531,9 +4499,8 @@
       <c r="M25" s="24" t="s">
         <v>163</v>
       </c>
-      <c r="N25" s="24" t="str">
-        <f>[1]!Table1330[[#This Row],['[sku']]]</f>
-        <v>soldiers</v>
+      <c r="N25" s="60" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="26" spans="2:14" x14ac:dyDescent="0.25">
@@ -4571,10 +4538,7 @@
       <c r="M26" s="48" t="s">
         <v>164</v>
       </c>
-      <c r="N26" s="48" t="str">
-        <f>[1]!Table1330[[#This Row],['[sku']]]</f>
-        <v>troll</v>
-      </c>
+      <c r="N26" s="59"/>
     </row>
     <row r="27" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B27" s="27" t="s">
@@ -4609,9 +4573,8 @@
         <v>73</v>
       </c>
       <c r="M27" s="24"/>
-      <c r="N27" s="24" t="str">
-        <f>[1]!Table1330[[#This Row],['[sku']]]</f>
-        <v>distance</v>
+      <c r="N27" s="60" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="28" spans="2:14" x14ac:dyDescent="0.25">
@@ -4649,10 +4612,7 @@
       <c r="M28" s="24" t="s">
         <v>156</v>
       </c>
-      <c r="N28" s="24" t="str">
-        <f>[1]!Table1330[[#This Row],['[sku']]]</f>
-        <v>eat_spec_anim_a_spiders</v>
-      </c>
+      <c r="N28" s="59"/>
     </row>
     <row r="29" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B29" s="27" t="s">
@@ -4689,9 +4649,8 @@
       <c r="M29" s="24" t="s">
         <v>213</v>
       </c>
-      <c r="N29" s="24" t="str">
-        <f>[1]!Table1330[[#This Row],['[sku']]]</f>
-        <v>eat_gold_gen</v>
+      <c r="N29" s="60" t="s">
+        <v>182</v>
       </c>
     </row>
     <row r="30" spans="2:14" x14ac:dyDescent="0.25">
@@ -4731,9 +4690,8 @@
       <c r="M30" s="24" t="s">
         <v>165</v>
       </c>
-      <c r="N30" s="24" t="str">
-        <f>[1]!Table1330[[#This Row],['[sku']]]</f>
-        <v>eat_gold_stingrays</v>
+      <c r="N30" s="59" t="s">
+        <v>190</v>
       </c>
     </row>
     <row r="31" spans="2:14" x14ac:dyDescent="0.25">
@@ -4773,9 +4731,8 @@
       <c r="M31" s="24" t="s">
         <v>212</v>
       </c>
-      <c r="N31" s="24" t="str">
-        <f>[1]!Table1330[[#This Row],['[sku']]]</f>
-        <v>eat_gold_cattle</v>
+      <c r="N31" s="60" t="s">
+        <v>188</v>
       </c>
     </row>
     <row r="32" spans="2:14" s="40" customFormat="1" x14ac:dyDescent="0.25">
@@ -4815,9 +4772,8 @@
       <c r="M32" s="24" t="s">
         <v>155</v>
       </c>
-      <c r="N32" s="24" t="str">
-        <f>[1]!Table1330[[#This Row],['[sku']]]</f>
-        <v>eat_gold_goblins</v>
+      <c r="N32" s="60" t="s">
+        <v>187</v>
       </c>
     </row>
     <row r="33" spans="2:14" s="40" customFormat="1" x14ac:dyDescent="0.25">
@@ -4851,10 +4807,7 @@
         <v>209</v>
       </c>
       <c r="M33" s="48"/>
-      <c r="N33" s="48" t="str">
-        <f>[1]!Table1330[[#This Row],['[sku']]]</f>
-        <v>critical_time</v>
-      </c>
+      <c r="N33" s="59"/>
     </row>
     <row r="34" spans="2:14" s="40" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B34" s="27" t="s">
@@ -4893,9 +4846,8 @@
       <c r="M34" s="24" t="s">
         <v>150</v>
       </c>
-      <c r="N34" s="24" t="str">
-        <f>[1]!Table1330[[#This Row],['[sku']]]</f>
-        <v>houses</v>
+      <c r="N34" s="60" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="35" spans="2:14" s="40" customFormat="1" x14ac:dyDescent="0.25">
@@ -4935,9 +4887,8 @@
       <c r="M35" s="24" t="s">
         <v>214</v>
       </c>
-      <c r="N35" s="24" t="str">
-        <f>[1]!Table1330[[#This Row],['[sku']]]</f>
-        <v>eat_gold_witch</v>
+      <c r="N35" s="59" t="s">
+        <v>195</v>
       </c>
     </row>
     <row r="36" spans="2:14" s="40" customFormat="1" x14ac:dyDescent="0.25">
@@ -4977,9 +4928,8 @@
       <c r="M36" s="24" t="s">
         <v>147</v>
       </c>
-      <c r="N36" s="24" t="str">
-        <f>[1]!Table1330[[#This Row],['[sku']]]</f>
-        <v>eat_gold_birds</v>
+      <c r="N36" s="60" t="s">
+        <v>186</v>
       </c>
     </row>
     <row r="37" spans="2:14" s="40" customFormat="1" x14ac:dyDescent="0.25">
@@ -5019,9 +4969,8 @@
       <c r="M37" s="24" t="s">
         <v>151</v>
       </c>
-      <c r="N37" s="24" t="str">
-        <f>[1]!Table1330[[#This Row],['[sku']]]</f>
-        <v>vulture</v>
+      <c r="N37" s="59" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="38" spans="2:14" s="40" customFormat="1" x14ac:dyDescent="0.25">
@@ -5059,10 +5008,7 @@
       <c r="M38" s="48" t="s">
         <v>147</v>
       </c>
-      <c r="N38" s="48" t="str">
-        <f>[1]!Table1330[[#This Row],['[sku']]]</f>
-        <v>kill_chain_canaries</v>
-      </c>
+      <c r="N38" s="60"/>
     </row>
     <row r="39" spans="2:14" s="40" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B39" s="47"/>
@@ -5099,10 +5045,7 @@
       <c r="M39" s="48" t="s">
         <v>149</v>
       </c>
-      <c r="N39" s="48" t="str">
-        <f>[1]!Table1330[[#This Row],['[sku']]]</f>
-        <v>kill_chain_humans</v>
-      </c>
+      <c r="N39" s="59"/>
     </row>
     <row r="40" spans="2:14" s="40" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B40" s="27" t="s">
@@ -5141,9 +5084,8 @@
       <c r="M40" s="24" t="s">
         <v>166</v>
       </c>
-      <c r="N40" s="24" t="str">
-        <f>[1]!Table1330[[#This Row],['[sku']]]</f>
-        <v>eat_gold_birdsOfPrey</v>
+      <c r="N40" s="60" t="s">
+        <v>189</v>
       </c>
     </row>
     <row r="41" spans="2:14" s="40" customFormat="1" x14ac:dyDescent="0.25">
@@ -5179,10 +5121,7 @@
         <v>208</v>
       </c>
       <c r="M41" s="48"/>
-      <c r="N41" s="48" t="str">
-        <f>[1]!Table1330[[#This Row],['[sku']]]</f>
-        <v>destroy_mineSmall</v>
-      </c>
+      <c r="N41" s="60"/>
     </row>
     <row r="42" spans="2:14" s="40" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B42" s="27" t="s">
@@ -5221,9 +5160,8 @@
       <c r="M42" s="24" t="s">
         <v>153</v>
       </c>
-      <c r="N42" s="24" t="str">
-        <f>[1]!Table1330[[#This Row],['[sku']]]</f>
-        <v>eggs</v>
+      <c r="N42" s="59" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="43" spans="2:14" s="40" customFormat="1" x14ac:dyDescent="0.25">
@@ -5263,9 +5201,8 @@
       <c r="M43" s="24" t="s">
         <v>157</v>
       </c>
-      <c r="N43" s="24" t="str">
-        <f>[1]!Table1330[[#This Row],['[sku']]]</f>
-        <v>flyingPig</v>
+      <c r="N43" s="60" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="44" spans="2:14" s="40" customFormat="1" x14ac:dyDescent="0.25">
@@ -5299,15 +5236,14 @@
       <c r="K44" s="23">
         <v>30</v>
       </c>
-      <c r="L44" s="59" t="s">
+      <c r="L44" s="58" t="s">
         <v>123</v>
       </c>
       <c r="M44" s="24" t="s">
         <v>462</v>
       </c>
-      <c r="N44" s="60" t="str">
-        <f>[1]!Table1330[[#This Row],['[sku']]]</f>
-        <v>halloween_zombie</v>
+      <c r="N44" s="59" t="s">
+        <v>484</v>
       </c>
     </row>
     <row r="45" spans="2:14" s="40" customFormat="1" x14ac:dyDescent="0.25">
@@ -5341,15 +5277,14 @@
       <c r="K45" s="23">
         <v>30</v>
       </c>
-      <c r="L45" s="58" t="s">
+      <c r="L45" s="57" t="s">
         <v>123</v>
       </c>
       <c r="M45" s="23" t="s">
         <v>466</v>
       </c>
-      <c r="N45" s="61" t="str">
-        <f>[1]!Table1330[[#This Row],['[sku']]]</f>
-        <v>halloween_creatures</v>
+      <c r="N45" s="60" t="s">
+        <v>485</v>
       </c>
     </row>
     <row r="46" spans="2:14" s="40" customFormat="1" x14ac:dyDescent="0.25">
@@ -5401,9 +5336,9 @@
       <c r="C49" s="20"/>
       <c r="D49" s="20"/>
       <c r="E49" s="20"/>
-      <c r="F49" s="63"/>
-      <c r="G49" s="63"/>
-      <c r="H49" s="63"/>
+      <c r="F49" s="62"/>
+      <c r="G49" s="62"/>
+      <c r="H49" s="62"/>
       <c r="I49" s="20"/>
       <c r="J49" s="20"/>
     </row>
@@ -5908,25 +5843,25 @@
       <c r="H71" s="26"/>
     </row>
     <row r="72" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B72" s="53" t="s">
-        <v>1</v>
-      </c>
-      <c r="C72" s="53" t="s">
+      <c r="B72" s="66" t="s">
+        <v>1</v>
+      </c>
+      <c r="C72" s="64" t="s">
         <v>464</v>
       </c>
-      <c r="D72" s="53">
-        <v>0</v>
-      </c>
-      <c r="E72" s="53">
+      <c r="D72" s="64">
+        <v>0</v>
+      </c>
+      <c r="E72" s="64">
         <v>7</v>
       </c>
-      <c r="F72" s="53">
+      <c r="F72" s="64">
         <v>2</v>
       </c>
-      <c r="G72" s="57" t="s">
+      <c r="G72" s="65" t="s">
         <v>467</v>
       </c>
-      <c r="H72" s="53" t="s">
+      <c r="H72" s="65" t="s">
         <v>468</v>
       </c>
     </row>
@@ -5955,10 +5890,10 @@
       <c r="F75" s="21" t="s">
         <v>40</v>
       </c>
-      <c r="G75" s="64" t="s">
+      <c r="G75" s="63" t="s">
         <v>39</v>
       </c>
-      <c r="H75" s="64"/>
+      <c r="H75" s="63"/>
       <c r="I75" s="20"/>
     </row>
     <row r="76" spans="2:13" ht="142.5" x14ac:dyDescent="0.25">
@@ -7306,10 +7241,10 @@
         <v>1</v>
       </c>
       <c r="C176" s="46" t="s">
-        <v>105</v>
+        <v>74</v>
       </c>
       <c r="D176" s="46" t="s">
-        <v>295</v>
+        <v>476</v>
       </c>
       <c r="E176" s="43" t="b">
         <v>1</v>
@@ -7320,10 +7255,10 @@
         <v>1</v>
       </c>
       <c r="C177" s="46" t="s">
-        <v>74</v>
+        <v>481</v>
       </c>
       <c r="D177" s="46" t="s">
-        <v>476</v>
+        <v>477</v>
       </c>
       <c r="E177" s="43" t="b">
         <v>1</v>
@@ -7334,10 +7269,10 @@
         <v>1</v>
       </c>
       <c r="C178" s="46" t="s">
-        <v>481</v>
+        <v>482</v>
       </c>
       <c r="D178" s="46" t="s">
-        <v>477</v>
+        <v>478</v>
       </c>
       <c r="E178" s="43" t="b">
         <v>1</v>
@@ -7348,10 +7283,10 @@
         <v>1</v>
       </c>
       <c r="C179" s="46" t="s">
-        <v>482</v>
+        <v>430</v>
       </c>
       <c r="D179" s="46" t="s">
-        <v>478</v>
+        <v>479</v>
       </c>
       <c r="E179" s="43" t="b">
         <v>1</v>
@@ -7362,26 +7297,12 @@
         <v>1</v>
       </c>
       <c r="C180" s="46" t="s">
-        <v>430</v>
+        <v>483</v>
       </c>
       <c r="D180" s="46" t="s">
-        <v>479</v>
+        <v>480</v>
       </c>
       <c r="E180" s="43" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="181" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B181" s="43" t="s">
-        <v>1</v>
-      </c>
-      <c r="C181" s="46" t="s">
-        <v>483</v>
-      </c>
-      <c r="D181" s="46" t="s">
-        <v>480</v>
-      </c>
-      <c r="E181" s="43" t="b">
         <v>1</v>
       </c>
     </row>
@@ -7393,7 +7314,7 @@
     <mergeCell ref="G75:H75"/>
   </mergeCells>
   <conditionalFormatting sqref="C77:E79">
-    <cfRule type="duplicateValues" dxfId="68" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Review FTUX missions. Now, 'easy' mission can be easily completed in 1 run, while 'hard' mission is a bit harder
Former-commit-id: 9321367be382403defb61d410839af757bacd225
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Missions.xlsx
+++ b/Docs/Content/HungryDragonContent_Missions.xlsx
@@ -2013,13 +2013,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2028,6 +2021,13 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2057,16 +2057,6 @@
           <color indexed="64"/>
         </horizontal>
       </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -3194,6 +3184,16 @@
         </bottom>
       </border>
     </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -3208,98 +3208,98 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="missionDifficultyDefinitions" displayName="missionDifficultyDefinitions" ref="B76:L79" totalsRowShown="0" headerRowBorderDxfId="68" tableBorderDxfId="67">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="missionDifficultyDefinitions" displayName="missionDifficultyDefinitions" ref="B76:L79" totalsRowShown="0" headerRowBorderDxfId="67" tableBorderDxfId="66">
   <autoFilter ref="B76:L79"/>
   <tableColumns count="11">
     <tableColumn id="1" name="{missionDifficultyDefinitions}"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="66"/>
-    <tableColumn id="11" name="[difficulty]" dataDxfId="65"/>
-    <tableColumn id="7" name="[index]" dataDxfId="64"/>
-    <tableColumn id="3" name="[dragonsToUnlock]" dataDxfId="63"/>
-    <tableColumn id="4" name="[cooldownMinutes]" dataDxfId="62"/>
-    <tableColumn id="9" name="[maxRewardCoins]" dataDxfId="61"/>
-    <tableColumn id="5" name="[removeMissionPCCoefA]" dataDxfId="60"/>
-    <tableColumn id="6" name="[removeMissionPCCoefB]" dataDxfId="59"/>
-    <tableColumn id="8" name="[tidName]" dataDxfId="58"/>
-    <tableColumn id="10" name="[color]" dataDxfId="57"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="65"/>
+    <tableColumn id="11" name="[difficulty]" dataDxfId="64"/>
+    <tableColumn id="7" name="[index]" dataDxfId="63"/>
+    <tableColumn id="3" name="[dragonsToUnlock]" dataDxfId="62"/>
+    <tableColumn id="4" name="[cooldownMinutes]" dataDxfId="61"/>
+    <tableColumn id="9" name="[maxRewardCoins]" dataDxfId="60"/>
+    <tableColumn id="5" name="[removeMissionPCCoefA]" dataDxfId="59"/>
+    <tableColumn id="6" name="[removeMissionPCCoefB]" dataDxfId="58"/>
+    <tableColumn id="8" name="[tidName]" dataDxfId="57"/>
+    <tableColumn id="10" name="[color]" dataDxfId="56"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table13303132" displayName="Table13303132" ref="B84:E102" totalsRowShown="0" headerRowDxfId="56" dataDxfId="54" headerRowBorderDxfId="55" tableBorderDxfId="53" totalsRowBorderDxfId="52">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table13303132" displayName="Table13303132" ref="B84:E102" totalsRowShown="0" headerRowDxfId="55" dataDxfId="53" headerRowBorderDxfId="54" tableBorderDxfId="52" totalsRowBorderDxfId="51">
   <autoFilter ref="B84:E102"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="{missionDragonModifiersDefinitions}" dataDxfId="51"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="50"/>
-    <tableColumn id="7" name="[quantityModifier]" dataDxfId="49"/>
-    <tableColumn id="3" name="[missionSCRewardMultiplier]" dataDxfId="48"/>
+    <tableColumn id="1" name="{missionDragonModifiersDefinitions}" dataDxfId="50"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="49"/>
+    <tableColumn id="7" name="[quantityModifier]" dataDxfId="48"/>
+    <tableColumn id="3" name="[missionSCRewardMultiplier]" dataDxfId="47"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table1330313234" displayName="Table1330313234" ref="B106:E109" totalsRowShown="0" headerRowDxfId="47" dataDxfId="45" headerRowBorderDxfId="46" tableBorderDxfId="44" totalsRowBorderDxfId="43">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table1330313234" displayName="Table1330313234" ref="B106:E109" totalsRowShown="0" headerRowDxfId="46" dataDxfId="44" headerRowBorderDxfId="45" tableBorderDxfId="43" totalsRowBorderDxfId="42">
   <autoFilter ref="B106:E109"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="{missionDifficultyModifiersDefinitions}" dataDxfId="42"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="41"/>
-    <tableColumn id="3" name="[difficulty]" dataDxfId="40"/>
-    <tableColumn id="7" name="[quantityModifier]" dataDxfId="39"/>
+    <tableColumn id="1" name="{missionDifficultyModifiersDefinitions}" dataDxfId="41"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="40"/>
+    <tableColumn id="3" name="[difficulty]" dataDxfId="39"/>
+    <tableColumn id="7" name="[quantityModifier]" dataDxfId="38"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table133031323435" displayName="Table133031323435" ref="B113:D114" totalsRowShown="0" headerRowDxfId="38" dataDxfId="36" headerRowBorderDxfId="37" tableBorderDxfId="35" totalsRowBorderDxfId="34">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table133031323435" displayName="Table133031323435" ref="B113:D114" totalsRowShown="0" headerRowDxfId="37" dataDxfId="35" headerRowBorderDxfId="36" tableBorderDxfId="34" totalsRowBorderDxfId="33">
   <autoFilter ref="B113:D114"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="{missionOtherModifiersDefinitions}" dataDxfId="33"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="32"/>
-    <tableColumn id="7" name="[quantityModifier]" dataDxfId="31"/>
+    <tableColumn id="1" name="{missionOtherModifiersDefinitions}" dataDxfId="32"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="31"/>
+    <tableColumn id="7" name="[quantityModifier]" dataDxfId="30"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table13" displayName="Table13" ref="B50:H72" totalsRowShown="0" headerRowDxfId="30" dataDxfId="28" headerRowBorderDxfId="29" tableBorderDxfId="27" totalsRowBorderDxfId="26">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table13" displayName="Table13" ref="B50:H72" totalsRowShown="0" headerRowDxfId="29" dataDxfId="27" headerRowBorderDxfId="28" tableBorderDxfId="26" totalsRowBorderDxfId="25">
   <autoFilter ref="B50:H72"/>
   <tableColumns count="7">
-    <tableColumn id="1" name="{missionTypeDefinitions}" dataDxfId="25"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="24"/>
-    <tableColumn id="3" name="[minTier]" dataDxfId="23"/>
-    <tableColumn id="6" name="[maxTier]" dataDxfId="22"/>
-    <tableColumn id="4" name="[weight]" dataDxfId="21"/>
-    <tableColumn id="9" name="[tidDescSingleRun]" dataDxfId="20"/>
-    <tableColumn id="10" name="[tidDescMultiRun]" dataDxfId="19"/>
+    <tableColumn id="1" name="{missionTypeDefinitions}" dataDxfId="24"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="23"/>
+    <tableColumn id="3" name="[minTier]" dataDxfId="22"/>
+    <tableColumn id="6" name="[maxTier]" dataDxfId="21"/>
+    <tableColumn id="4" name="[weight]" dataDxfId="20"/>
+    <tableColumn id="9" name="[tidDescSingleRun]" dataDxfId="19"/>
+    <tableColumn id="10" name="[tidDescMultiRun]" dataDxfId="18"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table1330" displayName="Table1330" ref="B4:N45" totalsRowShown="0" headerRowDxfId="18" dataDxfId="16" headerRowBorderDxfId="17" tableBorderDxfId="15" totalsRowBorderDxfId="14">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table1330" displayName="Table1330" ref="B4:N45" totalsRowShown="0" headerRowDxfId="17" dataDxfId="15" headerRowBorderDxfId="16" tableBorderDxfId="14" totalsRowBorderDxfId="13">
   <autoFilter ref="B4:N45"/>
   <sortState ref="B5:P43">
     <sortCondition descending="1" ref="J4:J43"/>
   </sortState>
   <tableColumns count="13">
-    <tableColumn id="1" name="{missionsDefinitions}" dataDxfId="13"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="12"/>
-    <tableColumn id="7" name="[type]" dataDxfId="11"/>
-    <tableColumn id="8" name="[weight]" dataDxfId="10"/>
-    <tableColumn id="13" name="[singleRunChance]" dataDxfId="9"/>
-    <tableColumn id="11" name="[minTier]" dataDxfId="8"/>
-    <tableColumn id="12" name="[maxTier]" dataDxfId="7"/>
-    <tableColumn id="6" name="[params]" dataDxfId="6"/>
-    <tableColumn id="3" name="[objectiveBaseQuantityMin]" dataDxfId="5"/>
-    <tableColumn id="9" name="[objectiveBaseQuantityMax]" dataDxfId="4"/>
-    <tableColumn id="4" name="[icon]" dataDxfId="3"/>
-    <tableColumn id="5" name="[tidObjective]" dataDxfId="2"/>
+    <tableColumn id="1" name="{missionsDefinitions}" dataDxfId="12"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="11"/>
+    <tableColumn id="7" name="[type]" dataDxfId="10"/>
+    <tableColumn id="8" name="[weight]" dataDxfId="9"/>
+    <tableColumn id="13" name="[singleRunChance]" dataDxfId="8"/>
+    <tableColumn id="11" name="[minTier]" dataDxfId="7"/>
+    <tableColumn id="12" name="[maxTier]" dataDxfId="6"/>
+    <tableColumn id="6" name="[params]" dataDxfId="5"/>
+    <tableColumn id="3" name="[objectiveBaseQuantityMin]" dataDxfId="4"/>
+    <tableColumn id="9" name="[objectiveBaseQuantityMax]" dataDxfId="3"/>
+    <tableColumn id="4" name="[icon]" dataDxfId="2"/>
+    <tableColumn id="5" name="[tidObjective]" dataDxfId="1"/>
     <tableColumn id="10" name="[trackingSku]" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -3574,8 +3574,8 @@
   </sheetPr>
   <dimension ref="B1:P180"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A139" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N5" sqref="N5:N17"/>
+    <sheetView tabSelected="1" topLeftCell="D4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3622,14 +3622,14 @@
         <v>140</v>
       </c>
       <c r="G3" s="38"/>
-      <c r="J3" s="61" t="s">
+      <c r="J3" s="64" t="s">
         <v>139</v>
       </c>
-      <c r="K3" s="61"/>
-      <c r="M3" s="61"/>
-      <c r="N3" s="61"/>
-      <c r="O3" s="61"/>
-      <c r="P3" s="61"/>
+      <c r="K3" s="64"/>
+      <c r="M3" s="64"/>
+      <c r="N3" s="64"/>
+      <c r="O3" s="64"/>
+      <c r="P3" s="64"/>
     </row>
     <row r="4" spans="2:16" ht="107.25" x14ac:dyDescent="0.25">
       <c r="B4" s="30" t="s">
@@ -3686,7 +3686,7 @@
         <v>0</v>
       </c>
       <c r="F5" s="24">
-        <v>0.3</v>
+        <v>1</v>
       </c>
       <c r="G5" s="24">
         <v>0</v>
@@ -3698,10 +3698,10 @@
         <v>126</v>
       </c>
       <c r="J5" s="24">
-        <v>500</v>
+        <v>120</v>
       </c>
       <c r="K5" s="33">
-        <v>600</v>
+        <v>120</v>
       </c>
       <c r="L5" s="24" t="s">
         <v>125</v>
@@ -3764,7 +3764,7 @@
         <v>0</v>
       </c>
       <c r="F7" s="24">
-        <v>0.3</v>
+        <v>0</v>
       </c>
       <c r="G7" s="24">
         <v>0</v>
@@ -3774,10 +3774,10 @@
       </c>
       <c r="I7" s="24"/>
       <c r="J7" s="24">
-        <v>10000</v>
+        <v>28000</v>
       </c>
       <c r="K7" s="33">
-        <v>10000</v>
+        <v>28000</v>
       </c>
       <c r="L7" s="24" t="s">
         <v>108</v>
@@ -5336,9 +5336,9 @@
       <c r="C49" s="20"/>
       <c r="D49" s="20"/>
       <c r="E49" s="20"/>
-      <c r="F49" s="62"/>
-      <c r="G49" s="62"/>
-      <c r="H49" s="62"/>
+      <c r="F49" s="65"/>
+      <c r="G49" s="65"/>
+      <c r="H49" s="65"/>
       <c r="I49" s="20"/>
       <c r="J49" s="20"/>
     </row>
@@ -5843,25 +5843,25 @@
       <c r="H71" s="26"/>
     </row>
     <row r="72" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B72" s="66" t="s">
-        <v>1</v>
-      </c>
-      <c r="C72" s="64" t="s">
+      <c r="B72" s="63" t="s">
+        <v>1</v>
+      </c>
+      <c r="C72" s="61" t="s">
         <v>464</v>
       </c>
-      <c r="D72" s="64">
-        <v>0</v>
-      </c>
-      <c r="E72" s="64">
+      <c r="D72" s="61">
+        <v>0</v>
+      </c>
+      <c r="E72" s="61">
         <v>7</v>
       </c>
-      <c r="F72" s="64">
+      <c r="F72" s="61">
         <v>2</v>
       </c>
-      <c r="G72" s="65" t="s">
+      <c r="G72" s="62" t="s">
         <v>467</v>
       </c>
-      <c r="H72" s="65" t="s">
+      <c r="H72" s="62" t="s">
         <v>468</v>
       </c>
     </row>
@@ -5890,10 +5890,10 @@
       <c r="F75" s="21" t="s">
         <v>40</v>
       </c>
-      <c r="G75" s="63" t="s">
+      <c r="G75" s="66" t="s">
         <v>39</v>
       </c>
-      <c r="H75" s="63"/>
+      <c r="H75" s="66"/>
       <c r="I75" s="20"/>
     </row>
     <row r="76" spans="2:13" ht="142.5" x14ac:dyDescent="0.25">
@@ -7314,7 +7314,7 @@
     <mergeCell ref="G75:H75"/>
   </mergeCells>
   <conditionalFormatting sqref="C77:E79">
-    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="68" priority="2"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Reduced quantity requiered for killing birds
Former-commit-id: e86732fd1460cf2f01e7478b2332992bd660dc2e
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Missions.xlsx
+++ b/Docs/Content/HungryDragonContent_Missions.xlsx
@@ -3574,8 +3574,8 @@
   </sheetPr>
   <dimension ref="B1:P180"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3813,10 +3813,10 @@
         <v>126</v>
       </c>
       <c r="J8" s="24">
+        <v>600</v>
+      </c>
+      <c r="K8" s="33">
         <v>700</v>
-      </c>
-      <c r="K8" s="33">
-        <v>750</v>
       </c>
       <c r="L8" s="24" t="s">
         <v>125</v>

</xml_diff>

<commit_message>
Fixing some missions quantities values
Former-commit-id: 3c54b6663be9ee55018d147010b0b9feb6a26f77
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Missions.xlsx
+++ b/Docs/Content/HungryDragonContent_Missions.xlsx
@@ -3575,7 +3575,7 @@
   <dimension ref="B1:P180"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+      <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3816,7 +3816,7 @@
         <v>600</v>
       </c>
       <c r="K8" s="33">
-        <v>700</v>
+        <v>650</v>
       </c>
       <c r="L8" s="24" t="s">
         <v>125</v>

</xml_diff>

<commit_message>
Reduced quantity modifier multiplier for Legendary dragons
Former-commit-id: 9d7295ffebb2eab32b8c4a4329525ff7d5fe331c
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Missions.xlsx
+++ b/Docs/Content/HungryDragonContent_Missions.xlsx
@@ -3574,8 +3574,8 @@
   </sheetPr>
   <dimension ref="B1:P180"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+    <sheetView tabSelected="1" topLeftCell="A85" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D101" sqref="D101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6047,7 +6047,7 @@
       <c r="F82" s="6"/>
       <c r="G82" s="6"/>
     </row>
-    <row r="84" spans="2:7" ht="135.75" x14ac:dyDescent="0.25">
+    <row r="84" spans="2:7" ht="135" x14ac:dyDescent="0.25">
       <c r="B84" s="5" t="s">
         <v>22</v>
       </c>
@@ -6251,7 +6251,7 @@
         <v>469</v>
       </c>
       <c r="D98" s="42">
-        <v>8.5</v>
+        <v>8.1</v>
       </c>
       <c r="E98" s="42">
         <v>75</v>
@@ -6265,7 +6265,7 @@
         <v>470</v>
       </c>
       <c r="D99" s="42">
-        <v>8.5</v>
+        <v>8</v>
       </c>
       <c r="E99" s="42">
         <v>75</v>
@@ -6279,7 +6279,7 @@
         <v>471</v>
       </c>
       <c r="D100" s="42">
-        <v>8.5</v>
+        <v>7.5</v>
       </c>
       <c r="E100" s="42">
         <v>75</v>
@@ -6293,7 +6293,7 @@
         <v>472</v>
       </c>
       <c r="D101" s="42">
-        <v>8.5</v>
+        <v>8</v>
       </c>
       <c r="E101" s="42">
         <v>75</v>
@@ -6307,7 +6307,7 @@
         <v>473</v>
       </c>
       <c r="D102" s="42">
-        <v>8.5</v>
+        <v>7.5</v>
       </c>
       <c r="E102" s="42">
         <v>75</v>
@@ -6391,7 +6391,7 @@
       <c r="F111" s="6"/>
       <c r="G111" s="6"/>
     </row>
-    <row r="113" spans="2:7" ht="132" x14ac:dyDescent="0.25">
+    <row r="113" spans="2:7" ht="131.25" x14ac:dyDescent="0.25">
       <c r="B113" s="5" t="s">
         <v>4</v>
       </c>

</xml_diff>

<commit_message>
deleted mission of zombies and mixed with custome/disguised mission
Former-commit-id: 6ac3df468e23ce7a271a3bc0fe2977df3e20cbf8
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Missions.xlsx
+++ b/Docs/Content/HungryDragonContent_Missions.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\dragon\Docs\Content\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\dragon\client\Docs\Content\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="645" uniqueCount="353">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="644" uniqueCount="353">
   <si>
     <t>single_run</t>
   </si>
@@ -1071,9 +1071,6 @@
     <t>kill_disguise</t>
   </si>
   <si>
-    <t>Villager02;Villager03;Villager04;Worker01;Worker02;WorkerWife;Troll;Cow;Horse;Sheep;EnemyTier0;EnemyTier1;EnemyTier2;EnemyTier3;EnemyTier4;EnemyTier5</t>
-  </si>
-  <si>
     <t>TID_ENTITY_DISGUISE_HALLOWEEN</t>
   </si>
   <si>
@@ -1132,6 +1129,9 @@
   </si>
   <si>
     <t>halloween</t>
+  </si>
+  <si>
+    <t>Villager02;Villager03;Villager04;Worker01;Worker02;WorkerWife;Troll;Cow;Horse;Sheep;EnemyTier0;EnemyTier1;EnemyTier2;EnemyTier3;EnemyTier4;EnemyTier5;Villager01;BakerWoman;BoatFisher;Ground_Zombie</t>
   </si>
 </sst>
 </file>
@@ -1456,7 +1456,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1"/>
@@ -1579,9 +1579,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3149,8 +3146,8 @@
   </sheetPr>
   <dimension ref="B1:P180"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A70" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D90" sqref="D90"/>
+    <sheetView tabSelected="1" topLeftCell="F16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I45" sqref="I45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3197,14 +3194,14 @@
         <v>140</v>
       </c>
       <c r="G3" s="38"/>
-      <c r="J3" s="58" t="s">
+      <c r="J3" s="57" t="s">
         <v>139</v>
       </c>
-      <c r="K3" s="58"/>
-      <c r="M3" s="58"/>
-      <c r="N3" s="58"/>
-      <c r="O3" s="58"/>
-      <c r="P3" s="58"/>
+      <c r="K3" s="57"/>
+      <c r="M3" s="57"/>
+      <c r="N3" s="57"/>
+      <c r="O3" s="57"/>
+      <c r="P3" s="57"/>
     </row>
     <row r="4" spans="2:16" ht="107.25" x14ac:dyDescent="0.25">
       <c r="B4" s="30" t="s">
@@ -3284,7 +3281,7 @@
       <c r="M5" s="24" t="s">
         <v>147</v>
       </c>
-      <c r="N5" s="53" t="s">
+      <c r="N5" s="52" t="s">
         <v>130</v>
       </c>
     </row>
@@ -3321,7 +3318,7 @@
         <v>109</v>
       </c>
       <c r="M6" s="24"/>
-      <c r="N6" s="54" t="s">
+      <c r="N6" s="53" t="s">
         <v>129</v>
       </c>
     </row>
@@ -3358,7 +3355,7 @@
         <v>108</v>
       </c>
       <c r="M7" s="24"/>
-      <c r="N7" s="53" t="s">
+      <c r="N7" s="52" t="s">
         <v>128</v>
       </c>
     </row>
@@ -3399,7 +3396,7 @@
       <c r="M8" s="24" t="s">
         <v>147</v>
       </c>
-      <c r="N8" s="54" t="s">
+      <c r="N8" s="53" t="s">
         <v>127</v>
       </c>
     </row>
@@ -3438,7 +3435,7 @@
       <c r="M9" s="24" t="s">
         <v>149</v>
       </c>
-      <c r="N9" s="53" t="s">
+      <c r="N9" s="52" t="s">
         <v>124</v>
       </c>
     </row>
@@ -3477,7 +3474,7 @@
       <c r="M10" s="48" t="s">
         <v>150</v>
       </c>
-      <c r="N10" s="54"/>
+      <c r="N10" s="53"/>
     </row>
     <row r="11" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B11" s="27" t="s">
@@ -3516,7 +3513,7 @@
       <c r="M11" s="24" t="s">
         <v>152</v>
       </c>
-      <c r="N11" s="53" t="s">
+      <c r="N11" s="52" t="s">
         <v>117</v>
       </c>
     </row>
@@ -3557,7 +3554,7 @@
       <c r="M12" s="24" t="s">
         <v>154</v>
       </c>
-      <c r="N12" s="54" t="s">
+      <c r="N12" s="53" t="s">
         <v>113</v>
       </c>
     </row>
@@ -3594,7 +3591,7 @@
         <v>246</v>
       </c>
       <c r="M13" s="24"/>
-      <c r="N13" s="54" t="s">
+      <c r="N13" s="53" t="s">
         <v>111</v>
       </c>
     </row>
@@ -3631,7 +3628,7 @@
         <v>110</v>
       </c>
       <c r="M14" s="24"/>
-      <c r="N14" s="53" t="s">
+      <c r="N14" s="52" t="s">
         <v>44</v>
       </c>
     </row>
@@ -3668,7 +3665,7 @@
         <v>109</v>
       </c>
       <c r="M15" s="24"/>
-      <c r="N15" s="54" t="s">
+      <c r="N15" s="53" t="s">
         <v>53</v>
       </c>
     </row>
@@ -3705,7 +3702,7 @@
         <v>108</v>
       </c>
       <c r="M16" s="24"/>
-      <c r="N16" s="53" t="s">
+      <c r="N16" s="52" t="s">
         <v>59</v>
       </c>
     </row>
@@ -3746,7 +3743,7 @@
       <c r="M17" s="24" t="s">
         <v>156</v>
       </c>
-      <c r="N17" s="54" t="s">
+      <c r="N17" s="53" t="s">
         <v>107</v>
       </c>
     </row>
@@ -3787,7 +3784,7 @@
       <c r="M18" s="24" t="s">
         <v>155</v>
       </c>
-      <c r="N18" s="54" t="s">
+      <c r="N18" s="53" t="s">
         <v>104</v>
       </c>
     </row>
@@ -3828,7 +3825,7 @@
       <c r="M19" s="24" t="s">
         <v>158</v>
       </c>
-      <c r="N19" s="53" t="s">
+      <c r="N19" s="52" t="s">
         <v>95</v>
       </c>
     </row>
@@ -3869,7 +3866,7 @@
       <c r="M20" s="24" t="s">
         <v>159</v>
       </c>
-      <c r="N20" s="54" t="s">
+      <c r="N20" s="53" t="s">
         <v>92</v>
       </c>
     </row>
@@ -3910,7 +3907,7 @@
       <c r="M21" s="24" t="s">
         <v>160</v>
       </c>
-      <c r="N21" s="54" t="s">
+      <c r="N21" s="53" t="s">
         <v>90</v>
       </c>
     </row>
@@ -3951,7 +3948,7 @@
       <c r="M22" s="24" t="s">
         <v>161</v>
       </c>
-      <c r="N22" s="53" t="s">
+      <c r="N22" s="52" t="s">
         <v>194</v>
       </c>
     </row>
@@ -3992,7 +3989,7 @@
       <c r="M23" s="24" t="s">
         <v>216</v>
       </c>
-      <c r="N23" s="54" t="s">
+      <c r="N23" s="53" t="s">
         <v>85</v>
       </c>
     </row>
@@ -4033,7 +4030,7 @@
       <c r="M24" s="24" t="s">
         <v>162</v>
       </c>
-      <c r="N24" s="53" t="s">
+      <c r="N24" s="52" t="s">
         <v>82</v>
       </c>
     </row>
@@ -4074,7 +4071,7 @@
       <c r="M25" s="24" t="s">
         <v>163</v>
       </c>
-      <c r="N25" s="54" t="s">
+      <c r="N25" s="53" t="s">
         <v>79</v>
       </c>
     </row>
@@ -4113,7 +4110,7 @@
       <c r="M26" s="48" t="s">
         <v>164</v>
       </c>
-      <c r="N26" s="53"/>
+      <c r="N26" s="52"/>
     </row>
     <row r="27" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B27" s="27" t="s">
@@ -4148,7 +4145,7 @@
         <v>73</v>
       </c>
       <c r="M27" s="24"/>
-      <c r="N27" s="54" t="s">
+      <c r="N27" s="53" t="s">
         <v>47</v>
       </c>
     </row>
@@ -4187,7 +4184,7 @@
       <c r="M28" s="24" t="s">
         <v>156</v>
       </c>
-      <c r="N28" s="53"/>
+      <c r="N28" s="52"/>
     </row>
     <row r="29" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B29" s="27" t="s">
@@ -4224,7 +4221,7 @@
       <c r="M29" s="24" t="s">
         <v>213</v>
       </c>
-      <c r="N29" s="54" t="s">
+      <c r="N29" s="53" t="s">
         <v>182</v>
       </c>
     </row>
@@ -4265,7 +4262,7 @@
       <c r="M30" s="24" t="s">
         <v>165</v>
       </c>
-      <c r="N30" s="53" t="s">
+      <c r="N30" s="52" t="s">
         <v>190</v>
       </c>
     </row>
@@ -4306,7 +4303,7 @@
       <c r="M31" s="24" t="s">
         <v>212</v>
       </c>
-      <c r="N31" s="54" t="s">
+      <c r="N31" s="53" t="s">
         <v>188</v>
       </c>
     </row>
@@ -4347,7 +4344,7 @@
       <c r="M32" s="24" t="s">
         <v>155</v>
       </c>
-      <c r="N32" s="54" t="s">
+      <c r="N32" s="53" t="s">
         <v>187</v>
       </c>
     </row>
@@ -4382,7 +4379,7 @@
         <v>209</v>
       </c>
       <c r="M33" s="48"/>
-      <c r="N33" s="53"/>
+      <c r="N33" s="52"/>
     </row>
     <row r="34" spans="2:14" s="40" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B34" s="27" t="s">
@@ -4421,7 +4418,7 @@
       <c r="M34" s="24" t="s">
         <v>150</v>
       </c>
-      <c r="N34" s="54" t="s">
+      <c r="N34" s="53" t="s">
         <v>122</v>
       </c>
     </row>
@@ -4462,7 +4459,7 @@
       <c r="M35" s="24" t="s">
         <v>214</v>
       </c>
-      <c r="N35" s="53" t="s">
+      <c r="N35" s="52" t="s">
         <v>195</v>
       </c>
     </row>
@@ -4503,7 +4500,7 @@
       <c r="M36" s="24" t="s">
         <v>147</v>
       </c>
-      <c r="N36" s="54" t="s">
+      <c r="N36" s="53" t="s">
         <v>186</v>
       </c>
     </row>
@@ -4544,7 +4541,7 @@
       <c r="M37" s="24" t="s">
         <v>151</v>
       </c>
-      <c r="N37" s="53" t="s">
+      <c r="N37" s="52" t="s">
         <v>101</v>
       </c>
     </row>
@@ -4583,7 +4580,7 @@
       <c r="M38" s="48" t="s">
         <v>147</v>
       </c>
-      <c r="N38" s="54"/>
+      <c r="N38" s="53"/>
     </row>
     <row r="39" spans="2:14" s="40" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B39" s="47"/>
@@ -4620,7 +4617,7 @@
       <c r="M39" s="48" t="s">
         <v>149</v>
       </c>
-      <c r="N39" s="53"/>
+      <c r="N39" s="52"/>
     </row>
     <row r="40" spans="2:14" s="40" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B40" s="27" t="s">
@@ -4659,7 +4656,7 @@
       <c r="M40" s="24" t="s">
         <v>166</v>
       </c>
-      <c r="N40" s="54" t="s">
+      <c r="N40" s="53" t="s">
         <v>189</v>
       </c>
     </row>
@@ -4696,7 +4693,7 @@
         <v>208</v>
       </c>
       <c r="M41" s="48"/>
-      <c r="N41" s="54"/>
+      <c r="N41" s="53"/>
     </row>
     <row r="42" spans="2:14" s="40" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B42" s="27" t="s">
@@ -4735,7 +4732,7 @@
       <c r="M42" s="24" t="s">
         <v>153</v>
       </c>
-      <c r="N42" s="53" t="s">
+      <c r="N42" s="52" t="s">
         <v>115</v>
       </c>
     </row>
@@ -4776,49 +4773,47 @@
       <c r="M43" s="24" t="s">
         <v>157</v>
       </c>
-      <c r="N43" s="54" t="s">
+      <c r="N43" s="53" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="44" spans="2:14" s="40" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B44" s="27" t="s">
-        <v>1</v>
-      </c>
-      <c r="C44" s="24" t="s">
+      <c r="B44" s="47"/>
+      <c r="C44" s="48" t="s">
         <v>327</v>
       </c>
-      <c r="D44" s="23" t="s">
+      <c r="D44" s="49" t="s">
         <v>65</v>
       </c>
-      <c r="E44" s="23">
-        <v>1</v>
-      </c>
-      <c r="F44" s="23">
+      <c r="E44" s="48">
+        <v>1</v>
+      </c>
+      <c r="F44" s="48">
         <v>0.3</v>
       </c>
-      <c r="G44" s="24">
-        <v>0</v>
-      </c>
-      <c r="H44" s="23">
+      <c r="G44" s="48">
+        <v>0</v>
+      </c>
+      <c r="H44" s="48">
         <v>7</v>
       </c>
-      <c r="I44" s="23" t="s">
+      <c r="I44" s="49" t="s">
         <v>328</v>
       </c>
-      <c r="J44" s="24">
+      <c r="J44" s="48">
         <v>25</v>
       </c>
-      <c r="K44" s="23">
+      <c r="K44" s="50">
         <v>30</v>
       </c>
-      <c r="L44" s="52" t="s">
+      <c r="L44" s="48" t="s">
         <v>123</v>
       </c>
-      <c r="M44" s="24" t="s">
+      <c r="M44" s="48" t="s">
         <v>329</v>
       </c>
       <c r="N44" s="53" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="45" spans="2:14" s="40" customFormat="1" x14ac:dyDescent="0.25">
@@ -4844,7 +4839,7 @@
         <v>7</v>
       </c>
       <c r="I45" s="23" t="s">
-        <v>332</v>
+        <v>352</v>
       </c>
       <c r="J45" s="23">
         <v>25</v>
@@ -4852,14 +4847,14 @@
       <c r="K45" s="23">
         <v>30</v>
       </c>
-      <c r="L45" s="55" t="s">
+      <c r="L45" s="54" t="s">
         <v>123</v>
       </c>
       <c r="M45" s="23" t="s">
-        <v>333</v>
-      </c>
-      <c r="N45" s="54" t="s">
-        <v>352</v>
+        <v>332</v>
+      </c>
+      <c r="N45" s="53" t="s">
+        <v>351</v>
       </c>
     </row>
     <row r="46" spans="2:14" s="40" customFormat="1" x14ac:dyDescent="0.25">
@@ -4911,9 +4906,9 @@
       <c r="C49" s="20"/>
       <c r="D49" s="20"/>
       <c r="E49" s="20"/>
-      <c r="F49" s="59"/>
-      <c r="G49" s="59"/>
-      <c r="H49" s="59"/>
+      <c r="F49" s="58"/>
+      <c r="G49" s="58"/>
+      <c r="H49" s="58"/>
       <c r="I49" s="20"/>
       <c r="J49" s="20"/>
     </row>
@@ -5418,26 +5413,26 @@
       <c r="H71" s="26"/>
     </row>
     <row r="72" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B72" s="57" t="s">
-        <v>1</v>
-      </c>
-      <c r="C72" s="55" t="s">
+      <c r="B72" s="56" t="s">
+        <v>1</v>
+      </c>
+      <c r="C72" s="54" t="s">
         <v>331</v>
       </c>
-      <c r="D72" s="55">
-        <v>0</v>
-      </c>
-      <c r="E72" s="55">
+      <c r="D72" s="54">
+        <v>0</v>
+      </c>
+      <c r="E72" s="54">
         <v>7</v>
       </c>
-      <c r="F72" s="55">
+      <c r="F72" s="54">
         <v>2</v>
       </c>
-      <c r="G72" s="56" t="s">
+      <c r="G72" s="55" t="s">
+        <v>333</v>
+      </c>
+      <c r="H72" s="55" t="s">
         <v>334</v>
-      </c>
-      <c r="H72" s="56" t="s">
-        <v>335</v>
       </c>
     </row>
     <row r="73" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -5465,10 +5460,10 @@
       <c r="F75" s="21" t="s">
         <v>40</v>
       </c>
-      <c r="G75" s="60" t="s">
+      <c r="G75" s="59" t="s">
         <v>39</v>
       </c>
-      <c r="H75" s="60"/>
+      <c r="H75" s="59"/>
       <c r="I75" s="20"/>
     </row>
     <row r="76" spans="2:13" ht="142.5" x14ac:dyDescent="0.25">
@@ -5823,7 +5818,7 @@
         <v>1</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="D98" s="42">
         <v>8.1</v>
@@ -5837,7 +5832,7 @@
         <v>1</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="D99" s="42">
         <v>8</v>
@@ -5851,7 +5846,7 @@
         <v>1</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="D100" s="42">
         <v>7.5</v>
@@ -5865,7 +5860,7 @@
         <v>1</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="D101" s="42">
         <v>8</v>
@@ -5879,7 +5874,7 @@
         <v>1</v>
       </c>
       <c r="C102" s="42" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="D102" s="42">
         <v>7.5</v>
@@ -6791,7 +6786,7 @@
         <v>317</v>
       </c>
       <c r="D174" s="46" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="E174" s="43" t="b">
         <v>1</v>
@@ -6805,7 +6800,7 @@
         <v>318</v>
       </c>
       <c r="D175" s="46" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="E175" s="43" t="b">
         <v>1</v>
@@ -6819,7 +6814,7 @@
         <v>74</v>
       </c>
       <c r="D176" s="46" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="E176" s="43" t="b">
         <v>1</v>
@@ -6830,10 +6825,10 @@
         <v>1</v>
       </c>
       <c r="C177" s="46" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="D177" s="46" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="E177" s="43" t="b">
         <v>1</v>
@@ -6844,10 +6839,10 @@
         <v>1</v>
       </c>
       <c r="C178" s="46" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="D178" s="46" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="E178" s="43" t="b">
         <v>1</v>
@@ -6861,7 +6856,7 @@
         <v>319</v>
       </c>
       <c r="D179" s="46" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="E179" s="43" t="b">
         <v>1</v>
@@ -6872,10 +6867,10 @@
         <v>1</v>
       </c>
       <c r="C180" s="46" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="D180" s="46" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="E180" s="43" t="b">
         <v>1</v>

</xml_diff>

<commit_message>
Removing Halloween mission and activating again Kill villagers mission
Former-commit-id: e74a6e693a6009c985bb70b365346408d5751f37
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Missions.xlsx
+++ b/Docs/Content/HungryDragonContent_Missions.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\dragon\client\Docs\Content\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\dragon\Docs\Content\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -21,30 +21,6 @@
     </ext>
   </extLst>
 </workbook>
-</file>
-
-<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <authors>
-    <author>Jose Camacho</author>
-  </authors>
-  <commentList>
-    <comment ref="B9" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>*Add this mission once Halloween is over</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1138,7 +1114,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1214,13 +1190,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="8"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="16">
@@ -3140,14 +3109,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="6"/>
   </sheetPr>
   <dimension ref="B1:P180"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F16" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I45" sqref="I45"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3401,7 +3370,9 @@
       </c>
     </row>
     <row r="9" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B9" s="27"/>
+      <c r="B9" s="27" t="s">
+        <v>1</v>
+      </c>
       <c r="C9" s="24" t="s">
         <v>124</v>
       </c>
@@ -4812,48 +4783,46 @@
       <c r="M44" s="48" t="s">
         <v>329</v>
       </c>
-      <c r="N44" s="53" t="s">
+      <c r="N44" s="48" t="s">
         <v>350</v>
       </c>
     </row>
     <row r="45" spans="2:14" s="40" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B45" s="25" t="s">
-        <v>1</v>
-      </c>
-      <c r="C45" s="23" t="s">
+      <c r="B45" s="47"/>
+      <c r="C45" s="48" t="s">
         <v>330</v>
       </c>
-      <c r="D45" s="23" t="s">
+      <c r="D45" s="49" t="s">
         <v>331</v>
       </c>
-      <c r="E45" s="23">
-        <v>1</v>
-      </c>
-      <c r="F45" s="23">
+      <c r="E45" s="48">
+        <v>1</v>
+      </c>
+      <c r="F45" s="48">
         <v>0.3</v>
       </c>
-      <c r="G45" s="23">
-        <v>0</v>
-      </c>
-      <c r="H45" s="23">
+      <c r="G45" s="48">
+        <v>0</v>
+      </c>
+      <c r="H45" s="48">
         <v>7</v>
       </c>
-      <c r="I45" s="23" t="s">
+      <c r="I45" s="49" t="s">
         <v>352</v>
       </c>
-      <c r="J45" s="23">
+      <c r="J45" s="48">
         <v>25</v>
       </c>
-      <c r="K45" s="23">
+      <c r="K45" s="50">
         <v>30</v>
       </c>
-      <c r="L45" s="54" t="s">
+      <c r="L45" s="48" t="s">
         <v>123</v>
       </c>
-      <c r="M45" s="23" t="s">
+      <c r="M45" s="48" t="s">
         <v>332</v>
       </c>
-      <c r="N45" s="53" t="s">
+      <c r="N45" s="48" t="s">
         <v>351</v>
       </c>
     </row>
@@ -6888,14 +6857,13 @@
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
   <tableParts count="6">
+    <tablePart r:id="rId2"/>
     <tablePart r:id="rId3"/>
     <tablePart r:id="rId4"/>
     <tablePart r:id="rId5"/>
     <tablePart r:id="rId6"/>
     <tablePart r:id="rId7"/>
-    <tablePart r:id="rId8"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Kill small spiders was wrong. Al spiders count for the mission. Fixed just to small
Former-commit-id: c9faaa6fa4eaa1732d209318cbd6f46144978c6e
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Missions.xlsx
+++ b/Docs/Content/HungryDragonContent_Missions.xlsx
@@ -344,9 +344,6 @@
     <t>icon_spiders</t>
   </si>
   <si>
-    <t>SpiderSmall;SpiderRed;SpiderGreenTurret</t>
-  </si>
-  <si>
     <t>spiders</t>
   </si>
   <si>
@@ -1108,6 +1105,9 @@
   </si>
   <si>
     <t>Villager02;Villager03;Villager04;Worker01;Worker02;WorkerWife;Troll;Cow;Horse;Sheep;EnemyTier0;EnemyTier1;EnemyTier2;EnemyTier3;EnemyTier4;EnemyTier5;Villager01;BakerWoman;BoatFisher;Ground_Zombie</t>
+  </si>
+  <si>
+    <t>SpiderSmall</t>
   </si>
 </sst>
 </file>
@@ -3115,8 +3115,8 @@
   </sheetPr>
   <dimension ref="B1:P180"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" topLeftCell="H4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3139,7 +3139,7 @@
     <row r="1" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:16" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B2" s="6" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C2" s="6"/>
       <c r="D2" s="6"/>
@@ -3157,14 +3157,14 @@
       <c r="C3" s="38"/>
       <c r="D3" s="38"/>
       <c r="E3" s="39" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="F3" s="39" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="G3" s="38"/>
       <c r="J3" s="57" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="K3" s="57"/>
       <c r="M3" s="57"/>
@@ -3174,19 +3174,19 @@
     </row>
     <row r="4" spans="2:16" ht="107.25" x14ac:dyDescent="0.25">
       <c r="B4" s="30" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C4" s="28" t="s">
         <v>3</v>
       </c>
       <c r="D4" s="37" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E4" s="37" t="s">
         <v>68</v>
       </c>
       <c r="F4" s="37" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G4" s="37" t="s">
         <v>70</v>
@@ -3195,22 +3195,22 @@
         <v>69</v>
       </c>
       <c r="I4" s="37" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="J4" s="37" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="K4" s="37" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="L4" s="36" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="M4" s="36" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="N4" s="35" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="5" spans="2:16" x14ac:dyDescent="0.25">
@@ -3218,7 +3218,7 @@
         <v>1</v>
       </c>
       <c r="C5" s="24" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D5" s="24" t="s">
         <v>65</v>
@@ -3236,7 +3236,7 @@
         <v>7</v>
       </c>
       <c r="I5" s="24" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="J5" s="24">
         <v>120</v>
@@ -3245,13 +3245,13 @@
         <v>120</v>
       </c>
       <c r="L5" s="24" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="M5" s="24" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="N5" s="52" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="6" spans="2:16" x14ac:dyDescent="0.25">
@@ -3259,7 +3259,7 @@
         <v>1</v>
       </c>
       <c r="C6" s="24" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D6" s="23" t="s">
         <v>53</v>
@@ -3284,11 +3284,11 @@
         <v>600</v>
       </c>
       <c r="L6" s="24" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="M6" s="24"/>
       <c r="N6" s="53" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="7" spans="2:16" x14ac:dyDescent="0.25">
@@ -3296,7 +3296,7 @@
         <v>1</v>
       </c>
       <c r="C7" s="24" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D7" s="24" t="s">
         <v>59</v>
@@ -3321,11 +3321,11 @@
         <v>28000</v>
       </c>
       <c r="L7" s="24" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="M7" s="24"/>
       <c r="N7" s="52" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="8" spans="2:16" x14ac:dyDescent="0.25">
@@ -3333,7 +3333,7 @@
         <v>1</v>
       </c>
       <c r="C8" s="24" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D8" s="24" t="s">
         <v>65</v>
@@ -3351,7 +3351,7 @@
         <v>7</v>
       </c>
       <c r="I8" s="24" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="J8" s="24">
         <v>600</v>
@@ -3360,13 +3360,13 @@
         <v>650</v>
       </c>
       <c r="L8" s="24" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="M8" s="24" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="N8" s="53" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="9" spans="2:16" x14ac:dyDescent="0.25">
@@ -3374,7 +3374,7 @@
         <v>1</v>
       </c>
       <c r="C9" s="24" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D9" s="24" t="s">
         <v>65</v>
@@ -3392,7 +3392,7 @@
         <v>7</v>
       </c>
       <c r="I9" s="24" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="J9" s="24">
         <v>25</v>
@@ -3401,19 +3401,19 @@
         <v>30</v>
       </c>
       <c r="L9" s="24" t="s">
+        <v>122</v>
+      </c>
+      <c r="M9" s="24" t="s">
+        <v>148</v>
+      </c>
+      <c r="N9" s="52" t="s">
         <v>123</v>
-      </c>
-      <c r="M9" s="24" t="s">
-        <v>149</v>
-      </c>
-      <c r="N9" s="52" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="10" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B10" s="47"/>
       <c r="C10" s="48" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D10" s="49" t="s">
         <v>56</v>
@@ -3431,7 +3431,7 @@
         <v>7</v>
       </c>
       <c r="I10" s="49" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="J10" s="48">
         <v>8</v>
@@ -3440,10 +3440,10 @@
         <v>9</v>
       </c>
       <c r="L10" s="48" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="M10" s="48" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="N10" s="53"/>
     </row>
@@ -3452,7 +3452,7 @@
         <v>1</v>
       </c>
       <c r="C11" s="24" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D11" s="23" t="s">
         <v>50</v>
@@ -3470,7 +3470,7 @@
         <v>7</v>
       </c>
       <c r="I11" s="23" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="J11" s="24">
         <v>1000</v>
@@ -3479,13 +3479,13 @@
         <v>1200</v>
       </c>
       <c r="L11" s="24" t="s">
+        <v>115</v>
+      </c>
+      <c r="M11" s="24" t="s">
+        <v>151</v>
+      </c>
+      <c r="N11" s="52" t="s">
         <v>116</v>
-      </c>
-      <c r="M11" s="24" t="s">
-        <v>152</v>
-      </c>
-      <c r="N11" s="52" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="12" spans="2:16" x14ac:dyDescent="0.25">
@@ -3493,7 +3493,7 @@
         <v>1</v>
       </c>
       <c r="C12" s="24" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D12" s="24" t="s">
         <v>65</v>
@@ -3511,7 +3511,7 @@
         <v>7</v>
       </c>
       <c r="I12" s="24" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="J12" s="24">
         <v>10</v>
@@ -3520,13 +3520,13 @@
         <v>11</v>
       </c>
       <c r="L12" s="24" t="s">
+        <v>111</v>
+      </c>
+      <c r="M12" s="24" t="s">
+        <v>153</v>
+      </c>
+      <c r="N12" s="53" t="s">
         <v>112</v>
-      </c>
-      <c r="M12" s="24" t="s">
-        <v>154</v>
-      </c>
-      <c r="N12" s="53" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="13" spans="2:16" x14ac:dyDescent="0.25">
@@ -3534,7 +3534,7 @@
         <v>1</v>
       </c>
       <c r="C13" s="23" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D13" s="24" t="s">
         <v>62</v>
@@ -3559,11 +3559,11 @@
         <v>6</v>
       </c>
       <c r="L13" s="24" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="M13" s="24"/>
       <c r="N13" s="53" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="14" spans="2:16" x14ac:dyDescent="0.25">
@@ -3596,7 +3596,7 @@
         <v>400</v>
       </c>
       <c r="L14" s="24" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="M14" s="24"/>
       <c r="N14" s="52" t="s">
@@ -3633,7 +3633,7 @@
         <v>400</v>
       </c>
       <c r="L15" s="24" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="M15" s="24"/>
       <c r="N15" s="53" t="s">
@@ -3670,7 +3670,7 @@
         <v>500000</v>
       </c>
       <c r="L16" s="24" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="M16" s="24"/>
       <c r="N16" s="52" t="s">
@@ -3682,7 +3682,7 @@
         <v>1</v>
       </c>
       <c r="C17" s="23" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D17" s="23" t="s">
         <v>65</v>
@@ -3700,7 +3700,7 @@
         <v>7</v>
       </c>
       <c r="I17" s="24" t="s">
-        <v>106</v>
+        <v>352</v>
       </c>
       <c r="J17" s="24">
         <v>45</v>
@@ -3712,10 +3712,10 @@
         <v>105</v>
       </c>
       <c r="M17" s="24" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="N17" s="53" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="18" spans="2:14" x14ac:dyDescent="0.25">
@@ -3753,7 +3753,7 @@
         <v>102</v>
       </c>
       <c r="M18" s="24" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="N18" s="53" t="s">
         <v>104</v>
@@ -3794,7 +3794,7 @@
         <v>93</v>
       </c>
       <c r="M19" s="24" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="N19" s="52" t="s">
         <v>95</v>
@@ -3823,7 +3823,7 @@
         <v>7</v>
       </c>
       <c r="I20" s="23" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="J20" s="24">
         <v>5</v>
@@ -3835,7 +3835,7 @@
         <v>91</v>
       </c>
       <c r="M20" s="24" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="N20" s="53" t="s">
         <v>92</v>
@@ -3876,7 +3876,7 @@
         <v>88</v>
       </c>
       <c r="M21" s="24" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="N21" s="53" t="s">
         <v>90</v>
@@ -3887,7 +3887,7 @@
         <v>1</v>
       </c>
       <c r="C22" s="24" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D22" s="23" t="s">
         <v>65</v>
@@ -3917,10 +3917,10 @@
         <v>86</v>
       </c>
       <c r="M22" s="24" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="N22" s="52" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="23" spans="2:14" x14ac:dyDescent="0.25">
@@ -3958,7 +3958,7 @@
         <v>83</v>
       </c>
       <c r="M23" s="24" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="N23" s="53" t="s">
         <v>85</v>
@@ -3999,7 +3999,7 @@
         <v>80</v>
       </c>
       <c r="M24" s="24" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="N24" s="52" t="s">
         <v>82</v>
@@ -4040,7 +4040,7 @@
         <v>77</v>
       </c>
       <c r="M25" s="24" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="N25" s="53" t="s">
         <v>79</v>
@@ -4079,7 +4079,7 @@
         <v>74</v>
       </c>
       <c r="M26" s="48" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="N26" s="52"/>
     </row>
@@ -4123,10 +4123,10 @@
     <row r="28" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B28" s="27"/>
       <c r="C28" s="23" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D28" s="24" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E28" s="24">
         <v>0</v>
@@ -4141,7 +4141,7 @@
         <v>7</v>
       </c>
       <c r="I28" s="24" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="J28" s="24">
         <v>8</v>
@@ -4150,10 +4150,10 @@
         <v>9</v>
       </c>
       <c r="L28" s="24" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="M28" s="24" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="N28" s="52"/>
     </row>
@@ -4162,10 +4162,10 @@
         <v>1</v>
       </c>
       <c r="C29" s="23" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D29" s="24" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E29" s="24">
         <v>1</v>
@@ -4187,13 +4187,13 @@
         <v>55</v>
       </c>
       <c r="L29" s="24" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="M29" s="24" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="N29" s="53" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="30" spans="2:14" x14ac:dyDescent="0.25">
@@ -4201,10 +4201,10 @@
         <v>1</v>
       </c>
       <c r="C30" s="23" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D30" s="23" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E30" s="24">
         <v>1</v>
@@ -4219,7 +4219,7 @@
         <v>7</v>
       </c>
       <c r="I30" s="24" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="J30" s="24">
         <v>4</v>
@@ -4228,13 +4228,13 @@
         <v>4</v>
       </c>
       <c r="L30" s="24" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="M30" s="24" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="N30" s="52" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="31" spans="2:14" x14ac:dyDescent="0.25">
@@ -4242,10 +4242,10 @@
         <v>1</v>
       </c>
       <c r="C31" s="23" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D31" s="23" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E31" s="24">
         <v>1</v>
@@ -4260,7 +4260,7 @@
         <v>7</v>
       </c>
       <c r="I31" s="23" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="J31" s="24">
         <v>5</v>
@@ -4269,13 +4269,13 @@
         <v>5</v>
       </c>
       <c r="L31" s="24" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="M31" s="24" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="N31" s="53" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="32" spans="2:14" s="40" customFormat="1" x14ac:dyDescent="0.25">
@@ -4283,10 +4283,10 @@
         <v>1</v>
       </c>
       <c r="C32" s="23" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D32" s="24" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E32" s="24">
         <v>1</v>
@@ -4310,22 +4310,22 @@
         <v>18</v>
       </c>
       <c r="L32" s="24" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="M32" s="24" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="N32" s="53" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="33" spans="2:14" s="40" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B33" s="47"/>
       <c r="C33" s="48" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D33" s="49" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E33" s="48">
         <v>0</v>
@@ -4347,7 +4347,7 @@
         <v>27</v>
       </c>
       <c r="L33" s="48" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="M33" s="48"/>
       <c r="N33" s="52"/>
@@ -4357,7 +4357,7 @@
         <v>1</v>
       </c>
       <c r="C34" s="23" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D34" s="23" t="s">
         <v>56</v>
@@ -4375,7 +4375,7 @@
         <v>3</v>
       </c>
       <c r="I34" s="23" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="J34" s="24">
         <v>10</v>
@@ -4384,13 +4384,13 @@
         <v>12</v>
       </c>
       <c r="L34" s="24" t="s">
+        <v>120</v>
+      </c>
+      <c r="M34" s="24" t="s">
+        <v>149</v>
+      </c>
+      <c r="N34" s="53" t="s">
         <v>121</v>
-      </c>
-      <c r="M34" s="24" t="s">
-        <v>150</v>
-      </c>
-      <c r="N34" s="53" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="35" spans="2:14" s="40" customFormat="1" x14ac:dyDescent="0.25">
@@ -4398,10 +4398,10 @@
         <v>1</v>
       </c>
       <c r="C35" s="23" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D35" s="23" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E35" s="23">
         <v>1</v>
@@ -4416,7 +4416,7 @@
         <v>3</v>
       </c>
       <c r="I35" s="24" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="J35" s="24">
         <v>3</v>
@@ -4425,13 +4425,13 @@
         <v>4</v>
       </c>
       <c r="L35" s="24" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="M35" s="24" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="N35" s="52" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="36" spans="2:14" s="40" customFormat="1" x14ac:dyDescent="0.25">
@@ -4439,10 +4439,10 @@
         <v>1</v>
       </c>
       <c r="C36" s="24" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D36" s="23" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E36" s="23">
         <v>1</v>
@@ -4457,7 +4457,7 @@
         <v>3</v>
       </c>
       <c r="I36" s="24" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="J36" s="24">
         <v>25</v>
@@ -4466,13 +4466,13 @@
         <v>27</v>
       </c>
       <c r="L36" s="24" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="M36" s="24" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="N36" s="53" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="37" spans="2:14" s="40" customFormat="1" x14ac:dyDescent="0.25">
@@ -4510,7 +4510,7 @@
         <v>99</v>
       </c>
       <c r="M37" s="24" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="N37" s="52" t="s">
         <v>101</v>
@@ -4519,10 +4519,10 @@
     <row r="38" spans="2:14" s="40" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B38" s="47"/>
       <c r="C38" s="48" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D38" s="49" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E38" s="48">
         <v>0</v>
@@ -4537,7 +4537,7 @@
         <v>2</v>
       </c>
       <c r="I38" s="49" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="J38" s="48">
         <v>150</v>
@@ -4546,20 +4546,20 @@
         <v>160</v>
       </c>
       <c r="L38" s="48" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="M38" s="48" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="N38" s="53"/>
     </row>
     <row r="39" spans="2:14" s="40" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B39" s="47"/>
       <c r="C39" s="48" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D39" s="49" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E39" s="48">
         <v>0</v>
@@ -4574,7 +4574,7 @@
         <v>2</v>
       </c>
       <c r="I39" s="49" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="J39" s="48">
         <v>15</v>
@@ -4583,10 +4583,10 @@
         <v>16</v>
       </c>
       <c r="L39" s="48" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="M39" s="48" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="N39" s="52"/>
     </row>
@@ -4595,10 +4595,10 @@
         <v>1</v>
       </c>
       <c r="C40" s="24" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D40" s="23" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E40" s="23">
         <v>1</v>
@@ -4613,7 +4613,7 @@
         <v>2</v>
       </c>
       <c r="I40" s="23" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="J40" s="24">
         <v>3</v>
@@ -4622,22 +4622,22 @@
         <v>3</v>
       </c>
       <c r="L40" s="24" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="M40" s="24" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="N40" s="53" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="41" spans="2:14" s="40" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B41" s="47"/>
       <c r="C41" s="48" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D41" s="49" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E41" s="48">
         <v>0</v>
@@ -4652,7 +4652,7 @@
         <v>2</v>
       </c>
       <c r="I41" s="49" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="J41" s="48">
         <v>50</v>
@@ -4661,7 +4661,7 @@
         <v>52</v>
       </c>
       <c r="L41" s="48" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="M41" s="48"/>
       <c r="N41" s="53"/>
@@ -4671,7 +4671,7 @@
         <v>1</v>
       </c>
       <c r="C42" s="24" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D42" s="24" t="s">
         <v>50</v>
@@ -4689,7 +4689,7 @@
         <v>1</v>
       </c>
       <c r="I42" s="23" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="J42" s="24">
         <v>1</v>
@@ -4698,13 +4698,13 @@
         <v>2</v>
       </c>
       <c r="L42" s="24" t="s">
+        <v>113</v>
+      </c>
+      <c r="M42" s="24" t="s">
+        <v>152</v>
+      </c>
+      <c r="N42" s="52" t="s">
         <v>114</v>
-      </c>
-      <c r="M42" s="24" t="s">
-        <v>153</v>
-      </c>
-      <c r="N42" s="52" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="43" spans="2:14" s="40" customFormat="1" x14ac:dyDescent="0.25">
@@ -4742,7 +4742,7 @@
         <v>96</v>
       </c>
       <c r="M43" s="24" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="N43" s="53" t="s">
         <v>98</v>
@@ -4751,7 +4751,7 @@
     <row r="44" spans="2:14" s="40" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B44" s="47"/>
       <c r="C44" s="48" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="D44" s="49" t="s">
         <v>65</v>
@@ -4769,7 +4769,7 @@
         <v>7</v>
       </c>
       <c r="I44" s="49" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="J44" s="48">
         <v>25</v>
@@ -4778,22 +4778,22 @@
         <v>30</v>
       </c>
       <c r="L44" s="48" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="M44" s="48" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="N44" s="48" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
     </row>
     <row r="45" spans="2:14" s="40" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B45" s="47"/>
       <c r="C45" s="48" t="s">
+        <v>329</v>
+      </c>
+      <c r="D45" s="49" t="s">
         <v>330</v>
-      </c>
-      <c r="D45" s="49" t="s">
-        <v>331</v>
       </c>
       <c r="E45" s="48">
         <v>1</v>
@@ -4808,7 +4808,7 @@
         <v>7</v>
       </c>
       <c r="I45" s="49" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="J45" s="48">
         <v>25</v>
@@ -4817,13 +4817,13 @@
         <v>30</v>
       </c>
       <c r="L45" s="48" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="M45" s="48" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="N45" s="48" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="46" spans="2:14" s="40" customFormat="1" x14ac:dyDescent="0.25">
@@ -5093,7 +5093,7 @@
         <v>1</v>
       </c>
       <c r="C59" s="24" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D59" s="24">
         <v>0</v>
@@ -5105,10 +5105,10 @@
         <v>0</v>
       </c>
       <c r="G59" s="26" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="H59" s="26" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="60" spans="2:10" x14ac:dyDescent="0.25">
@@ -5116,7 +5116,7 @@
         <v>1</v>
       </c>
       <c r="C60" s="24" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D60" s="24">
         <v>0</v>
@@ -5128,10 +5128,10 @@
         <v>0</v>
       </c>
       <c r="G60" s="26" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="H60" s="26" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="61" spans="2:10" x14ac:dyDescent="0.25">
@@ -5139,7 +5139,7 @@
         <v>1</v>
       </c>
       <c r="C61" s="24" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D61" s="24">
         <v>0</v>
@@ -5151,10 +5151,10 @@
         <v>2</v>
       </c>
       <c r="G61" s="26" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="H61" s="26" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="62" spans="2:10" x14ac:dyDescent="0.25">
@@ -5162,7 +5162,7 @@
         <v>1</v>
       </c>
       <c r="C62" s="24" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="D62" s="24">
         <v>0</v>
@@ -5174,10 +5174,10 @@
         <v>1</v>
       </c>
       <c r="G62" s="26" t="s">
+        <v>228</v>
+      </c>
+      <c r="H62" s="26" t="s">
         <v>229</v>
-      </c>
-      <c r="H62" s="26" t="s">
-        <v>230</v>
       </c>
     </row>
     <row r="63" spans="2:10" x14ac:dyDescent="0.25">
@@ -5185,7 +5185,7 @@
         <v>1</v>
       </c>
       <c r="C63" s="23" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="D63" s="23">
         <v>0</v>
@@ -5197,10 +5197,10 @@
         <v>1</v>
       </c>
       <c r="G63" s="26" t="s">
+        <v>231</v>
+      </c>
+      <c r="H63" s="26" t="s">
         <v>232</v>
-      </c>
-      <c r="H63" s="26" t="s">
-        <v>233</v>
       </c>
     </row>
     <row r="64" spans="2:10" x14ac:dyDescent="0.25">
@@ -5208,7 +5208,7 @@
         <v>1</v>
       </c>
       <c r="C64" s="24" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D64" s="24">
         <v>0</v>
@@ -5220,10 +5220,10 @@
         <v>1</v>
       </c>
       <c r="G64" s="26" t="s">
+        <v>234</v>
+      </c>
+      <c r="H64" s="26" t="s">
         <v>235</v>
-      </c>
-      <c r="H64" s="26" t="s">
-        <v>236</v>
       </c>
     </row>
     <row r="65" spans="2:13" x14ac:dyDescent="0.25">
@@ -5231,7 +5231,7 @@
         <v>1</v>
       </c>
       <c r="C65" s="24" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="D65" s="24">
         <v>0</v>
@@ -5243,10 +5243,10 @@
         <v>1</v>
       </c>
       <c r="G65" s="26" t="s">
+        <v>237</v>
+      </c>
+      <c r="H65" s="26" t="s">
         <v>238</v>
-      </c>
-      <c r="H65" s="26" t="s">
-        <v>239</v>
       </c>
     </row>
     <row r="66" spans="2:13" x14ac:dyDescent="0.25">
@@ -5254,7 +5254,7 @@
         <v>1</v>
       </c>
       <c r="C66" s="23" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D66" s="23">
         <v>0</v>
@@ -5266,10 +5266,10 @@
         <v>0</v>
       </c>
       <c r="G66" s="22" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="H66" s="22" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="67" spans="2:13" x14ac:dyDescent="0.25">
@@ -5277,7 +5277,7 @@
         <v>1</v>
       </c>
       <c r="C67" s="24" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D67" s="24">
         <v>0</v>
@@ -5289,7 +5289,7 @@
         <v>1</v>
       </c>
       <c r="G67" s="26" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="H67" s="26"/>
     </row>
@@ -5298,7 +5298,7 @@
         <v>1</v>
       </c>
       <c r="C68" s="24" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D68" s="24">
         <v>0</v>
@@ -5310,10 +5310,10 @@
         <v>0</v>
       </c>
       <c r="G68" s="26" t="s">
+        <v>183</v>
+      </c>
+      <c r="H68" s="26" t="s">
         <v>184</v>
-      </c>
-      <c r="H68" s="26" t="s">
-        <v>185</v>
       </c>
     </row>
     <row r="69" spans="2:13" x14ac:dyDescent="0.25">
@@ -5321,7 +5321,7 @@
         <v>1</v>
       </c>
       <c r="C69" s="24" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D69" s="24">
         <v>0</v>
@@ -5333,10 +5333,10 @@
         <v>1</v>
       </c>
       <c r="G69" s="26" t="s">
+        <v>209</v>
+      </c>
+      <c r="H69" s="26" t="s">
         <v>210</v>
-      </c>
-      <c r="H69" s="26" t="s">
-        <v>211</v>
       </c>
     </row>
     <row r="70" spans="2:13" x14ac:dyDescent="0.25">
@@ -5344,7 +5344,7 @@
         <v>1</v>
       </c>
       <c r="C70" s="24" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="D70" s="24">
         <v>0</v>
@@ -5356,7 +5356,7 @@
         <v>1</v>
       </c>
       <c r="G70" s="26" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="H70" s="26"/>
     </row>
@@ -5365,7 +5365,7 @@
         <v>1</v>
       </c>
       <c r="C71" s="24" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="D71" s="24">
         <v>0</v>
@@ -5377,7 +5377,7 @@
         <v>1</v>
       </c>
       <c r="G71" s="26" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="H71" s="26"/>
     </row>
@@ -5386,7 +5386,7 @@
         <v>1</v>
       </c>
       <c r="C72" s="54" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="D72" s="54">
         <v>0</v>
@@ -5398,10 +5398,10 @@
         <v>2</v>
       </c>
       <c r="G72" s="55" t="s">
+        <v>332</v>
+      </c>
+      <c r="H72" s="55" t="s">
         <v>333</v>
-      </c>
-      <c r="H72" s="55" t="s">
-        <v>334</v>
       </c>
     </row>
     <row r="73" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -5443,7 +5443,7 @@
         <v>3</v>
       </c>
       <c r="D76" s="18" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="E76" s="18" t="s">
         <v>37</v>
@@ -5475,7 +5475,7 @@
         <v>1</v>
       </c>
       <c r="C77" s="11" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="D77" s="11" t="s">
         <v>8</v>
@@ -5510,7 +5510,7 @@
         <v>1</v>
       </c>
       <c r="C78" s="11" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="D78" s="11" t="s">
         <v>7</v>
@@ -5545,7 +5545,7 @@
         <v>1</v>
       </c>
       <c r="C79" s="11" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D79" s="11" t="s">
         <v>6</v>
@@ -5586,7 +5586,7 @@
       <c r="F82" s="6"/>
       <c r="G82" s="6"/>
     </row>
-    <row r="84" spans="2:7" ht="135" x14ac:dyDescent="0.25">
+    <row r="84" spans="2:7" ht="135.75" x14ac:dyDescent="0.25">
       <c r="B84" s="5" t="s">
         <v>22</v>
       </c>
@@ -5717,7 +5717,7 @@
         <v>1</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D93" s="1">
         <v>4.5</v>
@@ -5759,7 +5759,7 @@
         <v>1</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="D96" s="42">
         <v>7.5</v>
@@ -5773,7 +5773,7 @@
         <v>1</v>
       </c>
       <c r="C97" s="42" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="D97" s="42">
         <v>8</v>
@@ -5787,7 +5787,7 @@
         <v>1</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="D98" s="42">
         <v>8.1</v>
@@ -5801,7 +5801,7 @@
         <v>1</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="D99" s="42">
         <v>8</v>
@@ -5815,7 +5815,7 @@
         <v>1</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="D100" s="42">
         <v>7.5</v>
@@ -5829,7 +5829,7 @@
         <v>1</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="D101" s="42">
         <v>8</v>
@@ -5843,7 +5843,7 @@
         <v>1</v>
       </c>
       <c r="C102" s="42" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="D102" s="42">
         <v>7.5</v>
@@ -5871,7 +5871,7 @@
         <v>3</v>
       </c>
       <c r="D106" s="4" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="E106" s="3" t="s">
         <v>2</v>
@@ -5882,7 +5882,7 @@
         <v>1</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D107" s="1" t="s">
         <v>8</v>
@@ -5896,7 +5896,7 @@
         <v>1</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="D108" s="1" t="s">
         <v>7</v>
@@ -5910,7 +5910,7 @@
         <v>1</v>
       </c>
       <c r="C109" s="1" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="D109" s="1" t="s">
         <v>6</v>
@@ -5930,7 +5930,7 @@
       <c r="F111" s="6"/>
       <c r="G111" s="6"/>
     </row>
-    <row r="113" spans="2:7" ht="131.25" x14ac:dyDescent="0.25">
+    <row r="113" spans="2:7" ht="132" x14ac:dyDescent="0.25">
       <c r="B113" s="5" t="s">
         <v>4</v>
       </c>
@@ -5955,7 +5955,7 @@
     <row r="115" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="116" spans="2:7" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B116" s="6" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C116" s="6"/>
       <c r="D116" s="6"/>
@@ -5965,16 +5965,16 @@
     </row>
     <row r="118" spans="2:7" ht="68.25" x14ac:dyDescent="0.25">
       <c r="B118" s="44" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C118" s="44" t="s">
         <v>3</v>
       </c>
       <c r="D118" s="45" t="s">
+        <v>241</v>
+      </c>
+      <c r="E118" s="45" t="s">
         <v>242</v>
-      </c>
-      <c r="E118" s="45" t="s">
-        <v>243</v>
       </c>
     </row>
     <row r="119" spans="2:7" x14ac:dyDescent="0.25">
@@ -5985,7 +5985,7 @@
         <v>80</v>
       </c>
       <c r="D119" s="46" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="E119" s="43" t="b">
         <v>1</v>
@@ -5999,7 +5999,7 @@
         <v>93</v>
       </c>
       <c r="D120" s="46" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="E120" s="43" t="b">
         <v>1</v>
@@ -6010,10 +6010,10 @@
         <v>1</v>
       </c>
       <c r="C121" s="46" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D121" s="46" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="E121" s="43" t="b">
         <v>1</v>
@@ -6024,10 +6024,10 @@
         <v>1</v>
       </c>
       <c r="C122" s="46" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D122" s="46" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E122" s="43" t="b">
         <v>0</v>
@@ -6038,10 +6038,10 @@
         <v>1</v>
       </c>
       <c r="C123" s="46" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D123" s="46" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E123" s="43" t="b">
         <v>0</v>
@@ -6052,10 +6052,10 @@
         <v>1</v>
       </c>
       <c r="C124" s="46" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D124" s="46" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E124" s="43" t="b">
         <v>0</v>
@@ -6066,10 +6066,10 @@
         <v>1</v>
       </c>
       <c r="C125" s="46" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D125" s="46" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="E125" s="43" t="b">
         <v>1</v>
@@ -6080,10 +6080,10 @@
         <v>1</v>
       </c>
       <c r="C126" s="46" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="D126" s="46" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="E126" s="43" t="b">
         <v>1</v>
@@ -6094,10 +6094,10 @@
         <v>1</v>
       </c>
       <c r="C127" s="46" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="D127" s="46" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="E127" s="43" t="b">
         <v>1</v>
@@ -6108,10 +6108,10 @@
         <v>1</v>
       </c>
       <c r="C128" s="46" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D128" s="46" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="E128" s="43" t="b">
         <v>1</v>
@@ -6122,10 +6122,10 @@
         <v>1</v>
       </c>
       <c r="C129" s="46" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D129" s="46" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="E129" s="43" t="b">
         <v>1</v>
@@ -6136,10 +6136,10 @@
         <v>1</v>
       </c>
       <c r="C130" s="46" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D130" s="46" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="E130" s="43" t="b">
         <v>1</v>
@@ -6150,10 +6150,10 @@
         <v>1</v>
       </c>
       <c r="C131" s="46" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D131" s="46" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="E131" s="43" t="b">
         <v>1</v>
@@ -6164,10 +6164,10 @@
         <v>1</v>
       </c>
       <c r="C132" s="46" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D132" s="46" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="E132" s="43" t="b">
         <v>1</v>
@@ -6178,10 +6178,10 @@
         <v>1</v>
       </c>
       <c r="C133" s="46" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D133" s="46" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="E133" s="43" t="b">
         <v>1</v>
@@ -6192,10 +6192,10 @@
         <v>1</v>
       </c>
       <c r="C134" s="46" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D134" s="46" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="E134" s="43" t="b">
         <v>1</v>
@@ -6206,10 +6206,10 @@
         <v>1</v>
       </c>
       <c r="C135" s="46" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D135" s="46" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="E135" s="43" t="b">
         <v>1</v>
@@ -6220,10 +6220,10 @@
         <v>1</v>
       </c>
       <c r="C136" s="46" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="D136" s="46" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="E136" s="43" t="b">
         <v>0</v>
@@ -6237,7 +6237,7 @@
         <v>83</v>
       </c>
       <c r="D137" s="46" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="E137" s="43" t="b">
         <v>1</v>
@@ -6251,7 +6251,7 @@
         <v>96</v>
       </c>
       <c r="D138" s="46" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="E138" s="43" t="b">
         <v>1</v>
@@ -6262,10 +6262,10 @@
         <v>1</v>
       </c>
       <c r="C139" s="46" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="D139" s="46" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="E139" s="43" t="b">
         <v>1</v>
@@ -6276,10 +6276,10 @@
         <v>1</v>
       </c>
       <c r="C140" s="46" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D140" s="46" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="E140" s="43" t="b">
         <v>1</v>
@@ -6293,7 +6293,7 @@
         <v>102</v>
       </c>
       <c r="D141" s="46" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="E141" s="43" t="b">
         <v>1</v>
@@ -6304,10 +6304,10 @@
         <v>1</v>
       </c>
       <c r="C142" s="46" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D142" s="46" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="E142" s="43" t="b">
         <v>1</v>
@@ -6318,10 +6318,10 @@
         <v>1</v>
       </c>
       <c r="C143" s="46" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D143" s="46" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="E143" s="43" t="b">
         <v>1</v>
@@ -6335,7 +6335,7 @@
         <v>88</v>
       </c>
       <c r="D144" s="46" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="E144" s="43" t="b">
         <v>1</v>
@@ -6346,10 +6346,10 @@
         <v>1</v>
       </c>
       <c r="C145" s="46" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="D145" s="46" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="E145" s="43" t="b">
         <v>1</v>
@@ -6360,10 +6360,10 @@
         <v>1</v>
       </c>
       <c r="C146" s="46" t="s">
+        <v>301</v>
+      </c>
+      <c r="D146" s="46" t="s">
         <v>302</v>
-      </c>
-      <c r="D146" s="46" t="s">
-        <v>303</v>
       </c>
       <c r="E146" s="43" t="b">
         <v>1</v>
@@ -6374,10 +6374,10 @@
         <v>1</v>
       </c>
       <c r="C147" s="46" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="D147" s="46" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="E147" s="43" t="b">
         <v>0</v>
@@ -6388,10 +6388,10 @@
         <v>1</v>
       </c>
       <c r="C148" s="46" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D148" s="46" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E148" s="43" t="b">
         <v>0</v>
@@ -6402,10 +6402,10 @@
         <v>1</v>
       </c>
       <c r="C149" s="46" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="D149" s="46" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="E149" s="43" t="b">
         <v>1</v>
@@ -6419,7 +6419,7 @@
         <v>91</v>
       </c>
       <c r="D150" s="46" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="E150" s="43" t="b">
         <v>1</v>
@@ -6430,10 +6430,10 @@
         <v>1</v>
       </c>
       <c r="C151" s="46" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="D151" s="46" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="E151" s="43" t="b">
         <v>1</v>
@@ -6444,10 +6444,10 @@
         <v>1</v>
       </c>
       <c r="C152" s="46" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D152" s="46" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="E152" s="43" t="b">
         <v>1</v>
@@ -6458,10 +6458,10 @@
         <v>1</v>
       </c>
       <c r="C153" s="46" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="D153" s="46" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="E153" s="43" t="b">
         <v>1</v>
@@ -6475,7 +6475,7 @@
         <v>86</v>
       </c>
       <c r="D154" s="46" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="E154" s="43" t="b">
         <v>1</v>
@@ -6500,10 +6500,10 @@
         <v>1</v>
       </c>
       <c r="C156" s="46" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D156" s="46" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E156" s="43" t="b">
         <v>0</v>
@@ -6514,10 +6514,10 @@
         <v>1</v>
       </c>
       <c r="C157" s="46" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="D157" s="46" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="E157" s="43" t="b">
         <v>1</v>
@@ -6528,10 +6528,10 @@
         <v>1</v>
       </c>
       <c r="C158" s="46" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D158" s="46" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="E158" s="43" t="b">
         <v>1</v>
@@ -6545,7 +6545,7 @@
         <v>77</v>
       </c>
       <c r="D159" s="46" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="E159" s="43" t="b">
         <v>1</v>
@@ -6559,7 +6559,7 @@
         <v>105</v>
       </c>
       <c r="D160" s="46" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="E160" s="43" t="b">
         <v>1</v>
@@ -6570,10 +6570,10 @@
         <v>1</v>
       </c>
       <c r="C161" s="46" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="D161" s="46" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="E161" s="43" t="b">
         <v>1</v>
@@ -6584,10 +6584,10 @@
         <v>1</v>
       </c>
       <c r="C162" s="46" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="D162" s="46" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="E162" s="43" t="b">
         <v>1</v>
@@ -6598,10 +6598,10 @@
         <v>1</v>
       </c>
       <c r="C163" s="46" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="D163" s="46" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="E163" s="43" t="b">
         <v>1</v>
@@ -6612,10 +6612,10 @@
         <v>1</v>
       </c>
       <c r="C164" s="46" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="D164" s="46" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="E164" s="43" t="b">
         <v>0</v>
@@ -6629,7 +6629,7 @@
         <v>99</v>
       </c>
       <c r="D165" s="46" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="E165" s="43" t="b">
         <v>1</v>
@@ -6640,10 +6640,10 @@
         <v>1</v>
       </c>
       <c r="C166" s="46" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="D166" s="46" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="E166" s="43" t="b">
         <v>1</v>
@@ -6654,10 +6654,10 @@
         <v>1</v>
       </c>
       <c r="C167" s="46" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="D167" s="46" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="E167" s="43" t="b">
         <v>1</v>
@@ -6668,10 +6668,10 @@
         <v>1</v>
       </c>
       <c r="C168" s="46" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="D168" s="46" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="E168" s="43" t="b">
         <v>1</v>
@@ -6682,10 +6682,10 @@
         <v>1</v>
       </c>
       <c r="C169" s="46" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="D169" s="46" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="E169" s="43" t="b">
         <v>1</v>
@@ -6696,10 +6696,10 @@
         <v>1</v>
       </c>
       <c r="C170" s="46" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D170" s="46" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="E170" s="43" t="b">
         <v>1</v>
@@ -6710,10 +6710,10 @@
         <v>1</v>
       </c>
       <c r="C171" s="46" t="s">
+        <v>319</v>
+      </c>
+      <c r="D171" s="46" t="s">
         <v>320</v>
-      </c>
-      <c r="D171" s="46" t="s">
-        <v>321</v>
       </c>
       <c r="E171" s="43" t="b">
         <v>1</v>
@@ -6724,10 +6724,10 @@
         <v>1</v>
       </c>
       <c r="C172" s="46" t="s">
+        <v>321</v>
+      </c>
+      <c r="D172" s="46" t="s">
         <v>322</v>
-      </c>
-      <c r="D172" s="46" t="s">
-        <v>323</v>
       </c>
       <c r="E172" s="43" t="b">
         <v>1</v>
@@ -6738,10 +6738,10 @@
         <v>1</v>
       </c>
       <c r="C173" s="46" t="s">
+        <v>323</v>
+      </c>
+      <c r="D173" s="46" t="s">
         <v>324</v>
-      </c>
-      <c r="D173" s="46" t="s">
-        <v>325</v>
       </c>
       <c r="E173" s="43" t="b">
         <v>1</v>
@@ -6752,10 +6752,10 @@
         <v>1</v>
       </c>
       <c r="C174" s="46" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="D174" s="46" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="E174" s="43" t="b">
         <v>1</v>
@@ -6766,10 +6766,10 @@
         <v>1</v>
       </c>
       <c r="C175" s="46" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="D175" s="46" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="E175" s="43" t="b">
         <v>1</v>
@@ -6783,7 +6783,7 @@
         <v>74</v>
       </c>
       <c r="D176" s="46" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="E176" s="43" t="b">
         <v>1</v>
@@ -6794,10 +6794,10 @@
         <v>1</v>
       </c>
       <c r="C177" s="46" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="D177" s="46" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="E177" s="43" t="b">
         <v>1</v>
@@ -6808,10 +6808,10 @@
         <v>1</v>
       </c>
       <c r="C178" s="46" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="D178" s="46" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="E178" s="43" t="b">
         <v>1</v>
@@ -6822,10 +6822,10 @@
         <v>1</v>
       </c>
       <c r="C179" s="46" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="D179" s="46" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="E179" s="43" t="b">
         <v>1</v>
@@ -6836,10 +6836,10 @@
         <v>1</v>
       </c>
       <c r="C180" s="46" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="D180" s="46" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="E180" s="43" t="b">
         <v>1</v>

</xml_diff>

<commit_message>
Adding new missions ( not active right now. Missing icons)
Former-commit-id: 409a7c75f4edec3891c7777630b62f67d0b12bff
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Missions.xlsx
+++ b/Docs/Content/HungryDragonContent_Missions.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="644" uniqueCount="353">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="674" uniqueCount="370">
   <si>
     <t>single_run</t>
   </si>
@@ -1109,12 +1109,63 @@
   <si>
     <t>SpiderSmall</t>
   </si>
+  <si>
+    <t>fishes</t>
+  </si>
+  <si>
+    <t>crocos</t>
+  </si>
+  <si>
+    <t>fireflies</t>
+  </si>
+  <si>
+    <t>carnivorousPlant</t>
+  </si>
+  <si>
+    <t>redGhost</t>
+  </si>
+  <si>
+    <t>Crocodile</t>
+  </si>
+  <si>
+    <t>Firefly</t>
+  </si>
+  <si>
+    <t>carnivorousPlant;CarnivorousPlantDark</t>
+  </si>
+  <si>
+    <t>Ghost03</t>
+  </si>
+  <si>
+    <t>TID_EDIBLE_FISH_PL</t>
+  </si>
+  <si>
+    <t>TID_EDIBLE_CROCODILES</t>
+  </si>
+  <si>
+    <t>TID_EDIBLE_FIREFLY_PL</t>
+  </si>
+  <si>
+    <t>TID_EDIBLE_CARNIVOROUS_PLANT_PL</t>
+  </si>
+  <si>
+    <t>plants</t>
+  </si>
+  <si>
+    <t>TID_EDIBLE_REDGHOSTS_PL</t>
+  </si>
+  <si>
+    <t>redGhosts</t>
+  </si>
+  <si>
+    <t>Fish01_Generic;Fish02_Generic;Fish03_Generic;FishDark;Piranha;PiranhaDark</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1187,6 +1238,13 @@
     <font>
       <sz val="11"/>
       <color theme="0" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1284,7 +1342,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -1421,11 +1479,39 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1"/>
@@ -1570,11 +1656,42 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="69">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -2725,16 +2842,6 @@
         </bottom>
       </border>
     </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -2749,99 +2856,99 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="missionDifficultyDefinitions" displayName="missionDifficultyDefinitions" ref="B76:L79" totalsRowShown="0" headerRowBorderDxfId="67" tableBorderDxfId="66">
-  <autoFilter ref="B76:L79"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="missionDifficultyDefinitions" displayName="missionDifficultyDefinitions" ref="B81:L84" totalsRowShown="0" headerRowBorderDxfId="68" tableBorderDxfId="67">
+  <autoFilter ref="B81:L84"/>
   <tableColumns count="11">
     <tableColumn id="1" name="{missionDifficultyDefinitions}"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="65"/>
-    <tableColumn id="11" name="[difficulty]" dataDxfId="64"/>
-    <tableColumn id="7" name="[index]" dataDxfId="63"/>
-    <tableColumn id="3" name="[dragonsToUnlock]" dataDxfId="62"/>
-    <tableColumn id="4" name="[cooldownMinutes]" dataDxfId="61"/>
-    <tableColumn id="9" name="[maxRewardCoins]" dataDxfId="60"/>
-    <tableColumn id="5" name="[removeMissionPCCoefA]" dataDxfId="59"/>
-    <tableColumn id="6" name="[removeMissionPCCoefB]" dataDxfId="58"/>
-    <tableColumn id="8" name="[tidName]" dataDxfId="57"/>
-    <tableColumn id="10" name="[color]" dataDxfId="56"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="66"/>
+    <tableColumn id="11" name="[difficulty]" dataDxfId="65"/>
+    <tableColumn id="7" name="[index]" dataDxfId="64"/>
+    <tableColumn id="3" name="[dragonsToUnlock]" dataDxfId="63"/>
+    <tableColumn id="4" name="[cooldownMinutes]" dataDxfId="62"/>
+    <tableColumn id="9" name="[maxRewardCoins]" dataDxfId="61"/>
+    <tableColumn id="5" name="[removeMissionPCCoefA]" dataDxfId="60"/>
+    <tableColumn id="6" name="[removeMissionPCCoefB]" dataDxfId="59"/>
+    <tableColumn id="8" name="[tidName]" dataDxfId="58"/>
+    <tableColumn id="10" name="[color]" dataDxfId="57"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table13303132" displayName="Table13303132" ref="B84:E102" totalsRowShown="0" headerRowDxfId="55" dataDxfId="53" headerRowBorderDxfId="54" tableBorderDxfId="52" totalsRowBorderDxfId="51">
-  <autoFilter ref="B84:E102"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table13303132" displayName="Table13303132" ref="B89:E107" totalsRowShown="0" headerRowDxfId="56" dataDxfId="54" headerRowBorderDxfId="55" tableBorderDxfId="53" totalsRowBorderDxfId="52">
+  <autoFilter ref="B89:E107"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="{missionDragonModifiersDefinitions}" dataDxfId="50"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="49"/>
-    <tableColumn id="7" name="[quantityModifier]" dataDxfId="48"/>
-    <tableColumn id="3" name="[missionSCRewardMultiplier]" dataDxfId="47"/>
+    <tableColumn id="1" name="{missionDragonModifiersDefinitions}" dataDxfId="51"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="50"/>
+    <tableColumn id="7" name="[quantityModifier]" dataDxfId="49"/>
+    <tableColumn id="3" name="[missionSCRewardMultiplier]" dataDxfId="48"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table1330313234" displayName="Table1330313234" ref="B106:E109" totalsRowShown="0" headerRowDxfId="46" dataDxfId="44" headerRowBorderDxfId="45" tableBorderDxfId="43" totalsRowBorderDxfId="42">
-  <autoFilter ref="B106:E109"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table1330313234" displayName="Table1330313234" ref="B111:E114" totalsRowShown="0" headerRowDxfId="47" dataDxfId="45" headerRowBorderDxfId="46" tableBorderDxfId="44" totalsRowBorderDxfId="43">
+  <autoFilter ref="B111:E114"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="{missionDifficultyModifiersDefinitions}" dataDxfId="41"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="40"/>
-    <tableColumn id="3" name="[difficulty]" dataDxfId="39"/>
-    <tableColumn id="7" name="[quantityModifier]" dataDxfId="38"/>
+    <tableColumn id="1" name="{missionDifficultyModifiersDefinitions}" dataDxfId="42"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="41"/>
+    <tableColumn id="3" name="[difficulty]" dataDxfId="40"/>
+    <tableColumn id="7" name="[quantityModifier]" dataDxfId="39"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table133031323435" displayName="Table133031323435" ref="B113:D114" totalsRowShown="0" headerRowDxfId="37" dataDxfId="35" headerRowBorderDxfId="36" tableBorderDxfId="34" totalsRowBorderDxfId="33">
-  <autoFilter ref="B113:D114"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table133031323435" displayName="Table133031323435" ref="B118:D119" totalsRowShown="0" headerRowDxfId="38" dataDxfId="36" headerRowBorderDxfId="37" tableBorderDxfId="35" totalsRowBorderDxfId="34">
+  <autoFilter ref="B118:D119"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="{missionOtherModifiersDefinitions}" dataDxfId="32"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="31"/>
-    <tableColumn id="7" name="[quantityModifier]" dataDxfId="30"/>
+    <tableColumn id="1" name="{missionOtherModifiersDefinitions}" dataDxfId="33"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="32"/>
+    <tableColumn id="7" name="[quantityModifier]" dataDxfId="31"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table13" displayName="Table13" ref="B50:H72" totalsRowShown="0" headerRowDxfId="29" dataDxfId="27" headerRowBorderDxfId="28" tableBorderDxfId="26" totalsRowBorderDxfId="25">
-  <autoFilter ref="B50:H72"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table13" displayName="Table13" ref="B55:H77" totalsRowShown="0" headerRowDxfId="30" dataDxfId="28" headerRowBorderDxfId="29" tableBorderDxfId="27" totalsRowBorderDxfId="26">
+  <autoFilter ref="B55:H77"/>
   <tableColumns count="7">
-    <tableColumn id="1" name="{missionTypeDefinitions}" dataDxfId="24"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="23"/>
-    <tableColumn id="3" name="[minTier]" dataDxfId="22"/>
-    <tableColumn id="6" name="[maxTier]" dataDxfId="21"/>
-    <tableColumn id="4" name="[weight]" dataDxfId="20"/>
-    <tableColumn id="9" name="[tidDescSingleRun]" dataDxfId="19"/>
-    <tableColumn id="10" name="[tidDescMultiRun]" dataDxfId="18"/>
+    <tableColumn id="1" name="{missionTypeDefinitions}" dataDxfId="25"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="24"/>
+    <tableColumn id="3" name="[minTier]" dataDxfId="23"/>
+    <tableColumn id="6" name="[maxTier]" dataDxfId="22"/>
+    <tableColumn id="4" name="[weight]" dataDxfId="21"/>
+    <tableColumn id="9" name="[tidDescSingleRun]" dataDxfId="20"/>
+    <tableColumn id="10" name="[tidDescMultiRun]" dataDxfId="19"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table1330" displayName="Table1330" ref="B4:N45" totalsRowShown="0" headerRowDxfId="17" dataDxfId="15" headerRowBorderDxfId="16" tableBorderDxfId="14" totalsRowBorderDxfId="13">
-  <autoFilter ref="B4:N45"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table1330" displayName="Table1330" ref="B4:N50" totalsRowShown="0" headerRowDxfId="18" dataDxfId="16" headerRowBorderDxfId="17" tableBorderDxfId="15" totalsRowBorderDxfId="14">
+  <autoFilter ref="B4:N50"/>
   <sortState ref="B5:P43">
     <sortCondition descending="1" ref="J4:J43"/>
   </sortState>
   <tableColumns count="13">
-    <tableColumn id="1" name="{missionsDefinitions}" dataDxfId="12"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="11"/>
-    <tableColumn id="7" name="[type]" dataDxfId="10"/>
-    <tableColumn id="8" name="[weight]" dataDxfId="9"/>
-    <tableColumn id="13" name="[singleRunChance]" dataDxfId="8"/>
-    <tableColumn id="11" name="[minTier]" dataDxfId="7"/>
-    <tableColumn id="12" name="[maxTier]" dataDxfId="6"/>
-    <tableColumn id="6" name="[params]" dataDxfId="5"/>
-    <tableColumn id="3" name="[objectiveBaseQuantityMin]" dataDxfId="4"/>
-    <tableColumn id="9" name="[objectiveBaseQuantityMax]" dataDxfId="3"/>
-    <tableColumn id="4" name="[icon]" dataDxfId="2"/>
-    <tableColumn id="5" name="[tidObjective]" dataDxfId="1"/>
-    <tableColumn id="10" name="[trackingSku]" dataDxfId="0"/>
+    <tableColumn id="1" name="{missionsDefinitions}" dataDxfId="13"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="12"/>
+    <tableColumn id="7" name="[type]" dataDxfId="11"/>
+    <tableColumn id="8" name="[weight]" dataDxfId="10"/>
+    <tableColumn id="13" name="[singleRunChance]" dataDxfId="9"/>
+    <tableColumn id="11" name="[minTier]" dataDxfId="8"/>
+    <tableColumn id="12" name="[maxTier]" dataDxfId="7"/>
+    <tableColumn id="6" name="[params]" dataDxfId="6"/>
+    <tableColumn id="3" name="[objectiveBaseQuantityMin]" dataDxfId="5"/>
+    <tableColumn id="9" name="[objectiveBaseQuantityMax]" dataDxfId="4"/>
+    <tableColumn id="4" name="[icon]" dataDxfId="3"/>
+    <tableColumn id="5" name="[tidObjective]" dataDxfId="2"/>
+    <tableColumn id="10" name="[trackingSku]" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3113,10 +3220,10 @@
   <sheetPr>
     <tabColor theme="6"/>
   </sheetPr>
-  <dimension ref="B1:P180"/>
+  <dimension ref="B1:P185"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C46" sqref="C46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4787,244 +4894,324 @@
         <v>349</v>
       </c>
     </row>
-    <row r="45" spans="2:14" s="40" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B45" s="47"/>
-      <c r="C45" s="48" t="s">
+    <row r="45" spans="2:14" s="40" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B45" s="60"/>
+      <c r="C45" s="49" t="s">
         <v>329</v>
       </c>
       <c r="D45" s="49" t="s">
         <v>330</v>
       </c>
-      <c r="E45" s="48">
-        <v>1</v>
-      </c>
-      <c r="F45" s="48">
+      <c r="E45" s="49">
+        <v>1</v>
+      </c>
+      <c r="F45" s="49">
         <v>0.3</v>
       </c>
-      <c r="G45" s="48">
-        <v>0</v>
-      </c>
-      <c r="H45" s="48">
+      <c r="G45" s="49">
+        <v>0</v>
+      </c>
+      <c r="H45" s="49">
         <v>7</v>
       </c>
       <c r="I45" s="49" t="s">
         <v>351</v>
       </c>
-      <c r="J45" s="48">
+      <c r="J45" s="49">
         <v>25</v>
       </c>
-      <c r="K45" s="50">
+      <c r="K45" s="61">
         <v>30</v>
       </c>
-      <c r="L45" s="48" t="s">
+      <c r="L45" s="49" t="s">
         <v>122</v>
       </c>
-      <c r="M45" s="48" t="s">
+      <c r="M45" s="49" t="s">
         <v>331</v>
       </c>
-      <c r="N45" s="48" t="s">
+      <c r="N45" s="49" t="s">
         <v>350</v>
       </c>
     </row>
     <row r="46" spans="2:14" s="40" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B46" s="41"/>
-      <c r="C46" s="41"/>
-      <c r="D46" s="41"/>
-      <c r="E46" s="41"/>
-      <c r="F46" s="41"/>
-      <c r="G46" s="41"/>
-      <c r="H46" s="41"/>
-      <c r="I46" s="41"/>
-      <c r="J46" s="41"/>
-      <c r="K46" s="41"/>
-      <c r="L46" s="41"/>
-      <c r="M46" s="41"/>
-      <c r="N46" s="41"/>
-    </row>
-    <row r="47" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B47" s="32"/>
-      <c r="C47" s="32"/>
-      <c r="D47" s="32"/>
-      <c r="E47" s="32"/>
-      <c r="F47" s="32"/>
-      <c r="G47" s="32"/>
-      <c r="H47" s="32"/>
-      <c r="I47" s="32"/>
-      <c r="J47" s="32"/>
-      <c r="K47" s="32"/>
-      <c r="L47" s="32"/>
-      <c r="M47" s="31"/>
-    </row>
-    <row r="48" spans="2:14" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B48" s="6" t="s">
+      <c r="B46" s="62"/>
+      <c r="C46" s="63" t="s">
+        <v>353</v>
+      </c>
+      <c r="D46" s="63" t="s">
+        <v>65</v>
+      </c>
+      <c r="E46" s="63">
+        <v>1</v>
+      </c>
+      <c r="F46" s="63">
+        <v>0.3</v>
+      </c>
+      <c r="G46" s="63">
+        <v>2</v>
+      </c>
+      <c r="H46" s="63">
+        <v>4</v>
+      </c>
+      <c r="I46" s="63" t="s">
+        <v>369</v>
+      </c>
+      <c r="J46" s="63">
+        <v>45</v>
+      </c>
+      <c r="K46" s="63">
+        <v>60</v>
+      </c>
+      <c r="L46" s="65" t="s">
+        <v>96</v>
+      </c>
+      <c r="M46" s="63" t="s">
+        <v>362</v>
+      </c>
+      <c r="N46" s="64" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="47" spans="2:14" s="40" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B47" s="25"/>
+      <c r="C47" s="23" t="s">
+        <v>354</v>
+      </c>
+      <c r="D47" s="23" t="s">
+        <v>65</v>
+      </c>
+      <c r="E47" s="23">
+        <v>1</v>
+      </c>
+      <c r="F47" s="23">
+        <v>0.3</v>
+      </c>
+      <c r="G47" s="23">
+        <v>3</v>
+      </c>
+      <c r="H47" s="23">
+        <v>7</v>
+      </c>
+      <c r="I47" s="23" t="s">
+        <v>358</v>
+      </c>
+      <c r="J47" s="23">
+        <v>2</v>
+      </c>
+      <c r="K47" s="23">
+        <v>4</v>
+      </c>
+      <c r="L47" s="66" t="s">
+        <v>96</v>
+      </c>
+      <c r="M47" s="23" t="s">
+        <v>363</v>
+      </c>
+      <c r="N47" s="53" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="48" spans="2:14" s="40" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B48" s="25"/>
+      <c r="C48" s="23" t="s">
+        <v>355</v>
+      </c>
+      <c r="D48" s="23" t="s">
+        <v>65</v>
+      </c>
+      <c r="E48" s="23">
+        <v>1</v>
+      </c>
+      <c r="F48" s="23">
+        <v>0.3</v>
+      </c>
+      <c r="G48" s="23">
+        <v>4</v>
+      </c>
+      <c r="H48" s="23">
+        <v>7</v>
+      </c>
+      <c r="I48" s="23" t="s">
+        <v>359</v>
+      </c>
+      <c r="J48" s="23">
+        <v>25</v>
+      </c>
+      <c r="K48" s="23">
+        <v>30</v>
+      </c>
+      <c r="L48" s="66" t="s">
+        <v>96</v>
+      </c>
+      <c r="M48" s="23" t="s">
+        <v>364</v>
+      </c>
+      <c r="N48" s="53" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="49" spans="2:14" s="40" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B49" s="25"/>
+      <c r="C49" s="23" t="s">
+        <v>356</v>
+      </c>
+      <c r="D49" s="23" t="s">
+        <v>65</v>
+      </c>
+      <c r="E49" s="23">
+        <v>1</v>
+      </c>
+      <c r="F49" s="23">
+        <v>0.3</v>
+      </c>
+      <c r="G49" s="23">
+        <v>4</v>
+      </c>
+      <c r="H49" s="23">
+        <v>7</v>
+      </c>
+      <c r="I49" s="23" t="s">
+        <v>360</v>
+      </c>
+      <c r="J49" s="23">
+        <v>3</v>
+      </c>
+      <c r="K49" s="23">
+        <v>5</v>
+      </c>
+      <c r="L49" s="66" t="s">
+        <v>96</v>
+      </c>
+      <c r="M49" s="23" t="s">
+        <v>365</v>
+      </c>
+      <c r="N49" s="53" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="50" spans="2:14" s="40" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B50" s="25"/>
+      <c r="C50" s="23" t="s">
+        <v>357</v>
+      </c>
+      <c r="D50" s="23" t="s">
+        <v>65</v>
+      </c>
+      <c r="E50" s="23">
+        <v>1</v>
+      </c>
+      <c r="F50" s="23">
+        <v>0.3</v>
+      </c>
+      <c r="G50" s="23">
+        <v>5</v>
+      </c>
+      <c r="H50" s="23">
+        <v>7</v>
+      </c>
+      <c r="I50" s="23" t="s">
+        <v>361</v>
+      </c>
+      <c r="J50" s="23">
+        <v>5</v>
+      </c>
+      <c r="K50" s="23">
+        <v>10</v>
+      </c>
+      <c r="L50" s="66" t="s">
+        <v>96</v>
+      </c>
+      <c r="M50" s="23" t="s">
+        <v>367</v>
+      </c>
+      <c r="N50" s="53" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="51" spans="2:14" s="40" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B51" s="41"/>
+      <c r="C51" s="41"/>
+      <c r="D51" s="41"/>
+      <c r="E51" s="41"/>
+      <c r="F51" s="41"/>
+      <c r="G51" s="41"/>
+      <c r="H51" s="41"/>
+      <c r="I51" s="41"/>
+      <c r="J51" s="41"/>
+      <c r="K51" s="41"/>
+      <c r="L51" s="41"/>
+      <c r="M51" s="41"/>
+      <c r="N51" s="41"/>
+    </row>
+    <row r="52" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B52" s="32"/>
+      <c r="C52" s="32"/>
+      <c r="D52" s="32"/>
+      <c r="E52" s="32"/>
+      <c r="F52" s="32"/>
+      <c r="G52" s="32"/>
+      <c r="H52" s="32"/>
+      <c r="I52" s="32"/>
+      <c r="J52" s="32"/>
+      <c r="K52" s="32"/>
+      <c r="L52" s="32"/>
+      <c r="M52" s="31"/>
+    </row>
+    <row r="53" spans="2:14" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B53" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="C48" s="6"/>
-      <c r="D48" s="6"/>
-      <c r="E48" s="6"/>
-      <c r="F48" s="6"/>
-      <c r="G48" s="6"/>
-      <c r="H48" s="6"/>
-      <c r="I48" s="6"/>
-      <c r="J48" s="6"/>
-      <c r="K48" s="6"/>
-      <c r="L48" s="6"/>
-    </row>
-    <row r="49" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B49" s="20"/>
-      <c r="C49" s="20"/>
-      <c r="D49" s="20"/>
-      <c r="E49" s="20"/>
-      <c r="F49" s="58"/>
-      <c r="G49" s="58"/>
-      <c r="H49" s="58"/>
-      <c r="I49" s="20"/>
-      <c r="J49" s="20"/>
-    </row>
-    <row r="50" spans="2:10" ht="96" x14ac:dyDescent="0.25">
-      <c r="B50" s="30" t="s">
+      <c r="C53" s="6"/>
+      <c r="D53" s="6"/>
+      <c r="E53" s="6"/>
+      <c r="F53" s="6"/>
+      <c r="G53" s="6"/>
+      <c r="H53" s="6"/>
+      <c r="I53" s="6"/>
+      <c r="J53" s="6"/>
+      <c r="K53" s="6"/>
+      <c r="L53" s="6"/>
+    </row>
+    <row r="54" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B54" s="20"/>
+      <c r="C54" s="20"/>
+      <c r="D54" s="20"/>
+      <c r="E54" s="20"/>
+      <c r="F54" s="58"/>
+      <c r="G54" s="58"/>
+      <c r="H54" s="58"/>
+      <c r="I54" s="20"/>
+      <c r="J54" s="20"/>
+    </row>
+    <row r="55" spans="2:14" ht="96" x14ac:dyDescent="0.25">
+      <c r="B55" s="30" t="s">
         <v>71</v>
       </c>
-      <c r="C50" s="28" t="s">
+      <c r="C55" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="D50" s="29" t="s">
+      <c r="D55" s="29" t="s">
         <v>70</v>
       </c>
-      <c r="E50" s="29" t="s">
+      <c r="E55" s="29" t="s">
         <v>69</v>
       </c>
-      <c r="F50" s="29" t="s">
+      <c r="F55" s="29" t="s">
         <v>68</v>
       </c>
-      <c r="G50" s="28" t="s">
+      <c r="G55" s="28" t="s">
         <v>67</v>
       </c>
-      <c r="H50" s="28" t="s">
+      <c r="H55" s="28" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="51" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B51" s="27" t="s">
-        <v>1</v>
-      </c>
-      <c r="C51" s="24" t="s">
+    <row r="56" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B56" s="27" t="s">
+        <v>1</v>
+      </c>
+      <c r="C56" s="24" t="s">
         <v>65</v>
-      </c>
-      <c r="D51" s="24">
-        <v>0</v>
-      </c>
-      <c r="E51" s="24">
-        <v>7</v>
-      </c>
-      <c r="F51" s="24">
-        <v>2</v>
-      </c>
-      <c r="G51" s="26" t="s">
-        <v>64</v>
-      </c>
-      <c r="H51" s="26" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="52" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B52" s="27" t="s">
-        <v>1</v>
-      </c>
-      <c r="C52" s="24" t="s">
-        <v>62</v>
-      </c>
-      <c r="D52" s="24">
-        <v>0</v>
-      </c>
-      <c r="E52" s="24">
-        <v>7</v>
-      </c>
-      <c r="F52" s="24">
-        <v>1</v>
-      </c>
-      <c r="G52" s="26" t="s">
-        <v>61</v>
-      </c>
-      <c r="H52" s="26" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="53" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B53" s="27" t="s">
-        <v>1</v>
-      </c>
-      <c r="C53" s="24" t="s">
-        <v>59</v>
-      </c>
-      <c r="D53" s="24">
-        <v>0</v>
-      </c>
-      <c r="E53" s="24">
-        <v>7</v>
-      </c>
-      <c r="F53" s="24">
-        <v>2</v>
-      </c>
-      <c r="G53" s="26" t="s">
-        <v>58</v>
-      </c>
-      <c r="H53" s="26" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="54" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B54" s="27" t="s">
-        <v>1</v>
-      </c>
-      <c r="C54" s="24" t="s">
-        <v>56</v>
-      </c>
-      <c r="D54" s="24">
-        <v>0</v>
-      </c>
-      <c r="E54" s="24">
-        <v>7</v>
-      </c>
-      <c r="F54" s="24">
-        <v>1</v>
-      </c>
-      <c r="G54" s="26" t="s">
-        <v>55</v>
-      </c>
-      <c r="H54" s="26" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="55" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B55" s="25" t="s">
-        <v>1</v>
-      </c>
-      <c r="C55" s="23" t="s">
-        <v>53</v>
-      </c>
-      <c r="D55" s="23">
-        <v>0</v>
-      </c>
-      <c r="E55" s="24">
-        <v>7</v>
-      </c>
-      <c r="F55" s="23">
-        <v>1</v>
-      </c>
-      <c r="G55" s="26" t="s">
-        <v>52</v>
-      </c>
-      <c r="H55" s="26" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="56" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B56" s="25" t="s">
-        <v>1</v>
-      </c>
-      <c r="C56" s="24" t="s">
-        <v>50</v>
       </c>
       <c r="D56" s="24">
         <v>0</v>
@@ -5033,21 +5220,21 @@
         <v>7</v>
       </c>
       <c r="F56" s="24">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G56" s="26" t="s">
-        <v>49</v>
+        <v>64</v>
       </c>
       <c r="H56" s="26" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="57" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B57" s="25" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="57" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B57" s="27" t="s">
         <v>1</v>
       </c>
       <c r="C57" s="24" t="s">
-        <v>47</v>
+        <v>62</v>
       </c>
       <c r="D57" s="24">
         <v>0</v>
@@ -5059,41 +5246,41 @@
         <v>1</v>
       </c>
       <c r="G57" s="26" t="s">
-        <v>46</v>
+        <v>61</v>
       </c>
       <c r="H57" s="26" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="58" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B58" s="25" t="s">
-        <v>1</v>
-      </c>
-      <c r="C58" s="23" t="s">
-        <v>44</v>
-      </c>
-      <c r="D58" s="23">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="58" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B58" s="27" t="s">
+        <v>1</v>
+      </c>
+      <c r="C58" s="24" t="s">
+        <v>59</v>
+      </c>
+      <c r="D58" s="24">
         <v>0</v>
       </c>
       <c r="E58" s="24">
         <v>7</v>
       </c>
-      <c r="F58" s="23">
-        <v>1</v>
-      </c>
-      <c r="G58" s="22" t="s">
-        <v>43</v>
-      </c>
-      <c r="H58" s="22" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="59" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="F58" s="24">
+        <v>2</v>
+      </c>
+      <c r="G58" s="26" t="s">
+        <v>58</v>
+      </c>
+      <c r="H58" s="26" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="59" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B59" s="27" t="s">
         <v>1</v>
       </c>
       <c r="C59" s="24" t="s">
-        <v>177</v>
+        <v>56</v>
       </c>
       <c r="D59" s="24">
         <v>0</v>
@@ -5102,44 +5289,44 @@
         <v>7</v>
       </c>
       <c r="F59" s="24">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G59" s="26" t="s">
-        <v>166</v>
+        <v>55</v>
       </c>
       <c r="H59" s="26" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="60" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B60" s="27" t="s">
-        <v>1</v>
-      </c>
-      <c r="C60" s="24" t="s">
-        <v>174</v>
-      </c>
-      <c r="D60" s="24">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="60" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B60" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="C60" s="23" t="s">
+        <v>53</v>
+      </c>
+      <c r="D60" s="23">
         <v>0</v>
       </c>
       <c r="E60" s="24">
         <v>7</v>
       </c>
-      <c r="F60" s="24">
-        <v>0</v>
+      <c r="F60" s="23">
+        <v>1</v>
       </c>
       <c r="G60" s="26" t="s">
-        <v>169</v>
+        <v>52</v>
       </c>
       <c r="H60" s="26" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="61" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B61" s="27" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="61" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B61" s="25" t="s">
         <v>1</v>
       </c>
       <c r="C61" s="24" t="s">
-        <v>144</v>
+        <v>50</v>
       </c>
       <c r="D61" s="24">
         <v>0</v>
@@ -5148,21 +5335,21 @@
         <v>7</v>
       </c>
       <c r="F61" s="24">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G61" s="26" t="s">
-        <v>167</v>
+        <v>49</v>
       </c>
       <c r="H61" s="26" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="62" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B62" s="27" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="62" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B62" s="25" t="s">
         <v>1</v>
       </c>
       <c r="C62" s="24" t="s">
-        <v>227</v>
+        <v>47</v>
       </c>
       <c r="D62" s="24">
         <v>0</v>
@@ -5174,18 +5361,18 @@
         <v>1</v>
       </c>
       <c r="G62" s="26" t="s">
-        <v>228</v>
+        <v>46</v>
       </c>
       <c r="H62" s="26" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="63" spans="2:10" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="63" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B63" s="25" t="s">
         <v>1</v>
       </c>
       <c r="C63" s="23" t="s">
-        <v>230</v>
+        <v>44</v>
       </c>
       <c r="D63" s="23">
         <v>0</v>
@@ -5196,19 +5383,19 @@
       <c r="F63" s="23">
         <v>1</v>
       </c>
-      <c r="G63" s="26" t="s">
-        <v>231</v>
-      </c>
-      <c r="H63" s="26" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="64" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B64" s="25" t="s">
+      <c r="G63" s="22" t="s">
+        <v>43</v>
+      </c>
+      <c r="H63" s="22" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="64" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B64" s="27" t="s">
         <v>1</v>
       </c>
       <c r="C64" s="24" t="s">
-        <v>233</v>
+        <v>177</v>
       </c>
       <c r="D64" s="24">
         <v>0</v>
@@ -5217,21 +5404,21 @@
         <v>7</v>
       </c>
       <c r="F64" s="24">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G64" s="26" t="s">
-        <v>234</v>
+        <v>166</v>
       </c>
       <c r="H64" s="26" t="s">
-        <v>235</v>
+        <v>170</v>
       </c>
     </row>
     <row r="65" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B65" s="25" t="s">
+      <c r="B65" s="27" t="s">
         <v>1</v>
       </c>
       <c r="C65" s="24" t="s">
-        <v>236</v>
+        <v>174</v>
       </c>
       <c r="D65" s="24">
         <v>0</v>
@@ -5240,36 +5427,36 @@
         <v>7</v>
       </c>
       <c r="F65" s="24">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G65" s="26" t="s">
-        <v>237</v>
+        <v>169</v>
       </c>
       <c r="H65" s="26" t="s">
-        <v>238</v>
+        <v>171</v>
       </c>
     </row>
     <row r="66" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B66" s="25" t="s">
-        <v>1</v>
-      </c>
-      <c r="C66" s="23" t="s">
-        <v>145</v>
-      </c>
-      <c r="D66" s="23">
+      <c r="B66" s="27" t="s">
+        <v>1</v>
+      </c>
+      <c r="C66" s="24" t="s">
+        <v>144</v>
+      </c>
+      <c r="D66" s="24">
         <v>0</v>
       </c>
       <c r="E66" s="24">
         <v>7</v>
       </c>
-      <c r="F66" s="23">
-        <v>0</v>
-      </c>
-      <c r="G66" s="22" t="s">
-        <v>168</v>
-      </c>
-      <c r="H66" s="22" t="s">
-        <v>173</v>
+      <c r="F66" s="24">
+        <v>2</v>
+      </c>
+      <c r="G66" s="26" t="s">
+        <v>167</v>
+      </c>
+      <c r="H66" s="26" t="s">
+        <v>172</v>
       </c>
     </row>
     <row r="67" spans="2:13" x14ac:dyDescent="0.25">
@@ -5277,7 +5464,7 @@
         <v>1</v>
       </c>
       <c r="C67" s="24" t="s">
-        <v>176</v>
+        <v>227</v>
       </c>
       <c r="D67" s="24">
         <v>0</v>
@@ -5289,39 +5476,41 @@
         <v>1</v>
       </c>
       <c r="G67" s="26" t="s">
-        <v>182</v>
-      </c>
-      <c r="H67" s="26"/>
+        <v>228</v>
+      </c>
+      <c r="H67" s="26" t="s">
+        <v>229</v>
+      </c>
     </row>
     <row r="68" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B68" s="27" t="s">
-        <v>1</v>
-      </c>
-      <c r="C68" s="24" t="s">
-        <v>178</v>
-      </c>
-      <c r="D68" s="24">
+      <c r="B68" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="C68" s="23" t="s">
+        <v>230</v>
+      </c>
+      <c r="D68" s="23">
         <v>0</v>
       </c>
       <c r="E68" s="24">
         <v>7</v>
       </c>
-      <c r="F68" s="24">
-        <v>0</v>
+      <c r="F68" s="23">
+        <v>1</v>
       </c>
       <c r="G68" s="26" t="s">
-        <v>183</v>
+        <v>231</v>
       </c>
       <c r="H68" s="26" t="s">
-        <v>184</v>
+        <v>232</v>
       </c>
     </row>
     <row r="69" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B69" s="27" t="s">
+      <c r="B69" s="25" t="s">
         <v>1</v>
       </c>
       <c r="C69" s="24" t="s">
-        <v>179</v>
+        <v>233</v>
       </c>
       <c r="D69" s="24">
         <v>0</v>
@@ -5333,18 +5522,18 @@
         <v>1</v>
       </c>
       <c r="G69" s="26" t="s">
-        <v>209</v>
+        <v>234</v>
       </c>
       <c r="H69" s="26" t="s">
-        <v>210</v>
+        <v>235</v>
       </c>
     </row>
     <row r="70" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B70" s="27" t="s">
+      <c r="B70" s="25" t="s">
         <v>1</v>
       </c>
       <c r="C70" s="24" t="s">
-        <v>312</v>
+        <v>236</v>
       </c>
       <c r="D70" s="24">
         <v>0</v>
@@ -5356,430 +5545,473 @@
         <v>1</v>
       </c>
       <c r="G70" s="26" t="s">
-        <v>313</v>
-      </c>
-      <c r="H70" s="26"/>
+        <v>237</v>
+      </c>
+      <c r="H70" s="26" t="s">
+        <v>238</v>
+      </c>
     </row>
     <row r="71" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B71" s="27" t="s">
-        <v>1</v>
-      </c>
-      <c r="C71" s="24" t="s">
-        <v>314</v>
-      </c>
-      <c r="D71" s="24">
+      <c r="B71" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="C71" s="23" t="s">
+        <v>145</v>
+      </c>
+      <c r="D71" s="23">
         <v>0</v>
       </c>
       <c r="E71" s="24">
         <v>7</v>
       </c>
-      <c r="F71" s="24">
-        <v>1</v>
-      </c>
-      <c r="G71" s="26" t="s">
+      <c r="F71" s="23">
+        <v>0</v>
+      </c>
+      <c r="G71" s="22" t="s">
+        <v>168</v>
+      </c>
+      <c r="H71" s="22" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="72" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B72" s="27" t="s">
+        <v>1</v>
+      </c>
+      <c r="C72" s="24" t="s">
+        <v>176</v>
+      </c>
+      <c r="D72" s="24">
+        <v>0</v>
+      </c>
+      <c r="E72" s="24">
+        <v>7</v>
+      </c>
+      <c r="F72" s="24">
+        <v>1</v>
+      </c>
+      <c r="G72" s="26" t="s">
+        <v>182</v>
+      </c>
+      <c r="H72" s="26"/>
+    </row>
+    <row r="73" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B73" s="27" t="s">
+        <v>1</v>
+      </c>
+      <c r="C73" s="24" t="s">
+        <v>178</v>
+      </c>
+      <c r="D73" s="24">
+        <v>0</v>
+      </c>
+      <c r="E73" s="24">
+        <v>7</v>
+      </c>
+      <c r="F73" s="24">
+        <v>0</v>
+      </c>
+      <c r="G73" s="26" t="s">
+        <v>183</v>
+      </c>
+      <c r="H73" s="26" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="74" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B74" s="27" t="s">
+        <v>1</v>
+      </c>
+      <c r="C74" s="24" t="s">
+        <v>179</v>
+      </c>
+      <c r="D74" s="24">
+        <v>0</v>
+      </c>
+      <c r="E74" s="24">
+        <v>7</v>
+      </c>
+      <c r="F74" s="24">
+        <v>1</v>
+      </c>
+      <c r="G74" s="26" t="s">
+        <v>209</v>
+      </c>
+      <c r="H74" s="26" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="75" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B75" s="27" t="s">
+        <v>1</v>
+      </c>
+      <c r="C75" s="24" t="s">
+        <v>312</v>
+      </c>
+      <c r="D75" s="24">
+        <v>0</v>
+      </c>
+      <c r="E75" s="24">
+        <v>7</v>
+      </c>
+      <c r="F75" s="24">
+        <v>1</v>
+      </c>
+      <c r="G75" s="26" t="s">
+        <v>313</v>
+      </c>
+      <c r="H75" s="26"/>
+    </row>
+    <row r="76" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B76" s="27" t="s">
+        <v>1</v>
+      </c>
+      <c r="C76" s="24" t="s">
+        <v>314</v>
+      </c>
+      <c r="D76" s="24">
+        <v>0</v>
+      </c>
+      <c r="E76" s="24">
+        <v>7</v>
+      </c>
+      <c r="F76" s="24">
+        <v>1</v>
+      </c>
+      <c r="G76" s="26" t="s">
         <v>315</v>
       </c>
-      <c r="H71" s="26"/>
-    </row>
-    <row r="72" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B72" s="56" t="s">
-        <v>1</v>
-      </c>
-      <c r="C72" s="54" t="s">
+      <c r="H76" s="26"/>
+    </row>
+    <row r="77" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B77" s="56" t="s">
+        <v>1</v>
+      </c>
+      <c r="C77" s="54" t="s">
         <v>330</v>
       </c>
-      <c r="D72" s="54">
-        <v>0</v>
-      </c>
-      <c r="E72" s="54">
+      <c r="D77" s="54">
+        <v>0</v>
+      </c>
+      <c r="E77" s="54">
         <v>7</v>
       </c>
-      <c r="F72" s="54">
+      <c r="F77" s="54">
         <v>2</v>
       </c>
-      <c r="G72" s="55" t="s">
+      <c r="G77" s="55" t="s">
         <v>332</v>
       </c>
-      <c r="H72" s="55" t="s">
+      <c r="H77" s="55" t="s">
         <v>333</v>
       </c>
     </row>
-    <row r="73" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="74" spans="2:13" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B74" s="6" t="s">
+    <row r="78" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="79" spans="2:13" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B79" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="C74" s="6"/>
-      <c r="D74" s="6"/>
-      <c r="E74" s="6"/>
-      <c r="F74" s="6"/>
-      <c r="G74" s="6"/>
-      <c r="H74" s="6"/>
-      <c r="I74" s="6"/>
-      <c r="J74" s="6"/>
-      <c r="K74" s="6"/>
-      <c r="L74" s="6"/>
-      <c r="M74" s="6"/>
-    </row>
-    <row r="75" spans="2:13" ht="60" x14ac:dyDescent="0.25">
-      <c r="B75" s="20"/>
-      <c r="C75" s="20"/>
-      <c r="D75" s="20"/>
-      <c r="E75" s="20"/>
-      <c r="F75" s="21" t="s">
+      <c r="C79" s="6"/>
+      <c r="D79" s="6"/>
+      <c r="E79" s="6"/>
+      <c r="F79" s="6"/>
+      <c r="G79" s="6"/>
+      <c r="H79" s="6"/>
+      <c r="I79" s="6"/>
+      <c r="J79" s="6"/>
+      <c r="K79" s="6"/>
+      <c r="L79" s="6"/>
+      <c r="M79" s="6"/>
+    </row>
+    <row r="80" spans="2:13" ht="60" x14ac:dyDescent="0.25">
+      <c r="B80" s="20"/>
+      <c r="C80" s="20"/>
+      <c r="D80" s="20"/>
+      <c r="E80" s="20"/>
+      <c r="F80" s="21" t="s">
         <v>40</v>
       </c>
-      <c r="G75" s="59" t="s">
+      <c r="G80" s="59" t="s">
         <v>39</v>
       </c>
-      <c r="H75" s="59"/>
-      <c r="I75" s="20"/>
-    </row>
-    <row r="76" spans="2:13" ht="142.5" x14ac:dyDescent="0.25">
-      <c r="B76" s="19" t="s">
+      <c r="H80" s="59"/>
+      <c r="I80" s="20"/>
+    </row>
+    <row r="81" spans="2:12" ht="142.5" x14ac:dyDescent="0.25">
+      <c r="B81" s="19" t="s">
         <v>38</v>
       </c>
-      <c r="C76" s="19" t="s">
+      <c r="C81" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="D76" s="18" t="s">
+      <c r="D81" s="18" t="s">
         <v>223</v>
       </c>
-      <c r="E76" s="18" t="s">
+      <c r="E81" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="F76" s="17" t="s">
+      <c r="F81" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="G76" s="17" t="s">
+      <c r="G81" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="H76" s="17" t="s">
+      <c r="H81" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="I76" s="16" t="s">
+      <c r="I81" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="J76" s="16" t="s">
+      <c r="J81" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="K76" s="15" t="s">
+      <c r="K81" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="L76" s="14" t="s">
+      <c r="L81" s="14" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="77" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B77" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="C77" s="11" t="s">
+    <row r="82" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B82" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="C82" s="11" t="s">
         <v>220</v>
       </c>
-      <c r="D77" s="11" t="s">
+      <c r="D82" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="E77" s="11">
-        <v>0</v>
-      </c>
-      <c r="F77" s="10">
-        <v>0</v>
-      </c>
-      <c r="G77" s="10">
+      <c r="E82" s="11">
+        <v>0</v>
+      </c>
+      <c r="F82" s="10">
+        <v>0</v>
+      </c>
+      <c r="G82" s="10">
         <v>15</v>
       </c>
-      <c r="H77" s="10">
+      <c r="H82" s="10">
         <v>200</v>
       </c>
-      <c r="I77" s="9">
+      <c r="I82" s="9">
         <v>0.5</v>
       </c>
-      <c r="J77" s="9">
-        <v>1</v>
-      </c>
-      <c r="K77" s="8" t="s">
+      <c r="J82" s="9">
+        <v>1</v>
+      </c>
+      <c r="K82" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="L77" s="13" t="s">
+      <c r="L82" s="13" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="78" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B78" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="C78" s="11" t="s">
+    <row r="83" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B83" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="C83" s="11" t="s">
         <v>221</v>
       </c>
-      <c r="D78" s="11" t="s">
+      <c r="D83" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="E78" s="11">
-        <v>1</v>
-      </c>
-      <c r="F78" s="10">
-        <v>0</v>
-      </c>
-      <c r="G78" s="10">
+      <c r="E83" s="11">
+        <v>1</v>
+      </c>
+      <c r="F83" s="10">
+        <v>0</v>
+      </c>
+      <c r="G83" s="10">
         <v>60</v>
       </c>
-      <c r="H78" s="10">
+      <c r="H83" s="10">
         <v>300</v>
       </c>
-      <c r="I78" s="9">
+      <c r="I83" s="9">
         <v>0.5</v>
       </c>
-      <c r="J78" s="9">
-        <v>1</v>
-      </c>
-      <c r="K78" s="8" t="s">
+      <c r="J83" s="9">
+        <v>1</v>
+      </c>
+      <c r="K83" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="L78" s="13" t="s">
+      <c r="L83" s="13" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="79" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B79" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="C79" s="11" t="s">
+    <row r="84" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B84" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="C84" s="11" t="s">
         <v>222</v>
       </c>
-      <c r="D79" s="11" t="s">
+      <c r="D84" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="E79" s="11">
+      <c r="E84" s="11">
         <v>2</v>
       </c>
-      <c r="F79" s="10">
-        <v>0</v>
-      </c>
-      <c r="G79" s="10">
+      <c r="F84" s="10">
+        <v>0</v>
+      </c>
+      <c r="G84" s="10">
         <v>240</v>
       </c>
-      <c r="H79" s="10">
+      <c r="H84" s="10">
         <v>600</v>
       </c>
-      <c r="I79" s="9">
+      <c r="I84" s="9">
         <v>0.5</v>
       </c>
-      <c r="J79" s="9">
-        <v>1</v>
-      </c>
-      <c r="K79" s="8" t="s">
+      <c r="J84" s="9">
+        <v>1</v>
+      </c>
+      <c r="K84" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="L79" s="7" t="s">
+      <c r="L84" s="7" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="81" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="82" spans="2:7" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B82" s="6" t="s">
+    <row r="86" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="87" spans="2:12" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B87" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="C82" s="6"/>
-      <c r="D82" s="6"/>
-      <c r="E82" s="6"/>
-      <c r="F82" s="6"/>
-      <c r="G82" s="6"/>
-    </row>
-    <row r="84" spans="2:7" ht="135.75" x14ac:dyDescent="0.25">
-      <c r="B84" s="5" t="s">
+      <c r="C87" s="6"/>
+      <c r="D87" s="6"/>
+      <c r="E87" s="6"/>
+      <c r="F87" s="6"/>
+      <c r="G87" s="6"/>
+    </row>
+    <row r="89" spans="2:12" ht="135.75" x14ac:dyDescent="0.25">
+      <c r="B89" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="C84" s="4" t="s">
+      <c r="C89" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D84" s="3" t="s">
+      <c r="D89" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E84" s="3" t="s">
+      <c r="E89" s="3" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="85" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B85" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C85" s="1" t="s">
+    <row r="90" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B90" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C90" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D85" s="1">
+      <c r="D90" s="1">
         <v>0.1</v>
       </c>
-      <c r="E85" s="1">
+      <c r="E90" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="86" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B86" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C86" s="1" t="s">
+    <row r="91" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B91" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C91" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D86" s="1">
+      <c r="D91" s="1">
         <v>0.7</v>
       </c>
-      <c r="E86" s="1">
+      <c r="E91" s="1">
         <v>6</v>
       </c>
     </row>
-    <row r="87" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B87" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C87" s="1" t="s">
+    <row r="92" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B92" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C92" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D87" s="1">
-        <v>1</v>
-      </c>
-      <c r="E87" s="1">
+      <c r="D92" s="1">
+        <v>1</v>
+      </c>
+      <c r="E92" s="1">
         <v>12</v>
       </c>
     </row>
-    <row r="88" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B88" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C88" s="1" t="s">
+    <row r="93" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B93" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C93" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D88" s="1">
+      <c r="D93" s="1">
         <v>1.5</v>
       </c>
-      <c r="E88" s="1">
+      <c r="E93" s="1">
         <v>18</v>
       </c>
     </row>
-    <row r="89" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B89" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C89" s="1" t="s">
+    <row r="94" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B94" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C94" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D89" s="1">
+      <c r="D94" s="1">
         <v>2</v>
       </c>
-      <c r="E89" s="1">
+      <c r="E94" s="1">
         <v>26</v>
       </c>
     </row>
-    <row r="90" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B90" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C90" s="1" t="s">
+    <row r="95" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B95" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C95" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D90" s="1">
+      <c r="D95" s="1">
         <v>2.5</v>
       </c>
-      <c r="E90" s="1">
+      <c r="E95" s="1">
         <v>35</v>
       </c>
     </row>
-    <row r="91" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B91" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C91" s="1" t="s">
+    <row r="96" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B96" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C96" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D91" s="1">
+      <c r="D96" s="1">
         <v>3</v>
       </c>
-      <c r="E91" s="1">
+      <c r="E96" s="1">
         <v>45</v>
       </c>
     </row>
-    <row r="92" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B92" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C92" s="1" t="s">
+    <row r="97" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B97" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C97" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D92" s="1">
+      <c r="D97" s="1">
         <v>4</v>
       </c>
-      <c r="E92" s="1">
+      <c r="E97" s="1">
         <v>56</v>
-      </c>
-    </row>
-    <row r="93" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B93" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C93" s="1" t="s">
-        <v>214</v>
-      </c>
-      <c r="D93" s="1">
-        <v>4.5</v>
-      </c>
-      <c r="E93" s="1">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="94" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B94" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C94" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D94" s="1">
-        <v>5</v>
-      </c>
-      <c r="E94" s="1">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="95" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B95" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C95" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D95" s="1">
-        <v>7</v>
-      </c>
-      <c r="E95" s="1">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="96" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B96" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C96" s="1" t="s">
-        <v>219</v>
-      </c>
-      <c r="D96" s="42">
-        <v>7.5</v>
-      </c>
-      <c r="E96" s="42">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="97" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B97" s="51" t="s">
-        <v>1</v>
-      </c>
-      <c r="C97" s="42" t="s">
-        <v>305</v>
-      </c>
-      <c r="D97" s="42">
-        <v>8</v>
-      </c>
-      <c r="E97" s="42">
-        <v>70</v>
       </c>
     </row>
     <row r="98" spans="2:7" x14ac:dyDescent="0.25">
@@ -5787,13 +6019,13 @@
         <v>1</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>334</v>
-      </c>
-      <c r="D98" s="42">
-        <v>8.1</v>
-      </c>
-      <c r="E98" s="42">
-        <v>75</v>
+        <v>214</v>
+      </c>
+      <c r="D98" s="1">
+        <v>4.5</v>
+      </c>
+      <c r="E98" s="1">
+        <v>62</v>
       </c>
     </row>
     <row r="99" spans="2:7" x14ac:dyDescent="0.25">
@@ -5801,13 +6033,13 @@
         <v>1</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>335</v>
-      </c>
-      <c r="D99" s="42">
-        <v>8</v>
-      </c>
-      <c r="E99" s="42">
-        <v>75</v>
+        <v>12</v>
+      </c>
+      <c r="D99" s="1">
+        <v>5</v>
+      </c>
+      <c r="E99" s="1">
+        <v>65</v>
       </c>
     </row>
     <row r="100" spans="2:7" x14ac:dyDescent="0.25">
@@ -5815,13 +6047,13 @@
         <v>1</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>336</v>
-      </c>
-      <c r="D100" s="42">
-        <v>7.5</v>
-      </c>
-      <c r="E100" s="42">
-        <v>75</v>
+        <v>11</v>
+      </c>
+      <c r="D100" s="1">
+        <v>7</v>
+      </c>
+      <c r="E100" s="1">
+        <v>70</v>
       </c>
     </row>
     <row r="101" spans="2:7" x14ac:dyDescent="0.25">
@@ -5829,13 +6061,13 @@
         <v>1</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>337</v>
+        <v>219</v>
       </c>
       <c r="D101" s="42">
-        <v>8</v>
+        <v>7.5</v>
       </c>
       <c r="E101" s="42">
-        <v>75</v>
+        <v>70</v>
       </c>
     </row>
     <row r="102" spans="2:7" x14ac:dyDescent="0.25">
@@ -5843,102 +6075,136 @@
         <v>1</v>
       </c>
       <c r="C102" s="42" t="s">
+        <v>305</v>
+      </c>
+      <c r="D102" s="42">
+        <v>8</v>
+      </c>
+      <c r="E102" s="42">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="103" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B103" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C103" s="1" t="s">
+        <v>334</v>
+      </c>
+      <c r="D103" s="42">
+        <v>8.1</v>
+      </c>
+      <c r="E103" s="42">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="104" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B104" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C104" s="1" t="s">
+        <v>335</v>
+      </c>
+      <c r="D104" s="42">
+        <v>8</v>
+      </c>
+      <c r="E104" s="42">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="105" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B105" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C105" s="1" t="s">
+        <v>336</v>
+      </c>
+      <c r="D105" s="42">
+        <v>7.5</v>
+      </c>
+      <c r="E105" s="42">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="106" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B106" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C106" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="D106" s="42">
+        <v>8</v>
+      </c>
+      <c r="E106" s="42">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="107" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B107" s="51" t="s">
+        <v>1</v>
+      </c>
+      <c r="C107" s="42" t="s">
         <v>338</v>
       </c>
-      <c r="D102" s="42">
+      <c r="D107" s="42">
         <v>7.5</v>
       </c>
-      <c r="E102" s="42">
+      <c r="E107" s="42">
         <v>75</v>
       </c>
     </row>
-    <row r="103" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="104" spans="2:7" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B104" s="6" t="s">
+    <row r="108" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="109" spans="2:7" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B109" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C104" s="6"/>
-      <c r="D104" s="6"/>
-      <c r="E104" s="6"/>
-      <c r="F104" s="6"/>
-      <c r="G104" s="6"/>
-    </row>
-    <row r="106" spans="2:7" ht="142.5" x14ac:dyDescent="0.25">
-      <c r="B106" s="5" t="s">
+      <c r="C109" s="6"/>
+      <c r="D109" s="6"/>
+      <c r="E109" s="6"/>
+      <c r="F109" s="6"/>
+      <c r="G109" s="6"/>
+    </row>
+    <row r="111" spans="2:7" ht="142.5" x14ac:dyDescent="0.25">
+      <c r="B111" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C106" s="4" t="s">
+      <c r="C111" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D106" s="4" t="s">
+      <c r="D111" s="4" t="s">
         <v>223</v>
       </c>
-      <c r="E106" s="3" t="s">
+      <c r="E111" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="107" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B107" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C107" s="1" t="s">
+    <row r="112" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B112" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C112" s="1" t="s">
         <v>224</v>
       </c>
-      <c r="D107" s="1" t="s">
+      <c r="D112" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E107" s="1">
+      <c r="E112" s="1">
         <v>0.05</v>
       </c>
     </row>
-    <row r="108" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B108" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C108" s="1" t="s">
+    <row r="113" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B113" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C113" s="1" t="s">
         <v>225</v>
       </c>
-      <c r="D108" s="1" t="s">
+      <c r="D113" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E108" s="1">
+      <c r="E113" s="1">
         <v>0.1</v>
-      </c>
-    </row>
-    <row r="109" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B109" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C109" s="1" t="s">
-        <v>226</v>
-      </c>
-      <c r="D109" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E109" s="1">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="110" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="111" spans="2:7" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B111" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C111" s="6"/>
-      <c r="D111" s="6"/>
-      <c r="E111" s="6"/>
-      <c r="F111" s="6"/>
-      <c r="G111" s="6"/>
-    </row>
-    <row r="113" spans="2:7" ht="132" x14ac:dyDescent="0.25">
-      <c r="B113" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C113" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D113" s="3" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="114" spans="2:7" x14ac:dyDescent="0.25">
@@ -5946,16 +6212,19 @@
         <v>1</v>
       </c>
       <c r="C114" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D114" s="1">
-        <v>0.7</v>
+        <v>226</v>
+      </c>
+      <c r="D114" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E114" s="1">
+        <v>0.2</v>
       </c>
     </row>
     <row r="115" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="116" spans="2:7" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B116" s="6" t="s">
-        <v>239</v>
+        <v>5</v>
       </c>
       <c r="C116" s="6"/>
       <c r="D116" s="6"/>
@@ -5963,88 +6232,51 @@
       <c r="F116" s="6"/>
       <c r="G116" s="6"/>
     </row>
-    <row r="118" spans="2:7" ht="68.25" x14ac:dyDescent="0.25">
-      <c r="B118" s="44" t="s">
+    <row r="118" spans="2:7" ht="132" x14ac:dyDescent="0.25">
+      <c r="B118" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C118" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D118" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="119" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B119" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C119" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D119" s="1">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="120" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="121" spans="2:7" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B121" s="6" t="s">
+        <v>239</v>
+      </c>
+      <c r="C121" s="6"/>
+      <c r="D121" s="6"/>
+      <c r="E121" s="6"/>
+      <c r="F121" s="6"/>
+      <c r="G121" s="6"/>
+    </row>
+    <row r="123" spans="2:7" ht="68.25" x14ac:dyDescent="0.25">
+      <c r="B123" s="44" t="s">
         <v>240</v>
       </c>
-      <c r="C118" s="44" t="s">
+      <c r="C123" s="44" t="s">
         <v>3</v>
       </c>
-      <c r="D118" s="45" t="s">
+      <c r="D123" s="45" t="s">
         <v>241</v>
       </c>
-      <c r="E118" s="45" t="s">
+      <c r="E123" s="45" t="s">
         <v>242</v>
-      </c>
-    </row>
-    <row r="119" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B119" s="43" t="s">
-        <v>1</v>
-      </c>
-      <c r="C119" s="46" t="s">
-        <v>80</v>
-      </c>
-      <c r="D119" s="46" t="s">
-        <v>263</v>
-      </c>
-      <c r="E119" s="43" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="120" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B120" s="43" t="s">
-        <v>1</v>
-      </c>
-      <c r="C120" s="46" t="s">
-        <v>93</v>
-      </c>
-      <c r="D120" s="46" t="s">
-        <v>264</v>
-      </c>
-      <c r="E120" s="43" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="121" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B121" s="43" t="s">
-        <v>1</v>
-      </c>
-      <c r="C121" s="46" t="s">
-        <v>124</v>
-      </c>
-      <c r="D121" s="46" t="s">
-        <v>265</v>
-      </c>
-      <c r="E121" s="43" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="122" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B122" s="43" t="s">
-        <v>1</v>
-      </c>
-      <c r="C122" s="46" t="s">
-        <v>108</v>
-      </c>
-      <c r="D122" s="46" t="s">
-        <v>108</v>
-      </c>
-      <c r="E122" s="43" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="123" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B123" s="43" t="s">
-        <v>1</v>
-      </c>
-      <c r="C123" s="46" t="s">
-        <v>120</v>
-      </c>
-      <c r="D123" s="46" t="s">
-        <v>120</v>
-      </c>
-      <c r="E123" s="43" t="b">
-        <v>0</v>
       </c>
     </row>
     <row r="124" spans="2:7" x14ac:dyDescent="0.25">
@@ -6052,13 +6284,13 @@
         <v>1</v>
       </c>
       <c r="C124" s="46" t="s">
-        <v>109</v>
+        <v>80</v>
       </c>
       <c r="D124" s="46" t="s">
-        <v>109</v>
+        <v>263</v>
       </c>
       <c r="E124" s="43" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="125" spans="2:7" x14ac:dyDescent="0.25">
@@ -6066,10 +6298,10 @@
         <v>1</v>
       </c>
       <c r="C125" s="46" t="s">
-        <v>111</v>
+        <v>93</v>
       </c>
       <c r="D125" s="46" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="E125" s="43" t="b">
         <v>1</v>
@@ -6080,10 +6312,10 @@
         <v>1</v>
       </c>
       <c r="C126" s="46" t="s">
-        <v>243</v>
+        <v>124</v>
       </c>
       <c r="D126" s="46" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="E126" s="43" t="b">
         <v>1</v>
@@ -6094,13 +6326,13 @@
         <v>1</v>
       </c>
       <c r="C127" s="46" t="s">
-        <v>244</v>
+        <v>108</v>
       </c>
       <c r="D127" s="46" t="s">
-        <v>268</v>
+        <v>108</v>
       </c>
       <c r="E127" s="43" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="128" spans="2:7" x14ac:dyDescent="0.25">
@@ -6108,13 +6340,13 @@
         <v>1</v>
       </c>
       <c r="C128" s="46" t="s">
-        <v>204</v>
+        <v>120</v>
       </c>
       <c r="D128" s="46" t="s">
-        <v>269</v>
+        <v>120</v>
       </c>
       <c r="E128" s="43" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="129" spans="2:5" x14ac:dyDescent="0.25">
@@ -6122,13 +6354,13 @@
         <v>1</v>
       </c>
       <c r="C129" s="46" t="s">
-        <v>203</v>
+        <v>109</v>
       </c>
       <c r="D129" s="46" t="s">
-        <v>270</v>
+        <v>109</v>
       </c>
       <c r="E129" s="43" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="130" spans="2:5" x14ac:dyDescent="0.25">
@@ -6136,10 +6368,10 @@
         <v>1</v>
       </c>
       <c r="C130" s="46" t="s">
-        <v>198</v>
+        <v>111</v>
       </c>
       <c r="D130" s="46" t="s">
-        <v>271</v>
+        <v>266</v>
       </c>
       <c r="E130" s="43" t="b">
         <v>1</v>
@@ -6150,10 +6382,10 @@
         <v>1</v>
       </c>
       <c r="C131" s="46" t="s">
-        <v>202</v>
+        <v>243</v>
       </c>
       <c r="D131" s="46" t="s">
-        <v>272</v>
+        <v>267</v>
       </c>
       <c r="E131" s="43" t="b">
         <v>1</v>
@@ -6164,10 +6396,10 @@
         <v>1</v>
       </c>
       <c r="C132" s="46" t="s">
-        <v>201</v>
+        <v>244</v>
       </c>
       <c r="D132" s="46" t="s">
-        <v>273</v>
+        <v>268</v>
       </c>
       <c r="E132" s="43" t="b">
         <v>1</v>
@@ -6178,10 +6410,10 @@
         <v>1</v>
       </c>
       <c r="C133" s="46" t="s">
-        <v>199</v>
+        <v>204</v>
       </c>
       <c r="D133" s="46" t="s">
-        <v>274</v>
+        <v>269</v>
       </c>
       <c r="E133" s="43" t="b">
         <v>1</v>
@@ -6192,10 +6424,10 @@
         <v>1</v>
       </c>
       <c r="C134" s="46" t="s">
-        <v>200</v>
+        <v>203</v>
       </c>
       <c r="D134" s="46" t="s">
-        <v>275</v>
+        <v>270</v>
       </c>
       <c r="E134" s="43" t="b">
         <v>1</v>
@@ -6206,10 +6438,10 @@
         <v>1</v>
       </c>
       <c r="C135" s="46" t="s">
-        <v>113</v>
+        <v>198</v>
       </c>
       <c r="D135" s="46" t="s">
-        <v>276</v>
+        <v>271</v>
       </c>
       <c r="E135" s="43" t="b">
         <v>1</v>
@@ -6220,13 +6452,13 @@
         <v>1</v>
       </c>
       <c r="C136" s="46" t="s">
-        <v>245</v>
+        <v>202</v>
       </c>
       <c r="D136" s="46" t="s">
-        <v>245</v>
+        <v>272</v>
       </c>
       <c r="E136" s="43" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="137" spans="2:5" x14ac:dyDescent="0.25">
@@ -6234,10 +6466,10 @@
         <v>1</v>
       </c>
       <c r="C137" s="46" t="s">
-        <v>83</v>
+        <v>201</v>
       </c>
       <c r="D137" s="46" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
       <c r="E137" s="43" t="b">
         <v>1</v>
@@ -6248,10 +6480,10 @@
         <v>1</v>
       </c>
       <c r="C138" s="46" t="s">
-        <v>96</v>
+        <v>199</v>
       </c>
       <c r="D138" s="46" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="E138" s="43" t="b">
         <v>1</v>
@@ -6262,10 +6494,10 @@
         <v>1</v>
       </c>
       <c r="C139" s="46" t="s">
-        <v>246</v>
+        <v>200</v>
       </c>
       <c r="D139" s="46" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="E139" s="43" t="b">
         <v>1</v>
@@ -6276,10 +6508,10 @@
         <v>1</v>
       </c>
       <c r="C140" s="46" t="s">
-        <v>247</v>
+        <v>113</v>
       </c>
       <c r="D140" s="46" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
       <c r="E140" s="43" t="b">
         <v>1</v>
@@ -6290,13 +6522,13 @@
         <v>1</v>
       </c>
       <c r="C141" s="46" t="s">
-        <v>102</v>
+        <v>245</v>
       </c>
       <c r="D141" s="46" t="s">
-        <v>281</v>
+        <v>245</v>
       </c>
       <c r="E141" s="43" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="142" spans="2:5" x14ac:dyDescent="0.25">
@@ -6304,10 +6536,10 @@
         <v>1</v>
       </c>
       <c r="C142" s="46" t="s">
-        <v>248</v>
+        <v>83</v>
       </c>
       <c r="D142" s="46" t="s">
-        <v>303</v>
+        <v>277</v>
       </c>
       <c r="E142" s="43" t="b">
         <v>1</v>
@@ -6318,10 +6550,10 @@
         <v>1</v>
       </c>
       <c r="C143" s="46" t="s">
-        <v>122</v>
+        <v>96</v>
       </c>
       <c r="D143" s="46" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
       <c r="E143" s="43" t="b">
         <v>1</v>
@@ -6332,10 +6564,10 @@
         <v>1</v>
       </c>
       <c r="C144" s="46" t="s">
-        <v>88</v>
+        <v>246</v>
       </c>
       <c r="D144" s="46" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
       <c r="E144" s="43" t="b">
         <v>1</v>
@@ -6346,10 +6578,10 @@
         <v>1</v>
       </c>
       <c r="C145" s="46" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="D145" s="46" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="E145" s="43" t="b">
         <v>1</v>
@@ -6360,10 +6592,10 @@
         <v>1</v>
       </c>
       <c r="C146" s="46" t="s">
-        <v>301</v>
+        <v>102</v>
       </c>
       <c r="D146" s="46" t="s">
-        <v>302</v>
+        <v>281</v>
       </c>
       <c r="E146" s="43" t="b">
         <v>1</v>
@@ -6374,13 +6606,13 @@
         <v>1</v>
       </c>
       <c r="C147" s="46" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="D147" s="46" t="s">
-        <v>250</v>
+        <v>303</v>
       </c>
       <c r="E147" s="43" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="148" spans="2:5" x14ac:dyDescent="0.25">
@@ -6388,13 +6620,13 @@
         <v>1</v>
       </c>
       <c r="C148" s="46" t="s">
-        <v>115</v>
+        <v>122</v>
       </c>
       <c r="D148" s="46" t="s">
-        <v>115</v>
+        <v>282</v>
       </c>
       <c r="E148" s="43" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="149" spans="2:5" x14ac:dyDescent="0.25">
@@ -6402,10 +6634,10 @@
         <v>1</v>
       </c>
       <c r="C149" s="46" t="s">
-        <v>251</v>
+        <v>88</v>
       </c>
       <c r="D149" s="46" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="E149" s="43" t="b">
         <v>1</v>
@@ -6416,10 +6648,10 @@
         <v>1</v>
       </c>
       <c r="C150" s="46" t="s">
-        <v>91</v>
+        <v>249</v>
       </c>
       <c r="D150" s="46" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="E150" s="43" t="b">
         <v>1</v>
@@ -6430,10 +6662,10 @@
         <v>1</v>
       </c>
       <c r="C151" s="46" t="s">
-        <v>252</v>
+        <v>301</v>
       </c>
       <c r="D151" s="46" t="s">
-        <v>287</v>
+        <v>302</v>
       </c>
       <c r="E151" s="43" t="b">
         <v>1</v>
@@ -6444,13 +6676,13 @@
         <v>1</v>
       </c>
       <c r="C152" s="46" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="D152" s="46" t="s">
-        <v>288</v>
+        <v>250</v>
       </c>
       <c r="E152" s="43" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="153" spans="2:5" x14ac:dyDescent="0.25">
@@ -6458,13 +6690,13 @@
         <v>1</v>
       </c>
       <c r="C153" s="46" t="s">
-        <v>254</v>
+        <v>115</v>
       </c>
       <c r="D153" s="46" t="s">
-        <v>289</v>
+        <v>115</v>
       </c>
       <c r="E153" s="43" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="154" spans="2:5" x14ac:dyDescent="0.25">
@@ -6472,10 +6704,10 @@
         <v>1</v>
       </c>
       <c r="C154" s="46" t="s">
-        <v>86</v>
+        <v>251</v>
       </c>
       <c r="D154" s="46" t="s">
-        <v>290</v>
+        <v>285</v>
       </c>
       <c r="E154" s="43" t="b">
         <v>1</v>
@@ -6486,13 +6718,13 @@
         <v>1</v>
       </c>
       <c r="C155" s="46" t="s">
-        <v>73</v>
+        <v>91</v>
       </c>
       <c r="D155" s="46" t="s">
-        <v>73</v>
+        <v>286</v>
       </c>
       <c r="E155" s="43" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="156" spans="2:5" x14ac:dyDescent="0.25">
@@ -6500,13 +6732,13 @@
         <v>1</v>
       </c>
       <c r="C156" s="46" t="s">
-        <v>107</v>
+        <v>252</v>
       </c>
       <c r="D156" s="46" t="s">
-        <v>107</v>
+        <v>287</v>
       </c>
       <c r="E156" s="43" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="157" spans="2:5" x14ac:dyDescent="0.25">
@@ -6514,10 +6746,10 @@
         <v>1</v>
       </c>
       <c r="C157" s="46" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="D157" s="46" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="E157" s="43" t="b">
         <v>1</v>
@@ -6528,10 +6760,10 @@
         <v>1</v>
       </c>
       <c r="C158" s="46" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="D158" s="46" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="E158" s="43" t="b">
         <v>1</v>
@@ -6542,10 +6774,10 @@
         <v>1</v>
       </c>
       <c r="C159" s="46" t="s">
-        <v>77</v>
+        <v>86</v>
       </c>
       <c r="D159" s="46" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="E159" s="43" t="b">
         <v>1</v>
@@ -6556,13 +6788,13 @@
         <v>1</v>
       </c>
       <c r="C160" s="46" t="s">
-        <v>105</v>
+        <v>73</v>
       </c>
       <c r="D160" s="46" t="s">
-        <v>294</v>
+        <v>73</v>
       </c>
       <c r="E160" s="43" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="161" spans="2:5" x14ac:dyDescent="0.25">
@@ -6570,13 +6802,13 @@
         <v>1</v>
       </c>
       <c r="C161" s="46" t="s">
-        <v>257</v>
+        <v>107</v>
       </c>
       <c r="D161" s="46" t="s">
-        <v>295</v>
+        <v>107</v>
       </c>
       <c r="E161" s="43" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="162" spans="2:5" x14ac:dyDescent="0.25">
@@ -6584,10 +6816,10 @@
         <v>1</v>
       </c>
       <c r="C162" s="46" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="D162" s="46" t="s">
-        <v>296</v>
+        <v>291</v>
       </c>
       <c r="E162" s="43" t="b">
         <v>1</v>
@@ -6598,10 +6830,10 @@
         <v>1</v>
       </c>
       <c r="C163" s="46" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="D163" s="46" t="s">
-        <v>297</v>
+        <v>292</v>
       </c>
       <c r="E163" s="43" t="b">
         <v>1</v>
@@ -6612,13 +6844,13 @@
         <v>1</v>
       </c>
       <c r="C164" s="46" t="s">
-        <v>260</v>
+        <v>77</v>
       </c>
       <c r="D164" s="46" t="s">
-        <v>260</v>
+        <v>293</v>
       </c>
       <c r="E164" s="43" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="165" spans="2:5" x14ac:dyDescent="0.25">
@@ -6626,10 +6858,10 @@
         <v>1</v>
       </c>
       <c r="C165" s="46" t="s">
-        <v>99</v>
+        <v>105</v>
       </c>
       <c r="D165" s="46" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="E165" s="43" t="b">
         <v>1</v>
@@ -6640,10 +6872,10 @@
         <v>1</v>
       </c>
       <c r="C166" s="46" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="D166" s="46" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="E166" s="43" t="b">
         <v>1</v>
@@ -6654,10 +6886,10 @@
         <v>1</v>
       </c>
       <c r="C167" s="46" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="D167" s="46" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="E167" s="43" t="b">
         <v>1</v>
@@ -6668,10 +6900,10 @@
         <v>1</v>
       </c>
       <c r="C168" s="46" t="s">
-        <v>309</v>
+        <v>259</v>
       </c>
       <c r="D168" s="46" t="s">
-        <v>306</v>
+        <v>297</v>
       </c>
       <c r="E168" s="43" t="b">
         <v>1</v>
@@ -6682,13 +6914,13 @@
         <v>1</v>
       </c>
       <c r="C169" s="46" t="s">
-        <v>310</v>
+        <v>260</v>
       </c>
       <c r="D169" s="46" t="s">
-        <v>307</v>
+        <v>260</v>
       </c>
       <c r="E169" s="43" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="170" spans="2:5" x14ac:dyDescent="0.25">
@@ -6696,10 +6928,10 @@
         <v>1</v>
       </c>
       <c r="C170" s="46" t="s">
-        <v>311</v>
+        <v>99</v>
       </c>
       <c r="D170" s="46" t="s">
-        <v>308</v>
+        <v>298</v>
       </c>
       <c r="E170" s="43" t="b">
         <v>1</v>
@@ -6710,10 +6942,10 @@
         <v>1</v>
       </c>
       <c r="C171" s="46" t="s">
-        <v>319</v>
+        <v>261</v>
       </c>
       <c r="D171" s="46" t="s">
-        <v>320</v>
+        <v>299</v>
       </c>
       <c r="E171" s="43" t="b">
         <v>1</v>
@@ -6724,10 +6956,10 @@
         <v>1</v>
       </c>
       <c r="C172" s="46" t="s">
-        <v>321</v>
+        <v>262</v>
       </c>
       <c r="D172" s="46" t="s">
-        <v>322</v>
+        <v>300</v>
       </c>
       <c r="E172" s="43" t="b">
         <v>1</v>
@@ -6738,10 +6970,10 @@
         <v>1</v>
       </c>
       <c r="C173" s="46" t="s">
-        <v>323</v>
+        <v>309</v>
       </c>
       <c r="D173" s="46" t="s">
-        <v>324</v>
+        <v>306</v>
       </c>
       <c r="E173" s="43" t="b">
         <v>1</v>
@@ -6752,10 +6984,10 @@
         <v>1</v>
       </c>
       <c r="C174" s="46" t="s">
-        <v>316</v>
+        <v>310</v>
       </c>
       <c r="D174" s="46" t="s">
-        <v>339</v>
+        <v>307</v>
       </c>
       <c r="E174" s="43" t="b">
         <v>1</v>
@@ -6766,10 +6998,10 @@
         <v>1</v>
       </c>
       <c r="C175" s="46" t="s">
-        <v>317</v>
+        <v>311</v>
       </c>
       <c r="D175" s="46" t="s">
-        <v>340</v>
+        <v>308</v>
       </c>
       <c r="E175" s="43" t="b">
         <v>1</v>
@@ -6780,10 +7012,10 @@
         <v>1</v>
       </c>
       <c r="C176" s="46" t="s">
-        <v>74</v>
+        <v>319</v>
       </c>
       <c r="D176" s="46" t="s">
-        <v>341</v>
+        <v>320</v>
       </c>
       <c r="E176" s="43" t="b">
         <v>1</v>
@@ -6794,10 +7026,10 @@
         <v>1</v>
       </c>
       <c r="C177" s="46" t="s">
-        <v>346</v>
+        <v>321</v>
       </c>
       <c r="D177" s="46" t="s">
-        <v>342</v>
+        <v>322</v>
       </c>
       <c r="E177" s="43" t="b">
         <v>1</v>
@@ -6808,10 +7040,10 @@
         <v>1</v>
       </c>
       <c r="C178" s="46" t="s">
-        <v>347</v>
+        <v>323</v>
       </c>
       <c r="D178" s="46" t="s">
-        <v>343</v>
+        <v>324</v>
       </c>
       <c r="E178" s="43" t="b">
         <v>1</v>
@@ -6822,10 +7054,10 @@
         <v>1</v>
       </c>
       <c r="C179" s="46" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="D179" s="46" t="s">
-        <v>344</v>
+        <v>339</v>
       </c>
       <c r="E179" s="43" t="b">
         <v>1</v>
@@ -6836,12 +7068,82 @@
         <v>1</v>
       </c>
       <c r="C180" s="46" t="s">
+        <v>317</v>
+      </c>
+      <c r="D180" s="46" t="s">
+        <v>340</v>
+      </c>
+      <c r="E180" s="43" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="181" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B181" s="43" t="s">
+        <v>1</v>
+      </c>
+      <c r="C181" s="46" t="s">
+        <v>74</v>
+      </c>
+      <c r="D181" s="46" t="s">
+        <v>341</v>
+      </c>
+      <c r="E181" s="43" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="182" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B182" s="43" t="s">
+        <v>1</v>
+      </c>
+      <c r="C182" s="46" t="s">
+        <v>346</v>
+      </c>
+      <c r="D182" s="46" t="s">
+        <v>342</v>
+      </c>
+      <c r="E182" s="43" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="183" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B183" s="43" t="s">
+        <v>1</v>
+      </c>
+      <c r="C183" s="46" t="s">
+        <v>347</v>
+      </c>
+      <c r="D183" s="46" t="s">
+        <v>343</v>
+      </c>
+      <c r="E183" s="43" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="184" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B184" s="43" t="s">
+        <v>1</v>
+      </c>
+      <c r="C184" s="46" t="s">
+        <v>318</v>
+      </c>
+      <c r="D184" s="46" t="s">
+        <v>344</v>
+      </c>
+      <c r="E184" s="43" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="185" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B185" s="43" t="s">
+        <v>1</v>
+      </c>
+      <c r="C185" s="46" t="s">
         <v>348</v>
       </c>
-      <c r="D180" s="46" t="s">
+      <c r="D185" s="46" t="s">
         <v>345</v>
       </c>
-      <c r="E180" s="43" t="b">
+      <c r="E185" s="43" t="b">
         <v>1</v>
       </c>
     </row>
@@ -6849,11 +7151,11 @@
   <mergeCells count="4">
     <mergeCell ref="J3:K3"/>
     <mergeCell ref="M3:P3"/>
-    <mergeCell ref="F49:H49"/>
-    <mergeCell ref="G75:H75"/>
+    <mergeCell ref="F54:H54"/>
+    <mergeCell ref="G80:H80"/>
   </mergeCells>
-  <conditionalFormatting sqref="C77:E79">
-    <cfRule type="duplicateValues" dxfId="68" priority="2"/>
+  <conditionalFormatting sqref="C82:E84">
+    <cfRule type="duplicateValues" dxfId="0" priority="2"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Adding new mission 'kill fishes'
Former-commit-id: 2df96a5ab35d69e9765c4c8b8d9d16dc7359c872
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Missions.xlsx
+++ b/Docs/Content/HungryDragonContent_Missions.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="674" uniqueCount="370">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="675" uniqueCount="370">
   <si>
     <t>single_run</t>
   </si>
@@ -1667,15 +1667,15 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3222,8 +3222,8 @@
   </sheetPr>
   <dimension ref="B1:P185"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A135" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C135" sqref="C135"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B47" sqref="B47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3270,14 +3270,14 @@
         <v>139</v>
       </c>
       <c r="G3" s="38"/>
-      <c r="J3" s="63" t="s">
+      <c r="J3" s="64" t="s">
         <v>138</v>
       </c>
-      <c r="K3" s="63"/>
-      <c r="M3" s="63"/>
-      <c r="N3" s="63"/>
-      <c r="O3" s="63"/>
-      <c r="P3" s="63"/>
+      <c r="K3" s="64"/>
+      <c r="M3" s="64"/>
+      <c r="N3" s="64"/>
+      <c r="O3" s="64"/>
+      <c r="P3" s="64"/>
     </row>
     <row r="4" spans="2:16" ht="107.25" x14ac:dyDescent="0.25">
       <c r="B4" s="30" t="s">
@@ -4934,7 +4934,9 @@
       </c>
     </row>
     <row r="46" spans="2:14" s="40" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B46" s="59"/>
+      <c r="B46" s="59" t="s">
+        <v>1</v>
+      </c>
       <c r="C46" s="60" t="s">
         <v>353</v>
       </c>
@@ -4962,7 +4964,7 @@
       <c r="K46" s="60">
         <v>60</v>
       </c>
-      <c r="L46" s="66" t="s">
+      <c r="L46" s="63" t="s">
         <v>316</v>
       </c>
       <c r="M46" s="60" t="s">
@@ -5177,9 +5179,9 @@
       <c r="C54" s="20"/>
       <c r="D54" s="20"/>
       <c r="E54" s="20"/>
-      <c r="F54" s="64"/>
-      <c r="G54" s="64"/>
-      <c r="H54" s="64"/>
+      <c r="F54" s="65"/>
+      <c r="G54" s="65"/>
+      <c r="H54" s="65"/>
       <c r="I54" s="20"/>
       <c r="J54" s="20"/>
     </row>
@@ -5731,10 +5733,10 @@
       <c r="F80" s="21" t="s">
         <v>40</v>
       </c>
-      <c r="G80" s="65" t="s">
+      <c r="G80" s="66" t="s">
         <v>39</v>
       </c>
-      <c r="H80" s="65"/>
+      <c r="H80" s="66"/>
       <c r="I80" s="20"/>
     </row>
     <row r="81" spans="2:12" ht="142.5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Adding mission mod for Alien dragon
Former-commit-id: 3ce33c422687416cff9d6e88b08001e66824c005
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Missions.xlsx
+++ b/Docs/Content/HungryDragonContent_Missions.xlsx
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="missions" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="162913" calcOnSave="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="675" uniqueCount="370">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="677" uniqueCount="371">
   <si>
     <t>single_run</t>
   </si>
@@ -1159,6 +1159,9 @@
   </si>
   <si>
     <t>Fish01_Generic;Fish02_Generic;Fish03_Generic;FishDark;Piranha;PiranhaDark</t>
+  </si>
+  <si>
+    <t>dragon_alien</t>
   </si>
 </sst>
 </file>
@@ -1683,6 +1686,16 @@
   </cellStyles>
   <dxfs count="69">
     <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
@@ -2832,16 +2845,6 @@
         </bottom>
       </border>
     </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -2856,99 +2859,99 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="missionDifficultyDefinitions" displayName="missionDifficultyDefinitions" ref="B81:L84" totalsRowShown="0" headerRowBorderDxfId="67" tableBorderDxfId="66">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="missionDifficultyDefinitions" displayName="missionDifficultyDefinitions" ref="B81:L84" totalsRowShown="0" headerRowBorderDxfId="68" tableBorderDxfId="67">
   <autoFilter ref="B81:L84"/>
   <tableColumns count="11">
     <tableColumn id="1" name="{missionDifficultyDefinitions}"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="65"/>
-    <tableColumn id="11" name="[difficulty]" dataDxfId="64"/>
-    <tableColumn id="7" name="[index]" dataDxfId="63"/>
-    <tableColumn id="3" name="[dragonsToUnlock]" dataDxfId="62"/>
-    <tableColumn id="4" name="[cooldownMinutes]" dataDxfId="61"/>
-    <tableColumn id="9" name="[maxRewardCoins]" dataDxfId="60"/>
-    <tableColumn id="5" name="[removeMissionPCCoefA]" dataDxfId="59"/>
-    <tableColumn id="6" name="[removeMissionPCCoefB]" dataDxfId="58"/>
-    <tableColumn id="8" name="[tidName]" dataDxfId="57"/>
-    <tableColumn id="10" name="[color]" dataDxfId="56"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="66"/>
+    <tableColumn id="11" name="[difficulty]" dataDxfId="65"/>
+    <tableColumn id="7" name="[index]" dataDxfId="64"/>
+    <tableColumn id="3" name="[dragonsToUnlock]" dataDxfId="63"/>
+    <tableColumn id="4" name="[cooldownMinutes]" dataDxfId="62"/>
+    <tableColumn id="9" name="[maxRewardCoins]" dataDxfId="61"/>
+    <tableColumn id="5" name="[removeMissionPCCoefA]" dataDxfId="60"/>
+    <tableColumn id="6" name="[removeMissionPCCoefB]" dataDxfId="59"/>
+    <tableColumn id="8" name="[tidName]" dataDxfId="58"/>
+    <tableColumn id="10" name="[color]" dataDxfId="57"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table13303132" displayName="Table13303132" ref="B89:E107" totalsRowShown="0" headerRowDxfId="55" dataDxfId="53" headerRowBorderDxfId="54" tableBorderDxfId="52" totalsRowBorderDxfId="51">
-  <autoFilter ref="B89:E107"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table13303132" displayName="Table13303132" ref="B89:E108" totalsRowShown="0" headerRowDxfId="56" dataDxfId="54" headerRowBorderDxfId="55" tableBorderDxfId="53" totalsRowBorderDxfId="52">
+  <autoFilter ref="B89:E108"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="{missionDragonModifiersDefinitions}" dataDxfId="50"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="49"/>
-    <tableColumn id="7" name="[quantityModifier]" dataDxfId="48"/>
-    <tableColumn id="3" name="[missionSCRewardMultiplier]" dataDxfId="47"/>
+    <tableColumn id="1" name="{missionDragonModifiersDefinitions}" dataDxfId="51"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="50"/>
+    <tableColumn id="7" name="[quantityModifier]" dataDxfId="49"/>
+    <tableColumn id="3" name="[missionSCRewardMultiplier]" dataDxfId="48"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table1330313234" displayName="Table1330313234" ref="B111:E114" totalsRowShown="0" headerRowDxfId="46" dataDxfId="44" headerRowBorderDxfId="45" tableBorderDxfId="43" totalsRowBorderDxfId="42">
-  <autoFilter ref="B111:E114"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table1330313234" displayName="Table1330313234" ref="B112:E115" totalsRowShown="0" headerRowDxfId="47" dataDxfId="45" headerRowBorderDxfId="46" tableBorderDxfId="44" totalsRowBorderDxfId="43">
+  <autoFilter ref="B112:E115"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="{missionDifficultyModifiersDefinitions}" dataDxfId="41"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="40"/>
-    <tableColumn id="3" name="[difficulty]" dataDxfId="39"/>
-    <tableColumn id="7" name="[quantityModifier]" dataDxfId="38"/>
+    <tableColumn id="1" name="{missionDifficultyModifiersDefinitions}" dataDxfId="42"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="41"/>
+    <tableColumn id="3" name="[difficulty]" dataDxfId="40"/>
+    <tableColumn id="7" name="[quantityModifier]" dataDxfId="39"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table133031323435" displayName="Table133031323435" ref="B118:D119" totalsRowShown="0" headerRowDxfId="37" dataDxfId="35" headerRowBorderDxfId="36" tableBorderDxfId="34" totalsRowBorderDxfId="33">
-  <autoFilter ref="B118:D119"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table133031323435" displayName="Table133031323435" ref="B119:D120" totalsRowShown="0" headerRowDxfId="38" dataDxfId="36" headerRowBorderDxfId="37" tableBorderDxfId="35" totalsRowBorderDxfId="34">
+  <autoFilter ref="B119:D120"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="{missionOtherModifiersDefinitions}" dataDxfId="32"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="31"/>
-    <tableColumn id="7" name="[quantityModifier]" dataDxfId="30"/>
+    <tableColumn id="1" name="{missionOtherModifiersDefinitions}" dataDxfId="33"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="32"/>
+    <tableColumn id="7" name="[quantityModifier]" dataDxfId="31"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table13" displayName="Table13" ref="B55:H77" totalsRowShown="0" headerRowDxfId="29" dataDxfId="27" headerRowBorderDxfId="28" tableBorderDxfId="26" totalsRowBorderDxfId="25">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table13" displayName="Table13" ref="B55:H77" totalsRowShown="0" headerRowDxfId="30" dataDxfId="28" headerRowBorderDxfId="29" tableBorderDxfId="27" totalsRowBorderDxfId="26">
   <autoFilter ref="B55:H77"/>
   <tableColumns count="7">
-    <tableColumn id="1" name="{missionTypeDefinitions}" dataDxfId="24"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="23"/>
-    <tableColumn id="3" name="[minTier]" dataDxfId="22"/>
-    <tableColumn id="6" name="[maxTier]" dataDxfId="21"/>
-    <tableColumn id="4" name="[weight]" dataDxfId="20"/>
-    <tableColumn id="9" name="[tidDescSingleRun]" dataDxfId="19"/>
-    <tableColumn id="10" name="[tidDescMultiRun]" dataDxfId="18"/>
+    <tableColumn id="1" name="{missionTypeDefinitions}" dataDxfId="25"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="24"/>
+    <tableColumn id="3" name="[minTier]" dataDxfId="23"/>
+    <tableColumn id="6" name="[maxTier]" dataDxfId="22"/>
+    <tableColumn id="4" name="[weight]" dataDxfId="21"/>
+    <tableColumn id="9" name="[tidDescSingleRun]" dataDxfId="20"/>
+    <tableColumn id="10" name="[tidDescMultiRun]" dataDxfId="19"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table1330" displayName="Table1330" ref="B4:N50" totalsRowShown="0" headerRowDxfId="17" dataDxfId="15" headerRowBorderDxfId="16" tableBorderDxfId="14" totalsRowBorderDxfId="13">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table1330" displayName="Table1330" ref="B4:N50" totalsRowShown="0" headerRowDxfId="18" dataDxfId="16" headerRowBorderDxfId="17" tableBorderDxfId="15" totalsRowBorderDxfId="14">
   <autoFilter ref="B4:N50"/>
   <sortState ref="B5:P43">
     <sortCondition descending="1" ref="J4:J43"/>
   </sortState>
   <tableColumns count="13">
-    <tableColumn id="1" name="{missionsDefinitions}" dataDxfId="12"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="11"/>
-    <tableColumn id="7" name="[type]" dataDxfId="10"/>
-    <tableColumn id="8" name="[weight]" dataDxfId="9"/>
-    <tableColumn id="13" name="[singleRunChance]" dataDxfId="8"/>
-    <tableColumn id="11" name="[minTier]" dataDxfId="7"/>
-    <tableColumn id="12" name="[maxTier]" dataDxfId="6"/>
-    <tableColumn id="6" name="[params]" dataDxfId="5"/>
-    <tableColumn id="3" name="[objectiveBaseQuantityMin]" dataDxfId="4"/>
-    <tableColumn id="9" name="[objectiveBaseQuantityMax]" dataDxfId="3"/>
-    <tableColumn id="4" name="[icon]" dataDxfId="2"/>
-    <tableColumn id="5" name="[tidObjective]" dataDxfId="1"/>
-    <tableColumn id="10" name="[trackingSku]" dataDxfId="0"/>
+    <tableColumn id="1" name="{missionsDefinitions}" dataDxfId="13"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="12"/>
+    <tableColumn id="7" name="[type]" dataDxfId="11"/>
+    <tableColumn id="8" name="[weight]" dataDxfId="10"/>
+    <tableColumn id="13" name="[singleRunChance]" dataDxfId="9"/>
+    <tableColumn id="11" name="[minTier]" dataDxfId="8"/>
+    <tableColumn id="12" name="[maxTier]" dataDxfId="7"/>
+    <tableColumn id="6" name="[params]" dataDxfId="6"/>
+    <tableColumn id="3" name="[objectiveBaseQuantityMin]" dataDxfId="5"/>
+    <tableColumn id="9" name="[objectiveBaseQuantityMax]" dataDxfId="4"/>
+    <tableColumn id="4" name="[icon]" dataDxfId="3"/>
+    <tableColumn id="5" name="[tidObjective]" dataDxfId="2"/>
+    <tableColumn id="10" name="[trackingSku]" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3220,10 +3223,10 @@
   <sheetPr>
     <tabColor theme="6"/>
   </sheetPr>
-  <dimension ref="B1:P185"/>
+  <dimension ref="B1:P186"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B47" sqref="B47"/>
+    <sheetView tabSelected="1" topLeftCell="A100" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C104" sqref="C104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6087,17 +6090,17 @@
       </c>
     </row>
     <row r="103" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B103" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C103" s="1" t="s">
-        <v>334</v>
+      <c r="B103" s="51" t="s">
+        <v>1</v>
+      </c>
+      <c r="C103" s="42" t="s">
+        <v>370</v>
       </c>
       <c r="D103" s="42">
-        <v>8.1</v>
+        <v>8</v>
       </c>
       <c r="E103" s="42">
-        <v>75</v>
+        <v>70</v>
       </c>
     </row>
     <row r="104" spans="2:7" x14ac:dyDescent="0.25">
@@ -6105,10 +6108,10 @@
         <v>1</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="D104" s="42">
-        <v>8</v>
+        <v>8.1</v>
       </c>
       <c r="E104" s="42">
         <v>75</v>
@@ -6119,10 +6122,10 @@
         <v>1</v>
       </c>
       <c r="C105" s="1" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="D105" s="42">
-        <v>7.5</v>
+        <v>8</v>
       </c>
       <c r="E105" s="42">
         <v>75</v>
@@ -6133,66 +6136,66 @@
         <v>1</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="D106" s="42">
-        <v>8</v>
+        <v>7.5</v>
       </c>
       <c r="E106" s="42">
         <v>75</v>
       </c>
     </row>
     <row r="107" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B107" s="51" t="s">
-        <v>1</v>
-      </c>
-      <c r="C107" s="42" t="s">
-        <v>338</v>
+      <c r="B107" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C107" s="1" t="s">
+        <v>337</v>
       </c>
       <c r="D107" s="42">
-        <v>7.5</v>
+        <v>8</v>
       </c>
       <c r="E107" s="42">
         <v>75</v>
       </c>
     </row>
-    <row r="108" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="109" spans="2:7" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B109" s="6" t="s">
+    <row r="108" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B108" s="51" t="s">
+        <v>1</v>
+      </c>
+      <c r="C108" s="42" t="s">
+        <v>338</v>
+      </c>
+      <c r="D108" s="42">
+        <v>7.5</v>
+      </c>
+      <c r="E108" s="42">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="109" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="110" spans="2:7" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B110" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C109" s="6"/>
-      <c r="D109" s="6"/>
-      <c r="E109" s="6"/>
-      <c r="F109" s="6"/>
-      <c r="G109" s="6"/>
-    </row>
-    <row r="111" spans="2:7" ht="142.5" x14ac:dyDescent="0.25">
-      <c r="B111" s="5" t="s">
+      <c r="C110" s="6"/>
+      <c r="D110" s="6"/>
+      <c r="E110" s="6"/>
+      <c r="F110" s="6"/>
+      <c r="G110" s="6"/>
+    </row>
+    <row r="112" spans="2:7" ht="142.5" x14ac:dyDescent="0.25">
+      <c r="B112" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C111" s="4" t="s">
+      <c r="C112" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D111" s="4" t="s">
+      <c r="D112" s="4" t="s">
         <v>223</v>
       </c>
-      <c r="E111" s="3" t="s">
+      <c r="E112" s="3" t="s">
         <v>2</v>
-      </c>
-    </row>
-    <row r="112" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B112" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C112" s="1" t="s">
-        <v>224</v>
-      </c>
-      <c r="D112" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E112" s="1">
-        <v>0.05</v>
       </c>
     </row>
     <row r="113" spans="2:7" x14ac:dyDescent="0.25">
@@ -6200,13 +6203,13 @@
         <v>1</v>
       </c>
       <c r="C113" s="1" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D113" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E113" s="1">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="114" spans="2:7" x14ac:dyDescent="0.25">
@@ -6214,85 +6217,85 @@
         <v>1</v>
       </c>
       <c r="C114" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="D114" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E114" s="1">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="115" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B115" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C115" s="1" t="s">
         <v>226</v>
       </c>
-      <c r="D114" s="1" t="s">
+      <c r="D115" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E114" s="1">
+      <c r="E115" s="1">
         <v>0.2</v>
       </c>
     </row>
-    <row r="115" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="116" spans="2:7" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B116" s="6" t="s">
+    <row r="116" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="117" spans="2:7" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B117" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C116" s="6"/>
-      <c r="D116" s="6"/>
-      <c r="E116" s="6"/>
-      <c r="F116" s="6"/>
-      <c r="G116" s="6"/>
-    </row>
-    <row r="118" spans="2:7" ht="132" x14ac:dyDescent="0.25">
-      <c r="B118" s="5" t="s">
+      <c r="C117" s="6"/>
+      <c r="D117" s="6"/>
+      <c r="E117" s="6"/>
+      <c r="F117" s="6"/>
+      <c r="G117" s="6"/>
+    </row>
+    <row r="119" spans="2:7" ht="132" x14ac:dyDescent="0.25">
+      <c r="B119" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C118" s="4" t="s">
+      <c r="C119" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D118" s="3" t="s">
+      <c r="D119" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="119" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B119" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C119" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D119" s="1">
+    <row r="120" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B120" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C120" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D120" s="1">
         <v>0.7</v>
       </c>
     </row>
-    <row r="120" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="121" spans="2:7" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B121" s="6" t="s">
+    <row r="121" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="122" spans="2:7" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B122" s="6" t="s">
         <v>239</v>
       </c>
-      <c r="C121" s="6"/>
-      <c r="D121" s="6"/>
-      <c r="E121" s="6"/>
-      <c r="F121" s="6"/>
-      <c r="G121" s="6"/>
-    </row>
-    <row r="123" spans="2:7" ht="68.25" x14ac:dyDescent="0.25">
-      <c r="B123" s="44" t="s">
+      <c r="C122" s="6"/>
+      <c r="D122" s="6"/>
+      <c r="E122" s="6"/>
+      <c r="F122" s="6"/>
+      <c r="G122" s="6"/>
+    </row>
+    <row r="124" spans="2:7" ht="68.25" x14ac:dyDescent="0.25">
+      <c r="B124" s="44" t="s">
         <v>240</v>
       </c>
-      <c r="C123" s="44" t="s">
+      <c r="C124" s="44" t="s">
         <v>3</v>
       </c>
-      <c r="D123" s="45" t="s">
+      <c r="D124" s="45" t="s">
         <v>241</v>
       </c>
-      <c r="E123" s="45" t="s">
+      <c r="E124" s="45" t="s">
         <v>242</v>
-      </c>
-    </row>
-    <row r="124" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B124" s="43" t="s">
-        <v>1</v>
-      </c>
-      <c r="C124" s="46" t="s">
-        <v>80</v>
-      </c>
-      <c r="D124" s="46" t="s">
-        <v>263</v>
-      </c>
-      <c r="E124" s="43" t="b">
-        <v>1</v>
       </c>
     </row>
     <row r="125" spans="2:7" x14ac:dyDescent="0.25">
@@ -6300,10 +6303,10 @@
         <v>1</v>
       </c>
       <c r="C125" s="46" t="s">
-        <v>93</v>
+        <v>80</v>
       </c>
       <c r="D125" s="46" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="E125" s="43" t="b">
         <v>1</v>
@@ -6314,10 +6317,10 @@
         <v>1</v>
       </c>
       <c r="C126" s="46" t="s">
-        <v>124</v>
+        <v>93</v>
       </c>
       <c r="D126" s="46" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="E126" s="43" t="b">
         <v>1</v>
@@ -6328,13 +6331,13 @@
         <v>1</v>
       </c>
       <c r="C127" s="46" t="s">
-        <v>108</v>
+        <v>124</v>
       </c>
       <c r="D127" s="46" t="s">
-        <v>108</v>
+        <v>265</v>
       </c>
       <c r="E127" s="43" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="128" spans="2:7" x14ac:dyDescent="0.25">
@@ -6342,10 +6345,10 @@
         <v>1</v>
       </c>
       <c r="C128" s="46" t="s">
-        <v>120</v>
+        <v>108</v>
       </c>
       <c r="D128" s="46" t="s">
-        <v>120</v>
+        <v>108</v>
       </c>
       <c r="E128" s="43" t="b">
         <v>0</v>
@@ -6356,10 +6359,10 @@
         <v>1</v>
       </c>
       <c r="C129" s="46" t="s">
-        <v>109</v>
+        <v>120</v>
       </c>
       <c r="D129" s="46" t="s">
-        <v>109</v>
+        <v>120</v>
       </c>
       <c r="E129" s="43" t="b">
         <v>0</v>
@@ -6370,13 +6373,13 @@
         <v>1</v>
       </c>
       <c r="C130" s="46" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D130" s="46" t="s">
-        <v>266</v>
+        <v>109</v>
       </c>
       <c r="E130" s="43" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="131" spans="2:5" x14ac:dyDescent="0.25">
@@ -6384,10 +6387,10 @@
         <v>1</v>
       </c>
       <c r="C131" s="46" t="s">
-        <v>243</v>
+        <v>111</v>
       </c>
       <c r="D131" s="46" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="E131" s="43" t="b">
         <v>1</v>
@@ -6398,10 +6401,10 @@
         <v>1</v>
       </c>
       <c r="C132" s="46" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="D132" s="46" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="E132" s="43" t="b">
         <v>1</v>
@@ -6412,10 +6415,10 @@
         <v>1</v>
       </c>
       <c r="C133" s="46" t="s">
-        <v>204</v>
+        <v>244</v>
       </c>
       <c r="D133" s="46" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="E133" s="43" t="b">
         <v>1</v>
@@ -6426,10 +6429,10 @@
         <v>1</v>
       </c>
       <c r="C134" s="46" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="D134" s="46" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="E134" s="43" t="b">
         <v>1</v>
@@ -6440,10 +6443,10 @@
         <v>1</v>
       </c>
       <c r="C135" s="46" t="s">
-        <v>198</v>
+        <v>203</v>
       </c>
       <c r="D135" s="46" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="E135" s="43" t="b">
         <v>1</v>
@@ -6454,10 +6457,10 @@
         <v>1</v>
       </c>
       <c r="C136" s="46" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="D136" s="46" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="E136" s="43" t="b">
         <v>1</v>
@@ -6468,10 +6471,10 @@
         <v>1</v>
       </c>
       <c r="C137" s="46" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="D137" s="46" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="E137" s="43" t="b">
         <v>1</v>
@@ -6482,10 +6485,10 @@
         <v>1</v>
       </c>
       <c r="C138" s="46" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="D138" s="46" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="E138" s="43" t="b">
         <v>1</v>
@@ -6496,10 +6499,10 @@
         <v>1</v>
       </c>
       <c r="C139" s="46" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D139" s="46" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="E139" s="43" t="b">
         <v>1</v>
@@ -6510,10 +6513,10 @@
         <v>1</v>
       </c>
       <c r="C140" s="46" t="s">
-        <v>113</v>
+        <v>200</v>
       </c>
       <c r="D140" s="46" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="E140" s="43" t="b">
         <v>1</v>
@@ -6524,13 +6527,13 @@
         <v>1</v>
       </c>
       <c r="C141" s="46" t="s">
-        <v>245</v>
+        <v>113</v>
       </c>
       <c r="D141" s="46" t="s">
-        <v>245</v>
+        <v>276</v>
       </c>
       <c r="E141" s="43" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="142" spans="2:5" x14ac:dyDescent="0.25">
@@ -6538,13 +6541,13 @@
         <v>1</v>
       </c>
       <c r="C142" s="46" t="s">
-        <v>83</v>
+        <v>245</v>
       </c>
       <c r="D142" s="46" t="s">
-        <v>277</v>
+        <v>245</v>
       </c>
       <c r="E142" s="43" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="143" spans="2:5" x14ac:dyDescent="0.25">
@@ -6552,10 +6555,10 @@
         <v>1</v>
       </c>
       <c r="C143" s="46" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="D143" s="46" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="E143" s="43" t="b">
         <v>1</v>
@@ -6566,10 +6569,10 @@
         <v>1</v>
       </c>
       <c r="C144" s="46" t="s">
-        <v>246</v>
+        <v>96</v>
       </c>
       <c r="D144" s="46" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="E144" s="43" t="b">
         <v>1</v>
@@ -6580,10 +6583,10 @@
         <v>1</v>
       </c>
       <c r="C145" s="46" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="D145" s="46" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="E145" s="43" t="b">
         <v>1</v>
@@ -6594,10 +6597,10 @@
         <v>1</v>
       </c>
       <c r="C146" s="46" t="s">
-        <v>102</v>
+        <v>247</v>
       </c>
       <c r="D146" s="46" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="E146" s="43" t="b">
         <v>1</v>
@@ -6608,10 +6611,10 @@
         <v>1</v>
       </c>
       <c r="C147" s="46" t="s">
-        <v>248</v>
+        <v>102</v>
       </c>
       <c r="D147" s="46" t="s">
-        <v>303</v>
+        <v>281</v>
       </c>
       <c r="E147" s="43" t="b">
         <v>1</v>
@@ -6622,10 +6625,10 @@
         <v>1</v>
       </c>
       <c r="C148" s="46" t="s">
-        <v>122</v>
+        <v>248</v>
       </c>
       <c r="D148" s="46" t="s">
-        <v>282</v>
+        <v>303</v>
       </c>
       <c r="E148" s="43" t="b">
         <v>1</v>
@@ -6636,10 +6639,10 @@
         <v>1</v>
       </c>
       <c r="C149" s="46" t="s">
-        <v>88</v>
+        <v>122</v>
       </c>
       <c r="D149" s="46" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="E149" s="43" t="b">
         <v>1</v>
@@ -6650,10 +6653,10 @@
         <v>1</v>
       </c>
       <c r="C150" s="46" t="s">
-        <v>249</v>
+        <v>88</v>
       </c>
       <c r="D150" s="46" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="E150" s="43" t="b">
         <v>1</v>
@@ -6664,10 +6667,10 @@
         <v>1</v>
       </c>
       <c r="C151" s="46" t="s">
-        <v>301</v>
+        <v>249</v>
       </c>
       <c r="D151" s="46" t="s">
-        <v>302</v>
+        <v>284</v>
       </c>
       <c r="E151" s="43" t="b">
         <v>1</v>
@@ -6678,13 +6681,13 @@
         <v>1</v>
       </c>
       <c r="C152" s="46" t="s">
-        <v>250</v>
+        <v>301</v>
       </c>
       <c r="D152" s="46" t="s">
-        <v>250</v>
+        <v>302</v>
       </c>
       <c r="E152" s="43" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="153" spans="2:5" x14ac:dyDescent="0.25">
@@ -6692,10 +6695,10 @@
         <v>1</v>
       </c>
       <c r="C153" s="46" t="s">
-        <v>115</v>
+        <v>250</v>
       </c>
       <c r="D153" s="46" t="s">
-        <v>115</v>
+        <v>250</v>
       </c>
       <c r="E153" s="43" t="b">
         <v>0</v>
@@ -6706,13 +6709,13 @@
         <v>1</v>
       </c>
       <c r="C154" s="46" t="s">
-        <v>251</v>
+        <v>115</v>
       </c>
       <c r="D154" s="46" t="s">
-        <v>285</v>
+        <v>115</v>
       </c>
       <c r="E154" s="43" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="155" spans="2:5" x14ac:dyDescent="0.25">
@@ -6720,10 +6723,10 @@
         <v>1</v>
       </c>
       <c r="C155" s="46" t="s">
-        <v>91</v>
+        <v>251</v>
       </c>
       <c r="D155" s="46" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="E155" s="43" t="b">
         <v>1</v>
@@ -6734,10 +6737,10 @@
         <v>1</v>
       </c>
       <c r="C156" s="46" t="s">
-        <v>252</v>
+        <v>91</v>
       </c>
       <c r="D156" s="46" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="E156" s="43" t="b">
         <v>1</v>
@@ -6748,10 +6751,10 @@
         <v>1</v>
       </c>
       <c r="C157" s="46" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="D157" s="46" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="E157" s="43" t="b">
         <v>1</v>
@@ -6762,10 +6765,10 @@
         <v>1</v>
       </c>
       <c r="C158" s="46" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D158" s="46" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="E158" s="43" t="b">
         <v>1</v>
@@ -6776,10 +6779,10 @@
         <v>1</v>
       </c>
       <c r="C159" s="46" t="s">
-        <v>86</v>
+        <v>254</v>
       </c>
       <c r="D159" s="46" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="E159" s="43" t="b">
         <v>1</v>
@@ -6790,13 +6793,13 @@
         <v>1</v>
       </c>
       <c r="C160" s="46" t="s">
-        <v>73</v>
+        <v>86</v>
       </c>
       <c r="D160" s="46" t="s">
-        <v>73</v>
+        <v>290</v>
       </c>
       <c r="E160" s="43" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="161" spans="2:5" x14ac:dyDescent="0.25">
@@ -6804,10 +6807,10 @@
         <v>1</v>
       </c>
       <c r="C161" s="46" t="s">
-        <v>107</v>
+        <v>73</v>
       </c>
       <c r="D161" s="46" t="s">
-        <v>107</v>
+        <v>73</v>
       </c>
       <c r="E161" s="43" t="b">
         <v>0</v>
@@ -6818,13 +6821,13 @@
         <v>1</v>
       </c>
       <c r="C162" s="46" t="s">
-        <v>255</v>
+        <v>107</v>
       </c>
       <c r="D162" s="46" t="s">
-        <v>291</v>
+        <v>107</v>
       </c>
       <c r="E162" s="43" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="163" spans="2:5" x14ac:dyDescent="0.25">
@@ -6832,10 +6835,10 @@
         <v>1</v>
       </c>
       <c r="C163" s="46" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="D163" s="46" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="E163" s="43" t="b">
         <v>1</v>
@@ -6846,10 +6849,10 @@
         <v>1</v>
       </c>
       <c r="C164" s="46" t="s">
-        <v>77</v>
+        <v>256</v>
       </c>
       <c r="D164" s="46" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="E164" s="43" t="b">
         <v>1</v>
@@ -6860,10 +6863,10 @@
         <v>1</v>
       </c>
       <c r="C165" s="46" t="s">
-        <v>105</v>
+        <v>77</v>
       </c>
       <c r="D165" s="46" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="E165" s="43" t="b">
         <v>1</v>
@@ -6874,10 +6877,10 @@
         <v>1</v>
       </c>
       <c r="C166" s="46" t="s">
-        <v>257</v>
+        <v>105</v>
       </c>
       <c r="D166" s="46" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="E166" s="43" t="b">
         <v>1</v>
@@ -6888,10 +6891,10 @@
         <v>1</v>
       </c>
       <c r="C167" s="46" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="D167" s="46" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="E167" s="43" t="b">
         <v>1</v>
@@ -6902,10 +6905,10 @@
         <v>1</v>
       </c>
       <c r="C168" s="46" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="D168" s="46" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="E168" s="43" t="b">
         <v>1</v>
@@ -6916,13 +6919,13 @@
         <v>1</v>
       </c>
       <c r="C169" s="46" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="D169" s="46" t="s">
-        <v>260</v>
+        <v>297</v>
       </c>
       <c r="E169" s="43" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="170" spans="2:5" x14ac:dyDescent="0.25">
@@ -6930,13 +6933,13 @@
         <v>1</v>
       </c>
       <c r="C170" s="46" t="s">
-        <v>99</v>
+        <v>260</v>
       </c>
       <c r="D170" s="46" t="s">
-        <v>298</v>
+        <v>260</v>
       </c>
       <c r="E170" s="43" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="171" spans="2:5" x14ac:dyDescent="0.25">
@@ -6944,10 +6947,10 @@
         <v>1</v>
       </c>
       <c r="C171" s="46" t="s">
-        <v>261</v>
+        <v>99</v>
       </c>
       <c r="D171" s="46" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="E171" s="43" t="b">
         <v>1</v>
@@ -6958,10 +6961,10 @@
         <v>1</v>
       </c>
       <c r="C172" s="46" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="D172" s="46" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="E172" s="43" t="b">
         <v>1</v>
@@ -6972,10 +6975,10 @@
         <v>1</v>
       </c>
       <c r="C173" s="46" t="s">
-        <v>309</v>
+        <v>262</v>
       </c>
       <c r="D173" s="46" t="s">
-        <v>306</v>
+        <v>300</v>
       </c>
       <c r="E173" s="43" t="b">
         <v>1</v>
@@ -6986,10 +6989,10 @@
         <v>1</v>
       </c>
       <c r="C174" s="46" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="D174" s="46" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="E174" s="43" t="b">
         <v>1</v>
@@ -7000,10 +7003,10 @@
         <v>1</v>
       </c>
       <c r="C175" s="46" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="D175" s="46" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="E175" s="43" t="b">
         <v>1</v>
@@ -7014,10 +7017,10 @@
         <v>1</v>
       </c>
       <c r="C176" s="46" t="s">
-        <v>319</v>
+        <v>311</v>
       </c>
       <c r="D176" s="46" t="s">
-        <v>320</v>
+        <v>308</v>
       </c>
       <c r="E176" s="43" t="b">
         <v>1</v>
@@ -7028,10 +7031,10 @@
         <v>1</v>
       </c>
       <c r="C177" s="46" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="D177" s="46" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="E177" s="43" t="b">
         <v>1</v>
@@ -7042,10 +7045,10 @@
         <v>1</v>
       </c>
       <c r="C178" s="46" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="D178" s="46" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="E178" s="43" t="b">
         <v>1</v>
@@ -7056,10 +7059,10 @@
         <v>1</v>
       </c>
       <c r="C179" s="46" t="s">
-        <v>316</v>
+        <v>323</v>
       </c>
       <c r="D179" s="46" t="s">
-        <v>339</v>
+        <v>324</v>
       </c>
       <c r="E179" s="43" t="b">
         <v>1</v>
@@ -7070,10 +7073,10 @@
         <v>1</v>
       </c>
       <c r="C180" s="46" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="D180" s="46" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="E180" s="43" t="b">
         <v>1</v>
@@ -7084,10 +7087,10 @@
         <v>1</v>
       </c>
       <c r="C181" s="46" t="s">
-        <v>74</v>
+        <v>317</v>
       </c>
       <c r="D181" s="46" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="E181" s="43" t="b">
         <v>1</v>
@@ -7098,10 +7101,10 @@
         <v>1</v>
       </c>
       <c r="C182" s="46" t="s">
-        <v>346</v>
+        <v>74</v>
       </c>
       <c r="D182" s="46" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="E182" s="43" t="b">
         <v>1</v>
@@ -7112,10 +7115,10 @@
         <v>1</v>
       </c>
       <c r="C183" s="46" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="D183" s="46" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="E183" s="43" t="b">
         <v>1</v>
@@ -7126,10 +7129,10 @@
         <v>1</v>
       </c>
       <c r="C184" s="46" t="s">
-        <v>318</v>
+        <v>347</v>
       </c>
       <c r="D184" s="46" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="E184" s="43" t="b">
         <v>1</v>
@@ -7140,12 +7143,26 @@
         <v>1</v>
       </c>
       <c r="C185" s="46" t="s">
+        <v>318</v>
+      </c>
+      <c r="D185" s="46" t="s">
+        <v>344</v>
+      </c>
+      <c r="E185" s="43" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="186" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B186" s="43" t="s">
+        <v>1</v>
+      </c>
+      <c r="C186" s="46" t="s">
         <v>348</v>
       </c>
-      <c r="D185" s="46" t="s">
+      <c r="D186" s="46" t="s">
         <v>345</v>
       </c>
-      <c r="E185" s="43" t="b">
+      <c r="E186" s="43" t="b">
         <v>1</v>
       </c>
     </row>
@@ -7157,7 +7174,7 @@
     <mergeCell ref="G80:H80"/>
   </mergeCells>
   <conditionalFormatting sqref="C82:E84">
-    <cfRule type="duplicateValues" dxfId="68" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="2"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Adding test space missions
Former-commit-id: 2d13aeed10e0656d72af18d05cecb14e6fa0fd16
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Missions.xlsx
+++ b/Docs/Content/HungryDragonContent_Missions.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="675" uniqueCount="370">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="694" uniqueCount="378">
   <si>
     <t>single_run</t>
   </si>
@@ -1159,6 +1159,30 @@
   </si>
   <si>
     <t>Fish01_Generic;Fish02_Generic;Fish03_Generic;FishDark;Piranha;PiranhaDark</t>
+  </si>
+  <si>
+    <t>icon_space</t>
+  </si>
+  <si>
+    <t>PF_icon_space</t>
+  </si>
+  <si>
+    <t>space</t>
+  </si>
+  <si>
+    <t>space_time</t>
+  </si>
+  <si>
+    <t>TID_MISSION_OBJECTIVE_SPACE_DESC_SINGLE_RUN</t>
+  </si>
+  <si>
+    <t>TID_MISSION_OBJECTIVE_SPACE_TIME_DESC_SINGLE_RUN</t>
+  </si>
+  <si>
+    <t>TID_MISSION_OBJECTIVE_SPACE_DESC_MULTI_RUN</t>
+  </si>
+  <si>
+    <t>TID_MISSION_OBJECTIVE_SPACE_TIME_DESC_MULTI_RUN</t>
   </si>
 </sst>
 </file>
@@ -1511,7 +1535,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="67">
+  <cellXfs count="68">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1"/>
@@ -1677,11 +1701,24 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="69">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -2832,16 +2869,6 @@
         </bottom>
       </border>
     </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -2856,99 +2883,99 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="missionDifficultyDefinitions" displayName="missionDifficultyDefinitions" ref="B81:L84" totalsRowShown="0" headerRowBorderDxfId="67" tableBorderDxfId="66">
-  <autoFilter ref="B81:L84"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="missionDifficultyDefinitions" displayName="missionDifficultyDefinitions" ref="B85:L88" totalsRowShown="0" headerRowBorderDxfId="68" tableBorderDxfId="67">
+  <autoFilter ref="B85:L88"/>
   <tableColumns count="11">
     <tableColumn id="1" name="{missionDifficultyDefinitions}"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="65"/>
-    <tableColumn id="11" name="[difficulty]" dataDxfId="64"/>
-    <tableColumn id="7" name="[index]" dataDxfId="63"/>
-    <tableColumn id="3" name="[dragonsToUnlock]" dataDxfId="62"/>
-    <tableColumn id="4" name="[cooldownMinutes]" dataDxfId="61"/>
-    <tableColumn id="9" name="[maxRewardCoins]" dataDxfId="60"/>
-    <tableColumn id="5" name="[removeMissionPCCoefA]" dataDxfId="59"/>
-    <tableColumn id="6" name="[removeMissionPCCoefB]" dataDxfId="58"/>
-    <tableColumn id="8" name="[tidName]" dataDxfId="57"/>
-    <tableColumn id="10" name="[color]" dataDxfId="56"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="66"/>
+    <tableColumn id="11" name="[difficulty]" dataDxfId="65"/>
+    <tableColumn id="7" name="[index]" dataDxfId="64"/>
+    <tableColumn id="3" name="[dragonsToUnlock]" dataDxfId="63"/>
+    <tableColumn id="4" name="[cooldownMinutes]" dataDxfId="62"/>
+    <tableColumn id="9" name="[maxRewardCoins]" dataDxfId="61"/>
+    <tableColumn id="5" name="[removeMissionPCCoefA]" dataDxfId="60"/>
+    <tableColumn id="6" name="[removeMissionPCCoefB]" dataDxfId="59"/>
+    <tableColumn id="8" name="[tidName]" dataDxfId="58"/>
+    <tableColumn id="10" name="[color]" dataDxfId="57"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table13303132" displayName="Table13303132" ref="B89:E107" totalsRowShown="0" headerRowDxfId="55" dataDxfId="53" headerRowBorderDxfId="54" tableBorderDxfId="52" totalsRowBorderDxfId="51">
-  <autoFilter ref="B89:E107"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table13303132" displayName="Table13303132" ref="B93:E111" totalsRowShown="0" headerRowDxfId="56" dataDxfId="54" headerRowBorderDxfId="55" tableBorderDxfId="53" totalsRowBorderDxfId="52">
+  <autoFilter ref="B93:E111"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="{missionDragonModifiersDefinitions}" dataDxfId="50"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="49"/>
-    <tableColumn id="7" name="[quantityModifier]" dataDxfId="48"/>
-    <tableColumn id="3" name="[missionSCRewardMultiplier]" dataDxfId="47"/>
+    <tableColumn id="1" name="{missionDragonModifiersDefinitions}" dataDxfId="51"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="50"/>
+    <tableColumn id="7" name="[quantityModifier]" dataDxfId="49"/>
+    <tableColumn id="3" name="[missionSCRewardMultiplier]" dataDxfId="48"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table1330313234" displayName="Table1330313234" ref="B111:E114" totalsRowShown="0" headerRowDxfId="46" dataDxfId="44" headerRowBorderDxfId="45" tableBorderDxfId="43" totalsRowBorderDxfId="42">
-  <autoFilter ref="B111:E114"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table1330313234" displayName="Table1330313234" ref="B115:E118" totalsRowShown="0" headerRowDxfId="47" dataDxfId="45" headerRowBorderDxfId="46" tableBorderDxfId="44" totalsRowBorderDxfId="43">
+  <autoFilter ref="B115:E118"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="{missionDifficultyModifiersDefinitions}" dataDxfId="41"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="40"/>
-    <tableColumn id="3" name="[difficulty]" dataDxfId="39"/>
-    <tableColumn id="7" name="[quantityModifier]" dataDxfId="38"/>
+    <tableColumn id="1" name="{missionDifficultyModifiersDefinitions}" dataDxfId="42"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="41"/>
+    <tableColumn id="3" name="[difficulty]" dataDxfId="40"/>
+    <tableColumn id="7" name="[quantityModifier]" dataDxfId="39"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table133031323435" displayName="Table133031323435" ref="B118:D119" totalsRowShown="0" headerRowDxfId="37" dataDxfId="35" headerRowBorderDxfId="36" tableBorderDxfId="34" totalsRowBorderDxfId="33">
-  <autoFilter ref="B118:D119"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table133031323435" displayName="Table133031323435" ref="B122:D123" totalsRowShown="0" headerRowDxfId="38" dataDxfId="36" headerRowBorderDxfId="37" tableBorderDxfId="35" totalsRowBorderDxfId="34">
+  <autoFilter ref="B122:D123"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="{missionOtherModifiersDefinitions}" dataDxfId="32"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="31"/>
-    <tableColumn id="7" name="[quantityModifier]" dataDxfId="30"/>
+    <tableColumn id="1" name="{missionOtherModifiersDefinitions}" dataDxfId="33"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="32"/>
+    <tableColumn id="7" name="[quantityModifier]" dataDxfId="31"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table13" displayName="Table13" ref="B55:H77" totalsRowShown="0" headerRowDxfId="29" dataDxfId="27" headerRowBorderDxfId="28" tableBorderDxfId="26" totalsRowBorderDxfId="25">
-  <autoFilter ref="B55:H77"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table13" displayName="Table13" ref="B57:H81" totalsRowShown="0" headerRowDxfId="30" dataDxfId="28" headerRowBorderDxfId="29" tableBorderDxfId="27" totalsRowBorderDxfId="26">
+  <autoFilter ref="B57:H81"/>
   <tableColumns count="7">
-    <tableColumn id="1" name="{missionTypeDefinitions}" dataDxfId="24"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="23"/>
-    <tableColumn id="3" name="[minTier]" dataDxfId="22"/>
-    <tableColumn id="6" name="[maxTier]" dataDxfId="21"/>
-    <tableColumn id="4" name="[weight]" dataDxfId="20"/>
-    <tableColumn id="9" name="[tidDescSingleRun]" dataDxfId="19"/>
-    <tableColumn id="10" name="[tidDescMultiRun]" dataDxfId="18"/>
+    <tableColumn id="1" name="{missionTypeDefinitions}" dataDxfId="25"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="24"/>
+    <tableColumn id="3" name="[minTier]" dataDxfId="23"/>
+    <tableColumn id="6" name="[maxTier]" dataDxfId="22"/>
+    <tableColumn id="4" name="[weight]" dataDxfId="21"/>
+    <tableColumn id="9" name="[tidDescSingleRun]" dataDxfId="20"/>
+    <tableColumn id="10" name="[tidDescMultiRun]" dataDxfId="19"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table1330" displayName="Table1330" ref="B4:N50" totalsRowShown="0" headerRowDxfId="17" dataDxfId="15" headerRowBorderDxfId="16" tableBorderDxfId="14" totalsRowBorderDxfId="13">
-  <autoFilter ref="B4:N50"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table1330" displayName="Table1330" ref="B4:N52" totalsRowShown="0" headerRowDxfId="18" dataDxfId="16" headerRowBorderDxfId="17" tableBorderDxfId="15" totalsRowBorderDxfId="14">
+  <autoFilter ref="B4:N52"/>
   <sortState ref="B5:P43">
     <sortCondition descending="1" ref="J4:J43"/>
   </sortState>
   <tableColumns count="13">
-    <tableColumn id="1" name="{missionsDefinitions}" dataDxfId="12"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="11"/>
-    <tableColumn id="7" name="[type]" dataDxfId="10"/>
-    <tableColumn id="8" name="[weight]" dataDxfId="9"/>
-    <tableColumn id="13" name="[singleRunChance]" dataDxfId="8"/>
-    <tableColumn id="11" name="[minTier]" dataDxfId="7"/>
-    <tableColumn id="12" name="[maxTier]" dataDxfId="6"/>
-    <tableColumn id="6" name="[params]" dataDxfId="5"/>
-    <tableColumn id="3" name="[objectiveBaseQuantityMin]" dataDxfId="4"/>
-    <tableColumn id="9" name="[objectiveBaseQuantityMax]" dataDxfId="3"/>
-    <tableColumn id="4" name="[icon]" dataDxfId="2"/>
-    <tableColumn id="5" name="[tidObjective]" dataDxfId="1"/>
-    <tableColumn id="10" name="[trackingSku]" dataDxfId="0"/>
+    <tableColumn id="1" name="{missionsDefinitions}" dataDxfId="13"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="12"/>
+    <tableColumn id="7" name="[type]" dataDxfId="11"/>
+    <tableColumn id="8" name="[weight]" dataDxfId="10"/>
+    <tableColumn id="13" name="[singleRunChance]" dataDxfId="9"/>
+    <tableColumn id="11" name="[minTier]" dataDxfId="8"/>
+    <tableColumn id="12" name="[maxTier]" dataDxfId="7"/>
+    <tableColumn id="6" name="[params]" dataDxfId="6"/>
+    <tableColumn id="3" name="[objectiveBaseQuantityMin]" dataDxfId="5"/>
+    <tableColumn id="9" name="[objectiveBaseQuantityMax]" dataDxfId="4"/>
+    <tableColumn id="4" name="[icon]" dataDxfId="3"/>
+    <tableColumn id="5" name="[tidObjective]" dataDxfId="2"/>
+    <tableColumn id="10" name="[trackingSku]" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3220,10 +3247,10 @@
   <sheetPr>
     <tabColor theme="6"/>
   </sheetPr>
-  <dimension ref="B1:P185"/>
+  <dimension ref="B1:P190"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B47" sqref="B47"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N54" sqref="N54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5131,127 +5158,151 @@
       </c>
     </row>
     <row r="51" spans="2:14" s="40" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B51" s="41"/>
-      <c r="C51" s="41"/>
-      <c r="D51" s="41"/>
-      <c r="E51" s="41"/>
-      <c r="F51" s="41"/>
-      <c r="G51" s="41"/>
-      <c r="H51" s="41"/>
-      <c r="I51" s="41"/>
-      <c r="J51" s="41"/>
-      <c r="K51" s="41"/>
-      <c r="L51" s="41"/>
-      <c r="M51" s="41"/>
-      <c r="N51" s="41"/>
-    </row>
-    <row r="52" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B52" s="32"/>
-      <c r="C52" s="32"/>
-      <c r="D52" s="32"/>
-      <c r="E52" s="32"/>
-      <c r="F52" s="32"/>
-      <c r="G52" s="32"/>
-      <c r="H52" s="32"/>
-      <c r="I52" s="32"/>
-      <c r="J52" s="32"/>
-      <c r="K52" s="32"/>
-      <c r="L52" s="32"/>
-      <c r="M52" s="31"/>
-    </row>
-    <row r="53" spans="2:14" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B53" s="6" t="s">
+      <c r="B51" s="27"/>
+      <c r="C51" s="24" t="s">
+        <v>372</v>
+      </c>
+      <c r="D51" s="23" t="s">
+        <v>372</v>
+      </c>
+      <c r="E51" s="23">
+        <v>1</v>
+      </c>
+      <c r="F51" s="23">
+        <v>0</v>
+      </c>
+      <c r="G51" s="24">
+        <v>1</v>
+      </c>
+      <c r="H51" s="23">
+        <v>4</v>
+      </c>
+      <c r="I51" s="23"/>
+      <c r="J51" s="24">
+        <v>350</v>
+      </c>
+      <c r="K51" s="23">
+        <v>500</v>
+      </c>
+      <c r="L51" s="67" t="s">
+        <v>370</v>
+      </c>
+      <c r="M51" s="24"/>
+      <c r="N51" s="52" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="52" spans="2:14" s="40" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B52" s="25"/>
+      <c r="C52" s="23" t="s">
+        <v>373</v>
+      </c>
+      <c r="D52" s="23" t="s">
+        <v>373</v>
+      </c>
+      <c r="E52" s="23">
+        <v>1</v>
+      </c>
+      <c r="F52" s="23">
+        <v>0</v>
+      </c>
+      <c r="G52" s="23">
+        <v>1</v>
+      </c>
+      <c r="H52" s="23">
+        <v>4</v>
+      </c>
+      <c r="I52" s="23"/>
+      <c r="J52" s="23">
+        <v>300</v>
+      </c>
+      <c r="K52" s="23">
+        <v>400</v>
+      </c>
+      <c r="L52" s="54" t="s">
+        <v>370</v>
+      </c>
+      <c r="M52" s="23"/>
+      <c r="N52" s="53" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="53" spans="2:14" s="40" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B53" s="41"/>
+      <c r="C53" s="41"/>
+      <c r="D53" s="41"/>
+      <c r="E53" s="41"/>
+      <c r="F53" s="41"/>
+      <c r="G53" s="41"/>
+      <c r="H53" s="41"/>
+      <c r="I53" s="41"/>
+      <c r="J53" s="41"/>
+      <c r="K53" s="41"/>
+      <c r="L53" s="41"/>
+      <c r="M53" s="41"/>
+      <c r="N53" s="41"/>
+    </row>
+    <row r="54" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B54" s="32"/>
+      <c r="C54" s="32"/>
+      <c r="D54" s="32"/>
+      <c r="E54" s="32"/>
+      <c r="F54" s="32"/>
+      <c r="G54" s="32"/>
+      <c r="H54" s="32"/>
+      <c r="I54" s="32"/>
+      <c r="J54" s="32"/>
+      <c r="K54" s="32"/>
+      <c r="L54" s="32"/>
+      <c r="M54" s="31"/>
+    </row>
+    <row r="55" spans="2:14" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B55" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="C53" s="6"/>
-      <c r="D53" s="6"/>
-      <c r="E53" s="6"/>
-      <c r="F53" s="6"/>
-      <c r="G53" s="6"/>
-      <c r="H53" s="6"/>
-      <c r="I53" s="6"/>
-      <c r="J53" s="6"/>
-      <c r="K53" s="6"/>
-      <c r="L53" s="6"/>
-    </row>
-    <row r="54" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B54" s="20"/>
-      <c r="C54" s="20"/>
-      <c r="D54" s="20"/>
-      <c r="E54" s="20"/>
-      <c r="F54" s="65"/>
-      <c r="G54" s="65"/>
-      <c r="H54" s="65"/>
-      <c r="I54" s="20"/>
-      <c r="J54" s="20"/>
-    </row>
-    <row r="55" spans="2:14" ht="96" x14ac:dyDescent="0.25">
-      <c r="B55" s="30" t="s">
+      <c r="C55" s="6"/>
+      <c r="D55" s="6"/>
+      <c r="E55" s="6"/>
+      <c r="F55" s="6"/>
+      <c r="G55" s="6"/>
+      <c r="H55" s="6"/>
+      <c r="I55" s="6"/>
+      <c r="J55" s="6"/>
+      <c r="K55" s="6"/>
+      <c r="L55" s="6"/>
+    </row>
+    <row r="56" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B56" s="20"/>
+      <c r="C56" s="20"/>
+      <c r="D56" s="20"/>
+      <c r="E56" s="20"/>
+      <c r="F56" s="65"/>
+      <c r="G56" s="65"/>
+      <c r="H56" s="65"/>
+      <c r="I56" s="20"/>
+      <c r="J56" s="20"/>
+    </row>
+    <row r="57" spans="2:14" ht="96" x14ac:dyDescent="0.25">
+      <c r="B57" s="30" t="s">
         <v>71</v>
       </c>
-      <c r="C55" s="28" t="s">
+      <c r="C57" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="D55" s="29" t="s">
+      <c r="D57" s="29" t="s">
         <v>70</v>
       </c>
-      <c r="E55" s="29" t="s">
+      <c r="E57" s="29" t="s">
         <v>69</v>
       </c>
-      <c r="F55" s="29" t="s">
+      <c r="F57" s="29" t="s">
         <v>68</v>
       </c>
-      <c r="G55" s="28" t="s">
+      <c r="G57" s="28" t="s">
         <v>67</v>
       </c>
-      <c r="H55" s="28" t="s">
+      <c r="H57" s="28" t="s">
         <v>66</v>
-      </c>
-    </row>
-    <row r="56" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B56" s="27" t="s">
-        <v>1</v>
-      </c>
-      <c r="C56" s="24" t="s">
-        <v>65</v>
-      </c>
-      <c r="D56" s="24">
-        <v>0</v>
-      </c>
-      <c r="E56" s="24">
-        <v>7</v>
-      </c>
-      <c r="F56" s="24">
-        <v>2</v>
-      </c>
-      <c r="G56" s="26" t="s">
-        <v>64</v>
-      </c>
-      <c r="H56" s="26" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="57" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B57" s="27" t="s">
-        <v>1</v>
-      </c>
-      <c r="C57" s="24" t="s">
-        <v>62</v>
-      </c>
-      <c r="D57" s="24">
-        <v>0</v>
-      </c>
-      <c r="E57" s="24">
-        <v>7</v>
-      </c>
-      <c r="F57" s="24">
-        <v>1</v>
-      </c>
-      <c r="G57" s="26" t="s">
-        <v>61</v>
-      </c>
-      <c r="H57" s="26" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="58" spans="2:14" x14ac:dyDescent="0.25">
@@ -5259,7 +5310,7 @@
         <v>1</v>
       </c>
       <c r="C58" s="24" t="s">
-        <v>59</v>
+        <v>65</v>
       </c>
       <c r="D58" s="24">
         <v>0</v>
@@ -5271,10 +5322,10 @@
         <v>2</v>
       </c>
       <c r="G58" s="26" t="s">
-        <v>58</v>
+        <v>64</v>
       </c>
       <c r="H58" s="26" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
     </row>
     <row r="59" spans="2:14" x14ac:dyDescent="0.25">
@@ -5282,7 +5333,7 @@
         <v>1</v>
       </c>
       <c r="C59" s="24" t="s">
-        <v>56</v>
+        <v>62</v>
       </c>
       <c r="D59" s="24">
         <v>0</v>
@@ -5294,41 +5345,41 @@
         <v>1</v>
       </c>
       <c r="G59" s="26" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="H59" s="26" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
     </row>
     <row r="60" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B60" s="25" t="s">
-        <v>1</v>
-      </c>
-      <c r="C60" s="23" t="s">
-        <v>53</v>
-      </c>
-      <c r="D60" s="23">
+      <c r="B60" s="27" t="s">
+        <v>1</v>
+      </c>
+      <c r="C60" s="24" t="s">
+        <v>59</v>
+      </c>
+      <c r="D60" s="24">
         <v>0</v>
       </c>
       <c r="E60" s="24">
         <v>7</v>
       </c>
-      <c r="F60" s="23">
-        <v>1</v>
+      <c r="F60" s="24">
+        <v>2</v>
       </c>
       <c r="G60" s="26" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="H60" s="26" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
     </row>
     <row r="61" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B61" s="25" t="s">
+      <c r="B61" s="27" t="s">
         <v>1</v>
       </c>
       <c r="C61" s="24" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="D61" s="24">
         <v>0</v>
@@ -5340,64 +5391,64 @@
         <v>1</v>
       </c>
       <c r="G61" s="26" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="H61" s="26" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
     </row>
     <row r="62" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B62" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="C62" s="24" t="s">
-        <v>47</v>
-      </c>
-      <c r="D62" s="24">
+      <c r="C62" s="23" t="s">
+        <v>53</v>
+      </c>
+      <c r="D62" s="23">
         <v>0</v>
       </c>
       <c r="E62" s="24">
         <v>7</v>
       </c>
-      <c r="F62" s="24">
+      <c r="F62" s="23">
         <v>1</v>
       </c>
       <c r="G62" s="26" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="H62" s="26" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
     </row>
     <row r="63" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B63" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="C63" s="23" t="s">
-        <v>44</v>
-      </c>
-      <c r="D63" s="23">
+      <c r="C63" s="24" t="s">
+        <v>50</v>
+      </c>
+      <c r="D63" s="24">
         <v>0</v>
       </c>
       <c r="E63" s="24">
         <v>7</v>
       </c>
-      <c r="F63" s="23">
-        <v>1</v>
-      </c>
-      <c r="G63" s="22" t="s">
-        <v>43</v>
-      </c>
-      <c r="H63" s="22" t="s">
-        <v>42</v>
+      <c r="F63" s="24">
+        <v>1</v>
+      </c>
+      <c r="G63" s="26" t="s">
+        <v>49</v>
+      </c>
+      <c r="H63" s="26" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="64" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B64" s="27" t="s">
+      <c r="B64" s="25" t="s">
         <v>1</v>
       </c>
       <c r="C64" s="24" t="s">
-        <v>177</v>
+        <v>47</v>
       </c>
       <c r="D64" s="24">
         <v>0</v>
@@ -5406,44 +5457,44 @@
         <v>7</v>
       </c>
       <c r="F64" s="24">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G64" s="26" t="s">
-        <v>166</v>
+        <v>46</v>
       </c>
       <c r="H64" s="26" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="65" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B65" s="27" t="s">
-        <v>1</v>
-      </c>
-      <c r="C65" s="24" t="s">
-        <v>174</v>
-      </c>
-      <c r="D65" s="24">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="65" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B65" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="C65" s="23" t="s">
+        <v>44</v>
+      </c>
+      <c r="D65" s="23">
         <v>0</v>
       </c>
       <c r="E65" s="24">
         <v>7</v>
       </c>
-      <c r="F65" s="24">
-        <v>0</v>
-      </c>
-      <c r="G65" s="26" t="s">
-        <v>169</v>
-      </c>
-      <c r="H65" s="26" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="66" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B66" s="27" t="s">
+      <c r="F65" s="23">
+        <v>1</v>
+      </c>
+      <c r="G65" s="22" t="s">
+        <v>43</v>
+      </c>
+      <c r="H65" s="22" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="66" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B66" s="25" t="s">
         <v>1</v>
       </c>
       <c r="C66" s="24" t="s">
-        <v>144</v>
+        <v>372</v>
       </c>
       <c r="D66" s="24">
         <v>0</v>
@@ -5452,21 +5503,21 @@
         <v>7</v>
       </c>
       <c r="F66" s="24">
-        <v>2</v>
-      </c>
-      <c r="G66" s="26" t="s">
-        <v>167</v>
-      </c>
-      <c r="H66" s="26" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="67" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B67" s="27" t="s">
+        <v>1</v>
+      </c>
+      <c r="G66" s="22" t="s">
+        <v>374</v>
+      </c>
+      <c r="H66" s="22" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="67" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B67" s="25" t="s">
         <v>1</v>
       </c>
       <c r="C67" s="24" t="s">
-        <v>227</v>
+        <v>373</v>
       </c>
       <c r="D67" s="24">
         <v>0</v>
@@ -5477,42 +5528,42 @@
       <c r="F67" s="24">
         <v>1</v>
       </c>
-      <c r="G67" s="26" t="s">
-        <v>228</v>
-      </c>
-      <c r="H67" s="26" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="68" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B68" s="25" t="s">
-        <v>1</v>
-      </c>
-      <c r="C68" s="23" t="s">
-        <v>230</v>
-      </c>
-      <c r="D68" s="23">
+      <c r="G67" s="22" t="s">
+        <v>375</v>
+      </c>
+      <c r="H67" s="22" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="68" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B68" s="27" t="s">
+        <v>1</v>
+      </c>
+      <c r="C68" s="24" t="s">
+        <v>177</v>
+      </c>
+      <c r="D68" s="24">
         <v>0</v>
       </c>
       <c r="E68" s="24">
         <v>7</v>
       </c>
-      <c r="F68" s="23">
-        <v>1</v>
+      <c r="F68" s="24">
+        <v>0</v>
       </c>
       <c r="G68" s="26" t="s">
-        <v>231</v>
+        <v>166</v>
       </c>
       <c r="H68" s="26" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="69" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B69" s="25" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="69" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B69" s="27" t="s">
         <v>1</v>
       </c>
       <c r="C69" s="24" t="s">
-        <v>233</v>
+        <v>174</v>
       </c>
       <c r="D69" s="24">
         <v>0</v>
@@ -5521,21 +5572,21 @@
         <v>7</v>
       </c>
       <c r="F69" s="24">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G69" s="26" t="s">
-        <v>234</v>
+        <v>169</v>
       </c>
       <c r="H69" s="26" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="70" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B70" s="25" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="70" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B70" s="27" t="s">
         <v>1</v>
       </c>
       <c r="C70" s="24" t="s">
-        <v>236</v>
+        <v>144</v>
       </c>
       <c r="D70" s="24">
         <v>0</v>
@@ -5544,65 +5595,67 @@
         <v>7</v>
       </c>
       <c r="F70" s="24">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G70" s="26" t="s">
-        <v>237</v>
+        <v>167</v>
       </c>
       <c r="H70" s="26" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="71" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B71" s="25" t="s">
-        <v>1</v>
-      </c>
-      <c r="C71" s="23" t="s">
-        <v>145</v>
-      </c>
-      <c r="D71" s="23">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="71" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B71" s="27" t="s">
+        <v>1</v>
+      </c>
+      <c r="C71" s="24" t="s">
+        <v>227</v>
+      </c>
+      <c r="D71" s="24">
         <v>0</v>
       </c>
       <c r="E71" s="24">
         <v>7</v>
       </c>
-      <c r="F71" s="23">
-        <v>0</v>
-      </c>
-      <c r="G71" s="22" t="s">
-        <v>168</v>
-      </c>
-      <c r="H71" s="22" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="72" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B72" s="27" t="s">
-        <v>1</v>
-      </c>
-      <c r="C72" s="24" t="s">
-        <v>176</v>
-      </c>
-      <c r="D72" s="24">
+      <c r="F71" s="24">
+        <v>1</v>
+      </c>
+      <c r="G71" s="26" t="s">
+        <v>228</v>
+      </c>
+      <c r="H71" s="26" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="72" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B72" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="C72" s="23" t="s">
+        <v>230</v>
+      </c>
+      <c r="D72" s="23">
         <v>0</v>
       </c>
       <c r="E72" s="24">
         <v>7</v>
       </c>
-      <c r="F72" s="24">
+      <c r="F72" s="23">
         <v>1</v>
       </c>
       <c r="G72" s="26" t="s">
-        <v>182</v>
-      </c>
-      <c r="H72" s="26"/>
-    </row>
-    <row r="73" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B73" s="27" t="s">
+        <v>231</v>
+      </c>
+      <c r="H72" s="26" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="73" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B73" s="25" t="s">
         <v>1</v>
       </c>
       <c r="C73" s="24" t="s">
-        <v>178</v>
+        <v>233</v>
       </c>
       <c r="D73" s="24">
         <v>0</v>
@@ -5611,21 +5664,21 @@
         <v>7</v>
       </c>
       <c r="F73" s="24">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G73" s="26" t="s">
-        <v>183</v>
+        <v>234</v>
       </c>
       <c r="H73" s="26" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="74" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B74" s="27" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="74" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B74" s="25" t="s">
         <v>1</v>
       </c>
       <c r="C74" s="24" t="s">
-        <v>179</v>
+        <v>236</v>
       </c>
       <c r="D74" s="24">
         <v>0</v>
@@ -5637,39 +5690,41 @@
         <v>1</v>
       </c>
       <c r="G74" s="26" t="s">
-        <v>209</v>
+        <v>237</v>
       </c>
       <c r="H74" s="26" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="75" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B75" s="27" t="s">
-        <v>1</v>
-      </c>
-      <c r="C75" s="24" t="s">
-        <v>312</v>
-      </c>
-      <c r="D75" s="24">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="75" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B75" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="C75" s="23" t="s">
+        <v>145</v>
+      </c>
+      <c r="D75" s="23">
         <v>0</v>
       </c>
       <c r="E75" s="24">
         <v>7</v>
       </c>
-      <c r="F75" s="24">
-        <v>1</v>
-      </c>
-      <c r="G75" s="26" t="s">
-        <v>313</v>
-      </c>
-      <c r="H75" s="26"/>
-    </row>
-    <row r="76" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="F75" s="23">
+        <v>0</v>
+      </c>
+      <c r="G75" s="22" t="s">
+        <v>168</v>
+      </c>
+      <c r="H75" s="22" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="76" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B76" s="27" t="s">
         <v>1</v>
       </c>
       <c r="C76" s="24" t="s">
-        <v>314</v>
+        <v>176</v>
       </c>
       <c r="D76" s="24">
         <v>0</v>
@@ -5681,660 +5736,692 @@
         <v>1</v>
       </c>
       <c r="G76" s="26" t="s">
+        <v>182</v>
+      </c>
+      <c r="H76" s="26"/>
+    </row>
+    <row r="77" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B77" s="27" t="s">
+        <v>1</v>
+      </c>
+      <c r="C77" s="24" t="s">
+        <v>178</v>
+      </c>
+      <c r="D77" s="24">
+        <v>0</v>
+      </c>
+      <c r="E77" s="24">
+        <v>7</v>
+      </c>
+      <c r="F77" s="24">
+        <v>0</v>
+      </c>
+      <c r="G77" s="26" t="s">
+        <v>183</v>
+      </c>
+      <c r="H77" s="26" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="78" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B78" s="27" t="s">
+        <v>1</v>
+      </c>
+      <c r="C78" s="24" t="s">
+        <v>179</v>
+      </c>
+      <c r="D78" s="24">
+        <v>0</v>
+      </c>
+      <c r="E78" s="24">
+        <v>7</v>
+      </c>
+      <c r="F78" s="24">
+        <v>1</v>
+      </c>
+      <c r="G78" s="26" t="s">
+        <v>209</v>
+      </c>
+      <c r="H78" s="26" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="79" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B79" s="27" t="s">
+        <v>1</v>
+      </c>
+      <c r="C79" s="24" t="s">
+        <v>312</v>
+      </c>
+      <c r="D79" s="24">
+        <v>0</v>
+      </c>
+      <c r="E79" s="24">
+        <v>7</v>
+      </c>
+      <c r="F79" s="24">
+        <v>1</v>
+      </c>
+      <c r="G79" s="26" t="s">
+        <v>313</v>
+      </c>
+      <c r="H79" s="26"/>
+    </row>
+    <row r="80" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B80" s="27" t="s">
+        <v>1</v>
+      </c>
+      <c r="C80" s="24" t="s">
+        <v>314</v>
+      </c>
+      <c r="D80" s="24">
+        <v>0</v>
+      </c>
+      <c r="E80" s="24">
+        <v>7</v>
+      </c>
+      <c r="F80" s="24">
+        <v>1</v>
+      </c>
+      <c r="G80" s="26" t="s">
         <v>315</v>
       </c>
-      <c r="H76" s="26"/>
-    </row>
-    <row r="77" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B77" s="56" t="s">
-        <v>1</v>
-      </c>
-      <c r="C77" s="54" t="s">
+      <c r="H80" s="26"/>
+    </row>
+    <row r="81" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B81" s="56" t="s">
+        <v>1</v>
+      </c>
+      <c r="C81" s="54" t="s">
         <v>330</v>
       </c>
-      <c r="D77" s="54">
-        <v>0</v>
-      </c>
-      <c r="E77" s="54">
+      <c r="D81" s="54">
+        <v>0</v>
+      </c>
+      <c r="E81" s="54">
         <v>7</v>
       </c>
-      <c r="F77" s="54">
+      <c r="F81" s="54">
         <v>2</v>
       </c>
-      <c r="G77" s="55" t="s">
+      <c r="G81" s="55" t="s">
         <v>332</v>
       </c>
-      <c r="H77" s="55" t="s">
+      <c r="H81" s="55" t="s">
         <v>333</v>
       </c>
     </row>
-    <row r="78" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="79" spans="2:13" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B79" s="6" t="s">
+    <row r="82" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="83" spans="2:13" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B83" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="C79" s="6"/>
-      <c r="D79" s="6"/>
-      <c r="E79" s="6"/>
-      <c r="F79" s="6"/>
-      <c r="G79" s="6"/>
-      <c r="H79" s="6"/>
-      <c r="I79" s="6"/>
-      <c r="J79" s="6"/>
-      <c r="K79" s="6"/>
-      <c r="L79" s="6"/>
-      <c r="M79" s="6"/>
-    </row>
-    <row r="80" spans="2:13" ht="60" x14ac:dyDescent="0.25">
-      <c r="B80" s="20"/>
-      <c r="C80" s="20"/>
-      <c r="D80" s="20"/>
-      <c r="E80" s="20"/>
-      <c r="F80" s="21" t="s">
+      <c r="C83" s="6"/>
+      <c r="D83" s="6"/>
+      <c r="E83" s="6"/>
+      <c r="F83" s="6"/>
+      <c r="G83" s="6"/>
+      <c r="H83" s="6"/>
+      <c r="I83" s="6"/>
+      <c r="J83" s="6"/>
+      <c r="K83" s="6"/>
+      <c r="L83" s="6"/>
+      <c r="M83" s="6"/>
+    </row>
+    <row r="84" spans="2:13" ht="60" x14ac:dyDescent="0.25">
+      <c r="B84" s="20"/>
+      <c r="C84" s="20"/>
+      <c r="D84" s="20"/>
+      <c r="E84" s="20"/>
+      <c r="F84" s="21" t="s">
         <v>40</v>
       </c>
-      <c r="G80" s="66" t="s">
+      <c r="G84" s="66" t="s">
         <v>39</v>
       </c>
-      <c r="H80" s="66"/>
-      <c r="I80" s="20"/>
-    </row>
-    <row r="81" spans="2:12" ht="142.5" x14ac:dyDescent="0.25">
-      <c r="B81" s="19" t="s">
+      <c r="H84" s="66"/>
+      <c r="I84" s="20"/>
+    </row>
+    <row r="85" spans="2:13" ht="142.5" x14ac:dyDescent="0.25">
+      <c r="B85" s="19" t="s">
         <v>38</v>
       </c>
-      <c r="C81" s="19" t="s">
+      <c r="C85" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="D81" s="18" t="s">
+      <c r="D85" s="18" t="s">
         <v>223</v>
       </c>
-      <c r="E81" s="18" t="s">
+      <c r="E85" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="F81" s="17" t="s">
+      <c r="F85" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="G81" s="17" t="s">
+      <c r="G85" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="H81" s="17" t="s">
+      <c r="H85" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="I81" s="16" t="s">
+      <c r="I85" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="J81" s="16" t="s">
+      <c r="J85" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="K81" s="15" t="s">
+      <c r="K85" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="L81" s="14" t="s">
+      <c r="L85" s="14" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="82" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B82" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="C82" s="11" t="s">
+    <row r="86" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B86" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="C86" s="11" t="s">
         <v>220</v>
       </c>
-      <c r="D82" s="11" t="s">
+      <c r="D86" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="E82" s="11">
-        <v>0</v>
-      </c>
-      <c r="F82" s="10">
-        <v>0</v>
-      </c>
-      <c r="G82" s="10">
+      <c r="E86" s="11">
+        <v>0</v>
+      </c>
+      <c r="F86" s="10">
+        <v>0</v>
+      </c>
+      <c r="G86" s="10">
         <v>15</v>
       </c>
-      <c r="H82" s="10">
+      <c r="H86" s="10">
         <v>200</v>
       </c>
-      <c r="I82" s="9">
+      <c r="I86" s="9">
         <v>0.5</v>
       </c>
-      <c r="J82" s="9">
-        <v>1</v>
-      </c>
-      <c r="K82" s="8" t="s">
+      <c r="J86" s="9">
+        <v>1</v>
+      </c>
+      <c r="K86" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="L82" s="13" t="s">
+      <c r="L86" s="13" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="83" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B83" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="C83" s="11" t="s">
+    <row r="87" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B87" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="C87" s="11" t="s">
         <v>221</v>
       </c>
-      <c r="D83" s="11" t="s">
+      <c r="D87" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="E83" s="11">
-        <v>1</v>
-      </c>
-      <c r="F83" s="10">
-        <v>0</v>
-      </c>
-      <c r="G83" s="10">
+      <c r="E87" s="11">
+        <v>1</v>
+      </c>
+      <c r="F87" s="10">
+        <v>0</v>
+      </c>
+      <c r="G87" s="10">
         <v>60</v>
       </c>
-      <c r="H83" s="10">
+      <c r="H87" s="10">
         <v>300</v>
       </c>
-      <c r="I83" s="9">
+      <c r="I87" s="9">
         <v>0.5</v>
       </c>
-      <c r="J83" s="9">
-        <v>1</v>
-      </c>
-      <c r="K83" s="8" t="s">
+      <c r="J87" s="9">
+        <v>1</v>
+      </c>
+      <c r="K87" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="L83" s="13" t="s">
+      <c r="L87" s="13" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="84" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B84" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="C84" s="11" t="s">
+    <row r="88" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B88" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="C88" s="11" t="s">
         <v>222</v>
       </c>
-      <c r="D84" s="11" t="s">
+      <c r="D88" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="E84" s="11">
+      <c r="E88" s="11">
         <v>2</v>
       </c>
-      <c r="F84" s="10">
-        <v>0</v>
-      </c>
-      <c r="G84" s="10">
+      <c r="F88" s="10">
+        <v>0</v>
+      </c>
+      <c r="G88" s="10">
         <v>240</v>
       </c>
-      <c r="H84" s="10">
+      <c r="H88" s="10">
         <v>600</v>
       </c>
-      <c r="I84" s="9">
+      <c r="I88" s="9">
         <v>0.5</v>
       </c>
-      <c r="J84" s="9">
-        <v>1</v>
-      </c>
-      <c r="K84" s="8" t="s">
+      <c r="J88" s="9">
+        <v>1</v>
+      </c>
+      <c r="K88" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="L84" s="7" t="s">
+      <c r="L88" s="7" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="86" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="87" spans="2:12" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B87" s="6" t="s">
+    <row r="90" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="91" spans="2:13" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B91" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="C87" s="6"/>
-      <c r="D87" s="6"/>
-      <c r="E87" s="6"/>
-      <c r="F87" s="6"/>
-      <c r="G87" s="6"/>
-    </row>
-    <row r="89" spans="2:12" ht="135.75" x14ac:dyDescent="0.25">
-      <c r="B89" s="5" t="s">
+      <c r="C91" s="6"/>
+      <c r="D91" s="6"/>
+      <c r="E91" s="6"/>
+      <c r="F91" s="6"/>
+      <c r="G91" s="6"/>
+    </row>
+    <row r="93" spans="2:13" ht="135.75" x14ac:dyDescent="0.25">
+      <c r="B93" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="C89" s="4" t="s">
+      <c r="C93" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D89" s="3" t="s">
+      <c r="D93" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E89" s="3" t="s">
+      <c r="E93" s="3" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="90" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B90" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C90" s="1" t="s">
+    <row r="94" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B94" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C94" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D90" s="1">
+      <c r="D94" s="1">
         <v>0.1</v>
       </c>
-      <c r="E90" s="1">
+      <c r="E94" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="91" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B91" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C91" s="1" t="s">
+    <row r="95" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B95" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C95" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D91" s="1">
+      <c r="D95" s="1">
         <v>0.7</v>
       </c>
-      <c r="E91" s="1">
+      <c r="E95" s="1">
         <v>6</v>
       </c>
     </row>
-    <row r="92" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B92" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C92" s="1" t="s">
+    <row r="96" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B96" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C96" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D92" s="1">
-        <v>1</v>
-      </c>
-      <c r="E92" s="1">
+      <c r="D96" s="1">
+        <v>1</v>
+      </c>
+      <c r="E96" s="1">
         <v>12</v>
       </c>
     </row>
-    <row r="93" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B93" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C93" s="1" t="s">
+    <row r="97" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B97" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C97" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D93" s="1">
+      <c r="D97" s="1">
         <v>1.5</v>
       </c>
-      <c r="E93" s="1">
+      <c r="E97" s="1">
         <v>18</v>
       </c>
     </row>
-    <row r="94" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B94" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C94" s="1" t="s">
+    <row r="98" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B98" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C98" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D94" s="1">
+      <c r="D98" s="1">
         <v>2</v>
       </c>
-      <c r="E94" s="1">
+      <c r="E98" s="1">
         <v>26</v>
       </c>
     </row>
-    <row r="95" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B95" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C95" s="1" t="s">
+    <row r="99" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B99" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C99" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D95" s="1">
+      <c r="D99" s="1">
         <v>2.5</v>
       </c>
-      <c r="E95" s="1">
+      <c r="E99" s="1">
         <v>35</v>
       </c>
     </row>
-    <row r="96" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B96" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C96" s="1" t="s">
+    <row r="100" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B100" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C100" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D96" s="1">
+      <c r="D100" s="1">
         <v>3</v>
       </c>
-      <c r="E96" s="1">
+      <c r="E100" s="1">
         <v>45</v>
       </c>
     </row>
-    <row r="97" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B97" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C97" s="1" t="s">
+    <row r="101" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B101" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C101" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D97" s="1">
+      <c r="D101" s="1">
         <v>4</v>
       </c>
-      <c r="E97" s="1">
+      <c r="E101" s="1">
         <v>56</v>
       </c>
     </row>
-    <row r="98" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B98" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C98" s="1" t="s">
+    <row r="102" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B102" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C102" s="1" t="s">
         <v>214</v>
       </c>
-      <c r="D98" s="1">
+      <c r="D102" s="1">
         <v>4.5</v>
       </c>
-      <c r="E98" s="1">
+      <c r="E102" s="1">
         <v>62</v>
       </c>
     </row>
-    <row r="99" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B99" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C99" s="1" t="s">
+    <row r="103" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B103" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C103" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D99" s="1">
+      <c r="D103" s="1">
         <v>5</v>
       </c>
-      <c r="E99" s="1">
+      <c r="E103" s="1">
         <v>65</v>
       </c>
     </row>
-    <row r="100" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B100" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C100" s="1" t="s">
+    <row r="104" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B104" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C104" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D100" s="1">
+      <c r="D104" s="1">
         <v>7</v>
       </c>
-      <c r="E100" s="1">
+      <c r="E104" s="1">
         <v>70</v>
       </c>
     </row>
-    <row r="101" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B101" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C101" s="1" t="s">
+    <row r="105" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B105" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C105" s="1" t="s">
         <v>219</v>
-      </c>
-      <c r="D101" s="42">
-        <v>7.5</v>
-      </c>
-      <c r="E101" s="42">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="102" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B102" s="51" t="s">
-        <v>1</v>
-      </c>
-      <c r="C102" s="42" t="s">
-        <v>305</v>
-      </c>
-      <c r="D102" s="42">
-        <v>8</v>
-      </c>
-      <c r="E102" s="42">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="103" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B103" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C103" s="1" t="s">
-        <v>334</v>
-      </c>
-      <c r="D103" s="42">
-        <v>8.1</v>
-      </c>
-      <c r="E103" s="42">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="104" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B104" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C104" s="1" t="s">
-        <v>335</v>
-      </c>
-      <c r="D104" s="42">
-        <v>8</v>
-      </c>
-      <c r="E104" s="42">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="105" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B105" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C105" s="1" t="s">
-        <v>336</v>
       </c>
       <c r="D105" s="42">
         <v>7.5</v>
       </c>
       <c r="E105" s="42">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="106" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B106" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C106" s="1" t="s">
-        <v>337</v>
+        <v>70</v>
+      </c>
+    </row>
+    <row r="106" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B106" s="51" t="s">
+        <v>1</v>
+      </c>
+      <c r="C106" s="42" t="s">
+        <v>305</v>
       </c>
       <c r="D106" s="42">
         <v>8</v>
       </c>
       <c r="E106" s="42">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="107" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B107" s="51" t="s">
-        <v>1</v>
-      </c>
-      <c r="C107" s="42" t="s">
-        <v>338</v>
+        <v>70</v>
+      </c>
+    </row>
+    <row r="107" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B107" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C107" s="1" t="s">
+        <v>334</v>
       </c>
       <c r="D107" s="42">
-        <v>7.5</v>
+        <v>8.1</v>
       </c>
       <c r="E107" s="42">
         <v>75</v>
       </c>
     </row>
-    <row r="108" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="109" spans="2:7" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B109" s="6" t="s">
+    <row r="108" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B108" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C108" s="1" t="s">
+        <v>335</v>
+      </c>
+      <c r="D108" s="42">
+        <v>8</v>
+      </c>
+      <c r="E108" s="42">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="109" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B109" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C109" s="1" t="s">
+        <v>336</v>
+      </c>
+      <c r="D109" s="42">
+        <v>7.5</v>
+      </c>
+      <c r="E109" s="42">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="110" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B110" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C110" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="D110" s="42">
+        <v>8</v>
+      </c>
+      <c r="E110" s="42">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="111" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B111" s="51" t="s">
+        <v>1</v>
+      </c>
+      <c r="C111" s="42" t="s">
+        <v>338</v>
+      </c>
+      <c r="D111" s="42">
+        <v>7.5</v>
+      </c>
+      <c r="E111" s="42">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="112" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="113" spans="2:7" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B113" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C109" s="6"/>
-      <c r="D109" s="6"/>
-      <c r="E109" s="6"/>
-      <c r="F109" s="6"/>
-      <c r="G109" s="6"/>
-    </row>
-    <row r="111" spans="2:7" ht="142.5" x14ac:dyDescent="0.25">
-      <c r="B111" s="5" t="s">
+      <c r="C113" s="6"/>
+      <c r="D113" s="6"/>
+      <c r="E113" s="6"/>
+      <c r="F113" s="6"/>
+      <c r="G113" s="6"/>
+    </row>
+    <row r="115" spans="2:7" ht="142.5" x14ac:dyDescent="0.25">
+      <c r="B115" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C111" s="4" t="s">
+      <c r="C115" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D111" s="4" t="s">
+      <c r="D115" s="4" t="s">
         <v>223</v>
       </c>
-      <c r="E111" s="3" t="s">
+      <c r="E115" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="112" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B112" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C112" s="1" t="s">
+    <row r="116" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B116" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C116" s="1" t="s">
         <v>224</v>
       </c>
-      <c r="D112" s="1" t="s">
+      <c r="D116" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E112" s="1">
+      <c r="E116" s="1">
         <v>0.05</v>
       </c>
     </row>
-    <row r="113" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B113" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C113" s="1" t="s">
+    <row r="117" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B117" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C117" s="1" t="s">
         <v>225</v>
       </c>
-      <c r="D113" s="1" t="s">
+      <c r="D117" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E113" s="1">
+      <c r="E117" s="1">
         <v>0.1</v>
       </c>
     </row>
-    <row r="114" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B114" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C114" s="1" t="s">
+    <row r="118" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B118" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C118" s="1" t="s">
         <v>226</v>
       </c>
-      <c r="D114" s="1" t="s">
+      <c r="D118" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E114" s="1">
+      <c r="E118" s="1">
         <v>0.2</v>
       </c>
     </row>
-    <row r="115" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="116" spans="2:7" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B116" s="6" t="s">
+    <row r="119" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="120" spans="2:7" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B120" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C116" s="6"/>
-      <c r="D116" s="6"/>
-      <c r="E116" s="6"/>
-      <c r="F116" s="6"/>
-      <c r="G116" s="6"/>
-    </row>
-    <row r="118" spans="2:7" ht="132" x14ac:dyDescent="0.25">
-      <c r="B118" s="5" t="s">
+      <c r="C120" s="6"/>
+      <c r="D120" s="6"/>
+      <c r="E120" s="6"/>
+      <c r="F120" s="6"/>
+      <c r="G120" s="6"/>
+    </row>
+    <row r="122" spans="2:7" ht="132" x14ac:dyDescent="0.25">
+      <c r="B122" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C118" s="4" t="s">
+      <c r="C122" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D118" s="3" t="s">
+      <c r="D122" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="119" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B119" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C119" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D119" s="1">
+    <row r="123" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B123" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C123" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D123" s="1">
         <v>0.7</v>
       </c>
     </row>
-    <row r="120" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="121" spans="2:7" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B121" s="6" t="s">
+    <row r="124" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="125" spans="2:7" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B125" s="6" t="s">
         <v>239</v>
       </c>
-      <c r="C121" s="6"/>
-      <c r="D121" s="6"/>
-      <c r="E121" s="6"/>
-      <c r="F121" s="6"/>
-      <c r="G121" s="6"/>
-    </row>
-    <row r="123" spans="2:7" ht="68.25" x14ac:dyDescent="0.25">
-      <c r="B123" s="44" t="s">
+      <c r="C125" s="6"/>
+      <c r="D125" s="6"/>
+      <c r="E125" s="6"/>
+      <c r="F125" s="6"/>
+      <c r="G125" s="6"/>
+    </row>
+    <row r="127" spans="2:7" ht="68.25" x14ac:dyDescent="0.25">
+      <c r="B127" s="44" t="s">
         <v>240</v>
       </c>
-      <c r="C123" s="44" t="s">
+      <c r="C127" s="44" t="s">
         <v>3</v>
       </c>
-      <c r="D123" s="45" t="s">
+      <c r="D127" s="45" t="s">
         <v>241</v>
       </c>
-      <c r="E123" s="45" t="s">
+      <c r="E127" s="45" t="s">
         <v>242</v>
-      </c>
-    </row>
-    <row r="124" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B124" s="43" t="s">
-        <v>1</v>
-      </c>
-      <c r="C124" s="46" t="s">
-        <v>80</v>
-      </c>
-      <c r="D124" s="46" t="s">
-        <v>263</v>
-      </c>
-      <c r="E124" s="43" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="125" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B125" s="43" t="s">
-        <v>1</v>
-      </c>
-      <c r="C125" s="46" t="s">
-        <v>93</v>
-      </c>
-      <c r="D125" s="46" t="s">
-        <v>264</v>
-      </c>
-      <c r="E125" s="43" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="126" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B126" s="43" t="s">
-        <v>1</v>
-      </c>
-      <c r="C126" s="46" t="s">
-        <v>124</v>
-      </c>
-      <c r="D126" s="46" t="s">
-        <v>265</v>
-      </c>
-      <c r="E126" s="43" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="127" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B127" s="43" t="s">
-        <v>1</v>
-      </c>
-      <c r="C127" s="46" t="s">
-        <v>108</v>
-      </c>
-      <c r="D127" s="46" t="s">
-        <v>108</v>
-      </c>
-      <c r="E127" s="43" t="b">
-        <v>0</v>
       </c>
     </row>
     <row r="128" spans="2:7" x14ac:dyDescent="0.25">
@@ -6342,13 +6429,13 @@
         <v>1</v>
       </c>
       <c r="C128" s="46" t="s">
-        <v>120</v>
+        <v>80</v>
       </c>
       <c r="D128" s="46" t="s">
-        <v>120</v>
+        <v>263</v>
       </c>
       <c r="E128" s="43" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="129" spans="2:5" x14ac:dyDescent="0.25">
@@ -6356,13 +6443,13 @@
         <v>1</v>
       </c>
       <c r="C129" s="46" t="s">
-        <v>109</v>
+        <v>93</v>
       </c>
       <c r="D129" s="46" t="s">
-        <v>109</v>
+        <v>264</v>
       </c>
       <c r="E129" s="43" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="130" spans="2:5" x14ac:dyDescent="0.25">
@@ -6370,10 +6457,10 @@
         <v>1</v>
       </c>
       <c r="C130" s="46" t="s">
-        <v>111</v>
+        <v>124</v>
       </c>
       <c r="D130" s="46" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="E130" s="43" t="b">
         <v>1</v>
@@ -6384,13 +6471,13 @@
         <v>1</v>
       </c>
       <c r="C131" s="46" t="s">
-        <v>243</v>
+        <v>108</v>
       </c>
       <c r="D131" s="46" t="s">
-        <v>267</v>
+        <v>108</v>
       </c>
       <c r="E131" s="43" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="132" spans="2:5" x14ac:dyDescent="0.25">
@@ -6398,13 +6485,13 @@
         <v>1</v>
       </c>
       <c r="C132" s="46" t="s">
-        <v>244</v>
+        <v>120</v>
       </c>
       <c r="D132" s="46" t="s">
-        <v>268</v>
+        <v>120</v>
       </c>
       <c r="E132" s="43" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="133" spans="2:5" x14ac:dyDescent="0.25">
@@ -6412,13 +6499,13 @@
         <v>1</v>
       </c>
       <c r="C133" s="46" t="s">
-        <v>204</v>
+        <v>109</v>
       </c>
       <c r="D133" s="46" t="s">
-        <v>269</v>
+        <v>109</v>
       </c>
       <c r="E133" s="43" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="134" spans="2:5" x14ac:dyDescent="0.25">
@@ -6426,10 +6513,10 @@
         <v>1</v>
       </c>
       <c r="C134" s="46" t="s">
-        <v>203</v>
+        <v>111</v>
       </c>
       <c r="D134" s="46" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="E134" s="43" t="b">
         <v>1</v>
@@ -6440,10 +6527,10 @@
         <v>1</v>
       </c>
       <c r="C135" s="46" t="s">
-        <v>198</v>
+        <v>243</v>
       </c>
       <c r="D135" s="46" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="E135" s="43" t="b">
         <v>1</v>
@@ -6454,10 +6541,10 @@
         <v>1</v>
       </c>
       <c r="C136" s="46" t="s">
-        <v>202</v>
+        <v>244</v>
       </c>
       <c r="D136" s="46" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
       <c r="E136" s="43" t="b">
         <v>1</v>
@@ -6468,10 +6555,10 @@
         <v>1</v>
       </c>
       <c r="C137" s="46" t="s">
-        <v>201</v>
+        <v>204</v>
       </c>
       <c r="D137" s="46" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
       <c r="E137" s="43" t="b">
         <v>1</v>
@@ -6482,10 +6569,10 @@
         <v>1</v>
       </c>
       <c r="C138" s="46" t="s">
-        <v>199</v>
+        <v>203</v>
       </c>
       <c r="D138" s="46" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="E138" s="43" t="b">
         <v>1</v>
@@ -6496,10 +6583,10 @@
         <v>1</v>
       </c>
       <c r="C139" s="46" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="D139" s="46" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="E139" s="43" t="b">
         <v>1</v>
@@ -6510,10 +6597,10 @@
         <v>1</v>
       </c>
       <c r="C140" s="46" t="s">
-        <v>113</v>
+        <v>202</v>
       </c>
       <c r="D140" s="46" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="E140" s="43" t="b">
         <v>1</v>
@@ -6524,13 +6611,13 @@
         <v>1</v>
       </c>
       <c r="C141" s="46" t="s">
-        <v>245</v>
+        <v>201</v>
       </c>
       <c r="D141" s="46" t="s">
-        <v>245</v>
+        <v>273</v>
       </c>
       <c r="E141" s="43" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="142" spans="2:5" x14ac:dyDescent="0.25">
@@ -6538,10 +6625,10 @@
         <v>1</v>
       </c>
       <c r="C142" s="46" t="s">
-        <v>83</v>
+        <v>199</v>
       </c>
       <c r="D142" s="46" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="E142" s="43" t="b">
         <v>1</v>
@@ -6552,10 +6639,10 @@
         <v>1</v>
       </c>
       <c r="C143" s="46" t="s">
-        <v>96</v>
+        <v>200</v>
       </c>
       <c r="D143" s="46" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="E143" s="43" t="b">
         <v>1</v>
@@ -6566,10 +6653,10 @@
         <v>1</v>
       </c>
       <c r="C144" s="46" t="s">
-        <v>246</v>
+        <v>113</v>
       </c>
       <c r="D144" s="46" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="E144" s="43" t="b">
         <v>1</v>
@@ -6580,13 +6667,13 @@
         <v>1</v>
       </c>
       <c r="C145" s="46" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="D145" s="46" t="s">
-        <v>280</v>
+        <v>245</v>
       </c>
       <c r="E145" s="43" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="146" spans="2:5" x14ac:dyDescent="0.25">
@@ -6594,10 +6681,10 @@
         <v>1</v>
       </c>
       <c r="C146" s="46" t="s">
-        <v>102</v>
+        <v>83</v>
       </c>
       <c r="D146" s="46" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
       <c r="E146" s="43" t="b">
         <v>1</v>
@@ -6608,10 +6695,10 @@
         <v>1</v>
       </c>
       <c r="C147" s="46" t="s">
-        <v>248</v>
+        <v>96</v>
       </c>
       <c r="D147" s="46" t="s">
-        <v>303</v>
+        <v>278</v>
       </c>
       <c r="E147" s="43" t="b">
         <v>1</v>
@@ -6622,10 +6709,10 @@
         <v>1</v>
       </c>
       <c r="C148" s="46" t="s">
-        <v>122</v>
+        <v>246</v>
       </c>
       <c r="D148" s="46" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="E148" s="43" t="b">
         <v>1</v>
@@ -6636,10 +6723,10 @@
         <v>1</v>
       </c>
       <c r="C149" s="46" t="s">
-        <v>88</v>
+        <v>247</v>
       </c>
       <c r="D149" s="46" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="E149" s="43" t="b">
         <v>1</v>
@@ -6650,10 +6737,10 @@
         <v>1</v>
       </c>
       <c r="C150" s="46" t="s">
-        <v>249</v>
+        <v>102</v>
       </c>
       <c r="D150" s="46" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="E150" s="43" t="b">
         <v>1</v>
@@ -6664,10 +6751,10 @@
         <v>1</v>
       </c>
       <c r="C151" s="46" t="s">
-        <v>301</v>
+        <v>248</v>
       </c>
       <c r="D151" s="46" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="E151" s="43" t="b">
         <v>1</v>
@@ -6678,13 +6765,13 @@
         <v>1</v>
       </c>
       <c r="C152" s="46" t="s">
-        <v>250</v>
+        <v>122</v>
       </c>
       <c r="D152" s="46" t="s">
-        <v>250</v>
+        <v>282</v>
       </c>
       <c r="E152" s="43" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="153" spans="2:5" x14ac:dyDescent="0.25">
@@ -6692,13 +6779,13 @@
         <v>1</v>
       </c>
       <c r="C153" s="46" t="s">
-        <v>115</v>
+        <v>88</v>
       </c>
       <c r="D153" s="46" t="s">
-        <v>115</v>
+        <v>283</v>
       </c>
       <c r="E153" s="43" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="154" spans="2:5" x14ac:dyDescent="0.25">
@@ -6706,10 +6793,10 @@
         <v>1</v>
       </c>
       <c r="C154" s="46" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="D154" s="46" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="E154" s="43" t="b">
         <v>1</v>
@@ -6720,10 +6807,10 @@
         <v>1</v>
       </c>
       <c r="C155" s="46" t="s">
-        <v>91</v>
+        <v>301</v>
       </c>
       <c r="D155" s="46" t="s">
-        <v>286</v>
+        <v>302</v>
       </c>
       <c r="E155" s="43" t="b">
         <v>1</v>
@@ -6734,13 +6821,13 @@
         <v>1</v>
       </c>
       <c r="C156" s="46" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="D156" s="46" t="s">
-        <v>287</v>
+        <v>250</v>
       </c>
       <c r="E156" s="43" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="157" spans="2:5" x14ac:dyDescent="0.25">
@@ -6748,13 +6835,13 @@
         <v>1</v>
       </c>
       <c r="C157" s="46" t="s">
-        <v>253</v>
+        <v>115</v>
       </c>
       <c r="D157" s="46" t="s">
-        <v>288</v>
+        <v>115</v>
       </c>
       <c r="E157" s="43" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="158" spans="2:5" x14ac:dyDescent="0.25">
@@ -6762,10 +6849,10 @@
         <v>1</v>
       </c>
       <c r="C158" s="46" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="D158" s="46" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
       <c r="E158" s="43" t="b">
         <v>1</v>
@@ -6776,10 +6863,10 @@
         <v>1</v>
       </c>
       <c r="C159" s="46" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="D159" s="46" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="E159" s="43" t="b">
         <v>1</v>
@@ -6790,13 +6877,13 @@
         <v>1</v>
       </c>
       <c r="C160" s="46" t="s">
-        <v>73</v>
+        <v>252</v>
       </c>
       <c r="D160" s="46" t="s">
-        <v>73</v>
+        <v>287</v>
       </c>
       <c r="E160" s="43" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="161" spans="2:5" x14ac:dyDescent="0.25">
@@ -6804,13 +6891,13 @@
         <v>1</v>
       </c>
       <c r="C161" s="46" t="s">
-        <v>107</v>
+        <v>253</v>
       </c>
       <c r="D161" s="46" t="s">
-        <v>107</v>
+        <v>288</v>
       </c>
       <c r="E161" s="43" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="162" spans="2:5" x14ac:dyDescent="0.25">
@@ -6818,10 +6905,10 @@
         <v>1</v>
       </c>
       <c r="C162" s="46" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="D162" s="46" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="E162" s="43" t="b">
         <v>1</v>
@@ -6832,10 +6919,10 @@
         <v>1</v>
       </c>
       <c r="C163" s="46" t="s">
-        <v>256</v>
+        <v>86</v>
       </c>
       <c r="D163" s="46" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="E163" s="43" t="b">
         <v>1</v>
@@ -6846,13 +6933,13 @@
         <v>1</v>
       </c>
       <c r="C164" s="46" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="D164" s="46" t="s">
-        <v>293</v>
+        <v>73</v>
       </c>
       <c r="E164" s="43" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="165" spans="2:5" x14ac:dyDescent="0.25">
@@ -6860,13 +6947,13 @@
         <v>1</v>
       </c>
       <c r="C165" s="46" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="D165" s="46" t="s">
-        <v>294</v>
+        <v>107</v>
       </c>
       <c r="E165" s="43" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="166" spans="2:5" x14ac:dyDescent="0.25">
@@ -6874,10 +6961,10 @@
         <v>1</v>
       </c>
       <c r="C166" s="46" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="D166" s="46" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
       <c r="E166" s="43" t="b">
         <v>1</v>
@@ -6888,10 +6975,10 @@
         <v>1</v>
       </c>
       <c r="C167" s="46" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="D167" s="46" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="E167" s="43" t="b">
         <v>1</v>
@@ -6902,10 +6989,10 @@
         <v>1</v>
       </c>
       <c r="C168" s="46" t="s">
-        <v>259</v>
+        <v>77</v>
       </c>
       <c r="D168" s="46" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="E168" s="43" t="b">
         <v>1</v>
@@ -6916,13 +7003,13 @@
         <v>1</v>
       </c>
       <c r="C169" s="46" t="s">
-        <v>260</v>
+        <v>105</v>
       </c>
       <c r="D169" s="46" t="s">
-        <v>260</v>
+        <v>294</v>
       </c>
       <c r="E169" s="43" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="170" spans="2:5" x14ac:dyDescent="0.25">
@@ -6930,10 +7017,10 @@
         <v>1</v>
       </c>
       <c r="C170" s="46" t="s">
-        <v>99</v>
+        <v>257</v>
       </c>
       <c r="D170" s="46" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="E170" s="43" t="b">
         <v>1</v>
@@ -6944,10 +7031,10 @@
         <v>1</v>
       </c>
       <c r="C171" s="46" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="D171" s="46" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="E171" s="43" t="b">
         <v>1</v>
@@ -6958,10 +7045,10 @@
         <v>1</v>
       </c>
       <c r="C172" s="46" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="D172" s="46" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="E172" s="43" t="b">
         <v>1</v>
@@ -6972,13 +7059,13 @@
         <v>1</v>
       </c>
       <c r="C173" s="46" t="s">
-        <v>309</v>
+        <v>260</v>
       </c>
       <c r="D173" s="46" t="s">
-        <v>306</v>
+        <v>260</v>
       </c>
       <c r="E173" s="43" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="174" spans="2:5" x14ac:dyDescent="0.25">
@@ -6986,10 +7073,10 @@
         <v>1</v>
       </c>
       <c r="C174" s="46" t="s">
-        <v>310</v>
+        <v>99</v>
       </c>
       <c r="D174" s="46" t="s">
-        <v>307</v>
+        <v>298</v>
       </c>
       <c r="E174" s="43" t="b">
         <v>1</v>
@@ -7000,10 +7087,10 @@
         <v>1</v>
       </c>
       <c r="C175" s="46" t="s">
-        <v>311</v>
+        <v>261</v>
       </c>
       <c r="D175" s="46" t="s">
-        <v>308</v>
+        <v>299</v>
       </c>
       <c r="E175" s="43" t="b">
         <v>1</v>
@@ -7014,10 +7101,10 @@
         <v>1</v>
       </c>
       <c r="C176" s="46" t="s">
-        <v>319</v>
+        <v>262</v>
       </c>
       <c r="D176" s="46" t="s">
-        <v>320</v>
+        <v>300</v>
       </c>
       <c r="E176" s="43" t="b">
         <v>1</v>
@@ -7028,10 +7115,10 @@
         <v>1</v>
       </c>
       <c r="C177" s="46" t="s">
-        <v>321</v>
+        <v>309</v>
       </c>
       <c r="D177" s="46" t="s">
-        <v>322</v>
+        <v>306</v>
       </c>
       <c r="E177" s="43" t="b">
         <v>1</v>
@@ -7042,10 +7129,10 @@
         <v>1</v>
       </c>
       <c r="C178" s="46" t="s">
-        <v>323</v>
+        <v>310</v>
       </c>
       <c r="D178" s="46" t="s">
-        <v>324</v>
+        <v>307</v>
       </c>
       <c r="E178" s="43" t="b">
         <v>1</v>
@@ -7056,10 +7143,10 @@
         <v>1</v>
       </c>
       <c r="C179" s="46" t="s">
-        <v>316</v>
+        <v>311</v>
       </c>
       <c r="D179" s="46" t="s">
-        <v>339</v>
+        <v>308</v>
       </c>
       <c r="E179" s="43" t="b">
         <v>1</v>
@@ -7070,10 +7157,10 @@
         <v>1</v>
       </c>
       <c r="C180" s="46" t="s">
-        <v>317</v>
+        <v>319</v>
       </c>
       <c r="D180" s="46" t="s">
-        <v>340</v>
+        <v>320</v>
       </c>
       <c r="E180" s="43" t="b">
         <v>1</v>
@@ -7084,10 +7171,10 @@
         <v>1</v>
       </c>
       <c r="C181" s="46" t="s">
-        <v>74</v>
+        <v>321</v>
       </c>
       <c r="D181" s="46" t="s">
-        <v>341</v>
+        <v>322</v>
       </c>
       <c r="E181" s="43" t="b">
         <v>1</v>
@@ -7098,10 +7185,10 @@
         <v>1</v>
       </c>
       <c r="C182" s="46" t="s">
-        <v>346</v>
+        <v>323</v>
       </c>
       <c r="D182" s="46" t="s">
-        <v>342</v>
+        <v>324</v>
       </c>
       <c r="E182" s="43" t="b">
         <v>1</v>
@@ -7112,10 +7199,10 @@
         <v>1</v>
       </c>
       <c r="C183" s="46" t="s">
-        <v>347</v>
+        <v>316</v>
       </c>
       <c r="D183" s="46" t="s">
-        <v>343</v>
+        <v>339</v>
       </c>
       <c r="E183" s="43" t="b">
         <v>1</v>
@@ -7126,10 +7213,10 @@
         <v>1</v>
       </c>
       <c r="C184" s="46" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="D184" s="46" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
       <c r="E184" s="43" t="b">
         <v>1</v>
@@ -7140,12 +7227,82 @@
         <v>1</v>
       </c>
       <c r="C185" s="46" t="s">
+        <v>74</v>
+      </c>
+      <c r="D185" s="46" t="s">
+        <v>341</v>
+      </c>
+      <c r="E185" s="43" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="186" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B186" s="43" t="s">
+        <v>1</v>
+      </c>
+      <c r="C186" s="46" t="s">
+        <v>346</v>
+      </c>
+      <c r="D186" s="46" t="s">
+        <v>342</v>
+      </c>
+      <c r="E186" s="43" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="187" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B187" s="43" t="s">
+        <v>1</v>
+      </c>
+      <c r="C187" s="46" t="s">
+        <v>347</v>
+      </c>
+      <c r="D187" s="46" t="s">
+        <v>343</v>
+      </c>
+      <c r="E187" s="43" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="188" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B188" s="43" t="s">
+        <v>1</v>
+      </c>
+      <c r="C188" s="46" t="s">
+        <v>318</v>
+      </c>
+      <c r="D188" s="46" t="s">
+        <v>344</v>
+      </c>
+      <c r="E188" s="43" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="189" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B189" s="43" t="s">
+        <v>1</v>
+      </c>
+      <c r="C189" s="46" t="s">
         <v>348</v>
       </c>
-      <c r="D185" s="46" t="s">
+      <c r="D189" s="46" t="s">
         <v>345</v>
       </c>
-      <c r="E185" s="43" t="b">
+      <c r="E189" s="43" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="190" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B190" s="43" t="s">
+        <v>1</v>
+      </c>
+      <c r="C190" s="46" t="s">
+        <v>370</v>
+      </c>
+      <c r="D190" s="46" t="s">
+        <v>371</v>
+      </c>
+      <c r="E190" s="43" t="b">
         <v>1</v>
       </c>
     </row>
@@ -7153,11 +7310,11 @@
   <mergeCells count="4">
     <mergeCell ref="J3:K3"/>
     <mergeCell ref="M3:P3"/>
-    <mergeCell ref="F54:H54"/>
-    <mergeCell ref="G80:H80"/>
+    <mergeCell ref="F56:H56"/>
+    <mergeCell ref="G84:H84"/>
   </mergeCells>
-  <conditionalFormatting sqref="C82:E84">
-    <cfRule type="duplicateValues" dxfId="68" priority="2"/>
+  <conditionalFormatting sqref="C86:E88">
+    <cfRule type="duplicateValues" dxfId="0" priority="2"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
fly in The beyond need to have an area selected
Former-commit-id: 3793dbe881f2b40c83356cc13b2254fb4b03f90d
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Missions.xlsx
+++ b/Docs/Content/HungryDragonContent_Missions.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="851" uniqueCount="468">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="853" uniqueCount="468">
   <si>
     <t>single_run</t>
   </si>
@@ -3559,8 +3559,8 @@
   </sheetPr>
   <dimension ref="B1:S203"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B65" sqref="B65"/>
+    <sheetView tabSelected="1" topLeftCell="I25" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N52" sqref="N52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5725,7 +5725,9 @@
         <v>370</v>
       </c>
       <c r="M51" s="24"/>
-      <c r="N51" s="24"/>
+      <c r="N51" s="24" t="s">
+        <v>440</v>
+      </c>
       <c r="O51" s="52" t="s">
         <v>372</v>
       </c>
@@ -5763,7 +5765,9 @@
         <v>370</v>
       </c>
       <c r="M52" s="23"/>
-      <c r="N52" s="23"/>
+      <c r="N52" s="23" t="s">
+        <v>440</v>
+      </c>
       <c r="O52" s="53" t="s">
         <v>373</v>
       </c>

</xml_diff>

<commit_message>
Fixing an sku in a mission
Former-commit-id: 3c839a81ba8ee38e0233382e149ad0d0675d8cc1
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Missions.xlsx
+++ b/Docs/Content/HungryDragonContent_Missions.xlsx
@@ -1491,10 +1491,10 @@
     <t>goblinsSpace_zone_beyond</t>
   </si>
   <si>
-    <t>WorkerSpace</t>
-  </si>
-  <si>
     <t>TID_EDIBLE_GOBLIN_ASTRONAUT_PL</t>
+  </si>
+  <si>
+    <t>Worker_Space</t>
   </si>
 </sst>
 </file>
@@ -3588,8 +3588,8 @@
   </sheetPr>
   <dimension ref="B1:S209"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M67" sqref="M67"/>
+    <sheetView tabSelected="1" topLeftCell="D34" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I65" sqref="I65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6352,7 +6352,7 @@
         <v>7</v>
       </c>
       <c r="I65" s="54" t="s">
-        <v>480</v>
+        <v>481</v>
       </c>
       <c r="J65" s="23">
         <v>10</v>
@@ -6364,7 +6364,7 @@
         <v>478</v>
       </c>
       <c r="M65" s="54" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="N65" s="23" t="s">
         <v>440</v>

</xml_diff>

<commit_message>
Adding missions for special dragons
Former-commit-id: 80ec2b092ad698ede4f53bbc9f223404027018c8
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Missions.xlsx
+++ b/Docs/Content/HungryDragonContent_Missions.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="937" uniqueCount="505">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1129" uniqueCount="531">
   <si>
     <t>single_run</t>
   </si>
@@ -1564,6 +1564,84 @@
   </si>
   <si>
     <t>electrify_villagers</t>
+  </si>
+  <si>
+    <t>freeze_dragons</t>
+  </si>
+  <si>
+    <t>shoot_dragons</t>
+  </si>
+  <si>
+    <t>smash_dragons</t>
+  </si>
+  <si>
+    <t>electrify_dragons</t>
+  </si>
+  <si>
+    <t>freeze_spiders</t>
+  </si>
+  <si>
+    <t>shoot_spiders</t>
+  </si>
+  <si>
+    <t>smash_spiders</t>
+  </si>
+  <si>
+    <t>electrify_spiders</t>
+  </si>
+  <si>
+    <t>SpiderSmall;SpiderRed;SpiderGreenTurret</t>
+  </si>
+  <si>
+    <t>TID_EDIBLE_ALL_SPIDER_PL</t>
+  </si>
+  <si>
+    <t>freeze_goblins</t>
+  </si>
+  <si>
+    <t>shoot_goblins</t>
+  </si>
+  <si>
+    <t>smash_goblins</t>
+  </si>
+  <si>
+    <t>electrify_goblins</t>
+  </si>
+  <si>
+    <t>freeze_bats</t>
+  </si>
+  <si>
+    <t>shoot_bats</t>
+  </si>
+  <si>
+    <t>smash_bats</t>
+  </si>
+  <si>
+    <t>electrify_bats</t>
+  </si>
+  <si>
+    <t>freeze_archers</t>
+  </si>
+  <si>
+    <t>shoot_archers</t>
+  </si>
+  <si>
+    <t>smash_archers</t>
+  </si>
+  <si>
+    <t>electrify_archers</t>
+  </si>
+  <si>
+    <t>freeze_fireflies</t>
+  </si>
+  <si>
+    <t>shoot_fireflies</t>
+  </si>
+  <si>
+    <t>smash_fireflies</t>
+  </si>
+  <si>
+    <t>electrify_fireflies</t>
   </si>
 </sst>
 </file>
@@ -2098,18 +2176,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2127,6 +2205,30 @@
       </fill>
     </dxf>
     <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
@@ -2141,30 +2243,6 @@
         <bottom/>
         <vertical/>
         <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
       </border>
     </dxf>
     <dxf>
@@ -3326,8 +3404,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="missionDifficultyDefinitions" displayName="missionDifficultyDefinitions" ref="B106:L109" totalsRowShown="0" headerRowBorderDxfId="70" tableBorderDxfId="69">
-  <autoFilter ref="B106:L109"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="missionDifficultyDefinitions" displayName="missionDifficultyDefinitions" ref="B130:L133" totalsRowShown="0" headerRowBorderDxfId="70" tableBorderDxfId="69">
+  <autoFilter ref="B130:L133"/>
   <tableColumns count="11">
     <tableColumn id="1" name="{missionDifficultyDefinitions}"/>
     <tableColumn id="2" name="[sku]" dataDxfId="68"/>
@@ -3346,8 +3424,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table13303132" displayName="Table13303132" ref="B114:E132" totalsRowShown="0" headerRowDxfId="58" dataDxfId="56" headerRowBorderDxfId="57" tableBorderDxfId="55" totalsRowBorderDxfId="54">
-  <autoFilter ref="B114:E132"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table13303132" displayName="Table13303132" ref="B138:E156" totalsRowShown="0" headerRowDxfId="58" dataDxfId="56" headerRowBorderDxfId="57" tableBorderDxfId="55" totalsRowBorderDxfId="54">
+  <autoFilter ref="B138:E156"/>
   <tableColumns count="4">
     <tableColumn id="1" name="{missionDragonModifiersDefinitions}" dataDxfId="53"/>
     <tableColumn id="2" name="[sku]" dataDxfId="52"/>
@@ -3359,8 +3437,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table1330313234" displayName="Table1330313234" ref="B136:E139" totalsRowShown="0" headerRowDxfId="49" dataDxfId="47" headerRowBorderDxfId="48" tableBorderDxfId="46" totalsRowBorderDxfId="45">
-  <autoFilter ref="B136:E139"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table1330313234" displayName="Table1330313234" ref="B160:E163" totalsRowShown="0" headerRowDxfId="49" dataDxfId="47" headerRowBorderDxfId="48" tableBorderDxfId="46" totalsRowBorderDxfId="45">
+  <autoFilter ref="B160:E163"/>
   <tableColumns count="4">
     <tableColumn id="1" name="{missionDifficultyModifiersDefinitions}" dataDxfId="44"/>
     <tableColumn id="2" name="[sku]" dataDxfId="43"/>
@@ -3372,8 +3450,8 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table133031323435" displayName="Table133031323435" ref="B143:D144" totalsRowShown="0" headerRowDxfId="40" dataDxfId="38" headerRowBorderDxfId="39" tableBorderDxfId="37" totalsRowBorderDxfId="36">
-  <autoFilter ref="B143:D144"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table133031323435" displayName="Table133031323435" ref="B167:D168" totalsRowShown="0" headerRowDxfId="40" dataDxfId="38" headerRowBorderDxfId="39" tableBorderDxfId="37" totalsRowBorderDxfId="36">
+  <autoFilter ref="B167:D168"/>
   <tableColumns count="3">
     <tableColumn id="1" name="{missionOtherModifiersDefinitions}" dataDxfId="35"/>
     <tableColumn id="2" name="[sku]" dataDxfId="34"/>
@@ -3384,8 +3462,8 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table13" displayName="Table13" ref="B74:H102" totalsRowShown="0" headerRowDxfId="32" dataDxfId="30" headerRowBorderDxfId="31" tableBorderDxfId="29" totalsRowBorderDxfId="28">
-  <autoFilter ref="B74:H102"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table13" displayName="Table13" ref="B98:H126" totalsRowShown="0" headerRowDxfId="32" dataDxfId="30" headerRowBorderDxfId="31" tableBorderDxfId="29" totalsRowBorderDxfId="28">
+  <autoFilter ref="B98:H126"/>
   <tableColumns count="7">
     <tableColumn id="1" name="{missionTypeDefinitions}" dataDxfId="27"/>
     <tableColumn id="2" name="[sku]" dataDxfId="26"/>
@@ -3400,8 +3478,8 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table1330" displayName="Table1330" ref="B4:P69" totalsRowShown="0" headerRowDxfId="20" dataDxfId="18" headerRowBorderDxfId="19" tableBorderDxfId="17" totalsRowBorderDxfId="16">
-  <autoFilter ref="B4:P69"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table1330" displayName="Table1330" ref="B4:P93" totalsRowShown="0" headerRowDxfId="20" dataDxfId="18" headerRowBorderDxfId="19" tableBorderDxfId="17" totalsRowBorderDxfId="16">
+  <autoFilter ref="B4:P93"/>
   <sortState ref="B5:P43">
     <sortCondition descending="1" ref="J4:J43"/>
   </sortState>
@@ -3419,8 +3497,8 @@
     <tableColumn id="4" name="[icon]" dataDxfId="5"/>
     <tableColumn id="5" name="[tidObjective]" dataDxfId="4"/>
     <tableColumn id="14" name="[zone]" dataDxfId="3"/>
-    <tableColumn id="15" name="[dragon]" dataDxfId="1"/>
-    <tableColumn id="10" name="[trackingSku]" dataDxfId="2"/>
+    <tableColumn id="15" name="[dragon]" dataDxfId="2"/>
+    <tableColumn id="10" name="[trackingSku]" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3692,10 +3770,10 @@
   <sheetPr>
     <tabColor theme="6"/>
   </sheetPr>
-  <dimension ref="B1:T220"/>
+  <dimension ref="B1:T244"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O6" sqref="O6"/>
+    <sheetView tabSelected="1" topLeftCell="J55" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="P94" sqref="P94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3746,16 +3824,16 @@
         <v>139</v>
       </c>
       <c r="G3" s="38"/>
-      <c r="J3" s="69" t="s">
+      <c r="J3" s="71" t="s">
         <v>138</v>
       </c>
-      <c r="K3" s="69"/>
-      <c r="M3" s="69"/>
-      <c r="N3" s="69"/>
-      <c r="O3" s="69"/>
-      <c r="P3" s="69"/>
-      <c r="Q3" s="69"/>
-      <c r="R3" s="69"/>
+      <c r="K3" s="71"/>
+      <c r="M3" s="71"/>
+      <c r="N3" s="71"/>
+      <c r="O3" s="71"/>
+      <c r="P3" s="71"/>
+      <c r="Q3" s="71"/>
+      <c r="R3" s="71"/>
       <c r="S3" s="63"/>
     </row>
     <row r="4" spans="2:20" ht="107.25" x14ac:dyDescent="0.25">
@@ -6551,28 +6629,28 @@
       <c r="C66" s="60" t="s">
         <v>501</v>
       </c>
-      <c r="D66" s="72" t="s">
+      <c r="D66" s="69" t="s">
         <v>489</v>
       </c>
-      <c r="E66" s="72">
-        <v>1</v>
-      </c>
-      <c r="F66" s="72">
+      <c r="E66" s="69">
+        <v>1</v>
+      </c>
+      <c r="F66" s="69">
         <v>0.3</v>
       </c>
       <c r="G66" s="60">
         <v>6</v>
       </c>
-      <c r="H66" s="72">
+      <c r="H66" s="69">
         <v>6</v>
       </c>
-      <c r="I66" s="73" t="s">
+      <c r="I66" s="70" t="s">
         <v>325</v>
       </c>
       <c r="J66" s="60">
         <v>10</v>
       </c>
-      <c r="K66" s="72">
+      <c r="K66" s="69">
         <v>20</v>
       </c>
       <c r="L66" s="60" t="s">
@@ -6582,7 +6660,7 @@
         <v>148</v>
       </c>
       <c r="N66" s="60"/>
-      <c r="O66" s="72" t="s">
+      <c r="O66" s="69" t="s">
         <v>337</v>
       </c>
       <c r="P66" s="61" t="s">
@@ -6725,1690 +6803,2434 @@
       </c>
     </row>
     <row r="70" spans="2:16" s="40" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B70" s="41"/>
-      <c r="C70" s="41"/>
-      <c r="D70" s="41"/>
-      <c r="E70" s="41"/>
-      <c r="F70" s="41"/>
-      <c r="G70" s="41"/>
-      <c r="H70" s="41"/>
-      <c r="I70" s="41"/>
-      <c r="J70" s="41"/>
-      <c r="K70" s="41"/>
-      <c r="L70" s="41"/>
-      <c r="M70" s="41"/>
-      <c r="N70" s="41"/>
-      <c r="O70" s="41"/>
-      <c r="P70" s="41"/>
-    </row>
-    <row r="71" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B71" s="32"/>
-      <c r="C71" s="32"/>
-      <c r="D71" s="32"/>
-      <c r="E71" s="32"/>
-      <c r="F71" s="32"/>
-      <c r="G71" s="32"/>
-      <c r="H71" s="32"/>
-      <c r="I71" s="32"/>
-      <c r="J71" s="32"/>
-      <c r="K71" s="32"/>
-      <c r="L71" s="32"/>
-      <c r="M71" s="31"/>
-      <c r="N71" s="31"/>
-      <c r="O71" s="31"/>
-    </row>
-    <row r="72" spans="2:16" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B72" s="6" t="s">
+      <c r="B70" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="C70" s="23" t="s">
+        <v>505</v>
+      </c>
+      <c r="D70" s="23" t="s">
+        <v>489</v>
+      </c>
+      <c r="E70" s="23">
+        <v>1</v>
+      </c>
+      <c r="F70" s="23">
+        <v>0.3</v>
+      </c>
+      <c r="G70" s="23">
+        <v>6</v>
+      </c>
+      <c r="H70" s="23">
+        <v>6</v>
+      </c>
+      <c r="I70" s="23" t="s">
+        <v>304</v>
+      </c>
+      <c r="J70" s="23">
+        <v>10</v>
+      </c>
+      <c r="K70" s="23">
+        <v>11</v>
+      </c>
+      <c r="L70" s="23" t="s">
+        <v>111</v>
+      </c>
+      <c r="M70" s="23" t="s">
+        <v>153</v>
+      </c>
+      <c r="N70" s="23"/>
+      <c r="O70" s="23" t="s">
+        <v>337</v>
+      </c>
+      <c r="P70" s="53" t="s">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="71" spans="2:16" s="40" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B71" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="C71" s="23" t="s">
+        <v>506</v>
+      </c>
+      <c r="D71" s="23" t="s">
+        <v>490</v>
+      </c>
+      <c r="E71" s="23">
+        <v>1</v>
+      </c>
+      <c r="F71" s="23">
+        <v>0.3</v>
+      </c>
+      <c r="G71" s="23">
+        <v>6</v>
+      </c>
+      <c r="H71" s="23">
+        <v>6</v>
+      </c>
+      <c r="I71" s="23" t="s">
+        <v>304</v>
+      </c>
+      <c r="J71" s="23">
+        <v>10</v>
+      </c>
+      <c r="K71" s="23">
+        <v>11</v>
+      </c>
+      <c r="L71" s="23" t="s">
+        <v>111</v>
+      </c>
+      <c r="M71" s="23" t="s">
+        <v>153</v>
+      </c>
+      <c r="N71" s="23"/>
+      <c r="O71" s="23" t="s">
+        <v>335</v>
+      </c>
+      <c r="P71" s="53" t="s">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="72" spans="2:16" s="40" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B72" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="C72" s="23" t="s">
+        <v>507</v>
+      </c>
+      <c r="D72" s="23" t="s">
+        <v>491</v>
+      </c>
+      <c r="E72" s="23">
+        <v>1</v>
+      </c>
+      <c r="F72" s="23">
+        <v>0.3</v>
+      </c>
+      <c r="G72" s="23">
+        <v>6</v>
+      </c>
+      <c r="H72" s="23">
+        <v>6</v>
+      </c>
+      <c r="I72" s="23" t="s">
+        <v>304</v>
+      </c>
+      <c r="J72" s="23">
+        <v>10</v>
+      </c>
+      <c r="K72" s="23">
+        <v>11</v>
+      </c>
+      <c r="L72" s="23" t="s">
+        <v>111</v>
+      </c>
+      <c r="M72" s="23" t="s">
+        <v>153</v>
+      </c>
+      <c r="N72" s="23"/>
+      <c r="O72" s="23" t="s">
+        <v>336</v>
+      </c>
+      <c r="P72" s="53" t="s">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="73" spans="2:16" s="40" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B73" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="C73" s="23" t="s">
+        <v>508</v>
+      </c>
+      <c r="D73" s="23" t="s">
+        <v>492</v>
+      </c>
+      <c r="E73" s="23">
+        <v>1</v>
+      </c>
+      <c r="F73" s="23">
+        <v>0.3</v>
+      </c>
+      <c r="G73" s="23">
+        <v>6</v>
+      </c>
+      <c r="H73" s="23">
+        <v>6</v>
+      </c>
+      <c r="I73" s="23" t="s">
+        <v>304</v>
+      </c>
+      <c r="J73" s="23">
+        <v>10</v>
+      </c>
+      <c r="K73" s="23">
+        <v>11</v>
+      </c>
+      <c r="L73" s="23" t="s">
+        <v>111</v>
+      </c>
+      <c r="M73" s="23" t="s">
+        <v>153</v>
+      </c>
+      <c r="N73" s="23"/>
+      <c r="O73" s="23" t="s">
+        <v>334</v>
+      </c>
+      <c r="P73" s="53" t="s">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="74" spans="2:16" s="40" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B74" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="C74" s="23" t="s">
+        <v>509</v>
+      </c>
+      <c r="D74" s="23" t="s">
+        <v>489</v>
+      </c>
+      <c r="E74" s="23">
+        <v>1</v>
+      </c>
+      <c r="F74" s="23">
+        <v>0.3</v>
+      </c>
+      <c r="G74" s="23">
+        <v>6</v>
+      </c>
+      <c r="H74" s="23">
+        <v>6</v>
+      </c>
+      <c r="I74" s="23" t="s">
+        <v>513</v>
+      </c>
+      <c r="J74" s="23">
+        <v>45</v>
+      </c>
+      <c r="K74" s="23">
+        <v>55</v>
+      </c>
+      <c r="L74" s="23" t="s">
+        <v>105</v>
+      </c>
+      <c r="M74" s="23" t="s">
+        <v>514</v>
+      </c>
+      <c r="N74" s="23"/>
+      <c r="O74" s="23" t="s">
+        <v>337</v>
+      </c>
+      <c r="P74" s="53" t="s">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="75" spans="2:16" s="40" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B75" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="C75" s="23" t="s">
+        <v>510</v>
+      </c>
+      <c r="D75" s="23" t="s">
+        <v>490</v>
+      </c>
+      <c r="E75" s="23">
+        <v>1</v>
+      </c>
+      <c r="F75" s="23">
+        <v>0.3</v>
+      </c>
+      <c r="G75" s="23">
+        <v>6</v>
+      </c>
+      <c r="H75" s="23">
+        <v>6</v>
+      </c>
+      <c r="I75" s="23" t="s">
+        <v>513</v>
+      </c>
+      <c r="J75" s="23">
+        <v>45</v>
+      </c>
+      <c r="K75" s="23">
+        <v>55</v>
+      </c>
+      <c r="L75" s="23" t="s">
+        <v>105</v>
+      </c>
+      <c r="M75" s="23" t="s">
+        <v>514</v>
+      </c>
+      <c r="N75" s="23"/>
+      <c r="O75" s="23" t="s">
+        <v>335</v>
+      </c>
+      <c r="P75" s="53" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="76" spans="2:16" s="40" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B76" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="C76" s="23" t="s">
+        <v>511</v>
+      </c>
+      <c r="D76" s="23" t="s">
+        <v>491</v>
+      </c>
+      <c r="E76" s="23">
+        <v>1</v>
+      </c>
+      <c r="F76" s="23">
+        <v>0.3</v>
+      </c>
+      <c r="G76" s="23">
+        <v>6</v>
+      </c>
+      <c r="H76" s="23">
+        <v>6</v>
+      </c>
+      <c r="I76" s="23" t="s">
+        <v>513</v>
+      </c>
+      <c r="J76" s="23">
+        <v>45</v>
+      </c>
+      <c r="K76" s="23">
+        <v>55</v>
+      </c>
+      <c r="L76" s="23" t="s">
+        <v>105</v>
+      </c>
+      <c r="M76" s="23" t="s">
+        <v>514</v>
+      </c>
+      <c r="N76" s="23"/>
+      <c r="O76" s="23" t="s">
+        <v>336</v>
+      </c>
+      <c r="P76" s="53" t="s">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="77" spans="2:16" s="40" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B77" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="C77" s="23" t="s">
+        <v>512</v>
+      </c>
+      <c r="D77" s="23" t="s">
+        <v>492</v>
+      </c>
+      <c r="E77" s="23">
+        <v>1</v>
+      </c>
+      <c r="F77" s="23">
+        <v>0.3</v>
+      </c>
+      <c r="G77" s="23">
+        <v>6</v>
+      </c>
+      <c r="H77" s="23">
+        <v>6</v>
+      </c>
+      <c r="I77" s="23" t="s">
+        <v>513</v>
+      </c>
+      <c r="J77" s="23">
+        <v>45</v>
+      </c>
+      <c r="K77" s="23">
+        <v>55</v>
+      </c>
+      <c r="L77" s="23" t="s">
+        <v>105</v>
+      </c>
+      <c r="M77" s="23" t="s">
+        <v>514</v>
+      </c>
+      <c r="N77" s="23"/>
+      <c r="O77" s="23" t="s">
+        <v>334</v>
+      </c>
+      <c r="P77" s="53" t="s">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="78" spans="2:16" s="40" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B78" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="C78" s="23" t="s">
+        <v>515</v>
+      </c>
+      <c r="D78" s="23" t="s">
+        <v>489</v>
+      </c>
+      <c r="E78" s="23">
+        <v>1</v>
+      </c>
+      <c r="F78" s="23">
+        <v>0.3</v>
+      </c>
+      <c r="G78" s="23">
+        <v>6</v>
+      </c>
+      <c r="H78" s="23">
+        <v>6</v>
+      </c>
+      <c r="I78" s="23" t="s">
+        <v>103</v>
+      </c>
+      <c r="J78" s="23">
+        <v>40</v>
+      </c>
+      <c r="K78" s="23">
+        <v>45</v>
+      </c>
+      <c r="L78" s="23" t="s">
+        <v>102</v>
+      </c>
+      <c r="M78" s="23" t="s">
+        <v>154</v>
+      </c>
+      <c r="N78" s="23"/>
+      <c r="O78" s="23" t="s">
+        <v>337</v>
+      </c>
+      <c r="P78" s="53" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="79" spans="2:16" s="40" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B79" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="C79" s="23" t="s">
+        <v>516</v>
+      </c>
+      <c r="D79" s="23" t="s">
+        <v>490</v>
+      </c>
+      <c r="E79" s="23">
+        <v>1</v>
+      </c>
+      <c r="F79" s="23">
+        <v>0.3</v>
+      </c>
+      <c r="G79" s="23">
+        <v>6</v>
+      </c>
+      <c r="H79" s="23">
+        <v>6</v>
+      </c>
+      <c r="I79" s="23" t="s">
+        <v>103</v>
+      </c>
+      <c r="J79" s="23">
+        <v>40</v>
+      </c>
+      <c r="K79" s="23">
+        <v>45</v>
+      </c>
+      <c r="L79" s="23" t="s">
+        <v>102</v>
+      </c>
+      <c r="M79" s="23" t="s">
+        <v>154</v>
+      </c>
+      <c r="N79" s="23"/>
+      <c r="O79" s="23" t="s">
+        <v>335</v>
+      </c>
+      <c r="P79" s="53" t="s">
+        <v>516</v>
+      </c>
+    </row>
+    <row r="80" spans="2:16" s="40" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B80" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="C80" s="23" t="s">
+        <v>517</v>
+      </c>
+      <c r="D80" s="23" t="s">
+        <v>491</v>
+      </c>
+      <c r="E80" s="23">
+        <v>1</v>
+      </c>
+      <c r="F80" s="23">
+        <v>0.3</v>
+      </c>
+      <c r="G80" s="23">
+        <v>6</v>
+      </c>
+      <c r="H80" s="23">
+        <v>6</v>
+      </c>
+      <c r="I80" s="23" t="s">
+        <v>103</v>
+      </c>
+      <c r="J80" s="23">
+        <v>40</v>
+      </c>
+      <c r="K80" s="23">
+        <v>45</v>
+      </c>
+      <c r="L80" s="23" t="s">
+        <v>102</v>
+      </c>
+      <c r="M80" s="23" t="s">
+        <v>154</v>
+      </c>
+      <c r="N80" s="23"/>
+      <c r="O80" s="23" t="s">
+        <v>336</v>
+      </c>
+      <c r="P80" s="53" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="81" spans="2:16" s="40" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B81" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="C81" s="23" t="s">
+        <v>518</v>
+      </c>
+      <c r="D81" s="23" t="s">
+        <v>492</v>
+      </c>
+      <c r="E81" s="23">
+        <v>1</v>
+      </c>
+      <c r="F81" s="23">
+        <v>0.3</v>
+      </c>
+      <c r="G81" s="23">
+        <v>6</v>
+      </c>
+      <c r="H81" s="23">
+        <v>6</v>
+      </c>
+      <c r="I81" s="23" t="s">
+        <v>103</v>
+      </c>
+      <c r="J81" s="23">
+        <v>40</v>
+      </c>
+      <c r="K81" s="23">
+        <v>45</v>
+      </c>
+      <c r="L81" s="23" t="s">
+        <v>102</v>
+      </c>
+      <c r="M81" s="23" t="s">
+        <v>154</v>
+      </c>
+      <c r="N81" s="23"/>
+      <c r="O81" s="23" t="s">
+        <v>334</v>
+      </c>
+      <c r="P81" s="53" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="82" spans="2:16" s="40" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B82" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="C82" s="23" t="s">
+        <v>519</v>
+      </c>
+      <c r="D82" s="23" t="s">
+        <v>489</v>
+      </c>
+      <c r="E82" s="23">
+        <v>1</v>
+      </c>
+      <c r="F82" s="23">
+        <v>0.3</v>
+      </c>
+      <c r="G82" s="23">
+        <v>6</v>
+      </c>
+      <c r="H82" s="23">
+        <v>6</v>
+      </c>
+      <c r="I82" s="23" t="s">
+        <v>94</v>
+      </c>
+      <c r="J82" s="23">
+        <v>150</v>
+      </c>
+      <c r="K82" s="23">
+        <v>200</v>
+      </c>
+      <c r="L82" s="23" t="s">
+        <v>93</v>
+      </c>
+      <c r="M82" s="23" t="s">
+        <v>157</v>
+      </c>
+      <c r="N82" s="23"/>
+      <c r="O82" s="23" t="s">
+        <v>337</v>
+      </c>
+      <c r="P82" s="53" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="83" spans="2:16" s="40" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B83" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="C83" s="23" t="s">
+        <v>520</v>
+      </c>
+      <c r="D83" s="23" t="s">
+        <v>490</v>
+      </c>
+      <c r="E83" s="23">
+        <v>1</v>
+      </c>
+      <c r="F83" s="23">
+        <v>0.3</v>
+      </c>
+      <c r="G83" s="23">
+        <v>6</v>
+      </c>
+      <c r="H83" s="23">
+        <v>6</v>
+      </c>
+      <c r="I83" s="23" t="s">
+        <v>94</v>
+      </c>
+      <c r="J83" s="23">
+        <v>150</v>
+      </c>
+      <c r="K83" s="23">
+        <v>200</v>
+      </c>
+      <c r="L83" s="23" t="s">
+        <v>93</v>
+      </c>
+      <c r="M83" s="23" t="s">
+        <v>157</v>
+      </c>
+      <c r="N83" s="23"/>
+      <c r="O83" s="23" t="s">
+        <v>335</v>
+      </c>
+      <c r="P83" s="53" t="s">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="84" spans="2:16" s="40" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B84" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="C84" s="23" t="s">
+        <v>521</v>
+      </c>
+      <c r="D84" s="23" t="s">
+        <v>491</v>
+      </c>
+      <c r="E84" s="23">
+        <v>1</v>
+      </c>
+      <c r="F84" s="23">
+        <v>0.3</v>
+      </c>
+      <c r="G84" s="23">
+        <v>6</v>
+      </c>
+      <c r="H84" s="23">
+        <v>6</v>
+      </c>
+      <c r="I84" s="23" t="s">
+        <v>94</v>
+      </c>
+      <c r="J84" s="23">
+        <v>150</v>
+      </c>
+      <c r="K84" s="23">
+        <v>200</v>
+      </c>
+      <c r="L84" s="23" t="s">
+        <v>93</v>
+      </c>
+      <c r="M84" s="23" t="s">
+        <v>157</v>
+      </c>
+      <c r="N84" s="23"/>
+      <c r="O84" s="23" t="s">
+        <v>336</v>
+      </c>
+      <c r="P84" s="53" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="85" spans="2:16" s="40" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B85" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="C85" s="23" t="s">
+        <v>522</v>
+      </c>
+      <c r="D85" s="23" t="s">
+        <v>492</v>
+      </c>
+      <c r="E85" s="23">
+        <v>1</v>
+      </c>
+      <c r="F85" s="23">
+        <v>0.3</v>
+      </c>
+      <c r="G85" s="23">
+        <v>6</v>
+      </c>
+      <c r="H85" s="23">
+        <v>6</v>
+      </c>
+      <c r="I85" s="23" t="s">
+        <v>94</v>
+      </c>
+      <c r="J85" s="23">
+        <v>150</v>
+      </c>
+      <c r="K85" s="23">
+        <v>200</v>
+      </c>
+      <c r="L85" s="23" t="s">
+        <v>93</v>
+      </c>
+      <c r="M85" s="23" t="s">
+        <v>157</v>
+      </c>
+      <c r="N85" s="23"/>
+      <c r="O85" s="23" t="s">
+        <v>334</v>
+      </c>
+      <c r="P85" s="53" t="s">
+        <v>522</v>
+      </c>
+    </row>
+    <row r="86" spans="2:16" s="40" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B86" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="C86" s="23" t="s">
+        <v>523</v>
+      </c>
+      <c r="D86" s="23" t="s">
+        <v>489</v>
+      </c>
+      <c r="E86" s="23">
+        <v>1</v>
+      </c>
+      <c r="F86" s="23">
+        <v>0.3</v>
+      </c>
+      <c r="G86" s="23">
+        <v>6</v>
+      </c>
+      <c r="H86" s="23">
+        <v>6</v>
+      </c>
+      <c r="I86" s="23" t="s">
+        <v>81</v>
+      </c>
+      <c r="J86" s="23">
+        <v>8</v>
+      </c>
+      <c r="K86" s="23">
+        <v>9</v>
+      </c>
+      <c r="L86" s="23" t="s">
+        <v>80</v>
+      </c>
+      <c r="M86" s="23" t="s">
+        <v>161</v>
+      </c>
+      <c r="N86" s="23"/>
+      <c r="O86" s="23" t="s">
+        <v>337</v>
+      </c>
+      <c r="P86" s="53" t="s">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="87" spans="2:16" s="40" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B87" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="C87" s="23" t="s">
+        <v>524</v>
+      </c>
+      <c r="D87" s="23" t="s">
+        <v>490</v>
+      </c>
+      <c r="E87" s="23">
+        <v>1</v>
+      </c>
+      <c r="F87" s="23">
+        <v>0.3</v>
+      </c>
+      <c r="G87" s="23">
+        <v>6</v>
+      </c>
+      <c r="H87" s="23">
+        <v>6</v>
+      </c>
+      <c r="I87" s="23" t="s">
+        <v>81</v>
+      </c>
+      <c r="J87" s="23">
+        <v>8</v>
+      </c>
+      <c r="K87" s="23">
+        <v>9</v>
+      </c>
+      <c r="L87" s="23" t="s">
+        <v>80</v>
+      </c>
+      <c r="M87" s="23" t="s">
+        <v>161</v>
+      </c>
+      <c r="N87" s="23"/>
+      <c r="O87" s="23" t="s">
+        <v>335</v>
+      </c>
+      <c r="P87" s="53" t="s">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="88" spans="2:16" s="40" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B88" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="C88" s="23" t="s">
+        <v>525</v>
+      </c>
+      <c r="D88" s="23" t="s">
+        <v>491</v>
+      </c>
+      <c r="E88" s="23">
+        <v>1</v>
+      </c>
+      <c r="F88" s="23">
+        <v>0.3</v>
+      </c>
+      <c r="G88" s="23">
+        <v>6</v>
+      </c>
+      <c r="H88" s="23">
+        <v>6</v>
+      </c>
+      <c r="I88" s="23" t="s">
+        <v>81</v>
+      </c>
+      <c r="J88" s="23">
+        <v>8</v>
+      </c>
+      <c r="K88" s="23">
+        <v>9</v>
+      </c>
+      <c r="L88" s="23" t="s">
+        <v>80</v>
+      </c>
+      <c r="M88" s="23" t="s">
+        <v>161</v>
+      </c>
+      <c r="N88" s="23"/>
+      <c r="O88" s="23" t="s">
+        <v>336</v>
+      </c>
+      <c r="